<commit_message>
add datasets and links
</commit_message>
<xml_diff>
--- a/PolData.xlsx
+++ b/PolData.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="65">
   <si>
     <t>name</t>
   </si>
@@ -150,16 +150,96 @@
   </si>
   <si>
     <t>http://www.worldvaluessurvey.org/wvs.jsp</t>
+  </si>
+  <si>
+    <t>Correlates of War</t>
+  </si>
+  <si>
+    <t>international relations</t>
+  </si>
+  <si>
+    <t>http://www.correlatesofwar.org/</t>
+  </si>
+  <si>
+    <t>Political attitudes</t>
+  </si>
+  <si>
+    <t>http://www.electionstudies.org/</t>
+  </si>
+  <si>
+    <t>cross-sectional, panel</t>
+  </si>
+  <si>
+    <t>http://www.vanderbilt.edu/lapop/about-americasbarometer.php</t>
+  </si>
+  <si>
+    <t>http://www.asianbarometer.org/</t>
+  </si>
+  <si>
+    <t>http://www.cses.org/</t>
+  </si>
+  <si>
+    <t>http://ec.europa.eu/commfrontoffice/publicopinion/index.cfm</t>
+  </si>
+  <si>
+    <t>https://www.eurofound.europa.eu/surveys/european-quality-of-life-surveys</t>
+  </si>
+  <si>
+    <t>http://www.afrobarometer.org/</t>
+  </si>
+  <si>
+    <t>http://caucasusbarometer.org/en/datasets/</t>
+  </si>
+  <si>
+    <t>http://www.europeanvaluesstudy.eu/</t>
+  </si>
+  <si>
+    <t>http://www.issp.org/menu-top/home/</t>
+  </si>
+  <si>
+    <t>Comparative Political Data Set</t>
+  </si>
+  <si>
+    <t>political institutions</t>
+  </si>
+  <si>
+    <t>http://www.cpds-data.org/</t>
+  </si>
+  <si>
+    <t>Parties, Governments and Legislatures Dataset</t>
+  </si>
+  <si>
+    <t>governments and parties</t>
+  </si>
+  <si>
+    <t>http://www.edac.eu/policies_desc.cfm?v_id=112</t>
+  </si>
+  <si>
+    <t>Democratic Accountability and Citizen-Politician Linkages</t>
+  </si>
+  <si>
+    <t>democracy</t>
+  </si>
+  <si>
+    <t>https://sites.duke.edu/democracylinkage/data/</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -182,16 +262,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -467,10 +550,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J15"/>
+  <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -525,6 +608,9 @@
       <c r="B2" t="s">
         <v>26</v>
       </c>
+      <c r="C2" s="2" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
@@ -533,8 +619,23 @@
       <c r="B3" t="s">
         <v>26</v>
       </c>
+      <c r="C3" s="2" t="s">
+        <v>45</v>
+      </c>
       <c r="E3" t="s">
         <v>35</v>
+      </c>
+      <c r="F3">
+        <v>1948</v>
+      </c>
+      <c r="H3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I3" t="s">
+        <v>21</v>
+      </c>
+      <c r="J3" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
@@ -544,6 +645,9 @@
       <c r="B4" t="s">
         <v>26</v>
       </c>
+      <c r="C4" s="2" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
@@ -552,6 +656,9 @@
       <c r="B5" t="s">
         <v>26</v>
       </c>
+      <c r="C5" s="2" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
@@ -560,164 +667,264 @@
       <c r="B6" t="s">
         <v>26</v>
       </c>
+      <c r="C6" s="2" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
+      <c r="A7" t="s">
+        <v>56</v>
+      </c>
+      <c r="B7" t="s">
+        <v>57</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B7" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>29</v>
-      </c>
       <c r="B8" t="s">
         <v>26</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="B9" t="s">
-        <v>26</v>
+        <v>42</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E9" t="s">
+        <v>15</v>
+      </c>
+      <c r="F9">
+        <v>1816</v>
+      </c>
+      <c r="G9">
+        <v>2007</v>
+      </c>
+      <c r="H9" t="s">
+        <v>17</v>
+      </c>
+      <c r="I9" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>5</v>
+        <v>62</v>
       </c>
       <c r="B10" t="s">
-        <v>26</v>
-      </c>
-      <c r="C10" t="s">
-        <v>6</v>
-      </c>
-      <c r="D10" t="s">
-        <v>7</v>
-      </c>
-      <c r="E10" t="s">
-        <v>10</v>
-      </c>
-      <c r="F10">
-        <v>2002</v>
-      </c>
-      <c r="H10" t="s">
-        <v>17</v>
-      </c>
-      <c r="I10" t="s">
-        <v>21</v>
-      </c>
-      <c r="J10" t="s">
-        <v>18</v>
+        <v>63</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A11" s="1" t="s">
-        <v>27</v>
+      <c r="A11" t="s">
+        <v>29</v>
       </c>
       <c r="B11" t="s">
         <v>26</v>
       </c>
+      <c r="C11" s="2" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A12" s="1" t="s">
-        <v>24</v>
+      <c r="A12" t="s">
+        <v>28</v>
       </c>
       <c r="B12" t="s">
         <v>26</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="B13" t="s">
         <v>26</v>
       </c>
-      <c r="C13" t="s">
-        <v>13</v>
+      <c r="C13" s="2" t="s">
+        <v>6</v>
       </c>
       <c r="D13" t="s">
-        <v>39</v>
+        <v>7</v>
       </c>
       <c r="E13" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F13">
-        <v>2007</v>
+        <v>2002</v>
       </c>
       <c r="H13" t="s">
         <v>17</v>
       </c>
       <c r="I13" t="s">
+        <v>21</v>
+      </c>
+      <c r="J13" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" t="s">
+        <v>26</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B15" t="s">
+        <v>26</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>12</v>
+      </c>
+      <c r="B16" t="s">
+        <v>26</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D16" t="s">
+        <v>39</v>
+      </c>
+      <c r="E16" t="s">
+        <v>11</v>
+      </c>
+      <c r="F16">
+        <v>2007</v>
+      </c>
+      <c r="H16" t="s">
+        <v>17</v>
+      </c>
+      <c r="I16" t="s">
         <v>22</v>
       </c>
-      <c r="J13" t="s">
+      <c r="J16" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>59</v>
+      </c>
+      <c r="B17" t="s">
+        <v>60</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
         <v>36</v>
       </c>
-      <c r="B14" t="s">
-        <v>26</v>
-      </c>
-      <c r="C14" t="s">
+      <c r="B18" t="s">
+        <v>26</v>
+      </c>
+      <c r="C18" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D18" t="s">
         <v>38</v>
       </c>
-      <c r="E14" t="s">
+      <c r="E18" t="s">
         <v>15</v>
       </c>
-      <c r="F14">
+      <c r="F18">
         <v>2001</v>
       </c>
-      <c r="H14" t="s">
+      <c r="H18" t="s">
         <v>17</v>
       </c>
-      <c r="I14" t="s">
+      <c r="I18" t="s">
         <v>21</v>
       </c>
-      <c r="J14" t="s">
+      <c r="J18" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
         <v>14</v>
       </c>
-      <c r="B15" t="s">
-        <v>26</v>
-      </c>
-      <c r="C15" t="s">
+      <c r="B19" t="s">
+        <v>26</v>
+      </c>
+      <c r="C19" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="E15" t="s">
+      <c r="D19" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E19" t="s">
         <v>15</v>
       </c>
-      <c r="F15">
+      <c r="F19">
         <v>1981</v>
       </c>
-      <c r="H15" t="s">
+      <c r="H19" t="s">
         <v>17</v>
       </c>
-      <c r="I15" t="s">
+      <c r="I19" t="s">
         <v>21</v>
       </c>
-      <c r="J15" t="s">
+      <c r="J19" t="s">
         <v>18</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:J15">
+  <sortState ref="A2:J19">
     <sortCondition ref="A2"/>
   </sortState>
+  <hyperlinks>
+    <hyperlink ref="C3" r:id="rId1"/>
+    <hyperlink ref="C13" r:id="rId2"/>
+    <hyperlink ref="C4" r:id="rId3"/>
+    <hyperlink ref="C5" r:id="rId4"/>
+    <hyperlink ref="C16" r:id="rId5"/>
+    <hyperlink ref="C18" r:id="rId6"/>
+    <hyperlink ref="C19" r:id="rId7"/>
+    <hyperlink ref="C9" r:id="rId8"/>
+    <hyperlink ref="C8" r:id="rId9"/>
+    <hyperlink ref="C11" r:id="rId10"/>
+    <hyperlink ref="C12" r:id="rId11"/>
+    <hyperlink ref="C2" r:id="rId12"/>
+    <hyperlink ref="C6" r:id="rId13"/>
+    <hyperlink ref="C14" r:id="rId14"/>
+    <hyperlink ref="C15" r:id="rId15"/>
+    <hyperlink ref="C7" r:id="rId16"/>
+    <hyperlink ref="C17" r:id="rId17"/>
+    <hyperlink ref="C10" r:id="rId18"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add an extra batch of datasets
</commit_message>
<xml_diff>
--- a/PolData.xlsx
+++ b/PolData.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="98">
   <si>
     <t>name</t>
   </si>
@@ -222,6 +222,105 @@
   </si>
   <si>
     <t>https://sites.duke.edu/democracylinkage/data/</t>
+  </si>
+  <si>
+    <t>German Socio-Economic Panel</t>
+  </si>
+  <si>
+    <t>https://www.eui.eu/Research/Library/ResearchGuides/Economics/Statistics/DataPortal/GSOEP</t>
+  </si>
+  <si>
+    <t>British Household Panel Survey</t>
+  </si>
+  <si>
+    <t>https://www.iser.essex.ac.uk/bhps</t>
+  </si>
+  <si>
+    <t>Understanding Society</t>
+  </si>
+  <si>
+    <t>https://www.understandingsociety.ac.uk/documentation/mainstage</t>
+  </si>
+  <si>
+    <t>Africa</t>
+  </si>
+  <si>
+    <t>Latin America</t>
+  </si>
+  <si>
+    <t>Arab Barometer</t>
+  </si>
+  <si>
+    <t>http://arabbarometer.org/</t>
+  </si>
+  <si>
+    <t>Middle East</t>
+  </si>
+  <si>
+    <t>Asia</t>
+  </si>
+  <si>
+    <t>Caucasus</t>
+  </si>
+  <si>
+    <t>Danish National Election Study</t>
+  </si>
+  <si>
+    <t>http://www.valgprojektet.dk/default.asp?l=eng</t>
+  </si>
+  <si>
+    <t>Denmark</t>
+  </si>
+  <si>
+    <t>European Election Studies: Voter Study</t>
+  </si>
+  <si>
+    <t>http://europeanelectionstudies.net/ees-study-components/voter-study/</t>
+  </si>
+  <si>
+    <t>Euromanifesto</t>
+  </si>
+  <si>
+    <t>http://europeanelectionstudies.net/ees-study-components/euromanifesto-study/</t>
+  </si>
+  <si>
+    <t>European Election Study: Elite Study</t>
+  </si>
+  <si>
+    <t>political elites</t>
+  </si>
+  <si>
+    <t>http://europeanelectionstudies.net/ees-study-components/elite-study/</t>
+  </si>
+  <si>
+    <t>European Election Study: Media Study</t>
+  </si>
+  <si>
+    <t>media</t>
+  </si>
+  <si>
+    <t>http://europeanelectionstudies.net/ees-study-components/media-study/</t>
+  </si>
+  <si>
+    <t>http://gss.norc.org/</t>
+  </si>
+  <si>
+    <t>General Social Survey​</t>
+  </si>
+  <si>
+    <t>Latinobarómetro</t>
+  </si>
+  <si>
+    <t>http://www.latinobarometro.org/lat.jsp</t>
+  </si>
+  <si>
+    <t>Swiss Household Panel</t>
+  </si>
+  <si>
+    <t>Switzerland</t>
+  </si>
+  <si>
+    <t>http://forscenter.ch/en/our-surveys/swiss-household-panel/</t>
   </si>
 </sst>
 </file>
@@ -266,12 +365,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -550,15 +652,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J19"/>
+  <dimension ref="A1:J31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="33" customWidth="1"/>
+    <col min="1" max="1" width="56.1640625" customWidth="1"/>
     <col min="2" max="2" width="24.33203125" customWidth="1"/>
     <col min="3" max="3" width="33.1640625" customWidth="1"/>
     <col min="4" max="4" width="22.5" customWidth="1"/>
@@ -611,6 +713,12 @@
       <c r="C2" s="2" t="s">
         <v>52</v>
       </c>
+      <c r="E2" t="s">
+        <v>71</v>
+      </c>
+      <c r="F2">
+        <v>1999</v>
+      </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
@@ -648,282 +756,525 @@
       <c r="C4" s="2" t="s">
         <v>47</v>
       </c>
+      <c r="E4" t="s">
+        <v>72</v>
+      </c>
+      <c r="F4">
+        <v>2004</v>
+      </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>32</v>
+        <v>73</v>
       </c>
       <c r="B5" t="s">
         <v>26</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>48</v>
+        <v>74</v>
+      </c>
+      <c r="E5" t="s">
+        <v>75</v>
+      </c>
+      <c r="F5">
+        <v>2006</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B6" t="s">
         <v>26</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>53</v>
+        <v>48</v>
+      </c>
+      <c r="E6" t="s">
+        <v>76</v>
+      </c>
+      <c r="F6">
+        <v>2001</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>56</v>
+        <v>67</v>
       </c>
       <c r="B7" t="s">
-        <v>57</v>
+        <v>26</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>58</v>
+        <v>68</v>
+      </c>
+      <c r="F7">
+        <v>1991</v>
+      </c>
+      <c r="G7">
+        <v>2009</v>
+      </c>
+      <c r="J7" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
-        <v>23</v>
+      <c r="A8" t="s">
+        <v>33</v>
       </c>
       <c r="B8" t="s">
         <v>26</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>49</v>
+        <v>53</v>
+      </c>
+      <c r="E8" t="s">
+        <v>77</v>
+      </c>
+      <c r="F8">
+        <v>2008</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>41</v>
+        <v>56</v>
       </c>
       <c r="B9" t="s">
-        <v>42</v>
+        <v>57</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="E9" t="s">
-        <v>15</v>
-      </c>
-      <c r="F9">
-        <v>1816</v>
-      </c>
-      <c r="G9">
-        <v>2007</v>
-      </c>
-      <c r="H9" t="s">
-        <v>17</v>
-      </c>
-      <c r="I9" t="s">
-        <v>21</v>
+        <v>58</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>62</v>
+      <c r="A10" s="1" t="s">
+        <v>23</v>
       </c>
       <c r="B10" t="s">
-        <v>63</v>
+        <v>26</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>64</v>
+        <v>49</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>29</v>
+        <v>41</v>
       </c>
       <c r="B11" t="s">
-        <v>26</v>
+        <v>42</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>50</v>
+        <v>43</v>
+      </c>
+      <c r="E11" t="s">
+        <v>15</v>
+      </c>
+      <c r="F11">
+        <v>1816</v>
+      </c>
+      <c r="G11">
+        <v>2007</v>
+      </c>
+      <c r="H11" t="s">
+        <v>17</v>
+      </c>
+      <c r="I11" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>28</v>
+        <v>78</v>
       </c>
       <c r="B12" t="s">
         <v>26</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>51</v>
+        <v>79</v>
+      </c>
+      <c r="E12" t="s">
+        <v>80</v>
+      </c>
+      <c r="F12">
+        <v>1971</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>5</v>
+        <v>62</v>
       </c>
       <c r="B13" t="s">
-        <v>26</v>
+        <v>63</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D13" t="s">
-        <v>7</v>
-      </c>
-      <c r="E13" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>29</v>
+      </c>
+      <c r="B14" t="s">
+        <v>26</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>83</v>
+      </c>
+      <c r="B15" t="s">
+        <v>60</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="E15" t="s">
         <v>10</v>
       </c>
-      <c r="F13">
-        <v>2002</v>
-      </c>
-      <c r="H13" t="s">
-        <v>17</v>
-      </c>
-      <c r="I13" t="s">
-        <v>21</v>
-      </c>
-      <c r="J13" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A14" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B14" t="s">
-        <v>26</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A15" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B15" t="s">
-        <v>26</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>55</v>
+      <c r="F15">
+        <v>1979</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>12</v>
+        <v>81</v>
       </c>
       <c r="B16" t="s">
         <v>26</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D16" t="s">
-        <v>39</v>
+        <v>82</v>
       </c>
       <c r="E16" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F16">
-        <v>2007</v>
-      </c>
-      <c r="H16" t="s">
-        <v>17</v>
-      </c>
-      <c r="I16" t="s">
-        <v>22</v>
-      </c>
-      <c r="J16" t="s">
-        <v>19</v>
+        <v>1979</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>59</v>
+      <c r="A17" s="3" t="s">
+        <v>85</v>
       </c>
       <c r="B17" t="s">
-        <v>60</v>
+        <v>86</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>61</v>
+        <v>87</v>
+      </c>
+      <c r="E17" t="s">
+        <v>10</v>
+      </c>
+      <c r="F17">
+        <v>1979</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>36</v>
+      <c r="A18" s="3" t="s">
+        <v>88</v>
       </c>
       <c r="B18" t="s">
-        <v>26</v>
+        <v>89</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="D18" t="s">
-        <v>38</v>
+        <v>90</v>
       </c>
       <c r="E18" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="F18">
-        <v>2001</v>
-      </c>
-      <c r="H18" t="s">
-        <v>17</v>
-      </c>
-      <c r="I18" t="s">
-        <v>21</v>
-      </c>
-      <c r="J18" t="s">
-        <v>18</v>
+        <v>1979</v>
+      </c>
+      <c r="G18">
+        <v>2009</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
+        <v>28</v>
+      </c>
+      <c r="B19" t="s">
+        <v>26</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>5</v>
+      </c>
+      <c r="B20" t="s">
+        <v>26</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D20" t="s">
+        <v>7</v>
+      </c>
+      <c r="E20" t="s">
+        <v>10</v>
+      </c>
+      <c r="F20">
+        <v>2002</v>
+      </c>
+      <c r="H20" t="s">
+        <v>17</v>
+      </c>
+      <c r="I20" t="s">
+        <v>21</v>
+      </c>
+      <c r="J20" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A21" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B21" t="s">
+        <v>26</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>92</v>
+      </c>
+      <c r="B22" t="s">
+        <v>26</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="E22" t="s">
+        <v>35</v>
+      </c>
+      <c r="F22">
+        <v>1972</v>
+      </c>
+      <c r="H22" t="s">
+        <v>17</v>
+      </c>
+      <c r="I22" t="s">
+        <v>21</v>
+      </c>
+      <c r="J22" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>65</v>
+      </c>
+      <c r="B23" t="s">
+        <v>26</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="J23" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A24" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B24" t="s">
+        <v>26</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>93</v>
+      </c>
+      <c r="B25" t="s">
+        <v>26</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="E25" t="s">
+        <v>72</v>
+      </c>
+      <c r="F25">
+        <v>1995</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>12</v>
+      </c>
+      <c r="B26" t="s">
+        <v>26</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D26" t="s">
+        <v>39</v>
+      </c>
+      <c r="E26" t="s">
+        <v>11</v>
+      </c>
+      <c r="F26">
+        <v>2007</v>
+      </c>
+      <c r="H26" t="s">
+        <v>17</v>
+      </c>
+      <c r="I26" t="s">
+        <v>22</v>
+      </c>
+      <c r="J26" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>59</v>
+      </c>
+      <c r="B27" t="s">
+        <v>60</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>36</v>
+      </c>
+      <c r="B28" t="s">
+        <v>26</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D28" t="s">
+        <v>38</v>
+      </c>
+      <c r="E28" t="s">
+        <v>15</v>
+      </c>
+      <c r="F28">
+        <v>2001</v>
+      </c>
+      <c r="H28" t="s">
+        <v>17</v>
+      </c>
+      <c r="I28" t="s">
+        <v>21</v>
+      </c>
+      <c r="J28" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>95</v>
+      </c>
+      <c r="B29" t="s">
+        <v>26</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="E29" t="s">
+        <v>96</v>
+      </c>
+      <c r="F29">
+        <v>1999</v>
+      </c>
+      <c r="J29" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>69</v>
+      </c>
+      <c r="B30" t="s">
+        <v>26</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
         <v>14</v>
       </c>
-      <c r="B19" t="s">
-        <v>26</v>
-      </c>
-      <c r="C19" s="2" t="s">
+      <c r="B31" t="s">
+        <v>26</v>
+      </c>
+      <c r="C31" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="D19" s="1" t="s">
+      <c r="D31" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="E19" t="s">
+      <c r="E31" t="s">
         <v>15</v>
       </c>
-      <c r="F19">
+      <c r="F31">
         <v>1981</v>
       </c>
-      <c r="H19" t="s">
+      <c r="H31" t="s">
         <v>17</v>
       </c>
-      <c r="I19" t="s">
+      <c r="I31" t="s">
         <v>21</v>
       </c>
-      <c r="J19" t="s">
+      <c r="J31" t="s">
         <v>18</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:J19">
+  <sortState ref="A2:J31">
     <sortCondition ref="A2"/>
   </sortState>
   <hyperlinks>
     <hyperlink ref="C3" r:id="rId1"/>
-    <hyperlink ref="C13" r:id="rId2"/>
+    <hyperlink ref="C20" r:id="rId2"/>
     <hyperlink ref="C4" r:id="rId3"/>
-    <hyperlink ref="C5" r:id="rId4"/>
-    <hyperlink ref="C16" r:id="rId5"/>
-    <hyperlink ref="C18" r:id="rId6"/>
-    <hyperlink ref="C19" r:id="rId7"/>
-    <hyperlink ref="C9" r:id="rId8"/>
-    <hyperlink ref="C8" r:id="rId9"/>
-    <hyperlink ref="C11" r:id="rId10"/>
-    <hyperlink ref="C12" r:id="rId11"/>
+    <hyperlink ref="C6" r:id="rId4"/>
+    <hyperlink ref="C26" r:id="rId5"/>
+    <hyperlink ref="C28" r:id="rId6"/>
+    <hyperlink ref="C31" r:id="rId7"/>
+    <hyperlink ref="C11" r:id="rId8"/>
+    <hyperlink ref="C10" r:id="rId9"/>
+    <hyperlink ref="C14" r:id="rId10"/>
+    <hyperlink ref="C19" r:id="rId11"/>
     <hyperlink ref="C2" r:id="rId12"/>
-    <hyperlink ref="C6" r:id="rId13"/>
-    <hyperlink ref="C14" r:id="rId14"/>
-    <hyperlink ref="C15" r:id="rId15"/>
-    <hyperlink ref="C7" r:id="rId16"/>
-    <hyperlink ref="C17" r:id="rId17"/>
-    <hyperlink ref="C10" r:id="rId18"/>
+    <hyperlink ref="C8" r:id="rId13"/>
+    <hyperlink ref="C21" r:id="rId14"/>
+    <hyperlink ref="C24" r:id="rId15"/>
+    <hyperlink ref="C9" r:id="rId16"/>
+    <hyperlink ref="C27" r:id="rId17"/>
+    <hyperlink ref="C13" r:id="rId18"/>
+    <hyperlink ref="C23" r:id="rId19"/>
+    <hyperlink ref="C7" r:id="rId20"/>
+    <hyperlink ref="C30" r:id="rId21"/>
+    <hyperlink ref="C5" r:id="rId22"/>
+    <hyperlink ref="C12" r:id="rId23"/>
+    <hyperlink ref="C16" r:id="rId24"/>
+    <hyperlink ref="C15" r:id="rId25"/>
+    <hyperlink ref="C17" r:id="rId26"/>
+    <hyperlink ref="C18" r:id="rId27"/>
+    <hyperlink ref="C22" r:id="rId28"/>
+    <hyperlink ref="C25" r:id="rId29"/>
+    <hyperlink ref="C29" r:id="rId30"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
add 17 datasets and two links to overviews
</commit_message>
<xml_diff>
--- a/PolData.xlsx
+++ b/PolData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17460" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17440" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="196">
   <si>
     <t>name</t>
   </si>
@@ -504,6 +504,117 @@
   </si>
   <si>
     <t>Seats and Votes, 1950-1995</t>
+  </si>
+  <si>
+    <t>Comparative Welfare Entitlements Dataset</t>
+  </si>
+  <si>
+    <t>http://cwed2.org/download.php</t>
+  </si>
+  <si>
+    <t>http://web.missouri.edu/~williamslaro/mipdata.html</t>
+  </si>
+  <si>
+    <t>The 'Most Important Problem' Dataset</t>
+  </si>
+  <si>
+    <t>http://www.rochester.edu/college/faculty/hgoemans/data.htm</t>
+  </si>
+  <si>
+    <t>Archigos: A Data Base on Leaders 1875-2004</t>
+  </si>
+  <si>
+    <t>Constituency-Level Elections Archive</t>
+  </si>
+  <si>
+    <t>elections</t>
+  </si>
+  <si>
+    <t>http://www.electiondataarchive.org/</t>
+  </si>
+  <si>
+    <t>http://www.humanrightsdata.com/p/data-documentation.html</t>
+  </si>
+  <si>
+    <t>The CIRI Human Rights Dataset</t>
+  </si>
+  <si>
+    <t>https://sites.google.com/site/mkmtwo/data</t>
+  </si>
+  <si>
+    <t>Boix-Miller-Rosato (BMR) dichotomous coding of democracy, 1800-2010</t>
+  </si>
+  <si>
+    <t>https://www.prio.org/Data/Governance/Vanhanens-index-of-democracy/</t>
+  </si>
+  <si>
+    <t>Vanhanen's index of democracy</t>
+  </si>
+  <si>
+    <t>Comparative Agendas Project</t>
+  </si>
+  <si>
+    <t>Comparative Agendas Project: Media</t>
+  </si>
+  <si>
+    <t>http://www.comparativeagendas.net/datasets_codebooks</t>
+  </si>
+  <si>
+    <t>Belgium, Hungary, Spain, State of Pennsylvania, Switzerland, United Kingdom, United States</t>
+  </si>
+  <si>
+    <t>Comparative Agendas Project: Public Opinion &amp; Interest Groups</t>
+  </si>
+  <si>
+    <t>Hungary, Switzerland, United Kingdom, United States</t>
+  </si>
+  <si>
+    <t>European Election Database</t>
+  </si>
+  <si>
+    <t>http://www.nsd.uib.no/european_election_database</t>
+  </si>
+  <si>
+    <t>https://www.idea.int/data-tools/data/voter-turnout</t>
+  </si>
+  <si>
+    <t>Voter Turnout Database</t>
+  </si>
+  <si>
+    <t>http://www.marquette.edu/polisci/faculty_swank.shtml</t>
+  </si>
+  <si>
+    <t>Comparative Parties Data Set</t>
+  </si>
+  <si>
+    <t>PIP: Left-Right Party Scores</t>
+  </si>
+  <si>
+    <t>http://comparativepolitics.uni-greifswald.de/data.html</t>
+  </si>
+  <si>
+    <t>Comparative Welfare States Data Set</t>
+  </si>
+  <si>
+    <t>http://www.lisdatacenter.org/resources/other-databases/</t>
+  </si>
+  <si>
+    <t>free</t>
+  </si>
+  <si>
+    <t>https://www.gesis.org/angebot/daten-analysieren/weitere-sekundaerdaten/weitere-internationale-daten/europaeische-wahlstudien/election-studies-eastern-europe/</t>
+  </si>
+  <si>
+    <t>Election Studies Eastern Europe</t>
+  </si>
+  <si>
+    <t>Belarus, Bulgaria, the Czech Republic, Croatia, Macedonia, Poland, Serbia, Slovakia, Slovenia, Ukraine</t>
+  </si>
+  <si>
+    <t>http://www.spin.su.se/datasets/scip</t>
+  </si>
+  <si>
+    <t>Social Citizenship Indicator Program</t>
   </si>
 </sst>
 </file>
@@ -835,10 +946,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J60"/>
+  <dimension ref="A1:J77"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="A53" sqref="A53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -965,725 +1076,707 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>31</v>
+        <v>164</v>
       </c>
       <c r="B6" t="s">
-        <v>25</v>
+        <v>83</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="E6" t="s">
-        <v>73</v>
-      </c>
-      <c r="F6">
-        <v>2001</v>
+        <v>163</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>113</v>
+        <v>31</v>
       </c>
       <c r="B7" t="s">
         <v>25</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>114</v>
+        <v>46</v>
       </c>
       <c r="E7" t="s">
-        <v>112</v>
+        <v>73</v>
       </c>
       <c r="F7">
-        <v>1964</v>
+        <v>2001</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>64</v>
+        <v>171</v>
       </c>
       <c r="B8" t="s">
-        <v>25</v>
+        <v>60</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="F8">
-        <v>1991</v>
-      </c>
-      <c r="G8">
-        <v>2009</v>
-      </c>
-      <c r="J8" t="s">
-        <v>18</v>
+        <v>170</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>107</v>
+        <v>113</v>
       </c>
       <c r="B9" t="s">
         <v>25</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>108</v>
+        <v>114</v>
       </c>
       <c r="E9" t="s">
         <v>112</v>
       </c>
+      <c r="F9">
+        <v>1964</v>
+      </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>124</v>
+        <v>64</v>
       </c>
       <c r="B10" t="s">
-        <v>119</v>
+        <v>25</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="I10" t="s">
-        <v>20</v>
+        <v>65</v>
+      </c>
+      <c r="F10">
+        <v>1991</v>
+      </c>
+      <c r="G10">
+        <v>2009</v>
+      </c>
+      <c r="J10" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>32</v>
+        <v>107</v>
       </c>
       <c r="B11" t="s">
         <v>25</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>51</v>
+        <v>108</v>
       </c>
       <c r="E11" t="s">
-        <v>74</v>
-      </c>
-      <c r="F11">
-        <v>2008</v>
+        <v>112</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>147</v>
+        <v>124</v>
       </c>
       <c r="B12" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>146</v>
+        <v>122</v>
+      </c>
+      <c r="I12" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>128</v>
+        <v>32</v>
       </c>
       <c r="B13" t="s">
-        <v>119</v>
+        <v>25</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="I13" t="s">
-        <v>20</v>
+        <v>51</v>
+      </c>
+      <c r="E13" t="s">
+        <v>74</v>
+      </c>
+      <c r="F13">
+        <v>2008</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>136</v>
+        <v>147</v>
       </c>
       <c r="B14" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>137</v>
+        <v>146</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>54</v>
+        <v>128</v>
       </c>
       <c r="B15" t="s">
-        <v>55</v>
+        <v>119</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>56</v>
+        <v>122</v>
+      </c>
+      <c r="I15" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A16" s="1" t="s">
-        <v>22</v>
+      <c r="A16" t="s">
+        <v>174</v>
       </c>
       <c r="B16" t="s">
-        <v>25</v>
+        <v>129</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>39</v>
+        <v>175</v>
       </c>
       <c r="B17" t="s">
-        <v>40</v>
+        <v>86</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>41</v>
+        <v>176</v>
       </c>
       <c r="E17" t="s">
-        <v>14</v>
-      </c>
-      <c r="F17">
-        <v>1816</v>
-      </c>
-      <c r="G17">
-        <v>2007</v>
-      </c>
-      <c r="H17" t="s">
-        <v>16</v>
-      </c>
-      <c r="I17" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>75</v>
+        <v>178</v>
       </c>
       <c r="B18" t="s">
         <v>25</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>76</v>
+        <v>176</v>
       </c>
       <c r="E18" t="s">
-        <v>77</v>
-      </c>
-      <c r="F18">
-        <v>1971</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>59</v>
+        <v>136</v>
       </c>
       <c r="B19" t="s">
-        <v>60</v>
+        <v>135</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>150</v>
+        <v>185</v>
       </c>
       <c r="B20" t="s">
         <v>129</v>
       </c>
       <c r="C20" s="2" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>54</v>
+      </c>
+      <c r="B21" t="s">
+        <v>55</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A22" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B22" t="s">
+        <v>25</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>159</v>
+      </c>
+      <c r="B23" t="s">
+        <v>99</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>188</v>
+      </c>
+      <c r="B24" t="s">
+        <v>99</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="F24">
+        <v>1960</v>
+      </c>
+      <c r="G24">
+        <v>2011</v>
+      </c>
+      <c r="H24" t="s">
+        <v>16</v>
+      </c>
+      <c r="I24" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>165</v>
+      </c>
+      <c r="B25" t="s">
+        <v>166</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>39</v>
+      </c>
+      <c r="B26" t="s">
+        <v>40</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E26" t="s">
+        <v>14</v>
+      </c>
+      <c r="F26">
+        <v>1816</v>
+      </c>
+      <c r="G26">
+        <v>2007</v>
+      </c>
+      <c r="H26" t="s">
+        <v>16</v>
+      </c>
+      <c r="I26" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>75</v>
+      </c>
+      <c r="B27" t="s">
+        <v>25</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="E27" t="s">
+        <v>77</v>
+      </c>
+      <c r="F27">
+        <v>1971</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>59</v>
+      </c>
+      <c r="B28" t="s">
+        <v>60</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>192</v>
+      </c>
+      <c r="B29" t="s">
+        <v>25</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="E29" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>150</v>
+      </c>
+      <c r="B30" t="s">
+        <v>129</v>
+      </c>
+      <c r="C30" s="2" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
         <v>28</v>
       </c>
-      <c r="B21" t="s">
-        <v>25</v>
-      </c>
-      <c r="C21" s="2" t="s">
+      <c r="B31" t="s">
+        <v>25</v>
+      </c>
+      <c r="C31" s="2" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
         <v>80</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B32" t="s">
         <v>129</v>
       </c>
-      <c r="C22" s="2" t="s">
+      <c r="C32" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="E22" t="s">
+      <c r="E32" t="s">
         <v>9</v>
       </c>
-      <c r="F22">
+      <c r="F32">
         <v>1979</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>126</v>
-      </c>
-      <c r="B23" t="s">
-        <v>125</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>78</v>
-      </c>
-      <c r="B24" t="s">
-        <v>25</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="E24" t="s">
-        <v>9</v>
-      </c>
-      <c r="F24">
-        <v>1979</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A25" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="B25" t="s">
-        <v>83</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="E25" t="s">
-        <v>9</v>
-      </c>
-      <c r="F25">
-        <v>1979</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A26" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="B26" t="s">
-        <v>86</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="E26" t="s">
-        <v>9</v>
-      </c>
-      <c r="F26">
-        <v>1979</v>
-      </c>
-      <c r="G26">
-        <v>2009</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
-        <v>27</v>
-      </c>
-      <c r="B27" t="s">
-        <v>25</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
-        <v>121</v>
-      </c>
-      <c r="B28" t="s">
-        <v>119</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="I28" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
-        <v>5</v>
-      </c>
-      <c r="B29" t="s">
-        <v>25</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D29" t="s">
-        <v>94</v>
-      </c>
-      <c r="E29" t="s">
-        <v>9</v>
-      </c>
-      <c r="F29">
-        <v>2002</v>
-      </c>
-      <c r="H29" t="s">
-        <v>16</v>
-      </c>
-      <c r="I29" t="s">
-        <v>20</v>
-      </c>
-      <c r="J29" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A30" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B30" t="s">
-        <v>25</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
-        <v>89</v>
-      </c>
-      <c r="B31" t="s">
-        <v>25</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="E31" t="s">
-        <v>34</v>
-      </c>
-      <c r="F31">
-        <v>1972</v>
-      </c>
-      <c r="H31" t="s">
-        <v>16</v>
-      </c>
-      <c r="I31" t="s">
-        <v>20</v>
-      </c>
-      <c r="J31" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
-        <v>104</v>
-      </c>
-      <c r="B32" t="s">
-        <v>25</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="E32" t="s">
-        <v>105</v>
-      </c>
-      <c r="F32">
-        <v>1980</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>62</v>
+        <v>126</v>
       </c>
       <c r="B33" t="s">
-        <v>25</v>
+        <v>125</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="J33" t="s">
-        <v>18</v>
+        <v>127</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>152</v>
+        <v>180</v>
       </c>
       <c r="B34" t="s">
-        <v>40</v>
+        <v>166</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="E34" t="s">
-        <v>14</v>
+        <v>181</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>154</v>
+        <v>78</v>
       </c>
       <c r="B35" t="s">
-        <v>119</v>
+        <v>25</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>155</v>
+        <v>79</v>
+      </c>
+      <c r="E35" t="s">
+        <v>9</v>
+      </c>
+      <c r="F35">
+        <v>1979</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
-        <v>100</v>
+      <c r="A36" s="3" t="s">
+        <v>82</v>
       </c>
       <c r="B36" t="s">
-        <v>99</v>
+        <v>83</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>101</v>
+        <v>84</v>
+      </c>
+      <c r="E36" t="s">
+        <v>9</v>
+      </c>
+      <c r="F36">
+        <v>1979</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
-        <v>117</v>
+      <c r="A37" s="3" t="s">
+        <v>85</v>
       </c>
       <c r="B37" t="s">
-        <v>55</v>
+        <v>86</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="I37" t="s">
-        <v>20</v>
+        <v>87</v>
+      </c>
+      <c r="E37" t="s">
+        <v>9</v>
+      </c>
+      <c r="F37">
+        <v>1979</v>
+      </c>
+      <c r="G37">
+        <v>2009</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A38" s="1" t="s">
-        <v>23</v>
+      <c r="A38" t="s">
+        <v>27</v>
       </c>
       <c r="B38" t="s">
         <v>25</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>96</v>
+        <v>121</v>
       </c>
       <c r="B39" t="s">
-        <v>25</v>
+        <v>119</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="E39" t="s">
-        <v>69</v>
-      </c>
-      <c r="F39">
-        <v>1995</v>
+        <v>120</v>
+      </c>
+      <c r="I39" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="B40" t="s">
         <v>25</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="D40" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E40" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F40">
-        <v>2007</v>
+        <v>2002</v>
       </c>
       <c r="H40" t="s">
         <v>16</v>
       </c>
       <c r="I40" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J40" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A41" t="s">
-        <v>97</v>
+      <c r="A41" s="1" t="s">
+        <v>26</v>
       </c>
       <c r="B41" t="s">
-        <v>129</v>
+        <v>25</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>98</v>
+        <v>52</v>
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>157</v>
+        <v>89</v>
       </c>
       <c r="B42" t="s">
         <v>25</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>155</v>
+        <v>88</v>
+      </c>
+      <c r="E42" t="s">
+        <v>34</v>
+      </c>
+      <c r="F42">
+        <v>1972</v>
+      </c>
+      <c r="H42" t="s">
+        <v>16</v>
+      </c>
+      <c r="I42" t="s">
+        <v>20</v>
+      </c>
+      <c r="J42" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="B43" t="s">
-        <v>99</v>
+        <v>25</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>103</v>
+        <v>106</v>
+      </c>
+      <c r="E43" t="s">
+        <v>105</v>
+      </c>
+      <c r="F43">
+        <v>1980</v>
       </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>138</v>
+        <v>62</v>
       </c>
       <c r="B44" t="s">
-        <v>119</v>
+        <v>25</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>139</v>
+        <v>63</v>
+      </c>
+      <c r="J44" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="B45" t="s">
-        <v>119</v>
+        <v>40</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>155</v>
+        <v>153</v>
+      </c>
+      <c r="E45" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>57</v>
+        <v>154</v>
       </c>
       <c r="B46" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>58</v>
+        <v>155</v>
       </c>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="B47" t="s">
-        <v>119</v>
+        <v>99</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="E47" t="s">
-        <v>132</v>
-      </c>
-      <c r="F47">
-        <v>1945</v>
-      </c>
-      <c r="G47">
-        <v>2008</v>
-      </c>
-      <c r="I47" t="s">
-        <v>20</v>
+        <v>101</v>
       </c>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>149</v>
+        <v>117</v>
       </c>
       <c r="B48" t="s">
-        <v>129</v>
+        <v>55</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>148</v>
+        <v>118</v>
+      </c>
+      <c r="I48" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A49" t="s">
-        <v>35</v>
+      <c r="A49" s="1" t="s">
+        <v>23</v>
       </c>
       <c r="B49" t="s">
         <v>25</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="D49" t="s">
-        <v>37</v>
-      </c>
-      <c r="E49" t="s">
-        <v>14</v>
-      </c>
-      <c r="F49">
-        <v>2001</v>
-      </c>
-      <c r="H49" t="s">
-        <v>16</v>
-      </c>
-      <c r="I49" t="s">
-        <v>20</v>
-      </c>
-      <c r="J49" t="s">
-        <v>17</v>
+        <v>53</v>
       </c>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>145</v>
+        <v>96</v>
       </c>
       <c r="B50" t="s">
-        <v>60</v>
+        <v>25</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>144</v>
+        <v>90</v>
+      </c>
+      <c r="E50" t="s">
+        <v>69</v>
       </c>
       <c r="F50">
-        <v>1800</v>
-      </c>
-      <c r="G50">
-        <v>2013</v>
+        <v>1995</v>
       </c>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>123</v>
+        <v>11</v>
       </c>
       <c r="B51" t="s">
-        <v>119</v>
+        <v>25</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>122</v>
+        <v>12</v>
+      </c>
+      <c r="D51" t="s">
+        <v>95</v>
+      </c>
+      <c r="E51" t="s">
+        <v>10</v>
+      </c>
+      <c r="F51">
+        <v>2007</v>
+      </c>
+      <c r="H51" t="s">
+        <v>16</v>
       </c>
       <c r="I51" t="s">
-        <v>20</v>
+        <v>21</v>
+      </c>
+      <c r="J51" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>142</v>
+        <v>97</v>
       </c>
       <c r="B52" t="s">
-        <v>60</v>
+        <v>129</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>143</v>
+        <v>98</v>
       </c>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B53" t="s">
-        <v>129</v>
+        <v>25</v>
       </c>
       <c r="C53" s="2" t="s">
         <v>155</v>
@@ -1691,106 +1784,100 @@
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="B54" t="s">
-        <v>25</v>
+        <v>99</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="E54" t="s">
-        <v>111</v>
-      </c>
-      <c r="F54">
-        <v>1956</v>
-      </c>
-      <c r="J54" t="s">
-        <v>17</v>
+        <v>103</v>
       </c>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>91</v>
+        <v>138</v>
       </c>
       <c r="B55" t="s">
-        <v>25</v>
+        <v>119</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="E55" t="s">
-        <v>92</v>
-      </c>
-      <c r="F55">
-        <v>1999</v>
-      </c>
-      <c r="J55" t="s">
-        <v>18</v>
+        <v>139</v>
       </c>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>66</v>
+        <v>156</v>
       </c>
       <c r="B56" t="s">
-        <v>25</v>
+        <v>119</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>67</v>
+        <v>155</v>
       </c>
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>140</v>
+        <v>57</v>
       </c>
       <c r="B57" t="s">
-        <v>40</v>
+        <v>129</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>141</v>
+        <v>58</v>
       </c>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="B58" t="s">
         <v>119</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
+      </c>
+      <c r="E58" t="s">
+        <v>132</v>
+      </c>
+      <c r="F58">
+        <v>1945</v>
+      </c>
+      <c r="G58">
+        <v>2008</v>
+      </c>
+      <c r="I58" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>115</v>
+        <v>149</v>
       </c>
       <c r="B59" t="s">
         <v>129</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>116</v>
+        <v>148</v>
       </c>
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>13</v>
+        <v>35</v>
       </c>
       <c r="B60" t="s">
         <v>25</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="D60" s="1" t="s">
-        <v>42</v>
+        <v>36</v>
+      </c>
+      <c r="D60" t="s">
+        <v>37</v>
       </c>
       <c r="E60" t="s">
         <v>14</v>
       </c>
       <c r="F60">
-        <v>1981</v>
+        <v>2001</v>
       </c>
       <c r="H60" t="s">
         <v>16</v>
@@ -1802,70 +1889,319 @@
         <v>17</v>
       </c>
     </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>186</v>
+      </c>
+      <c r="B61" t="s">
+        <v>129</v>
+      </c>
+      <c r="C61" s="2" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>145</v>
+      </c>
+      <c r="B62" t="s">
+        <v>60</v>
+      </c>
+      <c r="C62" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="F62">
+        <v>1800</v>
+      </c>
+      <c r="G62">
+        <v>2013</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>123</v>
+      </c>
+      <c r="B63" t="s">
+        <v>119</v>
+      </c>
+      <c r="C63" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="I63" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
+        <v>142</v>
+      </c>
+      <c r="B64" t="s">
+        <v>60</v>
+      </c>
+      <c r="C64" s="2" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
+        <v>158</v>
+      </c>
+      <c r="B65" t="s">
+        <v>129</v>
+      </c>
+      <c r="C65" s="2" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
+        <v>195</v>
+      </c>
+      <c r="B66" t="s">
+        <v>99</v>
+      </c>
+      <c r="C66" s="2" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
+        <v>109</v>
+      </c>
+      <c r="B67" t="s">
+        <v>25</v>
+      </c>
+      <c r="C67" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="E67" t="s">
+        <v>111</v>
+      </c>
+      <c r="F67">
+        <v>1956</v>
+      </c>
+      <c r="J67" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
+        <v>91</v>
+      </c>
+      <c r="B68" t="s">
+        <v>25</v>
+      </c>
+      <c r="C68" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="E68" t="s">
+        <v>92</v>
+      </c>
+      <c r="F68">
+        <v>1999</v>
+      </c>
+      <c r="J68" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
+        <v>162</v>
+      </c>
+      <c r="B69" t="s">
+        <v>25</v>
+      </c>
+      <c r="C69" s="2" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
+        <v>169</v>
+      </c>
+      <c r="B70" t="s">
+        <v>40</v>
+      </c>
+      <c r="C70" s="2" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A71" t="s">
+        <v>66</v>
+      </c>
+      <c r="B71" t="s">
+        <v>25</v>
+      </c>
+      <c r="C71" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="72" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A72" t="s">
+        <v>140</v>
+      </c>
+      <c r="B72" t="s">
+        <v>40</v>
+      </c>
+      <c r="C72" s="2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A73" t="s">
+        <v>173</v>
+      </c>
+      <c r="B73" t="s">
+        <v>60</v>
+      </c>
+      <c r="C73" s="2" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A74" t="s">
+        <v>133</v>
+      </c>
+      <c r="B74" t="s">
+        <v>119</v>
+      </c>
+      <c r="C74" s="2" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="75" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A75" t="s">
+        <v>183</v>
+      </c>
+      <c r="B75" t="s">
+        <v>166</v>
+      </c>
+      <c r="C75" s="2" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A76" t="s">
+        <v>115</v>
+      </c>
+      <c r="B76" t="s">
+        <v>129</v>
+      </c>
+      <c r="C76" s="2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A77" t="s">
+        <v>13</v>
+      </c>
+      <c r="B77" t="s">
+        <v>25</v>
+      </c>
+      <c r="C77" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D77" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E77" t="s">
+        <v>14</v>
+      </c>
+      <c r="F77">
+        <v>1981</v>
+      </c>
+      <c r="H77" t="s">
+        <v>16</v>
+      </c>
+      <c r="I77" t="s">
+        <v>20</v>
+      </c>
+      <c r="J77" t="s">
+        <v>17</v>
+      </c>
+    </row>
   </sheetData>
-  <sortState ref="A2:J60">
+  <sortState ref="A2:J77">
     <sortCondition ref="A2"/>
   </sortState>
   <hyperlinks>
     <hyperlink ref="C3" r:id="rId1"/>
-    <hyperlink ref="C29" r:id="rId2"/>
+    <hyperlink ref="C40" r:id="rId2"/>
     <hyperlink ref="C4" r:id="rId3"/>
-    <hyperlink ref="C6" r:id="rId4"/>
-    <hyperlink ref="C40" r:id="rId5"/>
-    <hyperlink ref="C49" r:id="rId6"/>
-    <hyperlink ref="C60" r:id="rId7"/>
-    <hyperlink ref="C17" r:id="rId8"/>
-    <hyperlink ref="C16" r:id="rId9"/>
-    <hyperlink ref="C21" r:id="rId10"/>
-    <hyperlink ref="C27" r:id="rId11"/>
+    <hyperlink ref="C7" r:id="rId4"/>
+    <hyperlink ref="C51" r:id="rId5"/>
+    <hyperlink ref="C60" r:id="rId6"/>
+    <hyperlink ref="C77" r:id="rId7"/>
+    <hyperlink ref="C26" r:id="rId8"/>
+    <hyperlink ref="C22" r:id="rId9"/>
+    <hyperlink ref="C31" r:id="rId10"/>
+    <hyperlink ref="C38" r:id="rId11"/>
     <hyperlink ref="C2" r:id="rId12"/>
-    <hyperlink ref="C11" r:id="rId13"/>
-    <hyperlink ref="C30" r:id="rId14"/>
-    <hyperlink ref="C38" r:id="rId15"/>
-    <hyperlink ref="C15" r:id="rId16"/>
-    <hyperlink ref="C46" r:id="rId17"/>
-    <hyperlink ref="C19" r:id="rId18"/>
-    <hyperlink ref="C33" r:id="rId19"/>
-    <hyperlink ref="C8" r:id="rId20"/>
-    <hyperlink ref="C56" r:id="rId21"/>
+    <hyperlink ref="C13" r:id="rId13"/>
+    <hyperlink ref="C41" r:id="rId14"/>
+    <hyperlink ref="C49" r:id="rId15"/>
+    <hyperlink ref="C21" r:id="rId16"/>
+    <hyperlink ref="C57" r:id="rId17"/>
+    <hyperlink ref="C28" r:id="rId18"/>
+    <hyperlink ref="C44" r:id="rId19"/>
+    <hyperlink ref="C10" r:id="rId20"/>
+    <hyperlink ref="C71" r:id="rId21"/>
     <hyperlink ref="C5" r:id="rId22"/>
-    <hyperlink ref="C18" r:id="rId23"/>
-    <hyperlink ref="C24" r:id="rId24"/>
-    <hyperlink ref="C22" r:id="rId25"/>
-    <hyperlink ref="C25" r:id="rId26"/>
-    <hyperlink ref="C26" r:id="rId27"/>
-    <hyperlink ref="C31" r:id="rId28"/>
-    <hyperlink ref="C39" r:id="rId29"/>
-    <hyperlink ref="C55" r:id="rId30"/>
-    <hyperlink ref="C41" r:id="rId31"/>
-    <hyperlink ref="C36" r:id="rId32"/>
-    <hyperlink ref="C43" r:id="rId33"/>
-    <hyperlink ref="C32" r:id="rId34"/>
-    <hyperlink ref="C9" r:id="rId35"/>
-    <hyperlink ref="C54" r:id="rId36"/>
-    <hyperlink ref="C7" r:id="rId37"/>
-    <hyperlink ref="C59" r:id="rId38"/>
-    <hyperlink ref="C37" r:id="rId39"/>
-    <hyperlink ref="C28" r:id="rId40"/>
-    <hyperlink ref="C51" r:id="rId41"/>
-    <hyperlink ref="C10" r:id="rId42"/>
-    <hyperlink ref="C23" r:id="rId43"/>
-    <hyperlink ref="C13" r:id="rId44"/>
-    <hyperlink ref="C47" r:id="rId45"/>
-    <hyperlink ref="C58" r:id="rId46"/>
-    <hyperlink ref="C14" r:id="rId47" display="http://comparativeconstitutionsproject.org/"/>
-    <hyperlink ref="C44" r:id="rId48"/>
-    <hyperlink ref="C57" r:id="rId49"/>
-    <hyperlink ref="C52" r:id="rId50"/>
-    <hyperlink ref="C50" r:id="rId51"/>
-    <hyperlink ref="C12" r:id="rId52"/>
-    <hyperlink ref="C48" r:id="rId53"/>
-    <hyperlink ref="C20" r:id="rId54"/>
-    <hyperlink ref="C34" r:id="rId55"/>
-    <hyperlink ref="C35" r:id="rId56"/>
-    <hyperlink ref="C45" r:id="rId57"/>
-    <hyperlink ref="C42" r:id="rId58"/>
-    <hyperlink ref="C53" r:id="rId59"/>
+    <hyperlink ref="C27" r:id="rId23"/>
+    <hyperlink ref="C35" r:id="rId24"/>
+    <hyperlink ref="C32" r:id="rId25"/>
+    <hyperlink ref="C36" r:id="rId26"/>
+    <hyperlink ref="C37" r:id="rId27"/>
+    <hyperlink ref="C42" r:id="rId28"/>
+    <hyperlink ref="C50" r:id="rId29"/>
+    <hyperlink ref="C68" r:id="rId30"/>
+    <hyperlink ref="C52" r:id="rId31"/>
+    <hyperlink ref="C47" r:id="rId32"/>
+    <hyperlink ref="C54" r:id="rId33"/>
+    <hyperlink ref="C43" r:id="rId34"/>
+    <hyperlink ref="C11" r:id="rId35"/>
+    <hyperlink ref="C67" r:id="rId36"/>
+    <hyperlink ref="C9" r:id="rId37"/>
+    <hyperlink ref="C76" r:id="rId38"/>
+    <hyperlink ref="C48" r:id="rId39"/>
+    <hyperlink ref="C39" r:id="rId40"/>
+    <hyperlink ref="C63" r:id="rId41"/>
+    <hyperlink ref="C12" r:id="rId42"/>
+    <hyperlink ref="C33" r:id="rId43"/>
+    <hyperlink ref="C15" r:id="rId44"/>
+    <hyperlink ref="C58" r:id="rId45"/>
+    <hyperlink ref="C74" r:id="rId46"/>
+    <hyperlink ref="C19" r:id="rId47" display="http://comparativeconstitutionsproject.org/"/>
+    <hyperlink ref="C55" r:id="rId48"/>
+    <hyperlink ref="C72" r:id="rId49"/>
+    <hyperlink ref="C64" r:id="rId50"/>
+    <hyperlink ref="C62" r:id="rId51"/>
+    <hyperlink ref="C14" r:id="rId52"/>
+    <hyperlink ref="C59" r:id="rId53"/>
+    <hyperlink ref="C30" r:id="rId54"/>
+    <hyperlink ref="C45" r:id="rId55"/>
+    <hyperlink ref="C46" r:id="rId56"/>
+    <hyperlink ref="C56" r:id="rId57"/>
+    <hyperlink ref="C53" r:id="rId58"/>
+    <hyperlink ref="C65" r:id="rId59"/>
+    <hyperlink ref="C23" r:id="rId60"/>
+    <hyperlink ref="C69" r:id="rId61"/>
+    <hyperlink ref="C6" r:id="rId62"/>
+    <hyperlink ref="C25" r:id="rId63"/>
+    <hyperlink ref="C70" r:id="rId64"/>
+    <hyperlink ref="C8" r:id="rId65"/>
+    <hyperlink ref="C73" r:id="rId66"/>
+    <hyperlink ref="C17" r:id="rId67"/>
+    <hyperlink ref="C16" r:id="rId68"/>
+    <hyperlink ref="C18" r:id="rId69"/>
+    <hyperlink ref="C34" r:id="rId70"/>
+    <hyperlink ref="C75" r:id="rId71"/>
+    <hyperlink ref="C20" r:id="rId72"/>
+    <hyperlink ref="C61" r:id="rId73"/>
+    <hyperlink ref="C24" r:id="rId74"/>
+    <hyperlink ref="C29" r:id="rId75"/>
+    <hyperlink ref="C66" r:id="rId76"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
add three datasets and change description
</commit_message>
<xml_diff>
--- a/PolData.xlsx
+++ b/PolData.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="203">
   <si>
     <t>name</t>
   </si>
@@ -615,6 +615,27 @@
   </si>
   <si>
     <t>Social Citizenship Indicator Program</t>
+  </si>
+  <si>
+    <t>http://mattgolder.com/elections</t>
+  </si>
+  <si>
+    <t>Democratic Electoral Systems</t>
+  </si>
+  <si>
+    <t>Database of Political Institutions</t>
+  </si>
+  <si>
+    <t>http://econ.worldbank.org/WBSITE/EXTERNAL/EXTDEC/EXTRESEARCH/0,,contentMDK:20649465~pagePK:64214825~piPK:64214943~theSitePK:469382,00.html</t>
+  </si>
+  <si>
+    <t>180 countries</t>
+  </si>
+  <si>
+    <t>fRDB-IZA Social Reforms Database</t>
+  </si>
+  <si>
+    <t>http://www.frdb.org/page/data/scheda/frdb-iza-social-reforms-database/doc_pk/9027</t>
   </si>
 </sst>
 </file>
@@ -946,10 +967,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J77"/>
+  <dimension ref="A1:J80"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A53" sqref="A53"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1393,133 +1414,142 @@
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>59</v>
+        <v>198</v>
       </c>
       <c r="B28" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>61</v>
+        <v>199</v>
+      </c>
+      <c r="E28" t="s">
+        <v>200</v>
+      </c>
+      <c r="F28">
+        <v>1975</v>
+      </c>
+      <c r="G28">
+        <v>2015</v>
+      </c>
+      <c r="H28" t="s">
+        <v>16</v>
+      </c>
+      <c r="I28" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>192</v>
+        <v>59</v>
       </c>
       <c r="B29" t="s">
-        <v>25</v>
+        <v>60</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>191</v>
-      </c>
-      <c r="E29" t="s">
-        <v>193</v>
+        <v>61</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>150</v>
+        <v>197</v>
       </c>
       <c r="B30" t="s">
-        <v>129</v>
+        <v>166</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>151</v>
+        <v>196</v>
+      </c>
+      <c r="F30">
+        <v>1946</v>
+      </c>
+      <c r="G30">
+        <v>2016</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>28</v>
+        <v>192</v>
       </c>
       <c r="B31" t="s">
         <v>25</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>48</v>
+        <v>191</v>
+      </c>
+      <c r="E31" t="s">
+        <v>193</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>80</v>
+        <v>150</v>
       </c>
       <c r="B32" t="s">
         <v>129</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="E32" t="s">
-        <v>9</v>
-      </c>
-      <c r="F32">
-        <v>1979</v>
+        <v>151</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>126</v>
+        <v>28</v>
       </c>
       <c r="B33" t="s">
-        <v>125</v>
+        <v>25</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>127</v>
+        <v>48</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>180</v>
+        <v>80</v>
       </c>
       <c r="B34" t="s">
-        <v>166</v>
+        <v>129</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>181</v>
+        <v>81</v>
+      </c>
+      <c r="E34" t="s">
+        <v>9</v>
+      </c>
+      <c r="F34">
+        <v>1979</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
+        <v>126</v>
+      </c>
+      <c r="B35" t="s">
+        <v>125</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>180</v>
+      </c>
+      <c r="B36" t="s">
+        <v>166</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
         <v>78</v>
       </c>
-      <c r="B35" t="s">
-        <v>25</v>
-      </c>
-      <c r="C35" s="2" t="s">
+      <c r="B37" t="s">
+        <v>25</v>
+      </c>
+      <c r="C37" s="2" t="s">
         <v>79</v>
-      </c>
-      <c r="E35" t="s">
-        <v>9</v>
-      </c>
-      <c r="F35">
-        <v>1979</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A36" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="B36" t="s">
-        <v>83</v>
-      </c>
-      <c r="C36" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="E36" t="s">
-        <v>9</v>
-      </c>
-      <c r="F36">
-        <v>1979</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A37" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="B37" t="s">
-        <v>86</v>
-      </c>
-      <c r="C37" s="2" t="s">
-        <v>87</v>
       </c>
       <c r="E37" t="s">
         <v>9</v>
@@ -1527,90 +1557,90 @@
       <c r="F37">
         <v>1979</v>
       </c>
-      <c r="G37">
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A38" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="B38" t="s">
+        <v>83</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="E38" t="s">
+        <v>9</v>
+      </c>
+      <c r="F38">
+        <v>1979</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A39" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="B39" t="s">
+        <v>86</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="E39" t="s">
+        <v>9</v>
+      </c>
+      <c r="F39">
+        <v>1979</v>
+      </c>
+      <c r="G39">
         <v>2009</v>
-      </c>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A38" t="s">
-        <v>27</v>
-      </c>
-      <c r="B38" t="s">
-        <v>25</v>
-      </c>
-      <c r="C38" s="2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A39" t="s">
-        <v>121</v>
-      </c>
-      <c r="B39" t="s">
-        <v>119</v>
-      </c>
-      <c r="C39" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="I39" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>5</v>
+        <v>27</v>
       </c>
       <c r="B40" t="s">
         <v>25</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D40" t="s">
-        <v>94</v>
-      </c>
-      <c r="E40" t="s">
-        <v>9</v>
-      </c>
-      <c r="F40">
-        <v>2002</v>
-      </c>
-      <c r="H40" t="s">
-        <v>16</v>
-      </c>
-      <c r="I40" t="s">
-        <v>20</v>
+        <v>49</v>
       </c>
       <c r="J40" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A41" s="1" t="s">
-        <v>26</v>
+      <c r="A41" t="s">
+        <v>121</v>
       </c>
       <c r="B41" t="s">
-        <v>25</v>
+        <v>119</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>52</v>
+        <v>120</v>
+      </c>
+      <c r="I41" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>89</v>
+        <v>5</v>
       </c>
       <c r="B42" t="s">
         <v>25</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>88</v>
+        <v>6</v>
+      </c>
+      <c r="D42" t="s">
+        <v>94</v>
       </c>
       <c r="E42" t="s">
-        <v>34</v>
+        <v>9</v>
       </c>
       <c r="F42">
-        <v>1972</v>
+        <v>2002</v>
       </c>
       <c r="H42" t="s">
         <v>16</v>
@@ -1623,31 +1653,31 @@
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A43" t="s">
-        <v>104</v>
+      <c r="A43" s="1" t="s">
+        <v>26</v>
       </c>
       <c r="B43" t="s">
         <v>25</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="E43" t="s">
-        <v>105</v>
-      </c>
-      <c r="F43">
-        <v>1980</v>
+        <v>52</v>
       </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>62</v>
+        <v>201</v>
       </c>
       <c r="B44" t="s">
-        <v>25</v>
+        <v>99</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>63</v>
+        <v>202</v>
+      </c>
+      <c r="F44">
+        <v>1980</v>
+      </c>
+      <c r="G44">
+        <v>2007</v>
       </c>
       <c r="J44" t="s">
         <v>18</v>
@@ -1655,161 +1685,179 @@
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>152</v>
+        <v>89</v>
       </c>
       <c r="B45" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>153</v>
+        <v>88</v>
       </c>
       <c r="E45" t="s">
-        <v>14</v>
+        <v>34</v>
+      </c>
+      <c r="F45">
+        <v>1972</v>
+      </c>
+      <c r="H45" t="s">
+        <v>16</v>
+      </c>
+      <c r="I45" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>154</v>
+        <v>104</v>
       </c>
       <c r="B46" t="s">
-        <v>119</v>
+        <v>25</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>155</v>
+        <v>106</v>
+      </c>
+      <c r="E46" t="s">
+        <v>105</v>
+      </c>
+      <c r="F46">
+        <v>1980</v>
       </c>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>100</v>
+        <v>62</v>
       </c>
       <c r="B47" t="s">
-        <v>99</v>
+        <v>25</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>101</v>
+        <v>63</v>
       </c>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>117</v>
+        <v>152</v>
       </c>
       <c r="B48" t="s">
-        <v>55</v>
+        <v>40</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="I48" t="s">
-        <v>20</v>
+        <v>153</v>
+      </c>
+      <c r="E48" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A49" s="1" t="s">
-        <v>23</v>
+      <c r="A49" t="s">
+        <v>154</v>
       </c>
       <c r="B49" t="s">
-        <v>25</v>
+        <v>119</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>53</v>
+        <v>155</v>
       </c>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="B50" t="s">
-        <v>25</v>
+        <v>99</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="E50" t="s">
-        <v>69</v>
-      </c>
-      <c r="F50">
-        <v>1995</v>
+        <v>101</v>
       </c>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>11</v>
+        <v>117</v>
       </c>
       <c r="B51" t="s">
-        <v>25</v>
+        <v>55</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D51" t="s">
-        <v>95</v>
-      </c>
-      <c r="E51" t="s">
-        <v>10</v>
-      </c>
-      <c r="F51">
-        <v>2007</v>
-      </c>
-      <c r="H51" t="s">
-        <v>16</v>
+        <v>118</v>
       </c>
       <c r="I51" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J51" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A52" t="s">
-        <v>97</v>
+      <c r="A52" s="1" t="s">
+        <v>23</v>
       </c>
       <c r="B52" t="s">
-        <v>129</v>
+        <v>25</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>98</v>
+        <v>53</v>
       </c>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>157</v>
+        <v>96</v>
       </c>
       <c r="B53" t="s">
         <v>25</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>155</v>
+        <v>90</v>
+      </c>
+      <c r="E53" t="s">
+        <v>69</v>
+      </c>
+      <c r="F53">
+        <v>1995</v>
       </c>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>102</v>
+        <v>11</v>
       </c>
       <c r="B54" t="s">
-        <v>99</v>
+        <v>25</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>103</v>
+        <v>12</v>
+      </c>
+      <c r="D54" t="s">
+        <v>95</v>
+      </c>
+      <c r="E54" t="s">
+        <v>10</v>
+      </c>
+      <c r="F54">
+        <v>2007</v>
+      </c>
+      <c r="H54" t="s">
+        <v>16</v>
+      </c>
+      <c r="I54" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>138</v>
+        <v>97</v>
       </c>
       <c r="B55" t="s">
-        <v>119</v>
+        <v>129</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>139</v>
+        <v>98</v>
       </c>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B56" t="s">
-        <v>119</v>
+        <v>25</v>
       </c>
       <c r="C56" s="2" t="s">
         <v>155</v>
@@ -1817,73 +1865,46 @@
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>57</v>
+        <v>102</v>
       </c>
       <c r="B57" t="s">
-        <v>129</v>
+        <v>99</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>58</v>
+        <v>103</v>
       </c>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>130</v>
+        <v>138</v>
       </c>
       <c r="B58" t="s">
         <v>119</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="E58" t="s">
-        <v>132</v>
-      </c>
-      <c r="F58">
-        <v>1945</v>
-      </c>
-      <c r="G58">
-        <v>2008</v>
-      </c>
-      <c r="I58" t="s">
-        <v>20</v>
+        <v>139</v>
       </c>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>149</v>
+        <v>156</v>
       </c>
       <c r="B59" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>148</v>
+        <v>155</v>
       </c>
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>35</v>
+        <v>57</v>
       </c>
       <c r="B60" t="s">
-        <v>25</v>
+        <v>129</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="D60" t="s">
-        <v>37</v>
-      </c>
-      <c r="E60" t="s">
-        <v>14</v>
-      </c>
-      <c r="F60">
-        <v>2001</v>
-      </c>
-      <c r="H60" t="s">
-        <v>16</v>
-      </c>
-      <c r="I60" t="s">
-        <v>20</v>
+        <v>58</v>
       </c>
       <c r="J60" t="s">
         <v>17</v>
@@ -1891,41 +1912,59 @@
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>186</v>
+        <v>130</v>
       </c>
       <c r="B61" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>187</v>
+        <v>131</v>
+      </c>
+      <c r="E61" t="s">
+        <v>132</v>
+      </c>
+      <c r="F61">
+        <v>1945</v>
+      </c>
+      <c r="G61">
+        <v>2008</v>
+      </c>
+      <c r="I61" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="B62" t="s">
-        <v>60</v>
+        <v>129</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="F62">
-        <v>1800</v>
-      </c>
-      <c r="G62">
-        <v>2013</v>
+        <v>148</v>
       </c>
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>123</v>
+        <v>35</v>
       </c>
       <c r="B63" t="s">
-        <v>119</v>
+        <v>25</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>122</v>
+        <v>36</v>
+      </c>
+      <c r="D63" t="s">
+        <v>37</v>
+      </c>
+      <c r="E63" t="s">
+        <v>14</v>
+      </c>
+      <c r="F63">
+        <v>2001</v>
+      </c>
+      <c r="H63" t="s">
+        <v>16</v>
       </c>
       <c r="I63" t="s">
         <v>20</v>
@@ -1933,52 +1972,55 @@
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>142</v>
+        <v>186</v>
       </c>
       <c r="B64" t="s">
-        <v>60</v>
+        <v>129</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>143</v>
+        <v>187</v>
       </c>
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>158</v>
+        <v>145</v>
       </c>
       <c r="B65" t="s">
-        <v>129</v>
+        <v>60</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>155</v>
+        <v>144</v>
+      </c>
+      <c r="F65">
+        <v>1800</v>
+      </c>
+      <c r="G65">
+        <v>2013</v>
       </c>
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>195</v>
+        <v>123</v>
       </c>
       <c r="B66" t="s">
-        <v>99</v>
+        <v>119</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>194</v>
+        <v>122</v>
+      </c>
+      <c r="I66" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>109</v>
+        <v>142</v>
       </c>
       <c r="B67" t="s">
-        <v>25</v>
+        <v>60</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="E67" t="s">
-        <v>111</v>
-      </c>
-      <c r="F67">
-        <v>1956</v>
+        <v>143</v>
       </c>
       <c r="J67" t="s">
         <v>17</v>
@@ -1986,19 +2028,13 @@
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>91</v>
+        <v>158</v>
       </c>
       <c r="B68" t="s">
-        <v>25</v>
+        <v>129</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="E68" t="s">
-        <v>92</v>
-      </c>
-      <c r="F68">
-        <v>1999</v>
+        <v>155</v>
       </c>
       <c r="J68" t="s">
         <v>18</v>
@@ -2006,202 +2042,250 @@
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>162</v>
+        <v>195</v>
       </c>
       <c r="B69" t="s">
-        <v>25</v>
+        <v>99</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>161</v>
+        <v>194</v>
       </c>
     </row>
     <row r="70" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>169</v>
+        <v>109</v>
       </c>
       <c r="B70" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>168</v>
+        <v>110</v>
+      </c>
+      <c r="E70" t="s">
+        <v>111</v>
+      </c>
+      <c r="F70">
+        <v>1956</v>
       </c>
     </row>
     <row r="71" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>66</v>
+        <v>91</v>
       </c>
       <c r="B71" t="s">
         <v>25</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>67</v>
+        <v>93</v>
+      </c>
+      <c r="E71" t="s">
+        <v>92</v>
+      </c>
+      <c r="F71">
+        <v>1999</v>
       </c>
     </row>
     <row r="72" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>140</v>
+        <v>162</v>
       </c>
       <c r="B72" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>141</v>
+        <v>161</v>
       </c>
     </row>
     <row r="73" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="B73" t="s">
-        <v>60</v>
+        <v>40</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
     </row>
     <row r="74" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>133</v>
+        <v>66</v>
       </c>
       <c r="B74" t="s">
-        <v>119</v>
+        <v>25</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>134</v>
+        <v>67</v>
       </c>
     </row>
     <row r="75" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>183</v>
+        <v>140</v>
       </c>
       <c r="B75" t="s">
-        <v>166</v>
+        <v>40</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>182</v>
+        <v>141</v>
       </c>
     </row>
     <row r="76" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>115</v>
+        <v>173</v>
       </c>
       <c r="B76" t="s">
-        <v>129</v>
+        <v>60</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>116</v>
+        <v>172</v>
       </c>
     </row>
     <row r="77" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>13</v>
+        <v>133</v>
       </c>
       <c r="B77" t="s">
-        <v>25</v>
+        <v>119</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="D77" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="E77" t="s">
-        <v>14</v>
-      </c>
-      <c r="F77">
-        <v>1981</v>
-      </c>
-      <c r="H77" t="s">
-        <v>16</v>
-      </c>
-      <c r="I77" t="s">
-        <v>20</v>
+        <v>134</v>
       </c>
       <c r="J77" t="s">
         <v>17</v>
       </c>
     </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A78" t="s">
+        <v>183</v>
+      </c>
+      <c r="B78" t="s">
+        <v>166</v>
+      </c>
+      <c r="C78" s="2" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A79" t="s">
+        <v>115</v>
+      </c>
+      <c r="B79" t="s">
+        <v>129</v>
+      </c>
+      <c r="C79" s="2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A80" t="s">
+        <v>13</v>
+      </c>
+      <c r="B80" t="s">
+        <v>25</v>
+      </c>
+      <c r="C80" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D80" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E80" t="s">
+        <v>14</v>
+      </c>
+      <c r="F80">
+        <v>1981</v>
+      </c>
+      <c r="H80" t="s">
+        <v>16</v>
+      </c>
+      <c r="I80" t="s">
+        <v>20</v>
+      </c>
+    </row>
   </sheetData>
-  <sortState ref="A2:J77">
+  <sortState ref="A2:I80">
     <sortCondition ref="A2"/>
   </sortState>
   <hyperlinks>
     <hyperlink ref="C3" r:id="rId1"/>
-    <hyperlink ref="C40" r:id="rId2"/>
+    <hyperlink ref="C42" r:id="rId2"/>
     <hyperlink ref="C4" r:id="rId3"/>
     <hyperlink ref="C7" r:id="rId4"/>
-    <hyperlink ref="C51" r:id="rId5"/>
-    <hyperlink ref="C60" r:id="rId6"/>
-    <hyperlink ref="C77" r:id="rId7"/>
+    <hyperlink ref="C54" r:id="rId5"/>
+    <hyperlink ref="C63" r:id="rId6"/>
+    <hyperlink ref="C80" r:id="rId7"/>
     <hyperlink ref="C26" r:id="rId8"/>
     <hyperlink ref="C22" r:id="rId9"/>
-    <hyperlink ref="C31" r:id="rId10"/>
-    <hyperlink ref="C38" r:id="rId11"/>
+    <hyperlink ref="C33" r:id="rId10"/>
+    <hyperlink ref="C40" r:id="rId11"/>
     <hyperlink ref="C2" r:id="rId12"/>
     <hyperlink ref="C13" r:id="rId13"/>
-    <hyperlink ref="C41" r:id="rId14"/>
-    <hyperlink ref="C49" r:id="rId15"/>
+    <hyperlink ref="C43" r:id="rId14"/>
+    <hyperlink ref="C52" r:id="rId15"/>
     <hyperlink ref="C21" r:id="rId16"/>
-    <hyperlink ref="C57" r:id="rId17"/>
-    <hyperlink ref="C28" r:id="rId18"/>
-    <hyperlink ref="C44" r:id="rId19"/>
+    <hyperlink ref="C60" r:id="rId17"/>
+    <hyperlink ref="C29" r:id="rId18"/>
+    <hyperlink ref="C47" r:id="rId19"/>
     <hyperlink ref="C10" r:id="rId20"/>
-    <hyperlink ref="C71" r:id="rId21"/>
+    <hyperlink ref="C74" r:id="rId21"/>
     <hyperlink ref="C5" r:id="rId22"/>
     <hyperlink ref="C27" r:id="rId23"/>
-    <hyperlink ref="C35" r:id="rId24"/>
-    <hyperlink ref="C32" r:id="rId25"/>
-    <hyperlink ref="C36" r:id="rId26"/>
-    <hyperlink ref="C37" r:id="rId27"/>
-    <hyperlink ref="C42" r:id="rId28"/>
-    <hyperlink ref="C50" r:id="rId29"/>
-    <hyperlink ref="C68" r:id="rId30"/>
-    <hyperlink ref="C52" r:id="rId31"/>
-    <hyperlink ref="C47" r:id="rId32"/>
-    <hyperlink ref="C54" r:id="rId33"/>
-    <hyperlink ref="C43" r:id="rId34"/>
+    <hyperlink ref="C37" r:id="rId24"/>
+    <hyperlink ref="C34" r:id="rId25"/>
+    <hyperlink ref="C38" r:id="rId26"/>
+    <hyperlink ref="C39" r:id="rId27"/>
+    <hyperlink ref="C45" r:id="rId28"/>
+    <hyperlink ref="C53" r:id="rId29"/>
+    <hyperlink ref="C71" r:id="rId30"/>
+    <hyperlink ref="C55" r:id="rId31"/>
+    <hyperlink ref="C50" r:id="rId32"/>
+    <hyperlink ref="C57" r:id="rId33"/>
+    <hyperlink ref="C46" r:id="rId34"/>
     <hyperlink ref="C11" r:id="rId35"/>
-    <hyperlink ref="C67" r:id="rId36"/>
+    <hyperlink ref="C70" r:id="rId36"/>
     <hyperlink ref="C9" r:id="rId37"/>
-    <hyperlink ref="C76" r:id="rId38"/>
-    <hyperlink ref="C48" r:id="rId39"/>
-    <hyperlink ref="C39" r:id="rId40"/>
-    <hyperlink ref="C63" r:id="rId41"/>
+    <hyperlink ref="C79" r:id="rId38"/>
+    <hyperlink ref="C51" r:id="rId39"/>
+    <hyperlink ref="C41" r:id="rId40"/>
+    <hyperlink ref="C66" r:id="rId41"/>
     <hyperlink ref="C12" r:id="rId42"/>
-    <hyperlink ref="C33" r:id="rId43"/>
+    <hyperlink ref="C35" r:id="rId43"/>
     <hyperlink ref="C15" r:id="rId44"/>
-    <hyperlink ref="C58" r:id="rId45"/>
-    <hyperlink ref="C74" r:id="rId46"/>
+    <hyperlink ref="C61" r:id="rId45"/>
+    <hyperlink ref="C77" r:id="rId46"/>
     <hyperlink ref="C19" r:id="rId47" display="http://comparativeconstitutionsproject.org/"/>
-    <hyperlink ref="C55" r:id="rId48"/>
-    <hyperlink ref="C72" r:id="rId49"/>
-    <hyperlink ref="C64" r:id="rId50"/>
-    <hyperlink ref="C62" r:id="rId51"/>
+    <hyperlink ref="C58" r:id="rId48"/>
+    <hyperlink ref="C75" r:id="rId49"/>
+    <hyperlink ref="C67" r:id="rId50"/>
+    <hyperlink ref="C65" r:id="rId51"/>
     <hyperlink ref="C14" r:id="rId52"/>
-    <hyperlink ref="C59" r:id="rId53"/>
-    <hyperlink ref="C30" r:id="rId54"/>
-    <hyperlink ref="C45" r:id="rId55"/>
-    <hyperlink ref="C46" r:id="rId56"/>
-    <hyperlink ref="C56" r:id="rId57"/>
-    <hyperlink ref="C53" r:id="rId58"/>
-    <hyperlink ref="C65" r:id="rId59"/>
+    <hyperlink ref="C62" r:id="rId53"/>
+    <hyperlink ref="C32" r:id="rId54"/>
+    <hyperlink ref="C48" r:id="rId55"/>
+    <hyperlink ref="C49" r:id="rId56"/>
+    <hyperlink ref="C59" r:id="rId57"/>
+    <hyperlink ref="C56" r:id="rId58"/>
+    <hyperlink ref="C68" r:id="rId59"/>
     <hyperlink ref="C23" r:id="rId60"/>
-    <hyperlink ref="C69" r:id="rId61"/>
+    <hyperlink ref="C72" r:id="rId61"/>
     <hyperlink ref="C6" r:id="rId62"/>
     <hyperlink ref="C25" r:id="rId63"/>
-    <hyperlink ref="C70" r:id="rId64"/>
+    <hyperlink ref="C73" r:id="rId64"/>
     <hyperlink ref="C8" r:id="rId65"/>
-    <hyperlink ref="C73" r:id="rId66"/>
+    <hyperlink ref="C76" r:id="rId66"/>
     <hyperlink ref="C17" r:id="rId67"/>
     <hyperlink ref="C16" r:id="rId68"/>
     <hyperlink ref="C18" r:id="rId69"/>
-    <hyperlink ref="C34" r:id="rId70"/>
-    <hyperlink ref="C75" r:id="rId71"/>
+    <hyperlink ref="C36" r:id="rId70"/>
+    <hyperlink ref="C78" r:id="rId71"/>
     <hyperlink ref="C20" r:id="rId72"/>
-    <hyperlink ref="C61" r:id="rId73"/>
+    <hyperlink ref="C64" r:id="rId73"/>
     <hyperlink ref="C24" r:id="rId74"/>
-    <hyperlink ref="C29" r:id="rId75"/>
-    <hyperlink ref="C66" r:id="rId76"/>
+    <hyperlink ref="C31" r:id="rId75"/>
+    <hyperlink ref="C69" r:id="rId76"/>
+    <hyperlink ref="C30" r:id="rId77"/>
+    <hyperlink ref="C28" r:id="rId78"/>
+    <hyperlink ref="C44" r:id="rId79"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
add 45 datasets and two overview links
</commit_message>
<xml_diff>
--- a/PolData.xlsx
+++ b/PolData.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="540" uniqueCount="293">
   <si>
     <t>name</t>
   </si>
@@ -386,9 +386,6 @@
     <t>https://havardhegre.net/iaep/</t>
   </si>
   <si>
-    <t>cabinets</t>
-  </si>
-  <si>
     <t>http://www.erdda.se/index.php/projects/erd/data-archive</t>
   </si>
   <si>
@@ -636,6 +633,279 @@
   </si>
   <si>
     <t>http://www.frdb.org/page/data/scheda/frdb-iza-social-reforms-database/doc_pk/9027</t>
+  </si>
+  <si>
+    <t>http://aiddata.org/data/aiddata-core-research-release-level-1-v3-0</t>
+  </si>
+  <si>
+    <t>AidData</t>
+  </si>
+  <si>
+    <t>http://fundforpeace.org/fsi/data/</t>
+  </si>
+  <si>
+    <t>Fragile States Index</t>
+  </si>
+  <si>
+    <t>https://sites.google.com/site/authoritarianregimedataset/data</t>
+  </si>
+  <si>
+    <t>Authoritarian Regimes Dataset</t>
+  </si>
+  <si>
+    <t>Oil and Gas Data</t>
+  </si>
+  <si>
+    <t>http://dx.doi.org/10.7910/DVN/ZTPW0Y</t>
+  </si>
+  <si>
+    <t>Political Terror Scale</t>
+  </si>
+  <si>
+    <t>http://www.politicalterrorscale.org/Data/Download.html</t>
+  </si>
+  <si>
+    <t>https://mgmt.wharton.upenn.edu/faculty/heniszpolcon/polcondataset/</t>
+  </si>
+  <si>
+    <t>The Political Constraint Index</t>
+  </si>
+  <si>
+    <t>https://www.transparency.org/research/cpi/</t>
+  </si>
+  <si>
+    <t>Corruption Perceptions Index</t>
+  </si>
+  <si>
+    <t>https://www.v-dem.net/en/data/</t>
+  </si>
+  <si>
+    <t>Varieties of Democracy</t>
+  </si>
+  <si>
+    <t>https://www.fraserinstitute.org/economic-freedom/dataset</t>
+  </si>
+  <si>
+    <t>Economic Freedom of the World</t>
+  </si>
+  <si>
+    <t>https://rsf.org/en/ranking_table</t>
+  </si>
+  <si>
+    <t>World Press Freedom Index</t>
+  </si>
+  <si>
+    <t>http://www.ggdc.net/maddison/maddison-project/data.htm</t>
+  </si>
+  <si>
+    <t>Maddison Project Database</t>
+  </si>
+  <si>
+    <t>Forcibly Displaced Populations</t>
+  </si>
+  <si>
+    <t>http://www.systemicpeace.org/inscrdata.html</t>
+  </si>
+  <si>
+    <t>Major Episodes of Political Violence</t>
+  </si>
+  <si>
+    <t>State Failure Problem Set</t>
+  </si>
+  <si>
+    <t>High Casualty Terrorist Bombings</t>
+  </si>
+  <si>
+    <t>Memberships in Conventional Intergovernmental Organizations</t>
+  </si>
+  <si>
+    <t>State Fragility Index</t>
+  </si>
+  <si>
+    <t>http://ec.europa.eu/eurostat/data/bulkdownload</t>
+  </si>
+  <si>
+    <t>Eurostat</t>
+  </si>
+  <si>
+    <t>Perceptions of Electoral Integrity</t>
+  </si>
+  <si>
+    <t>https://sites.google.com/site/electoralintegrityproject4/projects/expert-survey-2</t>
+  </si>
+  <si>
+    <t>Electoral Systems and the Personal Vote</t>
+  </si>
+  <si>
+    <t>http://hdl.handle.net/1902.1/17901</t>
+  </si>
+  <si>
+    <t>governance</t>
+  </si>
+  <si>
+    <t>Democratic Innovations Data</t>
+  </si>
+  <si>
+    <t>Infrastructure Governance Indicators</t>
+  </si>
+  <si>
+    <t>European Union Indicators</t>
+  </si>
+  <si>
+    <t>Administrative Capacities</t>
+  </si>
+  <si>
+    <t>Governance Challenges Indicators</t>
+  </si>
+  <si>
+    <t>https://www.hertie-school.org/en/governancereport/govreport-indicators/</t>
+  </si>
+  <si>
+    <t>http://mo.ibrahim.foundation/iiag/downloads/</t>
+  </si>
+  <si>
+    <t>Ibrahim Index of African Governance</t>
+  </si>
+  <si>
+    <t>National Elections Across Democracy and Autocracy</t>
+  </si>
+  <si>
+    <t>http://www.nelda.co/</t>
+  </si>
+  <si>
+    <t>free, online registration</t>
+  </si>
+  <si>
+    <t>free, online form</t>
+  </si>
+  <si>
+    <t>other</t>
+  </si>
+  <si>
+    <t>http://epi.yale.edu/downloads</t>
+  </si>
+  <si>
+    <t>Environmental Performance Index</t>
+  </si>
+  <si>
+    <t>http://www.uva-aias.net/en/ictwss</t>
+  </si>
+  <si>
+    <t>Institutional Characteristics of Trade Unions, Wage Setting, State Intervention and Social Pacts</t>
+  </si>
+  <si>
+    <t>51 countries</t>
+  </si>
+  <si>
+    <t>State Antiquity Index</t>
+  </si>
+  <si>
+    <t>http://www.brown.edu/Departments/Economics/Faculty/Louis_Putterman/antiquity%20index.htm</t>
+  </si>
+  <si>
+    <t>149 countries</t>
+  </si>
+  <si>
+    <t>cabinets and parliaments</t>
+  </si>
+  <si>
+    <t>Basic data on parliaments</t>
+  </si>
+  <si>
+    <t>http://archive.ipu.org/gpr-e/downloads/index.htm</t>
+  </si>
+  <si>
+    <t>Age, gender and profession of parliamentarians</t>
+  </si>
+  <si>
+    <t>World Migration Matrix</t>
+  </si>
+  <si>
+    <t>http://www.brown.edu/Departments/Economics/Faculty/Louis_Putterman/world%20migration%20matrix.htm</t>
+  </si>
+  <si>
+    <t>165 countries</t>
+  </si>
+  <si>
+    <t>http://globalization.kof.ethz.ch/</t>
+  </si>
+  <si>
+    <t>KOF Globalization Index</t>
+  </si>
+  <si>
+    <t>207 countries</t>
+  </si>
+  <si>
+    <t>economic globalization, political globalization, social globalization</t>
+  </si>
+  <si>
+    <t>Institutional Quality Dataset</t>
+  </si>
+  <si>
+    <t>https://sites.google.com/site/aljazkuncic/research</t>
+  </si>
+  <si>
+    <t>https://data.worldbank.org/data-catalog/worldwide-governance-indicators</t>
+  </si>
+  <si>
+    <t>The Worldwide Governance Indicators</t>
+  </si>
+  <si>
+    <t>Rule of Law Index</t>
+  </si>
+  <si>
+    <t>https://worldjusticeproject.org/our-work/wjp-rule-law-index/wjp-rule-law-index-2016/current-historical-data</t>
+  </si>
+  <si>
+    <t>Expanded Trade and GDP Data</t>
+  </si>
+  <si>
+    <t>http://privatewww.essex.ac.uk/~ksg/exptradegdp.html</t>
+  </si>
+  <si>
+    <t>Measuring Income Inequality Database</t>
+  </si>
+  <si>
+    <t>http://econ.worldbank.org/WBSITE/EXTERNAL/EXTDEC/EXTRESEARCH/0,,contentMDK:20699070~pagePK:64214825~piPK:64214943~theSitePK:469382,00.html</t>
+  </si>
+  <si>
+    <t>138 countries</t>
+  </si>
+  <si>
+    <t>Global Integrity Report</t>
+  </si>
+  <si>
+    <t>https://www.globalintegrity.org/downloads/</t>
+  </si>
+  <si>
+    <t>World Wealth and Income Database</t>
+  </si>
+  <si>
+    <t>http://wid.world/data/</t>
+  </si>
+  <si>
+    <t>Fractionalization</t>
+  </si>
+  <si>
+    <t>http://www.anderson.ucla.edu/faculty_pages/romain.wacziarg/papersum.html</t>
+  </si>
+  <si>
+    <t>Religion and State Project Constitutions Dataset</t>
+  </si>
+  <si>
+    <t>http://www.thearda.com/archive/files/Descriptions/RASCONS.asp</t>
+  </si>
+  <si>
+    <t>National Accounts Main Aggregates Database</t>
+  </si>
+  <si>
+    <t>https://unstats.un.org/unsd/snaama/dnlList.asp</t>
+  </si>
+  <si>
+    <t>https://www.wider.unu.edu/database/additional-data-files-grd</t>
+  </si>
+  <si>
+    <t>Government Revenue Dataset</t>
   </si>
 </sst>
 </file>
@@ -967,10 +1237,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J80"/>
+  <dimension ref="A1:J125"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="A74" sqref="A74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1020,180 +1290,201 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>30</v>
+        <v>241</v>
       </c>
       <c r="B2" t="s">
-        <v>25</v>
+        <v>237</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="E2" t="s">
-        <v>68</v>
-      </c>
-      <c r="F2">
-        <v>1999</v>
+        <v>243</v>
+      </c>
+      <c r="H2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I2" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B3" t="s">
         <v>25</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="E3" t="s">
-        <v>34</v>
+        <v>68</v>
       </c>
       <c r="F3">
-        <v>1948</v>
-      </c>
-      <c r="H3" t="s">
-        <v>16</v>
-      </c>
-      <c r="I3" t="s">
-        <v>20</v>
-      </c>
-      <c r="J3" t="s">
-        <v>44</v>
+        <v>1999</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>29</v>
+        <v>262</v>
       </c>
       <c r="B4" t="s">
-        <v>25</v>
+        <v>128</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="E4" t="s">
-        <v>69</v>
-      </c>
-      <c r="F4">
-        <v>2004</v>
+        <v>261</v>
+      </c>
+      <c r="H4" t="s">
+        <v>16</v>
+      </c>
+      <c r="I4" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>70</v>
+        <v>203</v>
       </c>
       <c r="B5" t="s">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="E5" t="s">
-        <v>72</v>
+        <v>202</v>
       </c>
       <c r="F5">
-        <v>2006</v>
+        <v>1947</v>
+      </c>
+      <c r="G5">
+        <v>2013</v>
+      </c>
+      <c r="H5" t="s">
+        <v>16</v>
+      </c>
+      <c r="I5" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>164</v>
+        <v>33</v>
       </c>
       <c r="B6" t="s">
-        <v>83</v>
+        <v>25</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>163</v>
+        <v>43</v>
+      </c>
+      <c r="E6" t="s">
+        <v>34</v>
+      </c>
+      <c r="F6">
+        <v>1948</v>
+      </c>
+      <c r="H6" t="s">
+        <v>16</v>
+      </c>
+      <c r="I6" t="s">
+        <v>20</v>
+      </c>
+      <c r="J6" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B7" t="s">
         <v>25</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E7" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="F7">
-        <v>2001</v>
+        <v>2004</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>171</v>
+        <v>70</v>
       </c>
       <c r="B8" t="s">
-        <v>60</v>
+        <v>25</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>170</v>
+        <v>71</v>
+      </c>
+      <c r="E8" t="s">
+        <v>72</v>
+      </c>
+      <c r="F8">
+        <v>2006</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>113</v>
+        <v>163</v>
       </c>
       <c r="B9" t="s">
-        <v>25</v>
+        <v>83</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="E9" t="s">
-        <v>112</v>
-      </c>
-      <c r="F9">
-        <v>1964</v>
+        <v>162</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>64</v>
+        <v>31</v>
       </c>
       <c r="B10" t="s">
         <v>25</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>65</v>
+        <v>46</v>
+      </c>
+      <c r="E10" t="s">
+        <v>73</v>
       </c>
       <c r="F10">
-        <v>1991</v>
-      </c>
-      <c r="G10">
-        <v>2009</v>
-      </c>
-      <c r="J10" t="s">
-        <v>18</v>
+        <v>2001</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>107</v>
+        <v>207</v>
       </c>
       <c r="B11" t="s">
-        <v>25</v>
+        <v>60</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="E11" t="s">
-        <v>112</v>
+        <v>206</v>
+      </c>
+      <c r="F11">
+        <v>1972</v>
+      </c>
+      <c r="G11">
+        <v>2014</v>
+      </c>
+      <c r="H11" t="s">
+        <v>16</v>
+      </c>
+      <c r="I11" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>124</v>
+        <v>260</v>
       </c>
       <c r="B12" t="s">
-        <v>119</v>
+        <v>259</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>122</v>
+        <v>261</v>
+      </c>
+      <c r="H12" t="s">
+        <v>16</v>
       </c>
       <c r="I12" t="s">
         <v>20</v>
@@ -1201,733 +1492,781 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>32</v>
+        <v>170</v>
       </c>
       <c r="B13" t="s">
-        <v>25</v>
+        <v>60</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="E13" t="s">
-        <v>74</v>
-      </c>
-      <c r="F13">
-        <v>2008</v>
+        <v>169</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>147</v>
+        <v>113</v>
       </c>
       <c r="B14" t="s">
-        <v>129</v>
+        <v>25</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>146</v>
+        <v>114</v>
+      </c>
+      <c r="E14" t="s">
+        <v>112</v>
+      </c>
+      <c r="F14">
+        <v>1964</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>128</v>
+        <v>64</v>
       </c>
       <c r="B15" t="s">
-        <v>119</v>
+        <v>25</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="I15" t="s">
-        <v>20</v>
+        <v>65</v>
+      </c>
+      <c r="F15">
+        <v>1991</v>
+      </c>
+      <c r="G15">
+        <v>2009</v>
+      </c>
+      <c r="J15" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>174</v>
+        <v>107</v>
       </c>
       <c r="B16" t="s">
-        <v>129</v>
+        <v>25</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>176</v>
+        <v>108</v>
+      </c>
+      <c r="E16" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>175</v>
+        <v>123</v>
       </c>
       <c r="B17" t="s">
-        <v>86</v>
+        <v>259</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>176</v>
-      </c>
-      <c r="E17" t="s">
-        <v>177</v>
+        <v>121</v>
+      </c>
+      <c r="I17" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>178</v>
+        <v>32</v>
       </c>
       <c r="B18" t="s">
         <v>25</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>176</v>
+        <v>51</v>
       </c>
       <c r="E18" t="s">
-        <v>179</v>
+        <v>74</v>
+      </c>
+      <c r="F18">
+        <v>2008</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>136</v>
+        <v>146</v>
       </c>
       <c r="B19" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>137</v>
+        <v>145</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>185</v>
+        <v>127</v>
       </c>
       <c r="B20" t="s">
-        <v>129</v>
+        <v>259</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>184</v>
+        <v>121</v>
+      </c>
+      <c r="I20" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>54</v>
+        <v>173</v>
       </c>
       <c r="B21" t="s">
-        <v>55</v>
+        <v>128</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>56</v>
+        <v>175</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A22" s="1" t="s">
-        <v>22</v>
+      <c r="A22" t="s">
+        <v>174</v>
       </c>
       <c r="B22" t="s">
-        <v>25</v>
+        <v>86</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>47</v>
+        <v>175</v>
+      </c>
+      <c r="E22" t="s">
+        <v>176</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>159</v>
+        <v>177</v>
       </c>
       <c r="B23" t="s">
-        <v>99</v>
+        <v>25</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>160</v>
+        <v>175</v>
+      </c>
+      <c r="E23" t="s">
+        <v>178</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>188</v>
+        <v>135</v>
       </c>
       <c r="B24" t="s">
-        <v>99</v>
+        <v>134</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>189</v>
-      </c>
-      <c r="F24">
-        <v>1960</v>
-      </c>
-      <c r="G24">
-        <v>2011</v>
-      </c>
-      <c r="H24" t="s">
-        <v>16</v>
-      </c>
-      <c r="I24" t="s">
-        <v>190</v>
+        <v>136</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>165</v>
+        <v>184</v>
       </c>
       <c r="B25" t="s">
-        <v>166</v>
+        <v>128</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>167</v>
+        <v>183</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>39</v>
+        <v>54</v>
       </c>
       <c r="B26" t="s">
-        <v>40</v>
+        <v>55</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="E26" t="s">
-        <v>14</v>
-      </c>
-      <c r="F26">
-        <v>1816</v>
-      </c>
-      <c r="G26">
-        <v>2007</v>
-      </c>
-      <c r="H26" t="s">
-        <v>16</v>
-      </c>
-      <c r="I26" t="s">
-        <v>20</v>
+        <v>56</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
-        <v>75</v>
+      <c r="A27" s="1" t="s">
+        <v>22</v>
       </c>
       <c r="B27" t="s">
         <v>25</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="E27" t="s">
-        <v>77</v>
-      </c>
-      <c r="F27">
-        <v>1971</v>
+        <v>47</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>198</v>
+        <v>158</v>
       </c>
       <c r="B28" t="s">
-        <v>55</v>
+        <v>99</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>199</v>
-      </c>
-      <c r="E28" t="s">
-        <v>200</v>
-      </c>
-      <c r="F28">
-        <v>1975</v>
-      </c>
-      <c r="G28">
-        <v>2015</v>
-      </c>
-      <c r="H28" t="s">
-        <v>16</v>
-      </c>
-      <c r="I28" t="s">
-        <v>20</v>
+        <v>159</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>59</v>
+        <v>187</v>
       </c>
       <c r="B29" t="s">
-        <v>60</v>
+        <v>99</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>61</v>
+        <v>188</v>
+      </c>
+      <c r="F29">
+        <v>1960</v>
+      </c>
+      <c r="G29">
+        <v>2011</v>
+      </c>
+      <c r="H29" t="s">
+        <v>16</v>
+      </c>
+      <c r="I29" t="s">
+        <v>189</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>197</v>
+        <v>164</v>
       </c>
       <c r="B30" t="s">
+        <v>165</v>
+      </c>
+      <c r="C30" s="2" t="s">
         <v>166</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="F30">
-        <v>1946</v>
-      </c>
-      <c r="G30">
-        <v>2016</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>192</v>
+        <v>39</v>
       </c>
       <c r="B31" t="s">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>191</v>
+        <v>41</v>
       </c>
       <c r="E31" t="s">
-        <v>193</v>
+        <v>14</v>
+      </c>
+      <c r="F31">
+        <v>1816</v>
+      </c>
+      <c r="G31">
+        <v>2007</v>
+      </c>
+      <c r="H31" t="s">
+        <v>16</v>
+      </c>
+      <c r="I31" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>150</v>
+        <v>215</v>
       </c>
       <c r="B32" t="s">
-        <v>129</v>
+        <v>237</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
+        <v>214</v>
+      </c>
+      <c r="F32">
+        <v>1995</v>
+      </c>
+      <c r="H32" t="s">
+        <v>16</v>
+      </c>
+      <c r="I32" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>28</v>
+        <v>75</v>
       </c>
       <c r="B33" t="s">
         <v>25</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
+        <v>76</v>
+      </c>
+      <c r="E33" t="s">
+        <v>77</v>
+      </c>
+      <c r="F33">
+        <v>1971</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>80</v>
+        <v>197</v>
       </c>
       <c r="B34" t="s">
-        <v>129</v>
+        <v>55</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>81</v>
+        <v>198</v>
       </c>
       <c r="E34" t="s">
-        <v>9</v>
+        <v>199</v>
       </c>
       <c r="F34">
-        <v>1979</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
+        <v>1975</v>
+      </c>
+      <c r="G34">
+        <v>2015</v>
+      </c>
+      <c r="H34" t="s">
+        <v>16</v>
+      </c>
+      <c r="I34" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>126</v>
+        <v>59</v>
       </c>
       <c r="B35" t="s">
-        <v>125</v>
+        <v>60</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>180</v>
+        <v>196</v>
       </c>
       <c r="B36" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
+        <v>195</v>
+      </c>
+      <c r="F36">
+        <v>1946</v>
+      </c>
+      <c r="G36">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>78</v>
+        <v>238</v>
       </c>
       <c r="B37" t="s">
+        <v>237</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="H37" t="s">
+        <v>16</v>
+      </c>
+      <c r="I37" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>219</v>
+      </c>
+      <c r="B38" t="s">
+        <v>124</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="F38">
+        <v>1970</v>
+      </c>
+      <c r="G38">
+        <v>2015</v>
+      </c>
+      <c r="H38" t="s">
+        <v>16</v>
+      </c>
+      <c r="I38" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>191</v>
+      </c>
+      <c r="B39" t="s">
         <v>25</v>
       </c>
-      <c r="C37" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="E37" t="s">
-        <v>9</v>
-      </c>
-      <c r="F37">
-        <v>1979</v>
-      </c>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A38" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="B38" t="s">
-        <v>83</v>
-      </c>
-      <c r="C38" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="E38" t="s">
-        <v>9</v>
-      </c>
-      <c r="F38">
-        <v>1979</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A39" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="B39" t="s">
-        <v>86</v>
-      </c>
       <c r="C39" s="2" t="s">
-        <v>87</v>
+        <v>190</v>
       </c>
       <c r="E39" t="s">
-        <v>9</v>
-      </c>
-      <c r="F39">
-        <v>1979</v>
-      </c>
-      <c r="G39">
-        <v>2009</v>
-      </c>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>27</v>
+        <v>235</v>
       </c>
       <c r="B40" t="s">
-        <v>25</v>
+        <v>60</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="J40" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
+        <v>236</v>
+      </c>
+      <c r="H40" t="s">
+        <v>16</v>
+      </c>
+      <c r="I40" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>121</v>
+        <v>252</v>
       </c>
       <c r="B41" t="s">
-        <v>119</v>
+        <v>250</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>120</v>
+        <v>251</v>
+      </c>
+      <c r="H41" t="s">
+        <v>16</v>
       </c>
       <c r="I41" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>5</v>
+        <v>149</v>
       </c>
       <c r="B42" t="s">
-        <v>25</v>
+        <v>128</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D42" t="s">
-        <v>94</v>
-      </c>
-      <c r="E42" t="s">
-        <v>9</v>
-      </c>
-      <c r="F42">
-        <v>2002</v>
-      </c>
-      <c r="H42" t="s">
-        <v>16</v>
-      </c>
-      <c r="I42" t="s">
-        <v>20</v>
-      </c>
-      <c r="J42" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A43" s="1" t="s">
-        <v>26</v>
+        <v>150</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>28</v>
       </c>
       <c r="B43" t="s">
         <v>25</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>201</v>
+        <v>80</v>
       </c>
       <c r="B44" t="s">
-        <v>99</v>
+        <v>128</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>202</v>
+        <v>81</v>
+      </c>
+      <c r="E44" t="s">
+        <v>9</v>
       </c>
       <c r="F44">
-        <v>1980</v>
-      </c>
-      <c r="G44">
-        <v>2007</v>
-      </c>
-      <c r="J44" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
+        <v>1979</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>89</v>
+        <v>125</v>
       </c>
       <c r="B45" t="s">
-        <v>25</v>
+        <v>124</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="E45" t="s">
-        <v>34</v>
-      </c>
-      <c r="F45">
-        <v>1972</v>
-      </c>
-      <c r="H45" t="s">
-        <v>16</v>
-      </c>
-      <c r="I45" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>104</v>
+        <v>179</v>
       </c>
       <c r="B46" t="s">
-        <v>25</v>
+        <v>165</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="E46" t="s">
-        <v>105</v>
-      </c>
-      <c r="F46">
-        <v>1980</v>
-      </c>
-    </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.2">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>62</v>
+        <v>78</v>
       </c>
       <c r="B47" t="s">
         <v>25</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A48" t="s">
-        <v>152</v>
+        <v>79</v>
+      </c>
+      <c r="E47" t="s">
+        <v>9</v>
+      </c>
+      <c r="F47">
+        <v>1979</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A48" s="3" t="s">
+        <v>82</v>
       </c>
       <c r="B48" t="s">
-        <v>40</v>
+        <v>83</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>153</v>
+        <v>84</v>
       </c>
       <c r="E48" t="s">
-        <v>14</v>
+        <v>9</v>
+      </c>
+      <c r="F48">
+        <v>1979</v>
       </c>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A49" t="s">
-        <v>154</v>
+      <c r="A49" s="3" t="s">
+        <v>85</v>
       </c>
       <c r="B49" t="s">
-        <v>119</v>
+        <v>86</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>155</v>
+        <v>87</v>
+      </c>
+      <c r="E49" t="s">
+        <v>9</v>
+      </c>
+      <c r="F49">
+        <v>1979</v>
+      </c>
+      <c r="G49">
+        <v>2009</v>
       </c>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>100</v>
+        <v>27</v>
       </c>
       <c r="B50" t="s">
-        <v>99</v>
+        <v>25</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>101</v>
+        <v>49</v>
+      </c>
+      <c r="J50" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="B51" t="s">
-        <v>55</v>
+        <v>259</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="I51" t="s">
         <v>20</v>
       </c>
-      <c r="J51" t="s">
-        <v>18</v>
-      </c>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A52" s="1" t="s">
-        <v>23</v>
+      <c r="A52" t="s">
+        <v>5</v>
       </c>
       <c r="B52" t="s">
         <v>25</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>53</v>
+        <v>6</v>
+      </c>
+      <c r="D52" t="s">
+        <v>94</v>
+      </c>
+      <c r="E52" t="s">
+        <v>9</v>
+      </c>
+      <c r="F52">
+        <v>2002</v>
+      </c>
+      <c r="H52" t="s">
+        <v>16</v>
+      </c>
+      <c r="I52" t="s">
+        <v>248</v>
+      </c>
+      <c r="J52" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>96</v>
+        <v>240</v>
       </c>
       <c r="B53" t="s">
-        <v>25</v>
+        <v>237</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="E53" t="s">
-        <v>69</v>
-      </c>
-      <c r="F53">
-        <v>1995</v>
+        <v>243</v>
+      </c>
+      <c r="H53" t="s">
+        <v>16</v>
+      </c>
+      <c r="I53" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A54" t="s">
-        <v>11</v>
+      <c r="A54" s="1" t="s">
+        <v>26</v>
       </c>
       <c r="B54" t="s">
         <v>25</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D54" t="s">
-        <v>95</v>
-      </c>
-      <c r="E54" t="s">
-        <v>10</v>
-      </c>
-      <c r="F54">
-        <v>2007</v>
-      </c>
-      <c r="H54" t="s">
-        <v>16</v>
-      </c>
-      <c r="I54" t="s">
-        <v>21</v>
+        <v>52</v>
       </c>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>97</v>
+        <v>232</v>
       </c>
       <c r="B55" t="s">
-        <v>129</v>
+        <v>250</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>98</v>
+        <v>231</v>
       </c>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>157</v>
+        <v>276</v>
       </c>
       <c r="B56" t="s">
-        <v>25</v>
+        <v>124</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>155</v>
+        <v>277</v>
+      </c>
+      <c r="F56">
+        <v>1948</v>
+      </c>
+      <c r="G56">
+        <v>2000</v>
+      </c>
+      <c r="H56" t="s">
+        <v>16</v>
+      </c>
+      <c r="I56" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>102</v>
+        <v>224</v>
       </c>
       <c r="B57" t="s">
-        <v>99</v>
+        <v>40</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>103</v>
+        <v>225</v>
+      </c>
+      <c r="F57">
+        <v>1964</v>
+      </c>
+      <c r="G57">
+        <v>2008</v>
+      </c>
+      <c r="H57" t="s">
+        <v>16</v>
+      </c>
+      <c r="I57" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>138</v>
+        <v>285</v>
       </c>
       <c r="B58" t="s">
-        <v>119</v>
+        <v>250</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>139</v>
+        <v>286</v>
+      </c>
+      <c r="H58" t="s">
+        <v>16</v>
+      </c>
+      <c r="I58" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>156</v>
+        <v>205</v>
       </c>
       <c r="B59" t="s">
-        <v>119</v>
+        <v>40</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>155</v>
+        <v>204</v>
+      </c>
+      <c r="F59">
+        <v>2006</v>
       </c>
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>57</v>
+        <v>200</v>
       </c>
       <c r="B60" t="s">
-        <v>129</v>
+        <v>99</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>58</v>
+        <v>201</v>
+      </c>
+      <c r="F60">
+        <v>1980</v>
+      </c>
+      <c r="G60">
+        <v>2007</v>
       </c>
       <c r="J60" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>130</v>
+        <v>89</v>
       </c>
       <c r="B61" t="s">
-        <v>119</v>
+        <v>25</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>131</v>
+        <v>88</v>
       </c>
       <c r="E61" t="s">
-        <v>132</v>
+        <v>34</v>
       </c>
       <c r="F61">
-        <v>1945</v>
-      </c>
-      <c r="G61">
-        <v>2008</v>
+        <v>1972</v>
+      </c>
+      <c r="H61" t="s">
+        <v>16</v>
       </c>
       <c r="I61" t="s">
         <v>20</v>
@@ -1935,78 +2274,75 @@
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>149</v>
+        <v>104</v>
       </c>
       <c r="B62" t="s">
-        <v>129</v>
+        <v>25</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>148</v>
+        <v>106</v>
+      </c>
+      <c r="E62" t="s">
+        <v>105</v>
+      </c>
+      <c r="F62">
+        <v>1980</v>
       </c>
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>35</v>
+        <v>62</v>
       </c>
       <c r="B63" t="s">
         <v>25</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="D63" t="s">
-        <v>37</v>
-      </c>
-      <c r="E63" t="s">
-        <v>14</v>
-      </c>
-      <c r="F63">
-        <v>2001</v>
-      </c>
-      <c r="H63" t="s">
-        <v>16</v>
-      </c>
-      <c r="I63" t="s">
-        <v>20</v>
+        <v>63</v>
       </c>
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>186</v>
+        <v>281</v>
       </c>
       <c r="B64" t="s">
-        <v>129</v>
+        <v>237</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>187</v>
+        <v>282</v>
+      </c>
+      <c r="H64" t="s">
+        <v>16</v>
+      </c>
+      <c r="I64" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>145</v>
+        <v>151</v>
       </c>
       <c r="B65" t="s">
-        <v>60</v>
+        <v>40</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="F65">
-        <v>1800</v>
-      </c>
-      <c r="G65">
-        <v>2013</v>
+        <v>152</v>
+      </c>
+      <c r="E65" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>123</v>
+        <v>242</v>
       </c>
       <c r="B66" t="s">
-        <v>119</v>
+        <v>237</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>122</v>
+        <v>243</v>
+      </c>
+      <c r="H66" t="s">
+        <v>16</v>
       </c>
       <c r="I66" t="s">
         <v>20</v>
@@ -2014,278 +2350,1169 @@
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>142</v>
+        <v>292</v>
       </c>
       <c r="B67" t="s">
-        <v>60</v>
+        <v>99</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="J67" t="s">
-        <v>17</v>
+        <v>291</v>
+      </c>
+      <c r="H67" t="s">
+        <v>16</v>
+      </c>
+      <c r="I67" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="B68" t="s">
-        <v>129</v>
+        <v>259</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>155</v>
-      </c>
-      <c r="J68" t="s">
-        <v>18</v>
+        <v>154</v>
       </c>
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>195</v>
+        <v>228</v>
       </c>
       <c r="B69" t="s">
-        <v>99</v>
+        <v>40</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>194</v>
+        <v>225</v>
+      </c>
+      <c r="F69">
+        <v>1989</v>
+      </c>
+      <c r="G69">
+        <v>2017</v>
+      </c>
+      <c r="H69" t="s">
+        <v>16</v>
+      </c>
+      <c r="I69" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="70" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>109</v>
+        <v>245</v>
       </c>
       <c r="B70" t="s">
-        <v>25</v>
+        <v>237</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="E70" t="s">
-        <v>111</v>
-      </c>
-      <c r="F70">
-        <v>1956</v>
+        <v>244</v>
+      </c>
+      <c r="H70" t="s">
+        <v>16</v>
+      </c>
+      <c r="I70" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="71" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>91</v>
+        <v>100</v>
       </c>
       <c r="B71" t="s">
-        <v>25</v>
+        <v>99</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="E71" t="s">
-        <v>92</v>
-      </c>
-      <c r="F71">
-        <v>1999</v>
+        <v>101</v>
       </c>
     </row>
     <row r="72" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>162</v>
+        <v>239</v>
       </c>
       <c r="B72" t="s">
-        <v>25</v>
+        <v>237</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>161</v>
+        <v>243</v>
+      </c>
+      <c r="H72" t="s">
+        <v>16</v>
+      </c>
+      <c r="I72" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="73" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>169</v>
+        <v>254</v>
       </c>
       <c r="B73" t="s">
-        <v>40</v>
+        <v>55</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>168</v>
+        <v>253</v>
+      </c>
+      <c r="E73" t="s">
+        <v>255</v>
+      </c>
+      <c r="F73">
+        <v>1960</v>
+      </c>
+      <c r="G73">
+        <v>2014</v>
+      </c>
+      <c r="H73" t="s">
+        <v>16</v>
+      </c>
+      <c r="I73" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="74" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>66</v>
+        <v>270</v>
       </c>
       <c r="B74" t="s">
-        <v>25</v>
+        <v>55</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>67</v>
+        <v>271</v>
+      </c>
+      <c r="F74">
+        <v>1990</v>
+      </c>
+      <c r="G74">
+        <v>2010</v>
+      </c>
+      <c r="H74" t="s">
+        <v>16</v>
+      </c>
+      <c r="I74" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="75" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>140</v>
+        <v>117</v>
       </c>
       <c r="B75" t="s">
-        <v>40</v>
+        <v>55</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>141</v>
+        <v>118</v>
+      </c>
+      <c r="I75" t="s">
+        <v>20</v>
+      </c>
+      <c r="J75" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="76" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A76" t="s">
-        <v>173</v>
+      <c r="A76" s="1" t="s">
+        <v>23</v>
       </c>
       <c r="B76" t="s">
-        <v>60</v>
+        <v>25</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>172</v>
+        <v>53</v>
       </c>
     </row>
     <row r="77" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>133</v>
+        <v>267</v>
       </c>
       <c r="B77" t="s">
-        <v>119</v>
+        <v>250</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="J77" t="s">
-        <v>17</v>
+        <v>266</v>
+      </c>
+      <c r="D77" t="s">
+        <v>269</v>
+      </c>
+      <c r="E77" t="s">
+        <v>268</v>
+      </c>
+      <c r="F77">
+        <v>1970</v>
+      </c>
+      <c r="G77">
+        <v>2014</v>
+      </c>
+      <c r="H77" t="s">
+        <v>16</v>
+      </c>
+      <c r="I77" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="78" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>183</v>
+        <v>96</v>
       </c>
       <c r="B78" t="s">
-        <v>166</v>
+        <v>25</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>182</v>
+        <v>90</v>
+      </c>
+      <c r="E78" t="s">
+        <v>69</v>
+      </c>
+      <c r="F78">
+        <v>1995</v>
       </c>
     </row>
     <row r="79" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>115</v>
+        <v>11</v>
       </c>
       <c r="B79" t="s">
-        <v>129</v>
+        <v>25</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>116</v>
+        <v>12</v>
+      </c>
+      <c r="D79" t="s">
+        <v>95</v>
+      </c>
+      <c r="E79" t="s">
+        <v>10</v>
+      </c>
+      <c r="F79">
+        <v>2007</v>
+      </c>
+      <c r="H79" t="s">
+        <v>16</v>
+      </c>
+      <c r="I79" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="80" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
+        <v>223</v>
+      </c>
+      <c r="B80" t="s">
+        <v>124</v>
+      </c>
+      <c r="C80" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="F80">
+        <v>1</v>
+      </c>
+      <c r="G80">
+        <v>2010</v>
+      </c>
+      <c r="H80" t="s">
+        <v>16</v>
+      </c>
+      <c r="I80" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A81" t="s">
+        <v>226</v>
+      </c>
+      <c r="B81" t="s">
+        <v>40</v>
+      </c>
+      <c r="C81" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="F81">
+        <v>1946</v>
+      </c>
+      <c r="G81">
+        <v>2016</v>
+      </c>
+      <c r="H81" t="s">
+        <v>16</v>
+      </c>
+      <c r="I81" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A82" t="s">
+        <v>97</v>
+      </c>
+      <c r="B82" t="s">
+        <v>128</v>
+      </c>
+      <c r="C82" s="2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A83" t="s">
+        <v>278</v>
+      </c>
+      <c r="B83" t="s">
+        <v>124</v>
+      </c>
+      <c r="C83" s="2" t="s">
+        <v>279</v>
+      </c>
+      <c r="E83" t="s">
+        <v>280</v>
+      </c>
+      <c r="F83">
+        <v>1890</v>
+      </c>
+      <c r="G83">
+        <v>1996</v>
+      </c>
+      <c r="H83" t="s">
+        <v>16</v>
+      </c>
+      <c r="I83" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A84" t="s">
+        <v>156</v>
+      </c>
+      <c r="B84" t="s">
+        <v>25</v>
+      </c>
+      <c r="C84" s="2" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A85" t="s">
+        <v>229</v>
+      </c>
+      <c r="B85" t="s">
+        <v>40</v>
+      </c>
+      <c r="C85" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="F85">
+        <v>1952</v>
+      </c>
+      <c r="G85">
+        <v>1997</v>
+      </c>
+      <c r="H85" t="s">
+        <v>16</v>
+      </c>
+      <c r="I85" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A86" t="s">
+        <v>102</v>
+      </c>
+      <c r="B86" t="s">
+        <v>99</v>
+      </c>
+      <c r="C86" s="2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A87" t="s">
+        <v>289</v>
+      </c>
+      <c r="B87" t="s">
+        <v>124</v>
+      </c>
+      <c r="C87" s="2" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A88" t="s">
+        <v>246</v>
+      </c>
+      <c r="B88" t="s">
+        <v>165</v>
+      </c>
+      <c r="C88" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="E88" t="s">
+        <v>14</v>
+      </c>
+      <c r="F88">
+        <v>1960</v>
+      </c>
+      <c r="G88">
+        <v>2006</v>
+      </c>
+      <c r="H88" t="s">
+        <v>16</v>
+      </c>
+      <c r="I88" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A89" t="s">
+        <v>208</v>
+      </c>
+      <c r="B89" t="s">
+        <v>124</v>
+      </c>
+      <c r="C89" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="F89">
+        <v>1932</v>
+      </c>
+      <c r="G89">
+        <v>2014</v>
+      </c>
+      <c r="H89" t="s">
+        <v>16</v>
+      </c>
+      <c r="I89" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="90" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A90" t="s">
+        <v>137</v>
+      </c>
+      <c r="B90" t="s">
+        <v>259</v>
+      </c>
+      <c r="C90" s="2" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="91" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A91" t="s">
+        <v>155</v>
+      </c>
+      <c r="B91" t="s">
+        <v>259</v>
+      </c>
+      <c r="C91" s="2" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="92" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A92" t="s">
+        <v>57</v>
+      </c>
+      <c r="B92" t="s">
+        <v>128</v>
+      </c>
+      <c r="C92" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="J92" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="93" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A93" t="s">
+        <v>129</v>
+      </c>
+      <c r="B93" t="s">
+        <v>259</v>
+      </c>
+      <c r="C93" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="E93" t="s">
+        <v>131</v>
+      </c>
+      <c r="F93">
+        <v>1945</v>
+      </c>
+      <c r="G93">
+        <v>2008</v>
+      </c>
+      <c r="I93" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="94" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A94" t="s">
+        <v>148</v>
+      </c>
+      <c r="B94" t="s">
+        <v>128</v>
+      </c>
+      <c r="C94" s="2" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="95" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A95" t="s">
+        <v>233</v>
+      </c>
+      <c r="B95" t="s">
+        <v>165</v>
+      </c>
+      <c r="C95" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="E95" t="s">
+        <v>14</v>
+      </c>
+      <c r="F95">
+        <v>2012</v>
+      </c>
+      <c r="G95">
+        <v>2016</v>
+      </c>
+      <c r="H95" t="s">
+        <v>16</v>
+      </c>
+      <c r="I95" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="96" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A96" t="s">
+        <v>35</v>
+      </c>
+      <c r="B96" t="s">
+        <v>25</v>
+      </c>
+      <c r="C96" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D96" t="s">
+        <v>37</v>
+      </c>
+      <c r="E96" t="s">
+        <v>14</v>
+      </c>
+      <c r="F96">
+        <v>2001</v>
+      </c>
+      <c r="H96" t="s">
+        <v>16</v>
+      </c>
+      <c r="I96" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="97" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A97" t="s">
+        <v>185</v>
+      </c>
+      <c r="B97" t="s">
+        <v>128</v>
+      </c>
+      <c r="C97" s="2" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="98" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A98" t="s">
+        <v>210</v>
+      </c>
+      <c r="B98" t="s">
+        <v>40</v>
+      </c>
+      <c r="C98" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="F98">
+        <v>1976</v>
+      </c>
+      <c r="G98">
+        <v>2016</v>
+      </c>
+      <c r="H98" t="s">
+        <v>16</v>
+      </c>
+      <c r="I98" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="99" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A99" t="s">
+        <v>144</v>
+      </c>
+      <c r="B99" t="s">
+        <v>60</v>
+      </c>
+      <c r="C99" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="F99">
+        <v>1800</v>
+      </c>
+      <c r="G99">
+        <v>2013</v>
+      </c>
+    </row>
+    <row r="100" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A100" t="s">
+        <v>122</v>
+      </c>
+      <c r="B100" t="s">
+        <v>259</v>
+      </c>
+      <c r="C100" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="I100" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="101" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A101" t="s">
+        <v>141</v>
+      </c>
+      <c r="B101" t="s">
+        <v>237</v>
+      </c>
+      <c r="C101" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="J101" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="102" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A102" t="s">
+        <v>287</v>
+      </c>
+      <c r="B102" t="s">
+        <v>134</v>
+      </c>
+      <c r="C102" s="2" t="s">
+        <v>288</v>
+      </c>
+      <c r="F102">
+        <v>1990</v>
+      </c>
+      <c r="G102">
+        <v>2008</v>
+      </c>
+    </row>
+    <row r="103" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A103" t="s">
+        <v>274</v>
+      </c>
+      <c r="B103" t="s">
+        <v>55</v>
+      </c>
+      <c r="C103" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="H103" t="s">
+        <v>16</v>
+      </c>
+      <c r="I103" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="104" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A104" t="s">
+        <v>157</v>
+      </c>
+      <c r="B104" t="s">
+        <v>128</v>
+      </c>
+      <c r="C104" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="J104" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="105" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A105" t="s">
+        <v>194</v>
+      </c>
+      <c r="B105" t="s">
+        <v>99</v>
+      </c>
+      <c r="C105" s="2" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="106" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A106" t="s">
+        <v>256</v>
+      </c>
+      <c r="B106" t="s">
+        <v>250</v>
+      </c>
+      <c r="C106" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="E106" t="s">
+        <v>258</v>
+      </c>
+      <c r="H106" t="s">
+        <v>16</v>
+      </c>
+      <c r="I106" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="107" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A107" t="s">
+        <v>227</v>
+      </c>
+      <c r="B107" t="s">
+        <v>40</v>
+      </c>
+      <c r="C107" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="F107">
+        <v>1955</v>
+      </c>
+      <c r="G107">
+        <v>2016</v>
+      </c>
+      <c r="H107" t="s">
+        <v>16</v>
+      </c>
+      <c r="I107" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="108" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A108" t="s">
+        <v>230</v>
+      </c>
+      <c r="B108" t="s">
+        <v>40</v>
+      </c>
+      <c r="C108" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="F108">
+        <v>1995</v>
+      </c>
+      <c r="G108">
+        <v>2016</v>
+      </c>
+      <c r="H108" t="s">
+        <v>16</v>
+      </c>
+      <c r="I108" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="109" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A109" t="s">
+        <v>109</v>
+      </c>
+      <c r="B109" t="s">
+        <v>25</v>
+      </c>
+      <c r="C109" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="E109" t="s">
+        <v>111</v>
+      </c>
+      <c r="F109">
+        <v>1956</v>
+      </c>
+    </row>
+    <row r="110" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A110" t="s">
+        <v>91</v>
+      </c>
+      <c r="B110" t="s">
+        <v>25</v>
+      </c>
+      <c r="C110" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="E110" t="s">
+        <v>92</v>
+      </c>
+      <c r="F110">
+        <v>1999</v>
+      </c>
+    </row>
+    <row r="111" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A111" t="s">
+        <v>161</v>
+      </c>
+      <c r="B111" t="s">
+        <v>25</v>
+      </c>
+      <c r="C111" s="2" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="112" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A112" t="s">
+        <v>168</v>
+      </c>
+      <c r="B112" t="s">
+        <v>40</v>
+      </c>
+      <c r="C112" s="2" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="113" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A113" t="s">
+        <v>213</v>
+      </c>
+      <c r="B113" t="s">
+        <v>55</v>
+      </c>
+      <c r="C113" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="H113" t="s">
+        <v>16</v>
+      </c>
+      <c r="I113" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="114" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A114" t="s">
+        <v>273</v>
+      </c>
+      <c r="B114" t="s">
+        <v>237</v>
+      </c>
+      <c r="C114" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="F114">
+        <v>1996</v>
+      </c>
+      <c r="G114">
+        <v>2016</v>
+      </c>
+      <c r="H114" t="s">
+        <v>16</v>
+      </c>
+      <c r="I114" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="115" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A115" t="s">
+        <v>66</v>
+      </c>
+      <c r="B115" t="s">
+        <v>25</v>
+      </c>
+      <c r="C115" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="116" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A116" t="s">
+        <v>139</v>
+      </c>
+      <c r="B116" t="s">
+        <v>40</v>
+      </c>
+      <c r="C116" s="2" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="117" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A117" t="s">
+        <v>172</v>
+      </c>
+      <c r="B117" t="s">
+        <v>60</v>
+      </c>
+      <c r="C117" s="2" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="118" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A118" t="s">
+        <v>217</v>
+      </c>
+      <c r="B118" t="s">
+        <v>60</v>
+      </c>
+      <c r="C118" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="E118" t="s">
+        <v>14</v>
+      </c>
+      <c r="F118">
+        <v>1900</v>
+      </c>
+      <c r="H118" t="s">
+        <v>16</v>
+      </c>
+      <c r="I118" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="119" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A119" t="s">
+        <v>132</v>
+      </c>
+      <c r="B119" t="s">
+        <v>259</v>
+      </c>
+      <c r="C119" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="J119" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="120" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A120" t="s">
+        <v>182</v>
+      </c>
+      <c r="B120" t="s">
+        <v>165</v>
+      </c>
+      <c r="C120" s="2" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="121" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A121" t="s">
+        <v>115</v>
+      </c>
+      <c r="B121" t="s">
+        <v>128</v>
+      </c>
+      <c r="C121" s="2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="122" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A122" t="s">
+        <v>263</v>
+      </c>
+      <c r="B122" t="s">
+        <v>250</v>
+      </c>
+      <c r="C122" s="2" t="s">
+        <v>264</v>
+      </c>
+      <c r="E122" t="s">
+        <v>265</v>
+      </c>
+      <c r="F122">
+        <v>1500</v>
+      </c>
+      <c r="G122">
+        <v>2000</v>
+      </c>
+      <c r="H122" t="s">
+        <v>16</v>
+      </c>
+      <c r="I122" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="123" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A123" t="s">
+        <v>221</v>
+      </c>
+      <c r="B123" t="s">
+        <v>86</v>
+      </c>
+      <c r="C123" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="F123">
+        <v>2013</v>
+      </c>
+      <c r="H123" t="s">
+        <v>16</v>
+      </c>
+      <c r="I123" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="124" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A124" t="s">
         <v>13</v>
       </c>
-      <c r="B80" t="s">
+      <c r="B124" t="s">
         <v>25</v>
       </c>
-      <c r="C80" s="2" t="s">
+      <c r="C124" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="D80" s="1" t="s">
+      <c r="D124" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="E80" t="s">
+      <c r="E124" t="s">
         <v>14</v>
       </c>
-      <c r="F80">
+      <c r="F124">
         <v>1981</v>
       </c>
-      <c r="H80" t="s">
-        <v>16</v>
-      </c>
-      <c r="I80" t="s">
+      <c r="H124" t="s">
+        <v>16</v>
+      </c>
+      <c r="I124" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="125" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A125" t="s">
+        <v>283</v>
+      </c>
+      <c r="B125" t="s">
+        <v>124</v>
+      </c>
+      <c r="C125" s="2" t="s">
+        <v>284</v>
+      </c>
+      <c r="H125" t="s">
+        <v>16</v>
+      </c>
+      <c r="I125" t="s">
         <v>20</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:I80">
+  <sortState ref="A2:J125">
     <sortCondition ref="A2"/>
   </sortState>
   <hyperlinks>
-    <hyperlink ref="C3" r:id="rId1"/>
-    <hyperlink ref="C42" r:id="rId2"/>
-    <hyperlink ref="C4" r:id="rId3"/>
-    <hyperlink ref="C7" r:id="rId4"/>
-    <hyperlink ref="C54" r:id="rId5"/>
-    <hyperlink ref="C63" r:id="rId6"/>
-    <hyperlink ref="C80" r:id="rId7"/>
-    <hyperlink ref="C26" r:id="rId8"/>
-    <hyperlink ref="C22" r:id="rId9"/>
-    <hyperlink ref="C33" r:id="rId10"/>
-    <hyperlink ref="C40" r:id="rId11"/>
-    <hyperlink ref="C2" r:id="rId12"/>
-    <hyperlink ref="C13" r:id="rId13"/>
-    <hyperlink ref="C43" r:id="rId14"/>
-    <hyperlink ref="C52" r:id="rId15"/>
-    <hyperlink ref="C21" r:id="rId16"/>
-    <hyperlink ref="C60" r:id="rId17"/>
-    <hyperlink ref="C29" r:id="rId18"/>
-    <hyperlink ref="C47" r:id="rId19"/>
-    <hyperlink ref="C10" r:id="rId20"/>
-    <hyperlink ref="C74" r:id="rId21"/>
-    <hyperlink ref="C5" r:id="rId22"/>
-    <hyperlink ref="C27" r:id="rId23"/>
-    <hyperlink ref="C37" r:id="rId24"/>
-    <hyperlink ref="C34" r:id="rId25"/>
-    <hyperlink ref="C38" r:id="rId26"/>
-    <hyperlink ref="C39" r:id="rId27"/>
-    <hyperlink ref="C45" r:id="rId28"/>
-    <hyperlink ref="C53" r:id="rId29"/>
-    <hyperlink ref="C71" r:id="rId30"/>
-    <hyperlink ref="C55" r:id="rId31"/>
-    <hyperlink ref="C50" r:id="rId32"/>
-    <hyperlink ref="C57" r:id="rId33"/>
-    <hyperlink ref="C46" r:id="rId34"/>
-    <hyperlink ref="C11" r:id="rId35"/>
-    <hyperlink ref="C70" r:id="rId36"/>
-    <hyperlink ref="C9" r:id="rId37"/>
-    <hyperlink ref="C79" r:id="rId38"/>
-    <hyperlink ref="C51" r:id="rId39"/>
-    <hyperlink ref="C41" r:id="rId40"/>
-    <hyperlink ref="C66" r:id="rId41"/>
-    <hyperlink ref="C12" r:id="rId42"/>
-    <hyperlink ref="C35" r:id="rId43"/>
-    <hyperlink ref="C15" r:id="rId44"/>
-    <hyperlink ref="C61" r:id="rId45"/>
-    <hyperlink ref="C77" r:id="rId46"/>
-    <hyperlink ref="C19" r:id="rId47" display="http://comparativeconstitutionsproject.org/"/>
-    <hyperlink ref="C58" r:id="rId48"/>
-    <hyperlink ref="C75" r:id="rId49"/>
-    <hyperlink ref="C67" r:id="rId50"/>
-    <hyperlink ref="C65" r:id="rId51"/>
-    <hyperlink ref="C14" r:id="rId52"/>
-    <hyperlink ref="C62" r:id="rId53"/>
-    <hyperlink ref="C32" r:id="rId54"/>
-    <hyperlink ref="C48" r:id="rId55"/>
-    <hyperlink ref="C49" r:id="rId56"/>
-    <hyperlink ref="C59" r:id="rId57"/>
-    <hyperlink ref="C56" r:id="rId58"/>
-    <hyperlink ref="C68" r:id="rId59"/>
-    <hyperlink ref="C23" r:id="rId60"/>
-    <hyperlink ref="C72" r:id="rId61"/>
-    <hyperlink ref="C6" r:id="rId62"/>
-    <hyperlink ref="C25" r:id="rId63"/>
-    <hyperlink ref="C73" r:id="rId64"/>
-    <hyperlink ref="C8" r:id="rId65"/>
-    <hyperlink ref="C76" r:id="rId66"/>
-    <hyperlink ref="C17" r:id="rId67"/>
-    <hyperlink ref="C16" r:id="rId68"/>
-    <hyperlink ref="C18" r:id="rId69"/>
-    <hyperlink ref="C36" r:id="rId70"/>
-    <hyperlink ref="C78" r:id="rId71"/>
-    <hyperlink ref="C20" r:id="rId72"/>
-    <hyperlink ref="C64" r:id="rId73"/>
-    <hyperlink ref="C24" r:id="rId74"/>
-    <hyperlink ref="C31" r:id="rId75"/>
-    <hyperlink ref="C69" r:id="rId76"/>
-    <hyperlink ref="C30" r:id="rId77"/>
-    <hyperlink ref="C28" r:id="rId78"/>
-    <hyperlink ref="C44" r:id="rId79"/>
+    <hyperlink ref="C6" r:id="rId1"/>
+    <hyperlink ref="C52" r:id="rId2"/>
+    <hyperlink ref="C7" r:id="rId3"/>
+    <hyperlink ref="C10" r:id="rId4"/>
+    <hyperlink ref="C79" r:id="rId5"/>
+    <hyperlink ref="C96" r:id="rId6"/>
+    <hyperlink ref="C124" r:id="rId7"/>
+    <hyperlink ref="C31" r:id="rId8"/>
+    <hyperlink ref="C27" r:id="rId9"/>
+    <hyperlink ref="C43" r:id="rId10"/>
+    <hyperlink ref="C50" r:id="rId11"/>
+    <hyperlink ref="C3" r:id="rId12"/>
+    <hyperlink ref="C18" r:id="rId13"/>
+    <hyperlink ref="C54" r:id="rId14"/>
+    <hyperlink ref="C76" r:id="rId15"/>
+    <hyperlink ref="C26" r:id="rId16"/>
+    <hyperlink ref="C92" r:id="rId17"/>
+    <hyperlink ref="C35" r:id="rId18"/>
+    <hyperlink ref="C63" r:id="rId19"/>
+    <hyperlink ref="C15" r:id="rId20"/>
+    <hyperlink ref="C115" r:id="rId21"/>
+    <hyperlink ref="C8" r:id="rId22"/>
+    <hyperlink ref="C33" r:id="rId23"/>
+    <hyperlink ref="C47" r:id="rId24"/>
+    <hyperlink ref="C44" r:id="rId25"/>
+    <hyperlink ref="C48" r:id="rId26"/>
+    <hyperlink ref="C49" r:id="rId27"/>
+    <hyperlink ref="C61" r:id="rId28"/>
+    <hyperlink ref="C78" r:id="rId29"/>
+    <hyperlink ref="C110" r:id="rId30"/>
+    <hyperlink ref="C82" r:id="rId31"/>
+    <hyperlink ref="C71" r:id="rId32"/>
+    <hyperlink ref="C86" r:id="rId33"/>
+    <hyperlink ref="C62" r:id="rId34"/>
+    <hyperlink ref="C16" r:id="rId35"/>
+    <hyperlink ref="C109" r:id="rId36"/>
+    <hyperlink ref="C14" r:id="rId37"/>
+    <hyperlink ref="C121" r:id="rId38"/>
+    <hyperlink ref="C75" r:id="rId39"/>
+    <hyperlink ref="C51" r:id="rId40"/>
+    <hyperlink ref="C100" r:id="rId41"/>
+    <hyperlink ref="C17" r:id="rId42"/>
+    <hyperlink ref="C45" r:id="rId43"/>
+    <hyperlink ref="C20" r:id="rId44"/>
+    <hyperlink ref="C93" r:id="rId45"/>
+    <hyperlink ref="C119" r:id="rId46"/>
+    <hyperlink ref="C24" r:id="rId47" display="http://comparativeconstitutionsproject.org/"/>
+    <hyperlink ref="C90" r:id="rId48"/>
+    <hyperlink ref="C116" r:id="rId49"/>
+    <hyperlink ref="C101" r:id="rId50"/>
+    <hyperlink ref="C99" r:id="rId51"/>
+    <hyperlink ref="C19" r:id="rId52"/>
+    <hyperlink ref="C94" r:id="rId53"/>
+    <hyperlink ref="C42" r:id="rId54"/>
+    <hyperlink ref="C65" r:id="rId55"/>
+    <hyperlink ref="C68" r:id="rId56"/>
+    <hyperlink ref="C91" r:id="rId57"/>
+    <hyperlink ref="C84" r:id="rId58"/>
+    <hyperlink ref="C104" r:id="rId59"/>
+    <hyperlink ref="C28" r:id="rId60"/>
+    <hyperlink ref="C111" r:id="rId61"/>
+    <hyperlink ref="C9" r:id="rId62"/>
+    <hyperlink ref="C30" r:id="rId63"/>
+    <hyperlink ref="C112" r:id="rId64"/>
+    <hyperlink ref="C13" r:id="rId65"/>
+    <hyperlink ref="C117" r:id="rId66"/>
+    <hyperlink ref="C22" r:id="rId67"/>
+    <hyperlink ref="C21" r:id="rId68"/>
+    <hyperlink ref="C23" r:id="rId69"/>
+    <hyperlink ref="C46" r:id="rId70"/>
+    <hyperlink ref="C120" r:id="rId71"/>
+    <hyperlink ref="C25" r:id="rId72"/>
+    <hyperlink ref="C97" r:id="rId73"/>
+    <hyperlink ref="C29" r:id="rId74"/>
+    <hyperlink ref="C39" r:id="rId75"/>
+    <hyperlink ref="C105" r:id="rId76"/>
+    <hyperlink ref="C36" r:id="rId77"/>
+    <hyperlink ref="C34" r:id="rId78"/>
+    <hyperlink ref="C60" r:id="rId79"/>
+    <hyperlink ref="C5" r:id="rId80"/>
+    <hyperlink ref="C59" r:id="rId81"/>
+    <hyperlink ref="C11" r:id="rId82"/>
+    <hyperlink ref="C89" r:id="rId83"/>
+    <hyperlink ref="C98" r:id="rId84"/>
+    <hyperlink ref="C113" r:id="rId85"/>
+    <hyperlink ref="C32" r:id="rId86"/>
+    <hyperlink ref="C118" r:id="rId87"/>
+    <hyperlink ref="C38" r:id="rId88"/>
+    <hyperlink ref="C123" r:id="rId89"/>
+    <hyperlink ref="C80" r:id="rId90"/>
+    <hyperlink ref="C57" r:id="rId91"/>
+    <hyperlink ref="C81" r:id="rId92"/>
+    <hyperlink ref="C107" r:id="rId93"/>
+    <hyperlink ref="C69" r:id="rId94"/>
+    <hyperlink ref="C85" r:id="rId95"/>
+    <hyperlink ref="C108" r:id="rId96"/>
+    <hyperlink ref="C55" r:id="rId97"/>
+    <hyperlink ref="C95" r:id="rId98"/>
+    <hyperlink ref="C40" r:id="rId99"/>
+    <hyperlink ref="C37" r:id="rId100"/>
+    <hyperlink ref="C72" r:id="rId101"/>
+    <hyperlink ref="C53" r:id="rId102"/>
+    <hyperlink ref="C2" r:id="rId103"/>
+    <hyperlink ref="C66" r:id="rId104"/>
+    <hyperlink ref="C70" r:id="rId105"/>
+    <hyperlink ref="C88" r:id="rId106"/>
+    <hyperlink ref="C41" r:id="rId107"/>
+    <hyperlink ref="C73" r:id="rId108"/>
+    <hyperlink ref="C106" r:id="rId109"/>
+    <hyperlink ref="C12" r:id="rId110"/>
+    <hyperlink ref="C4" r:id="rId111"/>
+    <hyperlink ref="C122" r:id="rId112"/>
+    <hyperlink ref="C77" r:id="rId113"/>
+    <hyperlink ref="C74" r:id="rId114"/>
+    <hyperlink ref="C114" r:id="rId115"/>
+    <hyperlink ref="C103" r:id="rId116"/>
+    <hyperlink ref="C56" r:id="rId117"/>
+    <hyperlink ref="C83" r:id="rId118"/>
+    <hyperlink ref="C64" r:id="rId119"/>
+    <hyperlink ref="C125" r:id="rId120"/>
+    <hyperlink ref="C58" r:id="rId121"/>
+    <hyperlink ref="C102" r:id="rId122"/>
+    <hyperlink ref="C87" r:id="rId123"/>
+    <hyperlink ref="C67" r:id="rId124"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
add 10 datasets and two overview links (ht and thanks to Daniel Bischof)
</commit_message>
<xml_diff>
--- a/PolData.xlsx
+++ b/PolData.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="540" uniqueCount="293">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="599" uniqueCount="321">
   <si>
     <t>name</t>
   </si>
@@ -906,6 +906,90 @@
   </si>
   <si>
     <t>Government Revenue Dataset</t>
+  </si>
+  <si>
+    <t>Minorities at Risk</t>
+  </si>
+  <si>
+    <t>http://www.mar.umd.edu/mar_data.asp</t>
+  </si>
+  <si>
+    <t>Social Conflict Analysis Database</t>
+  </si>
+  <si>
+    <t>https://www.strausscenter.org/scad.html</t>
+  </si>
+  <si>
+    <t>Africa, Mexico, Central America, the Caribbean</t>
+  </si>
+  <si>
+    <t>http://www.ines.tau.ac.il/elections.html</t>
+  </si>
+  <si>
+    <t>Israel</t>
+  </si>
+  <si>
+    <t>Israel National Election Studies</t>
+  </si>
+  <si>
+    <t>free, registration</t>
+  </si>
+  <si>
+    <t>http://www.autnes.at/en/data-download/</t>
+  </si>
+  <si>
+    <t>Austria</t>
+  </si>
+  <si>
+    <t>Austrian National Election Study</t>
+  </si>
+  <si>
+    <t>http://ces-eec.arts.ubc.ca/english-section/surveys/</t>
+  </si>
+  <si>
+    <t>Canadian Election Study</t>
+  </si>
+  <si>
+    <t>Canada</t>
+  </si>
+  <si>
+    <t>Regional Authority Index</t>
+  </si>
+  <si>
+    <t>https://www.arjanschakel.nl/regauth_dat.html</t>
+  </si>
+  <si>
+    <t>81 countries</t>
+  </si>
+  <si>
+    <t>Global Elections Database</t>
+  </si>
+  <si>
+    <t>http://www.globalelectionsdatabase.com/index.php/datasets</t>
+  </si>
+  <si>
+    <t>http://folk.uib.no/sspje/tweed.htm</t>
+  </si>
+  <si>
+    <t>Terrorism in Western Europe: Events Data</t>
+  </si>
+  <si>
+    <t>18 countries</t>
+  </si>
+  <si>
+    <t>Protest events in the Federal Republic of Germany</t>
+  </si>
+  <si>
+    <t>https://www.wzb.eu/en/research/completed-research-programs/civil-society-and-political-mobilization/projects/prodat-dokumentation-un</t>
+  </si>
+  <si>
+    <t>Protest events</t>
+  </si>
+  <si>
+    <t>https://www.unige.ch/sciences-societe/incite/welcome-to-the-incite-website/data/new-s/</t>
+  </si>
+  <si>
+    <t>France, Germany, Switzerland, the Netherlands</t>
   </si>
 </sst>
 </file>
@@ -1237,10 +1321,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J125"/>
+  <dimension ref="A1:J135"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="A74" sqref="A74"/>
+    <sheetView tabSelected="1" topLeftCell="A101" workbookViewId="0">
+      <selection activeCell="B53" sqref="B53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1452,36 +1536,42 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>207</v>
+        <v>304</v>
       </c>
       <c r="B11" t="s">
-        <v>60</v>
+        <v>25</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>206</v>
+        <v>302</v>
+      </c>
+      <c r="E11" t="s">
+        <v>303</v>
       </c>
       <c r="F11">
-        <v>1972</v>
-      </c>
-      <c r="G11">
-        <v>2014</v>
+        <v>2002</v>
       </c>
       <c r="H11" t="s">
         <v>16</v>
       </c>
       <c r="I11" t="s">
-        <v>20</v>
+        <v>301</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>260</v>
+        <v>207</v>
       </c>
       <c r="B12" t="s">
-        <v>259</v>
+        <v>60</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>261</v>
+        <v>206</v>
+      </c>
+      <c r="F12">
+        <v>1972</v>
+      </c>
+      <c r="G12">
+        <v>2014</v>
       </c>
       <c r="H12" t="s">
         <v>16</v>
@@ -1492,331 +1582,328 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>170</v>
+        <v>260</v>
       </c>
       <c r="B13" t="s">
-        <v>60</v>
+        <v>259</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>169</v>
+        <v>261</v>
+      </c>
+      <c r="H13" t="s">
+        <v>16</v>
+      </c>
+      <c r="I13" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>113</v>
+        <v>170</v>
       </c>
       <c r="B14" t="s">
-        <v>25</v>
+        <v>60</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="E14" t="s">
-        <v>112</v>
-      </c>
-      <c r="F14">
-        <v>1964</v>
+        <v>169</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>64</v>
+        <v>113</v>
       </c>
       <c r="B15" t="s">
         <v>25</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>65</v>
+        <v>114</v>
+      </c>
+      <c r="E15" t="s">
+        <v>112</v>
       </c>
       <c r="F15">
-        <v>1991</v>
-      </c>
-      <c r="G15">
-        <v>2009</v>
-      </c>
-      <c r="J15" t="s">
-        <v>18</v>
+        <v>1964</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>107</v>
+        <v>64</v>
       </c>
       <c r="B16" t="s">
         <v>25</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="E16" t="s">
-        <v>112</v>
+        <v>65</v>
+      </c>
+      <c r="F16">
+        <v>1991</v>
+      </c>
+      <c r="G16">
+        <v>2009</v>
+      </c>
+      <c r="J16" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>123</v>
+        <v>107</v>
       </c>
       <c r="B17" t="s">
-        <v>259</v>
+        <v>25</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="I17" t="s">
-        <v>20</v>
+        <v>108</v>
+      </c>
+      <c r="E17" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>32</v>
+        <v>123</v>
       </c>
       <c r="B18" t="s">
-        <v>25</v>
+        <v>259</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="E18" t="s">
-        <v>74</v>
-      </c>
-      <c r="F18">
-        <v>2008</v>
+        <v>121</v>
+      </c>
+      <c r="I18" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>146</v>
+        <v>306</v>
       </c>
       <c r="B19" t="s">
-        <v>128</v>
+        <v>25</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>145</v>
+        <v>305</v>
+      </c>
+      <c r="E19" t="s">
+        <v>307</v>
+      </c>
+      <c r="F19">
+        <v>2004</v>
+      </c>
+      <c r="H19" t="s">
+        <v>16</v>
+      </c>
+      <c r="I19" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>127</v>
+        <v>32</v>
       </c>
       <c r="B20" t="s">
-        <v>259</v>
+        <v>25</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="I20" t="s">
-        <v>20</v>
+        <v>51</v>
+      </c>
+      <c r="E20" t="s">
+        <v>74</v>
+      </c>
+      <c r="F20">
+        <v>2008</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>173</v>
+        <v>146</v>
       </c>
       <c r="B21" t="s">
         <v>128</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>175</v>
+        <v>145</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>174</v>
+        <v>127</v>
       </c>
       <c r="B22" t="s">
-        <v>86</v>
+        <v>259</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="E22" t="s">
-        <v>176</v>
+        <v>121</v>
+      </c>
+      <c r="I22" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="B23" t="s">
-        <v>25</v>
+        <v>128</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="E23" t="s">
-        <v>178</v>
-      </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>135</v>
+        <v>174</v>
       </c>
       <c r="B24" t="s">
-        <v>134</v>
+        <v>86</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>136</v>
+        <v>175</v>
+      </c>
+      <c r="E24" t="s">
+        <v>176</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>184</v>
+        <v>177</v>
       </c>
       <c r="B25" t="s">
-        <v>128</v>
+        <v>25</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>183</v>
+        <v>175</v>
+      </c>
+      <c r="E25" t="s">
+        <v>178</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>54</v>
+        <v>135</v>
       </c>
       <c r="B26" t="s">
-        <v>55</v>
+        <v>134</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>56</v>
+        <v>136</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A27" s="1" t="s">
-        <v>22</v>
+      <c r="A27" t="s">
+        <v>184</v>
       </c>
       <c r="B27" t="s">
-        <v>25</v>
+        <v>128</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>47</v>
+        <v>183</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>158</v>
+        <v>54</v>
       </c>
       <c r="B28" t="s">
-        <v>99</v>
+        <v>55</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>159</v>
+        <v>56</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
-        <v>187</v>
+      <c r="A29" s="1" t="s">
+        <v>22</v>
       </c>
       <c r="B29" t="s">
-        <v>99</v>
+        <v>25</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>188</v>
-      </c>
-      <c r="F29">
-        <v>1960</v>
-      </c>
-      <c r="G29">
-        <v>2011</v>
-      </c>
-      <c r="H29" t="s">
-        <v>16</v>
-      </c>
-      <c r="I29" t="s">
-        <v>189</v>
+        <v>47</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="B30" t="s">
-        <v>165</v>
+        <v>99</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>39</v>
+        <v>187</v>
       </c>
       <c r="B31" t="s">
-        <v>40</v>
+        <v>99</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="E31" t="s">
-        <v>14</v>
+        <v>188</v>
       </c>
       <c r="F31">
-        <v>1816</v>
+        <v>1960</v>
       </c>
       <c r="G31">
-        <v>2007</v>
+        <v>2011</v>
       </c>
       <c r="H31" t="s">
         <v>16</v>
       </c>
       <c r="I31" t="s">
-        <v>20</v>
+        <v>189</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>215</v>
+        <v>164</v>
       </c>
       <c r="B32" t="s">
-        <v>237</v>
+        <v>165</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="F32">
-        <v>1995</v>
-      </c>
-      <c r="H32" t="s">
-        <v>16</v>
-      </c>
-      <c r="I32" t="s">
-        <v>20</v>
+        <v>166</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>75</v>
+        <v>39</v>
       </c>
       <c r="B33" t="s">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>76</v>
+        <v>41</v>
       </c>
       <c r="E33" t="s">
-        <v>77</v>
+        <v>14</v>
       </c>
       <c r="F33">
-        <v>1971</v>
+        <v>1816</v>
+      </c>
+      <c r="G33">
+        <v>2007</v>
+      </c>
+      <c r="H33" t="s">
+        <v>16</v>
+      </c>
+      <c r="I33" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>197</v>
+        <v>215</v>
       </c>
       <c r="B34" t="s">
-        <v>55</v>
+        <v>237</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>198</v>
-      </c>
-      <c r="E34" t="s">
-        <v>199</v>
+        <v>214</v>
       </c>
       <c r="F34">
-        <v>1975</v>
-      </c>
-      <c r="G34">
-        <v>2015</v>
+        <v>1995</v>
       </c>
       <c r="H34" t="s">
         <v>16</v>
@@ -1827,95 +1914,107 @@
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>59</v>
+        <v>75</v>
       </c>
       <c r="B35" t="s">
-        <v>60</v>
+        <v>25</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>61</v>
+        <v>76</v>
+      </c>
+      <c r="E35" t="s">
+        <v>77</v>
+      </c>
+      <c r="F35">
+        <v>1971</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="B36" t="s">
-        <v>165</v>
+        <v>55</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>195</v>
+        <v>198</v>
+      </c>
+      <c r="E36" t="s">
+        <v>199</v>
       </c>
       <c r="F36">
-        <v>1946</v>
+        <v>1975</v>
       </c>
       <c r="G36">
-        <v>2016</v>
+        <v>2015</v>
+      </c>
+      <c r="H36" t="s">
+        <v>16</v>
+      </c>
+      <c r="I36" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>238</v>
+        <v>59</v>
       </c>
       <c r="B37" t="s">
-        <v>237</v>
+        <v>60</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>243</v>
-      </c>
-      <c r="H37" t="s">
-        <v>16</v>
-      </c>
-      <c r="I37" t="s">
-        <v>20</v>
+        <v>61</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>219</v>
+        <v>196</v>
       </c>
       <c r="B38" t="s">
-        <v>124</v>
+        <v>165</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>218</v>
+        <v>195</v>
       </c>
       <c r="F38">
-        <v>1970</v>
+        <v>1946</v>
       </c>
       <c r="G38">
-        <v>2015</v>
-      </c>
-      <c r="H38" t="s">
-        <v>16</v>
-      </c>
-      <c r="I38" t="s">
-        <v>20</v>
+        <v>2016</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>191</v>
+        <v>238</v>
       </c>
       <c r="B39" t="s">
-        <v>25</v>
+        <v>237</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="E39" t="s">
-        <v>192</v>
+        <v>243</v>
+      </c>
+      <c r="H39" t="s">
+        <v>16</v>
+      </c>
+      <c r="I39" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>235</v>
+        <v>219</v>
       </c>
       <c r="B40" t="s">
-        <v>60</v>
+        <v>124</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>236</v>
+        <v>218</v>
+      </c>
+      <c r="F40">
+        <v>1970</v>
+      </c>
+      <c r="G40">
+        <v>2015</v>
       </c>
       <c r="H40" t="s">
         <v>16</v>
@@ -1926,125 +2025,122 @@
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>252</v>
+        <v>191</v>
       </c>
       <c r="B41" t="s">
-        <v>250</v>
+        <v>25</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>251</v>
-      </c>
-      <c r="H41" t="s">
-        <v>16</v>
-      </c>
-      <c r="I41" t="s">
-        <v>20</v>
+        <v>190</v>
+      </c>
+      <c r="E41" t="s">
+        <v>192</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>149</v>
+        <v>235</v>
       </c>
       <c r="B42" t="s">
-        <v>128</v>
+        <v>60</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>150</v>
+        <v>236</v>
+      </c>
+      <c r="H42" t="s">
+        <v>16</v>
+      </c>
+      <c r="I42" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>28</v>
+        <v>252</v>
       </c>
       <c r="B43" t="s">
-        <v>25</v>
+        <v>250</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>48</v>
+        <v>251</v>
+      </c>
+      <c r="H43" t="s">
+        <v>16</v>
+      </c>
+      <c r="I43" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>80</v>
+        <v>149</v>
       </c>
       <c r="B44" t="s">
         <v>128</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="E44" t="s">
-        <v>9</v>
-      </c>
-      <c r="F44">
-        <v>1979</v>
+        <v>150</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>125</v>
+        <v>28</v>
       </c>
       <c r="B45" t="s">
-        <v>124</v>
+        <v>25</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>126</v>
+        <v>48</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>179</v>
+        <v>80</v>
       </c>
       <c r="B46" t="s">
-        <v>165</v>
+        <v>128</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>180</v>
+        <v>81</v>
+      </c>
+      <c r="E46" t="s">
+        <v>9</v>
+      </c>
+      <c r="F46">
+        <v>1979</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
+        <v>125</v>
+      </c>
+      <c r="B47" t="s">
+        <v>124</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>179</v>
+      </c>
+      <c r="B48" t="s">
+        <v>165</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
         <v>78</v>
       </c>
-      <c r="B47" t="s">
+      <c r="B49" t="s">
         <v>25</v>
       </c>
-      <c r="C47" s="2" t="s">
+      <c r="C49" s="2" t="s">
         <v>79</v>
-      </c>
-      <c r="E47" t="s">
-        <v>9</v>
-      </c>
-      <c r="F47">
-        <v>1979</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A48" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="B48" t="s">
-        <v>83</v>
-      </c>
-      <c r="C48" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="E48" t="s">
-        <v>9</v>
-      </c>
-      <c r="F48">
-        <v>1979</v>
-      </c>
-    </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A49" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="B49" t="s">
-        <v>86</v>
-      </c>
-      <c r="C49" s="2" t="s">
-        <v>87</v>
       </c>
       <c r="E49" t="s">
         <v>9</v>
@@ -2052,161 +2148,155 @@
       <c r="F49">
         <v>1979</v>
       </c>
-      <c r="G49">
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A50" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="B50" t="s">
+        <v>83</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="E50" t="s">
+        <v>9</v>
+      </c>
+      <c r="F50">
+        <v>1979</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A51" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="B51" t="s">
+        <v>86</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="E51" t="s">
+        <v>9</v>
+      </c>
+      <c r="F51">
+        <v>1979</v>
+      </c>
+      <c r="G51">
         <v>2009</v>
-      </c>
-    </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A50" t="s">
-        <v>27</v>
-      </c>
-      <c r="B50" t="s">
-        <v>25</v>
-      </c>
-      <c r="C50" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="J50" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A51" t="s">
-        <v>120</v>
-      </c>
-      <c r="B51" t="s">
-        <v>259</v>
-      </c>
-      <c r="C51" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="I51" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>5</v>
+        <v>27</v>
       </c>
       <c r="B52" t="s">
         <v>25</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D52" t="s">
-        <v>94</v>
-      </c>
-      <c r="E52" t="s">
-        <v>9</v>
-      </c>
-      <c r="F52">
-        <v>2002</v>
-      </c>
-      <c r="H52" t="s">
-        <v>16</v>
-      </c>
-      <c r="I52" t="s">
-        <v>248</v>
+        <v>49</v>
       </c>
       <c r="J52" t="s">
-        <v>44</v>
+        <v>17</v>
       </c>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>240</v>
+        <v>120</v>
       </c>
       <c r="B53" t="s">
-        <v>237</v>
+        <v>259</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>243</v>
-      </c>
-      <c r="H53" t="s">
-        <v>16</v>
+        <v>119</v>
       </c>
       <c r="I53" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A54" s="1" t="s">
-        <v>26</v>
+      <c r="A54" t="s">
+        <v>5</v>
       </c>
       <c r="B54" t="s">
         <v>25</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>52</v>
+        <v>6</v>
+      </c>
+      <c r="D54" t="s">
+        <v>94</v>
+      </c>
+      <c r="E54" t="s">
+        <v>9</v>
+      </c>
+      <c r="F54">
+        <v>2002</v>
+      </c>
+      <c r="H54" t="s">
+        <v>16</v>
+      </c>
+      <c r="I54" t="s">
+        <v>248</v>
+      </c>
+      <c r="J54" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>232</v>
+        <v>240</v>
       </c>
       <c r="B55" t="s">
-        <v>250</v>
+        <v>237</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>231</v>
+        <v>243</v>
+      </c>
+      <c r="H55" t="s">
+        <v>16</v>
+      </c>
+      <c r="I55" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A56" t="s">
-        <v>276</v>
+      <c r="A56" s="1" t="s">
+        <v>26</v>
       </c>
       <c r="B56" t="s">
-        <v>124</v>
+        <v>25</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>277</v>
-      </c>
-      <c r="F56">
-        <v>1948</v>
-      </c>
-      <c r="G56">
-        <v>2000</v>
-      </c>
-      <c r="H56" t="s">
-        <v>16</v>
-      </c>
-      <c r="I56" t="s">
-        <v>20</v>
+        <v>52</v>
       </c>
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="B57" t="s">
-        <v>40</v>
+        <v>250</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>225</v>
-      </c>
-      <c r="F57">
-        <v>1964</v>
-      </c>
-      <c r="G57">
-        <v>2008</v>
-      </c>
-      <c r="H57" t="s">
-        <v>16</v>
-      </c>
-      <c r="I57" t="s">
-        <v>20</v>
+        <v>231</v>
       </c>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>285</v>
+        <v>276</v>
       </c>
       <c r="B58" t="s">
-        <v>250</v>
+        <v>124</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>286</v>
+        <v>277</v>
+      </c>
+      <c r="F58">
+        <v>1948</v>
+      </c>
+      <c r="G58">
+        <v>2000</v>
       </c>
       <c r="H58" t="s">
         <v>16</v>
@@ -2217,146 +2307,158 @@
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>205</v>
+        <v>224</v>
       </c>
       <c r="B59" t="s">
         <v>40</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>204</v>
+        <v>225</v>
       </c>
       <c r="F59">
-        <v>2006</v>
+        <v>1964</v>
+      </c>
+      <c r="G59">
+        <v>2008</v>
+      </c>
+      <c r="H59" t="s">
+        <v>16</v>
+      </c>
+      <c r="I59" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>200</v>
+        <v>285</v>
       </c>
       <c r="B60" t="s">
-        <v>99</v>
+        <v>250</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>201</v>
-      </c>
-      <c r="F60">
-        <v>1980</v>
-      </c>
-      <c r="G60">
-        <v>2007</v>
-      </c>
-      <c r="J60" t="s">
-        <v>18</v>
+        <v>286</v>
+      </c>
+      <c r="H60" t="s">
+        <v>16</v>
+      </c>
+      <c r="I60" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>89</v>
+        <v>205</v>
       </c>
       <c r="B61" t="s">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="E61" t="s">
-        <v>34</v>
+        <v>204</v>
       </c>
       <c r="F61">
-        <v>1972</v>
-      </c>
-      <c r="H61" t="s">
-        <v>16</v>
-      </c>
-      <c r="I61" t="s">
-        <v>20</v>
+        <v>2006</v>
       </c>
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>104</v>
+        <v>200</v>
       </c>
       <c r="B62" t="s">
-        <v>25</v>
+        <v>99</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="E62" t="s">
-        <v>105</v>
+        <v>201</v>
       </c>
       <c r="F62">
         <v>1980</v>
       </c>
+      <c r="G62">
+        <v>2007</v>
+      </c>
+      <c r="J62" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>62</v>
+        <v>89</v>
       </c>
       <c r="B63" t="s">
         <v>25</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>63</v>
+        <v>88</v>
+      </c>
+      <c r="E63" t="s">
+        <v>34</v>
+      </c>
+      <c r="F63">
+        <v>1972</v>
+      </c>
+      <c r="H63" t="s">
+        <v>16</v>
+      </c>
+      <c r="I63" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>281</v>
+        <v>104</v>
       </c>
       <c r="B64" t="s">
-        <v>237</v>
+        <v>25</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>282</v>
-      </c>
-      <c r="H64" t="s">
-        <v>16</v>
-      </c>
-      <c r="I64" t="s">
-        <v>20</v>
+        <v>106</v>
+      </c>
+      <c r="E64" t="s">
+        <v>105</v>
+      </c>
+      <c r="F64">
+        <v>1980</v>
       </c>
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>151</v>
+        <v>62</v>
       </c>
       <c r="B65" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="E65" t="s">
-        <v>14</v>
+        <v>63</v>
       </c>
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>242</v>
+        <v>311</v>
       </c>
       <c r="B66" t="s">
-        <v>237</v>
+        <v>165</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>243</v>
+        <v>312</v>
+      </c>
+      <c r="E66" t="s">
+        <v>14</v>
       </c>
       <c r="H66" t="s">
         <v>16</v>
       </c>
       <c r="I66" t="s">
-        <v>20</v>
+        <v>301</v>
       </c>
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>292</v>
+        <v>281</v>
       </c>
       <c r="B67" t="s">
-        <v>99</v>
+        <v>237</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>291</v>
+        <v>282</v>
       </c>
       <c r="H67" t="s">
         <v>16</v>
@@ -2367,30 +2469,27 @@
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B68" t="s">
-        <v>259</v>
+        <v>40</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>154</v>
+        <v>152</v>
+      </c>
+      <c r="E68" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>228</v>
+        <v>242</v>
       </c>
       <c r="B69" t="s">
-        <v>40</v>
+        <v>237</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>225</v>
-      </c>
-      <c r="F69">
-        <v>1989</v>
-      </c>
-      <c r="G69">
-        <v>2017</v>
+        <v>243</v>
       </c>
       <c r="H69" t="s">
         <v>16</v>
@@ -2401,13 +2500,13 @@
     </row>
     <row r="70" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>245</v>
+        <v>292</v>
       </c>
       <c r="B70" t="s">
-        <v>237</v>
+        <v>99</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>244</v>
+        <v>291</v>
       </c>
       <c r="H70" t="s">
         <v>16</v>
@@ -2418,24 +2517,30 @@
     </row>
     <row r="71" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>100</v>
+        <v>153</v>
       </c>
       <c r="B71" t="s">
-        <v>99</v>
+        <v>259</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>101</v>
+        <v>154</v>
       </c>
     </row>
     <row r="72" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>239</v>
+        <v>228</v>
       </c>
       <c r="B72" t="s">
-        <v>237</v>
+        <v>40</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>243</v>
+        <v>225</v>
+      </c>
+      <c r="F72">
+        <v>1989</v>
+      </c>
+      <c r="G72">
+        <v>2017</v>
       </c>
       <c r="H72" t="s">
         <v>16</v>
@@ -2446,22 +2551,13 @@
     </row>
     <row r="73" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>254</v>
+        <v>245</v>
       </c>
       <c r="B73" t="s">
-        <v>55</v>
+        <v>237</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>253</v>
-      </c>
-      <c r="E73" t="s">
-        <v>255</v>
-      </c>
-      <c r="F73">
-        <v>1960</v>
-      </c>
-      <c r="G73">
-        <v>2014</v>
+        <v>244</v>
       </c>
       <c r="H73" t="s">
         <v>16</v>
@@ -2472,76 +2568,73 @@
     </row>
     <row r="74" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>270</v>
+        <v>100</v>
       </c>
       <c r="B74" t="s">
-        <v>55</v>
+        <v>99</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>271</v>
-      </c>
-      <c r="F74">
-        <v>1990</v>
-      </c>
-      <c r="G74">
-        <v>2010</v>
-      </c>
-      <c r="H74" t="s">
-        <v>16</v>
-      </c>
-      <c r="I74" t="s">
-        <v>20</v>
+        <v>101</v>
       </c>
     </row>
     <row r="75" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>117</v>
+        <v>239</v>
       </c>
       <c r="B75" t="s">
+        <v>237</v>
+      </c>
+      <c r="C75" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="H75" t="s">
+        <v>16</v>
+      </c>
+      <c r="I75" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A76" t="s">
+        <v>254</v>
+      </c>
+      <c r="B76" t="s">
         <v>55</v>
       </c>
-      <c r="C75" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="I75" t="s">
-        <v>20</v>
-      </c>
-      <c r="J75" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A76" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B76" t="s">
-        <v>25</v>
-      </c>
       <c r="C76" s="2" t="s">
-        <v>53</v>
+        <v>253</v>
+      </c>
+      <c r="E76" t="s">
+        <v>255</v>
+      </c>
+      <c r="F76">
+        <v>1960</v>
+      </c>
+      <c r="G76">
+        <v>2014</v>
+      </c>
+      <c r="H76" t="s">
+        <v>16</v>
+      </c>
+      <c r="I76" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="77" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>267</v>
+        <v>270</v>
       </c>
       <c r="B77" t="s">
-        <v>250</v>
+        <v>55</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>266</v>
-      </c>
-      <c r="D77" t="s">
-        <v>269</v>
-      </c>
-      <c r="E77" t="s">
-        <v>268</v>
+        <v>271</v>
       </c>
       <c r="F77">
-        <v>1970</v>
+        <v>1990</v>
       </c>
       <c r="G77">
-        <v>2014</v>
+        <v>2010</v>
       </c>
       <c r="H77" t="s">
         <v>16</v>
@@ -2552,144 +2645,153 @@
     </row>
     <row r="78" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>96</v>
+        <v>117</v>
       </c>
       <c r="B78" t="s">
-        <v>25</v>
+        <v>55</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="E78" t="s">
-        <v>69</v>
-      </c>
-      <c r="F78">
-        <v>1995</v>
+        <v>118</v>
+      </c>
+      <c r="I78" t="s">
+        <v>20</v>
+      </c>
+      <c r="J78" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="79" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A79" t="s">
-        <v>11</v>
+      <c r="A79" s="1" t="s">
+        <v>23</v>
       </c>
       <c r="B79" t="s">
         <v>25</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D79" t="s">
-        <v>95</v>
-      </c>
-      <c r="E79" t="s">
-        <v>10</v>
-      </c>
-      <c r="F79">
-        <v>2007</v>
-      </c>
-      <c r="H79" t="s">
-        <v>16</v>
-      </c>
-      <c r="I79" t="s">
-        <v>21</v>
+        <v>53</v>
       </c>
     </row>
     <row r="80" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
+        <v>300</v>
+      </c>
+      <c r="B80" t="s">
+        <v>25</v>
+      </c>
+      <c r="C80" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="E80" t="s">
+        <v>299</v>
+      </c>
+      <c r="F80">
+        <v>1969</v>
+      </c>
+      <c r="H80" t="s">
+        <v>16</v>
+      </c>
+      <c r="I80" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A81" t="s">
+        <v>267</v>
+      </c>
+      <c r="B81" t="s">
+        <v>250</v>
+      </c>
+      <c r="C81" s="2" t="s">
+        <v>266</v>
+      </c>
+      <c r="D81" t="s">
+        <v>269</v>
+      </c>
+      <c r="E81" t="s">
+        <v>268</v>
+      </c>
+      <c r="F81">
+        <v>1970</v>
+      </c>
+      <c r="G81">
+        <v>2014</v>
+      </c>
+      <c r="H81" t="s">
+        <v>16</v>
+      </c>
+      <c r="I81" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A82" t="s">
+        <v>96</v>
+      </c>
+      <c r="B82" t="s">
+        <v>25</v>
+      </c>
+      <c r="C82" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="E82" t="s">
+        <v>69</v>
+      </c>
+      <c r="F82">
+        <v>1995</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A83" t="s">
+        <v>11</v>
+      </c>
+      <c r="B83" t="s">
+        <v>25</v>
+      </c>
+      <c r="C83" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D83" t="s">
+        <v>95</v>
+      </c>
+      <c r="E83" t="s">
+        <v>10</v>
+      </c>
+      <c r="F83">
+        <v>2007</v>
+      </c>
+      <c r="H83" t="s">
+        <v>16</v>
+      </c>
+      <c r="I83" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A84" t="s">
         <v>223</v>
       </c>
-      <c r="B80" t="s">
+      <c r="B84" t="s">
         <v>124</v>
       </c>
-      <c r="C80" s="2" t="s">
+      <c r="C84" s="2" t="s">
         <v>222</v>
       </c>
-      <c r="F80">
+      <c r="F84">
         <v>1</v>
       </c>
-      <c r="G80">
+      <c r="G84">
         <v>2010</v>
       </c>
-      <c r="H80" t="s">
-        <v>16</v>
-      </c>
-      <c r="I80" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A81" t="s">
+      <c r="H84" t="s">
+        <v>16</v>
+      </c>
+      <c r="I84" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A85" t="s">
         <v>226</v>
-      </c>
-      <c r="B81" t="s">
-        <v>40</v>
-      </c>
-      <c r="C81" s="2" t="s">
-        <v>225</v>
-      </c>
-      <c r="F81">
-        <v>1946</v>
-      </c>
-      <c r="G81">
-        <v>2016</v>
-      </c>
-      <c r="H81" t="s">
-        <v>16</v>
-      </c>
-      <c r="I81" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A82" t="s">
-        <v>97</v>
-      </c>
-      <c r="B82" t="s">
-        <v>128</v>
-      </c>
-      <c r="C82" s="2" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A83" t="s">
-        <v>278</v>
-      </c>
-      <c r="B83" t="s">
-        <v>124</v>
-      </c>
-      <c r="C83" s="2" t="s">
-        <v>279</v>
-      </c>
-      <c r="E83" t="s">
-        <v>280</v>
-      </c>
-      <c r="F83">
-        <v>1890</v>
-      </c>
-      <c r="G83">
-        <v>1996</v>
-      </c>
-      <c r="H83" t="s">
-        <v>16</v>
-      </c>
-      <c r="I83" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A84" t="s">
-        <v>156</v>
-      </c>
-      <c r="B84" t="s">
-        <v>25</v>
-      </c>
-      <c r="C84" s="2" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A85" t="s">
-        <v>229</v>
       </c>
       <c r="B85" t="s">
         <v>40</v>
@@ -2698,10 +2800,10 @@
         <v>225</v>
       </c>
       <c r="F85">
-        <v>1952</v>
+        <v>1946</v>
       </c>
       <c r="G85">
-        <v>1997</v>
+        <v>2016</v>
       </c>
       <c r="H85" t="s">
         <v>16</v>
@@ -2710,228 +2812,225 @@
         <v>20</v>
       </c>
     </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="B86" t="s">
-        <v>99</v>
+        <v>128</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.2">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>289</v>
+        <v>278</v>
       </c>
       <c r="B87" t="s">
         <v>124</v>
       </c>
       <c r="C87" s="2" t="s">
+        <v>279</v>
+      </c>
+      <c r="E87" t="s">
+        <v>280</v>
+      </c>
+      <c r="F87">
+        <v>1890</v>
+      </c>
+      <c r="G87">
+        <v>1996</v>
+      </c>
+      <c r="H87" t="s">
+        <v>16</v>
+      </c>
+      <c r="I87" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A88" t="s">
+        <v>156</v>
+      </c>
+      <c r="B88" t="s">
+        <v>25</v>
+      </c>
+      <c r="C88" s="2" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A89" t="s">
+        <v>229</v>
+      </c>
+      <c r="B89" t="s">
+        <v>40</v>
+      </c>
+      <c r="C89" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="F89">
+        <v>1952</v>
+      </c>
+      <c r="G89">
+        <v>1997</v>
+      </c>
+      <c r="H89" t="s">
+        <v>16</v>
+      </c>
+      <c r="I89" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="90" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A90" t="s">
+        <v>293</v>
+      </c>
+      <c r="B90" t="s">
+        <v>40</v>
+      </c>
+      <c r="C90" s="2" t="s">
+        <v>294</v>
+      </c>
+      <c r="F90">
+        <v>2004</v>
+      </c>
+      <c r="G90">
+        <v>2006</v>
+      </c>
+      <c r="H90" t="s">
+        <v>16</v>
+      </c>
+      <c r="I90" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="91" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A91" t="s">
+        <v>102</v>
+      </c>
+      <c r="B91" t="s">
+        <v>99</v>
+      </c>
+      <c r="C91" s="2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="92" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A92" t="s">
+        <v>289</v>
+      </c>
+      <c r="B92" t="s">
+        <v>124</v>
+      </c>
+      <c r="C92" s="2" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A88" t="s">
+    <row r="93" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A93" t="s">
         <v>246</v>
       </c>
-      <c r="B88" t="s">
+      <c r="B93" t="s">
         <v>165</v>
       </c>
-      <c r="C88" s="2" t="s">
+      <c r="C93" s="2" t="s">
         <v>247</v>
       </c>
-      <c r="E88" t="s">
+      <c r="E93" t="s">
         <v>14</v>
       </c>
-      <c r="F88">
+      <c r="F93">
         <v>1960</v>
       </c>
-      <c r="G88">
+      <c r="G93">
         <v>2006</v>
       </c>
-      <c r="H88" t="s">
-        <v>16</v>
-      </c>
-      <c r="I88" t="s">
+      <c r="H93" t="s">
+        <v>16</v>
+      </c>
+      <c r="I93" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A89" t="s">
+    <row r="94" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A94" t="s">
         <v>208</v>
       </c>
-      <c r="B89" t="s">
+      <c r="B94" t="s">
         <v>124</v>
       </c>
-      <c r="C89" s="2" t="s">
+      <c r="C94" s="2" t="s">
         <v>209</v>
       </c>
-      <c r="F89">
+      <c r="F94">
         <v>1932</v>
       </c>
-      <c r="G89">
+      <c r="G94">
         <v>2014</v>
       </c>
-      <c r="H89" t="s">
-        <v>16</v>
-      </c>
-      <c r="I89" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A90" t="s">
+      <c r="H94" t="s">
+        <v>16</v>
+      </c>
+      <c r="I94" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="95" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A95" t="s">
         <v>137</v>
       </c>
-      <c r="B90" t="s">
+      <c r="B95" t="s">
         <v>259</v>
       </c>
-      <c r="C90" s="2" t="s">
+      <c r="C95" s="2" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A91" t="s">
+    <row r="96" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A96" t="s">
         <v>155</v>
       </c>
-      <c r="B91" t="s">
+      <c r="B96" t="s">
         <v>259</v>
       </c>
-      <c r="C91" s="2" t="s">
+      <c r="C96" s="2" t="s">
         <v>154</v>
-      </c>
-    </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A92" t="s">
-        <v>57</v>
-      </c>
-      <c r="B92" t="s">
-        <v>128</v>
-      </c>
-      <c r="C92" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="J92" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A93" t="s">
-        <v>129</v>
-      </c>
-      <c r="B93" t="s">
-        <v>259</v>
-      </c>
-      <c r="C93" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="E93" t="s">
-        <v>131</v>
-      </c>
-      <c r="F93">
-        <v>1945</v>
-      </c>
-      <c r="G93">
-        <v>2008</v>
-      </c>
-      <c r="I93" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A94" t="s">
-        <v>148</v>
-      </c>
-      <c r="B94" t="s">
-        <v>128</v>
-      </c>
-      <c r="C94" s="2" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A95" t="s">
-        <v>233</v>
-      </c>
-      <c r="B95" t="s">
-        <v>165</v>
-      </c>
-      <c r="C95" s="2" t="s">
-        <v>234</v>
-      </c>
-      <c r="E95" t="s">
-        <v>14</v>
-      </c>
-      <c r="F95">
-        <v>2012</v>
-      </c>
-      <c r="G95">
-        <v>2016</v>
-      </c>
-      <c r="H95" t="s">
-        <v>16</v>
-      </c>
-      <c r="I95" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A96" t="s">
-        <v>35</v>
-      </c>
-      <c r="B96" t="s">
-        <v>25</v>
-      </c>
-      <c r="C96" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="D96" t="s">
-        <v>37</v>
-      </c>
-      <c r="E96" t="s">
-        <v>14</v>
-      </c>
-      <c r="F96">
-        <v>2001</v>
-      </c>
-      <c r="H96" t="s">
-        <v>16</v>
-      </c>
-      <c r="I96" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="97" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>185</v>
+        <v>57</v>
       </c>
       <c r="B97" t="s">
         <v>128</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>186</v>
+        <v>58</v>
+      </c>
+      <c r="J97" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="98" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>210</v>
+        <v>129</v>
       </c>
       <c r="B98" t="s">
-        <v>40</v>
+        <v>259</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>211</v>
+        <v>130</v>
+      </c>
+      <c r="E98" t="s">
+        <v>131</v>
       </c>
       <c r="F98">
-        <v>1976</v>
+        <v>1945</v>
       </c>
       <c r="G98">
-        <v>2016</v>
-      </c>
-      <c r="H98" t="s">
-        <v>16</v>
+        <v>2008</v>
       </c>
       <c r="I98" t="s">
         <v>20</v>
@@ -2939,30 +3038,36 @@
     </row>
     <row r="99" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="B99" t="s">
-        <v>60</v>
+        <v>128</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="F99">
-        <v>1800</v>
-      </c>
-      <c r="G99">
-        <v>2013</v>
+        <v>147</v>
       </c>
     </row>
     <row r="100" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>122</v>
+        <v>233</v>
       </c>
       <c r="B100" t="s">
-        <v>259</v>
+        <v>165</v>
       </c>
       <c r="C100" s="2" t="s">
-        <v>121</v>
+        <v>234</v>
+      </c>
+      <c r="E100" t="s">
+        <v>14</v>
+      </c>
+      <c r="F100">
+        <v>2012</v>
+      </c>
+      <c r="G100">
+        <v>2016</v>
+      </c>
+      <c r="H100" t="s">
+        <v>16</v>
       </c>
       <c r="I100" t="s">
         <v>20</v>
@@ -2970,44 +3075,56 @@
     </row>
     <row r="101" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>141</v>
+        <v>35</v>
       </c>
       <c r="B101" t="s">
-        <v>237</v>
+        <v>25</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="J101" t="s">
-        <v>17</v>
+        <v>36</v>
+      </c>
+      <c r="D101" t="s">
+        <v>37</v>
+      </c>
+      <c r="E101" t="s">
+        <v>14</v>
+      </c>
+      <c r="F101">
+        <v>2001</v>
+      </c>
+      <c r="H101" t="s">
+        <v>16</v>
+      </c>
+      <c r="I101" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="102" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>287</v>
+        <v>185</v>
       </c>
       <c r="B102" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="C102" s="2" t="s">
-        <v>288</v>
-      </c>
-      <c r="F102">
-        <v>1990</v>
-      </c>
-      <c r="G102">
-        <v>2008</v>
+        <v>186</v>
       </c>
     </row>
     <row r="103" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>274</v>
+        <v>210</v>
       </c>
       <c r="B103" t="s">
-        <v>55</v>
+        <v>40</v>
       </c>
       <c r="C103" s="2" t="s">
-        <v>275</v>
+        <v>211</v>
+      </c>
+      <c r="F103">
+        <v>1976</v>
+      </c>
+      <c r="G103">
+        <v>2016</v>
       </c>
       <c r="H103" t="s">
         <v>16</v>
@@ -3018,41 +3135,53 @@
     </row>
     <row r="104" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>157</v>
+        <v>144</v>
       </c>
       <c r="B104" t="s">
-        <v>128</v>
+        <v>60</v>
       </c>
       <c r="C104" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="J104" t="s">
-        <v>18</v>
+        <v>143</v>
+      </c>
+      <c r="F104">
+        <v>1800</v>
+      </c>
+      <c r="G104">
+        <v>2013</v>
       </c>
     </row>
     <row r="105" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>194</v>
+        <v>122</v>
       </c>
       <c r="B105" t="s">
-        <v>99</v>
+        <v>259</v>
       </c>
       <c r="C105" s="2" t="s">
-        <v>193</v>
+        <v>121</v>
+      </c>
+      <c r="I105" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="106" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>256</v>
+        <v>318</v>
       </c>
       <c r="B106" t="s">
         <v>250</v>
       </c>
       <c r="C106" s="2" t="s">
-        <v>257</v>
+        <v>319</v>
       </c>
       <c r="E106" t="s">
-        <v>258</v>
+        <v>320</v>
+      </c>
+      <c r="F106">
+        <v>1975</v>
+      </c>
+      <c r="G106">
+        <v>1989</v>
       </c>
       <c r="H106" t="s">
         <v>16</v>
@@ -3063,19 +3192,22 @@
     </row>
     <row r="107" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>227</v>
+        <v>316</v>
       </c>
       <c r="B107" t="s">
-        <v>40</v>
+        <v>250</v>
       </c>
       <c r="C107" s="2" t="s">
-        <v>225</v>
+        <v>317</v>
+      </c>
+      <c r="E107" t="s">
+        <v>105</v>
       </c>
       <c r="F107">
-        <v>1955</v>
+        <v>1950</v>
       </c>
       <c r="G107">
-        <v>2016</v>
+        <v>1996</v>
       </c>
       <c r="H107" t="s">
         <v>16</v>
@@ -3086,433 +3218,637 @@
     </row>
     <row r="108" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>230</v>
+        <v>141</v>
       </c>
       <c r="B108" t="s">
-        <v>40</v>
+        <v>237</v>
       </c>
       <c r="C108" s="2" t="s">
-        <v>225</v>
-      </c>
-      <c r="F108">
-        <v>1995</v>
-      </c>
-      <c r="G108">
-        <v>2016</v>
-      </c>
-      <c r="H108" t="s">
-        <v>16</v>
-      </c>
-      <c r="I108" t="s">
-        <v>20</v>
+        <v>142</v>
+      </c>
+      <c r="J108" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="109" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>109</v>
+        <v>308</v>
       </c>
       <c r="B109" t="s">
-        <v>25</v>
+        <v>250</v>
       </c>
       <c r="C109" s="2" t="s">
-        <v>110</v>
+        <v>309</v>
       </c>
       <c r="E109" t="s">
-        <v>111</v>
+        <v>310</v>
       </c>
       <c r="F109">
-        <v>1956</v>
+        <v>1950</v>
+      </c>
+      <c r="G109">
+        <v>2010</v>
+      </c>
+      <c r="H109" t="s">
+        <v>16</v>
+      </c>
+      <c r="I109" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="110" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>91</v>
+        <v>287</v>
       </c>
       <c r="B110" t="s">
-        <v>25</v>
+        <v>134</v>
       </c>
       <c r="C110" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="E110" t="s">
-        <v>92</v>
+        <v>288</v>
       </c>
       <c r="F110">
-        <v>1999</v>
+        <v>1990</v>
+      </c>
+      <c r="G110">
+        <v>2008</v>
       </c>
     </row>
     <row r="111" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>161</v>
+        <v>274</v>
       </c>
       <c r="B111" t="s">
-        <v>25</v>
+        <v>55</v>
       </c>
       <c r="C111" s="2" t="s">
-        <v>160</v>
+        <v>275</v>
+      </c>
+      <c r="H111" t="s">
+        <v>16</v>
+      </c>
+      <c r="I111" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="112" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>168</v>
+        <v>157</v>
       </c>
       <c r="B112" t="s">
+        <v>128</v>
+      </c>
+      <c r="C112" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="J112" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="113" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A113" t="s">
+        <v>194</v>
+      </c>
+      <c r="B113" t="s">
+        <v>99</v>
+      </c>
+      <c r="C113" s="2" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="114" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A114" t="s">
+        <v>295</v>
+      </c>
+      <c r="B114" t="s">
         <v>40</v>
       </c>
-      <c r="C112" s="2" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="113" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A113" t="s">
-        <v>213</v>
-      </c>
-      <c r="B113" t="s">
-        <v>55</v>
-      </c>
-      <c r="C113" s="2" t="s">
-        <v>212</v>
-      </c>
-      <c r="H113" t="s">
-        <v>16</v>
-      </c>
-      <c r="I113" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="114" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A114" t="s">
-        <v>273</v>
-      </c>
-      <c r="B114" t="s">
-        <v>237</v>
-      </c>
       <c r="C114" s="2" t="s">
-        <v>272</v>
+        <v>296</v>
+      </c>
+      <c r="E114" t="s">
+        <v>297</v>
       </c>
       <c r="F114">
-        <v>1996</v>
+        <v>1990</v>
       </c>
       <c r="G114">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="H114" t="s">
         <v>16</v>
       </c>
       <c r="I114" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="115" spans="1:10" x14ac:dyDescent="0.2">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="115" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>66</v>
+        <v>256</v>
       </c>
       <c r="B115" t="s">
-        <v>25</v>
+        <v>250</v>
       </c>
       <c r="C115" s="2" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="116" spans="1:10" x14ac:dyDescent="0.2">
+        <v>257</v>
+      </c>
+      <c r="E115" t="s">
+        <v>258</v>
+      </c>
+      <c r="H115" t="s">
+        <v>16</v>
+      </c>
+      <c r="I115" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="116" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>139</v>
+        <v>227</v>
       </c>
       <c r="B116" t="s">
         <v>40</v>
       </c>
       <c r="C116" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="F116">
+        <v>1955</v>
+      </c>
+      <c r="G116">
+        <v>2016</v>
+      </c>
+      <c r="H116" t="s">
+        <v>16</v>
+      </c>
+      <c r="I116" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="117" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A117" t="s">
+        <v>230</v>
+      </c>
+      <c r="B117" t="s">
+        <v>40</v>
+      </c>
+      <c r="C117" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="F117">
+        <v>1995</v>
+      </c>
+      <c r="G117">
+        <v>2016</v>
+      </c>
+      <c r="H117" t="s">
+        <v>16</v>
+      </c>
+      <c r="I117" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="118" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A118" t="s">
+        <v>109</v>
+      </c>
+      <c r="B118" t="s">
+        <v>25</v>
+      </c>
+      <c r="C118" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="E118" t="s">
+        <v>111</v>
+      </c>
+      <c r="F118">
+        <v>1956</v>
+      </c>
+    </row>
+    <row r="119" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A119" t="s">
+        <v>91</v>
+      </c>
+      <c r="B119" t="s">
+        <v>25</v>
+      </c>
+      <c r="C119" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="E119" t="s">
+        <v>92</v>
+      </c>
+      <c r="F119">
+        <v>1999</v>
+      </c>
+    </row>
+    <row r="120" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A120" t="s">
+        <v>314</v>
+      </c>
+      <c r="B120" t="s">
+        <v>40</v>
+      </c>
+      <c r="C120" s="2" t="s">
+        <v>313</v>
+      </c>
+      <c r="E120" t="s">
+        <v>315</v>
+      </c>
+      <c r="F120">
+        <v>1950</v>
+      </c>
+      <c r="G120">
+        <v>2004</v>
+      </c>
+      <c r="H120" t="s">
+        <v>16</v>
+      </c>
+      <c r="I120" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="121" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A121" t="s">
+        <v>161</v>
+      </c>
+      <c r="B121" t="s">
+        <v>25</v>
+      </c>
+      <c r="C121" s="2" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="122" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A122" t="s">
+        <v>168</v>
+      </c>
+      <c r="B122" t="s">
+        <v>40</v>
+      </c>
+      <c r="C122" s="2" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="123" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A123" t="s">
+        <v>213</v>
+      </c>
+      <c r="B123" t="s">
+        <v>55</v>
+      </c>
+      <c r="C123" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="H123" t="s">
+        <v>16</v>
+      </c>
+      <c r="I123" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="124" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A124" t="s">
+        <v>273</v>
+      </c>
+      <c r="B124" t="s">
+        <v>237</v>
+      </c>
+      <c r="C124" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="F124">
+        <v>1996</v>
+      </c>
+      <c r="G124">
+        <v>2016</v>
+      </c>
+      <c r="H124" t="s">
+        <v>16</v>
+      </c>
+      <c r="I124" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="125" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A125" t="s">
+        <v>66</v>
+      </c>
+      <c r="B125" t="s">
+        <v>25</v>
+      </c>
+      <c r="C125" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="126" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A126" t="s">
+        <v>139</v>
+      </c>
+      <c r="B126" t="s">
+        <v>40</v>
+      </c>
+      <c r="C126" s="2" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="117" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A117" t="s">
+    <row r="127" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A127" t="s">
         <v>172</v>
       </c>
-      <c r="B117" t="s">
+      <c r="B127" t="s">
         <v>60</v>
       </c>
-      <c r="C117" s="2" t="s">
+      <c r="C127" s="2" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="118" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A118" t="s">
+    <row r="128" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A128" t="s">
         <v>217</v>
       </c>
-      <c r="B118" t="s">
+      <c r="B128" t="s">
         <v>60</v>
       </c>
-      <c r="C118" s="2" t="s">
+      <c r="C128" s="2" t="s">
         <v>216</v>
       </c>
-      <c r="E118" t="s">
+      <c r="E128" t="s">
         <v>14</v>
       </c>
-      <c r="F118">
+      <c r="F128">
         <v>1900</v>
       </c>
-      <c r="H118" t="s">
-        <v>16</v>
-      </c>
-      <c r="I118" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="119" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A119" t="s">
+      <c r="H128" t="s">
+        <v>16</v>
+      </c>
+      <c r="I128" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="129" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A129" t="s">
         <v>132</v>
       </c>
-      <c r="B119" t="s">
+      <c r="B129" t="s">
         <v>259</v>
       </c>
-      <c r="C119" s="2" t="s">
+      <c r="C129" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="J119" t="s">
+      <c r="J129" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="120" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A120" t="s">
+    <row r="130" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A130" t="s">
         <v>182</v>
       </c>
-      <c r="B120" t="s">
+      <c r="B130" t="s">
         <v>165</v>
       </c>
-      <c r="C120" s="2" t="s">
+      <c r="C130" s="2" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="121" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A121" t="s">
+    <row r="131" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A131" t="s">
         <v>115</v>
       </c>
-      <c r="B121" t="s">
+      <c r="B131" t="s">
         <v>128</v>
       </c>
-      <c r="C121" s="2" t="s">
+      <c r="C131" s="2" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="122" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A122" t="s">
+    <row r="132" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A132" t="s">
         <v>263</v>
       </c>
-      <c r="B122" t="s">
+      <c r="B132" t="s">
         <v>250</v>
       </c>
-      <c r="C122" s="2" t="s">
+      <c r="C132" s="2" t="s">
         <v>264</v>
       </c>
-      <c r="E122" t="s">
+      <c r="E132" t="s">
         <v>265</v>
       </c>
-      <c r="F122">
+      <c r="F132">
         <v>1500</v>
       </c>
-      <c r="G122">
+      <c r="G132">
         <v>2000</v>
       </c>
-      <c r="H122" t="s">
-        <v>16</v>
-      </c>
-      <c r="I122" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="123" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A123" t="s">
+      <c r="H132" t="s">
+        <v>16</v>
+      </c>
+      <c r="I132" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="133" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A133" t="s">
         <v>221</v>
       </c>
-      <c r="B123" t="s">
+      <c r="B133" t="s">
         <v>86</v>
       </c>
-      <c r="C123" s="2" t="s">
+      <c r="C133" s="2" t="s">
         <v>220</v>
       </c>
-      <c r="F123">
+      <c r="F133">
         <v>2013</v>
       </c>
-      <c r="H123" t="s">
-        <v>16</v>
-      </c>
-      <c r="I123" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="124" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A124" t="s">
+      <c r="H133" t="s">
+        <v>16</v>
+      </c>
+      <c r="I133" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="134" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A134" t="s">
         <v>13</v>
       </c>
-      <c r="B124" t="s">
+      <c r="B134" t="s">
         <v>25</v>
       </c>
-      <c r="C124" s="2" t="s">
+      <c r="C134" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="D124" s="1" t="s">
+      <c r="D134" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="E124" t="s">
+      <c r="E134" t="s">
         <v>14</v>
       </c>
-      <c r="F124">
+      <c r="F134">
         <v>1981</v>
       </c>
-      <c r="H124" t="s">
-        <v>16</v>
-      </c>
-      <c r="I124" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="125" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A125" t="s">
+      <c r="H134" t="s">
+        <v>16</v>
+      </c>
+      <c r="I134" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="135" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A135" t="s">
         <v>283</v>
       </c>
-      <c r="B125" t="s">
+      <c r="B135" t="s">
         <v>124</v>
       </c>
-      <c r="C125" s="2" t="s">
+      <c r="C135" s="2" t="s">
         <v>284</v>
       </c>
-      <c r="H125" t="s">
-        <v>16</v>
-      </c>
-      <c r="I125" t="s">
+      <c r="H135" t="s">
+        <v>16</v>
+      </c>
+      <c r="I135" t="s">
         <v>20</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:J125">
+  <sortState ref="A2:J135">
     <sortCondition ref="A2"/>
   </sortState>
   <hyperlinks>
     <hyperlink ref="C6" r:id="rId1"/>
-    <hyperlink ref="C52" r:id="rId2"/>
+    <hyperlink ref="C54" r:id="rId2"/>
     <hyperlink ref="C7" r:id="rId3"/>
     <hyperlink ref="C10" r:id="rId4"/>
-    <hyperlink ref="C79" r:id="rId5"/>
-    <hyperlink ref="C96" r:id="rId6"/>
-    <hyperlink ref="C124" r:id="rId7"/>
-    <hyperlink ref="C31" r:id="rId8"/>
-    <hyperlink ref="C27" r:id="rId9"/>
-    <hyperlink ref="C43" r:id="rId10"/>
-    <hyperlink ref="C50" r:id="rId11"/>
+    <hyperlink ref="C83" r:id="rId5"/>
+    <hyperlink ref="C101" r:id="rId6"/>
+    <hyperlink ref="C134" r:id="rId7"/>
+    <hyperlink ref="C33" r:id="rId8"/>
+    <hyperlink ref="C29" r:id="rId9"/>
+    <hyperlink ref="C45" r:id="rId10"/>
+    <hyperlink ref="C52" r:id="rId11"/>
     <hyperlink ref="C3" r:id="rId12"/>
-    <hyperlink ref="C18" r:id="rId13"/>
-    <hyperlink ref="C54" r:id="rId14"/>
-    <hyperlink ref="C76" r:id="rId15"/>
-    <hyperlink ref="C26" r:id="rId16"/>
-    <hyperlink ref="C92" r:id="rId17"/>
-    <hyperlink ref="C35" r:id="rId18"/>
-    <hyperlink ref="C63" r:id="rId19"/>
-    <hyperlink ref="C15" r:id="rId20"/>
-    <hyperlink ref="C115" r:id="rId21"/>
+    <hyperlink ref="C20" r:id="rId13"/>
+    <hyperlink ref="C56" r:id="rId14"/>
+    <hyperlink ref="C79" r:id="rId15"/>
+    <hyperlink ref="C28" r:id="rId16"/>
+    <hyperlink ref="C97" r:id="rId17"/>
+    <hyperlink ref="C37" r:id="rId18"/>
+    <hyperlink ref="C65" r:id="rId19"/>
+    <hyperlink ref="C16" r:id="rId20"/>
+    <hyperlink ref="C125" r:id="rId21"/>
     <hyperlink ref="C8" r:id="rId22"/>
-    <hyperlink ref="C33" r:id="rId23"/>
-    <hyperlink ref="C47" r:id="rId24"/>
-    <hyperlink ref="C44" r:id="rId25"/>
-    <hyperlink ref="C48" r:id="rId26"/>
-    <hyperlink ref="C49" r:id="rId27"/>
-    <hyperlink ref="C61" r:id="rId28"/>
-    <hyperlink ref="C78" r:id="rId29"/>
-    <hyperlink ref="C110" r:id="rId30"/>
-    <hyperlink ref="C82" r:id="rId31"/>
-    <hyperlink ref="C71" r:id="rId32"/>
-    <hyperlink ref="C86" r:id="rId33"/>
-    <hyperlink ref="C62" r:id="rId34"/>
-    <hyperlink ref="C16" r:id="rId35"/>
-    <hyperlink ref="C109" r:id="rId36"/>
-    <hyperlink ref="C14" r:id="rId37"/>
-    <hyperlink ref="C121" r:id="rId38"/>
-    <hyperlink ref="C75" r:id="rId39"/>
-    <hyperlink ref="C51" r:id="rId40"/>
-    <hyperlink ref="C100" r:id="rId41"/>
-    <hyperlink ref="C17" r:id="rId42"/>
-    <hyperlink ref="C45" r:id="rId43"/>
-    <hyperlink ref="C20" r:id="rId44"/>
-    <hyperlink ref="C93" r:id="rId45"/>
-    <hyperlink ref="C119" r:id="rId46"/>
-    <hyperlink ref="C24" r:id="rId47" display="http://comparativeconstitutionsproject.org/"/>
-    <hyperlink ref="C90" r:id="rId48"/>
-    <hyperlink ref="C116" r:id="rId49"/>
-    <hyperlink ref="C101" r:id="rId50"/>
-    <hyperlink ref="C99" r:id="rId51"/>
-    <hyperlink ref="C19" r:id="rId52"/>
-    <hyperlink ref="C94" r:id="rId53"/>
-    <hyperlink ref="C42" r:id="rId54"/>
-    <hyperlink ref="C65" r:id="rId55"/>
-    <hyperlink ref="C68" r:id="rId56"/>
-    <hyperlink ref="C91" r:id="rId57"/>
-    <hyperlink ref="C84" r:id="rId58"/>
-    <hyperlink ref="C104" r:id="rId59"/>
-    <hyperlink ref="C28" r:id="rId60"/>
-    <hyperlink ref="C111" r:id="rId61"/>
+    <hyperlink ref="C35" r:id="rId23"/>
+    <hyperlink ref="C49" r:id="rId24"/>
+    <hyperlink ref="C46" r:id="rId25"/>
+    <hyperlink ref="C50" r:id="rId26"/>
+    <hyperlink ref="C51" r:id="rId27"/>
+    <hyperlink ref="C63" r:id="rId28"/>
+    <hyperlink ref="C82" r:id="rId29"/>
+    <hyperlink ref="C119" r:id="rId30"/>
+    <hyperlink ref="C86" r:id="rId31"/>
+    <hyperlink ref="C74" r:id="rId32"/>
+    <hyperlink ref="C91" r:id="rId33"/>
+    <hyperlink ref="C64" r:id="rId34"/>
+    <hyperlink ref="C17" r:id="rId35"/>
+    <hyperlink ref="C118" r:id="rId36"/>
+    <hyperlink ref="C15" r:id="rId37"/>
+    <hyperlink ref="C131" r:id="rId38"/>
+    <hyperlink ref="C78" r:id="rId39"/>
+    <hyperlink ref="C53" r:id="rId40"/>
+    <hyperlink ref="C105" r:id="rId41"/>
+    <hyperlink ref="C18" r:id="rId42"/>
+    <hyperlink ref="C47" r:id="rId43"/>
+    <hyperlink ref="C22" r:id="rId44"/>
+    <hyperlink ref="C98" r:id="rId45"/>
+    <hyperlink ref="C129" r:id="rId46"/>
+    <hyperlink ref="C26" r:id="rId47" display="http://comparativeconstitutionsproject.org/"/>
+    <hyperlink ref="C95" r:id="rId48"/>
+    <hyperlink ref="C126" r:id="rId49"/>
+    <hyperlink ref="C108" r:id="rId50"/>
+    <hyperlink ref="C104" r:id="rId51"/>
+    <hyperlink ref="C21" r:id="rId52"/>
+    <hyperlink ref="C99" r:id="rId53"/>
+    <hyperlink ref="C44" r:id="rId54"/>
+    <hyperlink ref="C68" r:id="rId55"/>
+    <hyperlink ref="C71" r:id="rId56"/>
+    <hyperlink ref="C96" r:id="rId57"/>
+    <hyperlink ref="C88" r:id="rId58"/>
+    <hyperlink ref="C112" r:id="rId59"/>
+    <hyperlink ref="C30" r:id="rId60"/>
+    <hyperlink ref="C121" r:id="rId61"/>
     <hyperlink ref="C9" r:id="rId62"/>
-    <hyperlink ref="C30" r:id="rId63"/>
-    <hyperlink ref="C112" r:id="rId64"/>
-    <hyperlink ref="C13" r:id="rId65"/>
-    <hyperlink ref="C117" r:id="rId66"/>
-    <hyperlink ref="C22" r:id="rId67"/>
-    <hyperlink ref="C21" r:id="rId68"/>
-    <hyperlink ref="C23" r:id="rId69"/>
-    <hyperlink ref="C46" r:id="rId70"/>
-    <hyperlink ref="C120" r:id="rId71"/>
-    <hyperlink ref="C25" r:id="rId72"/>
-    <hyperlink ref="C97" r:id="rId73"/>
-    <hyperlink ref="C29" r:id="rId74"/>
-    <hyperlink ref="C39" r:id="rId75"/>
-    <hyperlink ref="C105" r:id="rId76"/>
-    <hyperlink ref="C36" r:id="rId77"/>
-    <hyperlink ref="C34" r:id="rId78"/>
-    <hyperlink ref="C60" r:id="rId79"/>
+    <hyperlink ref="C32" r:id="rId63"/>
+    <hyperlink ref="C122" r:id="rId64"/>
+    <hyperlink ref="C14" r:id="rId65"/>
+    <hyperlink ref="C127" r:id="rId66"/>
+    <hyperlink ref="C24" r:id="rId67"/>
+    <hyperlink ref="C23" r:id="rId68"/>
+    <hyperlink ref="C25" r:id="rId69"/>
+    <hyperlink ref="C48" r:id="rId70"/>
+    <hyperlink ref="C130" r:id="rId71"/>
+    <hyperlink ref="C27" r:id="rId72"/>
+    <hyperlink ref="C102" r:id="rId73"/>
+    <hyperlink ref="C31" r:id="rId74"/>
+    <hyperlink ref="C41" r:id="rId75"/>
+    <hyperlink ref="C113" r:id="rId76"/>
+    <hyperlink ref="C38" r:id="rId77"/>
+    <hyperlink ref="C36" r:id="rId78"/>
+    <hyperlink ref="C62" r:id="rId79"/>
     <hyperlink ref="C5" r:id="rId80"/>
-    <hyperlink ref="C59" r:id="rId81"/>
-    <hyperlink ref="C11" r:id="rId82"/>
-    <hyperlink ref="C89" r:id="rId83"/>
-    <hyperlink ref="C98" r:id="rId84"/>
-    <hyperlink ref="C113" r:id="rId85"/>
-    <hyperlink ref="C32" r:id="rId86"/>
-    <hyperlink ref="C118" r:id="rId87"/>
-    <hyperlink ref="C38" r:id="rId88"/>
-    <hyperlink ref="C123" r:id="rId89"/>
-    <hyperlink ref="C80" r:id="rId90"/>
-    <hyperlink ref="C57" r:id="rId91"/>
-    <hyperlink ref="C81" r:id="rId92"/>
-    <hyperlink ref="C107" r:id="rId93"/>
-    <hyperlink ref="C69" r:id="rId94"/>
-    <hyperlink ref="C85" r:id="rId95"/>
-    <hyperlink ref="C108" r:id="rId96"/>
-    <hyperlink ref="C55" r:id="rId97"/>
-    <hyperlink ref="C95" r:id="rId98"/>
-    <hyperlink ref="C40" r:id="rId99"/>
-    <hyperlink ref="C37" r:id="rId100"/>
-    <hyperlink ref="C72" r:id="rId101"/>
-    <hyperlink ref="C53" r:id="rId102"/>
+    <hyperlink ref="C61" r:id="rId81"/>
+    <hyperlink ref="C12" r:id="rId82"/>
+    <hyperlink ref="C94" r:id="rId83"/>
+    <hyperlink ref="C103" r:id="rId84"/>
+    <hyperlink ref="C123" r:id="rId85"/>
+    <hyperlink ref="C34" r:id="rId86"/>
+    <hyperlink ref="C128" r:id="rId87"/>
+    <hyperlink ref="C40" r:id="rId88"/>
+    <hyperlink ref="C133" r:id="rId89"/>
+    <hyperlink ref="C84" r:id="rId90"/>
+    <hyperlink ref="C59" r:id="rId91"/>
+    <hyperlink ref="C85" r:id="rId92"/>
+    <hyperlink ref="C116" r:id="rId93"/>
+    <hyperlink ref="C72" r:id="rId94"/>
+    <hyperlink ref="C89" r:id="rId95"/>
+    <hyperlink ref="C117" r:id="rId96"/>
+    <hyperlink ref="C57" r:id="rId97"/>
+    <hyperlink ref="C100" r:id="rId98"/>
+    <hyperlink ref="C42" r:id="rId99"/>
+    <hyperlink ref="C39" r:id="rId100"/>
+    <hyperlink ref="C75" r:id="rId101"/>
+    <hyperlink ref="C55" r:id="rId102"/>
     <hyperlink ref="C2" r:id="rId103"/>
-    <hyperlink ref="C66" r:id="rId104"/>
-    <hyperlink ref="C70" r:id="rId105"/>
-    <hyperlink ref="C88" r:id="rId106"/>
-    <hyperlink ref="C41" r:id="rId107"/>
-    <hyperlink ref="C73" r:id="rId108"/>
-    <hyperlink ref="C106" r:id="rId109"/>
-    <hyperlink ref="C12" r:id="rId110"/>
+    <hyperlink ref="C69" r:id="rId104"/>
+    <hyperlink ref="C73" r:id="rId105"/>
+    <hyperlink ref="C93" r:id="rId106"/>
+    <hyperlink ref="C43" r:id="rId107"/>
+    <hyperlink ref="C76" r:id="rId108"/>
+    <hyperlink ref="C115" r:id="rId109"/>
+    <hyperlink ref="C13" r:id="rId110"/>
     <hyperlink ref="C4" r:id="rId111"/>
-    <hyperlink ref="C122" r:id="rId112"/>
-    <hyperlink ref="C77" r:id="rId113"/>
-    <hyperlink ref="C74" r:id="rId114"/>
-    <hyperlink ref="C114" r:id="rId115"/>
-    <hyperlink ref="C103" r:id="rId116"/>
-    <hyperlink ref="C56" r:id="rId117"/>
-    <hyperlink ref="C83" r:id="rId118"/>
-    <hyperlink ref="C64" r:id="rId119"/>
-    <hyperlink ref="C125" r:id="rId120"/>
-    <hyperlink ref="C58" r:id="rId121"/>
-    <hyperlink ref="C102" r:id="rId122"/>
-    <hyperlink ref="C87" r:id="rId123"/>
-    <hyperlink ref="C67" r:id="rId124"/>
+    <hyperlink ref="C132" r:id="rId112"/>
+    <hyperlink ref="C81" r:id="rId113"/>
+    <hyperlink ref="C77" r:id="rId114"/>
+    <hyperlink ref="C124" r:id="rId115"/>
+    <hyperlink ref="C111" r:id="rId116"/>
+    <hyperlink ref="C58" r:id="rId117"/>
+    <hyperlink ref="C87" r:id="rId118"/>
+    <hyperlink ref="C67" r:id="rId119"/>
+    <hyperlink ref="C135" r:id="rId120"/>
+    <hyperlink ref="C60" r:id="rId121"/>
+    <hyperlink ref="C110" r:id="rId122"/>
+    <hyperlink ref="C92" r:id="rId123"/>
+    <hyperlink ref="C70" r:id="rId124"/>
+    <hyperlink ref="C90" r:id="rId125"/>
+    <hyperlink ref="C114" r:id="rId126"/>
+    <hyperlink ref="C80" r:id="rId127"/>
+    <hyperlink ref="C11" r:id="rId128"/>
+    <hyperlink ref="C19" r:id="rId129"/>
+    <hyperlink ref="C109" r:id="rId130"/>
+    <hyperlink ref="C66" r:id="rId131"/>
+    <hyperlink ref="C120" r:id="rId132"/>
+    <hyperlink ref="C107" r:id="rId133"/>
+    <hyperlink ref="C106" r:id="rId134"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
add 6 datasets (polls, judicial and election data)
</commit_message>
<xml_diff>
--- a/PolData.xlsx
+++ b/PolData.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="599" uniqueCount="321">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="635" uniqueCount="335">
   <si>
     <t>name</t>
   </si>
@@ -990,6 +990,48 @@
   </si>
   <si>
     <t>France, Germany, Switzerland, the Netherlands</t>
+  </si>
+  <si>
+    <t>https://github.com/erikgahner/polls</t>
+  </si>
+  <si>
+    <t>Public support for political parties in Denmark</t>
+  </si>
+  <si>
+    <t>The Timeline of Elections</t>
+  </si>
+  <si>
+    <t>http://doi.org/10.7910/DVN/28856</t>
+  </si>
+  <si>
+    <t>45 countries</t>
+  </si>
+  <si>
+    <t>SwedishPolls</t>
+  </si>
+  <si>
+    <t>https://github.com/MansMeg/SwedishPolls</t>
+  </si>
+  <si>
+    <t>https://github.com/zonination/election-history</t>
+  </si>
+  <si>
+    <t>US Presidential Elections</t>
+  </si>
+  <si>
+    <t>Danish General Election Results</t>
+  </si>
+  <si>
+    <t>https://github.com/Straubinger/folketingsvalg</t>
+  </si>
+  <si>
+    <t>Judicial Checks and Balances</t>
+  </si>
+  <si>
+    <t>http://faculty.tuck.dartmouth.edu/rafael-laporta/research-publications/</t>
+  </si>
+  <si>
+    <t>71 countries</t>
   </si>
 </sst>
 </file>
@@ -1321,10 +1363,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J135"/>
+  <dimension ref="A1:J141"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A101" workbookViewId="0">
-      <selection activeCell="B53" sqref="B53"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1914,107 +1956,107 @@
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>75</v>
+        <v>330</v>
       </c>
       <c r="B35" t="s">
-        <v>25</v>
+        <v>165</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>76</v>
+        <v>331</v>
       </c>
       <c r="E35" t="s">
         <v>77</v>
       </c>
       <c r="F35">
-        <v>1971</v>
+        <v>1953</v>
+      </c>
+      <c r="H35" t="s">
+        <v>16</v>
+      </c>
+      <c r="I35" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>197</v>
+        <v>75</v>
       </c>
       <c r="B36" t="s">
-        <v>55</v>
+        <v>25</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>198</v>
+        <v>76</v>
       </c>
       <c r="E36" t="s">
-        <v>199</v>
+        <v>77</v>
       </c>
       <c r="F36">
-        <v>1975</v>
-      </c>
-      <c r="G36">
-        <v>2015</v>
-      </c>
-      <c r="H36" t="s">
-        <v>16</v>
-      </c>
-      <c r="I36" t="s">
-        <v>20</v>
+        <v>1971</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>59</v>
+        <v>197</v>
       </c>
       <c r="B37" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>61</v>
+        <v>198</v>
+      </c>
+      <c r="E37" t="s">
+        <v>199</v>
+      </c>
+      <c r="F37">
+        <v>1975</v>
+      </c>
+      <c r="G37">
+        <v>2015</v>
+      </c>
+      <c r="H37" t="s">
+        <v>16</v>
+      </c>
+      <c r="I37" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>196</v>
+        <v>59</v>
       </c>
       <c r="B38" t="s">
-        <v>165</v>
+        <v>60</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>195</v>
-      </c>
-      <c r="F38">
-        <v>1946</v>
-      </c>
-      <c r="G38">
-        <v>2016</v>
+        <v>61</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>238</v>
+        <v>196</v>
       </c>
       <c r="B39" t="s">
-        <v>237</v>
+        <v>165</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>243</v>
-      </c>
-      <c r="H39" t="s">
-        <v>16</v>
-      </c>
-      <c r="I39" t="s">
-        <v>20</v>
+        <v>195</v>
+      </c>
+      <c r="F39">
+        <v>1946</v>
+      </c>
+      <c r="G39">
+        <v>2016</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>219</v>
+        <v>238</v>
       </c>
       <c r="B40" t="s">
-        <v>124</v>
+        <v>237</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>218</v>
-      </c>
-      <c r="F40">
-        <v>1970</v>
-      </c>
-      <c r="G40">
-        <v>2015</v>
+        <v>243</v>
       </c>
       <c r="H40" t="s">
         <v>16</v>
@@ -2025,44 +2067,50 @@
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>191</v>
+        <v>219</v>
       </c>
       <c r="B41" t="s">
-        <v>25</v>
+        <v>124</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="E41" t="s">
-        <v>192</v>
+        <v>218</v>
+      </c>
+      <c r="F41">
+        <v>1970</v>
+      </c>
+      <c r="G41">
+        <v>2015</v>
+      </c>
+      <c r="H41" t="s">
+        <v>16</v>
+      </c>
+      <c r="I41" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>235</v>
+        <v>191</v>
       </c>
       <c r="B42" t="s">
-        <v>60</v>
+        <v>25</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>236</v>
-      </c>
-      <c r="H42" t="s">
-        <v>16</v>
-      </c>
-      <c r="I42" t="s">
-        <v>20</v>
+        <v>190</v>
+      </c>
+      <c r="E42" t="s">
+        <v>192</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>252</v>
+        <v>235</v>
       </c>
       <c r="B43" t="s">
-        <v>250</v>
+        <v>60</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>251</v>
+        <v>236</v>
       </c>
       <c r="H43" t="s">
         <v>16</v>
@@ -2073,91 +2121,91 @@
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>149</v>
+        <v>252</v>
       </c>
       <c r="B44" t="s">
-        <v>128</v>
+        <v>250</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>150</v>
+        <v>251</v>
+      </c>
+      <c r="H44" t="s">
+        <v>16</v>
+      </c>
+      <c r="I44" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>28</v>
+        <v>149</v>
       </c>
       <c r="B45" t="s">
-        <v>25</v>
+        <v>128</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>48</v>
+        <v>150</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>80</v>
+        <v>28</v>
       </c>
       <c r="B46" t="s">
-        <v>128</v>
+        <v>25</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="E46" t="s">
-        <v>9</v>
-      </c>
-      <c r="F46">
-        <v>1979</v>
+        <v>48</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>125</v>
+        <v>80</v>
       </c>
       <c r="B47" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>126</v>
+        <v>81</v>
+      </c>
+      <c r="E47" t="s">
+        <v>9</v>
+      </c>
+      <c r="F47">
+        <v>1979</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>179</v>
+        <v>125</v>
       </c>
       <c r="B48" t="s">
-        <v>165</v>
+        <v>124</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>180</v>
+        <v>126</v>
       </c>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
+        <v>179</v>
+      </c>
+      <c r="B49" t="s">
+        <v>165</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
         <v>78</v>
       </c>
-      <c r="B49" t="s">
+      <c r="B50" t="s">
         <v>25</v>
       </c>
-      <c r="C49" s="2" t="s">
+      <c r="C50" s="2" t="s">
         <v>79</v>
-      </c>
-      <c r="E49" t="s">
-        <v>9</v>
-      </c>
-      <c r="F49">
-        <v>1979</v>
-      </c>
-    </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A50" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="B50" t="s">
-        <v>83</v>
-      </c>
-      <c r="C50" s="2" t="s">
-        <v>84</v>
       </c>
       <c r="E50" t="s">
         <v>9</v>
@@ -2168,13 +2216,13 @@
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A51" s="3" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B51" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="E51" t="s">
         <v>9</v>
@@ -2182,144 +2230,138 @@
       <c r="F51">
         <v>1979</v>
       </c>
-      <c r="G51">
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A52" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="B52" t="s">
+        <v>86</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="E52" t="s">
+        <v>9</v>
+      </c>
+      <c r="F52">
+        <v>1979</v>
+      </c>
+      <c r="G52">
         <v>2009</v>
-      </c>
-    </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A52" t="s">
-        <v>27</v>
-      </c>
-      <c r="B52" t="s">
-        <v>25</v>
-      </c>
-      <c r="C52" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="J52" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>120</v>
+        <v>27</v>
       </c>
       <c r="B53" t="s">
-        <v>259</v>
+        <v>25</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="I53" t="s">
-        <v>20</v>
+        <v>49</v>
+      </c>
+      <c r="J53" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>5</v>
+        <v>120</v>
       </c>
       <c r="B54" t="s">
-        <v>25</v>
+        <v>259</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D54" t="s">
-        <v>94</v>
-      </c>
-      <c r="E54" t="s">
-        <v>9</v>
-      </c>
-      <c r="F54">
-        <v>2002</v>
-      </c>
-      <c r="H54" t="s">
-        <v>16</v>
+        <v>119</v>
       </c>
       <c r="I54" t="s">
-        <v>248</v>
-      </c>
-      <c r="J54" t="s">
-        <v>44</v>
+        <v>20</v>
       </c>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
+        <v>5</v>
+      </c>
+      <c r="B55" t="s">
+        <v>25</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D55" t="s">
+        <v>94</v>
+      </c>
+      <c r="E55" t="s">
+        <v>9</v>
+      </c>
+      <c r="F55">
+        <v>2002</v>
+      </c>
+      <c r="H55" t="s">
+        <v>16</v>
+      </c>
+      <c r="I55" t="s">
+        <v>248</v>
+      </c>
+      <c r="J55" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
         <v>240</v>
       </c>
-      <c r="B55" t="s">
+      <c r="B56" t="s">
         <v>237</v>
       </c>
-      <c r="C55" s="2" t="s">
+      <c r="C56" s="2" t="s">
         <v>243</v>
       </c>
-      <c r="H55" t="s">
-        <v>16</v>
-      </c>
-      <c r="I55" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A56" s="1" t="s">
+      <c r="H56" t="s">
+        <v>16</v>
+      </c>
+      <c r="I56" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A57" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B56" t="s">
+      <c r="B57" t="s">
         <v>25</v>
       </c>
-      <c r="C56" s="2" t="s">
+      <c r="C57" s="2" t="s">
         <v>52</v>
-      </c>
-    </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A57" t="s">
-        <v>232</v>
-      </c>
-      <c r="B57" t="s">
-        <v>250</v>
-      </c>
-      <c r="C57" s="2" t="s">
-        <v>231</v>
       </c>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>276</v>
+        <v>232</v>
       </c>
       <c r="B58" t="s">
-        <v>124</v>
+        <v>250</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>277</v>
-      </c>
-      <c r="F58">
-        <v>1948</v>
-      </c>
-      <c r="G58">
-        <v>2000</v>
-      </c>
-      <c r="H58" t="s">
-        <v>16</v>
-      </c>
-      <c r="I58" t="s">
-        <v>20</v>
+        <v>231</v>
       </c>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>224</v>
+        <v>276</v>
       </c>
       <c r="B59" t="s">
-        <v>40</v>
+        <v>124</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>225</v>
+        <v>277</v>
       </c>
       <c r="F59">
-        <v>1964</v>
+        <v>1948</v>
       </c>
       <c r="G59">
-        <v>2008</v>
+        <v>2000</v>
       </c>
       <c r="H59" t="s">
         <v>16</v>
@@ -2330,13 +2372,19 @@
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>285</v>
+        <v>224</v>
       </c>
       <c r="B60" t="s">
-        <v>250</v>
+        <v>40</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>286</v>
+        <v>225</v>
+      </c>
+      <c r="F60">
+        <v>1964</v>
+      </c>
+      <c r="G60">
+        <v>2008</v>
       </c>
       <c r="H60" t="s">
         <v>16</v>
@@ -2347,166 +2395,166 @@
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>205</v>
+        <v>285</v>
       </c>
       <c r="B61" t="s">
-        <v>40</v>
+        <v>250</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>204</v>
-      </c>
-      <c r="F61">
-        <v>2006</v>
+        <v>286</v>
+      </c>
+      <c r="H61" t="s">
+        <v>16</v>
+      </c>
+      <c r="I61" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>200</v>
+        <v>205</v>
       </c>
       <c r="B62" t="s">
-        <v>99</v>
+        <v>40</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="F62">
-        <v>1980</v>
-      </c>
-      <c r="G62">
-        <v>2007</v>
-      </c>
-      <c r="J62" t="s">
-        <v>18</v>
+        <v>2006</v>
       </c>
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>89</v>
+        <v>200</v>
       </c>
       <c r="B63" t="s">
-        <v>25</v>
+        <v>99</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="E63" t="s">
-        <v>34</v>
+        <v>201</v>
       </c>
       <c r="F63">
-        <v>1972</v>
-      </c>
-      <c r="H63" t="s">
-        <v>16</v>
-      </c>
-      <c r="I63" t="s">
-        <v>20</v>
+        <v>1980</v>
+      </c>
+      <c r="G63">
+        <v>2007</v>
+      </c>
+      <c r="J63" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>104</v>
+        <v>89</v>
       </c>
       <c r="B64" t="s">
         <v>25</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>106</v>
+        <v>88</v>
       </c>
       <c r="E64" t="s">
-        <v>105</v>
+        <v>34</v>
       </c>
       <c r="F64">
-        <v>1980</v>
+        <v>1972</v>
+      </c>
+      <c r="H64" t="s">
+        <v>16</v>
+      </c>
+      <c r="I64" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>62</v>
+        <v>104</v>
       </c>
       <c r="B65" t="s">
         <v>25</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>63</v>
+        <v>106</v>
+      </c>
+      <c r="E65" t="s">
+        <v>105</v>
+      </c>
+      <c r="F65">
+        <v>1980</v>
       </c>
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>311</v>
+        <v>62</v>
       </c>
       <c r="B66" t="s">
-        <v>165</v>
+        <v>25</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>312</v>
-      </c>
-      <c r="E66" t="s">
-        <v>14</v>
-      </c>
-      <c r="H66" t="s">
-        <v>16</v>
-      </c>
-      <c r="I66" t="s">
-        <v>301</v>
+        <v>63</v>
       </c>
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>281</v>
+        <v>311</v>
       </c>
       <c r="B67" t="s">
-        <v>237</v>
+        <v>165</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>282</v>
+        <v>312</v>
+      </c>
+      <c r="E67" t="s">
+        <v>14</v>
       </c>
       <c r="H67" t="s">
         <v>16</v>
       </c>
       <c r="I67" t="s">
-        <v>20</v>
+        <v>301</v>
       </c>
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>151</v>
+        <v>281</v>
       </c>
       <c r="B68" t="s">
-        <v>40</v>
+        <v>237</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="E68" t="s">
-        <v>14</v>
+        <v>282</v>
+      </c>
+      <c r="H68" t="s">
+        <v>16</v>
+      </c>
+      <c r="I68" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>242</v>
+        <v>151</v>
       </c>
       <c r="B69" t="s">
-        <v>237</v>
+        <v>40</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>243</v>
-      </c>
-      <c r="H69" t="s">
-        <v>16</v>
-      </c>
-      <c r="I69" t="s">
-        <v>20</v>
+        <v>152</v>
+      </c>
+      <c r="E69" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="70" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>292</v>
+        <v>242</v>
       </c>
       <c r="B70" t="s">
-        <v>99</v>
+        <v>237</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>291</v>
+        <v>243</v>
       </c>
       <c r="H70" t="s">
         <v>16</v>
@@ -2517,47 +2565,47 @@
     </row>
     <row r="71" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>153</v>
+        <v>292</v>
       </c>
       <c r="B71" t="s">
-        <v>259</v>
+        <v>99</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>154</v>
+        <v>291</v>
+      </c>
+      <c r="H71" t="s">
+        <v>16</v>
+      </c>
+      <c r="I71" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="72" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>228</v>
+        <v>153</v>
       </c>
       <c r="B72" t="s">
-        <v>40</v>
+        <v>259</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>225</v>
-      </c>
-      <c r="F72">
-        <v>1989</v>
-      </c>
-      <c r="G72">
-        <v>2017</v>
-      </c>
-      <c r="H72" t="s">
-        <v>16</v>
-      </c>
-      <c r="I72" t="s">
-        <v>20</v>
+        <v>154</v>
       </c>
     </row>
     <row r="73" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>245</v>
+        <v>228</v>
       </c>
       <c r="B73" t="s">
-        <v>237</v>
+        <v>40</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>244</v>
+        <v>225</v>
+      </c>
+      <c r="F73">
+        <v>1989</v>
+      </c>
+      <c r="G73">
+        <v>2017</v>
       </c>
       <c r="H73" t="s">
         <v>16</v>
@@ -2568,50 +2616,41 @@
     </row>
     <row r="74" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>100</v>
+        <v>245</v>
       </c>
       <c r="B74" t="s">
-        <v>99</v>
+        <v>237</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>101</v>
+        <v>244</v>
+      </c>
+      <c r="H74" t="s">
+        <v>16</v>
+      </c>
+      <c r="I74" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="75" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>239</v>
+        <v>100</v>
       </c>
       <c r="B75" t="s">
-        <v>237</v>
+        <v>99</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>243</v>
-      </c>
-      <c r="H75" t="s">
-        <v>16</v>
-      </c>
-      <c r="I75" t="s">
-        <v>20</v>
+        <v>101</v>
       </c>
     </row>
     <row r="76" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>254</v>
+        <v>239</v>
       </c>
       <c r="B76" t="s">
-        <v>55</v>
+        <v>237</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>253</v>
-      </c>
-      <c r="E76" t="s">
-        <v>255</v>
-      </c>
-      <c r="F76">
-        <v>1960</v>
-      </c>
-      <c r="G76">
-        <v>2014</v>
+        <v>243</v>
       </c>
       <c r="H76" t="s">
         <v>16</v>
@@ -2622,19 +2661,22 @@
     </row>
     <row r="77" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>270</v>
+        <v>254</v>
       </c>
       <c r="B77" t="s">
         <v>55</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>271</v>
+        <v>253</v>
+      </c>
+      <c r="E77" t="s">
+        <v>255</v>
       </c>
       <c r="F77">
-        <v>1990</v>
+        <v>1960</v>
       </c>
       <c r="G77">
-        <v>2010</v>
+        <v>2014</v>
       </c>
       <c r="H77" t="s">
         <v>16</v>
@@ -2645,202 +2687,208 @@
     </row>
     <row r="78" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>117</v>
+        <v>270</v>
       </c>
       <c r="B78" t="s">
         <v>55</v>
       </c>
       <c r="C78" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="F78">
+        <v>1990</v>
+      </c>
+      <c r="G78">
+        <v>2010</v>
+      </c>
+      <c r="H78" t="s">
+        <v>16</v>
+      </c>
+      <c r="I78" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A79" t="s">
+        <v>117</v>
+      </c>
+      <c r="B79" t="s">
+        <v>55</v>
+      </c>
+      <c r="C79" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="I78" t="s">
-        <v>20</v>
-      </c>
-      <c r="J78" t="s">
+      <c r="I79" t="s">
+        <v>20</v>
+      </c>
+      <c r="J79" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A79" s="1" t="s">
+    <row r="80" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A80" s="1" t="s">
         <v>23</v>
-      </c>
-      <c r="B79" t="s">
-        <v>25</v>
-      </c>
-      <c r="C79" s="2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A80" t="s">
-        <v>300</v>
       </c>
       <c r="B80" t="s">
         <v>25</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>298</v>
-      </c>
-      <c r="E80" t="s">
-        <v>299</v>
-      </c>
-      <c r="F80">
-        <v>1969</v>
-      </c>
-      <c r="H80" t="s">
-        <v>16</v>
-      </c>
-      <c r="I80" t="s">
-        <v>249</v>
+        <v>53</v>
       </c>
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>267</v>
+        <v>300</v>
       </c>
       <c r="B81" t="s">
-        <v>250</v>
+        <v>25</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>266</v>
-      </c>
-      <c r="D81" t="s">
-        <v>269</v>
+        <v>298</v>
       </c>
       <c r="E81" t="s">
-        <v>268</v>
+        <v>299</v>
       </c>
       <c r="F81">
-        <v>1970</v>
-      </c>
-      <c r="G81">
-        <v>2014</v>
+        <v>1969</v>
       </c>
       <c r="H81" t="s">
         <v>16</v>
       </c>
       <c r="I81" t="s">
-        <v>20</v>
+        <v>249</v>
       </c>
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>96</v>
+        <v>332</v>
       </c>
       <c r="B82" t="s">
-        <v>25</v>
+        <v>134</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>90</v>
+        <v>333</v>
       </c>
       <c r="E82" t="s">
-        <v>69</v>
-      </c>
-      <c r="F82">
-        <v>1995</v>
+        <v>334</v>
+      </c>
+      <c r="H82" t="s">
+        <v>16</v>
+      </c>
+      <c r="I82" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>11</v>
+        <v>267</v>
       </c>
       <c r="B83" t="s">
-        <v>25</v>
+        <v>250</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>12</v>
+        <v>266</v>
       </c>
       <c r="D83" t="s">
-        <v>95</v>
+        <v>269</v>
       </c>
       <c r="E83" t="s">
-        <v>10</v>
+        <v>268</v>
       </c>
       <c r="F83">
-        <v>2007</v>
+        <v>1970</v>
+      </c>
+      <c r="G83">
+        <v>2014</v>
       </c>
       <c r="H83" t="s">
         <v>16</v>
       </c>
       <c r="I83" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>223</v>
+        <v>96</v>
       </c>
       <c r="B84" t="s">
-        <v>124</v>
+        <v>25</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>222</v>
+        <v>90</v>
+      </c>
+      <c r="E84" t="s">
+        <v>69</v>
       </c>
       <c r="F84">
-        <v>1</v>
-      </c>
-      <c r="G84">
-        <v>2010</v>
-      </c>
-      <c r="H84" t="s">
-        <v>16</v>
-      </c>
-      <c r="I84" t="s">
-        <v>20</v>
+        <v>1995</v>
       </c>
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>226</v>
+        <v>11</v>
       </c>
       <c r="B85" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>225</v>
+        <v>12</v>
+      </c>
+      <c r="D85" t="s">
+        <v>95</v>
+      </c>
+      <c r="E85" t="s">
+        <v>10</v>
       </c>
       <c r="F85">
-        <v>1946</v>
-      </c>
-      <c r="G85">
-        <v>2016</v>
+        <v>2007</v>
       </c>
       <c r="H85" t="s">
         <v>16</v>
       </c>
       <c r="I85" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>97</v>
+        <v>223</v>
       </c>
       <c r="B86" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>98</v>
+        <v>222</v>
+      </c>
+      <c r="F86">
+        <v>1</v>
+      </c>
+      <c r="G86">
+        <v>2010</v>
+      </c>
+      <c r="H86" t="s">
+        <v>16</v>
+      </c>
+      <c r="I86" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>278</v>
+        <v>226</v>
       </c>
       <c r="B87" t="s">
-        <v>124</v>
+        <v>40</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>279</v>
-      </c>
-      <c r="E87" t="s">
-        <v>280</v>
+        <v>225</v>
       </c>
       <c r="F87">
-        <v>1890</v>
+        <v>1946</v>
       </c>
       <c r="G87">
-        <v>1996</v>
+        <v>2016</v>
       </c>
       <c r="H87" t="s">
         <v>16</v>
@@ -2851,30 +2899,33 @@
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>156</v>
+        <v>97</v>
       </c>
       <c r="B88" t="s">
-        <v>25</v>
+        <v>128</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>154</v>
+        <v>98</v>
       </c>
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>229</v>
+        <v>278</v>
       </c>
       <c r="B89" t="s">
-        <v>40</v>
+        <v>124</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>225</v>
+        <v>279</v>
+      </c>
+      <c r="E89" t="s">
+        <v>280</v>
       </c>
       <c r="F89">
-        <v>1952</v>
+        <v>1890</v>
       </c>
       <c r="G89">
-        <v>1997</v>
+        <v>1996</v>
       </c>
       <c r="H89" t="s">
         <v>16</v>
@@ -2885,189 +2936,186 @@
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>293</v>
+        <v>156</v>
       </c>
       <c r="B90" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>294</v>
-      </c>
-      <c r="F90">
-        <v>2004</v>
-      </c>
-      <c r="G90">
-        <v>2006</v>
-      </c>
-      <c r="H90" t="s">
-        <v>16</v>
-      </c>
-      <c r="I90" t="s">
-        <v>20</v>
+        <v>154</v>
       </c>
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>102</v>
+        <v>229</v>
       </c>
       <c r="B91" t="s">
-        <v>99</v>
+        <v>40</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>103</v>
+        <v>225</v>
+      </c>
+      <c r="F91">
+        <v>1952</v>
+      </c>
+      <c r="G91">
+        <v>1997</v>
+      </c>
+      <c r="H91" t="s">
+        <v>16</v>
+      </c>
+      <c r="I91" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>289</v>
+        <v>293</v>
       </c>
       <c r="B92" t="s">
-        <v>124</v>
+        <v>40</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>290</v>
+        <v>294</v>
+      </c>
+      <c r="F92">
+        <v>2004</v>
+      </c>
+      <c r="G92">
+        <v>2006</v>
+      </c>
+      <c r="H92" t="s">
+        <v>16</v>
+      </c>
+      <c r="I92" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>246</v>
+        <v>102</v>
       </c>
       <c r="B93" t="s">
-        <v>165</v>
+        <v>99</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>247</v>
-      </c>
-      <c r="E93" t="s">
-        <v>14</v>
-      </c>
-      <c r="F93">
-        <v>1960</v>
-      </c>
-      <c r="G93">
-        <v>2006</v>
-      </c>
-      <c r="H93" t="s">
-        <v>16</v>
-      </c>
-      <c r="I93" t="s">
-        <v>249</v>
+        <v>103</v>
       </c>
     </row>
     <row r="94" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>208</v>
+        <v>289</v>
       </c>
       <c r="B94" t="s">
         <v>124</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>209</v>
-      </c>
-      <c r="F94">
-        <v>1932</v>
-      </c>
-      <c r="G94">
-        <v>2014</v>
-      </c>
-      <c r="H94" t="s">
-        <v>16</v>
-      </c>
-      <c r="I94" t="s">
-        <v>20</v>
+        <v>290</v>
       </c>
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>137</v>
+        <v>246</v>
       </c>
       <c r="B95" t="s">
-        <v>259</v>
+        <v>165</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>138</v>
+        <v>247</v>
+      </c>
+      <c r="E95" t="s">
+        <v>14</v>
+      </c>
+      <c r="F95">
+        <v>1960</v>
+      </c>
+      <c r="G95">
+        <v>2006</v>
+      </c>
+      <c r="H95" t="s">
+        <v>16</v>
+      </c>
+      <c r="I95" t="s">
+        <v>249</v>
       </c>
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>155</v>
+        <v>208</v>
       </c>
       <c r="B96" t="s">
-        <v>259</v>
+        <v>124</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>154</v>
+        <v>209</v>
+      </c>
+      <c r="F96">
+        <v>1932</v>
+      </c>
+      <c r="G96">
+        <v>2014</v>
+      </c>
+      <c r="H96" t="s">
+        <v>16</v>
+      </c>
+      <c r="I96" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="97" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>57</v>
+        <v>137</v>
       </c>
       <c r="B97" t="s">
-        <v>128</v>
+        <v>259</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="J97" t="s">
-        <v>17</v>
+        <v>138</v>
       </c>
     </row>
     <row r="98" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>129</v>
+        <v>155</v>
       </c>
       <c r="B98" t="s">
         <v>259</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="E98" t="s">
-        <v>131</v>
-      </c>
-      <c r="F98">
-        <v>1945</v>
-      </c>
-      <c r="G98">
-        <v>2008</v>
-      </c>
-      <c r="I98" t="s">
-        <v>20</v>
+        <v>154</v>
       </c>
     </row>
     <row r="99" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>148</v>
+        <v>57</v>
       </c>
       <c r="B99" t="s">
         <v>128</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>147</v>
+        <v>58</v>
+      </c>
+      <c r="J99" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="100" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>233</v>
+        <v>129</v>
       </c>
       <c r="B100" t="s">
-        <v>165</v>
+        <v>259</v>
       </c>
       <c r="C100" s="2" t="s">
-        <v>234</v>
+        <v>130</v>
       </c>
       <c r="E100" t="s">
-        <v>14</v>
+        <v>131</v>
       </c>
       <c r="F100">
-        <v>2012</v>
+        <v>1945</v>
       </c>
       <c r="G100">
-        <v>2016</v>
-      </c>
-      <c r="H100" t="s">
-        <v>16</v>
+        <v>2008</v>
       </c>
       <c r="I100" t="s">
         <v>20</v>
@@ -3075,56 +3123,59 @@
     </row>
     <row r="101" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>35</v>
+        <v>148</v>
       </c>
       <c r="B101" t="s">
-        <v>25</v>
+        <v>128</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="D101" t="s">
-        <v>37</v>
-      </c>
-      <c r="E101" t="s">
-        <v>14</v>
-      </c>
-      <c r="F101">
-        <v>2001</v>
-      </c>
-      <c r="H101" t="s">
-        <v>16</v>
-      </c>
-      <c r="I101" t="s">
-        <v>20</v>
+        <v>147</v>
       </c>
     </row>
     <row r="102" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>185</v>
+        <v>233</v>
       </c>
       <c r="B102" t="s">
-        <v>128</v>
+        <v>165</v>
       </c>
       <c r="C102" s="2" t="s">
-        <v>186</v>
+        <v>234</v>
+      </c>
+      <c r="E102" t="s">
+        <v>14</v>
+      </c>
+      <c r="F102">
+        <v>2012</v>
+      </c>
+      <c r="G102">
+        <v>2016</v>
+      </c>
+      <c r="H102" t="s">
+        <v>16</v>
+      </c>
+      <c r="I102" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="103" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>210</v>
+        <v>35</v>
       </c>
       <c r="B103" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="C103" s="2" t="s">
-        <v>211</v>
+        <v>36</v>
+      </c>
+      <c r="D103" t="s">
+        <v>37</v>
+      </c>
+      <c r="E103" t="s">
+        <v>14</v>
       </c>
       <c r="F103">
-        <v>1976</v>
-      </c>
-      <c r="G103">
-        <v>2016</v>
+        <v>2001</v>
       </c>
       <c r="H103" t="s">
         <v>16</v>
@@ -3135,30 +3186,33 @@
     </row>
     <row r="104" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>144</v>
+        <v>185</v>
       </c>
       <c r="B104" t="s">
-        <v>60</v>
+        <v>128</v>
       </c>
       <c r="C104" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="F104">
-        <v>1800</v>
-      </c>
-      <c r="G104">
-        <v>2013</v>
+        <v>186</v>
       </c>
     </row>
     <row r="105" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>122</v>
+        <v>210</v>
       </c>
       <c r="B105" t="s">
-        <v>259</v>
+        <v>40</v>
       </c>
       <c r="C105" s="2" t="s">
-        <v>121</v>
+        <v>211</v>
+      </c>
+      <c r="F105">
+        <v>1976</v>
+      </c>
+      <c r="G105">
+        <v>2016</v>
+      </c>
+      <c r="H105" t="s">
+        <v>16</v>
       </c>
       <c r="I105" t="s">
         <v>20</v>
@@ -3166,51 +3220,30 @@
     </row>
     <row r="106" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>318</v>
+        <v>144</v>
       </c>
       <c r="B106" t="s">
-        <v>250</v>
+        <v>60</v>
       </c>
       <c r="C106" s="2" t="s">
-        <v>319</v>
-      </c>
-      <c r="E106" t="s">
-        <v>320</v>
+        <v>143</v>
       </c>
       <c r="F106">
-        <v>1975</v>
+        <v>1800</v>
       </c>
       <c r="G106">
-        <v>1989</v>
-      </c>
-      <c r="H106" t="s">
-        <v>16</v>
-      </c>
-      <c r="I106" t="s">
-        <v>20</v>
+        <v>2013</v>
       </c>
     </row>
     <row r="107" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>316</v>
+        <v>122</v>
       </c>
       <c r="B107" t="s">
-        <v>250</v>
+        <v>259</v>
       </c>
       <c r="C107" s="2" t="s">
-        <v>317</v>
-      </c>
-      <c r="E107" t="s">
-        <v>105</v>
-      </c>
-      <c r="F107">
-        <v>1950</v>
-      </c>
-      <c r="G107">
-        <v>1996</v>
-      </c>
-      <c r="H107" t="s">
-        <v>16</v>
+        <v>121</v>
       </c>
       <c r="I107" t="s">
         <v>20</v>
@@ -3218,36 +3251,48 @@
     </row>
     <row r="108" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>141</v>
+        <v>318</v>
       </c>
       <c r="B108" t="s">
-        <v>237</v>
+        <v>250</v>
       </c>
       <c r="C108" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="J108" t="s">
-        <v>17</v>
+        <v>319</v>
+      </c>
+      <c r="E108" t="s">
+        <v>320</v>
+      </c>
+      <c r="F108">
+        <v>1975</v>
+      </c>
+      <c r="G108">
+        <v>1989</v>
+      </c>
+      <c r="H108" t="s">
+        <v>16</v>
+      </c>
+      <c r="I108" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="109" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>308</v>
+        <v>316</v>
       </c>
       <c r="B109" t="s">
         <v>250</v>
       </c>
       <c r="C109" s="2" t="s">
-        <v>309</v>
+        <v>317</v>
       </c>
       <c r="E109" t="s">
-        <v>310</v>
+        <v>105</v>
       </c>
       <c r="F109">
         <v>1950</v>
       </c>
       <c r="G109">
-        <v>2010</v>
+        <v>1996</v>
       </c>
       <c r="H109" t="s">
         <v>16</v>
@@ -3258,207 +3303,210 @@
     </row>
     <row r="110" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>287</v>
+        <v>322</v>
       </c>
       <c r="B110" t="s">
-        <v>134</v>
+        <v>25</v>
       </c>
       <c r="C110" s="2" t="s">
-        <v>288</v>
+        <v>321</v>
+      </c>
+      <c r="E110" t="s">
+        <v>77</v>
       </c>
       <c r="F110">
-        <v>1990</v>
-      </c>
-      <c r="G110">
-        <v>2008</v>
+        <v>2010</v>
+      </c>
+      <c r="H110" t="s">
+        <v>16</v>
+      </c>
+      <c r="I110" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="111" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>274</v>
+        <v>141</v>
       </c>
       <c r="B111" t="s">
-        <v>55</v>
+        <v>237</v>
       </c>
       <c r="C111" s="2" t="s">
-        <v>275</v>
-      </c>
-      <c r="H111" t="s">
-        <v>16</v>
-      </c>
-      <c r="I111" t="s">
-        <v>20</v>
+        <v>142</v>
+      </c>
+      <c r="J111" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="112" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
+        <v>308</v>
+      </c>
+      <c r="B112" t="s">
+        <v>250</v>
+      </c>
+      <c r="C112" s="2" t="s">
+        <v>309</v>
+      </c>
+      <c r="E112" t="s">
+        <v>310</v>
+      </c>
+      <c r="F112">
+        <v>1950</v>
+      </c>
+      <c r="G112">
+        <v>2010</v>
+      </c>
+      <c r="H112" t="s">
+        <v>16</v>
+      </c>
+      <c r="I112" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="113" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A113" t="s">
+        <v>287</v>
+      </c>
+      <c r="B113" t="s">
+        <v>134</v>
+      </c>
+      <c r="C113" s="2" t="s">
+        <v>288</v>
+      </c>
+      <c r="F113">
+        <v>1990</v>
+      </c>
+      <c r="G113">
+        <v>2008</v>
+      </c>
+    </row>
+    <row r="114" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A114" t="s">
+        <v>274</v>
+      </c>
+      <c r="B114" t="s">
+        <v>55</v>
+      </c>
+      <c r="C114" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="H114" t="s">
+        <v>16</v>
+      </c>
+      <c r="I114" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="115" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A115" t="s">
         <v>157</v>
       </c>
-      <c r="B112" t="s">
+      <c r="B115" t="s">
         <v>128</v>
       </c>
-      <c r="C112" s="2" t="s">
+      <c r="C115" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="J112" t="s">
+      <c r="J115" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="113" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A113" t="s">
+    <row r="116" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A116" t="s">
         <v>194</v>
       </c>
-      <c r="B113" t="s">
+      <c r="B116" t="s">
         <v>99</v>
       </c>
-      <c r="C113" s="2" t="s">
+      <c r="C116" s="2" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="114" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A114" t="s">
+    <row r="117" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A117" t="s">
         <v>295</v>
-      </c>
-      <c r="B114" t="s">
-        <v>40</v>
-      </c>
-      <c r="C114" s="2" t="s">
-        <v>296</v>
-      </c>
-      <c r="E114" t="s">
-        <v>297</v>
-      </c>
-      <c r="F114">
-        <v>1990</v>
-      </c>
-      <c r="G114">
-        <v>2015</v>
-      </c>
-      <c r="H114" t="s">
-        <v>16</v>
-      </c>
-      <c r="I114" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="115" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A115" t="s">
-        <v>256</v>
-      </c>
-      <c r="B115" t="s">
-        <v>250</v>
-      </c>
-      <c r="C115" s="2" t="s">
-        <v>257</v>
-      </c>
-      <c r="E115" t="s">
-        <v>258</v>
-      </c>
-      <c r="H115" t="s">
-        <v>16</v>
-      </c>
-      <c r="I115" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="116" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A116" t="s">
-        <v>227</v>
-      </c>
-      <c r="B116" t="s">
-        <v>40</v>
-      </c>
-      <c r="C116" s="2" t="s">
-        <v>225</v>
-      </c>
-      <c r="F116">
-        <v>1955</v>
-      </c>
-      <c r="G116">
-        <v>2016</v>
-      </c>
-      <c r="H116" t="s">
-        <v>16</v>
-      </c>
-      <c r="I116" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="117" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A117" t="s">
-        <v>230</v>
       </c>
       <c r="B117" t="s">
         <v>40</v>
       </c>
       <c r="C117" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="E117" t="s">
+        <v>297</v>
+      </c>
+      <c r="F117">
+        <v>1990</v>
+      </c>
+      <c r="G117">
+        <v>2015</v>
+      </c>
+      <c r="H117" t="s">
+        <v>16</v>
+      </c>
+      <c r="I117" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="118" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A118" t="s">
+        <v>256</v>
+      </c>
+      <c r="B118" t="s">
+        <v>250</v>
+      </c>
+      <c r="C118" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="E118" t="s">
+        <v>258</v>
+      </c>
+      <c r="H118" t="s">
+        <v>16</v>
+      </c>
+      <c r="I118" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="119" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A119" t="s">
+        <v>227</v>
+      </c>
+      <c r="B119" t="s">
+        <v>40</v>
+      </c>
+      <c r="C119" s="2" t="s">
         <v>225</v>
       </c>
-      <c r="F117">
-        <v>1995</v>
-      </c>
-      <c r="G117">
+      <c r="F119">
+        <v>1955</v>
+      </c>
+      <c r="G119">
         <v>2016</v>
       </c>
-      <c r="H117" t="s">
-        <v>16</v>
-      </c>
-      <c r="I117" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="118" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A118" t="s">
-        <v>109</v>
-      </c>
-      <c r="B118" t="s">
-        <v>25</v>
-      </c>
-      <c r="C118" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="E118" t="s">
-        <v>111</v>
-      </c>
-      <c r="F118">
-        <v>1956</v>
-      </c>
-    </row>
-    <row r="119" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A119" t="s">
-        <v>91</v>
-      </c>
-      <c r="B119" t="s">
-        <v>25</v>
-      </c>
-      <c r="C119" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="E119" t="s">
-        <v>92</v>
-      </c>
-      <c r="F119">
-        <v>1999</v>
-      </c>
-    </row>
-    <row r="120" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H119" t="s">
+        <v>16</v>
+      </c>
+      <c r="I119" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="120" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>314</v>
+        <v>230</v>
       </c>
       <c r="B120" t="s">
         <v>40</v>
       </c>
       <c r="C120" s="2" t="s">
-        <v>313</v>
-      </c>
-      <c r="E120" t="s">
-        <v>315</v>
+        <v>225</v>
       </c>
       <c r="F120">
-        <v>1950</v>
+        <v>1995</v>
       </c>
       <c r="G120">
-        <v>2004</v>
+        <v>2016</v>
       </c>
       <c r="H120" t="s">
         <v>16</v>
@@ -3467,60 +3515,81 @@
         <v>20</v>
       </c>
     </row>
-    <row r="121" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>161</v>
+        <v>109</v>
       </c>
       <c r="B121" t="s">
         <v>25</v>
       </c>
       <c r="C121" s="2" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="122" spans="1:9" x14ac:dyDescent="0.2">
+        <v>110</v>
+      </c>
+      <c r="E121" t="s">
+        <v>111</v>
+      </c>
+      <c r="F121">
+        <v>1956</v>
+      </c>
+    </row>
+    <row r="122" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>168</v>
+        <v>326</v>
       </c>
       <c r="B122" t="s">
+        <v>25</v>
+      </c>
+      <c r="C122" s="2" t="s">
+        <v>327</v>
+      </c>
+      <c r="E122" t="s">
+        <v>111</v>
+      </c>
+      <c r="F122">
+        <v>1998</v>
+      </c>
+      <c r="H122" t="s">
+        <v>16</v>
+      </c>
+      <c r="I122" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="123" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A123" t="s">
+        <v>91</v>
+      </c>
+      <c r="B123" t="s">
+        <v>25</v>
+      </c>
+      <c r="C123" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="E123" t="s">
+        <v>92</v>
+      </c>
+      <c r="F123">
+        <v>1999</v>
+      </c>
+    </row>
+    <row r="124" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A124" t="s">
+        <v>314</v>
+      </c>
+      <c r="B124" t="s">
         <v>40</v>
       </c>
-      <c r="C122" s="2" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="123" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A123" t="s">
-        <v>213</v>
-      </c>
-      <c r="B123" t="s">
-        <v>55</v>
-      </c>
-      <c r="C123" s="2" t="s">
-        <v>212</v>
-      </c>
-      <c r="H123" t="s">
-        <v>16</v>
-      </c>
-      <c r="I123" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="124" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A124" t="s">
-        <v>273</v>
-      </c>
-      <c r="B124" t="s">
-        <v>237</v>
-      </c>
       <c r="C124" s="2" t="s">
-        <v>272</v>
+        <v>313</v>
+      </c>
+      <c r="E124" t="s">
+        <v>315</v>
       </c>
       <c r="F124">
-        <v>1996</v>
+        <v>1950</v>
       </c>
       <c r="G124">
-        <v>2016</v>
+        <v>2004</v>
       </c>
       <c r="H124" t="s">
         <v>16</v>
@@ -3529,54 +3598,60 @@
         <v>20</v>
       </c>
     </row>
-    <row r="125" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>66</v>
+        <v>161</v>
       </c>
       <c r="B125" t="s">
         <v>25</v>
       </c>
       <c r="C125" s="2" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="126" spans="1:9" x14ac:dyDescent="0.2">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="126" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>139</v>
+        <v>168</v>
       </c>
       <c r="B126" t="s">
         <v>40</v>
       </c>
       <c r="C126" s="2" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="127" spans="1:9" x14ac:dyDescent="0.2">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="127" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>172</v>
+        <v>213</v>
       </c>
       <c r="B127" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="C127" s="2" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="128" spans="1:9" x14ac:dyDescent="0.2">
+        <v>212</v>
+      </c>
+      <c r="H127" t="s">
+        <v>16</v>
+      </c>
+      <c r="I127" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="128" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>217</v>
+        <v>323</v>
       </c>
       <c r="B128" t="s">
-        <v>60</v>
+        <v>25</v>
       </c>
       <c r="C128" s="2" t="s">
-        <v>216</v>
+        <v>324</v>
       </c>
       <c r="E128" t="s">
-        <v>14</v>
+        <v>325</v>
       </c>
       <c r="F128">
-        <v>1900</v>
+        <v>1942</v>
       </c>
       <c r="H128" t="s">
         <v>16</v>
@@ -3587,58 +3662,64 @@
     </row>
     <row r="129" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>132</v>
+        <v>273</v>
       </c>
       <c r="B129" t="s">
-        <v>259</v>
+        <v>237</v>
       </c>
       <c r="C129" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="J129" t="s">
-        <v>17</v>
+        <v>272</v>
+      </c>
+      <c r="F129">
+        <v>1996</v>
+      </c>
+      <c r="G129">
+        <v>2016</v>
+      </c>
+      <c r="H129" t="s">
+        <v>16</v>
+      </c>
+      <c r="I129" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="130" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
-        <v>182</v>
+        <v>66</v>
       </c>
       <c r="B130" t="s">
-        <v>165</v>
+        <v>25</v>
       </c>
       <c r="C130" s="2" t="s">
-        <v>181</v>
+        <v>67</v>
       </c>
     </row>
     <row r="131" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>115</v>
+        <v>139</v>
       </c>
       <c r="B131" t="s">
-        <v>128</v>
+        <v>40</v>
       </c>
       <c r="C131" s="2" t="s">
-        <v>116</v>
+        <v>140</v>
       </c>
     </row>
     <row r="132" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>263</v>
+        <v>329</v>
       </c>
       <c r="B132" t="s">
-        <v>250</v>
+        <v>165</v>
       </c>
       <c r="C132" s="2" t="s">
-        <v>264</v>
+        <v>328</v>
       </c>
       <c r="E132" t="s">
-        <v>265</v>
+        <v>34</v>
       </c>
       <c r="F132">
-        <v>1500</v>
-      </c>
-      <c r="G132">
-        <v>2000</v>
+        <v>1789</v>
       </c>
       <c r="H132" t="s">
         <v>16</v>
@@ -3649,42 +3730,30 @@
     </row>
     <row r="133" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
-        <v>221</v>
+        <v>172</v>
       </c>
       <c r="B133" t="s">
-        <v>86</v>
+        <v>60</v>
       </c>
       <c r="C133" s="2" t="s">
-        <v>220</v>
-      </c>
-      <c r="F133">
-        <v>2013</v>
-      </c>
-      <c r="H133" t="s">
-        <v>16</v>
-      </c>
-      <c r="I133" t="s">
-        <v>20</v>
+        <v>171</v>
       </c>
     </row>
     <row r="134" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
-        <v>13</v>
+        <v>217</v>
       </c>
       <c r="B134" t="s">
-        <v>25</v>
+        <v>60</v>
       </c>
       <c r="C134" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="D134" s="1" t="s">
-        <v>42</v>
+        <v>216</v>
       </c>
       <c r="E134" t="s">
         <v>14</v>
       </c>
       <c r="F134">
-        <v>1981</v>
+        <v>1900</v>
       </c>
       <c r="H134" t="s">
         <v>16</v>
@@ -3695,160 +3764,274 @@
     </row>
     <row r="135" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
+        <v>132</v>
+      </c>
+      <c r="B135" t="s">
+        <v>259</v>
+      </c>
+      <c r="C135" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="J135" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="136" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A136" t="s">
+        <v>182</v>
+      </c>
+      <c r="B136" t="s">
+        <v>165</v>
+      </c>
+      <c r="C136" s="2" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="137" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A137" t="s">
+        <v>115</v>
+      </c>
+      <c r="B137" t="s">
+        <v>128</v>
+      </c>
+      <c r="C137" s="2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="138" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A138" t="s">
+        <v>263</v>
+      </c>
+      <c r="B138" t="s">
+        <v>250</v>
+      </c>
+      <c r="C138" s="2" t="s">
+        <v>264</v>
+      </c>
+      <c r="E138" t="s">
+        <v>265</v>
+      </c>
+      <c r="F138">
+        <v>1500</v>
+      </c>
+      <c r="G138">
+        <v>2000</v>
+      </c>
+      <c r="H138" t="s">
+        <v>16</v>
+      </c>
+      <c r="I138" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="139" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A139" t="s">
+        <v>221</v>
+      </c>
+      <c r="B139" t="s">
+        <v>86</v>
+      </c>
+      <c r="C139" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="F139">
+        <v>2013</v>
+      </c>
+      <c r="H139" t="s">
+        <v>16</v>
+      </c>
+      <c r="I139" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="140" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A140" t="s">
+        <v>13</v>
+      </c>
+      <c r="B140" t="s">
+        <v>25</v>
+      </c>
+      <c r="C140" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D140" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E140" t="s">
+        <v>14</v>
+      </c>
+      <c r="F140">
+        <v>1981</v>
+      </c>
+      <c r="H140" t="s">
+        <v>16</v>
+      </c>
+      <c r="I140" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="141" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A141" t="s">
         <v>283</v>
       </c>
-      <c r="B135" t="s">
+      <c r="B141" t="s">
         <v>124</v>
       </c>
-      <c r="C135" s="2" t="s">
+      <c r="C141" s="2" t="s">
         <v>284</v>
       </c>
-      <c r="H135" t="s">
-        <v>16</v>
-      </c>
-      <c r="I135" t="s">
+      <c r="H141" t="s">
+        <v>16</v>
+      </c>
+      <c r="I141" t="s">
         <v>20</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:J135">
+  <sortState ref="A2:J141">
     <sortCondition ref="A2"/>
   </sortState>
   <hyperlinks>
     <hyperlink ref="C6" r:id="rId1"/>
-    <hyperlink ref="C54" r:id="rId2"/>
+    <hyperlink ref="C55" r:id="rId2"/>
     <hyperlink ref="C7" r:id="rId3"/>
     <hyperlink ref="C10" r:id="rId4"/>
-    <hyperlink ref="C83" r:id="rId5"/>
-    <hyperlink ref="C101" r:id="rId6"/>
-    <hyperlink ref="C134" r:id="rId7"/>
+    <hyperlink ref="C85" r:id="rId5"/>
+    <hyperlink ref="C103" r:id="rId6"/>
+    <hyperlink ref="C140" r:id="rId7"/>
     <hyperlink ref="C33" r:id="rId8"/>
     <hyperlink ref="C29" r:id="rId9"/>
-    <hyperlink ref="C45" r:id="rId10"/>
-    <hyperlink ref="C52" r:id="rId11"/>
+    <hyperlink ref="C46" r:id="rId10"/>
+    <hyperlink ref="C53" r:id="rId11"/>
     <hyperlink ref="C3" r:id="rId12"/>
     <hyperlink ref="C20" r:id="rId13"/>
-    <hyperlink ref="C56" r:id="rId14"/>
-    <hyperlink ref="C79" r:id="rId15"/>
+    <hyperlink ref="C57" r:id="rId14"/>
+    <hyperlink ref="C80" r:id="rId15"/>
     <hyperlink ref="C28" r:id="rId16"/>
-    <hyperlink ref="C97" r:id="rId17"/>
-    <hyperlink ref="C37" r:id="rId18"/>
-    <hyperlink ref="C65" r:id="rId19"/>
+    <hyperlink ref="C99" r:id="rId17"/>
+    <hyperlink ref="C38" r:id="rId18"/>
+    <hyperlink ref="C66" r:id="rId19"/>
     <hyperlink ref="C16" r:id="rId20"/>
-    <hyperlink ref="C125" r:id="rId21"/>
+    <hyperlink ref="C130" r:id="rId21"/>
     <hyperlink ref="C8" r:id="rId22"/>
-    <hyperlink ref="C35" r:id="rId23"/>
-    <hyperlink ref="C49" r:id="rId24"/>
-    <hyperlink ref="C46" r:id="rId25"/>
-    <hyperlink ref="C50" r:id="rId26"/>
-    <hyperlink ref="C51" r:id="rId27"/>
-    <hyperlink ref="C63" r:id="rId28"/>
-    <hyperlink ref="C82" r:id="rId29"/>
-    <hyperlink ref="C119" r:id="rId30"/>
-    <hyperlink ref="C86" r:id="rId31"/>
-    <hyperlink ref="C74" r:id="rId32"/>
-    <hyperlink ref="C91" r:id="rId33"/>
-    <hyperlink ref="C64" r:id="rId34"/>
+    <hyperlink ref="C36" r:id="rId23"/>
+    <hyperlink ref="C50" r:id="rId24"/>
+    <hyperlink ref="C47" r:id="rId25"/>
+    <hyperlink ref="C51" r:id="rId26"/>
+    <hyperlink ref="C52" r:id="rId27"/>
+    <hyperlink ref="C64" r:id="rId28"/>
+    <hyperlink ref="C84" r:id="rId29"/>
+    <hyperlink ref="C123" r:id="rId30"/>
+    <hyperlink ref="C88" r:id="rId31"/>
+    <hyperlink ref="C75" r:id="rId32"/>
+    <hyperlink ref="C93" r:id="rId33"/>
+    <hyperlink ref="C65" r:id="rId34"/>
     <hyperlink ref="C17" r:id="rId35"/>
-    <hyperlink ref="C118" r:id="rId36"/>
+    <hyperlink ref="C121" r:id="rId36"/>
     <hyperlink ref="C15" r:id="rId37"/>
-    <hyperlink ref="C131" r:id="rId38"/>
-    <hyperlink ref="C78" r:id="rId39"/>
-    <hyperlink ref="C53" r:id="rId40"/>
-    <hyperlink ref="C105" r:id="rId41"/>
+    <hyperlink ref="C137" r:id="rId38"/>
+    <hyperlink ref="C79" r:id="rId39"/>
+    <hyperlink ref="C54" r:id="rId40"/>
+    <hyperlink ref="C107" r:id="rId41"/>
     <hyperlink ref="C18" r:id="rId42"/>
-    <hyperlink ref="C47" r:id="rId43"/>
+    <hyperlink ref="C48" r:id="rId43"/>
     <hyperlink ref="C22" r:id="rId44"/>
-    <hyperlink ref="C98" r:id="rId45"/>
-    <hyperlink ref="C129" r:id="rId46"/>
+    <hyperlink ref="C100" r:id="rId45"/>
+    <hyperlink ref="C135" r:id="rId46"/>
     <hyperlink ref="C26" r:id="rId47" display="http://comparativeconstitutionsproject.org/"/>
-    <hyperlink ref="C95" r:id="rId48"/>
-    <hyperlink ref="C126" r:id="rId49"/>
-    <hyperlink ref="C108" r:id="rId50"/>
-    <hyperlink ref="C104" r:id="rId51"/>
+    <hyperlink ref="C97" r:id="rId48"/>
+    <hyperlink ref="C131" r:id="rId49"/>
+    <hyperlink ref="C111" r:id="rId50"/>
+    <hyperlink ref="C106" r:id="rId51"/>
     <hyperlink ref="C21" r:id="rId52"/>
-    <hyperlink ref="C99" r:id="rId53"/>
-    <hyperlink ref="C44" r:id="rId54"/>
-    <hyperlink ref="C68" r:id="rId55"/>
-    <hyperlink ref="C71" r:id="rId56"/>
-    <hyperlink ref="C96" r:id="rId57"/>
-    <hyperlink ref="C88" r:id="rId58"/>
-    <hyperlink ref="C112" r:id="rId59"/>
+    <hyperlink ref="C101" r:id="rId53"/>
+    <hyperlink ref="C45" r:id="rId54"/>
+    <hyperlink ref="C69" r:id="rId55"/>
+    <hyperlink ref="C72" r:id="rId56"/>
+    <hyperlink ref="C98" r:id="rId57"/>
+    <hyperlink ref="C90" r:id="rId58"/>
+    <hyperlink ref="C115" r:id="rId59"/>
     <hyperlink ref="C30" r:id="rId60"/>
-    <hyperlink ref="C121" r:id="rId61"/>
+    <hyperlink ref="C125" r:id="rId61"/>
     <hyperlink ref="C9" r:id="rId62"/>
     <hyperlink ref="C32" r:id="rId63"/>
-    <hyperlink ref="C122" r:id="rId64"/>
+    <hyperlink ref="C126" r:id="rId64"/>
     <hyperlink ref="C14" r:id="rId65"/>
-    <hyperlink ref="C127" r:id="rId66"/>
+    <hyperlink ref="C133" r:id="rId66"/>
     <hyperlink ref="C24" r:id="rId67"/>
     <hyperlink ref="C23" r:id="rId68"/>
     <hyperlink ref="C25" r:id="rId69"/>
-    <hyperlink ref="C48" r:id="rId70"/>
-    <hyperlink ref="C130" r:id="rId71"/>
+    <hyperlink ref="C49" r:id="rId70"/>
+    <hyperlink ref="C136" r:id="rId71"/>
     <hyperlink ref="C27" r:id="rId72"/>
-    <hyperlink ref="C102" r:id="rId73"/>
+    <hyperlink ref="C104" r:id="rId73"/>
     <hyperlink ref="C31" r:id="rId74"/>
-    <hyperlink ref="C41" r:id="rId75"/>
-    <hyperlink ref="C113" r:id="rId76"/>
-    <hyperlink ref="C38" r:id="rId77"/>
-    <hyperlink ref="C36" r:id="rId78"/>
-    <hyperlink ref="C62" r:id="rId79"/>
+    <hyperlink ref="C42" r:id="rId75"/>
+    <hyperlink ref="C116" r:id="rId76"/>
+    <hyperlink ref="C39" r:id="rId77"/>
+    <hyperlink ref="C37" r:id="rId78"/>
+    <hyperlink ref="C63" r:id="rId79"/>
     <hyperlink ref="C5" r:id="rId80"/>
-    <hyperlink ref="C61" r:id="rId81"/>
+    <hyperlink ref="C62" r:id="rId81"/>
     <hyperlink ref="C12" r:id="rId82"/>
-    <hyperlink ref="C94" r:id="rId83"/>
-    <hyperlink ref="C103" r:id="rId84"/>
-    <hyperlink ref="C123" r:id="rId85"/>
+    <hyperlink ref="C96" r:id="rId83"/>
+    <hyperlink ref="C105" r:id="rId84"/>
+    <hyperlink ref="C127" r:id="rId85"/>
     <hyperlink ref="C34" r:id="rId86"/>
-    <hyperlink ref="C128" r:id="rId87"/>
-    <hyperlink ref="C40" r:id="rId88"/>
-    <hyperlink ref="C133" r:id="rId89"/>
-    <hyperlink ref="C84" r:id="rId90"/>
-    <hyperlink ref="C59" r:id="rId91"/>
-    <hyperlink ref="C85" r:id="rId92"/>
-    <hyperlink ref="C116" r:id="rId93"/>
-    <hyperlink ref="C72" r:id="rId94"/>
-    <hyperlink ref="C89" r:id="rId95"/>
-    <hyperlink ref="C117" r:id="rId96"/>
-    <hyperlink ref="C57" r:id="rId97"/>
-    <hyperlink ref="C100" r:id="rId98"/>
-    <hyperlink ref="C42" r:id="rId99"/>
-    <hyperlink ref="C39" r:id="rId100"/>
-    <hyperlink ref="C75" r:id="rId101"/>
-    <hyperlink ref="C55" r:id="rId102"/>
+    <hyperlink ref="C134" r:id="rId87"/>
+    <hyperlink ref="C41" r:id="rId88"/>
+    <hyperlink ref="C139" r:id="rId89"/>
+    <hyperlink ref="C86" r:id="rId90"/>
+    <hyperlink ref="C60" r:id="rId91"/>
+    <hyperlink ref="C87" r:id="rId92"/>
+    <hyperlink ref="C119" r:id="rId93"/>
+    <hyperlink ref="C73" r:id="rId94"/>
+    <hyperlink ref="C91" r:id="rId95"/>
+    <hyperlink ref="C120" r:id="rId96"/>
+    <hyperlink ref="C58" r:id="rId97"/>
+    <hyperlink ref="C102" r:id="rId98"/>
+    <hyperlink ref="C43" r:id="rId99"/>
+    <hyperlink ref="C40" r:id="rId100"/>
+    <hyperlink ref="C76" r:id="rId101"/>
+    <hyperlink ref="C56" r:id="rId102"/>
     <hyperlink ref="C2" r:id="rId103"/>
-    <hyperlink ref="C69" r:id="rId104"/>
-    <hyperlink ref="C73" r:id="rId105"/>
-    <hyperlink ref="C93" r:id="rId106"/>
-    <hyperlink ref="C43" r:id="rId107"/>
-    <hyperlink ref="C76" r:id="rId108"/>
-    <hyperlink ref="C115" r:id="rId109"/>
+    <hyperlink ref="C70" r:id="rId104"/>
+    <hyperlink ref="C74" r:id="rId105"/>
+    <hyperlink ref="C95" r:id="rId106"/>
+    <hyperlink ref="C44" r:id="rId107"/>
+    <hyperlink ref="C77" r:id="rId108"/>
+    <hyperlink ref="C118" r:id="rId109"/>
     <hyperlink ref="C13" r:id="rId110"/>
     <hyperlink ref="C4" r:id="rId111"/>
-    <hyperlink ref="C132" r:id="rId112"/>
-    <hyperlink ref="C81" r:id="rId113"/>
-    <hyperlink ref="C77" r:id="rId114"/>
-    <hyperlink ref="C124" r:id="rId115"/>
-    <hyperlink ref="C111" r:id="rId116"/>
-    <hyperlink ref="C58" r:id="rId117"/>
-    <hyperlink ref="C87" r:id="rId118"/>
-    <hyperlink ref="C67" r:id="rId119"/>
-    <hyperlink ref="C135" r:id="rId120"/>
-    <hyperlink ref="C60" r:id="rId121"/>
-    <hyperlink ref="C110" r:id="rId122"/>
-    <hyperlink ref="C92" r:id="rId123"/>
-    <hyperlink ref="C70" r:id="rId124"/>
-    <hyperlink ref="C90" r:id="rId125"/>
-    <hyperlink ref="C114" r:id="rId126"/>
-    <hyperlink ref="C80" r:id="rId127"/>
+    <hyperlink ref="C138" r:id="rId112"/>
+    <hyperlink ref="C83" r:id="rId113"/>
+    <hyperlink ref="C78" r:id="rId114"/>
+    <hyperlink ref="C129" r:id="rId115"/>
+    <hyperlink ref="C114" r:id="rId116"/>
+    <hyperlink ref="C59" r:id="rId117"/>
+    <hyperlink ref="C89" r:id="rId118"/>
+    <hyperlink ref="C68" r:id="rId119"/>
+    <hyperlink ref="C141" r:id="rId120"/>
+    <hyperlink ref="C61" r:id="rId121"/>
+    <hyperlink ref="C113" r:id="rId122"/>
+    <hyperlink ref="C94" r:id="rId123"/>
+    <hyperlink ref="C71" r:id="rId124"/>
+    <hyperlink ref="C92" r:id="rId125"/>
+    <hyperlink ref="C117" r:id="rId126"/>
+    <hyperlink ref="C81" r:id="rId127"/>
     <hyperlink ref="C11" r:id="rId128"/>
     <hyperlink ref="C19" r:id="rId129"/>
-    <hyperlink ref="C109" r:id="rId130"/>
-    <hyperlink ref="C66" r:id="rId131"/>
-    <hyperlink ref="C120" r:id="rId132"/>
-    <hyperlink ref="C107" r:id="rId133"/>
-    <hyperlink ref="C106" r:id="rId134"/>
+    <hyperlink ref="C112" r:id="rId130"/>
+    <hyperlink ref="C67" r:id="rId131"/>
+    <hyperlink ref="C124" r:id="rId132"/>
+    <hyperlink ref="C109" r:id="rId133"/>
+    <hyperlink ref="C108" r:id="rId134"/>
+    <hyperlink ref="C110" r:id="rId135"/>
+    <hyperlink ref="C128" r:id="rId136"/>
+    <hyperlink ref="C122" r:id="rId137"/>
+    <hyperlink ref="C132" r:id="rId138"/>
+    <hyperlink ref="C35" r:id="rId139"/>
+    <hyperlink ref="C82" r:id="rId140"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
add 7 variables (codebook, file_csv, file_dta, file_sav, file_excel, file_r, file_zip)
</commit_message>
<xml_diff>
--- a/PolData.xlsx
+++ b/PolData.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="635" uniqueCount="335">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="665" uniqueCount="365">
   <si>
     <t>name</t>
   </si>
@@ -1032,13 +1032,110 @@
   </si>
   <si>
     <t>71 countries</t>
+  </si>
+  <si>
+    <t>https://www.hertie-school.org/fileadmin/2_Research/1_About_our_research/4_The_Governance_Report/Indicators/2014/Downloads/GovReport2014_Indicators_IndicatorsCodebook.pdf</t>
+  </si>
+  <si>
+    <t>file_csv</t>
+  </si>
+  <si>
+    <t>file_dta</t>
+  </si>
+  <si>
+    <t>file_sav</t>
+  </si>
+  <si>
+    <t>file_excel</t>
+  </si>
+  <si>
+    <t>file_r</t>
+  </si>
+  <si>
+    <t>file_zip</t>
+  </si>
+  <si>
+    <t>https://www.hertie-school.org/fileadmin/2_Research/1_About_our_research/4_The_Governance_Report/Indicators/2014/Downloads/GovReport2014_Indicators_Indicators.csv</t>
+  </si>
+  <si>
+    <t>https://www.hertie-school.org/fileadmin/2_Research/1_About_our_research/4_The_Governance_Report/Indicators/2014/Downloads/GovReport2014_Indicators_Indicators.xlsx</t>
+  </si>
+  <si>
+    <t>https://www.hertie-school.org/fileadmin/2_Research/1_About_our_research/4_The_Governance_Report/Indicators/2014/Downloads/GovReport2014_Indicators_Indicators.dta</t>
+  </si>
+  <si>
+    <t>https://www.hertie-school.org/fileadmin/2_Research/1_About_our_research/4_The_Governance_Report/Indicators/2014/Downloads/GovReport2014_Indicators_Indicators.RData</t>
+  </si>
+  <si>
+    <t>Crime control, education provision, civil justice provision, revenue collection capacity, legitimacy and effectiveness, regulatory capacity and quality, coordination capacity, self-monitoring</t>
+  </si>
+  <si>
+    <t>195 countries</t>
+  </si>
+  <si>
+    <t>online</t>
+  </si>
+  <si>
+    <t>free, no registration</t>
+  </si>
+  <si>
+    <t>Comprised of data from multiple organisations and data providers.</t>
+  </si>
+  <si>
+    <t>codebook</t>
+  </si>
+  <si>
+    <t>Conflict and crime, democracy, elections, gender equality, governance, identity, macroeconomics and markets, political participation, poverty, public services, social capital, tolerance, citizenship, energy</t>
+  </si>
+  <si>
+    <t>http://afrobarometer.org/sites/default/files/data/round-6/merged_r6_data_2016_36countries2.sav</t>
+  </si>
+  <si>
+    <t>http://afrobarometer.org/sites/default/files/data/round-6/merged_round_6_codebook_28082017.pdf</t>
+  </si>
+  <si>
+    <t>Cross-sectional. Data and codebook link is to the 2016 merged Round 6.</t>
+  </si>
+  <si>
+    <t>http://archive.ipu.org/gpr-e/downloads/data-age-gender-profession-e.xls</t>
+  </si>
+  <si>
+    <t>http://archive.ipu.org/gpr-e/downloads/dataset-notes-e.pdf</t>
+  </si>
+  <si>
+    <t>Chamber, gender, age, profession</t>
+  </si>
+  <si>
+    <t>https://github.com/AidData-WM/public_datasets/releases/download/v3.0/AidDataCore_ResearchRelease_Level1_v3.0.zip</t>
+  </si>
+  <si>
+    <t>96 countries</t>
+  </si>
+  <si>
+    <t>International development flows</t>
+  </si>
+  <si>
+    <t>http://docs.aiddata.org/ad4/files/inline/readme.pdf</t>
+  </si>
+  <si>
+    <t>Political attitudes, voting behavior, political participation, socio-demographic characteristics</t>
+  </si>
+  <si>
+    <t>Cross-sectional and panel datasetspanel</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1074,17 +1171,18 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1363,10 +1461,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J141"/>
+  <dimension ref="A1:Q141"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1378,11 +1476,16 @@
     <col min="5" max="5" width="18.1640625" customWidth="1"/>
     <col min="7" max="7" width="21.5" customWidth="1"/>
     <col min="8" max="8" width="21.83203125" customWidth="1"/>
-    <col min="9" max="9" width="26.83203125" customWidth="1"/>
-    <col min="10" max="10" width="24.33203125" customWidth="1"/>
+    <col min="9" max="11" width="26.83203125" customWidth="1"/>
+    <col min="12" max="12" width="45.5" customWidth="1"/>
+    <col min="13" max="13" width="45" customWidth="1"/>
+    <col min="14" max="14" width="41.6640625" customWidth="1"/>
+    <col min="15" max="15" width="39.33203125" customWidth="1"/>
+    <col min="16" max="16" width="45.1640625" customWidth="1"/>
+    <col min="17" max="17" width="61" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1411,10 +1514,31 @@
         <v>19</v>
       </c>
       <c r="J1" t="s">
+        <v>351</v>
+      </c>
+      <c r="K1" t="s">
+        <v>336</v>
+      </c>
+      <c r="L1" t="s">
+        <v>337</v>
+      </c>
+      <c r="M1" t="s">
+        <v>338</v>
+      </c>
+      <c r="N1" t="s">
+        <v>339</v>
+      </c>
+      <c r="O1" t="s">
+        <v>340</v>
+      </c>
+      <c r="P1" t="s">
+        <v>341</v>
+      </c>
+      <c r="Q1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>241</v>
       </c>
@@ -1424,14 +1548,46 @@
       <c r="C2" s="2" t="s">
         <v>243</v>
       </c>
+      <c r="D2" t="s">
+        <v>346</v>
+      </c>
+      <c r="E2" t="s">
+        <v>347</v>
+      </c>
+      <c r="F2">
+        <v>2014</v>
+      </c>
+      <c r="G2">
+        <v>2014</v>
+      </c>
       <c r="H2" t="s">
-        <v>16</v>
+        <v>348</v>
       </c>
       <c r="I2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+        <v>349</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>335</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>342</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>344</v>
+      </c>
+      <c r="M2" s="2"/>
+      <c r="N2" s="2" t="s">
+        <v>343</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>345</v>
+      </c>
+      <c r="P2" s="2"/>
+      <c r="Q2" s="4" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>30</v>
       </c>
@@ -1441,14 +1597,32 @@
       <c r="C3" s="2" t="s">
         <v>50</v>
       </c>
+      <c r="D3" t="s">
+        <v>352</v>
+      </c>
       <c r="E3" t="s">
         <v>68</v>
       </c>
       <c r="F3">
         <v>1999</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="H3" t="s">
+        <v>348</v>
+      </c>
+      <c r="I3" t="s">
+        <v>349</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>354</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>353</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>262</v>
       </c>
@@ -1458,14 +1632,32 @@
       <c r="C4" s="2" t="s">
         <v>261</v>
       </c>
+      <c r="D4" t="s">
+        <v>358</v>
+      </c>
+      <c r="E4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4">
+        <v>2012</v>
+      </c>
+      <c r="G4">
+        <v>2012</v>
+      </c>
       <c r="H4" t="s">
-        <v>16</v>
+        <v>348</v>
       </c>
       <c r="I4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+        <v>349</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>357</v>
+      </c>
+      <c r="N4" s="2" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>203</v>
       </c>
@@ -1475,6 +1667,12 @@
       <c r="C5" s="2" t="s">
         <v>202</v>
       </c>
+      <c r="D5" t="s">
+        <v>361</v>
+      </c>
+      <c r="E5" t="s">
+        <v>360</v>
+      </c>
       <c r="F5">
         <v>1947</v>
       </c>
@@ -1482,13 +1680,19 @@
         <v>2013</v>
       </c>
       <c r="H5" t="s">
-        <v>16</v>
+        <v>348</v>
       </c>
       <c r="I5" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+        <v>349</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>362</v>
+      </c>
+      <c r="P5" s="2" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>33</v>
       </c>
@@ -1498,6 +1702,9 @@
       <c r="C6" s="2" t="s">
         <v>43</v>
       </c>
+      <c r="D6" t="s">
+        <v>363</v>
+      </c>
       <c r="E6" t="s">
         <v>34</v>
       </c>
@@ -1505,16 +1712,16 @@
         <v>1948</v>
       </c>
       <c r="H6" t="s">
-        <v>16</v>
+        <v>348</v>
       </c>
       <c r="I6" t="s">
-        <v>20</v>
-      </c>
-      <c r="J6" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+        <v>248</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>29</v>
       </c>
@@ -1531,7 +1738,7 @@
         <v>2004</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>70</v>
       </c>
@@ -1548,7 +1755,7 @@
         <v>2006</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>163</v>
       </c>
@@ -1559,7 +1766,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>31</v>
       </c>
@@ -1576,7 +1783,7 @@
         <v>2001</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>304</v>
       </c>
@@ -1599,7 +1806,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>207</v>
       </c>
@@ -1622,7 +1829,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>260</v>
       </c>
@@ -1639,7 +1846,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>170</v>
       </c>
@@ -1650,7 +1857,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>113</v>
       </c>
@@ -1667,7 +1874,7 @@
         <v>1964</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>64</v>
       </c>
@@ -1683,7 +1890,7 @@
       <c r="G16">
         <v>2009</v>
       </c>
-      <c r="J16" t="s">
+      <c r="Q16" t="s">
         <v>18</v>
       </c>
     </row>
@@ -2186,7 +2393,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>179</v>
       </c>
@@ -2197,7 +2404,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>78</v>
       </c>
@@ -2214,7 +2421,7 @@
         <v>1979</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A51" s="3" t="s">
         <v>82</v>
       </c>
@@ -2231,7 +2438,7 @@
         <v>1979</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A52" s="3" t="s">
         <v>85</v>
       </c>
@@ -2251,7 +2458,7 @@
         <v>2009</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>27</v>
       </c>
@@ -2261,11 +2468,11 @@
       <c r="C53" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="J53" t="s">
+      <c r="Q53" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>120</v>
       </c>
@@ -2279,7 +2486,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>5</v>
       </c>
@@ -2304,11 +2511,11 @@
       <c r="I55" t="s">
         <v>248</v>
       </c>
-      <c r="J55" t="s">
+      <c r="Q55" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>240</v>
       </c>
@@ -2325,7 +2532,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
         <v>26</v>
       </c>
@@ -2336,7 +2543,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>232</v>
       </c>
@@ -2347,7 +2554,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>276</v>
       </c>
@@ -2370,7 +2577,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>224</v>
       </c>
@@ -2393,7 +2600,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>285</v>
       </c>
@@ -2410,7 +2617,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>205</v>
       </c>
@@ -2424,7 +2631,7 @@
         <v>2006</v>
       </c>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>200</v>
       </c>
@@ -2440,11 +2647,11 @@
       <c r="G63">
         <v>2007</v>
       </c>
-      <c r="J63" t="s">
+      <c r="Q63" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>89</v>
       </c>
@@ -2467,7 +2674,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>104</v>
       </c>
@@ -2484,7 +2691,7 @@
         <v>1980</v>
       </c>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>62</v>
       </c>
@@ -2495,7 +2702,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>311</v>
       </c>
@@ -2515,7 +2722,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>281</v>
       </c>
@@ -2532,7 +2739,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>151</v>
       </c>
@@ -2546,7 +2753,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>242</v>
       </c>
@@ -2563,7 +2770,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>292</v>
       </c>
@@ -2580,7 +2787,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>153</v>
       </c>
@@ -2591,7 +2798,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>228</v>
       </c>
@@ -2614,7 +2821,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>245</v>
       </c>
@@ -2631,7 +2838,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>100</v>
       </c>
@@ -2642,7 +2849,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>239</v>
       </c>
@@ -2659,7 +2866,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>254</v>
       </c>
@@ -2685,7 +2892,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>270</v>
       </c>
@@ -2708,7 +2915,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>117</v>
       </c>
@@ -2721,11 +2928,11 @@
       <c r="I79" t="s">
         <v>20</v>
       </c>
-      <c r="J79" t="s">
+      <c r="Q79" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
         <v>23</v>
       </c>
@@ -3062,7 +3269,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>137</v>
       </c>
@@ -3073,7 +3280,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>155</v>
       </c>
@@ -3084,7 +3291,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>57</v>
       </c>
@@ -3094,11 +3301,11 @@
       <c r="C99" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="J99" t="s">
+      <c r="Q99" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="100" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>129</v>
       </c>
@@ -3121,7 +3328,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="101" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>148</v>
       </c>
@@ -3132,7 +3339,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="102" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>233</v>
       </c>
@@ -3158,7 +3365,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="103" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>35</v>
       </c>
@@ -3184,7 +3391,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="104" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>185</v>
       </c>
@@ -3195,7 +3402,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="105" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>210</v>
       </c>
@@ -3218,7 +3425,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="106" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>144</v>
       </c>
@@ -3235,7 +3442,7 @@
         <v>2013</v>
       </c>
     </row>
-    <row r="107" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>122</v>
       </c>
@@ -3249,7 +3456,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="108" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>318</v>
       </c>
@@ -3275,7 +3482,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="109" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>316</v>
       </c>
@@ -3301,7 +3508,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="110" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>322</v>
       </c>
@@ -3324,7 +3531,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="111" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>141</v>
       </c>
@@ -3334,11 +3541,11 @@
       <c r="C111" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="J111" t="s">
+      <c r="Q111" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="112" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>308</v>
       </c>
@@ -3364,7 +3571,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="113" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>287</v>
       </c>
@@ -3381,7 +3588,7 @@
         <v>2008</v>
       </c>
     </row>
-    <row r="114" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>274</v>
       </c>
@@ -3398,7 +3605,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="115" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>157</v>
       </c>
@@ -3408,11 +3615,11 @@
       <c r="C115" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="J115" t="s">
+      <c r="Q115" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="116" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>194</v>
       </c>
@@ -3423,7 +3630,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="117" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>295</v>
       </c>
@@ -3449,7 +3656,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="118" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>256</v>
       </c>
@@ -3469,7 +3676,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="119" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>227</v>
       </c>
@@ -3492,7 +3699,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="120" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>230</v>
       </c>
@@ -3515,7 +3722,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="121" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>109</v>
       </c>
@@ -3532,7 +3739,7 @@
         <v>1956</v>
       </c>
     </row>
-    <row r="122" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
         <v>326</v>
       </c>
@@ -3555,7 +3762,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="123" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
         <v>91</v>
       </c>
@@ -3572,7 +3779,7 @@
         <v>1999</v>
       </c>
     </row>
-    <row r="124" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
         <v>314</v>
       </c>
@@ -3598,7 +3805,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="125" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
         <v>161</v>
       </c>
@@ -3609,7 +3816,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="126" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
         <v>168</v>
       </c>
@@ -3620,7 +3827,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="127" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
         <v>213</v>
       </c>
@@ -3637,7 +3844,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="128" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
         <v>323</v>
       </c>
@@ -3660,7 +3867,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="129" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
         <v>273</v>
       </c>
@@ -3683,7 +3890,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="130" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
         <v>66</v>
       </c>
@@ -3694,7 +3901,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="131" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
         <v>139</v>
       </c>
@@ -3705,7 +3912,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="132" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
         <v>329</v>
       </c>
@@ -3728,7 +3935,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="133" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
         <v>172</v>
       </c>
@@ -3739,7 +3946,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="134" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
         <v>217</v>
       </c>
@@ -3762,7 +3969,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="135" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
         <v>132</v>
       </c>
@@ -3772,11 +3979,11 @@
       <c r="C135" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="J135" t="s">
+      <c r="Q135" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="136" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
         <v>182</v>
       </c>
@@ -3787,7 +3994,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="137" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
         <v>115</v>
       </c>
@@ -3798,7 +4005,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="138" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
         <v>263</v>
       </c>
@@ -3824,7 +4031,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="139" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
         <v>221</v>
       </c>
@@ -3844,7 +4051,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="140" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
         <v>13</v>
       </c>
@@ -3870,7 +4077,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="141" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
         <v>283</v>
       </c>
@@ -4032,6 +4239,13 @@
     <hyperlink ref="C132" r:id="rId138"/>
     <hyperlink ref="C35" r:id="rId139"/>
     <hyperlink ref="C82" r:id="rId140"/>
+    <hyperlink ref="J2" r:id="rId141"/>
+    <hyperlink ref="M3" r:id="rId142"/>
+    <hyperlink ref="J3" r:id="rId143"/>
+    <hyperlink ref="N4" r:id="rId144"/>
+    <hyperlink ref="J4" r:id="rId145"/>
+    <hyperlink ref="P5" r:id="rId146"/>
+    <hyperlink ref="J5" r:id="rId147"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
add datasets, 'Norwegian Parliamentary Elections, 1906-2013' and 'Cooperative Congressional Election Study'
</commit_message>
<xml_diff>
--- a/PolData.xlsx
+++ b/PolData.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="665" uniqueCount="365">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="680" uniqueCount="374">
   <si>
     <t>name</t>
   </si>
@@ -1122,6 +1122,33 @@
   </si>
   <si>
     <t>Cross-sectional and panel datasetspanel</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.18712/NSD-NSD2405-V1</t>
+  </si>
+  <si>
+    <t>Norwegian Parliamentary Elections, 1906-2013</t>
+  </si>
+  <si>
+    <t>Norway</t>
+  </si>
+  <si>
+    <t>delivered after acceptance of form</t>
+  </si>
+  <si>
+    <t>free, order form and declaration of secrecy</t>
+  </si>
+  <si>
+    <t>Data on candidates running for parliamentary (Storting).</t>
+  </si>
+  <si>
+    <t>Elections, parliamentary elections, parliamentary candidates, politicians</t>
+  </si>
+  <si>
+    <t>Cooperative Congressional Election Study</t>
+  </si>
+  <si>
+    <t>https://cces.gov.harvard.edu/</t>
   </si>
 </sst>
 </file>
@@ -1461,10 +1488,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q141"/>
+  <dimension ref="A1:Q143"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="B112" sqref="B112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2117,42 +2144,48 @@
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>39</v>
+        <v>372</v>
       </c>
       <c r="B33" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>41</v>
+        <v>373</v>
+      </c>
+      <c r="D33" t="s">
+        <v>363</v>
       </c>
       <c r="E33" t="s">
-        <v>14</v>
+        <v>34</v>
       </c>
       <c r="F33">
-        <v>1816</v>
-      </c>
-      <c r="G33">
-        <v>2007</v>
+        <v>2006</v>
       </c>
       <c r="H33" t="s">
-        <v>16</v>
+        <v>348</v>
       </c>
       <c r="I33" t="s">
-        <v>20</v>
+        <v>349</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>215</v>
+        <v>39</v>
       </c>
       <c r="B34" t="s">
-        <v>237</v>
+        <v>40</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>214</v>
+        <v>41</v>
+      </c>
+      <c r="E34" t="s">
+        <v>14</v>
       </c>
       <c r="F34">
-        <v>1995</v>
+        <v>1816</v>
+      </c>
+      <c r="G34">
+        <v>2007</v>
       </c>
       <c r="H34" t="s">
         <v>16</v>
@@ -2163,19 +2196,16 @@
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>330</v>
+        <v>215</v>
       </c>
       <c r="B35" t="s">
-        <v>165</v>
+        <v>237</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>331</v>
-      </c>
-      <c r="E35" t="s">
-        <v>77</v>
+        <v>214</v>
       </c>
       <c r="F35">
-        <v>1953</v>
+        <v>1995</v>
       </c>
       <c r="H35" t="s">
         <v>16</v>
@@ -2186,107 +2216,107 @@
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>75</v>
+        <v>330</v>
       </c>
       <c r="B36" t="s">
-        <v>25</v>
+        <v>165</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>76</v>
+        <v>331</v>
       </c>
       <c r="E36" t="s">
         <v>77</v>
       </c>
       <c r="F36">
-        <v>1971</v>
+        <v>1953</v>
+      </c>
+      <c r="H36" t="s">
+        <v>16</v>
+      </c>
+      <c r="I36" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>197</v>
+        <v>75</v>
       </c>
       <c r="B37" t="s">
-        <v>55</v>
+        <v>25</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>198</v>
+        <v>76</v>
       </c>
       <c r="E37" t="s">
-        <v>199</v>
+        <v>77</v>
       </c>
       <c r="F37">
-        <v>1975</v>
-      </c>
-      <c r="G37">
-        <v>2015</v>
-      </c>
-      <c r="H37" t="s">
-        <v>16</v>
-      </c>
-      <c r="I37" t="s">
-        <v>20</v>
+        <v>1971</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>59</v>
+        <v>197</v>
       </c>
       <c r="B38" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>61</v>
+        <v>198</v>
+      </c>
+      <c r="E38" t="s">
+        <v>199</v>
+      </c>
+      <c r="F38">
+        <v>1975</v>
+      </c>
+      <c r="G38">
+        <v>2015</v>
+      </c>
+      <c r="H38" t="s">
+        <v>16</v>
+      </c>
+      <c r="I38" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>196</v>
+        <v>59</v>
       </c>
       <c r="B39" t="s">
-        <v>165</v>
+        <v>60</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>195</v>
-      </c>
-      <c r="F39">
-        <v>1946</v>
-      </c>
-      <c r="G39">
-        <v>2016</v>
+        <v>61</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>238</v>
+        <v>196</v>
       </c>
       <c r="B40" t="s">
-        <v>237</v>
+        <v>165</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>243</v>
-      </c>
-      <c r="H40" t="s">
-        <v>16</v>
-      </c>
-      <c r="I40" t="s">
-        <v>20</v>
+        <v>195</v>
+      </c>
+      <c r="F40">
+        <v>1946</v>
+      </c>
+      <c r="G40">
+        <v>2016</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>219</v>
+        <v>238</v>
       </c>
       <c r="B41" t="s">
-        <v>124</v>
+        <v>237</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>218</v>
-      </c>
-      <c r="F41">
-        <v>1970</v>
-      </c>
-      <c r="G41">
-        <v>2015</v>
+        <v>243</v>
       </c>
       <c r="H41" t="s">
         <v>16</v>
@@ -2297,44 +2327,50 @@
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>191</v>
+        <v>219</v>
       </c>
       <c r="B42" t="s">
-        <v>25</v>
+        <v>124</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="E42" t="s">
-        <v>192</v>
+        <v>218</v>
+      </c>
+      <c r="F42">
+        <v>1970</v>
+      </c>
+      <c r="G42">
+        <v>2015</v>
+      </c>
+      <c r="H42" t="s">
+        <v>16</v>
+      </c>
+      <c r="I42" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>235</v>
+        <v>191</v>
       </c>
       <c r="B43" t="s">
-        <v>60</v>
+        <v>25</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>236</v>
-      </c>
-      <c r="H43" t="s">
-        <v>16</v>
-      </c>
-      <c r="I43" t="s">
-        <v>20</v>
+        <v>190</v>
+      </c>
+      <c r="E43" t="s">
+        <v>192</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>252</v>
+        <v>235</v>
       </c>
       <c r="B44" t="s">
-        <v>250</v>
+        <v>60</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>251</v>
+        <v>236</v>
       </c>
       <c r="H44" t="s">
         <v>16</v>
@@ -2345,91 +2381,91 @@
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>149</v>
+        <v>252</v>
       </c>
       <c r="B45" t="s">
-        <v>128</v>
+        <v>250</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>150</v>
+        <v>251</v>
+      </c>
+      <c r="H45" t="s">
+        <v>16</v>
+      </c>
+      <c r="I45" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>28</v>
+        <v>149</v>
       </c>
       <c r="B46" t="s">
-        <v>25</v>
+        <v>128</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>48</v>
+        <v>150</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>80</v>
+        <v>28</v>
       </c>
       <c r="B47" t="s">
-        <v>128</v>
+        <v>25</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="E47" t="s">
-        <v>9</v>
-      </c>
-      <c r="F47">
-        <v>1979</v>
+        <v>48</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>125</v>
+        <v>80</v>
       </c>
       <c r="B48" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>126</v>
+        <v>81</v>
+      </c>
+      <c r="E48" t="s">
+        <v>9</v>
+      </c>
+      <c r="F48">
+        <v>1979</v>
       </c>
     </row>
     <row r="49" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>179</v>
+        <v>125</v>
       </c>
       <c r="B49" t="s">
-        <v>165</v>
+        <v>124</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>180</v>
+        <v>126</v>
       </c>
     </row>
     <row r="50" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
+        <v>179</v>
+      </c>
+      <c r="B50" t="s">
+        <v>165</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="51" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
         <v>78</v>
       </c>
-      <c r="B50" t="s">
+      <c r="B51" t="s">
         <v>25</v>
       </c>
-      <c r="C50" s="2" t="s">
+      <c r="C51" s="2" t="s">
         <v>79</v>
-      </c>
-      <c r="E50" t="s">
-        <v>9</v>
-      </c>
-      <c r="F50">
-        <v>1979</v>
-      </c>
-    </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A51" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="B51" t="s">
-        <v>83</v>
-      </c>
-      <c r="C51" s="2" t="s">
-        <v>84</v>
       </c>
       <c r="E51" t="s">
         <v>9</v>
@@ -2440,13 +2476,13 @@
     </row>
     <row r="52" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A52" s="3" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B52" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="E52" t="s">
         <v>9</v>
@@ -2454,144 +2490,138 @@
       <c r="F52">
         <v>1979</v>
       </c>
-      <c r="G52">
+    </row>
+    <row r="53" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A53" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="B53" t="s">
+        <v>86</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="E53" t="s">
+        <v>9</v>
+      </c>
+      <c r="F53">
+        <v>1979</v>
+      </c>
+      <c r="G53">
         <v>2009</v>
-      </c>
-    </row>
-    <row r="53" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A53" t="s">
-        <v>27</v>
-      </c>
-      <c r="B53" t="s">
-        <v>25</v>
-      </c>
-      <c r="C53" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="Q53" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="54" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>120</v>
+        <v>27</v>
       </c>
       <c r="B54" t="s">
-        <v>259</v>
+        <v>25</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="I54" t="s">
-        <v>20</v>
+        <v>49</v>
+      </c>
+      <c r="Q54" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="55" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>5</v>
+        <v>120</v>
       </c>
       <c r="B55" t="s">
-        <v>25</v>
+        <v>259</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D55" t="s">
-        <v>94</v>
-      </c>
-      <c r="E55" t="s">
-        <v>9</v>
-      </c>
-      <c r="F55">
-        <v>2002</v>
-      </c>
-      <c r="H55" t="s">
-        <v>16</v>
+        <v>119</v>
       </c>
       <c r="I55" t="s">
-        <v>248</v>
-      </c>
-      <c r="Q55" t="s">
-        <v>44</v>
+        <v>20</v>
       </c>
     </row>
     <row r="56" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
+        <v>5</v>
+      </c>
+      <c r="B56" t="s">
+        <v>25</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D56" t="s">
+        <v>94</v>
+      </c>
+      <c r="E56" t="s">
+        <v>9</v>
+      </c>
+      <c r="F56">
+        <v>2002</v>
+      </c>
+      <c r="H56" t="s">
+        <v>16</v>
+      </c>
+      <c r="I56" t="s">
+        <v>248</v>
+      </c>
+      <c r="Q56" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="57" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
         <v>240</v>
       </c>
-      <c r="B56" t="s">
+      <c r="B57" t="s">
         <v>237</v>
       </c>
-      <c r="C56" s="2" t="s">
+      <c r="C57" s="2" t="s">
         <v>243</v>
       </c>
-      <c r="H56" t="s">
-        <v>16</v>
-      </c>
-      <c r="I56" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="57" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A57" s="1" t="s">
+      <c r="H57" t="s">
+        <v>16</v>
+      </c>
+      <c r="I57" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="58" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A58" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B57" t="s">
+      <c r="B58" t="s">
         <v>25</v>
       </c>
-      <c r="C57" s="2" t="s">
+      <c r="C58" s="2" t="s">
         <v>52</v>
-      </c>
-    </row>
-    <row r="58" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A58" t="s">
-        <v>232</v>
-      </c>
-      <c r="B58" t="s">
-        <v>250</v>
-      </c>
-      <c r="C58" s="2" t="s">
-        <v>231</v>
       </c>
     </row>
     <row r="59" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>276</v>
+        <v>232</v>
       </c>
       <c r="B59" t="s">
-        <v>124</v>
+        <v>250</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>277</v>
-      </c>
-      <c r="F59">
-        <v>1948</v>
-      </c>
-      <c r="G59">
-        <v>2000</v>
-      </c>
-      <c r="H59" t="s">
-        <v>16</v>
-      </c>
-      <c r="I59" t="s">
-        <v>20</v>
+        <v>231</v>
       </c>
     </row>
     <row r="60" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>224</v>
+        <v>276</v>
       </c>
       <c r="B60" t="s">
-        <v>40</v>
+        <v>124</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>225</v>
+        <v>277</v>
       </c>
       <c r="F60">
-        <v>1964</v>
+        <v>1948</v>
       </c>
       <c r="G60">
-        <v>2008</v>
+        <v>2000</v>
       </c>
       <c r="H60" t="s">
         <v>16</v>
@@ -2602,13 +2632,19 @@
     </row>
     <row r="61" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>285</v>
+        <v>224</v>
       </c>
       <c r="B61" t="s">
-        <v>250</v>
+        <v>40</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>286</v>
+        <v>225</v>
+      </c>
+      <c r="F61">
+        <v>1964</v>
+      </c>
+      <c r="G61">
+        <v>2008</v>
       </c>
       <c r="H61" t="s">
         <v>16</v>
@@ -2619,166 +2655,166 @@
     </row>
     <row r="62" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>205</v>
+        <v>285</v>
       </c>
       <c r="B62" t="s">
-        <v>40</v>
+        <v>250</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>204</v>
-      </c>
-      <c r="F62">
-        <v>2006</v>
+        <v>286</v>
+      </c>
+      <c r="H62" t="s">
+        <v>16</v>
+      </c>
+      <c r="I62" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="63" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>200</v>
+        <v>205</v>
       </c>
       <c r="B63" t="s">
-        <v>99</v>
+        <v>40</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="F63">
-        <v>1980</v>
-      </c>
-      <c r="G63">
-        <v>2007</v>
-      </c>
-      <c r="Q63" t="s">
-        <v>18</v>
+        <v>2006</v>
       </c>
     </row>
     <row r="64" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>89</v>
+        <v>200</v>
       </c>
       <c r="B64" t="s">
-        <v>25</v>
+        <v>99</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="E64" t="s">
-        <v>34</v>
+        <v>201</v>
       </c>
       <c r="F64">
-        <v>1972</v>
-      </c>
-      <c r="H64" t="s">
-        <v>16</v>
-      </c>
-      <c r="I64" t="s">
-        <v>20</v>
+        <v>1980</v>
+      </c>
+      <c r="G64">
+        <v>2007</v>
+      </c>
+      <c r="Q64" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="65" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>104</v>
+        <v>89</v>
       </c>
       <c r="B65" t="s">
         <v>25</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>106</v>
+        <v>88</v>
       </c>
       <c r="E65" t="s">
-        <v>105</v>
+        <v>34</v>
       </c>
       <c r="F65">
-        <v>1980</v>
+        <v>1972</v>
+      </c>
+      <c r="H65" t="s">
+        <v>16</v>
+      </c>
+      <c r="I65" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="66" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>62</v>
+        <v>104</v>
       </c>
       <c r="B66" t="s">
         <v>25</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>63</v>
+        <v>106</v>
+      </c>
+      <c r="E66" t="s">
+        <v>105</v>
+      </c>
+      <c r="F66">
+        <v>1980</v>
       </c>
     </row>
     <row r="67" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>311</v>
+        <v>62</v>
       </c>
       <c r="B67" t="s">
-        <v>165</v>
+        <v>25</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>312</v>
-      </c>
-      <c r="E67" t="s">
-        <v>14</v>
-      </c>
-      <c r="H67" t="s">
-        <v>16</v>
-      </c>
-      <c r="I67" t="s">
-        <v>301</v>
+        <v>63</v>
       </c>
     </row>
     <row r="68" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>281</v>
+        <v>311</v>
       </c>
       <c r="B68" t="s">
-        <v>237</v>
+        <v>165</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>282</v>
+        <v>312</v>
+      </c>
+      <c r="E68" t="s">
+        <v>14</v>
       </c>
       <c r="H68" t="s">
         <v>16</v>
       </c>
       <c r="I68" t="s">
-        <v>20</v>
+        <v>301</v>
       </c>
     </row>
     <row r="69" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>151</v>
+        <v>281</v>
       </c>
       <c r="B69" t="s">
-        <v>40</v>
+        <v>237</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="E69" t="s">
-        <v>14</v>
+        <v>282</v>
+      </c>
+      <c r="H69" t="s">
+        <v>16</v>
+      </c>
+      <c r="I69" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="70" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>242</v>
+        <v>151</v>
       </c>
       <c r="B70" t="s">
-        <v>237</v>
+        <v>40</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>243</v>
-      </c>
-      <c r="H70" t="s">
-        <v>16</v>
-      </c>
-      <c r="I70" t="s">
-        <v>20</v>
+        <v>152</v>
+      </c>
+      <c r="E70" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="71" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>292</v>
+        <v>242</v>
       </c>
       <c r="B71" t="s">
-        <v>99</v>
+        <v>237</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>291</v>
+        <v>243</v>
       </c>
       <c r="H71" t="s">
         <v>16</v>
@@ -2789,47 +2825,47 @@
     </row>
     <row r="72" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>153</v>
+        <v>292</v>
       </c>
       <c r="B72" t="s">
-        <v>259</v>
+        <v>99</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>154</v>
+        <v>291</v>
+      </c>
+      <c r="H72" t="s">
+        <v>16</v>
+      </c>
+      <c r="I72" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="73" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>228</v>
+        <v>153</v>
       </c>
       <c r="B73" t="s">
-        <v>40</v>
+        <v>259</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>225</v>
-      </c>
-      <c r="F73">
-        <v>1989</v>
-      </c>
-      <c r="G73">
-        <v>2017</v>
-      </c>
-      <c r="H73" t="s">
-        <v>16</v>
-      </c>
-      <c r="I73" t="s">
-        <v>20</v>
+        <v>154</v>
       </c>
     </row>
     <row r="74" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>245</v>
+        <v>228</v>
       </c>
       <c r="B74" t="s">
-        <v>237</v>
+        <v>40</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>244</v>
+        <v>225</v>
+      </c>
+      <c r="F74">
+        <v>1989</v>
+      </c>
+      <c r="G74">
+        <v>2017</v>
       </c>
       <c r="H74" t="s">
         <v>16</v>
@@ -2840,50 +2876,41 @@
     </row>
     <row r="75" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>100</v>
+        <v>245</v>
       </c>
       <c r="B75" t="s">
-        <v>99</v>
+        <v>237</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>101</v>
+        <v>244</v>
+      </c>
+      <c r="H75" t="s">
+        <v>16</v>
+      </c>
+      <c r="I75" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="76" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>239</v>
+        <v>100</v>
       </c>
       <c r="B76" t="s">
-        <v>237</v>
+        <v>99</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>243</v>
-      </c>
-      <c r="H76" t="s">
-        <v>16</v>
-      </c>
-      <c r="I76" t="s">
-        <v>20</v>
+        <v>101</v>
       </c>
     </row>
     <row r="77" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>254</v>
+        <v>239</v>
       </c>
       <c r="B77" t="s">
-        <v>55</v>
+        <v>237</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>253</v>
-      </c>
-      <c r="E77" t="s">
-        <v>255</v>
-      </c>
-      <c r="F77">
-        <v>1960</v>
-      </c>
-      <c r="G77">
-        <v>2014</v>
+        <v>243</v>
       </c>
       <c r="H77" t="s">
         <v>16</v>
@@ -2894,19 +2921,22 @@
     </row>
     <row r="78" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>270</v>
+        <v>254</v>
       </c>
       <c r="B78" t="s">
         <v>55</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>271</v>
+        <v>253</v>
+      </c>
+      <c r="E78" t="s">
+        <v>255</v>
       </c>
       <c r="F78">
-        <v>1990</v>
+        <v>1960</v>
       </c>
       <c r="G78">
-        <v>2010</v>
+        <v>2014</v>
       </c>
       <c r="H78" t="s">
         <v>16</v>
@@ -2917,96 +2947,90 @@
     </row>
     <row r="79" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>117</v>
+        <v>270</v>
       </c>
       <c r="B79" t="s">
         <v>55</v>
       </c>
       <c r="C79" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="F79">
+        <v>1990</v>
+      </c>
+      <c r="G79">
+        <v>2010</v>
+      </c>
+      <c r="H79" t="s">
+        <v>16</v>
+      </c>
+      <c r="I79" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="80" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A80" t="s">
+        <v>117</v>
+      </c>
+      <c r="B80" t="s">
+        <v>55</v>
+      </c>
+      <c r="C80" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="I79" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q79" t="s">
+      <c r="I80" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q80" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="80" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A80" s="1" t="s">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A81" s="1" t="s">
         <v>23</v>
-      </c>
-      <c r="B80" t="s">
-        <v>25</v>
-      </c>
-      <c r="C80" s="2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A81" t="s">
-        <v>300</v>
       </c>
       <c r="B81" t="s">
         <v>25</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>298</v>
-      </c>
-      <c r="E81" t="s">
-        <v>299</v>
-      </c>
-      <c r="F81">
-        <v>1969</v>
-      </c>
-      <c r="H81" t="s">
-        <v>16</v>
-      </c>
-      <c r="I81" t="s">
-        <v>249</v>
+        <v>53</v>
       </c>
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>332</v>
+        <v>300</v>
       </c>
       <c r="B82" t="s">
-        <v>134</v>
+        <v>25</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>333</v>
+        <v>298</v>
       </c>
       <c r="E82" t="s">
-        <v>334</v>
+        <v>299</v>
+      </c>
+      <c r="F82">
+        <v>1969</v>
       </c>
       <c r="H82" t="s">
         <v>16</v>
       </c>
       <c r="I82" t="s">
-        <v>20</v>
+        <v>249</v>
       </c>
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>267</v>
+        <v>332</v>
       </c>
       <c r="B83" t="s">
-        <v>250</v>
+        <v>134</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>266</v>
-      </c>
-      <c r="D83" t="s">
-        <v>269</v>
+        <v>333</v>
       </c>
       <c r="E83" t="s">
-        <v>268</v>
-      </c>
-      <c r="F83">
-        <v>1970</v>
-      </c>
-      <c r="G83">
-        <v>2014</v>
+        <v>334</v>
       </c>
       <c r="H83" t="s">
         <v>16</v>
@@ -3017,85 +3041,91 @@
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>96</v>
+        <v>267</v>
       </c>
       <c r="B84" t="s">
-        <v>25</v>
+        <v>250</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>90</v>
+        <v>266</v>
+      </c>
+      <c r="D84" t="s">
+        <v>269</v>
       </c>
       <c r="E84" t="s">
-        <v>69</v>
+        <v>268</v>
       </c>
       <c r="F84">
-        <v>1995</v>
+        <v>1970</v>
+      </c>
+      <c r="G84">
+        <v>2014</v>
+      </c>
+      <c r="H84" t="s">
+        <v>16</v>
+      </c>
+      <c r="I84" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>11</v>
+        <v>96</v>
       </c>
       <c r="B85" t="s">
         <v>25</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D85" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="E85" t="s">
-        <v>10</v>
+        <v>69</v>
       </c>
       <c r="F85">
-        <v>2007</v>
-      </c>
-      <c r="H85" t="s">
-        <v>16</v>
-      </c>
-      <c r="I85" t="s">
-        <v>21</v>
+        <v>1995</v>
       </c>
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>223</v>
+        <v>11</v>
       </c>
       <c r="B86" t="s">
-        <v>124</v>
+        <v>25</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>222</v>
+        <v>12</v>
+      </c>
+      <c r="D86" t="s">
+        <v>95</v>
+      </c>
+      <c r="E86" t="s">
+        <v>10</v>
       </c>
       <c r="F86">
-        <v>1</v>
-      </c>
-      <c r="G86">
-        <v>2010</v>
+        <v>2007</v>
       </c>
       <c r="H86" t="s">
         <v>16</v>
       </c>
       <c r="I86" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="B87" t="s">
-        <v>40</v>
+        <v>124</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="F87">
-        <v>1946</v>
+        <v>1</v>
       </c>
       <c r="G87">
-        <v>2016</v>
+        <v>2010</v>
       </c>
       <c r="H87" t="s">
         <v>16</v>
@@ -3106,90 +3136,90 @@
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>97</v>
+        <v>226</v>
       </c>
       <c r="B88" t="s">
-        <v>128</v>
+        <v>40</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>98</v>
+        <v>225</v>
+      </c>
+      <c r="F88">
+        <v>1946</v>
+      </c>
+      <c r="G88">
+        <v>2016</v>
+      </c>
+      <c r="H88" t="s">
+        <v>16</v>
+      </c>
+      <c r="I88" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>278</v>
+        <v>97</v>
       </c>
       <c r="B89" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>279</v>
-      </c>
-      <c r="E89" t="s">
-        <v>280</v>
-      </c>
-      <c r="F89">
-        <v>1890</v>
-      </c>
-      <c r="G89">
-        <v>1996</v>
-      </c>
-      <c r="H89" t="s">
-        <v>16</v>
-      </c>
-      <c r="I89" t="s">
-        <v>20</v>
+        <v>98</v>
       </c>
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>156</v>
+        <v>278</v>
       </c>
       <c r="B90" t="s">
-        <v>25</v>
+        <v>124</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>154</v>
+        <v>279</v>
+      </c>
+      <c r="E90" t="s">
+        <v>280</v>
+      </c>
+      <c r="F90">
+        <v>1890</v>
+      </c>
+      <c r="G90">
+        <v>1996</v>
+      </c>
+      <c r="H90" t="s">
+        <v>16</v>
+      </c>
+      <c r="I90" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>229</v>
+        <v>156</v>
       </c>
       <c r="B91" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>225</v>
-      </c>
-      <c r="F91">
-        <v>1952</v>
-      </c>
-      <c r="G91">
-        <v>1997</v>
-      </c>
-      <c r="H91" t="s">
-        <v>16</v>
-      </c>
-      <c r="I91" t="s">
-        <v>20</v>
+        <v>154</v>
       </c>
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>293</v>
+        <v>229</v>
       </c>
       <c r="B92" t="s">
         <v>40</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>294</v>
+        <v>225</v>
       </c>
       <c r="F92">
-        <v>2004</v>
+        <v>1952</v>
       </c>
       <c r="G92">
-        <v>2006</v>
+        <v>1997</v>
       </c>
       <c r="H92" t="s">
         <v>16</v>
@@ -3200,166 +3230,184 @@
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>102</v>
+        <v>293</v>
       </c>
       <c r="B93" t="s">
-        <v>99</v>
+        <v>40</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>103</v>
+        <v>294</v>
+      </c>
+      <c r="F93">
+        <v>2004</v>
+      </c>
+      <c r="G93">
+        <v>2006</v>
+      </c>
+      <c r="H93" t="s">
+        <v>16</v>
+      </c>
+      <c r="I93" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="94" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>289</v>
+        <v>102</v>
       </c>
       <c r="B94" t="s">
-        <v>124</v>
+        <v>99</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>290</v>
+        <v>103</v>
       </c>
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>246</v>
+        <v>289</v>
       </c>
       <c r="B95" t="s">
-        <v>165</v>
+        <v>124</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>247</v>
-      </c>
-      <c r="E95" t="s">
-        <v>14</v>
-      </c>
-      <c r="F95">
-        <v>1960</v>
-      </c>
-      <c r="G95">
-        <v>2006</v>
-      </c>
-      <c r="H95" t="s">
-        <v>16</v>
-      </c>
-      <c r="I95" t="s">
-        <v>249</v>
+        <v>290</v>
       </c>
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>208</v>
+        <v>246</v>
       </c>
       <c r="B96" t="s">
-        <v>124</v>
+        <v>165</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>209</v>
+        <v>247</v>
+      </c>
+      <c r="E96" t="s">
+        <v>14</v>
       </c>
       <c r="F96">
-        <v>1932</v>
+        <v>1960</v>
       </c>
       <c r="G96">
-        <v>2014</v>
+        <v>2006</v>
       </c>
       <c r="H96" t="s">
         <v>16</v>
       </c>
       <c r="I96" t="s">
-        <v>20</v>
+        <v>249</v>
       </c>
     </row>
     <row r="97" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>137</v>
+        <v>366</v>
       </c>
       <c r="B97" t="s">
-        <v>259</v>
+        <v>128</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>138</v>
+        <v>365</v>
+      </c>
+      <c r="D97" t="s">
+        <v>371</v>
+      </c>
+      <c r="E97" t="s">
+        <v>367</v>
+      </c>
+      <c r="F97">
+        <v>1906</v>
+      </c>
+      <c r="G97">
+        <v>2013</v>
+      </c>
+      <c r="H97" t="s">
+        <v>368</v>
+      </c>
+      <c r="I97" t="s">
+        <v>369</v>
+      </c>
+      <c r="Q97" t="s">
+        <v>370</v>
       </c>
     </row>
     <row r="98" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>155</v>
+        <v>208</v>
       </c>
       <c r="B98" t="s">
-        <v>259</v>
+        <v>124</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>154</v>
+        <v>209</v>
+      </c>
+      <c r="F98">
+        <v>1932</v>
+      </c>
+      <c r="G98">
+        <v>2014</v>
+      </c>
+      <c r="H98" t="s">
+        <v>16</v>
+      </c>
+      <c r="I98" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="99" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>57</v>
+        <v>137</v>
       </c>
       <c r="B99" t="s">
-        <v>128</v>
+        <v>259</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="Q99" t="s">
-        <v>17</v>
+        <v>138</v>
       </c>
     </row>
     <row r="100" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>129</v>
+        <v>155</v>
       </c>
       <c r="B100" t="s">
         <v>259</v>
       </c>
       <c r="C100" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="E100" t="s">
-        <v>131</v>
-      </c>
-      <c r="F100">
-        <v>1945</v>
-      </c>
-      <c r="G100">
-        <v>2008</v>
-      </c>
-      <c r="I100" t="s">
-        <v>20</v>
+        <v>154</v>
       </c>
     </row>
     <row r="101" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>148</v>
+        <v>57</v>
       </c>
       <c r="B101" t="s">
         <v>128</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>147</v>
+        <v>58</v>
+      </c>
+      <c r="Q101" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="102" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>233</v>
+        <v>129</v>
       </c>
       <c r="B102" t="s">
-        <v>165</v>
+        <v>259</v>
       </c>
       <c r="C102" s="2" t="s">
-        <v>234</v>
+        <v>130</v>
       </c>
       <c r="E102" t="s">
-        <v>14</v>
+        <v>131</v>
       </c>
       <c r="F102">
-        <v>2012</v>
+        <v>1945</v>
       </c>
       <c r="G102">
-        <v>2016</v>
-      </c>
-      <c r="H102" t="s">
-        <v>16</v>
+        <v>2008</v>
       </c>
       <c r="I102" t="s">
         <v>20</v>
@@ -3367,56 +3415,59 @@
     </row>
     <row r="103" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>35</v>
+        <v>148</v>
       </c>
       <c r="B103" t="s">
-        <v>25</v>
+        <v>128</v>
       </c>
       <c r="C103" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="D103" t="s">
-        <v>37</v>
-      </c>
-      <c r="E103" t="s">
-        <v>14</v>
-      </c>
-      <c r="F103">
-        <v>2001</v>
-      </c>
-      <c r="H103" t="s">
-        <v>16</v>
-      </c>
-      <c r="I103" t="s">
-        <v>20</v>
+        <v>147</v>
       </c>
     </row>
     <row r="104" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>185</v>
+        <v>233</v>
       </c>
       <c r="B104" t="s">
-        <v>128</v>
+        <v>165</v>
       </c>
       <c r="C104" s="2" t="s">
-        <v>186</v>
+        <v>234</v>
+      </c>
+      <c r="E104" t="s">
+        <v>14</v>
+      </c>
+      <c r="F104">
+        <v>2012</v>
+      </c>
+      <c r="G104">
+        <v>2016</v>
+      </c>
+      <c r="H104" t="s">
+        <v>16</v>
+      </c>
+      <c r="I104" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="105" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>210</v>
+        <v>35</v>
       </c>
       <c r="B105" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="C105" s="2" t="s">
-        <v>211</v>
+        <v>36</v>
+      </c>
+      <c r="D105" t="s">
+        <v>37</v>
+      </c>
+      <c r="E105" t="s">
+        <v>14</v>
       </c>
       <c r="F105">
-        <v>1976</v>
-      </c>
-      <c r="G105">
-        <v>2016</v>
+        <v>2001</v>
       </c>
       <c r="H105" t="s">
         <v>16</v>
@@ -3427,30 +3478,33 @@
     </row>
     <row r="106" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>144</v>
+        <v>185</v>
       </c>
       <c r="B106" t="s">
-        <v>60</v>
+        <v>128</v>
       </c>
       <c r="C106" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="F106">
-        <v>1800</v>
-      </c>
-      <c r="G106">
-        <v>2013</v>
+        <v>186</v>
       </c>
     </row>
     <row r="107" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>122</v>
+        <v>210</v>
       </c>
       <c r="B107" t="s">
-        <v>259</v>
+        <v>40</v>
       </c>
       <c r="C107" s="2" t="s">
-        <v>121</v>
+        <v>211</v>
+      </c>
+      <c r="F107">
+        <v>1976</v>
+      </c>
+      <c r="G107">
+        <v>2016</v>
+      </c>
+      <c r="H107" t="s">
+        <v>16</v>
       </c>
       <c r="I107" t="s">
         <v>20</v>
@@ -3458,51 +3512,30 @@
     </row>
     <row r="108" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>318</v>
+        <v>144</v>
       </c>
       <c r="B108" t="s">
-        <v>250</v>
+        <v>60</v>
       </c>
       <c r="C108" s="2" t="s">
-        <v>319</v>
-      </c>
-      <c r="E108" t="s">
-        <v>320</v>
+        <v>143</v>
       </c>
       <c r="F108">
-        <v>1975</v>
+        <v>1800</v>
       </c>
       <c r="G108">
-        <v>1989</v>
-      </c>
-      <c r="H108" t="s">
-        <v>16</v>
-      </c>
-      <c r="I108" t="s">
-        <v>20</v>
+        <v>2013</v>
       </c>
     </row>
     <row r="109" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>316</v>
+        <v>122</v>
       </c>
       <c r="B109" t="s">
-        <v>250</v>
+        <v>259</v>
       </c>
       <c r="C109" s="2" t="s">
-        <v>317</v>
-      </c>
-      <c r="E109" t="s">
-        <v>105</v>
-      </c>
-      <c r="F109">
-        <v>1950</v>
-      </c>
-      <c r="G109">
-        <v>1996</v>
-      </c>
-      <c r="H109" t="s">
-        <v>16</v>
+        <v>121</v>
       </c>
       <c r="I109" t="s">
         <v>20</v>
@@ -3510,19 +3543,22 @@
     </row>
     <row r="110" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
       <c r="B110" t="s">
-        <v>25</v>
+        <v>250</v>
       </c>
       <c r="C110" s="2" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="E110" t="s">
-        <v>77</v>
+        <v>320</v>
       </c>
       <c r="F110">
-        <v>2010</v>
+        <v>1975</v>
+      </c>
+      <c r="G110">
+        <v>1989</v>
       </c>
       <c r="H110" t="s">
         <v>16</v>
@@ -3533,35 +3569,44 @@
     </row>
     <row r="111" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>141</v>
+        <v>316</v>
       </c>
       <c r="B111" t="s">
-        <v>237</v>
+        <v>250</v>
       </c>
       <c r="C111" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="Q111" t="s">
-        <v>17</v>
+        <v>317</v>
+      </c>
+      <c r="E111" t="s">
+        <v>105</v>
+      </c>
+      <c r="F111">
+        <v>1950</v>
+      </c>
+      <c r="G111">
+        <v>1996</v>
+      </c>
+      <c r="H111" t="s">
+        <v>16</v>
+      </c>
+      <c r="I111" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="112" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>308</v>
+        <v>322</v>
       </c>
       <c r="B112" t="s">
-        <v>250</v>
+        <v>25</v>
       </c>
       <c r="C112" s="2" t="s">
-        <v>309</v>
+        <v>321</v>
       </c>
       <c r="E112" t="s">
-        <v>310</v>
+        <v>77</v>
       </c>
       <c r="F112">
-        <v>1950</v>
-      </c>
-      <c r="G112">
         <v>2010</v>
       </c>
       <c r="H112" t="s">
@@ -3573,30 +3618,36 @@
     </row>
     <row r="113" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>287</v>
+        <v>141</v>
       </c>
       <c r="B113" t="s">
-        <v>134</v>
+        <v>237</v>
       </c>
       <c r="C113" s="2" t="s">
-        <v>288</v>
-      </c>
-      <c r="F113">
-        <v>1990</v>
-      </c>
-      <c r="G113">
-        <v>2008</v>
+        <v>142</v>
+      </c>
+      <c r="Q113" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="114" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>274</v>
+        <v>308</v>
       </c>
       <c r="B114" t="s">
-        <v>55</v>
+        <v>250</v>
       </c>
       <c r="C114" s="2" t="s">
-        <v>275</v>
+        <v>309</v>
+      </c>
+      <c r="E114" t="s">
+        <v>310</v>
+      </c>
+      <c r="F114">
+        <v>1950</v>
+      </c>
+      <c r="G114">
+        <v>2010</v>
       </c>
       <c r="H114" t="s">
         <v>16</v>
@@ -3607,113 +3658,101 @@
     </row>
     <row r="115" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>157</v>
+        <v>287</v>
       </c>
       <c r="B115" t="s">
-        <v>128</v>
+        <v>134</v>
       </c>
       <c r="C115" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="Q115" t="s">
-        <v>18</v>
+        <v>288</v>
+      </c>
+      <c r="F115">
+        <v>1990</v>
+      </c>
+      <c r="G115">
+        <v>2008</v>
       </c>
     </row>
     <row r="116" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>194</v>
+        <v>274</v>
       </c>
       <c r="B116" t="s">
-        <v>99</v>
+        <v>55</v>
       </c>
       <c r="C116" s="2" t="s">
-        <v>193</v>
+        <v>275</v>
+      </c>
+      <c r="H116" t="s">
+        <v>16</v>
+      </c>
+      <c r="I116" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="117" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>295</v>
+        <v>157</v>
       </c>
       <c r="B117" t="s">
-        <v>40</v>
+        <v>128</v>
       </c>
       <c r="C117" s="2" t="s">
-        <v>296</v>
-      </c>
-      <c r="E117" t="s">
-        <v>297</v>
-      </c>
-      <c r="F117">
-        <v>1990</v>
-      </c>
-      <c r="G117">
-        <v>2015</v>
-      </c>
-      <c r="H117" t="s">
-        <v>16</v>
-      </c>
-      <c r="I117" t="s">
-        <v>249</v>
+        <v>154</v>
+      </c>
+      <c r="Q117" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="118" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>256</v>
+        <v>194</v>
       </c>
       <c r="B118" t="s">
-        <v>250</v>
+        <v>99</v>
       </c>
       <c r="C118" s="2" t="s">
-        <v>257</v>
-      </c>
-      <c r="E118" t="s">
-        <v>258</v>
-      </c>
-      <c r="H118" t="s">
-        <v>16</v>
-      </c>
-      <c r="I118" t="s">
-        <v>20</v>
+        <v>193</v>
       </c>
     </row>
     <row r="119" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>227</v>
+        <v>295</v>
       </c>
       <c r="B119" t="s">
         <v>40</v>
       </c>
       <c r="C119" s="2" t="s">
-        <v>225</v>
+        <v>296</v>
+      </c>
+      <c r="E119" t="s">
+        <v>297</v>
       </c>
       <c r="F119">
-        <v>1955</v>
+        <v>1990</v>
       </c>
       <c r="G119">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="H119" t="s">
         <v>16</v>
       </c>
       <c r="I119" t="s">
-        <v>20</v>
+        <v>249</v>
       </c>
     </row>
     <row r="120" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>230</v>
+        <v>256</v>
       </c>
       <c r="B120" t="s">
-        <v>40</v>
+        <v>250</v>
       </c>
       <c r="C120" s="2" t="s">
-        <v>225</v>
-      </c>
-      <c r="F120">
-        <v>1995</v>
-      </c>
-      <c r="G120">
-        <v>2016</v>
+        <v>257</v>
+      </c>
+      <c r="E120" t="s">
+        <v>258</v>
       </c>
       <c r="H120" t="s">
         <v>16</v>
@@ -3724,36 +3763,42 @@
     </row>
     <row r="121" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>109</v>
+        <v>227</v>
       </c>
       <c r="B121" t="s">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="C121" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="E121" t="s">
-        <v>111</v>
+        <v>225</v>
       </c>
       <c r="F121">
-        <v>1956</v>
+        <v>1955</v>
+      </c>
+      <c r="G121">
+        <v>2016</v>
+      </c>
+      <c r="H121" t="s">
+        <v>16</v>
+      </c>
+      <c r="I121" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="122" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>326</v>
+        <v>230</v>
       </c>
       <c r="B122" t="s">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="C122" s="2" t="s">
-        <v>327</v>
-      </c>
-      <c r="E122" t="s">
-        <v>111</v>
+        <v>225</v>
       </c>
       <c r="F122">
-        <v>1998</v>
+        <v>1995</v>
+      </c>
+      <c r="G122">
+        <v>2016</v>
       </c>
       <c r="H122" t="s">
         <v>16</v>
@@ -3764,39 +3809,36 @@
     </row>
     <row r="123" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>91</v>
+        <v>109</v>
       </c>
       <c r="B123" t="s">
         <v>25</v>
       </c>
       <c r="C123" s="2" t="s">
-        <v>93</v>
+        <v>110</v>
       </c>
       <c r="E123" t="s">
-        <v>92</v>
+        <v>111</v>
       </c>
       <c r="F123">
-        <v>1999</v>
+        <v>1956</v>
       </c>
     </row>
     <row r="124" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>314</v>
+        <v>326</v>
       </c>
       <c r="B124" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="C124" s="2" t="s">
-        <v>313</v>
+        <v>327</v>
       </c>
       <c r="E124" t="s">
-        <v>315</v>
+        <v>111</v>
       </c>
       <c r="F124">
-        <v>1950</v>
-      </c>
-      <c r="G124">
-        <v>2004</v>
+        <v>1998</v>
       </c>
       <c r="H124" t="s">
         <v>16</v>
@@ -3807,81 +3849,78 @@
     </row>
     <row r="125" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>161</v>
+        <v>91</v>
       </c>
       <c r="B125" t="s">
         <v>25</v>
       </c>
       <c r="C125" s="2" t="s">
-        <v>160</v>
+        <v>93</v>
+      </c>
+      <c r="E125" t="s">
+        <v>92</v>
+      </c>
+      <c r="F125">
+        <v>1999</v>
       </c>
     </row>
     <row r="126" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>168</v>
+        <v>314</v>
       </c>
       <c r="B126" t="s">
         <v>40</v>
       </c>
       <c r="C126" s="2" t="s">
-        <v>167</v>
+        <v>313</v>
+      </c>
+      <c r="E126" t="s">
+        <v>315</v>
+      </c>
+      <c r="F126">
+        <v>1950</v>
+      </c>
+      <c r="G126">
+        <v>2004</v>
+      </c>
+      <c r="H126" t="s">
+        <v>16</v>
+      </c>
+      <c r="I126" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="127" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>213</v>
+        <v>161</v>
       </c>
       <c r="B127" t="s">
-        <v>55</v>
+        <v>25</v>
       </c>
       <c r="C127" s="2" t="s">
-        <v>212</v>
-      </c>
-      <c r="H127" t="s">
-        <v>16</v>
-      </c>
-      <c r="I127" t="s">
-        <v>20</v>
+        <v>160</v>
       </c>
     </row>
     <row r="128" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>323</v>
+        <v>168</v>
       </c>
       <c r="B128" t="s">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="C128" s="2" t="s">
-        <v>324</v>
-      </c>
-      <c r="E128" t="s">
-        <v>325</v>
-      </c>
-      <c r="F128">
-        <v>1942</v>
-      </c>
-      <c r="H128" t="s">
-        <v>16</v>
-      </c>
-      <c r="I128" t="s">
-        <v>20</v>
+        <v>167</v>
       </c>
     </row>
     <row r="129" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>273</v>
+        <v>213</v>
       </c>
       <c r="B129" t="s">
-        <v>237</v>
+        <v>55</v>
       </c>
       <c r="C129" s="2" t="s">
-        <v>272</v>
-      </c>
-      <c r="F129">
-        <v>1996</v>
-      </c>
-      <c r="G129">
-        <v>2016</v>
+        <v>212</v>
       </c>
       <c r="H129" t="s">
         <v>16</v>
@@ -3892,75 +3931,87 @@
     </row>
     <row r="130" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
-        <v>66</v>
+        <v>323</v>
       </c>
       <c r="B130" t="s">
         <v>25</v>
       </c>
       <c r="C130" s="2" t="s">
-        <v>67</v>
+        <v>324</v>
+      </c>
+      <c r="E130" t="s">
+        <v>325</v>
+      </c>
+      <c r="F130">
+        <v>1942</v>
+      </c>
+      <c r="H130" t="s">
+        <v>16</v>
+      </c>
+      <c r="I130" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="131" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>139</v>
+        <v>273</v>
       </c>
       <c r="B131" t="s">
-        <v>40</v>
+        <v>237</v>
       </c>
       <c r="C131" s="2" t="s">
-        <v>140</v>
+        <v>272</v>
+      </c>
+      <c r="F131">
+        <v>1996</v>
+      </c>
+      <c r="G131">
+        <v>2016</v>
+      </c>
+      <c r="H131" t="s">
+        <v>16</v>
+      </c>
+      <c r="I131" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="132" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>329</v>
+        <v>66</v>
       </c>
       <c r="B132" t="s">
-        <v>165</v>
+        <v>25</v>
       </c>
       <c r="C132" s="2" t="s">
-        <v>328</v>
-      </c>
-      <c r="E132" t="s">
-        <v>34</v>
-      </c>
-      <c r="F132">
-        <v>1789</v>
-      </c>
-      <c r="H132" t="s">
-        <v>16</v>
-      </c>
-      <c r="I132" t="s">
-        <v>20</v>
+        <v>67</v>
       </c>
     </row>
     <row r="133" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
-        <v>172</v>
+        <v>139</v>
       </c>
       <c r="B133" t="s">
-        <v>60</v>
+        <v>40</v>
       </c>
       <c r="C133" s="2" t="s">
-        <v>171</v>
+        <v>140</v>
       </c>
     </row>
     <row r="134" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
-        <v>217</v>
+        <v>329</v>
       </c>
       <c r="B134" t="s">
-        <v>60</v>
+        <v>165</v>
       </c>
       <c r="C134" s="2" t="s">
-        <v>216</v>
+        <v>328</v>
       </c>
       <c r="E134" t="s">
-        <v>14</v>
+        <v>34</v>
       </c>
       <c r="F134">
-        <v>1900</v>
+        <v>1789</v>
       </c>
       <c r="H134" t="s">
         <v>16</v>
@@ -3971,104 +4022,92 @@
     </row>
     <row r="135" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
-        <v>132</v>
+        <v>172</v>
       </c>
       <c r="B135" t="s">
-        <v>259</v>
+        <v>60</v>
       </c>
       <c r="C135" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="Q135" t="s">
-        <v>17</v>
+        <v>171</v>
       </c>
     </row>
     <row r="136" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
-        <v>182</v>
+        <v>217</v>
       </c>
       <c r="B136" t="s">
-        <v>165</v>
+        <v>60</v>
       </c>
       <c r="C136" s="2" t="s">
-        <v>181</v>
+        <v>216</v>
+      </c>
+      <c r="E136" t="s">
+        <v>14</v>
+      </c>
+      <c r="F136">
+        <v>1900</v>
+      </c>
+      <c r="H136" t="s">
+        <v>16</v>
+      </c>
+      <c r="I136" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="137" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
-        <v>115</v>
+        <v>132</v>
       </c>
       <c r="B137" t="s">
-        <v>128</v>
+        <v>259</v>
       </c>
       <c r="C137" s="2" t="s">
-        <v>116</v>
+        <v>133</v>
+      </c>
+      <c r="Q137" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="138" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
-        <v>263</v>
+        <v>182</v>
       </c>
       <c r="B138" t="s">
-        <v>250</v>
+        <v>165</v>
       </c>
       <c r="C138" s="2" t="s">
-        <v>264</v>
-      </c>
-      <c r="E138" t="s">
-        <v>265</v>
-      </c>
-      <c r="F138">
-        <v>1500</v>
-      </c>
-      <c r="G138">
-        <v>2000</v>
-      </c>
-      <c r="H138" t="s">
-        <v>16</v>
-      </c>
-      <c r="I138" t="s">
-        <v>20</v>
+        <v>181</v>
       </c>
     </row>
     <row r="139" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
-        <v>221</v>
+        <v>115</v>
       </c>
       <c r="B139" t="s">
-        <v>86</v>
+        <v>128</v>
       </c>
       <c r="C139" s="2" t="s">
-        <v>220</v>
-      </c>
-      <c r="F139">
-        <v>2013</v>
-      </c>
-      <c r="H139" t="s">
-        <v>16</v>
-      </c>
-      <c r="I139" t="s">
-        <v>20</v>
+        <v>116</v>
       </c>
     </row>
     <row r="140" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
-        <v>13</v>
+        <v>263</v>
       </c>
       <c r="B140" t="s">
-        <v>25</v>
+        <v>250</v>
       </c>
       <c r="C140" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="D140" s="1" t="s">
-        <v>42</v>
+        <v>264</v>
       </c>
       <c r="E140" t="s">
-        <v>14</v>
+        <v>265</v>
       </c>
       <c r="F140">
-        <v>1981</v>
+        <v>1500</v>
+      </c>
+      <c r="G140">
+        <v>2000</v>
       </c>
       <c r="H140" t="s">
         <v>16</v>
@@ -4079,166 +4118,212 @@
     </row>
     <row r="141" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
+        <v>221</v>
+      </c>
+      <c r="B141" t="s">
+        <v>86</v>
+      </c>
+      <c r="C141" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="F141">
+        <v>2013</v>
+      </c>
+      <c r="H141" t="s">
+        <v>16</v>
+      </c>
+      <c r="I141" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="142" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A142" t="s">
+        <v>13</v>
+      </c>
+      <c r="B142" t="s">
+        <v>25</v>
+      </c>
+      <c r="C142" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D142" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E142" t="s">
+        <v>14</v>
+      </c>
+      <c r="F142">
+        <v>1981</v>
+      </c>
+      <c r="H142" t="s">
+        <v>16</v>
+      </c>
+      <c r="I142" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="143" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A143" t="s">
         <v>283</v>
       </c>
-      <c r="B141" t="s">
+      <c r="B143" t="s">
         <v>124</v>
       </c>
-      <c r="C141" s="2" t="s">
+      <c r="C143" s="2" t="s">
         <v>284</v>
       </c>
-      <c r="H141" t="s">
-        <v>16</v>
-      </c>
-      <c r="I141" t="s">
+      <c r="H143" t="s">
+        <v>16</v>
+      </c>
+      <c r="I143" t="s">
         <v>20</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:J141">
+  <sortState ref="A2:Q143">
     <sortCondition ref="A2"/>
   </sortState>
   <hyperlinks>
     <hyperlink ref="C6" r:id="rId1"/>
-    <hyperlink ref="C55" r:id="rId2"/>
+    <hyperlink ref="C56" r:id="rId2"/>
     <hyperlink ref="C7" r:id="rId3"/>
     <hyperlink ref="C10" r:id="rId4"/>
-    <hyperlink ref="C85" r:id="rId5"/>
-    <hyperlink ref="C103" r:id="rId6"/>
-    <hyperlink ref="C140" r:id="rId7"/>
-    <hyperlink ref="C33" r:id="rId8"/>
+    <hyperlink ref="C86" r:id="rId5"/>
+    <hyperlink ref="C105" r:id="rId6"/>
+    <hyperlink ref="C142" r:id="rId7"/>
+    <hyperlink ref="C34" r:id="rId8"/>
     <hyperlink ref="C29" r:id="rId9"/>
-    <hyperlink ref="C46" r:id="rId10"/>
-    <hyperlink ref="C53" r:id="rId11"/>
+    <hyperlink ref="C47" r:id="rId10"/>
+    <hyperlink ref="C54" r:id="rId11"/>
     <hyperlink ref="C3" r:id="rId12"/>
     <hyperlink ref="C20" r:id="rId13"/>
-    <hyperlink ref="C57" r:id="rId14"/>
-    <hyperlink ref="C80" r:id="rId15"/>
+    <hyperlink ref="C58" r:id="rId14"/>
+    <hyperlink ref="C81" r:id="rId15"/>
     <hyperlink ref="C28" r:id="rId16"/>
-    <hyperlink ref="C99" r:id="rId17"/>
-    <hyperlink ref="C38" r:id="rId18"/>
-    <hyperlink ref="C66" r:id="rId19"/>
+    <hyperlink ref="C101" r:id="rId17"/>
+    <hyperlink ref="C39" r:id="rId18"/>
+    <hyperlink ref="C67" r:id="rId19"/>
     <hyperlink ref="C16" r:id="rId20"/>
-    <hyperlink ref="C130" r:id="rId21"/>
+    <hyperlink ref="C132" r:id="rId21"/>
     <hyperlink ref="C8" r:id="rId22"/>
-    <hyperlink ref="C36" r:id="rId23"/>
-    <hyperlink ref="C50" r:id="rId24"/>
-    <hyperlink ref="C47" r:id="rId25"/>
-    <hyperlink ref="C51" r:id="rId26"/>
-    <hyperlink ref="C52" r:id="rId27"/>
-    <hyperlink ref="C64" r:id="rId28"/>
-    <hyperlink ref="C84" r:id="rId29"/>
-    <hyperlink ref="C123" r:id="rId30"/>
-    <hyperlink ref="C88" r:id="rId31"/>
-    <hyperlink ref="C75" r:id="rId32"/>
-    <hyperlink ref="C93" r:id="rId33"/>
-    <hyperlink ref="C65" r:id="rId34"/>
+    <hyperlink ref="C37" r:id="rId23"/>
+    <hyperlink ref="C51" r:id="rId24"/>
+    <hyperlink ref="C48" r:id="rId25"/>
+    <hyperlink ref="C52" r:id="rId26"/>
+    <hyperlink ref="C53" r:id="rId27"/>
+    <hyperlink ref="C65" r:id="rId28"/>
+    <hyperlink ref="C85" r:id="rId29"/>
+    <hyperlink ref="C125" r:id="rId30"/>
+    <hyperlink ref="C89" r:id="rId31"/>
+    <hyperlink ref="C76" r:id="rId32"/>
+    <hyperlink ref="C94" r:id="rId33"/>
+    <hyperlink ref="C66" r:id="rId34"/>
     <hyperlink ref="C17" r:id="rId35"/>
-    <hyperlink ref="C121" r:id="rId36"/>
+    <hyperlink ref="C123" r:id="rId36"/>
     <hyperlink ref="C15" r:id="rId37"/>
-    <hyperlink ref="C137" r:id="rId38"/>
-    <hyperlink ref="C79" r:id="rId39"/>
-    <hyperlink ref="C54" r:id="rId40"/>
-    <hyperlink ref="C107" r:id="rId41"/>
+    <hyperlink ref="C139" r:id="rId38"/>
+    <hyperlink ref="C80" r:id="rId39"/>
+    <hyperlink ref="C55" r:id="rId40"/>
+    <hyperlink ref="C109" r:id="rId41"/>
     <hyperlink ref="C18" r:id="rId42"/>
-    <hyperlink ref="C48" r:id="rId43"/>
+    <hyperlink ref="C49" r:id="rId43"/>
     <hyperlink ref="C22" r:id="rId44"/>
-    <hyperlink ref="C100" r:id="rId45"/>
-    <hyperlink ref="C135" r:id="rId46"/>
+    <hyperlink ref="C102" r:id="rId45"/>
+    <hyperlink ref="C137" r:id="rId46"/>
     <hyperlink ref="C26" r:id="rId47" display="http://comparativeconstitutionsproject.org/"/>
-    <hyperlink ref="C97" r:id="rId48"/>
-    <hyperlink ref="C131" r:id="rId49"/>
-    <hyperlink ref="C111" r:id="rId50"/>
-    <hyperlink ref="C106" r:id="rId51"/>
+    <hyperlink ref="C99" r:id="rId48"/>
+    <hyperlink ref="C133" r:id="rId49"/>
+    <hyperlink ref="C113" r:id="rId50"/>
+    <hyperlink ref="C108" r:id="rId51"/>
     <hyperlink ref="C21" r:id="rId52"/>
-    <hyperlink ref="C101" r:id="rId53"/>
-    <hyperlink ref="C45" r:id="rId54"/>
-    <hyperlink ref="C69" r:id="rId55"/>
-    <hyperlink ref="C72" r:id="rId56"/>
-    <hyperlink ref="C98" r:id="rId57"/>
-    <hyperlink ref="C90" r:id="rId58"/>
-    <hyperlink ref="C115" r:id="rId59"/>
+    <hyperlink ref="C103" r:id="rId53"/>
+    <hyperlink ref="C46" r:id="rId54"/>
+    <hyperlink ref="C70" r:id="rId55"/>
+    <hyperlink ref="C73" r:id="rId56"/>
+    <hyperlink ref="C100" r:id="rId57"/>
+    <hyperlink ref="C91" r:id="rId58"/>
+    <hyperlink ref="C117" r:id="rId59"/>
     <hyperlink ref="C30" r:id="rId60"/>
-    <hyperlink ref="C125" r:id="rId61"/>
+    <hyperlink ref="C127" r:id="rId61"/>
     <hyperlink ref="C9" r:id="rId62"/>
     <hyperlink ref="C32" r:id="rId63"/>
-    <hyperlink ref="C126" r:id="rId64"/>
+    <hyperlink ref="C128" r:id="rId64"/>
     <hyperlink ref="C14" r:id="rId65"/>
-    <hyperlink ref="C133" r:id="rId66"/>
+    <hyperlink ref="C135" r:id="rId66"/>
     <hyperlink ref="C24" r:id="rId67"/>
     <hyperlink ref="C23" r:id="rId68"/>
     <hyperlink ref="C25" r:id="rId69"/>
-    <hyperlink ref="C49" r:id="rId70"/>
-    <hyperlink ref="C136" r:id="rId71"/>
+    <hyperlink ref="C50" r:id="rId70"/>
+    <hyperlink ref="C138" r:id="rId71"/>
     <hyperlink ref="C27" r:id="rId72"/>
-    <hyperlink ref="C104" r:id="rId73"/>
+    <hyperlink ref="C106" r:id="rId73"/>
     <hyperlink ref="C31" r:id="rId74"/>
-    <hyperlink ref="C42" r:id="rId75"/>
-    <hyperlink ref="C116" r:id="rId76"/>
-    <hyperlink ref="C39" r:id="rId77"/>
-    <hyperlink ref="C37" r:id="rId78"/>
-    <hyperlink ref="C63" r:id="rId79"/>
+    <hyperlink ref="C43" r:id="rId75"/>
+    <hyperlink ref="C118" r:id="rId76"/>
+    <hyperlink ref="C40" r:id="rId77"/>
+    <hyperlink ref="C38" r:id="rId78"/>
+    <hyperlink ref="C64" r:id="rId79"/>
     <hyperlink ref="C5" r:id="rId80"/>
-    <hyperlink ref="C62" r:id="rId81"/>
+    <hyperlink ref="C63" r:id="rId81"/>
     <hyperlink ref="C12" r:id="rId82"/>
-    <hyperlink ref="C96" r:id="rId83"/>
-    <hyperlink ref="C105" r:id="rId84"/>
-    <hyperlink ref="C127" r:id="rId85"/>
-    <hyperlink ref="C34" r:id="rId86"/>
-    <hyperlink ref="C134" r:id="rId87"/>
-    <hyperlink ref="C41" r:id="rId88"/>
-    <hyperlink ref="C139" r:id="rId89"/>
-    <hyperlink ref="C86" r:id="rId90"/>
-    <hyperlink ref="C60" r:id="rId91"/>
-    <hyperlink ref="C87" r:id="rId92"/>
-    <hyperlink ref="C119" r:id="rId93"/>
-    <hyperlink ref="C73" r:id="rId94"/>
-    <hyperlink ref="C91" r:id="rId95"/>
-    <hyperlink ref="C120" r:id="rId96"/>
-    <hyperlink ref="C58" r:id="rId97"/>
-    <hyperlink ref="C102" r:id="rId98"/>
-    <hyperlink ref="C43" r:id="rId99"/>
-    <hyperlink ref="C40" r:id="rId100"/>
-    <hyperlink ref="C76" r:id="rId101"/>
-    <hyperlink ref="C56" r:id="rId102"/>
+    <hyperlink ref="C98" r:id="rId83"/>
+    <hyperlink ref="C107" r:id="rId84"/>
+    <hyperlink ref="C129" r:id="rId85"/>
+    <hyperlink ref="C35" r:id="rId86"/>
+    <hyperlink ref="C136" r:id="rId87"/>
+    <hyperlink ref="C42" r:id="rId88"/>
+    <hyperlink ref="C141" r:id="rId89"/>
+    <hyperlink ref="C87" r:id="rId90"/>
+    <hyperlink ref="C61" r:id="rId91"/>
+    <hyperlink ref="C88" r:id="rId92"/>
+    <hyperlink ref="C121" r:id="rId93"/>
+    <hyperlink ref="C74" r:id="rId94"/>
+    <hyperlink ref="C92" r:id="rId95"/>
+    <hyperlink ref="C122" r:id="rId96"/>
+    <hyperlink ref="C59" r:id="rId97"/>
+    <hyperlink ref="C104" r:id="rId98"/>
+    <hyperlink ref="C44" r:id="rId99"/>
+    <hyperlink ref="C41" r:id="rId100"/>
+    <hyperlink ref="C77" r:id="rId101"/>
+    <hyperlink ref="C57" r:id="rId102"/>
     <hyperlink ref="C2" r:id="rId103"/>
-    <hyperlink ref="C70" r:id="rId104"/>
-    <hyperlink ref="C74" r:id="rId105"/>
-    <hyperlink ref="C95" r:id="rId106"/>
-    <hyperlink ref="C44" r:id="rId107"/>
-    <hyperlink ref="C77" r:id="rId108"/>
-    <hyperlink ref="C118" r:id="rId109"/>
+    <hyperlink ref="C71" r:id="rId104"/>
+    <hyperlink ref="C75" r:id="rId105"/>
+    <hyperlink ref="C96" r:id="rId106"/>
+    <hyperlink ref="C45" r:id="rId107"/>
+    <hyperlink ref="C78" r:id="rId108"/>
+    <hyperlink ref="C120" r:id="rId109"/>
     <hyperlink ref="C13" r:id="rId110"/>
     <hyperlink ref="C4" r:id="rId111"/>
-    <hyperlink ref="C138" r:id="rId112"/>
-    <hyperlink ref="C83" r:id="rId113"/>
-    <hyperlink ref="C78" r:id="rId114"/>
-    <hyperlink ref="C129" r:id="rId115"/>
-    <hyperlink ref="C114" r:id="rId116"/>
-    <hyperlink ref="C59" r:id="rId117"/>
-    <hyperlink ref="C89" r:id="rId118"/>
-    <hyperlink ref="C68" r:id="rId119"/>
-    <hyperlink ref="C141" r:id="rId120"/>
-    <hyperlink ref="C61" r:id="rId121"/>
-    <hyperlink ref="C113" r:id="rId122"/>
-    <hyperlink ref="C94" r:id="rId123"/>
-    <hyperlink ref="C71" r:id="rId124"/>
-    <hyperlink ref="C92" r:id="rId125"/>
-    <hyperlink ref="C117" r:id="rId126"/>
-    <hyperlink ref="C81" r:id="rId127"/>
+    <hyperlink ref="C140" r:id="rId112"/>
+    <hyperlink ref="C84" r:id="rId113"/>
+    <hyperlink ref="C79" r:id="rId114"/>
+    <hyperlink ref="C131" r:id="rId115"/>
+    <hyperlink ref="C116" r:id="rId116"/>
+    <hyperlink ref="C60" r:id="rId117"/>
+    <hyperlink ref="C90" r:id="rId118"/>
+    <hyperlink ref="C69" r:id="rId119"/>
+    <hyperlink ref="C143" r:id="rId120"/>
+    <hyperlink ref="C62" r:id="rId121"/>
+    <hyperlink ref="C115" r:id="rId122"/>
+    <hyperlink ref="C95" r:id="rId123"/>
+    <hyperlink ref="C72" r:id="rId124"/>
+    <hyperlink ref="C93" r:id="rId125"/>
+    <hyperlink ref="C119" r:id="rId126"/>
+    <hyperlink ref="C82" r:id="rId127"/>
     <hyperlink ref="C11" r:id="rId128"/>
     <hyperlink ref="C19" r:id="rId129"/>
-    <hyperlink ref="C112" r:id="rId130"/>
-    <hyperlink ref="C67" r:id="rId131"/>
-    <hyperlink ref="C124" r:id="rId132"/>
-    <hyperlink ref="C109" r:id="rId133"/>
-    <hyperlink ref="C108" r:id="rId134"/>
-    <hyperlink ref="C110" r:id="rId135"/>
-    <hyperlink ref="C128" r:id="rId136"/>
-    <hyperlink ref="C122" r:id="rId137"/>
-    <hyperlink ref="C132" r:id="rId138"/>
-    <hyperlink ref="C35" r:id="rId139"/>
-    <hyperlink ref="C82" r:id="rId140"/>
+    <hyperlink ref="C114" r:id="rId130"/>
+    <hyperlink ref="C68" r:id="rId131"/>
+    <hyperlink ref="C126" r:id="rId132"/>
+    <hyperlink ref="C111" r:id="rId133"/>
+    <hyperlink ref="C110" r:id="rId134"/>
+    <hyperlink ref="C112" r:id="rId135"/>
+    <hyperlink ref="C130" r:id="rId136"/>
+    <hyperlink ref="C124" r:id="rId137"/>
+    <hyperlink ref="C134" r:id="rId138"/>
+    <hyperlink ref="C36" r:id="rId139"/>
+    <hyperlink ref="C83" r:id="rId140"/>
     <hyperlink ref="J2" r:id="rId141"/>
     <hyperlink ref="M3" r:id="rId142"/>
     <hyperlink ref="J3" r:id="rId143"/>
@@ -4246,6 +4331,8 @@
     <hyperlink ref="J4" r:id="rId145"/>
     <hyperlink ref="P5" r:id="rId146"/>
     <hyperlink ref="J5" r:id="rId147"/>
+    <hyperlink ref="C97" r:id="rId148"/>
+    <hyperlink ref="C33" r:id="rId149"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
update info on Americas Barometer and Arab Barometer
</commit_message>
<xml_diff>
--- a/PolData.xlsx
+++ b/PolData.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="680" uniqueCount="374">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="693" uniqueCount="383">
   <si>
     <t>name</t>
   </si>
@@ -1121,9 +1121,6 @@
     <t>Political attitudes, voting behavior, political participation, socio-demographic characteristics</t>
   </si>
   <si>
-    <t>Cross-sectional and panel datasetspanel</t>
-  </si>
-  <si>
     <t>https://doi.org/10.18712/NSD-NSD2405-V1</t>
   </si>
   <si>
@@ -1149,6 +1146,36 @@
   </si>
   <si>
     <t>https://cces.gov.harvard.edu/</t>
+  </si>
+  <si>
+    <t>Cross-sectional and panel datasets</t>
+  </si>
+  <si>
+    <t>http://datasets.americasbarometer.org/database/files/746278534AmericasBarometer%20Grand%20Merge%202004-2014%20v3.0_FREE_dta.zip</t>
+  </si>
+  <si>
+    <t>Cross-sectional dataset. Link to zip file is to the 2004-2014 merged Stata file.</t>
+  </si>
+  <si>
+    <t>http://datasets.americasbarometer.org/database/files/12364388022004-2014%20Grand%20Merge%20Codebook_V3.0_Free_W.pdf</t>
+  </si>
+  <si>
+    <t>free, no registration (free registration for full data)</t>
+  </si>
+  <si>
+    <t>Political attitudes, political participation, socio-demographic characteristics</t>
+  </si>
+  <si>
+    <t>http://www.arabbarometer.org/sites/default/files/Arab_Barometer_Fourth_Wave_English_Data_Set_v1.sav</t>
+  </si>
+  <si>
+    <t>http://www.arabbarometer.org/sites/default/files/Arab_Barometer_Fourth_Wave_English_Data_Set_v1.dta</t>
+  </si>
+  <si>
+    <t>http://www.arabbarometer.org/sites/default/files/code_book/AB4%20English%20Codebook%20Final%20English.pdf</t>
+  </si>
+  <si>
+    <t>Cross-sectional dataset. Links are to the Arab Barometer IV data files.</t>
   </si>
 </sst>
 </file>
@@ -1491,7 +1518,7 @@
   <dimension ref="A1:Q143"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B112" sqref="B112"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1509,7 +1536,7 @@
     <col min="14" max="14" width="41.6640625" customWidth="1"/>
     <col min="15" max="15" width="39.33203125" customWidth="1"/>
     <col min="16" max="16" width="45.1640625" customWidth="1"/>
-    <col min="17" max="17" width="61" customWidth="1"/>
+    <col min="17" max="17" width="67.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.2">
@@ -1745,7 +1772,7 @@
         <v>248</v>
       </c>
       <c r="Q6" t="s">
-        <v>364</v>
+        <v>373</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.2">
@@ -1758,11 +1785,29 @@
       <c r="C7" s="2" t="s">
         <v>45</v>
       </c>
+      <c r="D7" t="s">
+        <v>378</v>
+      </c>
       <c r="E7" t="s">
         <v>69</v>
       </c>
       <c r="F7">
         <v>2004</v>
+      </c>
+      <c r="H7" t="s">
+        <v>348</v>
+      </c>
+      <c r="I7" t="s">
+        <v>377</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>376</v>
+      </c>
+      <c r="P7" s="2" t="s">
+        <v>374</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>375</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.2">
@@ -1775,11 +1820,32 @@
       <c r="C8" s="2" t="s">
         <v>71</v>
       </c>
+      <c r="D8" t="s">
+        <v>378</v>
+      </c>
       <c r="E8" t="s">
         <v>72</v>
       </c>
       <c r="F8">
         <v>2006</v>
+      </c>
+      <c r="H8" t="s">
+        <v>348</v>
+      </c>
+      <c r="I8" t="s">
+        <v>349</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>381</v>
+      </c>
+      <c r="L8" s="2" t="s">
+        <v>380</v>
+      </c>
+      <c r="M8" s="2" t="s">
+        <v>379</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>382</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.2">
@@ -2144,13 +2210,13 @@
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B33" t="s">
         <v>25</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="D33" t="s">
         <v>363</v>
@@ -3301,19 +3367,19 @@
     </row>
     <row r="97" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B97" t="s">
         <v>128</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="D97" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="E97" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="F97">
         <v>1906</v>
@@ -3322,13 +3388,13 @@
         <v>2013</v>
       </c>
       <c r="H97" t="s">
+        <v>367</v>
+      </c>
+      <c r="I97" t="s">
         <v>368</v>
       </c>
-      <c r="I97" t="s">
+      <c r="Q97" t="s">
         <v>369</v>
-      </c>
-      <c r="Q97" t="s">
-        <v>370</v>
       </c>
     </row>
     <row r="98" spans="1:17" x14ac:dyDescent="0.2">
@@ -4333,6 +4399,11 @@
     <hyperlink ref="J5" r:id="rId147"/>
     <hyperlink ref="C97" r:id="rId148"/>
     <hyperlink ref="C33" r:id="rId149"/>
+    <hyperlink ref="P7" r:id="rId150"/>
+    <hyperlink ref="J7" r:id="rId151"/>
+    <hyperlink ref="M8" r:id="rId152"/>
+    <hyperlink ref="L8" r:id="rId153"/>
+    <hyperlink ref="J8" r:id="rId154"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
add data on Central Bank Governors and United Nations Security Council membership
</commit_message>
<xml_diff>
--- a/PolData.xlsx
+++ b/PolData.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="693" uniqueCount="383">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="707" uniqueCount="390">
   <si>
     <t>name</t>
   </si>
@@ -1176,6 +1176,27 @@
   </si>
   <si>
     <t>Cross-sectional dataset. Links are to the Arab Barometer IV data files.</t>
+  </si>
+  <si>
+    <t>United Nations Security Council membership</t>
+  </si>
+  <si>
+    <t>http://www.uni-heidelberg.de/fakultaeten/wiso/awi/professuren/intwipol/datasets_en.html</t>
+  </si>
+  <si>
+    <t>http://www.axel-dreher.de/UNSCdata.xls</t>
+  </si>
+  <si>
+    <t>193 countries</t>
+  </si>
+  <si>
+    <t>Central Bank Governors</t>
+  </si>
+  <si>
+    <t>https://www.kof.ethz.ch/services/daten/data-on-central-bank-governors.html</t>
+  </si>
+  <si>
+    <t>https://www.ethz.ch/content/dam/ethz/special-interest/dual/kof-dam/documents/central_bank_governors/cbg_turnover.xlsx</t>
   </si>
 </sst>
 </file>
@@ -1515,10 +1536,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q143"/>
+  <dimension ref="A1:Q145"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1987,7 +2008,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>107</v>
       </c>
@@ -2001,7 +2022,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>123</v>
       </c>
@@ -2015,7 +2036,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>306</v>
       </c>
@@ -2038,7 +2059,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>32</v>
       </c>
@@ -2055,223 +2076,229 @@
         <v>2008</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
+        <v>387</v>
+      </c>
+      <c r="B21" t="s">
+        <v>124</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>388</v>
+      </c>
+      <c r="E21" t="s">
+        <v>14</v>
+      </c>
+      <c r="F21">
+        <v>1970</v>
+      </c>
+      <c r="H21" t="s">
+        <v>348</v>
+      </c>
+      <c r="I21" t="s">
+        <v>349</v>
+      </c>
+      <c r="N21" s="2" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
         <v>146</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B22" t="s">
         <v>128</v>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="C22" s="2" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
         <v>127</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B23" t="s">
         <v>259</v>
       </c>
-      <c r="C22" s="2" t="s">
+      <c r="C23" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="I22" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
+      <c r="I23" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
         <v>173</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B24" t="s">
         <v>128</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>174</v>
-      </c>
-      <c r="B24" t="s">
-        <v>86</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="E24" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="B25" t="s">
-        <v>25</v>
+        <v>86</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>175</v>
       </c>
       <c r="E25" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>177</v>
+      </c>
+      <c r="B26" t="s">
+        <v>25</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="E26" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
         <v>135</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B27" t="s">
         <v>134</v>
       </c>
-      <c r="C26" s="2" t="s">
+      <c r="C27" s="2" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
         <v>184</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B28" t="s">
         <v>128</v>
       </c>
-      <c r="C27" s="2" t="s">
+      <c r="C28" s="2" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
         <v>54</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B29" t="s">
         <v>55</v>
       </c>
-      <c r="C28" s="2" t="s">
+      <c r="C29" s="2" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A29" s="1" t="s">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A30" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B30" t="s">
         <v>25</v>
       </c>
-      <c r="C29" s="2" t="s">
+      <c r="C30" s="2" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
         <v>158</v>
-      </c>
-      <c r="B30" t="s">
-        <v>99</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
-        <v>187</v>
       </c>
       <c r="B31" t="s">
         <v>99</v>
       </c>
       <c r="C31" s="2" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>187</v>
+      </c>
+      <c r="B32" t="s">
+        <v>99</v>
+      </c>
+      <c r="C32" s="2" t="s">
         <v>188</v>
       </c>
-      <c r="F31">
+      <c r="F32">
         <v>1960</v>
       </c>
-      <c r="G31">
+      <c r="G32">
         <v>2011</v>
       </c>
-      <c r="H31" t="s">
-        <v>16</v>
-      </c>
-      <c r="I31" t="s">
+      <c r="H32" t="s">
+        <v>16</v>
+      </c>
+      <c r="I32" t="s">
         <v>189</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
-        <v>164</v>
-      </c>
-      <c r="B32" t="s">
-        <v>165</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>371</v>
+        <v>164</v>
       </c>
       <c r="B33" t="s">
-        <v>25</v>
+        <v>165</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>372</v>
-      </c>
-      <c r="D33" t="s">
-        <v>363</v>
-      </c>
-      <c r="E33" t="s">
-        <v>34</v>
-      </c>
-      <c r="F33">
-        <v>2006</v>
-      </c>
-      <c r="H33" t="s">
-        <v>348</v>
-      </c>
-      <c r="I33" t="s">
-        <v>349</v>
+        <v>166</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>39</v>
+        <v>371</v>
       </c>
       <c r="B34" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>41</v>
+        <v>372</v>
+      </c>
+      <c r="D34" t="s">
+        <v>363</v>
       </c>
       <c r="E34" t="s">
-        <v>14</v>
+        <v>34</v>
       </c>
       <c r="F34">
-        <v>1816</v>
-      </c>
-      <c r="G34">
-        <v>2007</v>
+        <v>2006</v>
       </c>
       <c r="H34" t="s">
-        <v>16</v>
+        <v>348</v>
       </c>
       <c r="I34" t="s">
-        <v>20</v>
+        <v>349</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>215</v>
+        <v>39</v>
       </c>
       <c r="B35" t="s">
-        <v>237</v>
+        <v>40</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>214</v>
+        <v>41</v>
+      </c>
+      <c r="E35" t="s">
+        <v>14</v>
       </c>
       <c r="F35">
-        <v>1995</v>
+        <v>1816</v>
+      </c>
+      <c r="G35">
+        <v>2007</v>
       </c>
       <c r="H35" t="s">
         <v>16</v>
@@ -2282,19 +2309,16 @@
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>330</v>
+        <v>215</v>
       </c>
       <c r="B36" t="s">
-        <v>165</v>
+        <v>237</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>331</v>
-      </c>
-      <c r="E36" t="s">
-        <v>77</v>
+        <v>214</v>
       </c>
       <c r="F36">
-        <v>1953</v>
+        <v>1995</v>
       </c>
       <c r="H36" t="s">
         <v>16</v>
@@ -2305,107 +2329,107 @@
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>75</v>
+        <v>330</v>
       </c>
       <c r="B37" t="s">
-        <v>25</v>
+        <v>165</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>76</v>
+        <v>331</v>
       </c>
       <c r="E37" t="s">
         <v>77</v>
       </c>
       <c r="F37">
-        <v>1971</v>
+        <v>1953</v>
+      </c>
+      <c r="H37" t="s">
+        <v>16</v>
+      </c>
+      <c r="I37" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>197</v>
+        <v>75</v>
       </c>
       <c r="B38" t="s">
-        <v>55</v>
+        <v>25</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>198</v>
+        <v>76</v>
       </c>
       <c r="E38" t="s">
-        <v>199</v>
+        <v>77</v>
       </c>
       <c r="F38">
-        <v>1975</v>
-      </c>
-      <c r="G38">
-        <v>2015</v>
-      </c>
-      <c r="H38" t="s">
-        <v>16</v>
-      </c>
-      <c r="I38" t="s">
-        <v>20</v>
+        <v>1971</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>59</v>
+        <v>197</v>
       </c>
       <c r="B39" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>61</v>
+        <v>198</v>
+      </c>
+      <c r="E39" t="s">
+        <v>199</v>
+      </c>
+      <c r="F39">
+        <v>1975</v>
+      </c>
+      <c r="G39">
+        <v>2015</v>
+      </c>
+      <c r="H39" t="s">
+        <v>16</v>
+      </c>
+      <c r="I39" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>196</v>
+        <v>59</v>
       </c>
       <c r="B40" t="s">
-        <v>165</v>
+        <v>60</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>195</v>
-      </c>
-      <c r="F40">
-        <v>1946</v>
-      </c>
-      <c r="G40">
-        <v>2016</v>
+        <v>61</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>238</v>
+        <v>196</v>
       </c>
       <c r="B41" t="s">
-        <v>237</v>
+        <v>165</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>243</v>
-      </c>
-      <c r="H41" t="s">
-        <v>16</v>
-      </c>
-      <c r="I41" t="s">
-        <v>20</v>
+        <v>195</v>
+      </c>
+      <c r="F41">
+        <v>1946</v>
+      </c>
+      <c r="G41">
+        <v>2016</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>219</v>
+        <v>238</v>
       </c>
       <c r="B42" t="s">
-        <v>124</v>
+        <v>237</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>218</v>
-      </c>
-      <c r="F42">
-        <v>1970</v>
-      </c>
-      <c r="G42">
-        <v>2015</v>
+        <v>243</v>
       </c>
       <c r="H42" t="s">
         <v>16</v>
@@ -2416,44 +2440,50 @@
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>191</v>
+        <v>219</v>
       </c>
       <c r="B43" t="s">
-        <v>25</v>
+        <v>124</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="E43" t="s">
-        <v>192</v>
+        <v>218</v>
+      </c>
+      <c r="F43">
+        <v>1970</v>
+      </c>
+      <c r="G43">
+        <v>2015</v>
+      </c>
+      <c r="H43" t="s">
+        <v>16</v>
+      </c>
+      <c r="I43" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>235</v>
+        <v>191</v>
       </c>
       <c r="B44" t="s">
-        <v>60</v>
+        <v>25</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>236</v>
-      </c>
-      <c r="H44" t="s">
-        <v>16</v>
-      </c>
-      <c r="I44" t="s">
-        <v>20</v>
+        <v>190</v>
+      </c>
+      <c r="E44" t="s">
+        <v>192</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>252</v>
+        <v>235</v>
       </c>
       <c r="B45" t="s">
-        <v>250</v>
+        <v>60</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>251</v>
+        <v>236</v>
       </c>
       <c r="H45" t="s">
         <v>16</v>
@@ -2464,91 +2494,91 @@
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>149</v>
+        <v>252</v>
       </c>
       <c r="B46" t="s">
-        <v>128</v>
+        <v>250</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>150</v>
+        <v>251</v>
+      </c>
+      <c r="H46" t="s">
+        <v>16</v>
+      </c>
+      <c r="I46" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>28</v>
+        <v>149</v>
       </c>
       <c r="B47" t="s">
-        <v>25</v>
+        <v>128</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>48</v>
+        <v>150</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>80</v>
+        <v>28</v>
       </c>
       <c r="B48" t="s">
-        <v>128</v>
+        <v>25</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="E48" t="s">
-        <v>9</v>
-      </c>
-      <c r="F48">
-        <v>1979</v>
+        <v>48</v>
       </c>
     </row>
     <row r="49" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>125</v>
+        <v>80</v>
       </c>
       <c r="B49" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>126</v>
+        <v>81</v>
+      </c>
+      <c r="E49" t="s">
+        <v>9</v>
+      </c>
+      <c r="F49">
+        <v>1979</v>
       </c>
     </row>
     <row r="50" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>179</v>
+        <v>125</v>
       </c>
       <c r="B50" t="s">
-        <v>165</v>
+        <v>124</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>180</v>
+        <v>126</v>
       </c>
     </row>
     <row r="51" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
+        <v>179</v>
+      </c>
+      <c r="B51" t="s">
+        <v>165</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="52" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
         <v>78</v>
       </c>
-      <c r="B51" t="s">
+      <c r="B52" t="s">
         <v>25</v>
       </c>
-      <c r="C51" s="2" t="s">
+      <c r="C52" s="2" t="s">
         <v>79</v>
-      </c>
-      <c r="E51" t="s">
-        <v>9</v>
-      </c>
-      <c r="F51">
-        <v>1979</v>
-      </c>
-    </row>
-    <row r="52" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A52" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="B52" t="s">
-        <v>83</v>
-      </c>
-      <c r="C52" s="2" t="s">
-        <v>84</v>
       </c>
       <c r="E52" t="s">
         <v>9</v>
@@ -2559,13 +2589,13 @@
     </row>
     <row r="53" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A53" s="3" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B53" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="E53" t="s">
         <v>9</v>
@@ -2573,144 +2603,138 @@
       <c r="F53">
         <v>1979</v>
       </c>
-      <c r="G53">
+    </row>
+    <row r="54" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A54" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="B54" t="s">
+        <v>86</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="E54" t="s">
+        <v>9</v>
+      </c>
+      <c r="F54">
+        <v>1979</v>
+      </c>
+      <c r="G54">
         <v>2009</v>
-      </c>
-    </row>
-    <row r="54" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A54" t="s">
-        <v>27</v>
-      </c>
-      <c r="B54" t="s">
-        <v>25</v>
-      </c>
-      <c r="C54" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="Q54" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="55" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>120</v>
+        <v>27</v>
       </c>
       <c r="B55" t="s">
-        <v>259</v>
+        <v>25</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="I55" t="s">
-        <v>20</v>
+        <v>49</v>
+      </c>
+      <c r="Q55" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="56" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>5</v>
+        <v>120</v>
       </c>
       <c r="B56" t="s">
-        <v>25</v>
+        <v>259</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D56" t="s">
-        <v>94</v>
-      </c>
-      <c r="E56" t="s">
-        <v>9</v>
-      </c>
-      <c r="F56">
-        <v>2002</v>
-      </c>
-      <c r="H56" t="s">
-        <v>16</v>
+        <v>119</v>
       </c>
       <c r="I56" t="s">
-        <v>248</v>
-      </c>
-      <c r="Q56" t="s">
-        <v>44</v>
+        <v>20</v>
       </c>
     </row>
     <row r="57" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
+        <v>5</v>
+      </c>
+      <c r="B57" t="s">
+        <v>25</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D57" t="s">
+        <v>94</v>
+      </c>
+      <c r="E57" t="s">
+        <v>9</v>
+      </c>
+      <c r="F57">
+        <v>2002</v>
+      </c>
+      <c r="H57" t="s">
+        <v>16</v>
+      </c>
+      <c r="I57" t="s">
+        <v>248</v>
+      </c>
+      <c r="Q57" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="58" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
         <v>240</v>
       </c>
-      <c r="B57" t="s">
+      <c r="B58" t="s">
         <v>237</v>
       </c>
-      <c r="C57" s="2" t="s">
+      <c r="C58" s="2" t="s">
         <v>243</v>
       </c>
-      <c r="H57" t="s">
-        <v>16</v>
-      </c>
-      <c r="I57" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="58" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A58" s="1" t="s">
+      <c r="H58" t="s">
+        <v>16</v>
+      </c>
+      <c r="I58" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="59" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A59" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B58" t="s">
+      <c r="B59" t="s">
         <v>25</v>
       </c>
-      <c r="C58" s="2" t="s">
+      <c r="C59" s="2" t="s">
         <v>52</v>
-      </c>
-    </row>
-    <row r="59" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A59" t="s">
-        <v>232</v>
-      </c>
-      <c r="B59" t="s">
-        <v>250</v>
-      </c>
-      <c r="C59" s="2" t="s">
-        <v>231</v>
       </c>
     </row>
     <row r="60" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>276</v>
+        <v>232</v>
       </c>
       <c r="B60" t="s">
-        <v>124</v>
+        <v>250</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>277</v>
-      </c>
-      <c r="F60">
-        <v>1948</v>
-      </c>
-      <c r="G60">
-        <v>2000</v>
-      </c>
-      <c r="H60" t="s">
-        <v>16</v>
-      </c>
-      <c r="I60" t="s">
-        <v>20</v>
+        <v>231</v>
       </c>
     </row>
     <row r="61" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>224</v>
+        <v>276</v>
       </c>
       <c r="B61" t="s">
-        <v>40</v>
+        <v>124</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>225</v>
+        <v>277</v>
       </c>
       <c r="F61">
-        <v>1964</v>
+        <v>1948</v>
       </c>
       <c r="G61">
-        <v>2008</v>
+        <v>2000</v>
       </c>
       <c r="H61" t="s">
         <v>16</v>
@@ -2721,13 +2745,19 @@
     </row>
     <row r="62" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>285</v>
+        <v>224</v>
       </c>
       <c r="B62" t="s">
-        <v>250</v>
+        <v>40</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>286</v>
+        <v>225</v>
+      </c>
+      <c r="F62">
+        <v>1964</v>
+      </c>
+      <c r="G62">
+        <v>2008</v>
       </c>
       <c r="H62" t="s">
         <v>16</v>
@@ -2738,166 +2768,166 @@
     </row>
     <row r="63" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>205</v>
+        <v>285</v>
       </c>
       <c r="B63" t="s">
-        <v>40</v>
+        <v>250</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>204</v>
-      </c>
-      <c r="F63">
-        <v>2006</v>
+        <v>286</v>
+      </c>
+      <c r="H63" t="s">
+        <v>16</v>
+      </c>
+      <c r="I63" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="64" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>200</v>
+        <v>205</v>
       </c>
       <c r="B64" t="s">
-        <v>99</v>
+        <v>40</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="F64">
-        <v>1980</v>
-      </c>
-      <c r="G64">
-        <v>2007</v>
-      </c>
-      <c r="Q64" t="s">
-        <v>18</v>
+        <v>2006</v>
       </c>
     </row>
     <row r="65" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>89</v>
+        <v>200</v>
       </c>
       <c r="B65" t="s">
-        <v>25</v>
+        <v>99</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="E65" t="s">
-        <v>34</v>
+        <v>201</v>
       </c>
       <c r="F65">
-        <v>1972</v>
-      </c>
-      <c r="H65" t="s">
-        <v>16</v>
-      </c>
-      <c r="I65" t="s">
-        <v>20</v>
+        <v>1980</v>
+      </c>
+      <c r="G65">
+        <v>2007</v>
+      </c>
+      <c r="Q65" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="66" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>104</v>
+        <v>89</v>
       </c>
       <c r="B66" t="s">
         <v>25</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>106</v>
+        <v>88</v>
       </c>
       <c r="E66" t="s">
-        <v>105</v>
+        <v>34</v>
       </c>
       <c r="F66">
-        <v>1980</v>
+        <v>1972</v>
+      </c>
+      <c r="H66" t="s">
+        <v>16</v>
+      </c>
+      <c r="I66" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="67" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>62</v>
+        <v>104</v>
       </c>
       <c r="B67" t="s">
         <v>25</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>63</v>
+        <v>106</v>
+      </c>
+      <c r="E67" t="s">
+        <v>105</v>
+      </c>
+      <c r="F67">
+        <v>1980</v>
       </c>
     </row>
     <row r="68" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>311</v>
+        <v>62</v>
       </c>
       <c r="B68" t="s">
-        <v>165</v>
+        <v>25</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>312</v>
-      </c>
-      <c r="E68" t="s">
-        <v>14</v>
-      </c>
-      <c r="H68" t="s">
-        <v>16</v>
-      </c>
-      <c r="I68" t="s">
-        <v>301</v>
+        <v>63</v>
       </c>
     </row>
     <row r="69" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>281</v>
+        <v>311</v>
       </c>
       <c r="B69" t="s">
-        <v>237</v>
+        <v>165</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>282</v>
+        <v>312</v>
+      </c>
+      <c r="E69" t="s">
+        <v>14</v>
       </c>
       <c r="H69" t="s">
         <v>16</v>
       </c>
       <c r="I69" t="s">
-        <v>20</v>
+        <v>301</v>
       </c>
     </row>
     <row r="70" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>151</v>
+        <v>281</v>
       </c>
       <c r="B70" t="s">
-        <v>40</v>
+        <v>237</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="E70" t="s">
-        <v>14</v>
+        <v>282</v>
+      </c>
+      <c r="H70" t="s">
+        <v>16</v>
+      </c>
+      <c r="I70" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="71" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>242</v>
+        <v>151</v>
       </c>
       <c r="B71" t="s">
-        <v>237</v>
+        <v>40</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>243</v>
-      </c>
-      <c r="H71" t="s">
-        <v>16</v>
-      </c>
-      <c r="I71" t="s">
-        <v>20</v>
+        <v>152</v>
+      </c>
+      <c r="E71" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="72" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>292</v>
+        <v>242</v>
       </c>
       <c r="B72" t="s">
-        <v>99</v>
+        <v>237</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>291</v>
+        <v>243</v>
       </c>
       <c r="H72" t="s">
         <v>16</v>
@@ -2908,47 +2938,47 @@
     </row>
     <row r="73" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>153</v>
+        <v>292</v>
       </c>
       <c r="B73" t="s">
-        <v>259</v>
+        <v>99</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>154</v>
+        <v>291</v>
+      </c>
+      <c r="H73" t="s">
+        <v>16</v>
+      </c>
+      <c r="I73" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="74" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>228</v>
+        <v>153</v>
       </c>
       <c r="B74" t="s">
-        <v>40</v>
+        <v>259</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>225</v>
-      </c>
-      <c r="F74">
-        <v>1989</v>
-      </c>
-      <c r="G74">
-        <v>2017</v>
-      </c>
-      <c r="H74" t="s">
-        <v>16</v>
-      </c>
-      <c r="I74" t="s">
-        <v>20</v>
+        <v>154</v>
       </c>
     </row>
     <row r="75" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>245</v>
+        <v>228</v>
       </c>
       <c r="B75" t="s">
-        <v>237</v>
+        <v>40</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>244</v>
+        <v>225</v>
+      </c>
+      <c r="F75">
+        <v>1989</v>
+      </c>
+      <c r="G75">
+        <v>2017</v>
       </c>
       <c r="H75" t="s">
         <v>16</v>
@@ -2959,50 +2989,41 @@
     </row>
     <row r="76" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>100</v>
+        <v>245</v>
       </c>
       <c r="B76" t="s">
-        <v>99</v>
+        <v>237</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>101</v>
+        <v>244</v>
+      </c>
+      <c r="H76" t="s">
+        <v>16</v>
+      </c>
+      <c r="I76" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="77" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>239</v>
+        <v>100</v>
       </c>
       <c r="B77" t="s">
-        <v>237</v>
+        <v>99</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>243</v>
-      </c>
-      <c r="H77" t="s">
-        <v>16</v>
-      </c>
-      <c r="I77" t="s">
-        <v>20</v>
+        <v>101</v>
       </c>
     </row>
     <row r="78" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>254</v>
+        <v>239</v>
       </c>
       <c r="B78" t="s">
-        <v>55</v>
+        <v>237</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>253</v>
-      </c>
-      <c r="E78" t="s">
-        <v>255</v>
-      </c>
-      <c r="F78">
-        <v>1960</v>
-      </c>
-      <c r="G78">
-        <v>2014</v>
+        <v>243</v>
       </c>
       <c r="H78" t="s">
         <v>16</v>
@@ -3013,19 +3034,22 @@
     </row>
     <row r="79" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>270</v>
+        <v>254</v>
       </c>
       <c r="B79" t="s">
         <v>55</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>271</v>
+        <v>253</v>
+      </c>
+      <c r="E79" t="s">
+        <v>255</v>
       </c>
       <c r="F79">
-        <v>1990</v>
+        <v>1960</v>
       </c>
       <c r="G79">
-        <v>2010</v>
+        <v>2014</v>
       </c>
       <c r="H79" t="s">
         <v>16</v>
@@ -3036,504 +3060,501 @@
     </row>
     <row r="80" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>117</v>
+        <v>270</v>
       </c>
       <c r="B80" t="s">
         <v>55</v>
       </c>
       <c r="C80" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="F80">
+        <v>1990</v>
+      </c>
+      <c r="G80">
+        <v>2010</v>
+      </c>
+      <c r="H80" t="s">
+        <v>16</v>
+      </c>
+      <c r="I80" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="81" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A81" t="s">
+        <v>117</v>
+      </c>
+      <c r="B81" t="s">
+        <v>55</v>
+      </c>
+      <c r="C81" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="I80" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q80" t="s">
+      <c r="I81" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q81" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A81" s="1" t="s">
+    <row r="82" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A82" s="1" t="s">
         <v>23</v>
-      </c>
-      <c r="B81" t="s">
-        <v>25</v>
-      </c>
-      <c r="C81" s="2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A82" t="s">
-        <v>300</v>
       </c>
       <c r="B82" t="s">
         <v>25</v>
       </c>
       <c r="C82" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="83" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A83" t="s">
+        <v>300</v>
+      </c>
+      <c r="B83" t="s">
+        <v>25</v>
+      </c>
+      <c r="C83" s="2" t="s">
         <v>298</v>
       </c>
-      <c r="E82" t="s">
+      <c r="E83" t="s">
         <v>299</v>
       </c>
-      <c r="F82">
+      <c r="F83">
         <v>1969</v>
       </c>
-      <c r="H82" t="s">
-        <v>16</v>
-      </c>
-      <c r="I82" t="s">
+      <c r="H83" t="s">
+        <v>16</v>
+      </c>
+      <c r="I83" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A83" t="s">
+    <row r="84" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A84" t="s">
         <v>332</v>
       </c>
-      <c r="B83" t="s">
+      <c r="B84" t="s">
         <v>134</v>
       </c>
-      <c r="C83" s="2" t="s">
+      <c r="C84" s="2" t="s">
         <v>333</v>
       </c>
-      <c r="E83" t="s">
+      <c r="E84" t="s">
         <v>334</v>
       </c>
-      <c r="H83" t="s">
-        <v>16</v>
-      </c>
-      <c r="I83" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A84" t="s">
+      <c r="H84" t="s">
+        <v>16</v>
+      </c>
+      <c r="I84" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="85" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A85" t="s">
         <v>267</v>
       </c>
-      <c r="B84" t="s">
+      <c r="B85" t="s">
         <v>250</v>
       </c>
-      <c r="C84" s="2" t="s">
+      <c r="C85" s="2" t="s">
         <v>266</v>
       </c>
-      <c r="D84" t="s">
+      <c r="D85" t="s">
         <v>269</v>
       </c>
-      <c r="E84" t="s">
+      <c r="E85" t="s">
         <v>268</v>
       </c>
-      <c r="F84">
+      <c r="F85">
         <v>1970</v>
       </c>
-      <c r="G84">
+      <c r="G85">
         <v>2014</v>
       </c>
-      <c r="H84" t="s">
-        <v>16</v>
-      </c>
-      <c r="I84" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A85" t="s">
+      <c r="H85" t="s">
+        <v>16</v>
+      </c>
+      <c r="I85" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="86" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A86" t="s">
         <v>96</v>
-      </c>
-      <c r="B85" t="s">
-        <v>25</v>
-      </c>
-      <c r="C85" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="E85" t="s">
-        <v>69</v>
-      </c>
-      <c r="F85">
-        <v>1995</v>
-      </c>
-    </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A86" t="s">
-        <v>11</v>
       </c>
       <c r="B86" t="s">
         <v>25</v>
       </c>
       <c r="C86" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="E86" t="s">
+        <v>69</v>
+      </c>
+      <c r="F86">
+        <v>1995</v>
+      </c>
+    </row>
+    <row r="87" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A87" t="s">
+        <v>11</v>
+      </c>
+      <c r="B87" t="s">
+        <v>25</v>
+      </c>
+      <c r="C87" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D86" t="s">
+      <c r="D87" t="s">
         <v>95</v>
       </c>
-      <c r="E86" t="s">
+      <c r="E87" t="s">
         <v>10</v>
       </c>
-      <c r="F86">
+      <c r="F87">
         <v>2007</v>
       </c>
-      <c r="H86" t="s">
-        <v>16</v>
-      </c>
-      <c r="I86" t="s">
+      <c r="H87" t="s">
+        <v>16</v>
+      </c>
+      <c r="I87" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A87" t="s">
+    <row r="88" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A88" t="s">
         <v>223</v>
       </c>
-      <c r="B87" t="s">
+      <c r="B88" t="s">
         <v>124</v>
       </c>
-      <c r="C87" s="2" t="s">
+      <c r="C88" s="2" t="s">
         <v>222</v>
       </c>
-      <c r="F87">
+      <c r="F88">
         <v>1</v>
       </c>
-      <c r="G87">
+      <c r="G88">
         <v>2010</v>
       </c>
-      <c r="H87" t="s">
-        <v>16</v>
-      </c>
-      <c r="I87" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A88" t="s">
+      <c r="H88" t="s">
+        <v>16</v>
+      </c>
+      <c r="I88" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="89" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A89" t="s">
         <v>226</v>
       </c>
-      <c r="B88" t="s">
+      <c r="B89" t="s">
         <v>40</v>
       </c>
-      <c r="C88" s="2" t="s">
+      <c r="C89" s="2" t="s">
         <v>225</v>
       </c>
-      <c r="F88">
+      <c r="F89">
         <v>1946</v>
       </c>
-      <c r="G88">
+      <c r="G89">
         <v>2016</v>
       </c>
-      <c r="H88" t="s">
-        <v>16</v>
-      </c>
-      <c r="I88" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A89" t="s">
+      <c r="H89" t="s">
+        <v>16</v>
+      </c>
+      <c r="I89" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="90" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A90" t="s">
         <v>97</v>
       </c>
-      <c r="B89" t="s">
+      <c r="B90" t="s">
         <v>128</v>
       </c>
-      <c r="C89" s="2" t="s">
+      <c r="C90" s="2" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A90" t="s">
+    <row r="91" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A91" t="s">
         <v>278</v>
       </c>
-      <c r="B90" t="s">
+      <c r="B91" t="s">
         <v>124</v>
       </c>
-      <c r="C90" s="2" t="s">
+      <c r="C91" s="2" t="s">
         <v>279</v>
       </c>
-      <c r="E90" t="s">
+      <c r="E91" t="s">
         <v>280</v>
       </c>
-      <c r="F90">
+      <c r="F91">
         <v>1890</v>
       </c>
-      <c r="G90">
+      <c r="G91">
         <v>1996</v>
       </c>
-      <c r="H90" t="s">
-        <v>16</v>
-      </c>
-      <c r="I90" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A91" t="s">
+      <c r="H91" t="s">
+        <v>16</v>
+      </c>
+      <c r="I91" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="92" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A92" t="s">
         <v>156</v>
       </c>
-      <c r="B91" t="s">
+      <c r="B92" t="s">
         <v>25</v>
       </c>
-      <c r="C91" s="2" t="s">
+      <c r="C92" s="2" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A92" t="s">
+    <row r="93" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A93" t="s">
         <v>229</v>
-      </c>
-      <c r="B92" t="s">
-        <v>40</v>
-      </c>
-      <c r="C92" s="2" t="s">
-        <v>225</v>
-      </c>
-      <c r="F92">
-        <v>1952</v>
-      </c>
-      <c r="G92">
-        <v>1997</v>
-      </c>
-      <c r="H92" t="s">
-        <v>16</v>
-      </c>
-      <c r="I92" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A93" t="s">
-        <v>293</v>
       </c>
       <c r="B93" t="s">
         <v>40</v>
       </c>
       <c r="C93" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="F93">
+        <v>1952</v>
+      </c>
+      <c r="G93">
+        <v>1997</v>
+      </c>
+      <c r="H93" t="s">
+        <v>16</v>
+      </c>
+      <c r="I93" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="94" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A94" t="s">
+        <v>293</v>
+      </c>
+      <c r="B94" t="s">
+        <v>40</v>
+      </c>
+      <c r="C94" s="2" t="s">
         <v>294</v>
       </c>
-      <c r="F93">
+      <c r="F94">
         <v>2004</v>
       </c>
-      <c r="G93">
+      <c r="G94">
         <v>2006</v>
       </c>
-      <c r="H93" t="s">
-        <v>16</v>
-      </c>
-      <c r="I93" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A94" t="s">
+      <c r="H94" t="s">
+        <v>16</v>
+      </c>
+      <c r="I94" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="95" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A95" t="s">
         <v>102</v>
       </c>
-      <c r="B94" t="s">
+      <c r="B95" t="s">
         <v>99</v>
       </c>
-      <c r="C94" s="2" t="s">
+      <c r="C95" s="2" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A95" t="s">
+    <row r="96" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A96" t="s">
         <v>289</v>
       </c>
-      <c r="B95" t="s">
+      <c r="B96" t="s">
         <v>124</v>
       </c>
-      <c r="C95" s="2" t="s">
+      <c r="C96" s="2" t="s">
         <v>290</v>
-      </c>
-    </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A96" t="s">
-        <v>246</v>
-      </c>
-      <c r="B96" t="s">
-        <v>165</v>
-      </c>
-      <c r="C96" s="2" t="s">
-        <v>247</v>
-      </c>
-      <c r="E96" t="s">
-        <v>14</v>
-      </c>
-      <c r="F96">
-        <v>1960</v>
-      </c>
-      <c r="G96">
-        <v>2006</v>
-      </c>
-      <c r="H96" t="s">
-        <v>16</v>
-      </c>
-      <c r="I96" t="s">
-        <v>249</v>
       </c>
     </row>
     <row r="97" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>365</v>
+        <v>246</v>
       </c>
       <c r="B97" t="s">
-        <v>128</v>
+        <v>165</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>364</v>
-      </c>
-      <c r="D97" t="s">
-        <v>370</v>
+        <v>247</v>
       </c>
       <c r="E97" t="s">
-        <v>366</v>
+        <v>14</v>
       </c>
       <c r="F97">
-        <v>1906</v>
+        <v>1960</v>
       </c>
       <c r="G97">
-        <v>2013</v>
+        <v>2006</v>
       </c>
       <c r="H97" t="s">
-        <v>367</v>
+        <v>16</v>
       </c>
       <c r="I97" t="s">
-        <v>368</v>
-      </c>
-      <c r="Q97" t="s">
-        <v>369</v>
+        <v>249</v>
       </c>
     </row>
     <row r="98" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>208</v>
+        <v>365</v>
       </c>
       <c r="B98" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>209</v>
+        <v>364</v>
+      </c>
+      <c r="D98" t="s">
+        <v>370</v>
+      </c>
+      <c r="E98" t="s">
+        <v>366</v>
       </c>
       <c r="F98">
-        <v>1932</v>
+        <v>1906</v>
       </c>
       <c r="G98">
-        <v>2014</v>
+        <v>2013</v>
       </c>
       <c r="H98" t="s">
-        <v>16</v>
+        <v>367</v>
       </c>
       <c r="I98" t="s">
-        <v>20</v>
+        <v>368</v>
+      </c>
+      <c r="Q98" t="s">
+        <v>369</v>
       </c>
     </row>
     <row r="99" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>137</v>
+        <v>208</v>
       </c>
       <c r="B99" t="s">
-        <v>259</v>
+        <v>124</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>138</v>
+        <v>209</v>
+      </c>
+      <c r="F99">
+        <v>1932</v>
+      </c>
+      <c r="G99">
+        <v>2014</v>
+      </c>
+      <c r="H99" t="s">
+        <v>16</v>
+      </c>
+      <c r="I99" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="100" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>155</v>
+        <v>137</v>
       </c>
       <c r="B100" t="s">
         <v>259</v>
       </c>
       <c r="C100" s="2" t="s">
-        <v>154</v>
+        <v>138</v>
       </c>
     </row>
     <row r="101" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>57</v>
+        <v>155</v>
       </c>
       <c r="B101" t="s">
-        <v>128</v>
+        <v>259</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="Q101" t="s">
-        <v>17</v>
+        <v>154</v>
       </c>
     </row>
     <row r="102" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>129</v>
+        <v>57</v>
       </c>
       <c r="B102" t="s">
-        <v>259</v>
+        <v>128</v>
       </c>
       <c r="C102" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="E102" t="s">
-        <v>131</v>
-      </c>
-      <c r="F102">
-        <v>1945</v>
-      </c>
-      <c r="G102">
-        <v>2008</v>
-      </c>
-      <c r="I102" t="s">
-        <v>20</v>
+        <v>58</v>
+      </c>
+      <c r="Q102" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="103" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>148</v>
+        <v>129</v>
       </c>
       <c r="B103" t="s">
-        <v>128</v>
+        <v>259</v>
       </c>
       <c r="C103" s="2" t="s">
-        <v>147</v>
+        <v>130</v>
+      </c>
+      <c r="E103" t="s">
+        <v>131</v>
+      </c>
+      <c r="F103">
+        <v>1945</v>
+      </c>
+      <c r="G103">
+        <v>2008</v>
+      </c>
+      <c r="I103" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="104" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>233</v>
+        <v>148</v>
       </c>
       <c r="B104" t="s">
-        <v>165</v>
+        <v>128</v>
       </c>
       <c r="C104" s="2" t="s">
-        <v>234</v>
-      </c>
-      <c r="E104" t="s">
-        <v>14</v>
-      </c>
-      <c r="F104">
-        <v>2012</v>
-      </c>
-      <c r="G104">
-        <v>2016</v>
-      </c>
-      <c r="H104" t="s">
-        <v>16</v>
-      </c>
-      <c r="I104" t="s">
-        <v>20</v>
+        <v>147</v>
       </c>
     </row>
     <row r="105" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>35</v>
+        <v>233</v>
       </c>
       <c r="B105" t="s">
-        <v>25</v>
+        <v>165</v>
       </c>
       <c r="C105" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="D105" t="s">
-        <v>37</v>
+        <v>234</v>
       </c>
       <c r="E105" t="s">
         <v>14</v>
       </c>
       <c r="F105">
-        <v>2001</v>
+        <v>2012</v>
+      </c>
+      <c r="G105">
+        <v>2016</v>
       </c>
       <c r="H105" t="s">
         <v>16</v>
@@ -3544,90 +3565,90 @@
     </row>
     <row r="106" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>185</v>
+        <v>35</v>
       </c>
       <c r="B106" t="s">
-        <v>128</v>
+        <v>25</v>
       </c>
       <c r="C106" s="2" t="s">
-        <v>186</v>
+        <v>36</v>
+      </c>
+      <c r="D106" t="s">
+        <v>37</v>
+      </c>
+      <c r="E106" t="s">
+        <v>14</v>
+      </c>
+      <c r="F106">
+        <v>2001</v>
+      </c>
+      <c r="H106" t="s">
+        <v>16</v>
+      </c>
+      <c r="I106" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="107" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>210</v>
+        <v>185</v>
       </c>
       <c r="B107" t="s">
-        <v>40</v>
+        <v>128</v>
       </c>
       <c r="C107" s="2" t="s">
-        <v>211</v>
-      </c>
-      <c r="F107">
-        <v>1976</v>
-      </c>
-      <c r="G107">
-        <v>2016</v>
-      </c>
-      <c r="H107" t="s">
-        <v>16</v>
-      </c>
-      <c r="I107" t="s">
-        <v>20</v>
+        <v>186</v>
       </c>
     </row>
     <row r="108" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>144</v>
+        <v>210</v>
       </c>
       <c r="B108" t="s">
-        <v>60</v>
+        <v>40</v>
       </c>
       <c r="C108" s="2" t="s">
-        <v>143</v>
+        <v>211</v>
       </c>
       <c r="F108">
-        <v>1800</v>
+        <v>1976</v>
       </c>
       <c r="G108">
-        <v>2013</v>
+        <v>2016</v>
+      </c>
+      <c r="H108" t="s">
+        <v>16</v>
+      </c>
+      <c r="I108" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="109" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>122</v>
+        <v>144</v>
       </c>
       <c r="B109" t="s">
-        <v>259</v>
+        <v>60</v>
       </c>
       <c r="C109" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="I109" t="s">
-        <v>20</v>
+        <v>143</v>
+      </c>
+      <c r="F109">
+        <v>1800</v>
+      </c>
+      <c r="G109">
+        <v>2013</v>
       </c>
     </row>
     <row r="110" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>318</v>
+        <v>122</v>
       </c>
       <c r="B110" t="s">
-        <v>250</v>
+        <v>259</v>
       </c>
       <c r="C110" s="2" t="s">
-        <v>319</v>
-      </c>
-      <c r="E110" t="s">
-        <v>320</v>
-      </c>
-      <c r="F110">
-        <v>1975</v>
-      </c>
-      <c r="G110">
-        <v>1989</v>
-      </c>
-      <c r="H110" t="s">
-        <v>16</v>
+        <v>121</v>
       </c>
       <c r="I110" t="s">
         <v>20</v>
@@ -3635,22 +3656,22 @@
     </row>
     <row r="111" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="B111" t="s">
         <v>250</v>
       </c>
       <c r="C111" s="2" t="s">
-        <v>317</v>
+        <v>319</v>
       </c>
       <c r="E111" t="s">
-        <v>105</v>
+        <v>320</v>
       </c>
       <c r="F111">
-        <v>1950</v>
+        <v>1975</v>
       </c>
       <c r="G111">
-        <v>1996</v>
+        <v>1989</v>
       </c>
       <c r="H111" t="s">
         <v>16</v>
@@ -3661,19 +3682,22 @@
     </row>
     <row r="112" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>322</v>
+        <v>316</v>
       </c>
       <c r="B112" t="s">
-        <v>25</v>
+        <v>250</v>
       </c>
       <c r="C112" s="2" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="E112" t="s">
-        <v>77</v>
+        <v>105</v>
       </c>
       <c r="F112">
-        <v>2010</v>
+        <v>1950</v>
+      </c>
+      <c r="G112">
+        <v>1996</v>
       </c>
       <c r="H112" t="s">
         <v>16</v>
@@ -3684,164 +3708,164 @@
     </row>
     <row r="113" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>141</v>
+        <v>322</v>
       </c>
       <c r="B113" t="s">
-        <v>237</v>
+        <v>25</v>
       </c>
       <c r="C113" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="Q113" t="s">
-        <v>17</v>
+        <v>321</v>
+      </c>
+      <c r="E113" t="s">
+        <v>77</v>
+      </c>
+      <c r="F113">
+        <v>2010</v>
+      </c>
+      <c r="H113" t="s">
+        <v>16</v>
+      </c>
+      <c r="I113" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="114" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>308</v>
+        <v>141</v>
       </c>
       <c r="B114" t="s">
-        <v>250</v>
+        <v>237</v>
       </c>
       <c r="C114" s="2" t="s">
-        <v>309</v>
-      </c>
-      <c r="E114" t="s">
-        <v>310</v>
-      </c>
-      <c r="F114">
-        <v>1950</v>
-      </c>
-      <c r="G114">
-        <v>2010</v>
-      </c>
-      <c r="H114" t="s">
-        <v>16</v>
-      </c>
-      <c r="I114" t="s">
-        <v>20</v>
+        <v>142</v>
+      </c>
+      <c r="Q114" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="115" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>287</v>
+        <v>308</v>
       </c>
       <c r="B115" t="s">
-        <v>134</v>
+        <v>250</v>
       </c>
       <c r="C115" s="2" t="s">
-        <v>288</v>
+        <v>309</v>
+      </c>
+      <c r="E115" t="s">
+        <v>310</v>
       </c>
       <c r="F115">
-        <v>1990</v>
+        <v>1950</v>
       </c>
       <c r="G115">
-        <v>2008</v>
+        <v>2010</v>
+      </c>
+      <c r="H115" t="s">
+        <v>16</v>
+      </c>
+      <c r="I115" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="116" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>274</v>
+        <v>287</v>
       </c>
       <c r="B116" t="s">
-        <v>55</v>
+        <v>134</v>
       </c>
       <c r="C116" s="2" t="s">
-        <v>275</v>
-      </c>
-      <c r="H116" t="s">
-        <v>16</v>
-      </c>
-      <c r="I116" t="s">
-        <v>20</v>
+        <v>288</v>
+      </c>
+      <c r="F116">
+        <v>1990</v>
+      </c>
+      <c r="G116">
+        <v>2008</v>
       </c>
     </row>
     <row r="117" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>157</v>
+        <v>274</v>
       </c>
       <c r="B117" t="s">
-        <v>128</v>
+        <v>55</v>
       </c>
       <c r="C117" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="Q117" t="s">
-        <v>18</v>
+        <v>275</v>
+      </c>
+      <c r="H117" t="s">
+        <v>16</v>
+      </c>
+      <c r="I117" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="118" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>194</v>
+        <v>157</v>
       </c>
       <c r="B118" t="s">
-        <v>99</v>
+        <v>128</v>
       </c>
       <c r="C118" s="2" t="s">
-        <v>193</v>
+        <v>154</v>
+      </c>
+      <c r="Q118" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="119" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>295</v>
+        <v>194</v>
       </c>
       <c r="B119" t="s">
-        <v>40</v>
+        <v>99</v>
       </c>
       <c r="C119" s="2" t="s">
-        <v>296</v>
-      </c>
-      <c r="E119" t="s">
-        <v>297</v>
-      </c>
-      <c r="F119">
-        <v>1990</v>
-      </c>
-      <c r="G119">
-        <v>2015</v>
-      </c>
-      <c r="H119" t="s">
-        <v>16</v>
-      </c>
-      <c r="I119" t="s">
-        <v>249</v>
+        <v>193</v>
       </c>
     </row>
     <row r="120" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>256</v>
+        <v>295</v>
       </c>
       <c r="B120" t="s">
-        <v>250</v>
+        <v>40</v>
       </c>
       <c r="C120" s="2" t="s">
-        <v>257</v>
+        <v>296</v>
       </c>
       <c r="E120" t="s">
-        <v>258</v>
+        <v>297</v>
+      </c>
+      <c r="F120">
+        <v>1990</v>
+      </c>
+      <c r="G120">
+        <v>2015</v>
       </c>
       <c r="H120" t="s">
         <v>16</v>
       </c>
       <c r="I120" t="s">
-        <v>20</v>
+        <v>249</v>
       </c>
     </row>
     <row r="121" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>227</v>
+        <v>256</v>
       </c>
       <c r="B121" t="s">
-        <v>40</v>
+        <v>250</v>
       </c>
       <c r="C121" s="2" t="s">
-        <v>225</v>
-      </c>
-      <c r="F121">
-        <v>1955</v>
-      </c>
-      <c r="G121">
-        <v>2016</v>
+        <v>257</v>
+      </c>
+      <c r="E121" t="s">
+        <v>258</v>
       </c>
       <c r="H121" t="s">
         <v>16</v>
@@ -3852,7 +3876,7 @@
     </row>
     <row r="122" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="B122" t="s">
         <v>40</v>
@@ -3861,7 +3885,7 @@
         <v>225</v>
       </c>
       <c r="F122">
-        <v>1995</v>
+        <v>1955</v>
       </c>
       <c r="G122">
         <v>2016</v>
@@ -3875,141 +3899,141 @@
     </row>
     <row r="123" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>109</v>
+        <v>230</v>
       </c>
       <c r="B123" t="s">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="C123" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="E123" t="s">
-        <v>111</v>
+        <v>225</v>
       </c>
       <c r="F123">
-        <v>1956</v>
+        <v>1995</v>
+      </c>
+      <c r="G123">
+        <v>2016</v>
+      </c>
+      <c r="H123" t="s">
+        <v>16</v>
+      </c>
+      <c r="I123" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="124" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>326</v>
+        <v>109</v>
       </c>
       <c r="B124" t="s">
         <v>25</v>
       </c>
       <c r="C124" s="2" t="s">
-        <v>327</v>
+        <v>110</v>
       </c>
       <c r="E124" t="s">
         <v>111</v>
       </c>
       <c r="F124">
-        <v>1998</v>
-      </c>
-      <c r="H124" t="s">
-        <v>16</v>
-      </c>
-      <c r="I124" t="s">
-        <v>20</v>
+        <v>1956</v>
       </c>
     </row>
     <row r="125" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>91</v>
+        <v>326</v>
       </c>
       <c r="B125" t="s">
         <v>25</v>
       </c>
       <c r="C125" s="2" t="s">
-        <v>93</v>
+        <v>327</v>
       </c>
       <c r="E125" t="s">
-        <v>92</v>
+        <v>111</v>
       </c>
       <c r="F125">
-        <v>1999</v>
+        <v>1998</v>
+      </c>
+      <c r="H125" t="s">
+        <v>16</v>
+      </c>
+      <c r="I125" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="126" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>314</v>
+        <v>91</v>
       </c>
       <c r="B126" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="C126" s="2" t="s">
-        <v>313</v>
+        <v>93</v>
       </c>
       <c r="E126" t="s">
-        <v>315</v>
+        <v>92</v>
       </c>
       <c r="F126">
-        <v>1950</v>
-      </c>
-      <c r="G126">
-        <v>2004</v>
-      </c>
-      <c r="H126" t="s">
-        <v>16</v>
-      </c>
-      <c r="I126" t="s">
-        <v>20</v>
+        <v>1999</v>
       </c>
     </row>
     <row r="127" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>161</v>
+        <v>314</v>
       </c>
       <c r="B127" t="s">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="C127" s="2" t="s">
-        <v>160</v>
+        <v>313</v>
+      </c>
+      <c r="E127" t="s">
+        <v>315</v>
+      </c>
+      <c r="F127">
+        <v>1950</v>
+      </c>
+      <c r="G127">
+        <v>2004</v>
+      </c>
+      <c r="H127" t="s">
+        <v>16</v>
+      </c>
+      <c r="I127" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="128" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="B128" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="C128" s="2" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
     </row>
     <row r="129" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>213</v>
+        <v>168</v>
       </c>
       <c r="B129" t="s">
-        <v>55</v>
+        <v>40</v>
       </c>
       <c r="C129" s="2" t="s">
-        <v>212</v>
-      </c>
-      <c r="H129" t="s">
-        <v>16</v>
-      </c>
-      <c r="I129" t="s">
-        <v>20</v>
+        <v>167</v>
       </c>
     </row>
     <row r="130" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
-        <v>323</v>
+        <v>213</v>
       </c>
       <c r="B130" t="s">
-        <v>25</v>
+        <v>55</v>
       </c>
       <c r="C130" s="2" t="s">
-        <v>324</v>
-      </c>
-      <c r="E130" t="s">
-        <v>325</v>
-      </c>
-      <c r="F130">
-        <v>1942</v>
+        <v>212</v>
       </c>
       <c r="H130" t="s">
         <v>16</v>
@@ -4020,19 +4044,19 @@
     </row>
     <row r="131" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>273</v>
+        <v>323</v>
       </c>
       <c r="B131" t="s">
-        <v>237</v>
+        <v>25</v>
       </c>
       <c r="C131" s="2" t="s">
-        <v>272</v>
+        <v>324</v>
+      </c>
+      <c r="E131" t="s">
+        <v>325</v>
       </c>
       <c r="F131">
-        <v>1996</v>
-      </c>
-      <c r="G131">
-        <v>2016</v>
+        <v>1942</v>
       </c>
       <c r="H131" t="s">
         <v>16</v>
@@ -4043,75 +4067,90 @@
     </row>
     <row r="132" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>66</v>
+        <v>273</v>
       </c>
       <c r="B132" t="s">
-        <v>25</v>
+        <v>237</v>
       </c>
       <c r="C132" s="2" t="s">
-        <v>67</v>
+        <v>272</v>
+      </c>
+      <c r="F132">
+        <v>1996</v>
+      </c>
+      <c r="G132">
+        <v>2016</v>
+      </c>
+      <c r="H132" t="s">
+        <v>16</v>
+      </c>
+      <c r="I132" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="133" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
-        <v>139</v>
+        <v>66</v>
       </c>
       <c r="B133" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="C133" s="2" t="s">
-        <v>140</v>
+        <v>67</v>
       </c>
     </row>
     <row r="134" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
-        <v>329</v>
+        <v>383</v>
       </c>
       <c r="B134" t="s">
-        <v>165</v>
+        <v>40</v>
       </c>
       <c r="C134" s="2" t="s">
-        <v>328</v>
+        <v>384</v>
       </c>
       <c r="E134" t="s">
-        <v>34</v>
+        <v>386</v>
       </c>
       <c r="F134">
-        <v>1789</v>
+        <v>1951</v>
       </c>
       <c r="H134" t="s">
-        <v>16</v>
+        <v>348</v>
       </c>
       <c r="I134" t="s">
-        <v>20</v>
+        <v>349</v>
+      </c>
+      <c r="N134" s="2" t="s">
+        <v>385</v>
       </c>
     </row>
     <row r="135" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
-        <v>172</v>
+        <v>139</v>
       </c>
       <c r="B135" t="s">
-        <v>60</v>
+        <v>40</v>
       </c>
       <c r="C135" s="2" t="s">
-        <v>171</v>
+        <v>140</v>
       </c>
     </row>
     <row r="136" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
-        <v>217</v>
+        <v>329</v>
       </c>
       <c r="B136" t="s">
-        <v>60</v>
+        <v>165</v>
       </c>
       <c r="C136" s="2" t="s">
-        <v>216</v>
+        <v>328</v>
       </c>
       <c r="E136" t="s">
-        <v>14</v>
+        <v>34</v>
       </c>
       <c r="F136">
-        <v>1900</v>
+        <v>1789</v>
       </c>
       <c r="H136" t="s">
         <v>16</v>
@@ -4122,104 +4161,92 @@
     </row>
     <row r="137" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
-        <v>132</v>
+        <v>172</v>
       </c>
       <c r="B137" t="s">
-        <v>259</v>
+        <v>60</v>
       </c>
       <c r="C137" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="Q137" t="s">
-        <v>17</v>
+        <v>171</v>
       </c>
     </row>
     <row r="138" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
-        <v>182</v>
+        <v>217</v>
       </c>
       <c r="B138" t="s">
-        <v>165</v>
+        <v>60</v>
       </c>
       <c r="C138" s="2" t="s">
-        <v>181</v>
+        <v>216</v>
+      </c>
+      <c r="E138" t="s">
+        <v>14</v>
+      </c>
+      <c r="F138">
+        <v>1900</v>
+      </c>
+      <c r="H138" t="s">
+        <v>16</v>
+      </c>
+      <c r="I138" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="139" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
-        <v>115</v>
+        <v>132</v>
       </c>
       <c r="B139" t="s">
-        <v>128</v>
+        <v>259</v>
       </c>
       <c r="C139" s="2" t="s">
-        <v>116</v>
+        <v>133</v>
+      </c>
+      <c r="Q139" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="140" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
-        <v>263</v>
+        <v>182</v>
       </c>
       <c r="B140" t="s">
-        <v>250</v>
+        <v>165</v>
       </c>
       <c r="C140" s="2" t="s">
-        <v>264</v>
-      </c>
-      <c r="E140" t="s">
-        <v>265</v>
-      </c>
-      <c r="F140">
-        <v>1500</v>
-      </c>
-      <c r="G140">
-        <v>2000</v>
-      </c>
-      <c r="H140" t="s">
-        <v>16</v>
-      </c>
-      <c r="I140" t="s">
-        <v>20</v>
+        <v>181</v>
       </c>
     </row>
     <row r="141" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
-        <v>221</v>
+        <v>115</v>
       </c>
       <c r="B141" t="s">
-        <v>86</v>
+        <v>128</v>
       </c>
       <c r="C141" s="2" t="s">
-        <v>220</v>
-      </c>
-      <c r="F141">
-        <v>2013</v>
-      </c>
-      <c r="H141" t="s">
-        <v>16</v>
-      </c>
-      <c r="I141" t="s">
-        <v>20</v>
+        <v>116</v>
       </c>
     </row>
     <row r="142" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
-        <v>13</v>
+        <v>263</v>
       </c>
       <c r="B142" t="s">
-        <v>25</v>
+        <v>250</v>
       </c>
       <c r="C142" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="D142" s="1" t="s">
-        <v>42</v>
+        <v>264</v>
       </c>
       <c r="E142" t="s">
-        <v>14</v>
+        <v>265</v>
       </c>
       <c r="F142">
-        <v>1981</v>
+        <v>1500</v>
+      </c>
+      <c r="G142">
+        <v>2000</v>
       </c>
       <c r="H142" t="s">
         <v>16</v>
@@ -4230,166 +4257,212 @@
     </row>
     <row r="143" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
+        <v>221</v>
+      </c>
+      <c r="B143" t="s">
+        <v>86</v>
+      </c>
+      <c r="C143" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="F143">
+        <v>2013</v>
+      </c>
+      <c r="H143" t="s">
+        <v>16</v>
+      </c>
+      <c r="I143" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="144" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A144" t="s">
+        <v>13</v>
+      </c>
+      <c r="B144" t="s">
+        <v>25</v>
+      </c>
+      <c r="C144" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D144" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E144" t="s">
+        <v>14</v>
+      </c>
+      <c r="F144">
+        <v>1981</v>
+      </c>
+      <c r="H144" t="s">
+        <v>16</v>
+      </c>
+      <c r="I144" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="145" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A145" t="s">
         <v>283</v>
       </c>
-      <c r="B143" t="s">
+      <c r="B145" t="s">
         <v>124</v>
       </c>
-      <c r="C143" s="2" t="s">
+      <c r="C145" s="2" t="s">
         <v>284</v>
       </c>
-      <c r="H143" t="s">
-        <v>16</v>
-      </c>
-      <c r="I143" t="s">
+      <c r="H145" t="s">
+        <v>16</v>
+      </c>
+      <c r="I145" t="s">
         <v>20</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:Q143">
+  <sortState ref="A2:Q145">
     <sortCondition ref="A2"/>
   </sortState>
   <hyperlinks>
     <hyperlink ref="C6" r:id="rId1"/>
-    <hyperlink ref="C56" r:id="rId2"/>
+    <hyperlink ref="C57" r:id="rId2"/>
     <hyperlink ref="C7" r:id="rId3"/>
     <hyperlink ref="C10" r:id="rId4"/>
-    <hyperlink ref="C86" r:id="rId5"/>
-    <hyperlink ref="C105" r:id="rId6"/>
-    <hyperlink ref="C142" r:id="rId7"/>
-    <hyperlink ref="C34" r:id="rId8"/>
-    <hyperlink ref="C29" r:id="rId9"/>
-    <hyperlink ref="C47" r:id="rId10"/>
-    <hyperlink ref="C54" r:id="rId11"/>
+    <hyperlink ref="C87" r:id="rId5"/>
+    <hyperlink ref="C106" r:id="rId6"/>
+    <hyperlink ref="C144" r:id="rId7"/>
+    <hyperlink ref="C35" r:id="rId8"/>
+    <hyperlink ref="C30" r:id="rId9"/>
+    <hyperlink ref="C48" r:id="rId10"/>
+    <hyperlink ref="C55" r:id="rId11"/>
     <hyperlink ref="C3" r:id="rId12"/>
     <hyperlink ref="C20" r:id="rId13"/>
-    <hyperlink ref="C58" r:id="rId14"/>
-    <hyperlink ref="C81" r:id="rId15"/>
-    <hyperlink ref="C28" r:id="rId16"/>
-    <hyperlink ref="C101" r:id="rId17"/>
-    <hyperlink ref="C39" r:id="rId18"/>
-    <hyperlink ref="C67" r:id="rId19"/>
+    <hyperlink ref="C59" r:id="rId14"/>
+    <hyperlink ref="C82" r:id="rId15"/>
+    <hyperlink ref="C29" r:id="rId16"/>
+    <hyperlink ref="C102" r:id="rId17"/>
+    <hyperlink ref="C40" r:id="rId18"/>
+    <hyperlink ref="C68" r:id="rId19"/>
     <hyperlink ref="C16" r:id="rId20"/>
-    <hyperlink ref="C132" r:id="rId21"/>
+    <hyperlink ref="C133" r:id="rId21"/>
     <hyperlink ref="C8" r:id="rId22"/>
-    <hyperlink ref="C37" r:id="rId23"/>
-    <hyperlink ref="C51" r:id="rId24"/>
-    <hyperlink ref="C48" r:id="rId25"/>
-    <hyperlink ref="C52" r:id="rId26"/>
-    <hyperlink ref="C53" r:id="rId27"/>
-    <hyperlink ref="C65" r:id="rId28"/>
-    <hyperlink ref="C85" r:id="rId29"/>
-    <hyperlink ref="C125" r:id="rId30"/>
-    <hyperlink ref="C89" r:id="rId31"/>
-    <hyperlink ref="C76" r:id="rId32"/>
-    <hyperlink ref="C94" r:id="rId33"/>
-    <hyperlink ref="C66" r:id="rId34"/>
+    <hyperlink ref="C38" r:id="rId23"/>
+    <hyperlink ref="C52" r:id="rId24"/>
+    <hyperlink ref="C49" r:id="rId25"/>
+    <hyperlink ref="C53" r:id="rId26"/>
+    <hyperlink ref="C54" r:id="rId27"/>
+    <hyperlink ref="C66" r:id="rId28"/>
+    <hyperlink ref="C86" r:id="rId29"/>
+    <hyperlink ref="C126" r:id="rId30"/>
+    <hyperlink ref="C90" r:id="rId31"/>
+    <hyperlink ref="C77" r:id="rId32"/>
+    <hyperlink ref="C95" r:id="rId33"/>
+    <hyperlink ref="C67" r:id="rId34"/>
     <hyperlink ref="C17" r:id="rId35"/>
-    <hyperlink ref="C123" r:id="rId36"/>
+    <hyperlink ref="C124" r:id="rId36"/>
     <hyperlink ref="C15" r:id="rId37"/>
-    <hyperlink ref="C139" r:id="rId38"/>
-    <hyperlink ref="C80" r:id="rId39"/>
-    <hyperlink ref="C55" r:id="rId40"/>
-    <hyperlink ref="C109" r:id="rId41"/>
+    <hyperlink ref="C141" r:id="rId38"/>
+    <hyperlink ref="C81" r:id="rId39"/>
+    <hyperlink ref="C56" r:id="rId40"/>
+    <hyperlink ref="C110" r:id="rId41"/>
     <hyperlink ref="C18" r:id="rId42"/>
-    <hyperlink ref="C49" r:id="rId43"/>
-    <hyperlink ref="C22" r:id="rId44"/>
-    <hyperlink ref="C102" r:id="rId45"/>
-    <hyperlink ref="C137" r:id="rId46"/>
-    <hyperlink ref="C26" r:id="rId47" display="http://comparativeconstitutionsproject.org/"/>
-    <hyperlink ref="C99" r:id="rId48"/>
-    <hyperlink ref="C133" r:id="rId49"/>
-    <hyperlink ref="C113" r:id="rId50"/>
-    <hyperlink ref="C108" r:id="rId51"/>
-    <hyperlink ref="C21" r:id="rId52"/>
-    <hyperlink ref="C103" r:id="rId53"/>
-    <hyperlink ref="C46" r:id="rId54"/>
-    <hyperlink ref="C70" r:id="rId55"/>
-    <hyperlink ref="C73" r:id="rId56"/>
-    <hyperlink ref="C100" r:id="rId57"/>
-    <hyperlink ref="C91" r:id="rId58"/>
-    <hyperlink ref="C117" r:id="rId59"/>
-    <hyperlink ref="C30" r:id="rId60"/>
-    <hyperlink ref="C127" r:id="rId61"/>
+    <hyperlink ref="C50" r:id="rId43"/>
+    <hyperlink ref="C23" r:id="rId44"/>
+    <hyperlink ref="C103" r:id="rId45"/>
+    <hyperlink ref="C139" r:id="rId46"/>
+    <hyperlink ref="C27" r:id="rId47" display="http://comparativeconstitutionsproject.org/"/>
+    <hyperlink ref="C100" r:id="rId48"/>
+    <hyperlink ref="C135" r:id="rId49"/>
+    <hyperlink ref="C114" r:id="rId50"/>
+    <hyperlink ref="C109" r:id="rId51"/>
+    <hyperlink ref="C22" r:id="rId52"/>
+    <hyperlink ref="C104" r:id="rId53"/>
+    <hyperlink ref="C47" r:id="rId54"/>
+    <hyperlink ref="C71" r:id="rId55"/>
+    <hyperlink ref="C74" r:id="rId56"/>
+    <hyperlink ref="C101" r:id="rId57"/>
+    <hyperlink ref="C92" r:id="rId58"/>
+    <hyperlink ref="C118" r:id="rId59"/>
+    <hyperlink ref="C31" r:id="rId60"/>
+    <hyperlink ref="C128" r:id="rId61"/>
     <hyperlink ref="C9" r:id="rId62"/>
-    <hyperlink ref="C32" r:id="rId63"/>
-    <hyperlink ref="C128" r:id="rId64"/>
+    <hyperlink ref="C33" r:id="rId63"/>
+    <hyperlink ref="C129" r:id="rId64"/>
     <hyperlink ref="C14" r:id="rId65"/>
-    <hyperlink ref="C135" r:id="rId66"/>
-    <hyperlink ref="C24" r:id="rId67"/>
-    <hyperlink ref="C23" r:id="rId68"/>
-    <hyperlink ref="C25" r:id="rId69"/>
-    <hyperlink ref="C50" r:id="rId70"/>
-    <hyperlink ref="C138" r:id="rId71"/>
-    <hyperlink ref="C27" r:id="rId72"/>
-    <hyperlink ref="C106" r:id="rId73"/>
-    <hyperlink ref="C31" r:id="rId74"/>
-    <hyperlink ref="C43" r:id="rId75"/>
-    <hyperlink ref="C118" r:id="rId76"/>
-    <hyperlink ref="C40" r:id="rId77"/>
-    <hyperlink ref="C38" r:id="rId78"/>
-    <hyperlink ref="C64" r:id="rId79"/>
+    <hyperlink ref="C137" r:id="rId66"/>
+    <hyperlink ref="C25" r:id="rId67"/>
+    <hyperlink ref="C24" r:id="rId68"/>
+    <hyperlink ref="C26" r:id="rId69"/>
+    <hyperlink ref="C51" r:id="rId70"/>
+    <hyperlink ref="C140" r:id="rId71"/>
+    <hyperlink ref="C28" r:id="rId72"/>
+    <hyperlink ref="C107" r:id="rId73"/>
+    <hyperlink ref="C32" r:id="rId74"/>
+    <hyperlink ref="C44" r:id="rId75"/>
+    <hyperlink ref="C119" r:id="rId76"/>
+    <hyperlink ref="C41" r:id="rId77"/>
+    <hyperlink ref="C39" r:id="rId78"/>
+    <hyperlink ref="C65" r:id="rId79"/>
     <hyperlink ref="C5" r:id="rId80"/>
-    <hyperlink ref="C63" r:id="rId81"/>
+    <hyperlink ref="C64" r:id="rId81"/>
     <hyperlink ref="C12" r:id="rId82"/>
-    <hyperlink ref="C98" r:id="rId83"/>
-    <hyperlink ref="C107" r:id="rId84"/>
-    <hyperlink ref="C129" r:id="rId85"/>
-    <hyperlink ref="C35" r:id="rId86"/>
-    <hyperlink ref="C136" r:id="rId87"/>
-    <hyperlink ref="C42" r:id="rId88"/>
-    <hyperlink ref="C141" r:id="rId89"/>
-    <hyperlink ref="C87" r:id="rId90"/>
-    <hyperlink ref="C61" r:id="rId91"/>
-    <hyperlink ref="C88" r:id="rId92"/>
-    <hyperlink ref="C121" r:id="rId93"/>
-    <hyperlink ref="C74" r:id="rId94"/>
-    <hyperlink ref="C92" r:id="rId95"/>
-    <hyperlink ref="C122" r:id="rId96"/>
-    <hyperlink ref="C59" r:id="rId97"/>
-    <hyperlink ref="C104" r:id="rId98"/>
-    <hyperlink ref="C44" r:id="rId99"/>
-    <hyperlink ref="C41" r:id="rId100"/>
-    <hyperlink ref="C77" r:id="rId101"/>
-    <hyperlink ref="C57" r:id="rId102"/>
+    <hyperlink ref="C99" r:id="rId83"/>
+    <hyperlink ref="C108" r:id="rId84"/>
+    <hyperlink ref="C130" r:id="rId85"/>
+    <hyperlink ref="C36" r:id="rId86"/>
+    <hyperlink ref="C138" r:id="rId87"/>
+    <hyperlink ref="C43" r:id="rId88"/>
+    <hyperlink ref="C143" r:id="rId89"/>
+    <hyperlink ref="C88" r:id="rId90"/>
+    <hyperlink ref="C62" r:id="rId91"/>
+    <hyperlink ref="C89" r:id="rId92"/>
+    <hyperlink ref="C122" r:id="rId93"/>
+    <hyperlink ref="C75" r:id="rId94"/>
+    <hyperlink ref="C93" r:id="rId95"/>
+    <hyperlink ref="C123" r:id="rId96"/>
+    <hyperlink ref="C60" r:id="rId97"/>
+    <hyperlink ref="C105" r:id="rId98"/>
+    <hyperlink ref="C45" r:id="rId99"/>
+    <hyperlink ref="C42" r:id="rId100"/>
+    <hyperlink ref="C78" r:id="rId101"/>
+    <hyperlink ref="C58" r:id="rId102"/>
     <hyperlink ref="C2" r:id="rId103"/>
-    <hyperlink ref="C71" r:id="rId104"/>
-    <hyperlink ref="C75" r:id="rId105"/>
-    <hyperlink ref="C96" r:id="rId106"/>
-    <hyperlink ref="C45" r:id="rId107"/>
-    <hyperlink ref="C78" r:id="rId108"/>
-    <hyperlink ref="C120" r:id="rId109"/>
+    <hyperlink ref="C72" r:id="rId104"/>
+    <hyperlink ref="C76" r:id="rId105"/>
+    <hyperlink ref="C97" r:id="rId106"/>
+    <hyperlink ref="C46" r:id="rId107"/>
+    <hyperlink ref="C79" r:id="rId108"/>
+    <hyperlink ref="C121" r:id="rId109"/>
     <hyperlink ref="C13" r:id="rId110"/>
     <hyperlink ref="C4" r:id="rId111"/>
-    <hyperlink ref="C140" r:id="rId112"/>
-    <hyperlink ref="C84" r:id="rId113"/>
-    <hyperlink ref="C79" r:id="rId114"/>
-    <hyperlink ref="C131" r:id="rId115"/>
-    <hyperlink ref="C116" r:id="rId116"/>
-    <hyperlink ref="C60" r:id="rId117"/>
-    <hyperlink ref="C90" r:id="rId118"/>
-    <hyperlink ref="C69" r:id="rId119"/>
-    <hyperlink ref="C143" r:id="rId120"/>
-    <hyperlink ref="C62" r:id="rId121"/>
-    <hyperlink ref="C115" r:id="rId122"/>
-    <hyperlink ref="C95" r:id="rId123"/>
-    <hyperlink ref="C72" r:id="rId124"/>
-    <hyperlink ref="C93" r:id="rId125"/>
-    <hyperlink ref="C119" r:id="rId126"/>
-    <hyperlink ref="C82" r:id="rId127"/>
+    <hyperlink ref="C142" r:id="rId112"/>
+    <hyperlink ref="C85" r:id="rId113"/>
+    <hyperlink ref="C80" r:id="rId114"/>
+    <hyperlink ref="C132" r:id="rId115"/>
+    <hyperlink ref="C117" r:id="rId116"/>
+    <hyperlink ref="C61" r:id="rId117"/>
+    <hyperlink ref="C91" r:id="rId118"/>
+    <hyperlink ref="C70" r:id="rId119"/>
+    <hyperlink ref="C145" r:id="rId120"/>
+    <hyperlink ref="C63" r:id="rId121"/>
+    <hyperlink ref="C116" r:id="rId122"/>
+    <hyperlink ref="C96" r:id="rId123"/>
+    <hyperlink ref="C73" r:id="rId124"/>
+    <hyperlink ref="C94" r:id="rId125"/>
+    <hyperlink ref="C120" r:id="rId126"/>
+    <hyperlink ref="C83" r:id="rId127"/>
     <hyperlink ref="C11" r:id="rId128"/>
     <hyperlink ref="C19" r:id="rId129"/>
-    <hyperlink ref="C114" r:id="rId130"/>
-    <hyperlink ref="C68" r:id="rId131"/>
-    <hyperlink ref="C126" r:id="rId132"/>
-    <hyperlink ref="C111" r:id="rId133"/>
-    <hyperlink ref="C110" r:id="rId134"/>
-    <hyperlink ref="C112" r:id="rId135"/>
-    <hyperlink ref="C130" r:id="rId136"/>
-    <hyperlink ref="C124" r:id="rId137"/>
-    <hyperlink ref="C134" r:id="rId138"/>
-    <hyperlink ref="C36" r:id="rId139"/>
-    <hyperlink ref="C83" r:id="rId140"/>
+    <hyperlink ref="C115" r:id="rId130"/>
+    <hyperlink ref="C69" r:id="rId131"/>
+    <hyperlink ref="C127" r:id="rId132"/>
+    <hyperlink ref="C112" r:id="rId133"/>
+    <hyperlink ref="C111" r:id="rId134"/>
+    <hyperlink ref="C113" r:id="rId135"/>
+    <hyperlink ref="C131" r:id="rId136"/>
+    <hyperlink ref="C125" r:id="rId137"/>
+    <hyperlink ref="C136" r:id="rId138"/>
+    <hyperlink ref="C37" r:id="rId139"/>
+    <hyperlink ref="C84" r:id="rId140"/>
     <hyperlink ref="J2" r:id="rId141"/>
     <hyperlink ref="M3" r:id="rId142"/>
     <hyperlink ref="J3" r:id="rId143"/>
@@ -4397,13 +4470,17 @@
     <hyperlink ref="J4" r:id="rId145"/>
     <hyperlink ref="P5" r:id="rId146"/>
     <hyperlink ref="J5" r:id="rId147"/>
-    <hyperlink ref="C97" r:id="rId148"/>
-    <hyperlink ref="C33" r:id="rId149"/>
+    <hyperlink ref="C98" r:id="rId148"/>
+    <hyperlink ref="C34" r:id="rId149"/>
     <hyperlink ref="P7" r:id="rId150"/>
     <hyperlink ref="J7" r:id="rId151"/>
     <hyperlink ref="M8" r:id="rId152"/>
     <hyperlink ref="L8" r:id="rId153"/>
     <hyperlink ref="J8" r:id="rId154"/>
+    <hyperlink ref="C134" r:id="rId155"/>
+    <hyperlink ref="N134" r:id="rId156"/>
+    <hyperlink ref="C21" r:id="rId157"/>
+    <hyperlink ref="N21" r:id="rId158"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
add data, 'The SOM Institute Cumulative Dataset' and 'The Dyadic Cyber Incident and Dispute Data
</commit_message>
<xml_diff>
--- a/PolData.xlsx
+++ b/PolData.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="715" uniqueCount="394">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="731" uniqueCount="403">
   <si>
     <t>name</t>
   </si>
@@ -1209,6 +1209,33 @@
   </si>
   <si>
     <t>Text data on leader speeches in the European Union.</t>
+  </si>
+  <si>
+    <t>https://snd.gu.se/en/catalogue/study/snd0905</t>
+  </si>
+  <si>
+    <t>The SOM Institute Cumulative Dataset</t>
+  </si>
+  <si>
+    <t>General health and well-being, media, information society, employment, unemployment, environment and conservation, political behaviour and attitudes, elections, international politics and organisations, social welfare policy, leisure, tourism and sport, social behaviour and attitudes, cultural activities and participation, Political Science, Media and Communications</t>
+  </si>
+  <si>
+    <t>https://snd.gu.se/catalogue/file/5665</t>
+  </si>
+  <si>
+    <t>free, order form</t>
+  </si>
+  <si>
+    <t>The Dyadic Cyber Incident and Dispute Data</t>
+  </si>
+  <si>
+    <t>https://drryanmaness.wixsite.com/cyberconflcit/cyber-conflict-dataset</t>
+  </si>
+  <si>
+    <t>https://docs.wixstatic.com/ugd/4b99a4_294fde43b8094872999ca63f62972765.xlsx?dn=DCID%20Version%201.1.xlsx</t>
+  </si>
+  <si>
+    <t>https://docs.wixstatic.com/ugd/4b99a4_4c7971ea7791464a8ac551fff85fb1f1.pdf</t>
   </si>
 </sst>
 </file>
@@ -1548,10 +1575,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q146"/>
+  <dimension ref="A1:Q148"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A113" workbookViewId="0">
-      <selection activeCell="A61" sqref="A61"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4071,36 +4098,45 @@
     </row>
     <row r="131" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>213</v>
+        <v>399</v>
       </c>
       <c r="B131" t="s">
-        <v>55</v>
+        <v>40</v>
       </c>
       <c r="C131" s="2" t="s">
-        <v>212</v>
+        <v>400</v>
+      </c>
+      <c r="E131" t="s">
+        <v>14</v>
+      </c>
+      <c r="F131">
+        <v>2000</v>
+      </c>
+      <c r="G131">
+        <v>2014</v>
       </c>
       <c r="H131" t="s">
-        <v>16</v>
+        <v>348</v>
       </c>
       <c r="I131" t="s">
-        <v>20</v>
+        <v>349</v>
+      </c>
+      <c r="J131" s="2" t="s">
+        <v>402</v>
+      </c>
+      <c r="N131" s="2" t="s">
+        <v>401</v>
       </c>
     </row>
     <row r="132" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>323</v>
+        <v>213</v>
       </c>
       <c r="B132" t="s">
-        <v>25</v>
+        <v>55</v>
       </c>
       <c r="C132" s="2" t="s">
-        <v>324</v>
-      </c>
-      <c r="E132" t="s">
-        <v>325</v>
-      </c>
-      <c r="F132">
-        <v>1942</v>
+        <v>212</v>
       </c>
       <c r="H132" t="s">
         <v>16</v>
@@ -4111,124 +4147,145 @@
     </row>
     <row r="133" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
-        <v>273</v>
+        <v>395</v>
       </c>
       <c r="B133" t="s">
-        <v>237</v>
+        <v>25</v>
       </c>
       <c r="C133" s="2" t="s">
-        <v>272</v>
+        <v>394</v>
+      </c>
+      <c r="D133" t="s">
+        <v>396</v>
+      </c>
+      <c r="E133" t="s">
+        <v>111</v>
       </c>
       <c r="F133">
-        <v>1996</v>
+        <v>1986</v>
       </c>
       <c r="G133">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="H133" t="s">
-        <v>16</v>
+        <v>367</v>
       </c>
       <c r="I133" t="s">
-        <v>20</v>
+        <v>398</v>
+      </c>
+      <c r="J133" s="2" t="s">
+        <v>397</v>
       </c>
     </row>
     <row r="134" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
-        <v>66</v>
+        <v>323</v>
       </c>
       <c r="B134" t="s">
         <v>25</v>
       </c>
       <c r="C134" s="2" t="s">
-        <v>67</v>
+        <v>324</v>
+      </c>
+      <c r="E134" t="s">
+        <v>325</v>
+      </c>
+      <c r="F134">
+        <v>1942</v>
+      </c>
+      <c r="H134" t="s">
+        <v>16</v>
+      </c>
+      <c r="I134" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="135" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
-        <v>383</v>
+        <v>273</v>
       </c>
       <c r="B135" t="s">
-        <v>40</v>
+        <v>237</v>
       </c>
       <c r="C135" s="2" t="s">
-        <v>384</v>
-      </c>
-      <c r="E135" t="s">
-        <v>386</v>
+        <v>272</v>
       </c>
       <c r="F135">
-        <v>1951</v>
+        <v>1996</v>
+      </c>
+      <c r="G135">
+        <v>2016</v>
       </c>
       <c r="H135" t="s">
-        <v>348</v>
+        <v>16</v>
       </c>
       <c r="I135" t="s">
-        <v>349</v>
-      </c>
-      <c r="N135" s="2" t="s">
-        <v>385</v>
+        <v>20</v>
       </c>
     </row>
     <row r="136" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
-        <v>139</v>
+        <v>66</v>
       </c>
       <c r="B136" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="C136" s="2" t="s">
-        <v>140</v>
+        <v>67</v>
       </c>
     </row>
     <row r="137" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
-        <v>329</v>
+        <v>383</v>
       </c>
       <c r="B137" t="s">
-        <v>165</v>
+        <v>40</v>
       </c>
       <c r="C137" s="2" t="s">
-        <v>328</v>
+        <v>384</v>
       </c>
       <c r="E137" t="s">
-        <v>34</v>
+        <v>386</v>
       </c>
       <c r="F137">
-        <v>1789</v>
+        <v>1951</v>
       </c>
       <c r="H137" t="s">
-        <v>16</v>
+        <v>348</v>
       </c>
       <c r="I137" t="s">
-        <v>20</v>
+        <v>349</v>
+      </c>
+      <c r="N137" s="2" t="s">
+        <v>385</v>
       </c>
     </row>
     <row r="138" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
-        <v>172</v>
+        <v>139</v>
       </c>
       <c r="B138" t="s">
-        <v>60</v>
+        <v>40</v>
       </c>
       <c r="C138" s="2" t="s">
-        <v>171</v>
+        <v>140</v>
       </c>
     </row>
     <row r="139" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
-        <v>217</v>
+        <v>329</v>
       </c>
       <c r="B139" t="s">
-        <v>60</v>
+        <v>165</v>
       </c>
       <c r="C139" s="2" t="s">
-        <v>216</v>
+        <v>328</v>
       </c>
       <c r="E139" t="s">
-        <v>14</v>
+        <v>34</v>
       </c>
       <c r="F139">
-        <v>1900</v>
+        <v>1789</v>
       </c>
       <c r="H139" t="s">
         <v>16</v>
@@ -4239,104 +4296,92 @@
     </row>
     <row r="140" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
-        <v>132</v>
+        <v>172</v>
       </c>
       <c r="B140" t="s">
-        <v>259</v>
+        <v>60</v>
       </c>
       <c r="C140" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="Q140" t="s">
-        <v>17</v>
+        <v>171</v>
       </c>
     </row>
     <row r="141" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
-        <v>182</v>
+        <v>217</v>
       </c>
       <c r="B141" t="s">
-        <v>165</v>
+        <v>60</v>
       </c>
       <c r="C141" s="2" t="s">
-        <v>181</v>
+        <v>216</v>
+      </c>
+      <c r="E141" t="s">
+        <v>14</v>
+      </c>
+      <c r="F141">
+        <v>1900</v>
+      </c>
+      <c r="H141" t="s">
+        <v>16</v>
+      </c>
+      <c r="I141" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="142" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
-        <v>115</v>
+        <v>132</v>
       </c>
       <c r="B142" t="s">
-        <v>128</v>
+        <v>259</v>
       </c>
       <c r="C142" s="2" t="s">
-        <v>116</v>
+        <v>133</v>
+      </c>
+      <c r="Q142" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="143" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
-        <v>263</v>
+        <v>182</v>
       </c>
       <c r="B143" t="s">
-        <v>250</v>
+        <v>165</v>
       </c>
       <c r="C143" s="2" t="s">
-        <v>264</v>
-      </c>
-      <c r="E143" t="s">
-        <v>265</v>
-      </c>
-      <c r="F143">
-        <v>1500</v>
-      </c>
-      <c r="G143">
-        <v>2000</v>
-      </c>
-      <c r="H143" t="s">
-        <v>16</v>
-      </c>
-      <c r="I143" t="s">
-        <v>20</v>
+        <v>181</v>
       </c>
     </row>
     <row r="144" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
-        <v>221</v>
+        <v>115</v>
       </c>
       <c r="B144" t="s">
-        <v>86</v>
+        <v>128</v>
       </c>
       <c r="C144" s="2" t="s">
-        <v>220</v>
-      </c>
-      <c r="F144">
-        <v>2013</v>
-      </c>
-      <c r="H144" t="s">
-        <v>16</v>
-      </c>
-      <c r="I144" t="s">
-        <v>20</v>
+        <v>116</v>
       </c>
     </row>
     <row r="145" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
-        <v>13</v>
+        <v>263</v>
       </c>
       <c r="B145" t="s">
-        <v>25</v>
+        <v>250</v>
       </c>
       <c r="C145" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="D145" s="1" t="s">
-        <v>42</v>
+        <v>264</v>
       </c>
       <c r="E145" t="s">
-        <v>14</v>
+        <v>265</v>
       </c>
       <c r="F145">
-        <v>1981</v>
+        <v>1500</v>
+      </c>
+      <c r="G145">
+        <v>2000</v>
       </c>
       <c r="H145" t="s">
         <v>16</v>
@@ -4347,23 +4392,69 @@
     </row>
     <row r="146" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
+        <v>221</v>
+      </c>
+      <c r="B146" t="s">
+        <v>86</v>
+      </c>
+      <c r="C146" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="F146">
+        <v>2013</v>
+      </c>
+      <c r="H146" t="s">
+        <v>16</v>
+      </c>
+      <c r="I146" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="147" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A147" t="s">
+        <v>13</v>
+      </c>
+      <c r="B147" t="s">
+        <v>25</v>
+      </c>
+      <c r="C147" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D147" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E147" t="s">
+        <v>14</v>
+      </c>
+      <c r="F147">
+        <v>1981</v>
+      </c>
+      <c r="H147" t="s">
+        <v>16</v>
+      </c>
+      <c r="I147" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="148" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A148" t="s">
         <v>283</v>
       </c>
-      <c r="B146" t="s">
+      <c r="B148" t="s">
         <v>124</v>
       </c>
-      <c r="C146" s="2" t="s">
+      <c r="C148" s="2" t="s">
         <v>284</v>
       </c>
-      <c r="H146" t="s">
-        <v>16</v>
-      </c>
-      <c r="I146" t="s">
+      <c r="H148" t="s">
+        <v>16</v>
+      </c>
+      <c r="I148" t="s">
         <v>20</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:Q146">
+  <sortState ref="A2:Q148">
     <sortCondition ref="A2"/>
   </sortState>
   <hyperlinks>
@@ -4373,7 +4464,7 @@
     <hyperlink ref="C10" r:id="rId4"/>
     <hyperlink ref="C88" r:id="rId5"/>
     <hyperlink ref="C107" r:id="rId6"/>
-    <hyperlink ref="C145" r:id="rId7"/>
+    <hyperlink ref="C147" r:id="rId7"/>
     <hyperlink ref="C35" r:id="rId8"/>
     <hyperlink ref="C30" r:id="rId9"/>
     <hyperlink ref="C48" r:id="rId10"/>
@@ -4387,7 +4478,7 @@
     <hyperlink ref="C40" r:id="rId18"/>
     <hyperlink ref="C69" r:id="rId19"/>
     <hyperlink ref="C16" r:id="rId20"/>
-    <hyperlink ref="C134" r:id="rId21"/>
+    <hyperlink ref="C136" r:id="rId21"/>
     <hyperlink ref="C8" r:id="rId22"/>
     <hyperlink ref="C38" r:id="rId23"/>
     <hyperlink ref="C52" r:id="rId24"/>
@@ -4404,7 +4495,7 @@
     <hyperlink ref="C17" r:id="rId35"/>
     <hyperlink ref="C125" r:id="rId36"/>
     <hyperlink ref="C15" r:id="rId37"/>
-    <hyperlink ref="C142" r:id="rId38"/>
+    <hyperlink ref="C144" r:id="rId38"/>
     <hyperlink ref="C82" r:id="rId39"/>
     <hyperlink ref="C56" r:id="rId40"/>
     <hyperlink ref="C111" r:id="rId41"/>
@@ -4412,10 +4503,10 @@
     <hyperlink ref="C50" r:id="rId43"/>
     <hyperlink ref="C23" r:id="rId44"/>
     <hyperlink ref="C104" r:id="rId45"/>
-    <hyperlink ref="C140" r:id="rId46"/>
+    <hyperlink ref="C142" r:id="rId46"/>
     <hyperlink ref="C27" r:id="rId47" display="http://comparativeconstitutionsproject.org/"/>
     <hyperlink ref="C101" r:id="rId48"/>
-    <hyperlink ref="C136" r:id="rId49"/>
+    <hyperlink ref="C138" r:id="rId49"/>
     <hyperlink ref="C115" r:id="rId50"/>
     <hyperlink ref="C110" r:id="rId51"/>
     <hyperlink ref="C22" r:id="rId52"/>
@@ -4432,12 +4523,12 @@
     <hyperlink ref="C33" r:id="rId63"/>
     <hyperlink ref="C130" r:id="rId64"/>
     <hyperlink ref="C14" r:id="rId65"/>
-    <hyperlink ref="C138" r:id="rId66"/>
+    <hyperlink ref="C140" r:id="rId66"/>
     <hyperlink ref="C25" r:id="rId67"/>
     <hyperlink ref="C24" r:id="rId68"/>
     <hyperlink ref="C26" r:id="rId69"/>
     <hyperlink ref="C51" r:id="rId70"/>
-    <hyperlink ref="C141" r:id="rId71"/>
+    <hyperlink ref="C143" r:id="rId71"/>
     <hyperlink ref="C28" r:id="rId72"/>
     <hyperlink ref="C108" r:id="rId73"/>
     <hyperlink ref="C32" r:id="rId74"/>
@@ -4451,11 +4542,11 @@
     <hyperlink ref="C12" r:id="rId82"/>
     <hyperlink ref="C100" r:id="rId83"/>
     <hyperlink ref="C109" r:id="rId84"/>
-    <hyperlink ref="C131" r:id="rId85"/>
+    <hyperlink ref="C132" r:id="rId85"/>
     <hyperlink ref="C36" r:id="rId86"/>
-    <hyperlink ref="C139" r:id="rId87"/>
+    <hyperlink ref="C141" r:id="rId87"/>
     <hyperlink ref="C43" r:id="rId88"/>
-    <hyperlink ref="C144" r:id="rId89"/>
+    <hyperlink ref="C146" r:id="rId89"/>
     <hyperlink ref="C89" r:id="rId90"/>
     <hyperlink ref="C63" r:id="rId91"/>
     <hyperlink ref="C90" r:id="rId92"/>
@@ -4478,15 +4569,15 @@
     <hyperlink ref="C122" r:id="rId109"/>
     <hyperlink ref="C13" r:id="rId110"/>
     <hyperlink ref="C4" r:id="rId111"/>
-    <hyperlink ref="C143" r:id="rId112"/>
+    <hyperlink ref="C145" r:id="rId112"/>
     <hyperlink ref="C86" r:id="rId113"/>
     <hyperlink ref="C81" r:id="rId114"/>
-    <hyperlink ref="C133" r:id="rId115"/>
+    <hyperlink ref="C135" r:id="rId115"/>
     <hyperlink ref="C118" r:id="rId116"/>
     <hyperlink ref="C62" r:id="rId117"/>
     <hyperlink ref="C92" r:id="rId118"/>
     <hyperlink ref="C71" r:id="rId119"/>
-    <hyperlink ref="C146" r:id="rId120"/>
+    <hyperlink ref="C148" r:id="rId120"/>
     <hyperlink ref="C64" r:id="rId121"/>
     <hyperlink ref="C117" r:id="rId122"/>
     <hyperlink ref="C97" r:id="rId123"/>
@@ -4502,9 +4593,9 @@
     <hyperlink ref="C113" r:id="rId133"/>
     <hyperlink ref="C112" r:id="rId134"/>
     <hyperlink ref="C114" r:id="rId135"/>
-    <hyperlink ref="C132" r:id="rId136"/>
+    <hyperlink ref="C134" r:id="rId136"/>
     <hyperlink ref="C126" r:id="rId137"/>
-    <hyperlink ref="C137" r:id="rId138"/>
+    <hyperlink ref="C139" r:id="rId138"/>
     <hyperlink ref="C37" r:id="rId139"/>
     <hyperlink ref="C85" r:id="rId140"/>
     <hyperlink ref="J2" r:id="rId141"/>
@@ -4521,11 +4612,16 @@
     <hyperlink ref="M8" r:id="rId152"/>
     <hyperlink ref="L8" r:id="rId153"/>
     <hyperlink ref="J8" r:id="rId154"/>
-    <hyperlink ref="C135" r:id="rId155"/>
-    <hyperlink ref="N135" r:id="rId156"/>
+    <hyperlink ref="C137" r:id="rId155"/>
+    <hyperlink ref="N137" r:id="rId156"/>
     <hyperlink ref="C21" r:id="rId157"/>
     <hyperlink ref="N21" r:id="rId158"/>
     <hyperlink ref="C61" r:id="rId159"/>
+    <hyperlink ref="C133" r:id="rId160"/>
+    <hyperlink ref="J133" r:id="rId161"/>
+    <hyperlink ref="C131" r:id="rId162"/>
+    <hyperlink ref="N131" r:id="rId163"/>
+    <hyperlink ref="J131" r:id="rId164"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
add data, 'Leader Experience and Attribute Descriptions'
</commit_message>
<xml_diff>
--- a/PolData.xlsx
+++ b/PolData.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="731" uniqueCount="403">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="738" uniqueCount="406">
   <si>
     <t>name</t>
   </si>
@@ -1236,6 +1236,15 @@
   </si>
   <si>
     <t>https://docs.wixstatic.com/ugd/4b99a4_4c7971ea7791464a8ac551fff85fb1f1.pdf</t>
+  </si>
+  <si>
+    <t>http://dx.doi.org/10.7910/DVN/SYZZEY</t>
+  </si>
+  <si>
+    <t>Leader Experience and Attribute Descriptions</t>
+  </si>
+  <si>
+    <t>Military experiences, childhood, education, personal, family life</t>
   </si>
 </sst>
 </file>
@@ -1575,10 +1584,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q148"/>
+  <dimension ref="A1:Q149"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="A37" sqref="A37"/>
+    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="A88" sqref="A88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3271,68 +3280,74 @@
     </row>
     <row r="88" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>11</v>
+        <v>404</v>
       </c>
       <c r="B88" t="s">
-        <v>25</v>
+        <v>83</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>12</v>
+        <v>403</v>
       </c>
       <c r="D88" t="s">
-        <v>95</v>
+        <v>405</v>
       </c>
       <c r="E88" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="F88">
-        <v>2007</v>
+        <v>1875</v>
+      </c>
+      <c r="G88">
+        <v>2004</v>
       </c>
       <c r="H88" t="s">
-        <v>16</v>
+        <v>348</v>
       </c>
       <c r="I88" t="s">
-        <v>21</v>
+        <v>349</v>
       </c>
     </row>
     <row r="89" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>223</v>
+        <v>11</v>
       </c>
       <c r="B89" t="s">
-        <v>124</v>
+        <v>25</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>222</v>
+        <v>12</v>
+      </c>
+      <c r="D89" t="s">
+        <v>95</v>
+      </c>
+      <c r="E89" t="s">
+        <v>10</v>
       </c>
       <c r="F89">
-        <v>1</v>
-      </c>
-      <c r="G89">
-        <v>2010</v>
+        <v>2007</v>
       </c>
       <c r="H89" t="s">
         <v>16</v>
       </c>
       <c r="I89" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="90" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="B90" t="s">
-        <v>40</v>
+        <v>124</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="F90">
-        <v>1946</v>
+        <v>1</v>
       </c>
       <c r="G90">
-        <v>2016</v>
+        <v>2010</v>
       </c>
       <c r="H90" t="s">
         <v>16</v>
@@ -3343,90 +3358,90 @@
     </row>
     <row r="91" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>97</v>
+        <v>226</v>
       </c>
       <c r="B91" t="s">
-        <v>128</v>
+        <v>40</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>98</v>
+        <v>225</v>
+      </c>
+      <c r="F91">
+        <v>1946</v>
+      </c>
+      <c r="G91">
+        <v>2016</v>
+      </c>
+      <c r="H91" t="s">
+        <v>16</v>
+      </c>
+      <c r="I91" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="92" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>278</v>
+        <v>97</v>
       </c>
       <c r="B92" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>279</v>
-      </c>
-      <c r="E92" t="s">
-        <v>280</v>
-      </c>
-      <c r="F92">
-        <v>1890</v>
-      </c>
-      <c r="G92">
-        <v>1996</v>
-      </c>
-      <c r="H92" t="s">
-        <v>16</v>
-      </c>
-      <c r="I92" t="s">
-        <v>20</v>
+        <v>98</v>
       </c>
     </row>
     <row r="93" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>156</v>
+        <v>278</v>
       </c>
       <c r="B93" t="s">
-        <v>25</v>
+        <v>124</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>154</v>
+        <v>279</v>
+      </c>
+      <c r="E93" t="s">
+        <v>280</v>
+      </c>
+      <c r="F93">
+        <v>1890</v>
+      </c>
+      <c r="G93">
+        <v>1996</v>
+      </c>
+      <c r="H93" t="s">
+        <v>16</v>
+      </c>
+      <c r="I93" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="94" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>229</v>
+        <v>156</v>
       </c>
       <c r="B94" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>225</v>
-      </c>
-      <c r="F94">
-        <v>1952</v>
-      </c>
-      <c r="G94">
-        <v>1997</v>
-      </c>
-      <c r="H94" t="s">
-        <v>16</v>
-      </c>
-      <c r="I94" t="s">
-        <v>20</v>
+        <v>154</v>
       </c>
     </row>
     <row r="95" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>293</v>
+        <v>229</v>
       </c>
       <c r="B95" t="s">
         <v>40</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>294</v>
+        <v>225</v>
       </c>
       <c r="F95">
-        <v>2004</v>
+        <v>1952</v>
       </c>
       <c r="G95">
-        <v>2006</v>
+        <v>1997</v>
       </c>
       <c r="H95" t="s">
         <v>16</v>
@@ -3437,221 +3452,218 @@
     </row>
     <row r="96" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>102</v>
+        <v>293</v>
       </c>
       <c r="B96" t="s">
-        <v>99</v>
+        <v>40</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>103</v>
+        <v>294</v>
+      </c>
+      <c r="F96">
+        <v>2004</v>
+      </c>
+      <c r="G96">
+        <v>2006</v>
+      </c>
+      <c r="H96" t="s">
+        <v>16</v>
+      </c>
+      <c r="I96" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="97" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>289</v>
+        <v>102</v>
       </c>
       <c r="B97" t="s">
-        <v>124</v>
+        <v>99</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>290</v>
+        <v>103</v>
       </c>
     </row>
     <row r="98" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>246</v>
+        <v>289</v>
       </c>
       <c r="B98" t="s">
-        <v>165</v>
+        <v>124</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>247</v>
-      </c>
-      <c r="E98" t="s">
-        <v>14</v>
-      </c>
-      <c r="F98">
-        <v>1960</v>
-      </c>
-      <c r="G98">
-        <v>2006</v>
-      </c>
-      <c r="H98" t="s">
-        <v>16</v>
-      </c>
-      <c r="I98" t="s">
-        <v>249</v>
+        <v>290</v>
       </c>
     </row>
     <row r="99" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>365</v>
+        <v>246</v>
       </c>
       <c r="B99" t="s">
-        <v>128</v>
+        <v>165</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>364</v>
-      </c>
-      <c r="D99" t="s">
-        <v>370</v>
+        <v>247</v>
       </c>
       <c r="E99" t="s">
-        <v>366</v>
+        <v>14</v>
       </c>
       <c r="F99">
-        <v>1906</v>
+        <v>1960</v>
       </c>
       <c r="G99">
-        <v>2013</v>
+        <v>2006</v>
       </c>
       <c r="H99" t="s">
-        <v>367</v>
+        <v>16</v>
       </c>
       <c r="I99" t="s">
-        <v>368</v>
-      </c>
-      <c r="Q99" t="s">
-        <v>369</v>
+        <v>249</v>
       </c>
     </row>
     <row r="100" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>208</v>
+        <v>365</v>
       </c>
       <c r="B100" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="C100" s="2" t="s">
-        <v>209</v>
+        <v>364</v>
+      </c>
+      <c r="D100" t="s">
+        <v>370</v>
+      </c>
+      <c r="E100" t="s">
+        <v>366</v>
       </c>
       <c r="F100">
-        <v>1932</v>
+        <v>1906</v>
       </c>
       <c r="G100">
-        <v>2014</v>
+        <v>2013</v>
       </c>
       <c r="H100" t="s">
-        <v>16</v>
+        <v>367</v>
       </c>
       <c r="I100" t="s">
-        <v>20</v>
+        <v>368</v>
+      </c>
+      <c r="Q100" t="s">
+        <v>369</v>
       </c>
     </row>
     <row r="101" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>137</v>
+        <v>208</v>
       </c>
       <c r="B101" t="s">
-        <v>259</v>
+        <v>124</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>138</v>
+        <v>209</v>
+      </c>
+      <c r="F101">
+        <v>1932</v>
+      </c>
+      <c r="G101">
+        <v>2014</v>
+      </c>
+      <c r="H101" t="s">
+        <v>16</v>
+      </c>
+      <c r="I101" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="102" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>155</v>
+        <v>137</v>
       </c>
       <c r="B102" t="s">
         <v>259</v>
       </c>
       <c r="C102" s="2" t="s">
-        <v>154</v>
+        <v>138</v>
       </c>
     </row>
     <row r="103" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>57</v>
+        <v>155</v>
       </c>
       <c r="B103" t="s">
-        <v>128</v>
+        <v>259</v>
       </c>
       <c r="C103" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="Q103" t="s">
-        <v>17</v>
+        <v>154</v>
       </c>
     </row>
     <row r="104" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>129</v>
+        <v>57</v>
       </c>
       <c r="B104" t="s">
-        <v>259</v>
+        <v>128</v>
       </c>
       <c r="C104" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="E104" t="s">
-        <v>131</v>
-      </c>
-      <c r="F104">
-        <v>1945</v>
-      </c>
-      <c r="G104">
-        <v>2008</v>
-      </c>
-      <c r="I104" t="s">
-        <v>20</v>
+        <v>58</v>
+      </c>
+      <c r="Q104" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="105" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>148</v>
+        <v>129</v>
       </c>
       <c r="B105" t="s">
-        <v>128</v>
+        <v>259</v>
       </c>
       <c r="C105" s="2" t="s">
-        <v>147</v>
+        <v>130</v>
+      </c>
+      <c r="E105" t="s">
+        <v>131</v>
+      </c>
+      <c r="F105">
+        <v>1945</v>
+      </c>
+      <c r="G105">
+        <v>2008</v>
+      </c>
+      <c r="I105" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="106" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>233</v>
+        <v>148</v>
       </c>
       <c r="B106" t="s">
-        <v>165</v>
+        <v>128</v>
       </c>
       <c r="C106" s="2" t="s">
-        <v>234</v>
-      </c>
-      <c r="E106" t="s">
-        <v>14</v>
-      </c>
-      <c r="F106">
-        <v>2012</v>
-      </c>
-      <c r="G106">
-        <v>2016</v>
-      </c>
-      <c r="H106" t="s">
-        <v>16</v>
-      </c>
-      <c r="I106" t="s">
-        <v>20</v>
+        <v>147</v>
       </c>
     </row>
     <row r="107" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>35</v>
+        <v>233</v>
       </c>
       <c r="B107" t="s">
-        <v>25</v>
+        <v>165</v>
       </c>
       <c r="C107" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="D107" t="s">
-        <v>37</v>
+        <v>234</v>
       </c>
       <c r="E107" t="s">
         <v>14</v>
       </c>
       <c r="F107">
-        <v>2001</v>
+        <v>2012</v>
+      </c>
+      <c r="G107">
+        <v>2016</v>
       </c>
       <c r="H107" t="s">
         <v>16</v>
@@ -3662,90 +3674,90 @@
     </row>
     <row r="108" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>185</v>
+        <v>35</v>
       </c>
       <c r="B108" t="s">
-        <v>128</v>
+        <v>25</v>
       </c>
       <c r="C108" s="2" t="s">
-        <v>186</v>
+        <v>36</v>
+      </c>
+      <c r="D108" t="s">
+        <v>37</v>
+      </c>
+      <c r="E108" t="s">
+        <v>14</v>
+      </c>
+      <c r="F108">
+        <v>2001</v>
+      </c>
+      <c r="H108" t="s">
+        <v>16</v>
+      </c>
+      <c r="I108" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="109" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>210</v>
+        <v>185</v>
       </c>
       <c r="B109" t="s">
-        <v>40</v>
+        <v>128</v>
       </c>
       <c r="C109" s="2" t="s">
-        <v>211</v>
-      </c>
-      <c r="F109">
-        <v>1976</v>
-      </c>
-      <c r="G109">
-        <v>2016</v>
-      </c>
-      <c r="H109" t="s">
-        <v>16</v>
-      </c>
-      <c r="I109" t="s">
-        <v>20</v>
+        <v>186</v>
       </c>
     </row>
     <row r="110" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>144</v>
+        <v>210</v>
       </c>
       <c r="B110" t="s">
-        <v>60</v>
+        <v>40</v>
       </c>
       <c r="C110" s="2" t="s">
-        <v>143</v>
+        <v>211</v>
       </c>
       <c r="F110">
-        <v>1800</v>
+        <v>1976</v>
       </c>
       <c r="G110">
-        <v>2013</v>
+        <v>2016</v>
+      </c>
+      <c r="H110" t="s">
+        <v>16</v>
+      </c>
+      <c r="I110" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="111" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>122</v>
+        <v>144</v>
       </c>
       <c r="B111" t="s">
-        <v>259</v>
+        <v>60</v>
       </c>
       <c r="C111" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="I111" t="s">
-        <v>20</v>
+        <v>143</v>
+      </c>
+      <c r="F111">
+        <v>1800</v>
+      </c>
+      <c r="G111">
+        <v>2013</v>
       </c>
     </row>
     <row r="112" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>318</v>
+        <v>122</v>
       </c>
       <c r="B112" t="s">
-        <v>250</v>
+        <v>259</v>
       </c>
       <c r="C112" s="2" t="s">
-        <v>319</v>
-      </c>
-      <c r="E112" t="s">
-        <v>320</v>
-      </c>
-      <c r="F112">
-        <v>1975</v>
-      </c>
-      <c r="G112">
-        <v>1989</v>
-      </c>
-      <c r="H112" t="s">
-        <v>16</v>
+        <v>121</v>
       </c>
       <c r="I112" t="s">
         <v>20</v>
@@ -3753,22 +3765,22 @@
     </row>
     <row r="113" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="B113" t="s">
         <v>250</v>
       </c>
       <c r="C113" s="2" t="s">
-        <v>317</v>
+        <v>319</v>
       </c>
       <c r="E113" t="s">
-        <v>105</v>
+        <v>320</v>
       </c>
       <c r="F113">
-        <v>1950</v>
+        <v>1975</v>
       </c>
       <c r="G113">
-        <v>1996</v>
+        <v>1989</v>
       </c>
       <c r="H113" t="s">
         <v>16</v>
@@ -3779,19 +3791,22 @@
     </row>
     <row r="114" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>322</v>
+        <v>316</v>
       </c>
       <c r="B114" t="s">
-        <v>25</v>
+        <v>250</v>
       </c>
       <c r="C114" s="2" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="E114" t="s">
-        <v>77</v>
+        <v>105</v>
       </c>
       <c r="F114">
-        <v>2010</v>
+        <v>1950</v>
+      </c>
+      <c r="G114">
+        <v>1996</v>
       </c>
       <c r="H114" t="s">
         <v>16</v>
@@ -3802,164 +3817,164 @@
     </row>
     <row r="115" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>141</v>
+        <v>322</v>
       </c>
       <c r="B115" t="s">
-        <v>237</v>
+        <v>25</v>
       </c>
       <c r="C115" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="Q115" t="s">
-        <v>17</v>
+        <v>321</v>
+      </c>
+      <c r="E115" t="s">
+        <v>77</v>
+      </c>
+      <c r="F115">
+        <v>2010</v>
+      </c>
+      <c r="H115" t="s">
+        <v>16</v>
+      </c>
+      <c r="I115" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="116" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>308</v>
+        <v>141</v>
       </c>
       <c r="B116" t="s">
-        <v>250</v>
+        <v>237</v>
       </c>
       <c r="C116" s="2" t="s">
-        <v>309</v>
-      </c>
-      <c r="E116" t="s">
-        <v>310</v>
-      </c>
-      <c r="F116">
-        <v>1950</v>
-      </c>
-      <c r="G116">
-        <v>2010</v>
-      </c>
-      <c r="H116" t="s">
-        <v>16</v>
-      </c>
-      <c r="I116" t="s">
-        <v>20</v>
+        <v>142</v>
+      </c>
+      <c r="Q116" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="117" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>287</v>
+        <v>308</v>
       </c>
       <c r="B117" t="s">
-        <v>134</v>
+        <v>250</v>
       </c>
       <c r="C117" s="2" t="s">
-        <v>288</v>
+        <v>309</v>
+      </c>
+      <c r="E117" t="s">
+        <v>310</v>
       </c>
       <c r="F117">
-        <v>1990</v>
+        <v>1950</v>
       </c>
       <c r="G117">
-        <v>2008</v>
+        <v>2010</v>
+      </c>
+      <c r="H117" t="s">
+        <v>16</v>
+      </c>
+      <c r="I117" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="118" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>274</v>
+        <v>287</v>
       </c>
       <c r="B118" t="s">
-        <v>55</v>
+        <v>134</v>
       </c>
       <c r="C118" s="2" t="s">
-        <v>275</v>
-      </c>
-      <c r="H118" t="s">
-        <v>16</v>
-      </c>
-      <c r="I118" t="s">
-        <v>20</v>
+        <v>288</v>
+      </c>
+      <c r="F118">
+        <v>1990</v>
+      </c>
+      <c r="G118">
+        <v>2008</v>
       </c>
     </row>
     <row r="119" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>157</v>
+        <v>274</v>
       </c>
       <c r="B119" t="s">
-        <v>128</v>
+        <v>55</v>
       </c>
       <c r="C119" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="Q119" t="s">
-        <v>18</v>
+        <v>275</v>
+      </c>
+      <c r="H119" t="s">
+        <v>16</v>
+      </c>
+      <c r="I119" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="120" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>194</v>
+        <v>157</v>
       </c>
       <c r="B120" t="s">
-        <v>99</v>
+        <v>128</v>
       </c>
       <c r="C120" s="2" t="s">
-        <v>193</v>
+        <v>154</v>
+      </c>
+      <c r="Q120" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="121" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>295</v>
+        <v>194</v>
       </c>
       <c r="B121" t="s">
-        <v>40</v>
+        <v>99</v>
       </c>
       <c r="C121" s="2" t="s">
-        <v>296</v>
-      </c>
-      <c r="E121" t="s">
-        <v>297</v>
-      </c>
-      <c r="F121">
-        <v>1990</v>
-      </c>
-      <c r="G121">
-        <v>2015</v>
-      </c>
-      <c r="H121" t="s">
-        <v>16</v>
-      </c>
-      <c r="I121" t="s">
-        <v>249</v>
+        <v>193</v>
       </c>
     </row>
     <row r="122" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>256</v>
+        <v>295</v>
       </c>
       <c r="B122" t="s">
-        <v>250</v>
+        <v>40</v>
       </c>
       <c r="C122" s="2" t="s">
-        <v>257</v>
+        <v>296</v>
       </c>
       <c r="E122" t="s">
-        <v>258</v>
+        <v>297</v>
+      </c>
+      <c r="F122">
+        <v>1990</v>
+      </c>
+      <c r="G122">
+        <v>2015</v>
       </c>
       <c r="H122" t="s">
         <v>16</v>
       </c>
       <c r="I122" t="s">
-        <v>20</v>
+        <v>249</v>
       </c>
     </row>
     <row r="123" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>227</v>
+        <v>256</v>
       </c>
       <c r="B123" t="s">
-        <v>40</v>
+        <v>250</v>
       </c>
       <c r="C123" s="2" t="s">
-        <v>225</v>
-      </c>
-      <c r="F123">
-        <v>1955</v>
-      </c>
-      <c r="G123">
-        <v>2016</v>
+        <v>257</v>
+      </c>
+      <c r="E123" t="s">
+        <v>258</v>
       </c>
       <c r="H123" t="s">
         <v>16</v>
@@ -3970,7 +3985,7 @@
     </row>
     <row r="124" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="B124" t="s">
         <v>40</v>
@@ -3979,7 +3994,7 @@
         <v>225</v>
       </c>
       <c r="F124">
-        <v>1995</v>
+        <v>1955</v>
       </c>
       <c r="G124">
         <v>2016</v>
@@ -3993,228 +4008,228 @@
     </row>
     <row r="125" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>109</v>
+        <v>230</v>
       </c>
       <c r="B125" t="s">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="C125" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="E125" t="s">
-        <v>111</v>
+        <v>225</v>
       </c>
       <c r="F125">
-        <v>1956</v>
+        <v>1995</v>
+      </c>
+      <c r="G125">
+        <v>2016</v>
+      </c>
+      <c r="H125" t="s">
+        <v>16</v>
+      </c>
+      <c r="I125" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="126" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>326</v>
+        <v>109</v>
       </c>
       <c r="B126" t="s">
         <v>25</v>
       </c>
       <c r="C126" s="2" t="s">
-        <v>327</v>
+        <v>110</v>
       </c>
       <c r="E126" t="s">
         <v>111</v>
       </c>
       <c r="F126">
-        <v>1998</v>
-      </c>
-      <c r="H126" t="s">
-        <v>16</v>
-      </c>
-      <c r="I126" t="s">
-        <v>20</v>
+        <v>1956</v>
       </c>
     </row>
     <row r="127" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>91</v>
+        <v>326</v>
       </c>
       <c r="B127" t="s">
         <v>25</v>
       </c>
       <c r="C127" s="2" t="s">
-        <v>93</v>
+        <v>327</v>
       </c>
       <c r="E127" t="s">
-        <v>92</v>
+        <v>111</v>
       </c>
       <c r="F127">
-        <v>1999</v>
+        <v>1998</v>
+      </c>
+      <c r="H127" t="s">
+        <v>16</v>
+      </c>
+      <c r="I127" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="128" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>314</v>
+        <v>91</v>
       </c>
       <c r="B128" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="C128" s="2" t="s">
-        <v>313</v>
+        <v>93</v>
       </c>
       <c r="E128" t="s">
-        <v>315</v>
+        <v>92</v>
       </c>
       <c r="F128">
-        <v>1950</v>
-      </c>
-      <c r="G128">
-        <v>2004</v>
-      </c>
-      <c r="H128" t="s">
-        <v>16</v>
-      </c>
-      <c r="I128" t="s">
-        <v>20</v>
+        <v>1999</v>
       </c>
     </row>
     <row r="129" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>161</v>
+        <v>314</v>
       </c>
       <c r="B129" t="s">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="C129" s="2" t="s">
-        <v>160</v>
+        <v>313</v>
+      </c>
+      <c r="E129" t="s">
+        <v>315</v>
+      </c>
+      <c r="F129">
+        <v>1950</v>
+      </c>
+      <c r="G129">
+        <v>2004</v>
+      </c>
+      <c r="H129" t="s">
+        <v>16</v>
+      </c>
+      <c r="I129" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="130" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="B130" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="C130" s="2" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
     </row>
     <row r="131" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>399</v>
+        <v>168</v>
       </c>
       <c r="B131" t="s">
         <v>40</v>
       </c>
       <c r="C131" s="2" t="s">
-        <v>400</v>
-      </c>
-      <c r="E131" t="s">
-        <v>14</v>
-      </c>
-      <c r="F131">
-        <v>2000</v>
-      </c>
-      <c r="G131">
-        <v>2014</v>
-      </c>
-      <c r="H131" t="s">
-        <v>348</v>
-      </c>
-      <c r="I131" t="s">
-        <v>349</v>
-      </c>
-      <c r="J131" s="2" t="s">
-        <v>402</v>
-      </c>
-      <c r="N131" s="2" t="s">
-        <v>401</v>
+        <v>167</v>
       </c>
     </row>
     <row r="132" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>213</v>
+        <v>399</v>
       </c>
       <c r="B132" t="s">
-        <v>55</v>
+        <v>40</v>
       </c>
       <c r="C132" s="2" t="s">
-        <v>212</v>
+        <v>400</v>
+      </c>
+      <c r="E132" t="s">
+        <v>14</v>
+      </c>
+      <c r="F132">
+        <v>2000</v>
+      </c>
+      <c r="G132">
+        <v>2014</v>
       </c>
       <c r="H132" t="s">
-        <v>16</v>
+        <v>348</v>
       </c>
       <c r="I132" t="s">
-        <v>20</v>
+        <v>349</v>
+      </c>
+      <c r="J132" s="2" t="s">
+        <v>402</v>
+      </c>
+      <c r="N132" s="2" t="s">
+        <v>401</v>
       </c>
     </row>
     <row r="133" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
-        <v>395</v>
+        <v>213</v>
       </c>
       <c r="B133" t="s">
-        <v>25</v>
+        <v>55</v>
       </c>
       <c r="C133" s="2" t="s">
-        <v>394</v>
-      </c>
-      <c r="D133" t="s">
-        <v>396</v>
-      </c>
-      <c r="E133" t="s">
-        <v>111</v>
-      </c>
-      <c r="F133">
-        <v>1986</v>
-      </c>
-      <c r="G133">
-        <v>2015</v>
+        <v>212</v>
       </c>
       <c r="H133" t="s">
-        <v>367</v>
+        <v>16</v>
       </c>
       <c r="I133" t="s">
-        <v>398</v>
-      </c>
-      <c r="J133" s="2" t="s">
-        <v>397</v>
+        <v>20</v>
       </c>
     </row>
     <row r="134" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
-        <v>323</v>
+        <v>395</v>
       </c>
       <c r="B134" t="s">
         <v>25</v>
       </c>
       <c r="C134" s="2" t="s">
-        <v>324</v>
+        <v>394</v>
+      </c>
+      <c r="D134" t="s">
+        <v>396</v>
       </c>
       <c r="E134" t="s">
-        <v>325</v>
+        <v>111</v>
       </c>
       <c r="F134">
-        <v>1942</v>
+        <v>1986</v>
+      </c>
+      <c r="G134">
+        <v>2015</v>
       </c>
       <c r="H134" t="s">
-        <v>16</v>
+        <v>367</v>
       </c>
       <c r="I134" t="s">
-        <v>20</v>
+        <v>398</v>
+      </c>
+      <c r="J134" s="2" t="s">
+        <v>397</v>
       </c>
     </row>
     <row r="135" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
-        <v>273</v>
+        <v>323</v>
       </c>
       <c r="B135" t="s">
-        <v>237</v>
+        <v>25</v>
       </c>
       <c r="C135" s="2" t="s">
-        <v>272</v>
+        <v>324</v>
+      </c>
+      <c r="E135" t="s">
+        <v>325</v>
       </c>
       <c r="F135">
-        <v>1996</v>
-      </c>
-      <c r="G135">
-        <v>2016</v>
+        <v>1942</v>
       </c>
       <c r="H135" t="s">
         <v>16</v>
@@ -4225,183 +4240,186 @@
     </row>
     <row r="136" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
-        <v>66</v>
+        <v>273</v>
       </c>
       <c r="B136" t="s">
-        <v>25</v>
+        <v>237</v>
       </c>
       <c r="C136" s="2" t="s">
-        <v>67</v>
+        <v>272</v>
+      </c>
+      <c r="F136">
+        <v>1996</v>
+      </c>
+      <c r="G136">
+        <v>2016</v>
+      </c>
+      <c r="H136" t="s">
+        <v>16</v>
+      </c>
+      <c r="I136" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="137" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
-        <v>383</v>
+        <v>66</v>
       </c>
       <c r="B137" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="C137" s="2" t="s">
-        <v>384</v>
-      </c>
-      <c r="E137" t="s">
-        <v>386</v>
-      </c>
-      <c r="F137">
-        <v>1951</v>
-      </c>
-      <c r="H137" t="s">
-        <v>348</v>
-      </c>
-      <c r="I137" t="s">
-        <v>349</v>
-      </c>
-      <c r="N137" s="2" t="s">
-        <v>385</v>
+        <v>67</v>
       </c>
     </row>
     <row r="138" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
-        <v>139</v>
+        <v>383</v>
       </c>
       <c r="B138" t="s">
         <v>40</v>
       </c>
       <c r="C138" s="2" t="s">
-        <v>140</v>
+        <v>384</v>
+      </c>
+      <c r="E138" t="s">
+        <v>386</v>
+      </c>
+      <c r="F138">
+        <v>1951</v>
+      </c>
+      <c r="H138" t="s">
+        <v>348</v>
+      </c>
+      <c r="I138" t="s">
+        <v>349</v>
+      </c>
+      <c r="N138" s="2" t="s">
+        <v>385</v>
       </c>
     </row>
     <row r="139" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
-        <v>329</v>
+        <v>139</v>
       </c>
       <c r="B139" t="s">
-        <v>165</v>
+        <v>40</v>
       </c>
       <c r="C139" s="2" t="s">
-        <v>328</v>
-      </c>
-      <c r="E139" t="s">
-        <v>34</v>
-      </c>
-      <c r="F139">
-        <v>1789</v>
-      </c>
-      <c r="H139" t="s">
-        <v>16</v>
-      </c>
-      <c r="I139" t="s">
-        <v>20</v>
+        <v>140</v>
       </c>
     </row>
     <row r="140" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
-        <v>172</v>
+        <v>329</v>
       </c>
       <c r="B140" t="s">
-        <v>60</v>
+        <v>165</v>
       </c>
       <c r="C140" s="2" t="s">
-        <v>171</v>
+        <v>328</v>
+      </c>
+      <c r="E140" t="s">
+        <v>34</v>
+      </c>
+      <c r="F140">
+        <v>1789</v>
+      </c>
+      <c r="H140" t="s">
+        <v>16</v>
+      </c>
+      <c r="I140" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="141" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
-        <v>217</v>
+        <v>172</v>
       </c>
       <c r="B141" t="s">
         <v>60</v>
       </c>
       <c r="C141" s="2" t="s">
-        <v>216</v>
-      </c>
-      <c r="E141" t="s">
-        <v>14</v>
-      </c>
-      <c r="F141">
-        <v>1900</v>
-      </c>
-      <c r="H141" t="s">
-        <v>16</v>
-      </c>
-      <c r="I141" t="s">
-        <v>20</v>
+        <v>171</v>
       </c>
     </row>
     <row r="142" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
-        <v>132</v>
+        <v>217</v>
       </c>
       <c r="B142" t="s">
-        <v>259</v>
+        <v>60</v>
       </c>
       <c r="C142" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="Q142" t="s">
-        <v>17</v>
+        <v>216</v>
+      </c>
+      <c r="E142" t="s">
+        <v>14</v>
+      </c>
+      <c r="F142">
+        <v>1900</v>
+      </c>
+      <c r="H142" t="s">
+        <v>16</v>
+      </c>
+      <c r="I142" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="143" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
-        <v>182</v>
+        <v>132</v>
       </c>
       <c r="B143" t="s">
-        <v>165</v>
+        <v>259</v>
       </c>
       <c r="C143" s="2" t="s">
-        <v>181</v>
+        <v>133</v>
+      </c>
+      <c r="Q143" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="144" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
-        <v>115</v>
+        <v>182</v>
       </c>
       <c r="B144" t="s">
-        <v>128</v>
+        <v>165</v>
       </c>
       <c r="C144" s="2" t="s">
-        <v>116</v>
+        <v>181</v>
       </c>
     </row>
     <row r="145" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
-        <v>263</v>
+        <v>115</v>
       </c>
       <c r="B145" t="s">
-        <v>250</v>
+        <v>128</v>
       </c>
       <c r="C145" s="2" t="s">
-        <v>264</v>
-      </c>
-      <c r="E145" t="s">
-        <v>265</v>
-      </c>
-      <c r="F145">
-        <v>1500</v>
-      </c>
-      <c r="G145">
-        <v>2000</v>
-      </c>
-      <c r="H145" t="s">
-        <v>16</v>
-      </c>
-      <c r="I145" t="s">
-        <v>20</v>
+        <v>116</v>
       </c>
     </row>
     <row r="146" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
-        <v>221</v>
+        <v>263</v>
       </c>
       <c r="B146" t="s">
-        <v>86</v>
+        <v>250</v>
       </c>
       <c r="C146" s="2" t="s">
-        <v>220</v>
+        <v>264</v>
+      </c>
+      <c r="E146" t="s">
+        <v>265</v>
       </c>
       <c r="F146">
-        <v>2013</v>
+        <v>1500</v>
+      </c>
+      <c r="G146">
+        <v>2000</v>
       </c>
       <c r="H146" t="s">
         <v>16</v>
@@ -4412,22 +4430,16 @@
     </row>
     <row r="147" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
-        <v>13</v>
+        <v>221</v>
       </c>
       <c r="B147" t="s">
-        <v>25</v>
+        <v>86</v>
       </c>
       <c r="C147" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="D147" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="E147" t="s">
-        <v>14</v>
+        <v>220</v>
       </c>
       <c r="F147">
-        <v>1981</v>
+        <v>2013</v>
       </c>
       <c r="H147" t="s">
         <v>16</v>
@@ -4438,23 +4450,49 @@
     </row>
     <row r="148" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
+        <v>13</v>
+      </c>
+      <c r="B148" t="s">
+        <v>25</v>
+      </c>
+      <c r="C148" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D148" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E148" t="s">
+        <v>14</v>
+      </c>
+      <c r="F148">
+        <v>1981</v>
+      </c>
+      <c r="H148" t="s">
+        <v>16</v>
+      </c>
+      <c r="I148" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="149" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A149" t="s">
         <v>283</v>
       </c>
-      <c r="B148" t="s">
+      <c r="B149" t="s">
         <v>124</v>
       </c>
-      <c r="C148" s="2" t="s">
+      <c r="C149" s="2" t="s">
         <v>284</v>
       </c>
-      <c r="H148" t="s">
-        <v>16</v>
-      </c>
-      <c r="I148" t="s">
+      <c r="H149" t="s">
+        <v>16</v>
+      </c>
+      <c r="I149" t="s">
         <v>20</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:Q148">
+  <sortState ref="A2:Q149">
     <sortCondition ref="A2"/>
   </sortState>
   <hyperlinks>
@@ -4462,9 +4500,9 @@
     <hyperlink ref="C57" r:id="rId2"/>
     <hyperlink ref="C7" r:id="rId3"/>
     <hyperlink ref="C10" r:id="rId4"/>
-    <hyperlink ref="C88" r:id="rId5"/>
-    <hyperlink ref="C107" r:id="rId6"/>
-    <hyperlink ref="C147" r:id="rId7"/>
+    <hyperlink ref="C89" r:id="rId5"/>
+    <hyperlink ref="C108" r:id="rId6"/>
+    <hyperlink ref="C148" r:id="rId7"/>
     <hyperlink ref="C35" r:id="rId8"/>
     <hyperlink ref="C30" r:id="rId9"/>
     <hyperlink ref="C48" r:id="rId10"/>
@@ -4474,11 +4512,11 @@
     <hyperlink ref="C59" r:id="rId14"/>
     <hyperlink ref="C83" r:id="rId15"/>
     <hyperlink ref="C29" r:id="rId16"/>
-    <hyperlink ref="C103" r:id="rId17"/>
+    <hyperlink ref="C104" r:id="rId17"/>
     <hyperlink ref="C40" r:id="rId18"/>
     <hyperlink ref="C69" r:id="rId19"/>
     <hyperlink ref="C16" r:id="rId20"/>
-    <hyperlink ref="C136" r:id="rId21"/>
+    <hyperlink ref="C137" r:id="rId21"/>
     <hyperlink ref="C8" r:id="rId22"/>
     <hyperlink ref="C38" r:id="rId23"/>
     <hyperlink ref="C52" r:id="rId24"/>
@@ -4487,75 +4525,75 @@
     <hyperlink ref="C54" r:id="rId27"/>
     <hyperlink ref="C67" r:id="rId28"/>
     <hyperlink ref="C87" r:id="rId29"/>
-    <hyperlink ref="C127" r:id="rId30"/>
-    <hyperlink ref="C91" r:id="rId31"/>
+    <hyperlink ref="C128" r:id="rId30"/>
+    <hyperlink ref="C92" r:id="rId31"/>
     <hyperlink ref="C78" r:id="rId32"/>
-    <hyperlink ref="C96" r:id="rId33"/>
+    <hyperlink ref="C97" r:id="rId33"/>
     <hyperlink ref="C68" r:id="rId34"/>
     <hyperlink ref="C17" r:id="rId35"/>
-    <hyperlink ref="C125" r:id="rId36"/>
+    <hyperlink ref="C126" r:id="rId36"/>
     <hyperlink ref="C15" r:id="rId37"/>
-    <hyperlink ref="C144" r:id="rId38"/>
+    <hyperlink ref="C145" r:id="rId38"/>
     <hyperlink ref="C82" r:id="rId39"/>
     <hyperlink ref="C56" r:id="rId40"/>
-    <hyperlink ref="C111" r:id="rId41"/>
+    <hyperlink ref="C112" r:id="rId41"/>
     <hyperlink ref="C18" r:id="rId42"/>
     <hyperlink ref="C50" r:id="rId43"/>
     <hyperlink ref="C23" r:id="rId44"/>
-    <hyperlink ref="C104" r:id="rId45"/>
-    <hyperlink ref="C142" r:id="rId46"/>
+    <hyperlink ref="C105" r:id="rId45"/>
+    <hyperlink ref="C143" r:id="rId46"/>
     <hyperlink ref="C27" r:id="rId47" display="http://comparativeconstitutionsproject.org/"/>
-    <hyperlink ref="C101" r:id="rId48"/>
-    <hyperlink ref="C138" r:id="rId49"/>
-    <hyperlink ref="C115" r:id="rId50"/>
-    <hyperlink ref="C110" r:id="rId51"/>
+    <hyperlink ref="C102" r:id="rId48"/>
+    <hyperlink ref="C139" r:id="rId49"/>
+    <hyperlink ref="C116" r:id="rId50"/>
+    <hyperlink ref="C111" r:id="rId51"/>
     <hyperlink ref="C22" r:id="rId52"/>
-    <hyperlink ref="C105" r:id="rId53"/>
+    <hyperlink ref="C106" r:id="rId53"/>
     <hyperlink ref="C47" r:id="rId54"/>
     <hyperlink ref="C72" r:id="rId55"/>
     <hyperlink ref="C75" r:id="rId56"/>
-    <hyperlink ref="C102" r:id="rId57"/>
-    <hyperlink ref="C93" r:id="rId58"/>
-    <hyperlink ref="C119" r:id="rId59"/>
+    <hyperlink ref="C103" r:id="rId57"/>
+    <hyperlink ref="C94" r:id="rId58"/>
+    <hyperlink ref="C120" r:id="rId59"/>
     <hyperlink ref="C31" r:id="rId60"/>
-    <hyperlink ref="C129" r:id="rId61"/>
+    <hyperlink ref="C130" r:id="rId61"/>
     <hyperlink ref="C9" r:id="rId62"/>
     <hyperlink ref="C33" r:id="rId63"/>
-    <hyperlink ref="C130" r:id="rId64"/>
+    <hyperlink ref="C131" r:id="rId64"/>
     <hyperlink ref="C14" r:id="rId65"/>
-    <hyperlink ref="C140" r:id="rId66"/>
+    <hyperlink ref="C141" r:id="rId66"/>
     <hyperlink ref="C25" r:id="rId67"/>
     <hyperlink ref="C24" r:id="rId68"/>
     <hyperlink ref="C26" r:id="rId69"/>
     <hyperlink ref="C51" r:id="rId70"/>
-    <hyperlink ref="C143" r:id="rId71"/>
+    <hyperlink ref="C144" r:id="rId71"/>
     <hyperlink ref="C28" r:id="rId72"/>
-    <hyperlink ref="C108" r:id="rId73"/>
+    <hyperlink ref="C109" r:id="rId73"/>
     <hyperlink ref="C32" r:id="rId74"/>
     <hyperlink ref="C44" r:id="rId75"/>
-    <hyperlink ref="C120" r:id="rId76"/>
+    <hyperlink ref="C121" r:id="rId76"/>
     <hyperlink ref="C41" r:id="rId77"/>
     <hyperlink ref="C39" r:id="rId78"/>
     <hyperlink ref="C66" r:id="rId79"/>
     <hyperlink ref="C5" r:id="rId80"/>
     <hyperlink ref="C65" r:id="rId81"/>
     <hyperlink ref="C12" r:id="rId82"/>
-    <hyperlink ref="C100" r:id="rId83"/>
-    <hyperlink ref="C109" r:id="rId84"/>
-    <hyperlink ref="C132" r:id="rId85"/>
+    <hyperlink ref="C101" r:id="rId83"/>
+    <hyperlink ref="C110" r:id="rId84"/>
+    <hyperlink ref="C133" r:id="rId85"/>
     <hyperlink ref="C36" r:id="rId86"/>
-    <hyperlink ref="C141" r:id="rId87"/>
+    <hyperlink ref="C142" r:id="rId87"/>
     <hyperlink ref="C43" r:id="rId88"/>
-    <hyperlink ref="C146" r:id="rId89"/>
-    <hyperlink ref="C89" r:id="rId90"/>
+    <hyperlink ref="C147" r:id="rId89"/>
+    <hyperlink ref="C90" r:id="rId90"/>
     <hyperlink ref="C63" r:id="rId91"/>
-    <hyperlink ref="C90" r:id="rId92"/>
-    <hyperlink ref="C123" r:id="rId93"/>
+    <hyperlink ref="C91" r:id="rId92"/>
+    <hyperlink ref="C124" r:id="rId93"/>
     <hyperlink ref="C76" r:id="rId94"/>
-    <hyperlink ref="C94" r:id="rId95"/>
-    <hyperlink ref="C124" r:id="rId96"/>
+    <hyperlink ref="C95" r:id="rId95"/>
+    <hyperlink ref="C125" r:id="rId96"/>
     <hyperlink ref="C60" r:id="rId97"/>
-    <hyperlink ref="C106" r:id="rId98"/>
+    <hyperlink ref="C107" r:id="rId98"/>
     <hyperlink ref="C45" r:id="rId99"/>
     <hyperlink ref="C42" r:id="rId100"/>
     <hyperlink ref="C79" r:id="rId101"/>
@@ -4563,39 +4601,39 @@
     <hyperlink ref="C2" r:id="rId103"/>
     <hyperlink ref="C73" r:id="rId104"/>
     <hyperlink ref="C77" r:id="rId105"/>
-    <hyperlink ref="C98" r:id="rId106"/>
+    <hyperlink ref="C99" r:id="rId106"/>
     <hyperlink ref="C46" r:id="rId107"/>
     <hyperlink ref="C80" r:id="rId108"/>
-    <hyperlink ref="C122" r:id="rId109"/>
+    <hyperlink ref="C123" r:id="rId109"/>
     <hyperlink ref="C13" r:id="rId110"/>
     <hyperlink ref="C4" r:id="rId111"/>
-    <hyperlink ref="C145" r:id="rId112"/>
+    <hyperlink ref="C146" r:id="rId112"/>
     <hyperlink ref="C86" r:id="rId113"/>
     <hyperlink ref="C81" r:id="rId114"/>
-    <hyperlink ref="C135" r:id="rId115"/>
-    <hyperlink ref="C118" r:id="rId116"/>
+    <hyperlink ref="C136" r:id="rId115"/>
+    <hyperlink ref="C119" r:id="rId116"/>
     <hyperlink ref="C62" r:id="rId117"/>
-    <hyperlink ref="C92" r:id="rId118"/>
+    <hyperlink ref="C93" r:id="rId118"/>
     <hyperlink ref="C71" r:id="rId119"/>
-    <hyperlink ref="C148" r:id="rId120"/>
+    <hyperlink ref="C149" r:id="rId120"/>
     <hyperlink ref="C64" r:id="rId121"/>
-    <hyperlink ref="C117" r:id="rId122"/>
-    <hyperlink ref="C97" r:id="rId123"/>
+    <hyperlink ref="C118" r:id="rId122"/>
+    <hyperlink ref="C98" r:id="rId123"/>
     <hyperlink ref="C74" r:id="rId124"/>
-    <hyperlink ref="C95" r:id="rId125"/>
-    <hyperlink ref="C121" r:id="rId126"/>
+    <hyperlink ref="C96" r:id="rId125"/>
+    <hyperlink ref="C122" r:id="rId126"/>
     <hyperlink ref="C84" r:id="rId127"/>
     <hyperlink ref="C11" r:id="rId128"/>
     <hyperlink ref="C19" r:id="rId129"/>
-    <hyperlink ref="C116" r:id="rId130"/>
+    <hyperlink ref="C117" r:id="rId130"/>
     <hyperlink ref="C70" r:id="rId131"/>
-    <hyperlink ref="C128" r:id="rId132"/>
-    <hyperlink ref="C113" r:id="rId133"/>
-    <hyperlink ref="C112" r:id="rId134"/>
-    <hyperlink ref="C114" r:id="rId135"/>
-    <hyperlink ref="C134" r:id="rId136"/>
-    <hyperlink ref="C126" r:id="rId137"/>
-    <hyperlink ref="C139" r:id="rId138"/>
+    <hyperlink ref="C129" r:id="rId132"/>
+    <hyperlink ref="C114" r:id="rId133"/>
+    <hyperlink ref="C113" r:id="rId134"/>
+    <hyperlink ref="C115" r:id="rId135"/>
+    <hyperlink ref="C135" r:id="rId136"/>
+    <hyperlink ref="C127" r:id="rId137"/>
+    <hyperlink ref="C140" r:id="rId138"/>
     <hyperlink ref="C37" r:id="rId139"/>
     <hyperlink ref="C85" r:id="rId140"/>
     <hyperlink ref="J2" r:id="rId141"/>
@@ -4605,23 +4643,24 @@
     <hyperlink ref="J4" r:id="rId145"/>
     <hyperlink ref="P5" r:id="rId146"/>
     <hyperlink ref="J5" r:id="rId147"/>
-    <hyperlink ref="C99" r:id="rId148"/>
+    <hyperlink ref="C100" r:id="rId148"/>
     <hyperlink ref="C34" r:id="rId149"/>
     <hyperlink ref="P7" r:id="rId150"/>
     <hyperlink ref="J7" r:id="rId151"/>
     <hyperlink ref="M8" r:id="rId152"/>
     <hyperlink ref="L8" r:id="rId153"/>
     <hyperlink ref="J8" r:id="rId154"/>
-    <hyperlink ref="C137" r:id="rId155"/>
-    <hyperlink ref="N137" r:id="rId156"/>
+    <hyperlink ref="C138" r:id="rId155"/>
+    <hyperlink ref="N138" r:id="rId156"/>
     <hyperlink ref="C21" r:id="rId157"/>
     <hyperlink ref="N21" r:id="rId158"/>
     <hyperlink ref="C61" r:id="rId159"/>
-    <hyperlink ref="C133" r:id="rId160"/>
-    <hyperlink ref="J133" r:id="rId161"/>
-    <hyperlink ref="C131" r:id="rId162"/>
-    <hyperlink ref="N131" r:id="rId163"/>
-    <hyperlink ref="J131" r:id="rId164"/>
+    <hyperlink ref="C134" r:id="rId160"/>
+    <hyperlink ref="J134" r:id="rId161"/>
+    <hyperlink ref="C132" r:id="rId162"/>
+    <hyperlink ref="N132" r:id="rId163"/>
+    <hyperlink ref="J132" r:id="rId164"/>
+    <hyperlink ref="C88" r:id="rId165"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
add Latent Human Rights Protection Scores
</commit_message>
<xml_diff>
--- a/PolData.xlsx
+++ b/PolData.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="738" uniqueCount="406">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="745" uniqueCount="409">
   <si>
     <t>name</t>
   </si>
@@ -1245,6 +1245,15 @@
   </si>
   <si>
     <t>Military experiences, childhood, education, personal, family life</t>
+  </si>
+  <si>
+    <t>http://dx.doi.org/10.7910/DVN/24872</t>
+  </si>
+  <si>
+    <t>Latent Human Rights Protection Scores</t>
+  </si>
+  <si>
+    <t>Accountability, repression, human rights</t>
   </si>
 </sst>
 </file>
@@ -1584,10 +1593,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q149"/>
+  <dimension ref="A1:Q150"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
-      <selection activeCell="A88" sqref="A88"/>
+    <sheetView tabSelected="1" topLeftCell="A125" workbookViewId="0">
+      <selection activeCell="A87" sqref="A87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3263,114 +3272,120 @@
     </row>
     <row r="87" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>96</v>
+        <v>407</v>
       </c>
       <c r="B87" t="s">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>90</v>
+        <v>406</v>
+      </c>
+      <c r="D87" t="s">
+        <v>408</v>
       </c>
       <c r="E87" t="s">
-        <v>69</v>
+        <v>14</v>
       </c>
       <c r="F87">
-        <v>1995</v>
+        <v>1949</v>
+      </c>
+      <c r="G87">
+        <v>2013</v>
+      </c>
+      <c r="H87" t="s">
+        <v>348</v>
+      </c>
+      <c r="I87" t="s">
+        <v>349</v>
       </c>
     </row>
     <row r="88" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>404</v>
+        <v>96</v>
       </c>
       <c r="B88" t="s">
-        <v>83</v>
+        <v>25</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>403</v>
-      </c>
-      <c r="D88" t="s">
-        <v>405</v>
+        <v>90</v>
       </c>
       <c r="E88" t="s">
-        <v>14</v>
+        <v>69</v>
       </c>
       <c r="F88">
-        <v>1875</v>
-      </c>
-      <c r="G88">
-        <v>2004</v>
-      </c>
-      <c r="H88" t="s">
-        <v>348</v>
-      </c>
-      <c r="I88" t="s">
-        <v>349</v>
+        <v>1995</v>
       </c>
     </row>
     <row r="89" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>11</v>
+        <v>404</v>
       </c>
       <c r="B89" t="s">
-        <v>25</v>
+        <v>83</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>12</v>
+        <v>403</v>
       </c>
       <c r="D89" t="s">
-        <v>95</v>
+        <v>405</v>
       </c>
       <c r="E89" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="F89">
-        <v>2007</v>
+        <v>1875</v>
+      </c>
+      <c r="G89">
+        <v>2004</v>
       </c>
       <c r="H89" t="s">
-        <v>16</v>
+        <v>348</v>
       </c>
       <c r="I89" t="s">
-        <v>21</v>
+        <v>349</v>
       </c>
     </row>
     <row r="90" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>223</v>
+        <v>11</v>
       </c>
       <c r="B90" t="s">
-        <v>124</v>
+        <v>25</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>222</v>
+        <v>12</v>
+      </c>
+      <c r="D90" t="s">
+        <v>95</v>
+      </c>
+      <c r="E90" t="s">
+        <v>10</v>
       </c>
       <c r="F90">
-        <v>1</v>
-      </c>
-      <c r="G90">
-        <v>2010</v>
+        <v>2007</v>
       </c>
       <c r="H90" t="s">
         <v>16</v>
       </c>
       <c r="I90" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="91" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="B91" t="s">
-        <v>40</v>
+        <v>124</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="F91">
-        <v>1946</v>
+        <v>1</v>
       </c>
       <c r="G91">
-        <v>2016</v>
+        <v>2010</v>
       </c>
       <c r="H91" t="s">
         <v>16</v>
@@ -3381,90 +3396,90 @@
     </row>
     <row r="92" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>97</v>
+        <v>226</v>
       </c>
       <c r="B92" t="s">
-        <v>128</v>
+        <v>40</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>98</v>
+        <v>225</v>
+      </c>
+      <c r="F92">
+        <v>1946</v>
+      </c>
+      <c r="G92">
+        <v>2016</v>
+      </c>
+      <c r="H92" t="s">
+        <v>16</v>
+      </c>
+      <c r="I92" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="93" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>278</v>
+        <v>97</v>
       </c>
       <c r="B93" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>279</v>
-      </c>
-      <c r="E93" t="s">
-        <v>280</v>
-      </c>
-      <c r="F93">
-        <v>1890</v>
-      </c>
-      <c r="G93">
-        <v>1996</v>
-      </c>
-      <c r="H93" t="s">
-        <v>16</v>
-      </c>
-      <c r="I93" t="s">
-        <v>20</v>
+        <v>98</v>
       </c>
     </row>
     <row r="94" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>156</v>
+        <v>278</v>
       </c>
       <c r="B94" t="s">
-        <v>25</v>
+        <v>124</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>154</v>
+        <v>279</v>
+      </c>
+      <c r="E94" t="s">
+        <v>280</v>
+      </c>
+      <c r="F94">
+        <v>1890</v>
+      </c>
+      <c r="G94">
+        <v>1996</v>
+      </c>
+      <c r="H94" t="s">
+        <v>16</v>
+      </c>
+      <c r="I94" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="95" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>229</v>
+        <v>156</v>
       </c>
       <c r="B95" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>225</v>
-      </c>
-      <c r="F95">
-        <v>1952</v>
-      </c>
-      <c r="G95">
-        <v>1997</v>
-      </c>
-      <c r="H95" t="s">
-        <v>16</v>
-      </c>
-      <c r="I95" t="s">
-        <v>20</v>
+        <v>154</v>
       </c>
     </row>
     <row r="96" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>293</v>
+        <v>229</v>
       </c>
       <c r="B96" t="s">
         <v>40</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>294</v>
+        <v>225</v>
       </c>
       <c r="F96">
-        <v>2004</v>
+        <v>1952</v>
       </c>
       <c r="G96">
-        <v>2006</v>
+        <v>1997</v>
       </c>
       <c r="H96" t="s">
         <v>16</v>
@@ -3475,221 +3490,218 @@
     </row>
     <row r="97" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>102</v>
+        <v>293</v>
       </c>
       <c r="B97" t="s">
-        <v>99</v>
+        <v>40</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>103</v>
+        <v>294</v>
+      </c>
+      <c r="F97">
+        <v>2004</v>
+      </c>
+      <c r="G97">
+        <v>2006</v>
+      </c>
+      <c r="H97" t="s">
+        <v>16</v>
+      </c>
+      <c r="I97" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="98" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>289</v>
+        <v>102</v>
       </c>
       <c r="B98" t="s">
-        <v>124</v>
+        <v>99</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>290</v>
+        <v>103</v>
       </c>
     </row>
     <row r="99" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>246</v>
+        <v>289</v>
       </c>
       <c r="B99" t="s">
-        <v>165</v>
+        <v>124</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>247</v>
-      </c>
-      <c r="E99" t="s">
-        <v>14</v>
-      </c>
-      <c r="F99">
-        <v>1960</v>
-      </c>
-      <c r="G99">
-        <v>2006</v>
-      </c>
-      <c r="H99" t="s">
-        <v>16</v>
-      </c>
-      <c r="I99" t="s">
-        <v>249</v>
+        <v>290</v>
       </c>
     </row>
     <row r="100" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>365</v>
+        <v>246</v>
       </c>
       <c r="B100" t="s">
-        <v>128</v>
+        <v>165</v>
       </c>
       <c r="C100" s="2" t="s">
-        <v>364</v>
-      </c>
-      <c r="D100" t="s">
-        <v>370</v>
+        <v>247</v>
       </c>
       <c r="E100" t="s">
-        <v>366</v>
+        <v>14</v>
       </c>
       <c r="F100">
-        <v>1906</v>
+        <v>1960</v>
       </c>
       <c r="G100">
-        <v>2013</v>
+        <v>2006</v>
       </c>
       <c r="H100" t="s">
-        <v>367</v>
+        <v>16</v>
       </c>
       <c r="I100" t="s">
-        <v>368</v>
-      </c>
-      <c r="Q100" t="s">
-        <v>369</v>
+        <v>249</v>
       </c>
     </row>
     <row r="101" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>208</v>
+        <v>365</v>
       </c>
       <c r="B101" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>209</v>
+        <v>364</v>
+      </c>
+      <c r="D101" t="s">
+        <v>370</v>
+      </c>
+      <c r="E101" t="s">
+        <v>366</v>
       </c>
       <c r="F101">
-        <v>1932</v>
+        <v>1906</v>
       </c>
       <c r="G101">
-        <v>2014</v>
+        <v>2013</v>
       </c>
       <c r="H101" t="s">
-        <v>16</v>
+        <v>367</v>
       </c>
       <c r="I101" t="s">
-        <v>20</v>
+        <v>368</v>
+      </c>
+      <c r="Q101" t="s">
+        <v>369</v>
       </c>
     </row>
     <row r="102" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>137</v>
+        <v>208</v>
       </c>
       <c r="B102" t="s">
-        <v>259</v>
+        <v>124</v>
       </c>
       <c r="C102" s="2" t="s">
-        <v>138</v>
+        <v>209</v>
+      </c>
+      <c r="F102">
+        <v>1932</v>
+      </c>
+      <c r="G102">
+        <v>2014</v>
+      </c>
+      <c r="H102" t="s">
+        <v>16</v>
+      </c>
+      <c r="I102" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="103" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>155</v>
+        <v>137</v>
       </c>
       <c r="B103" t="s">
         <v>259</v>
       </c>
       <c r="C103" s="2" t="s">
-        <v>154</v>
+        <v>138</v>
       </c>
     </row>
     <row r="104" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>57</v>
+        <v>155</v>
       </c>
       <c r="B104" t="s">
-        <v>128</v>
+        <v>259</v>
       </c>
       <c r="C104" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="Q104" t="s">
-        <v>17</v>
+        <v>154</v>
       </c>
     </row>
     <row r="105" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>129</v>
+        <v>57</v>
       </c>
       <c r="B105" t="s">
-        <v>259</v>
+        <v>128</v>
       </c>
       <c r="C105" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="E105" t="s">
-        <v>131</v>
-      </c>
-      <c r="F105">
-        <v>1945</v>
-      </c>
-      <c r="G105">
-        <v>2008</v>
-      </c>
-      <c r="I105" t="s">
-        <v>20</v>
+        <v>58</v>
+      </c>
+      <c r="Q105" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="106" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>148</v>
+        <v>129</v>
       </c>
       <c r="B106" t="s">
-        <v>128</v>
+        <v>259</v>
       </c>
       <c r="C106" s="2" t="s">
-        <v>147</v>
+        <v>130</v>
+      </c>
+      <c r="E106" t="s">
+        <v>131</v>
+      </c>
+      <c r="F106">
+        <v>1945</v>
+      </c>
+      <c r="G106">
+        <v>2008</v>
+      </c>
+      <c r="I106" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="107" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>233</v>
+        <v>148</v>
       </c>
       <c r="B107" t="s">
-        <v>165</v>
+        <v>128</v>
       </c>
       <c r="C107" s="2" t="s">
-        <v>234</v>
-      </c>
-      <c r="E107" t="s">
-        <v>14</v>
-      </c>
-      <c r="F107">
-        <v>2012</v>
-      </c>
-      <c r="G107">
-        <v>2016</v>
-      </c>
-      <c r="H107" t="s">
-        <v>16</v>
-      </c>
-      <c r="I107" t="s">
-        <v>20</v>
+        <v>147</v>
       </c>
     </row>
     <row r="108" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>35</v>
+        <v>233</v>
       </c>
       <c r="B108" t="s">
-        <v>25</v>
+        <v>165</v>
       </c>
       <c r="C108" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="D108" t="s">
-        <v>37</v>
+        <v>234</v>
       </c>
       <c r="E108" t="s">
         <v>14</v>
       </c>
       <c r="F108">
-        <v>2001</v>
+        <v>2012</v>
+      </c>
+      <c r="G108">
+        <v>2016</v>
       </c>
       <c r="H108" t="s">
         <v>16</v>
@@ -3700,90 +3712,90 @@
     </row>
     <row r="109" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>185</v>
+        <v>35</v>
       </c>
       <c r="B109" t="s">
-        <v>128</v>
+        <v>25</v>
       </c>
       <c r="C109" s="2" t="s">
-        <v>186</v>
+        <v>36</v>
+      </c>
+      <c r="D109" t="s">
+        <v>37</v>
+      </c>
+      <c r="E109" t="s">
+        <v>14</v>
+      </c>
+      <c r="F109">
+        <v>2001</v>
+      </c>
+      <c r="H109" t="s">
+        <v>16</v>
+      </c>
+      <c r="I109" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="110" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>210</v>
+        <v>185</v>
       </c>
       <c r="B110" t="s">
-        <v>40</v>
+        <v>128</v>
       </c>
       <c r="C110" s="2" t="s">
-        <v>211</v>
-      </c>
-      <c r="F110">
-        <v>1976</v>
-      </c>
-      <c r="G110">
-        <v>2016</v>
-      </c>
-      <c r="H110" t="s">
-        <v>16</v>
-      </c>
-      <c r="I110" t="s">
-        <v>20</v>
+        <v>186</v>
       </c>
     </row>
     <row r="111" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>144</v>
+        <v>210</v>
       </c>
       <c r="B111" t="s">
-        <v>60</v>
+        <v>40</v>
       </c>
       <c r="C111" s="2" t="s">
-        <v>143</v>
+        <v>211</v>
       </c>
       <c r="F111">
-        <v>1800</v>
+        <v>1976</v>
       </c>
       <c r="G111">
-        <v>2013</v>
+        <v>2016</v>
+      </c>
+      <c r="H111" t="s">
+        <v>16</v>
+      </c>
+      <c r="I111" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="112" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>122</v>
+        <v>144</v>
       </c>
       <c r="B112" t="s">
-        <v>259</v>
+        <v>60</v>
       </c>
       <c r="C112" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="I112" t="s">
-        <v>20</v>
+        <v>143</v>
+      </c>
+      <c r="F112">
+        <v>1800</v>
+      </c>
+      <c r="G112">
+        <v>2013</v>
       </c>
     </row>
     <row r="113" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>318</v>
+        <v>122</v>
       </c>
       <c r="B113" t="s">
-        <v>250</v>
+        <v>259</v>
       </c>
       <c r="C113" s="2" t="s">
-        <v>319</v>
-      </c>
-      <c r="E113" t="s">
-        <v>320</v>
-      </c>
-      <c r="F113">
-        <v>1975</v>
-      </c>
-      <c r="G113">
-        <v>1989</v>
-      </c>
-      <c r="H113" t="s">
-        <v>16</v>
+        <v>121</v>
       </c>
       <c r="I113" t="s">
         <v>20</v>
@@ -3791,22 +3803,22 @@
     </row>
     <row r="114" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="B114" t="s">
         <v>250</v>
       </c>
       <c r="C114" s="2" t="s">
-        <v>317</v>
+        <v>319</v>
       </c>
       <c r="E114" t="s">
-        <v>105</v>
+        <v>320</v>
       </c>
       <c r="F114">
-        <v>1950</v>
+        <v>1975</v>
       </c>
       <c r="G114">
-        <v>1996</v>
+        <v>1989</v>
       </c>
       <c r="H114" t="s">
         <v>16</v>
@@ -3817,19 +3829,22 @@
     </row>
     <row r="115" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>322</v>
+        <v>316</v>
       </c>
       <c r="B115" t="s">
-        <v>25</v>
+        <v>250</v>
       </c>
       <c r="C115" s="2" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="E115" t="s">
-        <v>77</v>
+        <v>105</v>
       </c>
       <c r="F115">
-        <v>2010</v>
+        <v>1950</v>
+      </c>
+      <c r="G115">
+        <v>1996</v>
       </c>
       <c r="H115" t="s">
         <v>16</v>
@@ -3840,164 +3855,164 @@
     </row>
     <row r="116" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>141</v>
+        <v>322</v>
       </c>
       <c r="B116" t="s">
-        <v>237</v>
+        <v>25</v>
       </c>
       <c r="C116" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="Q116" t="s">
-        <v>17</v>
+        <v>321</v>
+      </c>
+      <c r="E116" t="s">
+        <v>77</v>
+      </c>
+      <c r="F116">
+        <v>2010</v>
+      </c>
+      <c r="H116" t="s">
+        <v>16</v>
+      </c>
+      <c r="I116" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="117" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>308</v>
+        <v>141</v>
       </c>
       <c r="B117" t="s">
-        <v>250</v>
+        <v>237</v>
       </c>
       <c r="C117" s="2" t="s">
-        <v>309</v>
-      </c>
-      <c r="E117" t="s">
-        <v>310</v>
-      </c>
-      <c r="F117">
-        <v>1950</v>
-      </c>
-      <c r="G117">
-        <v>2010</v>
-      </c>
-      <c r="H117" t="s">
-        <v>16</v>
-      </c>
-      <c r="I117" t="s">
-        <v>20</v>
+        <v>142</v>
+      </c>
+      <c r="Q117" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="118" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>287</v>
+        <v>308</v>
       </c>
       <c r="B118" t="s">
-        <v>134</v>
+        <v>250</v>
       </c>
       <c r="C118" s="2" t="s">
-        <v>288</v>
+        <v>309</v>
+      </c>
+      <c r="E118" t="s">
+        <v>310</v>
       </c>
       <c r="F118">
-        <v>1990</v>
+        <v>1950</v>
       </c>
       <c r="G118">
-        <v>2008</v>
+        <v>2010</v>
+      </c>
+      <c r="H118" t="s">
+        <v>16</v>
+      </c>
+      <c r="I118" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="119" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>274</v>
+        <v>287</v>
       </c>
       <c r="B119" t="s">
-        <v>55</v>
+        <v>134</v>
       </c>
       <c r="C119" s="2" t="s">
-        <v>275</v>
-      </c>
-      <c r="H119" t="s">
-        <v>16</v>
-      </c>
-      <c r="I119" t="s">
-        <v>20</v>
+        <v>288</v>
+      </c>
+      <c r="F119">
+        <v>1990</v>
+      </c>
+      <c r="G119">
+        <v>2008</v>
       </c>
     </row>
     <row r="120" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>157</v>
+        <v>274</v>
       </c>
       <c r="B120" t="s">
-        <v>128</v>
+        <v>55</v>
       </c>
       <c r="C120" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="Q120" t="s">
-        <v>18</v>
+        <v>275</v>
+      </c>
+      <c r="H120" t="s">
+        <v>16</v>
+      </c>
+      <c r="I120" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="121" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>194</v>
+        <v>157</v>
       </c>
       <c r="B121" t="s">
-        <v>99</v>
+        <v>128</v>
       </c>
       <c r="C121" s="2" t="s">
-        <v>193</v>
+        <v>154</v>
+      </c>
+      <c r="Q121" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="122" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>295</v>
+        <v>194</v>
       </c>
       <c r="B122" t="s">
-        <v>40</v>
+        <v>99</v>
       </c>
       <c r="C122" s="2" t="s">
-        <v>296</v>
-      </c>
-      <c r="E122" t="s">
-        <v>297</v>
-      </c>
-      <c r="F122">
-        <v>1990</v>
-      </c>
-      <c r="G122">
-        <v>2015</v>
-      </c>
-      <c r="H122" t="s">
-        <v>16</v>
-      </c>
-      <c r="I122" t="s">
-        <v>249</v>
+        <v>193</v>
       </c>
     </row>
     <row r="123" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>256</v>
+        <v>295</v>
       </c>
       <c r="B123" t="s">
-        <v>250</v>
+        <v>40</v>
       </c>
       <c r="C123" s="2" t="s">
-        <v>257</v>
+        <v>296</v>
       </c>
       <c r="E123" t="s">
-        <v>258</v>
+        <v>297</v>
+      </c>
+      <c r="F123">
+        <v>1990</v>
+      </c>
+      <c r="G123">
+        <v>2015</v>
       </c>
       <c r="H123" t="s">
         <v>16</v>
       </c>
       <c r="I123" t="s">
-        <v>20</v>
+        <v>249</v>
       </c>
     </row>
     <row r="124" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>227</v>
+        <v>256</v>
       </c>
       <c r="B124" t="s">
-        <v>40</v>
+        <v>250</v>
       </c>
       <c r="C124" s="2" t="s">
-        <v>225</v>
-      </c>
-      <c r="F124">
-        <v>1955</v>
-      </c>
-      <c r="G124">
-        <v>2016</v>
+        <v>257</v>
+      </c>
+      <c r="E124" t="s">
+        <v>258</v>
       </c>
       <c r="H124" t="s">
         <v>16</v>
@@ -4008,7 +4023,7 @@
     </row>
     <row r="125" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="B125" t="s">
         <v>40</v>
@@ -4017,7 +4032,7 @@
         <v>225</v>
       </c>
       <c r="F125">
-        <v>1995</v>
+        <v>1955</v>
       </c>
       <c r="G125">
         <v>2016</v>
@@ -4031,228 +4046,228 @@
     </row>
     <row r="126" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>109</v>
+        <v>230</v>
       </c>
       <c r="B126" t="s">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="C126" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="E126" t="s">
-        <v>111</v>
+        <v>225</v>
       </c>
       <c r="F126">
-        <v>1956</v>
+        <v>1995</v>
+      </c>
+      <c r="G126">
+        <v>2016</v>
+      </c>
+      <c r="H126" t="s">
+        <v>16</v>
+      </c>
+      <c r="I126" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="127" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>326</v>
+        <v>109</v>
       </c>
       <c r="B127" t="s">
         <v>25</v>
       </c>
       <c r="C127" s="2" t="s">
-        <v>327</v>
+        <v>110</v>
       </c>
       <c r="E127" t="s">
         <v>111</v>
       </c>
       <c r="F127">
-        <v>1998</v>
-      </c>
-      <c r="H127" t="s">
-        <v>16</v>
-      </c>
-      <c r="I127" t="s">
-        <v>20</v>
+        <v>1956</v>
       </c>
     </row>
     <row r="128" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>91</v>
+        <v>326</v>
       </c>
       <c r="B128" t="s">
         <v>25</v>
       </c>
       <c r="C128" s="2" t="s">
-        <v>93</v>
+        <v>327</v>
       </c>
       <c r="E128" t="s">
-        <v>92</v>
+        <v>111</v>
       </c>
       <c r="F128">
-        <v>1999</v>
+        <v>1998</v>
+      </c>
+      <c r="H128" t="s">
+        <v>16</v>
+      </c>
+      <c r="I128" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="129" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>314</v>
+        <v>91</v>
       </c>
       <c r="B129" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="C129" s="2" t="s">
-        <v>313</v>
+        <v>93</v>
       </c>
       <c r="E129" t="s">
-        <v>315</v>
+        <v>92</v>
       </c>
       <c r="F129">
-        <v>1950</v>
-      </c>
-      <c r="G129">
-        <v>2004</v>
-      </c>
-      <c r="H129" t="s">
-        <v>16</v>
-      </c>
-      <c r="I129" t="s">
-        <v>20</v>
+        <v>1999</v>
       </c>
     </row>
     <row r="130" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
-        <v>161</v>
+        <v>314</v>
       </c>
       <c r="B130" t="s">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="C130" s="2" t="s">
-        <v>160</v>
+        <v>313</v>
+      </c>
+      <c r="E130" t="s">
+        <v>315</v>
+      </c>
+      <c r="F130">
+        <v>1950</v>
+      </c>
+      <c r="G130">
+        <v>2004</v>
+      </c>
+      <c r="H130" t="s">
+        <v>16</v>
+      </c>
+      <c r="I130" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="131" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="B131" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="C131" s="2" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
     </row>
     <row r="132" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>399</v>
+        <v>168</v>
       </c>
       <c r="B132" t="s">
         <v>40</v>
       </c>
       <c r="C132" s="2" t="s">
-        <v>400</v>
-      </c>
-      <c r="E132" t="s">
-        <v>14</v>
-      </c>
-      <c r="F132">
-        <v>2000</v>
-      </c>
-      <c r="G132">
-        <v>2014</v>
-      </c>
-      <c r="H132" t="s">
-        <v>348</v>
-      </c>
-      <c r="I132" t="s">
-        <v>349</v>
-      </c>
-      <c r="J132" s="2" t="s">
-        <v>402</v>
-      </c>
-      <c r="N132" s="2" t="s">
-        <v>401</v>
+        <v>167</v>
       </c>
     </row>
     <row r="133" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
-        <v>213</v>
+        <v>399</v>
       </c>
       <c r="B133" t="s">
-        <v>55</v>
+        <v>40</v>
       </c>
       <c r="C133" s="2" t="s">
-        <v>212</v>
+        <v>400</v>
+      </c>
+      <c r="E133" t="s">
+        <v>14</v>
+      </c>
+      <c r="F133">
+        <v>2000</v>
+      </c>
+      <c r="G133">
+        <v>2014</v>
       </c>
       <c r="H133" t="s">
-        <v>16</v>
+        <v>348</v>
       </c>
       <c r="I133" t="s">
-        <v>20</v>
+        <v>349</v>
+      </c>
+      <c r="J133" s="2" t="s">
+        <v>402</v>
+      </c>
+      <c r="N133" s="2" t="s">
+        <v>401</v>
       </c>
     </row>
     <row r="134" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
-        <v>395</v>
+        <v>213</v>
       </c>
       <c r="B134" t="s">
-        <v>25</v>
+        <v>55</v>
       </c>
       <c r="C134" s="2" t="s">
-        <v>394</v>
-      </c>
-      <c r="D134" t="s">
-        <v>396</v>
-      </c>
-      <c r="E134" t="s">
-        <v>111</v>
-      </c>
-      <c r="F134">
-        <v>1986</v>
-      </c>
-      <c r="G134">
-        <v>2015</v>
+        <v>212</v>
       </c>
       <c r="H134" t="s">
-        <v>367</v>
+        <v>16</v>
       </c>
       <c r="I134" t="s">
-        <v>398</v>
-      </c>
-      <c r="J134" s="2" t="s">
-        <v>397</v>
+        <v>20</v>
       </c>
     </row>
     <row r="135" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
-        <v>323</v>
+        <v>395</v>
       </c>
       <c r="B135" t="s">
         <v>25</v>
       </c>
       <c r="C135" s="2" t="s">
-        <v>324</v>
+        <v>394</v>
+      </c>
+      <c r="D135" t="s">
+        <v>396</v>
       </c>
       <c r="E135" t="s">
-        <v>325</v>
+        <v>111</v>
       </c>
       <c r="F135">
-        <v>1942</v>
+        <v>1986</v>
+      </c>
+      <c r="G135">
+        <v>2015</v>
       </c>
       <c r="H135" t="s">
-        <v>16</v>
+        <v>367</v>
       </c>
       <c r="I135" t="s">
-        <v>20</v>
+        <v>398</v>
+      </c>
+      <c r="J135" s="2" t="s">
+        <v>397</v>
       </c>
     </row>
     <row r="136" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
-        <v>273</v>
+        <v>323</v>
       </c>
       <c r="B136" t="s">
-        <v>237</v>
+        <v>25</v>
       </c>
       <c r="C136" s="2" t="s">
-        <v>272</v>
+        <v>324</v>
+      </c>
+      <c r="E136" t="s">
+        <v>325</v>
       </c>
       <c r="F136">
-        <v>1996</v>
-      </c>
-      <c r="G136">
-        <v>2016</v>
+        <v>1942</v>
       </c>
       <c r="H136" t="s">
         <v>16</v>
@@ -4263,183 +4278,186 @@
     </row>
     <row r="137" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
-        <v>66</v>
+        <v>273</v>
       </c>
       <c r="B137" t="s">
-        <v>25</v>
+        <v>237</v>
       </c>
       <c r="C137" s="2" t="s">
-        <v>67</v>
+        <v>272</v>
+      </c>
+      <c r="F137">
+        <v>1996</v>
+      </c>
+      <c r="G137">
+        <v>2016</v>
+      </c>
+      <c r="H137" t="s">
+        <v>16</v>
+      </c>
+      <c r="I137" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="138" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
-        <v>383</v>
+        <v>66</v>
       </c>
       <c r="B138" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="C138" s="2" t="s">
-        <v>384</v>
-      </c>
-      <c r="E138" t="s">
-        <v>386</v>
-      </c>
-      <c r="F138">
-        <v>1951</v>
-      </c>
-      <c r="H138" t="s">
-        <v>348</v>
-      </c>
-      <c r="I138" t="s">
-        <v>349</v>
-      </c>
-      <c r="N138" s="2" t="s">
-        <v>385</v>
+        <v>67</v>
       </c>
     </row>
     <row r="139" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
-        <v>139</v>
+        <v>383</v>
       </c>
       <c r="B139" t="s">
         <v>40</v>
       </c>
       <c r="C139" s="2" t="s">
-        <v>140</v>
+        <v>384</v>
+      </c>
+      <c r="E139" t="s">
+        <v>386</v>
+      </c>
+      <c r="F139">
+        <v>1951</v>
+      </c>
+      <c r="H139" t="s">
+        <v>348</v>
+      </c>
+      <c r="I139" t="s">
+        <v>349</v>
+      </c>
+      <c r="N139" s="2" t="s">
+        <v>385</v>
       </c>
     </row>
     <row r="140" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
-        <v>329</v>
+        <v>139</v>
       </c>
       <c r="B140" t="s">
-        <v>165</v>
+        <v>40</v>
       </c>
       <c r="C140" s="2" t="s">
-        <v>328</v>
-      </c>
-      <c r="E140" t="s">
-        <v>34</v>
-      </c>
-      <c r="F140">
-        <v>1789</v>
-      </c>
-      <c r="H140" t="s">
-        <v>16</v>
-      </c>
-      <c r="I140" t="s">
-        <v>20</v>
+        <v>140</v>
       </c>
     </row>
     <row r="141" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
-        <v>172</v>
+        <v>329</v>
       </c>
       <c r="B141" t="s">
-        <v>60</v>
+        <v>165</v>
       </c>
       <c r="C141" s="2" t="s">
-        <v>171</v>
+        <v>328</v>
+      </c>
+      <c r="E141" t="s">
+        <v>34</v>
+      </c>
+      <c r="F141">
+        <v>1789</v>
+      </c>
+      <c r="H141" t="s">
+        <v>16</v>
+      </c>
+      <c r="I141" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="142" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
-        <v>217</v>
+        <v>172</v>
       </c>
       <c r="B142" t="s">
         <v>60</v>
       </c>
       <c r="C142" s="2" t="s">
-        <v>216</v>
-      </c>
-      <c r="E142" t="s">
-        <v>14</v>
-      </c>
-      <c r="F142">
-        <v>1900</v>
-      </c>
-      <c r="H142" t="s">
-        <v>16</v>
-      </c>
-      <c r="I142" t="s">
-        <v>20</v>
+        <v>171</v>
       </c>
     </row>
     <row r="143" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
-        <v>132</v>
+        <v>217</v>
       </c>
       <c r="B143" t="s">
-        <v>259</v>
+        <v>60</v>
       </c>
       <c r="C143" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="Q143" t="s">
-        <v>17</v>
+        <v>216</v>
+      </c>
+      <c r="E143" t="s">
+        <v>14</v>
+      </c>
+      <c r="F143">
+        <v>1900</v>
+      </c>
+      <c r="H143" t="s">
+        <v>16</v>
+      </c>
+      <c r="I143" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="144" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
-        <v>182</v>
+        <v>132</v>
       </c>
       <c r="B144" t="s">
-        <v>165</v>
+        <v>259</v>
       </c>
       <c r="C144" s="2" t="s">
-        <v>181</v>
+        <v>133</v>
+      </c>
+      <c r="Q144" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="145" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
-        <v>115</v>
+        <v>182</v>
       </c>
       <c r="B145" t="s">
-        <v>128</v>
+        <v>165</v>
       </c>
       <c r="C145" s="2" t="s">
-        <v>116</v>
+        <v>181</v>
       </c>
     </row>
     <row r="146" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
-        <v>263</v>
+        <v>115</v>
       </c>
       <c r="B146" t="s">
-        <v>250</v>
+        <v>128</v>
       </c>
       <c r="C146" s="2" t="s">
-        <v>264</v>
-      </c>
-      <c r="E146" t="s">
-        <v>265</v>
-      </c>
-      <c r="F146">
-        <v>1500</v>
-      </c>
-      <c r="G146">
-        <v>2000</v>
-      </c>
-      <c r="H146" t="s">
-        <v>16</v>
-      </c>
-      <c r="I146" t="s">
-        <v>20</v>
+        <v>116</v>
       </c>
     </row>
     <row r="147" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
-        <v>221</v>
+        <v>263</v>
       </c>
       <c r="B147" t="s">
-        <v>86</v>
+        <v>250</v>
       </c>
       <c r="C147" s="2" t="s">
-        <v>220</v>
+        <v>264</v>
+      </c>
+      <c r="E147" t="s">
+        <v>265</v>
       </c>
       <c r="F147">
-        <v>2013</v>
+        <v>1500</v>
+      </c>
+      <c r="G147">
+        <v>2000</v>
       </c>
       <c r="H147" t="s">
         <v>16</v>
@@ -4450,22 +4468,16 @@
     </row>
     <row r="148" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
-        <v>13</v>
+        <v>221</v>
       </c>
       <c r="B148" t="s">
-        <v>25</v>
+        <v>86</v>
       </c>
       <c r="C148" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="D148" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="E148" t="s">
-        <v>14</v>
+        <v>220</v>
       </c>
       <c r="F148">
-        <v>1981</v>
+        <v>2013</v>
       </c>
       <c r="H148" t="s">
         <v>16</v>
@@ -4476,23 +4488,49 @@
     </row>
     <row r="149" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
+        <v>13</v>
+      </c>
+      <c r="B149" t="s">
+        <v>25</v>
+      </c>
+      <c r="C149" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D149" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E149" t="s">
+        <v>14</v>
+      </c>
+      <c r="F149">
+        <v>1981</v>
+      </c>
+      <c r="H149" t="s">
+        <v>16</v>
+      </c>
+      <c r="I149" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="150" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A150" t="s">
         <v>283</v>
       </c>
-      <c r="B149" t="s">
+      <c r="B150" t="s">
         <v>124</v>
       </c>
-      <c r="C149" s="2" t="s">
+      <c r="C150" s="2" t="s">
         <v>284</v>
       </c>
-      <c r="H149" t="s">
-        <v>16</v>
-      </c>
-      <c r="I149" t="s">
+      <c r="H150" t="s">
+        <v>16</v>
+      </c>
+      <c r="I150" t="s">
         <v>20</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:Q149">
+  <sortState ref="A2:Q150">
     <sortCondition ref="A2"/>
   </sortState>
   <hyperlinks>
@@ -4500,9 +4538,9 @@
     <hyperlink ref="C57" r:id="rId2"/>
     <hyperlink ref="C7" r:id="rId3"/>
     <hyperlink ref="C10" r:id="rId4"/>
-    <hyperlink ref="C89" r:id="rId5"/>
-    <hyperlink ref="C108" r:id="rId6"/>
-    <hyperlink ref="C148" r:id="rId7"/>
+    <hyperlink ref="C90" r:id="rId5"/>
+    <hyperlink ref="C109" r:id="rId6"/>
+    <hyperlink ref="C149" r:id="rId7"/>
     <hyperlink ref="C35" r:id="rId8"/>
     <hyperlink ref="C30" r:id="rId9"/>
     <hyperlink ref="C48" r:id="rId10"/>
@@ -4512,11 +4550,11 @@
     <hyperlink ref="C59" r:id="rId14"/>
     <hyperlink ref="C83" r:id="rId15"/>
     <hyperlink ref="C29" r:id="rId16"/>
-    <hyperlink ref="C104" r:id="rId17"/>
+    <hyperlink ref="C105" r:id="rId17"/>
     <hyperlink ref="C40" r:id="rId18"/>
     <hyperlink ref="C69" r:id="rId19"/>
     <hyperlink ref="C16" r:id="rId20"/>
-    <hyperlink ref="C137" r:id="rId21"/>
+    <hyperlink ref="C138" r:id="rId21"/>
     <hyperlink ref="C8" r:id="rId22"/>
     <hyperlink ref="C38" r:id="rId23"/>
     <hyperlink ref="C52" r:id="rId24"/>
@@ -4524,76 +4562,76 @@
     <hyperlink ref="C53" r:id="rId26"/>
     <hyperlink ref="C54" r:id="rId27"/>
     <hyperlink ref="C67" r:id="rId28"/>
-    <hyperlink ref="C87" r:id="rId29"/>
-    <hyperlink ref="C128" r:id="rId30"/>
-    <hyperlink ref="C92" r:id="rId31"/>
+    <hyperlink ref="C88" r:id="rId29"/>
+    <hyperlink ref="C129" r:id="rId30"/>
+    <hyperlink ref="C93" r:id="rId31"/>
     <hyperlink ref="C78" r:id="rId32"/>
-    <hyperlink ref="C97" r:id="rId33"/>
+    <hyperlink ref="C98" r:id="rId33"/>
     <hyperlink ref="C68" r:id="rId34"/>
     <hyperlink ref="C17" r:id="rId35"/>
-    <hyperlink ref="C126" r:id="rId36"/>
+    <hyperlink ref="C127" r:id="rId36"/>
     <hyperlink ref="C15" r:id="rId37"/>
-    <hyperlink ref="C145" r:id="rId38"/>
+    <hyperlink ref="C146" r:id="rId38"/>
     <hyperlink ref="C82" r:id="rId39"/>
     <hyperlink ref="C56" r:id="rId40"/>
-    <hyperlink ref="C112" r:id="rId41"/>
+    <hyperlink ref="C113" r:id="rId41"/>
     <hyperlink ref="C18" r:id="rId42"/>
     <hyperlink ref="C50" r:id="rId43"/>
     <hyperlink ref="C23" r:id="rId44"/>
-    <hyperlink ref="C105" r:id="rId45"/>
-    <hyperlink ref="C143" r:id="rId46"/>
+    <hyperlink ref="C106" r:id="rId45"/>
+    <hyperlink ref="C144" r:id="rId46"/>
     <hyperlink ref="C27" r:id="rId47" display="http://comparativeconstitutionsproject.org/"/>
-    <hyperlink ref="C102" r:id="rId48"/>
-    <hyperlink ref="C139" r:id="rId49"/>
-    <hyperlink ref="C116" r:id="rId50"/>
-    <hyperlink ref="C111" r:id="rId51"/>
+    <hyperlink ref="C103" r:id="rId48"/>
+    <hyperlink ref="C140" r:id="rId49"/>
+    <hyperlink ref="C117" r:id="rId50"/>
+    <hyperlink ref="C112" r:id="rId51"/>
     <hyperlink ref="C22" r:id="rId52"/>
-    <hyperlink ref="C106" r:id="rId53"/>
+    <hyperlink ref="C107" r:id="rId53"/>
     <hyperlink ref="C47" r:id="rId54"/>
     <hyperlink ref="C72" r:id="rId55"/>
     <hyperlink ref="C75" r:id="rId56"/>
-    <hyperlink ref="C103" r:id="rId57"/>
-    <hyperlink ref="C94" r:id="rId58"/>
-    <hyperlink ref="C120" r:id="rId59"/>
+    <hyperlink ref="C104" r:id="rId57"/>
+    <hyperlink ref="C95" r:id="rId58"/>
+    <hyperlink ref="C121" r:id="rId59"/>
     <hyperlink ref="C31" r:id="rId60"/>
-    <hyperlink ref="C130" r:id="rId61"/>
+    <hyperlink ref="C131" r:id="rId61"/>
     <hyperlink ref="C9" r:id="rId62"/>
     <hyperlink ref="C33" r:id="rId63"/>
-    <hyperlink ref="C131" r:id="rId64"/>
+    <hyperlink ref="C132" r:id="rId64"/>
     <hyperlink ref="C14" r:id="rId65"/>
-    <hyperlink ref="C141" r:id="rId66"/>
+    <hyperlink ref="C142" r:id="rId66"/>
     <hyperlink ref="C25" r:id="rId67"/>
     <hyperlink ref="C24" r:id="rId68"/>
     <hyperlink ref="C26" r:id="rId69"/>
     <hyperlink ref="C51" r:id="rId70"/>
-    <hyperlink ref="C144" r:id="rId71"/>
+    <hyperlink ref="C145" r:id="rId71"/>
     <hyperlink ref="C28" r:id="rId72"/>
-    <hyperlink ref="C109" r:id="rId73"/>
+    <hyperlink ref="C110" r:id="rId73"/>
     <hyperlink ref="C32" r:id="rId74"/>
     <hyperlink ref="C44" r:id="rId75"/>
-    <hyperlink ref="C121" r:id="rId76"/>
+    <hyperlink ref="C122" r:id="rId76"/>
     <hyperlink ref="C41" r:id="rId77"/>
     <hyperlink ref="C39" r:id="rId78"/>
     <hyperlink ref="C66" r:id="rId79"/>
     <hyperlink ref="C5" r:id="rId80"/>
     <hyperlink ref="C65" r:id="rId81"/>
     <hyperlink ref="C12" r:id="rId82"/>
-    <hyperlink ref="C101" r:id="rId83"/>
-    <hyperlink ref="C110" r:id="rId84"/>
-    <hyperlink ref="C133" r:id="rId85"/>
+    <hyperlink ref="C102" r:id="rId83"/>
+    <hyperlink ref="C111" r:id="rId84"/>
+    <hyperlink ref="C134" r:id="rId85"/>
     <hyperlink ref="C36" r:id="rId86"/>
-    <hyperlink ref="C142" r:id="rId87"/>
+    <hyperlink ref="C143" r:id="rId87"/>
     <hyperlink ref="C43" r:id="rId88"/>
-    <hyperlink ref="C147" r:id="rId89"/>
-    <hyperlink ref="C90" r:id="rId90"/>
+    <hyperlink ref="C148" r:id="rId89"/>
+    <hyperlink ref="C91" r:id="rId90"/>
     <hyperlink ref="C63" r:id="rId91"/>
-    <hyperlink ref="C91" r:id="rId92"/>
-    <hyperlink ref="C124" r:id="rId93"/>
+    <hyperlink ref="C92" r:id="rId92"/>
+    <hyperlink ref="C125" r:id="rId93"/>
     <hyperlink ref="C76" r:id="rId94"/>
-    <hyperlink ref="C95" r:id="rId95"/>
-    <hyperlink ref="C125" r:id="rId96"/>
+    <hyperlink ref="C96" r:id="rId95"/>
+    <hyperlink ref="C126" r:id="rId96"/>
     <hyperlink ref="C60" r:id="rId97"/>
-    <hyperlink ref="C107" r:id="rId98"/>
+    <hyperlink ref="C108" r:id="rId98"/>
     <hyperlink ref="C45" r:id="rId99"/>
     <hyperlink ref="C42" r:id="rId100"/>
     <hyperlink ref="C79" r:id="rId101"/>
@@ -4601,39 +4639,39 @@
     <hyperlink ref="C2" r:id="rId103"/>
     <hyperlink ref="C73" r:id="rId104"/>
     <hyperlink ref="C77" r:id="rId105"/>
-    <hyperlink ref="C99" r:id="rId106"/>
+    <hyperlink ref="C100" r:id="rId106"/>
     <hyperlink ref="C46" r:id="rId107"/>
     <hyperlink ref="C80" r:id="rId108"/>
-    <hyperlink ref="C123" r:id="rId109"/>
+    <hyperlink ref="C124" r:id="rId109"/>
     <hyperlink ref="C13" r:id="rId110"/>
     <hyperlink ref="C4" r:id="rId111"/>
-    <hyperlink ref="C146" r:id="rId112"/>
+    <hyperlink ref="C147" r:id="rId112"/>
     <hyperlink ref="C86" r:id="rId113"/>
     <hyperlink ref="C81" r:id="rId114"/>
-    <hyperlink ref="C136" r:id="rId115"/>
-    <hyperlink ref="C119" r:id="rId116"/>
+    <hyperlink ref="C137" r:id="rId115"/>
+    <hyperlink ref="C120" r:id="rId116"/>
     <hyperlink ref="C62" r:id="rId117"/>
-    <hyperlink ref="C93" r:id="rId118"/>
+    <hyperlink ref="C94" r:id="rId118"/>
     <hyperlink ref="C71" r:id="rId119"/>
-    <hyperlink ref="C149" r:id="rId120"/>
+    <hyperlink ref="C150" r:id="rId120"/>
     <hyperlink ref="C64" r:id="rId121"/>
-    <hyperlink ref="C118" r:id="rId122"/>
-    <hyperlink ref="C98" r:id="rId123"/>
+    <hyperlink ref="C119" r:id="rId122"/>
+    <hyperlink ref="C99" r:id="rId123"/>
     <hyperlink ref="C74" r:id="rId124"/>
-    <hyperlink ref="C96" r:id="rId125"/>
-    <hyperlink ref="C122" r:id="rId126"/>
+    <hyperlink ref="C97" r:id="rId125"/>
+    <hyperlink ref="C123" r:id="rId126"/>
     <hyperlink ref="C84" r:id="rId127"/>
     <hyperlink ref="C11" r:id="rId128"/>
     <hyperlink ref="C19" r:id="rId129"/>
-    <hyperlink ref="C117" r:id="rId130"/>
+    <hyperlink ref="C118" r:id="rId130"/>
     <hyperlink ref="C70" r:id="rId131"/>
-    <hyperlink ref="C129" r:id="rId132"/>
-    <hyperlink ref="C114" r:id="rId133"/>
-    <hyperlink ref="C113" r:id="rId134"/>
-    <hyperlink ref="C115" r:id="rId135"/>
-    <hyperlink ref="C135" r:id="rId136"/>
-    <hyperlink ref="C127" r:id="rId137"/>
-    <hyperlink ref="C140" r:id="rId138"/>
+    <hyperlink ref="C130" r:id="rId132"/>
+    <hyperlink ref="C115" r:id="rId133"/>
+    <hyperlink ref="C114" r:id="rId134"/>
+    <hyperlink ref="C116" r:id="rId135"/>
+    <hyperlink ref="C136" r:id="rId136"/>
+    <hyperlink ref="C128" r:id="rId137"/>
+    <hyperlink ref="C141" r:id="rId138"/>
     <hyperlink ref="C37" r:id="rId139"/>
     <hyperlink ref="C85" r:id="rId140"/>
     <hyperlink ref="J2" r:id="rId141"/>
@@ -4643,24 +4681,25 @@
     <hyperlink ref="J4" r:id="rId145"/>
     <hyperlink ref="P5" r:id="rId146"/>
     <hyperlink ref="J5" r:id="rId147"/>
-    <hyperlink ref="C100" r:id="rId148"/>
+    <hyperlink ref="C101" r:id="rId148"/>
     <hyperlink ref="C34" r:id="rId149"/>
     <hyperlink ref="P7" r:id="rId150"/>
     <hyperlink ref="J7" r:id="rId151"/>
     <hyperlink ref="M8" r:id="rId152"/>
     <hyperlink ref="L8" r:id="rId153"/>
     <hyperlink ref="J8" r:id="rId154"/>
-    <hyperlink ref="C138" r:id="rId155"/>
-    <hyperlink ref="N138" r:id="rId156"/>
+    <hyperlink ref="C139" r:id="rId155"/>
+    <hyperlink ref="N139" r:id="rId156"/>
     <hyperlink ref="C21" r:id="rId157"/>
     <hyperlink ref="N21" r:id="rId158"/>
     <hyperlink ref="C61" r:id="rId159"/>
-    <hyperlink ref="C134" r:id="rId160"/>
-    <hyperlink ref="J134" r:id="rId161"/>
-    <hyperlink ref="C132" r:id="rId162"/>
-    <hyperlink ref="N132" r:id="rId163"/>
-    <hyperlink ref="J132" r:id="rId164"/>
-    <hyperlink ref="C88" r:id="rId165"/>
+    <hyperlink ref="C135" r:id="rId160"/>
+    <hyperlink ref="J135" r:id="rId161"/>
+    <hyperlink ref="C133" r:id="rId162"/>
+    <hyperlink ref="N133" r:id="rId163"/>
+    <hyperlink ref="J133" r:id="rId164"/>
+    <hyperlink ref="C89" r:id="rId165"/>
+    <hyperlink ref="C87" r:id="rId166"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
add Decision-making in the European Union
</commit_message>
<xml_diff>
--- a/PolData.xlsx
+++ b/PolData.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="745" uniqueCount="409">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="753" uniqueCount="413">
   <si>
     <t>name</t>
   </si>
@@ -1254,6 +1254,18 @@
   </si>
   <si>
     <t>Accountability, repression, human rights</t>
+  </si>
+  <si>
+    <t>Decision-making in the European Union</t>
+  </si>
+  <si>
+    <t>http://www.robertthomson.info/research/resolving-controversy-in-the-eu</t>
+  </si>
+  <si>
+    <t>http://www.robertthomson.info/wp-content/uploads/2011/01/Issues_list_new_26March2012.pdf</t>
+  </si>
+  <si>
+    <t>http://www.robertthomson.info/wp-content/uploads/2011/01/deu15_27_26March2012.csv</t>
   </si>
 </sst>
 </file>
@@ -1593,10 +1605,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q150"/>
+  <dimension ref="A1:Q151"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A125" workbookViewId="0">
-      <selection activeCell="A87" sqref="A87"/>
+    <sheetView tabSelected="1" topLeftCell="A131" workbookViewId="0">
+      <selection activeCell="A151" sqref="A151"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2301,7 +2313,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>164</v>
       </c>
@@ -2312,7 +2324,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>371</v>
       </c>
@@ -2338,7 +2350,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>39</v>
       </c>
@@ -2364,7 +2376,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>215</v>
       </c>
@@ -2384,7 +2396,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>330</v>
       </c>
@@ -2407,7 +2419,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>75</v>
       </c>
@@ -2424,7 +2436,7 @@
         <v>1971</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>197</v>
       </c>
@@ -2450,209 +2462,218 @@
         <v>20</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
+        <v>409</v>
+      </c>
+      <c r="B40" t="s">
+        <v>250</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>410</v>
+      </c>
+      <c r="E40" t="s">
+        <v>9</v>
+      </c>
+      <c r="H40" t="s">
+        <v>348</v>
+      </c>
+      <c r="I40" t="s">
+        <v>349</v>
+      </c>
+      <c r="J40" s="2" t="s">
+        <v>411</v>
+      </c>
+      <c r="K40" s="2" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
         <v>59</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B41" t="s">
         <v>60</v>
       </c>
-      <c r="C40" s="2" t="s">
+      <c r="C41" s="2" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A41" t="s">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
         <v>196</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B42" t="s">
         <v>165</v>
       </c>
-      <c r="C41" s="2" t="s">
+      <c r="C42" s="2" t="s">
         <v>195</v>
       </c>
-      <c r="F41">
+      <c r="F42">
         <v>1946</v>
       </c>
-      <c r="G41">
+      <c r="G42">
         <v>2016</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A42" t="s">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
         <v>238</v>
       </c>
-      <c r="B42" t="s">
+      <c r="B43" t="s">
         <v>237</v>
       </c>
-      <c r="C42" s="2" t="s">
+      <c r="C43" s="2" t="s">
         <v>243</v>
       </c>
-      <c r="H42" t="s">
-        <v>16</v>
-      </c>
-      <c r="I42" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A43" t="s">
+      <c r="H43" t="s">
+        <v>16</v>
+      </c>
+      <c r="I43" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
         <v>219</v>
       </c>
-      <c r="B43" t="s">
+      <c r="B44" t="s">
         <v>124</v>
       </c>
-      <c r="C43" s="2" t="s">
+      <c r="C44" s="2" t="s">
         <v>218</v>
       </c>
-      <c r="F43">
+      <c r="F44">
         <v>1970</v>
       </c>
-      <c r="G43">
+      <c r="G44">
         <v>2015</v>
       </c>
-      <c r="H43" t="s">
-        <v>16</v>
-      </c>
-      <c r="I43" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A44" t="s">
+      <c r="H44" t="s">
+        <v>16</v>
+      </c>
+      <c r="I44" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
         <v>191</v>
       </c>
-      <c r="B44" t="s">
+      <c r="B45" t="s">
         <v>25</v>
       </c>
-      <c r="C44" s="2" t="s">
+      <c r="C45" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="E44" t="s">
+      <c r="E45" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A45" t="s">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
         <v>235</v>
       </c>
-      <c r="B45" t="s">
+      <c r="B46" t="s">
         <v>60</v>
       </c>
-      <c r="C45" s="2" t="s">
+      <c r="C46" s="2" t="s">
         <v>236</v>
       </c>
-      <c r="H45" t="s">
-        <v>16</v>
-      </c>
-      <c r="I45" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A46" t="s">
+      <c r="H46" t="s">
+        <v>16</v>
+      </c>
+      <c r="I46" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
         <v>252</v>
       </c>
-      <c r="B46" t="s">
+      <c r="B47" t="s">
         <v>250</v>
       </c>
-      <c r="C46" s="2" t="s">
+      <c r="C47" s="2" t="s">
         <v>251</v>
       </c>
-      <c r="H46" t="s">
-        <v>16</v>
-      </c>
-      <c r="I46" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A47" t="s">
+      <c r="H47" t="s">
+        <v>16</v>
+      </c>
+      <c r="I47" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
         <v>149</v>
       </c>
-      <c r="B47" t="s">
+      <c r="B48" t="s">
         <v>128</v>
       </c>
-      <c r="C47" s="2" t="s">
+      <c r="C48" s="2" t="s">
         <v>150</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A48" t="s">
-        <v>28</v>
-      </c>
-      <c r="B48" t="s">
-        <v>25</v>
-      </c>
-      <c r="C48" s="2" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="49" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>80</v>
+        <v>28</v>
       </c>
       <c r="B49" t="s">
-        <v>128</v>
+        <v>25</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="E49" t="s">
-        <v>9</v>
-      </c>
-      <c r="F49">
-        <v>1979</v>
+        <v>48</v>
       </c>
     </row>
     <row r="50" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>125</v>
+        <v>80</v>
       </c>
       <c r="B50" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>126</v>
+        <v>81</v>
+      </c>
+      <c r="E50" t="s">
+        <v>9</v>
+      </c>
+      <c r="F50">
+        <v>1979</v>
       </c>
     </row>
     <row r="51" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>179</v>
+        <v>125</v>
       </c>
       <c r="B51" t="s">
-        <v>165</v>
+        <v>124</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>180</v>
+        <v>126</v>
       </c>
     </row>
     <row r="52" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
+        <v>179</v>
+      </c>
+      <c r="B52" t="s">
+        <v>165</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="53" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
         <v>78</v>
       </c>
-      <c r="B52" t="s">
+      <c r="B53" t="s">
         <v>25</v>
       </c>
-      <c r="C52" s="2" t="s">
+      <c r="C53" s="2" t="s">
         <v>79</v>
-      </c>
-      <c r="E52" t="s">
-        <v>9</v>
-      </c>
-      <c r="F52">
-        <v>1979</v>
-      </c>
-    </row>
-    <row r="53" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A53" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="B53" t="s">
-        <v>83</v>
-      </c>
-      <c r="C53" s="2" t="s">
-        <v>84</v>
       </c>
       <c r="E53" t="s">
         <v>9</v>
@@ -2663,13 +2684,13 @@
     </row>
     <row r="54" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A54" s="3" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B54" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="E54" t="s">
         <v>9</v>
@@ -2677,176 +2698,170 @@
       <c r="F54">
         <v>1979</v>
       </c>
-      <c r="G54">
+    </row>
+    <row r="55" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A55" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="B55" t="s">
+        <v>86</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="E55" t="s">
+        <v>9</v>
+      </c>
+      <c r="F55">
+        <v>1979</v>
+      </c>
+      <c r="G55">
         <v>2009</v>
-      </c>
-    </row>
-    <row r="55" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A55" t="s">
-        <v>27</v>
-      </c>
-      <c r="B55" t="s">
-        <v>25</v>
-      </c>
-      <c r="C55" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="Q55" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="56" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>120</v>
+        <v>27</v>
       </c>
       <c r="B56" t="s">
-        <v>259</v>
+        <v>25</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="I56" t="s">
-        <v>20</v>
+        <v>49</v>
+      </c>
+      <c r="Q56" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="57" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>5</v>
+        <v>120</v>
       </c>
       <c r="B57" t="s">
-        <v>25</v>
+        <v>259</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D57" t="s">
-        <v>94</v>
-      </c>
-      <c r="E57" t="s">
-        <v>9</v>
-      </c>
-      <c r="F57">
-        <v>2002</v>
-      </c>
-      <c r="H57" t="s">
-        <v>16</v>
+        <v>119</v>
       </c>
       <c r="I57" t="s">
-        <v>248</v>
-      </c>
-      <c r="Q57" t="s">
-        <v>44</v>
+        <v>20</v>
       </c>
     </row>
     <row r="58" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
+        <v>5</v>
+      </c>
+      <c r="B58" t="s">
+        <v>25</v>
+      </c>
+      <c r="C58" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D58" t="s">
+        <v>94</v>
+      </c>
+      <c r="E58" t="s">
+        <v>9</v>
+      </c>
+      <c r="F58">
+        <v>2002</v>
+      </c>
+      <c r="H58" t="s">
+        <v>16</v>
+      </c>
+      <c r="I58" t="s">
+        <v>248</v>
+      </c>
+      <c r="Q58" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="59" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
         <v>240</v>
       </c>
-      <c r="B58" t="s">
+      <c r="B59" t="s">
         <v>237</v>
       </c>
-      <c r="C58" s="2" t="s">
+      <c r="C59" s="2" t="s">
         <v>243</v>
       </c>
-      <c r="H58" t="s">
-        <v>16</v>
-      </c>
-      <c r="I58" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="59" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A59" s="1" t="s">
+      <c r="H59" t="s">
+        <v>16</v>
+      </c>
+      <c r="I59" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="60" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A60" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B59" t="s">
+      <c r="B60" t="s">
         <v>25</v>
       </c>
-      <c r="C59" s="2" t="s">
+      <c r="C60" s="2" t="s">
         <v>52</v>
-      </c>
-    </row>
-    <row r="60" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A60" t="s">
-        <v>232</v>
-      </c>
-      <c r="B60" t="s">
-        <v>250</v>
-      </c>
-      <c r="C60" s="2" t="s">
-        <v>231</v>
       </c>
     </row>
     <row r="61" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>390</v>
+        <v>232</v>
       </c>
       <c r="B61" t="s">
-        <v>83</v>
+        <v>250</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>392</v>
-      </c>
-      <c r="D61" t="s">
-        <v>391</v>
-      </c>
-      <c r="E61" t="s">
-        <v>9</v>
-      </c>
-      <c r="F61">
-        <v>2007</v>
-      </c>
-      <c r="G61">
-        <v>2015</v>
-      </c>
-      <c r="H61" t="s">
-        <v>348</v>
-      </c>
-      <c r="I61" t="s">
-        <v>349</v>
-      </c>
-      <c r="Q61" t="s">
-        <v>393</v>
+        <v>231</v>
       </c>
     </row>
     <row r="62" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>276</v>
+        <v>390</v>
       </c>
       <c r="B62" t="s">
-        <v>124</v>
+        <v>83</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>277</v>
+        <v>392</v>
+      </c>
+      <c r="D62" t="s">
+        <v>391</v>
+      </c>
+      <c r="E62" t="s">
+        <v>9</v>
       </c>
       <c r="F62">
-        <v>1948</v>
+        <v>2007</v>
       </c>
       <c r="G62">
-        <v>2000</v>
+        <v>2015</v>
       </c>
       <c r="H62" t="s">
-        <v>16</v>
+        <v>348</v>
       </c>
       <c r="I62" t="s">
-        <v>20</v>
+        <v>349</v>
+      </c>
+      <c r="Q62" t="s">
+        <v>393</v>
       </c>
     </row>
     <row r="63" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>224</v>
+        <v>276</v>
       </c>
       <c r="B63" t="s">
-        <v>40</v>
+        <v>124</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>225</v>
+        <v>277</v>
       </c>
       <c r="F63">
-        <v>1964</v>
+        <v>1948</v>
       </c>
       <c r="G63">
-        <v>2008</v>
+        <v>2000</v>
       </c>
       <c r="H63" t="s">
         <v>16</v>
@@ -2857,13 +2872,19 @@
     </row>
     <row r="64" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>285</v>
+        <v>224</v>
       </c>
       <c r="B64" t="s">
-        <v>250</v>
+        <v>40</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>286</v>
+        <v>225</v>
+      </c>
+      <c r="F64">
+        <v>1964</v>
+      </c>
+      <c r="G64">
+        <v>2008</v>
       </c>
       <c r="H64" t="s">
         <v>16</v>
@@ -2874,166 +2895,166 @@
     </row>
     <row r="65" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>205</v>
+        <v>285</v>
       </c>
       <c r="B65" t="s">
-        <v>40</v>
+        <v>250</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>204</v>
-      </c>
-      <c r="F65">
-        <v>2006</v>
+        <v>286</v>
+      </c>
+      <c r="H65" t="s">
+        <v>16</v>
+      </c>
+      <c r="I65" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="66" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>200</v>
+        <v>205</v>
       </c>
       <c r="B66" t="s">
-        <v>99</v>
+        <v>40</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="F66">
-        <v>1980</v>
-      </c>
-      <c r="G66">
-        <v>2007</v>
-      </c>
-      <c r="Q66" t="s">
-        <v>18</v>
+        <v>2006</v>
       </c>
     </row>
     <row r="67" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>89</v>
+        <v>200</v>
       </c>
       <c r="B67" t="s">
-        <v>25</v>
+        <v>99</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="E67" t="s">
-        <v>34</v>
+        <v>201</v>
       </c>
       <c r="F67">
-        <v>1972</v>
-      </c>
-      <c r="H67" t="s">
-        <v>16</v>
-      </c>
-      <c r="I67" t="s">
-        <v>20</v>
+        <v>1980</v>
+      </c>
+      <c r="G67">
+        <v>2007</v>
+      </c>
+      <c r="Q67" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="68" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>104</v>
+        <v>89</v>
       </c>
       <c r="B68" t="s">
         <v>25</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>106</v>
+        <v>88</v>
       </c>
       <c r="E68" t="s">
-        <v>105</v>
+        <v>34</v>
       </c>
       <c r="F68">
-        <v>1980</v>
+        <v>1972</v>
+      </c>
+      <c r="H68" t="s">
+        <v>16</v>
+      </c>
+      <c r="I68" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="69" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>62</v>
+        <v>104</v>
       </c>
       <c r="B69" t="s">
         <v>25</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>63</v>
+        <v>106</v>
+      </c>
+      <c r="E69" t="s">
+        <v>105</v>
+      </c>
+      <c r="F69">
+        <v>1980</v>
       </c>
     </row>
     <row r="70" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>311</v>
+        <v>62</v>
       </c>
       <c r="B70" t="s">
-        <v>165</v>
+        <v>25</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>312</v>
-      </c>
-      <c r="E70" t="s">
-        <v>14</v>
-      </c>
-      <c r="H70" t="s">
-        <v>16</v>
-      </c>
-      <c r="I70" t="s">
-        <v>301</v>
+        <v>63</v>
       </c>
     </row>
     <row r="71" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>281</v>
+        <v>311</v>
       </c>
       <c r="B71" t="s">
-        <v>237</v>
+        <v>165</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>282</v>
+        <v>312</v>
+      </c>
+      <c r="E71" t="s">
+        <v>14</v>
       </c>
       <c r="H71" t="s">
         <v>16</v>
       </c>
       <c r="I71" t="s">
-        <v>20</v>
+        <v>301</v>
       </c>
     </row>
     <row r="72" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>151</v>
+        <v>281</v>
       </c>
       <c r="B72" t="s">
-        <v>40</v>
+        <v>237</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="E72" t="s">
-        <v>14</v>
+        <v>282</v>
+      </c>
+      <c r="H72" t="s">
+        <v>16</v>
+      </c>
+      <c r="I72" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="73" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>242</v>
+        <v>151</v>
       </c>
       <c r="B73" t="s">
-        <v>237</v>
+        <v>40</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>243</v>
-      </c>
-      <c r="H73" t="s">
-        <v>16</v>
-      </c>
-      <c r="I73" t="s">
-        <v>20</v>
+        <v>152</v>
+      </c>
+      <c r="E73" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="74" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>292</v>
+        <v>242</v>
       </c>
       <c r="B74" t="s">
-        <v>99</v>
+        <v>237</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>291</v>
+        <v>243</v>
       </c>
       <c r="H74" t="s">
         <v>16</v>
@@ -3044,47 +3065,47 @@
     </row>
     <row r="75" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>153</v>
+        <v>292</v>
       </c>
       <c r="B75" t="s">
-        <v>259</v>
+        <v>99</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>154</v>
+        <v>291</v>
+      </c>
+      <c r="H75" t="s">
+        <v>16</v>
+      </c>
+      <c r="I75" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="76" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>228</v>
+        <v>153</v>
       </c>
       <c r="B76" t="s">
-        <v>40</v>
+        <v>259</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>225</v>
-      </c>
-      <c r="F76">
-        <v>1989</v>
-      </c>
-      <c r="G76">
-        <v>2017</v>
-      </c>
-      <c r="H76" t="s">
-        <v>16</v>
-      </c>
-      <c r="I76" t="s">
-        <v>20</v>
+        <v>154</v>
       </c>
     </row>
     <row r="77" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>245</v>
+        <v>228</v>
       </c>
       <c r="B77" t="s">
-        <v>237</v>
+        <v>40</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>244</v>
+        <v>225</v>
+      </c>
+      <c r="F77">
+        <v>1989</v>
+      </c>
+      <c r="G77">
+        <v>2017</v>
       </c>
       <c r="H77" t="s">
         <v>16</v>
@@ -3095,50 +3116,41 @@
     </row>
     <row r="78" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>100</v>
+        <v>245</v>
       </c>
       <c r="B78" t="s">
-        <v>99</v>
+        <v>237</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>101</v>
+        <v>244</v>
+      </c>
+      <c r="H78" t="s">
+        <v>16</v>
+      </c>
+      <c r="I78" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="79" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>239</v>
+        <v>100</v>
       </c>
       <c r="B79" t="s">
-        <v>237</v>
+        <v>99</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>243</v>
-      </c>
-      <c r="H79" t="s">
-        <v>16</v>
-      </c>
-      <c r="I79" t="s">
-        <v>20</v>
+        <v>101</v>
       </c>
     </row>
     <row r="80" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>254</v>
+        <v>239</v>
       </c>
       <c r="B80" t="s">
-        <v>55</v>
+        <v>237</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>253</v>
-      </c>
-      <c r="E80" t="s">
-        <v>255</v>
-      </c>
-      <c r="F80">
-        <v>1960</v>
-      </c>
-      <c r="G80">
-        <v>2014</v>
+        <v>243</v>
       </c>
       <c r="H80" t="s">
         <v>16</v>
@@ -3149,19 +3161,22 @@
     </row>
     <row r="81" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>270</v>
+        <v>254</v>
       </c>
       <c r="B81" t="s">
         <v>55</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>271</v>
+        <v>253</v>
+      </c>
+      <c r="E81" t="s">
+        <v>255</v>
       </c>
       <c r="F81">
-        <v>1990</v>
+        <v>1960</v>
       </c>
       <c r="G81">
-        <v>2010</v>
+        <v>2014</v>
       </c>
       <c r="H81" t="s">
         <v>16</v>
@@ -3172,96 +3187,90 @@
     </row>
     <row r="82" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>117</v>
+        <v>270</v>
       </c>
       <c r="B82" t="s">
         <v>55</v>
       </c>
       <c r="C82" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="F82">
+        <v>1990</v>
+      </c>
+      <c r="G82">
+        <v>2010</v>
+      </c>
+      <c r="H82" t="s">
+        <v>16</v>
+      </c>
+      <c r="I82" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="83" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A83" t="s">
+        <v>117</v>
+      </c>
+      <c r="B83" t="s">
+        <v>55</v>
+      </c>
+      <c r="C83" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="I82" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q82" t="s">
+      <c r="I83" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q83" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="83" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A83" s="1" t="s">
+    <row r="84" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A84" s="1" t="s">
         <v>23</v>
-      </c>
-      <c r="B83" t="s">
-        <v>25</v>
-      </c>
-      <c r="C83" s="2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="84" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A84" t="s">
-        <v>300</v>
       </c>
       <c r="B84" t="s">
         <v>25</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>298</v>
-      </c>
-      <c r="E84" t="s">
-        <v>299</v>
-      </c>
-      <c r="F84">
-        <v>1969</v>
-      </c>
-      <c r="H84" t="s">
-        <v>16</v>
-      </c>
-      <c r="I84" t="s">
-        <v>249</v>
+        <v>53</v>
       </c>
     </row>
     <row r="85" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>332</v>
+        <v>300</v>
       </c>
       <c r="B85" t="s">
-        <v>134</v>
+        <v>25</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>333</v>
+        <v>298</v>
       </c>
       <c r="E85" t="s">
-        <v>334</v>
+        <v>299</v>
+      </c>
+      <c r="F85">
+        <v>1969</v>
       </c>
       <c r="H85" t="s">
         <v>16</v>
       </c>
       <c r="I85" t="s">
-        <v>20</v>
+        <v>249</v>
       </c>
     </row>
     <row r="86" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>267</v>
+        <v>332</v>
       </c>
       <c r="B86" t="s">
-        <v>250</v>
+        <v>134</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>266</v>
-      </c>
-      <c r="D86" t="s">
-        <v>269</v>
+        <v>333</v>
       </c>
       <c r="E86" t="s">
-        <v>268</v>
-      </c>
-      <c r="F86">
-        <v>1970</v>
-      </c>
-      <c r="G86">
-        <v>2014</v>
+        <v>334</v>
       </c>
       <c r="H86" t="s">
         <v>16</v>
@@ -3272,143 +3281,149 @@
     </row>
     <row r="87" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>407</v>
+        <v>267</v>
       </c>
       <c r="B87" t="s">
-        <v>40</v>
+        <v>250</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>406</v>
+        <v>266</v>
       </c>
       <c r="D87" t="s">
-        <v>408</v>
+        <v>269</v>
       </c>
       <c r="E87" t="s">
-        <v>14</v>
+        <v>268</v>
       </c>
       <c r="F87">
-        <v>1949</v>
+        <v>1970</v>
       </c>
       <c r="G87">
-        <v>2013</v>
+        <v>2014</v>
       </c>
       <c r="H87" t="s">
-        <v>348</v>
+        <v>16</v>
       </c>
       <c r="I87" t="s">
-        <v>349</v>
+        <v>20</v>
       </c>
     </row>
     <row r="88" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>96</v>
+        <v>407</v>
       </c>
       <c r="B88" t="s">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>90</v>
+        <v>406</v>
+      </c>
+      <c r="D88" t="s">
+        <v>408</v>
       </c>
       <c r="E88" t="s">
-        <v>69</v>
+        <v>14</v>
       </c>
       <c r="F88">
-        <v>1995</v>
+        <v>1949</v>
+      </c>
+      <c r="G88">
+        <v>2013</v>
+      </c>
+      <c r="H88" t="s">
+        <v>348</v>
+      </c>
+      <c r="I88" t="s">
+        <v>349</v>
       </c>
     </row>
     <row r="89" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>404</v>
+        <v>96</v>
       </c>
       <c r="B89" t="s">
-        <v>83</v>
+        <v>25</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>403</v>
-      </c>
-      <c r="D89" t="s">
-        <v>405</v>
+        <v>90</v>
       </c>
       <c r="E89" t="s">
-        <v>14</v>
+        <v>69</v>
       </c>
       <c r="F89">
-        <v>1875</v>
-      </c>
-      <c r="G89">
-        <v>2004</v>
-      </c>
-      <c r="H89" t="s">
-        <v>348</v>
-      </c>
-      <c r="I89" t="s">
-        <v>349</v>
+        <v>1995</v>
       </c>
     </row>
     <row r="90" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>11</v>
+        <v>404</v>
       </c>
       <c r="B90" t="s">
-        <v>25</v>
+        <v>83</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>12</v>
+        <v>403</v>
       </c>
       <c r="D90" t="s">
-        <v>95</v>
+        <v>405</v>
       </c>
       <c r="E90" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="F90">
-        <v>2007</v>
+        <v>1875</v>
+      </c>
+      <c r="G90">
+        <v>2004</v>
       </c>
       <c r="H90" t="s">
-        <v>16</v>
+        <v>348</v>
       </c>
       <c r="I90" t="s">
-        <v>21</v>
+        <v>349</v>
       </c>
     </row>
     <row r="91" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>223</v>
+        <v>11</v>
       </c>
       <c r="B91" t="s">
-        <v>124</v>
+        <v>25</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>222</v>
+        <v>12</v>
+      </c>
+      <c r="D91" t="s">
+        <v>95</v>
+      </c>
+      <c r="E91" t="s">
+        <v>10</v>
       </c>
       <c r="F91">
-        <v>1</v>
-      </c>
-      <c r="G91">
-        <v>2010</v>
+        <v>2007</v>
       </c>
       <c r="H91" t="s">
         <v>16</v>
       </c>
       <c r="I91" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="92" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="B92" t="s">
-        <v>40</v>
+        <v>124</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="F92">
-        <v>1946</v>
+        <v>1</v>
       </c>
       <c r="G92">
-        <v>2016</v>
+        <v>2010</v>
       </c>
       <c r="H92" t="s">
         <v>16</v>
@@ -3419,90 +3434,90 @@
     </row>
     <row r="93" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>97</v>
+        <v>226</v>
       </c>
       <c r="B93" t="s">
-        <v>128</v>
+        <v>40</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>98</v>
+        <v>225</v>
+      </c>
+      <c r="F93">
+        <v>1946</v>
+      </c>
+      <c r="G93">
+        <v>2016</v>
+      </c>
+      <c r="H93" t="s">
+        <v>16</v>
+      </c>
+      <c r="I93" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="94" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>278</v>
+        <v>97</v>
       </c>
       <c r="B94" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>279</v>
-      </c>
-      <c r="E94" t="s">
-        <v>280</v>
-      </c>
-      <c r="F94">
-        <v>1890</v>
-      </c>
-      <c r="G94">
-        <v>1996</v>
-      </c>
-      <c r="H94" t="s">
-        <v>16</v>
-      </c>
-      <c r="I94" t="s">
-        <v>20</v>
+        <v>98</v>
       </c>
     </row>
     <row r="95" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>156</v>
+        <v>278</v>
       </c>
       <c r="B95" t="s">
-        <v>25</v>
+        <v>124</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>154</v>
+        <v>279</v>
+      </c>
+      <c r="E95" t="s">
+        <v>280</v>
+      </c>
+      <c r="F95">
+        <v>1890</v>
+      </c>
+      <c r="G95">
+        <v>1996</v>
+      </c>
+      <c r="H95" t="s">
+        <v>16</v>
+      </c>
+      <c r="I95" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="96" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>229</v>
+        <v>156</v>
       </c>
       <c r="B96" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>225</v>
-      </c>
-      <c r="F96">
-        <v>1952</v>
-      </c>
-      <c r="G96">
-        <v>1997</v>
-      </c>
-      <c r="H96" t="s">
-        <v>16</v>
-      </c>
-      <c r="I96" t="s">
-        <v>20</v>
+        <v>154</v>
       </c>
     </row>
     <row r="97" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>293</v>
+        <v>229</v>
       </c>
       <c r="B97" t="s">
         <v>40</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>294</v>
+        <v>225</v>
       </c>
       <c r="F97">
-        <v>2004</v>
+        <v>1952</v>
       </c>
       <c r="G97">
-        <v>2006</v>
+        <v>1997</v>
       </c>
       <c r="H97" t="s">
         <v>16</v>
@@ -3513,221 +3528,218 @@
     </row>
     <row r="98" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>102</v>
+        <v>293</v>
       </c>
       <c r="B98" t="s">
-        <v>99</v>
+        <v>40</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>103</v>
+        <v>294</v>
+      </c>
+      <c r="F98">
+        <v>2004</v>
+      </c>
+      <c r="G98">
+        <v>2006</v>
+      </c>
+      <c r="H98" t="s">
+        <v>16</v>
+      </c>
+      <c r="I98" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="99" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>289</v>
+        <v>102</v>
       </c>
       <c r="B99" t="s">
-        <v>124</v>
+        <v>99</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>290</v>
+        <v>103</v>
       </c>
     </row>
     <row r="100" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>246</v>
+        <v>289</v>
       </c>
       <c r="B100" t="s">
-        <v>165</v>
+        <v>124</v>
       </c>
       <c r="C100" s="2" t="s">
-        <v>247</v>
-      </c>
-      <c r="E100" t="s">
-        <v>14</v>
-      </c>
-      <c r="F100">
-        <v>1960</v>
-      </c>
-      <c r="G100">
-        <v>2006</v>
-      </c>
-      <c r="H100" t="s">
-        <v>16</v>
-      </c>
-      <c r="I100" t="s">
-        <v>249</v>
+        <v>290</v>
       </c>
     </row>
     <row r="101" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>365</v>
+        <v>246</v>
       </c>
       <c r="B101" t="s">
-        <v>128</v>
+        <v>165</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>364</v>
-      </c>
-      <c r="D101" t="s">
-        <v>370</v>
+        <v>247</v>
       </c>
       <c r="E101" t="s">
-        <v>366</v>
+        <v>14</v>
       </c>
       <c r="F101">
-        <v>1906</v>
+        <v>1960</v>
       </c>
       <c r="G101">
-        <v>2013</v>
+        <v>2006</v>
       </c>
       <c r="H101" t="s">
-        <v>367</v>
+        <v>16</v>
       </c>
       <c r="I101" t="s">
-        <v>368</v>
-      </c>
-      <c r="Q101" t="s">
-        <v>369</v>
+        <v>249</v>
       </c>
     </row>
     <row r="102" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>208</v>
+        <v>365</v>
       </c>
       <c r="B102" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="C102" s="2" t="s">
-        <v>209</v>
+        <v>364</v>
+      </c>
+      <c r="D102" t="s">
+        <v>370</v>
+      </c>
+      <c r="E102" t="s">
+        <v>366</v>
       </c>
       <c r="F102">
-        <v>1932</v>
+        <v>1906</v>
       </c>
       <c r="G102">
-        <v>2014</v>
+        <v>2013</v>
       </c>
       <c r="H102" t="s">
-        <v>16</v>
+        <v>367</v>
       </c>
       <c r="I102" t="s">
-        <v>20</v>
+        <v>368</v>
+      </c>
+      <c r="Q102" t="s">
+        <v>369</v>
       </c>
     </row>
     <row r="103" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>137</v>
+        <v>208</v>
       </c>
       <c r="B103" t="s">
-        <v>259</v>
+        <v>124</v>
       </c>
       <c r="C103" s="2" t="s">
-        <v>138</v>
+        <v>209</v>
+      </c>
+      <c r="F103">
+        <v>1932</v>
+      </c>
+      <c r="G103">
+        <v>2014</v>
+      </c>
+      <c r="H103" t="s">
+        <v>16</v>
+      </c>
+      <c r="I103" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="104" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>155</v>
+        <v>137</v>
       </c>
       <c r="B104" t="s">
         <v>259</v>
       </c>
       <c r="C104" s="2" t="s">
-        <v>154</v>
+        <v>138</v>
       </c>
     </row>
     <row r="105" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>57</v>
+        <v>155</v>
       </c>
       <c r="B105" t="s">
-        <v>128</v>
+        <v>259</v>
       </c>
       <c r="C105" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="Q105" t="s">
-        <v>17</v>
+        <v>154</v>
       </c>
     </row>
     <row r="106" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>129</v>
+        <v>57</v>
       </c>
       <c r="B106" t="s">
-        <v>259</v>
+        <v>128</v>
       </c>
       <c r="C106" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="E106" t="s">
-        <v>131</v>
-      </c>
-      <c r="F106">
-        <v>1945</v>
-      </c>
-      <c r="G106">
-        <v>2008</v>
-      </c>
-      <c r="I106" t="s">
-        <v>20</v>
+        <v>58</v>
+      </c>
+      <c r="Q106" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="107" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>148</v>
+        <v>129</v>
       </c>
       <c r="B107" t="s">
-        <v>128</v>
+        <v>259</v>
       </c>
       <c r="C107" s="2" t="s">
-        <v>147</v>
+        <v>130</v>
+      </c>
+      <c r="E107" t="s">
+        <v>131</v>
+      </c>
+      <c r="F107">
+        <v>1945</v>
+      </c>
+      <c r="G107">
+        <v>2008</v>
+      </c>
+      <c r="I107" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="108" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>233</v>
+        <v>148</v>
       </c>
       <c r="B108" t="s">
-        <v>165</v>
+        <v>128</v>
       </c>
       <c r="C108" s="2" t="s">
-        <v>234</v>
-      </c>
-      <c r="E108" t="s">
-        <v>14</v>
-      </c>
-      <c r="F108">
-        <v>2012</v>
-      </c>
-      <c r="G108">
-        <v>2016</v>
-      </c>
-      <c r="H108" t="s">
-        <v>16</v>
-      </c>
-      <c r="I108" t="s">
-        <v>20</v>
+        <v>147</v>
       </c>
     </row>
     <row r="109" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>35</v>
+        <v>233</v>
       </c>
       <c r="B109" t="s">
-        <v>25</v>
+        <v>165</v>
       </c>
       <c r="C109" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="D109" t="s">
-        <v>37</v>
+        <v>234</v>
       </c>
       <c r="E109" t="s">
         <v>14</v>
       </c>
       <c r="F109">
-        <v>2001</v>
+        <v>2012</v>
+      </c>
+      <c r="G109">
+        <v>2016</v>
       </c>
       <c r="H109" t="s">
         <v>16</v>
@@ -3738,90 +3750,90 @@
     </row>
     <row r="110" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>185</v>
+        <v>35</v>
       </c>
       <c r="B110" t="s">
-        <v>128</v>
+        <v>25</v>
       </c>
       <c r="C110" s="2" t="s">
-        <v>186</v>
+        <v>36</v>
+      </c>
+      <c r="D110" t="s">
+        <v>37</v>
+      </c>
+      <c r="E110" t="s">
+        <v>14</v>
+      </c>
+      <c r="F110">
+        <v>2001</v>
+      </c>
+      <c r="H110" t="s">
+        <v>16</v>
+      </c>
+      <c r="I110" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="111" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>210</v>
+        <v>185</v>
       </c>
       <c r="B111" t="s">
-        <v>40</v>
+        <v>128</v>
       </c>
       <c r="C111" s="2" t="s">
-        <v>211</v>
-      </c>
-      <c r="F111">
-        <v>1976</v>
-      </c>
-      <c r="G111">
-        <v>2016</v>
-      </c>
-      <c r="H111" t="s">
-        <v>16</v>
-      </c>
-      <c r="I111" t="s">
-        <v>20</v>
+        <v>186</v>
       </c>
     </row>
     <row r="112" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>144</v>
+        <v>210</v>
       </c>
       <c r="B112" t="s">
-        <v>60</v>
+        <v>40</v>
       </c>
       <c r="C112" s="2" t="s">
-        <v>143</v>
+        <v>211</v>
       </c>
       <c r="F112">
-        <v>1800</v>
+        <v>1976</v>
       </c>
       <c r="G112">
-        <v>2013</v>
+        <v>2016</v>
+      </c>
+      <c r="H112" t="s">
+        <v>16</v>
+      </c>
+      <c r="I112" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="113" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>122</v>
+        <v>144</v>
       </c>
       <c r="B113" t="s">
-        <v>259</v>
+        <v>60</v>
       </c>
       <c r="C113" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="I113" t="s">
-        <v>20</v>
+        <v>143</v>
+      </c>
+      <c r="F113">
+        <v>1800</v>
+      </c>
+      <c r="G113">
+        <v>2013</v>
       </c>
     </row>
     <row r="114" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>318</v>
+        <v>122</v>
       </c>
       <c r="B114" t="s">
-        <v>250</v>
+        <v>259</v>
       </c>
       <c r="C114" s="2" t="s">
-        <v>319</v>
-      </c>
-      <c r="E114" t="s">
-        <v>320</v>
-      </c>
-      <c r="F114">
-        <v>1975</v>
-      </c>
-      <c r="G114">
-        <v>1989</v>
-      </c>
-      <c r="H114" t="s">
-        <v>16</v>
+        <v>121</v>
       </c>
       <c r="I114" t="s">
         <v>20</v>
@@ -3829,22 +3841,22 @@
     </row>
     <row r="115" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="B115" t="s">
         <v>250</v>
       </c>
       <c r="C115" s="2" t="s">
-        <v>317</v>
+        <v>319</v>
       </c>
       <c r="E115" t="s">
-        <v>105</v>
+        <v>320</v>
       </c>
       <c r="F115">
-        <v>1950</v>
+        <v>1975</v>
       </c>
       <c r="G115">
-        <v>1996</v>
+        <v>1989</v>
       </c>
       <c r="H115" t="s">
         <v>16</v>
@@ -3855,19 +3867,22 @@
     </row>
     <row r="116" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>322</v>
+        <v>316</v>
       </c>
       <c r="B116" t="s">
-        <v>25</v>
+        <v>250</v>
       </c>
       <c r="C116" s="2" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="E116" t="s">
-        <v>77</v>
+        <v>105</v>
       </c>
       <c r="F116">
-        <v>2010</v>
+        <v>1950</v>
+      </c>
+      <c r="G116">
+        <v>1996</v>
       </c>
       <c r="H116" t="s">
         <v>16</v>
@@ -3878,164 +3893,164 @@
     </row>
     <row r="117" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>141</v>
+        <v>322</v>
       </c>
       <c r="B117" t="s">
-        <v>237</v>
+        <v>25</v>
       </c>
       <c r="C117" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="Q117" t="s">
-        <v>17</v>
+        <v>321</v>
+      </c>
+      <c r="E117" t="s">
+        <v>77</v>
+      </c>
+      <c r="F117">
+        <v>2010</v>
+      </c>
+      <c r="H117" t="s">
+        <v>16</v>
+      </c>
+      <c r="I117" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="118" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>308</v>
+        <v>141</v>
       </c>
       <c r="B118" t="s">
-        <v>250</v>
+        <v>237</v>
       </c>
       <c r="C118" s="2" t="s">
-        <v>309</v>
-      </c>
-      <c r="E118" t="s">
-        <v>310</v>
-      </c>
-      <c r="F118">
-        <v>1950</v>
-      </c>
-      <c r="G118">
-        <v>2010</v>
-      </c>
-      <c r="H118" t="s">
-        <v>16</v>
-      </c>
-      <c r="I118" t="s">
-        <v>20</v>
+        <v>142</v>
+      </c>
+      <c r="Q118" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="119" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>287</v>
+        <v>308</v>
       </c>
       <c r="B119" t="s">
-        <v>134</v>
+        <v>250</v>
       </c>
       <c r="C119" s="2" t="s">
-        <v>288</v>
+        <v>309</v>
+      </c>
+      <c r="E119" t="s">
+        <v>310</v>
       </c>
       <c r="F119">
-        <v>1990</v>
+        <v>1950</v>
       </c>
       <c r="G119">
-        <v>2008</v>
+        <v>2010</v>
+      </c>
+      <c r="H119" t="s">
+        <v>16</v>
+      </c>
+      <c r="I119" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="120" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>274</v>
+        <v>287</v>
       </c>
       <c r="B120" t="s">
-        <v>55</v>
+        <v>134</v>
       </c>
       <c r="C120" s="2" t="s">
-        <v>275</v>
-      </c>
-      <c r="H120" t="s">
-        <v>16</v>
-      </c>
-      <c r="I120" t="s">
-        <v>20</v>
+        <v>288</v>
+      </c>
+      <c r="F120">
+        <v>1990</v>
+      </c>
+      <c r="G120">
+        <v>2008</v>
       </c>
     </row>
     <row r="121" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>157</v>
+        <v>274</v>
       </c>
       <c r="B121" t="s">
-        <v>128</v>
+        <v>55</v>
       </c>
       <c r="C121" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="Q121" t="s">
-        <v>18</v>
+        <v>275</v>
+      </c>
+      <c r="H121" t="s">
+        <v>16</v>
+      </c>
+      <c r="I121" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="122" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>194</v>
+        <v>157</v>
       </c>
       <c r="B122" t="s">
-        <v>99</v>
+        <v>128</v>
       </c>
       <c r="C122" s="2" t="s">
-        <v>193</v>
+        <v>154</v>
+      </c>
+      <c r="Q122" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="123" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>295</v>
+        <v>194</v>
       </c>
       <c r="B123" t="s">
-        <v>40</v>
+        <v>99</v>
       </c>
       <c r="C123" s="2" t="s">
-        <v>296</v>
-      </c>
-      <c r="E123" t="s">
-        <v>297</v>
-      </c>
-      <c r="F123">
-        <v>1990</v>
-      </c>
-      <c r="G123">
-        <v>2015</v>
-      </c>
-      <c r="H123" t="s">
-        <v>16</v>
-      </c>
-      <c r="I123" t="s">
-        <v>249</v>
+        <v>193</v>
       </c>
     </row>
     <row r="124" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>256</v>
+        <v>295</v>
       </c>
       <c r="B124" t="s">
-        <v>250</v>
+        <v>40</v>
       </c>
       <c r="C124" s="2" t="s">
-        <v>257</v>
+        <v>296</v>
       </c>
       <c r="E124" t="s">
-        <v>258</v>
+        <v>297</v>
+      </c>
+      <c r="F124">
+        <v>1990</v>
+      </c>
+      <c r="G124">
+        <v>2015</v>
       </c>
       <c r="H124" t="s">
         <v>16</v>
       </c>
       <c r="I124" t="s">
-        <v>20</v>
+        <v>249</v>
       </c>
     </row>
     <row r="125" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>227</v>
+        <v>256</v>
       </c>
       <c r="B125" t="s">
-        <v>40</v>
+        <v>250</v>
       </c>
       <c r="C125" s="2" t="s">
-        <v>225</v>
-      </c>
-      <c r="F125">
-        <v>1955</v>
-      </c>
-      <c r="G125">
-        <v>2016</v>
+        <v>257</v>
+      </c>
+      <c r="E125" t="s">
+        <v>258</v>
       </c>
       <c r="H125" t="s">
         <v>16</v>
@@ -4046,7 +4061,7 @@
     </row>
     <row r="126" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="B126" t="s">
         <v>40</v>
@@ -4055,7 +4070,7 @@
         <v>225</v>
       </c>
       <c r="F126">
-        <v>1995</v>
+        <v>1955</v>
       </c>
       <c r="G126">
         <v>2016</v>
@@ -4069,611 +4084,634 @@
     </row>
     <row r="127" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>109</v>
+        <v>230</v>
       </c>
       <c r="B127" t="s">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="C127" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="E127" t="s">
-        <v>111</v>
+        <v>225</v>
       </c>
       <c r="F127">
-        <v>1956</v>
+        <v>1995</v>
+      </c>
+      <c r="G127">
+        <v>2016</v>
+      </c>
+      <c r="H127" t="s">
+        <v>16</v>
+      </c>
+      <c r="I127" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="128" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>326</v>
+        <v>109</v>
       </c>
       <c r="B128" t="s">
         <v>25</v>
       </c>
       <c r="C128" s="2" t="s">
-        <v>327</v>
+        <v>110</v>
       </c>
       <c r="E128" t="s">
         <v>111</v>
       </c>
       <c r="F128">
-        <v>1998</v>
-      </c>
-      <c r="H128" t="s">
-        <v>16</v>
-      </c>
-      <c r="I128" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="129" spans="1:17" x14ac:dyDescent="0.2">
+        <v>1956</v>
+      </c>
+    </row>
+    <row r="129" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>91</v>
+        <v>326</v>
       </c>
       <c r="B129" t="s">
         <v>25</v>
       </c>
       <c r="C129" s="2" t="s">
+        <v>327</v>
+      </c>
+      <c r="E129" t="s">
+        <v>111</v>
+      </c>
+      <c r="F129">
+        <v>1998</v>
+      </c>
+      <c r="H129" t="s">
+        <v>16</v>
+      </c>
+      <c r="I129" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="130" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A130" t="s">
+        <v>91</v>
+      </c>
+      <c r="B130" t="s">
+        <v>25</v>
+      </c>
+      <c r="C130" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="E129" t="s">
+      <c r="E130" t="s">
         <v>92</v>
       </c>
-      <c r="F129">
+      <c r="F130">
         <v>1999</v>
       </c>
     </row>
-    <row r="130" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A130" t="s">
+    <row r="131" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A131" t="s">
         <v>314</v>
       </c>
-      <c r="B130" t="s">
+      <c r="B131" t="s">
         <v>40</v>
       </c>
-      <c r="C130" s="2" t="s">
+      <c r="C131" s="2" t="s">
         <v>313</v>
       </c>
-      <c r="E130" t="s">
+      <c r="E131" t="s">
         <v>315</v>
       </c>
-      <c r="F130">
+      <c r="F131">
         <v>1950</v>
       </c>
-      <c r="G130">
+      <c r="G131">
         <v>2004</v>
       </c>
-      <c r="H130" t="s">
-        <v>16</v>
-      </c>
-      <c r="I130" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="131" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A131" t="s">
+      <c r="H131" t="s">
+        <v>16</v>
+      </c>
+      <c r="I131" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="132" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A132" t="s">
         <v>161</v>
       </c>
-      <c r="B131" t="s">
+      <c r="B132" t="s">
         <v>25</v>
       </c>
-      <c r="C131" s="2" t="s">
+      <c r="C132" s="2" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="132" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A132" t="s">
+    <row r="133" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A133" t="s">
         <v>168</v>
-      </c>
-      <c r="B132" t="s">
-        <v>40</v>
-      </c>
-      <c r="C132" s="2" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="133" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A133" t="s">
-        <v>399</v>
       </c>
       <c r="B133" t="s">
         <v>40</v>
       </c>
       <c r="C133" s="2" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="134" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A134" t="s">
+        <v>399</v>
+      </c>
+      <c r="B134" t="s">
+        <v>40</v>
+      </c>
+      <c r="C134" s="2" t="s">
         <v>400</v>
       </c>
-      <c r="E133" t="s">
+      <c r="E134" t="s">
         <v>14</v>
       </c>
-      <c r="F133">
+      <c r="F134">
         <v>2000</v>
       </c>
-      <c r="G133">
+      <c r="G134">
         <v>2014</v>
       </c>
-      <c r="H133" t="s">
+      <c r="H134" t="s">
         <v>348</v>
       </c>
-      <c r="I133" t="s">
+      <c r="I134" t="s">
         <v>349</v>
       </c>
-      <c r="J133" s="2" t="s">
+      <c r="J134" s="2" t="s">
         <v>402</v>
       </c>
-      <c r="N133" s="2" t="s">
+      <c r="N134" s="2" t="s">
         <v>401</v>
       </c>
     </row>
-    <row r="134" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A134" t="s">
+    <row r="135" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A135" t="s">
         <v>213</v>
       </c>
-      <c r="B134" t="s">
+      <c r="B135" t="s">
         <v>55</v>
       </c>
-      <c r="C134" s="2" t="s">
+      <c r="C135" s="2" t="s">
         <v>212</v>
       </c>
-      <c r="H134" t="s">
-        <v>16</v>
-      </c>
-      <c r="I134" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="135" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A135" t="s">
+      <c r="H135" t="s">
+        <v>16</v>
+      </c>
+      <c r="I135" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="136" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A136" t="s">
         <v>395</v>
-      </c>
-      <c r="B135" t="s">
-        <v>25</v>
-      </c>
-      <c r="C135" s="2" t="s">
-        <v>394</v>
-      </c>
-      <c r="D135" t="s">
-        <v>396</v>
-      </c>
-      <c r="E135" t="s">
-        <v>111</v>
-      </c>
-      <c r="F135">
-        <v>1986</v>
-      </c>
-      <c r="G135">
-        <v>2015</v>
-      </c>
-      <c r="H135" t="s">
-        <v>367</v>
-      </c>
-      <c r="I135" t="s">
-        <v>398</v>
-      </c>
-      <c r="J135" s="2" t="s">
-        <v>397</v>
-      </c>
-    </row>
-    <row r="136" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A136" t="s">
-        <v>323</v>
       </c>
       <c r="B136" t="s">
         <v>25</v>
       </c>
       <c r="C136" s="2" t="s">
+        <v>394</v>
+      </c>
+      <c r="D136" t="s">
+        <v>396</v>
+      </c>
+      <c r="E136" t="s">
+        <v>111</v>
+      </c>
+      <c r="F136">
+        <v>1986</v>
+      </c>
+      <c r="G136">
+        <v>2015</v>
+      </c>
+      <c r="H136" t="s">
+        <v>367</v>
+      </c>
+      <c r="I136" t="s">
+        <v>398</v>
+      </c>
+      <c r="J136" s="2" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="137" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A137" t="s">
+        <v>323</v>
+      </c>
+      <c r="B137" t="s">
+        <v>25</v>
+      </c>
+      <c r="C137" s="2" t="s">
         <v>324</v>
       </c>
-      <c r="E136" t="s">
+      <c r="E137" t="s">
         <v>325</v>
       </c>
-      <c r="F136">
+      <c r="F137">
         <v>1942</v>
       </c>
-      <c r="H136" t="s">
-        <v>16</v>
-      </c>
-      <c r="I136" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="137" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A137" t="s">
+      <c r="H137" t="s">
+        <v>16</v>
+      </c>
+      <c r="I137" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="138" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A138" t="s">
         <v>273</v>
       </c>
-      <c r="B137" t="s">
+      <c r="B138" t="s">
         <v>237</v>
       </c>
-      <c r="C137" s="2" t="s">
+      <c r="C138" s="2" t="s">
         <v>272</v>
       </c>
-      <c r="F137">
+      <c r="F138">
         <v>1996</v>
       </c>
-      <c r="G137">
+      <c r="G138">
         <v>2016</v>
       </c>
-      <c r="H137" t="s">
-        <v>16</v>
-      </c>
-      <c r="I137" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="138" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A138" t="s">
+      <c r="H138" t="s">
+        <v>16</v>
+      </c>
+      <c r="I138" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="139" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A139" t="s">
         <v>66</v>
       </c>
-      <c r="B138" t="s">
+      <c r="B139" t="s">
         <v>25</v>
       </c>
-      <c r="C138" s="2" t="s">
+      <c r="C139" s="2" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="139" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A139" t="s">
+    <row r="140" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A140" t="s">
         <v>383</v>
-      </c>
-      <c r="B139" t="s">
-        <v>40</v>
-      </c>
-      <c r="C139" s="2" t="s">
-        <v>384</v>
-      </c>
-      <c r="E139" t="s">
-        <v>386</v>
-      </c>
-      <c r="F139">
-        <v>1951</v>
-      </c>
-      <c r="H139" t="s">
-        <v>348</v>
-      </c>
-      <c r="I139" t="s">
-        <v>349</v>
-      </c>
-      <c r="N139" s="2" t="s">
-        <v>385</v>
-      </c>
-    </row>
-    <row r="140" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A140" t="s">
-        <v>139</v>
       </c>
       <c r="B140" t="s">
         <v>40</v>
       </c>
       <c r="C140" s="2" t="s">
+        <v>384</v>
+      </c>
+      <c r="E140" t="s">
+        <v>386</v>
+      </c>
+      <c r="F140">
+        <v>1951</v>
+      </c>
+      <c r="H140" t="s">
+        <v>348</v>
+      </c>
+      <c r="I140" t="s">
+        <v>349</v>
+      </c>
+      <c r="N140" s="2" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="141" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A141" t="s">
+        <v>139</v>
+      </c>
+      <c r="B141" t="s">
+        <v>40</v>
+      </c>
+      <c r="C141" s="2" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="141" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A141" t="s">
+    <row r="142" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A142" t="s">
         <v>329</v>
       </c>
-      <c r="B141" t="s">
+      <c r="B142" t="s">
         <v>165</v>
       </c>
-      <c r="C141" s="2" t="s">
+      <c r="C142" s="2" t="s">
         <v>328</v>
       </c>
-      <c r="E141" t="s">
+      <c r="E142" t="s">
         <v>34</v>
       </c>
-      <c r="F141">
+      <c r="F142">
         <v>1789</v>
       </c>
-      <c r="H141" t="s">
-        <v>16</v>
-      </c>
-      <c r="I141" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="142" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A142" t="s">
+      <c r="H142" t="s">
+        <v>16</v>
+      </c>
+      <c r="I142" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="143" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A143" t="s">
         <v>172</v>
-      </c>
-      <c r="B142" t="s">
-        <v>60</v>
-      </c>
-      <c r="C142" s="2" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="143" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A143" t="s">
-        <v>217</v>
       </c>
       <c r="B143" t="s">
         <v>60</v>
       </c>
       <c r="C143" s="2" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="144" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A144" t="s">
+        <v>217</v>
+      </c>
+      <c r="B144" t="s">
+        <v>60</v>
+      </c>
+      <c r="C144" s="2" t="s">
         <v>216</v>
       </c>
-      <c r="E143" t="s">
+      <c r="E144" t="s">
         <v>14</v>
       </c>
-      <c r="F143">
+      <c r="F144">
         <v>1900</v>
       </c>
-      <c r="H143" t="s">
-        <v>16</v>
-      </c>
-      <c r="I143" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="144" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A144" t="s">
+      <c r="H144" t="s">
+        <v>16</v>
+      </c>
+      <c r="I144" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="145" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A145" t="s">
         <v>132</v>
       </c>
-      <c r="B144" t="s">
+      <c r="B145" t="s">
         <v>259</v>
       </c>
-      <c r="C144" s="2" t="s">
+      <c r="C145" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="Q144" t="s">
+      <c r="Q145" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="145" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A145" t="s">
+    <row r="146" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A146" t="s">
         <v>182</v>
       </c>
-      <c r="B145" t="s">
+      <c r="B146" t="s">
         <v>165</v>
       </c>
-      <c r="C145" s="2" t="s">
+      <c r="C146" s="2" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="146" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A146" t="s">
+    <row r="147" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A147" t="s">
         <v>115</v>
       </c>
-      <c r="B146" t="s">
+      <c r="B147" t="s">
         <v>128</v>
       </c>
-      <c r="C146" s="2" t="s">
+      <c r="C147" s="2" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="147" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A147" t="s">
+    <row r="148" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A148" t="s">
         <v>263</v>
       </c>
-      <c r="B147" t="s">
+      <c r="B148" t="s">
         <v>250</v>
       </c>
-      <c r="C147" s="2" t="s">
+      <c r="C148" s="2" t="s">
         <v>264</v>
       </c>
-      <c r="E147" t="s">
+      <c r="E148" t="s">
         <v>265</v>
       </c>
-      <c r="F147">
+      <c r="F148">
         <v>1500</v>
       </c>
-      <c r="G147">
+      <c r="G148">
         <v>2000</v>
       </c>
-      <c r="H147" t="s">
-        <v>16</v>
-      </c>
-      <c r="I147" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="148" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A148" t="s">
+      <c r="H148" t="s">
+        <v>16</v>
+      </c>
+      <c r="I148" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="149" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A149" t="s">
         <v>221</v>
       </c>
-      <c r="B148" t="s">
+      <c r="B149" t="s">
         <v>86</v>
       </c>
-      <c r="C148" s="2" t="s">
+      <c r="C149" s="2" t="s">
         <v>220</v>
       </c>
-      <c r="F148">
+      <c r="F149">
         <v>2013</v>
       </c>
-      <c r="H148" t="s">
-        <v>16</v>
-      </c>
-      <c r="I148" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="149" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A149" t="s">
+      <c r="H149" t="s">
+        <v>16</v>
+      </c>
+      <c r="I149" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="150" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A150" t="s">
         <v>13</v>
       </c>
-      <c r="B149" t="s">
+      <c r="B150" t="s">
         <v>25</v>
       </c>
-      <c r="C149" s="2" t="s">
+      <c r="C150" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="D149" s="1" t="s">
+      <c r="D150" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="E149" t="s">
+      <c r="E150" t="s">
         <v>14</v>
       </c>
-      <c r="F149">
+      <c r="F150">
         <v>1981</v>
       </c>
-      <c r="H149" t="s">
-        <v>16</v>
-      </c>
-      <c r="I149" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="150" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A150" t="s">
+      <c r="H150" t="s">
+        <v>16</v>
+      </c>
+      <c r="I150" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="151" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A151" t="s">
         <v>283</v>
       </c>
-      <c r="B150" t="s">
+      <c r="B151" t="s">
         <v>124</v>
       </c>
-      <c r="C150" s="2" t="s">
+      <c r="C151" s="2" t="s">
         <v>284</v>
       </c>
-      <c r="H150" t="s">
-        <v>16</v>
-      </c>
-      <c r="I150" t="s">
+      <c r="H151" t="s">
+        <v>16</v>
+      </c>
+      <c r="I151" t="s">
         <v>20</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:Q150">
+  <sortState ref="A2:Q151">
     <sortCondition ref="A2"/>
   </sortState>
   <hyperlinks>
     <hyperlink ref="C6" r:id="rId1"/>
-    <hyperlink ref="C57" r:id="rId2"/>
+    <hyperlink ref="C58" r:id="rId2"/>
     <hyperlink ref="C7" r:id="rId3"/>
     <hyperlink ref="C10" r:id="rId4"/>
-    <hyperlink ref="C90" r:id="rId5"/>
-    <hyperlink ref="C109" r:id="rId6"/>
-    <hyperlink ref="C149" r:id="rId7"/>
+    <hyperlink ref="C91" r:id="rId5"/>
+    <hyperlink ref="C110" r:id="rId6"/>
+    <hyperlink ref="C150" r:id="rId7"/>
     <hyperlink ref="C35" r:id="rId8"/>
     <hyperlink ref="C30" r:id="rId9"/>
-    <hyperlink ref="C48" r:id="rId10"/>
-    <hyperlink ref="C55" r:id="rId11"/>
+    <hyperlink ref="C49" r:id="rId10"/>
+    <hyperlink ref="C56" r:id="rId11"/>
     <hyperlink ref="C3" r:id="rId12"/>
     <hyperlink ref="C20" r:id="rId13"/>
-    <hyperlink ref="C59" r:id="rId14"/>
-    <hyperlink ref="C83" r:id="rId15"/>
+    <hyperlink ref="C60" r:id="rId14"/>
+    <hyperlink ref="C84" r:id="rId15"/>
     <hyperlink ref="C29" r:id="rId16"/>
-    <hyperlink ref="C105" r:id="rId17"/>
-    <hyperlink ref="C40" r:id="rId18"/>
-    <hyperlink ref="C69" r:id="rId19"/>
+    <hyperlink ref="C106" r:id="rId17"/>
+    <hyperlink ref="C41" r:id="rId18"/>
+    <hyperlink ref="C70" r:id="rId19"/>
     <hyperlink ref="C16" r:id="rId20"/>
-    <hyperlink ref="C138" r:id="rId21"/>
+    <hyperlink ref="C139" r:id="rId21"/>
     <hyperlink ref="C8" r:id="rId22"/>
     <hyperlink ref="C38" r:id="rId23"/>
-    <hyperlink ref="C52" r:id="rId24"/>
-    <hyperlink ref="C49" r:id="rId25"/>
-    <hyperlink ref="C53" r:id="rId26"/>
-    <hyperlink ref="C54" r:id="rId27"/>
-    <hyperlink ref="C67" r:id="rId28"/>
-    <hyperlink ref="C88" r:id="rId29"/>
-    <hyperlink ref="C129" r:id="rId30"/>
-    <hyperlink ref="C93" r:id="rId31"/>
-    <hyperlink ref="C78" r:id="rId32"/>
-    <hyperlink ref="C98" r:id="rId33"/>
-    <hyperlink ref="C68" r:id="rId34"/>
+    <hyperlink ref="C53" r:id="rId24"/>
+    <hyperlink ref="C50" r:id="rId25"/>
+    <hyperlink ref="C54" r:id="rId26"/>
+    <hyperlink ref="C55" r:id="rId27"/>
+    <hyperlink ref="C68" r:id="rId28"/>
+    <hyperlink ref="C89" r:id="rId29"/>
+    <hyperlink ref="C130" r:id="rId30"/>
+    <hyperlink ref="C94" r:id="rId31"/>
+    <hyperlink ref="C79" r:id="rId32"/>
+    <hyperlink ref="C99" r:id="rId33"/>
+    <hyperlink ref="C69" r:id="rId34"/>
     <hyperlink ref="C17" r:id="rId35"/>
-    <hyperlink ref="C127" r:id="rId36"/>
+    <hyperlink ref="C128" r:id="rId36"/>
     <hyperlink ref="C15" r:id="rId37"/>
-    <hyperlink ref="C146" r:id="rId38"/>
-    <hyperlink ref="C82" r:id="rId39"/>
-    <hyperlink ref="C56" r:id="rId40"/>
-    <hyperlink ref="C113" r:id="rId41"/>
+    <hyperlink ref="C147" r:id="rId38"/>
+    <hyperlink ref="C83" r:id="rId39"/>
+    <hyperlink ref="C57" r:id="rId40"/>
+    <hyperlink ref="C114" r:id="rId41"/>
     <hyperlink ref="C18" r:id="rId42"/>
-    <hyperlink ref="C50" r:id="rId43"/>
+    <hyperlink ref="C51" r:id="rId43"/>
     <hyperlink ref="C23" r:id="rId44"/>
-    <hyperlink ref="C106" r:id="rId45"/>
-    <hyperlink ref="C144" r:id="rId46"/>
+    <hyperlink ref="C107" r:id="rId45"/>
+    <hyperlink ref="C145" r:id="rId46"/>
     <hyperlink ref="C27" r:id="rId47" display="http://comparativeconstitutionsproject.org/"/>
-    <hyperlink ref="C103" r:id="rId48"/>
-    <hyperlink ref="C140" r:id="rId49"/>
-    <hyperlink ref="C117" r:id="rId50"/>
-    <hyperlink ref="C112" r:id="rId51"/>
+    <hyperlink ref="C104" r:id="rId48"/>
+    <hyperlink ref="C141" r:id="rId49"/>
+    <hyperlink ref="C118" r:id="rId50"/>
+    <hyperlink ref="C113" r:id="rId51"/>
     <hyperlink ref="C22" r:id="rId52"/>
-    <hyperlink ref="C107" r:id="rId53"/>
-    <hyperlink ref="C47" r:id="rId54"/>
-    <hyperlink ref="C72" r:id="rId55"/>
-    <hyperlink ref="C75" r:id="rId56"/>
-    <hyperlink ref="C104" r:id="rId57"/>
-    <hyperlink ref="C95" r:id="rId58"/>
-    <hyperlink ref="C121" r:id="rId59"/>
+    <hyperlink ref="C108" r:id="rId53"/>
+    <hyperlink ref="C48" r:id="rId54"/>
+    <hyperlink ref="C73" r:id="rId55"/>
+    <hyperlink ref="C76" r:id="rId56"/>
+    <hyperlink ref="C105" r:id="rId57"/>
+    <hyperlink ref="C96" r:id="rId58"/>
+    <hyperlink ref="C122" r:id="rId59"/>
     <hyperlink ref="C31" r:id="rId60"/>
-    <hyperlink ref="C131" r:id="rId61"/>
+    <hyperlink ref="C132" r:id="rId61"/>
     <hyperlink ref="C9" r:id="rId62"/>
     <hyperlink ref="C33" r:id="rId63"/>
-    <hyperlink ref="C132" r:id="rId64"/>
+    <hyperlink ref="C133" r:id="rId64"/>
     <hyperlink ref="C14" r:id="rId65"/>
-    <hyperlink ref="C142" r:id="rId66"/>
+    <hyperlink ref="C143" r:id="rId66"/>
     <hyperlink ref="C25" r:id="rId67"/>
     <hyperlink ref="C24" r:id="rId68"/>
     <hyperlink ref="C26" r:id="rId69"/>
-    <hyperlink ref="C51" r:id="rId70"/>
-    <hyperlink ref="C145" r:id="rId71"/>
+    <hyperlink ref="C52" r:id="rId70"/>
+    <hyperlink ref="C146" r:id="rId71"/>
     <hyperlink ref="C28" r:id="rId72"/>
-    <hyperlink ref="C110" r:id="rId73"/>
+    <hyperlink ref="C111" r:id="rId73"/>
     <hyperlink ref="C32" r:id="rId74"/>
-    <hyperlink ref="C44" r:id="rId75"/>
-    <hyperlink ref="C122" r:id="rId76"/>
-    <hyperlink ref="C41" r:id="rId77"/>
+    <hyperlink ref="C45" r:id="rId75"/>
+    <hyperlink ref="C123" r:id="rId76"/>
+    <hyperlink ref="C42" r:id="rId77"/>
     <hyperlink ref="C39" r:id="rId78"/>
-    <hyperlink ref="C66" r:id="rId79"/>
+    <hyperlink ref="C67" r:id="rId79"/>
     <hyperlink ref="C5" r:id="rId80"/>
-    <hyperlink ref="C65" r:id="rId81"/>
+    <hyperlink ref="C66" r:id="rId81"/>
     <hyperlink ref="C12" r:id="rId82"/>
-    <hyperlink ref="C102" r:id="rId83"/>
-    <hyperlink ref="C111" r:id="rId84"/>
-    <hyperlink ref="C134" r:id="rId85"/>
+    <hyperlink ref="C103" r:id="rId83"/>
+    <hyperlink ref="C112" r:id="rId84"/>
+    <hyperlink ref="C135" r:id="rId85"/>
     <hyperlink ref="C36" r:id="rId86"/>
-    <hyperlink ref="C143" r:id="rId87"/>
-    <hyperlink ref="C43" r:id="rId88"/>
-    <hyperlink ref="C148" r:id="rId89"/>
-    <hyperlink ref="C91" r:id="rId90"/>
-    <hyperlink ref="C63" r:id="rId91"/>
-    <hyperlink ref="C92" r:id="rId92"/>
-    <hyperlink ref="C125" r:id="rId93"/>
-    <hyperlink ref="C76" r:id="rId94"/>
-    <hyperlink ref="C96" r:id="rId95"/>
-    <hyperlink ref="C126" r:id="rId96"/>
-    <hyperlink ref="C60" r:id="rId97"/>
-    <hyperlink ref="C108" r:id="rId98"/>
-    <hyperlink ref="C45" r:id="rId99"/>
-    <hyperlink ref="C42" r:id="rId100"/>
-    <hyperlink ref="C79" r:id="rId101"/>
-    <hyperlink ref="C58" r:id="rId102"/>
+    <hyperlink ref="C144" r:id="rId87"/>
+    <hyperlink ref="C44" r:id="rId88"/>
+    <hyperlink ref="C149" r:id="rId89"/>
+    <hyperlink ref="C92" r:id="rId90"/>
+    <hyperlink ref="C64" r:id="rId91"/>
+    <hyperlink ref="C93" r:id="rId92"/>
+    <hyperlink ref="C126" r:id="rId93"/>
+    <hyperlink ref="C77" r:id="rId94"/>
+    <hyperlink ref="C97" r:id="rId95"/>
+    <hyperlink ref="C127" r:id="rId96"/>
+    <hyperlink ref="C61" r:id="rId97"/>
+    <hyperlink ref="C109" r:id="rId98"/>
+    <hyperlink ref="C46" r:id="rId99"/>
+    <hyperlink ref="C43" r:id="rId100"/>
+    <hyperlink ref="C80" r:id="rId101"/>
+    <hyperlink ref="C59" r:id="rId102"/>
     <hyperlink ref="C2" r:id="rId103"/>
-    <hyperlink ref="C73" r:id="rId104"/>
-    <hyperlink ref="C77" r:id="rId105"/>
-    <hyperlink ref="C100" r:id="rId106"/>
-    <hyperlink ref="C46" r:id="rId107"/>
-    <hyperlink ref="C80" r:id="rId108"/>
-    <hyperlink ref="C124" r:id="rId109"/>
+    <hyperlink ref="C74" r:id="rId104"/>
+    <hyperlink ref="C78" r:id="rId105"/>
+    <hyperlink ref="C101" r:id="rId106"/>
+    <hyperlink ref="C47" r:id="rId107"/>
+    <hyperlink ref="C81" r:id="rId108"/>
+    <hyperlink ref="C125" r:id="rId109"/>
     <hyperlink ref="C13" r:id="rId110"/>
     <hyperlink ref="C4" r:id="rId111"/>
-    <hyperlink ref="C147" r:id="rId112"/>
-    <hyperlink ref="C86" r:id="rId113"/>
-    <hyperlink ref="C81" r:id="rId114"/>
-    <hyperlink ref="C137" r:id="rId115"/>
-    <hyperlink ref="C120" r:id="rId116"/>
-    <hyperlink ref="C62" r:id="rId117"/>
-    <hyperlink ref="C94" r:id="rId118"/>
-    <hyperlink ref="C71" r:id="rId119"/>
-    <hyperlink ref="C150" r:id="rId120"/>
-    <hyperlink ref="C64" r:id="rId121"/>
-    <hyperlink ref="C119" r:id="rId122"/>
-    <hyperlink ref="C99" r:id="rId123"/>
-    <hyperlink ref="C74" r:id="rId124"/>
-    <hyperlink ref="C97" r:id="rId125"/>
-    <hyperlink ref="C123" r:id="rId126"/>
-    <hyperlink ref="C84" r:id="rId127"/>
+    <hyperlink ref="C148" r:id="rId112"/>
+    <hyperlink ref="C87" r:id="rId113"/>
+    <hyperlink ref="C82" r:id="rId114"/>
+    <hyperlink ref="C138" r:id="rId115"/>
+    <hyperlink ref="C121" r:id="rId116"/>
+    <hyperlink ref="C63" r:id="rId117"/>
+    <hyperlink ref="C95" r:id="rId118"/>
+    <hyperlink ref="C72" r:id="rId119"/>
+    <hyperlink ref="C151" r:id="rId120"/>
+    <hyperlink ref="C65" r:id="rId121"/>
+    <hyperlink ref="C120" r:id="rId122"/>
+    <hyperlink ref="C100" r:id="rId123"/>
+    <hyperlink ref="C75" r:id="rId124"/>
+    <hyperlink ref="C98" r:id="rId125"/>
+    <hyperlink ref="C124" r:id="rId126"/>
+    <hyperlink ref="C85" r:id="rId127"/>
     <hyperlink ref="C11" r:id="rId128"/>
     <hyperlink ref="C19" r:id="rId129"/>
-    <hyperlink ref="C118" r:id="rId130"/>
-    <hyperlink ref="C70" r:id="rId131"/>
-    <hyperlink ref="C130" r:id="rId132"/>
-    <hyperlink ref="C115" r:id="rId133"/>
-    <hyperlink ref="C114" r:id="rId134"/>
-    <hyperlink ref="C116" r:id="rId135"/>
-    <hyperlink ref="C136" r:id="rId136"/>
-    <hyperlink ref="C128" r:id="rId137"/>
-    <hyperlink ref="C141" r:id="rId138"/>
+    <hyperlink ref="C119" r:id="rId130"/>
+    <hyperlink ref="C71" r:id="rId131"/>
+    <hyperlink ref="C131" r:id="rId132"/>
+    <hyperlink ref="C116" r:id="rId133"/>
+    <hyperlink ref="C115" r:id="rId134"/>
+    <hyperlink ref="C117" r:id="rId135"/>
+    <hyperlink ref="C137" r:id="rId136"/>
+    <hyperlink ref="C129" r:id="rId137"/>
+    <hyperlink ref="C142" r:id="rId138"/>
     <hyperlink ref="C37" r:id="rId139"/>
-    <hyperlink ref="C85" r:id="rId140"/>
+    <hyperlink ref="C86" r:id="rId140"/>
     <hyperlink ref="J2" r:id="rId141"/>
     <hyperlink ref="M3" r:id="rId142"/>
     <hyperlink ref="J3" r:id="rId143"/>
@@ -4681,25 +4719,28 @@
     <hyperlink ref="J4" r:id="rId145"/>
     <hyperlink ref="P5" r:id="rId146"/>
     <hyperlink ref="J5" r:id="rId147"/>
-    <hyperlink ref="C101" r:id="rId148"/>
+    <hyperlink ref="C102" r:id="rId148"/>
     <hyperlink ref="C34" r:id="rId149"/>
     <hyperlink ref="P7" r:id="rId150"/>
     <hyperlink ref="J7" r:id="rId151"/>
     <hyperlink ref="M8" r:id="rId152"/>
     <hyperlink ref="L8" r:id="rId153"/>
     <hyperlink ref="J8" r:id="rId154"/>
-    <hyperlink ref="C139" r:id="rId155"/>
-    <hyperlink ref="N139" r:id="rId156"/>
+    <hyperlink ref="C140" r:id="rId155"/>
+    <hyperlink ref="N140" r:id="rId156"/>
     <hyperlink ref="C21" r:id="rId157"/>
     <hyperlink ref="N21" r:id="rId158"/>
-    <hyperlink ref="C61" r:id="rId159"/>
-    <hyperlink ref="C135" r:id="rId160"/>
-    <hyperlink ref="J135" r:id="rId161"/>
-    <hyperlink ref="C133" r:id="rId162"/>
-    <hyperlink ref="N133" r:id="rId163"/>
-    <hyperlink ref="J133" r:id="rId164"/>
-    <hyperlink ref="C89" r:id="rId165"/>
-    <hyperlink ref="C87" r:id="rId166"/>
+    <hyperlink ref="C62" r:id="rId159"/>
+    <hyperlink ref="C136" r:id="rId160"/>
+    <hyperlink ref="J136" r:id="rId161"/>
+    <hyperlink ref="C134" r:id="rId162"/>
+    <hyperlink ref="N134" r:id="rId163"/>
+    <hyperlink ref="J134" r:id="rId164"/>
+    <hyperlink ref="C90" r:id="rId165"/>
+    <hyperlink ref="C88" r:id="rId166"/>
+    <hyperlink ref="C40" r:id="rId167"/>
+    <hyperlink ref="J40" r:id="rId168"/>
+    <hyperlink ref="K40" r:id="rId169"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
add two datasets, 'Members and Activists of Political Parties' and 'Global Media Freedom Dataset'
</commit_message>
<xml_diff>
--- a/PolData.xlsx
+++ b/PolData.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="753" uniqueCount="413">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="769" uniqueCount="423">
   <si>
     <t>name</t>
   </si>
@@ -1266,6 +1266,36 @@
   </si>
   <si>
     <t>http://www.robertthomson.info/wp-content/uploads/2011/01/deu15_27_26March2012.csv</t>
+  </si>
+  <si>
+    <t>Members and Activists of Political Parties</t>
+  </si>
+  <si>
+    <t>https://zenodo.org/record/61234</t>
+  </si>
+  <si>
+    <t>Australia, Austria, Belgium, Brazil, Canada, Croatia, Cyprus, Czech Republic, Denmark, Estonia, Finland, France, Germany, Hungary, Iceland, Ireland, Israel, Italy, Lithuania, Mexico, Netherlands, Norway, Poland, Portugal, Romania, Slovakia, Slovenia, Spain, Spain, Sweden, Switzerland, United Kingdom</t>
+  </si>
+  <si>
+    <t>https://zenodo.org/record/61234/files/MAPP_dataset_-_Version_2.0.xlsx</t>
+  </si>
+  <si>
+    <t>See also this link for more documentation https://doi.org/10.1057/s41304-016-0098-z</t>
+  </si>
+  <si>
+    <t>Global Media Freedom Dataset</t>
+  </si>
+  <si>
+    <t>http://faculty.uml.edu/Jenifer_whittenwoodring/MediaFreedomData_000.aspx</t>
+  </si>
+  <si>
+    <t>196 countries</t>
+  </si>
+  <si>
+    <t>http://faculty.uml.edu/Jenifer_whittenwoodring/GMFD_V2.csv</t>
+  </si>
+  <si>
+    <t>See also this article for more info https://doi.org/10.1017/psrm.2015.68</t>
   </si>
 </sst>
 </file>
@@ -1605,10 +1635,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q151"/>
+  <dimension ref="A1:Q153"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A131" workbookViewId="0">
-      <selection activeCell="A151" sqref="A151"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R73" sqref="R73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3034,44 +3064,59 @@
     </row>
     <row r="73" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>151</v>
+        <v>418</v>
       </c>
       <c r="B73" t="s">
-        <v>40</v>
+        <v>86</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>152</v>
+        <v>419</v>
       </c>
       <c r="E73" t="s">
-        <v>14</v>
+        <v>420</v>
+      </c>
+      <c r="F73">
+        <v>1948</v>
+      </c>
+      <c r="G73">
+        <v>2012</v>
+      </c>
+      <c r="H73" t="s">
+        <v>348</v>
+      </c>
+      <c r="I73" t="s">
+        <v>349</v>
+      </c>
+      <c r="K73" s="2" t="s">
+        <v>421</v>
+      </c>
+      <c r="Q73" t="s">
+        <v>422</v>
       </c>
     </row>
     <row r="74" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>242</v>
+        <v>151</v>
       </c>
       <c r="B74" t="s">
-        <v>237</v>
+        <v>40</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>243</v>
-      </c>
-      <c r="H74" t="s">
-        <v>16</v>
-      </c>
-      <c r="I74" t="s">
-        <v>20</v>
+        <v>152</v>
+      </c>
+      <c r="E74" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="75" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>292</v>
+        <v>242</v>
       </c>
       <c r="B75" t="s">
-        <v>99</v>
+        <v>237</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>291</v>
+        <v>243</v>
       </c>
       <c r="H75" t="s">
         <v>16</v>
@@ -3082,47 +3127,47 @@
     </row>
     <row r="76" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>153</v>
+        <v>292</v>
       </c>
       <c r="B76" t="s">
-        <v>259</v>
+        <v>99</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>154</v>
+        <v>291</v>
+      </c>
+      <c r="H76" t="s">
+        <v>16</v>
+      </c>
+      <c r="I76" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="77" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>228</v>
+        <v>153</v>
       </c>
       <c r="B77" t="s">
-        <v>40</v>
+        <v>259</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>225</v>
-      </c>
-      <c r="F77">
-        <v>1989</v>
-      </c>
-      <c r="G77">
-        <v>2017</v>
-      </c>
-      <c r="H77" t="s">
-        <v>16</v>
-      </c>
-      <c r="I77" t="s">
-        <v>20</v>
+        <v>154</v>
       </c>
     </row>
     <row r="78" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>245</v>
+        <v>228</v>
       </c>
       <c r="B78" t="s">
-        <v>237</v>
+        <v>40</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>244</v>
+        <v>225</v>
+      </c>
+      <c r="F78">
+        <v>1989</v>
+      </c>
+      <c r="G78">
+        <v>2017</v>
       </c>
       <c r="H78" t="s">
         <v>16</v>
@@ -3133,50 +3178,41 @@
     </row>
     <row r="79" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>100</v>
+        <v>245</v>
       </c>
       <c r="B79" t="s">
-        <v>99</v>
+        <v>237</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>101</v>
+        <v>244</v>
+      </c>
+      <c r="H79" t="s">
+        <v>16</v>
+      </c>
+      <c r="I79" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="80" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>239</v>
+        <v>100</v>
       </c>
       <c r="B80" t="s">
-        <v>237</v>
+        <v>99</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>243</v>
-      </c>
-      <c r="H80" t="s">
-        <v>16</v>
-      </c>
-      <c r="I80" t="s">
-        <v>20</v>
+        <v>101</v>
       </c>
     </row>
     <row r="81" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>254</v>
+        <v>239</v>
       </c>
       <c r="B81" t="s">
-        <v>55</v>
+        <v>237</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>253</v>
-      </c>
-      <c r="E81" t="s">
-        <v>255</v>
-      </c>
-      <c r="F81">
-        <v>1960</v>
-      </c>
-      <c r="G81">
-        <v>2014</v>
+        <v>243</v>
       </c>
       <c r="H81" t="s">
         <v>16</v>
@@ -3187,19 +3223,22 @@
     </row>
     <row r="82" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>270</v>
+        <v>254</v>
       </c>
       <c r="B82" t="s">
         <v>55</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>271</v>
+        <v>253</v>
+      </c>
+      <c r="E82" t="s">
+        <v>255</v>
       </c>
       <c r="F82">
-        <v>1990</v>
+        <v>1960</v>
       </c>
       <c r="G82">
-        <v>2010</v>
+        <v>2014</v>
       </c>
       <c r="H82" t="s">
         <v>16</v>
@@ -3210,96 +3249,90 @@
     </row>
     <row r="83" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>117</v>
+        <v>270</v>
       </c>
       <c r="B83" t="s">
         <v>55</v>
       </c>
       <c r="C83" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="F83">
+        <v>1990</v>
+      </c>
+      <c r="G83">
+        <v>2010</v>
+      </c>
+      <c r="H83" t="s">
+        <v>16</v>
+      </c>
+      <c r="I83" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="84" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A84" t="s">
+        <v>117</v>
+      </c>
+      <c r="B84" t="s">
+        <v>55</v>
+      </c>
+      <c r="C84" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="I83" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q83" t="s">
+      <c r="I84" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q84" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="84" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A84" s="1" t="s">
+    <row r="85" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A85" s="1" t="s">
         <v>23</v>
-      </c>
-      <c r="B84" t="s">
-        <v>25</v>
-      </c>
-      <c r="C84" s="2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="85" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A85" t="s">
-        <v>300</v>
       </c>
       <c r="B85" t="s">
         <v>25</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>298</v>
-      </c>
-      <c r="E85" t="s">
-        <v>299</v>
-      </c>
-      <c r="F85">
-        <v>1969</v>
-      </c>
-      <c r="H85" t="s">
-        <v>16</v>
-      </c>
-      <c r="I85" t="s">
-        <v>249</v>
+        <v>53</v>
       </c>
     </row>
     <row r="86" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>332</v>
+        <v>300</v>
       </c>
       <c r="B86" t="s">
-        <v>134</v>
+        <v>25</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>333</v>
+        <v>298</v>
       </c>
       <c r="E86" t="s">
-        <v>334</v>
+        <v>299</v>
+      </c>
+      <c r="F86">
+        <v>1969</v>
       </c>
       <c r="H86" t="s">
         <v>16</v>
       </c>
       <c r="I86" t="s">
-        <v>20</v>
+        <v>249</v>
       </c>
     </row>
     <row r="87" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>267</v>
+        <v>332</v>
       </c>
       <c r="B87" t="s">
-        <v>250</v>
+        <v>134</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>266</v>
-      </c>
-      <c r="D87" t="s">
-        <v>269</v>
+        <v>333</v>
       </c>
       <c r="E87" t="s">
-        <v>268</v>
-      </c>
-      <c r="F87">
-        <v>1970</v>
-      </c>
-      <c r="G87">
-        <v>2014</v>
+        <v>334</v>
       </c>
       <c r="H87" t="s">
         <v>16</v>
@@ -3310,143 +3343,149 @@
     </row>
     <row r="88" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>407</v>
+        <v>267</v>
       </c>
       <c r="B88" t="s">
-        <v>40</v>
+        <v>250</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>406</v>
+        <v>266</v>
       </c>
       <c r="D88" t="s">
-        <v>408</v>
+        <v>269</v>
       </c>
       <c r="E88" t="s">
-        <v>14</v>
+        <v>268</v>
       </c>
       <c r="F88">
-        <v>1949</v>
+        <v>1970</v>
       </c>
       <c r="G88">
-        <v>2013</v>
+        <v>2014</v>
       </c>
       <c r="H88" t="s">
-        <v>348</v>
+        <v>16</v>
       </c>
       <c r="I88" t="s">
-        <v>349</v>
+        <v>20</v>
       </c>
     </row>
     <row r="89" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>96</v>
+        <v>407</v>
       </c>
       <c r="B89" t="s">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>90</v>
+        <v>406</v>
+      </c>
+      <c r="D89" t="s">
+        <v>408</v>
       </c>
       <c r="E89" t="s">
-        <v>69</v>
+        <v>14</v>
       </c>
       <c r="F89">
-        <v>1995</v>
+        <v>1949</v>
+      </c>
+      <c r="G89">
+        <v>2013</v>
+      </c>
+      <c r="H89" t="s">
+        <v>348</v>
+      </c>
+      <c r="I89" t="s">
+        <v>349</v>
       </c>
     </row>
     <row r="90" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>404</v>
+        <v>96</v>
       </c>
       <c r="B90" t="s">
-        <v>83</v>
+        <v>25</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>403</v>
-      </c>
-      <c r="D90" t="s">
-        <v>405</v>
+        <v>90</v>
       </c>
       <c r="E90" t="s">
-        <v>14</v>
+        <v>69</v>
       </c>
       <c r="F90">
-        <v>1875</v>
-      </c>
-      <c r="G90">
-        <v>2004</v>
-      </c>
-      <c r="H90" t="s">
-        <v>348</v>
-      </c>
-      <c r="I90" t="s">
-        <v>349</v>
+        <v>1995</v>
       </c>
     </row>
     <row r="91" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>11</v>
+        <v>404</v>
       </c>
       <c r="B91" t="s">
-        <v>25</v>
+        <v>83</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>12</v>
+        <v>403</v>
       </c>
       <c r="D91" t="s">
-        <v>95</v>
+        <v>405</v>
       </c>
       <c r="E91" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="F91">
-        <v>2007</v>
+        <v>1875</v>
+      </c>
+      <c r="G91">
+        <v>2004</v>
       </c>
       <c r="H91" t="s">
-        <v>16</v>
+        <v>348</v>
       </c>
       <c r="I91" t="s">
-        <v>21</v>
+        <v>349</v>
       </c>
     </row>
     <row r="92" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>223</v>
+        <v>11</v>
       </c>
       <c r="B92" t="s">
-        <v>124</v>
+        <v>25</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>222</v>
+        <v>12</v>
+      </c>
+      <c r="D92" t="s">
+        <v>95</v>
+      </c>
+      <c r="E92" t="s">
+        <v>10</v>
       </c>
       <c r="F92">
-        <v>1</v>
-      </c>
-      <c r="G92">
-        <v>2010</v>
+        <v>2007</v>
       </c>
       <c r="H92" t="s">
         <v>16</v>
       </c>
       <c r="I92" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="93" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="B93" t="s">
-        <v>40</v>
+        <v>124</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="F93">
-        <v>1946</v>
+        <v>1</v>
       </c>
       <c r="G93">
-        <v>2016</v>
+        <v>2010</v>
       </c>
       <c r="H93" t="s">
         <v>16</v>
@@ -3457,292 +3496,310 @@
     </row>
     <row r="94" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>97</v>
+        <v>226</v>
       </c>
       <c r="B94" t="s">
-        <v>128</v>
+        <v>40</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>98</v>
+        <v>225</v>
+      </c>
+      <c r="F94">
+        <v>1946</v>
+      </c>
+      <c r="G94">
+        <v>2016</v>
+      </c>
+      <c r="H94" t="s">
+        <v>16</v>
+      </c>
+      <c r="I94" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="95" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>278</v>
+        <v>97</v>
       </c>
       <c r="B95" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>279</v>
-      </c>
-      <c r="E95" t="s">
-        <v>280</v>
-      </c>
-      <c r="F95">
-        <v>1890</v>
-      </c>
-      <c r="G95">
-        <v>1996</v>
-      </c>
-      <c r="H95" t="s">
-        <v>16</v>
-      </c>
-      <c r="I95" t="s">
-        <v>20</v>
+        <v>98</v>
       </c>
     </row>
     <row r="96" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>156</v>
+        <v>278</v>
       </c>
       <c r="B96" t="s">
-        <v>25</v>
+        <v>124</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>154</v>
+        <v>279</v>
+      </c>
+      <c r="E96" t="s">
+        <v>280</v>
+      </c>
+      <c r="F96">
+        <v>1890</v>
+      </c>
+      <c r="G96">
+        <v>1996</v>
+      </c>
+      <c r="H96" t="s">
+        <v>16</v>
+      </c>
+      <c r="I96" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="97" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>229</v>
+        <v>156</v>
       </c>
       <c r="B97" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>225</v>
-      </c>
-      <c r="F97">
-        <v>1952</v>
-      </c>
-      <c r="G97">
-        <v>1997</v>
-      </c>
-      <c r="H97" t="s">
-        <v>16</v>
-      </c>
-      <c r="I97" t="s">
-        <v>20</v>
+        <v>154</v>
       </c>
     </row>
     <row r="98" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>293</v>
+        <v>413</v>
       </c>
       <c r="B98" t="s">
-        <v>40</v>
+        <v>128</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>294</v>
+        <v>414</v>
+      </c>
+      <c r="E98" t="s">
+        <v>415</v>
       </c>
       <c r="F98">
-        <v>2004</v>
+        <v>1946</v>
       </c>
       <c r="G98">
-        <v>2006</v>
+        <v>2014</v>
       </c>
       <c r="H98" t="s">
-        <v>16</v>
+        <v>348</v>
       </c>
       <c r="I98" t="s">
-        <v>20</v>
+        <v>349</v>
+      </c>
+      <c r="N98" s="2" t="s">
+        <v>416</v>
+      </c>
+      <c r="Q98" t="s">
+        <v>417</v>
       </c>
     </row>
     <row r="99" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>102</v>
+        <v>229</v>
       </c>
       <c r="B99" t="s">
-        <v>99</v>
+        <v>40</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>103</v>
+        <v>225</v>
+      </c>
+      <c r="F99">
+        <v>1952</v>
+      </c>
+      <c r="G99">
+        <v>1997</v>
+      </c>
+      <c r="H99" t="s">
+        <v>16</v>
+      </c>
+      <c r="I99" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="100" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>289</v>
+        <v>293</v>
       </c>
       <c r="B100" t="s">
-        <v>124</v>
+        <v>40</v>
       </c>
       <c r="C100" s="2" t="s">
-        <v>290</v>
+        <v>294</v>
+      </c>
+      <c r="F100">
+        <v>2004</v>
+      </c>
+      <c r="G100">
+        <v>2006</v>
+      </c>
+      <c r="H100" t="s">
+        <v>16</v>
+      </c>
+      <c r="I100" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="101" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>246</v>
+        <v>102</v>
       </c>
       <c r="B101" t="s">
-        <v>165</v>
+        <v>99</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>247</v>
-      </c>
-      <c r="E101" t="s">
-        <v>14</v>
-      </c>
-      <c r="F101">
-        <v>1960</v>
-      </c>
-      <c r="G101">
-        <v>2006</v>
-      </c>
-      <c r="H101" t="s">
-        <v>16</v>
-      </c>
-      <c r="I101" t="s">
-        <v>249</v>
+        <v>103</v>
       </c>
     </row>
     <row r="102" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>365</v>
+        <v>289</v>
       </c>
       <c r="B102" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="C102" s="2" t="s">
-        <v>364</v>
-      </c>
-      <c r="D102" t="s">
-        <v>370</v>
-      </c>
-      <c r="E102" t="s">
-        <v>366</v>
-      </c>
-      <c r="F102">
-        <v>1906</v>
-      </c>
-      <c r="G102">
-        <v>2013</v>
-      </c>
-      <c r="H102" t="s">
-        <v>367</v>
-      </c>
-      <c r="I102" t="s">
-        <v>368</v>
-      </c>
-      <c r="Q102" t="s">
-        <v>369</v>
+        <v>290</v>
       </c>
     </row>
     <row r="103" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>208</v>
+        <v>246</v>
       </c>
       <c r="B103" t="s">
-        <v>124</v>
+        <v>165</v>
       </c>
       <c r="C103" s="2" t="s">
-        <v>209</v>
+        <v>247</v>
+      </c>
+      <c r="E103" t="s">
+        <v>14</v>
       </c>
       <c r="F103">
-        <v>1932</v>
+        <v>1960</v>
       </c>
       <c r="G103">
-        <v>2014</v>
+        <v>2006</v>
       </c>
       <c r="H103" t="s">
         <v>16</v>
       </c>
       <c r="I103" t="s">
-        <v>20</v>
+        <v>249</v>
       </c>
     </row>
     <row r="104" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>137</v>
+        <v>365</v>
       </c>
       <c r="B104" t="s">
-        <v>259</v>
+        <v>128</v>
       </c>
       <c r="C104" s="2" t="s">
-        <v>138</v>
+        <v>364</v>
+      </c>
+      <c r="D104" t="s">
+        <v>370</v>
+      </c>
+      <c r="E104" t="s">
+        <v>366</v>
+      </c>
+      <c r="F104">
+        <v>1906</v>
+      </c>
+      <c r="G104">
+        <v>2013</v>
+      </c>
+      <c r="H104" t="s">
+        <v>367</v>
+      </c>
+      <c r="I104" t="s">
+        <v>368</v>
+      </c>
+      <c r="Q104" t="s">
+        <v>369</v>
       </c>
     </row>
     <row r="105" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>155</v>
+        <v>208</v>
       </c>
       <c r="B105" t="s">
-        <v>259</v>
+        <v>124</v>
       </c>
       <c r="C105" s="2" t="s">
-        <v>154</v>
+        <v>209</v>
+      </c>
+      <c r="F105">
+        <v>1932</v>
+      </c>
+      <c r="G105">
+        <v>2014</v>
+      </c>
+      <c r="H105" t="s">
+        <v>16</v>
+      </c>
+      <c r="I105" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="106" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>57</v>
+        <v>137</v>
       </c>
       <c r="B106" t="s">
-        <v>128</v>
+        <v>259</v>
       </c>
       <c r="C106" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="Q106" t="s">
-        <v>17</v>
+        <v>138</v>
       </c>
     </row>
     <row r="107" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>129</v>
+        <v>155</v>
       </c>
       <c r="B107" t="s">
         <v>259</v>
       </c>
       <c r="C107" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="E107" t="s">
-        <v>131</v>
-      </c>
-      <c r="F107">
-        <v>1945</v>
-      </c>
-      <c r="G107">
-        <v>2008</v>
-      </c>
-      <c r="I107" t="s">
-        <v>20</v>
+        <v>154</v>
       </c>
     </row>
     <row r="108" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>148</v>
+        <v>57</v>
       </c>
       <c r="B108" t="s">
         <v>128</v>
       </c>
       <c r="C108" s="2" t="s">
-        <v>147</v>
+        <v>58</v>
+      </c>
+      <c r="Q108" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="109" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>233</v>
+        <v>129</v>
       </c>
       <c r="B109" t="s">
-        <v>165</v>
+        <v>259</v>
       </c>
       <c r="C109" s="2" t="s">
-        <v>234</v>
+        <v>130</v>
       </c>
       <c r="E109" t="s">
-        <v>14</v>
+        <v>131</v>
       </c>
       <c r="F109">
-        <v>2012</v>
+        <v>1945</v>
       </c>
       <c r="G109">
-        <v>2016</v>
-      </c>
-      <c r="H109" t="s">
-        <v>16</v>
+        <v>2008</v>
       </c>
       <c r="I109" t="s">
         <v>20</v>
@@ -3750,56 +3807,59 @@
     </row>
     <row r="110" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>35</v>
+        <v>148</v>
       </c>
       <c r="B110" t="s">
-        <v>25</v>
+        <v>128</v>
       </c>
       <c r="C110" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="D110" t="s">
-        <v>37</v>
-      </c>
-      <c r="E110" t="s">
-        <v>14</v>
-      </c>
-      <c r="F110">
-        <v>2001</v>
-      </c>
-      <c r="H110" t="s">
-        <v>16</v>
-      </c>
-      <c r="I110" t="s">
-        <v>20</v>
+        <v>147</v>
       </c>
     </row>
     <row r="111" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>185</v>
+        <v>233</v>
       </c>
       <c r="B111" t="s">
-        <v>128</v>
+        <v>165</v>
       </c>
       <c r="C111" s="2" t="s">
-        <v>186</v>
+        <v>234</v>
+      </c>
+      <c r="E111" t="s">
+        <v>14</v>
+      </c>
+      <c r="F111">
+        <v>2012</v>
+      </c>
+      <c r="G111">
+        <v>2016</v>
+      </c>
+      <c r="H111" t="s">
+        <v>16</v>
+      </c>
+      <c r="I111" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="112" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>210</v>
+        <v>35</v>
       </c>
       <c r="B112" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="C112" s="2" t="s">
-        <v>211</v>
+        <v>36</v>
+      </c>
+      <c r="D112" t="s">
+        <v>37</v>
+      </c>
+      <c r="E112" t="s">
+        <v>14</v>
       </c>
       <c r="F112">
-        <v>1976</v>
-      </c>
-      <c r="G112">
-        <v>2016</v>
+        <v>2001</v>
       </c>
       <c r="H112" t="s">
         <v>16</v>
@@ -3810,30 +3870,33 @@
     </row>
     <row r="113" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>144</v>
+        <v>185</v>
       </c>
       <c r="B113" t="s">
-        <v>60</v>
+        <v>128</v>
       </c>
       <c r="C113" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="F113">
-        <v>1800</v>
-      </c>
-      <c r="G113">
-        <v>2013</v>
+        <v>186</v>
       </c>
     </row>
     <row r="114" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>122</v>
+        <v>210</v>
       </c>
       <c r="B114" t="s">
-        <v>259</v>
+        <v>40</v>
       </c>
       <c r="C114" s="2" t="s">
-        <v>121</v>
+        <v>211</v>
+      </c>
+      <c r="F114">
+        <v>1976</v>
+      </c>
+      <c r="G114">
+        <v>2016</v>
+      </c>
+      <c r="H114" t="s">
+        <v>16</v>
       </c>
       <c r="I114" t="s">
         <v>20</v>
@@ -3841,51 +3904,30 @@
     </row>
     <row r="115" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>318</v>
+        <v>144</v>
       </c>
       <c r="B115" t="s">
-        <v>250</v>
+        <v>60</v>
       </c>
       <c r="C115" s="2" t="s">
-        <v>319</v>
-      </c>
-      <c r="E115" t="s">
-        <v>320</v>
+        <v>143</v>
       </c>
       <c r="F115">
-        <v>1975</v>
+        <v>1800</v>
       </c>
       <c r="G115">
-        <v>1989</v>
-      </c>
-      <c r="H115" t="s">
-        <v>16</v>
-      </c>
-      <c r="I115" t="s">
-        <v>20</v>
+        <v>2013</v>
       </c>
     </row>
     <row r="116" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>316</v>
+        <v>122</v>
       </c>
       <c r="B116" t="s">
-        <v>250</v>
+        <v>259</v>
       </c>
       <c r="C116" s="2" t="s">
-        <v>317</v>
-      </c>
-      <c r="E116" t="s">
-        <v>105</v>
-      </c>
-      <c r="F116">
-        <v>1950</v>
-      </c>
-      <c r="G116">
-        <v>1996</v>
-      </c>
-      <c r="H116" t="s">
-        <v>16</v>
+        <v>121</v>
       </c>
       <c r="I116" t="s">
         <v>20</v>
@@ -3893,19 +3935,22 @@
     </row>
     <row r="117" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
       <c r="B117" t="s">
-        <v>25</v>
+        <v>250</v>
       </c>
       <c r="C117" s="2" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="E117" t="s">
-        <v>77</v>
+        <v>320</v>
       </c>
       <c r="F117">
-        <v>2010</v>
+        <v>1975</v>
+      </c>
+      <c r="G117">
+        <v>1989</v>
       </c>
       <c r="H117" t="s">
         <v>16</v>
@@ -3916,35 +3961,44 @@
     </row>
     <row r="118" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>141</v>
+        <v>316</v>
       </c>
       <c r="B118" t="s">
-        <v>237</v>
+        <v>250</v>
       </c>
       <c r="C118" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="Q118" t="s">
-        <v>17</v>
+        <v>317</v>
+      </c>
+      <c r="E118" t="s">
+        <v>105</v>
+      </c>
+      <c r="F118">
+        <v>1950</v>
+      </c>
+      <c r="G118">
+        <v>1996</v>
+      </c>
+      <c r="H118" t="s">
+        <v>16</v>
+      </c>
+      <c r="I118" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="119" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>308</v>
+        <v>322</v>
       </c>
       <c r="B119" t="s">
-        <v>250</v>
+        <v>25</v>
       </c>
       <c r="C119" s="2" t="s">
-        <v>309</v>
+        <v>321</v>
       </c>
       <c r="E119" t="s">
-        <v>310</v>
+        <v>77</v>
       </c>
       <c r="F119">
-        <v>1950</v>
-      </c>
-      <c r="G119">
         <v>2010</v>
       </c>
       <c r="H119" t="s">
@@ -3956,30 +4010,36 @@
     </row>
     <row r="120" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>287</v>
+        <v>141</v>
       </c>
       <c r="B120" t="s">
-        <v>134</v>
+        <v>237</v>
       </c>
       <c r="C120" s="2" t="s">
-        <v>288</v>
-      </c>
-      <c r="F120">
-        <v>1990</v>
-      </c>
-      <c r="G120">
-        <v>2008</v>
+        <v>142</v>
+      </c>
+      <c r="Q120" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="121" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>274</v>
+        <v>308</v>
       </c>
       <c r="B121" t="s">
-        <v>55</v>
+        <v>250</v>
       </c>
       <c r="C121" s="2" t="s">
-        <v>275</v>
+        <v>309</v>
+      </c>
+      <c r="E121" t="s">
+        <v>310</v>
+      </c>
+      <c r="F121">
+        <v>1950</v>
+      </c>
+      <c r="G121">
+        <v>2010</v>
       </c>
       <c r="H121" t="s">
         <v>16</v>
@@ -3990,113 +4050,101 @@
     </row>
     <row r="122" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>157</v>
+        <v>287</v>
       </c>
       <c r="B122" t="s">
-        <v>128</v>
+        <v>134</v>
       </c>
       <c r="C122" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="Q122" t="s">
-        <v>18</v>
+        <v>288</v>
+      </c>
+      <c r="F122">
+        <v>1990</v>
+      </c>
+      <c r="G122">
+        <v>2008</v>
       </c>
     </row>
     <row r="123" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>194</v>
+        <v>274</v>
       </c>
       <c r="B123" t="s">
-        <v>99</v>
+        <v>55</v>
       </c>
       <c r="C123" s="2" t="s">
-        <v>193</v>
+        <v>275</v>
+      </c>
+      <c r="H123" t="s">
+        <v>16</v>
+      </c>
+      <c r="I123" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="124" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>295</v>
+        <v>157</v>
       </c>
       <c r="B124" t="s">
-        <v>40</v>
+        <v>128</v>
       </c>
       <c r="C124" s="2" t="s">
-        <v>296</v>
-      </c>
-      <c r="E124" t="s">
-        <v>297</v>
-      </c>
-      <c r="F124">
-        <v>1990</v>
-      </c>
-      <c r="G124">
-        <v>2015</v>
-      </c>
-      <c r="H124" t="s">
-        <v>16</v>
-      </c>
-      <c r="I124" t="s">
-        <v>249</v>
+        <v>154</v>
+      </c>
+      <c r="Q124" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="125" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>256</v>
+        <v>194</v>
       </c>
       <c r="B125" t="s">
-        <v>250</v>
+        <v>99</v>
       </c>
       <c r="C125" s="2" t="s">
-        <v>257</v>
-      </c>
-      <c r="E125" t="s">
-        <v>258</v>
-      </c>
-      <c r="H125" t="s">
-        <v>16</v>
-      </c>
-      <c r="I125" t="s">
-        <v>20</v>
+        <v>193</v>
       </c>
     </row>
     <row r="126" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>227</v>
+        <v>295</v>
       </c>
       <c r="B126" t="s">
         <v>40</v>
       </c>
       <c r="C126" s="2" t="s">
-        <v>225</v>
+        <v>296</v>
+      </c>
+      <c r="E126" t="s">
+        <v>297</v>
       </c>
       <c r="F126">
-        <v>1955</v>
+        <v>1990</v>
       </c>
       <c r="G126">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="H126" t="s">
         <v>16</v>
       </c>
       <c r="I126" t="s">
-        <v>20</v>
+        <v>249</v>
       </c>
     </row>
     <row r="127" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>230</v>
+        <v>256</v>
       </c>
       <c r="B127" t="s">
-        <v>40</v>
+        <v>250</v>
       </c>
       <c r="C127" s="2" t="s">
-        <v>225</v>
-      </c>
-      <c r="F127">
-        <v>1995</v>
-      </c>
-      <c r="G127">
-        <v>2016</v>
+        <v>257</v>
+      </c>
+      <c r="E127" t="s">
+        <v>258</v>
       </c>
       <c r="H127" t="s">
         <v>16</v>
@@ -4107,36 +4155,42 @@
     </row>
     <row r="128" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>109</v>
+        <v>227</v>
       </c>
       <c r="B128" t="s">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="C128" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="E128" t="s">
-        <v>111</v>
+        <v>225</v>
       </c>
       <c r="F128">
-        <v>1956</v>
+        <v>1955</v>
+      </c>
+      <c r="G128">
+        <v>2016</v>
+      </c>
+      <c r="H128" t="s">
+        <v>16</v>
+      </c>
+      <c r="I128" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="129" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>326</v>
+        <v>230</v>
       </c>
       <c r="B129" t="s">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="C129" s="2" t="s">
-        <v>327</v>
-      </c>
-      <c r="E129" t="s">
-        <v>111</v>
+        <v>225</v>
       </c>
       <c r="F129">
-        <v>1998</v>
+        <v>1995</v>
+      </c>
+      <c r="G129">
+        <v>2016</v>
       </c>
       <c r="H129" t="s">
         <v>16</v>
@@ -4147,39 +4201,36 @@
     </row>
     <row r="130" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
-        <v>91</v>
+        <v>109</v>
       </c>
       <c r="B130" t="s">
         <v>25</v>
       </c>
       <c r="C130" s="2" t="s">
-        <v>93</v>
+        <v>110</v>
       </c>
       <c r="E130" t="s">
-        <v>92</v>
+        <v>111</v>
       </c>
       <c r="F130">
-        <v>1999</v>
+        <v>1956</v>
       </c>
     </row>
     <row r="131" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>314</v>
+        <v>326</v>
       </c>
       <c r="B131" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="C131" s="2" t="s">
-        <v>313</v>
+        <v>327</v>
       </c>
       <c r="E131" t="s">
-        <v>315</v>
+        <v>111</v>
       </c>
       <c r="F131">
-        <v>1950</v>
-      </c>
-      <c r="G131">
-        <v>2004</v>
+        <v>1998</v>
       </c>
       <c r="H131" t="s">
         <v>16</v>
@@ -4190,122 +4241,110 @@
     </row>
     <row r="132" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>161</v>
+        <v>91</v>
       </c>
       <c r="B132" t="s">
         <v>25</v>
       </c>
       <c r="C132" s="2" t="s">
-        <v>160</v>
+        <v>93</v>
+      </c>
+      <c r="E132" t="s">
+        <v>92</v>
+      </c>
+      <c r="F132">
+        <v>1999</v>
       </c>
     </row>
     <row r="133" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
-        <v>168</v>
+        <v>314</v>
       </c>
       <c r="B133" t="s">
         <v>40</v>
       </c>
       <c r="C133" s="2" t="s">
-        <v>167</v>
+        <v>313</v>
+      </c>
+      <c r="E133" t="s">
+        <v>315</v>
+      </c>
+      <c r="F133">
+        <v>1950</v>
+      </c>
+      <c r="G133">
+        <v>2004</v>
+      </c>
+      <c r="H133" t="s">
+        <v>16</v>
+      </c>
+      <c r="I133" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="134" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
-        <v>399</v>
+        <v>161</v>
       </c>
       <c r="B134" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="C134" s="2" t="s">
-        <v>400</v>
-      </c>
-      <c r="E134" t="s">
-        <v>14</v>
-      </c>
-      <c r="F134">
-        <v>2000</v>
-      </c>
-      <c r="G134">
-        <v>2014</v>
-      </c>
-      <c r="H134" t="s">
-        <v>348</v>
-      </c>
-      <c r="I134" t="s">
-        <v>349</v>
-      </c>
-      <c r="J134" s="2" t="s">
-        <v>402</v>
-      </c>
-      <c r="N134" s="2" t="s">
-        <v>401</v>
+        <v>160</v>
       </c>
     </row>
     <row r="135" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
-        <v>213</v>
+        <v>168</v>
       </c>
       <c r="B135" t="s">
-        <v>55</v>
+        <v>40</v>
       </c>
       <c r="C135" s="2" t="s">
-        <v>212</v>
-      </c>
-      <c r="H135" t="s">
-        <v>16</v>
-      </c>
-      <c r="I135" t="s">
-        <v>20</v>
+        <v>167</v>
       </c>
     </row>
     <row r="136" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
-        <v>395</v>
+        <v>399</v>
       </c>
       <c r="B136" t="s">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="C136" s="2" t="s">
-        <v>394</v>
-      </c>
-      <c r="D136" t="s">
-        <v>396</v>
+        <v>400</v>
       </c>
       <c r="E136" t="s">
-        <v>111</v>
+        <v>14</v>
       </c>
       <c r="F136">
-        <v>1986</v>
+        <v>2000</v>
       </c>
       <c r="G136">
-        <v>2015</v>
+        <v>2014</v>
       </c>
       <c r="H136" t="s">
-        <v>367</v>
+        <v>348</v>
       </c>
       <c r="I136" t="s">
-        <v>398</v>
+        <v>349</v>
       </c>
       <c r="J136" s="2" t="s">
-        <v>397</v>
+        <v>402</v>
+      </c>
+      <c r="N136" s="2" t="s">
+        <v>401</v>
       </c>
     </row>
     <row r="137" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
-        <v>323</v>
+        <v>213</v>
       </c>
       <c r="B137" t="s">
-        <v>25</v>
+        <v>55</v>
       </c>
       <c r="C137" s="2" t="s">
-        <v>324</v>
-      </c>
-      <c r="E137" t="s">
-        <v>325</v>
-      </c>
-      <c r="F137">
-        <v>1942</v>
+        <v>212</v>
       </c>
       <c r="H137" t="s">
         <v>16</v>
@@ -4316,124 +4355,145 @@
     </row>
     <row r="138" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
-        <v>273</v>
+        <v>395</v>
       </c>
       <c r="B138" t="s">
-        <v>237</v>
+        <v>25</v>
       </c>
       <c r="C138" s="2" t="s">
-        <v>272</v>
+        <v>394</v>
+      </c>
+      <c r="D138" t="s">
+        <v>396</v>
+      </c>
+      <c r="E138" t="s">
+        <v>111</v>
       </c>
       <c r="F138">
-        <v>1996</v>
+        <v>1986</v>
       </c>
       <c r="G138">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="H138" t="s">
-        <v>16</v>
+        <v>367</v>
       </c>
       <c r="I138" t="s">
-        <v>20</v>
+        <v>398</v>
+      </c>
+      <c r="J138" s="2" t="s">
+        <v>397</v>
       </c>
     </row>
     <row r="139" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
-        <v>66</v>
+        <v>323</v>
       </c>
       <c r="B139" t="s">
         <v>25</v>
       </c>
       <c r="C139" s="2" t="s">
-        <v>67</v>
+        <v>324</v>
+      </c>
+      <c r="E139" t="s">
+        <v>325</v>
+      </c>
+      <c r="F139">
+        <v>1942</v>
+      </c>
+      <c r="H139" t="s">
+        <v>16</v>
+      </c>
+      <c r="I139" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="140" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
-        <v>383</v>
+        <v>273</v>
       </c>
       <c r="B140" t="s">
-        <v>40</v>
+        <v>237</v>
       </c>
       <c r="C140" s="2" t="s">
-        <v>384</v>
-      </c>
-      <c r="E140" t="s">
-        <v>386</v>
+        <v>272</v>
       </c>
       <c r="F140">
-        <v>1951</v>
+        <v>1996</v>
+      </c>
+      <c r="G140">
+        <v>2016</v>
       </c>
       <c r="H140" t="s">
-        <v>348</v>
+        <v>16</v>
       </c>
       <c r="I140" t="s">
-        <v>349</v>
-      </c>
-      <c r="N140" s="2" t="s">
-        <v>385</v>
+        <v>20</v>
       </c>
     </row>
     <row r="141" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
-        <v>139</v>
+        <v>66</v>
       </c>
       <c r="B141" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="C141" s="2" t="s">
-        <v>140</v>
+        <v>67</v>
       </c>
     </row>
     <row r="142" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
-        <v>329</v>
+        <v>383</v>
       </c>
       <c r="B142" t="s">
-        <v>165</v>
+        <v>40</v>
       </c>
       <c r="C142" s="2" t="s">
-        <v>328</v>
+        <v>384</v>
       </c>
       <c r="E142" t="s">
-        <v>34</v>
+        <v>386</v>
       </c>
       <c r="F142">
-        <v>1789</v>
+        <v>1951</v>
       </c>
       <c r="H142" t="s">
-        <v>16</v>
+        <v>348</v>
       </c>
       <c r="I142" t="s">
-        <v>20</v>
+        <v>349</v>
+      </c>
+      <c r="N142" s="2" t="s">
+        <v>385</v>
       </c>
     </row>
     <row r="143" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
-        <v>172</v>
+        <v>139</v>
       </c>
       <c r="B143" t="s">
-        <v>60</v>
+        <v>40</v>
       </c>
       <c r="C143" s="2" t="s">
-        <v>171</v>
+        <v>140</v>
       </c>
     </row>
     <row r="144" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
-        <v>217</v>
+        <v>329</v>
       </c>
       <c r="B144" t="s">
-        <v>60</v>
+        <v>165</v>
       </c>
       <c r="C144" s="2" t="s">
-        <v>216</v>
+        <v>328</v>
       </c>
       <c r="E144" t="s">
-        <v>14</v>
+        <v>34</v>
       </c>
       <c r="F144">
-        <v>1900</v>
+        <v>1789</v>
       </c>
       <c r="H144" t="s">
         <v>16</v>
@@ -4444,104 +4504,92 @@
     </row>
     <row r="145" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
-        <v>132</v>
+        <v>172</v>
       </c>
       <c r="B145" t="s">
-        <v>259</v>
+        <v>60</v>
       </c>
       <c r="C145" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="Q145" t="s">
-        <v>17</v>
+        <v>171</v>
       </c>
     </row>
     <row r="146" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
-        <v>182</v>
+        <v>217</v>
       </c>
       <c r="B146" t="s">
-        <v>165</v>
+        <v>60</v>
       </c>
       <c r="C146" s="2" t="s">
-        <v>181</v>
+        <v>216</v>
+      </c>
+      <c r="E146" t="s">
+        <v>14</v>
+      </c>
+      <c r="F146">
+        <v>1900</v>
+      </c>
+      <c r="H146" t="s">
+        <v>16</v>
+      </c>
+      <c r="I146" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="147" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
-        <v>115</v>
+        <v>132</v>
       </c>
       <c r="B147" t="s">
-        <v>128</v>
+        <v>259</v>
       </c>
       <c r="C147" s="2" t="s">
-        <v>116</v>
+        <v>133</v>
+      </c>
+      <c r="Q147" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="148" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
-        <v>263</v>
+        <v>182</v>
       </c>
       <c r="B148" t="s">
-        <v>250</v>
+        <v>165</v>
       </c>
       <c r="C148" s="2" t="s">
-        <v>264</v>
-      </c>
-      <c r="E148" t="s">
-        <v>265</v>
-      </c>
-      <c r="F148">
-        <v>1500</v>
-      </c>
-      <c r="G148">
-        <v>2000</v>
-      </c>
-      <c r="H148" t="s">
-        <v>16</v>
-      </c>
-      <c r="I148" t="s">
-        <v>20</v>
+        <v>181</v>
       </c>
     </row>
     <row r="149" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
-        <v>221</v>
+        <v>115</v>
       </c>
       <c r="B149" t="s">
-        <v>86</v>
+        <v>128</v>
       </c>
       <c r="C149" s="2" t="s">
-        <v>220</v>
-      </c>
-      <c r="F149">
-        <v>2013</v>
-      </c>
-      <c r="H149" t="s">
-        <v>16</v>
-      </c>
-      <c r="I149" t="s">
-        <v>20</v>
+        <v>116</v>
       </c>
     </row>
     <row r="150" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
-        <v>13</v>
+        <v>263</v>
       </c>
       <c r="B150" t="s">
-        <v>25</v>
+        <v>250</v>
       </c>
       <c r="C150" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="D150" s="1" t="s">
-        <v>42</v>
+        <v>264</v>
       </c>
       <c r="E150" t="s">
-        <v>14</v>
+        <v>265</v>
       </c>
       <c r="F150">
-        <v>1981</v>
+        <v>1500</v>
+      </c>
+      <c r="G150">
+        <v>2000</v>
       </c>
       <c r="H150" t="s">
         <v>16</v>
@@ -4552,23 +4600,69 @@
     </row>
     <row r="151" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
+        <v>221</v>
+      </c>
+      <c r="B151" t="s">
+        <v>86</v>
+      </c>
+      <c r="C151" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="F151">
+        <v>2013</v>
+      </c>
+      <c r="H151" t="s">
+        <v>16</v>
+      </c>
+      <c r="I151" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="152" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A152" t="s">
+        <v>13</v>
+      </c>
+      <c r="B152" t="s">
+        <v>25</v>
+      </c>
+      <c r="C152" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D152" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E152" t="s">
+        <v>14</v>
+      </c>
+      <c r="F152">
+        <v>1981</v>
+      </c>
+      <c r="H152" t="s">
+        <v>16</v>
+      </c>
+      <c r="I152" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="153" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A153" t="s">
         <v>283</v>
       </c>
-      <c r="B151" t="s">
+      <c r="B153" t="s">
         <v>124</v>
       </c>
-      <c r="C151" s="2" t="s">
+      <c r="C153" s="2" t="s">
         <v>284</v>
       </c>
-      <c r="H151" t="s">
-        <v>16</v>
-      </c>
-      <c r="I151" t="s">
+      <c r="H153" t="s">
+        <v>16</v>
+      </c>
+      <c r="I153" t="s">
         <v>20</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:Q151">
+  <sortState ref="A2:Q153">
     <sortCondition ref="A2"/>
   </sortState>
   <hyperlinks>
@@ -4576,9 +4670,9 @@
     <hyperlink ref="C58" r:id="rId2"/>
     <hyperlink ref="C7" r:id="rId3"/>
     <hyperlink ref="C10" r:id="rId4"/>
-    <hyperlink ref="C91" r:id="rId5"/>
-    <hyperlink ref="C110" r:id="rId6"/>
-    <hyperlink ref="C150" r:id="rId7"/>
+    <hyperlink ref="C92" r:id="rId5"/>
+    <hyperlink ref="C112" r:id="rId6"/>
+    <hyperlink ref="C152" r:id="rId7"/>
     <hyperlink ref="C35" r:id="rId8"/>
     <hyperlink ref="C30" r:id="rId9"/>
     <hyperlink ref="C49" r:id="rId10"/>
@@ -4586,13 +4680,13 @@
     <hyperlink ref="C3" r:id="rId12"/>
     <hyperlink ref="C20" r:id="rId13"/>
     <hyperlink ref="C60" r:id="rId14"/>
-    <hyperlink ref="C84" r:id="rId15"/>
+    <hyperlink ref="C85" r:id="rId15"/>
     <hyperlink ref="C29" r:id="rId16"/>
-    <hyperlink ref="C106" r:id="rId17"/>
+    <hyperlink ref="C108" r:id="rId17"/>
     <hyperlink ref="C41" r:id="rId18"/>
     <hyperlink ref="C70" r:id="rId19"/>
     <hyperlink ref="C16" r:id="rId20"/>
-    <hyperlink ref="C139" r:id="rId21"/>
+    <hyperlink ref="C141" r:id="rId21"/>
     <hyperlink ref="C8" r:id="rId22"/>
     <hyperlink ref="C38" r:id="rId23"/>
     <hyperlink ref="C53" r:id="rId24"/>
@@ -4600,118 +4694,118 @@
     <hyperlink ref="C54" r:id="rId26"/>
     <hyperlink ref="C55" r:id="rId27"/>
     <hyperlink ref="C68" r:id="rId28"/>
-    <hyperlink ref="C89" r:id="rId29"/>
-    <hyperlink ref="C130" r:id="rId30"/>
-    <hyperlink ref="C94" r:id="rId31"/>
-    <hyperlink ref="C79" r:id="rId32"/>
-    <hyperlink ref="C99" r:id="rId33"/>
+    <hyperlink ref="C90" r:id="rId29"/>
+    <hyperlink ref="C132" r:id="rId30"/>
+    <hyperlink ref="C95" r:id="rId31"/>
+    <hyperlink ref="C80" r:id="rId32"/>
+    <hyperlink ref="C101" r:id="rId33"/>
     <hyperlink ref="C69" r:id="rId34"/>
     <hyperlink ref="C17" r:id="rId35"/>
-    <hyperlink ref="C128" r:id="rId36"/>
+    <hyperlink ref="C130" r:id="rId36"/>
     <hyperlink ref="C15" r:id="rId37"/>
-    <hyperlink ref="C147" r:id="rId38"/>
-    <hyperlink ref="C83" r:id="rId39"/>
+    <hyperlink ref="C149" r:id="rId38"/>
+    <hyperlink ref="C84" r:id="rId39"/>
     <hyperlink ref="C57" r:id="rId40"/>
-    <hyperlink ref="C114" r:id="rId41"/>
+    <hyperlink ref="C116" r:id="rId41"/>
     <hyperlink ref="C18" r:id="rId42"/>
     <hyperlink ref="C51" r:id="rId43"/>
     <hyperlink ref="C23" r:id="rId44"/>
-    <hyperlink ref="C107" r:id="rId45"/>
-    <hyperlink ref="C145" r:id="rId46"/>
+    <hyperlink ref="C109" r:id="rId45"/>
+    <hyperlink ref="C147" r:id="rId46"/>
     <hyperlink ref="C27" r:id="rId47" display="http://comparativeconstitutionsproject.org/"/>
-    <hyperlink ref="C104" r:id="rId48"/>
-    <hyperlink ref="C141" r:id="rId49"/>
-    <hyperlink ref="C118" r:id="rId50"/>
-    <hyperlink ref="C113" r:id="rId51"/>
+    <hyperlink ref="C106" r:id="rId48"/>
+    <hyperlink ref="C143" r:id="rId49"/>
+    <hyperlink ref="C120" r:id="rId50"/>
+    <hyperlink ref="C115" r:id="rId51"/>
     <hyperlink ref="C22" r:id="rId52"/>
-    <hyperlink ref="C108" r:id="rId53"/>
+    <hyperlink ref="C110" r:id="rId53"/>
     <hyperlink ref="C48" r:id="rId54"/>
-    <hyperlink ref="C73" r:id="rId55"/>
-    <hyperlink ref="C76" r:id="rId56"/>
-    <hyperlink ref="C105" r:id="rId57"/>
-    <hyperlink ref="C96" r:id="rId58"/>
-    <hyperlink ref="C122" r:id="rId59"/>
+    <hyperlink ref="C74" r:id="rId55"/>
+    <hyperlink ref="C77" r:id="rId56"/>
+    <hyperlink ref="C107" r:id="rId57"/>
+    <hyperlink ref="C97" r:id="rId58"/>
+    <hyperlink ref="C124" r:id="rId59"/>
     <hyperlink ref="C31" r:id="rId60"/>
-    <hyperlink ref="C132" r:id="rId61"/>
+    <hyperlink ref="C134" r:id="rId61"/>
     <hyperlink ref="C9" r:id="rId62"/>
     <hyperlink ref="C33" r:id="rId63"/>
-    <hyperlink ref="C133" r:id="rId64"/>
+    <hyperlink ref="C135" r:id="rId64"/>
     <hyperlink ref="C14" r:id="rId65"/>
-    <hyperlink ref="C143" r:id="rId66"/>
+    <hyperlink ref="C145" r:id="rId66"/>
     <hyperlink ref="C25" r:id="rId67"/>
     <hyperlink ref="C24" r:id="rId68"/>
     <hyperlink ref="C26" r:id="rId69"/>
     <hyperlink ref="C52" r:id="rId70"/>
-    <hyperlink ref="C146" r:id="rId71"/>
+    <hyperlink ref="C148" r:id="rId71"/>
     <hyperlink ref="C28" r:id="rId72"/>
-    <hyperlink ref="C111" r:id="rId73"/>
+    <hyperlink ref="C113" r:id="rId73"/>
     <hyperlink ref="C32" r:id="rId74"/>
     <hyperlink ref="C45" r:id="rId75"/>
-    <hyperlink ref="C123" r:id="rId76"/>
+    <hyperlink ref="C125" r:id="rId76"/>
     <hyperlink ref="C42" r:id="rId77"/>
     <hyperlink ref="C39" r:id="rId78"/>
     <hyperlink ref="C67" r:id="rId79"/>
     <hyperlink ref="C5" r:id="rId80"/>
     <hyperlink ref="C66" r:id="rId81"/>
     <hyperlink ref="C12" r:id="rId82"/>
-    <hyperlink ref="C103" r:id="rId83"/>
-    <hyperlink ref="C112" r:id="rId84"/>
-    <hyperlink ref="C135" r:id="rId85"/>
+    <hyperlink ref="C105" r:id="rId83"/>
+    <hyperlink ref="C114" r:id="rId84"/>
+    <hyperlink ref="C137" r:id="rId85"/>
     <hyperlink ref="C36" r:id="rId86"/>
-    <hyperlink ref="C144" r:id="rId87"/>
+    <hyperlink ref="C146" r:id="rId87"/>
     <hyperlink ref="C44" r:id="rId88"/>
-    <hyperlink ref="C149" r:id="rId89"/>
-    <hyperlink ref="C92" r:id="rId90"/>
+    <hyperlink ref="C151" r:id="rId89"/>
+    <hyperlink ref="C93" r:id="rId90"/>
     <hyperlink ref="C64" r:id="rId91"/>
-    <hyperlink ref="C93" r:id="rId92"/>
-    <hyperlink ref="C126" r:id="rId93"/>
-    <hyperlink ref="C77" r:id="rId94"/>
-    <hyperlink ref="C97" r:id="rId95"/>
-    <hyperlink ref="C127" r:id="rId96"/>
+    <hyperlink ref="C94" r:id="rId92"/>
+    <hyperlink ref="C128" r:id="rId93"/>
+    <hyperlink ref="C78" r:id="rId94"/>
+    <hyperlink ref="C99" r:id="rId95"/>
+    <hyperlink ref="C129" r:id="rId96"/>
     <hyperlink ref="C61" r:id="rId97"/>
-    <hyperlink ref="C109" r:id="rId98"/>
+    <hyperlink ref="C111" r:id="rId98"/>
     <hyperlink ref="C46" r:id="rId99"/>
     <hyperlink ref="C43" r:id="rId100"/>
-    <hyperlink ref="C80" r:id="rId101"/>
+    <hyperlink ref="C81" r:id="rId101"/>
     <hyperlink ref="C59" r:id="rId102"/>
     <hyperlink ref="C2" r:id="rId103"/>
-    <hyperlink ref="C74" r:id="rId104"/>
-    <hyperlink ref="C78" r:id="rId105"/>
-    <hyperlink ref="C101" r:id="rId106"/>
+    <hyperlink ref="C75" r:id="rId104"/>
+    <hyperlink ref="C79" r:id="rId105"/>
+    <hyperlink ref="C103" r:id="rId106"/>
     <hyperlink ref="C47" r:id="rId107"/>
-    <hyperlink ref="C81" r:id="rId108"/>
-    <hyperlink ref="C125" r:id="rId109"/>
+    <hyperlink ref="C82" r:id="rId108"/>
+    <hyperlink ref="C127" r:id="rId109"/>
     <hyperlink ref="C13" r:id="rId110"/>
     <hyperlink ref="C4" r:id="rId111"/>
-    <hyperlink ref="C148" r:id="rId112"/>
-    <hyperlink ref="C87" r:id="rId113"/>
-    <hyperlink ref="C82" r:id="rId114"/>
-    <hyperlink ref="C138" r:id="rId115"/>
-    <hyperlink ref="C121" r:id="rId116"/>
+    <hyperlink ref="C150" r:id="rId112"/>
+    <hyperlink ref="C88" r:id="rId113"/>
+    <hyperlink ref="C83" r:id="rId114"/>
+    <hyperlink ref="C140" r:id="rId115"/>
+    <hyperlink ref="C123" r:id="rId116"/>
     <hyperlink ref="C63" r:id="rId117"/>
-    <hyperlink ref="C95" r:id="rId118"/>
+    <hyperlink ref="C96" r:id="rId118"/>
     <hyperlink ref="C72" r:id="rId119"/>
-    <hyperlink ref="C151" r:id="rId120"/>
+    <hyperlink ref="C153" r:id="rId120"/>
     <hyperlink ref="C65" r:id="rId121"/>
-    <hyperlink ref="C120" r:id="rId122"/>
-    <hyperlink ref="C100" r:id="rId123"/>
-    <hyperlink ref="C75" r:id="rId124"/>
-    <hyperlink ref="C98" r:id="rId125"/>
-    <hyperlink ref="C124" r:id="rId126"/>
-    <hyperlink ref="C85" r:id="rId127"/>
+    <hyperlink ref="C122" r:id="rId122"/>
+    <hyperlink ref="C102" r:id="rId123"/>
+    <hyperlink ref="C76" r:id="rId124"/>
+    <hyperlink ref="C100" r:id="rId125"/>
+    <hyperlink ref="C126" r:id="rId126"/>
+    <hyperlink ref="C86" r:id="rId127"/>
     <hyperlink ref="C11" r:id="rId128"/>
     <hyperlink ref="C19" r:id="rId129"/>
-    <hyperlink ref="C119" r:id="rId130"/>
+    <hyperlink ref="C121" r:id="rId130"/>
     <hyperlink ref="C71" r:id="rId131"/>
-    <hyperlink ref="C131" r:id="rId132"/>
-    <hyperlink ref="C116" r:id="rId133"/>
-    <hyperlink ref="C115" r:id="rId134"/>
-    <hyperlink ref="C117" r:id="rId135"/>
-    <hyperlink ref="C137" r:id="rId136"/>
-    <hyperlink ref="C129" r:id="rId137"/>
-    <hyperlink ref="C142" r:id="rId138"/>
+    <hyperlink ref="C133" r:id="rId132"/>
+    <hyperlink ref="C118" r:id="rId133"/>
+    <hyperlink ref="C117" r:id="rId134"/>
+    <hyperlink ref="C119" r:id="rId135"/>
+    <hyperlink ref="C139" r:id="rId136"/>
+    <hyperlink ref="C131" r:id="rId137"/>
+    <hyperlink ref="C144" r:id="rId138"/>
     <hyperlink ref="C37" r:id="rId139"/>
-    <hyperlink ref="C86" r:id="rId140"/>
+    <hyperlink ref="C87" r:id="rId140"/>
     <hyperlink ref="J2" r:id="rId141"/>
     <hyperlink ref="M3" r:id="rId142"/>
     <hyperlink ref="J3" r:id="rId143"/>
@@ -4719,28 +4813,32 @@
     <hyperlink ref="J4" r:id="rId145"/>
     <hyperlink ref="P5" r:id="rId146"/>
     <hyperlink ref="J5" r:id="rId147"/>
-    <hyperlink ref="C102" r:id="rId148"/>
+    <hyperlink ref="C104" r:id="rId148"/>
     <hyperlink ref="C34" r:id="rId149"/>
     <hyperlink ref="P7" r:id="rId150"/>
     <hyperlink ref="J7" r:id="rId151"/>
     <hyperlink ref="M8" r:id="rId152"/>
     <hyperlink ref="L8" r:id="rId153"/>
     <hyperlink ref="J8" r:id="rId154"/>
-    <hyperlink ref="C140" r:id="rId155"/>
-    <hyperlink ref="N140" r:id="rId156"/>
+    <hyperlink ref="C142" r:id="rId155"/>
+    <hyperlink ref="N142" r:id="rId156"/>
     <hyperlink ref="C21" r:id="rId157"/>
     <hyperlink ref="N21" r:id="rId158"/>
     <hyperlink ref="C62" r:id="rId159"/>
-    <hyperlink ref="C136" r:id="rId160"/>
-    <hyperlink ref="J136" r:id="rId161"/>
-    <hyperlink ref="C134" r:id="rId162"/>
-    <hyperlink ref="N134" r:id="rId163"/>
-    <hyperlink ref="J134" r:id="rId164"/>
-    <hyperlink ref="C90" r:id="rId165"/>
-    <hyperlink ref="C88" r:id="rId166"/>
+    <hyperlink ref="C138" r:id="rId160"/>
+    <hyperlink ref="J138" r:id="rId161"/>
+    <hyperlink ref="C136" r:id="rId162"/>
+    <hyperlink ref="N136" r:id="rId163"/>
+    <hyperlink ref="J136" r:id="rId164"/>
+    <hyperlink ref="C91" r:id="rId165"/>
+    <hyperlink ref="C89" r:id="rId166"/>
     <hyperlink ref="C40" r:id="rId167"/>
     <hyperlink ref="J40" r:id="rId168"/>
     <hyperlink ref="K40" r:id="rId169"/>
+    <hyperlink ref="C98" r:id="rId170"/>
+    <hyperlink ref="N98" r:id="rId171"/>
+    <hyperlink ref="C73" r:id="rId172"/>
+    <hyperlink ref="K73" r:id="rId173"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
add data, 'Wesleyan Media Project: Media Advertising' and 'Political TV Ad Archive'
</commit_message>
<xml_diff>
--- a/PolData.xlsx
+++ b/PolData.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="769" uniqueCount="423">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="782" uniqueCount="429">
   <si>
     <t>name</t>
   </si>
@@ -1296,6 +1296,24 @@
   </si>
   <si>
     <t>See also this article for more info https://doi.org/10.1017/psrm.2015.68</t>
+  </si>
+  <si>
+    <t>Wesleyan Media Project: Media Advertising</t>
+  </si>
+  <si>
+    <t>http://mediaproject.wesleyan.edu/dataaccess/</t>
+  </si>
+  <si>
+    <t>not free</t>
+  </si>
+  <si>
+    <t>Political TV Ad Archive</t>
+  </si>
+  <si>
+    <t>http://politicaladarchive.org/data/</t>
+  </si>
+  <si>
+    <t>http://politicaladarchive.org/api/v1/ad_instances?output=csv</t>
   </si>
 </sst>
 </file>
@@ -1635,10 +1653,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q153"/>
+  <dimension ref="A1:Q155"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R73" sqref="R73"/>
+      <selection activeCell="A150" sqref="A150"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3904,56 +3922,59 @@
     </row>
     <row r="115" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>144</v>
+        <v>426</v>
       </c>
       <c r="B115" t="s">
-        <v>60</v>
+        <v>86</v>
       </c>
       <c r="C115" s="2" t="s">
-        <v>143</v>
+        <v>427</v>
+      </c>
+      <c r="E115" t="s">
+        <v>34</v>
       </c>
       <c r="F115">
-        <v>1800</v>
+        <v>2015</v>
       </c>
       <c r="G115">
-        <v>2013</v>
+        <v>2016</v>
+      </c>
+      <c r="H115" t="s">
+        <v>348</v>
+      </c>
+      <c r="I115" t="s">
+        <v>349</v>
+      </c>
+      <c r="K115" s="2" t="s">
+        <v>428</v>
       </c>
     </row>
     <row r="116" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>122</v>
+        <v>144</v>
       </c>
       <c r="B116" t="s">
-        <v>259</v>
+        <v>60</v>
       </c>
       <c r="C116" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="I116" t="s">
-        <v>20</v>
+        <v>143</v>
+      </c>
+      <c r="F116">
+        <v>1800</v>
+      </c>
+      <c r="G116">
+        <v>2013</v>
       </c>
     </row>
     <row r="117" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>318</v>
+        <v>122</v>
       </c>
       <c r="B117" t="s">
-        <v>250</v>
+        <v>259</v>
       </c>
       <c r="C117" s="2" t="s">
-        <v>319</v>
-      </c>
-      <c r="E117" t="s">
-        <v>320</v>
-      </c>
-      <c r="F117">
-        <v>1975</v>
-      </c>
-      <c r="G117">
-        <v>1989</v>
-      </c>
-      <c r="H117" t="s">
-        <v>16</v>
+        <v>121</v>
       </c>
       <c r="I117" t="s">
         <v>20</v>
@@ -3961,22 +3982,22 @@
     </row>
     <row r="118" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="B118" t="s">
         <v>250</v>
       </c>
       <c r="C118" s="2" t="s">
-        <v>317</v>
+        <v>319</v>
       </c>
       <c r="E118" t="s">
-        <v>105</v>
+        <v>320</v>
       </c>
       <c r="F118">
-        <v>1950</v>
+        <v>1975</v>
       </c>
       <c r="G118">
-        <v>1996</v>
+        <v>1989</v>
       </c>
       <c r="H118" t="s">
         <v>16</v>
@@ -3987,19 +4008,22 @@
     </row>
     <row r="119" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>322</v>
+        <v>316</v>
       </c>
       <c r="B119" t="s">
-        <v>25</v>
+        <v>250</v>
       </c>
       <c r="C119" s="2" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="E119" t="s">
-        <v>77</v>
+        <v>105</v>
       </c>
       <c r="F119">
-        <v>2010</v>
+        <v>1950</v>
+      </c>
+      <c r="G119">
+        <v>1996</v>
       </c>
       <c r="H119" t="s">
         <v>16</v>
@@ -4010,164 +4034,164 @@
     </row>
     <row r="120" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>141</v>
+        <v>322</v>
       </c>
       <c r="B120" t="s">
-        <v>237</v>
+        <v>25</v>
       </c>
       <c r="C120" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="Q120" t="s">
-        <v>17</v>
+        <v>321</v>
+      </c>
+      <c r="E120" t="s">
+        <v>77</v>
+      </c>
+      <c r="F120">
+        <v>2010</v>
+      </c>
+      <c r="H120" t="s">
+        <v>16</v>
+      </c>
+      <c r="I120" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="121" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>308</v>
+        <v>141</v>
       </c>
       <c r="B121" t="s">
-        <v>250</v>
+        <v>237</v>
       </c>
       <c r="C121" s="2" t="s">
-        <v>309</v>
-      </c>
-      <c r="E121" t="s">
-        <v>310</v>
-      </c>
-      <c r="F121">
-        <v>1950</v>
-      </c>
-      <c r="G121">
-        <v>2010</v>
-      </c>
-      <c r="H121" t="s">
-        <v>16</v>
-      </c>
-      <c r="I121" t="s">
-        <v>20</v>
+        <v>142</v>
+      </c>
+      <c r="Q121" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="122" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>287</v>
+        <v>308</v>
       </c>
       <c r="B122" t="s">
-        <v>134</v>
+        <v>250</v>
       </c>
       <c r="C122" s="2" t="s">
-        <v>288</v>
+        <v>309</v>
+      </c>
+      <c r="E122" t="s">
+        <v>310</v>
       </c>
       <c r="F122">
-        <v>1990</v>
+        <v>1950</v>
       </c>
       <c r="G122">
-        <v>2008</v>
+        <v>2010</v>
+      </c>
+      <c r="H122" t="s">
+        <v>16</v>
+      </c>
+      <c r="I122" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="123" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>274</v>
+        <v>287</v>
       </c>
       <c r="B123" t="s">
-        <v>55</v>
+        <v>134</v>
       </c>
       <c r="C123" s="2" t="s">
-        <v>275</v>
-      </c>
-      <c r="H123" t="s">
-        <v>16</v>
-      </c>
-      <c r="I123" t="s">
-        <v>20</v>
+        <v>288</v>
+      </c>
+      <c r="F123">
+        <v>1990</v>
+      </c>
+      <c r="G123">
+        <v>2008</v>
       </c>
     </row>
     <row r="124" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>157</v>
+        <v>274</v>
       </c>
       <c r="B124" t="s">
-        <v>128</v>
+        <v>55</v>
       </c>
       <c r="C124" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="Q124" t="s">
-        <v>18</v>
+        <v>275</v>
+      </c>
+      <c r="H124" t="s">
+        <v>16</v>
+      </c>
+      <c r="I124" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="125" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>194</v>
+        <v>157</v>
       </c>
       <c r="B125" t="s">
-        <v>99</v>
+        <v>128</v>
       </c>
       <c r="C125" s="2" t="s">
-        <v>193</v>
+        <v>154</v>
+      </c>
+      <c r="Q125" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="126" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>295</v>
+        <v>194</v>
       </c>
       <c r="B126" t="s">
-        <v>40</v>
+        <v>99</v>
       </c>
       <c r="C126" s="2" t="s">
-        <v>296</v>
-      </c>
-      <c r="E126" t="s">
-        <v>297</v>
-      </c>
-      <c r="F126">
-        <v>1990</v>
-      </c>
-      <c r="G126">
-        <v>2015</v>
-      </c>
-      <c r="H126" t="s">
-        <v>16</v>
-      </c>
-      <c r="I126" t="s">
-        <v>249</v>
+        <v>193</v>
       </c>
     </row>
     <row r="127" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>256</v>
+        <v>295</v>
       </c>
       <c r="B127" t="s">
-        <v>250</v>
+        <v>40</v>
       </c>
       <c r="C127" s="2" t="s">
-        <v>257</v>
+        <v>296</v>
       </c>
       <c r="E127" t="s">
-        <v>258</v>
+        <v>297</v>
+      </c>
+      <c r="F127">
+        <v>1990</v>
+      </c>
+      <c r="G127">
+        <v>2015</v>
       </c>
       <c r="H127" t="s">
         <v>16</v>
       </c>
       <c r="I127" t="s">
-        <v>20</v>
+        <v>249</v>
       </c>
     </row>
     <row r="128" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>227</v>
+        <v>256</v>
       </c>
       <c r="B128" t="s">
-        <v>40</v>
+        <v>250</v>
       </c>
       <c r="C128" s="2" t="s">
-        <v>225</v>
-      </c>
-      <c r="F128">
-        <v>1955</v>
-      </c>
-      <c r="G128">
-        <v>2016</v>
+        <v>257</v>
+      </c>
+      <c r="E128" t="s">
+        <v>258</v>
       </c>
       <c r="H128" t="s">
         <v>16</v>
@@ -4178,7 +4202,7 @@
     </row>
     <row r="129" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="B129" t="s">
         <v>40</v>
@@ -4187,7 +4211,7 @@
         <v>225</v>
       </c>
       <c r="F129">
-        <v>1995</v>
+        <v>1955</v>
       </c>
       <c r="G129">
         <v>2016</v>
@@ -4201,228 +4225,228 @@
     </row>
     <row r="130" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
-        <v>109</v>
+        <v>230</v>
       </c>
       <c r="B130" t="s">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="C130" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="E130" t="s">
-        <v>111</v>
+        <v>225</v>
       </c>
       <c r="F130">
-        <v>1956</v>
+        <v>1995</v>
+      </c>
+      <c r="G130">
+        <v>2016</v>
+      </c>
+      <c r="H130" t="s">
+        <v>16</v>
+      </c>
+      <c r="I130" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="131" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>326</v>
+        <v>109</v>
       </c>
       <c r="B131" t="s">
         <v>25</v>
       </c>
       <c r="C131" s="2" t="s">
-        <v>327</v>
+        <v>110</v>
       </c>
       <c r="E131" t="s">
         <v>111</v>
       </c>
       <c r="F131">
-        <v>1998</v>
-      </c>
-      <c r="H131" t="s">
-        <v>16</v>
-      </c>
-      <c r="I131" t="s">
-        <v>20</v>
+        <v>1956</v>
       </c>
     </row>
     <row r="132" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>91</v>
+        <v>326</v>
       </c>
       <c r="B132" t="s">
         <v>25</v>
       </c>
       <c r="C132" s="2" t="s">
-        <v>93</v>
+        <v>327</v>
       </c>
       <c r="E132" t="s">
-        <v>92</v>
+        <v>111</v>
       </c>
       <c r="F132">
-        <v>1999</v>
+        <v>1998</v>
+      </c>
+      <c r="H132" t="s">
+        <v>16</v>
+      </c>
+      <c r="I132" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="133" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
-        <v>314</v>
+        <v>91</v>
       </c>
       <c r="B133" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="C133" s="2" t="s">
-        <v>313</v>
+        <v>93</v>
       </c>
       <c r="E133" t="s">
-        <v>315</v>
+        <v>92</v>
       </c>
       <c r="F133">
-        <v>1950</v>
-      </c>
-      <c r="G133">
-        <v>2004</v>
-      </c>
-      <c r="H133" t="s">
-        <v>16</v>
-      </c>
-      <c r="I133" t="s">
-        <v>20</v>
+        <v>1999</v>
       </c>
     </row>
     <row r="134" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
-        <v>161</v>
+        <v>314</v>
       </c>
       <c r="B134" t="s">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="C134" s="2" t="s">
-        <v>160</v>
+        <v>313</v>
+      </c>
+      <c r="E134" t="s">
+        <v>315</v>
+      </c>
+      <c r="F134">
+        <v>1950</v>
+      </c>
+      <c r="G134">
+        <v>2004</v>
+      </c>
+      <c r="H134" t="s">
+        <v>16</v>
+      </c>
+      <c r="I134" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="135" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="B135" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="C135" s="2" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
     </row>
     <row r="136" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
-        <v>399</v>
+        <v>168</v>
       </c>
       <c r="B136" t="s">
         <v>40</v>
       </c>
       <c r="C136" s="2" t="s">
-        <v>400</v>
-      </c>
-      <c r="E136" t="s">
-        <v>14</v>
-      </c>
-      <c r="F136">
-        <v>2000</v>
-      </c>
-      <c r="G136">
-        <v>2014</v>
-      </c>
-      <c r="H136" t="s">
-        <v>348</v>
-      </c>
-      <c r="I136" t="s">
-        <v>349</v>
-      </c>
-      <c r="J136" s="2" t="s">
-        <v>402</v>
-      </c>
-      <c r="N136" s="2" t="s">
-        <v>401</v>
+        <v>167</v>
       </c>
     </row>
     <row r="137" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
-        <v>213</v>
+        <v>399</v>
       </c>
       <c r="B137" t="s">
-        <v>55</v>
+        <v>40</v>
       </c>
       <c r="C137" s="2" t="s">
-        <v>212</v>
+        <v>400</v>
+      </c>
+      <c r="E137" t="s">
+        <v>14</v>
+      </c>
+      <c r="F137">
+        <v>2000</v>
+      </c>
+      <c r="G137">
+        <v>2014</v>
       </c>
       <c r="H137" t="s">
-        <v>16</v>
+        <v>348</v>
       </c>
       <c r="I137" t="s">
-        <v>20</v>
+        <v>349</v>
+      </c>
+      <c r="J137" s="2" t="s">
+        <v>402</v>
+      </c>
+      <c r="N137" s="2" t="s">
+        <v>401</v>
       </c>
     </row>
     <row r="138" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
-        <v>395</v>
+        <v>213</v>
       </c>
       <c r="B138" t="s">
-        <v>25</v>
+        <v>55</v>
       </c>
       <c r="C138" s="2" t="s">
-        <v>394</v>
-      </c>
-      <c r="D138" t="s">
-        <v>396</v>
-      </c>
-      <c r="E138" t="s">
-        <v>111</v>
-      </c>
-      <c r="F138">
-        <v>1986</v>
-      </c>
-      <c r="G138">
-        <v>2015</v>
+        <v>212</v>
       </c>
       <c r="H138" t="s">
-        <v>367</v>
+        <v>16</v>
       </c>
       <c r="I138" t="s">
-        <v>398</v>
-      </c>
-      <c r="J138" s="2" t="s">
-        <v>397</v>
+        <v>20</v>
       </c>
     </row>
     <row r="139" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
-        <v>323</v>
+        <v>395</v>
       </c>
       <c r="B139" t="s">
         <v>25</v>
       </c>
       <c r="C139" s="2" t="s">
-        <v>324</v>
+        <v>394</v>
+      </c>
+      <c r="D139" t="s">
+        <v>396</v>
       </c>
       <c r="E139" t="s">
-        <v>325</v>
+        <v>111</v>
       </c>
       <c r="F139">
-        <v>1942</v>
+        <v>1986</v>
+      </c>
+      <c r="G139">
+        <v>2015</v>
       </c>
       <c r="H139" t="s">
-        <v>16</v>
+        <v>367</v>
       </c>
       <c r="I139" t="s">
-        <v>20</v>
+        <v>398</v>
+      </c>
+      <c r="J139" s="2" t="s">
+        <v>397</v>
       </c>
     </row>
     <row r="140" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
-        <v>273</v>
+        <v>323</v>
       </c>
       <c r="B140" t="s">
-        <v>237</v>
+        <v>25</v>
       </c>
       <c r="C140" s="2" t="s">
-        <v>272</v>
+        <v>324</v>
+      </c>
+      <c r="E140" t="s">
+        <v>325</v>
       </c>
       <c r="F140">
-        <v>1996</v>
-      </c>
-      <c r="G140">
-        <v>2016</v>
+        <v>1942</v>
       </c>
       <c r="H140" t="s">
         <v>16</v>
@@ -4433,209 +4457,212 @@
     </row>
     <row r="141" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
-        <v>66</v>
+        <v>273</v>
       </c>
       <c r="B141" t="s">
-        <v>25</v>
+        <v>237</v>
       </c>
       <c r="C141" s="2" t="s">
-        <v>67</v>
+        <v>272</v>
+      </c>
+      <c r="F141">
+        <v>1996</v>
+      </c>
+      <c r="G141">
+        <v>2016</v>
+      </c>
+      <c r="H141" t="s">
+        <v>16</v>
+      </c>
+      <c r="I141" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="142" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
-        <v>383</v>
+        <v>66</v>
       </c>
       <c r="B142" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="C142" s="2" t="s">
-        <v>384</v>
-      </c>
-      <c r="E142" t="s">
-        <v>386</v>
-      </c>
-      <c r="F142">
-        <v>1951</v>
-      </c>
-      <c r="H142" t="s">
-        <v>348</v>
-      </c>
-      <c r="I142" t="s">
-        <v>349</v>
-      </c>
-      <c r="N142" s="2" t="s">
-        <v>385</v>
+        <v>67</v>
       </c>
     </row>
     <row r="143" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
-        <v>139</v>
+        <v>383</v>
       </c>
       <c r="B143" t="s">
         <v>40</v>
       </c>
       <c r="C143" s="2" t="s">
-        <v>140</v>
+        <v>384</v>
+      </c>
+      <c r="E143" t="s">
+        <v>386</v>
+      </c>
+      <c r="F143">
+        <v>1951</v>
+      </c>
+      <c r="H143" t="s">
+        <v>348</v>
+      </c>
+      <c r="I143" t="s">
+        <v>349</v>
+      </c>
+      <c r="N143" s="2" t="s">
+        <v>385</v>
       </c>
     </row>
     <row r="144" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
-        <v>329</v>
+        <v>139</v>
       </c>
       <c r="B144" t="s">
-        <v>165</v>
+        <v>40</v>
       </c>
       <c r="C144" s="2" t="s">
-        <v>328</v>
-      </c>
-      <c r="E144" t="s">
-        <v>34</v>
-      </c>
-      <c r="F144">
-        <v>1789</v>
-      </c>
-      <c r="H144" t="s">
-        <v>16</v>
-      </c>
-      <c r="I144" t="s">
-        <v>20</v>
+        <v>140</v>
       </c>
     </row>
     <row r="145" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
-        <v>172</v>
+        <v>329</v>
       </c>
       <c r="B145" t="s">
-        <v>60</v>
+        <v>165</v>
       </c>
       <c r="C145" s="2" t="s">
-        <v>171</v>
+        <v>328</v>
+      </c>
+      <c r="E145" t="s">
+        <v>34</v>
+      </c>
+      <c r="F145">
+        <v>1789</v>
+      </c>
+      <c r="H145" t="s">
+        <v>16</v>
+      </c>
+      <c r="I145" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="146" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
-        <v>217</v>
+        <v>172</v>
       </c>
       <c r="B146" t="s">
         <v>60</v>
       </c>
       <c r="C146" s="2" t="s">
-        <v>216</v>
-      </c>
-      <c r="E146" t="s">
-        <v>14</v>
-      </c>
-      <c r="F146">
-        <v>1900</v>
-      </c>
-      <c r="H146" t="s">
-        <v>16</v>
-      </c>
-      <c r="I146" t="s">
-        <v>20</v>
+        <v>171</v>
       </c>
     </row>
     <row r="147" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
-        <v>132</v>
+        <v>217</v>
       </c>
       <c r="B147" t="s">
-        <v>259</v>
+        <v>60</v>
       </c>
       <c r="C147" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="Q147" t="s">
-        <v>17</v>
+        <v>216</v>
+      </c>
+      <c r="E147" t="s">
+        <v>14</v>
+      </c>
+      <c r="F147">
+        <v>1900</v>
+      </c>
+      <c r="H147" t="s">
+        <v>16</v>
+      </c>
+      <c r="I147" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="148" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
-        <v>182</v>
+        <v>132</v>
       </c>
       <c r="B148" t="s">
-        <v>165</v>
+        <v>259</v>
       </c>
       <c r="C148" s="2" t="s">
-        <v>181</v>
+        <v>133</v>
+      </c>
+      <c r="Q148" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="149" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
-        <v>115</v>
+        <v>182</v>
       </c>
       <c r="B149" t="s">
-        <v>128</v>
+        <v>165</v>
       </c>
       <c r="C149" s="2" t="s">
-        <v>116</v>
+        <v>181</v>
       </c>
     </row>
     <row r="150" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
-        <v>263</v>
+        <v>423</v>
       </c>
       <c r="B150" t="s">
-        <v>250</v>
+        <v>86</v>
       </c>
       <c r="C150" s="2" t="s">
-        <v>264</v>
+        <v>424</v>
       </c>
       <c r="E150" t="s">
-        <v>265</v>
+        <v>34</v>
       </c>
       <c r="F150">
-        <v>1500</v>
+        <v>1996</v>
       </c>
       <c r="G150">
-        <v>2000</v>
+        <v>2016</v>
       </c>
       <c r="H150" t="s">
-        <v>16</v>
+        <v>348</v>
       </c>
       <c r="I150" t="s">
-        <v>20</v>
+        <v>425</v>
       </c>
     </row>
     <row r="151" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
-        <v>221</v>
+        <v>115</v>
       </c>
       <c r="B151" t="s">
-        <v>86</v>
+        <v>128</v>
       </c>
       <c r="C151" s="2" t="s">
-        <v>220</v>
-      </c>
-      <c r="F151">
-        <v>2013</v>
-      </c>
-      <c r="H151" t="s">
-        <v>16</v>
-      </c>
-      <c r="I151" t="s">
-        <v>20</v>
+        <v>116</v>
       </c>
     </row>
     <row r="152" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
-        <v>13</v>
+        <v>263</v>
       </c>
       <c r="B152" t="s">
-        <v>25</v>
+        <v>250</v>
       </c>
       <c r="C152" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="D152" s="1" t="s">
-        <v>42</v>
+        <v>264</v>
       </c>
       <c r="E152" t="s">
-        <v>14</v>
+        <v>265</v>
       </c>
       <c r="F152">
-        <v>1981</v>
+        <v>1500</v>
+      </c>
+      <c r="G152">
+        <v>2000</v>
       </c>
       <c r="H152" t="s">
         <v>16</v>
@@ -4646,23 +4673,69 @@
     </row>
     <row r="153" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
+        <v>221</v>
+      </c>
+      <c r="B153" t="s">
+        <v>86</v>
+      </c>
+      <c r="C153" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="F153">
+        <v>2013</v>
+      </c>
+      <c r="H153" t="s">
+        <v>16</v>
+      </c>
+      <c r="I153" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="154" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A154" t="s">
+        <v>13</v>
+      </c>
+      <c r="B154" t="s">
+        <v>25</v>
+      </c>
+      <c r="C154" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D154" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E154" t="s">
+        <v>14</v>
+      </c>
+      <c r="F154">
+        <v>1981</v>
+      </c>
+      <c r="H154" t="s">
+        <v>16</v>
+      </c>
+      <c r="I154" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="155" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A155" t="s">
         <v>283</v>
       </c>
-      <c r="B153" t="s">
+      <c r="B155" t="s">
         <v>124</v>
       </c>
-      <c r="C153" s="2" t="s">
+      <c r="C155" s="2" t="s">
         <v>284</v>
       </c>
-      <c r="H153" t="s">
-        <v>16</v>
-      </c>
-      <c r="I153" t="s">
+      <c r="H155" t="s">
+        <v>16</v>
+      </c>
+      <c r="I155" t="s">
         <v>20</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:Q153">
+  <sortState ref="A2:Q155">
     <sortCondition ref="A2"/>
   </sortState>
   <hyperlinks>
@@ -4672,7 +4745,7 @@
     <hyperlink ref="C10" r:id="rId4"/>
     <hyperlink ref="C92" r:id="rId5"/>
     <hyperlink ref="C112" r:id="rId6"/>
-    <hyperlink ref="C152" r:id="rId7"/>
+    <hyperlink ref="C154" r:id="rId7"/>
     <hyperlink ref="C35" r:id="rId8"/>
     <hyperlink ref="C30" r:id="rId9"/>
     <hyperlink ref="C49" r:id="rId10"/>
@@ -4686,7 +4759,7 @@
     <hyperlink ref="C41" r:id="rId18"/>
     <hyperlink ref="C70" r:id="rId19"/>
     <hyperlink ref="C16" r:id="rId20"/>
-    <hyperlink ref="C141" r:id="rId21"/>
+    <hyperlink ref="C142" r:id="rId21"/>
     <hyperlink ref="C8" r:id="rId22"/>
     <hyperlink ref="C38" r:id="rId23"/>
     <hyperlink ref="C53" r:id="rId24"/>
@@ -4695,28 +4768,28 @@
     <hyperlink ref="C55" r:id="rId27"/>
     <hyperlink ref="C68" r:id="rId28"/>
     <hyperlink ref="C90" r:id="rId29"/>
-    <hyperlink ref="C132" r:id="rId30"/>
+    <hyperlink ref="C133" r:id="rId30"/>
     <hyperlink ref="C95" r:id="rId31"/>
     <hyperlink ref="C80" r:id="rId32"/>
     <hyperlink ref="C101" r:id="rId33"/>
     <hyperlink ref="C69" r:id="rId34"/>
     <hyperlink ref="C17" r:id="rId35"/>
-    <hyperlink ref="C130" r:id="rId36"/>
+    <hyperlink ref="C131" r:id="rId36"/>
     <hyperlink ref="C15" r:id="rId37"/>
-    <hyperlink ref="C149" r:id="rId38"/>
+    <hyperlink ref="C151" r:id="rId38"/>
     <hyperlink ref="C84" r:id="rId39"/>
     <hyperlink ref="C57" r:id="rId40"/>
-    <hyperlink ref="C116" r:id="rId41"/>
+    <hyperlink ref="C117" r:id="rId41"/>
     <hyperlink ref="C18" r:id="rId42"/>
     <hyperlink ref="C51" r:id="rId43"/>
     <hyperlink ref="C23" r:id="rId44"/>
     <hyperlink ref="C109" r:id="rId45"/>
-    <hyperlink ref="C147" r:id="rId46"/>
+    <hyperlink ref="C148" r:id="rId46"/>
     <hyperlink ref="C27" r:id="rId47" display="http://comparativeconstitutionsproject.org/"/>
     <hyperlink ref="C106" r:id="rId48"/>
-    <hyperlink ref="C143" r:id="rId49"/>
-    <hyperlink ref="C120" r:id="rId50"/>
-    <hyperlink ref="C115" r:id="rId51"/>
+    <hyperlink ref="C144" r:id="rId49"/>
+    <hyperlink ref="C121" r:id="rId50"/>
+    <hyperlink ref="C116" r:id="rId51"/>
     <hyperlink ref="C22" r:id="rId52"/>
     <hyperlink ref="C110" r:id="rId53"/>
     <hyperlink ref="C48" r:id="rId54"/>
@@ -4724,24 +4797,24 @@
     <hyperlink ref="C77" r:id="rId56"/>
     <hyperlink ref="C107" r:id="rId57"/>
     <hyperlink ref="C97" r:id="rId58"/>
-    <hyperlink ref="C124" r:id="rId59"/>
+    <hyperlink ref="C125" r:id="rId59"/>
     <hyperlink ref="C31" r:id="rId60"/>
-    <hyperlink ref="C134" r:id="rId61"/>
+    <hyperlink ref="C135" r:id="rId61"/>
     <hyperlink ref="C9" r:id="rId62"/>
     <hyperlink ref="C33" r:id="rId63"/>
-    <hyperlink ref="C135" r:id="rId64"/>
+    <hyperlink ref="C136" r:id="rId64"/>
     <hyperlink ref="C14" r:id="rId65"/>
-    <hyperlink ref="C145" r:id="rId66"/>
+    <hyperlink ref="C146" r:id="rId66"/>
     <hyperlink ref="C25" r:id="rId67"/>
     <hyperlink ref="C24" r:id="rId68"/>
     <hyperlink ref="C26" r:id="rId69"/>
     <hyperlink ref="C52" r:id="rId70"/>
-    <hyperlink ref="C148" r:id="rId71"/>
+    <hyperlink ref="C149" r:id="rId71"/>
     <hyperlink ref="C28" r:id="rId72"/>
     <hyperlink ref="C113" r:id="rId73"/>
     <hyperlink ref="C32" r:id="rId74"/>
     <hyperlink ref="C45" r:id="rId75"/>
-    <hyperlink ref="C125" r:id="rId76"/>
+    <hyperlink ref="C126" r:id="rId76"/>
     <hyperlink ref="C42" r:id="rId77"/>
     <hyperlink ref="C39" r:id="rId78"/>
     <hyperlink ref="C67" r:id="rId79"/>
@@ -4750,18 +4823,18 @@
     <hyperlink ref="C12" r:id="rId82"/>
     <hyperlink ref="C105" r:id="rId83"/>
     <hyperlink ref="C114" r:id="rId84"/>
-    <hyperlink ref="C137" r:id="rId85"/>
+    <hyperlink ref="C138" r:id="rId85"/>
     <hyperlink ref="C36" r:id="rId86"/>
-    <hyperlink ref="C146" r:id="rId87"/>
+    <hyperlink ref="C147" r:id="rId87"/>
     <hyperlink ref="C44" r:id="rId88"/>
-    <hyperlink ref="C151" r:id="rId89"/>
+    <hyperlink ref="C153" r:id="rId89"/>
     <hyperlink ref="C93" r:id="rId90"/>
     <hyperlink ref="C64" r:id="rId91"/>
     <hyperlink ref="C94" r:id="rId92"/>
-    <hyperlink ref="C128" r:id="rId93"/>
+    <hyperlink ref="C129" r:id="rId93"/>
     <hyperlink ref="C78" r:id="rId94"/>
     <hyperlink ref="C99" r:id="rId95"/>
-    <hyperlink ref="C129" r:id="rId96"/>
+    <hyperlink ref="C130" r:id="rId96"/>
     <hyperlink ref="C61" r:id="rId97"/>
     <hyperlink ref="C111" r:id="rId98"/>
     <hyperlink ref="C46" r:id="rId99"/>
@@ -4774,36 +4847,36 @@
     <hyperlink ref="C103" r:id="rId106"/>
     <hyperlink ref="C47" r:id="rId107"/>
     <hyperlink ref="C82" r:id="rId108"/>
-    <hyperlink ref="C127" r:id="rId109"/>
+    <hyperlink ref="C128" r:id="rId109"/>
     <hyperlink ref="C13" r:id="rId110"/>
     <hyperlink ref="C4" r:id="rId111"/>
-    <hyperlink ref="C150" r:id="rId112"/>
+    <hyperlink ref="C152" r:id="rId112"/>
     <hyperlink ref="C88" r:id="rId113"/>
     <hyperlink ref="C83" r:id="rId114"/>
-    <hyperlink ref="C140" r:id="rId115"/>
-    <hyperlink ref="C123" r:id="rId116"/>
+    <hyperlink ref="C141" r:id="rId115"/>
+    <hyperlink ref="C124" r:id="rId116"/>
     <hyperlink ref="C63" r:id="rId117"/>
     <hyperlink ref="C96" r:id="rId118"/>
     <hyperlink ref="C72" r:id="rId119"/>
-    <hyperlink ref="C153" r:id="rId120"/>
+    <hyperlink ref="C155" r:id="rId120"/>
     <hyperlink ref="C65" r:id="rId121"/>
-    <hyperlink ref="C122" r:id="rId122"/>
+    <hyperlink ref="C123" r:id="rId122"/>
     <hyperlink ref="C102" r:id="rId123"/>
     <hyperlink ref="C76" r:id="rId124"/>
     <hyperlink ref="C100" r:id="rId125"/>
-    <hyperlink ref="C126" r:id="rId126"/>
+    <hyperlink ref="C127" r:id="rId126"/>
     <hyperlink ref="C86" r:id="rId127"/>
     <hyperlink ref="C11" r:id="rId128"/>
     <hyperlink ref="C19" r:id="rId129"/>
-    <hyperlink ref="C121" r:id="rId130"/>
+    <hyperlink ref="C122" r:id="rId130"/>
     <hyperlink ref="C71" r:id="rId131"/>
-    <hyperlink ref="C133" r:id="rId132"/>
-    <hyperlink ref="C118" r:id="rId133"/>
-    <hyperlink ref="C117" r:id="rId134"/>
-    <hyperlink ref="C119" r:id="rId135"/>
-    <hyperlink ref="C139" r:id="rId136"/>
-    <hyperlink ref="C131" r:id="rId137"/>
-    <hyperlink ref="C144" r:id="rId138"/>
+    <hyperlink ref="C134" r:id="rId132"/>
+    <hyperlink ref="C119" r:id="rId133"/>
+    <hyperlink ref="C118" r:id="rId134"/>
+    <hyperlink ref="C120" r:id="rId135"/>
+    <hyperlink ref="C140" r:id="rId136"/>
+    <hyperlink ref="C132" r:id="rId137"/>
+    <hyperlink ref="C145" r:id="rId138"/>
     <hyperlink ref="C37" r:id="rId139"/>
     <hyperlink ref="C87" r:id="rId140"/>
     <hyperlink ref="J2" r:id="rId141"/>
@@ -4820,16 +4893,16 @@
     <hyperlink ref="M8" r:id="rId152"/>
     <hyperlink ref="L8" r:id="rId153"/>
     <hyperlink ref="J8" r:id="rId154"/>
-    <hyperlink ref="C142" r:id="rId155"/>
-    <hyperlink ref="N142" r:id="rId156"/>
+    <hyperlink ref="C143" r:id="rId155"/>
+    <hyperlink ref="N143" r:id="rId156"/>
     <hyperlink ref="C21" r:id="rId157"/>
     <hyperlink ref="N21" r:id="rId158"/>
     <hyperlink ref="C62" r:id="rId159"/>
-    <hyperlink ref="C138" r:id="rId160"/>
-    <hyperlink ref="J138" r:id="rId161"/>
-    <hyperlink ref="C136" r:id="rId162"/>
-    <hyperlink ref="N136" r:id="rId163"/>
-    <hyperlink ref="J136" r:id="rId164"/>
+    <hyperlink ref="C139" r:id="rId160"/>
+    <hyperlink ref="J139" r:id="rId161"/>
+    <hyperlink ref="C137" r:id="rId162"/>
+    <hyperlink ref="N137" r:id="rId163"/>
+    <hyperlink ref="J137" r:id="rId164"/>
     <hyperlink ref="C91" r:id="rId165"/>
     <hyperlink ref="C89" r:id="rId166"/>
     <hyperlink ref="C40" r:id="rId167"/>
@@ -4839,6 +4912,9 @@
     <hyperlink ref="N98" r:id="rId171"/>
     <hyperlink ref="C73" r:id="rId172"/>
     <hyperlink ref="K73" r:id="rId173"/>
+    <hyperlink ref="C150" r:id="rId174"/>
+    <hyperlink ref="C115" r:id="rId175"/>
+    <hyperlink ref="K115" r:id="rId176"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
update csv and add more info on Archigos data
</commit_message>
<xml_diff>
--- a/PolData.xlsx
+++ b/PolData.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="782" uniqueCount="429">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="789" uniqueCount="433">
   <si>
     <t>name</t>
   </si>
@@ -1314,6 +1314,18 @@
   </si>
   <si>
     <t>http://politicaladarchive.org/api/v1/ad_instances?output=csv</t>
+  </si>
+  <si>
+    <t>http://www.rochester.edu/college/faculty/hgoemans/Archigos_4.1_stata14.dta</t>
+  </si>
+  <si>
+    <t>http://www.rochester.edu/college/faculty/hgoemans/Archigos_4.1.pdf</t>
+  </si>
+  <si>
+    <t>Political leaders, leader characteristics</t>
+  </si>
+  <si>
+    <t>Stata link is to Version 4.1.</t>
   </si>
 </sst>
 </file>
@@ -1656,7 +1668,7 @@
   <dimension ref="A1:Q155"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A150" sqref="A150"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1995,6 +2007,33 @@
       </c>
       <c r="C9" s="2" t="s">
         <v>162</v>
+      </c>
+      <c r="D9" t="s">
+        <v>431</v>
+      </c>
+      <c r="E9" t="s">
+        <v>14</v>
+      </c>
+      <c r="F9">
+        <v>1875</v>
+      </c>
+      <c r="G9">
+        <v>2015</v>
+      </c>
+      <c r="H9" t="s">
+        <v>348</v>
+      </c>
+      <c r="I9" t="s">
+        <v>349</v>
+      </c>
+      <c r="J9" s="2" t="s">
+        <v>430</v>
+      </c>
+      <c r="L9" s="2" t="s">
+        <v>429</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>432</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.2">
@@ -4915,6 +4954,8 @@
     <hyperlink ref="C150" r:id="rId174"/>
     <hyperlink ref="C115" r:id="rId175"/>
     <hyperlink ref="K115" r:id="rId176"/>
+    <hyperlink ref="L9" r:id="rId177"/>
+    <hyperlink ref="J9" r:id="rId178"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
update info on Asian Barometer
</commit_message>
<xml_diff>
--- a/PolData.xlsx
+++ b/PolData.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="789" uniqueCount="433">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="794" uniqueCount="438">
   <si>
     <t>name</t>
   </si>
@@ -1326,6 +1326,21 @@
   </si>
   <si>
     <t>Stata link is to Version 4.1.</t>
+  </si>
+  <si>
+    <t>http://www.asianbarometer.org/pdf/core_questionnaire_wave4.pdf</t>
+  </si>
+  <si>
+    <t>Codebook link is to questionnaire for the 4th wave</t>
+  </si>
+  <si>
+    <t>free, application form</t>
+  </si>
+  <si>
+    <t>mail</t>
+  </si>
+  <si>
+    <t>Economic evaluations, trust in institutions, social capital, political participation, access to public service, internet and social media, partisanship</t>
   </si>
 </sst>
 </file>
@@ -1668,7 +1683,7 @@
   <dimension ref="A1:Q155"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2046,11 +2061,26 @@
       <c r="C10" s="2" t="s">
         <v>46</v>
       </c>
+      <c r="D10" t="s">
+        <v>437</v>
+      </c>
       <c r="E10" t="s">
         <v>73</v>
       </c>
       <c r="F10">
         <v>2001</v>
+      </c>
+      <c r="H10" t="s">
+        <v>436</v>
+      </c>
+      <c r="I10" t="s">
+        <v>435</v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>433</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>434</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.2">
@@ -4956,6 +4986,7 @@
     <hyperlink ref="K115" r:id="rId176"/>
     <hyperlink ref="L9" r:id="rId177"/>
     <hyperlink ref="J9" r:id="rId178"/>
+    <hyperlink ref="J10" r:id="rId179"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
add two datasets, Seki-Williams Governments/Ministers
</commit_message>
<xml_diff>
--- a/PolData.xlsx
+++ b/PolData.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="794" uniqueCount="438">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="811" uniqueCount="448">
   <si>
     <t>name</t>
   </si>
@@ -1341,6 +1341,36 @@
   </si>
   <si>
     <t>Economic evaluations, trust in institutions, social capital, political participation, access to public service, internet and social media, partisanship</t>
+  </si>
+  <si>
+    <t>http://faculty.missouri.edu/williamslaro/govtdata.html</t>
+  </si>
+  <si>
+    <t>Seki-Williams Governments Dataset</t>
+  </si>
+  <si>
+    <t>http://faculty.missouri.edu/williamslaro/SW%202016%20Codebook--Governments.pdf</t>
+  </si>
+  <si>
+    <t>http://faculty.missouri.edu/williamslaro/Seki-Williams%20Governments--Version%202.0.dta</t>
+  </si>
+  <si>
+    <t>http://faculty.missouri.edu/williamslaro/Seki-Williams%20Governments--Version%202.0.csv</t>
+  </si>
+  <si>
+    <t>Seki-Williams Ministers Dataset</t>
+  </si>
+  <si>
+    <t>http://faculty.missouri.edu/williamslaro/SW%202016%20Codebook--Ministers.pdf</t>
+  </si>
+  <si>
+    <t>http://faculty.missouri.edu/williamslaro/Seki-Williams%20Ministers--Version%202.0.csv</t>
+  </si>
+  <si>
+    <t>http://faculty.missouri.edu/williamslaro/Seki-Williams%20Ministers--Version%202.0.dta</t>
+  </si>
+  <si>
+    <t>Ministry, tenure</t>
   </si>
 </sst>
 </file>
@@ -1680,10 +1710,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q155"/>
+  <dimension ref="A1:Q157"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView tabSelected="1" topLeftCell="C110" workbookViewId="0">
+      <selection activeCell="A131" sqref="A131"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4214,99 +4244,114 @@
     </row>
     <row r="126" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>194</v>
+        <v>439</v>
       </c>
       <c r="B126" t="s">
-        <v>99</v>
+        <v>259</v>
       </c>
       <c r="C126" s="2" t="s">
-        <v>193</v>
+        <v>438</v>
+      </c>
+      <c r="H126" t="s">
+        <v>348</v>
+      </c>
+      <c r="I126" t="s">
+        <v>349</v>
+      </c>
+      <c r="J126" s="2" t="s">
+        <v>440</v>
+      </c>
+      <c r="K126" s="2" t="s">
+        <v>442</v>
+      </c>
+      <c r="L126" s="2" t="s">
+        <v>441</v>
       </c>
     </row>
     <row r="127" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>295</v>
+        <v>443</v>
       </c>
       <c r="B127" t="s">
-        <v>40</v>
+        <v>259</v>
       </c>
       <c r="C127" s="2" t="s">
-        <v>296</v>
-      </c>
-      <c r="E127" t="s">
-        <v>297</v>
+        <v>438</v>
+      </c>
+      <c r="D127" t="s">
+        <v>447</v>
       </c>
       <c r="F127">
         <v>1990</v>
       </c>
       <c r="G127">
-        <v>2015</v>
+        <v>2014</v>
       </c>
       <c r="H127" t="s">
-        <v>16</v>
+        <v>348</v>
       </c>
       <c r="I127" t="s">
-        <v>249</v>
+        <v>349</v>
+      </c>
+      <c r="J127" s="2" t="s">
+        <v>444</v>
+      </c>
+      <c r="K127" s="2" t="s">
+        <v>445</v>
+      </c>
+      <c r="L127" s="2" t="s">
+        <v>446</v>
       </c>
     </row>
     <row r="128" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>256</v>
+        <v>194</v>
       </c>
       <c r="B128" t="s">
-        <v>250</v>
+        <v>99</v>
       </c>
       <c r="C128" s="2" t="s">
-        <v>257</v>
-      </c>
-      <c r="E128" t="s">
-        <v>258</v>
-      </c>
-      <c r="H128" t="s">
-        <v>16</v>
-      </c>
-      <c r="I128" t="s">
-        <v>20</v>
+        <v>193</v>
       </c>
     </row>
     <row r="129" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>227</v>
+        <v>295</v>
       </c>
       <c r="B129" t="s">
         <v>40</v>
       </c>
       <c r="C129" s="2" t="s">
-        <v>225</v>
+        <v>296</v>
+      </c>
+      <c r="E129" t="s">
+        <v>297</v>
       </c>
       <c r="F129">
-        <v>1955</v>
+        <v>1990</v>
       </c>
       <c r="G129">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="H129" t="s">
         <v>16</v>
       </c>
       <c r="I129" t="s">
-        <v>20</v>
+        <v>249</v>
       </c>
     </row>
     <row r="130" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
-        <v>230</v>
+        <v>256</v>
       </c>
       <c r="B130" t="s">
-        <v>40</v>
+        <v>250</v>
       </c>
       <c r="C130" s="2" t="s">
-        <v>225</v>
-      </c>
-      <c r="F130">
-        <v>1995</v>
-      </c>
-      <c r="G130">
-        <v>2016</v>
+        <v>257</v>
+      </c>
+      <c r="E130" t="s">
+        <v>258</v>
       </c>
       <c r="H130" t="s">
         <v>16</v>
@@ -4317,36 +4362,42 @@
     </row>
     <row r="131" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>109</v>
+        <v>227</v>
       </c>
       <c r="B131" t="s">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="C131" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="E131" t="s">
-        <v>111</v>
+        <v>225</v>
       </c>
       <c r="F131">
-        <v>1956</v>
+        <v>1955</v>
+      </c>
+      <c r="G131">
+        <v>2016</v>
+      </c>
+      <c r="H131" t="s">
+        <v>16</v>
+      </c>
+      <c r="I131" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="132" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>326</v>
+        <v>230</v>
       </c>
       <c r="B132" t="s">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="C132" s="2" t="s">
-        <v>327</v>
-      </c>
-      <c r="E132" t="s">
-        <v>111</v>
+        <v>225</v>
       </c>
       <c r="F132">
-        <v>1998</v>
+        <v>1995</v>
+      </c>
+      <c r="G132">
+        <v>2016</v>
       </c>
       <c r="H132" t="s">
         <v>16</v>
@@ -4357,39 +4408,36 @@
     </row>
     <row r="133" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
-        <v>91</v>
+        <v>109</v>
       </c>
       <c r="B133" t="s">
         <v>25</v>
       </c>
       <c r="C133" s="2" t="s">
-        <v>93</v>
+        <v>110</v>
       </c>
       <c r="E133" t="s">
-        <v>92</v>
+        <v>111</v>
       </c>
       <c r="F133">
-        <v>1999</v>
+        <v>1956</v>
       </c>
     </row>
     <row r="134" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
-        <v>314</v>
+        <v>326</v>
       </c>
       <c r="B134" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="C134" s="2" t="s">
-        <v>313</v>
+        <v>327</v>
       </c>
       <c r="E134" t="s">
-        <v>315</v>
+        <v>111</v>
       </c>
       <c r="F134">
-        <v>1950</v>
-      </c>
-      <c r="G134">
-        <v>2004</v>
+        <v>1998</v>
       </c>
       <c r="H134" t="s">
         <v>16</v>
@@ -4400,122 +4448,110 @@
     </row>
     <row r="135" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
-        <v>161</v>
+        <v>91</v>
       </c>
       <c r="B135" t="s">
         <v>25</v>
       </c>
       <c r="C135" s="2" t="s">
-        <v>160</v>
+        <v>93</v>
+      </c>
+      <c r="E135" t="s">
+        <v>92</v>
+      </c>
+      <c r="F135">
+        <v>1999</v>
       </c>
     </row>
     <row r="136" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
-        <v>168</v>
+        <v>314</v>
       </c>
       <c r="B136" t="s">
         <v>40</v>
       </c>
       <c r="C136" s="2" t="s">
-        <v>167</v>
+        <v>313</v>
+      </c>
+      <c r="E136" t="s">
+        <v>315</v>
+      </c>
+      <c r="F136">
+        <v>1950</v>
+      </c>
+      <c r="G136">
+        <v>2004</v>
+      </c>
+      <c r="H136" t="s">
+        <v>16</v>
+      </c>
+      <c r="I136" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="137" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
-        <v>399</v>
+        <v>161</v>
       </c>
       <c r="B137" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="C137" s="2" t="s">
-        <v>400</v>
-      </c>
-      <c r="E137" t="s">
-        <v>14</v>
-      </c>
-      <c r="F137">
-        <v>2000</v>
-      </c>
-      <c r="G137">
-        <v>2014</v>
-      </c>
-      <c r="H137" t="s">
-        <v>348</v>
-      </c>
-      <c r="I137" t="s">
-        <v>349</v>
-      </c>
-      <c r="J137" s="2" t="s">
-        <v>402</v>
-      </c>
-      <c r="N137" s="2" t="s">
-        <v>401</v>
+        <v>160</v>
       </c>
     </row>
     <row r="138" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
-        <v>213</v>
+        <v>168</v>
       </c>
       <c r="B138" t="s">
-        <v>55</v>
+        <v>40</v>
       </c>
       <c r="C138" s="2" t="s">
-        <v>212</v>
-      </c>
-      <c r="H138" t="s">
-        <v>16</v>
-      </c>
-      <c r="I138" t="s">
-        <v>20</v>
+        <v>167</v>
       </c>
     </row>
     <row r="139" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
-        <v>395</v>
+        <v>399</v>
       </c>
       <c r="B139" t="s">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="C139" s="2" t="s">
-        <v>394</v>
-      </c>
-      <c r="D139" t="s">
-        <v>396</v>
+        <v>400</v>
       </c>
       <c r="E139" t="s">
-        <v>111</v>
+        <v>14</v>
       </c>
       <c r="F139">
-        <v>1986</v>
+        <v>2000</v>
       </c>
       <c r="G139">
-        <v>2015</v>
+        <v>2014</v>
       </c>
       <c r="H139" t="s">
-        <v>367</v>
+        <v>348</v>
       </c>
       <c r="I139" t="s">
-        <v>398</v>
+        <v>349</v>
       </c>
       <c r="J139" s="2" t="s">
-        <v>397</v>
+        <v>402</v>
+      </c>
+      <c r="N139" s="2" t="s">
+        <v>401</v>
       </c>
     </row>
     <row r="140" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
-        <v>323</v>
+        <v>213</v>
       </c>
       <c r="B140" t="s">
-        <v>25</v>
+        <v>55</v>
       </c>
       <c r="C140" s="2" t="s">
-        <v>324</v>
-      </c>
-      <c r="E140" t="s">
-        <v>325</v>
-      </c>
-      <c r="F140">
-        <v>1942</v>
+        <v>212</v>
       </c>
       <c r="H140" t="s">
         <v>16</v>
@@ -4526,124 +4562,145 @@
     </row>
     <row r="141" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
-        <v>273</v>
+        <v>395</v>
       </c>
       <c r="B141" t="s">
-        <v>237</v>
+        <v>25</v>
       </c>
       <c r="C141" s="2" t="s">
-        <v>272</v>
+        <v>394</v>
+      </c>
+      <c r="D141" t="s">
+        <v>396</v>
+      </c>
+      <c r="E141" t="s">
+        <v>111</v>
       </c>
       <c r="F141">
-        <v>1996</v>
+        <v>1986</v>
       </c>
       <c r="G141">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="H141" t="s">
-        <v>16</v>
+        <v>367</v>
       </c>
       <c r="I141" t="s">
-        <v>20</v>
+        <v>398</v>
+      </c>
+      <c r="J141" s="2" t="s">
+        <v>397</v>
       </c>
     </row>
     <row r="142" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
-        <v>66</v>
+        <v>323</v>
       </c>
       <c r="B142" t="s">
         <v>25</v>
       </c>
       <c r="C142" s="2" t="s">
-        <v>67</v>
+        <v>324</v>
+      </c>
+      <c r="E142" t="s">
+        <v>325</v>
+      </c>
+      <c r="F142">
+        <v>1942</v>
+      </c>
+      <c r="H142" t="s">
+        <v>16</v>
+      </c>
+      <c r="I142" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="143" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
-        <v>383</v>
+        <v>273</v>
       </c>
       <c r="B143" t="s">
-        <v>40</v>
+        <v>237</v>
       </c>
       <c r="C143" s="2" t="s">
-        <v>384</v>
-      </c>
-      <c r="E143" t="s">
-        <v>386</v>
+        <v>272</v>
       </c>
       <c r="F143">
-        <v>1951</v>
+        <v>1996</v>
+      </c>
+      <c r="G143">
+        <v>2016</v>
       </c>
       <c r="H143" t="s">
-        <v>348</v>
+        <v>16</v>
       </c>
       <c r="I143" t="s">
-        <v>349</v>
-      </c>
-      <c r="N143" s="2" t="s">
-        <v>385</v>
+        <v>20</v>
       </c>
     </row>
     <row r="144" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
-        <v>139</v>
+        <v>66</v>
       </c>
       <c r="B144" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="C144" s="2" t="s">
-        <v>140</v>
+        <v>67</v>
       </c>
     </row>
     <row r="145" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
-        <v>329</v>
+        <v>383</v>
       </c>
       <c r="B145" t="s">
-        <v>165</v>
+        <v>40</v>
       </c>
       <c r="C145" s="2" t="s">
-        <v>328</v>
+        <v>384</v>
       </c>
       <c r="E145" t="s">
-        <v>34</v>
+        <v>386</v>
       </c>
       <c r="F145">
-        <v>1789</v>
+        <v>1951</v>
       </c>
       <c r="H145" t="s">
-        <v>16</v>
+        <v>348</v>
       </c>
       <c r="I145" t="s">
-        <v>20</v>
+        <v>349</v>
+      </c>
+      <c r="N145" s="2" t="s">
+        <v>385</v>
       </c>
     </row>
     <row r="146" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
-        <v>172</v>
+        <v>139</v>
       </c>
       <c r="B146" t="s">
-        <v>60</v>
+        <v>40</v>
       </c>
       <c r="C146" s="2" t="s">
-        <v>171</v>
+        <v>140</v>
       </c>
     </row>
     <row r="147" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
-        <v>217</v>
+        <v>329</v>
       </c>
       <c r="B147" t="s">
-        <v>60</v>
+        <v>165</v>
       </c>
       <c r="C147" s="2" t="s">
-        <v>216</v>
+        <v>328</v>
       </c>
       <c r="E147" t="s">
-        <v>14</v>
+        <v>34</v>
       </c>
       <c r="F147">
-        <v>1900</v>
+        <v>1789</v>
       </c>
       <c r="H147" t="s">
         <v>16</v>
@@ -4654,130 +4711,118 @@
     </row>
     <row r="148" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
-        <v>132</v>
+        <v>172</v>
       </c>
       <c r="B148" t="s">
-        <v>259</v>
+        <v>60</v>
       </c>
       <c r="C148" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="Q148" t="s">
-        <v>17</v>
+        <v>171</v>
       </c>
     </row>
     <row r="149" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
-        <v>182</v>
+        <v>217</v>
       </c>
       <c r="B149" t="s">
-        <v>165</v>
+        <v>60</v>
       </c>
       <c r="C149" s="2" t="s">
-        <v>181</v>
+        <v>216</v>
+      </c>
+      <c r="E149" t="s">
+        <v>14</v>
+      </c>
+      <c r="F149">
+        <v>1900</v>
+      </c>
+      <c r="H149" t="s">
+        <v>16</v>
+      </c>
+      <c r="I149" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="150" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
-        <v>423</v>
+        <v>132</v>
       </c>
       <c r="B150" t="s">
-        <v>86</v>
+        <v>259</v>
       </c>
       <c r="C150" s="2" t="s">
-        <v>424</v>
-      </c>
-      <c r="E150" t="s">
-        <v>34</v>
-      </c>
-      <c r="F150">
-        <v>1996</v>
-      </c>
-      <c r="G150">
-        <v>2016</v>
-      </c>
-      <c r="H150" t="s">
-        <v>348</v>
-      </c>
-      <c r="I150" t="s">
-        <v>425</v>
+        <v>133</v>
+      </c>
+      <c r="Q150" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="151" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
-        <v>115</v>
+        <v>182</v>
       </c>
       <c r="B151" t="s">
-        <v>128</v>
+        <v>165</v>
       </c>
       <c r="C151" s="2" t="s">
-        <v>116</v>
+        <v>181</v>
       </c>
     </row>
     <row r="152" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
-        <v>263</v>
+        <v>423</v>
       </c>
       <c r="B152" t="s">
-        <v>250</v>
+        <v>86</v>
       </c>
       <c r="C152" s="2" t="s">
-        <v>264</v>
+        <v>424</v>
       </c>
       <c r="E152" t="s">
-        <v>265</v>
+        <v>34</v>
       </c>
       <c r="F152">
-        <v>1500</v>
+        <v>1996</v>
       </c>
       <c r="G152">
-        <v>2000</v>
+        <v>2016</v>
       </c>
       <c r="H152" t="s">
-        <v>16</v>
+        <v>348</v>
       </c>
       <c r="I152" t="s">
-        <v>20</v>
+        <v>425</v>
       </c>
     </row>
     <row r="153" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
-        <v>221</v>
+        <v>115</v>
       </c>
       <c r="B153" t="s">
-        <v>86</v>
+        <v>128</v>
       </c>
       <c r="C153" s="2" t="s">
-        <v>220</v>
-      </c>
-      <c r="F153">
-        <v>2013</v>
-      </c>
-      <c r="H153" t="s">
-        <v>16</v>
-      </c>
-      <c r="I153" t="s">
-        <v>20</v>
+        <v>116</v>
       </c>
     </row>
     <row r="154" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
-        <v>13</v>
+        <v>263</v>
       </c>
       <c r="B154" t="s">
-        <v>25</v>
+        <v>250</v>
       </c>
       <c r="C154" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="D154" s="1" t="s">
-        <v>42</v>
+        <v>264</v>
       </c>
       <c r="E154" t="s">
-        <v>14</v>
+        <v>265</v>
       </c>
       <c r="F154">
-        <v>1981</v>
+        <v>1500</v>
+      </c>
+      <c r="G154">
+        <v>2000</v>
       </c>
       <c r="H154" t="s">
         <v>16</v>
@@ -4788,23 +4833,69 @@
     </row>
     <row r="155" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
+        <v>221</v>
+      </c>
+      <c r="B155" t="s">
+        <v>86</v>
+      </c>
+      <c r="C155" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="F155">
+        <v>2013</v>
+      </c>
+      <c r="H155" t="s">
+        <v>16</v>
+      </c>
+      <c r="I155" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="156" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A156" t="s">
+        <v>13</v>
+      </c>
+      <c r="B156" t="s">
+        <v>25</v>
+      </c>
+      <c r="C156" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D156" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E156" t="s">
+        <v>14</v>
+      </c>
+      <c r="F156">
+        <v>1981</v>
+      </c>
+      <c r="H156" t="s">
+        <v>16</v>
+      </c>
+      <c r="I156" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="157" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A157" t="s">
         <v>283</v>
       </c>
-      <c r="B155" t="s">
+      <c r="B157" t="s">
         <v>124</v>
       </c>
-      <c r="C155" s="2" t="s">
+      <c r="C157" s="2" t="s">
         <v>284</v>
       </c>
-      <c r="H155" t="s">
-        <v>16</v>
-      </c>
-      <c r="I155" t="s">
+      <c r="H157" t="s">
+        <v>16</v>
+      </c>
+      <c r="I157" t="s">
         <v>20</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:Q155">
+  <sortState ref="A2:Q157">
     <sortCondition ref="A2"/>
   </sortState>
   <hyperlinks>
@@ -4814,7 +4905,7 @@
     <hyperlink ref="C10" r:id="rId4"/>
     <hyperlink ref="C92" r:id="rId5"/>
     <hyperlink ref="C112" r:id="rId6"/>
-    <hyperlink ref="C154" r:id="rId7"/>
+    <hyperlink ref="C156" r:id="rId7"/>
     <hyperlink ref="C35" r:id="rId8"/>
     <hyperlink ref="C30" r:id="rId9"/>
     <hyperlink ref="C49" r:id="rId10"/>
@@ -4828,7 +4919,7 @@
     <hyperlink ref="C41" r:id="rId18"/>
     <hyperlink ref="C70" r:id="rId19"/>
     <hyperlink ref="C16" r:id="rId20"/>
-    <hyperlink ref="C142" r:id="rId21"/>
+    <hyperlink ref="C144" r:id="rId21"/>
     <hyperlink ref="C8" r:id="rId22"/>
     <hyperlink ref="C38" r:id="rId23"/>
     <hyperlink ref="C53" r:id="rId24"/>
@@ -4837,15 +4928,15 @@
     <hyperlink ref="C55" r:id="rId27"/>
     <hyperlink ref="C68" r:id="rId28"/>
     <hyperlink ref="C90" r:id="rId29"/>
-    <hyperlink ref="C133" r:id="rId30"/>
+    <hyperlink ref="C135" r:id="rId30"/>
     <hyperlink ref="C95" r:id="rId31"/>
     <hyperlink ref="C80" r:id="rId32"/>
     <hyperlink ref="C101" r:id="rId33"/>
     <hyperlink ref="C69" r:id="rId34"/>
     <hyperlink ref="C17" r:id="rId35"/>
-    <hyperlink ref="C131" r:id="rId36"/>
+    <hyperlink ref="C133" r:id="rId36"/>
     <hyperlink ref="C15" r:id="rId37"/>
-    <hyperlink ref="C151" r:id="rId38"/>
+    <hyperlink ref="C153" r:id="rId38"/>
     <hyperlink ref="C84" r:id="rId39"/>
     <hyperlink ref="C57" r:id="rId40"/>
     <hyperlink ref="C117" r:id="rId41"/>
@@ -4853,10 +4944,10 @@
     <hyperlink ref="C51" r:id="rId43"/>
     <hyperlink ref="C23" r:id="rId44"/>
     <hyperlink ref="C109" r:id="rId45"/>
-    <hyperlink ref="C148" r:id="rId46"/>
+    <hyperlink ref="C150" r:id="rId46"/>
     <hyperlink ref="C27" r:id="rId47" display="http://comparativeconstitutionsproject.org/"/>
     <hyperlink ref="C106" r:id="rId48"/>
-    <hyperlink ref="C144" r:id="rId49"/>
+    <hyperlink ref="C146" r:id="rId49"/>
     <hyperlink ref="C121" r:id="rId50"/>
     <hyperlink ref="C116" r:id="rId51"/>
     <hyperlink ref="C22" r:id="rId52"/>
@@ -4868,22 +4959,22 @@
     <hyperlink ref="C97" r:id="rId58"/>
     <hyperlink ref="C125" r:id="rId59"/>
     <hyperlink ref="C31" r:id="rId60"/>
-    <hyperlink ref="C135" r:id="rId61"/>
+    <hyperlink ref="C137" r:id="rId61"/>
     <hyperlink ref="C9" r:id="rId62"/>
     <hyperlink ref="C33" r:id="rId63"/>
-    <hyperlink ref="C136" r:id="rId64"/>
+    <hyperlink ref="C138" r:id="rId64"/>
     <hyperlink ref="C14" r:id="rId65"/>
-    <hyperlink ref="C146" r:id="rId66"/>
+    <hyperlink ref="C148" r:id="rId66"/>
     <hyperlink ref="C25" r:id="rId67"/>
     <hyperlink ref="C24" r:id="rId68"/>
     <hyperlink ref="C26" r:id="rId69"/>
     <hyperlink ref="C52" r:id="rId70"/>
-    <hyperlink ref="C149" r:id="rId71"/>
+    <hyperlink ref="C151" r:id="rId71"/>
     <hyperlink ref="C28" r:id="rId72"/>
     <hyperlink ref="C113" r:id="rId73"/>
     <hyperlink ref="C32" r:id="rId74"/>
     <hyperlink ref="C45" r:id="rId75"/>
-    <hyperlink ref="C126" r:id="rId76"/>
+    <hyperlink ref="C128" r:id="rId76"/>
     <hyperlink ref="C42" r:id="rId77"/>
     <hyperlink ref="C39" r:id="rId78"/>
     <hyperlink ref="C67" r:id="rId79"/>
@@ -4892,18 +4983,18 @@
     <hyperlink ref="C12" r:id="rId82"/>
     <hyperlink ref="C105" r:id="rId83"/>
     <hyperlink ref="C114" r:id="rId84"/>
-    <hyperlink ref="C138" r:id="rId85"/>
+    <hyperlink ref="C140" r:id="rId85"/>
     <hyperlink ref="C36" r:id="rId86"/>
-    <hyperlink ref="C147" r:id="rId87"/>
+    <hyperlink ref="C149" r:id="rId87"/>
     <hyperlink ref="C44" r:id="rId88"/>
-    <hyperlink ref="C153" r:id="rId89"/>
+    <hyperlink ref="C155" r:id="rId89"/>
     <hyperlink ref="C93" r:id="rId90"/>
     <hyperlink ref="C64" r:id="rId91"/>
     <hyperlink ref="C94" r:id="rId92"/>
-    <hyperlink ref="C129" r:id="rId93"/>
+    <hyperlink ref="C131" r:id="rId93"/>
     <hyperlink ref="C78" r:id="rId94"/>
     <hyperlink ref="C99" r:id="rId95"/>
-    <hyperlink ref="C130" r:id="rId96"/>
+    <hyperlink ref="C132" r:id="rId96"/>
     <hyperlink ref="C61" r:id="rId97"/>
     <hyperlink ref="C111" r:id="rId98"/>
     <hyperlink ref="C46" r:id="rId99"/>
@@ -4916,36 +5007,36 @@
     <hyperlink ref="C103" r:id="rId106"/>
     <hyperlink ref="C47" r:id="rId107"/>
     <hyperlink ref="C82" r:id="rId108"/>
-    <hyperlink ref="C128" r:id="rId109"/>
+    <hyperlink ref="C130" r:id="rId109"/>
     <hyperlink ref="C13" r:id="rId110"/>
     <hyperlink ref="C4" r:id="rId111"/>
-    <hyperlink ref="C152" r:id="rId112"/>
+    <hyperlink ref="C154" r:id="rId112"/>
     <hyperlink ref="C88" r:id="rId113"/>
     <hyperlink ref="C83" r:id="rId114"/>
-    <hyperlink ref="C141" r:id="rId115"/>
+    <hyperlink ref="C143" r:id="rId115"/>
     <hyperlink ref="C124" r:id="rId116"/>
     <hyperlink ref="C63" r:id="rId117"/>
     <hyperlink ref="C96" r:id="rId118"/>
     <hyperlink ref="C72" r:id="rId119"/>
-    <hyperlink ref="C155" r:id="rId120"/>
+    <hyperlink ref="C157" r:id="rId120"/>
     <hyperlink ref="C65" r:id="rId121"/>
     <hyperlink ref="C123" r:id="rId122"/>
     <hyperlink ref="C102" r:id="rId123"/>
     <hyperlink ref="C76" r:id="rId124"/>
     <hyperlink ref="C100" r:id="rId125"/>
-    <hyperlink ref="C127" r:id="rId126"/>
+    <hyperlink ref="C129" r:id="rId126"/>
     <hyperlink ref="C86" r:id="rId127"/>
     <hyperlink ref="C11" r:id="rId128"/>
     <hyperlink ref="C19" r:id="rId129"/>
     <hyperlink ref="C122" r:id="rId130"/>
     <hyperlink ref="C71" r:id="rId131"/>
-    <hyperlink ref="C134" r:id="rId132"/>
+    <hyperlink ref="C136" r:id="rId132"/>
     <hyperlink ref="C119" r:id="rId133"/>
     <hyperlink ref="C118" r:id="rId134"/>
     <hyperlink ref="C120" r:id="rId135"/>
-    <hyperlink ref="C140" r:id="rId136"/>
-    <hyperlink ref="C132" r:id="rId137"/>
-    <hyperlink ref="C145" r:id="rId138"/>
+    <hyperlink ref="C142" r:id="rId136"/>
+    <hyperlink ref="C134" r:id="rId137"/>
+    <hyperlink ref="C147" r:id="rId138"/>
     <hyperlink ref="C37" r:id="rId139"/>
     <hyperlink ref="C87" r:id="rId140"/>
     <hyperlink ref="J2" r:id="rId141"/>
@@ -4962,16 +5053,16 @@
     <hyperlink ref="M8" r:id="rId152"/>
     <hyperlink ref="L8" r:id="rId153"/>
     <hyperlink ref="J8" r:id="rId154"/>
-    <hyperlink ref="C143" r:id="rId155"/>
-    <hyperlink ref="N143" r:id="rId156"/>
+    <hyperlink ref="C145" r:id="rId155"/>
+    <hyperlink ref="N145" r:id="rId156"/>
     <hyperlink ref="C21" r:id="rId157"/>
     <hyperlink ref="N21" r:id="rId158"/>
     <hyperlink ref="C62" r:id="rId159"/>
-    <hyperlink ref="C139" r:id="rId160"/>
-    <hyperlink ref="J139" r:id="rId161"/>
-    <hyperlink ref="C137" r:id="rId162"/>
-    <hyperlink ref="N137" r:id="rId163"/>
-    <hyperlink ref="J137" r:id="rId164"/>
+    <hyperlink ref="C141" r:id="rId160"/>
+    <hyperlink ref="J141" r:id="rId161"/>
+    <hyperlink ref="C139" r:id="rId162"/>
+    <hyperlink ref="N139" r:id="rId163"/>
+    <hyperlink ref="J139" r:id="rId164"/>
     <hyperlink ref="C91" r:id="rId165"/>
     <hyperlink ref="C89" r:id="rId166"/>
     <hyperlink ref="C40" r:id="rId167"/>
@@ -4981,12 +5072,20 @@
     <hyperlink ref="N98" r:id="rId171"/>
     <hyperlink ref="C73" r:id="rId172"/>
     <hyperlink ref="K73" r:id="rId173"/>
-    <hyperlink ref="C150" r:id="rId174"/>
+    <hyperlink ref="C152" r:id="rId174"/>
     <hyperlink ref="C115" r:id="rId175"/>
     <hyperlink ref="K115" r:id="rId176"/>
     <hyperlink ref="L9" r:id="rId177"/>
     <hyperlink ref="J9" r:id="rId178"/>
     <hyperlink ref="J10" r:id="rId179"/>
+    <hyperlink ref="C126" r:id="rId180"/>
+    <hyperlink ref="J126" r:id="rId181"/>
+    <hyperlink ref="L126" r:id="rId182"/>
+    <hyperlink ref="K126" r:id="rId183"/>
+    <hyperlink ref="C127" r:id="rId184"/>
+    <hyperlink ref="J127" r:id="rId185"/>
+    <hyperlink ref="K127" r:id="rId186"/>
+    <hyperlink ref="L127" r:id="rId187"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
add dataset, Extended State History Index
</commit_message>
<xml_diff>
--- a/PolData.xlsx
+++ b/PolData.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="811" uniqueCount="448">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="819" uniqueCount="452">
   <si>
     <t>name</t>
   </si>
@@ -1371,6 +1371,18 @@
   </si>
   <si>
     <t>Ministry, tenure</t>
+  </si>
+  <si>
+    <t>https://sites.google.com/site/econolaols/extended-state-history-index</t>
+  </si>
+  <si>
+    <t>Extended State History Index</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1t5p1USIivXK-38urc2d5Fx7X5rHTzxzQ/view?usp=sharing</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1OExJ70t0YBzlV1vhUE11bbQTW8tJH7cW/view?usp=sharing</t>
   </si>
 </sst>
 </file>
@@ -1710,10 +1722,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q157"/>
+  <dimension ref="A1:Q158"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C110" workbookViewId="0">
-      <selection activeCell="A131" sqref="A131"/>
+    <sheetView tabSelected="1" topLeftCell="A137" workbookViewId="0">
+      <selection activeCell="B159" sqref="B159"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3019,36 +3031,51 @@
     </row>
     <row r="64" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>224</v>
+        <v>449</v>
       </c>
       <c r="B64" t="s">
-        <v>40</v>
+        <v>250</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>225</v>
+        <v>448</v>
+      </c>
+      <c r="E64" t="s">
+        <v>14</v>
       </c>
       <c r="F64">
-        <v>1964</v>
+        <v>-4000</v>
       </c>
       <c r="G64">
-        <v>2008</v>
+        <v>2000</v>
       </c>
       <c r="H64" t="s">
-        <v>16</v>
+        <v>348</v>
       </c>
       <c r="I64" t="s">
-        <v>20</v>
+        <v>349</v>
+      </c>
+      <c r="J64" s="2" t="s">
+        <v>450</v>
+      </c>
+      <c r="N64" s="2" t="s">
+        <v>451</v>
       </c>
     </row>
     <row r="65" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>285</v>
+        <v>224</v>
       </c>
       <c r="B65" t="s">
-        <v>250</v>
+        <v>40</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>286</v>
+        <v>225</v>
+      </c>
+      <c r="F65">
+        <v>1964</v>
+      </c>
+      <c r="G65">
+        <v>2008</v>
       </c>
       <c r="H65" t="s">
         <v>16</v>
@@ -3059,198 +3086,198 @@
     </row>
     <row r="66" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>205</v>
+        <v>285</v>
       </c>
       <c r="B66" t="s">
-        <v>40</v>
+        <v>250</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>204</v>
-      </c>
-      <c r="F66">
-        <v>2006</v>
+        <v>286</v>
+      </c>
+      <c r="H66" t="s">
+        <v>16</v>
+      </c>
+      <c r="I66" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="67" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>200</v>
+        <v>205</v>
       </c>
       <c r="B67" t="s">
-        <v>99</v>
+        <v>40</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="F67">
-        <v>1980</v>
-      </c>
-      <c r="G67">
-        <v>2007</v>
-      </c>
-      <c r="Q67" t="s">
-        <v>18</v>
+        <v>2006</v>
       </c>
     </row>
     <row r="68" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>89</v>
+        <v>200</v>
       </c>
       <c r="B68" t="s">
-        <v>25</v>
+        <v>99</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="E68" t="s">
-        <v>34</v>
+        <v>201</v>
       </c>
       <c r="F68">
-        <v>1972</v>
-      </c>
-      <c r="H68" t="s">
-        <v>16</v>
-      </c>
-      <c r="I68" t="s">
-        <v>20</v>
+        <v>1980</v>
+      </c>
+      <c r="G68">
+        <v>2007</v>
+      </c>
+      <c r="Q68" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="69" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>104</v>
+        <v>89</v>
       </c>
       <c r="B69" t="s">
         <v>25</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>106</v>
+        <v>88</v>
       </c>
       <c r="E69" t="s">
-        <v>105</v>
+        <v>34</v>
       </c>
       <c r="F69">
-        <v>1980</v>
+        <v>1972</v>
+      </c>
+      <c r="H69" t="s">
+        <v>16</v>
+      </c>
+      <c r="I69" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="70" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>62</v>
+        <v>104</v>
       </c>
       <c r="B70" t="s">
         <v>25</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>63</v>
+        <v>106</v>
+      </c>
+      <c r="E70" t="s">
+        <v>105</v>
+      </c>
+      <c r="F70">
+        <v>1980</v>
       </c>
     </row>
     <row r="71" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>311</v>
+        <v>62</v>
       </c>
       <c r="B71" t="s">
-        <v>165</v>
+        <v>25</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>312</v>
-      </c>
-      <c r="E71" t="s">
-        <v>14</v>
-      </c>
-      <c r="H71" t="s">
-        <v>16</v>
-      </c>
-      <c r="I71" t="s">
-        <v>301</v>
+        <v>63</v>
       </c>
     </row>
     <row r="72" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>281</v>
+        <v>311</v>
       </c>
       <c r="B72" t="s">
-        <v>237</v>
+        <v>165</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>282</v>
+        <v>312</v>
+      </c>
+      <c r="E72" t="s">
+        <v>14</v>
       </c>
       <c r="H72" t="s">
         <v>16</v>
       </c>
       <c r="I72" t="s">
-        <v>20</v>
+        <v>301</v>
       </c>
     </row>
     <row r="73" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>418</v>
+        <v>281</v>
       </c>
       <c r="B73" t="s">
-        <v>86</v>
+        <v>237</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>419</v>
-      </c>
-      <c r="E73" t="s">
-        <v>420</v>
-      </c>
-      <c r="F73">
-        <v>1948</v>
-      </c>
-      <c r="G73">
-        <v>2012</v>
+        <v>282</v>
       </c>
       <c r="H73" t="s">
-        <v>348</v>
+        <v>16</v>
       </c>
       <c r="I73" t="s">
-        <v>349</v>
-      </c>
-      <c r="K73" s="2" t="s">
-        <v>421</v>
-      </c>
-      <c r="Q73" t="s">
-        <v>422</v>
+        <v>20</v>
       </c>
     </row>
     <row r="74" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>151</v>
+        <v>418</v>
       </c>
       <c r="B74" t="s">
-        <v>40</v>
+        <v>86</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>152</v>
+        <v>419</v>
       </c>
       <c r="E74" t="s">
-        <v>14</v>
+        <v>420</v>
+      </c>
+      <c r="F74">
+        <v>1948</v>
+      </c>
+      <c r="G74">
+        <v>2012</v>
+      </c>
+      <c r="H74" t="s">
+        <v>348</v>
+      </c>
+      <c r="I74" t="s">
+        <v>349</v>
+      </c>
+      <c r="K74" s="2" t="s">
+        <v>421</v>
+      </c>
+      <c r="Q74" t="s">
+        <v>422</v>
       </c>
     </row>
     <row r="75" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>242</v>
+        <v>151</v>
       </c>
       <c r="B75" t="s">
-        <v>237</v>
+        <v>40</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>243</v>
-      </c>
-      <c r="H75" t="s">
-        <v>16</v>
-      </c>
-      <c r="I75" t="s">
-        <v>20</v>
+        <v>152</v>
+      </c>
+      <c r="E75" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="76" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>292</v>
+        <v>242</v>
       </c>
       <c r="B76" t="s">
-        <v>99</v>
+        <v>237</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>291</v>
+        <v>243</v>
       </c>
       <c r="H76" t="s">
         <v>16</v>
@@ -3261,47 +3288,47 @@
     </row>
     <row r="77" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>153</v>
+        <v>292</v>
       </c>
       <c r="B77" t="s">
-        <v>259</v>
+        <v>99</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>154</v>
+        <v>291</v>
+      </c>
+      <c r="H77" t="s">
+        <v>16</v>
+      </c>
+      <c r="I77" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="78" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>228</v>
+        <v>153</v>
       </c>
       <c r="B78" t="s">
-        <v>40</v>
+        <v>259</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>225</v>
-      </c>
-      <c r="F78">
-        <v>1989</v>
-      </c>
-      <c r="G78">
-        <v>2017</v>
-      </c>
-      <c r="H78" t="s">
-        <v>16</v>
-      </c>
-      <c r="I78" t="s">
-        <v>20</v>
+        <v>154</v>
       </c>
     </row>
     <row r="79" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>245</v>
+        <v>228</v>
       </c>
       <c r="B79" t="s">
-        <v>237</v>
+        <v>40</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>244</v>
+        <v>225</v>
+      </c>
+      <c r="F79">
+        <v>1989</v>
+      </c>
+      <c r="G79">
+        <v>2017</v>
       </c>
       <c r="H79" t="s">
         <v>16</v>
@@ -3312,50 +3339,41 @@
     </row>
     <row r="80" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>100</v>
+        <v>245</v>
       </c>
       <c r="B80" t="s">
-        <v>99</v>
+        <v>237</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>101</v>
+        <v>244</v>
+      </c>
+      <c r="H80" t="s">
+        <v>16</v>
+      </c>
+      <c r="I80" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="81" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>239</v>
+        <v>100</v>
       </c>
       <c r="B81" t="s">
-        <v>237</v>
+        <v>99</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>243</v>
-      </c>
-      <c r="H81" t="s">
-        <v>16</v>
-      </c>
-      <c r="I81" t="s">
-        <v>20</v>
+        <v>101</v>
       </c>
     </row>
     <row r="82" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>254</v>
+        <v>239</v>
       </c>
       <c r="B82" t="s">
-        <v>55</v>
+        <v>237</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>253</v>
-      </c>
-      <c r="E82" t="s">
-        <v>255</v>
-      </c>
-      <c r="F82">
-        <v>1960</v>
-      </c>
-      <c r="G82">
-        <v>2014</v>
+        <v>243</v>
       </c>
       <c r="H82" t="s">
         <v>16</v>
@@ -3366,19 +3384,22 @@
     </row>
     <row r="83" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>270</v>
+        <v>254</v>
       </c>
       <c r="B83" t="s">
         <v>55</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>271</v>
+        <v>253</v>
+      </c>
+      <c r="E83" t="s">
+        <v>255</v>
       </c>
       <c r="F83">
-        <v>1990</v>
+        <v>1960</v>
       </c>
       <c r="G83">
-        <v>2010</v>
+        <v>2014</v>
       </c>
       <c r="H83" t="s">
         <v>16</v>
@@ -3389,96 +3410,90 @@
     </row>
     <row r="84" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>117</v>
+        <v>270</v>
       </c>
       <c r="B84" t="s">
         <v>55</v>
       </c>
       <c r="C84" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="F84">
+        <v>1990</v>
+      </c>
+      <c r="G84">
+        <v>2010</v>
+      </c>
+      <c r="H84" t="s">
+        <v>16</v>
+      </c>
+      <c r="I84" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="85" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A85" t="s">
+        <v>117</v>
+      </c>
+      <c r="B85" t="s">
+        <v>55</v>
+      </c>
+      <c r="C85" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="I84" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q84" t="s">
+      <c r="I85" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q85" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="85" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A85" s="1" t="s">
+    <row r="86" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A86" s="1" t="s">
         <v>23</v>
-      </c>
-      <c r="B85" t="s">
-        <v>25</v>
-      </c>
-      <c r="C85" s="2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="86" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A86" t="s">
-        <v>300</v>
       </c>
       <c r="B86" t="s">
         <v>25</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>298</v>
-      </c>
-      <c r="E86" t="s">
-        <v>299</v>
-      </c>
-      <c r="F86">
-        <v>1969</v>
-      </c>
-      <c r="H86" t="s">
-        <v>16</v>
-      </c>
-      <c r="I86" t="s">
-        <v>249</v>
+        <v>53</v>
       </c>
     </row>
     <row r="87" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>332</v>
+        <v>300</v>
       </c>
       <c r="B87" t="s">
-        <v>134</v>
+        <v>25</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>333</v>
+        <v>298</v>
       </c>
       <c r="E87" t="s">
-        <v>334</v>
+        <v>299</v>
+      </c>
+      <c r="F87">
+        <v>1969</v>
       </c>
       <c r="H87" t="s">
         <v>16</v>
       </c>
       <c r="I87" t="s">
-        <v>20</v>
+        <v>249</v>
       </c>
     </row>
     <row r="88" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>267</v>
+        <v>332</v>
       </c>
       <c r="B88" t="s">
-        <v>250</v>
+        <v>134</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>266</v>
-      </c>
-      <c r="D88" t="s">
-        <v>269</v>
+        <v>333</v>
       </c>
       <c r="E88" t="s">
-        <v>268</v>
-      </c>
-      <c r="F88">
-        <v>1970</v>
-      </c>
-      <c r="G88">
-        <v>2014</v>
+        <v>334</v>
       </c>
       <c r="H88" t="s">
         <v>16</v>
@@ -3489,143 +3504,149 @@
     </row>
     <row r="89" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>407</v>
+        <v>267</v>
       </c>
       <c r="B89" t="s">
-        <v>40</v>
+        <v>250</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>406</v>
+        <v>266</v>
       </c>
       <c r="D89" t="s">
-        <v>408</v>
+        <v>269</v>
       </c>
       <c r="E89" t="s">
-        <v>14</v>
+        <v>268</v>
       </c>
       <c r="F89">
-        <v>1949</v>
+        <v>1970</v>
       </c>
       <c r="G89">
-        <v>2013</v>
+        <v>2014</v>
       </c>
       <c r="H89" t="s">
-        <v>348</v>
+        <v>16</v>
       </c>
       <c r="I89" t="s">
-        <v>349</v>
+        <v>20</v>
       </c>
     </row>
     <row r="90" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>96</v>
+        <v>407</v>
       </c>
       <c r="B90" t="s">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>90</v>
+        <v>406</v>
+      </c>
+      <c r="D90" t="s">
+        <v>408</v>
       </c>
       <c r="E90" t="s">
-        <v>69</v>
+        <v>14</v>
       </c>
       <c r="F90">
-        <v>1995</v>
+        <v>1949</v>
+      </c>
+      <c r="G90">
+        <v>2013</v>
+      </c>
+      <c r="H90" t="s">
+        <v>348</v>
+      </c>
+      <c r="I90" t="s">
+        <v>349</v>
       </c>
     </row>
     <row r="91" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>404</v>
+        <v>96</v>
       </c>
       <c r="B91" t="s">
-        <v>83</v>
+        <v>25</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>403</v>
-      </c>
-      <c r="D91" t="s">
-        <v>405</v>
+        <v>90</v>
       </c>
       <c r="E91" t="s">
-        <v>14</v>
+        <v>69</v>
       </c>
       <c r="F91">
-        <v>1875</v>
-      </c>
-      <c r="G91">
-        <v>2004</v>
-      </c>
-      <c r="H91" t="s">
-        <v>348</v>
-      </c>
-      <c r="I91" t="s">
-        <v>349</v>
+        <v>1995</v>
       </c>
     </row>
     <row r="92" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>11</v>
+        <v>404</v>
       </c>
       <c r="B92" t="s">
-        <v>25</v>
+        <v>83</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>12</v>
+        <v>403</v>
       </c>
       <c r="D92" t="s">
-        <v>95</v>
+        <v>405</v>
       </c>
       <c r="E92" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="F92">
-        <v>2007</v>
+        <v>1875</v>
+      </c>
+      <c r="G92">
+        <v>2004</v>
       </c>
       <c r="H92" t="s">
-        <v>16</v>
+        <v>348</v>
       </c>
       <c r="I92" t="s">
-        <v>21</v>
+        <v>349</v>
       </c>
     </row>
     <row r="93" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>223</v>
+        <v>11</v>
       </c>
       <c r="B93" t="s">
-        <v>124</v>
+        <v>25</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>222</v>
+        <v>12</v>
+      </c>
+      <c r="D93" t="s">
+        <v>95</v>
+      </c>
+      <c r="E93" t="s">
+        <v>10</v>
       </c>
       <c r="F93">
-        <v>1</v>
-      </c>
-      <c r="G93">
-        <v>2010</v>
+        <v>2007</v>
       </c>
       <c r="H93" t="s">
         <v>16</v>
       </c>
       <c r="I93" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="94" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="B94" t="s">
-        <v>40</v>
+        <v>124</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="F94">
-        <v>1946</v>
+        <v>1</v>
       </c>
       <c r="G94">
-        <v>2016</v>
+        <v>2010</v>
       </c>
       <c r="H94" t="s">
         <v>16</v>
@@ -3636,122 +3657,122 @@
     </row>
     <row r="95" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>97</v>
+        <v>226</v>
       </c>
       <c r="B95" t="s">
-        <v>128</v>
+        <v>40</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>98</v>
+        <v>225</v>
+      </c>
+      <c r="F95">
+        <v>1946</v>
+      </c>
+      <c r="G95">
+        <v>2016</v>
+      </c>
+      <c r="H95" t="s">
+        <v>16</v>
+      </c>
+      <c r="I95" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="96" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>278</v>
+        <v>97</v>
       </c>
       <c r="B96" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>279</v>
-      </c>
-      <c r="E96" t="s">
-        <v>280</v>
-      </c>
-      <c r="F96">
-        <v>1890</v>
-      </c>
-      <c r="G96">
-        <v>1996</v>
-      </c>
-      <c r="H96" t="s">
-        <v>16</v>
-      </c>
-      <c r="I96" t="s">
-        <v>20</v>
+        <v>98</v>
       </c>
     </row>
     <row r="97" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>156</v>
+        <v>278</v>
       </c>
       <c r="B97" t="s">
-        <v>25</v>
+        <v>124</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>154</v>
+        <v>279</v>
+      </c>
+      <c r="E97" t="s">
+        <v>280</v>
+      </c>
+      <c r="F97">
+        <v>1890</v>
+      </c>
+      <c r="G97">
+        <v>1996</v>
+      </c>
+      <c r="H97" t="s">
+        <v>16</v>
+      </c>
+      <c r="I97" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="98" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>413</v>
+        <v>156</v>
       </c>
       <c r="B98" t="s">
-        <v>128</v>
+        <v>25</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>414</v>
-      </c>
-      <c r="E98" t="s">
-        <v>415</v>
-      </c>
-      <c r="F98">
-        <v>1946</v>
-      </c>
-      <c r="G98">
-        <v>2014</v>
-      </c>
-      <c r="H98" t="s">
-        <v>348</v>
-      </c>
-      <c r="I98" t="s">
-        <v>349</v>
-      </c>
-      <c r="N98" s="2" t="s">
-        <v>416</v>
-      </c>
-      <c r="Q98" t="s">
-        <v>417</v>
+        <v>154</v>
       </c>
     </row>
     <row r="99" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>229</v>
+        <v>413</v>
       </c>
       <c r="B99" t="s">
-        <v>40</v>
+        <v>128</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>225</v>
+        <v>414</v>
+      </c>
+      <c r="E99" t="s">
+        <v>415</v>
       </c>
       <c r="F99">
-        <v>1952</v>
+        <v>1946</v>
       </c>
       <c r="G99">
-        <v>1997</v>
+        <v>2014</v>
       </c>
       <c r="H99" t="s">
-        <v>16</v>
+        <v>348</v>
       </c>
       <c r="I99" t="s">
-        <v>20</v>
+        <v>349</v>
+      </c>
+      <c r="N99" s="2" t="s">
+        <v>416</v>
+      </c>
+      <c r="Q99" t="s">
+        <v>417</v>
       </c>
     </row>
     <row r="100" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>293</v>
+        <v>229</v>
       </c>
       <c r="B100" t="s">
         <v>40</v>
       </c>
       <c r="C100" s="2" t="s">
-        <v>294</v>
+        <v>225</v>
       </c>
       <c r="F100">
-        <v>2004</v>
+        <v>1952</v>
       </c>
       <c r="G100">
-        <v>2006</v>
+        <v>1997</v>
       </c>
       <c r="H100" t="s">
         <v>16</v>
@@ -3762,221 +3783,218 @@
     </row>
     <row r="101" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>102</v>
+        <v>293</v>
       </c>
       <c r="B101" t="s">
-        <v>99</v>
+        <v>40</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>103</v>
+        <v>294</v>
+      </c>
+      <c r="F101">
+        <v>2004</v>
+      </c>
+      <c r="G101">
+        <v>2006</v>
+      </c>
+      <c r="H101" t="s">
+        <v>16</v>
+      </c>
+      <c r="I101" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="102" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>289</v>
+        <v>102</v>
       </c>
       <c r="B102" t="s">
-        <v>124</v>
+        <v>99</v>
       </c>
       <c r="C102" s="2" t="s">
-        <v>290</v>
+        <v>103</v>
       </c>
     </row>
     <row r="103" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>246</v>
+        <v>289</v>
       </c>
       <c r="B103" t="s">
-        <v>165</v>
+        <v>124</v>
       </c>
       <c r="C103" s="2" t="s">
-        <v>247</v>
-      </c>
-      <c r="E103" t="s">
-        <v>14</v>
-      </c>
-      <c r="F103">
-        <v>1960</v>
-      </c>
-      <c r="G103">
-        <v>2006</v>
-      </c>
-      <c r="H103" t="s">
-        <v>16</v>
-      </c>
-      <c r="I103" t="s">
-        <v>249</v>
+        <v>290</v>
       </c>
     </row>
     <row r="104" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>365</v>
+        <v>246</v>
       </c>
       <c r="B104" t="s">
-        <v>128</v>
+        <v>165</v>
       </c>
       <c r="C104" s="2" t="s">
-        <v>364</v>
-      </c>
-      <c r="D104" t="s">
-        <v>370</v>
+        <v>247</v>
       </c>
       <c r="E104" t="s">
-        <v>366</v>
+        <v>14</v>
       </c>
       <c r="F104">
-        <v>1906</v>
+        <v>1960</v>
       </c>
       <c r="G104">
-        <v>2013</v>
+        <v>2006</v>
       </c>
       <c r="H104" t="s">
-        <v>367</v>
+        <v>16</v>
       </c>
       <c r="I104" t="s">
-        <v>368</v>
-      </c>
-      <c r="Q104" t="s">
-        <v>369</v>
+        <v>249</v>
       </c>
     </row>
     <row r="105" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>208</v>
+        <v>365</v>
       </c>
       <c r="B105" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="C105" s="2" t="s">
-        <v>209</v>
+        <v>364</v>
+      </c>
+      <c r="D105" t="s">
+        <v>370</v>
+      </c>
+      <c r="E105" t="s">
+        <v>366</v>
       </c>
       <c r="F105">
-        <v>1932</v>
+        <v>1906</v>
       </c>
       <c r="G105">
-        <v>2014</v>
+        <v>2013</v>
       </c>
       <c r="H105" t="s">
-        <v>16</v>
+        <v>367</v>
       </c>
       <c r="I105" t="s">
-        <v>20</v>
+        <v>368</v>
+      </c>
+      <c r="Q105" t="s">
+        <v>369</v>
       </c>
     </row>
     <row r="106" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>137</v>
+        <v>208</v>
       </c>
       <c r="B106" t="s">
-        <v>259</v>
+        <v>124</v>
       </c>
       <c r="C106" s="2" t="s">
-        <v>138</v>
+        <v>209</v>
+      </c>
+      <c r="F106">
+        <v>1932</v>
+      </c>
+      <c r="G106">
+        <v>2014</v>
+      </c>
+      <c r="H106" t="s">
+        <v>16</v>
+      </c>
+      <c r="I106" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="107" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>155</v>
+        <v>137</v>
       </c>
       <c r="B107" t="s">
         <v>259</v>
       </c>
       <c r="C107" s="2" t="s">
-        <v>154</v>
+        <v>138</v>
       </c>
     </row>
     <row r="108" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>57</v>
+        <v>155</v>
       </c>
       <c r="B108" t="s">
-        <v>128</v>
+        <v>259</v>
       </c>
       <c r="C108" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="Q108" t="s">
-        <v>17</v>
+        <v>154</v>
       </c>
     </row>
     <row r="109" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>129</v>
+        <v>57</v>
       </c>
       <c r="B109" t="s">
-        <v>259</v>
+        <v>128</v>
       </c>
       <c r="C109" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="E109" t="s">
-        <v>131</v>
-      </c>
-      <c r="F109">
-        <v>1945</v>
-      </c>
-      <c r="G109">
-        <v>2008</v>
-      </c>
-      <c r="I109" t="s">
-        <v>20</v>
+        <v>58</v>
+      </c>
+      <c r="Q109" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="110" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>148</v>
+        <v>129</v>
       </c>
       <c r="B110" t="s">
-        <v>128</v>
+        <v>259</v>
       </c>
       <c r="C110" s="2" t="s">
-        <v>147</v>
+        <v>130</v>
+      </c>
+      <c r="E110" t="s">
+        <v>131</v>
+      </c>
+      <c r="F110">
+        <v>1945</v>
+      </c>
+      <c r="G110">
+        <v>2008</v>
+      </c>
+      <c r="I110" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="111" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>233</v>
+        <v>148</v>
       </c>
       <c r="B111" t="s">
-        <v>165</v>
+        <v>128</v>
       </c>
       <c r="C111" s="2" t="s">
-        <v>234</v>
-      </c>
-      <c r="E111" t="s">
-        <v>14</v>
-      </c>
-      <c r="F111">
-        <v>2012</v>
-      </c>
-      <c r="G111">
-        <v>2016</v>
-      </c>
-      <c r="H111" t="s">
-        <v>16</v>
-      </c>
-      <c r="I111" t="s">
-        <v>20</v>
+        <v>147</v>
       </c>
     </row>
     <row r="112" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>35</v>
+        <v>233</v>
       </c>
       <c r="B112" t="s">
-        <v>25</v>
+        <v>165</v>
       </c>
       <c r="C112" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="D112" t="s">
-        <v>37</v>
+        <v>234</v>
       </c>
       <c r="E112" t="s">
         <v>14</v>
       </c>
       <c r="F112">
-        <v>2001</v>
+        <v>2012</v>
+      </c>
+      <c r="G112">
+        <v>2016</v>
       </c>
       <c r="H112" t="s">
         <v>16</v>
@@ -3987,119 +4005,119 @@
     </row>
     <row r="113" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>185</v>
+        <v>35</v>
       </c>
       <c r="B113" t="s">
-        <v>128</v>
+        <v>25</v>
       </c>
       <c r="C113" s="2" t="s">
-        <v>186</v>
+        <v>36</v>
+      </c>
+      <c r="D113" t="s">
+        <v>37</v>
+      </c>
+      <c r="E113" t="s">
+        <v>14</v>
+      </c>
+      <c r="F113">
+        <v>2001</v>
+      </c>
+      <c r="H113" t="s">
+        <v>16</v>
+      </c>
+      <c r="I113" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="114" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>210</v>
+        <v>185</v>
       </c>
       <c r="B114" t="s">
-        <v>40</v>
+        <v>128</v>
       </c>
       <c r="C114" s="2" t="s">
-        <v>211</v>
-      </c>
-      <c r="F114">
-        <v>1976</v>
-      </c>
-      <c r="G114">
-        <v>2016</v>
-      </c>
-      <c r="H114" t="s">
-        <v>16</v>
-      </c>
-      <c r="I114" t="s">
-        <v>20</v>
+        <v>186</v>
       </c>
     </row>
     <row r="115" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>426</v>
+        <v>210</v>
       </c>
       <c r="B115" t="s">
-        <v>86</v>
+        <v>40</v>
       </c>
       <c r="C115" s="2" t="s">
-        <v>427</v>
-      </c>
-      <c r="E115" t="s">
-        <v>34</v>
+        <v>211</v>
       </c>
       <c r="F115">
-        <v>2015</v>
+        <v>1976</v>
       </c>
       <c r="G115">
         <v>2016</v>
       </c>
       <c r="H115" t="s">
-        <v>348</v>
+        <v>16</v>
       </c>
       <c r="I115" t="s">
-        <v>349</v>
-      </c>
-      <c r="K115" s="2" t="s">
-        <v>428</v>
+        <v>20</v>
       </c>
     </row>
     <row r="116" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>144</v>
+        <v>426</v>
       </c>
       <c r="B116" t="s">
-        <v>60</v>
+        <v>86</v>
       </c>
       <c r="C116" s="2" t="s">
-        <v>143</v>
+        <v>427</v>
+      </c>
+      <c r="E116" t="s">
+        <v>34</v>
       </c>
       <c r="F116">
-        <v>1800</v>
+        <v>2015</v>
       </c>
       <c r="G116">
-        <v>2013</v>
+        <v>2016</v>
+      </c>
+      <c r="H116" t="s">
+        <v>348</v>
+      </c>
+      <c r="I116" t="s">
+        <v>349</v>
+      </c>
+      <c r="K116" s="2" t="s">
+        <v>428</v>
       </c>
     </row>
     <row r="117" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>122</v>
+        <v>144</v>
       </c>
       <c r="B117" t="s">
-        <v>259</v>
+        <v>60</v>
       </c>
       <c r="C117" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="I117" t="s">
-        <v>20</v>
+        <v>143</v>
+      </c>
+      <c r="F117">
+        <v>1800</v>
+      </c>
+      <c r="G117">
+        <v>2013</v>
       </c>
     </row>
     <row r="118" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>318</v>
+        <v>122</v>
       </c>
       <c r="B118" t="s">
-        <v>250</v>
+        <v>259</v>
       </c>
       <c r="C118" s="2" t="s">
-        <v>319</v>
-      </c>
-      <c r="E118" t="s">
-        <v>320</v>
-      </c>
-      <c r="F118">
-        <v>1975</v>
-      </c>
-      <c r="G118">
-        <v>1989</v>
-      </c>
-      <c r="H118" t="s">
-        <v>16</v>
+        <v>121</v>
       </c>
       <c r="I118" t="s">
         <v>20</v>
@@ -4107,22 +4125,22 @@
     </row>
     <row r="119" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="B119" t="s">
         <v>250</v>
       </c>
       <c r="C119" s="2" t="s">
-        <v>317</v>
+        <v>319</v>
       </c>
       <c r="E119" t="s">
-        <v>105</v>
+        <v>320</v>
       </c>
       <c r="F119">
-        <v>1950</v>
+        <v>1975</v>
       </c>
       <c r="G119">
-        <v>1996</v>
+        <v>1989</v>
       </c>
       <c r="H119" t="s">
         <v>16</v>
@@ -4133,19 +4151,22 @@
     </row>
     <row r="120" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>322</v>
+        <v>316</v>
       </c>
       <c r="B120" t="s">
-        <v>25</v>
+        <v>250</v>
       </c>
       <c r="C120" s="2" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="E120" t="s">
-        <v>77</v>
+        <v>105</v>
       </c>
       <c r="F120">
-        <v>2010</v>
+        <v>1950</v>
+      </c>
+      <c r="G120">
+        <v>1996</v>
       </c>
       <c r="H120" t="s">
         <v>16</v>
@@ -4156,121 +4177,118 @@
     </row>
     <row r="121" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>141</v>
+        <v>322</v>
       </c>
       <c r="B121" t="s">
-        <v>237</v>
+        <v>25</v>
       </c>
       <c r="C121" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="Q121" t="s">
-        <v>17</v>
+        <v>321</v>
+      </c>
+      <c r="E121" t="s">
+        <v>77</v>
+      </c>
+      <c r="F121">
+        <v>2010</v>
+      </c>
+      <c r="H121" t="s">
+        <v>16</v>
+      </c>
+      <c r="I121" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="122" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>308</v>
+        <v>141</v>
       </c>
       <c r="B122" t="s">
-        <v>250</v>
+        <v>237</v>
       </c>
       <c r="C122" s="2" t="s">
-        <v>309</v>
-      </c>
-      <c r="E122" t="s">
-        <v>310</v>
-      </c>
-      <c r="F122">
-        <v>1950</v>
-      </c>
-      <c r="G122">
-        <v>2010</v>
-      </c>
-      <c r="H122" t="s">
-        <v>16</v>
-      </c>
-      <c r="I122" t="s">
-        <v>20</v>
+        <v>142</v>
+      </c>
+      <c r="Q122" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="123" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>287</v>
+        <v>308</v>
       </c>
       <c r="B123" t="s">
-        <v>134</v>
+        <v>250</v>
       </c>
       <c r="C123" s="2" t="s">
-        <v>288</v>
+        <v>309</v>
+      </c>
+      <c r="E123" t="s">
+        <v>310</v>
       </c>
       <c r="F123">
-        <v>1990</v>
+        <v>1950</v>
       </c>
       <c r="G123">
-        <v>2008</v>
+        <v>2010</v>
+      </c>
+      <c r="H123" t="s">
+        <v>16</v>
+      </c>
+      <c r="I123" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="124" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>274</v>
+        <v>287</v>
       </c>
       <c r="B124" t="s">
-        <v>55</v>
+        <v>134</v>
       </c>
       <c r="C124" s="2" t="s">
-        <v>275</v>
-      </c>
-      <c r="H124" t="s">
-        <v>16</v>
-      </c>
-      <c r="I124" t="s">
-        <v>20</v>
+        <v>288</v>
+      </c>
+      <c r="F124">
+        <v>1990</v>
+      </c>
+      <c r="G124">
+        <v>2008</v>
       </c>
     </row>
     <row r="125" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>157</v>
+        <v>274</v>
       </c>
       <c r="B125" t="s">
-        <v>128</v>
+        <v>55</v>
       </c>
       <c r="C125" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="Q125" t="s">
-        <v>18</v>
+        <v>275</v>
+      </c>
+      <c r="H125" t="s">
+        <v>16</v>
+      </c>
+      <c r="I125" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="126" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>439</v>
+        <v>157</v>
       </c>
       <c r="B126" t="s">
-        <v>259</v>
+        <v>128</v>
       </c>
       <c r="C126" s="2" t="s">
-        <v>438</v>
-      </c>
-      <c r="H126" t="s">
-        <v>348</v>
-      </c>
-      <c r="I126" t="s">
-        <v>349</v>
-      </c>
-      <c r="J126" s="2" t="s">
-        <v>440</v>
-      </c>
-      <c r="K126" s="2" t="s">
-        <v>442</v>
-      </c>
-      <c r="L126" s="2" t="s">
-        <v>441</v>
+        <v>154</v>
+      </c>
+      <c r="Q126" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="127" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>443</v>
+        <v>439</v>
       </c>
       <c r="B127" t="s">
         <v>259</v>
@@ -4278,15 +4296,6 @@
       <c r="C127" s="2" t="s">
         <v>438</v>
       </c>
-      <c r="D127" t="s">
-        <v>447</v>
-      </c>
-      <c r="F127">
-        <v>1990</v>
-      </c>
-      <c r="G127">
-        <v>2014</v>
-      </c>
       <c r="H127" t="s">
         <v>348</v>
       </c>
@@ -4294,87 +4303,99 @@
         <v>349</v>
       </c>
       <c r="J127" s="2" t="s">
-        <v>444</v>
+        <v>440</v>
       </c>
       <c r="K127" s="2" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
       <c r="L127" s="2" t="s">
-        <v>446</v>
+        <v>441</v>
       </c>
     </row>
     <row r="128" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>194</v>
+        <v>443</v>
       </c>
       <c r="B128" t="s">
-        <v>99</v>
+        <v>259</v>
       </c>
       <c r="C128" s="2" t="s">
-        <v>193</v>
+        <v>438</v>
+      </c>
+      <c r="D128" t="s">
+        <v>447</v>
+      </c>
+      <c r="F128">
+        <v>1990</v>
+      </c>
+      <c r="G128">
+        <v>2014</v>
+      </c>
+      <c r="H128" t="s">
+        <v>348</v>
+      </c>
+      <c r="I128" t="s">
+        <v>349</v>
+      </c>
+      <c r="J128" s="2" t="s">
+        <v>444</v>
+      </c>
+      <c r="K128" s="2" t="s">
+        <v>445</v>
+      </c>
+      <c r="L128" s="2" t="s">
+        <v>446</v>
       </c>
     </row>
     <row r="129" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>295</v>
+        <v>194</v>
       </c>
       <c r="B129" t="s">
-        <v>40</v>
+        <v>99</v>
       </c>
       <c r="C129" s="2" t="s">
-        <v>296</v>
-      </c>
-      <c r="E129" t="s">
-        <v>297</v>
-      </c>
-      <c r="F129">
-        <v>1990</v>
-      </c>
-      <c r="G129">
-        <v>2015</v>
-      </c>
-      <c r="H129" t="s">
-        <v>16</v>
-      </c>
-      <c r="I129" t="s">
-        <v>249</v>
+        <v>193</v>
       </c>
     </row>
     <row r="130" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
-        <v>256</v>
+        <v>295</v>
       </c>
       <c r="B130" t="s">
-        <v>250</v>
+        <v>40</v>
       </c>
       <c r="C130" s="2" t="s">
-        <v>257</v>
+        <v>296</v>
       </c>
       <c r="E130" t="s">
-        <v>258</v>
+        <v>297</v>
+      </c>
+      <c r="F130">
+        <v>1990</v>
+      </c>
+      <c r="G130">
+        <v>2015</v>
       </c>
       <c r="H130" t="s">
         <v>16</v>
       </c>
       <c r="I130" t="s">
-        <v>20</v>
+        <v>249</v>
       </c>
     </row>
     <row r="131" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>227</v>
+        <v>256</v>
       </c>
       <c r="B131" t="s">
-        <v>40</v>
+        <v>250</v>
       </c>
       <c r="C131" s="2" t="s">
-        <v>225</v>
-      </c>
-      <c r="F131">
-        <v>1955</v>
-      </c>
-      <c r="G131">
-        <v>2016</v>
+        <v>257</v>
+      </c>
+      <c r="E131" t="s">
+        <v>258</v>
       </c>
       <c r="H131" t="s">
         <v>16</v>
@@ -4385,7 +4406,7 @@
     </row>
     <row r="132" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="B132" t="s">
         <v>40</v>
@@ -4394,7 +4415,7 @@
         <v>225</v>
       </c>
       <c r="F132">
-        <v>1995</v>
+        <v>1955</v>
       </c>
       <c r="G132">
         <v>2016</v>
@@ -4408,228 +4429,228 @@
     </row>
     <row r="133" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
-        <v>109</v>
+        <v>230</v>
       </c>
       <c r="B133" t="s">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="C133" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="E133" t="s">
-        <v>111</v>
+        <v>225</v>
       </c>
       <c r="F133">
-        <v>1956</v>
+        <v>1995</v>
+      </c>
+      <c r="G133">
+        <v>2016</v>
+      </c>
+      <c r="H133" t="s">
+        <v>16</v>
+      </c>
+      <c r="I133" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="134" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
-        <v>326</v>
+        <v>109</v>
       </c>
       <c r="B134" t="s">
         <v>25</v>
       </c>
       <c r="C134" s="2" t="s">
-        <v>327</v>
+        <v>110</v>
       </c>
       <c r="E134" t="s">
         <v>111</v>
       </c>
       <c r="F134">
-        <v>1998</v>
-      </c>
-      <c r="H134" t="s">
-        <v>16</v>
-      </c>
-      <c r="I134" t="s">
-        <v>20</v>
+        <v>1956</v>
       </c>
     </row>
     <row r="135" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
-        <v>91</v>
+        <v>326</v>
       </c>
       <c r="B135" t="s">
         <v>25</v>
       </c>
       <c r="C135" s="2" t="s">
-        <v>93</v>
+        <v>327</v>
       </c>
       <c r="E135" t="s">
-        <v>92</v>
+        <v>111</v>
       </c>
       <c r="F135">
-        <v>1999</v>
+        <v>1998</v>
+      </c>
+      <c r="H135" t="s">
+        <v>16</v>
+      </c>
+      <c r="I135" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="136" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
-        <v>314</v>
+        <v>91</v>
       </c>
       <c r="B136" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="C136" s="2" t="s">
-        <v>313</v>
+        <v>93</v>
       </c>
       <c r="E136" t="s">
-        <v>315</v>
+        <v>92</v>
       </c>
       <c r="F136">
-        <v>1950</v>
-      </c>
-      <c r="G136">
-        <v>2004</v>
-      </c>
-      <c r="H136" t="s">
-        <v>16</v>
-      </c>
-      <c r="I136" t="s">
-        <v>20</v>
+        <v>1999</v>
       </c>
     </row>
     <row r="137" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
-        <v>161</v>
+        <v>314</v>
       </c>
       <c r="B137" t="s">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="C137" s="2" t="s">
-        <v>160</v>
+        <v>313</v>
+      </c>
+      <c r="E137" t="s">
+        <v>315</v>
+      </c>
+      <c r="F137">
+        <v>1950</v>
+      </c>
+      <c r="G137">
+        <v>2004</v>
+      </c>
+      <c r="H137" t="s">
+        <v>16</v>
+      </c>
+      <c r="I137" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="138" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="B138" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="C138" s="2" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
     </row>
     <row r="139" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
-        <v>399</v>
+        <v>168</v>
       </c>
       <c r="B139" t="s">
         <v>40</v>
       </c>
       <c r="C139" s="2" t="s">
-        <v>400</v>
-      </c>
-      <c r="E139" t="s">
-        <v>14</v>
-      </c>
-      <c r="F139">
-        <v>2000</v>
-      </c>
-      <c r="G139">
-        <v>2014</v>
-      </c>
-      <c r="H139" t="s">
-        <v>348</v>
-      </c>
-      <c r="I139" t="s">
-        <v>349</v>
-      </c>
-      <c r="J139" s="2" t="s">
-        <v>402</v>
-      </c>
-      <c r="N139" s="2" t="s">
-        <v>401</v>
+        <v>167</v>
       </c>
     </row>
     <row r="140" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
-        <v>213</v>
+        <v>399</v>
       </c>
       <c r="B140" t="s">
-        <v>55</v>
+        <v>40</v>
       </c>
       <c r="C140" s="2" t="s">
-        <v>212</v>
+        <v>400</v>
+      </c>
+      <c r="E140" t="s">
+        <v>14</v>
+      </c>
+      <c r="F140">
+        <v>2000</v>
+      </c>
+      <c r="G140">
+        <v>2014</v>
       </c>
       <c r="H140" t="s">
-        <v>16</v>
+        <v>348</v>
       </c>
       <c r="I140" t="s">
-        <v>20</v>
+        <v>349</v>
+      </c>
+      <c r="J140" s="2" t="s">
+        <v>402</v>
+      </c>
+      <c r="N140" s="2" t="s">
+        <v>401</v>
       </c>
     </row>
     <row r="141" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
-        <v>395</v>
+        <v>213</v>
       </c>
       <c r="B141" t="s">
-        <v>25</v>
+        <v>55</v>
       </c>
       <c r="C141" s="2" t="s">
-        <v>394</v>
-      </c>
-      <c r="D141" t="s">
-        <v>396</v>
-      </c>
-      <c r="E141" t="s">
-        <v>111</v>
-      </c>
-      <c r="F141">
-        <v>1986</v>
-      </c>
-      <c r="G141">
-        <v>2015</v>
+        <v>212</v>
       </c>
       <c r="H141" t="s">
-        <v>367</v>
+        <v>16</v>
       </c>
       <c r="I141" t="s">
-        <v>398</v>
-      </c>
-      <c r="J141" s="2" t="s">
-        <v>397</v>
+        <v>20</v>
       </c>
     </row>
     <row r="142" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
-        <v>323</v>
+        <v>395</v>
       </c>
       <c r="B142" t="s">
         <v>25</v>
       </c>
       <c r="C142" s="2" t="s">
-        <v>324</v>
+        <v>394</v>
+      </c>
+      <c r="D142" t="s">
+        <v>396</v>
       </c>
       <c r="E142" t="s">
-        <v>325</v>
+        <v>111</v>
       </c>
       <c r="F142">
-        <v>1942</v>
+        <v>1986</v>
+      </c>
+      <c r="G142">
+        <v>2015</v>
       </c>
       <c r="H142" t="s">
-        <v>16</v>
+        <v>367</v>
       </c>
       <c r="I142" t="s">
-        <v>20</v>
+        <v>398</v>
+      </c>
+      <c r="J142" s="2" t="s">
+        <v>397</v>
       </c>
     </row>
     <row r="143" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
-        <v>273</v>
+        <v>323</v>
       </c>
       <c r="B143" t="s">
-        <v>237</v>
+        <v>25</v>
       </c>
       <c r="C143" s="2" t="s">
-        <v>272</v>
+        <v>324</v>
+      </c>
+      <c r="E143" t="s">
+        <v>325</v>
       </c>
       <c r="F143">
-        <v>1996</v>
-      </c>
-      <c r="G143">
-        <v>2016</v>
+        <v>1942</v>
       </c>
       <c r="H143" t="s">
         <v>16</v>
@@ -4640,209 +4661,212 @@
     </row>
     <row r="144" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
-        <v>66</v>
+        <v>273</v>
       </c>
       <c r="B144" t="s">
-        <v>25</v>
+        <v>237</v>
       </c>
       <c r="C144" s="2" t="s">
-        <v>67</v>
+        <v>272</v>
+      </c>
+      <c r="F144">
+        <v>1996</v>
+      </c>
+      <c r="G144">
+        <v>2016</v>
+      </c>
+      <c r="H144" t="s">
+        <v>16</v>
+      </c>
+      <c r="I144" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="145" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
-        <v>383</v>
+        <v>66</v>
       </c>
       <c r="B145" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="C145" s="2" t="s">
-        <v>384</v>
-      </c>
-      <c r="E145" t="s">
-        <v>386</v>
-      </c>
-      <c r="F145">
-        <v>1951</v>
-      </c>
-      <c r="H145" t="s">
-        <v>348</v>
-      </c>
-      <c r="I145" t="s">
-        <v>349</v>
-      </c>
-      <c r="N145" s="2" t="s">
-        <v>385</v>
+        <v>67</v>
       </c>
     </row>
     <row r="146" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
-        <v>139</v>
+        <v>383</v>
       </c>
       <c r="B146" t="s">
         <v>40</v>
       </c>
       <c r="C146" s="2" t="s">
-        <v>140</v>
+        <v>384</v>
+      </c>
+      <c r="E146" t="s">
+        <v>386</v>
+      </c>
+      <c r="F146">
+        <v>1951</v>
+      </c>
+      <c r="H146" t="s">
+        <v>348</v>
+      </c>
+      <c r="I146" t="s">
+        <v>349</v>
+      </c>
+      <c r="N146" s="2" t="s">
+        <v>385</v>
       </c>
     </row>
     <row r="147" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
-        <v>329</v>
+        <v>139</v>
       </c>
       <c r="B147" t="s">
-        <v>165</v>
+        <v>40</v>
       </c>
       <c r="C147" s="2" t="s">
-        <v>328</v>
-      </c>
-      <c r="E147" t="s">
-        <v>34</v>
-      </c>
-      <c r="F147">
-        <v>1789</v>
-      </c>
-      <c r="H147" t="s">
-        <v>16</v>
-      </c>
-      <c r="I147" t="s">
-        <v>20</v>
+        <v>140</v>
       </c>
     </row>
     <row r="148" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
-        <v>172</v>
+        <v>329</v>
       </c>
       <c r="B148" t="s">
-        <v>60</v>
+        <v>165</v>
       </c>
       <c r="C148" s="2" t="s">
-        <v>171</v>
+        <v>328</v>
+      </c>
+      <c r="E148" t="s">
+        <v>34</v>
+      </c>
+      <c r="F148">
+        <v>1789</v>
+      </c>
+      <c r="H148" t="s">
+        <v>16</v>
+      </c>
+      <c r="I148" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="149" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
-        <v>217</v>
+        <v>172</v>
       </c>
       <c r="B149" t="s">
         <v>60</v>
       </c>
       <c r="C149" s="2" t="s">
-        <v>216</v>
-      </c>
-      <c r="E149" t="s">
-        <v>14</v>
-      </c>
-      <c r="F149">
-        <v>1900</v>
-      </c>
-      <c r="H149" t="s">
-        <v>16</v>
-      </c>
-      <c r="I149" t="s">
-        <v>20</v>
+        <v>171</v>
       </c>
     </row>
     <row r="150" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
-        <v>132</v>
+        <v>217</v>
       </c>
       <c r="B150" t="s">
-        <v>259</v>
+        <v>60</v>
       </c>
       <c r="C150" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="Q150" t="s">
-        <v>17</v>
+        <v>216</v>
+      </c>
+      <c r="E150" t="s">
+        <v>14</v>
+      </c>
+      <c r="F150">
+        <v>1900</v>
+      </c>
+      <c r="H150" t="s">
+        <v>16</v>
+      </c>
+      <c r="I150" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="151" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
-        <v>182</v>
+        <v>132</v>
       </c>
       <c r="B151" t="s">
-        <v>165</v>
+        <v>259</v>
       </c>
       <c r="C151" s="2" t="s">
-        <v>181</v>
+        <v>133</v>
+      </c>
+      <c r="Q151" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="152" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
-        <v>423</v>
+        <v>182</v>
       </c>
       <c r="B152" t="s">
-        <v>86</v>
+        <v>165</v>
       </c>
       <c r="C152" s="2" t="s">
-        <v>424</v>
-      </c>
-      <c r="E152" t="s">
-        <v>34</v>
-      </c>
-      <c r="F152">
-        <v>1996</v>
-      </c>
-      <c r="G152">
-        <v>2016</v>
-      </c>
-      <c r="H152" t="s">
-        <v>348</v>
-      </c>
-      <c r="I152" t="s">
-        <v>425</v>
+        <v>181</v>
       </c>
     </row>
     <row r="153" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
-        <v>115</v>
+        <v>423</v>
       </c>
       <c r="B153" t="s">
-        <v>128</v>
+        <v>86</v>
       </c>
       <c r="C153" s="2" t="s">
-        <v>116</v>
+        <v>424</v>
+      </c>
+      <c r="E153" t="s">
+        <v>34</v>
+      </c>
+      <c r="F153">
+        <v>1996</v>
+      </c>
+      <c r="G153">
+        <v>2016</v>
+      </c>
+      <c r="H153" t="s">
+        <v>348</v>
+      </c>
+      <c r="I153" t="s">
+        <v>425</v>
       </c>
     </row>
     <row r="154" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
-        <v>263</v>
+        <v>115</v>
       </c>
       <c r="B154" t="s">
-        <v>250</v>
+        <v>128</v>
       </c>
       <c r="C154" s="2" t="s">
-        <v>264</v>
-      </c>
-      <c r="E154" t="s">
-        <v>265</v>
-      </c>
-      <c r="F154">
-        <v>1500</v>
-      </c>
-      <c r="G154">
-        <v>2000</v>
-      </c>
-      <c r="H154" t="s">
-        <v>16</v>
-      </c>
-      <c r="I154" t="s">
-        <v>20</v>
+        <v>116</v>
       </c>
     </row>
     <row r="155" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
-        <v>221</v>
+        <v>263</v>
       </c>
       <c r="B155" t="s">
-        <v>86</v>
+        <v>250</v>
       </c>
       <c r="C155" s="2" t="s">
-        <v>220</v>
+        <v>264</v>
+      </c>
+      <c r="E155" t="s">
+        <v>265</v>
       </c>
       <c r="F155">
-        <v>2013</v>
+        <v>1500</v>
+      </c>
+      <c r="G155">
+        <v>2000</v>
       </c>
       <c r="H155" t="s">
         <v>16</v>
@@ -4853,22 +4877,16 @@
     </row>
     <row r="156" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
-        <v>13</v>
+        <v>221</v>
       </c>
       <c r="B156" t="s">
-        <v>25</v>
+        <v>86</v>
       </c>
       <c r="C156" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="D156" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="E156" t="s">
-        <v>14</v>
+        <v>220</v>
       </c>
       <c r="F156">
-        <v>1981</v>
+        <v>2013</v>
       </c>
       <c r="H156" t="s">
         <v>16</v>
@@ -4879,23 +4897,49 @@
     </row>
     <row r="157" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
+        <v>13</v>
+      </c>
+      <c r="B157" t="s">
+        <v>25</v>
+      </c>
+      <c r="C157" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D157" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E157" t="s">
+        <v>14</v>
+      </c>
+      <c r="F157">
+        <v>1981</v>
+      </c>
+      <c r="H157" t="s">
+        <v>16</v>
+      </c>
+      <c r="I157" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="158" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A158" t="s">
         <v>283</v>
       </c>
-      <c r="B157" t="s">
+      <c r="B158" t="s">
         <v>124</v>
       </c>
-      <c r="C157" s="2" t="s">
+      <c r="C158" s="2" t="s">
         <v>284</v>
       </c>
-      <c r="H157" t="s">
-        <v>16</v>
-      </c>
-      <c r="I157" t="s">
+      <c r="H158" t="s">
+        <v>16</v>
+      </c>
+      <c r="I158" t="s">
         <v>20</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:Q157">
+  <sortState ref="A2:Q158">
     <sortCondition ref="A2"/>
   </sortState>
   <hyperlinks>
@@ -4903,9 +4947,9 @@
     <hyperlink ref="C58" r:id="rId2"/>
     <hyperlink ref="C7" r:id="rId3"/>
     <hyperlink ref="C10" r:id="rId4"/>
-    <hyperlink ref="C92" r:id="rId5"/>
-    <hyperlink ref="C112" r:id="rId6"/>
-    <hyperlink ref="C156" r:id="rId7"/>
+    <hyperlink ref="C93" r:id="rId5"/>
+    <hyperlink ref="C113" r:id="rId6"/>
+    <hyperlink ref="C157" r:id="rId7"/>
     <hyperlink ref="C35" r:id="rId8"/>
     <hyperlink ref="C30" r:id="rId9"/>
     <hyperlink ref="C49" r:id="rId10"/>
@@ -4913,132 +4957,132 @@
     <hyperlink ref="C3" r:id="rId12"/>
     <hyperlink ref="C20" r:id="rId13"/>
     <hyperlink ref="C60" r:id="rId14"/>
-    <hyperlink ref="C85" r:id="rId15"/>
+    <hyperlink ref="C86" r:id="rId15"/>
     <hyperlink ref="C29" r:id="rId16"/>
-    <hyperlink ref="C108" r:id="rId17"/>
+    <hyperlink ref="C109" r:id="rId17"/>
     <hyperlink ref="C41" r:id="rId18"/>
-    <hyperlink ref="C70" r:id="rId19"/>
+    <hyperlink ref="C71" r:id="rId19"/>
     <hyperlink ref="C16" r:id="rId20"/>
-    <hyperlink ref="C144" r:id="rId21"/>
+    <hyperlink ref="C145" r:id="rId21"/>
     <hyperlink ref="C8" r:id="rId22"/>
     <hyperlink ref="C38" r:id="rId23"/>
     <hyperlink ref="C53" r:id="rId24"/>
     <hyperlink ref="C50" r:id="rId25"/>
     <hyperlink ref="C54" r:id="rId26"/>
     <hyperlink ref="C55" r:id="rId27"/>
-    <hyperlink ref="C68" r:id="rId28"/>
-    <hyperlink ref="C90" r:id="rId29"/>
-    <hyperlink ref="C135" r:id="rId30"/>
-    <hyperlink ref="C95" r:id="rId31"/>
-    <hyperlink ref="C80" r:id="rId32"/>
-    <hyperlink ref="C101" r:id="rId33"/>
-    <hyperlink ref="C69" r:id="rId34"/>
+    <hyperlink ref="C69" r:id="rId28"/>
+    <hyperlink ref="C91" r:id="rId29"/>
+    <hyperlink ref="C136" r:id="rId30"/>
+    <hyperlink ref="C96" r:id="rId31"/>
+    <hyperlink ref="C81" r:id="rId32"/>
+    <hyperlink ref="C102" r:id="rId33"/>
+    <hyperlink ref="C70" r:id="rId34"/>
     <hyperlink ref="C17" r:id="rId35"/>
-    <hyperlink ref="C133" r:id="rId36"/>
+    <hyperlink ref="C134" r:id="rId36"/>
     <hyperlink ref="C15" r:id="rId37"/>
-    <hyperlink ref="C153" r:id="rId38"/>
-    <hyperlink ref="C84" r:id="rId39"/>
+    <hyperlink ref="C154" r:id="rId38"/>
+    <hyperlink ref="C85" r:id="rId39"/>
     <hyperlink ref="C57" r:id="rId40"/>
-    <hyperlink ref="C117" r:id="rId41"/>
+    <hyperlink ref="C118" r:id="rId41"/>
     <hyperlink ref="C18" r:id="rId42"/>
     <hyperlink ref="C51" r:id="rId43"/>
     <hyperlink ref="C23" r:id="rId44"/>
-    <hyperlink ref="C109" r:id="rId45"/>
-    <hyperlink ref="C150" r:id="rId46"/>
+    <hyperlink ref="C110" r:id="rId45"/>
+    <hyperlink ref="C151" r:id="rId46"/>
     <hyperlink ref="C27" r:id="rId47" display="http://comparativeconstitutionsproject.org/"/>
-    <hyperlink ref="C106" r:id="rId48"/>
-    <hyperlink ref="C146" r:id="rId49"/>
-    <hyperlink ref="C121" r:id="rId50"/>
-    <hyperlink ref="C116" r:id="rId51"/>
+    <hyperlink ref="C107" r:id="rId48"/>
+    <hyperlink ref="C147" r:id="rId49"/>
+    <hyperlink ref="C122" r:id="rId50"/>
+    <hyperlink ref="C117" r:id="rId51"/>
     <hyperlink ref="C22" r:id="rId52"/>
-    <hyperlink ref="C110" r:id="rId53"/>
+    <hyperlink ref="C111" r:id="rId53"/>
     <hyperlink ref="C48" r:id="rId54"/>
-    <hyperlink ref="C74" r:id="rId55"/>
-    <hyperlink ref="C77" r:id="rId56"/>
-    <hyperlink ref="C107" r:id="rId57"/>
-    <hyperlink ref="C97" r:id="rId58"/>
-    <hyperlink ref="C125" r:id="rId59"/>
+    <hyperlink ref="C75" r:id="rId55"/>
+    <hyperlink ref="C78" r:id="rId56"/>
+    <hyperlink ref="C108" r:id="rId57"/>
+    <hyperlink ref="C98" r:id="rId58"/>
+    <hyperlink ref="C126" r:id="rId59"/>
     <hyperlink ref="C31" r:id="rId60"/>
-    <hyperlink ref="C137" r:id="rId61"/>
+    <hyperlink ref="C138" r:id="rId61"/>
     <hyperlink ref="C9" r:id="rId62"/>
     <hyperlink ref="C33" r:id="rId63"/>
-    <hyperlink ref="C138" r:id="rId64"/>
+    <hyperlink ref="C139" r:id="rId64"/>
     <hyperlink ref="C14" r:id="rId65"/>
-    <hyperlink ref="C148" r:id="rId66"/>
+    <hyperlink ref="C149" r:id="rId66"/>
     <hyperlink ref="C25" r:id="rId67"/>
     <hyperlink ref="C24" r:id="rId68"/>
     <hyperlink ref="C26" r:id="rId69"/>
     <hyperlink ref="C52" r:id="rId70"/>
-    <hyperlink ref="C151" r:id="rId71"/>
+    <hyperlink ref="C152" r:id="rId71"/>
     <hyperlink ref="C28" r:id="rId72"/>
-    <hyperlink ref="C113" r:id="rId73"/>
+    <hyperlink ref="C114" r:id="rId73"/>
     <hyperlink ref="C32" r:id="rId74"/>
     <hyperlink ref="C45" r:id="rId75"/>
-    <hyperlink ref="C128" r:id="rId76"/>
+    <hyperlink ref="C129" r:id="rId76"/>
     <hyperlink ref="C42" r:id="rId77"/>
     <hyperlink ref="C39" r:id="rId78"/>
-    <hyperlink ref="C67" r:id="rId79"/>
+    <hyperlink ref="C68" r:id="rId79"/>
     <hyperlink ref="C5" r:id="rId80"/>
-    <hyperlink ref="C66" r:id="rId81"/>
+    <hyperlink ref="C67" r:id="rId81"/>
     <hyperlink ref="C12" r:id="rId82"/>
-    <hyperlink ref="C105" r:id="rId83"/>
-    <hyperlink ref="C114" r:id="rId84"/>
-    <hyperlink ref="C140" r:id="rId85"/>
+    <hyperlink ref="C106" r:id="rId83"/>
+    <hyperlink ref="C115" r:id="rId84"/>
+    <hyperlink ref="C141" r:id="rId85"/>
     <hyperlink ref="C36" r:id="rId86"/>
-    <hyperlink ref="C149" r:id="rId87"/>
+    <hyperlink ref="C150" r:id="rId87"/>
     <hyperlink ref="C44" r:id="rId88"/>
-    <hyperlink ref="C155" r:id="rId89"/>
-    <hyperlink ref="C93" r:id="rId90"/>
-    <hyperlink ref="C64" r:id="rId91"/>
-    <hyperlink ref="C94" r:id="rId92"/>
-    <hyperlink ref="C131" r:id="rId93"/>
-    <hyperlink ref="C78" r:id="rId94"/>
-    <hyperlink ref="C99" r:id="rId95"/>
-    <hyperlink ref="C132" r:id="rId96"/>
+    <hyperlink ref="C156" r:id="rId89"/>
+    <hyperlink ref="C94" r:id="rId90"/>
+    <hyperlink ref="C65" r:id="rId91"/>
+    <hyperlink ref="C95" r:id="rId92"/>
+    <hyperlink ref="C132" r:id="rId93"/>
+    <hyperlink ref="C79" r:id="rId94"/>
+    <hyperlink ref="C100" r:id="rId95"/>
+    <hyperlink ref="C133" r:id="rId96"/>
     <hyperlink ref="C61" r:id="rId97"/>
-    <hyperlink ref="C111" r:id="rId98"/>
+    <hyperlink ref="C112" r:id="rId98"/>
     <hyperlink ref="C46" r:id="rId99"/>
     <hyperlink ref="C43" r:id="rId100"/>
-    <hyperlink ref="C81" r:id="rId101"/>
+    <hyperlink ref="C82" r:id="rId101"/>
     <hyperlink ref="C59" r:id="rId102"/>
     <hyperlink ref="C2" r:id="rId103"/>
-    <hyperlink ref="C75" r:id="rId104"/>
-    <hyperlink ref="C79" r:id="rId105"/>
-    <hyperlink ref="C103" r:id="rId106"/>
+    <hyperlink ref="C76" r:id="rId104"/>
+    <hyperlink ref="C80" r:id="rId105"/>
+    <hyperlink ref="C104" r:id="rId106"/>
     <hyperlink ref="C47" r:id="rId107"/>
-    <hyperlink ref="C82" r:id="rId108"/>
-    <hyperlink ref="C130" r:id="rId109"/>
+    <hyperlink ref="C83" r:id="rId108"/>
+    <hyperlink ref="C131" r:id="rId109"/>
     <hyperlink ref="C13" r:id="rId110"/>
     <hyperlink ref="C4" r:id="rId111"/>
-    <hyperlink ref="C154" r:id="rId112"/>
-    <hyperlink ref="C88" r:id="rId113"/>
-    <hyperlink ref="C83" r:id="rId114"/>
-    <hyperlink ref="C143" r:id="rId115"/>
-    <hyperlink ref="C124" r:id="rId116"/>
+    <hyperlink ref="C155" r:id="rId112"/>
+    <hyperlink ref="C89" r:id="rId113"/>
+    <hyperlink ref="C84" r:id="rId114"/>
+    <hyperlink ref="C144" r:id="rId115"/>
+    <hyperlink ref="C125" r:id="rId116"/>
     <hyperlink ref="C63" r:id="rId117"/>
-    <hyperlink ref="C96" r:id="rId118"/>
-    <hyperlink ref="C72" r:id="rId119"/>
-    <hyperlink ref="C157" r:id="rId120"/>
-    <hyperlink ref="C65" r:id="rId121"/>
-    <hyperlink ref="C123" r:id="rId122"/>
-    <hyperlink ref="C102" r:id="rId123"/>
-    <hyperlink ref="C76" r:id="rId124"/>
-    <hyperlink ref="C100" r:id="rId125"/>
-    <hyperlink ref="C129" r:id="rId126"/>
-    <hyperlink ref="C86" r:id="rId127"/>
+    <hyperlink ref="C97" r:id="rId118"/>
+    <hyperlink ref="C73" r:id="rId119"/>
+    <hyperlink ref="C158" r:id="rId120"/>
+    <hyperlink ref="C66" r:id="rId121"/>
+    <hyperlink ref="C124" r:id="rId122"/>
+    <hyperlink ref="C103" r:id="rId123"/>
+    <hyperlink ref="C77" r:id="rId124"/>
+    <hyperlink ref="C101" r:id="rId125"/>
+    <hyperlink ref="C130" r:id="rId126"/>
+    <hyperlink ref="C87" r:id="rId127"/>
     <hyperlink ref="C11" r:id="rId128"/>
     <hyperlink ref="C19" r:id="rId129"/>
-    <hyperlink ref="C122" r:id="rId130"/>
-    <hyperlink ref="C71" r:id="rId131"/>
-    <hyperlink ref="C136" r:id="rId132"/>
-    <hyperlink ref="C119" r:id="rId133"/>
-    <hyperlink ref="C118" r:id="rId134"/>
-    <hyperlink ref="C120" r:id="rId135"/>
-    <hyperlink ref="C142" r:id="rId136"/>
-    <hyperlink ref="C134" r:id="rId137"/>
-    <hyperlink ref="C147" r:id="rId138"/>
+    <hyperlink ref="C123" r:id="rId130"/>
+    <hyperlink ref="C72" r:id="rId131"/>
+    <hyperlink ref="C137" r:id="rId132"/>
+    <hyperlink ref="C120" r:id="rId133"/>
+    <hyperlink ref="C119" r:id="rId134"/>
+    <hyperlink ref="C121" r:id="rId135"/>
+    <hyperlink ref="C143" r:id="rId136"/>
+    <hyperlink ref="C135" r:id="rId137"/>
+    <hyperlink ref="C148" r:id="rId138"/>
     <hyperlink ref="C37" r:id="rId139"/>
-    <hyperlink ref="C87" r:id="rId140"/>
+    <hyperlink ref="C88" r:id="rId140"/>
     <hyperlink ref="J2" r:id="rId141"/>
     <hyperlink ref="M3" r:id="rId142"/>
     <hyperlink ref="J3" r:id="rId143"/>
@@ -5046,46 +5090,49 @@
     <hyperlink ref="J4" r:id="rId145"/>
     <hyperlink ref="P5" r:id="rId146"/>
     <hyperlink ref="J5" r:id="rId147"/>
-    <hyperlink ref="C104" r:id="rId148"/>
+    <hyperlink ref="C105" r:id="rId148"/>
     <hyperlink ref="C34" r:id="rId149"/>
     <hyperlink ref="P7" r:id="rId150"/>
     <hyperlink ref="J7" r:id="rId151"/>
     <hyperlink ref="M8" r:id="rId152"/>
     <hyperlink ref="L8" r:id="rId153"/>
     <hyperlink ref="J8" r:id="rId154"/>
-    <hyperlink ref="C145" r:id="rId155"/>
-    <hyperlink ref="N145" r:id="rId156"/>
+    <hyperlink ref="C146" r:id="rId155"/>
+    <hyperlink ref="N146" r:id="rId156"/>
     <hyperlink ref="C21" r:id="rId157"/>
     <hyperlink ref="N21" r:id="rId158"/>
     <hyperlink ref="C62" r:id="rId159"/>
-    <hyperlink ref="C141" r:id="rId160"/>
-    <hyperlink ref="J141" r:id="rId161"/>
-    <hyperlink ref="C139" r:id="rId162"/>
-    <hyperlink ref="N139" r:id="rId163"/>
-    <hyperlink ref="J139" r:id="rId164"/>
-    <hyperlink ref="C91" r:id="rId165"/>
-    <hyperlink ref="C89" r:id="rId166"/>
+    <hyperlink ref="C142" r:id="rId160"/>
+    <hyperlink ref="J142" r:id="rId161"/>
+    <hyperlink ref="C140" r:id="rId162"/>
+    <hyperlink ref="N140" r:id="rId163"/>
+    <hyperlink ref="J140" r:id="rId164"/>
+    <hyperlink ref="C92" r:id="rId165"/>
+    <hyperlink ref="C90" r:id="rId166"/>
     <hyperlink ref="C40" r:id="rId167"/>
     <hyperlink ref="J40" r:id="rId168"/>
     <hyperlink ref="K40" r:id="rId169"/>
-    <hyperlink ref="C98" r:id="rId170"/>
-    <hyperlink ref="N98" r:id="rId171"/>
-    <hyperlink ref="C73" r:id="rId172"/>
-    <hyperlink ref="K73" r:id="rId173"/>
-    <hyperlink ref="C152" r:id="rId174"/>
-    <hyperlink ref="C115" r:id="rId175"/>
-    <hyperlink ref="K115" r:id="rId176"/>
+    <hyperlink ref="C99" r:id="rId170"/>
+    <hyperlink ref="N99" r:id="rId171"/>
+    <hyperlink ref="C74" r:id="rId172"/>
+    <hyperlink ref="K74" r:id="rId173"/>
+    <hyperlink ref="C153" r:id="rId174"/>
+    <hyperlink ref="C116" r:id="rId175"/>
+    <hyperlink ref="K116" r:id="rId176"/>
     <hyperlink ref="L9" r:id="rId177"/>
     <hyperlink ref="J9" r:id="rId178"/>
     <hyperlink ref="J10" r:id="rId179"/>
-    <hyperlink ref="C126" r:id="rId180"/>
-    <hyperlink ref="J126" r:id="rId181"/>
-    <hyperlink ref="L126" r:id="rId182"/>
-    <hyperlink ref="K126" r:id="rId183"/>
-    <hyperlink ref="C127" r:id="rId184"/>
-    <hyperlink ref="J127" r:id="rId185"/>
-    <hyperlink ref="K127" r:id="rId186"/>
-    <hyperlink ref="L127" r:id="rId187"/>
+    <hyperlink ref="C127" r:id="rId180"/>
+    <hyperlink ref="J127" r:id="rId181"/>
+    <hyperlink ref="L127" r:id="rId182"/>
+    <hyperlink ref="K127" r:id="rId183"/>
+    <hyperlink ref="C128" r:id="rId184"/>
+    <hyperlink ref="J128" r:id="rId185"/>
+    <hyperlink ref="K128" r:id="rId186"/>
+    <hyperlink ref="L128" r:id="rId187"/>
+    <hyperlink ref="C64" r:id="rId188"/>
+    <hyperlink ref="J64" r:id="rId189"/>
+    <hyperlink ref="N64" r:id="rId190"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
add 'Survey of Health, Ageing and Retirement in Europe' and 'Life in Transition Survey'
</commit_message>
<xml_diff>
--- a/PolData.xlsx
+++ b/PolData.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="819" uniqueCount="452">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="834" uniqueCount="460">
   <si>
     <t>name</t>
   </si>
@@ -1383,6 +1383,30 @@
   </si>
   <si>
     <t>https://drive.google.com/file/d/1OExJ70t0YBzlV1vhUE11bbQTW8tJH7cW/view?usp=sharing</t>
+  </si>
+  <si>
+    <t>Survey of Health, Ageing and Retirement in Europe</t>
+  </si>
+  <si>
+    <t>http://www.share-project.org/data-documentation/share-data-releases.html</t>
+  </si>
+  <si>
+    <t>Life in Transition Survey</t>
+  </si>
+  <si>
+    <t>http://www.ebrd.com/what-we-do/economic-research-and-data/data/lits.html</t>
+  </si>
+  <si>
+    <t>Central and Eastern Europe</t>
+  </si>
+  <si>
+    <t>http://www.ebrd.com/cs/Satellite?c=Content&amp;cid=1395256887325&amp;d=&amp;pagename=EBRD%2FContent%2FDownloadDocument</t>
+  </si>
+  <si>
+    <t>http://www.ebrd.com/cs/Satellite?c=Content&amp;cid=1395256887465&amp;d=&amp;pagename=EBRD%2FContent%2FDownloadDocument</t>
+  </si>
+  <si>
+    <t>links are to LiTS III</t>
   </si>
 </sst>
 </file>
@@ -1722,10 +1746,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q158"/>
+  <dimension ref="A1:Q160"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A137" workbookViewId="0">
-      <selection activeCell="B159" sqref="B159"/>
+    <sheetView tabSelected="1" topLeftCell="A139" workbookViewId="0">
+      <selection activeCell="A160" sqref="A160"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3608,68 +3632,80 @@
     </row>
     <row r="93" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>11</v>
+        <v>454</v>
       </c>
       <c r="B93" t="s">
         <v>25</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D93" t="s">
-        <v>95</v>
+        <v>455</v>
       </c>
       <c r="E93" t="s">
-        <v>10</v>
+        <v>456</v>
       </c>
       <c r="F93">
-        <v>2007</v>
+        <v>2006</v>
+      </c>
+      <c r="G93">
+        <v>2016</v>
       </c>
       <c r="H93" t="s">
-        <v>16</v>
+        <v>348</v>
       </c>
       <c r="I93" t="s">
-        <v>21</v>
+        <v>349</v>
+      </c>
+      <c r="J93" s="2" t="s">
+        <v>457</v>
+      </c>
+      <c r="L93" s="2" t="s">
+        <v>458</v>
+      </c>
+      <c r="Q93" t="s">
+        <v>459</v>
       </c>
     </row>
     <row r="94" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>223</v>
+        <v>11</v>
       </c>
       <c r="B94" t="s">
-        <v>124</v>
+        <v>25</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>222</v>
+        <v>12</v>
+      </c>
+      <c r="D94" t="s">
+        <v>95</v>
+      </c>
+      <c r="E94" t="s">
+        <v>10</v>
       </c>
       <c r="F94">
-        <v>1</v>
-      </c>
-      <c r="G94">
-        <v>2010</v>
+        <v>2007</v>
       </c>
       <c r="H94" t="s">
         <v>16</v>
       </c>
       <c r="I94" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="95" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="B95" t="s">
-        <v>40</v>
+        <v>124</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="F95">
-        <v>1946</v>
+        <v>1</v>
       </c>
       <c r="G95">
-        <v>2016</v>
+        <v>2010</v>
       </c>
       <c r="H95" t="s">
         <v>16</v>
@@ -3680,122 +3716,122 @@
     </row>
     <row r="96" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>97</v>
+        <v>226</v>
       </c>
       <c r="B96" t="s">
-        <v>128</v>
+        <v>40</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>98</v>
+        <v>225</v>
+      </c>
+      <c r="F96">
+        <v>1946</v>
+      </c>
+      <c r="G96">
+        <v>2016</v>
+      </c>
+      <c r="H96" t="s">
+        <v>16</v>
+      </c>
+      <c r="I96" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="97" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>278</v>
+        <v>97</v>
       </c>
       <c r="B97" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>279</v>
-      </c>
-      <c r="E97" t="s">
-        <v>280</v>
-      </c>
-      <c r="F97">
-        <v>1890</v>
-      </c>
-      <c r="G97">
-        <v>1996</v>
-      </c>
-      <c r="H97" t="s">
-        <v>16</v>
-      </c>
-      <c r="I97" t="s">
-        <v>20</v>
+        <v>98</v>
       </c>
     </row>
     <row r="98" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>156</v>
+        <v>278</v>
       </c>
       <c r="B98" t="s">
-        <v>25</v>
+        <v>124</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>154</v>
+        <v>279</v>
+      </c>
+      <c r="E98" t="s">
+        <v>280</v>
+      </c>
+      <c r="F98">
+        <v>1890</v>
+      </c>
+      <c r="G98">
+        <v>1996</v>
+      </c>
+      <c r="H98" t="s">
+        <v>16</v>
+      </c>
+      <c r="I98" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="99" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>413</v>
+        <v>156</v>
       </c>
       <c r="B99" t="s">
-        <v>128</v>
+        <v>25</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>414</v>
-      </c>
-      <c r="E99" t="s">
-        <v>415</v>
-      </c>
-      <c r="F99">
-        <v>1946</v>
-      </c>
-      <c r="G99">
-        <v>2014</v>
-      </c>
-      <c r="H99" t="s">
-        <v>348</v>
-      </c>
-      <c r="I99" t="s">
-        <v>349</v>
-      </c>
-      <c r="N99" s="2" t="s">
-        <v>416</v>
-      </c>
-      <c r="Q99" t="s">
-        <v>417</v>
+        <v>154</v>
       </c>
     </row>
     <row r="100" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>229</v>
+        <v>413</v>
       </c>
       <c r="B100" t="s">
-        <v>40</v>
+        <v>128</v>
       </c>
       <c r="C100" s="2" t="s">
-        <v>225</v>
+        <v>414</v>
+      </c>
+      <c r="E100" t="s">
+        <v>415</v>
       </c>
       <c r="F100">
-        <v>1952</v>
+        <v>1946</v>
       </c>
       <c r="G100">
-        <v>1997</v>
+        <v>2014</v>
       </c>
       <c r="H100" t="s">
-        <v>16</v>
+        <v>348</v>
       </c>
       <c r="I100" t="s">
-        <v>20</v>
+        <v>349</v>
+      </c>
+      <c r="N100" s="2" t="s">
+        <v>416</v>
+      </c>
+      <c r="Q100" t="s">
+        <v>417</v>
       </c>
     </row>
     <row r="101" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>293</v>
+        <v>229</v>
       </c>
       <c r="B101" t="s">
         <v>40</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>294</v>
+        <v>225</v>
       </c>
       <c r="F101">
-        <v>2004</v>
+        <v>1952</v>
       </c>
       <c r="G101">
-        <v>2006</v>
+        <v>1997</v>
       </c>
       <c r="H101" t="s">
         <v>16</v>
@@ -3806,221 +3842,218 @@
     </row>
     <row r="102" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>102</v>
+        <v>293</v>
       </c>
       <c r="B102" t="s">
-        <v>99</v>
+        <v>40</v>
       </c>
       <c r="C102" s="2" t="s">
-        <v>103</v>
+        <v>294</v>
+      </c>
+      <c r="F102">
+        <v>2004</v>
+      </c>
+      <c r="G102">
+        <v>2006</v>
+      </c>
+      <c r="H102" t="s">
+        <v>16</v>
+      </c>
+      <c r="I102" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="103" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>289</v>
+        <v>102</v>
       </c>
       <c r="B103" t="s">
-        <v>124</v>
+        <v>99</v>
       </c>
       <c r="C103" s="2" t="s">
-        <v>290</v>
+        <v>103</v>
       </c>
     </row>
     <row r="104" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>246</v>
+        <v>289</v>
       </c>
       <c r="B104" t="s">
-        <v>165</v>
+        <v>124</v>
       </c>
       <c r="C104" s="2" t="s">
-        <v>247</v>
-      </c>
-      <c r="E104" t="s">
-        <v>14</v>
-      </c>
-      <c r="F104">
-        <v>1960</v>
-      </c>
-      <c r="G104">
-        <v>2006</v>
-      </c>
-      <c r="H104" t="s">
-        <v>16</v>
-      </c>
-      <c r="I104" t="s">
-        <v>249</v>
+        <v>290</v>
       </c>
     </row>
     <row r="105" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>365</v>
+        <v>246</v>
       </c>
       <c r="B105" t="s">
-        <v>128</v>
+        <v>165</v>
       </c>
       <c r="C105" s="2" t="s">
-        <v>364</v>
-      </c>
-      <c r="D105" t="s">
-        <v>370</v>
+        <v>247</v>
       </c>
       <c r="E105" t="s">
-        <v>366</v>
+        <v>14</v>
       </c>
       <c r="F105">
-        <v>1906</v>
+        <v>1960</v>
       </c>
       <c r="G105">
-        <v>2013</v>
+        <v>2006</v>
       </c>
       <c r="H105" t="s">
-        <v>367</v>
+        <v>16</v>
       </c>
       <c r="I105" t="s">
-        <v>368</v>
-      </c>
-      <c r="Q105" t="s">
-        <v>369</v>
+        <v>249</v>
       </c>
     </row>
     <row r="106" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>208</v>
+        <v>365</v>
       </c>
       <c r="B106" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="C106" s="2" t="s">
-        <v>209</v>
+        <v>364</v>
+      </c>
+      <c r="D106" t="s">
+        <v>370</v>
+      </c>
+      <c r="E106" t="s">
+        <v>366</v>
       </c>
       <c r="F106">
-        <v>1932</v>
+        <v>1906</v>
       </c>
       <c r="G106">
-        <v>2014</v>
+        <v>2013</v>
       </c>
       <c r="H106" t="s">
-        <v>16</v>
+        <v>367</v>
       </c>
       <c r="I106" t="s">
-        <v>20</v>
+        <v>368</v>
+      </c>
+      <c r="Q106" t="s">
+        <v>369</v>
       </c>
     </row>
     <row r="107" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>137</v>
+        <v>208</v>
       </c>
       <c r="B107" t="s">
-        <v>259</v>
+        <v>124</v>
       </c>
       <c r="C107" s="2" t="s">
-        <v>138</v>
+        <v>209</v>
+      </c>
+      <c r="F107">
+        <v>1932</v>
+      </c>
+      <c r="G107">
+        <v>2014</v>
+      </c>
+      <c r="H107" t="s">
+        <v>16</v>
+      </c>
+      <c r="I107" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="108" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>155</v>
+        <v>137</v>
       </c>
       <c r="B108" t="s">
         <v>259</v>
       </c>
       <c r="C108" s="2" t="s">
-        <v>154</v>
+        <v>138</v>
       </c>
     </row>
     <row r="109" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>57</v>
+        <v>155</v>
       </c>
       <c r="B109" t="s">
-        <v>128</v>
+        <v>259</v>
       </c>
       <c r="C109" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="Q109" t="s">
-        <v>17</v>
+        <v>154</v>
       </c>
     </row>
     <row r="110" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>129</v>
+        <v>57</v>
       </c>
       <c r="B110" t="s">
-        <v>259</v>
+        <v>128</v>
       </c>
       <c r="C110" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="E110" t="s">
-        <v>131</v>
-      </c>
-      <c r="F110">
-        <v>1945</v>
-      </c>
-      <c r="G110">
-        <v>2008</v>
-      </c>
-      <c r="I110" t="s">
-        <v>20</v>
+        <v>58</v>
+      </c>
+      <c r="Q110" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="111" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>148</v>
+        <v>129</v>
       </c>
       <c r="B111" t="s">
-        <v>128</v>
+        <v>259</v>
       </c>
       <c r="C111" s="2" t="s">
-        <v>147</v>
+        <v>130</v>
+      </c>
+      <c r="E111" t="s">
+        <v>131</v>
+      </c>
+      <c r="F111">
+        <v>1945</v>
+      </c>
+      <c r="G111">
+        <v>2008</v>
+      </c>
+      <c r="I111" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="112" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>233</v>
+        <v>148</v>
       </c>
       <c r="B112" t="s">
-        <v>165</v>
+        <v>128</v>
       </c>
       <c r="C112" s="2" t="s">
-        <v>234</v>
-      </c>
-      <c r="E112" t="s">
-        <v>14</v>
-      </c>
-      <c r="F112">
-        <v>2012</v>
-      </c>
-      <c r="G112">
-        <v>2016</v>
-      </c>
-      <c r="H112" t="s">
-        <v>16</v>
-      </c>
-      <c r="I112" t="s">
-        <v>20</v>
+        <v>147</v>
       </c>
     </row>
     <row r="113" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>35</v>
+        <v>233</v>
       </c>
       <c r="B113" t="s">
-        <v>25</v>
+        <v>165</v>
       </c>
       <c r="C113" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="D113" t="s">
-        <v>37</v>
+        <v>234</v>
       </c>
       <c r="E113" t="s">
         <v>14</v>
       </c>
       <c r="F113">
-        <v>2001</v>
+        <v>2012</v>
+      </c>
+      <c r="G113">
+        <v>2016</v>
       </c>
       <c r="H113" t="s">
         <v>16</v>
@@ -4031,119 +4064,119 @@
     </row>
     <row r="114" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>185</v>
+        <v>35</v>
       </c>
       <c r="B114" t="s">
-        <v>128</v>
+        <v>25</v>
       </c>
       <c r="C114" s="2" t="s">
-        <v>186</v>
+        <v>36</v>
+      </c>
+      <c r="D114" t="s">
+        <v>37</v>
+      </c>
+      <c r="E114" t="s">
+        <v>14</v>
+      </c>
+      <c r="F114">
+        <v>2001</v>
+      </c>
+      <c r="H114" t="s">
+        <v>16</v>
+      </c>
+      <c r="I114" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="115" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>210</v>
+        <v>185</v>
       </c>
       <c r="B115" t="s">
-        <v>40</v>
+        <v>128</v>
       </c>
       <c r="C115" s="2" t="s">
-        <v>211</v>
-      </c>
-      <c r="F115">
-        <v>1976</v>
-      </c>
-      <c r="G115">
-        <v>2016</v>
-      </c>
-      <c r="H115" t="s">
-        <v>16</v>
-      </c>
-      <c r="I115" t="s">
-        <v>20</v>
+        <v>186</v>
       </c>
     </row>
     <row r="116" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>426</v>
+        <v>210</v>
       </c>
       <c r="B116" t="s">
-        <v>86</v>
+        <v>40</v>
       </c>
       <c r="C116" s="2" t="s">
-        <v>427</v>
-      </c>
-      <c r="E116" t="s">
-        <v>34</v>
+        <v>211</v>
       </c>
       <c r="F116">
-        <v>2015</v>
+        <v>1976</v>
       </c>
       <c r="G116">
         <v>2016</v>
       </c>
       <c r="H116" t="s">
-        <v>348</v>
+        <v>16</v>
       </c>
       <c r="I116" t="s">
-        <v>349</v>
-      </c>
-      <c r="K116" s="2" t="s">
-        <v>428</v>
+        <v>20</v>
       </c>
     </row>
     <row r="117" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>144</v>
+        <v>426</v>
       </c>
       <c r="B117" t="s">
-        <v>60</v>
+        <v>86</v>
       </c>
       <c r="C117" s="2" t="s">
-        <v>143</v>
+        <v>427</v>
+      </c>
+      <c r="E117" t="s">
+        <v>34</v>
       </c>
       <c r="F117">
-        <v>1800</v>
+        <v>2015</v>
       </c>
       <c r="G117">
-        <v>2013</v>
+        <v>2016</v>
+      </c>
+      <c r="H117" t="s">
+        <v>348</v>
+      </c>
+      <c r="I117" t="s">
+        <v>349</v>
+      </c>
+      <c r="K117" s="2" t="s">
+        <v>428</v>
       </c>
     </row>
     <row r="118" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>122</v>
+        <v>144</v>
       </c>
       <c r="B118" t="s">
-        <v>259</v>
+        <v>60</v>
       </c>
       <c r="C118" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="I118" t="s">
-        <v>20</v>
+        <v>143</v>
+      </c>
+      <c r="F118">
+        <v>1800</v>
+      </c>
+      <c r="G118">
+        <v>2013</v>
       </c>
     </row>
     <row r="119" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>318</v>
+        <v>122</v>
       </c>
       <c r="B119" t="s">
-        <v>250</v>
+        <v>259</v>
       </c>
       <c r="C119" s="2" t="s">
-        <v>319</v>
-      </c>
-      <c r="E119" t="s">
-        <v>320</v>
-      </c>
-      <c r="F119">
-        <v>1975</v>
-      </c>
-      <c r="G119">
-        <v>1989</v>
-      </c>
-      <c r="H119" t="s">
-        <v>16</v>
+        <v>121</v>
       </c>
       <c r="I119" t="s">
         <v>20</v>
@@ -4151,22 +4184,22 @@
     </row>
     <row r="120" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="B120" t="s">
         <v>250</v>
       </c>
       <c r="C120" s="2" t="s">
-        <v>317</v>
+        <v>319</v>
       </c>
       <c r="E120" t="s">
-        <v>105</v>
+        <v>320</v>
       </c>
       <c r="F120">
-        <v>1950</v>
+        <v>1975</v>
       </c>
       <c r="G120">
-        <v>1996</v>
+        <v>1989</v>
       </c>
       <c r="H120" t="s">
         <v>16</v>
@@ -4177,19 +4210,22 @@
     </row>
     <row r="121" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>322</v>
+        <v>316</v>
       </c>
       <c r="B121" t="s">
-        <v>25</v>
+        <v>250</v>
       </c>
       <c r="C121" s="2" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="E121" t="s">
-        <v>77</v>
+        <v>105</v>
       </c>
       <c r="F121">
-        <v>2010</v>
+        <v>1950</v>
+      </c>
+      <c r="G121">
+        <v>1996</v>
       </c>
       <c r="H121" t="s">
         <v>16</v>
@@ -4200,121 +4236,118 @@
     </row>
     <row r="122" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>141</v>
+        <v>322</v>
       </c>
       <c r="B122" t="s">
-        <v>237</v>
+        <v>25</v>
       </c>
       <c r="C122" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="Q122" t="s">
-        <v>17</v>
+        <v>321</v>
+      </c>
+      <c r="E122" t="s">
+        <v>77</v>
+      </c>
+      <c r="F122">
+        <v>2010</v>
+      </c>
+      <c r="H122" t="s">
+        <v>16</v>
+      </c>
+      <c r="I122" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="123" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>308</v>
+        <v>141</v>
       </c>
       <c r="B123" t="s">
-        <v>250</v>
+        <v>237</v>
       </c>
       <c r="C123" s="2" t="s">
-        <v>309</v>
-      </c>
-      <c r="E123" t="s">
-        <v>310</v>
-      </c>
-      <c r="F123">
-        <v>1950</v>
-      </c>
-      <c r="G123">
-        <v>2010</v>
-      </c>
-      <c r="H123" t="s">
-        <v>16</v>
-      </c>
-      <c r="I123" t="s">
-        <v>20</v>
+        <v>142</v>
+      </c>
+      <c r="Q123" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="124" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>287</v>
+        <v>308</v>
       </c>
       <c r="B124" t="s">
-        <v>134</v>
+        <v>250</v>
       </c>
       <c r="C124" s="2" t="s">
-        <v>288</v>
+        <v>309</v>
+      </c>
+      <c r="E124" t="s">
+        <v>310</v>
       </c>
       <c r="F124">
-        <v>1990</v>
+        <v>1950</v>
       </c>
       <c r="G124">
-        <v>2008</v>
+        <v>2010</v>
+      </c>
+      <c r="H124" t="s">
+        <v>16</v>
+      </c>
+      <c r="I124" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="125" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>274</v>
+        <v>287</v>
       </c>
       <c r="B125" t="s">
-        <v>55</v>
+        <v>134</v>
       </c>
       <c r="C125" s="2" t="s">
-        <v>275</v>
-      </c>
-      <c r="H125" t="s">
-        <v>16</v>
-      </c>
-      <c r="I125" t="s">
-        <v>20</v>
+        <v>288</v>
+      </c>
+      <c r="F125">
+        <v>1990</v>
+      </c>
+      <c r="G125">
+        <v>2008</v>
       </c>
     </row>
     <row r="126" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>157</v>
+        <v>274</v>
       </c>
       <c r="B126" t="s">
-        <v>128</v>
+        <v>55</v>
       </c>
       <c r="C126" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="Q126" t="s">
-        <v>18</v>
+        <v>275</v>
+      </c>
+      <c r="H126" t="s">
+        <v>16</v>
+      </c>
+      <c r="I126" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="127" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>439</v>
+        <v>157</v>
       </c>
       <c r="B127" t="s">
-        <v>259</v>
+        <v>128</v>
       </c>
       <c r="C127" s="2" t="s">
-        <v>438</v>
-      </c>
-      <c r="H127" t="s">
-        <v>348</v>
-      </c>
-      <c r="I127" t="s">
-        <v>349</v>
-      </c>
-      <c r="J127" s="2" t="s">
-        <v>440</v>
-      </c>
-      <c r="K127" s="2" t="s">
-        <v>442</v>
-      </c>
-      <c r="L127" s="2" t="s">
-        <v>441</v>
+        <v>154</v>
+      </c>
+      <c r="Q127" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="128" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>443</v>
+        <v>439</v>
       </c>
       <c r="B128" t="s">
         <v>259</v>
@@ -4322,15 +4355,6 @@
       <c r="C128" s="2" t="s">
         <v>438</v>
       </c>
-      <c r="D128" t="s">
-        <v>447</v>
-      </c>
-      <c r="F128">
-        <v>1990</v>
-      </c>
-      <c r="G128">
-        <v>2014</v>
-      </c>
       <c r="H128" t="s">
         <v>348</v>
       </c>
@@ -4338,87 +4362,99 @@
         <v>349</v>
       </c>
       <c r="J128" s="2" t="s">
-        <v>444</v>
+        <v>440</v>
       </c>
       <c r="K128" s="2" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
       <c r="L128" s="2" t="s">
-        <v>446</v>
+        <v>441</v>
       </c>
     </row>
     <row r="129" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>194</v>
+        <v>443</v>
       </c>
       <c r="B129" t="s">
-        <v>99</v>
+        <v>259</v>
       </c>
       <c r="C129" s="2" t="s">
-        <v>193</v>
+        <v>438</v>
+      </c>
+      <c r="D129" t="s">
+        <v>447</v>
+      </c>
+      <c r="F129">
+        <v>1990</v>
+      </c>
+      <c r="G129">
+        <v>2014</v>
+      </c>
+      <c r="H129" t="s">
+        <v>348</v>
+      </c>
+      <c r="I129" t="s">
+        <v>349</v>
+      </c>
+      <c r="J129" s="2" t="s">
+        <v>444</v>
+      </c>
+      <c r="K129" s="2" t="s">
+        <v>445</v>
+      </c>
+      <c r="L129" s="2" t="s">
+        <v>446</v>
       </c>
     </row>
     <row r="130" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
-        <v>295</v>
+        <v>194</v>
       </c>
       <c r="B130" t="s">
-        <v>40</v>
+        <v>99</v>
       </c>
       <c r="C130" s="2" t="s">
-        <v>296</v>
-      </c>
-      <c r="E130" t="s">
-        <v>297</v>
-      </c>
-      <c r="F130">
-        <v>1990</v>
-      </c>
-      <c r="G130">
-        <v>2015</v>
-      </c>
-      <c r="H130" t="s">
-        <v>16</v>
-      </c>
-      <c r="I130" t="s">
-        <v>249</v>
+        <v>193</v>
       </c>
     </row>
     <row r="131" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>256</v>
+        <v>295</v>
       </c>
       <c r="B131" t="s">
-        <v>250</v>
+        <v>40</v>
       </c>
       <c r="C131" s="2" t="s">
-        <v>257</v>
+        <v>296</v>
       </c>
       <c r="E131" t="s">
-        <v>258</v>
+        <v>297</v>
+      </c>
+      <c r="F131">
+        <v>1990</v>
+      </c>
+      <c r="G131">
+        <v>2015</v>
       </c>
       <c r="H131" t="s">
         <v>16</v>
       </c>
       <c r="I131" t="s">
-        <v>20</v>
+        <v>249</v>
       </c>
     </row>
     <row r="132" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>227</v>
+        <v>256</v>
       </c>
       <c r="B132" t="s">
-        <v>40</v>
+        <v>250</v>
       </c>
       <c r="C132" s="2" t="s">
-        <v>225</v>
-      </c>
-      <c r="F132">
-        <v>1955</v>
-      </c>
-      <c r="G132">
-        <v>2016</v>
+        <v>257</v>
+      </c>
+      <c r="E132" t="s">
+        <v>258</v>
       </c>
       <c r="H132" t="s">
         <v>16</v>
@@ -4429,7 +4465,7 @@
     </row>
     <row r="133" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="B133" t="s">
         <v>40</v>
@@ -4438,7 +4474,7 @@
         <v>225</v>
       </c>
       <c r="F133">
-        <v>1995</v>
+        <v>1955</v>
       </c>
       <c r="G133">
         <v>2016</v>
@@ -4452,79 +4488,79 @@
     </row>
     <row r="134" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
-        <v>109</v>
+        <v>230</v>
       </c>
       <c r="B134" t="s">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="C134" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="E134" t="s">
-        <v>111</v>
+        <v>225</v>
       </c>
       <c r="F134">
-        <v>1956</v>
+        <v>1995</v>
+      </c>
+      <c r="G134">
+        <v>2016</v>
+      </c>
+      <c r="H134" t="s">
+        <v>16</v>
+      </c>
+      <c r="I134" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="135" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
-        <v>326</v>
+        <v>452</v>
       </c>
       <c r="B135" t="s">
         <v>25</v>
       </c>
       <c r="C135" s="2" t="s">
-        <v>327</v>
+        <v>453</v>
       </c>
       <c r="E135" t="s">
-        <v>111</v>
-      </c>
-      <c r="F135">
-        <v>1998</v>
+        <v>9</v>
       </c>
       <c r="H135" t="s">
-        <v>16</v>
+        <v>348</v>
       </c>
       <c r="I135" t="s">
-        <v>20</v>
+        <v>435</v>
       </c>
     </row>
     <row r="136" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
-        <v>91</v>
+        <v>109</v>
       </c>
       <c r="B136" t="s">
         <v>25</v>
       </c>
       <c r="C136" s="2" t="s">
-        <v>93</v>
+        <v>110</v>
       </c>
       <c r="E136" t="s">
-        <v>92</v>
+        <v>111</v>
       </c>
       <c r="F136">
-        <v>1999</v>
+        <v>1956</v>
       </c>
     </row>
     <row r="137" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
-        <v>314</v>
+        <v>326</v>
       </c>
       <c r="B137" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="C137" s="2" t="s">
-        <v>313</v>
+        <v>327</v>
       </c>
       <c r="E137" t="s">
-        <v>315</v>
+        <v>111</v>
       </c>
       <c r="F137">
-        <v>1950</v>
-      </c>
-      <c r="G137">
-        <v>2004</v>
+        <v>1998</v>
       </c>
       <c r="H137" t="s">
         <v>16</v>
@@ -4535,122 +4571,110 @@
     </row>
     <row r="138" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
-        <v>161</v>
+        <v>91</v>
       </c>
       <c r="B138" t="s">
         <v>25</v>
       </c>
       <c r="C138" s="2" t="s">
-        <v>160</v>
+        <v>93</v>
+      </c>
+      <c r="E138" t="s">
+        <v>92</v>
+      </c>
+      <c r="F138">
+        <v>1999</v>
       </c>
     </row>
     <row r="139" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
-        <v>168</v>
+        <v>314</v>
       </c>
       <c r="B139" t="s">
         <v>40</v>
       </c>
       <c r="C139" s="2" t="s">
-        <v>167</v>
+        <v>313</v>
+      </c>
+      <c r="E139" t="s">
+        <v>315</v>
+      </c>
+      <c r="F139">
+        <v>1950</v>
+      </c>
+      <c r="G139">
+        <v>2004</v>
+      </c>
+      <c r="H139" t="s">
+        <v>16</v>
+      </c>
+      <c r="I139" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="140" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
-        <v>399</v>
+        <v>161</v>
       </c>
       <c r="B140" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="C140" s="2" t="s">
-        <v>400</v>
-      </c>
-      <c r="E140" t="s">
-        <v>14</v>
-      </c>
-      <c r="F140">
-        <v>2000</v>
-      </c>
-      <c r="G140">
-        <v>2014</v>
-      </c>
-      <c r="H140" t="s">
-        <v>348</v>
-      </c>
-      <c r="I140" t="s">
-        <v>349</v>
-      </c>
-      <c r="J140" s="2" t="s">
-        <v>402</v>
-      </c>
-      <c r="N140" s="2" t="s">
-        <v>401</v>
+        <v>160</v>
       </c>
     </row>
     <row r="141" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
-        <v>213</v>
+        <v>168</v>
       </c>
       <c r="B141" t="s">
-        <v>55</v>
+        <v>40</v>
       </c>
       <c r="C141" s="2" t="s">
-        <v>212</v>
-      </c>
-      <c r="H141" t="s">
-        <v>16</v>
-      </c>
-      <c r="I141" t="s">
-        <v>20</v>
+        <v>167</v>
       </c>
     </row>
     <row r="142" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
-        <v>395</v>
+        <v>399</v>
       </c>
       <c r="B142" t="s">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="C142" s="2" t="s">
-        <v>394</v>
-      </c>
-      <c r="D142" t="s">
-        <v>396</v>
+        <v>400</v>
       </c>
       <c r="E142" t="s">
-        <v>111</v>
+        <v>14</v>
       </c>
       <c r="F142">
-        <v>1986</v>
+        <v>2000</v>
       </c>
       <c r="G142">
-        <v>2015</v>
+        <v>2014</v>
       </c>
       <c r="H142" t="s">
-        <v>367</v>
+        <v>348</v>
       </c>
       <c r="I142" t="s">
-        <v>398</v>
+        <v>349</v>
       </c>
       <c r="J142" s="2" t="s">
-        <v>397</v>
+        <v>402</v>
+      </c>
+      <c r="N142" s="2" t="s">
+        <v>401</v>
       </c>
     </row>
     <row r="143" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
-        <v>323</v>
+        <v>213</v>
       </c>
       <c r="B143" t="s">
-        <v>25</v>
+        <v>55</v>
       </c>
       <c r="C143" s="2" t="s">
-        <v>324</v>
-      </c>
-      <c r="E143" t="s">
-        <v>325</v>
-      </c>
-      <c r="F143">
-        <v>1942</v>
+        <v>212</v>
       </c>
       <c r="H143" t="s">
         <v>16</v>
@@ -4661,124 +4685,145 @@
     </row>
     <row r="144" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
-        <v>273</v>
+        <v>395</v>
       </c>
       <c r="B144" t="s">
-        <v>237</v>
+        <v>25</v>
       </c>
       <c r="C144" s="2" t="s">
-        <v>272</v>
+        <v>394</v>
+      </c>
+      <c r="D144" t="s">
+        <v>396</v>
+      </c>
+      <c r="E144" t="s">
+        <v>111</v>
       </c>
       <c r="F144">
-        <v>1996</v>
+        <v>1986</v>
       </c>
       <c r="G144">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="H144" t="s">
-        <v>16</v>
+        <v>367</v>
       </c>
       <c r="I144" t="s">
-        <v>20</v>
+        <v>398</v>
+      </c>
+      <c r="J144" s="2" t="s">
+        <v>397</v>
       </c>
     </row>
     <row r="145" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
-        <v>66</v>
+        <v>323</v>
       </c>
       <c r="B145" t="s">
         <v>25</v>
       </c>
       <c r="C145" s="2" t="s">
-        <v>67</v>
+        <v>324</v>
+      </c>
+      <c r="E145" t="s">
+        <v>325</v>
+      </c>
+      <c r="F145">
+        <v>1942</v>
+      </c>
+      <c r="H145" t="s">
+        <v>16</v>
+      </c>
+      <c r="I145" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="146" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
-        <v>383</v>
+        <v>273</v>
       </c>
       <c r="B146" t="s">
-        <v>40</v>
+        <v>237</v>
       </c>
       <c r="C146" s="2" t="s">
-        <v>384</v>
-      </c>
-      <c r="E146" t="s">
-        <v>386</v>
+        <v>272</v>
       </c>
       <c r="F146">
-        <v>1951</v>
+        <v>1996</v>
+      </c>
+      <c r="G146">
+        <v>2016</v>
       </c>
       <c r="H146" t="s">
-        <v>348</v>
+        <v>16</v>
       </c>
       <c r="I146" t="s">
-        <v>349</v>
-      </c>
-      <c r="N146" s="2" t="s">
-        <v>385</v>
+        <v>20</v>
       </c>
     </row>
     <row r="147" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
-        <v>139</v>
+        <v>66</v>
       </c>
       <c r="B147" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="C147" s="2" t="s">
-        <v>140</v>
+        <v>67</v>
       </c>
     </row>
     <row r="148" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
-        <v>329</v>
+        <v>383</v>
       </c>
       <c r="B148" t="s">
-        <v>165</v>
+        <v>40</v>
       </c>
       <c r="C148" s="2" t="s">
-        <v>328</v>
+        <v>384</v>
       </c>
       <c r="E148" t="s">
-        <v>34</v>
+        <v>386</v>
       </c>
       <c r="F148">
-        <v>1789</v>
+        <v>1951</v>
       </c>
       <c r="H148" t="s">
-        <v>16</v>
+        <v>348</v>
       </c>
       <c r="I148" t="s">
-        <v>20</v>
+        <v>349</v>
+      </c>
+      <c r="N148" s="2" t="s">
+        <v>385</v>
       </c>
     </row>
     <row r="149" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
-        <v>172</v>
+        <v>139</v>
       </c>
       <c r="B149" t="s">
-        <v>60</v>
+        <v>40</v>
       </c>
       <c r="C149" s="2" t="s">
-        <v>171</v>
+        <v>140</v>
       </c>
     </row>
     <row r="150" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
-        <v>217</v>
+        <v>329</v>
       </c>
       <c r="B150" t="s">
-        <v>60</v>
+        <v>165</v>
       </c>
       <c r="C150" s="2" t="s">
-        <v>216</v>
+        <v>328</v>
       </c>
       <c r="E150" t="s">
-        <v>14</v>
+        <v>34</v>
       </c>
       <c r="F150">
-        <v>1900</v>
+        <v>1789</v>
       </c>
       <c r="H150" t="s">
         <v>16</v>
@@ -4789,130 +4834,118 @@
     </row>
     <row r="151" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
-        <v>132</v>
+        <v>172</v>
       </c>
       <c r="B151" t="s">
-        <v>259</v>
+        <v>60</v>
       </c>
       <c r="C151" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="Q151" t="s">
-        <v>17</v>
+        <v>171</v>
       </c>
     </row>
     <row r="152" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
-        <v>182</v>
+        <v>217</v>
       </c>
       <c r="B152" t="s">
-        <v>165</v>
+        <v>60</v>
       </c>
       <c r="C152" s="2" t="s">
-        <v>181</v>
+        <v>216</v>
+      </c>
+      <c r="E152" t="s">
+        <v>14</v>
+      </c>
+      <c r="F152">
+        <v>1900</v>
+      </c>
+      <c r="H152" t="s">
+        <v>16</v>
+      </c>
+      <c r="I152" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="153" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
-        <v>423</v>
+        <v>132</v>
       </c>
       <c r="B153" t="s">
-        <v>86</v>
+        <v>259</v>
       </c>
       <c r="C153" s="2" t="s">
-        <v>424</v>
-      </c>
-      <c r="E153" t="s">
-        <v>34</v>
-      </c>
-      <c r="F153">
-        <v>1996</v>
-      </c>
-      <c r="G153">
-        <v>2016</v>
-      </c>
-      <c r="H153" t="s">
-        <v>348</v>
-      </c>
-      <c r="I153" t="s">
-        <v>425</v>
+        <v>133</v>
+      </c>
+      <c r="Q153" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="154" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
-        <v>115</v>
+        <v>182</v>
       </c>
       <c r="B154" t="s">
-        <v>128</v>
+        <v>165</v>
       </c>
       <c r="C154" s="2" t="s">
-        <v>116</v>
+        <v>181</v>
       </c>
     </row>
     <row r="155" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
-        <v>263</v>
+        <v>423</v>
       </c>
       <c r="B155" t="s">
-        <v>250</v>
+        <v>86</v>
       </c>
       <c r="C155" s="2" t="s">
-        <v>264</v>
+        <v>424</v>
       </c>
       <c r="E155" t="s">
-        <v>265</v>
+        <v>34</v>
       </c>
       <c r="F155">
-        <v>1500</v>
+        <v>1996</v>
       </c>
       <c r="G155">
-        <v>2000</v>
+        <v>2016</v>
       </c>
       <c r="H155" t="s">
-        <v>16</v>
+        <v>348</v>
       </c>
       <c r="I155" t="s">
-        <v>20</v>
+        <v>425</v>
       </c>
     </row>
     <row r="156" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
-        <v>221</v>
+        <v>115</v>
       </c>
       <c r="B156" t="s">
-        <v>86</v>
+        <v>128</v>
       </c>
       <c r="C156" s="2" t="s">
-        <v>220</v>
-      </c>
-      <c r="F156">
-        <v>2013</v>
-      </c>
-      <c r="H156" t="s">
-        <v>16</v>
-      </c>
-      <c r="I156" t="s">
-        <v>20</v>
+        <v>116</v>
       </c>
     </row>
     <row r="157" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
-        <v>13</v>
+        <v>263</v>
       </c>
       <c r="B157" t="s">
-        <v>25</v>
+        <v>250</v>
       </c>
       <c r="C157" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="D157" s="1" t="s">
-        <v>42</v>
+        <v>264</v>
       </c>
       <c r="E157" t="s">
-        <v>14</v>
+        <v>265</v>
       </c>
       <c r="F157">
-        <v>1981</v>
+        <v>1500</v>
+      </c>
+      <c r="G157">
+        <v>2000</v>
       </c>
       <c r="H157" t="s">
         <v>16</v>
@@ -4923,23 +4956,69 @@
     </row>
     <row r="158" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
+        <v>221</v>
+      </c>
+      <c r="B158" t="s">
+        <v>86</v>
+      </c>
+      <c r="C158" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="F158">
+        <v>2013</v>
+      </c>
+      <c r="H158" t="s">
+        <v>16</v>
+      </c>
+      <c r="I158" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="159" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A159" t="s">
+        <v>13</v>
+      </c>
+      <c r="B159" t="s">
+        <v>25</v>
+      </c>
+      <c r="C159" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D159" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E159" t="s">
+        <v>14</v>
+      </c>
+      <c r="F159">
+        <v>1981</v>
+      </c>
+      <c r="H159" t="s">
+        <v>16</v>
+      </c>
+      <c r="I159" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="160" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A160" t="s">
         <v>283</v>
       </c>
-      <c r="B158" t="s">
+      <c r="B160" t="s">
         <v>124</v>
       </c>
-      <c r="C158" s="2" t="s">
+      <c r="C160" s="2" t="s">
         <v>284</v>
       </c>
-      <c r="H158" t="s">
-        <v>16</v>
-      </c>
-      <c r="I158" t="s">
+      <c r="H160" t="s">
+        <v>16</v>
+      </c>
+      <c r="I160" t="s">
         <v>20</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:Q158">
+  <sortState ref="A2:Q160">
     <sortCondition ref="A2"/>
   </sortState>
   <hyperlinks>
@@ -4947,9 +5026,9 @@
     <hyperlink ref="C58" r:id="rId2"/>
     <hyperlink ref="C7" r:id="rId3"/>
     <hyperlink ref="C10" r:id="rId4"/>
-    <hyperlink ref="C93" r:id="rId5"/>
-    <hyperlink ref="C113" r:id="rId6"/>
-    <hyperlink ref="C157" r:id="rId7"/>
+    <hyperlink ref="C94" r:id="rId5"/>
+    <hyperlink ref="C114" r:id="rId6"/>
+    <hyperlink ref="C159" r:id="rId7"/>
     <hyperlink ref="C35" r:id="rId8"/>
     <hyperlink ref="C30" r:id="rId9"/>
     <hyperlink ref="C49" r:id="rId10"/>
@@ -4959,11 +5038,11 @@
     <hyperlink ref="C60" r:id="rId14"/>
     <hyperlink ref="C86" r:id="rId15"/>
     <hyperlink ref="C29" r:id="rId16"/>
-    <hyperlink ref="C109" r:id="rId17"/>
+    <hyperlink ref="C110" r:id="rId17"/>
     <hyperlink ref="C41" r:id="rId18"/>
     <hyperlink ref="C71" r:id="rId19"/>
     <hyperlink ref="C16" r:id="rId20"/>
-    <hyperlink ref="C145" r:id="rId21"/>
+    <hyperlink ref="C147" r:id="rId21"/>
     <hyperlink ref="C8" r:id="rId22"/>
     <hyperlink ref="C38" r:id="rId23"/>
     <hyperlink ref="C53" r:id="rId24"/>
@@ -4972,75 +5051,75 @@
     <hyperlink ref="C55" r:id="rId27"/>
     <hyperlink ref="C69" r:id="rId28"/>
     <hyperlink ref="C91" r:id="rId29"/>
-    <hyperlink ref="C136" r:id="rId30"/>
-    <hyperlink ref="C96" r:id="rId31"/>
+    <hyperlink ref="C138" r:id="rId30"/>
+    <hyperlink ref="C97" r:id="rId31"/>
     <hyperlink ref="C81" r:id="rId32"/>
-    <hyperlink ref="C102" r:id="rId33"/>
+    <hyperlink ref="C103" r:id="rId33"/>
     <hyperlink ref="C70" r:id="rId34"/>
     <hyperlink ref="C17" r:id="rId35"/>
-    <hyperlink ref="C134" r:id="rId36"/>
+    <hyperlink ref="C136" r:id="rId36"/>
     <hyperlink ref="C15" r:id="rId37"/>
-    <hyperlink ref="C154" r:id="rId38"/>
+    <hyperlink ref="C156" r:id="rId38"/>
     <hyperlink ref="C85" r:id="rId39"/>
     <hyperlink ref="C57" r:id="rId40"/>
-    <hyperlink ref="C118" r:id="rId41"/>
+    <hyperlink ref="C119" r:id="rId41"/>
     <hyperlink ref="C18" r:id="rId42"/>
     <hyperlink ref="C51" r:id="rId43"/>
     <hyperlink ref="C23" r:id="rId44"/>
-    <hyperlink ref="C110" r:id="rId45"/>
-    <hyperlink ref="C151" r:id="rId46"/>
+    <hyperlink ref="C111" r:id="rId45"/>
+    <hyperlink ref="C153" r:id="rId46"/>
     <hyperlink ref="C27" r:id="rId47" display="http://comparativeconstitutionsproject.org/"/>
-    <hyperlink ref="C107" r:id="rId48"/>
-    <hyperlink ref="C147" r:id="rId49"/>
-    <hyperlink ref="C122" r:id="rId50"/>
-    <hyperlink ref="C117" r:id="rId51"/>
+    <hyperlink ref="C108" r:id="rId48"/>
+    <hyperlink ref="C149" r:id="rId49"/>
+    <hyperlink ref="C123" r:id="rId50"/>
+    <hyperlink ref="C118" r:id="rId51"/>
     <hyperlink ref="C22" r:id="rId52"/>
-    <hyperlink ref="C111" r:id="rId53"/>
+    <hyperlink ref="C112" r:id="rId53"/>
     <hyperlink ref="C48" r:id="rId54"/>
     <hyperlink ref="C75" r:id="rId55"/>
     <hyperlink ref="C78" r:id="rId56"/>
-    <hyperlink ref="C108" r:id="rId57"/>
-    <hyperlink ref="C98" r:id="rId58"/>
-    <hyperlink ref="C126" r:id="rId59"/>
+    <hyperlink ref="C109" r:id="rId57"/>
+    <hyperlink ref="C99" r:id="rId58"/>
+    <hyperlink ref="C127" r:id="rId59"/>
     <hyperlink ref="C31" r:id="rId60"/>
-    <hyperlink ref="C138" r:id="rId61"/>
+    <hyperlink ref="C140" r:id="rId61"/>
     <hyperlink ref="C9" r:id="rId62"/>
     <hyperlink ref="C33" r:id="rId63"/>
-    <hyperlink ref="C139" r:id="rId64"/>
+    <hyperlink ref="C141" r:id="rId64"/>
     <hyperlink ref="C14" r:id="rId65"/>
-    <hyperlink ref="C149" r:id="rId66"/>
+    <hyperlink ref="C151" r:id="rId66"/>
     <hyperlink ref="C25" r:id="rId67"/>
     <hyperlink ref="C24" r:id="rId68"/>
     <hyperlink ref="C26" r:id="rId69"/>
     <hyperlink ref="C52" r:id="rId70"/>
-    <hyperlink ref="C152" r:id="rId71"/>
+    <hyperlink ref="C154" r:id="rId71"/>
     <hyperlink ref="C28" r:id="rId72"/>
-    <hyperlink ref="C114" r:id="rId73"/>
+    <hyperlink ref="C115" r:id="rId73"/>
     <hyperlink ref="C32" r:id="rId74"/>
     <hyperlink ref="C45" r:id="rId75"/>
-    <hyperlink ref="C129" r:id="rId76"/>
+    <hyperlink ref="C130" r:id="rId76"/>
     <hyperlink ref="C42" r:id="rId77"/>
     <hyperlink ref="C39" r:id="rId78"/>
     <hyperlink ref="C68" r:id="rId79"/>
     <hyperlink ref="C5" r:id="rId80"/>
     <hyperlink ref="C67" r:id="rId81"/>
     <hyperlink ref="C12" r:id="rId82"/>
-    <hyperlink ref="C106" r:id="rId83"/>
-    <hyperlink ref="C115" r:id="rId84"/>
-    <hyperlink ref="C141" r:id="rId85"/>
+    <hyperlink ref="C107" r:id="rId83"/>
+    <hyperlink ref="C116" r:id="rId84"/>
+    <hyperlink ref="C143" r:id="rId85"/>
     <hyperlink ref="C36" r:id="rId86"/>
-    <hyperlink ref="C150" r:id="rId87"/>
+    <hyperlink ref="C152" r:id="rId87"/>
     <hyperlink ref="C44" r:id="rId88"/>
-    <hyperlink ref="C156" r:id="rId89"/>
-    <hyperlink ref="C94" r:id="rId90"/>
+    <hyperlink ref="C158" r:id="rId89"/>
+    <hyperlink ref="C95" r:id="rId90"/>
     <hyperlink ref="C65" r:id="rId91"/>
-    <hyperlink ref="C95" r:id="rId92"/>
-    <hyperlink ref="C132" r:id="rId93"/>
+    <hyperlink ref="C96" r:id="rId92"/>
+    <hyperlink ref="C133" r:id="rId93"/>
     <hyperlink ref="C79" r:id="rId94"/>
-    <hyperlink ref="C100" r:id="rId95"/>
-    <hyperlink ref="C133" r:id="rId96"/>
+    <hyperlink ref="C101" r:id="rId95"/>
+    <hyperlink ref="C134" r:id="rId96"/>
     <hyperlink ref="C61" r:id="rId97"/>
-    <hyperlink ref="C112" r:id="rId98"/>
+    <hyperlink ref="C113" r:id="rId98"/>
     <hyperlink ref="C46" r:id="rId99"/>
     <hyperlink ref="C43" r:id="rId100"/>
     <hyperlink ref="C82" r:id="rId101"/>
@@ -5048,39 +5127,39 @@
     <hyperlink ref="C2" r:id="rId103"/>
     <hyperlink ref="C76" r:id="rId104"/>
     <hyperlink ref="C80" r:id="rId105"/>
-    <hyperlink ref="C104" r:id="rId106"/>
+    <hyperlink ref="C105" r:id="rId106"/>
     <hyperlink ref="C47" r:id="rId107"/>
     <hyperlink ref="C83" r:id="rId108"/>
-    <hyperlink ref="C131" r:id="rId109"/>
+    <hyperlink ref="C132" r:id="rId109"/>
     <hyperlink ref="C13" r:id="rId110"/>
     <hyperlink ref="C4" r:id="rId111"/>
-    <hyperlink ref="C155" r:id="rId112"/>
+    <hyperlink ref="C157" r:id="rId112"/>
     <hyperlink ref="C89" r:id="rId113"/>
     <hyperlink ref="C84" r:id="rId114"/>
-    <hyperlink ref="C144" r:id="rId115"/>
-    <hyperlink ref="C125" r:id="rId116"/>
+    <hyperlink ref="C146" r:id="rId115"/>
+    <hyperlink ref="C126" r:id="rId116"/>
     <hyperlink ref="C63" r:id="rId117"/>
-    <hyperlink ref="C97" r:id="rId118"/>
+    <hyperlink ref="C98" r:id="rId118"/>
     <hyperlink ref="C73" r:id="rId119"/>
-    <hyperlink ref="C158" r:id="rId120"/>
+    <hyperlink ref="C160" r:id="rId120"/>
     <hyperlink ref="C66" r:id="rId121"/>
-    <hyperlink ref="C124" r:id="rId122"/>
-    <hyperlink ref="C103" r:id="rId123"/>
+    <hyperlink ref="C125" r:id="rId122"/>
+    <hyperlink ref="C104" r:id="rId123"/>
     <hyperlink ref="C77" r:id="rId124"/>
-    <hyperlink ref="C101" r:id="rId125"/>
-    <hyperlink ref="C130" r:id="rId126"/>
+    <hyperlink ref="C102" r:id="rId125"/>
+    <hyperlink ref="C131" r:id="rId126"/>
     <hyperlink ref="C87" r:id="rId127"/>
     <hyperlink ref="C11" r:id="rId128"/>
     <hyperlink ref="C19" r:id="rId129"/>
-    <hyperlink ref="C123" r:id="rId130"/>
+    <hyperlink ref="C124" r:id="rId130"/>
     <hyperlink ref="C72" r:id="rId131"/>
-    <hyperlink ref="C137" r:id="rId132"/>
-    <hyperlink ref="C120" r:id="rId133"/>
-    <hyperlink ref="C119" r:id="rId134"/>
-    <hyperlink ref="C121" r:id="rId135"/>
-    <hyperlink ref="C143" r:id="rId136"/>
-    <hyperlink ref="C135" r:id="rId137"/>
-    <hyperlink ref="C148" r:id="rId138"/>
+    <hyperlink ref="C139" r:id="rId132"/>
+    <hyperlink ref="C121" r:id="rId133"/>
+    <hyperlink ref="C120" r:id="rId134"/>
+    <hyperlink ref="C122" r:id="rId135"/>
+    <hyperlink ref="C145" r:id="rId136"/>
+    <hyperlink ref="C137" r:id="rId137"/>
+    <hyperlink ref="C150" r:id="rId138"/>
     <hyperlink ref="C37" r:id="rId139"/>
     <hyperlink ref="C88" r:id="rId140"/>
     <hyperlink ref="J2" r:id="rId141"/>
@@ -5090,49 +5169,53 @@
     <hyperlink ref="J4" r:id="rId145"/>
     <hyperlink ref="P5" r:id="rId146"/>
     <hyperlink ref="J5" r:id="rId147"/>
-    <hyperlink ref="C105" r:id="rId148"/>
+    <hyperlink ref="C106" r:id="rId148"/>
     <hyperlink ref="C34" r:id="rId149"/>
     <hyperlink ref="P7" r:id="rId150"/>
     <hyperlink ref="J7" r:id="rId151"/>
     <hyperlink ref="M8" r:id="rId152"/>
     <hyperlink ref="L8" r:id="rId153"/>
     <hyperlink ref="J8" r:id="rId154"/>
-    <hyperlink ref="C146" r:id="rId155"/>
-    <hyperlink ref="N146" r:id="rId156"/>
+    <hyperlink ref="C148" r:id="rId155"/>
+    <hyperlink ref="N148" r:id="rId156"/>
     <hyperlink ref="C21" r:id="rId157"/>
     <hyperlink ref="N21" r:id="rId158"/>
     <hyperlink ref="C62" r:id="rId159"/>
-    <hyperlink ref="C142" r:id="rId160"/>
-    <hyperlink ref="J142" r:id="rId161"/>
-    <hyperlink ref="C140" r:id="rId162"/>
-    <hyperlink ref="N140" r:id="rId163"/>
-    <hyperlink ref="J140" r:id="rId164"/>
+    <hyperlink ref="C144" r:id="rId160"/>
+    <hyperlink ref="J144" r:id="rId161"/>
+    <hyperlink ref="C142" r:id="rId162"/>
+    <hyperlink ref="N142" r:id="rId163"/>
+    <hyperlink ref="J142" r:id="rId164"/>
     <hyperlink ref="C92" r:id="rId165"/>
     <hyperlink ref="C90" r:id="rId166"/>
     <hyperlink ref="C40" r:id="rId167"/>
     <hyperlink ref="J40" r:id="rId168"/>
     <hyperlink ref="K40" r:id="rId169"/>
-    <hyperlink ref="C99" r:id="rId170"/>
-    <hyperlink ref="N99" r:id="rId171"/>
+    <hyperlink ref="C100" r:id="rId170"/>
+    <hyperlink ref="N100" r:id="rId171"/>
     <hyperlink ref="C74" r:id="rId172"/>
     <hyperlink ref="K74" r:id="rId173"/>
-    <hyperlink ref="C153" r:id="rId174"/>
-    <hyperlink ref="C116" r:id="rId175"/>
-    <hyperlink ref="K116" r:id="rId176"/>
+    <hyperlink ref="C155" r:id="rId174"/>
+    <hyperlink ref="C117" r:id="rId175"/>
+    <hyperlink ref="K117" r:id="rId176"/>
     <hyperlink ref="L9" r:id="rId177"/>
     <hyperlink ref="J9" r:id="rId178"/>
     <hyperlink ref="J10" r:id="rId179"/>
-    <hyperlink ref="C127" r:id="rId180"/>
-    <hyperlink ref="J127" r:id="rId181"/>
-    <hyperlink ref="L127" r:id="rId182"/>
-    <hyperlink ref="K127" r:id="rId183"/>
-    <hyperlink ref="C128" r:id="rId184"/>
-    <hyperlink ref="J128" r:id="rId185"/>
-    <hyperlink ref="K128" r:id="rId186"/>
-    <hyperlink ref="L128" r:id="rId187"/>
+    <hyperlink ref="C128" r:id="rId180"/>
+    <hyperlink ref="J128" r:id="rId181"/>
+    <hyperlink ref="L128" r:id="rId182"/>
+    <hyperlink ref="K128" r:id="rId183"/>
+    <hyperlink ref="C129" r:id="rId184"/>
+    <hyperlink ref="J129" r:id="rId185"/>
+    <hyperlink ref="K129" r:id="rId186"/>
+    <hyperlink ref="L129" r:id="rId187"/>
     <hyperlink ref="C64" r:id="rId188"/>
     <hyperlink ref="J64" r:id="rId189"/>
     <hyperlink ref="N64" r:id="rId190"/>
+    <hyperlink ref="C135" r:id="rId191"/>
+    <hyperlink ref="C93" r:id="rId192"/>
+    <hyperlink ref="J93" r:id="rId193"/>
+    <hyperlink ref="L93" r:id="rId194"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
add 'German Longitudinal Election Study'
</commit_message>
<xml_diff>
--- a/PolData.xlsx
+++ b/PolData.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="834" uniqueCount="460">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="841" uniqueCount="462">
   <si>
     <t>name</t>
   </si>
@@ -1407,6 +1407,12 @@
   </si>
   <si>
     <t>links are to LiTS III</t>
+  </si>
+  <si>
+    <t>German Longitudinal Election Study</t>
+  </si>
+  <si>
+    <t>https://www.gesis.org/en/elections-home/gles/data/</t>
   </si>
 </sst>
 </file>
@@ -1746,10 +1752,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q160"/>
+  <dimension ref="A1:Q161"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A139" workbookViewId="0">
-      <selection activeCell="A160" sqref="A160"/>
+    <sheetView tabSelected="1" topLeftCell="A146" workbookViewId="0">
+      <selection activeCell="A71" sqref="A71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3201,124 +3207,133 @@
     </row>
     <row r="71" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>62</v>
+        <v>460</v>
       </c>
       <c r="B71" t="s">
         <v>25</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>63</v>
+        <v>461</v>
+      </c>
+      <c r="D71" t="s">
+        <v>363</v>
+      </c>
+      <c r="E71" t="s">
+        <v>105</v>
+      </c>
+      <c r="F71">
+        <v>2009</v>
+      </c>
+      <c r="H71" t="s">
+        <v>348</v>
+      </c>
+      <c r="I71" t="s">
+        <v>301</v>
       </c>
     </row>
     <row r="72" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>311</v>
+        <v>62</v>
       </c>
       <c r="B72" t="s">
-        <v>165</v>
+        <v>25</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>312</v>
-      </c>
-      <c r="E72" t="s">
-        <v>14</v>
-      </c>
-      <c r="H72" t="s">
-        <v>16</v>
-      </c>
-      <c r="I72" t="s">
-        <v>301</v>
+        <v>63</v>
       </c>
     </row>
     <row r="73" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>281</v>
+        <v>311</v>
       </c>
       <c r="B73" t="s">
-        <v>237</v>
+        <v>165</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>282</v>
+        <v>312</v>
+      </c>
+      <c r="E73" t="s">
+        <v>14</v>
       </c>
       <c r="H73" t="s">
         <v>16</v>
       </c>
       <c r="I73" t="s">
-        <v>20</v>
+        <v>301</v>
       </c>
     </row>
     <row r="74" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>418</v>
+        <v>281</v>
       </c>
       <c r="B74" t="s">
-        <v>86</v>
+        <v>237</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>419</v>
-      </c>
-      <c r="E74" t="s">
-        <v>420</v>
-      </c>
-      <c r="F74">
-        <v>1948</v>
-      </c>
-      <c r="G74">
-        <v>2012</v>
+        <v>282</v>
       </c>
       <c r="H74" t="s">
-        <v>348</v>
+        <v>16</v>
       </c>
       <c r="I74" t="s">
-        <v>349</v>
-      </c>
-      <c r="K74" s="2" t="s">
-        <v>421</v>
-      </c>
-      <c r="Q74" t="s">
-        <v>422</v>
+        <v>20</v>
       </c>
     </row>
     <row r="75" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>151</v>
+        <v>418</v>
       </c>
       <c r="B75" t="s">
-        <v>40</v>
+        <v>86</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>152</v>
+        <v>419</v>
       </c>
       <c r="E75" t="s">
-        <v>14</v>
+        <v>420</v>
+      </c>
+      <c r="F75">
+        <v>1948</v>
+      </c>
+      <c r="G75">
+        <v>2012</v>
+      </c>
+      <c r="H75" t="s">
+        <v>348</v>
+      </c>
+      <c r="I75" t="s">
+        <v>349</v>
+      </c>
+      <c r="K75" s="2" t="s">
+        <v>421</v>
+      </c>
+      <c r="Q75" t="s">
+        <v>422</v>
       </c>
     </row>
     <row r="76" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>242</v>
+        <v>151</v>
       </c>
       <c r="B76" t="s">
-        <v>237</v>
+        <v>40</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>243</v>
-      </c>
-      <c r="H76" t="s">
-        <v>16</v>
-      </c>
-      <c r="I76" t="s">
-        <v>20</v>
+        <v>152</v>
+      </c>
+      <c r="E76" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="77" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>292</v>
+        <v>242</v>
       </c>
       <c r="B77" t="s">
-        <v>99</v>
+        <v>237</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>291</v>
+        <v>243</v>
       </c>
       <c r="H77" t="s">
         <v>16</v>
@@ -3329,47 +3344,47 @@
     </row>
     <row r="78" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>153</v>
+        <v>292</v>
       </c>
       <c r="B78" t="s">
-        <v>259</v>
+        <v>99</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>154</v>
+        <v>291</v>
+      </c>
+      <c r="H78" t="s">
+        <v>16</v>
+      </c>
+      <c r="I78" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="79" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>228</v>
+        <v>153</v>
       </c>
       <c r="B79" t="s">
-        <v>40</v>
+        <v>259</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>225</v>
-      </c>
-      <c r="F79">
-        <v>1989</v>
-      </c>
-      <c r="G79">
-        <v>2017</v>
-      </c>
-      <c r="H79" t="s">
-        <v>16</v>
-      </c>
-      <c r="I79" t="s">
-        <v>20</v>
+        <v>154</v>
       </c>
     </row>
     <row r="80" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>245</v>
+        <v>228</v>
       </c>
       <c r="B80" t="s">
-        <v>237</v>
+        <v>40</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>244</v>
+        <v>225</v>
+      </c>
+      <c r="F80">
+        <v>1989</v>
+      </c>
+      <c r="G80">
+        <v>2017</v>
       </c>
       <c r="H80" t="s">
         <v>16</v>
@@ -3380,50 +3395,41 @@
     </row>
     <row r="81" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>100</v>
+        <v>245</v>
       </c>
       <c r="B81" t="s">
-        <v>99</v>
+        <v>237</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>101</v>
+        <v>244</v>
+      </c>
+      <c r="H81" t="s">
+        <v>16</v>
+      </c>
+      <c r="I81" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="82" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>239</v>
+        <v>100</v>
       </c>
       <c r="B82" t="s">
-        <v>237</v>
+        <v>99</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>243</v>
-      </c>
-      <c r="H82" t="s">
-        <v>16</v>
-      </c>
-      <c r="I82" t="s">
-        <v>20</v>
+        <v>101</v>
       </c>
     </row>
     <row r="83" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>254</v>
+        <v>239</v>
       </c>
       <c r="B83" t="s">
-        <v>55</v>
+        <v>237</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>253</v>
-      </c>
-      <c r="E83" t="s">
-        <v>255</v>
-      </c>
-      <c r="F83">
-        <v>1960</v>
-      </c>
-      <c r="G83">
-        <v>2014</v>
+        <v>243</v>
       </c>
       <c r="H83" t="s">
         <v>16</v>
@@ -3434,19 +3440,22 @@
     </row>
     <row r="84" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>270</v>
+        <v>254</v>
       </c>
       <c r="B84" t="s">
         <v>55</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>271</v>
+        <v>253</v>
+      </c>
+      <c r="E84" t="s">
+        <v>255</v>
       </c>
       <c r="F84">
-        <v>1990</v>
+        <v>1960</v>
       </c>
       <c r="G84">
-        <v>2010</v>
+        <v>2014</v>
       </c>
       <c r="H84" t="s">
         <v>16</v>
@@ -3457,96 +3466,90 @@
     </row>
     <row r="85" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>117</v>
+        <v>270</v>
       </c>
       <c r="B85" t="s">
         <v>55</v>
       </c>
       <c r="C85" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="F85">
+        <v>1990</v>
+      </c>
+      <c r="G85">
+        <v>2010</v>
+      </c>
+      <c r="H85" t="s">
+        <v>16</v>
+      </c>
+      <c r="I85" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="86" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A86" t="s">
+        <v>117</v>
+      </c>
+      <c r="B86" t="s">
+        <v>55</v>
+      </c>
+      <c r="C86" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="I85" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q85" t="s">
+      <c r="I86" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q86" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="86" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A86" s="1" t="s">
+    <row r="87" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A87" s="1" t="s">
         <v>23</v>
-      </c>
-      <c r="B86" t="s">
-        <v>25</v>
-      </c>
-      <c r="C86" s="2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="87" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A87" t="s">
-        <v>300</v>
       </c>
       <c r="B87" t="s">
         <v>25</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>298</v>
-      </c>
-      <c r="E87" t="s">
-        <v>299</v>
-      </c>
-      <c r="F87">
-        <v>1969</v>
-      </c>
-      <c r="H87" t="s">
-        <v>16</v>
-      </c>
-      <c r="I87" t="s">
-        <v>249</v>
+        <v>53</v>
       </c>
     </row>
     <row r="88" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>332</v>
+        <v>300</v>
       </c>
       <c r="B88" t="s">
-        <v>134</v>
+        <v>25</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>333</v>
+        <v>298</v>
       </c>
       <c r="E88" t="s">
-        <v>334</v>
+        <v>299</v>
+      </c>
+      <c r="F88">
+        <v>1969</v>
       </c>
       <c r="H88" t="s">
         <v>16</v>
       </c>
       <c r="I88" t="s">
-        <v>20</v>
+        <v>249</v>
       </c>
     </row>
     <row r="89" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>267</v>
+        <v>332</v>
       </c>
       <c r="B89" t="s">
-        <v>250</v>
+        <v>134</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>266</v>
-      </c>
-      <c r="D89" t="s">
-        <v>269</v>
+        <v>333</v>
       </c>
       <c r="E89" t="s">
-        <v>268</v>
-      </c>
-      <c r="F89">
-        <v>1970</v>
-      </c>
-      <c r="G89">
-        <v>2014</v>
+        <v>334</v>
       </c>
       <c r="H89" t="s">
         <v>16</v>
@@ -3557,97 +3560,100 @@
     </row>
     <row r="90" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>407</v>
+        <v>267</v>
       </c>
       <c r="B90" t="s">
-        <v>40</v>
+        <v>250</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>406</v>
+        <v>266</v>
       </c>
       <c r="D90" t="s">
-        <v>408</v>
+        <v>269</v>
       </c>
       <c r="E90" t="s">
-        <v>14</v>
+        <v>268</v>
       </c>
       <c r="F90">
-        <v>1949</v>
+        <v>1970</v>
       </c>
       <c r="G90">
-        <v>2013</v>
+        <v>2014</v>
       </c>
       <c r="H90" t="s">
-        <v>348</v>
+        <v>16</v>
       </c>
       <c r="I90" t="s">
-        <v>349</v>
+        <v>20</v>
       </c>
     </row>
     <row r="91" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>96</v>
+        <v>407</v>
       </c>
       <c r="B91" t="s">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>90</v>
+        <v>406</v>
+      </c>
+      <c r="D91" t="s">
+        <v>408</v>
       </c>
       <c r="E91" t="s">
-        <v>69</v>
+        <v>14</v>
       </c>
       <c r="F91">
-        <v>1995</v>
+        <v>1949</v>
+      </c>
+      <c r="G91">
+        <v>2013</v>
+      </c>
+      <c r="H91" t="s">
+        <v>348</v>
+      </c>
+      <c r="I91" t="s">
+        <v>349</v>
       </c>
     </row>
     <row r="92" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>404</v>
+        <v>96</v>
       </c>
       <c r="B92" t="s">
-        <v>83</v>
+        <v>25</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>403</v>
-      </c>
-      <c r="D92" t="s">
-        <v>405</v>
+        <v>90</v>
       </c>
       <c r="E92" t="s">
-        <v>14</v>
+        <v>69</v>
       </c>
       <c r="F92">
-        <v>1875</v>
-      </c>
-      <c r="G92">
-        <v>2004</v>
-      </c>
-      <c r="H92" t="s">
-        <v>348</v>
-      </c>
-      <c r="I92" t="s">
-        <v>349</v>
+        <v>1995</v>
       </c>
     </row>
     <row r="93" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>454</v>
+        <v>404</v>
       </c>
       <c r="B93" t="s">
-        <v>25</v>
+        <v>83</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>455</v>
+        <v>403</v>
+      </c>
+      <c r="D93" t="s">
+        <v>405</v>
       </c>
       <c r="E93" t="s">
-        <v>456</v>
+        <v>14</v>
       </c>
       <c r="F93">
-        <v>2006</v>
+        <v>1875</v>
       </c>
       <c r="G93">
-        <v>2016</v>
+        <v>2004</v>
       </c>
       <c r="H93" t="s">
         <v>348</v>
@@ -3655,80 +3661,83 @@
       <c r="I93" t="s">
         <v>349</v>
       </c>
-      <c r="J93" s="2" t="s">
-        <v>457</v>
-      </c>
-      <c r="L93" s="2" t="s">
-        <v>458</v>
-      </c>
-      <c r="Q93" t="s">
-        <v>459</v>
-      </c>
     </row>
     <row r="94" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>11</v>
+        <v>454</v>
       </c>
       <c r="B94" t="s">
         <v>25</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D94" t="s">
-        <v>95</v>
+        <v>455</v>
       </c>
       <c r="E94" t="s">
-        <v>10</v>
+        <v>456</v>
       </c>
       <c r="F94">
-        <v>2007</v>
+        <v>2006</v>
+      </c>
+      <c r="G94">
+        <v>2016</v>
       </c>
       <c r="H94" t="s">
-        <v>16</v>
+        <v>348</v>
       </c>
       <c r="I94" t="s">
-        <v>21</v>
+        <v>349</v>
+      </c>
+      <c r="J94" s="2" t="s">
+        <v>457</v>
+      </c>
+      <c r="L94" s="2" t="s">
+        <v>458</v>
+      </c>
+      <c r="Q94" t="s">
+        <v>459</v>
       </c>
     </row>
     <row r="95" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>223</v>
+        <v>11</v>
       </c>
       <c r="B95" t="s">
-        <v>124</v>
+        <v>25</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>222</v>
+        <v>12</v>
+      </c>
+      <c r="D95" t="s">
+        <v>95</v>
+      </c>
+      <c r="E95" t="s">
+        <v>10</v>
       </c>
       <c r="F95">
-        <v>1</v>
-      </c>
-      <c r="G95">
-        <v>2010</v>
+        <v>2007</v>
       </c>
       <c r="H95" t="s">
         <v>16</v>
       </c>
       <c r="I95" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="96" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="B96" t="s">
-        <v>40</v>
+        <v>124</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="F96">
-        <v>1946</v>
+        <v>1</v>
       </c>
       <c r="G96">
-        <v>2016</v>
+        <v>2010</v>
       </c>
       <c r="H96" t="s">
         <v>16</v>
@@ -3739,122 +3748,122 @@
     </row>
     <row r="97" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>97</v>
+        <v>226</v>
       </c>
       <c r="B97" t="s">
-        <v>128</v>
+        <v>40</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>98</v>
+        <v>225</v>
+      </c>
+      <c r="F97">
+        <v>1946</v>
+      </c>
+      <c r="G97">
+        <v>2016</v>
+      </c>
+      <c r="H97" t="s">
+        <v>16</v>
+      </c>
+      <c r="I97" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="98" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>278</v>
+        <v>97</v>
       </c>
       <c r="B98" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>279</v>
-      </c>
-      <c r="E98" t="s">
-        <v>280</v>
-      </c>
-      <c r="F98">
-        <v>1890</v>
-      </c>
-      <c r="G98">
-        <v>1996</v>
-      </c>
-      <c r="H98" t="s">
-        <v>16</v>
-      </c>
-      <c r="I98" t="s">
-        <v>20</v>
+        <v>98</v>
       </c>
     </row>
     <row r="99" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>156</v>
+        <v>278</v>
       </c>
       <c r="B99" t="s">
-        <v>25</v>
+        <v>124</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>154</v>
+        <v>279</v>
+      </c>
+      <c r="E99" t="s">
+        <v>280</v>
+      </c>
+      <c r="F99">
+        <v>1890</v>
+      </c>
+      <c r="G99">
+        <v>1996</v>
+      </c>
+      <c r="H99" t="s">
+        <v>16</v>
+      </c>
+      <c r="I99" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="100" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>413</v>
+        <v>156</v>
       </c>
       <c r="B100" t="s">
-        <v>128</v>
+        <v>25</v>
       </c>
       <c r="C100" s="2" t="s">
-        <v>414</v>
-      </c>
-      <c r="E100" t="s">
-        <v>415</v>
-      </c>
-      <c r="F100">
-        <v>1946</v>
-      </c>
-      <c r="G100">
-        <v>2014</v>
-      </c>
-      <c r="H100" t="s">
-        <v>348</v>
-      </c>
-      <c r="I100" t="s">
-        <v>349</v>
-      </c>
-      <c r="N100" s="2" t="s">
-        <v>416</v>
-      </c>
-      <c r="Q100" t="s">
-        <v>417</v>
+        <v>154</v>
       </c>
     </row>
     <row r="101" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>229</v>
+        <v>413</v>
       </c>
       <c r="B101" t="s">
-        <v>40</v>
+        <v>128</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>225</v>
+        <v>414</v>
+      </c>
+      <c r="E101" t="s">
+        <v>415</v>
       </c>
       <c r="F101">
-        <v>1952</v>
+        <v>1946</v>
       </c>
       <c r="G101">
-        <v>1997</v>
+        <v>2014</v>
       </c>
       <c r="H101" t="s">
-        <v>16</v>
+        <v>348</v>
       </c>
       <c r="I101" t="s">
-        <v>20</v>
+        <v>349</v>
+      </c>
+      <c r="N101" s="2" t="s">
+        <v>416</v>
+      </c>
+      <c r="Q101" t="s">
+        <v>417</v>
       </c>
     </row>
     <row r="102" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>293</v>
+        <v>229</v>
       </c>
       <c r="B102" t="s">
         <v>40</v>
       </c>
       <c r="C102" s="2" t="s">
-        <v>294</v>
+        <v>225</v>
       </c>
       <c r="F102">
-        <v>2004</v>
+        <v>1952</v>
       </c>
       <c r="G102">
-        <v>2006</v>
+        <v>1997</v>
       </c>
       <c r="H102" t="s">
         <v>16</v>
@@ -3865,221 +3874,218 @@
     </row>
     <row r="103" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>102</v>
+        <v>293</v>
       </c>
       <c r="B103" t="s">
-        <v>99</v>
+        <v>40</v>
       </c>
       <c r="C103" s="2" t="s">
-        <v>103</v>
+        <v>294</v>
+      </c>
+      <c r="F103">
+        <v>2004</v>
+      </c>
+      <c r="G103">
+        <v>2006</v>
+      </c>
+      <c r="H103" t="s">
+        <v>16</v>
+      </c>
+      <c r="I103" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="104" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>289</v>
+        <v>102</v>
       </c>
       <c r="B104" t="s">
-        <v>124</v>
+        <v>99</v>
       </c>
       <c r="C104" s="2" t="s">
-        <v>290</v>
+        <v>103</v>
       </c>
     </row>
     <row r="105" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>246</v>
+        <v>289</v>
       </c>
       <c r="B105" t="s">
-        <v>165</v>
+        <v>124</v>
       </c>
       <c r="C105" s="2" t="s">
-        <v>247</v>
-      </c>
-      <c r="E105" t="s">
-        <v>14</v>
-      </c>
-      <c r="F105">
-        <v>1960</v>
-      </c>
-      <c r="G105">
-        <v>2006</v>
-      </c>
-      <c r="H105" t="s">
-        <v>16</v>
-      </c>
-      <c r="I105" t="s">
-        <v>249</v>
+        <v>290</v>
       </c>
     </row>
     <row r="106" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>365</v>
+        <v>246</v>
       </c>
       <c r="B106" t="s">
-        <v>128</v>
+        <v>165</v>
       </c>
       <c r="C106" s="2" t="s">
-        <v>364</v>
-      </c>
-      <c r="D106" t="s">
-        <v>370</v>
+        <v>247</v>
       </c>
       <c r="E106" t="s">
-        <v>366</v>
+        <v>14</v>
       </c>
       <c r="F106">
-        <v>1906</v>
+        <v>1960</v>
       </c>
       <c r="G106">
-        <v>2013</v>
+        <v>2006</v>
       </c>
       <c r="H106" t="s">
-        <v>367</v>
+        <v>16</v>
       </c>
       <c r="I106" t="s">
-        <v>368</v>
-      </c>
-      <c r="Q106" t="s">
-        <v>369</v>
+        <v>249</v>
       </c>
     </row>
     <row r="107" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>208</v>
+        <v>365</v>
       </c>
       <c r="B107" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="C107" s="2" t="s">
-        <v>209</v>
+        <v>364</v>
+      </c>
+      <c r="D107" t="s">
+        <v>370</v>
+      </c>
+      <c r="E107" t="s">
+        <v>366</v>
       </c>
       <c r="F107">
-        <v>1932</v>
+        <v>1906</v>
       </c>
       <c r="G107">
-        <v>2014</v>
+        <v>2013</v>
       </c>
       <c r="H107" t="s">
-        <v>16</v>
+        <v>367</v>
       </c>
       <c r="I107" t="s">
-        <v>20</v>
+        <v>368</v>
+      </c>
+      <c r="Q107" t="s">
+        <v>369</v>
       </c>
     </row>
     <row r="108" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>137</v>
+        <v>208</v>
       </c>
       <c r="B108" t="s">
-        <v>259</v>
+        <v>124</v>
       </c>
       <c r="C108" s="2" t="s">
-        <v>138</v>
+        <v>209</v>
+      </c>
+      <c r="F108">
+        <v>1932</v>
+      </c>
+      <c r="G108">
+        <v>2014</v>
+      </c>
+      <c r="H108" t="s">
+        <v>16</v>
+      </c>
+      <c r="I108" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="109" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>155</v>
+        <v>137</v>
       </c>
       <c r="B109" t="s">
         <v>259</v>
       </c>
       <c r="C109" s="2" t="s">
-        <v>154</v>
+        <v>138</v>
       </c>
     </row>
     <row r="110" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>57</v>
+        <v>155</v>
       </c>
       <c r="B110" t="s">
-        <v>128</v>
+        <v>259</v>
       </c>
       <c r="C110" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="Q110" t="s">
-        <v>17</v>
+        <v>154</v>
       </c>
     </row>
     <row r="111" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>129</v>
+        <v>57</v>
       </c>
       <c r="B111" t="s">
-        <v>259</v>
+        <v>128</v>
       </c>
       <c r="C111" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="E111" t="s">
-        <v>131</v>
-      </c>
-      <c r="F111">
-        <v>1945</v>
-      </c>
-      <c r="G111">
-        <v>2008</v>
-      </c>
-      <c r="I111" t="s">
-        <v>20</v>
+        <v>58</v>
+      </c>
+      <c r="Q111" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="112" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>148</v>
+        <v>129</v>
       </c>
       <c r="B112" t="s">
-        <v>128</v>
+        <v>259</v>
       </c>
       <c r="C112" s="2" t="s">
-        <v>147</v>
+        <v>130</v>
+      </c>
+      <c r="E112" t="s">
+        <v>131</v>
+      </c>
+      <c r="F112">
+        <v>1945</v>
+      </c>
+      <c r="G112">
+        <v>2008</v>
+      </c>
+      <c r="I112" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="113" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>233</v>
+        <v>148</v>
       </c>
       <c r="B113" t="s">
-        <v>165</v>
+        <v>128</v>
       </c>
       <c r="C113" s="2" t="s">
-        <v>234</v>
-      </c>
-      <c r="E113" t="s">
-        <v>14</v>
-      </c>
-      <c r="F113">
-        <v>2012</v>
-      </c>
-      <c r="G113">
-        <v>2016</v>
-      </c>
-      <c r="H113" t="s">
-        <v>16</v>
-      </c>
-      <c r="I113" t="s">
-        <v>20</v>
+        <v>147</v>
       </c>
     </row>
     <row r="114" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>35</v>
+        <v>233</v>
       </c>
       <c r="B114" t="s">
-        <v>25</v>
+        <v>165</v>
       </c>
       <c r="C114" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="D114" t="s">
-        <v>37</v>
+        <v>234</v>
       </c>
       <c r="E114" t="s">
         <v>14</v>
       </c>
       <c r="F114">
-        <v>2001</v>
+        <v>2012</v>
+      </c>
+      <c r="G114">
+        <v>2016</v>
       </c>
       <c r="H114" t="s">
         <v>16</v>
@@ -4090,119 +4096,119 @@
     </row>
     <row r="115" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>185</v>
+        <v>35</v>
       </c>
       <c r="B115" t="s">
-        <v>128</v>
+        <v>25</v>
       </c>
       <c r="C115" s="2" t="s">
-        <v>186</v>
+        <v>36</v>
+      </c>
+      <c r="D115" t="s">
+        <v>37</v>
+      </c>
+      <c r="E115" t="s">
+        <v>14</v>
+      </c>
+      <c r="F115">
+        <v>2001</v>
+      </c>
+      <c r="H115" t="s">
+        <v>16</v>
+      </c>
+      <c r="I115" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="116" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>210</v>
+        <v>185</v>
       </c>
       <c r="B116" t="s">
-        <v>40</v>
+        <v>128</v>
       </c>
       <c r="C116" s="2" t="s">
-        <v>211</v>
-      </c>
-      <c r="F116">
-        <v>1976</v>
-      </c>
-      <c r="G116">
-        <v>2016</v>
-      </c>
-      <c r="H116" t="s">
-        <v>16</v>
-      </c>
-      <c r="I116" t="s">
-        <v>20</v>
+        <v>186</v>
       </c>
     </row>
     <row r="117" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>426</v>
+        <v>210</v>
       </c>
       <c r="B117" t="s">
-        <v>86</v>
+        <v>40</v>
       </c>
       <c r="C117" s="2" t="s">
-        <v>427</v>
-      </c>
-      <c r="E117" t="s">
-        <v>34</v>
+        <v>211</v>
       </c>
       <c r="F117">
-        <v>2015</v>
+        <v>1976</v>
       </c>
       <c r="G117">
         <v>2016</v>
       </c>
       <c r="H117" t="s">
-        <v>348</v>
+        <v>16</v>
       </c>
       <c r="I117" t="s">
-        <v>349</v>
-      </c>
-      <c r="K117" s="2" t="s">
-        <v>428</v>
+        <v>20</v>
       </c>
     </row>
     <row r="118" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>144</v>
+        <v>426</v>
       </c>
       <c r="B118" t="s">
-        <v>60</v>
+        <v>86</v>
       </c>
       <c r="C118" s="2" t="s">
-        <v>143</v>
+        <v>427</v>
+      </c>
+      <c r="E118" t="s">
+        <v>34</v>
       </c>
       <c r="F118">
-        <v>1800</v>
+        <v>2015</v>
       </c>
       <c r="G118">
-        <v>2013</v>
+        <v>2016</v>
+      </c>
+      <c r="H118" t="s">
+        <v>348</v>
+      </c>
+      <c r="I118" t="s">
+        <v>349</v>
+      </c>
+      <c r="K118" s="2" t="s">
+        <v>428</v>
       </c>
     </row>
     <row r="119" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>122</v>
+        <v>144</v>
       </c>
       <c r="B119" t="s">
-        <v>259</v>
+        <v>60</v>
       </c>
       <c r="C119" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="I119" t="s">
-        <v>20</v>
+        <v>143</v>
+      </c>
+      <c r="F119">
+        <v>1800</v>
+      </c>
+      <c r="G119">
+        <v>2013</v>
       </c>
     </row>
     <row r="120" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>318</v>
+        <v>122</v>
       </c>
       <c r="B120" t="s">
-        <v>250</v>
+        <v>259</v>
       </c>
       <c r="C120" s="2" t="s">
-        <v>319</v>
-      </c>
-      <c r="E120" t="s">
-        <v>320</v>
-      </c>
-      <c r="F120">
-        <v>1975</v>
-      </c>
-      <c r="G120">
-        <v>1989</v>
-      </c>
-      <c r="H120" t="s">
-        <v>16</v>
+        <v>121</v>
       </c>
       <c r="I120" t="s">
         <v>20</v>
@@ -4210,22 +4216,22 @@
     </row>
     <row r="121" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="B121" t="s">
         <v>250</v>
       </c>
       <c r="C121" s="2" t="s">
-        <v>317</v>
+        <v>319</v>
       </c>
       <c r="E121" t="s">
-        <v>105</v>
+        <v>320</v>
       </c>
       <c r="F121">
-        <v>1950</v>
+        <v>1975</v>
       </c>
       <c r="G121">
-        <v>1996</v>
+        <v>1989</v>
       </c>
       <c r="H121" t="s">
         <v>16</v>
@@ -4236,19 +4242,22 @@
     </row>
     <row r="122" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>322</v>
+        <v>316</v>
       </c>
       <c r="B122" t="s">
-        <v>25</v>
+        <v>250</v>
       </c>
       <c r="C122" s="2" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="E122" t="s">
-        <v>77</v>
+        <v>105</v>
       </c>
       <c r="F122">
-        <v>2010</v>
+        <v>1950</v>
+      </c>
+      <c r="G122">
+        <v>1996</v>
       </c>
       <c r="H122" t="s">
         <v>16</v>
@@ -4259,121 +4268,118 @@
     </row>
     <row r="123" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>141</v>
+        <v>322</v>
       </c>
       <c r="B123" t="s">
-        <v>237</v>
+        <v>25</v>
       </c>
       <c r="C123" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="Q123" t="s">
-        <v>17</v>
+        <v>321</v>
+      </c>
+      <c r="E123" t="s">
+        <v>77</v>
+      </c>
+      <c r="F123">
+        <v>2010</v>
+      </c>
+      <c r="H123" t="s">
+        <v>16</v>
+      </c>
+      <c r="I123" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="124" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>308</v>
+        <v>141</v>
       </c>
       <c r="B124" t="s">
-        <v>250</v>
+        <v>237</v>
       </c>
       <c r="C124" s="2" t="s">
-        <v>309</v>
-      </c>
-      <c r="E124" t="s">
-        <v>310</v>
-      </c>
-      <c r="F124">
-        <v>1950</v>
-      </c>
-      <c r="G124">
-        <v>2010</v>
-      </c>
-      <c r="H124" t="s">
-        <v>16</v>
-      </c>
-      <c r="I124" t="s">
-        <v>20</v>
+        <v>142</v>
+      </c>
+      <c r="Q124" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="125" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>287</v>
+        <v>308</v>
       </c>
       <c r="B125" t="s">
-        <v>134</v>
+        <v>250</v>
       </c>
       <c r="C125" s="2" t="s">
-        <v>288</v>
+        <v>309</v>
+      </c>
+      <c r="E125" t="s">
+        <v>310</v>
       </c>
       <c r="F125">
-        <v>1990</v>
+        <v>1950</v>
       </c>
       <c r="G125">
-        <v>2008</v>
+        <v>2010</v>
+      </c>
+      <c r="H125" t="s">
+        <v>16</v>
+      </c>
+      <c r="I125" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="126" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>274</v>
+        <v>287</v>
       </c>
       <c r="B126" t="s">
-        <v>55</v>
+        <v>134</v>
       </c>
       <c r="C126" s="2" t="s">
-        <v>275</v>
-      </c>
-      <c r="H126" t="s">
-        <v>16</v>
-      </c>
-      <c r="I126" t="s">
-        <v>20</v>
+        <v>288</v>
+      </c>
+      <c r="F126">
+        <v>1990</v>
+      </c>
+      <c r="G126">
+        <v>2008</v>
       </c>
     </row>
     <row r="127" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>157</v>
+        <v>274</v>
       </c>
       <c r="B127" t="s">
-        <v>128</v>
+        <v>55</v>
       </c>
       <c r="C127" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="Q127" t="s">
-        <v>18</v>
+        <v>275</v>
+      </c>
+      <c r="H127" t="s">
+        <v>16</v>
+      </c>
+      <c r="I127" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="128" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>439</v>
+        <v>157</v>
       </c>
       <c r="B128" t="s">
-        <v>259</v>
+        <v>128</v>
       </c>
       <c r="C128" s="2" t="s">
-        <v>438</v>
-      </c>
-      <c r="H128" t="s">
-        <v>348</v>
-      </c>
-      <c r="I128" t="s">
-        <v>349</v>
-      </c>
-      <c r="J128" s="2" t="s">
-        <v>440</v>
-      </c>
-      <c r="K128" s="2" t="s">
-        <v>442</v>
-      </c>
-      <c r="L128" s="2" t="s">
-        <v>441</v>
+        <v>154</v>
+      </c>
+      <c r="Q128" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="129" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>443</v>
+        <v>439</v>
       </c>
       <c r="B129" t="s">
         <v>259</v>
@@ -4381,15 +4387,6 @@
       <c r="C129" s="2" t="s">
         <v>438</v>
       </c>
-      <c r="D129" t="s">
-        <v>447</v>
-      </c>
-      <c r="F129">
-        <v>1990</v>
-      </c>
-      <c r="G129">
-        <v>2014</v>
-      </c>
       <c r="H129" t="s">
         <v>348</v>
       </c>
@@ -4397,87 +4394,99 @@
         <v>349</v>
       </c>
       <c r="J129" s="2" t="s">
-        <v>444</v>
+        <v>440</v>
       </c>
       <c r="K129" s="2" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
       <c r="L129" s="2" t="s">
-        <v>446</v>
+        <v>441</v>
       </c>
     </row>
     <row r="130" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
-        <v>194</v>
+        <v>443</v>
       </c>
       <c r="B130" t="s">
-        <v>99</v>
+        <v>259</v>
       </c>
       <c r="C130" s="2" t="s">
-        <v>193</v>
+        <v>438</v>
+      </c>
+      <c r="D130" t="s">
+        <v>447</v>
+      </c>
+      <c r="F130">
+        <v>1990</v>
+      </c>
+      <c r="G130">
+        <v>2014</v>
+      </c>
+      <c r="H130" t="s">
+        <v>348</v>
+      </c>
+      <c r="I130" t="s">
+        <v>349</v>
+      </c>
+      <c r="J130" s="2" t="s">
+        <v>444</v>
+      </c>
+      <c r="K130" s="2" t="s">
+        <v>445</v>
+      </c>
+      <c r="L130" s="2" t="s">
+        <v>446</v>
       </c>
     </row>
     <row r="131" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>295</v>
+        <v>194</v>
       </c>
       <c r="B131" t="s">
-        <v>40</v>
+        <v>99</v>
       </c>
       <c r="C131" s="2" t="s">
-        <v>296</v>
-      </c>
-      <c r="E131" t="s">
-        <v>297</v>
-      </c>
-      <c r="F131">
-        <v>1990</v>
-      </c>
-      <c r="G131">
-        <v>2015</v>
-      </c>
-      <c r="H131" t="s">
-        <v>16</v>
-      </c>
-      <c r="I131" t="s">
-        <v>249</v>
+        <v>193</v>
       </c>
     </row>
     <row r="132" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>256</v>
+        <v>295</v>
       </c>
       <c r="B132" t="s">
-        <v>250</v>
+        <v>40</v>
       </c>
       <c r="C132" s="2" t="s">
-        <v>257</v>
+        <v>296</v>
       </c>
       <c r="E132" t="s">
-        <v>258</v>
+        <v>297</v>
+      </c>
+      <c r="F132">
+        <v>1990</v>
+      </c>
+      <c r="G132">
+        <v>2015</v>
       </c>
       <c r="H132" t="s">
         <v>16</v>
       </c>
       <c r="I132" t="s">
-        <v>20</v>
+        <v>249</v>
       </c>
     </row>
     <row r="133" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
-        <v>227</v>
+        <v>256</v>
       </c>
       <c r="B133" t="s">
-        <v>40</v>
+        <v>250</v>
       </c>
       <c r="C133" s="2" t="s">
-        <v>225</v>
-      </c>
-      <c r="F133">
-        <v>1955</v>
-      </c>
-      <c r="G133">
-        <v>2016</v>
+        <v>257</v>
+      </c>
+      <c r="E133" t="s">
+        <v>258</v>
       </c>
       <c r="H133" t="s">
         <v>16</v>
@@ -4488,7 +4497,7 @@
     </row>
     <row r="134" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="B134" t="s">
         <v>40</v>
@@ -4497,7 +4506,7 @@
         <v>225</v>
       </c>
       <c r="F134">
-        <v>1995</v>
+        <v>1955</v>
       </c>
       <c r="G134">
         <v>2016</v>
@@ -4511,248 +4520,248 @@
     </row>
     <row r="135" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
-        <v>452</v>
+        <v>230</v>
       </c>
       <c r="B135" t="s">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="C135" s="2" t="s">
-        <v>453</v>
-      </c>
-      <c r="E135" t="s">
-        <v>9</v>
+        <v>225</v>
+      </c>
+      <c r="F135">
+        <v>1995</v>
+      </c>
+      <c r="G135">
+        <v>2016</v>
       </c>
       <c r="H135" t="s">
-        <v>348</v>
+        <v>16</v>
       </c>
       <c r="I135" t="s">
-        <v>435</v>
+        <v>20</v>
       </c>
     </row>
     <row r="136" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
-        <v>109</v>
+        <v>452</v>
       </c>
       <c r="B136" t="s">
         <v>25</v>
       </c>
       <c r="C136" s="2" t="s">
-        <v>110</v>
+        <v>453</v>
       </c>
       <c r="E136" t="s">
-        <v>111</v>
-      </c>
-      <c r="F136">
-        <v>1956</v>
+        <v>9</v>
+      </c>
+      <c r="H136" t="s">
+        <v>348</v>
+      </c>
+      <c r="I136" t="s">
+        <v>435</v>
       </c>
     </row>
     <row r="137" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
-        <v>326</v>
+        <v>109</v>
       </c>
       <c r="B137" t="s">
         <v>25</v>
       </c>
       <c r="C137" s="2" t="s">
-        <v>327</v>
+        <v>110</v>
       </c>
       <c r="E137" t="s">
         <v>111</v>
       </c>
       <c r="F137">
-        <v>1998</v>
-      </c>
-      <c r="H137" t="s">
-        <v>16</v>
-      </c>
-      <c r="I137" t="s">
-        <v>20</v>
+        <v>1956</v>
       </c>
     </row>
     <row r="138" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
-        <v>91</v>
+        <v>326</v>
       </c>
       <c r="B138" t="s">
         <v>25</v>
       </c>
       <c r="C138" s="2" t="s">
-        <v>93</v>
+        <v>327</v>
       </c>
       <c r="E138" t="s">
-        <v>92</v>
+        <v>111</v>
       </c>
       <c r="F138">
-        <v>1999</v>
+        <v>1998</v>
+      </c>
+      <c r="H138" t="s">
+        <v>16</v>
+      </c>
+      <c r="I138" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="139" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
-        <v>314</v>
+        <v>91</v>
       </c>
       <c r="B139" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="C139" s="2" t="s">
-        <v>313</v>
+        <v>93</v>
       </c>
       <c r="E139" t="s">
-        <v>315</v>
+        <v>92</v>
       </c>
       <c r="F139">
-        <v>1950</v>
-      </c>
-      <c r="G139">
-        <v>2004</v>
-      </c>
-      <c r="H139" t="s">
-        <v>16</v>
-      </c>
-      <c r="I139" t="s">
-        <v>20</v>
+        <v>1999</v>
       </c>
     </row>
     <row r="140" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
-        <v>161</v>
+        <v>314</v>
       </c>
       <c r="B140" t="s">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="C140" s="2" t="s">
-        <v>160</v>
+        <v>313</v>
+      </c>
+      <c r="E140" t="s">
+        <v>315</v>
+      </c>
+      <c r="F140">
+        <v>1950</v>
+      </c>
+      <c r="G140">
+        <v>2004</v>
+      </c>
+      <c r="H140" t="s">
+        <v>16</v>
+      </c>
+      <c r="I140" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="141" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="B141" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="C141" s="2" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
     </row>
     <row r="142" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
-        <v>399</v>
+        <v>168</v>
       </c>
       <c r="B142" t="s">
         <v>40</v>
       </c>
       <c r="C142" s="2" t="s">
-        <v>400</v>
-      </c>
-      <c r="E142" t="s">
-        <v>14</v>
-      </c>
-      <c r="F142">
-        <v>2000</v>
-      </c>
-      <c r="G142">
-        <v>2014</v>
-      </c>
-      <c r="H142" t="s">
-        <v>348</v>
-      </c>
-      <c r="I142" t="s">
-        <v>349</v>
-      </c>
-      <c r="J142" s="2" t="s">
-        <v>402</v>
-      </c>
-      <c r="N142" s="2" t="s">
-        <v>401</v>
+        <v>167</v>
       </c>
     </row>
     <row r="143" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
-        <v>213</v>
+        <v>399</v>
       </c>
       <c r="B143" t="s">
-        <v>55</v>
+        <v>40</v>
       </c>
       <c r="C143" s="2" t="s">
-        <v>212</v>
+        <v>400</v>
+      </c>
+      <c r="E143" t="s">
+        <v>14</v>
+      </c>
+      <c r="F143">
+        <v>2000</v>
+      </c>
+      <c r="G143">
+        <v>2014</v>
       </c>
       <c r="H143" t="s">
-        <v>16</v>
+        <v>348</v>
       </c>
       <c r="I143" t="s">
-        <v>20</v>
+        <v>349</v>
+      </c>
+      <c r="J143" s="2" t="s">
+        <v>402</v>
+      </c>
+      <c r="N143" s="2" t="s">
+        <v>401</v>
       </c>
     </row>
     <row r="144" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
-        <v>395</v>
+        <v>213</v>
       </c>
       <c r="B144" t="s">
-        <v>25</v>
+        <v>55</v>
       </c>
       <c r="C144" s="2" t="s">
-        <v>394</v>
-      </c>
-      <c r="D144" t="s">
-        <v>396</v>
-      </c>
-      <c r="E144" t="s">
-        <v>111</v>
-      </c>
-      <c r="F144">
-        <v>1986</v>
-      </c>
-      <c r="G144">
-        <v>2015</v>
+        <v>212</v>
       </c>
       <c r="H144" t="s">
-        <v>367</v>
+        <v>16</v>
       </c>
       <c r="I144" t="s">
-        <v>398</v>
-      </c>
-      <c r="J144" s="2" t="s">
-        <v>397</v>
+        <v>20</v>
       </c>
     </row>
     <row r="145" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
-        <v>323</v>
+        <v>395</v>
       </c>
       <c r="B145" t="s">
         <v>25</v>
       </c>
       <c r="C145" s="2" t="s">
-        <v>324</v>
+        <v>394</v>
+      </c>
+      <c r="D145" t="s">
+        <v>396</v>
       </c>
       <c r="E145" t="s">
-        <v>325</v>
+        <v>111</v>
       </c>
       <c r="F145">
-        <v>1942</v>
+        <v>1986</v>
+      </c>
+      <c r="G145">
+        <v>2015</v>
       </c>
       <c r="H145" t="s">
-        <v>16</v>
+        <v>367</v>
       </c>
       <c r="I145" t="s">
-        <v>20</v>
+        <v>398</v>
+      </c>
+      <c r="J145" s="2" t="s">
+        <v>397</v>
       </c>
     </row>
     <row r="146" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
-        <v>273</v>
+        <v>323</v>
       </c>
       <c r="B146" t="s">
-        <v>237</v>
+        <v>25</v>
       </c>
       <c r="C146" s="2" t="s">
-        <v>272</v>
+        <v>324</v>
+      </c>
+      <c r="E146" t="s">
+        <v>325</v>
       </c>
       <c r="F146">
-        <v>1996</v>
-      </c>
-      <c r="G146">
-        <v>2016</v>
+        <v>1942</v>
       </c>
       <c r="H146" t="s">
         <v>16</v>
@@ -4763,209 +4772,212 @@
     </row>
     <row r="147" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
-        <v>66</v>
+        <v>273</v>
       </c>
       <c r="B147" t="s">
-        <v>25</v>
+        <v>237</v>
       </c>
       <c r="C147" s="2" t="s">
-        <v>67</v>
+        <v>272</v>
+      </c>
+      <c r="F147">
+        <v>1996</v>
+      </c>
+      <c r="G147">
+        <v>2016</v>
+      </c>
+      <c r="H147" t="s">
+        <v>16</v>
+      </c>
+      <c r="I147" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="148" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
-        <v>383</v>
+        <v>66</v>
       </c>
       <c r="B148" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="C148" s="2" t="s">
-        <v>384</v>
-      </c>
-      <c r="E148" t="s">
-        <v>386</v>
-      </c>
-      <c r="F148">
-        <v>1951</v>
-      </c>
-      <c r="H148" t="s">
-        <v>348</v>
-      </c>
-      <c r="I148" t="s">
-        <v>349</v>
-      </c>
-      <c r="N148" s="2" t="s">
-        <v>385</v>
+        <v>67</v>
       </c>
     </row>
     <row r="149" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
-        <v>139</v>
+        <v>383</v>
       </c>
       <c r="B149" t="s">
         <v>40</v>
       </c>
       <c r="C149" s="2" t="s">
-        <v>140</v>
+        <v>384</v>
+      </c>
+      <c r="E149" t="s">
+        <v>386</v>
+      </c>
+      <c r="F149">
+        <v>1951</v>
+      </c>
+      <c r="H149" t="s">
+        <v>348</v>
+      </c>
+      <c r="I149" t="s">
+        <v>349</v>
+      </c>
+      <c r="N149" s="2" t="s">
+        <v>385</v>
       </c>
     </row>
     <row r="150" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
-        <v>329</v>
+        <v>139</v>
       </c>
       <c r="B150" t="s">
-        <v>165</v>
+        <v>40</v>
       </c>
       <c r="C150" s="2" t="s">
-        <v>328</v>
-      </c>
-      <c r="E150" t="s">
-        <v>34</v>
-      </c>
-      <c r="F150">
-        <v>1789</v>
-      </c>
-      <c r="H150" t="s">
-        <v>16</v>
-      </c>
-      <c r="I150" t="s">
-        <v>20</v>
+        <v>140</v>
       </c>
     </row>
     <row r="151" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
-        <v>172</v>
+        <v>329</v>
       </c>
       <c r="B151" t="s">
-        <v>60</v>
+        <v>165</v>
       </c>
       <c r="C151" s="2" t="s">
-        <v>171</v>
+        <v>328</v>
+      </c>
+      <c r="E151" t="s">
+        <v>34</v>
+      </c>
+      <c r="F151">
+        <v>1789</v>
+      </c>
+      <c r="H151" t="s">
+        <v>16</v>
+      </c>
+      <c r="I151" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="152" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
-        <v>217</v>
+        <v>172</v>
       </c>
       <c r="B152" t="s">
         <v>60</v>
       </c>
       <c r="C152" s="2" t="s">
-        <v>216</v>
-      </c>
-      <c r="E152" t="s">
-        <v>14</v>
-      </c>
-      <c r="F152">
-        <v>1900</v>
-      </c>
-      <c r="H152" t="s">
-        <v>16</v>
-      </c>
-      <c r="I152" t="s">
-        <v>20</v>
+        <v>171</v>
       </c>
     </row>
     <row r="153" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
-        <v>132</v>
+        <v>217</v>
       </c>
       <c r="B153" t="s">
-        <v>259</v>
+        <v>60</v>
       </c>
       <c r="C153" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="Q153" t="s">
-        <v>17</v>
+        <v>216</v>
+      </c>
+      <c r="E153" t="s">
+        <v>14</v>
+      </c>
+      <c r="F153">
+        <v>1900</v>
+      </c>
+      <c r="H153" t="s">
+        <v>16</v>
+      </c>
+      <c r="I153" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="154" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
-        <v>182</v>
+        <v>132</v>
       </c>
       <c r="B154" t="s">
-        <v>165</v>
+        <v>259</v>
       </c>
       <c r="C154" s="2" t="s">
-        <v>181</v>
+        <v>133</v>
+      </c>
+      <c r="Q154" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="155" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
-        <v>423</v>
+        <v>182</v>
       </c>
       <c r="B155" t="s">
-        <v>86</v>
+        <v>165</v>
       </c>
       <c r="C155" s="2" t="s">
-        <v>424</v>
-      </c>
-      <c r="E155" t="s">
-        <v>34</v>
-      </c>
-      <c r="F155">
-        <v>1996</v>
-      </c>
-      <c r="G155">
-        <v>2016</v>
-      </c>
-      <c r="H155" t="s">
-        <v>348</v>
-      </c>
-      <c r="I155" t="s">
-        <v>425</v>
+        <v>181</v>
       </c>
     </row>
     <row r="156" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
-        <v>115</v>
+        <v>423</v>
       </c>
       <c r="B156" t="s">
-        <v>128</v>
+        <v>86</v>
       </c>
       <c r="C156" s="2" t="s">
-        <v>116</v>
+        <v>424</v>
+      </c>
+      <c r="E156" t="s">
+        <v>34</v>
+      </c>
+      <c r="F156">
+        <v>1996</v>
+      </c>
+      <c r="G156">
+        <v>2016</v>
+      </c>
+      <c r="H156" t="s">
+        <v>348</v>
+      </c>
+      <c r="I156" t="s">
+        <v>425</v>
       </c>
     </row>
     <row r="157" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
-        <v>263</v>
+        <v>115</v>
       </c>
       <c r="B157" t="s">
-        <v>250</v>
+        <v>128</v>
       </c>
       <c r="C157" s="2" t="s">
-        <v>264</v>
-      </c>
-      <c r="E157" t="s">
-        <v>265</v>
-      </c>
-      <c r="F157">
-        <v>1500</v>
-      </c>
-      <c r="G157">
-        <v>2000</v>
-      </c>
-      <c r="H157" t="s">
-        <v>16</v>
-      </c>
-      <c r="I157" t="s">
-        <v>20</v>
+        <v>116</v>
       </c>
     </row>
     <row r="158" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
-        <v>221</v>
+        <v>263</v>
       </c>
       <c r="B158" t="s">
-        <v>86</v>
+        <v>250</v>
       </c>
       <c r="C158" s="2" t="s">
-        <v>220</v>
+        <v>264</v>
+      </c>
+      <c r="E158" t="s">
+        <v>265</v>
       </c>
       <c r="F158">
-        <v>2013</v>
+        <v>1500</v>
+      </c>
+      <c r="G158">
+        <v>2000</v>
       </c>
       <c r="H158" t="s">
         <v>16</v>
@@ -4976,22 +4988,16 @@
     </row>
     <row r="159" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
-        <v>13</v>
+        <v>221</v>
       </c>
       <c r="B159" t="s">
-        <v>25</v>
+        <v>86</v>
       </c>
       <c r="C159" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="D159" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="E159" t="s">
-        <v>14</v>
+        <v>220</v>
       </c>
       <c r="F159">
-        <v>1981</v>
+        <v>2013</v>
       </c>
       <c r="H159" t="s">
         <v>16</v>
@@ -5002,23 +5008,49 @@
     </row>
     <row r="160" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
+        <v>13</v>
+      </c>
+      <c r="B160" t="s">
+        <v>25</v>
+      </c>
+      <c r="C160" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D160" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E160" t="s">
+        <v>14</v>
+      </c>
+      <c r="F160">
+        <v>1981</v>
+      </c>
+      <c r="H160" t="s">
+        <v>16</v>
+      </c>
+      <c r="I160" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="161" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A161" t="s">
         <v>283</v>
       </c>
-      <c r="B160" t="s">
+      <c r="B161" t="s">
         <v>124</v>
       </c>
-      <c r="C160" s="2" t="s">
+      <c r="C161" s="2" t="s">
         <v>284</v>
       </c>
-      <c r="H160" t="s">
-        <v>16</v>
-      </c>
-      <c r="I160" t="s">
+      <c r="H161" t="s">
+        <v>16</v>
+      </c>
+      <c r="I161" t="s">
         <v>20</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:Q160">
+  <sortState ref="A2:Q161">
     <sortCondition ref="A2"/>
   </sortState>
   <hyperlinks>
@@ -5026,9 +5058,9 @@
     <hyperlink ref="C58" r:id="rId2"/>
     <hyperlink ref="C7" r:id="rId3"/>
     <hyperlink ref="C10" r:id="rId4"/>
-    <hyperlink ref="C94" r:id="rId5"/>
-    <hyperlink ref="C114" r:id="rId6"/>
-    <hyperlink ref="C159" r:id="rId7"/>
+    <hyperlink ref="C95" r:id="rId5"/>
+    <hyperlink ref="C115" r:id="rId6"/>
+    <hyperlink ref="C160" r:id="rId7"/>
     <hyperlink ref="C35" r:id="rId8"/>
     <hyperlink ref="C30" r:id="rId9"/>
     <hyperlink ref="C49" r:id="rId10"/>
@@ -5036,13 +5068,13 @@
     <hyperlink ref="C3" r:id="rId12"/>
     <hyperlink ref="C20" r:id="rId13"/>
     <hyperlink ref="C60" r:id="rId14"/>
-    <hyperlink ref="C86" r:id="rId15"/>
+    <hyperlink ref="C87" r:id="rId15"/>
     <hyperlink ref="C29" r:id="rId16"/>
-    <hyperlink ref="C110" r:id="rId17"/>
+    <hyperlink ref="C111" r:id="rId17"/>
     <hyperlink ref="C41" r:id="rId18"/>
-    <hyperlink ref="C71" r:id="rId19"/>
+    <hyperlink ref="C72" r:id="rId19"/>
     <hyperlink ref="C16" r:id="rId20"/>
-    <hyperlink ref="C147" r:id="rId21"/>
+    <hyperlink ref="C148" r:id="rId21"/>
     <hyperlink ref="C8" r:id="rId22"/>
     <hyperlink ref="C38" r:id="rId23"/>
     <hyperlink ref="C53" r:id="rId24"/>
@@ -5050,118 +5082,118 @@
     <hyperlink ref="C54" r:id="rId26"/>
     <hyperlink ref="C55" r:id="rId27"/>
     <hyperlink ref="C69" r:id="rId28"/>
-    <hyperlink ref="C91" r:id="rId29"/>
-    <hyperlink ref="C138" r:id="rId30"/>
-    <hyperlink ref="C97" r:id="rId31"/>
-    <hyperlink ref="C81" r:id="rId32"/>
-    <hyperlink ref="C103" r:id="rId33"/>
+    <hyperlink ref="C92" r:id="rId29"/>
+    <hyperlink ref="C139" r:id="rId30"/>
+    <hyperlink ref="C98" r:id="rId31"/>
+    <hyperlink ref="C82" r:id="rId32"/>
+    <hyperlink ref="C104" r:id="rId33"/>
     <hyperlink ref="C70" r:id="rId34"/>
     <hyperlink ref="C17" r:id="rId35"/>
-    <hyperlink ref="C136" r:id="rId36"/>
+    <hyperlink ref="C137" r:id="rId36"/>
     <hyperlink ref="C15" r:id="rId37"/>
-    <hyperlink ref="C156" r:id="rId38"/>
-    <hyperlink ref="C85" r:id="rId39"/>
+    <hyperlink ref="C157" r:id="rId38"/>
+    <hyperlink ref="C86" r:id="rId39"/>
     <hyperlink ref="C57" r:id="rId40"/>
-    <hyperlink ref="C119" r:id="rId41"/>
+    <hyperlink ref="C120" r:id="rId41"/>
     <hyperlink ref="C18" r:id="rId42"/>
     <hyperlink ref="C51" r:id="rId43"/>
     <hyperlink ref="C23" r:id="rId44"/>
-    <hyperlink ref="C111" r:id="rId45"/>
-    <hyperlink ref="C153" r:id="rId46"/>
+    <hyperlink ref="C112" r:id="rId45"/>
+    <hyperlink ref="C154" r:id="rId46"/>
     <hyperlink ref="C27" r:id="rId47" display="http://comparativeconstitutionsproject.org/"/>
-    <hyperlink ref="C108" r:id="rId48"/>
-    <hyperlink ref="C149" r:id="rId49"/>
-    <hyperlink ref="C123" r:id="rId50"/>
-    <hyperlink ref="C118" r:id="rId51"/>
+    <hyperlink ref="C109" r:id="rId48"/>
+    <hyperlink ref="C150" r:id="rId49"/>
+    <hyperlink ref="C124" r:id="rId50"/>
+    <hyperlink ref="C119" r:id="rId51"/>
     <hyperlink ref="C22" r:id="rId52"/>
-    <hyperlink ref="C112" r:id="rId53"/>
+    <hyperlink ref="C113" r:id="rId53"/>
     <hyperlink ref="C48" r:id="rId54"/>
-    <hyperlink ref="C75" r:id="rId55"/>
-    <hyperlink ref="C78" r:id="rId56"/>
-    <hyperlink ref="C109" r:id="rId57"/>
-    <hyperlink ref="C99" r:id="rId58"/>
-    <hyperlink ref="C127" r:id="rId59"/>
+    <hyperlink ref="C76" r:id="rId55"/>
+    <hyperlink ref="C79" r:id="rId56"/>
+    <hyperlink ref="C110" r:id="rId57"/>
+    <hyperlink ref="C100" r:id="rId58"/>
+    <hyperlink ref="C128" r:id="rId59"/>
     <hyperlink ref="C31" r:id="rId60"/>
-    <hyperlink ref="C140" r:id="rId61"/>
+    <hyperlink ref="C141" r:id="rId61"/>
     <hyperlink ref="C9" r:id="rId62"/>
     <hyperlink ref="C33" r:id="rId63"/>
-    <hyperlink ref="C141" r:id="rId64"/>
+    <hyperlink ref="C142" r:id="rId64"/>
     <hyperlink ref="C14" r:id="rId65"/>
-    <hyperlink ref="C151" r:id="rId66"/>
+    <hyperlink ref="C152" r:id="rId66"/>
     <hyperlink ref="C25" r:id="rId67"/>
     <hyperlink ref="C24" r:id="rId68"/>
     <hyperlink ref="C26" r:id="rId69"/>
     <hyperlink ref="C52" r:id="rId70"/>
-    <hyperlink ref="C154" r:id="rId71"/>
+    <hyperlink ref="C155" r:id="rId71"/>
     <hyperlink ref="C28" r:id="rId72"/>
-    <hyperlink ref="C115" r:id="rId73"/>
+    <hyperlink ref="C116" r:id="rId73"/>
     <hyperlink ref="C32" r:id="rId74"/>
     <hyperlink ref="C45" r:id="rId75"/>
-    <hyperlink ref="C130" r:id="rId76"/>
+    <hyperlink ref="C131" r:id="rId76"/>
     <hyperlink ref="C42" r:id="rId77"/>
     <hyperlink ref="C39" r:id="rId78"/>
     <hyperlink ref="C68" r:id="rId79"/>
     <hyperlink ref="C5" r:id="rId80"/>
     <hyperlink ref="C67" r:id="rId81"/>
     <hyperlink ref="C12" r:id="rId82"/>
-    <hyperlink ref="C107" r:id="rId83"/>
-    <hyperlink ref="C116" r:id="rId84"/>
-    <hyperlink ref="C143" r:id="rId85"/>
+    <hyperlink ref="C108" r:id="rId83"/>
+    <hyperlink ref="C117" r:id="rId84"/>
+    <hyperlink ref="C144" r:id="rId85"/>
     <hyperlink ref="C36" r:id="rId86"/>
-    <hyperlink ref="C152" r:id="rId87"/>
+    <hyperlink ref="C153" r:id="rId87"/>
     <hyperlink ref="C44" r:id="rId88"/>
-    <hyperlink ref="C158" r:id="rId89"/>
-    <hyperlink ref="C95" r:id="rId90"/>
+    <hyperlink ref="C159" r:id="rId89"/>
+    <hyperlink ref="C96" r:id="rId90"/>
     <hyperlink ref="C65" r:id="rId91"/>
-    <hyperlink ref="C96" r:id="rId92"/>
-    <hyperlink ref="C133" r:id="rId93"/>
-    <hyperlink ref="C79" r:id="rId94"/>
-    <hyperlink ref="C101" r:id="rId95"/>
-    <hyperlink ref="C134" r:id="rId96"/>
+    <hyperlink ref="C97" r:id="rId92"/>
+    <hyperlink ref="C134" r:id="rId93"/>
+    <hyperlink ref="C80" r:id="rId94"/>
+    <hyperlink ref="C102" r:id="rId95"/>
+    <hyperlink ref="C135" r:id="rId96"/>
     <hyperlink ref="C61" r:id="rId97"/>
-    <hyperlink ref="C113" r:id="rId98"/>
+    <hyperlink ref="C114" r:id="rId98"/>
     <hyperlink ref="C46" r:id="rId99"/>
     <hyperlink ref="C43" r:id="rId100"/>
-    <hyperlink ref="C82" r:id="rId101"/>
+    <hyperlink ref="C83" r:id="rId101"/>
     <hyperlink ref="C59" r:id="rId102"/>
     <hyperlink ref="C2" r:id="rId103"/>
-    <hyperlink ref="C76" r:id="rId104"/>
-    <hyperlink ref="C80" r:id="rId105"/>
-    <hyperlink ref="C105" r:id="rId106"/>
+    <hyperlink ref="C77" r:id="rId104"/>
+    <hyperlink ref="C81" r:id="rId105"/>
+    <hyperlink ref="C106" r:id="rId106"/>
     <hyperlink ref="C47" r:id="rId107"/>
-    <hyperlink ref="C83" r:id="rId108"/>
-    <hyperlink ref="C132" r:id="rId109"/>
+    <hyperlink ref="C84" r:id="rId108"/>
+    <hyperlink ref="C133" r:id="rId109"/>
     <hyperlink ref="C13" r:id="rId110"/>
     <hyperlink ref="C4" r:id="rId111"/>
-    <hyperlink ref="C157" r:id="rId112"/>
-    <hyperlink ref="C89" r:id="rId113"/>
-    <hyperlink ref="C84" r:id="rId114"/>
-    <hyperlink ref="C146" r:id="rId115"/>
-    <hyperlink ref="C126" r:id="rId116"/>
+    <hyperlink ref="C158" r:id="rId112"/>
+    <hyperlink ref="C90" r:id="rId113"/>
+    <hyperlink ref="C85" r:id="rId114"/>
+    <hyperlink ref="C147" r:id="rId115"/>
+    <hyperlink ref="C127" r:id="rId116"/>
     <hyperlink ref="C63" r:id="rId117"/>
-    <hyperlink ref="C98" r:id="rId118"/>
-    <hyperlink ref="C73" r:id="rId119"/>
-    <hyperlink ref="C160" r:id="rId120"/>
+    <hyperlink ref="C99" r:id="rId118"/>
+    <hyperlink ref="C74" r:id="rId119"/>
+    <hyperlink ref="C161" r:id="rId120"/>
     <hyperlink ref="C66" r:id="rId121"/>
-    <hyperlink ref="C125" r:id="rId122"/>
-    <hyperlink ref="C104" r:id="rId123"/>
-    <hyperlink ref="C77" r:id="rId124"/>
-    <hyperlink ref="C102" r:id="rId125"/>
-    <hyperlink ref="C131" r:id="rId126"/>
-    <hyperlink ref="C87" r:id="rId127"/>
+    <hyperlink ref="C126" r:id="rId122"/>
+    <hyperlink ref="C105" r:id="rId123"/>
+    <hyperlink ref="C78" r:id="rId124"/>
+    <hyperlink ref="C103" r:id="rId125"/>
+    <hyperlink ref="C132" r:id="rId126"/>
+    <hyperlink ref="C88" r:id="rId127"/>
     <hyperlink ref="C11" r:id="rId128"/>
     <hyperlink ref="C19" r:id="rId129"/>
-    <hyperlink ref="C124" r:id="rId130"/>
-    <hyperlink ref="C72" r:id="rId131"/>
-    <hyperlink ref="C139" r:id="rId132"/>
-    <hyperlink ref="C121" r:id="rId133"/>
-    <hyperlink ref="C120" r:id="rId134"/>
-    <hyperlink ref="C122" r:id="rId135"/>
-    <hyperlink ref="C145" r:id="rId136"/>
-    <hyperlink ref="C137" r:id="rId137"/>
-    <hyperlink ref="C150" r:id="rId138"/>
+    <hyperlink ref="C125" r:id="rId130"/>
+    <hyperlink ref="C73" r:id="rId131"/>
+    <hyperlink ref="C140" r:id="rId132"/>
+    <hyperlink ref="C122" r:id="rId133"/>
+    <hyperlink ref="C121" r:id="rId134"/>
+    <hyperlink ref="C123" r:id="rId135"/>
+    <hyperlink ref="C146" r:id="rId136"/>
+    <hyperlink ref="C138" r:id="rId137"/>
+    <hyperlink ref="C151" r:id="rId138"/>
     <hyperlink ref="C37" r:id="rId139"/>
-    <hyperlink ref="C88" r:id="rId140"/>
+    <hyperlink ref="C89" r:id="rId140"/>
     <hyperlink ref="J2" r:id="rId141"/>
     <hyperlink ref="M3" r:id="rId142"/>
     <hyperlink ref="J3" r:id="rId143"/>
@@ -5169,53 +5201,54 @@
     <hyperlink ref="J4" r:id="rId145"/>
     <hyperlink ref="P5" r:id="rId146"/>
     <hyperlink ref="J5" r:id="rId147"/>
-    <hyperlink ref="C106" r:id="rId148"/>
+    <hyperlink ref="C107" r:id="rId148"/>
     <hyperlink ref="C34" r:id="rId149"/>
     <hyperlink ref="P7" r:id="rId150"/>
     <hyperlink ref="J7" r:id="rId151"/>
     <hyperlink ref="M8" r:id="rId152"/>
     <hyperlink ref="L8" r:id="rId153"/>
     <hyperlink ref="J8" r:id="rId154"/>
-    <hyperlink ref="C148" r:id="rId155"/>
-    <hyperlink ref="N148" r:id="rId156"/>
+    <hyperlink ref="C149" r:id="rId155"/>
+    <hyperlink ref="N149" r:id="rId156"/>
     <hyperlink ref="C21" r:id="rId157"/>
     <hyperlink ref="N21" r:id="rId158"/>
     <hyperlink ref="C62" r:id="rId159"/>
-    <hyperlink ref="C144" r:id="rId160"/>
-    <hyperlink ref="J144" r:id="rId161"/>
-    <hyperlink ref="C142" r:id="rId162"/>
-    <hyperlink ref="N142" r:id="rId163"/>
-    <hyperlink ref="J142" r:id="rId164"/>
-    <hyperlink ref="C92" r:id="rId165"/>
-    <hyperlink ref="C90" r:id="rId166"/>
+    <hyperlink ref="C145" r:id="rId160"/>
+    <hyperlink ref="J145" r:id="rId161"/>
+    <hyperlink ref="C143" r:id="rId162"/>
+    <hyperlink ref="N143" r:id="rId163"/>
+    <hyperlink ref="J143" r:id="rId164"/>
+    <hyperlink ref="C93" r:id="rId165"/>
+    <hyperlink ref="C91" r:id="rId166"/>
     <hyperlink ref="C40" r:id="rId167"/>
     <hyperlink ref="J40" r:id="rId168"/>
     <hyperlink ref="K40" r:id="rId169"/>
-    <hyperlink ref="C100" r:id="rId170"/>
-    <hyperlink ref="N100" r:id="rId171"/>
-    <hyperlink ref="C74" r:id="rId172"/>
-    <hyperlink ref="K74" r:id="rId173"/>
-    <hyperlink ref="C155" r:id="rId174"/>
-    <hyperlink ref="C117" r:id="rId175"/>
-    <hyperlink ref="K117" r:id="rId176"/>
+    <hyperlink ref="C101" r:id="rId170"/>
+    <hyperlink ref="N101" r:id="rId171"/>
+    <hyperlink ref="C75" r:id="rId172"/>
+    <hyperlink ref="K75" r:id="rId173"/>
+    <hyperlink ref="C156" r:id="rId174"/>
+    <hyperlink ref="C118" r:id="rId175"/>
+    <hyperlink ref="K118" r:id="rId176"/>
     <hyperlink ref="L9" r:id="rId177"/>
     <hyperlink ref="J9" r:id="rId178"/>
     <hyperlink ref="J10" r:id="rId179"/>
-    <hyperlink ref="C128" r:id="rId180"/>
-    <hyperlink ref="J128" r:id="rId181"/>
-    <hyperlink ref="L128" r:id="rId182"/>
-    <hyperlink ref="K128" r:id="rId183"/>
-    <hyperlink ref="C129" r:id="rId184"/>
-    <hyperlink ref="J129" r:id="rId185"/>
-    <hyperlink ref="K129" r:id="rId186"/>
-    <hyperlink ref="L129" r:id="rId187"/>
+    <hyperlink ref="C129" r:id="rId180"/>
+    <hyperlink ref="J129" r:id="rId181"/>
+    <hyperlink ref="L129" r:id="rId182"/>
+    <hyperlink ref="K129" r:id="rId183"/>
+    <hyperlink ref="C130" r:id="rId184"/>
+    <hyperlink ref="J130" r:id="rId185"/>
+    <hyperlink ref="K130" r:id="rId186"/>
+    <hyperlink ref="L130" r:id="rId187"/>
     <hyperlink ref="C64" r:id="rId188"/>
     <hyperlink ref="J64" r:id="rId189"/>
     <hyperlink ref="N64" r:id="rId190"/>
-    <hyperlink ref="C135" r:id="rId191"/>
-    <hyperlink ref="C93" r:id="rId192"/>
-    <hyperlink ref="J93" r:id="rId193"/>
-    <hyperlink ref="L93" r:id="rId194"/>
+    <hyperlink ref="C136" r:id="rId191"/>
+    <hyperlink ref="C94" r:id="rId192"/>
+    <hyperlink ref="J94" r:id="rId193"/>
+    <hyperlink ref="L94" r:id="rId194"/>
+    <hyperlink ref="C71" r:id="rId195"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
add data, 'Ethnic Power Relations' and 'From Empire to Nation-State'
</commit_message>
<xml_diff>
--- a/PolData.xlsx
+++ b/PolData.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="841" uniqueCount="462">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="860" uniqueCount="472">
   <si>
     <t>name</t>
   </si>
@@ -1413,6 +1413,36 @@
   </si>
   <si>
     <t>https://www.gesis.org/en/elections-home/gles/data/</t>
+  </si>
+  <si>
+    <t>Ethnic Power Relations</t>
+  </si>
+  <si>
+    <t>Ethnic groups, state power</t>
+  </si>
+  <si>
+    <t>http://www.columbia.edu/~aw2951/Datasets.html</t>
+  </si>
+  <si>
+    <t>http://www.columbia.edu/~aw2951/EPR3CountryNewReduced.dta</t>
+  </si>
+  <si>
+    <t>http://www.columbia.edu/~aw2951/eprnew301.xlsx</t>
+  </si>
+  <si>
+    <t>http://www.columbia.edu/~aw2951/AppendixEthnicPolitics.pdf</t>
+  </si>
+  <si>
+    <t>From Empire to Nation-State</t>
+  </si>
+  <si>
+    <t>http://www.columbia.edu/~aw2951/EmpireNSdataset.pdf</t>
+  </si>
+  <si>
+    <t>http://www.columbia.edu/~aw2951/WimmerMin1.0.xls</t>
+  </si>
+  <si>
+    <t>http://www.columbia.edu/~aw2951/WimmerMin1.0.dta</t>
   </si>
 </sst>
 </file>
@@ -1752,10 +1782,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q161"/>
+  <dimension ref="A1:Q163"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A146" workbookViewId="0">
-      <selection activeCell="A71" sqref="A71"/>
+    <sheetView tabSelected="1" topLeftCell="A137" workbookViewId="0">
+      <selection activeCell="A70" sqref="A70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2806,80 +2836,101 @@
     </row>
     <row r="49" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>28</v>
+        <v>462</v>
       </c>
       <c r="B49" t="s">
-        <v>25</v>
+        <v>250</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>48</v>
+        <v>464</v>
+      </c>
+      <c r="D49" t="s">
+        <v>463</v>
+      </c>
+      <c r="E49" t="s">
+        <v>14</v>
+      </c>
+      <c r="F49">
+        <v>1946</v>
+      </c>
+      <c r="G49">
+        <v>2010</v>
+      </c>
+      <c r="H49" t="s">
+        <v>348</v>
+      </c>
+      <c r="I49" t="s">
+        <v>349</v>
+      </c>
+      <c r="J49" s="2" t="s">
+        <v>467</v>
+      </c>
+      <c r="K49" s="2" t="s">
+        <v>466</v>
+      </c>
+      <c r="L49" s="2" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="50" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>80</v>
+        <v>28</v>
       </c>
       <c r="B50" t="s">
-        <v>128</v>
+        <v>25</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="E50" t="s">
-        <v>9</v>
-      </c>
-      <c r="F50">
-        <v>1979</v>
+        <v>48</v>
       </c>
     </row>
     <row r="51" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>125</v>
+        <v>80</v>
       </c>
       <c r="B51" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>126</v>
+        <v>81</v>
+      </c>
+      <c r="E51" t="s">
+        <v>9</v>
+      </c>
+      <c r="F51">
+        <v>1979</v>
       </c>
     </row>
     <row r="52" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>179</v>
+        <v>125</v>
       </c>
       <c r="B52" t="s">
-        <v>165</v>
+        <v>124</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>180</v>
+        <v>126</v>
       </c>
     </row>
     <row r="53" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
+        <v>179</v>
+      </c>
+      <c r="B53" t="s">
+        <v>165</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="54" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
         <v>78</v>
       </c>
-      <c r="B53" t="s">
+      <c r="B54" t="s">
         <v>25</v>
       </c>
-      <c r="C53" s="2" t="s">
+      <c r="C54" s="2" t="s">
         <v>79</v>
-      </c>
-      <c r="E53" t="s">
-        <v>9</v>
-      </c>
-      <c r="F53">
-        <v>1979</v>
-      </c>
-    </row>
-    <row r="54" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A54" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="B54" t="s">
-        <v>83</v>
-      </c>
-      <c r="C54" s="2" t="s">
-        <v>84</v>
       </c>
       <c r="E54" t="s">
         <v>9</v>
@@ -2890,13 +2941,13 @@
     </row>
     <row r="55" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A55" s="3" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B55" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="E55" t="s">
         <v>9</v>
@@ -2904,225 +2955,225 @@
       <c r="F55">
         <v>1979</v>
       </c>
-      <c r="G55">
+    </row>
+    <row r="56" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A56" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="B56" t="s">
+        <v>86</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="E56" t="s">
+        <v>9</v>
+      </c>
+      <c r="F56">
+        <v>1979</v>
+      </c>
+      <c r="G56">
         <v>2009</v>
-      </c>
-    </row>
-    <row r="56" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A56" t="s">
-        <v>27</v>
-      </c>
-      <c r="B56" t="s">
-        <v>25</v>
-      </c>
-      <c r="C56" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="Q56" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="57" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>120</v>
+        <v>27</v>
       </c>
       <c r="B57" t="s">
-        <v>259</v>
+        <v>25</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="I57" t="s">
-        <v>20</v>
+        <v>49</v>
+      </c>
+      <c r="Q57" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="58" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>5</v>
+        <v>120</v>
       </c>
       <c r="B58" t="s">
-        <v>25</v>
+        <v>259</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D58" t="s">
-        <v>94</v>
-      </c>
-      <c r="E58" t="s">
-        <v>9</v>
-      </c>
-      <c r="F58">
-        <v>2002</v>
-      </c>
-      <c r="H58" t="s">
-        <v>16</v>
+        <v>119</v>
       </c>
       <c r="I58" t="s">
-        <v>248</v>
-      </c>
-      <c r="Q58" t="s">
-        <v>44</v>
+        <v>20</v>
       </c>
     </row>
     <row r="59" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
+        <v>5</v>
+      </c>
+      <c r="B59" t="s">
+        <v>25</v>
+      </c>
+      <c r="C59" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D59" t="s">
+        <v>94</v>
+      </c>
+      <c r="E59" t="s">
+        <v>9</v>
+      </c>
+      <c r="F59">
+        <v>2002</v>
+      </c>
+      <c r="H59" t="s">
+        <v>16</v>
+      </c>
+      <c r="I59" t="s">
+        <v>248</v>
+      </c>
+      <c r="Q59" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="60" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
         <v>240</v>
       </c>
-      <c r="B59" t="s">
+      <c r="B60" t="s">
         <v>237</v>
       </c>
-      <c r="C59" s="2" t="s">
+      <c r="C60" s="2" t="s">
         <v>243</v>
       </c>
-      <c r="H59" t="s">
-        <v>16</v>
-      </c>
-      <c r="I59" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="60" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A60" s="1" t="s">
+      <c r="H60" t="s">
+        <v>16</v>
+      </c>
+      <c r="I60" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="61" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A61" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B60" t="s">
+      <c r="B61" t="s">
         <v>25</v>
       </c>
-      <c r="C60" s="2" t="s">
+      <c r="C61" s="2" t="s">
         <v>52</v>
-      </c>
-    </row>
-    <row r="61" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A61" t="s">
-        <v>232</v>
-      </c>
-      <c r="B61" t="s">
-        <v>250</v>
-      </c>
-      <c r="C61" s="2" t="s">
-        <v>231</v>
       </c>
     </row>
     <row r="62" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>390</v>
+        <v>232</v>
       </c>
       <c r="B62" t="s">
-        <v>83</v>
+        <v>250</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>392</v>
-      </c>
-      <c r="D62" t="s">
-        <v>391</v>
-      </c>
-      <c r="E62" t="s">
-        <v>9</v>
-      </c>
-      <c r="F62">
-        <v>2007</v>
-      </c>
-      <c r="G62">
-        <v>2015</v>
-      </c>
-      <c r="H62" t="s">
-        <v>348</v>
-      </c>
-      <c r="I62" t="s">
-        <v>349</v>
-      </c>
-      <c r="Q62" t="s">
-        <v>393</v>
+        <v>231</v>
       </c>
     </row>
     <row r="63" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>276</v>
+        <v>390</v>
       </c>
       <c r="B63" t="s">
-        <v>124</v>
+        <v>83</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>277</v>
+        <v>392</v>
+      </c>
+      <c r="D63" t="s">
+        <v>391</v>
+      </c>
+      <c r="E63" t="s">
+        <v>9</v>
       </c>
       <c r="F63">
-        <v>1948</v>
+        <v>2007</v>
       </c>
       <c r="G63">
-        <v>2000</v>
+        <v>2015</v>
       </c>
       <c r="H63" t="s">
-        <v>16</v>
+        <v>348</v>
       </c>
       <c r="I63" t="s">
-        <v>20</v>
+        <v>349</v>
+      </c>
+      <c r="Q63" t="s">
+        <v>393</v>
       </c>
     </row>
     <row r="64" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>449</v>
+        <v>276</v>
       </c>
       <c r="B64" t="s">
-        <v>250</v>
+        <v>124</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>448</v>
-      </c>
-      <c r="E64" t="s">
-        <v>14</v>
+        <v>277</v>
       </c>
       <c r="F64">
-        <v>-4000</v>
+        <v>1948</v>
       </c>
       <c r="G64">
         <v>2000</v>
       </c>
       <c r="H64" t="s">
-        <v>348</v>
+        <v>16</v>
       </c>
       <c r="I64" t="s">
-        <v>349</v>
-      </c>
-      <c r="J64" s="2" t="s">
-        <v>450</v>
-      </c>
-      <c r="N64" s="2" t="s">
-        <v>451</v>
+        <v>20</v>
       </c>
     </row>
     <row r="65" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>224</v>
+        <v>449</v>
       </c>
       <c r="B65" t="s">
-        <v>40</v>
+        <v>250</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>225</v>
+        <v>448</v>
+      </c>
+      <c r="E65" t="s">
+        <v>14</v>
       </c>
       <c r="F65">
-        <v>1964</v>
+        <v>-4000</v>
       </c>
       <c r="G65">
-        <v>2008</v>
+        <v>2000</v>
       </c>
       <c r="H65" t="s">
-        <v>16</v>
+        <v>348</v>
       </c>
       <c r="I65" t="s">
-        <v>20</v>
+        <v>349</v>
+      </c>
+      <c r="J65" s="2" t="s">
+        <v>450</v>
+      </c>
+      <c r="N65" s="2" t="s">
+        <v>451</v>
       </c>
     </row>
     <row r="66" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>285</v>
+        <v>224</v>
       </c>
       <c r="B66" t="s">
-        <v>250</v>
+        <v>40</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>286</v>
+        <v>225</v>
+      </c>
+      <c r="F66">
+        <v>1964</v>
+      </c>
+      <c r="G66">
+        <v>2008</v>
       </c>
       <c r="H66" t="s">
         <v>16</v>
@@ -3133,130 +3184,151 @@
     </row>
     <row r="67" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>205</v>
+        <v>285</v>
       </c>
       <c r="B67" t="s">
-        <v>40</v>
+        <v>250</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>204</v>
-      </c>
-      <c r="F67">
-        <v>2006</v>
+        <v>286</v>
+      </c>
+      <c r="H67" t="s">
+        <v>16</v>
+      </c>
+      <c r="I67" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="68" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>200</v>
+        <v>205</v>
       </c>
       <c r="B68" t="s">
-        <v>99</v>
+        <v>40</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="F68">
-        <v>1980</v>
-      </c>
-      <c r="G68">
-        <v>2007</v>
-      </c>
-      <c r="Q68" t="s">
-        <v>18</v>
+        <v>2006</v>
       </c>
     </row>
     <row r="69" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>89</v>
+        <v>200</v>
       </c>
       <c r="B69" t="s">
-        <v>25</v>
+        <v>99</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="E69" t="s">
-        <v>34</v>
+        <v>201</v>
       </c>
       <c r="F69">
-        <v>1972</v>
-      </c>
-      <c r="H69" t="s">
-        <v>16</v>
-      </c>
-      <c r="I69" t="s">
-        <v>20</v>
+        <v>1980</v>
+      </c>
+      <c r="G69">
+        <v>2007</v>
+      </c>
+      <c r="Q69" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="70" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>104</v>
+        <v>468</v>
       </c>
       <c r="B70" t="s">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>106</v>
+        <v>464</v>
       </c>
       <c r="E70" t="s">
-        <v>105</v>
+        <v>14</v>
       </c>
       <c r="F70">
-        <v>1980</v>
+        <v>1816</v>
+      </c>
+      <c r="G70">
+        <v>2001</v>
+      </c>
+      <c r="H70" t="s">
+        <v>348</v>
+      </c>
+      <c r="I70" t="s">
+        <v>349</v>
+      </c>
+      <c r="J70" s="2" t="s">
+        <v>469</v>
+      </c>
+      <c r="K70" s="2" t="s">
+        <v>470</v>
+      </c>
+      <c r="L70" s="2" t="s">
+        <v>471</v>
       </c>
     </row>
     <row r="71" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>460</v>
+        <v>89</v>
       </c>
       <c r="B71" t="s">
         <v>25</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>461</v>
-      </c>
-      <c r="D71" t="s">
-        <v>363</v>
+        <v>88</v>
       </c>
       <c r="E71" t="s">
-        <v>105</v>
+        <v>34</v>
       </c>
       <c r="F71">
-        <v>2009</v>
+        <v>1972</v>
       </c>
       <c r="H71" t="s">
-        <v>348</v>
+        <v>16</v>
       </c>
       <c r="I71" t="s">
-        <v>301</v>
+        <v>20</v>
       </c>
     </row>
     <row r="72" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>62</v>
+        <v>104</v>
       </c>
       <c r="B72" t="s">
         <v>25</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>63</v>
+        <v>106</v>
+      </c>
+      <c r="E72" t="s">
+        <v>105</v>
+      </c>
+      <c r="F72">
+        <v>1980</v>
       </c>
     </row>
     <row r="73" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>311</v>
+        <v>460</v>
       </c>
       <c r="B73" t="s">
-        <v>165</v>
+        <v>25</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>312</v>
+        <v>461</v>
+      </c>
+      <c r="D73" t="s">
+        <v>363</v>
       </c>
       <c r="E73" t="s">
-        <v>14</v>
+        <v>105</v>
+      </c>
+      <c r="F73">
+        <v>2009</v>
       </c>
       <c r="H73" t="s">
-        <v>16</v>
+        <v>348</v>
       </c>
       <c r="I73" t="s">
         <v>301</v>
@@ -3264,127 +3336,124 @@
     </row>
     <row r="74" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>281</v>
+        <v>62</v>
       </c>
       <c r="B74" t="s">
-        <v>237</v>
+        <v>25</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>282</v>
-      </c>
-      <c r="H74" t="s">
-        <v>16</v>
-      </c>
-      <c r="I74" t="s">
-        <v>20</v>
+        <v>63</v>
       </c>
     </row>
     <row r="75" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>418</v>
+        <v>311</v>
       </c>
       <c r="B75" t="s">
-        <v>86</v>
+        <v>165</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>419</v>
+        <v>312</v>
       </c>
       <c r="E75" t="s">
-        <v>420</v>
-      </c>
-      <c r="F75">
-        <v>1948</v>
-      </c>
-      <c r="G75">
-        <v>2012</v>
+        <v>14</v>
       </c>
       <c r="H75" t="s">
-        <v>348</v>
+        <v>16</v>
       </c>
       <c r="I75" t="s">
-        <v>349</v>
-      </c>
-      <c r="K75" s="2" t="s">
-        <v>421</v>
-      </c>
-      <c r="Q75" t="s">
-        <v>422</v>
+        <v>301</v>
       </c>
     </row>
     <row r="76" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>151</v>
+        <v>281</v>
       </c>
       <c r="B76" t="s">
-        <v>40</v>
+        <v>237</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="E76" t="s">
-        <v>14</v>
+        <v>282</v>
+      </c>
+      <c r="H76" t="s">
+        <v>16</v>
+      </c>
+      <c r="I76" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="77" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>242</v>
+        <v>418</v>
       </c>
       <c r="B77" t="s">
-        <v>237</v>
+        <v>86</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>243</v>
+        <v>419</v>
+      </c>
+      <c r="E77" t="s">
+        <v>420</v>
+      </c>
+      <c r="F77">
+        <v>1948</v>
+      </c>
+      <c r="G77">
+        <v>2012</v>
       </c>
       <c r="H77" t="s">
-        <v>16</v>
+        <v>348</v>
       </c>
       <c r="I77" t="s">
-        <v>20</v>
+        <v>349</v>
+      </c>
+      <c r="K77" s="2" t="s">
+        <v>421</v>
+      </c>
+      <c r="Q77" t="s">
+        <v>422</v>
       </c>
     </row>
     <row r="78" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>292</v>
+        <v>151</v>
       </c>
       <c r="B78" t="s">
-        <v>99</v>
+        <v>40</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>291</v>
-      </c>
-      <c r="H78" t="s">
-        <v>16</v>
-      </c>
-      <c r="I78" t="s">
-        <v>20</v>
+        <v>152</v>
+      </c>
+      <c r="E78" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="79" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>153</v>
+        <v>242</v>
       </c>
       <c r="B79" t="s">
-        <v>259</v>
+        <v>237</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>154</v>
+        <v>243</v>
+      </c>
+      <c r="H79" t="s">
+        <v>16</v>
+      </c>
+      <c r="I79" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="80" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>228</v>
+        <v>292</v>
       </c>
       <c r="B80" t="s">
-        <v>40</v>
+        <v>99</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>225</v>
-      </c>
-      <c r="F80">
-        <v>1989</v>
-      </c>
-      <c r="G80">
-        <v>2017</v>
+        <v>291</v>
       </c>
       <c r="H80" t="s">
         <v>16</v>
@@ -3395,41 +3464,47 @@
     </row>
     <row r="81" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>245</v>
+        <v>153</v>
       </c>
       <c r="B81" t="s">
-        <v>237</v>
+        <v>259</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>244</v>
-      </c>
-      <c r="H81" t="s">
-        <v>16</v>
-      </c>
-      <c r="I81" t="s">
-        <v>20</v>
+        <v>154</v>
       </c>
     </row>
     <row r="82" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>100</v>
+        <v>228</v>
       </c>
       <c r="B82" t="s">
-        <v>99</v>
+        <v>40</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>101</v>
+        <v>225</v>
+      </c>
+      <c r="F82">
+        <v>1989</v>
+      </c>
+      <c r="G82">
+        <v>2017</v>
+      </c>
+      <c r="H82" t="s">
+        <v>16</v>
+      </c>
+      <c r="I82" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="83" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>239</v>
+        <v>245</v>
       </c>
       <c r="B83" t="s">
         <v>237</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="H83" t="s">
         <v>16</v>
@@ -3440,45 +3515,24 @@
     </row>
     <row r="84" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>254</v>
+        <v>100</v>
       </c>
       <c r="B84" t="s">
-        <v>55</v>
+        <v>99</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>253</v>
-      </c>
-      <c r="E84" t="s">
-        <v>255</v>
-      </c>
-      <c r="F84">
-        <v>1960</v>
-      </c>
-      <c r="G84">
-        <v>2014</v>
-      </c>
-      <c r="H84" t="s">
-        <v>16</v>
-      </c>
-      <c r="I84" t="s">
-        <v>20</v>
+        <v>101</v>
       </c>
     </row>
     <row r="85" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>270</v>
+        <v>239</v>
       </c>
       <c r="B85" t="s">
-        <v>55</v>
+        <v>237</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>271</v>
-      </c>
-      <c r="F85">
-        <v>1990</v>
-      </c>
-      <c r="G85">
-        <v>2010</v>
+        <v>243</v>
       </c>
       <c r="H85" t="s">
         <v>16</v>
@@ -3489,171 +3543,174 @@
     </row>
     <row r="86" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>117</v>
+        <v>254</v>
       </c>
       <c r="B86" t="s">
         <v>55</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>118</v>
+        <v>253</v>
+      </c>
+      <c r="E86" t="s">
+        <v>255</v>
+      </c>
+      <c r="F86">
+        <v>1960</v>
+      </c>
+      <c r="G86">
+        <v>2014</v>
+      </c>
+      <c r="H86" t="s">
+        <v>16</v>
       </c>
       <c r="I86" t="s">
         <v>20</v>
       </c>
-      <c r="Q86" t="s">
-        <v>18</v>
-      </c>
     </row>
     <row r="87" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A87" s="1" t="s">
-        <v>23</v>
+      <c r="A87" t="s">
+        <v>270</v>
       </c>
       <c r="B87" t="s">
-        <v>25</v>
+        <v>55</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>53</v>
+        <v>271</v>
+      </c>
+      <c r="F87">
+        <v>1990</v>
+      </c>
+      <c r="G87">
+        <v>2010</v>
+      </c>
+      <c r="H87" t="s">
+        <v>16</v>
+      </c>
+      <c r="I87" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="88" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>300</v>
+        <v>117</v>
       </c>
       <c r="B88" t="s">
+        <v>55</v>
+      </c>
+      <c r="C88" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="I88" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q88" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="89" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A89" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B89" t="s">
         <v>25</v>
       </c>
-      <c r="C88" s="2" t="s">
-        <v>298</v>
-      </c>
-      <c r="E88" t="s">
-        <v>299</v>
-      </c>
-      <c r="F88">
-        <v>1969</v>
-      </c>
-      <c r="H88" t="s">
-        <v>16</v>
-      </c>
-      <c r="I88" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="89" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A89" t="s">
-        <v>332</v>
-      </c>
-      <c r="B89" t="s">
-        <v>134</v>
-      </c>
       <c r="C89" s="2" t="s">
-        <v>333</v>
-      </c>
-      <c r="E89" t="s">
-        <v>334</v>
-      </c>
-      <c r="H89" t="s">
-        <v>16</v>
-      </c>
-      <c r="I89" t="s">
-        <v>20</v>
+        <v>53</v>
       </c>
     </row>
     <row r="90" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>267</v>
+        <v>300</v>
       </c>
       <c r="B90" t="s">
-        <v>250</v>
+        <v>25</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>266</v>
-      </c>
-      <c r="D90" t="s">
-        <v>269</v>
+        <v>298</v>
       </c>
       <c r="E90" t="s">
-        <v>268</v>
+        <v>299</v>
       </c>
       <c r="F90">
-        <v>1970</v>
-      </c>
-      <c r="G90">
-        <v>2014</v>
+        <v>1969</v>
       </c>
       <c r="H90" t="s">
         <v>16</v>
       </c>
       <c r="I90" t="s">
-        <v>20</v>
+        <v>249</v>
       </c>
     </row>
     <row r="91" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>407</v>
+        <v>332</v>
       </c>
       <c r="B91" t="s">
-        <v>40</v>
+        <v>134</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>406</v>
-      </c>
-      <c r="D91" t="s">
-        <v>408</v>
+        <v>333</v>
       </c>
       <c r="E91" t="s">
-        <v>14</v>
-      </c>
-      <c r="F91">
-        <v>1949</v>
-      </c>
-      <c r="G91">
-        <v>2013</v>
+        <v>334</v>
       </c>
       <c r="H91" t="s">
-        <v>348</v>
+        <v>16</v>
       </c>
       <c r="I91" t="s">
-        <v>349</v>
+        <v>20</v>
       </c>
     </row>
     <row r="92" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>96</v>
+        <v>267</v>
       </c>
       <c r="B92" t="s">
-        <v>25</v>
+        <v>250</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>90</v>
+        <v>266</v>
+      </c>
+      <c r="D92" t="s">
+        <v>269</v>
       </c>
       <c r="E92" t="s">
-        <v>69</v>
+        <v>268</v>
       </c>
       <c r="F92">
-        <v>1995</v>
+        <v>1970</v>
+      </c>
+      <c r="G92">
+        <v>2014</v>
+      </c>
+      <c r="H92" t="s">
+        <v>16</v>
+      </c>
+      <c r="I92" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="93" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>404</v>
+        <v>407</v>
       </c>
       <c r="B93" t="s">
-        <v>83</v>
+        <v>40</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>403</v>
+        <v>406</v>
       </c>
       <c r="D93" t="s">
-        <v>405</v>
+        <v>408</v>
       </c>
       <c r="E93" t="s">
         <v>14</v>
       </c>
       <c r="F93">
-        <v>1875</v>
+        <v>1949</v>
       </c>
       <c r="G93">
-        <v>2004</v>
+        <v>2013</v>
       </c>
       <c r="H93" t="s">
         <v>348</v>
@@ -3664,140 +3721,149 @@
     </row>
     <row r="94" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>454</v>
+        <v>96</v>
       </c>
       <c r="B94" t="s">
         <v>25</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>455</v>
+        <v>90</v>
       </c>
       <c r="E94" t="s">
-        <v>456</v>
+        <v>69</v>
       </c>
       <c r="F94">
-        <v>2006</v>
-      </c>
-      <c r="G94">
-        <v>2016</v>
-      </c>
-      <c r="H94" t="s">
-        <v>348</v>
-      </c>
-      <c r="I94" t="s">
-        <v>349</v>
-      </c>
-      <c r="J94" s="2" t="s">
-        <v>457</v>
-      </c>
-      <c r="L94" s="2" t="s">
-        <v>458</v>
-      </c>
-      <c r="Q94" t="s">
-        <v>459</v>
+        <v>1995</v>
       </c>
     </row>
     <row r="95" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>11</v>
+        <v>404</v>
       </c>
       <c r="B95" t="s">
-        <v>25</v>
+        <v>83</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>12</v>
+        <v>403</v>
       </c>
       <c r="D95" t="s">
-        <v>95</v>
+        <v>405</v>
       </c>
       <c r="E95" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="F95">
-        <v>2007</v>
+        <v>1875</v>
+      </c>
+      <c r="G95">
+        <v>2004</v>
       </c>
       <c r="H95" t="s">
-        <v>16</v>
+        <v>348</v>
       </c>
       <c r="I95" t="s">
-        <v>21</v>
+        <v>349</v>
       </c>
     </row>
     <row r="96" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>223</v>
+        <v>454</v>
       </c>
       <c r="B96" t="s">
-        <v>124</v>
+        <v>25</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>222</v>
+        <v>455</v>
+      </c>
+      <c r="E96" t="s">
+        <v>456</v>
       </c>
       <c r="F96">
-        <v>1</v>
+        <v>2006</v>
       </c>
       <c r="G96">
-        <v>2010</v>
+        <v>2016</v>
       </c>
       <c r="H96" t="s">
-        <v>16</v>
+        <v>348</v>
       </c>
       <c r="I96" t="s">
-        <v>20</v>
+        <v>349</v>
+      </c>
+      <c r="J96" s="2" t="s">
+        <v>457</v>
+      </c>
+      <c r="L96" s="2" t="s">
+        <v>458</v>
+      </c>
+      <c r="Q96" t="s">
+        <v>459</v>
       </c>
     </row>
     <row r="97" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>226</v>
+        <v>11</v>
       </c>
       <c r="B97" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>225</v>
+        <v>12</v>
+      </c>
+      <c r="D97" t="s">
+        <v>95</v>
+      </c>
+      <c r="E97" t="s">
+        <v>10</v>
       </c>
       <c r="F97">
-        <v>1946</v>
-      </c>
-      <c r="G97">
-        <v>2016</v>
+        <v>2007</v>
       </c>
       <c r="H97" t="s">
         <v>16</v>
       </c>
       <c r="I97" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="98" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>97</v>
+        <v>223</v>
       </c>
       <c r="B98" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>98</v>
+        <v>222</v>
+      </c>
+      <c r="F98">
+        <v>1</v>
+      </c>
+      <c r="G98">
+        <v>2010</v>
+      </c>
+      <c r="H98" t="s">
+        <v>16</v>
+      </c>
+      <c r="I98" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="99" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>278</v>
+        <v>226</v>
       </c>
       <c r="B99" t="s">
-        <v>124</v>
+        <v>40</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>279</v>
-      </c>
-      <c r="E99" t="s">
-        <v>280</v>
+        <v>225</v>
       </c>
       <c r="F99">
-        <v>1890</v>
+        <v>1946</v>
       </c>
       <c r="G99">
-        <v>1996</v>
+        <v>2016</v>
       </c>
       <c r="H99" t="s">
         <v>16</v>
@@ -3808,287 +3874,287 @@
     </row>
     <row r="100" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>156</v>
+        <v>97</v>
       </c>
       <c r="B100" t="s">
-        <v>25</v>
+        <v>128</v>
       </c>
       <c r="C100" s="2" t="s">
-        <v>154</v>
+        <v>98</v>
       </c>
     </row>
     <row r="101" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>413</v>
+        <v>278</v>
       </c>
       <c r="B101" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>414</v>
+        <v>279</v>
       </c>
       <c r="E101" t="s">
-        <v>415</v>
+        <v>280</v>
       </c>
       <c r="F101">
-        <v>1946</v>
+        <v>1890</v>
       </c>
       <c r="G101">
-        <v>2014</v>
+        <v>1996</v>
       </c>
       <c r="H101" t="s">
-        <v>348</v>
+        <v>16</v>
       </c>
       <c r="I101" t="s">
-        <v>349</v>
-      </c>
-      <c r="N101" s="2" t="s">
-        <v>416</v>
-      </c>
-      <c r="Q101" t="s">
-        <v>417</v>
+        <v>20</v>
       </c>
     </row>
     <row r="102" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>229</v>
+        <v>156</v>
       </c>
       <c r="B102" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="C102" s="2" t="s">
-        <v>225</v>
-      </c>
-      <c r="F102">
-        <v>1952</v>
-      </c>
-      <c r="G102">
-        <v>1997</v>
-      </c>
-      <c r="H102" t="s">
-        <v>16</v>
-      </c>
-      <c r="I102" t="s">
-        <v>20</v>
+        <v>154</v>
       </c>
     </row>
     <row r="103" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>293</v>
+        <v>413</v>
       </c>
       <c r="B103" t="s">
-        <v>40</v>
+        <v>128</v>
       </c>
       <c r="C103" s="2" t="s">
-        <v>294</v>
+        <v>414</v>
+      </c>
+      <c r="E103" t="s">
+        <v>415</v>
       </c>
       <c r="F103">
-        <v>2004</v>
+        <v>1946</v>
       </c>
       <c r="G103">
-        <v>2006</v>
+        <v>2014</v>
       </c>
       <c r="H103" t="s">
-        <v>16</v>
+        <v>348</v>
       </c>
       <c r="I103" t="s">
-        <v>20</v>
+        <v>349</v>
+      </c>
+      <c r="N103" s="2" t="s">
+        <v>416</v>
+      </c>
+      <c r="Q103" t="s">
+        <v>417</v>
       </c>
     </row>
     <row r="104" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>102</v>
+        <v>229</v>
       </c>
       <c r="B104" t="s">
-        <v>99</v>
+        <v>40</v>
       </c>
       <c r="C104" s="2" t="s">
-        <v>103</v>
+        <v>225</v>
+      </c>
+      <c r="F104">
+        <v>1952</v>
+      </c>
+      <c r="G104">
+        <v>1997</v>
+      </c>
+      <c r="H104" t="s">
+        <v>16</v>
+      </c>
+      <c r="I104" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="105" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>289</v>
+        <v>293</v>
       </c>
       <c r="B105" t="s">
-        <v>124</v>
+        <v>40</v>
       </c>
       <c r="C105" s="2" t="s">
-        <v>290</v>
+        <v>294</v>
+      </c>
+      <c r="F105">
+        <v>2004</v>
+      </c>
+      <c r="G105">
+        <v>2006</v>
+      </c>
+      <c r="H105" t="s">
+        <v>16</v>
+      </c>
+      <c r="I105" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="106" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>246</v>
+        <v>102</v>
       </c>
       <c r="B106" t="s">
-        <v>165</v>
+        <v>99</v>
       </c>
       <c r="C106" s="2" t="s">
-        <v>247</v>
-      </c>
-      <c r="E106" t="s">
-        <v>14</v>
-      </c>
-      <c r="F106">
-        <v>1960</v>
-      </c>
-      <c r="G106">
-        <v>2006</v>
-      </c>
-      <c r="H106" t="s">
-        <v>16</v>
-      </c>
-      <c r="I106" t="s">
-        <v>249</v>
+        <v>103</v>
       </c>
     </row>
     <row r="107" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>365</v>
+        <v>289</v>
       </c>
       <c r="B107" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="C107" s="2" t="s">
-        <v>364</v>
-      </c>
-      <c r="D107" t="s">
-        <v>370</v>
-      </c>
-      <c r="E107" t="s">
-        <v>366</v>
-      </c>
-      <c r="F107">
-        <v>1906</v>
-      </c>
-      <c r="G107">
-        <v>2013</v>
-      </c>
-      <c r="H107" t="s">
-        <v>367</v>
-      </c>
-      <c r="I107" t="s">
-        <v>368</v>
-      </c>
-      <c r="Q107" t="s">
-        <v>369</v>
+        <v>290</v>
       </c>
     </row>
     <row r="108" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>208</v>
+        <v>246</v>
       </c>
       <c r="B108" t="s">
-        <v>124</v>
+        <v>165</v>
       </c>
       <c r="C108" s="2" t="s">
-        <v>209</v>
+        <v>247</v>
+      </c>
+      <c r="E108" t="s">
+        <v>14</v>
       </c>
       <c r="F108">
-        <v>1932</v>
+        <v>1960</v>
       </c>
       <c r="G108">
-        <v>2014</v>
+        <v>2006</v>
       </c>
       <c r="H108" t="s">
         <v>16</v>
       </c>
       <c r="I108" t="s">
-        <v>20</v>
+        <v>249</v>
       </c>
     </row>
     <row r="109" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>137</v>
+        <v>365</v>
       </c>
       <c r="B109" t="s">
-        <v>259</v>
+        <v>128</v>
       </c>
       <c r="C109" s="2" t="s">
-        <v>138</v>
+        <v>364</v>
+      </c>
+      <c r="D109" t="s">
+        <v>370</v>
+      </c>
+      <c r="E109" t="s">
+        <v>366</v>
+      </c>
+      <c r="F109">
+        <v>1906</v>
+      </c>
+      <c r="G109">
+        <v>2013</v>
+      </c>
+      <c r="H109" t="s">
+        <v>367</v>
+      </c>
+      <c r="I109" t="s">
+        <v>368</v>
+      </c>
+      <c r="Q109" t="s">
+        <v>369</v>
       </c>
     </row>
     <row r="110" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>155</v>
+        <v>208</v>
       </c>
       <c r="B110" t="s">
-        <v>259</v>
+        <v>124</v>
       </c>
       <c r="C110" s="2" t="s">
-        <v>154</v>
+        <v>209</v>
+      </c>
+      <c r="F110">
+        <v>1932</v>
+      </c>
+      <c r="G110">
+        <v>2014</v>
+      </c>
+      <c r="H110" t="s">
+        <v>16</v>
+      </c>
+      <c r="I110" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="111" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>57</v>
+        <v>137</v>
       </c>
       <c r="B111" t="s">
-        <v>128</v>
+        <v>259</v>
       </c>
       <c r="C111" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="Q111" t="s">
-        <v>17</v>
+        <v>138</v>
       </c>
     </row>
     <row r="112" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>129</v>
+        <v>155</v>
       </c>
       <c r="B112" t="s">
         <v>259</v>
       </c>
       <c r="C112" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="E112" t="s">
-        <v>131</v>
-      </c>
-      <c r="F112">
-        <v>1945</v>
-      </c>
-      <c r="G112">
-        <v>2008</v>
-      </c>
-      <c r="I112" t="s">
-        <v>20</v>
+        <v>154</v>
       </c>
     </row>
     <row r="113" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>148</v>
+        <v>57</v>
       </c>
       <c r="B113" t="s">
         <v>128</v>
       </c>
       <c r="C113" s="2" t="s">
-        <v>147</v>
+        <v>58</v>
+      </c>
+      <c r="Q113" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="114" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>233</v>
+        <v>129</v>
       </c>
       <c r="B114" t="s">
-        <v>165</v>
+        <v>259</v>
       </c>
       <c r="C114" s="2" t="s">
-        <v>234</v>
+        <v>130</v>
       </c>
       <c r="E114" t="s">
-        <v>14</v>
+        <v>131</v>
       </c>
       <c r="F114">
-        <v>2012</v>
+        <v>1945</v>
       </c>
       <c r="G114">
-        <v>2016</v>
-      </c>
-      <c r="H114" t="s">
-        <v>16</v>
+        <v>2008</v>
       </c>
       <c r="I114" t="s">
         <v>20</v>
@@ -4096,56 +4162,59 @@
     </row>
     <row r="115" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>35</v>
+        <v>148</v>
       </c>
       <c r="B115" t="s">
-        <v>25</v>
+        <v>128</v>
       </c>
       <c r="C115" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="D115" t="s">
-        <v>37</v>
-      </c>
-      <c r="E115" t="s">
-        <v>14</v>
-      </c>
-      <c r="F115">
-        <v>2001</v>
-      </c>
-      <c r="H115" t="s">
-        <v>16</v>
-      </c>
-      <c r="I115" t="s">
-        <v>20</v>
+        <v>147</v>
       </c>
     </row>
     <row r="116" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>185</v>
+        <v>233</v>
       </c>
       <c r="B116" t="s">
-        <v>128</v>
+        <v>165</v>
       </c>
       <c r="C116" s="2" t="s">
-        <v>186</v>
+        <v>234</v>
+      </c>
+      <c r="E116" t="s">
+        <v>14</v>
+      </c>
+      <c r="F116">
+        <v>2012</v>
+      </c>
+      <c r="G116">
+        <v>2016</v>
+      </c>
+      <c r="H116" t="s">
+        <v>16</v>
+      </c>
+      <c r="I116" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="117" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>210</v>
+        <v>35</v>
       </c>
       <c r="B117" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="C117" s="2" t="s">
-        <v>211</v>
+        <v>36</v>
+      </c>
+      <c r="D117" t="s">
+        <v>37</v>
+      </c>
+      <c r="E117" t="s">
+        <v>14</v>
       </c>
       <c r="F117">
-        <v>1976</v>
-      </c>
-      <c r="G117">
-        <v>2016</v>
+        <v>2001</v>
       </c>
       <c r="H117" t="s">
         <v>16</v>
@@ -4156,111 +4225,93 @@
     </row>
     <row r="118" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>426</v>
+        <v>185</v>
       </c>
       <c r="B118" t="s">
-        <v>86</v>
+        <v>128</v>
       </c>
       <c r="C118" s="2" t="s">
-        <v>427</v>
-      </c>
-      <c r="E118" t="s">
-        <v>34</v>
-      </c>
-      <c r="F118">
-        <v>2015</v>
-      </c>
-      <c r="G118">
-        <v>2016</v>
-      </c>
-      <c r="H118" t="s">
-        <v>348</v>
-      </c>
-      <c r="I118" t="s">
-        <v>349</v>
-      </c>
-      <c r="K118" s="2" t="s">
-        <v>428</v>
+        <v>186</v>
       </c>
     </row>
     <row r="119" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>144</v>
+        <v>210</v>
       </c>
       <c r="B119" t="s">
-        <v>60</v>
+        <v>40</v>
       </c>
       <c r="C119" s="2" t="s">
-        <v>143</v>
+        <v>211</v>
       </c>
       <c r="F119">
-        <v>1800</v>
+        <v>1976</v>
       </c>
       <c r="G119">
-        <v>2013</v>
+        <v>2016</v>
+      </c>
+      <c r="H119" t="s">
+        <v>16</v>
+      </c>
+      <c r="I119" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="120" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>122</v>
+        <v>426</v>
       </c>
       <c r="B120" t="s">
-        <v>259</v>
+        <v>86</v>
       </c>
       <c r="C120" s="2" t="s">
-        <v>121</v>
+        <v>427</v>
+      </c>
+      <c r="E120" t="s">
+        <v>34</v>
+      </c>
+      <c r="F120">
+        <v>2015</v>
+      </c>
+      <c r="G120">
+        <v>2016</v>
+      </c>
+      <c r="H120" t="s">
+        <v>348</v>
       </c>
       <c r="I120" t="s">
-        <v>20</v>
+        <v>349</v>
+      </c>
+      <c r="K120" s="2" t="s">
+        <v>428</v>
       </c>
     </row>
     <row r="121" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>318</v>
+        <v>144</v>
       </c>
       <c r="B121" t="s">
-        <v>250</v>
+        <v>60</v>
       </c>
       <c r="C121" s="2" t="s">
-        <v>319</v>
-      </c>
-      <c r="E121" t="s">
-        <v>320</v>
+        <v>143</v>
       </c>
       <c r="F121">
-        <v>1975</v>
+        <v>1800</v>
       </c>
       <c r="G121">
-        <v>1989</v>
-      </c>
-      <c r="H121" t="s">
-        <v>16</v>
-      </c>
-      <c r="I121" t="s">
-        <v>20</v>
+        <v>2013</v>
       </c>
     </row>
     <row r="122" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>316</v>
+        <v>122</v>
       </c>
       <c r="B122" t="s">
-        <v>250</v>
+        <v>259</v>
       </c>
       <c r="C122" s="2" t="s">
-        <v>317</v>
-      </c>
-      <c r="E122" t="s">
-        <v>105</v>
-      </c>
-      <c r="F122">
-        <v>1950</v>
-      </c>
-      <c r="G122">
-        <v>1996</v>
-      </c>
-      <c r="H122" t="s">
-        <v>16</v>
+        <v>121</v>
       </c>
       <c r="I122" t="s">
         <v>20</v>
@@ -4268,19 +4319,22 @@
     </row>
     <row r="123" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
       <c r="B123" t="s">
-        <v>25</v>
+        <v>250</v>
       </c>
       <c r="C123" s="2" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="E123" t="s">
-        <v>77</v>
+        <v>320</v>
       </c>
       <c r="F123">
-        <v>2010</v>
+        <v>1975</v>
+      </c>
+      <c r="G123">
+        <v>1989</v>
       </c>
       <c r="H123" t="s">
         <v>16</v>
@@ -4291,35 +4345,44 @@
     </row>
     <row r="124" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>141</v>
+        <v>316</v>
       </c>
       <c r="B124" t="s">
-        <v>237</v>
+        <v>250</v>
       </c>
       <c r="C124" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="Q124" t="s">
-        <v>17</v>
+        <v>317</v>
+      </c>
+      <c r="E124" t="s">
+        <v>105</v>
+      </c>
+      <c r="F124">
+        <v>1950</v>
+      </c>
+      <c r="G124">
+        <v>1996</v>
+      </c>
+      <c r="H124" t="s">
+        <v>16</v>
+      </c>
+      <c r="I124" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="125" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>308</v>
+        <v>322</v>
       </c>
       <c r="B125" t="s">
-        <v>250</v>
+        <v>25</v>
       </c>
       <c r="C125" s="2" t="s">
-        <v>309</v>
+        <v>321</v>
       </c>
       <c r="E125" t="s">
-        <v>310</v>
+        <v>77</v>
       </c>
       <c r="F125">
-        <v>1950</v>
-      </c>
-      <c r="G125">
         <v>2010</v>
       </c>
       <c r="H125" t="s">
@@ -4331,30 +4394,36 @@
     </row>
     <row r="126" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>287</v>
+        <v>141</v>
       </c>
       <c r="B126" t="s">
-        <v>134</v>
+        <v>237</v>
       </c>
       <c r="C126" s="2" t="s">
-        <v>288</v>
-      </c>
-      <c r="F126">
-        <v>1990</v>
-      </c>
-      <c r="G126">
-        <v>2008</v>
+        <v>142</v>
+      </c>
+      <c r="Q126" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="127" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>274</v>
+        <v>308</v>
       </c>
       <c r="B127" t="s">
-        <v>55</v>
+        <v>250</v>
       </c>
       <c r="C127" s="2" t="s">
-        <v>275</v>
+        <v>309</v>
+      </c>
+      <c r="E127" t="s">
+        <v>310</v>
+      </c>
+      <c r="F127">
+        <v>1950</v>
+      </c>
+      <c r="G127">
+        <v>2010</v>
       </c>
       <c r="H127" t="s">
         <v>16</v>
@@ -4365,277 +4434,268 @@
     </row>
     <row r="128" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
+        <v>287</v>
+      </c>
+      <c r="B128" t="s">
+        <v>134</v>
+      </c>
+      <c r="C128" s="2" t="s">
+        <v>288</v>
+      </c>
+      <c r="F128">
+        <v>1990</v>
+      </c>
+      <c r="G128">
+        <v>2008</v>
+      </c>
+    </row>
+    <row r="129" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A129" t="s">
+        <v>274</v>
+      </c>
+      <c r="B129" t="s">
+        <v>55</v>
+      </c>
+      <c r="C129" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="H129" t="s">
+        <v>16</v>
+      </c>
+      <c r="I129" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="130" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A130" t="s">
         <v>157</v>
       </c>
-      <c r="B128" t="s">
+      <c r="B130" t="s">
         <v>128</v>
       </c>
-      <c r="C128" s="2" t="s">
+      <c r="C130" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="Q128" t="s">
+      <c r="Q130" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="129" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A129" t="s">
+    <row r="131" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A131" t="s">
         <v>439</v>
       </c>
-      <c r="B129" t="s">
+      <c r="B131" t="s">
         <v>259</v>
       </c>
-      <c r="C129" s="2" t="s">
+      <c r="C131" s="2" t="s">
         <v>438</v>
       </c>
-      <c r="H129" t="s">
+      <c r="H131" t="s">
         <v>348</v>
       </c>
-      <c r="I129" t="s">
+      <c r="I131" t="s">
         <v>349</v>
       </c>
-      <c r="J129" s="2" t="s">
+      <c r="J131" s="2" t="s">
         <v>440</v>
       </c>
-      <c r="K129" s="2" t="s">
+      <c r="K131" s="2" t="s">
         <v>442</v>
       </c>
-      <c r="L129" s="2" t="s">
+      <c r="L131" s="2" t="s">
         <v>441</v>
       </c>
     </row>
-    <row r="130" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A130" t="s">
+    <row r="132" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A132" t="s">
         <v>443</v>
       </c>
-      <c r="B130" t="s">
+      <c r="B132" t="s">
         <v>259</v>
       </c>
-      <c r="C130" s="2" t="s">
+      <c r="C132" s="2" t="s">
         <v>438</v>
       </c>
-      <c r="D130" t="s">
+      <c r="D132" t="s">
         <v>447</v>
-      </c>
-      <c r="F130">
-        <v>1990</v>
-      </c>
-      <c r="G130">
-        <v>2014</v>
-      </c>
-      <c r="H130" t="s">
-        <v>348</v>
-      </c>
-      <c r="I130" t="s">
-        <v>349</v>
-      </c>
-      <c r="J130" s="2" t="s">
-        <v>444</v>
-      </c>
-      <c r="K130" s="2" t="s">
-        <v>445</v>
-      </c>
-      <c r="L130" s="2" t="s">
-        <v>446</v>
-      </c>
-    </row>
-    <row r="131" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A131" t="s">
-        <v>194</v>
-      </c>
-      <c r="B131" t="s">
-        <v>99</v>
-      </c>
-      <c r="C131" s="2" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="132" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A132" t="s">
-        <v>295</v>
-      </c>
-      <c r="B132" t="s">
-        <v>40</v>
-      </c>
-      <c r="C132" s="2" t="s">
-        <v>296</v>
-      </c>
-      <c r="E132" t="s">
-        <v>297</v>
       </c>
       <c r="F132">
         <v>1990</v>
       </c>
       <c r="G132">
-        <v>2015</v>
+        <v>2014</v>
       </c>
       <c r="H132" t="s">
-        <v>16</v>
+        <v>348</v>
       </c>
       <c r="I132" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="133" spans="1:14" x14ac:dyDescent="0.2">
+        <v>349</v>
+      </c>
+      <c r="J132" s="2" t="s">
+        <v>444</v>
+      </c>
+      <c r="K132" s="2" t="s">
+        <v>445</v>
+      </c>
+      <c r="L132" s="2" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="133" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
-        <v>256</v>
+        <v>194</v>
       </c>
       <c r="B133" t="s">
-        <v>250</v>
+        <v>99</v>
       </c>
       <c r="C133" s="2" t="s">
-        <v>257</v>
-      </c>
-      <c r="E133" t="s">
-        <v>258</v>
-      </c>
-      <c r="H133" t="s">
-        <v>16</v>
-      </c>
-      <c r="I133" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="134" spans="1:14" x14ac:dyDescent="0.2">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="134" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
-        <v>227</v>
+        <v>295</v>
       </c>
       <c r="B134" t="s">
         <v>40</v>
       </c>
       <c r="C134" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="E134" t="s">
+        <v>297</v>
+      </c>
+      <c r="F134">
+        <v>1990</v>
+      </c>
+      <c r="G134">
+        <v>2015</v>
+      </c>
+      <c r="H134" t="s">
+        <v>16</v>
+      </c>
+      <c r="I134" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="135" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A135" t="s">
+        <v>256</v>
+      </c>
+      <c r="B135" t="s">
+        <v>250</v>
+      </c>
+      <c r="C135" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="E135" t="s">
+        <v>258</v>
+      </c>
+      <c r="H135" t="s">
+        <v>16</v>
+      </c>
+      <c r="I135" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="136" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A136" t="s">
+        <v>227</v>
+      </c>
+      <c r="B136" t="s">
+        <v>40</v>
+      </c>
+      <c r="C136" s="2" t="s">
         <v>225</v>
       </c>
-      <c r="F134">
+      <c r="F136">
         <v>1955</v>
       </c>
-      <c r="G134">
+      <c r="G136">
         <v>2016</v>
       </c>
-      <c r="H134" t="s">
-        <v>16</v>
-      </c>
-      <c r="I134" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="135" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A135" t="s">
+      <c r="H136" t="s">
+        <v>16</v>
+      </c>
+      <c r="I136" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="137" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A137" t="s">
         <v>230</v>
       </c>
-      <c r="B135" t="s">
+      <c r="B137" t="s">
         <v>40</v>
       </c>
-      <c r="C135" s="2" t="s">
+      <c r="C137" s="2" t="s">
         <v>225</v>
       </c>
-      <c r="F135">
+      <c r="F137">
         <v>1995</v>
       </c>
-      <c r="G135">
+      <c r="G137">
         <v>2016</v>
       </c>
-      <c r="H135" t="s">
-        <v>16</v>
-      </c>
-      <c r="I135" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="136" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A136" t="s">
+      <c r="H137" t="s">
+        <v>16</v>
+      </c>
+      <c r="I137" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="138" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A138" t="s">
         <v>452</v>
-      </c>
-      <c r="B136" t="s">
-        <v>25</v>
-      </c>
-      <c r="C136" s="2" t="s">
-        <v>453</v>
-      </c>
-      <c r="E136" t="s">
-        <v>9</v>
-      </c>
-      <c r="H136" t="s">
-        <v>348</v>
-      </c>
-      <c r="I136" t="s">
-        <v>435</v>
-      </c>
-    </row>
-    <row r="137" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A137" t="s">
-        <v>109</v>
-      </c>
-      <c r="B137" t="s">
-        <v>25</v>
-      </c>
-      <c r="C137" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="E137" t="s">
-        <v>111</v>
-      </c>
-      <c r="F137">
-        <v>1956</v>
-      </c>
-    </row>
-    <row r="138" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A138" t="s">
-        <v>326</v>
       </c>
       <c r="B138" t="s">
         <v>25</v>
       </c>
       <c r="C138" s="2" t="s">
-        <v>327</v>
+        <v>453</v>
       </c>
       <c r="E138" t="s">
-        <v>111</v>
-      </c>
-      <c r="F138">
-        <v>1998</v>
+        <v>9</v>
       </c>
       <c r="H138" t="s">
-        <v>16</v>
+        <v>348</v>
       </c>
       <c r="I138" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="139" spans="1:14" x14ac:dyDescent="0.2">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="139" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
-        <v>91</v>
+        <v>109</v>
       </c>
       <c r="B139" t="s">
         <v>25</v>
       </c>
       <c r="C139" s="2" t="s">
-        <v>93</v>
+        <v>110</v>
       </c>
       <c r="E139" t="s">
-        <v>92</v>
+        <v>111</v>
       </c>
       <c r="F139">
-        <v>1999</v>
-      </c>
-    </row>
-    <row r="140" spans="1:14" x14ac:dyDescent="0.2">
+        <v>1956</v>
+      </c>
+    </row>
+    <row r="140" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
-        <v>314</v>
+        <v>326</v>
       </c>
       <c r="B140" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="C140" s="2" t="s">
-        <v>313</v>
+        <v>327</v>
       </c>
       <c r="E140" t="s">
-        <v>315</v>
+        <v>111</v>
       </c>
       <c r="F140">
-        <v>1950</v>
-      </c>
-      <c r="G140">
-        <v>2004</v>
+        <v>1998</v>
       </c>
       <c r="H140" t="s">
         <v>16</v>
@@ -4644,124 +4704,112 @@
         <v>20</v>
       </c>
     </row>
-    <row r="141" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
-        <v>161</v>
+        <v>91</v>
       </c>
       <c r="B141" t="s">
         <v>25</v>
       </c>
       <c r="C141" s="2" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="142" spans="1:14" x14ac:dyDescent="0.2">
+        <v>93</v>
+      </c>
+      <c r="E141" t="s">
+        <v>92</v>
+      </c>
+      <c r="F141">
+        <v>1999</v>
+      </c>
+    </row>
+    <row r="142" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
-        <v>168</v>
+        <v>314</v>
       </c>
       <c r="B142" t="s">
         <v>40</v>
       </c>
       <c r="C142" s="2" t="s">
+        <v>313</v>
+      </c>
+      <c r="E142" t="s">
+        <v>315</v>
+      </c>
+      <c r="F142">
+        <v>1950</v>
+      </c>
+      <c r="G142">
+        <v>2004</v>
+      </c>
+      <c r="H142" t="s">
+        <v>16</v>
+      </c>
+      <c r="I142" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="143" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A143" t="s">
+        <v>161</v>
+      </c>
+      <c r="B143" t="s">
+        <v>25</v>
+      </c>
+      <c r="C143" s="2" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="144" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A144" t="s">
+        <v>168</v>
+      </c>
+      <c r="B144" t="s">
+        <v>40</v>
+      </c>
+      <c r="C144" s="2" t="s">
         <v>167</v>
-      </c>
-    </row>
-    <row r="143" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A143" t="s">
-        <v>399</v>
-      </c>
-      <c r="B143" t="s">
-        <v>40</v>
-      </c>
-      <c r="C143" s="2" t="s">
-        <v>400</v>
-      </c>
-      <c r="E143" t="s">
-        <v>14</v>
-      </c>
-      <c r="F143">
-        <v>2000</v>
-      </c>
-      <c r="G143">
-        <v>2014</v>
-      </c>
-      <c r="H143" t="s">
-        <v>348</v>
-      </c>
-      <c r="I143" t="s">
-        <v>349</v>
-      </c>
-      <c r="J143" s="2" t="s">
-        <v>402</v>
-      </c>
-      <c r="N143" s="2" t="s">
-        <v>401</v>
-      </c>
-    </row>
-    <row r="144" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A144" t="s">
-        <v>213</v>
-      </c>
-      <c r="B144" t="s">
-        <v>55</v>
-      </c>
-      <c r="C144" s="2" t="s">
-        <v>212</v>
-      </c>
-      <c r="H144" t="s">
-        <v>16</v>
-      </c>
-      <c r="I144" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="145" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
-        <v>395</v>
+        <v>399</v>
       </c>
       <c r="B145" t="s">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="C145" s="2" t="s">
-        <v>394</v>
-      </c>
-      <c r="D145" t="s">
-        <v>396</v>
+        <v>400</v>
       </c>
       <c r="E145" t="s">
-        <v>111</v>
+        <v>14</v>
       </c>
       <c r="F145">
-        <v>1986</v>
+        <v>2000</v>
       </c>
       <c r="G145">
-        <v>2015</v>
+        <v>2014</v>
       </c>
       <c r="H145" t="s">
-        <v>367</v>
+        <v>348</v>
       </c>
       <c r="I145" t="s">
-        <v>398</v>
+        <v>349</v>
       </c>
       <c r="J145" s="2" t="s">
-        <v>397</v>
+        <v>402</v>
+      </c>
+      <c r="N145" s="2" t="s">
+        <v>401</v>
       </c>
     </row>
     <row r="146" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
-        <v>323</v>
+        <v>213</v>
       </c>
       <c r="B146" t="s">
-        <v>25</v>
+        <v>55</v>
       </c>
       <c r="C146" s="2" t="s">
-        <v>324</v>
-      </c>
-      <c r="E146" t="s">
-        <v>325</v>
-      </c>
-      <c r="F146">
-        <v>1942</v>
+        <v>212</v>
       </c>
       <c r="H146" t="s">
         <v>16</v>
@@ -4772,124 +4820,145 @@
     </row>
     <row r="147" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
-        <v>273</v>
+        <v>395</v>
       </c>
       <c r="B147" t="s">
-        <v>237</v>
+        <v>25</v>
       </c>
       <c r="C147" s="2" t="s">
-        <v>272</v>
+        <v>394</v>
+      </c>
+      <c r="D147" t="s">
+        <v>396</v>
+      </c>
+      <c r="E147" t="s">
+        <v>111</v>
       </c>
       <c r="F147">
-        <v>1996</v>
+        <v>1986</v>
       </c>
       <c r="G147">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="H147" t="s">
-        <v>16</v>
+        <v>367</v>
       </c>
       <c r="I147" t="s">
-        <v>20</v>
+        <v>398</v>
+      </c>
+      <c r="J147" s="2" t="s">
+        <v>397</v>
       </c>
     </row>
     <row r="148" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
-        <v>66</v>
+        <v>323</v>
       </c>
       <c r="B148" t="s">
         <v>25</v>
       </c>
       <c r="C148" s="2" t="s">
-        <v>67</v>
+        <v>324</v>
+      </c>
+      <c r="E148" t="s">
+        <v>325</v>
+      </c>
+      <c r="F148">
+        <v>1942</v>
+      </c>
+      <c r="H148" t="s">
+        <v>16</v>
+      </c>
+      <c r="I148" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="149" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
-        <v>383</v>
+        <v>273</v>
       </c>
       <c r="B149" t="s">
-        <v>40</v>
+        <v>237</v>
       </c>
       <c r="C149" s="2" t="s">
-        <v>384</v>
-      </c>
-      <c r="E149" t="s">
-        <v>386</v>
+        <v>272</v>
       </c>
       <c r="F149">
-        <v>1951</v>
+        <v>1996</v>
+      </c>
+      <c r="G149">
+        <v>2016</v>
       </c>
       <c r="H149" t="s">
-        <v>348</v>
+        <v>16</v>
       </c>
       <c r="I149" t="s">
-        <v>349</v>
-      </c>
-      <c r="N149" s="2" t="s">
-        <v>385</v>
+        <v>20</v>
       </c>
     </row>
     <row r="150" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
-        <v>139</v>
+        <v>66</v>
       </c>
       <c r="B150" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="C150" s="2" t="s">
-        <v>140</v>
+        <v>67</v>
       </c>
     </row>
     <row r="151" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
-        <v>329</v>
+        <v>383</v>
       </c>
       <c r="B151" t="s">
-        <v>165</v>
+        <v>40</v>
       </c>
       <c r="C151" s="2" t="s">
-        <v>328</v>
+        <v>384</v>
       </c>
       <c r="E151" t="s">
-        <v>34</v>
+        <v>386</v>
       </c>
       <c r="F151">
-        <v>1789</v>
+        <v>1951</v>
       </c>
       <c r="H151" t="s">
-        <v>16</v>
+        <v>348</v>
       </c>
       <c r="I151" t="s">
-        <v>20</v>
+        <v>349</v>
+      </c>
+      <c r="N151" s="2" t="s">
+        <v>385</v>
       </c>
     </row>
     <row r="152" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
-        <v>172</v>
+        <v>139</v>
       </c>
       <c r="B152" t="s">
-        <v>60</v>
+        <v>40</v>
       </c>
       <c r="C152" s="2" t="s">
-        <v>171</v>
+        <v>140</v>
       </c>
     </row>
     <row r="153" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
-        <v>217</v>
+        <v>329</v>
       </c>
       <c r="B153" t="s">
-        <v>60</v>
+        <v>165</v>
       </c>
       <c r="C153" s="2" t="s">
-        <v>216</v>
+        <v>328</v>
       </c>
       <c r="E153" t="s">
-        <v>14</v>
+        <v>34</v>
       </c>
       <c r="F153">
-        <v>1900</v>
+        <v>1789</v>
       </c>
       <c r="H153" t="s">
         <v>16</v>
@@ -4900,130 +4969,118 @@
     </row>
     <row r="154" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
-        <v>132</v>
+        <v>172</v>
       </c>
       <c r="B154" t="s">
-        <v>259</v>
+        <v>60</v>
       </c>
       <c r="C154" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="Q154" t="s">
-        <v>17</v>
+        <v>171</v>
       </c>
     </row>
     <row r="155" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
-        <v>182</v>
+        <v>217</v>
       </c>
       <c r="B155" t="s">
-        <v>165</v>
+        <v>60</v>
       </c>
       <c r="C155" s="2" t="s">
-        <v>181</v>
+        <v>216</v>
+      </c>
+      <c r="E155" t="s">
+        <v>14</v>
+      </c>
+      <c r="F155">
+        <v>1900</v>
+      </c>
+      <c r="H155" t="s">
+        <v>16</v>
+      </c>
+      <c r="I155" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="156" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
-        <v>423</v>
+        <v>132</v>
       </c>
       <c r="B156" t="s">
-        <v>86</v>
+        <v>259</v>
       </c>
       <c r="C156" s="2" t="s">
-        <v>424</v>
-      </c>
-      <c r="E156" t="s">
-        <v>34</v>
-      </c>
-      <c r="F156">
-        <v>1996</v>
-      </c>
-      <c r="G156">
-        <v>2016</v>
-      </c>
-      <c r="H156" t="s">
-        <v>348</v>
-      </c>
-      <c r="I156" t="s">
-        <v>425</v>
+        <v>133</v>
+      </c>
+      <c r="Q156" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="157" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
-        <v>115</v>
+        <v>182</v>
       </c>
       <c r="B157" t="s">
-        <v>128</v>
+        <v>165</v>
       </c>
       <c r="C157" s="2" t="s">
-        <v>116</v>
+        <v>181</v>
       </c>
     </row>
     <row r="158" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
-        <v>263</v>
+        <v>423</v>
       </c>
       <c r="B158" t="s">
-        <v>250</v>
+        <v>86</v>
       </c>
       <c r="C158" s="2" t="s">
-        <v>264</v>
+        <v>424</v>
       </c>
       <c r="E158" t="s">
-        <v>265</v>
+        <v>34</v>
       </c>
       <c r="F158">
-        <v>1500</v>
+        <v>1996</v>
       </c>
       <c r="G158">
-        <v>2000</v>
+        <v>2016</v>
       </c>
       <c r="H158" t="s">
-        <v>16</v>
+        <v>348</v>
       </c>
       <c r="I158" t="s">
-        <v>20</v>
+        <v>425</v>
       </c>
     </row>
     <row r="159" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
-        <v>221</v>
+        <v>115</v>
       </c>
       <c r="B159" t="s">
-        <v>86</v>
+        <v>128</v>
       </c>
       <c r="C159" s="2" t="s">
-        <v>220</v>
-      </c>
-      <c r="F159">
-        <v>2013</v>
-      </c>
-      <c r="H159" t="s">
-        <v>16</v>
-      </c>
-      <c r="I159" t="s">
-        <v>20</v>
+        <v>116</v>
       </c>
     </row>
     <row r="160" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
-        <v>13</v>
+        <v>263</v>
       </c>
       <c r="B160" t="s">
-        <v>25</v>
+        <v>250</v>
       </c>
       <c r="C160" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="D160" s="1" t="s">
-        <v>42</v>
+        <v>264</v>
       </c>
       <c r="E160" t="s">
-        <v>14</v>
+        <v>265</v>
       </c>
       <c r="F160">
-        <v>1981</v>
+        <v>1500</v>
+      </c>
+      <c r="G160">
+        <v>2000</v>
       </c>
       <c r="H160" t="s">
         <v>16</v>
@@ -5034,166 +5091,212 @@
     </row>
     <row r="161" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
+        <v>221</v>
+      </c>
+      <c r="B161" t="s">
+        <v>86</v>
+      </c>
+      <c r="C161" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="F161">
+        <v>2013</v>
+      </c>
+      <c r="H161" t="s">
+        <v>16</v>
+      </c>
+      <c r="I161" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="162" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A162" t="s">
+        <v>13</v>
+      </c>
+      <c r="B162" t="s">
+        <v>25</v>
+      </c>
+      <c r="C162" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D162" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E162" t="s">
+        <v>14</v>
+      </c>
+      <c r="F162">
+        <v>1981</v>
+      </c>
+      <c r="H162" t="s">
+        <v>16</v>
+      </c>
+      <c r="I162" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="163" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A163" t="s">
         <v>283</v>
       </c>
-      <c r="B161" t="s">
+      <c r="B163" t="s">
         <v>124</v>
       </c>
-      <c r="C161" s="2" t="s">
+      <c r="C163" s="2" t="s">
         <v>284</v>
       </c>
-      <c r="H161" t="s">
-        <v>16</v>
-      </c>
-      <c r="I161" t="s">
+      <c r="H163" t="s">
+        <v>16</v>
+      </c>
+      <c r="I163" t="s">
         <v>20</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:Q161">
+  <sortState ref="A2:Q163">
     <sortCondition ref="A2"/>
   </sortState>
   <hyperlinks>
     <hyperlink ref="C6" r:id="rId1"/>
-    <hyperlink ref="C58" r:id="rId2"/>
+    <hyperlink ref="C59" r:id="rId2"/>
     <hyperlink ref="C7" r:id="rId3"/>
     <hyperlink ref="C10" r:id="rId4"/>
-    <hyperlink ref="C95" r:id="rId5"/>
-    <hyperlink ref="C115" r:id="rId6"/>
-    <hyperlink ref="C160" r:id="rId7"/>
+    <hyperlink ref="C97" r:id="rId5"/>
+    <hyperlink ref="C117" r:id="rId6"/>
+    <hyperlink ref="C162" r:id="rId7"/>
     <hyperlink ref="C35" r:id="rId8"/>
     <hyperlink ref="C30" r:id="rId9"/>
-    <hyperlink ref="C49" r:id="rId10"/>
-    <hyperlink ref="C56" r:id="rId11"/>
+    <hyperlink ref="C50" r:id="rId10"/>
+    <hyperlink ref="C57" r:id="rId11"/>
     <hyperlink ref="C3" r:id="rId12"/>
     <hyperlink ref="C20" r:id="rId13"/>
-    <hyperlink ref="C60" r:id="rId14"/>
-    <hyperlink ref="C87" r:id="rId15"/>
+    <hyperlink ref="C61" r:id="rId14"/>
+    <hyperlink ref="C89" r:id="rId15"/>
     <hyperlink ref="C29" r:id="rId16"/>
-    <hyperlink ref="C111" r:id="rId17"/>
+    <hyperlink ref="C113" r:id="rId17"/>
     <hyperlink ref="C41" r:id="rId18"/>
-    <hyperlink ref="C72" r:id="rId19"/>
+    <hyperlink ref="C74" r:id="rId19"/>
     <hyperlink ref="C16" r:id="rId20"/>
-    <hyperlink ref="C148" r:id="rId21"/>
+    <hyperlink ref="C150" r:id="rId21"/>
     <hyperlink ref="C8" r:id="rId22"/>
     <hyperlink ref="C38" r:id="rId23"/>
-    <hyperlink ref="C53" r:id="rId24"/>
-    <hyperlink ref="C50" r:id="rId25"/>
-    <hyperlink ref="C54" r:id="rId26"/>
-    <hyperlink ref="C55" r:id="rId27"/>
-    <hyperlink ref="C69" r:id="rId28"/>
-    <hyperlink ref="C92" r:id="rId29"/>
-    <hyperlink ref="C139" r:id="rId30"/>
-    <hyperlink ref="C98" r:id="rId31"/>
-    <hyperlink ref="C82" r:id="rId32"/>
-    <hyperlink ref="C104" r:id="rId33"/>
-    <hyperlink ref="C70" r:id="rId34"/>
+    <hyperlink ref="C54" r:id="rId24"/>
+    <hyperlink ref="C51" r:id="rId25"/>
+    <hyperlink ref="C55" r:id="rId26"/>
+    <hyperlink ref="C56" r:id="rId27"/>
+    <hyperlink ref="C71" r:id="rId28"/>
+    <hyperlink ref="C94" r:id="rId29"/>
+    <hyperlink ref="C141" r:id="rId30"/>
+    <hyperlink ref="C100" r:id="rId31"/>
+    <hyperlink ref="C84" r:id="rId32"/>
+    <hyperlink ref="C106" r:id="rId33"/>
+    <hyperlink ref="C72" r:id="rId34"/>
     <hyperlink ref="C17" r:id="rId35"/>
-    <hyperlink ref="C137" r:id="rId36"/>
+    <hyperlink ref="C139" r:id="rId36"/>
     <hyperlink ref="C15" r:id="rId37"/>
-    <hyperlink ref="C157" r:id="rId38"/>
-    <hyperlink ref="C86" r:id="rId39"/>
-    <hyperlink ref="C57" r:id="rId40"/>
-    <hyperlink ref="C120" r:id="rId41"/>
+    <hyperlink ref="C159" r:id="rId38"/>
+    <hyperlink ref="C88" r:id="rId39"/>
+    <hyperlink ref="C58" r:id="rId40"/>
+    <hyperlink ref="C122" r:id="rId41"/>
     <hyperlink ref="C18" r:id="rId42"/>
-    <hyperlink ref="C51" r:id="rId43"/>
+    <hyperlink ref="C52" r:id="rId43"/>
     <hyperlink ref="C23" r:id="rId44"/>
-    <hyperlink ref="C112" r:id="rId45"/>
-    <hyperlink ref="C154" r:id="rId46"/>
+    <hyperlink ref="C114" r:id="rId45"/>
+    <hyperlink ref="C156" r:id="rId46"/>
     <hyperlink ref="C27" r:id="rId47" display="http://comparativeconstitutionsproject.org/"/>
-    <hyperlink ref="C109" r:id="rId48"/>
-    <hyperlink ref="C150" r:id="rId49"/>
-    <hyperlink ref="C124" r:id="rId50"/>
-    <hyperlink ref="C119" r:id="rId51"/>
+    <hyperlink ref="C111" r:id="rId48"/>
+    <hyperlink ref="C152" r:id="rId49"/>
+    <hyperlink ref="C126" r:id="rId50"/>
+    <hyperlink ref="C121" r:id="rId51"/>
     <hyperlink ref="C22" r:id="rId52"/>
-    <hyperlink ref="C113" r:id="rId53"/>
+    <hyperlink ref="C115" r:id="rId53"/>
     <hyperlink ref="C48" r:id="rId54"/>
-    <hyperlink ref="C76" r:id="rId55"/>
-    <hyperlink ref="C79" r:id="rId56"/>
-    <hyperlink ref="C110" r:id="rId57"/>
-    <hyperlink ref="C100" r:id="rId58"/>
-    <hyperlink ref="C128" r:id="rId59"/>
+    <hyperlink ref="C78" r:id="rId55"/>
+    <hyperlink ref="C81" r:id="rId56"/>
+    <hyperlink ref="C112" r:id="rId57"/>
+    <hyperlink ref="C102" r:id="rId58"/>
+    <hyperlink ref="C130" r:id="rId59"/>
     <hyperlink ref="C31" r:id="rId60"/>
-    <hyperlink ref="C141" r:id="rId61"/>
+    <hyperlink ref="C143" r:id="rId61"/>
     <hyperlink ref="C9" r:id="rId62"/>
     <hyperlink ref="C33" r:id="rId63"/>
-    <hyperlink ref="C142" r:id="rId64"/>
+    <hyperlink ref="C144" r:id="rId64"/>
     <hyperlink ref="C14" r:id="rId65"/>
-    <hyperlink ref="C152" r:id="rId66"/>
+    <hyperlink ref="C154" r:id="rId66"/>
     <hyperlink ref="C25" r:id="rId67"/>
     <hyperlink ref="C24" r:id="rId68"/>
     <hyperlink ref="C26" r:id="rId69"/>
-    <hyperlink ref="C52" r:id="rId70"/>
-    <hyperlink ref="C155" r:id="rId71"/>
+    <hyperlink ref="C53" r:id="rId70"/>
+    <hyperlink ref="C157" r:id="rId71"/>
     <hyperlink ref="C28" r:id="rId72"/>
-    <hyperlink ref="C116" r:id="rId73"/>
+    <hyperlink ref="C118" r:id="rId73"/>
     <hyperlink ref="C32" r:id="rId74"/>
     <hyperlink ref="C45" r:id="rId75"/>
-    <hyperlink ref="C131" r:id="rId76"/>
+    <hyperlink ref="C133" r:id="rId76"/>
     <hyperlink ref="C42" r:id="rId77"/>
     <hyperlink ref="C39" r:id="rId78"/>
-    <hyperlink ref="C68" r:id="rId79"/>
+    <hyperlink ref="C69" r:id="rId79"/>
     <hyperlink ref="C5" r:id="rId80"/>
-    <hyperlink ref="C67" r:id="rId81"/>
+    <hyperlink ref="C68" r:id="rId81"/>
     <hyperlink ref="C12" r:id="rId82"/>
-    <hyperlink ref="C108" r:id="rId83"/>
-    <hyperlink ref="C117" r:id="rId84"/>
-    <hyperlink ref="C144" r:id="rId85"/>
+    <hyperlink ref="C110" r:id="rId83"/>
+    <hyperlink ref="C119" r:id="rId84"/>
+    <hyperlink ref="C146" r:id="rId85"/>
     <hyperlink ref="C36" r:id="rId86"/>
-    <hyperlink ref="C153" r:id="rId87"/>
+    <hyperlink ref="C155" r:id="rId87"/>
     <hyperlink ref="C44" r:id="rId88"/>
-    <hyperlink ref="C159" r:id="rId89"/>
-    <hyperlink ref="C96" r:id="rId90"/>
-    <hyperlink ref="C65" r:id="rId91"/>
-    <hyperlink ref="C97" r:id="rId92"/>
-    <hyperlink ref="C134" r:id="rId93"/>
-    <hyperlink ref="C80" r:id="rId94"/>
-    <hyperlink ref="C102" r:id="rId95"/>
-    <hyperlink ref="C135" r:id="rId96"/>
-    <hyperlink ref="C61" r:id="rId97"/>
-    <hyperlink ref="C114" r:id="rId98"/>
+    <hyperlink ref="C161" r:id="rId89"/>
+    <hyperlink ref="C98" r:id="rId90"/>
+    <hyperlink ref="C66" r:id="rId91"/>
+    <hyperlink ref="C99" r:id="rId92"/>
+    <hyperlink ref="C136" r:id="rId93"/>
+    <hyperlink ref="C82" r:id="rId94"/>
+    <hyperlink ref="C104" r:id="rId95"/>
+    <hyperlink ref="C137" r:id="rId96"/>
+    <hyperlink ref="C62" r:id="rId97"/>
+    <hyperlink ref="C116" r:id="rId98"/>
     <hyperlink ref="C46" r:id="rId99"/>
     <hyperlink ref="C43" r:id="rId100"/>
-    <hyperlink ref="C83" r:id="rId101"/>
-    <hyperlink ref="C59" r:id="rId102"/>
+    <hyperlink ref="C85" r:id="rId101"/>
+    <hyperlink ref="C60" r:id="rId102"/>
     <hyperlink ref="C2" r:id="rId103"/>
-    <hyperlink ref="C77" r:id="rId104"/>
-    <hyperlink ref="C81" r:id="rId105"/>
-    <hyperlink ref="C106" r:id="rId106"/>
+    <hyperlink ref="C79" r:id="rId104"/>
+    <hyperlink ref="C83" r:id="rId105"/>
+    <hyperlink ref="C108" r:id="rId106"/>
     <hyperlink ref="C47" r:id="rId107"/>
-    <hyperlink ref="C84" r:id="rId108"/>
-    <hyperlink ref="C133" r:id="rId109"/>
+    <hyperlink ref="C86" r:id="rId108"/>
+    <hyperlink ref="C135" r:id="rId109"/>
     <hyperlink ref="C13" r:id="rId110"/>
     <hyperlink ref="C4" r:id="rId111"/>
-    <hyperlink ref="C158" r:id="rId112"/>
-    <hyperlink ref="C90" r:id="rId113"/>
-    <hyperlink ref="C85" r:id="rId114"/>
-    <hyperlink ref="C147" r:id="rId115"/>
-    <hyperlink ref="C127" r:id="rId116"/>
-    <hyperlink ref="C63" r:id="rId117"/>
-    <hyperlink ref="C99" r:id="rId118"/>
-    <hyperlink ref="C74" r:id="rId119"/>
-    <hyperlink ref="C161" r:id="rId120"/>
-    <hyperlink ref="C66" r:id="rId121"/>
-    <hyperlink ref="C126" r:id="rId122"/>
-    <hyperlink ref="C105" r:id="rId123"/>
-    <hyperlink ref="C78" r:id="rId124"/>
-    <hyperlink ref="C103" r:id="rId125"/>
-    <hyperlink ref="C132" r:id="rId126"/>
-    <hyperlink ref="C88" r:id="rId127"/>
+    <hyperlink ref="C160" r:id="rId112"/>
+    <hyperlink ref="C92" r:id="rId113"/>
+    <hyperlink ref="C87" r:id="rId114"/>
+    <hyperlink ref="C149" r:id="rId115"/>
+    <hyperlink ref="C129" r:id="rId116"/>
+    <hyperlink ref="C64" r:id="rId117"/>
+    <hyperlink ref="C101" r:id="rId118"/>
+    <hyperlink ref="C76" r:id="rId119"/>
+    <hyperlink ref="C163" r:id="rId120"/>
+    <hyperlink ref="C67" r:id="rId121"/>
+    <hyperlink ref="C128" r:id="rId122"/>
+    <hyperlink ref="C107" r:id="rId123"/>
+    <hyperlink ref="C80" r:id="rId124"/>
+    <hyperlink ref="C105" r:id="rId125"/>
+    <hyperlink ref="C134" r:id="rId126"/>
+    <hyperlink ref="C90" r:id="rId127"/>
     <hyperlink ref="C11" r:id="rId128"/>
     <hyperlink ref="C19" r:id="rId129"/>
-    <hyperlink ref="C125" r:id="rId130"/>
-    <hyperlink ref="C73" r:id="rId131"/>
-    <hyperlink ref="C140" r:id="rId132"/>
-    <hyperlink ref="C122" r:id="rId133"/>
-    <hyperlink ref="C121" r:id="rId134"/>
-    <hyperlink ref="C123" r:id="rId135"/>
-    <hyperlink ref="C146" r:id="rId136"/>
-    <hyperlink ref="C138" r:id="rId137"/>
-    <hyperlink ref="C151" r:id="rId138"/>
+    <hyperlink ref="C127" r:id="rId130"/>
+    <hyperlink ref="C75" r:id="rId131"/>
+    <hyperlink ref="C142" r:id="rId132"/>
+    <hyperlink ref="C124" r:id="rId133"/>
+    <hyperlink ref="C123" r:id="rId134"/>
+    <hyperlink ref="C125" r:id="rId135"/>
+    <hyperlink ref="C148" r:id="rId136"/>
+    <hyperlink ref="C140" r:id="rId137"/>
+    <hyperlink ref="C153" r:id="rId138"/>
     <hyperlink ref="C37" r:id="rId139"/>
-    <hyperlink ref="C89" r:id="rId140"/>
+    <hyperlink ref="C91" r:id="rId140"/>
     <hyperlink ref="J2" r:id="rId141"/>
     <hyperlink ref="M3" r:id="rId142"/>
     <hyperlink ref="J3" r:id="rId143"/>
@@ -5201,54 +5304,62 @@
     <hyperlink ref="J4" r:id="rId145"/>
     <hyperlink ref="P5" r:id="rId146"/>
     <hyperlink ref="J5" r:id="rId147"/>
-    <hyperlink ref="C107" r:id="rId148"/>
+    <hyperlink ref="C109" r:id="rId148"/>
     <hyperlink ref="C34" r:id="rId149"/>
     <hyperlink ref="P7" r:id="rId150"/>
     <hyperlink ref="J7" r:id="rId151"/>
     <hyperlink ref="M8" r:id="rId152"/>
     <hyperlink ref="L8" r:id="rId153"/>
     <hyperlink ref="J8" r:id="rId154"/>
-    <hyperlink ref="C149" r:id="rId155"/>
-    <hyperlink ref="N149" r:id="rId156"/>
+    <hyperlink ref="C151" r:id="rId155"/>
+    <hyperlink ref="N151" r:id="rId156"/>
     <hyperlink ref="C21" r:id="rId157"/>
     <hyperlink ref="N21" r:id="rId158"/>
-    <hyperlink ref="C62" r:id="rId159"/>
-    <hyperlink ref="C145" r:id="rId160"/>
-    <hyperlink ref="J145" r:id="rId161"/>
-    <hyperlink ref="C143" r:id="rId162"/>
-    <hyperlink ref="N143" r:id="rId163"/>
-    <hyperlink ref="J143" r:id="rId164"/>
-    <hyperlink ref="C93" r:id="rId165"/>
-    <hyperlink ref="C91" r:id="rId166"/>
+    <hyperlink ref="C63" r:id="rId159"/>
+    <hyperlink ref="C147" r:id="rId160"/>
+    <hyperlink ref="J147" r:id="rId161"/>
+    <hyperlink ref="C145" r:id="rId162"/>
+    <hyperlink ref="N145" r:id="rId163"/>
+    <hyperlink ref="J145" r:id="rId164"/>
+    <hyperlink ref="C95" r:id="rId165"/>
+    <hyperlink ref="C93" r:id="rId166"/>
     <hyperlink ref="C40" r:id="rId167"/>
     <hyperlink ref="J40" r:id="rId168"/>
     <hyperlink ref="K40" r:id="rId169"/>
-    <hyperlink ref="C101" r:id="rId170"/>
-    <hyperlink ref="N101" r:id="rId171"/>
-    <hyperlink ref="C75" r:id="rId172"/>
-    <hyperlink ref="K75" r:id="rId173"/>
-    <hyperlink ref="C156" r:id="rId174"/>
-    <hyperlink ref="C118" r:id="rId175"/>
-    <hyperlink ref="K118" r:id="rId176"/>
+    <hyperlink ref="C103" r:id="rId170"/>
+    <hyperlink ref="N103" r:id="rId171"/>
+    <hyperlink ref="C77" r:id="rId172"/>
+    <hyperlink ref="K77" r:id="rId173"/>
+    <hyperlink ref="C158" r:id="rId174"/>
+    <hyperlink ref="C120" r:id="rId175"/>
+    <hyperlink ref="K120" r:id="rId176"/>
     <hyperlink ref="L9" r:id="rId177"/>
     <hyperlink ref="J9" r:id="rId178"/>
     <hyperlink ref="J10" r:id="rId179"/>
-    <hyperlink ref="C129" r:id="rId180"/>
-    <hyperlink ref="J129" r:id="rId181"/>
-    <hyperlink ref="L129" r:id="rId182"/>
-    <hyperlink ref="K129" r:id="rId183"/>
-    <hyperlink ref="C130" r:id="rId184"/>
-    <hyperlink ref="J130" r:id="rId185"/>
-    <hyperlink ref="K130" r:id="rId186"/>
-    <hyperlink ref="L130" r:id="rId187"/>
-    <hyperlink ref="C64" r:id="rId188"/>
-    <hyperlink ref="J64" r:id="rId189"/>
-    <hyperlink ref="N64" r:id="rId190"/>
-    <hyperlink ref="C136" r:id="rId191"/>
-    <hyperlink ref="C94" r:id="rId192"/>
-    <hyperlink ref="J94" r:id="rId193"/>
-    <hyperlink ref="L94" r:id="rId194"/>
-    <hyperlink ref="C71" r:id="rId195"/>
+    <hyperlink ref="C131" r:id="rId180"/>
+    <hyperlink ref="J131" r:id="rId181"/>
+    <hyperlink ref="L131" r:id="rId182"/>
+    <hyperlink ref="K131" r:id="rId183"/>
+    <hyperlink ref="C132" r:id="rId184"/>
+    <hyperlink ref="J132" r:id="rId185"/>
+    <hyperlink ref="K132" r:id="rId186"/>
+    <hyperlink ref="L132" r:id="rId187"/>
+    <hyperlink ref="C65" r:id="rId188"/>
+    <hyperlink ref="J65" r:id="rId189"/>
+    <hyperlink ref="N65" r:id="rId190"/>
+    <hyperlink ref="C138" r:id="rId191"/>
+    <hyperlink ref="C96" r:id="rId192"/>
+    <hyperlink ref="J96" r:id="rId193"/>
+    <hyperlink ref="L96" r:id="rId194"/>
+    <hyperlink ref="C73" r:id="rId195"/>
+    <hyperlink ref="C49" r:id="rId196"/>
+    <hyperlink ref="L49" r:id="rId197"/>
+    <hyperlink ref="K49" r:id="rId198"/>
+    <hyperlink ref="J49" r:id="rId199"/>
+    <hyperlink ref="C70" r:id="rId200"/>
+    <hyperlink ref="J70" r:id="rId201"/>
+    <hyperlink ref="K70" r:id="rId202"/>
+    <hyperlink ref="L70" r:id="rId203"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
add 'PollBase' and 'Counter Trafficking Data Collaborative'
</commit_message>
<xml_diff>
--- a/PolData.xlsx
+++ b/PolData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17440" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="860" uniqueCount="472">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="877" uniqueCount="481">
   <si>
     <t>name</t>
   </si>
@@ -1443,6 +1443,33 @@
   </si>
   <si>
     <t>http://www.columbia.edu/~aw2951/WimmerMin1.0.dta</t>
+  </si>
+  <si>
+    <t>PollBase</t>
+  </si>
+  <si>
+    <t>https://www.markpack.org.uk/opinion-polls/</t>
+  </si>
+  <si>
+    <t>Opinion polls</t>
+  </si>
+  <si>
+    <t>https://www.markpack.org.uk/files/2017/10/PollBase.xls</t>
+  </si>
+  <si>
+    <t>Counter Trafficking Data Collaborative</t>
+  </si>
+  <si>
+    <t>https://www.ctdatacollaborative.org/download-global-dataset</t>
+  </si>
+  <si>
+    <t>Human trafficking, victims</t>
+  </si>
+  <si>
+    <t>https://www.ctdatacollaborative.org/sites/default/files/The%20Global%20Dataset%2027%20Nov%202017_0.csv</t>
+  </si>
+  <si>
+    <t>https://www.ctdatacollaborative.org/sites/default/files/CTDC%20codebook%20v6_0.pdf</t>
   </si>
 </sst>
 </file>
@@ -1782,10 +1809,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q163"/>
+  <dimension ref="A1:Q165"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A137" workbookViewId="0">
-      <selection activeCell="A70" sqref="A70"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2617,156 +2644,165 @@
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>330</v>
+        <v>476</v>
       </c>
       <c r="B37" t="s">
-        <v>165</v>
+        <v>40</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>331</v>
+        <v>477</v>
+      </c>
+      <c r="D37" t="s">
+        <v>478</v>
       </c>
       <c r="E37" t="s">
-        <v>77</v>
+        <v>14</v>
       </c>
       <c r="F37">
-        <v>1953</v>
+        <v>2002</v>
       </c>
       <c r="H37" t="s">
-        <v>16</v>
+        <v>348</v>
       </c>
       <c r="I37" t="s">
-        <v>20</v>
+        <v>349</v>
+      </c>
+      <c r="J37" s="2" t="s">
+        <v>480</v>
+      </c>
+      <c r="K37" s="2" t="s">
+        <v>479</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>75</v>
+        <v>330</v>
       </c>
       <c r="B38" t="s">
-        <v>25</v>
+        <v>165</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>76</v>
+        <v>331</v>
       </c>
       <c r="E38" t="s">
         <v>77</v>
       </c>
       <c r="F38">
-        <v>1971</v>
+        <v>1953</v>
+      </c>
+      <c r="H38" t="s">
+        <v>16</v>
+      </c>
+      <c r="I38" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>197</v>
+        <v>75</v>
       </c>
       <c r="B39" t="s">
-        <v>55</v>
+        <v>25</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>198</v>
+        <v>76</v>
       </c>
       <c r="E39" t="s">
-        <v>199</v>
+        <v>77</v>
       </c>
       <c r="F39">
-        <v>1975</v>
-      </c>
-      <c r="G39">
-        <v>2015</v>
-      </c>
-      <c r="H39" t="s">
-        <v>16</v>
-      </c>
-      <c r="I39" t="s">
-        <v>20</v>
+        <v>1971</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>409</v>
+        <v>197</v>
       </c>
       <c r="B40" t="s">
-        <v>250</v>
+        <v>55</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>410</v>
+        <v>198</v>
       </c>
       <c r="E40" t="s">
-        <v>9</v>
+        <v>199</v>
+      </c>
+      <c r="F40">
+        <v>1975</v>
+      </c>
+      <c r="G40">
+        <v>2015</v>
       </c>
       <c r="H40" t="s">
-        <v>348</v>
+        <v>16</v>
       </c>
       <c r="I40" t="s">
-        <v>349</v>
-      </c>
-      <c r="J40" s="2" t="s">
-        <v>411</v>
-      </c>
-      <c r="K40" s="2" t="s">
-        <v>412</v>
+        <v>20</v>
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>59</v>
+        <v>409</v>
       </c>
       <c r="B41" t="s">
-        <v>60</v>
+        <v>250</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>61</v>
+        <v>410</v>
+      </c>
+      <c r="E41" t="s">
+        <v>9</v>
+      </c>
+      <c r="H41" t="s">
+        <v>348</v>
+      </c>
+      <c r="I41" t="s">
+        <v>349</v>
+      </c>
+      <c r="J41" s="2" t="s">
+        <v>411</v>
+      </c>
+      <c r="K41" s="2" t="s">
+        <v>412</v>
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>196</v>
+        <v>59</v>
       </c>
       <c r="B42" t="s">
-        <v>165</v>
+        <v>60</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>195</v>
-      </c>
-      <c r="F42">
-        <v>1946</v>
-      </c>
-      <c r="G42">
-        <v>2016</v>
+        <v>61</v>
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>238</v>
+        <v>196</v>
       </c>
       <c r="B43" t="s">
-        <v>237</v>
+        <v>165</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>243</v>
-      </c>
-      <c r="H43" t="s">
-        <v>16</v>
-      </c>
-      <c r="I43" t="s">
-        <v>20</v>
+        <v>195</v>
+      </c>
+      <c r="F43">
+        <v>1946</v>
+      </c>
+      <c r="G43">
+        <v>2016</v>
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>219</v>
+        <v>238</v>
       </c>
       <c r="B44" t="s">
-        <v>124</v>
+        <v>237</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>218</v>
-      </c>
-      <c r="F44">
-        <v>1970</v>
-      </c>
-      <c r="G44">
-        <v>2015</v>
+        <v>243</v>
       </c>
       <c r="H44" t="s">
         <v>16</v>
@@ -2777,44 +2813,50 @@
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>191</v>
+        <v>219</v>
       </c>
       <c r="B45" t="s">
-        <v>25</v>
+        <v>124</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="E45" t="s">
-        <v>192</v>
+        <v>218</v>
+      </c>
+      <c r="F45">
+        <v>1970</v>
+      </c>
+      <c r="G45">
+        <v>2015</v>
+      </c>
+      <c r="H45" t="s">
+        <v>16</v>
+      </c>
+      <c r="I45" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>235</v>
+        <v>191</v>
       </c>
       <c r="B46" t="s">
-        <v>60</v>
+        <v>25</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>236</v>
-      </c>
-      <c r="H46" t="s">
-        <v>16</v>
-      </c>
-      <c r="I46" t="s">
-        <v>20</v>
+        <v>190</v>
+      </c>
+      <c r="E46" t="s">
+        <v>192</v>
       </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>252</v>
+        <v>235</v>
       </c>
       <c r="B47" t="s">
-        <v>250</v>
+        <v>60</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>251</v>
+        <v>236</v>
       </c>
       <c r="H47" t="s">
         <v>16</v>
@@ -2825,129 +2867,129 @@
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>149</v>
+        <v>252</v>
       </c>
       <c r="B48" t="s">
-        <v>128</v>
+        <v>250</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>150</v>
+        <v>251</v>
+      </c>
+      <c r="H48" t="s">
+        <v>16</v>
+      </c>
+      <c r="I48" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="49" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>462</v>
+        <v>149</v>
       </c>
       <c r="B49" t="s">
-        <v>250</v>
+        <v>128</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>464</v>
-      </c>
-      <c r="D49" t="s">
-        <v>463</v>
-      </c>
-      <c r="E49" t="s">
-        <v>14</v>
-      </c>
-      <c r="F49">
-        <v>1946</v>
-      </c>
-      <c r="G49">
-        <v>2010</v>
-      </c>
-      <c r="H49" t="s">
-        <v>348</v>
-      </c>
-      <c r="I49" t="s">
-        <v>349</v>
-      </c>
-      <c r="J49" s="2" t="s">
-        <v>467</v>
-      </c>
-      <c r="K49" s="2" t="s">
-        <v>466</v>
-      </c>
-      <c r="L49" s="2" t="s">
-        <v>465</v>
+        <v>150</v>
       </c>
     </row>
     <row r="50" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>28</v>
+        <v>462</v>
       </c>
       <c r="B50" t="s">
-        <v>25</v>
+        <v>250</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>48</v>
+        <v>464</v>
+      </c>
+      <c r="D50" t="s">
+        <v>463</v>
+      </c>
+      <c r="E50" t="s">
+        <v>14</v>
+      </c>
+      <c r="F50">
+        <v>1946</v>
+      </c>
+      <c r="G50">
+        <v>2010</v>
+      </c>
+      <c r="H50" t="s">
+        <v>348</v>
+      </c>
+      <c r="I50" t="s">
+        <v>349</v>
+      </c>
+      <c r="J50" s="2" t="s">
+        <v>467</v>
+      </c>
+      <c r="K50" s="2" t="s">
+        <v>466</v>
+      </c>
+      <c r="L50" s="2" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="51" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>80</v>
+        <v>28</v>
       </c>
       <c r="B51" t="s">
-        <v>128</v>
+        <v>25</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="E51" t="s">
-        <v>9</v>
-      </c>
-      <c r="F51">
-        <v>1979</v>
+        <v>48</v>
       </c>
     </row>
     <row r="52" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>125</v>
+        <v>80</v>
       </c>
       <c r="B52" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>126</v>
+        <v>81</v>
+      </c>
+      <c r="E52" t="s">
+        <v>9</v>
+      </c>
+      <c r="F52">
+        <v>1979</v>
       </c>
     </row>
     <row r="53" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>179</v>
+        <v>125</v>
       </c>
       <c r="B53" t="s">
-        <v>165</v>
+        <v>124</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>180</v>
+        <v>126</v>
       </c>
     </row>
     <row r="54" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
+        <v>179</v>
+      </c>
+      <c r="B54" t="s">
+        <v>165</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="55" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
         <v>78</v>
       </c>
-      <c r="B54" t="s">
+      <c r="B55" t="s">
         <v>25</v>
       </c>
-      <c r="C54" s="2" t="s">
+      <c r="C55" s="2" t="s">
         <v>79</v>
-      </c>
-      <c r="E54" t="s">
-        <v>9</v>
-      </c>
-      <c r="F54">
-        <v>1979</v>
-      </c>
-    </row>
-    <row r="55" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A55" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="B55" t="s">
-        <v>83</v>
-      </c>
-      <c r="C55" s="2" t="s">
-        <v>84</v>
       </c>
       <c r="E55" t="s">
         <v>9</v>
@@ -2958,13 +3000,13 @@
     </row>
     <row r="56" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A56" s="3" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B56" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="E56" t="s">
         <v>9</v>
@@ -2972,225 +3014,225 @@
       <c r="F56">
         <v>1979</v>
       </c>
-      <c r="G56">
+    </row>
+    <row r="57" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A57" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="B57" t="s">
+        <v>86</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="E57" t="s">
+        <v>9</v>
+      </c>
+      <c r="F57">
+        <v>1979</v>
+      </c>
+      <c r="G57">
         <v>2009</v>
-      </c>
-    </row>
-    <row r="57" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A57" t="s">
-        <v>27</v>
-      </c>
-      <c r="B57" t="s">
-        <v>25</v>
-      </c>
-      <c r="C57" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="Q57" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="58" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>120</v>
+        <v>27</v>
       </c>
       <c r="B58" t="s">
-        <v>259</v>
+        <v>25</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="I58" t="s">
-        <v>20</v>
+        <v>49</v>
+      </c>
+      <c r="Q58" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="59" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>5</v>
+        <v>120</v>
       </c>
       <c r="B59" t="s">
-        <v>25</v>
+        <v>259</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D59" t="s">
-        <v>94</v>
-      </c>
-      <c r="E59" t="s">
-        <v>9</v>
-      </c>
-      <c r="F59">
-        <v>2002</v>
-      </c>
-      <c r="H59" t="s">
-        <v>16</v>
+        <v>119</v>
       </c>
       <c r="I59" t="s">
-        <v>248</v>
-      </c>
-      <c r="Q59" t="s">
-        <v>44</v>
+        <v>20</v>
       </c>
     </row>
     <row r="60" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
+        <v>5</v>
+      </c>
+      <c r="B60" t="s">
+        <v>25</v>
+      </c>
+      <c r="C60" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D60" t="s">
+        <v>94</v>
+      </c>
+      <c r="E60" t="s">
+        <v>9</v>
+      </c>
+      <c r="F60">
+        <v>2002</v>
+      </c>
+      <c r="H60" t="s">
+        <v>16</v>
+      </c>
+      <c r="I60" t="s">
+        <v>248</v>
+      </c>
+      <c r="Q60" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="61" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
         <v>240</v>
       </c>
-      <c r="B60" t="s">
+      <c r="B61" t="s">
         <v>237</v>
       </c>
-      <c r="C60" s="2" t="s">
+      <c r="C61" s="2" t="s">
         <v>243</v>
       </c>
-      <c r="H60" t="s">
-        <v>16</v>
-      </c>
-      <c r="I60" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="61" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A61" s="1" t="s">
+      <c r="H61" t="s">
+        <v>16</v>
+      </c>
+      <c r="I61" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="62" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A62" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B61" t="s">
+      <c r="B62" t="s">
         <v>25</v>
       </c>
-      <c r="C61" s="2" t="s">
+      <c r="C62" s="2" t="s">
         <v>52</v>
-      </c>
-    </row>
-    <row r="62" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A62" t="s">
-        <v>232</v>
-      </c>
-      <c r="B62" t="s">
-        <v>250</v>
-      </c>
-      <c r="C62" s="2" t="s">
-        <v>231</v>
       </c>
     </row>
     <row r="63" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>390</v>
+        <v>232</v>
       </c>
       <c r="B63" t="s">
-        <v>83</v>
+        <v>250</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>392</v>
-      </c>
-      <c r="D63" t="s">
-        <v>391</v>
-      </c>
-      <c r="E63" t="s">
-        <v>9</v>
-      </c>
-      <c r="F63">
-        <v>2007</v>
-      </c>
-      <c r="G63">
-        <v>2015</v>
-      </c>
-      <c r="H63" t="s">
-        <v>348</v>
-      </c>
-      <c r="I63" t="s">
-        <v>349</v>
-      </c>
-      <c r="Q63" t="s">
-        <v>393</v>
+        <v>231</v>
       </c>
     </row>
     <row r="64" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>276</v>
+        <v>390</v>
       </c>
       <c r="B64" t="s">
-        <v>124</v>
+        <v>83</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>277</v>
+        <v>392</v>
+      </c>
+      <c r="D64" t="s">
+        <v>391</v>
+      </c>
+      <c r="E64" t="s">
+        <v>9</v>
       </c>
       <c r="F64">
-        <v>1948</v>
+        <v>2007</v>
       </c>
       <c r="G64">
-        <v>2000</v>
+        <v>2015</v>
       </c>
       <c r="H64" t="s">
-        <v>16</v>
+        <v>348</v>
       </c>
       <c r="I64" t="s">
-        <v>20</v>
+        <v>349</v>
+      </c>
+      <c r="Q64" t="s">
+        <v>393</v>
       </c>
     </row>
     <row r="65" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>449</v>
+        <v>276</v>
       </c>
       <c r="B65" t="s">
-        <v>250</v>
+        <v>124</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>448</v>
-      </c>
-      <c r="E65" t="s">
-        <v>14</v>
+        <v>277</v>
       </c>
       <c r="F65">
-        <v>-4000</v>
+        <v>1948</v>
       </c>
       <c r="G65">
         <v>2000</v>
       </c>
       <c r="H65" t="s">
-        <v>348</v>
+        <v>16</v>
       </c>
       <c r="I65" t="s">
-        <v>349</v>
-      </c>
-      <c r="J65" s="2" t="s">
-        <v>450</v>
-      </c>
-      <c r="N65" s="2" t="s">
-        <v>451</v>
+        <v>20</v>
       </c>
     </row>
     <row r="66" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>224</v>
+        <v>449</v>
       </c>
       <c r="B66" t="s">
-        <v>40</v>
+        <v>250</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>225</v>
+        <v>448</v>
+      </c>
+      <c r="E66" t="s">
+        <v>14</v>
       </c>
       <c r="F66">
-        <v>1964</v>
+        <v>-4000</v>
       </c>
       <c r="G66">
-        <v>2008</v>
+        <v>2000</v>
       </c>
       <c r="H66" t="s">
-        <v>16</v>
+        <v>348</v>
       </c>
       <c r="I66" t="s">
-        <v>20</v>
+        <v>349</v>
+      </c>
+      <c r="J66" s="2" t="s">
+        <v>450</v>
+      </c>
+      <c r="N66" s="2" t="s">
+        <v>451</v>
       </c>
     </row>
     <row r="67" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>285</v>
+        <v>224</v>
       </c>
       <c r="B67" t="s">
-        <v>250</v>
+        <v>40</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>286</v>
+        <v>225</v>
+      </c>
+      <c r="F67">
+        <v>1964</v>
+      </c>
+      <c r="G67">
+        <v>2008</v>
       </c>
       <c r="H67" t="s">
         <v>16</v>
@@ -3201,259 +3243,259 @@
     </row>
     <row r="68" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>205</v>
+        <v>285</v>
       </c>
       <c r="B68" t="s">
-        <v>40</v>
+        <v>250</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>204</v>
-      </c>
-      <c r="F68">
-        <v>2006</v>
+        <v>286</v>
+      </c>
+      <c r="H68" t="s">
+        <v>16</v>
+      </c>
+      <c r="I68" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="69" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>200</v>
+        <v>205</v>
       </c>
       <c r="B69" t="s">
-        <v>99</v>
+        <v>40</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="F69">
-        <v>1980</v>
-      </c>
-      <c r="G69">
-        <v>2007</v>
-      </c>
-      <c r="Q69" t="s">
-        <v>18</v>
+        <v>2006</v>
       </c>
     </row>
     <row r="70" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>468</v>
+        <v>200</v>
       </c>
       <c r="B70" t="s">
-        <v>40</v>
+        <v>99</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>464</v>
-      </c>
-      <c r="E70" t="s">
-        <v>14</v>
+        <v>201</v>
       </c>
       <c r="F70">
-        <v>1816</v>
+        <v>1980</v>
       </c>
       <c r="G70">
-        <v>2001</v>
-      </c>
-      <c r="H70" t="s">
-        <v>348</v>
-      </c>
-      <c r="I70" t="s">
-        <v>349</v>
-      </c>
-      <c r="J70" s="2" t="s">
-        <v>469</v>
-      </c>
-      <c r="K70" s="2" t="s">
-        <v>470</v>
-      </c>
-      <c r="L70" s="2" t="s">
-        <v>471</v>
+        <v>2007</v>
+      </c>
+      <c r="Q70" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="71" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>89</v>
+        <v>468</v>
       </c>
       <c r="B71" t="s">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>88</v>
+        <v>464</v>
       </c>
       <c r="E71" t="s">
-        <v>34</v>
+        <v>14</v>
       </c>
       <c r="F71">
-        <v>1972</v>
+        <v>1816</v>
+      </c>
+      <c r="G71">
+        <v>2001</v>
       </c>
       <c r="H71" t="s">
-        <v>16</v>
+        <v>348</v>
       </c>
       <c r="I71" t="s">
-        <v>20</v>
+        <v>349</v>
+      </c>
+      <c r="J71" s="2" t="s">
+        <v>469</v>
+      </c>
+      <c r="K71" s="2" t="s">
+        <v>470</v>
+      </c>
+      <c r="L71" s="2" t="s">
+        <v>471</v>
       </c>
     </row>
     <row r="72" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>104</v>
+        <v>89</v>
       </c>
       <c r="B72" t="s">
         <v>25</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>106</v>
+        <v>88</v>
       </c>
       <c r="E72" t="s">
-        <v>105</v>
+        <v>34</v>
       </c>
       <c r="F72">
-        <v>1980</v>
+        <v>1972</v>
+      </c>
+      <c r="H72" t="s">
+        <v>16</v>
+      </c>
+      <c r="I72" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="73" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>460</v>
+        <v>104</v>
       </c>
       <c r="B73" t="s">
         <v>25</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>461</v>
-      </c>
-      <c r="D73" t="s">
-        <v>363</v>
+        <v>106</v>
       </c>
       <c r="E73" t="s">
         <v>105</v>
       </c>
       <c r="F73">
-        <v>2009</v>
-      </c>
-      <c r="H73" t="s">
-        <v>348</v>
-      </c>
-      <c r="I73" t="s">
-        <v>301</v>
+        <v>1980</v>
       </c>
     </row>
     <row r="74" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>62</v>
+        <v>460</v>
       </c>
       <c r="B74" t="s">
         <v>25</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>63</v>
+        <v>461</v>
+      </c>
+      <c r="D74" t="s">
+        <v>363</v>
+      </c>
+      <c r="E74" t="s">
+        <v>105</v>
+      </c>
+      <c r="F74">
+        <v>2009</v>
+      </c>
+      <c r="H74" t="s">
+        <v>348</v>
+      </c>
+      <c r="I74" t="s">
+        <v>301</v>
       </c>
     </row>
     <row r="75" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>311</v>
+        <v>62</v>
       </c>
       <c r="B75" t="s">
-        <v>165</v>
+        <v>25</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>312</v>
-      </c>
-      <c r="E75" t="s">
-        <v>14</v>
-      </c>
-      <c r="H75" t="s">
-        <v>16</v>
-      </c>
-      <c r="I75" t="s">
-        <v>301</v>
+        <v>63</v>
       </c>
     </row>
     <row r="76" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>281</v>
+        <v>311</v>
       </c>
       <c r="B76" t="s">
-        <v>237</v>
+        <v>165</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>282</v>
+        <v>312</v>
+      </c>
+      <c r="E76" t="s">
+        <v>14</v>
       </c>
       <c r="H76" t="s">
         <v>16</v>
       </c>
       <c r="I76" t="s">
-        <v>20</v>
+        <v>301</v>
       </c>
     </row>
     <row r="77" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>418</v>
+        <v>281</v>
       </c>
       <c r="B77" t="s">
-        <v>86</v>
+        <v>237</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>419</v>
-      </c>
-      <c r="E77" t="s">
-        <v>420</v>
-      </c>
-      <c r="F77">
-        <v>1948</v>
-      </c>
-      <c r="G77">
-        <v>2012</v>
+        <v>282</v>
       </c>
       <c r="H77" t="s">
-        <v>348</v>
+        <v>16</v>
       </c>
       <c r="I77" t="s">
-        <v>349</v>
-      </c>
-      <c r="K77" s="2" t="s">
-        <v>421</v>
-      </c>
-      <c r="Q77" t="s">
-        <v>422</v>
+        <v>20</v>
       </c>
     </row>
     <row r="78" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>151</v>
+        <v>418</v>
       </c>
       <c r="B78" t="s">
-        <v>40</v>
+        <v>86</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>152</v>
+        <v>419</v>
       </c>
       <c r="E78" t="s">
-        <v>14</v>
+        <v>420</v>
+      </c>
+      <c r="F78">
+        <v>1948</v>
+      </c>
+      <c r="G78">
+        <v>2012</v>
+      </c>
+      <c r="H78" t="s">
+        <v>348</v>
+      </c>
+      <c r="I78" t="s">
+        <v>349</v>
+      </c>
+      <c r="K78" s="2" t="s">
+        <v>421</v>
+      </c>
+      <c r="Q78" t="s">
+        <v>422</v>
       </c>
     </row>
     <row r="79" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>242</v>
+        <v>151</v>
       </c>
       <c r="B79" t="s">
-        <v>237</v>
+        <v>40</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>243</v>
-      </c>
-      <c r="H79" t="s">
-        <v>16</v>
-      </c>
-      <c r="I79" t="s">
-        <v>20</v>
+        <v>152</v>
+      </c>
+      <c r="E79" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="80" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>292</v>
+        <v>242</v>
       </c>
       <c r="B80" t="s">
-        <v>99</v>
+        <v>237</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>291</v>
+        <v>243</v>
       </c>
       <c r="H80" t="s">
         <v>16</v>
@@ -3464,47 +3506,47 @@
     </row>
     <row r="81" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>153</v>
+        <v>292</v>
       </c>
       <c r="B81" t="s">
-        <v>259</v>
+        <v>99</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>154</v>
+        <v>291</v>
+      </c>
+      <c r="H81" t="s">
+        <v>16</v>
+      </c>
+      <c r="I81" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="82" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>228</v>
+        <v>153</v>
       </c>
       <c r="B82" t="s">
-        <v>40</v>
+        <v>259</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>225</v>
-      </c>
-      <c r="F82">
-        <v>1989</v>
-      </c>
-      <c r="G82">
-        <v>2017</v>
-      </c>
-      <c r="H82" t="s">
-        <v>16</v>
-      </c>
-      <c r="I82" t="s">
-        <v>20</v>
+        <v>154</v>
       </c>
     </row>
     <row r="83" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>245</v>
+        <v>228</v>
       </c>
       <c r="B83" t="s">
-        <v>237</v>
+        <v>40</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>244</v>
+        <v>225</v>
+      </c>
+      <c r="F83">
+        <v>1989</v>
+      </c>
+      <c r="G83">
+        <v>2017</v>
       </c>
       <c r="H83" t="s">
         <v>16</v>
@@ -3515,50 +3557,41 @@
     </row>
     <row r="84" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>100</v>
+        <v>245</v>
       </c>
       <c r="B84" t="s">
-        <v>99</v>
+        <v>237</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>101</v>
+        <v>244</v>
+      </c>
+      <c r="H84" t="s">
+        <v>16</v>
+      </c>
+      <c r="I84" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="85" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>239</v>
+        <v>100</v>
       </c>
       <c r="B85" t="s">
-        <v>237</v>
+        <v>99</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>243</v>
-      </c>
-      <c r="H85" t="s">
-        <v>16</v>
-      </c>
-      <c r="I85" t="s">
-        <v>20</v>
+        <v>101</v>
       </c>
     </row>
     <row r="86" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>254</v>
+        <v>239</v>
       </c>
       <c r="B86" t="s">
-        <v>55</v>
+        <v>237</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>253</v>
-      </c>
-      <c r="E86" t="s">
-        <v>255</v>
-      </c>
-      <c r="F86">
-        <v>1960</v>
-      </c>
-      <c r="G86">
-        <v>2014</v>
+        <v>243</v>
       </c>
       <c r="H86" t="s">
         <v>16</v>
@@ -3569,19 +3602,22 @@
     </row>
     <row r="87" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>270</v>
+        <v>254</v>
       </c>
       <c r="B87" t="s">
         <v>55</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>271</v>
+        <v>253</v>
+      </c>
+      <c r="E87" t="s">
+        <v>255</v>
       </c>
       <c r="F87">
-        <v>1990</v>
+        <v>1960</v>
       </c>
       <c r="G87">
-        <v>2010</v>
+        <v>2014</v>
       </c>
       <c r="H87" t="s">
         <v>16</v>
@@ -3592,96 +3628,90 @@
     </row>
     <row r="88" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>117</v>
+        <v>270</v>
       </c>
       <c r="B88" t="s">
         <v>55</v>
       </c>
       <c r="C88" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="F88">
+        <v>1990</v>
+      </c>
+      <c r="G88">
+        <v>2010</v>
+      </c>
+      <c r="H88" t="s">
+        <v>16</v>
+      </c>
+      <c r="I88" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="89" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A89" t="s">
+        <v>117</v>
+      </c>
+      <c r="B89" t="s">
+        <v>55</v>
+      </c>
+      <c r="C89" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="I88" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q88" t="s">
+      <c r="I89" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q89" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="89" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A89" s="1" t="s">
+    <row r="90" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A90" s="1" t="s">
         <v>23</v>
-      </c>
-      <c r="B89" t="s">
-        <v>25</v>
-      </c>
-      <c r="C89" s="2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="90" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A90" t="s">
-        <v>300</v>
       </c>
       <c r="B90" t="s">
         <v>25</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>298</v>
-      </c>
-      <c r="E90" t="s">
-        <v>299</v>
-      </c>
-      <c r="F90">
-        <v>1969</v>
-      </c>
-      <c r="H90" t="s">
-        <v>16</v>
-      </c>
-      <c r="I90" t="s">
-        <v>249</v>
+        <v>53</v>
       </c>
     </row>
     <row r="91" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>332</v>
+        <v>300</v>
       </c>
       <c r="B91" t="s">
-        <v>134</v>
+        <v>25</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>333</v>
+        <v>298</v>
       </c>
       <c r="E91" t="s">
-        <v>334</v>
+        <v>299</v>
+      </c>
+      <c r="F91">
+        <v>1969</v>
       </c>
       <c r="H91" t="s">
         <v>16</v>
       </c>
       <c r="I91" t="s">
-        <v>20</v>
+        <v>249</v>
       </c>
     </row>
     <row r="92" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>267</v>
+        <v>332</v>
       </c>
       <c r="B92" t="s">
-        <v>250</v>
+        <v>134</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>266</v>
-      </c>
-      <c r="D92" t="s">
-        <v>269</v>
+        <v>333</v>
       </c>
       <c r="E92" t="s">
-        <v>268</v>
-      </c>
-      <c r="F92">
-        <v>1970</v>
-      </c>
-      <c r="G92">
-        <v>2014</v>
+        <v>334</v>
       </c>
       <c r="H92" t="s">
         <v>16</v>
@@ -3692,97 +3722,100 @@
     </row>
     <row r="93" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>407</v>
+        <v>267</v>
       </c>
       <c r="B93" t="s">
-        <v>40</v>
+        <v>250</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>406</v>
+        <v>266</v>
       </c>
       <c r="D93" t="s">
-        <v>408</v>
+        <v>269</v>
       </c>
       <c r="E93" t="s">
-        <v>14</v>
+        <v>268</v>
       </c>
       <c r="F93">
-        <v>1949</v>
+        <v>1970</v>
       </c>
       <c r="G93">
-        <v>2013</v>
+        <v>2014</v>
       </c>
       <c r="H93" t="s">
-        <v>348</v>
+        <v>16</v>
       </c>
       <c r="I93" t="s">
-        <v>349</v>
+        <v>20</v>
       </c>
     </row>
     <row r="94" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>96</v>
+        <v>407</v>
       </c>
       <c r="B94" t="s">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>90</v>
+        <v>406</v>
+      </c>
+      <c r="D94" t="s">
+        <v>408</v>
       </c>
       <c r="E94" t="s">
-        <v>69</v>
+        <v>14</v>
       </c>
       <c r="F94">
-        <v>1995</v>
+        <v>1949</v>
+      </c>
+      <c r="G94">
+        <v>2013</v>
+      </c>
+      <c r="H94" t="s">
+        <v>348</v>
+      </c>
+      <c r="I94" t="s">
+        <v>349</v>
       </c>
     </row>
     <row r="95" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>404</v>
+        <v>96</v>
       </c>
       <c r="B95" t="s">
-        <v>83</v>
+        <v>25</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>403</v>
-      </c>
-      <c r="D95" t="s">
-        <v>405</v>
+        <v>90</v>
       </c>
       <c r="E95" t="s">
-        <v>14</v>
+        <v>69</v>
       </c>
       <c r="F95">
-        <v>1875</v>
-      </c>
-      <c r="G95">
-        <v>2004</v>
-      </c>
-      <c r="H95" t="s">
-        <v>348</v>
-      </c>
-      <c r="I95" t="s">
-        <v>349</v>
+        <v>1995</v>
       </c>
     </row>
     <row r="96" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>454</v>
+        <v>404</v>
       </c>
       <c r="B96" t="s">
-        <v>25</v>
+        <v>83</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>455</v>
+        <v>403</v>
+      </c>
+      <c r="D96" t="s">
+        <v>405</v>
       </c>
       <c r="E96" t="s">
-        <v>456</v>
+        <v>14</v>
       </c>
       <c r="F96">
-        <v>2006</v>
+        <v>1875</v>
       </c>
       <c r="G96">
-        <v>2016</v>
+        <v>2004</v>
       </c>
       <c r="H96" t="s">
         <v>348</v>
@@ -3790,80 +3823,83 @@
       <c r="I96" t="s">
         <v>349</v>
       </c>
-      <c r="J96" s="2" t="s">
-        <v>457</v>
-      </c>
-      <c r="L96" s="2" t="s">
-        <v>458</v>
-      </c>
-      <c r="Q96" t="s">
-        <v>459</v>
-      </c>
     </row>
     <row r="97" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>11</v>
+        <v>454</v>
       </c>
       <c r="B97" t="s">
         <v>25</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D97" t="s">
-        <v>95</v>
+        <v>455</v>
       </c>
       <c r="E97" t="s">
-        <v>10</v>
+        <v>456</v>
       </c>
       <c r="F97">
-        <v>2007</v>
+        <v>2006</v>
+      </c>
+      <c r="G97">
+        <v>2016</v>
       </c>
       <c r="H97" t="s">
-        <v>16</v>
+        <v>348</v>
       </c>
       <c r="I97" t="s">
-        <v>21</v>
+        <v>349</v>
+      </c>
+      <c r="J97" s="2" t="s">
+        <v>457</v>
+      </c>
+      <c r="L97" s="2" t="s">
+        <v>458</v>
+      </c>
+      <c r="Q97" t="s">
+        <v>459</v>
       </c>
     </row>
     <row r="98" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>223</v>
+        <v>11</v>
       </c>
       <c r="B98" t="s">
-        <v>124</v>
+        <v>25</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>222</v>
+        <v>12</v>
+      </c>
+      <c r="D98" t="s">
+        <v>95</v>
+      </c>
+      <c r="E98" t="s">
+        <v>10</v>
       </c>
       <c r="F98">
-        <v>1</v>
-      </c>
-      <c r="G98">
-        <v>2010</v>
+        <v>2007</v>
       </c>
       <c r="H98" t="s">
         <v>16</v>
       </c>
       <c r="I98" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="99" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="B99" t="s">
-        <v>40</v>
+        <v>124</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="F99">
-        <v>1946</v>
+        <v>1</v>
       </c>
       <c r="G99">
-        <v>2016</v>
+        <v>2010</v>
       </c>
       <c r="H99" t="s">
         <v>16</v>
@@ -3874,122 +3910,122 @@
     </row>
     <row r="100" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>97</v>
+        <v>226</v>
       </c>
       <c r="B100" t="s">
-        <v>128</v>
+        <v>40</v>
       </c>
       <c r="C100" s="2" t="s">
-        <v>98</v>
+        <v>225</v>
+      </c>
+      <c r="F100">
+        <v>1946</v>
+      </c>
+      <c r="G100">
+        <v>2016</v>
+      </c>
+      <c r="H100" t="s">
+        <v>16</v>
+      </c>
+      <c r="I100" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="101" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>278</v>
+        <v>97</v>
       </c>
       <c r="B101" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>279</v>
-      </c>
-      <c r="E101" t="s">
-        <v>280</v>
-      </c>
-      <c r="F101">
-        <v>1890</v>
-      </c>
-      <c r="G101">
-        <v>1996</v>
-      </c>
-      <c r="H101" t="s">
-        <v>16</v>
-      </c>
-      <c r="I101" t="s">
-        <v>20</v>
+        <v>98</v>
       </c>
     </row>
     <row r="102" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>156</v>
+        <v>278</v>
       </c>
       <c r="B102" t="s">
-        <v>25</v>
+        <v>124</v>
       </c>
       <c r="C102" s="2" t="s">
-        <v>154</v>
+        <v>279</v>
+      </c>
+      <c r="E102" t="s">
+        <v>280</v>
+      </c>
+      <c r="F102">
+        <v>1890</v>
+      </c>
+      <c r="G102">
+        <v>1996</v>
+      </c>
+      <c r="H102" t="s">
+        <v>16</v>
+      </c>
+      <c r="I102" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="103" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>413</v>
+        <v>156</v>
       </c>
       <c r="B103" t="s">
-        <v>128</v>
+        <v>25</v>
       </c>
       <c r="C103" s="2" t="s">
-        <v>414</v>
-      </c>
-      <c r="E103" t="s">
-        <v>415</v>
-      </c>
-      <c r="F103">
-        <v>1946</v>
-      </c>
-      <c r="G103">
-        <v>2014</v>
-      </c>
-      <c r="H103" t="s">
-        <v>348</v>
-      </c>
-      <c r="I103" t="s">
-        <v>349</v>
-      </c>
-      <c r="N103" s="2" t="s">
-        <v>416</v>
-      </c>
-      <c r="Q103" t="s">
-        <v>417</v>
+        <v>154</v>
       </c>
     </row>
     <row r="104" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>229</v>
+        <v>413</v>
       </c>
       <c r="B104" t="s">
-        <v>40</v>
+        <v>128</v>
       </c>
       <c r="C104" s="2" t="s">
-        <v>225</v>
+        <v>414</v>
+      </c>
+      <c r="E104" t="s">
+        <v>415</v>
       </c>
       <c r="F104">
-        <v>1952</v>
+        <v>1946</v>
       </c>
       <c r="G104">
-        <v>1997</v>
+        <v>2014</v>
       </c>
       <c r="H104" t="s">
-        <v>16</v>
+        <v>348</v>
       </c>
       <c r="I104" t="s">
-        <v>20</v>
+        <v>349</v>
+      </c>
+      <c r="N104" s="2" t="s">
+        <v>416</v>
+      </c>
+      <c r="Q104" t="s">
+        <v>417</v>
       </c>
     </row>
     <row r="105" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>293</v>
+        <v>229</v>
       </c>
       <c r="B105" t="s">
         <v>40</v>
       </c>
       <c r="C105" s="2" t="s">
-        <v>294</v>
+        <v>225</v>
       </c>
       <c r="F105">
-        <v>2004</v>
+        <v>1952</v>
       </c>
       <c r="G105">
-        <v>2006</v>
+        <v>1997</v>
       </c>
       <c r="H105" t="s">
         <v>16</v>
@@ -4000,221 +4036,218 @@
     </row>
     <row r="106" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>102</v>
+        <v>293</v>
       </c>
       <c r="B106" t="s">
-        <v>99</v>
+        <v>40</v>
       </c>
       <c r="C106" s="2" t="s">
-        <v>103</v>
+        <v>294</v>
+      </c>
+      <c r="F106">
+        <v>2004</v>
+      </c>
+      <c r="G106">
+        <v>2006</v>
+      </c>
+      <c r="H106" t="s">
+        <v>16</v>
+      </c>
+      <c r="I106" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="107" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>289</v>
+        <v>102</v>
       </c>
       <c r="B107" t="s">
-        <v>124</v>
+        <v>99</v>
       </c>
       <c r="C107" s="2" t="s">
-        <v>290</v>
+        <v>103</v>
       </c>
     </row>
     <row r="108" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>246</v>
+        <v>289</v>
       </c>
       <c r="B108" t="s">
-        <v>165</v>
+        <v>124</v>
       </c>
       <c r="C108" s="2" t="s">
-        <v>247</v>
-      </c>
-      <c r="E108" t="s">
-        <v>14</v>
-      </c>
-      <c r="F108">
-        <v>1960</v>
-      </c>
-      <c r="G108">
-        <v>2006</v>
-      </c>
-      <c r="H108" t="s">
-        <v>16</v>
-      </c>
-      <c r="I108" t="s">
-        <v>249</v>
+        <v>290</v>
       </c>
     </row>
     <row r="109" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>365</v>
+        <v>246</v>
       </c>
       <c r="B109" t="s">
-        <v>128</v>
+        <v>165</v>
       </c>
       <c r="C109" s="2" t="s">
-        <v>364</v>
-      </c>
-      <c r="D109" t="s">
-        <v>370</v>
+        <v>247</v>
       </c>
       <c r="E109" t="s">
-        <v>366</v>
+        <v>14</v>
       </c>
       <c r="F109">
-        <v>1906</v>
+        <v>1960</v>
       </c>
       <c r="G109">
-        <v>2013</v>
+        <v>2006</v>
       </c>
       <c r="H109" t="s">
-        <v>367</v>
+        <v>16</v>
       </c>
       <c r="I109" t="s">
-        <v>368</v>
-      </c>
-      <c r="Q109" t="s">
-        <v>369</v>
+        <v>249</v>
       </c>
     </row>
     <row r="110" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>208</v>
+        <v>365</v>
       </c>
       <c r="B110" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="C110" s="2" t="s">
-        <v>209</v>
+        <v>364</v>
+      </c>
+      <c r="D110" t="s">
+        <v>370</v>
+      </c>
+      <c r="E110" t="s">
+        <v>366</v>
       </c>
       <c r="F110">
-        <v>1932</v>
+        <v>1906</v>
       </c>
       <c r="G110">
-        <v>2014</v>
+        <v>2013</v>
       </c>
       <c r="H110" t="s">
-        <v>16</v>
+        <v>367</v>
       </c>
       <c r="I110" t="s">
-        <v>20</v>
+        <v>368</v>
+      </c>
+      <c r="Q110" t="s">
+        <v>369</v>
       </c>
     </row>
     <row r="111" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>137</v>
+        <v>208</v>
       </c>
       <c r="B111" t="s">
-        <v>259</v>
+        <v>124</v>
       </c>
       <c r="C111" s="2" t="s">
-        <v>138</v>
+        <v>209</v>
+      </c>
+      <c r="F111">
+        <v>1932</v>
+      </c>
+      <c r="G111">
+        <v>2014</v>
+      </c>
+      <c r="H111" t="s">
+        <v>16</v>
+      </c>
+      <c r="I111" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="112" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>155</v>
+        <v>137</v>
       </c>
       <c r="B112" t="s">
         <v>259</v>
       </c>
       <c r="C112" s="2" t="s">
-        <v>154</v>
+        <v>138</v>
       </c>
     </row>
     <row r="113" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>57</v>
+        <v>155</v>
       </c>
       <c r="B113" t="s">
-        <v>128</v>
+        <v>259</v>
       </c>
       <c r="C113" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="Q113" t="s">
-        <v>17</v>
+        <v>154</v>
       </c>
     </row>
     <row r="114" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>129</v>
+        <v>57</v>
       </c>
       <c r="B114" t="s">
-        <v>259</v>
+        <v>128</v>
       </c>
       <c r="C114" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="E114" t="s">
-        <v>131</v>
-      </c>
-      <c r="F114">
-        <v>1945</v>
-      </c>
-      <c r="G114">
-        <v>2008</v>
-      </c>
-      <c r="I114" t="s">
-        <v>20</v>
+        <v>58</v>
+      </c>
+      <c r="Q114" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="115" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>148</v>
+        <v>129</v>
       </c>
       <c r="B115" t="s">
-        <v>128</v>
+        <v>259</v>
       </c>
       <c r="C115" s="2" t="s">
-        <v>147</v>
+        <v>130</v>
+      </c>
+      <c r="E115" t="s">
+        <v>131</v>
+      </c>
+      <c r="F115">
+        <v>1945</v>
+      </c>
+      <c r="G115">
+        <v>2008</v>
+      </c>
+      <c r="I115" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="116" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>233</v>
+        <v>148</v>
       </c>
       <c r="B116" t="s">
-        <v>165</v>
+        <v>128</v>
       </c>
       <c r="C116" s="2" t="s">
-        <v>234</v>
-      </c>
-      <c r="E116" t="s">
-        <v>14</v>
-      </c>
-      <c r="F116">
-        <v>2012</v>
-      </c>
-      <c r="G116">
-        <v>2016</v>
-      </c>
-      <c r="H116" t="s">
-        <v>16</v>
-      </c>
-      <c r="I116" t="s">
-        <v>20</v>
+        <v>147</v>
       </c>
     </row>
     <row r="117" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>35</v>
+        <v>233</v>
       </c>
       <c r="B117" t="s">
-        <v>25</v>
+        <v>165</v>
       </c>
       <c r="C117" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="D117" t="s">
-        <v>37</v>
+        <v>234</v>
       </c>
       <c r="E117" t="s">
         <v>14</v>
       </c>
       <c r="F117">
-        <v>2001</v>
+        <v>2012</v>
+      </c>
+      <c r="G117">
+        <v>2016</v>
       </c>
       <c r="H117" t="s">
         <v>16</v>
@@ -4225,145 +4258,148 @@
     </row>
     <row r="118" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>185</v>
+        <v>35</v>
       </c>
       <c r="B118" t="s">
-        <v>128</v>
+        <v>25</v>
       </c>
       <c r="C118" s="2" t="s">
-        <v>186</v>
+        <v>36</v>
+      </c>
+      <c r="D118" t="s">
+        <v>37</v>
+      </c>
+      <c r="E118" t="s">
+        <v>14</v>
+      </c>
+      <c r="F118">
+        <v>2001</v>
+      </c>
+      <c r="H118" t="s">
+        <v>16</v>
+      </c>
+      <c r="I118" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="119" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>210</v>
+        <v>185</v>
       </c>
       <c r="B119" t="s">
-        <v>40</v>
+        <v>128</v>
       </c>
       <c r="C119" s="2" t="s">
-        <v>211</v>
-      </c>
-      <c r="F119">
-        <v>1976</v>
-      </c>
-      <c r="G119">
-        <v>2016</v>
-      </c>
-      <c r="H119" t="s">
-        <v>16</v>
-      </c>
-      <c r="I119" t="s">
-        <v>20</v>
+        <v>186</v>
       </c>
     </row>
     <row r="120" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>426</v>
+        <v>210</v>
       </c>
       <c r="B120" t="s">
-        <v>86</v>
+        <v>40</v>
       </c>
       <c r="C120" s="2" t="s">
-        <v>427</v>
-      </c>
-      <c r="E120" t="s">
-        <v>34</v>
+        <v>211</v>
       </c>
       <c r="F120">
-        <v>2015</v>
+        <v>1976</v>
       </c>
       <c r="G120">
         <v>2016</v>
       </c>
       <c r="H120" t="s">
-        <v>348</v>
+        <v>16</v>
       </c>
       <c r="I120" t="s">
-        <v>349</v>
-      </c>
-      <c r="K120" s="2" t="s">
-        <v>428</v>
+        <v>20</v>
       </c>
     </row>
     <row r="121" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>144</v>
+        <v>426</v>
       </c>
       <c r="B121" t="s">
-        <v>60</v>
+        <v>86</v>
       </c>
       <c r="C121" s="2" t="s">
-        <v>143</v>
+        <v>427</v>
+      </c>
+      <c r="E121" t="s">
+        <v>34</v>
       </c>
       <c r="F121">
-        <v>1800</v>
+        <v>2015</v>
       </c>
       <c r="G121">
-        <v>2013</v>
+        <v>2016</v>
+      </c>
+      <c r="H121" t="s">
+        <v>348</v>
+      </c>
+      <c r="I121" t="s">
+        <v>349</v>
+      </c>
+      <c r="K121" s="2" t="s">
+        <v>428</v>
       </c>
     </row>
     <row r="122" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>122</v>
+        <v>144</v>
       </c>
       <c r="B122" t="s">
-        <v>259</v>
+        <v>60</v>
       </c>
       <c r="C122" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="I122" t="s">
-        <v>20</v>
+        <v>143</v>
+      </c>
+      <c r="F122">
+        <v>1800</v>
+      </c>
+      <c r="G122">
+        <v>2013</v>
       </c>
     </row>
     <row r="123" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>318</v>
+        <v>472</v>
       </c>
       <c r="B123" t="s">
-        <v>250</v>
+        <v>25</v>
       </c>
       <c r="C123" s="2" t="s">
-        <v>319</v>
+        <v>473</v>
+      </c>
+      <c r="D123" t="s">
+        <v>474</v>
       </c>
       <c r="E123" t="s">
-        <v>320</v>
+        <v>112</v>
       </c>
       <c r="F123">
-        <v>1975</v>
-      </c>
-      <c r="G123">
-        <v>1989</v>
+        <v>1943</v>
       </c>
       <c r="H123" t="s">
-        <v>16</v>
+        <v>348</v>
       </c>
       <c r="I123" t="s">
-        <v>20</v>
+        <v>349</v>
+      </c>
+      <c r="N123" s="2" t="s">
+        <v>475</v>
       </c>
     </row>
     <row r="124" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>316</v>
+        <v>122</v>
       </c>
       <c r="B124" t="s">
-        <v>250</v>
+        <v>259</v>
       </c>
       <c r="C124" s="2" t="s">
-        <v>317</v>
-      </c>
-      <c r="E124" t="s">
-        <v>105</v>
-      </c>
-      <c r="F124">
-        <v>1950</v>
-      </c>
-      <c r="G124">
-        <v>1996</v>
-      </c>
-      <c r="H124" t="s">
-        <v>16</v>
+        <v>121</v>
       </c>
       <c r="I124" t="s">
         <v>20</v>
@@ -4371,19 +4407,22 @@
     </row>
     <row r="125" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
       <c r="B125" t="s">
-        <v>25</v>
+        <v>250</v>
       </c>
       <c r="C125" s="2" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="E125" t="s">
-        <v>77</v>
+        <v>320</v>
       </c>
       <c r="F125">
-        <v>2010</v>
+        <v>1975</v>
+      </c>
+      <c r="G125">
+        <v>1989</v>
       </c>
       <c r="H125" t="s">
         <v>16</v>
@@ -4394,35 +4433,44 @@
     </row>
     <row r="126" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>141</v>
+        <v>316</v>
       </c>
       <c r="B126" t="s">
-        <v>237</v>
+        <v>250</v>
       </c>
       <c r="C126" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="Q126" t="s">
-        <v>17</v>
+        <v>317</v>
+      </c>
+      <c r="E126" t="s">
+        <v>105</v>
+      </c>
+      <c r="F126">
+        <v>1950</v>
+      </c>
+      <c r="G126">
+        <v>1996</v>
+      </c>
+      <c r="H126" t="s">
+        <v>16</v>
+      </c>
+      <c r="I126" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="127" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>308</v>
+        <v>322</v>
       </c>
       <c r="B127" t="s">
-        <v>250</v>
+        <v>25</v>
       </c>
       <c r="C127" s="2" t="s">
-        <v>309</v>
+        <v>321</v>
       </c>
       <c r="E127" t="s">
-        <v>310</v>
+        <v>77</v>
       </c>
       <c r="F127">
-        <v>1950</v>
-      </c>
-      <c r="G127">
         <v>2010</v>
       </c>
       <c r="H127" t="s">
@@ -4434,30 +4482,36 @@
     </row>
     <row r="128" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>287</v>
+        <v>141</v>
       </c>
       <c r="B128" t="s">
-        <v>134</v>
+        <v>237</v>
       </c>
       <c r="C128" s="2" t="s">
-        <v>288</v>
-      </c>
-      <c r="F128">
-        <v>1990</v>
-      </c>
-      <c r="G128">
-        <v>2008</v>
+        <v>142</v>
+      </c>
+      <c r="Q128" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="129" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>274</v>
+        <v>308</v>
       </c>
       <c r="B129" t="s">
-        <v>55</v>
+        <v>250</v>
       </c>
       <c r="C129" s="2" t="s">
-        <v>275</v>
+        <v>309</v>
+      </c>
+      <c r="E129" t="s">
+        <v>310</v>
+      </c>
+      <c r="F129">
+        <v>1950</v>
+      </c>
+      <c r="G129">
+        <v>2010</v>
       </c>
       <c r="H129" t="s">
         <v>16</v>
@@ -4468,174 +4522,162 @@
     </row>
     <row r="130" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
-        <v>157</v>
+        <v>287</v>
       </c>
       <c r="B130" t="s">
-        <v>128</v>
+        <v>134</v>
       </c>
       <c r="C130" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="Q130" t="s">
-        <v>18</v>
+        <v>288</v>
+      </c>
+      <c r="F130">
+        <v>1990</v>
+      </c>
+      <c r="G130">
+        <v>2008</v>
       </c>
     </row>
     <row r="131" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>439</v>
+        <v>274</v>
       </c>
       <c r="B131" t="s">
-        <v>259</v>
+        <v>55</v>
       </c>
       <c r="C131" s="2" t="s">
-        <v>438</v>
+        <v>275</v>
       </c>
       <c r="H131" t="s">
-        <v>348</v>
+        <v>16</v>
       </c>
       <c r="I131" t="s">
-        <v>349</v>
-      </c>
-      <c r="J131" s="2" t="s">
-        <v>440</v>
-      </c>
-      <c r="K131" s="2" t="s">
-        <v>442</v>
-      </c>
-      <c r="L131" s="2" t="s">
-        <v>441</v>
+        <v>20</v>
       </c>
     </row>
     <row r="132" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>443</v>
+        <v>157</v>
       </c>
       <c r="B132" t="s">
-        <v>259</v>
+        <v>128</v>
       </c>
       <c r="C132" s="2" t="s">
-        <v>438</v>
-      </c>
-      <c r="D132" t="s">
-        <v>447</v>
-      </c>
-      <c r="F132">
-        <v>1990</v>
-      </c>
-      <c r="G132">
-        <v>2014</v>
-      </c>
-      <c r="H132" t="s">
-        <v>348</v>
-      </c>
-      <c r="I132" t="s">
-        <v>349</v>
-      </c>
-      <c r="J132" s="2" t="s">
-        <v>444</v>
-      </c>
-      <c r="K132" s="2" t="s">
-        <v>445</v>
-      </c>
-      <c r="L132" s="2" t="s">
-        <v>446</v>
+        <v>154</v>
+      </c>
+      <c r="Q132" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="133" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
-        <v>194</v>
+        <v>439</v>
       </c>
       <c r="B133" t="s">
-        <v>99</v>
+        <v>259</v>
       </c>
       <c r="C133" s="2" t="s">
-        <v>193</v>
+        <v>438</v>
+      </c>
+      <c r="H133" t="s">
+        <v>348</v>
+      </c>
+      <c r="I133" t="s">
+        <v>349</v>
+      </c>
+      <c r="J133" s="2" t="s">
+        <v>440</v>
+      </c>
+      <c r="K133" s="2" t="s">
+        <v>442</v>
+      </c>
+      <c r="L133" s="2" t="s">
+        <v>441</v>
       </c>
     </row>
     <row r="134" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
-        <v>295</v>
+        <v>443</v>
       </c>
       <c r="B134" t="s">
-        <v>40</v>
+        <v>259</v>
       </c>
       <c r="C134" s="2" t="s">
-        <v>296</v>
-      </c>
-      <c r="E134" t="s">
-        <v>297</v>
+        <v>438</v>
+      </c>
+      <c r="D134" t="s">
+        <v>447</v>
       </c>
       <c r="F134">
         <v>1990</v>
       </c>
       <c r="G134">
-        <v>2015</v>
+        <v>2014</v>
       </c>
       <c r="H134" t="s">
-        <v>16</v>
+        <v>348</v>
       </c>
       <c r="I134" t="s">
-        <v>249</v>
+        <v>349</v>
+      </c>
+      <c r="J134" s="2" t="s">
+        <v>444</v>
+      </c>
+      <c r="K134" s="2" t="s">
+        <v>445</v>
+      </c>
+      <c r="L134" s="2" t="s">
+        <v>446</v>
       </c>
     </row>
     <row r="135" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
-        <v>256</v>
+        <v>194</v>
       </c>
       <c r="B135" t="s">
-        <v>250</v>
+        <v>99</v>
       </c>
       <c r="C135" s="2" t="s">
-        <v>257</v>
-      </c>
-      <c r="E135" t="s">
-        <v>258</v>
-      </c>
-      <c r="H135" t="s">
-        <v>16</v>
-      </c>
-      <c r="I135" t="s">
-        <v>20</v>
+        <v>193</v>
       </c>
     </row>
     <row r="136" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
-        <v>227</v>
+        <v>295</v>
       </c>
       <c r="B136" t="s">
         <v>40</v>
       </c>
       <c r="C136" s="2" t="s">
-        <v>225</v>
+        <v>296</v>
+      </c>
+      <c r="E136" t="s">
+        <v>297</v>
       </c>
       <c r="F136">
-        <v>1955</v>
+        <v>1990</v>
       </c>
       <c r="G136">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="H136" t="s">
         <v>16</v>
       </c>
       <c r="I136" t="s">
-        <v>20</v>
+        <v>249</v>
       </c>
     </row>
     <row r="137" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
-        <v>230</v>
+        <v>256</v>
       </c>
       <c r="B137" t="s">
-        <v>40</v>
+        <v>250</v>
       </c>
       <c r="C137" s="2" t="s">
-        <v>225</v>
-      </c>
-      <c r="F137">
-        <v>1995</v>
-      </c>
-      <c r="G137">
-        <v>2016</v>
+        <v>257</v>
+      </c>
+      <c r="E137" t="s">
+        <v>258</v>
       </c>
       <c r="H137" t="s">
         <v>16</v>
@@ -4646,99 +4688,102 @@
     </row>
     <row r="138" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
-        <v>452</v>
+        <v>227</v>
       </c>
       <c r="B138" t="s">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="C138" s="2" t="s">
-        <v>453</v>
-      </c>
-      <c r="E138" t="s">
-        <v>9</v>
+        <v>225</v>
+      </c>
+      <c r="F138">
+        <v>1955</v>
+      </c>
+      <c r="G138">
+        <v>2016</v>
       </c>
       <c r="H138" t="s">
-        <v>348</v>
+        <v>16</v>
       </c>
       <c r="I138" t="s">
-        <v>435</v>
+        <v>20</v>
       </c>
     </row>
     <row r="139" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
-        <v>109</v>
+        <v>230</v>
       </c>
       <c r="B139" t="s">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="C139" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="E139" t="s">
-        <v>111</v>
+        <v>225</v>
       </c>
       <c r="F139">
-        <v>1956</v>
+        <v>1995</v>
+      </c>
+      <c r="G139">
+        <v>2016</v>
+      </c>
+      <c r="H139" t="s">
+        <v>16</v>
+      </c>
+      <c r="I139" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="140" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
-        <v>326</v>
+        <v>452</v>
       </c>
       <c r="B140" t="s">
         <v>25</v>
       </c>
       <c r="C140" s="2" t="s">
-        <v>327</v>
+        <v>453</v>
       </c>
       <c r="E140" t="s">
-        <v>111</v>
-      </c>
-      <c r="F140">
-        <v>1998</v>
+        <v>9</v>
       </c>
       <c r="H140" t="s">
-        <v>16</v>
+        <v>348</v>
       </c>
       <c r="I140" t="s">
-        <v>20</v>
+        <v>435</v>
       </c>
     </row>
     <row r="141" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
-        <v>91</v>
+        <v>109</v>
       </c>
       <c r="B141" t="s">
         <v>25</v>
       </c>
       <c r="C141" s="2" t="s">
-        <v>93</v>
+        <v>110</v>
       </c>
       <c r="E141" t="s">
-        <v>92</v>
+        <v>111</v>
       </c>
       <c r="F141">
-        <v>1999</v>
+        <v>1956</v>
       </c>
     </row>
     <row r="142" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
-        <v>314</v>
+        <v>326</v>
       </c>
       <c r="B142" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="C142" s="2" t="s">
-        <v>313</v>
+        <v>327</v>
       </c>
       <c r="E142" t="s">
-        <v>315</v>
+        <v>111</v>
       </c>
       <c r="F142">
-        <v>1950</v>
-      </c>
-      <c r="G142">
-        <v>2004</v>
+        <v>1998</v>
       </c>
       <c r="H142" t="s">
         <v>16</v>
@@ -4749,122 +4794,110 @@
     </row>
     <row r="143" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
-        <v>161</v>
+        <v>91</v>
       </c>
       <c r="B143" t="s">
         <v>25</v>
       </c>
       <c r="C143" s="2" t="s">
-        <v>160</v>
+        <v>93</v>
+      </c>
+      <c r="E143" t="s">
+        <v>92</v>
+      </c>
+      <c r="F143">
+        <v>1999</v>
       </c>
     </row>
     <row r="144" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
-        <v>168</v>
+        <v>314</v>
       </c>
       <c r="B144" t="s">
         <v>40</v>
       </c>
       <c r="C144" s="2" t="s">
-        <v>167</v>
+        <v>313</v>
+      </c>
+      <c r="E144" t="s">
+        <v>315</v>
+      </c>
+      <c r="F144">
+        <v>1950</v>
+      </c>
+      <c r="G144">
+        <v>2004</v>
+      </c>
+      <c r="H144" t="s">
+        <v>16</v>
+      </c>
+      <c r="I144" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="145" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
-        <v>399</v>
+        <v>161</v>
       </c>
       <c r="B145" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="C145" s="2" t="s">
-        <v>400</v>
-      </c>
-      <c r="E145" t="s">
-        <v>14</v>
-      </c>
-      <c r="F145">
-        <v>2000</v>
-      </c>
-      <c r="G145">
-        <v>2014</v>
-      </c>
-      <c r="H145" t="s">
-        <v>348</v>
-      </c>
-      <c r="I145" t="s">
-        <v>349</v>
-      </c>
-      <c r="J145" s="2" t="s">
-        <v>402</v>
-      </c>
-      <c r="N145" s="2" t="s">
-        <v>401</v>
+        <v>160</v>
       </c>
     </row>
     <row r="146" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
-        <v>213</v>
+        <v>168</v>
       </c>
       <c r="B146" t="s">
-        <v>55</v>
+        <v>40</v>
       </c>
       <c r="C146" s="2" t="s">
-        <v>212</v>
-      </c>
-      <c r="H146" t="s">
-        <v>16</v>
-      </c>
-      <c r="I146" t="s">
-        <v>20</v>
+        <v>167</v>
       </c>
     </row>
     <row r="147" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
-        <v>395</v>
+        <v>399</v>
       </c>
       <c r="B147" t="s">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="C147" s="2" t="s">
-        <v>394</v>
-      </c>
-      <c r="D147" t="s">
-        <v>396</v>
+        <v>400</v>
       </c>
       <c r="E147" t="s">
-        <v>111</v>
+        <v>14</v>
       </c>
       <c r="F147">
-        <v>1986</v>
+        <v>2000</v>
       </c>
       <c r="G147">
-        <v>2015</v>
+        <v>2014</v>
       </c>
       <c r="H147" t="s">
-        <v>367</v>
+        <v>348</v>
       </c>
       <c r="I147" t="s">
-        <v>398</v>
+        <v>349</v>
       </c>
       <c r="J147" s="2" t="s">
-        <v>397</v>
+        <v>402</v>
+      </c>
+      <c r="N147" s="2" t="s">
+        <v>401</v>
       </c>
     </row>
     <row r="148" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
-        <v>323</v>
+        <v>213</v>
       </c>
       <c r="B148" t="s">
-        <v>25</v>
+        <v>55</v>
       </c>
       <c r="C148" s="2" t="s">
-        <v>324</v>
-      </c>
-      <c r="E148" t="s">
-        <v>325</v>
-      </c>
-      <c r="F148">
-        <v>1942</v>
+        <v>212</v>
       </c>
       <c r="H148" t="s">
         <v>16</v>
@@ -4875,124 +4908,145 @@
     </row>
     <row r="149" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
-        <v>273</v>
+        <v>395</v>
       </c>
       <c r="B149" t="s">
-        <v>237</v>
+        <v>25</v>
       </c>
       <c r="C149" s="2" t="s">
-        <v>272</v>
+        <v>394</v>
+      </c>
+      <c r="D149" t="s">
+        <v>396</v>
+      </c>
+      <c r="E149" t="s">
+        <v>111</v>
       </c>
       <c r="F149">
-        <v>1996</v>
+        <v>1986</v>
       </c>
       <c r="G149">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="H149" t="s">
-        <v>16</v>
+        <v>367</v>
       </c>
       <c r="I149" t="s">
-        <v>20</v>
+        <v>398</v>
+      </c>
+      <c r="J149" s="2" t="s">
+        <v>397</v>
       </c>
     </row>
     <row r="150" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
-        <v>66</v>
+        <v>323</v>
       </c>
       <c r="B150" t="s">
         <v>25</v>
       </c>
       <c r="C150" s="2" t="s">
-        <v>67</v>
+        <v>324</v>
+      </c>
+      <c r="E150" t="s">
+        <v>325</v>
+      </c>
+      <c r="F150">
+        <v>1942</v>
+      </c>
+      <c r="H150" t="s">
+        <v>16</v>
+      </c>
+      <c r="I150" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="151" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
-        <v>383</v>
+        <v>273</v>
       </c>
       <c r="B151" t="s">
-        <v>40</v>
+        <v>237</v>
       </c>
       <c r="C151" s="2" t="s">
-        <v>384</v>
-      </c>
-      <c r="E151" t="s">
-        <v>386</v>
+        <v>272</v>
       </c>
       <c r="F151">
-        <v>1951</v>
+        <v>1996</v>
+      </c>
+      <c r="G151">
+        <v>2016</v>
       </c>
       <c r="H151" t="s">
-        <v>348</v>
+        <v>16</v>
       </c>
       <c r="I151" t="s">
-        <v>349</v>
-      </c>
-      <c r="N151" s="2" t="s">
-        <v>385</v>
+        <v>20</v>
       </c>
     </row>
     <row r="152" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
-        <v>139</v>
+        <v>66</v>
       </c>
       <c r="B152" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="C152" s="2" t="s">
-        <v>140</v>
+        <v>67</v>
       </c>
     </row>
     <row r="153" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
-        <v>329</v>
+        <v>383</v>
       </c>
       <c r="B153" t="s">
-        <v>165</v>
+        <v>40</v>
       </c>
       <c r="C153" s="2" t="s">
-        <v>328</v>
+        <v>384</v>
       </c>
       <c r="E153" t="s">
-        <v>34</v>
+        <v>386</v>
       </c>
       <c r="F153">
-        <v>1789</v>
+        <v>1951</v>
       </c>
       <c r="H153" t="s">
-        <v>16</v>
+        <v>348</v>
       </c>
       <c r="I153" t="s">
-        <v>20</v>
+        <v>349</v>
+      </c>
+      <c r="N153" s="2" t="s">
+        <v>385</v>
       </c>
     </row>
     <row r="154" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
-        <v>172</v>
+        <v>139</v>
       </c>
       <c r="B154" t="s">
-        <v>60</v>
+        <v>40</v>
       </c>
       <c r="C154" s="2" t="s">
-        <v>171</v>
+        <v>140</v>
       </c>
     </row>
     <row r="155" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
-        <v>217</v>
+        <v>329</v>
       </c>
       <c r="B155" t="s">
-        <v>60</v>
+        <v>165</v>
       </c>
       <c r="C155" s="2" t="s">
-        <v>216</v>
+        <v>328</v>
       </c>
       <c r="E155" t="s">
-        <v>14</v>
+        <v>34</v>
       </c>
       <c r="F155">
-        <v>1900</v>
+        <v>1789</v>
       </c>
       <c r="H155" t="s">
         <v>16</v>
@@ -5003,130 +5057,118 @@
     </row>
     <row r="156" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
-        <v>132</v>
+        <v>172</v>
       </c>
       <c r="B156" t="s">
-        <v>259</v>
+        <v>60</v>
       </c>
       <c r="C156" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="Q156" t="s">
-        <v>17</v>
+        <v>171</v>
       </c>
     </row>
     <row r="157" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
-        <v>182</v>
+        <v>217</v>
       </c>
       <c r="B157" t="s">
-        <v>165</v>
+        <v>60</v>
       </c>
       <c r="C157" s="2" t="s">
-        <v>181</v>
+        <v>216</v>
+      </c>
+      <c r="E157" t="s">
+        <v>14</v>
+      </c>
+      <c r="F157">
+        <v>1900</v>
+      </c>
+      <c r="H157" t="s">
+        <v>16</v>
+      </c>
+      <c r="I157" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="158" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
-        <v>423</v>
+        <v>132</v>
       </c>
       <c r="B158" t="s">
-        <v>86</v>
+        <v>259</v>
       </c>
       <c r="C158" s="2" t="s">
-        <v>424</v>
-      </c>
-      <c r="E158" t="s">
-        <v>34</v>
-      </c>
-      <c r="F158">
-        <v>1996</v>
-      </c>
-      <c r="G158">
-        <v>2016</v>
-      </c>
-      <c r="H158" t="s">
-        <v>348</v>
-      </c>
-      <c r="I158" t="s">
-        <v>425</v>
+        <v>133</v>
+      </c>
+      <c r="Q158" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="159" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
-        <v>115</v>
+        <v>182</v>
       </c>
       <c r="B159" t="s">
-        <v>128</v>
+        <v>165</v>
       </c>
       <c r="C159" s="2" t="s">
-        <v>116</v>
+        <v>181</v>
       </c>
     </row>
     <row r="160" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
-        <v>263</v>
+        <v>423</v>
       </c>
       <c r="B160" t="s">
-        <v>250</v>
+        <v>86</v>
       </c>
       <c r="C160" s="2" t="s">
-        <v>264</v>
+        <v>424</v>
       </c>
       <c r="E160" t="s">
-        <v>265</v>
+        <v>34</v>
       </c>
       <c r="F160">
-        <v>1500</v>
+        <v>1996</v>
       </c>
       <c r="G160">
-        <v>2000</v>
+        <v>2016</v>
       </c>
       <c r="H160" t="s">
-        <v>16</v>
+        <v>348</v>
       </c>
       <c r="I160" t="s">
-        <v>20</v>
+        <v>425</v>
       </c>
     </row>
     <row r="161" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
-        <v>221</v>
+        <v>115</v>
       </c>
       <c r="B161" t="s">
-        <v>86</v>
+        <v>128</v>
       </c>
       <c r="C161" s="2" t="s">
-        <v>220</v>
-      </c>
-      <c r="F161">
-        <v>2013</v>
-      </c>
-      <c r="H161" t="s">
-        <v>16</v>
-      </c>
-      <c r="I161" t="s">
-        <v>20</v>
+        <v>116</v>
       </c>
     </row>
     <row r="162" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
-        <v>13</v>
+        <v>263</v>
       </c>
       <c r="B162" t="s">
-        <v>25</v>
+        <v>250</v>
       </c>
       <c r="C162" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="D162" s="1" t="s">
-        <v>42</v>
+        <v>264</v>
       </c>
       <c r="E162" t="s">
-        <v>14</v>
+        <v>265</v>
       </c>
       <c r="F162">
-        <v>1981</v>
+        <v>1500</v>
+      </c>
+      <c r="G162">
+        <v>2000</v>
       </c>
       <c r="H162" t="s">
         <v>16</v>
@@ -5137,166 +5179,212 @@
     </row>
     <row r="163" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
+        <v>221</v>
+      </c>
+      <c r="B163" t="s">
+        <v>86</v>
+      </c>
+      <c r="C163" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="F163">
+        <v>2013</v>
+      </c>
+      <c r="H163" t="s">
+        <v>16</v>
+      </c>
+      <c r="I163" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="164" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A164" t="s">
+        <v>13</v>
+      </c>
+      <c r="B164" t="s">
+        <v>25</v>
+      </c>
+      <c r="C164" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D164" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E164" t="s">
+        <v>14</v>
+      </c>
+      <c r="F164">
+        <v>1981</v>
+      </c>
+      <c r="H164" t="s">
+        <v>16</v>
+      </c>
+      <c r="I164" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="165" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A165" t="s">
         <v>283</v>
       </c>
-      <c r="B163" t="s">
+      <c r="B165" t="s">
         <v>124</v>
       </c>
-      <c r="C163" s="2" t="s">
+      <c r="C165" s="2" t="s">
         <v>284</v>
       </c>
-      <c r="H163" t="s">
-        <v>16</v>
-      </c>
-      <c r="I163" t="s">
+      <c r="H165" t="s">
+        <v>16</v>
+      </c>
+      <c r="I165" t="s">
         <v>20</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:Q163">
+  <sortState ref="A2:Q165">
     <sortCondition ref="A2"/>
   </sortState>
   <hyperlinks>
     <hyperlink ref="C6" r:id="rId1"/>
-    <hyperlink ref="C59" r:id="rId2"/>
+    <hyperlink ref="C60" r:id="rId2"/>
     <hyperlink ref="C7" r:id="rId3"/>
     <hyperlink ref="C10" r:id="rId4"/>
-    <hyperlink ref="C97" r:id="rId5"/>
-    <hyperlink ref="C117" r:id="rId6"/>
-    <hyperlink ref="C162" r:id="rId7"/>
+    <hyperlink ref="C98" r:id="rId5"/>
+    <hyperlink ref="C118" r:id="rId6"/>
+    <hyperlink ref="C164" r:id="rId7"/>
     <hyperlink ref="C35" r:id="rId8"/>
     <hyperlink ref="C30" r:id="rId9"/>
-    <hyperlink ref="C50" r:id="rId10"/>
-    <hyperlink ref="C57" r:id="rId11"/>
+    <hyperlink ref="C51" r:id="rId10"/>
+    <hyperlink ref="C58" r:id="rId11"/>
     <hyperlink ref="C3" r:id="rId12"/>
     <hyperlink ref="C20" r:id="rId13"/>
-    <hyperlink ref="C61" r:id="rId14"/>
-    <hyperlink ref="C89" r:id="rId15"/>
+    <hyperlink ref="C62" r:id="rId14"/>
+    <hyperlink ref="C90" r:id="rId15"/>
     <hyperlink ref="C29" r:id="rId16"/>
-    <hyperlink ref="C113" r:id="rId17"/>
-    <hyperlink ref="C41" r:id="rId18"/>
-    <hyperlink ref="C74" r:id="rId19"/>
+    <hyperlink ref="C114" r:id="rId17"/>
+    <hyperlink ref="C42" r:id="rId18"/>
+    <hyperlink ref="C75" r:id="rId19"/>
     <hyperlink ref="C16" r:id="rId20"/>
-    <hyperlink ref="C150" r:id="rId21"/>
+    <hyperlink ref="C152" r:id="rId21"/>
     <hyperlink ref="C8" r:id="rId22"/>
-    <hyperlink ref="C38" r:id="rId23"/>
-    <hyperlink ref="C54" r:id="rId24"/>
-    <hyperlink ref="C51" r:id="rId25"/>
-    <hyperlink ref="C55" r:id="rId26"/>
-    <hyperlink ref="C56" r:id="rId27"/>
-    <hyperlink ref="C71" r:id="rId28"/>
-    <hyperlink ref="C94" r:id="rId29"/>
-    <hyperlink ref="C141" r:id="rId30"/>
-    <hyperlink ref="C100" r:id="rId31"/>
-    <hyperlink ref="C84" r:id="rId32"/>
-    <hyperlink ref="C106" r:id="rId33"/>
-    <hyperlink ref="C72" r:id="rId34"/>
+    <hyperlink ref="C39" r:id="rId23"/>
+    <hyperlink ref="C55" r:id="rId24"/>
+    <hyperlink ref="C52" r:id="rId25"/>
+    <hyperlink ref="C56" r:id="rId26"/>
+    <hyperlink ref="C57" r:id="rId27"/>
+    <hyperlink ref="C72" r:id="rId28"/>
+    <hyperlink ref="C95" r:id="rId29"/>
+    <hyperlink ref="C143" r:id="rId30"/>
+    <hyperlink ref="C101" r:id="rId31"/>
+    <hyperlink ref="C85" r:id="rId32"/>
+    <hyperlink ref="C107" r:id="rId33"/>
+    <hyperlink ref="C73" r:id="rId34"/>
     <hyperlink ref="C17" r:id="rId35"/>
-    <hyperlink ref="C139" r:id="rId36"/>
+    <hyperlink ref="C141" r:id="rId36"/>
     <hyperlink ref="C15" r:id="rId37"/>
-    <hyperlink ref="C159" r:id="rId38"/>
-    <hyperlink ref="C88" r:id="rId39"/>
-    <hyperlink ref="C58" r:id="rId40"/>
-    <hyperlink ref="C122" r:id="rId41"/>
+    <hyperlink ref="C161" r:id="rId38"/>
+    <hyperlink ref="C89" r:id="rId39"/>
+    <hyperlink ref="C59" r:id="rId40"/>
+    <hyperlink ref="C124" r:id="rId41"/>
     <hyperlink ref="C18" r:id="rId42"/>
-    <hyperlink ref="C52" r:id="rId43"/>
+    <hyperlink ref="C53" r:id="rId43"/>
     <hyperlink ref="C23" r:id="rId44"/>
-    <hyperlink ref="C114" r:id="rId45"/>
-    <hyperlink ref="C156" r:id="rId46"/>
+    <hyperlink ref="C115" r:id="rId45"/>
+    <hyperlink ref="C158" r:id="rId46"/>
     <hyperlink ref="C27" r:id="rId47" display="http://comparativeconstitutionsproject.org/"/>
-    <hyperlink ref="C111" r:id="rId48"/>
-    <hyperlink ref="C152" r:id="rId49"/>
-    <hyperlink ref="C126" r:id="rId50"/>
-    <hyperlink ref="C121" r:id="rId51"/>
+    <hyperlink ref="C112" r:id="rId48"/>
+    <hyperlink ref="C154" r:id="rId49"/>
+    <hyperlink ref="C128" r:id="rId50"/>
+    <hyperlink ref="C122" r:id="rId51"/>
     <hyperlink ref="C22" r:id="rId52"/>
-    <hyperlink ref="C115" r:id="rId53"/>
-    <hyperlink ref="C48" r:id="rId54"/>
-    <hyperlink ref="C78" r:id="rId55"/>
-    <hyperlink ref="C81" r:id="rId56"/>
-    <hyperlink ref="C112" r:id="rId57"/>
-    <hyperlink ref="C102" r:id="rId58"/>
-    <hyperlink ref="C130" r:id="rId59"/>
+    <hyperlink ref="C116" r:id="rId53"/>
+    <hyperlink ref="C49" r:id="rId54"/>
+    <hyperlink ref="C79" r:id="rId55"/>
+    <hyperlink ref="C82" r:id="rId56"/>
+    <hyperlink ref="C113" r:id="rId57"/>
+    <hyperlink ref="C103" r:id="rId58"/>
+    <hyperlink ref="C132" r:id="rId59"/>
     <hyperlink ref="C31" r:id="rId60"/>
-    <hyperlink ref="C143" r:id="rId61"/>
+    <hyperlink ref="C145" r:id="rId61"/>
     <hyperlink ref="C9" r:id="rId62"/>
     <hyperlink ref="C33" r:id="rId63"/>
-    <hyperlink ref="C144" r:id="rId64"/>
+    <hyperlink ref="C146" r:id="rId64"/>
     <hyperlink ref="C14" r:id="rId65"/>
-    <hyperlink ref="C154" r:id="rId66"/>
+    <hyperlink ref="C156" r:id="rId66"/>
     <hyperlink ref="C25" r:id="rId67"/>
     <hyperlink ref="C24" r:id="rId68"/>
     <hyperlink ref="C26" r:id="rId69"/>
-    <hyperlink ref="C53" r:id="rId70"/>
-    <hyperlink ref="C157" r:id="rId71"/>
+    <hyperlink ref="C54" r:id="rId70"/>
+    <hyperlink ref="C159" r:id="rId71"/>
     <hyperlink ref="C28" r:id="rId72"/>
-    <hyperlink ref="C118" r:id="rId73"/>
+    <hyperlink ref="C119" r:id="rId73"/>
     <hyperlink ref="C32" r:id="rId74"/>
-    <hyperlink ref="C45" r:id="rId75"/>
-    <hyperlink ref="C133" r:id="rId76"/>
-    <hyperlink ref="C42" r:id="rId77"/>
-    <hyperlink ref="C39" r:id="rId78"/>
-    <hyperlink ref="C69" r:id="rId79"/>
+    <hyperlink ref="C46" r:id="rId75"/>
+    <hyperlink ref="C135" r:id="rId76"/>
+    <hyperlink ref="C43" r:id="rId77"/>
+    <hyperlink ref="C40" r:id="rId78"/>
+    <hyperlink ref="C70" r:id="rId79"/>
     <hyperlink ref="C5" r:id="rId80"/>
-    <hyperlink ref="C68" r:id="rId81"/>
+    <hyperlink ref="C69" r:id="rId81"/>
     <hyperlink ref="C12" r:id="rId82"/>
-    <hyperlink ref="C110" r:id="rId83"/>
-    <hyperlink ref="C119" r:id="rId84"/>
-    <hyperlink ref="C146" r:id="rId85"/>
+    <hyperlink ref="C111" r:id="rId83"/>
+    <hyperlink ref="C120" r:id="rId84"/>
+    <hyperlink ref="C148" r:id="rId85"/>
     <hyperlink ref="C36" r:id="rId86"/>
-    <hyperlink ref="C155" r:id="rId87"/>
-    <hyperlink ref="C44" r:id="rId88"/>
-    <hyperlink ref="C161" r:id="rId89"/>
-    <hyperlink ref="C98" r:id="rId90"/>
-    <hyperlink ref="C66" r:id="rId91"/>
-    <hyperlink ref="C99" r:id="rId92"/>
-    <hyperlink ref="C136" r:id="rId93"/>
-    <hyperlink ref="C82" r:id="rId94"/>
-    <hyperlink ref="C104" r:id="rId95"/>
-    <hyperlink ref="C137" r:id="rId96"/>
-    <hyperlink ref="C62" r:id="rId97"/>
-    <hyperlink ref="C116" r:id="rId98"/>
-    <hyperlink ref="C46" r:id="rId99"/>
-    <hyperlink ref="C43" r:id="rId100"/>
-    <hyperlink ref="C85" r:id="rId101"/>
-    <hyperlink ref="C60" r:id="rId102"/>
+    <hyperlink ref="C157" r:id="rId87"/>
+    <hyperlink ref="C45" r:id="rId88"/>
+    <hyperlink ref="C163" r:id="rId89"/>
+    <hyperlink ref="C99" r:id="rId90"/>
+    <hyperlink ref="C67" r:id="rId91"/>
+    <hyperlink ref="C100" r:id="rId92"/>
+    <hyperlink ref="C138" r:id="rId93"/>
+    <hyperlink ref="C83" r:id="rId94"/>
+    <hyperlink ref="C105" r:id="rId95"/>
+    <hyperlink ref="C139" r:id="rId96"/>
+    <hyperlink ref="C63" r:id="rId97"/>
+    <hyperlink ref="C117" r:id="rId98"/>
+    <hyperlink ref="C47" r:id="rId99"/>
+    <hyperlink ref="C44" r:id="rId100"/>
+    <hyperlink ref="C86" r:id="rId101"/>
+    <hyperlink ref="C61" r:id="rId102"/>
     <hyperlink ref="C2" r:id="rId103"/>
-    <hyperlink ref="C79" r:id="rId104"/>
-    <hyperlink ref="C83" r:id="rId105"/>
-    <hyperlink ref="C108" r:id="rId106"/>
-    <hyperlink ref="C47" r:id="rId107"/>
-    <hyperlink ref="C86" r:id="rId108"/>
-    <hyperlink ref="C135" r:id="rId109"/>
+    <hyperlink ref="C80" r:id="rId104"/>
+    <hyperlink ref="C84" r:id="rId105"/>
+    <hyperlink ref="C109" r:id="rId106"/>
+    <hyperlink ref="C48" r:id="rId107"/>
+    <hyperlink ref="C87" r:id="rId108"/>
+    <hyperlink ref="C137" r:id="rId109"/>
     <hyperlink ref="C13" r:id="rId110"/>
     <hyperlink ref="C4" r:id="rId111"/>
-    <hyperlink ref="C160" r:id="rId112"/>
-    <hyperlink ref="C92" r:id="rId113"/>
-    <hyperlink ref="C87" r:id="rId114"/>
-    <hyperlink ref="C149" r:id="rId115"/>
-    <hyperlink ref="C129" r:id="rId116"/>
-    <hyperlink ref="C64" r:id="rId117"/>
-    <hyperlink ref="C101" r:id="rId118"/>
-    <hyperlink ref="C76" r:id="rId119"/>
-    <hyperlink ref="C163" r:id="rId120"/>
-    <hyperlink ref="C67" r:id="rId121"/>
-    <hyperlink ref="C128" r:id="rId122"/>
-    <hyperlink ref="C107" r:id="rId123"/>
-    <hyperlink ref="C80" r:id="rId124"/>
-    <hyperlink ref="C105" r:id="rId125"/>
-    <hyperlink ref="C134" r:id="rId126"/>
-    <hyperlink ref="C90" r:id="rId127"/>
+    <hyperlink ref="C162" r:id="rId112"/>
+    <hyperlink ref="C93" r:id="rId113"/>
+    <hyperlink ref="C88" r:id="rId114"/>
+    <hyperlink ref="C151" r:id="rId115"/>
+    <hyperlink ref="C131" r:id="rId116"/>
+    <hyperlink ref="C65" r:id="rId117"/>
+    <hyperlink ref="C102" r:id="rId118"/>
+    <hyperlink ref="C77" r:id="rId119"/>
+    <hyperlink ref="C165" r:id="rId120"/>
+    <hyperlink ref="C68" r:id="rId121"/>
+    <hyperlink ref="C130" r:id="rId122"/>
+    <hyperlink ref="C108" r:id="rId123"/>
+    <hyperlink ref="C81" r:id="rId124"/>
+    <hyperlink ref="C106" r:id="rId125"/>
+    <hyperlink ref="C136" r:id="rId126"/>
+    <hyperlink ref="C91" r:id="rId127"/>
     <hyperlink ref="C11" r:id="rId128"/>
     <hyperlink ref="C19" r:id="rId129"/>
-    <hyperlink ref="C127" r:id="rId130"/>
-    <hyperlink ref="C75" r:id="rId131"/>
-    <hyperlink ref="C142" r:id="rId132"/>
-    <hyperlink ref="C124" r:id="rId133"/>
-    <hyperlink ref="C123" r:id="rId134"/>
-    <hyperlink ref="C125" r:id="rId135"/>
-    <hyperlink ref="C148" r:id="rId136"/>
-    <hyperlink ref="C140" r:id="rId137"/>
-    <hyperlink ref="C153" r:id="rId138"/>
-    <hyperlink ref="C37" r:id="rId139"/>
-    <hyperlink ref="C91" r:id="rId140"/>
+    <hyperlink ref="C129" r:id="rId130"/>
+    <hyperlink ref="C76" r:id="rId131"/>
+    <hyperlink ref="C144" r:id="rId132"/>
+    <hyperlink ref="C126" r:id="rId133"/>
+    <hyperlink ref="C125" r:id="rId134"/>
+    <hyperlink ref="C127" r:id="rId135"/>
+    <hyperlink ref="C150" r:id="rId136"/>
+    <hyperlink ref="C142" r:id="rId137"/>
+    <hyperlink ref="C155" r:id="rId138"/>
+    <hyperlink ref="C38" r:id="rId139"/>
+    <hyperlink ref="C92" r:id="rId140"/>
     <hyperlink ref="J2" r:id="rId141"/>
     <hyperlink ref="M3" r:id="rId142"/>
     <hyperlink ref="J3" r:id="rId143"/>
@@ -5304,62 +5392,67 @@
     <hyperlink ref="J4" r:id="rId145"/>
     <hyperlink ref="P5" r:id="rId146"/>
     <hyperlink ref="J5" r:id="rId147"/>
-    <hyperlink ref="C109" r:id="rId148"/>
+    <hyperlink ref="C110" r:id="rId148"/>
     <hyperlink ref="C34" r:id="rId149"/>
     <hyperlink ref="P7" r:id="rId150"/>
     <hyperlink ref="J7" r:id="rId151"/>
     <hyperlink ref="M8" r:id="rId152"/>
     <hyperlink ref="L8" r:id="rId153"/>
     <hyperlink ref="J8" r:id="rId154"/>
-    <hyperlink ref="C151" r:id="rId155"/>
-    <hyperlink ref="N151" r:id="rId156"/>
+    <hyperlink ref="C153" r:id="rId155"/>
+    <hyperlink ref="N153" r:id="rId156"/>
     <hyperlink ref="C21" r:id="rId157"/>
     <hyperlink ref="N21" r:id="rId158"/>
-    <hyperlink ref="C63" r:id="rId159"/>
-    <hyperlink ref="C147" r:id="rId160"/>
-    <hyperlink ref="J147" r:id="rId161"/>
-    <hyperlink ref="C145" r:id="rId162"/>
-    <hyperlink ref="N145" r:id="rId163"/>
-    <hyperlink ref="J145" r:id="rId164"/>
-    <hyperlink ref="C95" r:id="rId165"/>
-    <hyperlink ref="C93" r:id="rId166"/>
-    <hyperlink ref="C40" r:id="rId167"/>
-    <hyperlink ref="J40" r:id="rId168"/>
-    <hyperlink ref="K40" r:id="rId169"/>
-    <hyperlink ref="C103" r:id="rId170"/>
-    <hyperlink ref="N103" r:id="rId171"/>
-    <hyperlink ref="C77" r:id="rId172"/>
-    <hyperlink ref="K77" r:id="rId173"/>
-    <hyperlink ref="C158" r:id="rId174"/>
-    <hyperlink ref="C120" r:id="rId175"/>
-    <hyperlink ref="K120" r:id="rId176"/>
+    <hyperlink ref="C64" r:id="rId159"/>
+    <hyperlink ref="C149" r:id="rId160"/>
+    <hyperlink ref="J149" r:id="rId161"/>
+    <hyperlink ref="C147" r:id="rId162"/>
+    <hyperlink ref="N147" r:id="rId163"/>
+    <hyperlink ref="J147" r:id="rId164"/>
+    <hyperlink ref="C96" r:id="rId165"/>
+    <hyperlink ref="C94" r:id="rId166"/>
+    <hyperlink ref="C41" r:id="rId167"/>
+    <hyperlink ref="J41" r:id="rId168"/>
+    <hyperlink ref="K41" r:id="rId169"/>
+    <hyperlink ref="C104" r:id="rId170"/>
+    <hyperlink ref="N104" r:id="rId171"/>
+    <hyperlink ref="C78" r:id="rId172"/>
+    <hyperlink ref="K78" r:id="rId173"/>
+    <hyperlink ref="C160" r:id="rId174"/>
+    <hyperlink ref="C121" r:id="rId175"/>
+    <hyperlink ref="K121" r:id="rId176"/>
     <hyperlink ref="L9" r:id="rId177"/>
     <hyperlink ref="J9" r:id="rId178"/>
     <hyperlink ref="J10" r:id="rId179"/>
-    <hyperlink ref="C131" r:id="rId180"/>
-    <hyperlink ref="J131" r:id="rId181"/>
-    <hyperlink ref="L131" r:id="rId182"/>
-    <hyperlink ref="K131" r:id="rId183"/>
-    <hyperlink ref="C132" r:id="rId184"/>
-    <hyperlink ref="J132" r:id="rId185"/>
-    <hyperlink ref="K132" r:id="rId186"/>
-    <hyperlink ref="L132" r:id="rId187"/>
-    <hyperlink ref="C65" r:id="rId188"/>
-    <hyperlink ref="J65" r:id="rId189"/>
-    <hyperlink ref="N65" r:id="rId190"/>
-    <hyperlink ref="C138" r:id="rId191"/>
-    <hyperlink ref="C96" r:id="rId192"/>
-    <hyperlink ref="J96" r:id="rId193"/>
-    <hyperlink ref="L96" r:id="rId194"/>
-    <hyperlink ref="C73" r:id="rId195"/>
-    <hyperlink ref="C49" r:id="rId196"/>
-    <hyperlink ref="L49" r:id="rId197"/>
-    <hyperlink ref="K49" r:id="rId198"/>
-    <hyperlink ref="J49" r:id="rId199"/>
-    <hyperlink ref="C70" r:id="rId200"/>
-    <hyperlink ref="J70" r:id="rId201"/>
-    <hyperlink ref="K70" r:id="rId202"/>
-    <hyperlink ref="L70" r:id="rId203"/>
+    <hyperlink ref="C133" r:id="rId180"/>
+    <hyperlink ref="J133" r:id="rId181"/>
+    <hyperlink ref="L133" r:id="rId182"/>
+    <hyperlink ref="K133" r:id="rId183"/>
+    <hyperlink ref="C134" r:id="rId184"/>
+    <hyperlink ref="J134" r:id="rId185"/>
+    <hyperlink ref="K134" r:id="rId186"/>
+    <hyperlink ref="L134" r:id="rId187"/>
+    <hyperlink ref="C66" r:id="rId188"/>
+    <hyperlink ref="J66" r:id="rId189"/>
+    <hyperlink ref="N66" r:id="rId190"/>
+    <hyperlink ref="C140" r:id="rId191"/>
+    <hyperlink ref="C97" r:id="rId192"/>
+    <hyperlink ref="J97" r:id="rId193"/>
+    <hyperlink ref="L97" r:id="rId194"/>
+    <hyperlink ref="C74" r:id="rId195"/>
+    <hyperlink ref="C50" r:id="rId196"/>
+    <hyperlink ref="L50" r:id="rId197"/>
+    <hyperlink ref="K50" r:id="rId198"/>
+    <hyperlink ref="J50" r:id="rId199"/>
+    <hyperlink ref="C71" r:id="rId200"/>
+    <hyperlink ref="J71" r:id="rId201"/>
+    <hyperlink ref="K71" r:id="rId202"/>
+    <hyperlink ref="L71" r:id="rId203"/>
+    <hyperlink ref="C123" r:id="rId204"/>
+    <hyperlink ref="N123" r:id="rId205"/>
+    <hyperlink ref="C37" r:id="rId206"/>
+    <hyperlink ref="K37" r:id="rId207"/>
+    <hyperlink ref="J37" r:id="rId208"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
add Armed Conflict Location & Event Data
</commit_message>
<xml_diff>
--- a/PolData.xlsx
+++ b/PolData.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="877" uniqueCount="481">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="888" uniqueCount="488">
   <si>
     <t>name</t>
   </si>
@@ -1470,6 +1470,27 @@
   </si>
   <si>
     <t>https://www.ctdatacollaborative.org/sites/default/files/CTDC%20codebook%20v6_0.pdf</t>
+  </si>
+  <si>
+    <t>Armed Conflict Location &amp; Event Data Project</t>
+  </si>
+  <si>
+    <t>https://www.acleddata.com/data/acled-version-7-1997-2016/</t>
+  </si>
+  <si>
+    <t>Conflict, protest</t>
+  </si>
+  <si>
+    <t>https://www.acleddata.com/wp-content/uploads/2017/01/ACLED_Codebook_2017.pdf</t>
+  </si>
+  <si>
+    <t>https://www.acleddata.com/wp-content/uploads/2017/01/ACLED-Version-7-All-Africa-1997-2016_dyadic-file.xlsx</t>
+  </si>
+  <si>
+    <t>https://www.acleddata.com/wp-content/uploads/2017/01/ACLED-Version-7-All-Africa-1997-2016_csv_dyadic-file.zip</t>
+  </si>
+  <si>
+    <t>csv in zip file</t>
   </si>
 </sst>
 </file>
@@ -1809,10 +1830,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q165"/>
+  <dimension ref="A1:Q166"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" topLeftCell="A143" workbookViewId="0">
+      <selection activeCell="A166" sqref="A166"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2182,91 +2203,116 @@
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>31</v>
+        <v>481</v>
       </c>
       <c r="B10" t="s">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>46</v>
+        <v>482</v>
       </c>
       <c r="D10" t="s">
-        <v>437</v>
+        <v>483</v>
       </c>
       <c r="E10" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="F10">
-        <v>2001</v>
+        <v>1997</v>
+      </c>
+      <c r="G10">
+        <v>2016</v>
       </c>
       <c r="H10" t="s">
-        <v>436</v>
+        <v>348</v>
       </c>
       <c r="I10" t="s">
-        <v>435</v>
+        <v>349</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>433</v>
+        <v>484</v>
+      </c>
+      <c r="K10" s="2"/>
+      <c r="N10" s="2" t="s">
+        <v>485</v>
+      </c>
+      <c r="P10" s="2" t="s">
+        <v>486</v>
       </c>
       <c r="Q10" t="s">
-        <v>434</v>
+        <v>487</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>304</v>
+        <v>31</v>
       </c>
       <c r="B11" t="s">
         <v>25</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>302</v>
+        <v>46</v>
+      </c>
+      <c r="D11" t="s">
+        <v>437</v>
       </c>
       <c r="E11" t="s">
-        <v>303</v>
+        <v>73</v>
       </c>
       <c r="F11">
-        <v>2002</v>
+        <v>2001</v>
       </c>
       <c r="H11" t="s">
-        <v>16</v>
+        <v>436</v>
       </c>
       <c r="I11" t="s">
-        <v>301</v>
+        <v>435</v>
+      </c>
+      <c r="J11" s="2" t="s">
+        <v>433</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>434</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>207</v>
+        <v>304</v>
       </c>
       <c r="B12" t="s">
-        <v>60</v>
+        <v>25</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>206</v>
+        <v>302</v>
+      </c>
+      <c r="E12" t="s">
+        <v>303</v>
       </c>
       <c r="F12">
-        <v>1972</v>
-      </c>
-      <c r="G12">
-        <v>2014</v>
+        <v>2002</v>
       </c>
       <c r="H12" t="s">
         <v>16</v>
       </c>
       <c r="I12" t="s">
-        <v>20</v>
+        <v>301</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>260</v>
+        <v>207</v>
       </c>
       <c r="B13" t="s">
-        <v>259</v>
+        <v>60</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>261</v>
+        <v>206</v>
+      </c>
+      <c r="F13">
+        <v>1972</v>
+      </c>
+      <c r="G13">
+        <v>2014</v>
       </c>
       <c r="H13" t="s">
         <v>16</v>
@@ -2277,363 +2323,360 @@
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>170</v>
+        <v>260</v>
       </c>
       <c r="B14" t="s">
-        <v>60</v>
+        <v>259</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>169</v>
+        <v>261</v>
+      </c>
+      <c r="H14" t="s">
+        <v>16</v>
+      </c>
+      <c r="I14" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>113</v>
+        <v>170</v>
       </c>
       <c r="B15" t="s">
-        <v>25</v>
+        <v>60</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="E15" t="s">
-        <v>112</v>
-      </c>
-      <c r="F15">
-        <v>1964</v>
+        <v>169</v>
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>64</v>
+        <v>113</v>
       </c>
       <c r="B16" t="s">
         <v>25</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>65</v>
+        <v>114</v>
+      </c>
+      <c r="E16" t="s">
+        <v>112</v>
       </c>
       <c r="F16">
-        <v>1991</v>
-      </c>
-      <c r="G16">
-        <v>2009</v>
-      </c>
-      <c r="Q16" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
+        <v>1964</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>107</v>
+        <v>64</v>
       </c>
       <c r="B17" t="s">
         <v>25</v>
       </c>
       <c r="C17" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="F17">
+        <v>1991</v>
+      </c>
+      <c r="G17">
+        <v>2009</v>
+      </c>
+      <c r="Q17" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>107</v>
+      </c>
+      <c r="B18" t="s">
+        <v>25</v>
+      </c>
+      <c r="C18" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="E17" t="s">
+      <c r="E18" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
         <v>123</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B19" t="s">
         <v>259</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="C19" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="I18" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
+      <c r="I19" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
         <v>306</v>
-      </c>
-      <c r="B19" t="s">
-        <v>25</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>305</v>
-      </c>
-      <c r="E19" t="s">
-        <v>307</v>
-      </c>
-      <c r="F19">
-        <v>2004</v>
-      </c>
-      <c r="H19" t="s">
-        <v>16</v>
-      </c>
-      <c r="I19" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>32</v>
       </c>
       <c r="B20" t="s">
         <v>25</v>
       </c>
       <c r="C20" s="2" t="s">
+        <v>305</v>
+      </c>
+      <c r="E20" t="s">
+        <v>307</v>
+      </c>
+      <c r="F20">
+        <v>2004</v>
+      </c>
+      <c r="H20" t="s">
+        <v>16</v>
+      </c>
+      <c r="I20" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>32</v>
+      </c>
+      <c r="B21" t="s">
+        <v>25</v>
+      </c>
+      <c r="C21" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="E20" t="s">
+      <c r="E21" t="s">
         <v>74</v>
       </c>
-      <c r="F20">
+      <c r="F21">
         <v>2008</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
         <v>387</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B22" t="s">
         <v>124</v>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="C22" s="2" t="s">
         <v>388</v>
       </c>
-      <c r="E21" t="s">
+      <c r="E22" t="s">
         <v>14</v>
       </c>
-      <c r="F21">
+      <c r="F22">
         <v>1970</v>
       </c>
-      <c r="H21" t="s">
+      <c r="H22" t="s">
         <v>348</v>
       </c>
-      <c r="I21" t="s">
+      <c r="I22" t="s">
         <v>349</v>
       </c>
-      <c r="N21" s="2" t="s">
+      <c r="N22" s="2" t="s">
         <v>389</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
         <v>146</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B23" t="s">
         <v>128</v>
       </c>
-      <c r="C22" s="2" t="s">
+      <c r="C23" s="2" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
         <v>127</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B24" t="s">
         <v>259</v>
       </c>
-      <c r="C23" s="2" t="s">
+      <c r="C24" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="I23" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
+      <c r="I24" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
         <v>173</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B25" t="s">
         <v>128</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
-        <v>174</v>
-      </c>
-      <c r="B25" t="s">
-        <v>86</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="E25" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="B26" t="s">
-        <v>25</v>
+        <v>86</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>175</v>
       </c>
       <c r="E26" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>177</v>
+      </c>
+      <c r="B27" t="s">
+        <v>25</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="E27" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
         <v>135</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B28" t="s">
         <v>134</v>
       </c>
-      <c r="C27" s="2" t="s">
+      <c r="C28" s="2" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
         <v>184</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B29" t="s">
         <v>128</v>
       </c>
-      <c r="C28" s="2" t="s">
+      <c r="C29" s="2" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
         <v>54</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B30" t="s">
         <v>55</v>
       </c>
-      <c r="C29" s="2" t="s">
+      <c r="C30" s="2" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A30" s="1" t="s">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A31" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B31" t="s">
         <v>25</v>
       </c>
-      <c r="C30" s="2" t="s">
+      <c r="C31" s="2" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
         <v>158</v>
-      </c>
-      <c r="B31" t="s">
-        <v>99</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
-        <v>187</v>
       </c>
       <c r="B32" t="s">
         <v>99</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>188</v>
-      </c>
-      <c r="F32">
-        <v>1960</v>
-      </c>
-      <c r="G32">
-        <v>2011</v>
-      </c>
-      <c r="H32" t="s">
-        <v>16</v>
-      </c>
-      <c r="I32" t="s">
-        <v>189</v>
+        <v>159</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>164</v>
+        <v>187</v>
       </c>
       <c r="B33" t="s">
-        <v>165</v>
+        <v>99</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>166</v>
+        <v>188</v>
+      </c>
+      <c r="F33">
+        <v>1960</v>
+      </c>
+      <c r="G33">
+        <v>2011</v>
+      </c>
+      <c r="H33" t="s">
+        <v>16</v>
+      </c>
+      <c r="I33" t="s">
+        <v>189</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>371</v>
+        <v>164</v>
       </c>
       <c r="B34" t="s">
-        <v>25</v>
+        <v>165</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>372</v>
-      </c>
-      <c r="D34" t="s">
-        <v>363</v>
-      </c>
-      <c r="E34" t="s">
-        <v>34</v>
-      </c>
-      <c r="F34">
-        <v>2006</v>
-      </c>
-      <c r="H34" t="s">
-        <v>348</v>
-      </c>
-      <c r="I34" t="s">
-        <v>349</v>
+        <v>166</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>39</v>
+        <v>371</v>
       </c>
       <c r="B35" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>41</v>
+        <v>372</v>
+      </c>
+      <c r="D35" t="s">
+        <v>363</v>
       </c>
       <c r="E35" t="s">
-        <v>14</v>
+        <v>34</v>
       </c>
       <c r="F35">
-        <v>1816</v>
-      </c>
-      <c r="G35">
-        <v>2007</v>
+        <v>2006</v>
       </c>
       <c r="H35" t="s">
-        <v>16</v>
+        <v>348</v>
       </c>
       <c r="I35" t="s">
-        <v>20</v>
+        <v>349</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>215</v>
+        <v>39</v>
       </c>
       <c r="B36" t="s">
-        <v>237</v>
+        <v>40</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>214</v>
+        <v>41</v>
+      </c>
+      <c r="E36" t="s">
+        <v>14</v>
       </c>
       <c r="F36">
-        <v>1995</v>
+        <v>1816</v>
+      </c>
+      <c r="G36">
+        <v>2007</v>
       </c>
       <c r="H36" t="s">
         <v>16</v>
@@ -2644,188 +2687,185 @@
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>476</v>
+        <v>215</v>
       </c>
       <c r="B37" t="s">
-        <v>40</v>
+        <v>237</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>477</v>
-      </c>
-      <c r="D37" t="s">
-        <v>478</v>
-      </c>
-      <c r="E37" t="s">
-        <v>14</v>
+        <v>214</v>
       </c>
       <c r="F37">
-        <v>2002</v>
+        <v>1995</v>
       </c>
       <c r="H37" t="s">
-        <v>348</v>
+        <v>16</v>
       </c>
       <c r="I37" t="s">
-        <v>349</v>
-      </c>
-      <c r="J37" s="2" t="s">
-        <v>480</v>
-      </c>
-      <c r="K37" s="2" t="s">
-        <v>479</v>
+        <v>20</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>330</v>
+        <v>476</v>
       </c>
       <c r="B38" t="s">
-        <v>165</v>
+        <v>40</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>331</v>
+        <v>477</v>
+      </c>
+      <c r="D38" t="s">
+        <v>478</v>
       </c>
       <c r="E38" t="s">
-        <v>77</v>
+        <v>14</v>
       </c>
       <c r="F38">
-        <v>1953</v>
+        <v>2002</v>
       </c>
       <c r="H38" t="s">
-        <v>16</v>
+        <v>348</v>
       </c>
       <c r="I38" t="s">
-        <v>20</v>
+        <v>349</v>
+      </c>
+      <c r="J38" s="2" t="s">
+        <v>480</v>
+      </c>
+      <c r="K38" s="2" t="s">
+        <v>479</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>75</v>
+        <v>330</v>
       </c>
       <c r="B39" t="s">
-        <v>25</v>
+        <v>165</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>76</v>
+        <v>331</v>
       </c>
       <c r="E39" t="s">
         <v>77</v>
       </c>
       <c r="F39">
-        <v>1971</v>
+        <v>1953</v>
+      </c>
+      <c r="H39" t="s">
+        <v>16</v>
+      </c>
+      <c r="I39" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>197</v>
+        <v>75</v>
       </c>
       <c r="B40" t="s">
-        <v>55</v>
+        <v>25</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>198</v>
+        <v>76</v>
       </c>
       <c r="E40" t="s">
-        <v>199</v>
+        <v>77</v>
       </c>
       <c r="F40">
-        <v>1975</v>
-      </c>
-      <c r="G40">
-        <v>2015</v>
-      </c>
-      <c r="H40" t="s">
-        <v>16</v>
-      </c>
-      <c r="I40" t="s">
-        <v>20</v>
+        <v>1971</v>
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>409</v>
+        <v>197</v>
       </c>
       <c r="B41" t="s">
-        <v>250</v>
+        <v>55</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>410</v>
+        <v>198</v>
       </c>
       <c r="E41" t="s">
-        <v>9</v>
+        <v>199</v>
+      </c>
+      <c r="F41">
+        <v>1975</v>
+      </c>
+      <c r="G41">
+        <v>2015</v>
       </c>
       <c r="H41" t="s">
-        <v>348</v>
+        <v>16</v>
       </c>
       <c r="I41" t="s">
-        <v>349</v>
-      </c>
-      <c r="J41" s="2" t="s">
-        <v>411</v>
-      </c>
-      <c r="K41" s="2" t="s">
-        <v>412</v>
+        <v>20</v>
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>59</v>
+        <v>409</v>
       </c>
       <c r="B42" t="s">
-        <v>60</v>
+        <v>250</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>61</v>
+        <v>410</v>
+      </c>
+      <c r="E42" t="s">
+        <v>9</v>
+      </c>
+      <c r="H42" t="s">
+        <v>348</v>
+      </c>
+      <c r="I42" t="s">
+        <v>349</v>
+      </c>
+      <c r="J42" s="2" t="s">
+        <v>411</v>
+      </c>
+      <c r="K42" s="2" t="s">
+        <v>412</v>
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>196</v>
+        <v>59</v>
       </c>
       <c r="B43" t="s">
-        <v>165</v>
+        <v>60</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>195</v>
-      </c>
-      <c r="F43">
-        <v>1946</v>
-      </c>
-      <c r="G43">
-        <v>2016</v>
+        <v>61</v>
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>238</v>
+        <v>196</v>
       </c>
       <c r="B44" t="s">
-        <v>237</v>
+        <v>165</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>243</v>
-      </c>
-      <c r="H44" t="s">
-        <v>16</v>
-      </c>
-      <c r="I44" t="s">
-        <v>20</v>
+        <v>195</v>
+      </c>
+      <c r="F44">
+        <v>1946</v>
+      </c>
+      <c r="G44">
+        <v>2016</v>
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>219</v>
+        <v>238</v>
       </c>
       <c r="B45" t="s">
-        <v>124</v>
+        <v>237</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>218</v>
-      </c>
-      <c r="F45">
-        <v>1970</v>
-      </c>
-      <c r="G45">
-        <v>2015</v>
+        <v>243</v>
       </c>
       <c r="H45" t="s">
         <v>16</v>
@@ -2836,44 +2876,50 @@
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>191</v>
+        <v>219</v>
       </c>
       <c r="B46" t="s">
-        <v>25</v>
+        <v>124</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="E46" t="s">
-        <v>192</v>
+        <v>218</v>
+      </c>
+      <c r="F46">
+        <v>1970</v>
+      </c>
+      <c r="G46">
+        <v>2015</v>
+      </c>
+      <c r="H46" t="s">
+        <v>16</v>
+      </c>
+      <c r="I46" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>235</v>
+        <v>191</v>
       </c>
       <c r="B47" t="s">
-        <v>60</v>
+        <v>25</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>236</v>
-      </c>
-      <c r="H47" t="s">
-        <v>16</v>
-      </c>
-      <c r="I47" t="s">
-        <v>20</v>
+        <v>190</v>
+      </c>
+      <c r="E47" t="s">
+        <v>192</v>
       </c>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>252</v>
+        <v>235</v>
       </c>
       <c r="B48" t="s">
-        <v>250</v>
+        <v>60</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>251</v>
+        <v>236</v>
       </c>
       <c r="H48" t="s">
         <v>16</v>
@@ -2884,129 +2930,129 @@
     </row>
     <row r="49" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>149</v>
+        <v>252</v>
       </c>
       <c r="B49" t="s">
-        <v>128</v>
+        <v>250</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>150</v>
+        <v>251</v>
+      </c>
+      <c r="H49" t="s">
+        <v>16</v>
+      </c>
+      <c r="I49" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="50" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>462</v>
+        <v>149</v>
       </c>
       <c r="B50" t="s">
-        <v>250</v>
+        <v>128</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>464</v>
-      </c>
-      <c r="D50" t="s">
-        <v>463</v>
-      </c>
-      <c r="E50" t="s">
-        <v>14</v>
-      </c>
-      <c r="F50">
-        <v>1946</v>
-      </c>
-      <c r="G50">
-        <v>2010</v>
-      </c>
-      <c r="H50" t="s">
-        <v>348</v>
-      </c>
-      <c r="I50" t="s">
-        <v>349</v>
-      </c>
-      <c r="J50" s="2" t="s">
-        <v>467</v>
-      </c>
-      <c r="K50" s="2" t="s">
-        <v>466</v>
-      </c>
-      <c r="L50" s="2" t="s">
-        <v>465</v>
+        <v>150</v>
       </c>
     </row>
     <row r="51" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>28</v>
+        <v>462</v>
       </c>
       <c r="B51" t="s">
-        <v>25</v>
+        <v>250</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>48</v>
+        <v>464</v>
+      </c>
+      <c r="D51" t="s">
+        <v>463</v>
+      </c>
+      <c r="E51" t="s">
+        <v>14</v>
+      </c>
+      <c r="F51">
+        <v>1946</v>
+      </c>
+      <c r="G51">
+        <v>2010</v>
+      </c>
+      <c r="H51" t="s">
+        <v>348</v>
+      </c>
+      <c r="I51" t="s">
+        <v>349</v>
+      </c>
+      <c r="J51" s="2" t="s">
+        <v>467</v>
+      </c>
+      <c r="K51" s="2" t="s">
+        <v>466</v>
+      </c>
+      <c r="L51" s="2" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="52" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>80</v>
+        <v>28</v>
       </c>
       <c r="B52" t="s">
-        <v>128</v>
+        <v>25</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="E52" t="s">
-        <v>9</v>
-      </c>
-      <c r="F52">
-        <v>1979</v>
+        <v>48</v>
       </c>
     </row>
     <row r="53" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>125</v>
+        <v>80</v>
       </c>
       <c r="B53" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>126</v>
+        <v>81</v>
+      </c>
+      <c r="E53" t="s">
+        <v>9</v>
+      </c>
+      <c r="F53">
+        <v>1979</v>
       </c>
     </row>
     <row r="54" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>179</v>
+        <v>125</v>
       </c>
       <c r="B54" t="s">
-        <v>165</v>
+        <v>124</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>180</v>
+        <v>126</v>
       </c>
     </row>
     <row r="55" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
+        <v>179</v>
+      </c>
+      <c r="B55" t="s">
+        <v>165</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="56" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
         <v>78</v>
       </c>
-      <c r="B55" t="s">
+      <c r="B56" t="s">
         <v>25</v>
       </c>
-      <c r="C55" s="2" t="s">
+      <c r="C56" s="2" t="s">
         <v>79</v>
-      </c>
-      <c r="E55" t="s">
-        <v>9</v>
-      </c>
-      <c r="F55">
-        <v>1979</v>
-      </c>
-    </row>
-    <row r="56" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A56" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="B56" t="s">
-        <v>83</v>
-      </c>
-      <c r="C56" s="2" t="s">
-        <v>84</v>
       </c>
       <c r="E56" t="s">
         <v>9</v>
@@ -3017,13 +3063,13 @@
     </row>
     <row r="57" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A57" s="3" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B57" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="E57" t="s">
         <v>9</v>
@@ -3031,225 +3077,225 @@
       <c r="F57">
         <v>1979</v>
       </c>
-      <c r="G57">
+    </row>
+    <row r="58" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A58" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="B58" t="s">
+        <v>86</v>
+      </c>
+      <c r="C58" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="E58" t="s">
+        <v>9</v>
+      </c>
+      <c r="F58">
+        <v>1979</v>
+      </c>
+      <c r="G58">
         <v>2009</v>
-      </c>
-    </row>
-    <row r="58" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A58" t="s">
-        <v>27</v>
-      </c>
-      <c r="B58" t="s">
-        <v>25</v>
-      </c>
-      <c r="C58" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="Q58" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="59" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>120</v>
+        <v>27</v>
       </c>
       <c r="B59" t="s">
-        <v>259</v>
+        <v>25</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="I59" t="s">
-        <v>20</v>
+        <v>49</v>
+      </c>
+      <c r="Q59" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="60" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>5</v>
+        <v>120</v>
       </c>
       <c r="B60" t="s">
-        <v>25</v>
+        <v>259</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D60" t="s">
-        <v>94</v>
-      </c>
-      <c r="E60" t="s">
-        <v>9</v>
-      </c>
-      <c r="F60">
-        <v>2002</v>
-      </c>
-      <c r="H60" t="s">
-        <v>16</v>
+        <v>119</v>
       </c>
       <c r="I60" t="s">
-        <v>248</v>
-      </c>
-      <c r="Q60" t="s">
-        <v>44</v>
+        <v>20</v>
       </c>
     </row>
     <row r="61" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
+        <v>5</v>
+      </c>
+      <c r="B61" t="s">
+        <v>25</v>
+      </c>
+      <c r="C61" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D61" t="s">
+        <v>94</v>
+      </c>
+      <c r="E61" t="s">
+        <v>9</v>
+      </c>
+      <c r="F61">
+        <v>2002</v>
+      </c>
+      <c r="H61" t="s">
+        <v>16</v>
+      </c>
+      <c r="I61" t="s">
+        <v>248</v>
+      </c>
+      <c r="Q61" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="62" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
         <v>240</v>
       </c>
-      <c r="B61" t="s">
+      <c r="B62" t="s">
         <v>237</v>
       </c>
-      <c r="C61" s="2" t="s">
+      <c r="C62" s="2" t="s">
         <v>243</v>
       </c>
-      <c r="H61" t="s">
-        <v>16</v>
-      </c>
-      <c r="I61" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="62" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A62" s="1" t="s">
+      <c r="H62" t="s">
+        <v>16</v>
+      </c>
+      <c r="I62" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="63" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A63" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B62" t="s">
+      <c r="B63" t="s">
         <v>25</v>
       </c>
-      <c r="C62" s="2" t="s">
+      <c r="C63" s="2" t="s">
         <v>52</v>
-      </c>
-    </row>
-    <row r="63" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A63" t="s">
-        <v>232</v>
-      </c>
-      <c r="B63" t="s">
-        <v>250</v>
-      </c>
-      <c r="C63" s="2" t="s">
-        <v>231</v>
       </c>
     </row>
     <row r="64" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>390</v>
+        <v>232</v>
       </c>
       <c r="B64" t="s">
-        <v>83</v>
+        <v>250</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>392</v>
-      </c>
-      <c r="D64" t="s">
-        <v>391</v>
-      </c>
-      <c r="E64" t="s">
-        <v>9</v>
-      </c>
-      <c r="F64">
-        <v>2007</v>
-      </c>
-      <c r="G64">
-        <v>2015</v>
-      </c>
-      <c r="H64" t="s">
-        <v>348</v>
-      </c>
-      <c r="I64" t="s">
-        <v>349</v>
-      </c>
-      <c r="Q64" t="s">
-        <v>393</v>
+        <v>231</v>
       </c>
     </row>
     <row r="65" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>276</v>
+        <v>390</v>
       </c>
       <c r="B65" t="s">
-        <v>124</v>
+        <v>83</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>277</v>
+        <v>392</v>
+      </c>
+      <c r="D65" t="s">
+        <v>391</v>
+      </c>
+      <c r="E65" t="s">
+        <v>9</v>
       </c>
       <c r="F65">
-        <v>1948</v>
+        <v>2007</v>
       </c>
       <c r="G65">
-        <v>2000</v>
+        <v>2015</v>
       </c>
       <c r="H65" t="s">
-        <v>16</v>
+        <v>348</v>
       </c>
       <c r="I65" t="s">
-        <v>20</v>
+        <v>349</v>
+      </c>
+      <c r="Q65" t="s">
+        <v>393</v>
       </c>
     </row>
     <row r="66" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>449</v>
+        <v>276</v>
       </c>
       <c r="B66" t="s">
-        <v>250</v>
+        <v>124</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>448</v>
-      </c>
-      <c r="E66" t="s">
-        <v>14</v>
+        <v>277</v>
       </c>
       <c r="F66">
-        <v>-4000</v>
+        <v>1948</v>
       </c>
       <c r="G66">
         <v>2000</v>
       </c>
       <c r="H66" t="s">
-        <v>348</v>
+        <v>16</v>
       </c>
       <c r="I66" t="s">
-        <v>349</v>
-      </c>
-      <c r="J66" s="2" t="s">
-        <v>450</v>
-      </c>
-      <c r="N66" s="2" t="s">
-        <v>451</v>
+        <v>20</v>
       </c>
     </row>
     <row r="67" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>224</v>
+        <v>449</v>
       </c>
       <c r="B67" t="s">
-        <v>40</v>
+        <v>250</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>225</v>
+        <v>448</v>
+      </c>
+      <c r="E67" t="s">
+        <v>14</v>
       </c>
       <c r="F67">
-        <v>1964</v>
+        <v>-4000</v>
       </c>
       <c r="G67">
-        <v>2008</v>
+        <v>2000</v>
       </c>
       <c r="H67" t="s">
-        <v>16</v>
+        <v>348</v>
       </c>
       <c r="I67" t="s">
-        <v>20</v>
+        <v>349</v>
+      </c>
+      <c r="J67" s="2" t="s">
+        <v>450</v>
+      </c>
+      <c r="N67" s="2" t="s">
+        <v>451</v>
       </c>
     </row>
     <row r="68" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>285</v>
+        <v>224</v>
       </c>
       <c r="B68" t="s">
-        <v>250</v>
+        <v>40</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>286</v>
+        <v>225</v>
+      </c>
+      <c r="F68">
+        <v>1964</v>
+      </c>
+      <c r="G68">
+        <v>2008</v>
       </c>
       <c r="H68" t="s">
         <v>16</v>
@@ -3260,259 +3306,259 @@
     </row>
     <row r="69" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>205</v>
+        <v>285</v>
       </c>
       <c r="B69" t="s">
-        <v>40</v>
+        <v>250</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>204</v>
-      </c>
-      <c r="F69">
-        <v>2006</v>
+        <v>286</v>
+      </c>
+      <c r="H69" t="s">
+        <v>16</v>
+      </c>
+      <c r="I69" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="70" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>200</v>
+        <v>205</v>
       </c>
       <c r="B70" t="s">
-        <v>99</v>
+        <v>40</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="F70">
-        <v>1980</v>
-      </c>
-      <c r="G70">
-        <v>2007</v>
-      </c>
-      <c r="Q70" t="s">
-        <v>18</v>
+        <v>2006</v>
       </c>
     </row>
     <row r="71" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>468</v>
+        <v>200</v>
       </c>
       <c r="B71" t="s">
-        <v>40</v>
+        <v>99</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>464</v>
-      </c>
-      <c r="E71" t="s">
-        <v>14</v>
+        <v>201</v>
       </c>
       <c r="F71">
-        <v>1816</v>
+        <v>1980</v>
       </c>
       <c r="G71">
-        <v>2001</v>
-      </c>
-      <c r="H71" t="s">
-        <v>348</v>
-      </c>
-      <c r="I71" t="s">
-        <v>349</v>
-      </c>
-      <c r="J71" s="2" t="s">
-        <v>469</v>
-      </c>
-      <c r="K71" s="2" t="s">
-        <v>470</v>
-      </c>
-      <c r="L71" s="2" t="s">
-        <v>471</v>
+        <v>2007</v>
+      </c>
+      <c r="Q71" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="72" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>89</v>
+        <v>468</v>
       </c>
       <c r="B72" t="s">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>88</v>
+        <v>464</v>
       </c>
       <c r="E72" t="s">
-        <v>34</v>
+        <v>14</v>
       </c>
       <c r="F72">
-        <v>1972</v>
+        <v>1816</v>
+      </c>
+      <c r="G72">
+        <v>2001</v>
       </c>
       <c r="H72" t="s">
-        <v>16</v>
+        <v>348</v>
       </c>
       <c r="I72" t="s">
-        <v>20</v>
+        <v>349</v>
+      </c>
+      <c r="J72" s="2" t="s">
+        <v>469</v>
+      </c>
+      <c r="K72" s="2" t="s">
+        <v>470</v>
+      </c>
+      <c r="L72" s="2" t="s">
+        <v>471</v>
       </c>
     </row>
     <row r="73" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>104</v>
+        <v>89</v>
       </c>
       <c r="B73" t="s">
         <v>25</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>106</v>
+        <v>88</v>
       </c>
       <c r="E73" t="s">
-        <v>105</v>
+        <v>34</v>
       </c>
       <c r="F73">
-        <v>1980</v>
+        <v>1972</v>
+      </c>
+      <c r="H73" t="s">
+        <v>16</v>
+      </c>
+      <c r="I73" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="74" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>460</v>
+        <v>104</v>
       </c>
       <c r="B74" t="s">
         <v>25</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>461</v>
-      </c>
-      <c r="D74" t="s">
-        <v>363</v>
+        <v>106</v>
       </c>
       <c r="E74" t="s">
         <v>105</v>
       </c>
       <c r="F74">
-        <v>2009</v>
-      </c>
-      <c r="H74" t="s">
-        <v>348</v>
-      </c>
-      <c r="I74" t="s">
-        <v>301</v>
+        <v>1980</v>
       </c>
     </row>
     <row r="75" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>62</v>
+        <v>460</v>
       </c>
       <c r="B75" t="s">
         <v>25</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>63</v>
+        <v>461</v>
+      </c>
+      <c r="D75" t="s">
+        <v>363</v>
+      </c>
+      <c r="E75" t="s">
+        <v>105</v>
+      </c>
+      <c r="F75">
+        <v>2009</v>
+      </c>
+      <c r="H75" t="s">
+        <v>348</v>
+      </c>
+      <c r="I75" t="s">
+        <v>301</v>
       </c>
     </row>
     <row r="76" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>311</v>
+        <v>62</v>
       </c>
       <c r="B76" t="s">
-        <v>165</v>
+        <v>25</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>312</v>
-      </c>
-      <c r="E76" t="s">
-        <v>14</v>
-      </c>
-      <c r="H76" t="s">
-        <v>16</v>
-      </c>
-      <c r="I76" t="s">
-        <v>301</v>
+        <v>63</v>
       </c>
     </row>
     <row r="77" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>281</v>
+        <v>311</v>
       </c>
       <c r="B77" t="s">
-        <v>237</v>
+        <v>165</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>282</v>
+        <v>312</v>
+      </c>
+      <c r="E77" t="s">
+        <v>14</v>
       </c>
       <c r="H77" t="s">
         <v>16</v>
       </c>
       <c r="I77" t="s">
-        <v>20</v>
+        <v>301</v>
       </c>
     </row>
     <row r="78" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>418</v>
+        <v>281</v>
       </c>
       <c r="B78" t="s">
-        <v>86</v>
+        <v>237</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>419</v>
-      </c>
-      <c r="E78" t="s">
-        <v>420</v>
-      </c>
-      <c r="F78">
-        <v>1948</v>
-      </c>
-      <c r="G78">
-        <v>2012</v>
+        <v>282</v>
       </c>
       <c r="H78" t="s">
-        <v>348</v>
+        <v>16</v>
       </c>
       <c r="I78" t="s">
-        <v>349</v>
-      </c>
-      <c r="K78" s="2" t="s">
-        <v>421</v>
-      </c>
-      <c r="Q78" t="s">
-        <v>422</v>
+        <v>20</v>
       </c>
     </row>
     <row r="79" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>151</v>
+        <v>418</v>
       </c>
       <c r="B79" t="s">
-        <v>40</v>
+        <v>86</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>152</v>
+        <v>419</v>
       </c>
       <c r="E79" t="s">
-        <v>14</v>
+        <v>420</v>
+      </c>
+      <c r="F79">
+        <v>1948</v>
+      </c>
+      <c r="G79">
+        <v>2012</v>
+      </c>
+      <c r="H79" t="s">
+        <v>348</v>
+      </c>
+      <c r="I79" t="s">
+        <v>349</v>
+      </c>
+      <c r="K79" s="2" t="s">
+        <v>421</v>
+      </c>
+      <c r="Q79" t="s">
+        <v>422</v>
       </c>
     </row>
     <row r="80" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>242</v>
+        <v>151</v>
       </c>
       <c r="B80" t="s">
-        <v>237</v>
+        <v>40</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>243</v>
-      </c>
-      <c r="H80" t="s">
-        <v>16</v>
-      </c>
-      <c r="I80" t="s">
-        <v>20</v>
+        <v>152</v>
+      </c>
+      <c r="E80" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="81" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>292</v>
+        <v>242</v>
       </c>
       <c r="B81" t="s">
-        <v>99</v>
+        <v>237</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>291</v>
+        <v>243</v>
       </c>
       <c r="H81" t="s">
         <v>16</v>
@@ -3523,47 +3569,47 @@
     </row>
     <row r="82" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>153</v>
+        <v>292</v>
       </c>
       <c r="B82" t="s">
-        <v>259</v>
+        <v>99</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>154</v>
+        <v>291</v>
+      </c>
+      <c r="H82" t="s">
+        <v>16</v>
+      </c>
+      <c r="I82" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="83" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>228</v>
+        <v>153</v>
       </c>
       <c r="B83" t="s">
-        <v>40</v>
+        <v>259</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>225</v>
-      </c>
-      <c r="F83">
-        <v>1989</v>
-      </c>
-      <c r="G83">
-        <v>2017</v>
-      </c>
-      <c r="H83" t="s">
-        <v>16</v>
-      </c>
-      <c r="I83" t="s">
-        <v>20</v>
+        <v>154</v>
       </c>
     </row>
     <row r="84" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>245</v>
+        <v>228</v>
       </c>
       <c r="B84" t="s">
-        <v>237</v>
+        <v>40</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>244</v>
+        <v>225</v>
+      </c>
+      <c r="F84">
+        <v>1989</v>
+      </c>
+      <c r="G84">
+        <v>2017</v>
       </c>
       <c r="H84" t="s">
         <v>16</v>
@@ -3574,50 +3620,41 @@
     </row>
     <row r="85" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>100</v>
+        <v>245</v>
       </c>
       <c r="B85" t="s">
-        <v>99</v>
+        <v>237</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>101</v>
+        <v>244</v>
+      </c>
+      <c r="H85" t="s">
+        <v>16</v>
+      </c>
+      <c r="I85" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="86" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>239</v>
+        <v>100</v>
       </c>
       <c r="B86" t="s">
-        <v>237</v>
+        <v>99</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>243</v>
-      </c>
-      <c r="H86" t="s">
-        <v>16</v>
-      </c>
-      <c r="I86" t="s">
-        <v>20</v>
+        <v>101</v>
       </c>
     </row>
     <row r="87" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>254</v>
+        <v>239</v>
       </c>
       <c r="B87" t="s">
-        <v>55</v>
+        <v>237</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>253</v>
-      </c>
-      <c r="E87" t="s">
-        <v>255</v>
-      </c>
-      <c r="F87">
-        <v>1960</v>
-      </c>
-      <c r="G87">
-        <v>2014</v>
+        <v>243</v>
       </c>
       <c r="H87" t="s">
         <v>16</v>
@@ -3628,19 +3665,22 @@
     </row>
     <row r="88" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>270</v>
+        <v>254</v>
       </c>
       <c r="B88" t="s">
         <v>55</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>271</v>
+        <v>253</v>
+      </c>
+      <c r="E88" t="s">
+        <v>255</v>
       </c>
       <c r="F88">
-        <v>1990</v>
+        <v>1960</v>
       </c>
       <c r="G88">
-        <v>2010</v>
+        <v>2014</v>
       </c>
       <c r="H88" t="s">
         <v>16</v>
@@ -3651,96 +3691,90 @@
     </row>
     <row r="89" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>117</v>
+        <v>270</v>
       </c>
       <c r="B89" t="s">
         <v>55</v>
       </c>
       <c r="C89" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="F89">
+        <v>1990</v>
+      </c>
+      <c r="G89">
+        <v>2010</v>
+      </c>
+      <c r="H89" t="s">
+        <v>16</v>
+      </c>
+      <c r="I89" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="90" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A90" t="s">
+        <v>117</v>
+      </c>
+      <c r="B90" t="s">
+        <v>55</v>
+      </c>
+      <c r="C90" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="I89" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q89" t="s">
+      <c r="I90" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q90" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="90" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A90" s="1" t="s">
+    <row r="91" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A91" s="1" t="s">
         <v>23</v>
-      </c>
-      <c r="B90" t="s">
-        <v>25</v>
-      </c>
-      <c r="C90" s="2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="91" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A91" t="s">
-        <v>300</v>
       </c>
       <c r="B91" t="s">
         <v>25</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>298</v>
-      </c>
-      <c r="E91" t="s">
-        <v>299</v>
-      </c>
-      <c r="F91">
-        <v>1969</v>
-      </c>
-      <c r="H91" t="s">
-        <v>16</v>
-      </c>
-      <c r="I91" t="s">
-        <v>249</v>
+        <v>53</v>
       </c>
     </row>
     <row r="92" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>332</v>
+        <v>300</v>
       </c>
       <c r="B92" t="s">
-        <v>134</v>
+        <v>25</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>333</v>
+        <v>298</v>
       </c>
       <c r="E92" t="s">
-        <v>334</v>
+        <v>299</v>
+      </c>
+      <c r="F92">
+        <v>1969</v>
       </c>
       <c r="H92" t="s">
         <v>16</v>
       </c>
       <c r="I92" t="s">
-        <v>20</v>
+        <v>249</v>
       </c>
     </row>
     <row r="93" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>267</v>
+        <v>332</v>
       </c>
       <c r="B93" t="s">
-        <v>250</v>
+        <v>134</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>266</v>
-      </c>
-      <c r="D93" t="s">
-        <v>269</v>
+        <v>333</v>
       </c>
       <c r="E93" t="s">
-        <v>268</v>
-      </c>
-      <c r="F93">
-        <v>1970</v>
-      </c>
-      <c r="G93">
-        <v>2014</v>
+        <v>334</v>
       </c>
       <c r="H93" t="s">
         <v>16</v>
@@ -3751,97 +3785,100 @@
     </row>
     <row r="94" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>407</v>
+        <v>267</v>
       </c>
       <c r="B94" t="s">
-        <v>40</v>
+        <v>250</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>406</v>
+        <v>266</v>
       </c>
       <c r="D94" t="s">
-        <v>408</v>
+        <v>269</v>
       </c>
       <c r="E94" t="s">
-        <v>14</v>
+        <v>268</v>
       </c>
       <c r="F94">
-        <v>1949</v>
+        <v>1970</v>
       </c>
       <c r="G94">
-        <v>2013</v>
+        <v>2014</v>
       </c>
       <c r="H94" t="s">
-        <v>348</v>
+        <v>16</v>
       </c>
       <c r="I94" t="s">
-        <v>349</v>
+        <v>20</v>
       </c>
     </row>
     <row r="95" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>96</v>
+        <v>407</v>
       </c>
       <c r="B95" t="s">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>90</v>
+        <v>406</v>
+      </c>
+      <c r="D95" t="s">
+        <v>408</v>
       </c>
       <c r="E95" t="s">
-        <v>69</v>
+        <v>14</v>
       </c>
       <c r="F95">
-        <v>1995</v>
+        <v>1949</v>
+      </c>
+      <c r="G95">
+        <v>2013</v>
+      </c>
+      <c r="H95" t="s">
+        <v>348</v>
+      </c>
+      <c r="I95" t="s">
+        <v>349</v>
       </c>
     </row>
     <row r="96" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>404</v>
+        <v>96</v>
       </c>
       <c r="B96" t="s">
-        <v>83</v>
+        <v>25</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>403</v>
-      </c>
-      <c r="D96" t="s">
-        <v>405</v>
+        <v>90</v>
       </c>
       <c r="E96" t="s">
-        <v>14</v>
+        <v>69</v>
       </c>
       <c r="F96">
-        <v>1875</v>
-      </c>
-      <c r="G96">
-        <v>2004</v>
-      </c>
-      <c r="H96" t="s">
-        <v>348</v>
-      </c>
-      <c r="I96" t="s">
-        <v>349</v>
+        <v>1995</v>
       </c>
     </row>
     <row r="97" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>454</v>
+        <v>404</v>
       </c>
       <c r="B97" t="s">
-        <v>25</v>
+        <v>83</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>455</v>
+        <v>403</v>
+      </c>
+      <c r="D97" t="s">
+        <v>405</v>
       </c>
       <c r="E97" t="s">
-        <v>456</v>
+        <v>14</v>
       </c>
       <c r="F97">
-        <v>2006</v>
+        <v>1875</v>
       </c>
       <c r="G97">
-        <v>2016</v>
+        <v>2004</v>
       </c>
       <c r="H97" t="s">
         <v>348</v>
@@ -3849,80 +3886,83 @@
       <c r="I97" t="s">
         <v>349</v>
       </c>
-      <c r="J97" s="2" t="s">
-        <v>457</v>
-      </c>
-      <c r="L97" s="2" t="s">
-        <v>458</v>
-      </c>
-      <c r="Q97" t="s">
-        <v>459</v>
-      </c>
     </row>
     <row r="98" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>11</v>
+        <v>454</v>
       </c>
       <c r="B98" t="s">
         <v>25</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D98" t="s">
-        <v>95</v>
+        <v>455</v>
       </c>
       <c r="E98" t="s">
-        <v>10</v>
+        <v>456</v>
       </c>
       <c r="F98">
-        <v>2007</v>
+        <v>2006</v>
+      </c>
+      <c r="G98">
+        <v>2016</v>
       </c>
       <c r="H98" t="s">
-        <v>16</v>
+        <v>348</v>
       </c>
       <c r="I98" t="s">
-        <v>21</v>
+        <v>349</v>
+      </c>
+      <c r="J98" s="2" t="s">
+        <v>457</v>
+      </c>
+      <c r="L98" s="2" t="s">
+        <v>458</v>
+      </c>
+      <c r="Q98" t="s">
+        <v>459</v>
       </c>
     </row>
     <row r="99" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>223</v>
+        <v>11</v>
       </c>
       <c r="B99" t="s">
-        <v>124</v>
+        <v>25</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>222</v>
+        <v>12</v>
+      </c>
+      <c r="D99" t="s">
+        <v>95</v>
+      </c>
+      <c r="E99" t="s">
+        <v>10</v>
       </c>
       <c r="F99">
-        <v>1</v>
-      </c>
-      <c r="G99">
-        <v>2010</v>
+        <v>2007</v>
       </c>
       <c r="H99" t="s">
         <v>16</v>
       </c>
       <c r="I99" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="100" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="B100" t="s">
-        <v>40</v>
+        <v>124</v>
       </c>
       <c r="C100" s="2" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="F100">
-        <v>1946</v>
+        <v>1</v>
       </c>
       <c r="G100">
-        <v>2016</v>
+        <v>2010</v>
       </c>
       <c r="H100" t="s">
         <v>16</v>
@@ -3933,122 +3973,122 @@
     </row>
     <row r="101" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>97</v>
+        <v>226</v>
       </c>
       <c r="B101" t="s">
-        <v>128</v>
+        <v>40</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>98</v>
+        <v>225</v>
+      </c>
+      <c r="F101">
+        <v>1946</v>
+      </c>
+      <c r="G101">
+        <v>2016</v>
+      </c>
+      <c r="H101" t="s">
+        <v>16</v>
+      </c>
+      <c r="I101" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="102" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>278</v>
+        <v>97</v>
       </c>
       <c r="B102" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="C102" s="2" t="s">
-        <v>279</v>
-      </c>
-      <c r="E102" t="s">
-        <v>280</v>
-      </c>
-      <c r="F102">
-        <v>1890</v>
-      </c>
-      <c r="G102">
-        <v>1996</v>
-      </c>
-      <c r="H102" t="s">
-        <v>16</v>
-      </c>
-      <c r="I102" t="s">
-        <v>20</v>
+        <v>98</v>
       </c>
     </row>
     <row r="103" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>156</v>
+        <v>278</v>
       </c>
       <c r="B103" t="s">
-        <v>25</v>
+        <v>124</v>
       </c>
       <c r="C103" s="2" t="s">
-        <v>154</v>
+        <v>279</v>
+      </c>
+      <c r="E103" t="s">
+        <v>280</v>
+      </c>
+      <c r="F103">
+        <v>1890</v>
+      </c>
+      <c r="G103">
+        <v>1996</v>
+      </c>
+      <c r="H103" t="s">
+        <v>16</v>
+      </c>
+      <c r="I103" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="104" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>413</v>
+        <v>156</v>
       </c>
       <c r="B104" t="s">
-        <v>128</v>
+        <v>25</v>
       </c>
       <c r="C104" s="2" t="s">
-        <v>414</v>
-      </c>
-      <c r="E104" t="s">
-        <v>415</v>
-      </c>
-      <c r="F104">
-        <v>1946</v>
-      </c>
-      <c r="G104">
-        <v>2014</v>
-      </c>
-      <c r="H104" t="s">
-        <v>348</v>
-      </c>
-      <c r="I104" t="s">
-        <v>349</v>
-      </c>
-      <c r="N104" s="2" t="s">
-        <v>416</v>
-      </c>
-      <c r="Q104" t="s">
-        <v>417</v>
+        <v>154</v>
       </c>
     </row>
     <row r="105" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>229</v>
+        <v>413</v>
       </c>
       <c r="B105" t="s">
-        <v>40</v>
+        <v>128</v>
       </c>
       <c r="C105" s="2" t="s">
-        <v>225</v>
+        <v>414</v>
+      </c>
+      <c r="E105" t="s">
+        <v>415</v>
       </c>
       <c r="F105">
-        <v>1952</v>
+        <v>1946</v>
       </c>
       <c r="G105">
-        <v>1997</v>
+        <v>2014</v>
       </c>
       <c r="H105" t="s">
-        <v>16</v>
+        <v>348</v>
       </c>
       <c r="I105" t="s">
-        <v>20</v>
+        <v>349</v>
+      </c>
+      <c r="N105" s="2" t="s">
+        <v>416</v>
+      </c>
+      <c r="Q105" t="s">
+        <v>417</v>
       </c>
     </row>
     <row r="106" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>293</v>
+        <v>229</v>
       </c>
       <c r="B106" t="s">
         <v>40</v>
       </c>
       <c r="C106" s="2" t="s">
-        <v>294</v>
+        <v>225</v>
       </c>
       <c r="F106">
-        <v>2004</v>
+        <v>1952</v>
       </c>
       <c r="G106">
-        <v>2006</v>
+        <v>1997</v>
       </c>
       <c r="H106" t="s">
         <v>16</v>
@@ -4059,221 +4099,218 @@
     </row>
     <row r="107" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>102</v>
+        <v>293</v>
       </c>
       <c r="B107" t="s">
-        <v>99</v>
+        <v>40</v>
       </c>
       <c r="C107" s="2" t="s">
-        <v>103</v>
+        <v>294</v>
+      </c>
+      <c r="F107">
+        <v>2004</v>
+      </c>
+      <c r="G107">
+        <v>2006</v>
+      </c>
+      <c r="H107" t="s">
+        <v>16</v>
+      </c>
+      <c r="I107" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="108" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>289</v>
+        <v>102</v>
       </c>
       <c r="B108" t="s">
-        <v>124</v>
+        <v>99</v>
       </c>
       <c r="C108" s="2" t="s">
-        <v>290</v>
+        <v>103</v>
       </c>
     </row>
     <row r="109" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>246</v>
+        <v>289</v>
       </c>
       <c r="B109" t="s">
-        <v>165</v>
+        <v>124</v>
       </c>
       <c r="C109" s="2" t="s">
-        <v>247</v>
-      </c>
-      <c r="E109" t="s">
-        <v>14</v>
-      </c>
-      <c r="F109">
-        <v>1960</v>
-      </c>
-      <c r="G109">
-        <v>2006</v>
-      </c>
-      <c r="H109" t="s">
-        <v>16</v>
-      </c>
-      <c r="I109" t="s">
-        <v>249</v>
+        <v>290</v>
       </c>
     </row>
     <row r="110" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>365</v>
+        <v>246</v>
       </c>
       <c r="B110" t="s">
-        <v>128</v>
+        <v>165</v>
       </c>
       <c r="C110" s="2" t="s">
-        <v>364</v>
-      </c>
-      <c r="D110" t="s">
-        <v>370</v>
+        <v>247</v>
       </c>
       <c r="E110" t="s">
-        <v>366</v>
+        <v>14</v>
       </c>
       <c r="F110">
-        <v>1906</v>
+        <v>1960</v>
       </c>
       <c r="G110">
-        <v>2013</v>
+        <v>2006</v>
       </c>
       <c r="H110" t="s">
-        <v>367</v>
+        <v>16</v>
       </c>
       <c r="I110" t="s">
-        <v>368</v>
-      </c>
-      <c r="Q110" t="s">
-        <v>369</v>
+        <v>249</v>
       </c>
     </row>
     <row r="111" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>208</v>
+        <v>365</v>
       </c>
       <c r="B111" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="C111" s="2" t="s">
-        <v>209</v>
+        <v>364</v>
+      </c>
+      <c r="D111" t="s">
+        <v>370</v>
+      </c>
+      <c r="E111" t="s">
+        <v>366</v>
       </c>
       <c r="F111">
-        <v>1932</v>
+        <v>1906</v>
       </c>
       <c r="G111">
-        <v>2014</v>
+        <v>2013</v>
       </c>
       <c r="H111" t="s">
-        <v>16</v>
+        <v>367</v>
       </c>
       <c r="I111" t="s">
-        <v>20</v>
+        <v>368</v>
+      </c>
+      <c r="Q111" t="s">
+        <v>369</v>
       </c>
     </row>
     <row r="112" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>137</v>
+        <v>208</v>
       </c>
       <c r="B112" t="s">
-        <v>259</v>
+        <v>124</v>
       </c>
       <c r="C112" s="2" t="s">
-        <v>138</v>
+        <v>209</v>
+      </c>
+      <c r="F112">
+        <v>1932</v>
+      </c>
+      <c r="G112">
+        <v>2014</v>
+      </c>
+      <c r="H112" t="s">
+        <v>16</v>
+      </c>
+      <c r="I112" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="113" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>155</v>
+        <v>137</v>
       </c>
       <c r="B113" t="s">
         <v>259</v>
       </c>
       <c r="C113" s="2" t="s">
-        <v>154</v>
+        <v>138</v>
       </c>
     </row>
     <row r="114" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>57</v>
+        <v>155</v>
       </c>
       <c r="B114" t="s">
-        <v>128</v>
+        <v>259</v>
       </c>
       <c r="C114" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="Q114" t="s">
-        <v>17</v>
+        <v>154</v>
       </c>
     </row>
     <row r="115" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>129</v>
+        <v>57</v>
       </c>
       <c r="B115" t="s">
-        <v>259</v>
+        <v>128</v>
       </c>
       <c r="C115" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="E115" t="s">
-        <v>131</v>
-      </c>
-      <c r="F115">
-        <v>1945</v>
-      </c>
-      <c r="G115">
-        <v>2008</v>
-      </c>
-      <c r="I115" t="s">
-        <v>20</v>
+        <v>58</v>
+      </c>
+      <c r="Q115" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="116" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>148</v>
+        <v>129</v>
       </c>
       <c r="B116" t="s">
-        <v>128</v>
+        <v>259</v>
       </c>
       <c r="C116" s="2" t="s">
-        <v>147</v>
+        <v>130</v>
+      </c>
+      <c r="E116" t="s">
+        <v>131</v>
+      </c>
+      <c r="F116">
+        <v>1945</v>
+      </c>
+      <c r="G116">
+        <v>2008</v>
+      </c>
+      <c r="I116" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="117" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>233</v>
+        <v>148</v>
       </c>
       <c r="B117" t="s">
-        <v>165</v>
+        <v>128</v>
       </c>
       <c r="C117" s="2" t="s">
-        <v>234</v>
-      </c>
-      <c r="E117" t="s">
-        <v>14</v>
-      </c>
-      <c r="F117">
-        <v>2012</v>
-      </c>
-      <c r="G117">
-        <v>2016</v>
-      </c>
-      <c r="H117" t="s">
-        <v>16</v>
-      </c>
-      <c r="I117" t="s">
-        <v>20</v>
+        <v>147</v>
       </c>
     </row>
     <row r="118" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>35</v>
+        <v>233</v>
       </c>
       <c r="B118" t="s">
-        <v>25</v>
+        <v>165</v>
       </c>
       <c r="C118" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="D118" t="s">
-        <v>37</v>
+        <v>234</v>
       </c>
       <c r="E118" t="s">
         <v>14</v>
       </c>
       <c r="F118">
-        <v>2001</v>
+        <v>2012</v>
+      </c>
+      <c r="G118">
+        <v>2016</v>
       </c>
       <c r="H118" t="s">
         <v>16</v>
@@ -4284,148 +4321,148 @@
     </row>
     <row r="119" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>185</v>
+        <v>35</v>
       </c>
       <c r="B119" t="s">
-        <v>128</v>
+        <v>25</v>
       </c>
       <c r="C119" s="2" t="s">
-        <v>186</v>
+        <v>36</v>
+      </c>
+      <c r="D119" t="s">
+        <v>37</v>
+      </c>
+      <c r="E119" t="s">
+        <v>14</v>
+      </c>
+      <c r="F119">
+        <v>2001</v>
+      </c>
+      <c r="H119" t="s">
+        <v>16</v>
+      </c>
+      <c r="I119" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="120" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>210</v>
+        <v>185</v>
       </c>
       <c r="B120" t="s">
-        <v>40</v>
+        <v>128</v>
       </c>
       <c r="C120" s="2" t="s">
-        <v>211</v>
-      </c>
-      <c r="F120">
-        <v>1976</v>
-      </c>
-      <c r="G120">
-        <v>2016</v>
-      </c>
-      <c r="H120" t="s">
-        <v>16</v>
-      </c>
-      <c r="I120" t="s">
-        <v>20</v>
+        <v>186</v>
       </c>
     </row>
     <row r="121" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>426</v>
+        <v>210</v>
       </c>
       <c r="B121" t="s">
-        <v>86</v>
+        <v>40</v>
       </c>
       <c r="C121" s="2" t="s">
-        <v>427</v>
-      </c>
-      <c r="E121" t="s">
-        <v>34</v>
+        <v>211</v>
       </c>
       <c r="F121">
-        <v>2015</v>
+        <v>1976</v>
       </c>
       <c r="G121">
         <v>2016</v>
       </c>
       <c r="H121" t="s">
-        <v>348</v>
+        <v>16</v>
       </c>
       <c r="I121" t="s">
-        <v>349</v>
-      </c>
-      <c r="K121" s="2" t="s">
-        <v>428</v>
+        <v>20</v>
       </c>
     </row>
     <row r="122" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>144</v>
+        <v>426</v>
       </c>
       <c r="B122" t="s">
-        <v>60</v>
+        <v>86</v>
       </c>
       <c r="C122" s="2" t="s">
-        <v>143</v>
+        <v>427</v>
+      </c>
+      <c r="E122" t="s">
+        <v>34</v>
       </c>
       <c r="F122">
-        <v>1800</v>
+        <v>2015</v>
       </c>
       <c r="G122">
-        <v>2013</v>
+        <v>2016</v>
+      </c>
+      <c r="H122" t="s">
+        <v>348</v>
+      </c>
+      <c r="I122" t="s">
+        <v>349</v>
+      </c>
+      <c r="K122" s="2" t="s">
+        <v>428</v>
       </c>
     </row>
     <row r="123" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>472</v>
+        <v>144</v>
       </c>
       <c r="B123" t="s">
-        <v>25</v>
+        <v>60</v>
       </c>
       <c r="C123" s="2" t="s">
-        <v>473</v>
-      </c>
-      <c r="D123" t="s">
-        <v>474</v>
-      </c>
-      <c r="E123" t="s">
-        <v>112</v>
+        <v>143</v>
       </c>
       <c r="F123">
-        <v>1943</v>
-      </c>
-      <c r="H123" t="s">
-        <v>348</v>
-      </c>
-      <c r="I123" t="s">
-        <v>349</v>
-      </c>
-      <c r="N123" s="2" t="s">
-        <v>475</v>
+        <v>1800</v>
+      </c>
+      <c r="G123">
+        <v>2013</v>
       </c>
     </row>
     <row r="124" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>122</v>
+        <v>472</v>
       </c>
       <c r="B124" t="s">
-        <v>259</v>
+        <v>25</v>
       </c>
       <c r="C124" s="2" t="s">
-        <v>121</v>
+        <v>473</v>
+      </c>
+      <c r="D124" t="s">
+        <v>474</v>
+      </c>
+      <c r="E124" t="s">
+        <v>112</v>
+      </c>
+      <c r="F124">
+        <v>1943</v>
+      </c>
+      <c r="H124" t="s">
+        <v>348</v>
       </c>
       <c r="I124" t="s">
-        <v>20</v>
+        <v>349</v>
+      </c>
+      <c r="N124" s="2" t="s">
+        <v>475</v>
       </c>
     </row>
     <row r="125" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>318</v>
+        <v>122</v>
       </c>
       <c r="B125" t="s">
-        <v>250</v>
+        <v>259</v>
       </c>
       <c r="C125" s="2" t="s">
-        <v>319</v>
-      </c>
-      <c r="E125" t="s">
-        <v>320</v>
-      </c>
-      <c r="F125">
-        <v>1975</v>
-      </c>
-      <c r="G125">
-        <v>1989</v>
-      </c>
-      <c r="H125" t="s">
-        <v>16</v>
+        <v>121</v>
       </c>
       <c r="I125" t="s">
         <v>20</v>
@@ -4433,22 +4470,22 @@
     </row>
     <row r="126" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="B126" t="s">
         <v>250</v>
       </c>
       <c r="C126" s="2" t="s">
-        <v>317</v>
+        <v>319</v>
       </c>
       <c r="E126" t="s">
-        <v>105</v>
+        <v>320</v>
       </c>
       <c r="F126">
-        <v>1950</v>
+        <v>1975</v>
       </c>
       <c r="G126">
-        <v>1996</v>
+        <v>1989</v>
       </c>
       <c r="H126" t="s">
         <v>16</v>
@@ -4459,19 +4496,22 @@
     </row>
     <row r="127" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>322</v>
+        <v>316</v>
       </c>
       <c r="B127" t="s">
-        <v>25</v>
+        <v>250</v>
       </c>
       <c r="C127" s="2" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="E127" t="s">
-        <v>77</v>
+        <v>105</v>
       </c>
       <c r="F127">
-        <v>2010</v>
+        <v>1950</v>
+      </c>
+      <c r="G127">
+        <v>1996</v>
       </c>
       <c r="H127" t="s">
         <v>16</v>
@@ -4482,121 +4522,118 @@
     </row>
     <row r="128" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>141</v>
+        <v>322</v>
       </c>
       <c r="B128" t="s">
-        <v>237</v>
+        <v>25</v>
       </c>
       <c r="C128" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="Q128" t="s">
-        <v>17</v>
+        <v>321</v>
+      </c>
+      <c r="E128" t="s">
+        <v>77</v>
+      </c>
+      <c r="F128">
+        <v>2010</v>
+      </c>
+      <c r="H128" t="s">
+        <v>16</v>
+      </c>
+      <c r="I128" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="129" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>308</v>
+        <v>141</v>
       </c>
       <c r="B129" t="s">
-        <v>250</v>
+        <v>237</v>
       </c>
       <c r="C129" s="2" t="s">
-        <v>309</v>
-      </c>
-      <c r="E129" t="s">
-        <v>310</v>
-      </c>
-      <c r="F129">
-        <v>1950</v>
-      </c>
-      <c r="G129">
-        <v>2010</v>
-      </c>
-      <c r="H129" t="s">
-        <v>16</v>
-      </c>
-      <c r="I129" t="s">
-        <v>20</v>
+        <v>142</v>
+      </c>
+      <c r="Q129" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="130" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
-        <v>287</v>
+        <v>308</v>
       </c>
       <c r="B130" t="s">
-        <v>134</v>
+        <v>250</v>
       </c>
       <c r="C130" s="2" t="s">
-        <v>288</v>
+        <v>309</v>
+      </c>
+      <c r="E130" t="s">
+        <v>310</v>
       </c>
       <c r="F130">
-        <v>1990</v>
+        <v>1950</v>
       </c>
       <c r="G130">
-        <v>2008</v>
+        <v>2010</v>
+      </c>
+      <c r="H130" t="s">
+        <v>16</v>
+      </c>
+      <c r="I130" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="131" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>274</v>
+        <v>287</v>
       </c>
       <c r="B131" t="s">
-        <v>55</v>
+        <v>134</v>
       </c>
       <c r="C131" s="2" t="s">
-        <v>275</v>
-      </c>
-      <c r="H131" t="s">
-        <v>16</v>
-      </c>
-      <c r="I131" t="s">
-        <v>20</v>
+        <v>288</v>
+      </c>
+      <c r="F131">
+        <v>1990</v>
+      </c>
+      <c r="G131">
+        <v>2008</v>
       </c>
     </row>
     <row r="132" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>157</v>
+        <v>274</v>
       </c>
       <c r="B132" t="s">
-        <v>128</v>
+        <v>55</v>
       </c>
       <c r="C132" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="Q132" t="s">
-        <v>18</v>
+        <v>275</v>
+      </c>
+      <c r="H132" t="s">
+        <v>16</v>
+      </c>
+      <c r="I132" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="133" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
-        <v>439</v>
+        <v>157</v>
       </c>
       <c r="B133" t="s">
-        <v>259</v>
+        <v>128</v>
       </c>
       <c r="C133" s="2" t="s">
-        <v>438</v>
-      </c>
-      <c r="H133" t="s">
-        <v>348</v>
-      </c>
-      <c r="I133" t="s">
-        <v>349</v>
-      </c>
-      <c r="J133" s="2" t="s">
-        <v>440</v>
-      </c>
-      <c r="K133" s="2" t="s">
-        <v>442</v>
-      </c>
-      <c r="L133" s="2" t="s">
-        <v>441</v>
+        <v>154</v>
+      </c>
+      <c r="Q133" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="134" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
-        <v>443</v>
+        <v>439</v>
       </c>
       <c r="B134" t="s">
         <v>259</v>
@@ -4604,15 +4641,6 @@
       <c r="C134" s="2" t="s">
         <v>438</v>
       </c>
-      <c r="D134" t="s">
-        <v>447</v>
-      </c>
-      <c r="F134">
-        <v>1990</v>
-      </c>
-      <c r="G134">
-        <v>2014</v>
-      </c>
       <c r="H134" t="s">
         <v>348</v>
       </c>
@@ -4620,87 +4648,99 @@
         <v>349</v>
       </c>
       <c r="J134" s="2" t="s">
-        <v>444</v>
+        <v>440</v>
       </c>
       <c r="K134" s="2" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
       <c r="L134" s="2" t="s">
-        <v>446</v>
+        <v>441</v>
       </c>
     </row>
     <row r="135" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
-        <v>194</v>
+        <v>443</v>
       </c>
       <c r="B135" t="s">
-        <v>99</v>
+        <v>259</v>
       </c>
       <c r="C135" s="2" t="s">
-        <v>193</v>
+        <v>438</v>
+      </c>
+      <c r="D135" t="s">
+        <v>447</v>
+      </c>
+      <c r="F135">
+        <v>1990</v>
+      </c>
+      <c r="G135">
+        <v>2014</v>
+      </c>
+      <c r="H135" t="s">
+        <v>348</v>
+      </c>
+      <c r="I135" t="s">
+        <v>349</v>
+      </c>
+      <c r="J135" s="2" t="s">
+        <v>444</v>
+      </c>
+      <c r="K135" s="2" t="s">
+        <v>445</v>
+      </c>
+      <c r="L135" s="2" t="s">
+        <v>446</v>
       </c>
     </row>
     <row r="136" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
-        <v>295</v>
+        <v>194</v>
       </c>
       <c r="B136" t="s">
-        <v>40</v>
+        <v>99</v>
       </c>
       <c r="C136" s="2" t="s">
-        <v>296</v>
-      </c>
-      <c r="E136" t="s">
-        <v>297</v>
-      </c>
-      <c r="F136">
-        <v>1990</v>
-      </c>
-      <c r="G136">
-        <v>2015</v>
-      </c>
-      <c r="H136" t="s">
-        <v>16</v>
-      </c>
-      <c r="I136" t="s">
-        <v>249</v>
+        <v>193</v>
       </c>
     </row>
     <row r="137" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
-        <v>256</v>
+        <v>295</v>
       </c>
       <c r="B137" t="s">
-        <v>250</v>
+        <v>40</v>
       </c>
       <c r="C137" s="2" t="s">
-        <v>257</v>
+        <v>296</v>
       </c>
       <c r="E137" t="s">
-        <v>258</v>
+        <v>297</v>
+      </c>
+      <c r="F137">
+        <v>1990</v>
+      </c>
+      <c r="G137">
+        <v>2015</v>
       </c>
       <c r="H137" t="s">
         <v>16</v>
       </c>
       <c r="I137" t="s">
-        <v>20</v>
+        <v>249</v>
       </c>
     </row>
     <row r="138" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
-        <v>227</v>
+        <v>256</v>
       </c>
       <c r="B138" t="s">
-        <v>40</v>
+        <v>250</v>
       </c>
       <c r="C138" s="2" t="s">
-        <v>225</v>
-      </c>
-      <c r="F138">
-        <v>1955</v>
-      </c>
-      <c r="G138">
-        <v>2016</v>
+        <v>257</v>
+      </c>
+      <c r="E138" t="s">
+        <v>258</v>
       </c>
       <c r="H138" t="s">
         <v>16</v>
@@ -4711,7 +4751,7 @@
     </row>
     <row r="139" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="B139" t="s">
         <v>40</v>
@@ -4720,7 +4760,7 @@
         <v>225</v>
       </c>
       <c r="F139">
-        <v>1995</v>
+        <v>1955</v>
       </c>
       <c r="G139">
         <v>2016</v>
@@ -4734,248 +4774,248 @@
     </row>
     <row r="140" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
-        <v>452</v>
+        <v>230</v>
       </c>
       <c r="B140" t="s">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="C140" s="2" t="s">
-        <v>453</v>
-      </c>
-      <c r="E140" t="s">
-        <v>9</v>
+        <v>225</v>
+      </c>
+      <c r="F140">
+        <v>1995</v>
+      </c>
+      <c r="G140">
+        <v>2016</v>
       </c>
       <c r="H140" t="s">
-        <v>348</v>
+        <v>16</v>
       </c>
       <c r="I140" t="s">
-        <v>435</v>
+        <v>20</v>
       </c>
     </row>
     <row r="141" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
-        <v>109</v>
+        <v>452</v>
       </c>
       <c r="B141" t="s">
         <v>25</v>
       </c>
       <c r="C141" s="2" t="s">
-        <v>110</v>
+        <v>453</v>
       </c>
       <c r="E141" t="s">
-        <v>111</v>
-      </c>
-      <c r="F141">
-        <v>1956</v>
+        <v>9</v>
+      </c>
+      <c r="H141" t="s">
+        <v>348</v>
+      </c>
+      <c r="I141" t="s">
+        <v>435</v>
       </c>
     </row>
     <row r="142" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
-        <v>326</v>
+        <v>109</v>
       </c>
       <c r="B142" t="s">
         <v>25</v>
       </c>
       <c r="C142" s="2" t="s">
-        <v>327</v>
+        <v>110</v>
       </c>
       <c r="E142" t="s">
         <v>111</v>
       </c>
       <c r="F142">
-        <v>1998</v>
-      </c>
-      <c r="H142" t="s">
-        <v>16</v>
-      </c>
-      <c r="I142" t="s">
-        <v>20</v>
+        <v>1956</v>
       </c>
     </row>
     <row r="143" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
-        <v>91</v>
+        <v>326</v>
       </c>
       <c r="B143" t="s">
         <v>25</v>
       </c>
       <c r="C143" s="2" t="s">
-        <v>93</v>
+        <v>327</v>
       </c>
       <c r="E143" t="s">
-        <v>92</v>
+        <v>111</v>
       </c>
       <c r="F143">
-        <v>1999</v>
+        <v>1998</v>
+      </c>
+      <c r="H143" t="s">
+        <v>16</v>
+      </c>
+      <c r="I143" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="144" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
-        <v>314</v>
+        <v>91</v>
       </c>
       <c r="B144" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="C144" s="2" t="s">
-        <v>313</v>
+        <v>93</v>
       </c>
       <c r="E144" t="s">
-        <v>315</v>
+        <v>92</v>
       </c>
       <c r="F144">
-        <v>1950</v>
-      </c>
-      <c r="G144">
-        <v>2004</v>
-      </c>
-      <c r="H144" t="s">
-        <v>16</v>
-      </c>
-      <c r="I144" t="s">
-        <v>20</v>
+        <v>1999</v>
       </c>
     </row>
     <row r="145" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
-        <v>161</v>
+        <v>314</v>
       </c>
       <c r="B145" t="s">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="C145" s="2" t="s">
-        <v>160</v>
+        <v>313</v>
+      </c>
+      <c r="E145" t="s">
+        <v>315</v>
+      </c>
+      <c r="F145">
+        <v>1950</v>
+      </c>
+      <c r="G145">
+        <v>2004</v>
+      </c>
+      <c r="H145" t="s">
+        <v>16</v>
+      </c>
+      <c r="I145" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="146" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="B146" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="C146" s="2" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
     </row>
     <row r="147" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
-        <v>399</v>
+        <v>168</v>
       </c>
       <c r="B147" t="s">
         <v>40</v>
       </c>
       <c r="C147" s="2" t="s">
-        <v>400</v>
-      </c>
-      <c r="E147" t="s">
-        <v>14</v>
-      </c>
-      <c r="F147">
-        <v>2000</v>
-      </c>
-      <c r="G147">
-        <v>2014</v>
-      </c>
-      <c r="H147" t="s">
-        <v>348</v>
-      </c>
-      <c r="I147" t="s">
-        <v>349</v>
-      </c>
-      <c r="J147" s="2" t="s">
-        <v>402</v>
-      </c>
-      <c r="N147" s="2" t="s">
-        <v>401</v>
+        <v>167</v>
       </c>
     </row>
     <row r="148" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
-        <v>213</v>
+        <v>399</v>
       </c>
       <c r="B148" t="s">
-        <v>55</v>
+        <v>40</v>
       </c>
       <c r="C148" s="2" t="s">
-        <v>212</v>
+        <v>400</v>
+      </c>
+      <c r="E148" t="s">
+        <v>14</v>
+      </c>
+      <c r="F148">
+        <v>2000</v>
+      </c>
+      <c r="G148">
+        <v>2014</v>
       </c>
       <c r="H148" t="s">
-        <v>16</v>
+        <v>348</v>
       </c>
       <c r="I148" t="s">
-        <v>20</v>
+        <v>349</v>
+      </c>
+      <c r="J148" s="2" t="s">
+        <v>402</v>
+      </c>
+      <c r="N148" s="2" t="s">
+        <v>401</v>
       </c>
     </row>
     <row r="149" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
-        <v>395</v>
+        <v>213</v>
       </c>
       <c r="B149" t="s">
-        <v>25</v>
+        <v>55</v>
       </c>
       <c r="C149" s="2" t="s">
-        <v>394</v>
-      </c>
-      <c r="D149" t="s">
-        <v>396</v>
-      </c>
-      <c r="E149" t="s">
-        <v>111</v>
-      </c>
-      <c r="F149">
-        <v>1986</v>
-      </c>
-      <c r="G149">
-        <v>2015</v>
+        <v>212</v>
       </c>
       <c r="H149" t="s">
-        <v>367</v>
+        <v>16</v>
       </c>
       <c r="I149" t="s">
-        <v>398</v>
-      </c>
-      <c r="J149" s="2" t="s">
-        <v>397</v>
+        <v>20</v>
       </c>
     </row>
     <row r="150" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
-        <v>323</v>
+        <v>395</v>
       </c>
       <c r="B150" t="s">
         <v>25</v>
       </c>
       <c r="C150" s="2" t="s">
-        <v>324</v>
+        <v>394</v>
+      </c>
+      <c r="D150" t="s">
+        <v>396</v>
       </c>
       <c r="E150" t="s">
-        <v>325</v>
+        <v>111</v>
       </c>
       <c r="F150">
-        <v>1942</v>
+        <v>1986</v>
+      </c>
+      <c r="G150">
+        <v>2015</v>
       </c>
       <c r="H150" t="s">
-        <v>16</v>
+        <v>367</v>
       </c>
       <c r="I150" t="s">
-        <v>20</v>
+        <v>398</v>
+      </c>
+      <c r="J150" s="2" t="s">
+        <v>397</v>
       </c>
     </row>
     <row r="151" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
-        <v>273</v>
+        <v>323</v>
       </c>
       <c r="B151" t="s">
-        <v>237</v>
+        <v>25</v>
       </c>
       <c r="C151" s="2" t="s">
-        <v>272</v>
+        <v>324</v>
+      </c>
+      <c r="E151" t="s">
+        <v>325</v>
       </c>
       <c r="F151">
-        <v>1996</v>
-      </c>
-      <c r="G151">
-        <v>2016</v>
+        <v>1942</v>
       </c>
       <c r="H151" t="s">
         <v>16</v>
@@ -4986,209 +5026,212 @@
     </row>
     <row r="152" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
-        <v>66</v>
+        <v>273</v>
       </c>
       <c r="B152" t="s">
-        <v>25</v>
+        <v>237</v>
       </c>
       <c r="C152" s="2" t="s">
-        <v>67</v>
+        <v>272</v>
+      </c>
+      <c r="F152">
+        <v>1996</v>
+      </c>
+      <c r="G152">
+        <v>2016</v>
+      </c>
+      <c r="H152" t="s">
+        <v>16</v>
+      </c>
+      <c r="I152" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="153" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
-        <v>383</v>
+        <v>66</v>
       </c>
       <c r="B153" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="C153" s="2" t="s">
-        <v>384</v>
-      </c>
-      <c r="E153" t="s">
-        <v>386</v>
-      </c>
-      <c r="F153">
-        <v>1951</v>
-      </c>
-      <c r="H153" t="s">
-        <v>348</v>
-      </c>
-      <c r="I153" t="s">
-        <v>349</v>
-      </c>
-      <c r="N153" s="2" t="s">
-        <v>385</v>
+        <v>67</v>
       </c>
     </row>
     <row r="154" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
-        <v>139</v>
+        <v>383</v>
       </c>
       <c r="B154" t="s">
         <v>40</v>
       </c>
       <c r="C154" s="2" t="s">
-        <v>140</v>
+        <v>384</v>
+      </c>
+      <c r="E154" t="s">
+        <v>386</v>
+      </c>
+      <c r="F154">
+        <v>1951</v>
+      </c>
+      <c r="H154" t="s">
+        <v>348</v>
+      </c>
+      <c r="I154" t="s">
+        <v>349</v>
+      </c>
+      <c r="N154" s="2" t="s">
+        <v>385</v>
       </c>
     </row>
     <row r="155" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
-        <v>329</v>
+        <v>139</v>
       </c>
       <c r="B155" t="s">
-        <v>165</v>
+        <v>40</v>
       </c>
       <c r="C155" s="2" t="s">
-        <v>328</v>
-      </c>
-      <c r="E155" t="s">
-        <v>34</v>
-      </c>
-      <c r="F155">
-        <v>1789</v>
-      </c>
-      <c r="H155" t="s">
-        <v>16</v>
-      </c>
-      <c r="I155" t="s">
-        <v>20</v>
+        <v>140</v>
       </c>
     </row>
     <row r="156" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
-        <v>172</v>
+        <v>329</v>
       </c>
       <c r="B156" t="s">
-        <v>60</v>
+        <v>165</v>
       </c>
       <c r="C156" s="2" t="s">
-        <v>171</v>
+        <v>328</v>
+      </c>
+      <c r="E156" t="s">
+        <v>34</v>
+      </c>
+      <c r="F156">
+        <v>1789</v>
+      </c>
+      <c r="H156" t="s">
+        <v>16</v>
+      </c>
+      <c r="I156" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="157" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
-        <v>217</v>
+        <v>172</v>
       </c>
       <c r="B157" t="s">
         <v>60</v>
       </c>
       <c r="C157" s="2" t="s">
-        <v>216</v>
-      </c>
-      <c r="E157" t="s">
-        <v>14</v>
-      </c>
-      <c r="F157">
-        <v>1900</v>
-      </c>
-      <c r="H157" t="s">
-        <v>16</v>
-      </c>
-      <c r="I157" t="s">
-        <v>20</v>
+        <v>171</v>
       </c>
     </row>
     <row r="158" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
-        <v>132</v>
+        <v>217</v>
       </c>
       <c r="B158" t="s">
-        <v>259</v>
+        <v>60</v>
       </c>
       <c r="C158" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="Q158" t="s">
-        <v>17</v>
+        <v>216</v>
+      </c>
+      <c r="E158" t="s">
+        <v>14</v>
+      </c>
+      <c r="F158">
+        <v>1900</v>
+      </c>
+      <c r="H158" t="s">
+        <v>16</v>
+      </c>
+      <c r="I158" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="159" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
-        <v>182</v>
+        <v>132</v>
       </c>
       <c r="B159" t="s">
-        <v>165</v>
+        <v>259</v>
       </c>
       <c r="C159" s="2" t="s">
-        <v>181</v>
+        <v>133</v>
+      </c>
+      <c r="Q159" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="160" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
-        <v>423</v>
+        <v>182</v>
       </c>
       <c r="B160" t="s">
-        <v>86</v>
+        <v>165</v>
       </c>
       <c r="C160" s="2" t="s">
-        <v>424</v>
-      </c>
-      <c r="E160" t="s">
-        <v>34</v>
-      </c>
-      <c r="F160">
-        <v>1996</v>
-      </c>
-      <c r="G160">
-        <v>2016</v>
-      </c>
-      <c r="H160" t="s">
-        <v>348</v>
-      </c>
-      <c r="I160" t="s">
-        <v>425</v>
+        <v>181</v>
       </c>
     </row>
     <row r="161" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
-        <v>115</v>
+        <v>423</v>
       </c>
       <c r="B161" t="s">
-        <v>128</v>
+        <v>86</v>
       </c>
       <c r="C161" s="2" t="s">
-        <v>116</v>
+        <v>424</v>
+      </c>
+      <c r="E161" t="s">
+        <v>34</v>
+      </c>
+      <c r="F161">
+        <v>1996</v>
+      </c>
+      <c r="G161">
+        <v>2016</v>
+      </c>
+      <c r="H161" t="s">
+        <v>348</v>
+      </c>
+      <c r="I161" t="s">
+        <v>425</v>
       </c>
     </row>
     <row r="162" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
-        <v>263</v>
+        <v>115</v>
       </c>
       <c r="B162" t="s">
-        <v>250</v>
+        <v>128</v>
       </c>
       <c r="C162" s="2" t="s">
-        <v>264</v>
-      </c>
-      <c r="E162" t="s">
-        <v>265</v>
-      </c>
-      <c r="F162">
-        <v>1500</v>
-      </c>
-      <c r="G162">
-        <v>2000</v>
-      </c>
-      <c r="H162" t="s">
-        <v>16</v>
-      </c>
-      <c r="I162" t="s">
-        <v>20</v>
+        <v>116</v>
       </c>
     </row>
     <row r="163" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
-        <v>221</v>
+        <v>263</v>
       </c>
       <c r="B163" t="s">
-        <v>86</v>
+        <v>250</v>
       </c>
       <c r="C163" s="2" t="s">
-        <v>220</v>
+        <v>264</v>
+      </c>
+      <c r="E163" t="s">
+        <v>265</v>
       </c>
       <c r="F163">
-        <v>2013</v>
+        <v>1500</v>
+      </c>
+      <c r="G163">
+        <v>2000</v>
       </c>
       <c r="H163" t="s">
         <v>16</v>
@@ -5199,22 +5242,16 @@
     </row>
     <row r="164" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
-        <v>13</v>
+        <v>221</v>
       </c>
       <c r="B164" t="s">
-        <v>25</v>
+        <v>86</v>
       </c>
       <c r="C164" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="D164" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="E164" t="s">
-        <v>14</v>
+        <v>220</v>
       </c>
       <c r="F164">
-        <v>1981</v>
+        <v>2013</v>
       </c>
       <c r="H164" t="s">
         <v>16</v>
@@ -5225,166 +5262,192 @@
     </row>
     <row r="165" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
+        <v>13</v>
+      </c>
+      <c r="B165" t="s">
+        <v>25</v>
+      </c>
+      <c r="C165" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D165" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E165" t="s">
+        <v>14</v>
+      </c>
+      <c r="F165">
+        <v>1981</v>
+      </c>
+      <c r="H165" t="s">
+        <v>16</v>
+      </c>
+      <c r="I165" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="166" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A166" t="s">
         <v>283</v>
       </c>
-      <c r="B165" t="s">
+      <c r="B166" t="s">
         <v>124</v>
       </c>
-      <c r="C165" s="2" t="s">
+      <c r="C166" s="2" t="s">
         <v>284</v>
       </c>
-      <c r="H165" t="s">
-        <v>16</v>
-      </c>
-      <c r="I165" t="s">
+      <c r="H166" t="s">
+        <v>16</v>
+      </c>
+      <c r="I166" t="s">
         <v>20</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:Q165">
+  <sortState ref="A2:Q166">
     <sortCondition ref="A2"/>
   </sortState>
   <hyperlinks>
     <hyperlink ref="C6" r:id="rId1"/>
-    <hyperlink ref="C60" r:id="rId2"/>
+    <hyperlink ref="C61" r:id="rId2"/>
     <hyperlink ref="C7" r:id="rId3"/>
-    <hyperlink ref="C10" r:id="rId4"/>
-    <hyperlink ref="C98" r:id="rId5"/>
-    <hyperlink ref="C118" r:id="rId6"/>
-    <hyperlink ref="C164" r:id="rId7"/>
-    <hyperlink ref="C35" r:id="rId8"/>
-    <hyperlink ref="C30" r:id="rId9"/>
-    <hyperlink ref="C51" r:id="rId10"/>
-    <hyperlink ref="C58" r:id="rId11"/>
+    <hyperlink ref="C11" r:id="rId4"/>
+    <hyperlink ref="C99" r:id="rId5"/>
+    <hyperlink ref="C119" r:id="rId6"/>
+    <hyperlink ref="C165" r:id="rId7"/>
+    <hyperlink ref="C36" r:id="rId8"/>
+    <hyperlink ref="C31" r:id="rId9"/>
+    <hyperlink ref="C52" r:id="rId10"/>
+    <hyperlink ref="C59" r:id="rId11"/>
     <hyperlink ref="C3" r:id="rId12"/>
-    <hyperlink ref="C20" r:id="rId13"/>
-    <hyperlink ref="C62" r:id="rId14"/>
-    <hyperlink ref="C90" r:id="rId15"/>
-    <hyperlink ref="C29" r:id="rId16"/>
-    <hyperlink ref="C114" r:id="rId17"/>
-    <hyperlink ref="C42" r:id="rId18"/>
-    <hyperlink ref="C75" r:id="rId19"/>
-    <hyperlink ref="C16" r:id="rId20"/>
-    <hyperlink ref="C152" r:id="rId21"/>
+    <hyperlink ref="C21" r:id="rId13"/>
+    <hyperlink ref="C63" r:id="rId14"/>
+    <hyperlink ref="C91" r:id="rId15"/>
+    <hyperlink ref="C30" r:id="rId16"/>
+    <hyperlink ref="C115" r:id="rId17"/>
+    <hyperlink ref="C43" r:id="rId18"/>
+    <hyperlink ref="C76" r:id="rId19"/>
+    <hyperlink ref="C17" r:id="rId20"/>
+    <hyperlink ref="C153" r:id="rId21"/>
     <hyperlink ref="C8" r:id="rId22"/>
-    <hyperlink ref="C39" r:id="rId23"/>
-    <hyperlink ref="C55" r:id="rId24"/>
-    <hyperlink ref="C52" r:id="rId25"/>
-    <hyperlink ref="C56" r:id="rId26"/>
-    <hyperlink ref="C57" r:id="rId27"/>
-    <hyperlink ref="C72" r:id="rId28"/>
-    <hyperlink ref="C95" r:id="rId29"/>
-    <hyperlink ref="C143" r:id="rId30"/>
-    <hyperlink ref="C101" r:id="rId31"/>
-    <hyperlink ref="C85" r:id="rId32"/>
-    <hyperlink ref="C107" r:id="rId33"/>
-    <hyperlink ref="C73" r:id="rId34"/>
-    <hyperlink ref="C17" r:id="rId35"/>
-    <hyperlink ref="C141" r:id="rId36"/>
-    <hyperlink ref="C15" r:id="rId37"/>
-    <hyperlink ref="C161" r:id="rId38"/>
-    <hyperlink ref="C89" r:id="rId39"/>
-    <hyperlink ref="C59" r:id="rId40"/>
-    <hyperlink ref="C124" r:id="rId41"/>
-    <hyperlink ref="C18" r:id="rId42"/>
-    <hyperlink ref="C53" r:id="rId43"/>
-    <hyperlink ref="C23" r:id="rId44"/>
-    <hyperlink ref="C115" r:id="rId45"/>
-    <hyperlink ref="C158" r:id="rId46"/>
-    <hyperlink ref="C27" r:id="rId47" display="http://comparativeconstitutionsproject.org/"/>
-    <hyperlink ref="C112" r:id="rId48"/>
-    <hyperlink ref="C154" r:id="rId49"/>
-    <hyperlink ref="C128" r:id="rId50"/>
-    <hyperlink ref="C122" r:id="rId51"/>
-    <hyperlink ref="C22" r:id="rId52"/>
-    <hyperlink ref="C116" r:id="rId53"/>
-    <hyperlink ref="C49" r:id="rId54"/>
-    <hyperlink ref="C79" r:id="rId55"/>
-    <hyperlink ref="C82" r:id="rId56"/>
-    <hyperlink ref="C113" r:id="rId57"/>
-    <hyperlink ref="C103" r:id="rId58"/>
-    <hyperlink ref="C132" r:id="rId59"/>
-    <hyperlink ref="C31" r:id="rId60"/>
-    <hyperlink ref="C145" r:id="rId61"/>
+    <hyperlink ref="C40" r:id="rId23"/>
+    <hyperlink ref="C56" r:id="rId24"/>
+    <hyperlink ref="C53" r:id="rId25"/>
+    <hyperlink ref="C57" r:id="rId26"/>
+    <hyperlink ref="C58" r:id="rId27"/>
+    <hyperlink ref="C73" r:id="rId28"/>
+    <hyperlink ref="C96" r:id="rId29"/>
+    <hyperlink ref="C144" r:id="rId30"/>
+    <hyperlink ref="C102" r:id="rId31"/>
+    <hyperlink ref="C86" r:id="rId32"/>
+    <hyperlink ref="C108" r:id="rId33"/>
+    <hyperlink ref="C74" r:id="rId34"/>
+    <hyperlink ref="C18" r:id="rId35"/>
+    <hyperlink ref="C142" r:id="rId36"/>
+    <hyperlink ref="C16" r:id="rId37"/>
+    <hyperlink ref="C162" r:id="rId38"/>
+    <hyperlink ref="C90" r:id="rId39"/>
+    <hyperlink ref="C60" r:id="rId40"/>
+    <hyperlink ref="C125" r:id="rId41"/>
+    <hyperlink ref="C19" r:id="rId42"/>
+    <hyperlink ref="C54" r:id="rId43"/>
+    <hyperlink ref="C24" r:id="rId44"/>
+    <hyperlink ref="C116" r:id="rId45"/>
+    <hyperlink ref="C159" r:id="rId46"/>
+    <hyperlink ref="C28" r:id="rId47" display="http://comparativeconstitutionsproject.org/"/>
+    <hyperlink ref="C113" r:id="rId48"/>
+    <hyperlink ref="C155" r:id="rId49"/>
+    <hyperlink ref="C129" r:id="rId50"/>
+    <hyperlink ref="C123" r:id="rId51"/>
+    <hyperlink ref="C23" r:id="rId52"/>
+    <hyperlink ref="C117" r:id="rId53"/>
+    <hyperlink ref="C50" r:id="rId54"/>
+    <hyperlink ref="C80" r:id="rId55"/>
+    <hyperlink ref="C83" r:id="rId56"/>
+    <hyperlink ref="C114" r:id="rId57"/>
+    <hyperlink ref="C104" r:id="rId58"/>
+    <hyperlink ref="C133" r:id="rId59"/>
+    <hyperlink ref="C32" r:id="rId60"/>
+    <hyperlink ref="C146" r:id="rId61"/>
     <hyperlink ref="C9" r:id="rId62"/>
-    <hyperlink ref="C33" r:id="rId63"/>
-    <hyperlink ref="C146" r:id="rId64"/>
-    <hyperlink ref="C14" r:id="rId65"/>
-    <hyperlink ref="C156" r:id="rId66"/>
-    <hyperlink ref="C25" r:id="rId67"/>
-    <hyperlink ref="C24" r:id="rId68"/>
-    <hyperlink ref="C26" r:id="rId69"/>
-    <hyperlink ref="C54" r:id="rId70"/>
-    <hyperlink ref="C159" r:id="rId71"/>
-    <hyperlink ref="C28" r:id="rId72"/>
-    <hyperlink ref="C119" r:id="rId73"/>
-    <hyperlink ref="C32" r:id="rId74"/>
-    <hyperlink ref="C46" r:id="rId75"/>
-    <hyperlink ref="C135" r:id="rId76"/>
-    <hyperlink ref="C43" r:id="rId77"/>
-    <hyperlink ref="C40" r:id="rId78"/>
-    <hyperlink ref="C70" r:id="rId79"/>
+    <hyperlink ref="C34" r:id="rId63"/>
+    <hyperlink ref="C147" r:id="rId64"/>
+    <hyperlink ref="C15" r:id="rId65"/>
+    <hyperlink ref="C157" r:id="rId66"/>
+    <hyperlink ref="C26" r:id="rId67"/>
+    <hyperlink ref="C25" r:id="rId68"/>
+    <hyperlink ref="C27" r:id="rId69"/>
+    <hyperlink ref="C55" r:id="rId70"/>
+    <hyperlink ref="C160" r:id="rId71"/>
+    <hyperlink ref="C29" r:id="rId72"/>
+    <hyperlink ref="C120" r:id="rId73"/>
+    <hyperlink ref="C33" r:id="rId74"/>
+    <hyperlink ref="C47" r:id="rId75"/>
+    <hyperlink ref="C136" r:id="rId76"/>
+    <hyperlink ref="C44" r:id="rId77"/>
+    <hyperlink ref="C41" r:id="rId78"/>
+    <hyperlink ref="C71" r:id="rId79"/>
     <hyperlink ref="C5" r:id="rId80"/>
-    <hyperlink ref="C69" r:id="rId81"/>
-    <hyperlink ref="C12" r:id="rId82"/>
-    <hyperlink ref="C111" r:id="rId83"/>
-    <hyperlink ref="C120" r:id="rId84"/>
-    <hyperlink ref="C148" r:id="rId85"/>
-    <hyperlink ref="C36" r:id="rId86"/>
-    <hyperlink ref="C157" r:id="rId87"/>
-    <hyperlink ref="C45" r:id="rId88"/>
-    <hyperlink ref="C163" r:id="rId89"/>
-    <hyperlink ref="C99" r:id="rId90"/>
-    <hyperlink ref="C67" r:id="rId91"/>
-    <hyperlink ref="C100" r:id="rId92"/>
-    <hyperlink ref="C138" r:id="rId93"/>
-    <hyperlink ref="C83" r:id="rId94"/>
-    <hyperlink ref="C105" r:id="rId95"/>
-    <hyperlink ref="C139" r:id="rId96"/>
-    <hyperlink ref="C63" r:id="rId97"/>
-    <hyperlink ref="C117" r:id="rId98"/>
-    <hyperlink ref="C47" r:id="rId99"/>
-    <hyperlink ref="C44" r:id="rId100"/>
-    <hyperlink ref="C86" r:id="rId101"/>
-    <hyperlink ref="C61" r:id="rId102"/>
+    <hyperlink ref="C70" r:id="rId81"/>
+    <hyperlink ref="C13" r:id="rId82"/>
+    <hyperlink ref="C112" r:id="rId83"/>
+    <hyperlink ref="C121" r:id="rId84"/>
+    <hyperlink ref="C149" r:id="rId85"/>
+    <hyperlink ref="C37" r:id="rId86"/>
+    <hyperlink ref="C158" r:id="rId87"/>
+    <hyperlink ref="C46" r:id="rId88"/>
+    <hyperlink ref="C164" r:id="rId89"/>
+    <hyperlink ref="C100" r:id="rId90"/>
+    <hyperlink ref="C68" r:id="rId91"/>
+    <hyperlink ref="C101" r:id="rId92"/>
+    <hyperlink ref="C139" r:id="rId93"/>
+    <hyperlink ref="C84" r:id="rId94"/>
+    <hyperlink ref="C106" r:id="rId95"/>
+    <hyperlink ref="C140" r:id="rId96"/>
+    <hyperlink ref="C64" r:id="rId97"/>
+    <hyperlink ref="C118" r:id="rId98"/>
+    <hyperlink ref="C48" r:id="rId99"/>
+    <hyperlink ref="C45" r:id="rId100"/>
+    <hyperlink ref="C87" r:id="rId101"/>
+    <hyperlink ref="C62" r:id="rId102"/>
     <hyperlink ref="C2" r:id="rId103"/>
-    <hyperlink ref="C80" r:id="rId104"/>
-    <hyperlink ref="C84" r:id="rId105"/>
-    <hyperlink ref="C109" r:id="rId106"/>
-    <hyperlink ref="C48" r:id="rId107"/>
-    <hyperlink ref="C87" r:id="rId108"/>
-    <hyperlink ref="C137" r:id="rId109"/>
-    <hyperlink ref="C13" r:id="rId110"/>
+    <hyperlink ref="C81" r:id="rId104"/>
+    <hyperlink ref="C85" r:id="rId105"/>
+    <hyperlink ref="C110" r:id="rId106"/>
+    <hyperlink ref="C49" r:id="rId107"/>
+    <hyperlink ref="C88" r:id="rId108"/>
+    <hyperlink ref="C138" r:id="rId109"/>
+    <hyperlink ref="C14" r:id="rId110"/>
     <hyperlink ref="C4" r:id="rId111"/>
-    <hyperlink ref="C162" r:id="rId112"/>
-    <hyperlink ref="C93" r:id="rId113"/>
-    <hyperlink ref="C88" r:id="rId114"/>
-    <hyperlink ref="C151" r:id="rId115"/>
-    <hyperlink ref="C131" r:id="rId116"/>
-    <hyperlink ref="C65" r:id="rId117"/>
-    <hyperlink ref="C102" r:id="rId118"/>
-    <hyperlink ref="C77" r:id="rId119"/>
-    <hyperlink ref="C165" r:id="rId120"/>
-    <hyperlink ref="C68" r:id="rId121"/>
-    <hyperlink ref="C130" r:id="rId122"/>
-    <hyperlink ref="C108" r:id="rId123"/>
-    <hyperlink ref="C81" r:id="rId124"/>
-    <hyperlink ref="C106" r:id="rId125"/>
-    <hyperlink ref="C136" r:id="rId126"/>
-    <hyperlink ref="C91" r:id="rId127"/>
-    <hyperlink ref="C11" r:id="rId128"/>
-    <hyperlink ref="C19" r:id="rId129"/>
-    <hyperlink ref="C129" r:id="rId130"/>
-    <hyperlink ref="C76" r:id="rId131"/>
-    <hyperlink ref="C144" r:id="rId132"/>
-    <hyperlink ref="C126" r:id="rId133"/>
-    <hyperlink ref="C125" r:id="rId134"/>
-    <hyperlink ref="C127" r:id="rId135"/>
-    <hyperlink ref="C150" r:id="rId136"/>
-    <hyperlink ref="C142" r:id="rId137"/>
-    <hyperlink ref="C155" r:id="rId138"/>
-    <hyperlink ref="C38" r:id="rId139"/>
-    <hyperlink ref="C92" r:id="rId140"/>
+    <hyperlink ref="C163" r:id="rId112"/>
+    <hyperlink ref="C94" r:id="rId113"/>
+    <hyperlink ref="C89" r:id="rId114"/>
+    <hyperlink ref="C152" r:id="rId115"/>
+    <hyperlink ref="C132" r:id="rId116"/>
+    <hyperlink ref="C66" r:id="rId117"/>
+    <hyperlink ref="C103" r:id="rId118"/>
+    <hyperlink ref="C78" r:id="rId119"/>
+    <hyperlink ref="C166" r:id="rId120"/>
+    <hyperlink ref="C69" r:id="rId121"/>
+    <hyperlink ref="C131" r:id="rId122"/>
+    <hyperlink ref="C109" r:id="rId123"/>
+    <hyperlink ref="C82" r:id="rId124"/>
+    <hyperlink ref="C107" r:id="rId125"/>
+    <hyperlink ref="C137" r:id="rId126"/>
+    <hyperlink ref="C92" r:id="rId127"/>
+    <hyperlink ref="C12" r:id="rId128"/>
+    <hyperlink ref="C20" r:id="rId129"/>
+    <hyperlink ref="C130" r:id="rId130"/>
+    <hyperlink ref="C77" r:id="rId131"/>
+    <hyperlink ref="C145" r:id="rId132"/>
+    <hyperlink ref="C127" r:id="rId133"/>
+    <hyperlink ref="C126" r:id="rId134"/>
+    <hyperlink ref="C128" r:id="rId135"/>
+    <hyperlink ref="C151" r:id="rId136"/>
+    <hyperlink ref="C143" r:id="rId137"/>
+    <hyperlink ref="C156" r:id="rId138"/>
+    <hyperlink ref="C39" r:id="rId139"/>
+    <hyperlink ref="C93" r:id="rId140"/>
     <hyperlink ref="J2" r:id="rId141"/>
     <hyperlink ref="M3" r:id="rId142"/>
     <hyperlink ref="J3" r:id="rId143"/>
@@ -5392,67 +5455,71 @@
     <hyperlink ref="J4" r:id="rId145"/>
     <hyperlink ref="P5" r:id="rId146"/>
     <hyperlink ref="J5" r:id="rId147"/>
-    <hyperlink ref="C110" r:id="rId148"/>
-    <hyperlink ref="C34" r:id="rId149"/>
+    <hyperlink ref="C111" r:id="rId148"/>
+    <hyperlink ref="C35" r:id="rId149"/>
     <hyperlink ref="P7" r:id="rId150"/>
     <hyperlink ref="J7" r:id="rId151"/>
     <hyperlink ref="M8" r:id="rId152"/>
     <hyperlink ref="L8" r:id="rId153"/>
     <hyperlink ref="J8" r:id="rId154"/>
-    <hyperlink ref="C153" r:id="rId155"/>
-    <hyperlink ref="N153" r:id="rId156"/>
-    <hyperlink ref="C21" r:id="rId157"/>
-    <hyperlink ref="N21" r:id="rId158"/>
-    <hyperlink ref="C64" r:id="rId159"/>
-    <hyperlink ref="C149" r:id="rId160"/>
-    <hyperlink ref="J149" r:id="rId161"/>
-    <hyperlink ref="C147" r:id="rId162"/>
-    <hyperlink ref="N147" r:id="rId163"/>
-    <hyperlink ref="J147" r:id="rId164"/>
-    <hyperlink ref="C96" r:id="rId165"/>
-    <hyperlink ref="C94" r:id="rId166"/>
-    <hyperlink ref="C41" r:id="rId167"/>
-    <hyperlink ref="J41" r:id="rId168"/>
-    <hyperlink ref="K41" r:id="rId169"/>
-    <hyperlink ref="C104" r:id="rId170"/>
-    <hyperlink ref="N104" r:id="rId171"/>
-    <hyperlink ref="C78" r:id="rId172"/>
-    <hyperlink ref="K78" r:id="rId173"/>
-    <hyperlink ref="C160" r:id="rId174"/>
-    <hyperlink ref="C121" r:id="rId175"/>
-    <hyperlink ref="K121" r:id="rId176"/>
+    <hyperlink ref="C154" r:id="rId155"/>
+    <hyperlink ref="N154" r:id="rId156"/>
+    <hyperlink ref="C22" r:id="rId157"/>
+    <hyperlink ref="N22" r:id="rId158"/>
+    <hyperlink ref="C65" r:id="rId159"/>
+    <hyperlink ref="C150" r:id="rId160"/>
+    <hyperlink ref="J150" r:id="rId161"/>
+    <hyperlink ref="C148" r:id="rId162"/>
+    <hyperlink ref="N148" r:id="rId163"/>
+    <hyperlink ref="J148" r:id="rId164"/>
+    <hyperlink ref="C97" r:id="rId165"/>
+    <hyperlink ref="C95" r:id="rId166"/>
+    <hyperlink ref="C42" r:id="rId167"/>
+    <hyperlink ref="J42" r:id="rId168"/>
+    <hyperlink ref="K42" r:id="rId169"/>
+    <hyperlink ref="C105" r:id="rId170"/>
+    <hyperlink ref="N105" r:id="rId171"/>
+    <hyperlink ref="C79" r:id="rId172"/>
+    <hyperlink ref="K79" r:id="rId173"/>
+    <hyperlink ref="C161" r:id="rId174"/>
+    <hyperlink ref="C122" r:id="rId175"/>
+    <hyperlink ref="K122" r:id="rId176"/>
     <hyperlink ref="L9" r:id="rId177"/>
     <hyperlink ref="J9" r:id="rId178"/>
-    <hyperlink ref="J10" r:id="rId179"/>
-    <hyperlink ref="C133" r:id="rId180"/>
-    <hyperlink ref="J133" r:id="rId181"/>
-    <hyperlink ref="L133" r:id="rId182"/>
-    <hyperlink ref="K133" r:id="rId183"/>
-    <hyperlink ref="C134" r:id="rId184"/>
-    <hyperlink ref="J134" r:id="rId185"/>
-    <hyperlink ref="K134" r:id="rId186"/>
-    <hyperlink ref="L134" r:id="rId187"/>
-    <hyperlink ref="C66" r:id="rId188"/>
-    <hyperlink ref="J66" r:id="rId189"/>
-    <hyperlink ref="N66" r:id="rId190"/>
-    <hyperlink ref="C140" r:id="rId191"/>
-    <hyperlink ref="C97" r:id="rId192"/>
-    <hyperlink ref="J97" r:id="rId193"/>
-    <hyperlink ref="L97" r:id="rId194"/>
-    <hyperlink ref="C74" r:id="rId195"/>
-    <hyperlink ref="C50" r:id="rId196"/>
-    <hyperlink ref="L50" r:id="rId197"/>
-    <hyperlink ref="K50" r:id="rId198"/>
-    <hyperlink ref="J50" r:id="rId199"/>
-    <hyperlink ref="C71" r:id="rId200"/>
-    <hyperlink ref="J71" r:id="rId201"/>
-    <hyperlink ref="K71" r:id="rId202"/>
-    <hyperlink ref="L71" r:id="rId203"/>
-    <hyperlink ref="C123" r:id="rId204"/>
-    <hyperlink ref="N123" r:id="rId205"/>
-    <hyperlink ref="C37" r:id="rId206"/>
-    <hyperlink ref="K37" r:id="rId207"/>
-    <hyperlink ref="J37" r:id="rId208"/>
+    <hyperlink ref="J11" r:id="rId179"/>
+    <hyperlink ref="C134" r:id="rId180"/>
+    <hyperlink ref="J134" r:id="rId181"/>
+    <hyperlink ref="L134" r:id="rId182"/>
+    <hyperlink ref="K134" r:id="rId183"/>
+    <hyperlink ref="C135" r:id="rId184"/>
+    <hyperlink ref="J135" r:id="rId185"/>
+    <hyperlink ref="K135" r:id="rId186"/>
+    <hyperlink ref="L135" r:id="rId187"/>
+    <hyperlink ref="C67" r:id="rId188"/>
+    <hyperlink ref="J67" r:id="rId189"/>
+    <hyperlink ref="N67" r:id="rId190"/>
+    <hyperlink ref="C141" r:id="rId191"/>
+    <hyperlink ref="C98" r:id="rId192"/>
+    <hyperlink ref="J98" r:id="rId193"/>
+    <hyperlink ref="L98" r:id="rId194"/>
+    <hyperlink ref="C75" r:id="rId195"/>
+    <hyperlink ref="C51" r:id="rId196"/>
+    <hyperlink ref="L51" r:id="rId197"/>
+    <hyperlink ref="K51" r:id="rId198"/>
+    <hyperlink ref="J51" r:id="rId199"/>
+    <hyperlink ref="C72" r:id="rId200"/>
+    <hyperlink ref="J72" r:id="rId201"/>
+    <hyperlink ref="K72" r:id="rId202"/>
+    <hyperlink ref="L72" r:id="rId203"/>
+    <hyperlink ref="C124" r:id="rId204"/>
+    <hyperlink ref="N124" r:id="rId205"/>
+    <hyperlink ref="C38" r:id="rId206"/>
+    <hyperlink ref="K38" r:id="rId207"/>
+    <hyperlink ref="J38" r:id="rId208"/>
+    <hyperlink ref="C10" r:id="rId209"/>
+    <hyperlink ref="J10" r:id="rId210"/>
+    <hyperlink ref="P10" r:id="rId211"/>
+    <hyperlink ref="N10" r:id="rId212"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
add Democracy Crossnational Data
</commit_message>
<xml_diff>
--- a/PolData.xlsx
+++ b/PolData.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="888" uniqueCount="488">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="899" uniqueCount="496">
   <si>
     <t>name</t>
   </si>
@@ -1491,6 +1491,30 @@
   </si>
   <si>
     <t>csv in zip file</t>
+  </si>
+  <si>
+    <t>https://sites.hks.harvard.edu/fs/pnorris/Data/Data.htm</t>
+  </si>
+  <si>
+    <t>Democracy Crossnational Data</t>
+  </si>
+  <si>
+    <t>191 countries</t>
+  </si>
+  <si>
+    <t>https://sites.hks.harvard.edu/fs/pnorris/Data/Democracy%20CrossNational%20Data/Democracy%20Crossnational%20Codebook%20March%202009.pdf</t>
+  </si>
+  <si>
+    <t>https://sites.hks.harvard.edu/fs/pnorris/Data/Democracy%20CrossNational%20Data/Democracy%20Crossnational%20Data%20Spring%202009.csv</t>
+  </si>
+  <si>
+    <t>https://sites.hks.harvard.edu/fs/pnorris/Data/Democracy%20CrossNational%20Data/Democracy%20Crossnational%20Data%20Spring%202009%20StataSE.dta</t>
+  </si>
+  <si>
+    <t>https://sites.hks.harvard.edu/fs/pnorris/Data/Democracy%20CrossNational%20Data/Democracy%20Crossnational%20Data%20Spring%202009.sav</t>
+  </si>
+  <si>
+    <t>https://sites.hks.harvard.edu/fs/pnorris/Data/Democracy%20CrossNational%20Data/Democracy%20Crossnational%20Data%20Spring%202009%20Excel.xlsx</t>
   </si>
 </sst>
 </file>
@@ -1830,10 +1854,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q166"/>
+  <dimension ref="A1:Q167"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A143" workbookViewId="0">
-      <selection activeCell="A166" sqref="A166"/>
+    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="A43" sqref="A43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2599,7 +2623,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>187</v>
       </c>
@@ -2622,7 +2646,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>164</v>
       </c>
@@ -2633,7 +2657,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>371</v>
       </c>
@@ -2659,7 +2683,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>39</v>
       </c>
@@ -2685,7 +2709,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>215</v>
       </c>
@@ -2705,7 +2729,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>476</v>
       </c>
@@ -2737,7 +2761,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>330</v>
       </c>
@@ -2760,7 +2784,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>75</v>
       </c>
@@ -2777,7 +2801,7 @@
         <v>1971</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>197</v>
       </c>
@@ -2803,7 +2827,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>409</v>
       </c>
@@ -2829,114 +2853,132 @@
         <v>412</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>59</v>
+        <v>489</v>
       </c>
       <c r="B43" t="s">
         <v>60</v>
       </c>
       <c r="C43" s="2" t="s">
+        <v>488</v>
+      </c>
+      <c r="E43" t="s">
+        <v>490</v>
+      </c>
+      <c r="H43" t="s">
+        <v>348</v>
+      </c>
+      <c r="I43" t="s">
+        <v>349</v>
+      </c>
+      <c r="J43" s="2" t="s">
+        <v>491</v>
+      </c>
+      <c r="K43" s="2" t="s">
+        <v>492</v>
+      </c>
+      <c r="L43" s="2" t="s">
+        <v>493</v>
+      </c>
+      <c r="M43" s="2" t="s">
+        <v>494</v>
+      </c>
+      <c r="N43" s="2" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>59</v>
+      </c>
+      <c r="B44" t="s">
+        <v>60</v>
+      </c>
+      <c r="C44" s="2" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A44" t="s">
+    <row r="45" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
         <v>196</v>
       </c>
-      <c r="B44" t="s">
+      <c r="B45" t="s">
         <v>165</v>
       </c>
-      <c r="C44" s="2" t="s">
+      <c r="C45" s="2" t="s">
         <v>195</v>
       </c>
-      <c r="F44">
+      <c r="F45">
         <v>1946</v>
       </c>
-      <c r="G44">
+      <c r="G45">
         <v>2016</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A45" t="s">
+    <row r="46" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
         <v>238</v>
       </c>
-      <c r="B45" t="s">
+      <c r="B46" t="s">
         <v>237</v>
       </c>
-      <c r="C45" s="2" t="s">
+      <c r="C46" s="2" t="s">
         <v>243</v>
       </c>
-      <c r="H45" t="s">
-        <v>16</v>
-      </c>
-      <c r="I45" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A46" t="s">
+      <c r="H46" t="s">
+        <v>16</v>
+      </c>
+      <c r="I46" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
         <v>219</v>
       </c>
-      <c r="B46" t="s">
+      <c r="B47" t="s">
         <v>124</v>
       </c>
-      <c r="C46" s="2" t="s">
+      <c r="C47" s="2" t="s">
         <v>218</v>
       </c>
-      <c r="F46">
+      <c r="F47">
         <v>1970</v>
       </c>
-      <c r="G46">
+      <c r="G47">
         <v>2015</v>
       </c>
-      <c r="H46" t="s">
-        <v>16</v>
-      </c>
-      <c r="I46" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A47" t="s">
+      <c r="H47" t="s">
+        <v>16</v>
+      </c>
+      <c r="I47" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
         <v>191</v>
       </c>
-      <c r="B47" t="s">
+      <c r="B48" t="s">
         <v>25</v>
       </c>
-      <c r="C47" s="2" t="s">
+      <c r="C48" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="E47" t="s">
+      <c r="E48" t="s">
         <v>192</v>
-      </c>
-    </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A48" t="s">
-        <v>235</v>
-      </c>
-      <c r="B48" t="s">
-        <v>60</v>
-      </c>
-      <c r="C48" s="2" t="s">
-        <v>236</v>
-      </c>
-      <c r="H48" t="s">
-        <v>16</v>
-      </c>
-      <c r="I48" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="49" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>252</v>
+        <v>235</v>
       </c>
       <c r="B49" t="s">
-        <v>250</v>
+        <v>60</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>251</v>
+        <v>236</v>
       </c>
       <c r="H49" t="s">
         <v>16</v>
@@ -2947,129 +2989,129 @@
     </row>
     <row r="50" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>149</v>
+        <v>252</v>
       </c>
       <c r="B50" t="s">
-        <v>128</v>
+        <v>250</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>150</v>
+        <v>251</v>
+      </c>
+      <c r="H50" t="s">
+        <v>16</v>
+      </c>
+      <c r="I50" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="51" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>462</v>
+        <v>149</v>
       </c>
       <c r="B51" t="s">
-        <v>250</v>
+        <v>128</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>464</v>
-      </c>
-      <c r="D51" t="s">
-        <v>463</v>
-      </c>
-      <c r="E51" t="s">
-        <v>14</v>
-      </c>
-      <c r="F51">
-        <v>1946</v>
-      </c>
-      <c r="G51">
-        <v>2010</v>
-      </c>
-      <c r="H51" t="s">
-        <v>348</v>
-      </c>
-      <c r="I51" t="s">
-        <v>349</v>
-      </c>
-      <c r="J51" s="2" t="s">
-        <v>467</v>
-      </c>
-      <c r="K51" s="2" t="s">
-        <v>466</v>
-      </c>
-      <c r="L51" s="2" t="s">
-        <v>465</v>
+        <v>150</v>
       </c>
     </row>
     <row r="52" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>28</v>
+        <v>462</v>
       </c>
       <c r="B52" t="s">
-        <v>25</v>
+        <v>250</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>48</v>
+        <v>464</v>
+      </c>
+      <c r="D52" t="s">
+        <v>463</v>
+      </c>
+      <c r="E52" t="s">
+        <v>14</v>
+      </c>
+      <c r="F52">
+        <v>1946</v>
+      </c>
+      <c r="G52">
+        <v>2010</v>
+      </c>
+      <c r="H52" t="s">
+        <v>348</v>
+      </c>
+      <c r="I52" t="s">
+        <v>349</v>
+      </c>
+      <c r="J52" s="2" t="s">
+        <v>467</v>
+      </c>
+      <c r="K52" s="2" t="s">
+        <v>466</v>
+      </c>
+      <c r="L52" s="2" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="53" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>80</v>
+        <v>28</v>
       </c>
       <c r="B53" t="s">
-        <v>128</v>
+        <v>25</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="E53" t="s">
-        <v>9</v>
-      </c>
-      <c r="F53">
-        <v>1979</v>
+        <v>48</v>
       </c>
     </row>
     <row r="54" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>125</v>
+        <v>80</v>
       </c>
       <c r="B54" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>126</v>
+        <v>81</v>
+      </c>
+      <c r="E54" t="s">
+        <v>9</v>
+      </c>
+      <c r="F54">
+        <v>1979</v>
       </c>
     </row>
     <row r="55" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>179</v>
+        <v>125</v>
       </c>
       <c r="B55" t="s">
-        <v>165</v>
+        <v>124</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>180</v>
+        <v>126</v>
       </c>
     </row>
     <row r="56" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
+        <v>179</v>
+      </c>
+      <c r="B56" t="s">
+        <v>165</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="57" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
         <v>78</v>
       </c>
-      <c r="B56" t="s">
+      <c r="B57" t="s">
         <v>25</v>
       </c>
-      <c r="C56" s="2" t="s">
+      <c r="C57" s="2" t="s">
         <v>79</v>
-      </c>
-      <c r="E56" t="s">
-        <v>9</v>
-      </c>
-      <c r="F56">
-        <v>1979</v>
-      </c>
-    </row>
-    <row r="57" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A57" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="B57" t="s">
-        <v>83</v>
-      </c>
-      <c r="C57" s="2" t="s">
-        <v>84</v>
       </c>
       <c r="E57" t="s">
         <v>9</v>
@@ -3080,13 +3122,13 @@
     </row>
     <row r="58" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A58" s="3" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B58" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="E58" t="s">
         <v>9</v>
@@ -3094,225 +3136,225 @@
       <c r="F58">
         <v>1979</v>
       </c>
-      <c r="G58">
+    </row>
+    <row r="59" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A59" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="B59" t="s">
+        <v>86</v>
+      </c>
+      <c r="C59" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="E59" t="s">
+        <v>9</v>
+      </c>
+      <c r="F59">
+        <v>1979</v>
+      </c>
+      <c r="G59">
         <v>2009</v>
-      </c>
-    </row>
-    <row r="59" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A59" t="s">
-        <v>27</v>
-      </c>
-      <c r="B59" t="s">
-        <v>25</v>
-      </c>
-      <c r="C59" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="Q59" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="60" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>120</v>
+        <v>27</v>
       </c>
       <c r="B60" t="s">
-        <v>259</v>
+        <v>25</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="I60" t="s">
-        <v>20</v>
+        <v>49</v>
+      </c>
+      <c r="Q60" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="61" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>5</v>
+        <v>120</v>
       </c>
       <c r="B61" t="s">
-        <v>25</v>
+        <v>259</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D61" t="s">
-        <v>94</v>
-      </c>
-      <c r="E61" t="s">
-        <v>9</v>
-      </c>
-      <c r="F61">
-        <v>2002</v>
-      </c>
-      <c r="H61" t="s">
-        <v>16</v>
+        <v>119</v>
       </c>
       <c r="I61" t="s">
-        <v>248</v>
-      </c>
-      <c r="Q61" t="s">
-        <v>44</v>
+        <v>20</v>
       </c>
     </row>
     <row r="62" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
+        <v>5</v>
+      </c>
+      <c r="B62" t="s">
+        <v>25</v>
+      </c>
+      <c r="C62" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D62" t="s">
+        <v>94</v>
+      </c>
+      <c r="E62" t="s">
+        <v>9</v>
+      </c>
+      <c r="F62">
+        <v>2002</v>
+      </c>
+      <c r="H62" t="s">
+        <v>16</v>
+      </c>
+      <c r="I62" t="s">
+        <v>248</v>
+      </c>
+      <c r="Q62" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="63" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
         <v>240</v>
       </c>
-      <c r="B62" t="s">
+      <c r="B63" t="s">
         <v>237</v>
       </c>
-      <c r="C62" s="2" t="s">
+      <c r="C63" s="2" t="s">
         <v>243</v>
       </c>
-      <c r="H62" t="s">
-        <v>16</v>
-      </c>
-      <c r="I62" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="63" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A63" s="1" t="s">
+      <c r="H63" t="s">
+        <v>16</v>
+      </c>
+      <c r="I63" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="64" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A64" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B63" t="s">
+      <c r="B64" t="s">
         <v>25</v>
       </c>
-      <c r="C63" s="2" t="s">
+      <c r="C64" s="2" t="s">
         <v>52</v>
-      </c>
-    </row>
-    <row r="64" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A64" t="s">
-        <v>232</v>
-      </c>
-      <c r="B64" t="s">
-        <v>250</v>
-      </c>
-      <c r="C64" s="2" t="s">
-        <v>231</v>
       </c>
     </row>
     <row r="65" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>390</v>
+        <v>232</v>
       </c>
       <c r="B65" t="s">
-        <v>83</v>
+        <v>250</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>392</v>
-      </c>
-      <c r="D65" t="s">
-        <v>391</v>
-      </c>
-      <c r="E65" t="s">
-        <v>9</v>
-      </c>
-      <c r="F65">
-        <v>2007</v>
-      </c>
-      <c r="G65">
-        <v>2015</v>
-      </c>
-      <c r="H65" t="s">
-        <v>348</v>
-      </c>
-      <c r="I65" t="s">
-        <v>349</v>
-      </c>
-      <c r="Q65" t="s">
-        <v>393</v>
+        <v>231</v>
       </c>
     </row>
     <row r="66" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>276</v>
+        <v>390</v>
       </c>
       <c r="B66" t="s">
-        <v>124</v>
+        <v>83</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>277</v>
+        <v>392</v>
+      </c>
+      <c r="D66" t="s">
+        <v>391</v>
+      </c>
+      <c r="E66" t="s">
+        <v>9</v>
       </c>
       <c r="F66">
-        <v>1948</v>
+        <v>2007</v>
       </c>
       <c r="G66">
-        <v>2000</v>
+        <v>2015</v>
       </c>
       <c r="H66" t="s">
-        <v>16</v>
+        <v>348</v>
       </c>
       <c r="I66" t="s">
-        <v>20</v>
+        <v>349</v>
+      </c>
+      <c r="Q66" t="s">
+        <v>393</v>
       </c>
     </row>
     <row r="67" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>449</v>
+        <v>276</v>
       </c>
       <c r="B67" t="s">
-        <v>250</v>
+        <v>124</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>448</v>
-      </c>
-      <c r="E67" t="s">
-        <v>14</v>
+        <v>277</v>
       </c>
       <c r="F67">
-        <v>-4000</v>
+        <v>1948</v>
       </c>
       <c r="G67">
         <v>2000</v>
       </c>
       <c r="H67" t="s">
-        <v>348</v>
+        <v>16</v>
       </c>
       <c r="I67" t="s">
-        <v>349</v>
-      </c>
-      <c r="J67" s="2" t="s">
-        <v>450</v>
-      </c>
-      <c r="N67" s="2" t="s">
-        <v>451</v>
+        <v>20</v>
       </c>
     </row>
     <row r="68" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>224</v>
+        <v>449</v>
       </c>
       <c r="B68" t="s">
-        <v>40</v>
+        <v>250</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>225</v>
+        <v>448</v>
+      </c>
+      <c r="E68" t="s">
+        <v>14</v>
       </c>
       <c r="F68">
-        <v>1964</v>
+        <v>-4000</v>
       </c>
       <c r="G68">
-        <v>2008</v>
+        <v>2000</v>
       </c>
       <c r="H68" t="s">
-        <v>16</v>
+        <v>348</v>
       </c>
       <c r="I68" t="s">
-        <v>20</v>
+        <v>349</v>
+      </c>
+      <c r="J68" s="2" t="s">
+        <v>450</v>
+      </c>
+      <c r="N68" s="2" t="s">
+        <v>451</v>
       </c>
     </row>
     <row r="69" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>285</v>
+        <v>224</v>
       </c>
       <c r="B69" t="s">
-        <v>250</v>
+        <v>40</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>286</v>
+        <v>225</v>
+      </c>
+      <c r="F69">
+        <v>1964</v>
+      </c>
+      <c r="G69">
+        <v>2008</v>
       </c>
       <c r="H69" t="s">
         <v>16</v>
@@ -3323,259 +3365,259 @@
     </row>
     <row r="70" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>205</v>
+        <v>285</v>
       </c>
       <c r="B70" t="s">
-        <v>40</v>
+        <v>250</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>204</v>
-      </c>
-      <c r="F70">
-        <v>2006</v>
+        <v>286</v>
+      </c>
+      <c r="H70" t="s">
+        <v>16</v>
+      </c>
+      <c r="I70" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="71" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>200</v>
+        <v>205</v>
       </c>
       <c r="B71" t="s">
-        <v>99</v>
+        <v>40</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="F71">
-        <v>1980</v>
-      </c>
-      <c r="G71">
-        <v>2007</v>
-      </c>
-      <c r="Q71" t="s">
-        <v>18</v>
+        <v>2006</v>
       </c>
     </row>
     <row r="72" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>468</v>
+        <v>200</v>
       </c>
       <c r="B72" t="s">
-        <v>40</v>
+        <v>99</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>464</v>
-      </c>
-      <c r="E72" t="s">
-        <v>14</v>
+        <v>201</v>
       </c>
       <c r="F72">
-        <v>1816</v>
+        <v>1980</v>
       </c>
       <c r="G72">
-        <v>2001</v>
-      </c>
-      <c r="H72" t="s">
-        <v>348</v>
-      </c>
-      <c r="I72" t="s">
-        <v>349</v>
-      </c>
-      <c r="J72" s="2" t="s">
-        <v>469</v>
-      </c>
-      <c r="K72" s="2" t="s">
-        <v>470</v>
-      </c>
-      <c r="L72" s="2" t="s">
-        <v>471</v>
+        <v>2007</v>
+      </c>
+      <c r="Q72" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="73" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>89</v>
+        <v>468</v>
       </c>
       <c r="B73" t="s">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>88</v>
+        <v>464</v>
       </c>
       <c r="E73" t="s">
-        <v>34</v>
+        <v>14</v>
       </c>
       <c r="F73">
-        <v>1972</v>
+        <v>1816</v>
+      </c>
+      <c r="G73">
+        <v>2001</v>
       </c>
       <c r="H73" t="s">
-        <v>16</v>
+        <v>348</v>
       </c>
       <c r="I73" t="s">
-        <v>20</v>
+        <v>349</v>
+      </c>
+      <c r="J73" s="2" t="s">
+        <v>469</v>
+      </c>
+      <c r="K73" s="2" t="s">
+        <v>470</v>
+      </c>
+      <c r="L73" s="2" t="s">
+        <v>471</v>
       </c>
     </row>
     <row r="74" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>104</v>
+        <v>89</v>
       </c>
       <c r="B74" t="s">
         <v>25</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>106</v>
+        <v>88</v>
       </c>
       <c r="E74" t="s">
-        <v>105</v>
+        <v>34</v>
       </c>
       <c r="F74">
-        <v>1980</v>
+        <v>1972</v>
+      </c>
+      <c r="H74" t="s">
+        <v>16</v>
+      </c>
+      <c r="I74" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="75" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>460</v>
+        <v>104</v>
       </c>
       <c r="B75" t="s">
         <v>25</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>461</v>
-      </c>
-      <c r="D75" t="s">
-        <v>363</v>
+        <v>106</v>
       </c>
       <c r="E75" t="s">
         <v>105</v>
       </c>
       <c r="F75">
-        <v>2009</v>
-      </c>
-      <c r="H75" t="s">
-        <v>348</v>
-      </c>
-      <c r="I75" t="s">
-        <v>301</v>
+        <v>1980</v>
       </c>
     </row>
     <row r="76" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>62</v>
+        <v>460</v>
       </c>
       <c r="B76" t="s">
         <v>25</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>63</v>
+        <v>461</v>
+      </c>
+      <c r="D76" t="s">
+        <v>363</v>
+      </c>
+      <c r="E76" t="s">
+        <v>105</v>
+      </c>
+      <c r="F76">
+        <v>2009</v>
+      </c>
+      <c r="H76" t="s">
+        <v>348</v>
+      </c>
+      <c r="I76" t="s">
+        <v>301</v>
       </c>
     </row>
     <row r="77" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>311</v>
+        <v>62</v>
       </c>
       <c r="B77" t="s">
-        <v>165</v>
+        <v>25</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>312</v>
-      </c>
-      <c r="E77" t="s">
-        <v>14</v>
-      </c>
-      <c r="H77" t="s">
-        <v>16</v>
-      </c>
-      <c r="I77" t="s">
-        <v>301</v>
+        <v>63</v>
       </c>
     </row>
     <row r="78" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>281</v>
+        <v>311</v>
       </c>
       <c r="B78" t="s">
-        <v>237</v>
+        <v>165</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>282</v>
+        <v>312</v>
+      </c>
+      <c r="E78" t="s">
+        <v>14</v>
       </c>
       <c r="H78" t="s">
         <v>16</v>
       </c>
       <c r="I78" t="s">
-        <v>20</v>
+        <v>301</v>
       </c>
     </row>
     <row r="79" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>418</v>
+        <v>281</v>
       </c>
       <c r="B79" t="s">
-        <v>86</v>
+        <v>237</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>419</v>
-      </c>
-      <c r="E79" t="s">
-        <v>420</v>
-      </c>
-      <c r="F79">
-        <v>1948</v>
-      </c>
-      <c r="G79">
-        <v>2012</v>
+        <v>282</v>
       </c>
       <c r="H79" t="s">
-        <v>348</v>
+        <v>16</v>
       </c>
       <c r="I79" t="s">
-        <v>349</v>
-      </c>
-      <c r="K79" s="2" t="s">
-        <v>421</v>
-      </c>
-      <c r="Q79" t="s">
-        <v>422</v>
+        <v>20</v>
       </c>
     </row>
     <row r="80" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>151</v>
+        <v>418</v>
       </c>
       <c r="B80" t="s">
-        <v>40</v>
+        <v>86</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>152</v>
+        <v>419</v>
       </c>
       <c r="E80" t="s">
-        <v>14</v>
+        <v>420</v>
+      </c>
+      <c r="F80">
+        <v>1948</v>
+      </c>
+      <c r="G80">
+        <v>2012</v>
+      </c>
+      <c r="H80" t="s">
+        <v>348</v>
+      </c>
+      <c r="I80" t="s">
+        <v>349</v>
+      </c>
+      <c r="K80" s="2" t="s">
+        <v>421</v>
+      </c>
+      <c r="Q80" t="s">
+        <v>422</v>
       </c>
     </row>
     <row r="81" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>242</v>
+        <v>151</v>
       </c>
       <c r="B81" t="s">
-        <v>237</v>
+        <v>40</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>243</v>
-      </c>
-      <c r="H81" t="s">
-        <v>16</v>
-      </c>
-      <c r="I81" t="s">
-        <v>20</v>
+        <v>152</v>
+      </c>
+      <c r="E81" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="82" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>292</v>
+        <v>242</v>
       </c>
       <c r="B82" t="s">
-        <v>99</v>
+        <v>237</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>291</v>
+        <v>243</v>
       </c>
       <c r="H82" t="s">
         <v>16</v>
@@ -3586,47 +3628,47 @@
     </row>
     <row r="83" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>153</v>
+        <v>292</v>
       </c>
       <c r="B83" t="s">
-        <v>259</v>
+        <v>99</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>154</v>
+        <v>291</v>
+      </c>
+      <c r="H83" t="s">
+        <v>16</v>
+      </c>
+      <c r="I83" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="84" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>228</v>
+        <v>153</v>
       </c>
       <c r="B84" t="s">
-        <v>40</v>
+        <v>259</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>225</v>
-      </c>
-      <c r="F84">
-        <v>1989</v>
-      </c>
-      <c r="G84">
-        <v>2017</v>
-      </c>
-      <c r="H84" t="s">
-        <v>16</v>
-      </c>
-      <c r="I84" t="s">
-        <v>20</v>
+        <v>154</v>
       </c>
     </row>
     <row r="85" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>245</v>
+        <v>228</v>
       </c>
       <c r="B85" t="s">
-        <v>237</v>
+        <v>40</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>244</v>
+        <v>225</v>
+      </c>
+      <c r="F85">
+        <v>1989</v>
+      </c>
+      <c r="G85">
+        <v>2017</v>
       </c>
       <c r="H85" t="s">
         <v>16</v>
@@ -3637,50 +3679,41 @@
     </row>
     <row r="86" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>100</v>
+        <v>245</v>
       </c>
       <c r="B86" t="s">
-        <v>99</v>
+        <v>237</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>101</v>
+        <v>244</v>
+      </c>
+      <c r="H86" t="s">
+        <v>16</v>
+      </c>
+      <c r="I86" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="87" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>239</v>
+        <v>100</v>
       </c>
       <c r="B87" t="s">
-        <v>237</v>
+        <v>99</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>243</v>
-      </c>
-      <c r="H87" t="s">
-        <v>16</v>
-      </c>
-      <c r="I87" t="s">
-        <v>20</v>
+        <v>101</v>
       </c>
     </row>
     <row r="88" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>254</v>
+        <v>239</v>
       </c>
       <c r="B88" t="s">
-        <v>55</v>
+        <v>237</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>253</v>
-      </c>
-      <c r="E88" t="s">
-        <v>255</v>
-      </c>
-      <c r="F88">
-        <v>1960</v>
-      </c>
-      <c r="G88">
-        <v>2014</v>
+        <v>243</v>
       </c>
       <c r="H88" t="s">
         <v>16</v>
@@ -3691,19 +3724,22 @@
     </row>
     <row r="89" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>270</v>
+        <v>254</v>
       </c>
       <c r="B89" t="s">
         <v>55</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>271</v>
+        <v>253</v>
+      </c>
+      <c r="E89" t="s">
+        <v>255</v>
       </c>
       <c r="F89">
-        <v>1990</v>
+        <v>1960</v>
       </c>
       <c r="G89">
-        <v>2010</v>
+        <v>2014</v>
       </c>
       <c r="H89" t="s">
         <v>16</v>
@@ -3714,96 +3750,90 @@
     </row>
     <row r="90" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>117</v>
+        <v>270</v>
       </c>
       <c r="B90" t="s">
         <v>55</v>
       </c>
       <c r="C90" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="F90">
+        <v>1990</v>
+      </c>
+      <c r="G90">
+        <v>2010</v>
+      </c>
+      <c r="H90" t="s">
+        <v>16</v>
+      </c>
+      <c r="I90" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="91" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A91" t="s">
+        <v>117</v>
+      </c>
+      <c r="B91" t="s">
+        <v>55</v>
+      </c>
+      <c r="C91" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="I90" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q90" t="s">
+      <c r="I91" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q91" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="91" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A91" s="1" t="s">
+    <row r="92" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A92" s="1" t="s">
         <v>23</v>
-      </c>
-      <c r="B91" t="s">
-        <v>25</v>
-      </c>
-      <c r="C91" s="2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="92" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A92" t="s">
-        <v>300</v>
       </c>
       <c r="B92" t="s">
         <v>25</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>298</v>
-      </c>
-      <c r="E92" t="s">
-        <v>299</v>
-      </c>
-      <c r="F92">
-        <v>1969</v>
-      </c>
-      <c r="H92" t="s">
-        <v>16</v>
-      </c>
-      <c r="I92" t="s">
-        <v>249</v>
+        <v>53</v>
       </c>
     </row>
     <row r="93" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>332</v>
+        <v>300</v>
       </c>
       <c r="B93" t="s">
-        <v>134</v>
+        <v>25</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>333</v>
+        <v>298</v>
       </c>
       <c r="E93" t="s">
-        <v>334</v>
+        <v>299</v>
+      </c>
+      <c r="F93">
+        <v>1969</v>
       </c>
       <c r="H93" t="s">
         <v>16</v>
       </c>
       <c r="I93" t="s">
-        <v>20</v>
+        <v>249</v>
       </c>
     </row>
     <row r="94" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>267</v>
+        <v>332</v>
       </c>
       <c r="B94" t="s">
-        <v>250</v>
+        <v>134</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>266</v>
-      </c>
-      <c r="D94" t="s">
-        <v>269</v>
+        <v>333</v>
       </c>
       <c r="E94" t="s">
-        <v>268</v>
-      </c>
-      <c r="F94">
-        <v>1970</v>
-      </c>
-      <c r="G94">
-        <v>2014</v>
+        <v>334</v>
       </c>
       <c r="H94" t="s">
         <v>16</v>
@@ -3814,97 +3844,100 @@
     </row>
     <row r="95" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>407</v>
+        <v>267</v>
       </c>
       <c r="B95" t="s">
-        <v>40</v>
+        <v>250</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>406</v>
+        <v>266</v>
       </c>
       <c r="D95" t="s">
-        <v>408</v>
+        <v>269</v>
       </c>
       <c r="E95" t="s">
-        <v>14</v>
+        <v>268</v>
       </c>
       <c r="F95">
-        <v>1949</v>
+        <v>1970</v>
       </c>
       <c r="G95">
-        <v>2013</v>
+        <v>2014</v>
       </c>
       <c r="H95" t="s">
-        <v>348</v>
+        <v>16</v>
       </c>
       <c r="I95" t="s">
-        <v>349</v>
+        <v>20</v>
       </c>
     </row>
     <row r="96" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>96</v>
+        <v>407</v>
       </c>
       <c r="B96" t="s">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>90</v>
+        <v>406</v>
+      </c>
+      <c r="D96" t="s">
+        <v>408</v>
       </c>
       <c r="E96" t="s">
-        <v>69</v>
+        <v>14</v>
       </c>
       <c r="F96">
-        <v>1995</v>
+        <v>1949</v>
+      </c>
+      <c r="G96">
+        <v>2013</v>
+      </c>
+      <c r="H96" t="s">
+        <v>348</v>
+      </c>
+      <c r="I96" t="s">
+        <v>349</v>
       </c>
     </row>
     <row r="97" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>404</v>
+        <v>96</v>
       </c>
       <c r="B97" t="s">
-        <v>83</v>
+        <v>25</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>403</v>
-      </c>
-      <c r="D97" t="s">
-        <v>405</v>
+        <v>90</v>
       </c>
       <c r="E97" t="s">
-        <v>14</v>
+        <v>69</v>
       </c>
       <c r="F97">
-        <v>1875</v>
-      </c>
-      <c r="G97">
-        <v>2004</v>
-      </c>
-      <c r="H97" t="s">
-        <v>348</v>
-      </c>
-      <c r="I97" t="s">
-        <v>349</v>
+        <v>1995</v>
       </c>
     </row>
     <row r="98" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>454</v>
+        <v>404</v>
       </c>
       <c r="B98" t="s">
-        <v>25</v>
+        <v>83</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>455</v>
+        <v>403</v>
+      </c>
+      <c r="D98" t="s">
+        <v>405</v>
       </c>
       <c r="E98" t="s">
-        <v>456</v>
+        <v>14</v>
       </c>
       <c r="F98">
-        <v>2006</v>
+        <v>1875</v>
       </c>
       <c r="G98">
-        <v>2016</v>
+        <v>2004</v>
       </c>
       <c r="H98" t="s">
         <v>348</v>
@@ -3912,80 +3945,83 @@
       <c r="I98" t="s">
         <v>349</v>
       </c>
-      <c r="J98" s="2" t="s">
-        <v>457</v>
-      </c>
-      <c r="L98" s="2" t="s">
-        <v>458</v>
-      </c>
-      <c r="Q98" t="s">
-        <v>459</v>
-      </c>
     </row>
     <row r="99" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>11</v>
+        <v>454</v>
       </c>
       <c r="B99" t="s">
         <v>25</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D99" t="s">
-        <v>95</v>
+        <v>455</v>
       </c>
       <c r="E99" t="s">
-        <v>10</v>
+        <v>456</v>
       </c>
       <c r="F99">
-        <v>2007</v>
+        <v>2006</v>
+      </c>
+      <c r="G99">
+        <v>2016</v>
       </c>
       <c r="H99" t="s">
-        <v>16</v>
+        <v>348</v>
       </c>
       <c r="I99" t="s">
-        <v>21</v>
+        <v>349</v>
+      </c>
+      <c r="J99" s="2" t="s">
+        <v>457</v>
+      </c>
+      <c r="L99" s="2" t="s">
+        <v>458</v>
+      </c>
+      <c r="Q99" t="s">
+        <v>459</v>
       </c>
     </row>
     <row r="100" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>223</v>
+        <v>11</v>
       </c>
       <c r="B100" t="s">
-        <v>124</v>
+        <v>25</v>
       </c>
       <c r="C100" s="2" t="s">
-        <v>222</v>
+        <v>12</v>
+      </c>
+      <c r="D100" t="s">
+        <v>95</v>
+      </c>
+      <c r="E100" t="s">
+        <v>10</v>
       </c>
       <c r="F100">
-        <v>1</v>
-      </c>
-      <c r="G100">
-        <v>2010</v>
+        <v>2007</v>
       </c>
       <c r="H100" t="s">
         <v>16</v>
       </c>
       <c r="I100" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="101" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="B101" t="s">
-        <v>40</v>
+        <v>124</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="F101">
-        <v>1946</v>
+        <v>1</v>
       </c>
       <c r="G101">
-        <v>2016</v>
+        <v>2010</v>
       </c>
       <c r="H101" t="s">
         <v>16</v>
@@ -3996,122 +4032,122 @@
     </row>
     <row r="102" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>97</v>
+        <v>226</v>
       </c>
       <c r="B102" t="s">
-        <v>128</v>
+        <v>40</v>
       </c>
       <c r="C102" s="2" t="s">
-        <v>98</v>
+        <v>225</v>
+      </c>
+      <c r="F102">
+        <v>1946</v>
+      </c>
+      <c r="G102">
+        <v>2016</v>
+      </c>
+      <c r="H102" t="s">
+        <v>16</v>
+      </c>
+      <c r="I102" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="103" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>278</v>
+        <v>97</v>
       </c>
       <c r="B103" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="C103" s="2" t="s">
-        <v>279</v>
-      </c>
-      <c r="E103" t="s">
-        <v>280</v>
-      </c>
-      <c r="F103">
-        <v>1890</v>
-      </c>
-      <c r="G103">
-        <v>1996</v>
-      </c>
-      <c r="H103" t="s">
-        <v>16</v>
-      </c>
-      <c r="I103" t="s">
-        <v>20</v>
+        <v>98</v>
       </c>
     </row>
     <row r="104" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>156</v>
+        <v>278</v>
       </c>
       <c r="B104" t="s">
-        <v>25</v>
+        <v>124</v>
       </c>
       <c r="C104" s="2" t="s">
-        <v>154</v>
+        <v>279</v>
+      </c>
+      <c r="E104" t="s">
+        <v>280</v>
+      </c>
+      <c r="F104">
+        <v>1890</v>
+      </c>
+      <c r="G104">
+        <v>1996</v>
+      </c>
+      <c r="H104" t="s">
+        <v>16</v>
+      </c>
+      <c r="I104" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="105" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>413</v>
+        <v>156</v>
       </c>
       <c r="B105" t="s">
-        <v>128</v>
+        <v>25</v>
       </c>
       <c r="C105" s="2" t="s">
-        <v>414</v>
-      </c>
-      <c r="E105" t="s">
-        <v>415</v>
-      </c>
-      <c r="F105">
-        <v>1946</v>
-      </c>
-      <c r="G105">
-        <v>2014</v>
-      </c>
-      <c r="H105" t="s">
-        <v>348</v>
-      </c>
-      <c r="I105" t="s">
-        <v>349</v>
-      </c>
-      <c r="N105" s="2" t="s">
-        <v>416</v>
-      </c>
-      <c r="Q105" t="s">
-        <v>417</v>
+        <v>154</v>
       </c>
     </row>
     <row r="106" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>229</v>
+        <v>413</v>
       </c>
       <c r="B106" t="s">
-        <v>40</v>
+        <v>128</v>
       </c>
       <c r="C106" s="2" t="s">
-        <v>225</v>
+        <v>414</v>
+      </c>
+      <c r="E106" t="s">
+        <v>415</v>
       </c>
       <c r="F106">
-        <v>1952</v>
+        <v>1946</v>
       </c>
       <c r="G106">
-        <v>1997</v>
+        <v>2014</v>
       </c>
       <c r="H106" t="s">
-        <v>16</v>
+        <v>348</v>
       </c>
       <c r="I106" t="s">
-        <v>20</v>
+        <v>349</v>
+      </c>
+      <c r="N106" s="2" t="s">
+        <v>416</v>
+      </c>
+      <c r="Q106" t="s">
+        <v>417</v>
       </c>
     </row>
     <row r="107" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>293</v>
+        <v>229</v>
       </c>
       <c r="B107" t="s">
         <v>40</v>
       </c>
       <c r="C107" s="2" t="s">
-        <v>294</v>
+        <v>225</v>
       </c>
       <c r="F107">
-        <v>2004</v>
+        <v>1952</v>
       </c>
       <c r="G107">
-        <v>2006</v>
+        <v>1997</v>
       </c>
       <c r="H107" t="s">
         <v>16</v>
@@ -4122,221 +4158,218 @@
     </row>
     <row r="108" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>102</v>
+        <v>293</v>
       </c>
       <c r="B108" t="s">
-        <v>99</v>
+        <v>40</v>
       </c>
       <c r="C108" s="2" t="s">
-        <v>103</v>
+        <v>294</v>
+      </c>
+      <c r="F108">
+        <v>2004</v>
+      </c>
+      <c r="G108">
+        <v>2006</v>
+      </c>
+      <c r="H108" t="s">
+        <v>16</v>
+      </c>
+      <c r="I108" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="109" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>289</v>
+        <v>102</v>
       </c>
       <c r="B109" t="s">
-        <v>124</v>
+        <v>99</v>
       </c>
       <c r="C109" s="2" t="s">
-        <v>290</v>
+        <v>103</v>
       </c>
     </row>
     <row r="110" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>246</v>
+        <v>289</v>
       </c>
       <c r="B110" t="s">
-        <v>165</v>
+        <v>124</v>
       </c>
       <c r="C110" s="2" t="s">
-        <v>247</v>
-      </c>
-      <c r="E110" t="s">
-        <v>14</v>
-      </c>
-      <c r="F110">
-        <v>1960</v>
-      </c>
-      <c r="G110">
-        <v>2006</v>
-      </c>
-      <c r="H110" t="s">
-        <v>16</v>
-      </c>
-      <c r="I110" t="s">
-        <v>249</v>
+        <v>290</v>
       </c>
     </row>
     <row r="111" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>365</v>
+        <v>246</v>
       </c>
       <c r="B111" t="s">
-        <v>128</v>
+        <v>165</v>
       </c>
       <c r="C111" s="2" t="s">
-        <v>364</v>
-      </c>
-      <c r="D111" t="s">
-        <v>370</v>
+        <v>247</v>
       </c>
       <c r="E111" t="s">
-        <v>366</v>
+        <v>14</v>
       </c>
       <c r="F111">
-        <v>1906</v>
+        <v>1960</v>
       </c>
       <c r="G111">
-        <v>2013</v>
+        <v>2006</v>
       </c>
       <c r="H111" t="s">
-        <v>367</v>
+        <v>16</v>
       </c>
       <c r="I111" t="s">
-        <v>368</v>
-      </c>
-      <c r="Q111" t="s">
-        <v>369</v>
+        <v>249</v>
       </c>
     </row>
     <row r="112" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>208</v>
+        <v>365</v>
       </c>
       <c r="B112" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="C112" s="2" t="s">
-        <v>209</v>
+        <v>364</v>
+      </c>
+      <c r="D112" t="s">
+        <v>370</v>
+      </c>
+      <c r="E112" t="s">
+        <v>366</v>
       </c>
       <c r="F112">
-        <v>1932</v>
+        <v>1906</v>
       </c>
       <c r="G112">
-        <v>2014</v>
+        <v>2013</v>
       </c>
       <c r="H112" t="s">
-        <v>16</v>
+        <v>367</v>
       </c>
       <c r="I112" t="s">
-        <v>20</v>
+        <v>368</v>
+      </c>
+      <c r="Q112" t="s">
+        <v>369</v>
       </c>
     </row>
     <row r="113" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>137</v>
+        <v>208</v>
       </c>
       <c r="B113" t="s">
-        <v>259</v>
+        <v>124</v>
       </c>
       <c r="C113" s="2" t="s">
-        <v>138</v>
+        <v>209</v>
+      </c>
+      <c r="F113">
+        <v>1932</v>
+      </c>
+      <c r="G113">
+        <v>2014</v>
+      </c>
+      <c r="H113" t="s">
+        <v>16</v>
+      </c>
+      <c r="I113" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="114" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>155</v>
+        <v>137</v>
       </c>
       <c r="B114" t="s">
         <v>259</v>
       </c>
       <c r="C114" s="2" t="s">
-        <v>154</v>
+        <v>138</v>
       </c>
     </row>
     <row r="115" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>57</v>
+        <v>155</v>
       </c>
       <c r="B115" t="s">
-        <v>128</v>
+        <v>259</v>
       </c>
       <c r="C115" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="Q115" t="s">
-        <v>17</v>
+        <v>154</v>
       </c>
     </row>
     <row r="116" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>129</v>
+        <v>57</v>
       </c>
       <c r="B116" t="s">
-        <v>259</v>
+        <v>128</v>
       </c>
       <c r="C116" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="E116" t="s">
-        <v>131</v>
-      </c>
-      <c r="F116">
-        <v>1945</v>
-      </c>
-      <c r="G116">
-        <v>2008</v>
-      </c>
-      <c r="I116" t="s">
-        <v>20</v>
+        <v>58</v>
+      </c>
+      <c r="Q116" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="117" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>148</v>
+        <v>129</v>
       </c>
       <c r="B117" t="s">
-        <v>128</v>
+        <v>259</v>
       </c>
       <c r="C117" s="2" t="s">
-        <v>147</v>
+        <v>130</v>
+      </c>
+      <c r="E117" t="s">
+        <v>131</v>
+      </c>
+      <c r="F117">
+        <v>1945</v>
+      </c>
+      <c r="G117">
+        <v>2008</v>
+      </c>
+      <c r="I117" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="118" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>233</v>
+        <v>148</v>
       </c>
       <c r="B118" t="s">
-        <v>165</v>
+        <v>128</v>
       </c>
       <c r="C118" s="2" t="s">
-        <v>234</v>
-      </c>
-      <c r="E118" t="s">
-        <v>14</v>
-      </c>
-      <c r="F118">
-        <v>2012</v>
-      </c>
-      <c r="G118">
-        <v>2016</v>
-      </c>
-      <c r="H118" t="s">
-        <v>16</v>
-      </c>
-      <c r="I118" t="s">
-        <v>20</v>
+        <v>147</v>
       </c>
     </row>
     <row r="119" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>35</v>
+        <v>233</v>
       </c>
       <c r="B119" t="s">
-        <v>25</v>
+        <v>165</v>
       </c>
       <c r="C119" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="D119" t="s">
-        <v>37</v>
+        <v>234</v>
       </c>
       <c r="E119" t="s">
         <v>14</v>
       </c>
       <c r="F119">
-        <v>2001</v>
+        <v>2012</v>
+      </c>
+      <c r="G119">
+        <v>2016</v>
       </c>
       <c r="H119" t="s">
         <v>16</v>
@@ -4347,148 +4380,148 @@
     </row>
     <row r="120" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>185</v>
+        <v>35</v>
       </c>
       <c r="B120" t="s">
-        <v>128</v>
+        <v>25</v>
       </c>
       <c r="C120" s="2" t="s">
-        <v>186</v>
+        <v>36</v>
+      </c>
+      <c r="D120" t="s">
+        <v>37</v>
+      </c>
+      <c r="E120" t="s">
+        <v>14</v>
+      </c>
+      <c r="F120">
+        <v>2001</v>
+      </c>
+      <c r="H120" t="s">
+        <v>16</v>
+      </c>
+      <c r="I120" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="121" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>210</v>
+        <v>185</v>
       </c>
       <c r="B121" t="s">
-        <v>40</v>
+        <v>128</v>
       </c>
       <c r="C121" s="2" t="s">
-        <v>211</v>
-      </c>
-      <c r="F121">
-        <v>1976</v>
-      </c>
-      <c r="G121">
-        <v>2016</v>
-      </c>
-      <c r="H121" t="s">
-        <v>16</v>
-      </c>
-      <c r="I121" t="s">
-        <v>20</v>
+        <v>186</v>
       </c>
     </row>
     <row r="122" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>426</v>
+        <v>210</v>
       </c>
       <c r="B122" t="s">
-        <v>86</v>
+        <v>40</v>
       </c>
       <c r="C122" s="2" t="s">
-        <v>427</v>
-      </c>
-      <c r="E122" t="s">
-        <v>34</v>
+        <v>211</v>
       </c>
       <c r="F122">
-        <v>2015</v>
+        <v>1976</v>
       </c>
       <c r="G122">
         <v>2016</v>
       </c>
       <c r="H122" t="s">
-        <v>348</v>
+        <v>16</v>
       </c>
       <c r="I122" t="s">
-        <v>349</v>
-      </c>
-      <c r="K122" s="2" t="s">
-        <v>428</v>
+        <v>20</v>
       </c>
     </row>
     <row r="123" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>144</v>
+        <v>426</v>
       </c>
       <c r="B123" t="s">
-        <v>60</v>
+        <v>86</v>
       </c>
       <c r="C123" s="2" t="s">
-        <v>143</v>
+        <v>427</v>
+      </c>
+      <c r="E123" t="s">
+        <v>34</v>
       </c>
       <c r="F123">
-        <v>1800</v>
+        <v>2015</v>
       </c>
       <c r="G123">
-        <v>2013</v>
+        <v>2016</v>
+      </c>
+      <c r="H123" t="s">
+        <v>348</v>
+      </c>
+      <c r="I123" t="s">
+        <v>349</v>
+      </c>
+      <c r="K123" s="2" t="s">
+        <v>428</v>
       </c>
     </row>
     <row r="124" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>472</v>
+        <v>144</v>
       </c>
       <c r="B124" t="s">
-        <v>25</v>
+        <v>60</v>
       </c>
       <c r="C124" s="2" t="s">
-        <v>473</v>
-      </c>
-      <c r="D124" t="s">
-        <v>474</v>
-      </c>
-      <c r="E124" t="s">
-        <v>112</v>
+        <v>143</v>
       </c>
       <c r="F124">
-        <v>1943</v>
-      </c>
-      <c r="H124" t="s">
-        <v>348</v>
-      </c>
-      <c r="I124" t="s">
-        <v>349</v>
-      </c>
-      <c r="N124" s="2" t="s">
-        <v>475</v>
+        <v>1800</v>
+      </c>
+      <c r="G124">
+        <v>2013</v>
       </c>
     </row>
     <row r="125" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>122</v>
+        <v>472</v>
       </c>
       <c r="B125" t="s">
-        <v>259</v>
+        <v>25</v>
       </c>
       <c r="C125" s="2" t="s">
-        <v>121</v>
+        <v>473</v>
+      </c>
+      <c r="D125" t="s">
+        <v>474</v>
+      </c>
+      <c r="E125" t="s">
+        <v>112</v>
+      </c>
+      <c r="F125">
+        <v>1943</v>
+      </c>
+      <c r="H125" t="s">
+        <v>348</v>
       </c>
       <c r="I125" t="s">
-        <v>20</v>
+        <v>349</v>
+      </c>
+      <c r="N125" s="2" t="s">
+        <v>475</v>
       </c>
     </row>
     <row r="126" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>318</v>
+        <v>122</v>
       </c>
       <c r="B126" t="s">
-        <v>250</v>
+        <v>259</v>
       </c>
       <c r="C126" s="2" t="s">
-        <v>319</v>
-      </c>
-      <c r="E126" t="s">
-        <v>320</v>
-      </c>
-      <c r="F126">
-        <v>1975</v>
-      </c>
-      <c r="G126">
-        <v>1989</v>
-      </c>
-      <c r="H126" t="s">
-        <v>16</v>
+        <v>121</v>
       </c>
       <c r="I126" t="s">
         <v>20</v>
@@ -4496,22 +4529,22 @@
     </row>
     <row r="127" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="B127" t="s">
         <v>250</v>
       </c>
       <c r="C127" s="2" t="s">
-        <v>317</v>
+        <v>319</v>
       </c>
       <c r="E127" t="s">
-        <v>105</v>
+        <v>320</v>
       </c>
       <c r="F127">
-        <v>1950</v>
+        <v>1975</v>
       </c>
       <c r="G127">
-        <v>1996</v>
+        <v>1989</v>
       </c>
       <c r="H127" t="s">
         <v>16</v>
@@ -4522,19 +4555,22 @@
     </row>
     <row r="128" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>322</v>
+        <v>316</v>
       </c>
       <c r="B128" t="s">
-        <v>25</v>
+        <v>250</v>
       </c>
       <c r="C128" s="2" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="E128" t="s">
-        <v>77</v>
+        <v>105</v>
       </c>
       <c r="F128">
-        <v>2010</v>
+        <v>1950</v>
+      </c>
+      <c r="G128">
+        <v>1996</v>
       </c>
       <c r="H128" t="s">
         <v>16</v>
@@ -4545,121 +4581,118 @@
     </row>
     <row r="129" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>141</v>
+        <v>322</v>
       </c>
       <c r="B129" t="s">
-        <v>237</v>
+        <v>25</v>
       </c>
       <c r="C129" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="Q129" t="s">
-        <v>17</v>
+        <v>321</v>
+      </c>
+      <c r="E129" t="s">
+        <v>77</v>
+      </c>
+      <c r="F129">
+        <v>2010</v>
+      </c>
+      <c r="H129" t="s">
+        <v>16</v>
+      </c>
+      <c r="I129" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="130" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
-        <v>308</v>
+        <v>141</v>
       </c>
       <c r="B130" t="s">
-        <v>250</v>
+        <v>237</v>
       </c>
       <c r="C130" s="2" t="s">
-        <v>309</v>
-      </c>
-      <c r="E130" t="s">
-        <v>310</v>
-      </c>
-      <c r="F130">
-        <v>1950</v>
-      </c>
-      <c r="G130">
-        <v>2010</v>
-      </c>
-      <c r="H130" t="s">
-        <v>16</v>
-      </c>
-      <c r="I130" t="s">
-        <v>20</v>
+        <v>142</v>
+      </c>
+      <c r="Q130" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="131" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>287</v>
+        <v>308</v>
       </c>
       <c r="B131" t="s">
-        <v>134</v>
+        <v>250</v>
       </c>
       <c r="C131" s="2" t="s">
-        <v>288</v>
+        <v>309</v>
+      </c>
+      <c r="E131" t="s">
+        <v>310</v>
       </c>
       <c r="F131">
-        <v>1990</v>
+        <v>1950</v>
       </c>
       <c r="G131">
-        <v>2008</v>
+        <v>2010</v>
+      </c>
+      <c r="H131" t="s">
+        <v>16</v>
+      </c>
+      <c r="I131" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="132" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>274</v>
+        <v>287</v>
       </c>
       <c r="B132" t="s">
-        <v>55</v>
+        <v>134</v>
       </c>
       <c r="C132" s="2" t="s">
-        <v>275</v>
-      </c>
-      <c r="H132" t="s">
-        <v>16</v>
-      </c>
-      <c r="I132" t="s">
-        <v>20</v>
+        <v>288</v>
+      </c>
+      <c r="F132">
+        <v>1990</v>
+      </c>
+      <c r="G132">
+        <v>2008</v>
       </c>
     </row>
     <row r="133" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
-        <v>157</v>
+        <v>274</v>
       </c>
       <c r="B133" t="s">
-        <v>128</v>
+        <v>55</v>
       </c>
       <c r="C133" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="Q133" t="s">
-        <v>18</v>
+        <v>275</v>
+      </c>
+      <c r="H133" t="s">
+        <v>16</v>
+      </c>
+      <c r="I133" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="134" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
-        <v>439</v>
+        <v>157</v>
       </c>
       <c r="B134" t="s">
-        <v>259</v>
+        <v>128</v>
       </c>
       <c r="C134" s="2" t="s">
-        <v>438</v>
-      </c>
-      <c r="H134" t="s">
-        <v>348</v>
-      </c>
-      <c r="I134" t="s">
-        <v>349</v>
-      </c>
-      <c r="J134" s="2" t="s">
-        <v>440</v>
-      </c>
-      <c r="K134" s="2" t="s">
-        <v>442</v>
-      </c>
-      <c r="L134" s="2" t="s">
-        <v>441</v>
+        <v>154</v>
+      </c>
+      <c r="Q134" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="135" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
-        <v>443</v>
+        <v>439</v>
       </c>
       <c r="B135" t="s">
         <v>259</v>
@@ -4667,15 +4700,6 @@
       <c r="C135" s="2" t="s">
         <v>438</v>
       </c>
-      <c r="D135" t="s">
-        <v>447</v>
-      </c>
-      <c r="F135">
-        <v>1990</v>
-      </c>
-      <c r="G135">
-        <v>2014</v>
-      </c>
       <c r="H135" t="s">
         <v>348</v>
       </c>
@@ -4683,87 +4707,99 @@
         <v>349</v>
       </c>
       <c r="J135" s="2" t="s">
-        <v>444</v>
+        <v>440</v>
       </c>
       <c r="K135" s="2" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
       <c r="L135" s="2" t="s">
-        <v>446</v>
+        <v>441</v>
       </c>
     </row>
     <row r="136" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
-        <v>194</v>
+        <v>443</v>
       </c>
       <c r="B136" t="s">
-        <v>99</v>
+        <v>259</v>
       </c>
       <c r="C136" s="2" t="s">
-        <v>193</v>
+        <v>438</v>
+      </c>
+      <c r="D136" t="s">
+        <v>447</v>
+      </c>
+      <c r="F136">
+        <v>1990</v>
+      </c>
+      <c r="G136">
+        <v>2014</v>
+      </c>
+      <c r="H136" t="s">
+        <v>348</v>
+      </c>
+      <c r="I136" t="s">
+        <v>349</v>
+      </c>
+      <c r="J136" s="2" t="s">
+        <v>444</v>
+      </c>
+      <c r="K136" s="2" t="s">
+        <v>445</v>
+      </c>
+      <c r="L136" s="2" t="s">
+        <v>446</v>
       </c>
     </row>
     <row r="137" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
-        <v>295</v>
+        <v>194</v>
       </c>
       <c r="B137" t="s">
-        <v>40</v>
+        <v>99</v>
       </c>
       <c r="C137" s="2" t="s">
-        <v>296</v>
-      </c>
-      <c r="E137" t="s">
-        <v>297</v>
-      </c>
-      <c r="F137">
-        <v>1990</v>
-      </c>
-      <c r="G137">
-        <v>2015</v>
-      </c>
-      <c r="H137" t="s">
-        <v>16</v>
-      </c>
-      <c r="I137" t="s">
-        <v>249</v>
+        <v>193</v>
       </c>
     </row>
     <row r="138" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
-        <v>256</v>
+        <v>295</v>
       </c>
       <c r="B138" t="s">
-        <v>250</v>
+        <v>40</v>
       </c>
       <c r="C138" s="2" t="s">
-        <v>257</v>
+        <v>296</v>
       </c>
       <c r="E138" t="s">
-        <v>258</v>
+        <v>297</v>
+      </c>
+      <c r="F138">
+        <v>1990</v>
+      </c>
+      <c r="G138">
+        <v>2015</v>
       </c>
       <c r="H138" t="s">
         <v>16</v>
       </c>
       <c r="I138" t="s">
-        <v>20</v>
+        <v>249</v>
       </c>
     </row>
     <row r="139" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
-        <v>227</v>
+        <v>256</v>
       </c>
       <c r="B139" t="s">
-        <v>40</v>
+        <v>250</v>
       </c>
       <c r="C139" s="2" t="s">
-        <v>225</v>
-      </c>
-      <c r="F139">
-        <v>1955</v>
-      </c>
-      <c r="G139">
-        <v>2016</v>
+        <v>257</v>
+      </c>
+      <c r="E139" t="s">
+        <v>258</v>
       </c>
       <c r="H139" t="s">
         <v>16</v>
@@ -4774,7 +4810,7 @@
     </row>
     <row r="140" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="B140" t="s">
         <v>40</v>
@@ -4783,7 +4819,7 @@
         <v>225</v>
       </c>
       <c r="F140">
-        <v>1995</v>
+        <v>1955</v>
       </c>
       <c r="G140">
         <v>2016</v>
@@ -4797,248 +4833,248 @@
     </row>
     <row r="141" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
-        <v>452</v>
+        <v>230</v>
       </c>
       <c r="B141" t="s">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="C141" s="2" t="s">
-        <v>453</v>
-      </c>
-      <c r="E141" t="s">
-        <v>9</v>
+        <v>225</v>
+      </c>
+      <c r="F141">
+        <v>1995</v>
+      </c>
+      <c r="G141">
+        <v>2016</v>
       </c>
       <c r="H141" t="s">
-        <v>348</v>
+        <v>16</v>
       </c>
       <c r="I141" t="s">
-        <v>435</v>
+        <v>20</v>
       </c>
     </row>
     <row r="142" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
-        <v>109</v>
+        <v>452</v>
       </c>
       <c r="B142" t="s">
         <v>25</v>
       </c>
       <c r="C142" s="2" t="s">
-        <v>110</v>
+        <v>453</v>
       </c>
       <c r="E142" t="s">
-        <v>111</v>
-      </c>
-      <c r="F142">
-        <v>1956</v>
+        <v>9</v>
+      </c>
+      <c r="H142" t="s">
+        <v>348</v>
+      </c>
+      <c r="I142" t="s">
+        <v>435</v>
       </c>
     </row>
     <row r="143" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
-        <v>326</v>
+        <v>109</v>
       </c>
       <c r="B143" t="s">
         <v>25</v>
       </c>
       <c r="C143" s="2" t="s">
-        <v>327</v>
+        <v>110</v>
       </c>
       <c r="E143" t="s">
         <v>111</v>
       </c>
       <c r="F143">
-        <v>1998</v>
-      </c>
-      <c r="H143" t="s">
-        <v>16</v>
-      </c>
-      <c r="I143" t="s">
-        <v>20</v>
+        <v>1956</v>
       </c>
     </row>
     <row r="144" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
-        <v>91</v>
+        <v>326</v>
       </c>
       <c r="B144" t="s">
         <v>25</v>
       </c>
       <c r="C144" s="2" t="s">
-        <v>93</v>
+        <v>327</v>
       </c>
       <c r="E144" t="s">
-        <v>92</v>
+        <v>111</v>
       </c>
       <c r="F144">
-        <v>1999</v>
+        <v>1998</v>
+      </c>
+      <c r="H144" t="s">
+        <v>16</v>
+      </c>
+      <c r="I144" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="145" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
-        <v>314</v>
+        <v>91</v>
       </c>
       <c r="B145" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="C145" s="2" t="s">
-        <v>313</v>
+        <v>93</v>
       </c>
       <c r="E145" t="s">
-        <v>315</v>
+        <v>92</v>
       </c>
       <c r="F145">
-        <v>1950</v>
-      </c>
-      <c r="G145">
-        <v>2004</v>
-      </c>
-      <c r="H145" t="s">
-        <v>16</v>
-      </c>
-      <c r="I145" t="s">
-        <v>20</v>
+        <v>1999</v>
       </c>
     </row>
     <row r="146" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
-        <v>161</v>
+        <v>314</v>
       </c>
       <c r="B146" t="s">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="C146" s="2" t="s">
-        <v>160</v>
+        <v>313</v>
+      </c>
+      <c r="E146" t="s">
+        <v>315</v>
+      </c>
+      <c r="F146">
+        <v>1950</v>
+      </c>
+      <c r="G146">
+        <v>2004</v>
+      </c>
+      <c r="H146" t="s">
+        <v>16</v>
+      </c>
+      <c r="I146" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="147" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="B147" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="C147" s="2" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
     </row>
     <row r="148" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
-        <v>399</v>
+        <v>168</v>
       </c>
       <c r="B148" t="s">
         <v>40</v>
       </c>
       <c r="C148" s="2" t="s">
-        <v>400</v>
-      </c>
-      <c r="E148" t="s">
-        <v>14</v>
-      </c>
-      <c r="F148">
-        <v>2000</v>
-      </c>
-      <c r="G148">
-        <v>2014</v>
-      </c>
-      <c r="H148" t="s">
-        <v>348</v>
-      </c>
-      <c r="I148" t="s">
-        <v>349</v>
-      </c>
-      <c r="J148" s="2" t="s">
-        <v>402</v>
-      </c>
-      <c r="N148" s="2" t="s">
-        <v>401</v>
+        <v>167</v>
       </c>
     </row>
     <row r="149" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
-        <v>213</v>
+        <v>399</v>
       </c>
       <c r="B149" t="s">
-        <v>55</v>
+        <v>40</v>
       </c>
       <c r="C149" s="2" t="s">
-        <v>212</v>
+        <v>400</v>
+      </c>
+      <c r="E149" t="s">
+        <v>14</v>
+      </c>
+      <c r="F149">
+        <v>2000</v>
+      </c>
+      <c r="G149">
+        <v>2014</v>
       </c>
       <c r="H149" t="s">
-        <v>16</v>
+        <v>348</v>
       </c>
       <c r="I149" t="s">
-        <v>20</v>
+        <v>349</v>
+      </c>
+      <c r="J149" s="2" t="s">
+        <v>402</v>
+      </c>
+      <c r="N149" s="2" t="s">
+        <v>401</v>
       </c>
     </row>
     <row r="150" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
-        <v>395</v>
+        <v>213</v>
       </c>
       <c r="B150" t="s">
-        <v>25</v>
+        <v>55</v>
       </c>
       <c r="C150" s="2" t="s">
-        <v>394</v>
-      </c>
-      <c r="D150" t="s">
-        <v>396</v>
-      </c>
-      <c r="E150" t="s">
-        <v>111</v>
-      </c>
-      <c r="F150">
-        <v>1986</v>
-      </c>
-      <c r="G150">
-        <v>2015</v>
+        <v>212</v>
       </c>
       <c r="H150" t="s">
-        <v>367</v>
+        <v>16</v>
       </c>
       <c r="I150" t="s">
-        <v>398</v>
-      </c>
-      <c r="J150" s="2" t="s">
-        <v>397</v>
+        <v>20</v>
       </c>
     </row>
     <row r="151" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
-        <v>323</v>
+        <v>395</v>
       </c>
       <c r="B151" t="s">
         <v>25</v>
       </c>
       <c r="C151" s="2" t="s">
-        <v>324</v>
+        <v>394</v>
+      </c>
+      <c r="D151" t="s">
+        <v>396</v>
       </c>
       <c r="E151" t="s">
-        <v>325</v>
+        <v>111</v>
       </c>
       <c r="F151">
-        <v>1942</v>
+        <v>1986</v>
+      </c>
+      <c r="G151">
+        <v>2015</v>
       </c>
       <c r="H151" t="s">
-        <v>16</v>
+        <v>367</v>
       </c>
       <c r="I151" t="s">
-        <v>20</v>
+        <v>398</v>
+      </c>
+      <c r="J151" s="2" t="s">
+        <v>397</v>
       </c>
     </row>
     <row r="152" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
-        <v>273</v>
+        <v>323</v>
       </c>
       <c r="B152" t="s">
-        <v>237</v>
+        <v>25</v>
       </c>
       <c r="C152" s="2" t="s">
-        <v>272</v>
+        <v>324</v>
+      </c>
+      <c r="E152" t="s">
+        <v>325</v>
       </c>
       <c r="F152">
-        <v>1996</v>
-      </c>
-      <c r="G152">
-        <v>2016</v>
+        <v>1942</v>
       </c>
       <c r="H152" t="s">
         <v>16</v>
@@ -5049,209 +5085,212 @@
     </row>
     <row r="153" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
-        <v>66</v>
+        <v>273</v>
       </c>
       <c r="B153" t="s">
-        <v>25</v>
+        <v>237</v>
       </c>
       <c r="C153" s="2" t="s">
-        <v>67</v>
+        <v>272</v>
+      </c>
+      <c r="F153">
+        <v>1996</v>
+      </c>
+      <c r="G153">
+        <v>2016</v>
+      </c>
+      <c r="H153" t="s">
+        <v>16</v>
+      </c>
+      <c r="I153" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="154" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
-        <v>383</v>
+        <v>66</v>
       </c>
       <c r="B154" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="C154" s="2" t="s">
-        <v>384</v>
-      </c>
-      <c r="E154" t="s">
-        <v>386</v>
-      </c>
-      <c r="F154">
-        <v>1951</v>
-      </c>
-      <c r="H154" t="s">
-        <v>348</v>
-      </c>
-      <c r="I154" t="s">
-        <v>349</v>
-      </c>
-      <c r="N154" s="2" t="s">
-        <v>385</v>
+        <v>67</v>
       </c>
     </row>
     <row r="155" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
-        <v>139</v>
+        <v>383</v>
       </c>
       <c r="B155" t="s">
         <v>40</v>
       </c>
       <c r="C155" s="2" t="s">
-        <v>140</v>
+        <v>384</v>
+      </c>
+      <c r="E155" t="s">
+        <v>386</v>
+      </c>
+      <c r="F155">
+        <v>1951</v>
+      </c>
+      <c r="H155" t="s">
+        <v>348</v>
+      </c>
+      <c r="I155" t="s">
+        <v>349</v>
+      </c>
+      <c r="N155" s="2" t="s">
+        <v>385</v>
       </c>
     </row>
     <row r="156" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
-        <v>329</v>
+        <v>139</v>
       </c>
       <c r="B156" t="s">
-        <v>165</v>
+        <v>40</v>
       </c>
       <c r="C156" s="2" t="s">
-        <v>328</v>
-      </c>
-      <c r="E156" t="s">
-        <v>34</v>
-      </c>
-      <c r="F156">
-        <v>1789</v>
-      </c>
-      <c r="H156" t="s">
-        <v>16</v>
-      </c>
-      <c r="I156" t="s">
-        <v>20</v>
+        <v>140</v>
       </c>
     </row>
     <row r="157" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
-        <v>172</v>
+        <v>329</v>
       </c>
       <c r="B157" t="s">
-        <v>60</v>
+        <v>165</v>
       </c>
       <c r="C157" s="2" t="s">
-        <v>171</v>
+        <v>328</v>
+      </c>
+      <c r="E157" t="s">
+        <v>34</v>
+      </c>
+      <c r="F157">
+        <v>1789</v>
+      </c>
+      <c r="H157" t="s">
+        <v>16</v>
+      </c>
+      <c r="I157" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="158" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
-        <v>217</v>
+        <v>172</v>
       </c>
       <c r="B158" t="s">
         <v>60</v>
       </c>
       <c r="C158" s="2" t="s">
-        <v>216</v>
-      </c>
-      <c r="E158" t="s">
-        <v>14</v>
-      </c>
-      <c r="F158">
-        <v>1900</v>
-      </c>
-      <c r="H158" t="s">
-        <v>16</v>
-      </c>
-      <c r="I158" t="s">
-        <v>20</v>
+        <v>171</v>
       </c>
     </row>
     <row r="159" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
-        <v>132</v>
+        <v>217</v>
       </c>
       <c r="B159" t="s">
-        <v>259</v>
+        <v>60</v>
       </c>
       <c r="C159" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="Q159" t="s">
-        <v>17</v>
+        <v>216</v>
+      </c>
+      <c r="E159" t="s">
+        <v>14</v>
+      </c>
+      <c r="F159">
+        <v>1900</v>
+      </c>
+      <c r="H159" t="s">
+        <v>16</v>
+      </c>
+      <c r="I159" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="160" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
-        <v>182</v>
+        <v>132</v>
       </c>
       <c r="B160" t="s">
-        <v>165</v>
+        <v>259</v>
       </c>
       <c r="C160" s="2" t="s">
-        <v>181</v>
+        <v>133</v>
+      </c>
+      <c r="Q160" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="161" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
-        <v>423</v>
+        <v>182</v>
       </c>
       <c r="B161" t="s">
-        <v>86</v>
+        <v>165</v>
       </c>
       <c r="C161" s="2" t="s">
-        <v>424</v>
-      </c>
-      <c r="E161" t="s">
-        <v>34</v>
-      </c>
-      <c r="F161">
-        <v>1996</v>
-      </c>
-      <c r="G161">
-        <v>2016</v>
-      </c>
-      <c r="H161" t="s">
-        <v>348</v>
-      </c>
-      <c r="I161" t="s">
-        <v>425</v>
+        <v>181</v>
       </c>
     </row>
     <row r="162" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
-        <v>115</v>
+        <v>423</v>
       </c>
       <c r="B162" t="s">
-        <v>128</v>
+        <v>86</v>
       </c>
       <c r="C162" s="2" t="s">
-        <v>116</v>
+        <v>424</v>
+      </c>
+      <c r="E162" t="s">
+        <v>34</v>
+      </c>
+      <c r="F162">
+        <v>1996</v>
+      </c>
+      <c r="G162">
+        <v>2016</v>
+      </c>
+      <c r="H162" t="s">
+        <v>348</v>
+      </c>
+      <c r="I162" t="s">
+        <v>425</v>
       </c>
     </row>
     <row r="163" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
-        <v>263</v>
+        <v>115</v>
       </c>
       <c r="B163" t="s">
-        <v>250</v>
+        <v>128</v>
       </c>
       <c r="C163" s="2" t="s">
-        <v>264</v>
-      </c>
-      <c r="E163" t="s">
-        <v>265</v>
-      </c>
-      <c r="F163">
-        <v>1500</v>
-      </c>
-      <c r="G163">
-        <v>2000</v>
-      </c>
-      <c r="H163" t="s">
-        <v>16</v>
-      </c>
-      <c r="I163" t="s">
-        <v>20</v>
+        <v>116</v>
       </c>
     </row>
     <row r="164" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
-        <v>221</v>
+        <v>263</v>
       </c>
       <c r="B164" t="s">
-        <v>86</v>
+        <v>250</v>
       </c>
       <c r="C164" s="2" t="s">
-        <v>220</v>
+        <v>264</v>
+      </c>
+      <c r="E164" t="s">
+        <v>265</v>
       </c>
       <c r="F164">
-        <v>2013</v>
+        <v>1500</v>
+      </c>
+      <c r="G164">
+        <v>2000</v>
       </c>
       <c r="H164" t="s">
         <v>16</v>
@@ -5262,22 +5301,16 @@
     </row>
     <row r="165" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
-        <v>13</v>
+        <v>221</v>
       </c>
       <c r="B165" t="s">
-        <v>25</v>
+        <v>86</v>
       </c>
       <c r="C165" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="D165" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="E165" t="s">
-        <v>14</v>
+        <v>220</v>
       </c>
       <c r="F165">
-        <v>1981</v>
+        <v>2013</v>
       </c>
       <c r="H165" t="s">
         <v>16</v>
@@ -5288,166 +5321,192 @@
     </row>
     <row r="166" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
+        <v>13</v>
+      </c>
+      <c r="B166" t="s">
+        <v>25</v>
+      </c>
+      <c r="C166" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D166" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E166" t="s">
+        <v>14</v>
+      </c>
+      <c r="F166">
+        <v>1981</v>
+      </c>
+      <c r="H166" t="s">
+        <v>16</v>
+      </c>
+      <c r="I166" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="167" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A167" t="s">
         <v>283</v>
       </c>
-      <c r="B166" t="s">
+      <c r="B167" t="s">
         <v>124</v>
       </c>
-      <c r="C166" s="2" t="s">
+      <c r="C167" s="2" t="s">
         <v>284</v>
       </c>
-      <c r="H166" t="s">
-        <v>16</v>
-      </c>
-      <c r="I166" t="s">
+      <c r="H167" t="s">
+        <v>16</v>
+      </c>
+      <c r="I167" t="s">
         <v>20</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:Q166">
+  <sortState ref="A2:Q167">
     <sortCondition ref="A2"/>
   </sortState>
   <hyperlinks>
     <hyperlink ref="C6" r:id="rId1"/>
-    <hyperlink ref="C61" r:id="rId2"/>
+    <hyperlink ref="C62" r:id="rId2"/>
     <hyperlink ref="C7" r:id="rId3"/>
     <hyperlink ref="C11" r:id="rId4"/>
-    <hyperlink ref="C99" r:id="rId5"/>
-    <hyperlink ref="C119" r:id="rId6"/>
-    <hyperlink ref="C165" r:id="rId7"/>
+    <hyperlink ref="C100" r:id="rId5"/>
+    <hyperlink ref="C120" r:id="rId6"/>
+    <hyperlink ref="C166" r:id="rId7"/>
     <hyperlink ref="C36" r:id="rId8"/>
     <hyperlink ref="C31" r:id="rId9"/>
-    <hyperlink ref="C52" r:id="rId10"/>
-    <hyperlink ref="C59" r:id="rId11"/>
+    <hyperlink ref="C53" r:id="rId10"/>
+    <hyperlink ref="C60" r:id="rId11"/>
     <hyperlink ref="C3" r:id="rId12"/>
     <hyperlink ref="C21" r:id="rId13"/>
-    <hyperlink ref="C63" r:id="rId14"/>
-    <hyperlink ref="C91" r:id="rId15"/>
+    <hyperlink ref="C64" r:id="rId14"/>
+    <hyperlink ref="C92" r:id="rId15"/>
     <hyperlink ref="C30" r:id="rId16"/>
-    <hyperlink ref="C115" r:id="rId17"/>
-    <hyperlink ref="C43" r:id="rId18"/>
-    <hyperlink ref="C76" r:id="rId19"/>
+    <hyperlink ref="C116" r:id="rId17"/>
+    <hyperlink ref="C44" r:id="rId18"/>
+    <hyperlink ref="C77" r:id="rId19"/>
     <hyperlink ref="C17" r:id="rId20"/>
-    <hyperlink ref="C153" r:id="rId21"/>
+    <hyperlink ref="C154" r:id="rId21"/>
     <hyperlink ref="C8" r:id="rId22"/>
     <hyperlink ref="C40" r:id="rId23"/>
-    <hyperlink ref="C56" r:id="rId24"/>
-    <hyperlink ref="C53" r:id="rId25"/>
-    <hyperlink ref="C57" r:id="rId26"/>
-    <hyperlink ref="C58" r:id="rId27"/>
-    <hyperlink ref="C73" r:id="rId28"/>
-    <hyperlink ref="C96" r:id="rId29"/>
-    <hyperlink ref="C144" r:id="rId30"/>
-    <hyperlink ref="C102" r:id="rId31"/>
-    <hyperlink ref="C86" r:id="rId32"/>
-    <hyperlink ref="C108" r:id="rId33"/>
-    <hyperlink ref="C74" r:id="rId34"/>
+    <hyperlink ref="C57" r:id="rId24"/>
+    <hyperlink ref="C54" r:id="rId25"/>
+    <hyperlink ref="C58" r:id="rId26"/>
+    <hyperlink ref="C59" r:id="rId27"/>
+    <hyperlink ref="C74" r:id="rId28"/>
+    <hyperlink ref="C97" r:id="rId29"/>
+    <hyperlink ref="C145" r:id="rId30"/>
+    <hyperlink ref="C103" r:id="rId31"/>
+    <hyperlink ref="C87" r:id="rId32"/>
+    <hyperlink ref="C109" r:id="rId33"/>
+    <hyperlink ref="C75" r:id="rId34"/>
     <hyperlink ref="C18" r:id="rId35"/>
-    <hyperlink ref="C142" r:id="rId36"/>
+    <hyperlink ref="C143" r:id="rId36"/>
     <hyperlink ref="C16" r:id="rId37"/>
-    <hyperlink ref="C162" r:id="rId38"/>
-    <hyperlink ref="C90" r:id="rId39"/>
-    <hyperlink ref="C60" r:id="rId40"/>
-    <hyperlink ref="C125" r:id="rId41"/>
+    <hyperlink ref="C163" r:id="rId38"/>
+    <hyperlink ref="C91" r:id="rId39"/>
+    <hyperlink ref="C61" r:id="rId40"/>
+    <hyperlink ref="C126" r:id="rId41"/>
     <hyperlink ref="C19" r:id="rId42"/>
-    <hyperlink ref="C54" r:id="rId43"/>
+    <hyperlink ref="C55" r:id="rId43"/>
     <hyperlink ref="C24" r:id="rId44"/>
-    <hyperlink ref="C116" r:id="rId45"/>
-    <hyperlink ref="C159" r:id="rId46"/>
+    <hyperlink ref="C117" r:id="rId45"/>
+    <hyperlink ref="C160" r:id="rId46"/>
     <hyperlink ref="C28" r:id="rId47" display="http://comparativeconstitutionsproject.org/"/>
-    <hyperlink ref="C113" r:id="rId48"/>
-    <hyperlink ref="C155" r:id="rId49"/>
-    <hyperlink ref="C129" r:id="rId50"/>
-    <hyperlink ref="C123" r:id="rId51"/>
+    <hyperlink ref="C114" r:id="rId48"/>
+    <hyperlink ref="C156" r:id="rId49"/>
+    <hyperlink ref="C130" r:id="rId50"/>
+    <hyperlink ref="C124" r:id="rId51"/>
     <hyperlink ref="C23" r:id="rId52"/>
-    <hyperlink ref="C117" r:id="rId53"/>
-    <hyperlink ref="C50" r:id="rId54"/>
-    <hyperlink ref="C80" r:id="rId55"/>
-    <hyperlink ref="C83" r:id="rId56"/>
-    <hyperlink ref="C114" r:id="rId57"/>
-    <hyperlink ref="C104" r:id="rId58"/>
-    <hyperlink ref="C133" r:id="rId59"/>
+    <hyperlink ref="C118" r:id="rId53"/>
+    <hyperlink ref="C51" r:id="rId54"/>
+    <hyperlink ref="C81" r:id="rId55"/>
+    <hyperlink ref="C84" r:id="rId56"/>
+    <hyperlink ref="C115" r:id="rId57"/>
+    <hyperlink ref="C105" r:id="rId58"/>
+    <hyperlink ref="C134" r:id="rId59"/>
     <hyperlink ref="C32" r:id="rId60"/>
-    <hyperlink ref="C146" r:id="rId61"/>
+    <hyperlink ref="C147" r:id="rId61"/>
     <hyperlink ref="C9" r:id="rId62"/>
     <hyperlink ref="C34" r:id="rId63"/>
-    <hyperlink ref="C147" r:id="rId64"/>
+    <hyperlink ref="C148" r:id="rId64"/>
     <hyperlink ref="C15" r:id="rId65"/>
-    <hyperlink ref="C157" r:id="rId66"/>
+    <hyperlink ref="C158" r:id="rId66"/>
     <hyperlink ref="C26" r:id="rId67"/>
     <hyperlink ref="C25" r:id="rId68"/>
     <hyperlink ref="C27" r:id="rId69"/>
-    <hyperlink ref="C55" r:id="rId70"/>
-    <hyperlink ref="C160" r:id="rId71"/>
+    <hyperlink ref="C56" r:id="rId70"/>
+    <hyperlink ref="C161" r:id="rId71"/>
     <hyperlink ref="C29" r:id="rId72"/>
-    <hyperlink ref="C120" r:id="rId73"/>
+    <hyperlink ref="C121" r:id="rId73"/>
     <hyperlink ref="C33" r:id="rId74"/>
-    <hyperlink ref="C47" r:id="rId75"/>
-    <hyperlink ref="C136" r:id="rId76"/>
-    <hyperlink ref="C44" r:id="rId77"/>
+    <hyperlink ref="C48" r:id="rId75"/>
+    <hyperlink ref="C137" r:id="rId76"/>
+    <hyperlink ref="C45" r:id="rId77"/>
     <hyperlink ref="C41" r:id="rId78"/>
-    <hyperlink ref="C71" r:id="rId79"/>
+    <hyperlink ref="C72" r:id="rId79"/>
     <hyperlink ref="C5" r:id="rId80"/>
-    <hyperlink ref="C70" r:id="rId81"/>
+    <hyperlink ref="C71" r:id="rId81"/>
     <hyperlink ref="C13" r:id="rId82"/>
-    <hyperlink ref="C112" r:id="rId83"/>
-    <hyperlink ref="C121" r:id="rId84"/>
-    <hyperlink ref="C149" r:id="rId85"/>
+    <hyperlink ref="C113" r:id="rId83"/>
+    <hyperlink ref="C122" r:id="rId84"/>
+    <hyperlink ref="C150" r:id="rId85"/>
     <hyperlink ref="C37" r:id="rId86"/>
-    <hyperlink ref="C158" r:id="rId87"/>
-    <hyperlink ref="C46" r:id="rId88"/>
-    <hyperlink ref="C164" r:id="rId89"/>
-    <hyperlink ref="C100" r:id="rId90"/>
-    <hyperlink ref="C68" r:id="rId91"/>
-    <hyperlink ref="C101" r:id="rId92"/>
-    <hyperlink ref="C139" r:id="rId93"/>
-    <hyperlink ref="C84" r:id="rId94"/>
-    <hyperlink ref="C106" r:id="rId95"/>
-    <hyperlink ref="C140" r:id="rId96"/>
-    <hyperlink ref="C64" r:id="rId97"/>
-    <hyperlink ref="C118" r:id="rId98"/>
-    <hyperlink ref="C48" r:id="rId99"/>
-    <hyperlink ref="C45" r:id="rId100"/>
-    <hyperlink ref="C87" r:id="rId101"/>
-    <hyperlink ref="C62" r:id="rId102"/>
+    <hyperlink ref="C159" r:id="rId87"/>
+    <hyperlink ref="C47" r:id="rId88"/>
+    <hyperlink ref="C165" r:id="rId89"/>
+    <hyperlink ref="C101" r:id="rId90"/>
+    <hyperlink ref="C69" r:id="rId91"/>
+    <hyperlink ref="C102" r:id="rId92"/>
+    <hyperlink ref="C140" r:id="rId93"/>
+    <hyperlink ref="C85" r:id="rId94"/>
+    <hyperlink ref="C107" r:id="rId95"/>
+    <hyperlink ref="C141" r:id="rId96"/>
+    <hyperlink ref="C65" r:id="rId97"/>
+    <hyperlink ref="C119" r:id="rId98"/>
+    <hyperlink ref="C49" r:id="rId99"/>
+    <hyperlink ref="C46" r:id="rId100"/>
+    <hyperlink ref="C88" r:id="rId101"/>
+    <hyperlink ref="C63" r:id="rId102"/>
     <hyperlink ref="C2" r:id="rId103"/>
-    <hyperlink ref="C81" r:id="rId104"/>
-    <hyperlink ref="C85" r:id="rId105"/>
-    <hyperlink ref="C110" r:id="rId106"/>
-    <hyperlink ref="C49" r:id="rId107"/>
-    <hyperlink ref="C88" r:id="rId108"/>
-    <hyperlink ref="C138" r:id="rId109"/>
+    <hyperlink ref="C82" r:id="rId104"/>
+    <hyperlink ref="C86" r:id="rId105"/>
+    <hyperlink ref="C111" r:id="rId106"/>
+    <hyperlink ref="C50" r:id="rId107"/>
+    <hyperlink ref="C89" r:id="rId108"/>
+    <hyperlink ref="C139" r:id="rId109"/>
     <hyperlink ref="C14" r:id="rId110"/>
     <hyperlink ref="C4" r:id="rId111"/>
-    <hyperlink ref="C163" r:id="rId112"/>
-    <hyperlink ref="C94" r:id="rId113"/>
-    <hyperlink ref="C89" r:id="rId114"/>
-    <hyperlink ref="C152" r:id="rId115"/>
-    <hyperlink ref="C132" r:id="rId116"/>
-    <hyperlink ref="C66" r:id="rId117"/>
-    <hyperlink ref="C103" r:id="rId118"/>
-    <hyperlink ref="C78" r:id="rId119"/>
-    <hyperlink ref="C166" r:id="rId120"/>
-    <hyperlink ref="C69" r:id="rId121"/>
-    <hyperlink ref="C131" r:id="rId122"/>
-    <hyperlink ref="C109" r:id="rId123"/>
-    <hyperlink ref="C82" r:id="rId124"/>
-    <hyperlink ref="C107" r:id="rId125"/>
-    <hyperlink ref="C137" r:id="rId126"/>
-    <hyperlink ref="C92" r:id="rId127"/>
+    <hyperlink ref="C164" r:id="rId112"/>
+    <hyperlink ref="C95" r:id="rId113"/>
+    <hyperlink ref="C90" r:id="rId114"/>
+    <hyperlink ref="C153" r:id="rId115"/>
+    <hyperlink ref="C133" r:id="rId116"/>
+    <hyperlink ref="C67" r:id="rId117"/>
+    <hyperlink ref="C104" r:id="rId118"/>
+    <hyperlink ref="C79" r:id="rId119"/>
+    <hyperlink ref="C167" r:id="rId120"/>
+    <hyperlink ref="C70" r:id="rId121"/>
+    <hyperlink ref="C132" r:id="rId122"/>
+    <hyperlink ref="C110" r:id="rId123"/>
+    <hyperlink ref="C83" r:id="rId124"/>
+    <hyperlink ref="C108" r:id="rId125"/>
+    <hyperlink ref="C138" r:id="rId126"/>
+    <hyperlink ref="C93" r:id="rId127"/>
     <hyperlink ref="C12" r:id="rId128"/>
     <hyperlink ref="C20" r:id="rId129"/>
-    <hyperlink ref="C130" r:id="rId130"/>
-    <hyperlink ref="C77" r:id="rId131"/>
-    <hyperlink ref="C145" r:id="rId132"/>
-    <hyperlink ref="C127" r:id="rId133"/>
-    <hyperlink ref="C126" r:id="rId134"/>
-    <hyperlink ref="C128" r:id="rId135"/>
-    <hyperlink ref="C151" r:id="rId136"/>
-    <hyperlink ref="C143" r:id="rId137"/>
-    <hyperlink ref="C156" r:id="rId138"/>
+    <hyperlink ref="C131" r:id="rId130"/>
+    <hyperlink ref="C78" r:id="rId131"/>
+    <hyperlink ref="C146" r:id="rId132"/>
+    <hyperlink ref="C128" r:id="rId133"/>
+    <hyperlink ref="C127" r:id="rId134"/>
+    <hyperlink ref="C129" r:id="rId135"/>
+    <hyperlink ref="C152" r:id="rId136"/>
+    <hyperlink ref="C144" r:id="rId137"/>
+    <hyperlink ref="C157" r:id="rId138"/>
     <hyperlink ref="C39" r:id="rId139"/>
-    <hyperlink ref="C93" r:id="rId140"/>
+    <hyperlink ref="C94" r:id="rId140"/>
     <hyperlink ref="J2" r:id="rId141"/>
     <hyperlink ref="M3" r:id="rId142"/>
     <hyperlink ref="J3" r:id="rId143"/>
@@ -5455,64 +5514,64 @@
     <hyperlink ref="J4" r:id="rId145"/>
     <hyperlink ref="P5" r:id="rId146"/>
     <hyperlink ref="J5" r:id="rId147"/>
-    <hyperlink ref="C111" r:id="rId148"/>
+    <hyperlink ref="C112" r:id="rId148"/>
     <hyperlink ref="C35" r:id="rId149"/>
     <hyperlink ref="P7" r:id="rId150"/>
     <hyperlink ref="J7" r:id="rId151"/>
     <hyperlink ref="M8" r:id="rId152"/>
     <hyperlink ref="L8" r:id="rId153"/>
     <hyperlink ref="J8" r:id="rId154"/>
-    <hyperlink ref="C154" r:id="rId155"/>
-    <hyperlink ref="N154" r:id="rId156"/>
+    <hyperlink ref="C155" r:id="rId155"/>
+    <hyperlink ref="N155" r:id="rId156"/>
     <hyperlink ref="C22" r:id="rId157"/>
     <hyperlink ref="N22" r:id="rId158"/>
-    <hyperlink ref="C65" r:id="rId159"/>
-    <hyperlink ref="C150" r:id="rId160"/>
-    <hyperlink ref="J150" r:id="rId161"/>
-    <hyperlink ref="C148" r:id="rId162"/>
-    <hyperlink ref="N148" r:id="rId163"/>
-    <hyperlink ref="J148" r:id="rId164"/>
-    <hyperlink ref="C97" r:id="rId165"/>
-    <hyperlink ref="C95" r:id="rId166"/>
+    <hyperlink ref="C66" r:id="rId159"/>
+    <hyperlink ref="C151" r:id="rId160"/>
+    <hyperlink ref="J151" r:id="rId161"/>
+    <hyperlink ref="C149" r:id="rId162"/>
+    <hyperlink ref="N149" r:id="rId163"/>
+    <hyperlink ref="J149" r:id="rId164"/>
+    <hyperlink ref="C98" r:id="rId165"/>
+    <hyperlink ref="C96" r:id="rId166"/>
     <hyperlink ref="C42" r:id="rId167"/>
     <hyperlink ref="J42" r:id="rId168"/>
     <hyperlink ref="K42" r:id="rId169"/>
-    <hyperlink ref="C105" r:id="rId170"/>
-    <hyperlink ref="N105" r:id="rId171"/>
-    <hyperlink ref="C79" r:id="rId172"/>
-    <hyperlink ref="K79" r:id="rId173"/>
-    <hyperlink ref="C161" r:id="rId174"/>
-    <hyperlink ref="C122" r:id="rId175"/>
-    <hyperlink ref="K122" r:id="rId176"/>
+    <hyperlink ref="C106" r:id="rId170"/>
+    <hyperlink ref="N106" r:id="rId171"/>
+    <hyperlink ref="C80" r:id="rId172"/>
+    <hyperlink ref="K80" r:id="rId173"/>
+    <hyperlink ref="C162" r:id="rId174"/>
+    <hyperlink ref="C123" r:id="rId175"/>
+    <hyperlink ref="K123" r:id="rId176"/>
     <hyperlink ref="L9" r:id="rId177"/>
     <hyperlink ref="J9" r:id="rId178"/>
     <hyperlink ref="J11" r:id="rId179"/>
-    <hyperlink ref="C134" r:id="rId180"/>
-    <hyperlink ref="J134" r:id="rId181"/>
-    <hyperlink ref="L134" r:id="rId182"/>
-    <hyperlink ref="K134" r:id="rId183"/>
-    <hyperlink ref="C135" r:id="rId184"/>
-    <hyperlink ref="J135" r:id="rId185"/>
-    <hyperlink ref="K135" r:id="rId186"/>
-    <hyperlink ref="L135" r:id="rId187"/>
-    <hyperlink ref="C67" r:id="rId188"/>
-    <hyperlink ref="J67" r:id="rId189"/>
-    <hyperlink ref="N67" r:id="rId190"/>
-    <hyperlink ref="C141" r:id="rId191"/>
-    <hyperlink ref="C98" r:id="rId192"/>
-    <hyperlink ref="J98" r:id="rId193"/>
-    <hyperlink ref="L98" r:id="rId194"/>
-    <hyperlink ref="C75" r:id="rId195"/>
-    <hyperlink ref="C51" r:id="rId196"/>
-    <hyperlink ref="L51" r:id="rId197"/>
-    <hyperlink ref="K51" r:id="rId198"/>
-    <hyperlink ref="J51" r:id="rId199"/>
-    <hyperlink ref="C72" r:id="rId200"/>
-    <hyperlink ref="J72" r:id="rId201"/>
-    <hyperlink ref="K72" r:id="rId202"/>
-    <hyperlink ref="L72" r:id="rId203"/>
-    <hyperlink ref="C124" r:id="rId204"/>
-    <hyperlink ref="N124" r:id="rId205"/>
+    <hyperlink ref="C135" r:id="rId180"/>
+    <hyperlink ref="J135" r:id="rId181"/>
+    <hyperlink ref="L135" r:id="rId182"/>
+    <hyperlink ref="K135" r:id="rId183"/>
+    <hyperlink ref="C136" r:id="rId184"/>
+    <hyperlink ref="J136" r:id="rId185"/>
+    <hyperlink ref="K136" r:id="rId186"/>
+    <hyperlink ref="L136" r:id="rId187"/>
+    <hyperlink ref="C68" r:id="rId188"/>
+    <hyperlink ref="J68" r:id="rId189"/>
+    <hyperlink ref="N68" r:id="rId190"/>
+    <hyperlink ref="C142" r:id="rId191"/>
+    <hyperlink ref="C99" r:id="rId192"/>
+    <hyperlink ref="J99" r:id="rId193"/>
+    <hyperlink ref="L99" r:id="rId194"/>
+    <hyperlink ref="C76" r:id="rId195"/>
+    <hyperlink ref="C52" r:id="rId196"/>
+    <hyperlink ref="L52" r:id="rId197"/>
+    <hyperlink ref="K52" r:id="rId198"/>
+    <hyperlink ref="J52" r:id="rId199"/>
+    <hyperlink ref="C73" r:id="rId200"/>
+    <hyperlink ref="J73" r:id="rId201"/>
+    <hyperlink ref="K73" r:id="rId202"/>
+    <hyperlink ref="L73" r:id="rId203"/>
+    <hyperlink ref="C125" r:id="rId204"/>
+    <hyperlink ref="N125" r:id="rId205"/>
     <hyperlink ref="C38" r:id="rId206"/>
     <hyperlink ref="K38" r:id="rId207"/>
     <hyperlink ref="J38" r:id="rId208"/>
@@ -5520,6 +5579,12 @@
     <hyperlink ref="J10" r:id="rId210"/>
     <hyperlink ref="P10" r:id="rId211"/>
     <hyperlink ref="N10" r:id="rId212"/>
+    <hyperlink ref="C43" r:id="rId213"/>
+    <hyperlink ref="J43" r:id="rId214"/>
+    <hyperlink ref="K43" r:id="rId215"/>
+    <hyperlink ref="L43" r:id="rId216"/>
+    <hyperlink ref="M43" r:id="rId217"/>
+    <hyperlink ref="N43" r:id="rId218"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
add 'United Nations General Assembly Voting Data' and 'Chance-Corrected Measures of Foreign Policy Similarity'
</commit_message>
<xml_diff>
--- a/PolData.xlsx
+++ b/PolData.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="899" uniqueCount="496">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="913" uniqueCount="502">
   <si>
     <t>name</t>
   </si>
@@ -1515,6 +1515,24 @@
   </si>
   <si>
     <t>https://sites.hks.harvard.edu/fs/pnorris/Data/Democracy%20CrossNational%20Data/Democracy%20Crossnational%20Data%20Spring%202009%20Excel.xlsx</t>
+  </si>
+  <si>
+    <t>http://dx.doi.org/10.7910/DVN/ALVXLM</t>
+  </si>
+  <si>
+    <t>Chance-Corrected Measures of Foreign Policy Similarity</t>
+  </si>
+  <si>
+    <t>Foreign policy</t>
+  </si>
+  <si>
+    <t>http://hdl.handle.net/1902.1/12379</t>
+  </si>
+  <si>
+    <t>United Nations General Assembly Voting Data</t>
+  </si>
+  <si>
+    <t>United Nations, roll-calls</t>
   </si>
 </sst>
 </file>
@@ -1854,10 +1872,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q167"/>
+  <dimension ref="A1:Q169"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="A43" sqref="A43"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2506,221 +2524,230 @@
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>146</v>
+        <v>497</v>
       </c>
       <c r="B23" t="s">
-        <v>128</v>
+        <v>40</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>145</v>
+        <v>496</v>
+      </c>
+      <c r="D23" t="s">
+        <v>498</v>
+      </c>
+      <c r="E23" t="s">
+        <v>14</v>
+      </c>
+      <c r="F23">
+        <v>1946</v>
+      </c>
+      <c r="G23">
+        <v>2012</v>
+      </c>
+      <c r="H23" t="s">
+        <v>348</v>
+      </c>
+      <c r="I23" t="s">
+        <v>349</v>
       </c>
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>127</v>
+        <v>146</v>
       </c>
       <c r="B24" t="s">
-        <v>259</v>
+        <v>128</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="I24" t="s">
-        <v>20</v>
+        <v>145</v>
       </c>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>173</v>
+        <v>127</v>
       </c>
       <c r="B25" t="s">
-        <v>128</v>
+        <v>259</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>175</v>
+        <v>121</v>
+      </c>
+      <c r="I25" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B26" t="s">
-        <v>86</v>
+        <v>128</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="E26" t="s">
-        <v>176</v>
-      </c>
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="B27" t="s">
-        <v>25</v>
+        <v>86</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>175</v>
       </c>
       <c r="E27" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>135</v>
+        <v>177</v>
       </c>
       <c r="B28" t="s">
-        <v>134</v>
+        <v>25</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>136</v>
+        <v>175</v>
+      </c>
+      <c r="E28" t="s">
+        <v>178</v>
       </c>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>184</v>
+        <v>135</v>
       </c>
       <c r="B29" t="s">
-        <v>128</v>
+        <v>134</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>183</v>
+        <v>136</v>
       </c>
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
+        <v>184</v>
+      </c>
+      <c r="B30" t="s">
+        <v>128</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
         <v>54</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B31" t="s">
         <v>55</v>
       </c>
-      <c r="C30" s="2" t="s">
+      <c r="C31" s="2" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A31" s="1" t="s">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A32" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B32" t="s">
         <v>25</v>
       </c>
-      <c r="C31" s="2" t="s">
+      <c r="C32" s="2" t="s">
         <v>47</v>
-      </c>
-    </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
-        <v>158</v>
-      </c>
-      <c r="B32" t="s">
-        <v>99</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>187</v>
+        <v>158</v>
       </c>
       <c r="B33" t="s">
         <v>99</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>188</v>
-      </c>
-      <c r="F33">
-        <v>1960</v>
-      </c>
-      <c r="G33">
-        <v>2011</v>
-      </c>
-      <c r="H33" t="s">
-        <v>16</v>
-      </c>
-      <c r="I33" t="s">
-        <v>189</v>
+        <v>159</v>
       </c>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>164</v>
+        <v>187</v>
       </c>
       <c r="B34" t="s">
-        <v>165</v>
+        <v>99</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>166</v>
+        <v>188</v>
+      </c>
+      <c r="F34">
+        <v>1960</v>
+      </c>
+      <c r="G34">
+        <v>2011</v>
+      </c>
+      <c r="H34" t="s">
+        <v>16</v>
+      </c>
+      <c r="I34" t="s">
+        <v>189</v>
       </c>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>371</v>
+        <v>164</v>
       </c>
       <c r="B35" t="s">
-        <v>25</v>
+        <v>165</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>372</v>
-      </c>
-      <c r="D35" t="s">
-        <v>363</v>
-      </c>
-      <c r="E35" t="s">
-        <v>34</v>
-      </c>
-      <c r="F35">
-        <v>2006</v>
-      </c>
-      <c r="H35" t="s">
-        <v>348</v>
-      </c>
-      <c r="I35" t="s">
-        <v>349</v>
+        <v>166</v>
       </c>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>39</v>
+        <v>371</v>
       </c>
       <c r="B36" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>41</v>
+        <v>372</v>
+      </c>
+      <c r="D36" t="s">
+        <v>363</v>
       </c>
       <c r="E36" t="s">
-        <v>14</v>
+        <v>34</v>
       </c>
       <c r="F36">
-        <v>1816</v>
-      </c>
-      <c r="G36">
-        <v>2007</v>
+        <v>2006</v>
       </c>
       <c r="H36" t="s">
-        <v>16</v>
+        <v>348</v>
       </c>
       <c r="I36" t="s">
-        <v>20</v>
+        <v>349</v>
       </c>
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>215</v>
+        <v>39</v>
       </c>
       <c r="B37" t="s">
-        <v>237</v>
+        <v>40</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>214</v>
+        <v>41</v>
+      </c>
+      <c r="E37" t="s">
+        <v>14</v>
       </c>
       <c r="F37">
-        <v>1995</v>
+        <v>1816</v>
+      </c>
+      <c r="G37">
+        <v>2007</v>
       </c>
       <c r="H37" t="s">
         <v>16</v>
@@ -2731,140 +2758,134 @@
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>476</v>
+        <v>215</v>
       </c>
       <c r="B38" t="s">
-        <v>40</v>
+        <v>237</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>477</v>
-      </c>
-      <c r="D38" t="s">
-        <v>478</v>
-      </c>
-      <c r="E38" t="s">
-        <v>14</v>
+        <v>214</v>
       </c>
       <c r="F38">
-        <v>2002</v>
+        <v>1995</v>
       </c>
       <c r="H38" t="s">
-        <v>348</v>
+        <v>16</v>
       </c>
       <c r="I38" t="s">
-        <v>349</v>
-      </c>
-      <c r="J38" s="2" t="s">
-        <v>480</v>
-      </c>
-      <c r="K38" s="2" t="s">
-        <v>479</v>
+        <v>20</v>
       </c>
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>330</v>
+        <v>476</v>
       </c>
       <c r="B39" t="s">
-        <v>165</v>
+        <v>40</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>331</v>
+        <v>477</v>
+      </c>
+      <c r="D39" t="s">
+        <v>478</v>
       </c>
       <c r="E39" t="s">
-        <v>77</v>
+        <v>14</v>
       </c>
       <c r="F39">
-        <v>1953</v>
+        <v>2002</v>
       </c>
       <c r="H39" t="s">
-        <v>16</v>
+        <v>348</v>
       </c>
       <c r="I39" t="s">
-        <v>20</v>
+        <v>349</v>
+      </c>
+      <c r="J39" s="2" t="s">
+        <v>480</v>
+      </c>
+      <c r="K39" s="2" t="s">
+        <v>479</v>
       </c>
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>75</v>
+        <v>330</v>
       </c>
       <c r="B40" t="s">
-        <v>25</v>
+        <v>165</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>76</v>
+        <v>331</v>
       </c>
       <c r="E40" t="s">
         <v>77</v>
       </c>
       <c r="F40">
-        <v>1971</v>
+        <v>1953</v>
+      </c>
+      <c r="H40" t="s">
+        <v>16</v>
+      </c>
+      <c r="I40" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>197</v>
+        <v>75</v>
       </c>
       <c r="B41" t="s">
-        <v>55</v>
+        <v>25</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>198</v>
+        <v>76</v>
       </c>
       <c r="E41" t="s">
-        <v>199</v>
+        <v>77</v>
       </c>
       <c r="F41">
-        <v>1975</v>
-      </c>
-      <c r="G41">
-        <v>2015</v>
-      </c>
-      <c r="H41" t="s">
-        <v>16</v>
-      </c>
-      <c r="I41" t="s">
-        <v>20</v>
+        <v>1971</v>
       </c>
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>409</v>
+        <v>197</v>
       </c>
       <c r="B42" t="s">
-        <v>250</v>
+        <v>55</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>410</v>
+        <v>198</v>
       </c>
       <c r="E42" t="s">
-        <v>9</v>
+        <v>199</v>
+      </c>
+      <c r="F42">
+        <v>1975</v>
+      </c>
+      <c r="G42">
+        <v>2015</v>
       </c>
       <c r="H42" t="s">
-        <v>348</v>
+        <v>16</v>
       </c>
       <c r="I42" t="s">
-        <v>349</v>
-      </c>
-      <c r="J42" s="2" t="s">
-        <v>411</v>
-      </c>
-      <c r="K42" s="2" t="s">
-        <v>412</v>
+        <v>20</v>
       </c>
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>489</v>
+        <v>409</v>
       </c>
       <c r="B43" t="s">
-        <v>60</v>
+        <v>250</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>488</v>
+        <v>410</v>
       </c>
       <c r="E43" t="s">
-        <v>490</v>
+        <v>9</v>
       </c>
       <c r="H43" t="s">
         <v>348</v>
@@ -2873,81 +2894,84 @@
         <v>349</v>
       </c>
       <c r="J43" s="2" t="s">
-        <v>491</v>
+        <v>411</v>
       </c>
       <c r="K43" s="2" t="s">
-        <v>492</v>
-      </c>
-      <c r="L43" s="2" t="s">
-        <v>493</v>
-      </c>
-      <c r="M43" s="2" t="s">
-        <v>494</v>
-      </c>
-      <c r="N43" s="2" t="s">
-        <v>495</v>
+        <v>412</v>
       </c>
     </row>
     <row r="44" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>59</v>
+        <v>489</v>
       </c>
       <c r="B44" t="s">
         <v>60</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>61</v>
+        <v>488</v>
+      </c>
+      <c r="E44" t="s">
+        <v>490</v>
+      </c>
+      <c r="H44" t="s">
+        <v>348</v>
+      </c>
+      <c r="I44" t="s">
+        <v>349</v>
+      </c>
+      <c r="J44" s="2" t="s">
+        <v>491</v>
+      </c>
+      <c r="K44" s="2" t="s">
+        <v>492</v>
+      </c>
+      <c r="L44" s="2" t="s">
+        <v>493</v>
+      </c>
+      <c r="M44" s="2" t="s">
+        <v>494</v>
+      </c>
+      <c r="N44" s="2" t="s">
+        <v>495</v>
       </c>
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>196</v>
+        <v>59</v>
       </c>
       <c r="B45" t="s">
-        <v>165</v>
+        <v>60</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>195</v>
-      </c>
-      <c r="F45">
-        <v>1946</v>
-      </c>
-      <c r="G45">
-        <v>2016</v>
+        <v>61</v>
       </c>
     </row>
     <row r="46" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>238</v>
+        <v>196</v>
       </c>
       <c r="B46" t="s">
-        <v>237</v>
+        <v>165</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>243</v>
-      </c>
-      <c r="H46" t="s">
-        <v>16</v>
-      </c>
-      <c r="I46" t="s">
-        <v>20</v>
+        <v>195</v>
+      </c>
+      <c r="F46">
+        <v>1946</v>
+      </c>
+      <c r="G46">
+        <v>2016</v>
       </c>
     </row>
     <row r="47" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>219</v>
+        <v>238</v>
       </c>
       <c r="B47" t="s">
-        <v>124</v>
+        <v>237</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>218</v>
-      </c>
-      <c r="F47">
-        <v>1970</v>
-      </c>
-      <c r="G47">
-        <v>2015</v>
+        <v>243</v>
       </c>
       <c r="H47" t="s">
         <v>16</v>
@@ -2958,44 +2982,50 @@
     </row>
     <row r="48" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>191</v>
+        <v>219</v>
       </c>
       <c r="B48" t="s">
-        <v>25</v>
+        <v>124</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="E48" t="s">
-        <v>192</v>
+        <v>218</v>
+      </c>
+      <c r="F48">
+        <v>1970</v>
+      </c>
+      <c r="G48">
+        <v>2015</v>
+      </c>
+      <c r="H48" t="s">
+        <v>16</v>
+      </c>
+      <c r="I48" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="49" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>235</v>
+        <v>191</v>
       </c>
       <c r="B49" t="s">
-        <v>60</v>
+        <v>25</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>236</v>
-      </c>
-      <c r="H49" t="s">
-        <v>16</v>
-      </c>
-      <c r="I49" t="s">
-        <v>20</v>
+        <v>190</v>
+      </c>
+      <c r="E49" t="s">
+        <v>192</v>
       </c>
     </row>
     <row r="50" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>252</v>
+        <v>235</v>
       </c>
       <c r="B50" t="s">
-        <v>250</v>
+        <v>60</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>251</v>
+        <v>236</v>
       </c>
       <c r="H50" t="s">
         <v>16</v>
@@ -3006,129 +3036,129 @@
     </row>
     <row r="51" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>149</v>
+        <v>252</v>
       </c>
       <c r="B51" t="s">
-        <v>128</v>
+        <v>250</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>150</v>
+        <v>251</v>
+      </c>
+      <c r="H51" t="s">
+        <v>16</v>
+      </c>
+      <c r="I51" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="52" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>462</v>
+        <v>149</v>
       </c>
       <c r="B52" t="s">
-        <v>250</v>
+        <v>128</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>464</v>
-      </c>
-      <c r="D52" t="s">
-        <v>463</v>
-      </c>
-      <c r="E52" t="s">
-        <v>14</v>
-      </c>
-      <c r="F52">
-        <v>1946</v>
-      </c>
-      <c r="G52">
-        <v>2010</v>
-      </c>
-      <c r="H52" t="s">
-        <v>348</v>
-      </c>
-      <c r="I52" t="s">
-        <v>349</v>
-      </c>
-      <c r="J52" s="2" t="s">
-        <v>467</v>
-      </c>
-      <c r="K52" s="2" t="s">
-        <v>466</v>
-      </c>
-      <c r="L52" s="2" t="s">
-        <v>465</v>
+        <v>150</v>
       </c>
     </row>
     <row r="53" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>28</v>
+        <v>462</v>
       </c>
       <c r="B53" t="s">
-        <v>25</v>
+        <v>250</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>48</v>
+        <v>464</v>
+      </c>
+      <c r="D53" t="s">
+        <v>463</v>
+      </c>
+      <c r="E53" t="s">
+        <v>14</v>
+      </c>
+      <c r="F53">
+        <v>1946</v>
+      </c>
+      <c r="G53">
+        <v>2010</v>
+      </c>
+      <c r="H53" t="s">
+        <v>348</v>
+      </c>
+      <c r="I53" t="s">
+        <v>349</v>
+      </c>
+      <c r="J53" s="2" t="s">
+        <v>467</v>
+      </c>
+      <c r="K53" s="2" t="s">
+        <v>466</v>
+      </c>
+      <c r="L53" s="2" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="54" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>80</v>
+        <v>28</v>
       </c>
       <c r="B54" t="s">
-        <v>128</v>
+        <v>25</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="E54" t="s">
-        <v>9</v>
-      </c>
-      <c r="F54">
-        <v>1979</v>
+        <v>48</v>
       </c>
     </row>
     <row r="55" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>125</v>
+        <v>80</v>
       </c>
       <c r="B55" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>126</v>
+        <v>81</v>
+      </c>
+      <c r="E55" t="s">
+        <v>9</v>
+      </c>
+      <c r="F55">
+        <v>1979</v>
       </c>
     </row>
     <row r="56" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>179</v>
+        <v>125</v>
       </c>
       <c r="B56" t="s">
-        <v>165</v>
+        <v>124</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>180</v>
+        <v>126</v>
       </c>
     </row>
     <row r="57" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
+        <v>179</v>
+      </c>
+      <c r="B57" t="s">
+        <v>165</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="58" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
         <v>78</v>
       </c>
-      <c r="B57" t="s">
+      <c r="B58" t="s">
         <v>25</v>
       </c>
-      <c r="C57" s="2" t="s">
+      <c r="C58" s="2" t="s">
         <v>79</v>
-      </c>
-      <c r="E57" t="s">
-        <v>9</v>
-      </c>
-      <c r="F57">
-        <v>1979</v>
-      </c>
-    </row>
-    <row r="58" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A58" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="B58" t="s">
-        <v>83</v>
-      </c>
-      <c r="C58" s="2" t="s">
-        <v>84</v>
       </c>
       <c r="E58" t="s">
         <v>9</v>
@@ -3139,13 +3169,13 @@
     </row>
     <row r="59" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A59" s="3" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B59" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="E59" t="s">
         <v>9</v>
@@ -3153,225 +3183,225 @@
       <c r="F59">
         <v>1979</v>
       </c>
-      <c r="G59">
+    </row>
+    <row r="60" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A60" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="B60" t="s">
+        <v>86</v>
+      </c>
+      <c r="C60" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="E60" t="s">
+        <v>9</v>
+      </c>
+      <c r="F60">
+        <v>1979</v>
+      </c>
+      <c r="G60">
         <v>2009</v>
-      </c>
-    </row>
-    <row r="60" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A60" t="s">
-        <v>27</v>
-      </c>
-      <c r="B60" t="s">
-        <v>25</v>
-      </c>
-      <c r="C60" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="Q60" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="61" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>120</v>
+        <v>27</v>
       </c>
       <c r="B61" t="s">
-        <v>259</v>
+        <v>25</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="I61" t="s">
-        <v>20</v>
+        <v>49</v>
+      </c>
+      <c r="Q61" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="62" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>5</v>
+        <v>120</v>
       </c>
       <c r="B62" t="s">
-        <v>25</v>
+        <v>259</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D62" t="s">
-        <v>94</v>
-      </c>
-      <c r="E62" t="s">
-        <v>9</v>
-      </c>
-      <c r="F62">
-        <v>2002</v>
-      </c>
-      <c r="H62" t="s">
-        <v>16</v>
+        <v>119</v>
       </c>
       <c r="I62" t="s">
-        <v>248</v>
-      </c>
-      <c r="Q62" t="s">
-        <v>44</v>
+        <v>20</v>
       </c>
     </row>
     <row r="63" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
+        <v>5</v>
+      </c>
+      <c r="B63" t="s">
+        <v>25</v>
+      </c>
+      <c r="C63" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D63" t="s">
+        <v>94</v>
+      </c>
+      <c r="E63" t="s">
+        <v>9</v>
+      </c>
+      <c r="F63">
+        <v>2002</v>
+      </c>
+      <c r="H63" t="s">
+        <v>16</v>
+      </c>
+      <c r="I63" t="s">
+        <v>248</v>
+      </c>
+      <c r="Q63" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="64" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
         <v>240</v>
       </c>
-      <c r="B63" t="s">
+      <c r="B64" t="s">
         <v>237</v>
       </c>
-      <c r="C63" s="2" t="s">
+      <c r="C64" s="2" t="s">
         <v>243</v>
       </c>
-      <c r="H63" t="s">
-        <v>16</v>
-      </c>
-      <c r="I63" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="64" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A64" s="1" t="s">
+      <c r="H64" t="s">
+        <v>16</v>
+      </c>
+      <c r="I64" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="65" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A65" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B64" t="s">
+      <c r="B65" t="s">
         <v>25</v>
       </c>
-      <c r="C64" s="2" t="s">
+      <c r="C65" s="2" t="s">
         <v>52</v>
-      </c>
-    </row>
-    <row r="65" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A65" t="s">
-        <v>232</v>
-      </c>
-      <c r="B65" t="s">
-        <v>250</v>
-      </c>
-      <c r="C65" s="2" t="s">
-        <v>231</v>
       </c>
     </row>
     <row r="66" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>390</v>
+        <v>232</v>
       </c>
       <c r="B66" t="s">
-        <v>83</v>
+        <v>250</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>392</v>
-      </c>
-      <c r="D66" t="s">
-        <v>391</v>
-      </c>
-      <c r="E66" t="s">
-        <v>9</v>
-      </c>
-      <c r="F66">
-        <v>2007</v>
-      </c>
-      <c r="G66">
-        <v>2015</v>
-      </c>
-      <c r="H66" t="s">
-        <v>348</v>
-      </c>
-      <c r="I66" t="s">
-        <v>349</v>
-      </c>
-      <c r="Q66" t="s">
-        <v>393</v>
+        <v>231</v>
       </c>
     </row>
     <row r="67" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>276</v>
+        <v>390</v>
       </c>
       <c r="B67" t="s">
-        <v>124</v>
+        <v>83</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>277</v>
+        <v>392</v>
+      </c>
+      <c r="D67" t="s">
+        <v>391</v>
+      </c>
+      <c r="E67" t="s">
+        <v>9</v>
       </c>
       <c r="F67">
-        <v>1948</v>
+        <v>2007</v>
       </c>
       <c r="G67">
-        <v>2000</v>
+        <v>2015</v>
       </c>
       <c r="H67" t="s">
-        <v>16</v>
+        <v>348</v>
       </c>
       <c r="I67" t="s">
-        <v>20</v>
+        <v>349</v>
+      </c>
+      <c r="Q67" t="s">
+        <v>393</v>
       </c>
     </row>
     <row r="68" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>449</v>
+        <v>276</v>
       </c>
       <c r="B68" t="s">
-        <v>250</v>
+        <v>124</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>448</v>
-      </c>
-      <c r="E68" t="s">
-        <v>14</v>
+        <v>277</v>
       </c>
       <c r="F68">
-        <v>-4000</v>
+        <v>1948</v>
       </c>
       <c r="G68">
         <v>2000</v>
       </c>
       <c r="H68" t="s">
-        <v>348</v>
+        <v>16</v>
       </c>
       <c r="I68" t="s">
-        <v>349</v>
-      </c>
-      <c r="J68" s="2" t="s">
-        <v>450</v>
-      </c>
-      <c r="N68" s="2" t="s">
-        <v>451</v>
+        <v>20</v>
       </c>
     </row>
     <row r="69" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>224</v>
+        <v>449</v>
       </c>
       <c r="B69" t="s">
-        <v>40</v>
+        <v>250</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>225</v>
+        <v>448</v>
+      </c>
+      <c r="E69" t="s">
+        <v>14</v>
       </c>
       <c r="F69">
-        <v>1964</v>
+        <v>-4000</v>
       </c>
       <c r="G69">
-        <v>2008</v>
+        <v>2000</v>
       </c>
       <c r="H69" t="s">
-        <v>16</v>
+        <v>348</v>
       </c>
       <c r="I69" t="s">
-        <v>20</v>
+        <v>349</v>
+      </c>
+      <c r="J69" s="2" t="s">
+        <v>450</v>
+      </c>
+      <c r="N69" s="2" t="s">
+        <v>451</v>
       </c>
     </row>
     <row r="70" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>285</v>
+        <v>224</v>
       </c>
       <c r="B70" t="s">
-        <v>250</v>
+        <v>40</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>286</v>
+        <v>225</v>
+      </c>
+      <c r="F70">
+        <v>1964</v>
+      </c>
+      <c r="G70">
+        <v>2008</v>
       </c>
       <c r="H70" t="s">
         <v>16</v>
@@ -3382,259 +3412,259 @@
     </row>
     <row r="71" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>205</v>
+        <v>285</v>
       </c>
       <c r="B71" t="s">
-        <v>40</v>
+        <v>250</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>204</v>
-      </c>
-      <c r="F71">
-        <v>2006</v>
+        <v>286</v>
+      </c>
+      <c r="H71" t="s">
+        <v>16</v>
+      </c>
+      <c r="I71" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="72" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>200</v>
+        <v>205</v>
       </c>
       <c r="B72" t="s">
-        <v>99</v>
+        <v>40</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="F72">
-        <v>1980</v>
-      </c>
-      <c r="G72">
-        <v>2007</v>
-      </c>
-      <c r="Q72" t="s">
-        <v>18</v>
+        <v>2006</v>
       </c>
     </row>
     <row r="73" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>468</v>
+        <v>200</v>
       </c>
       <c r="B73" t="s">
-        <v>40</v>
+        <v>99</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>464</v>
-      </c>
-      <c r="E73" t="s">
-        <v>14</v>
+        <v>201</v>
       </c>
       <c r="F73">
-        <v>1816</v>
+        <v>1980</v>
       </c>
       <c r="G73">
-        <v>2001</v>
-      </c>
-      <c r="H73" t="s">
-        <v>348</v>
-      </c>
-      <c r="I73" t="s">
-        <v>349</v>
-      </c>
-      <c r="J73" s="2" t="s">
-        <v>469</v>
-      </c>
-      <c r="K73" s="2" t="s">
-        <v>470</v>
-      </c>
-      <c r="L73" s="2" t="s">
-        <v>471</v>
+        <v>2007</v>
+      </c>
+      <c r="Q73" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="74" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>89</v>
+        <v>468</v>
       </c>
       <c r="B74" t="s">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>88</v>
+        <v>464</v>
       </c>
       <c r="E74" t="s">
-        <v>34</v>
+        <v>14</v>
       </c>
       <c r="F74">
-        <v>1972</v>
+        <v>1816</v>
+      </c>
+      <c r="G74">
+        <v>2001</v>
       </c>
       <c r="H74" t="s">
-        <v>16</v>
+        <v>348</v>
       </c>
       <c r="I74" t="s">
-        <v>20</v>
+        <v>349</v>
+      </c>
+      <c r="J74" s="2" t="s">
+        <v>469</v>
+      </c>
+      <c r="K74" s="2" t="s">
+        <v>470</v>
+      </c>
+      <c r="L74" s="2" t="s">
+        <v>471</v>
       </c>
     </row>
     <row r="75" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>104</v>
+        <v>89</v>
       </c>
       <c r="B75" t="s">
         <v>25</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>106</v>
+        <v>88</v>
       </c>
       <c r="E75" t="s">
-        <v>105</v>
+        <v>34</v>
       </c>
       <c r="F75">
-        <v>1980</v>
+        <v>1972</v>
+      </c>
+      <c r="H75" t="s">
+        <v>16</v>
+      </c>
+      <c r="I75" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="76" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>460</v>
+        <v>104</v>
       </c>
       <c r="B76" t="s">
         <v>25</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>461</v>
-      </c>
-      <c r="D76" t="s">
-        <v>363</v>
+        <v>106</v>
       </c>
       <c r="E76" t="s">
         <v>105</v>
       </c>
       <c r="F76">
-        <v>2009</v>
-      </c>
-      <c r="H76" t="s">
-        <v>348</v>
-      </c>
-      <c r="I76" t="s">
-        <v>301</v>
+        <v>1980</v>
       </c>
     </row>
     <row r="77" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>62</v>
+        <v>460</v>
       </c>
       <c r="B77" t="s">
         <v>25</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>63</v>
+        <v>461</v>
+      </c>
+      <c r="D77" t="s">
+        <v>363</v>
+      </c>
+      <c r="E77" t="s">
+        <v>105</v>
+      </c>
+      <c r="F77">
+        <v>2009</v>
+      </c>
+      <c r="H77" t="s">
+        <v>348</v>
+      </c>
+      <c r="I77" t="s">
+        <v>301</v>
       </c>
     </row>
     <row r="78" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>311</v>
+        <v>62</v>
       </c>
       <c r="B78" t="s">
-        <v>165</v>
+        <v>25</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>312</v>
-      </c>
-      <c r="E78" t="s">
-        <v>14</v>
-      </c>
-      <c r="H78" t="s">
-        <v>16</v>
-      </c>
-      <c r="I78" t="s">
-        <v>301</v>
+        <v>63</v>
       </c>
     </row>
     <row r="79" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>281</v>
+        <v>311</v>
       </c>
       <c r="B79" t="s">
-        <v>237</v>
+        <v>165</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>282</v>
+        <v>312</v>
+      </c>
+      <c r="E79" t="s">
+        <v>14</v>
       </c>
       <c r="H79" t="s">
         <v>16</v>
       </c>
       <c r="I79" t="s">
-        <v>20</v>
+        <v>301</v>
       </c>
     </row>
     <row r="80" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>418</v>
+        <v>281</v>
       </c>
       <c r="B80" t="s">
-        <v>86</v>
+        <v>237</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>419</v>
-      </c>
-      <c r="E80" t="s">
-        <v>420</v>
-      </c>
-      <c r="F80">
-        <v>1948</v>
-      </c>
-      <c r="G80">
-        <v>2012</v>
+        <v>282</v>
       </c>
       <c r="H80" t="s">
-        <v>348</v>
+        <v>16</v>
       </c>
       <c r="I80" t="s">
-        <v>349</v>
-      </c>
-      <c r="K80" s="2" t="s">
-        <v>421</v>
-      </c>
-      <c r="Q80" t="s">
-        <v>422</v>
+        <v>20</v>
       </c>
     </row>
     <row r="81" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>151</v>
+        <v>418</v>
       </c>
       <c r="B81" t="s">
-        <v>40</v>
+        <v>86</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>152</v>
+        <v>419</v>
       </c>
       <c r="E81" t="s">
-        <v>14</v>
+        <v>420</v>
+      </c>
+      <c r="F81">
+        <v>1948</v>
+      </c>
+      <c r="G81">
+        <v>2012</v>
+      </c>
+      <c r="H81" t="s">
+        <v>348</v>
+      </c>
+      <c r="I81" t="s">
+        <v>349</v>
+      </c>
+      <c r="K81" s="2" t="s">
+        <v>421</v>
+      </c>
+      <c r="Q81" t="s">
+        <v>422</v>
       </c>
     </row>
     <row r="82" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>242</v>
+        <v>151</v>
       </c>
       <c r="B82" t="s">
-        <v>237</v>
+        <v>40</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>243</v>
-      </c>
-      <c r="H82" t="s">
-        <v>16</v>
-      </c>
-      <c r="I82" t="s">
-        <v>20</v>
+        <v>152</v>
+      </c>
+      <c r="E82" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="83" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>292</v>
+        <v>242</v>
       </c>
       <c r="B83" t="s">
-        <v>99</v>
+        <v>237</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>291</v>
+        <v>243</v>
       </c>
       <c r="H83" t="s">
         <v>16</v>
@@ -3645,47 +3675,47 @@
     </row>
     <row r="84" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>153</v>
+        <v>292</v>
       </c>
       <c r="B84" t="s">
-        <v>259</v>
+        <v>99</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>154</v>
+        <v>291</v>
+      </c>
+      <c r="H84" t="s">
+        <v>16</v>
+      </c>
+      <c r="I84" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="85" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>228</v>
+        <v>153</v>
       </c>
       <c r="B85" t="s">
-        <v>40</v>
+        <v>259</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>225</v>
-      </c>
-      <c r="F85">
-        <v>1989</v>
-      </c>
-      <c r="G85">
-        <v>2017</v>
-      </c>
-      <c r="H85" t="s">
-        <v>16</v>
-      </c>
-      <c r="I85" t="s">
-        <v>20</v>
+        <v>154</v>
       </c>
     </row>
     <row r="86" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>245</v>
+        <v>228</v>
       </c>
       <c r="B86" t="s">
-        <v>237</v>
+        <v>40</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>244</v>
+        <v>225</v>
+      </c>
+      <c r="F86">
+        <v>1989</v>
+      </c>
+      <c r="G86">
+        <v>2017</v>
       </c>
       <c r="H86" t="s">
         <v>16</v>
@@ -3696,50 +3726,41 @@
     </row>
     <row r="87" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>100</v>
+        <v>245</v>
       </c>
       <c r="B87" t="s">
-        <v>99</v>
+        <v>237</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>101</v>
+        <v>244</v>
+      </c>
+      <c r="H87" t="s">
+        <v>16</v>
+      </c>
+      <c r="I87" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="88" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>239</v>
+        <v>100</v>
       </c>
       <c r="B88" t="s">
-        <v>237</v>
+        <v>99</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>243</v>
-      </c>
-      <c r="H88" t="s">
-        <v>16</v>
-      </c>
-      <c r="I88" t="s">
-        <v>20</v>
+        <v>101</v>
       </c>
     </row>
     <row r="89" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>254</v>
+        <v>239</v>
       </c>
       <c r="B89" t="s">
-        <v>55</v>
+        <v>237</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>253</v>
-      </c>
-      <c r="E89" t="s">
-        <v>255</v>
-      </c>
-      <c r="F89">
-        <v>1960</v>
-      </c>
-      <c r="G89">
-        <v>2014</v>
+        <v>243</v>
       </c>
       <c r="H89" t="s">
         <v>16</v>
@@ -3750,19 +3771,22 @@
     </row>
     <row r="90" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>270</v>
+        <v>254</v>
       </c>
       <c r="B90" t="s">
         <v>55</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>271</v>
+        <v>253</v>
+      </c>
+      <c r="E90" t="s">
+        <v>255</v>
       </c>
       <c r="F90">
-        <v>1990</v>
+        <v>1960</v>
       </c>
       <c r="G90">
-        <v>2010</v>
+        <v>2014</v>
       </c>
       <c r="H90" t="s">
         <v>16</v>
@@ -3773,96 +3797,90 @@
     </row>
     <row r="91" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>117</v>
+        <v>270</v>
       </c>
       <c r="B91" t="s">
         <v>55</v>
       </c>
       <c r="C91" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="F91">
+        <v>1990</v>
+      </c>
+      <c r="G91">
+        <v>2010</v>
+      </c>
+      <c r="H91" t="s">
+        <v>16</v>
+      </c>
+      <c r="I91" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="92" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A92" t="s">
+        <v>117</v>
+      </c>
+      <c r="B92" t="s">
+        <v>55</v>
+      </c>
+      <c r="C92" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="I91" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q91" t="s">
+      <c r="I92" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q92" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="92" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A92" s="1" t="s">
+    <row r="93" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A93" s="1" t="s">
         <v>23</v>
-      </c>
-      <c r="B92" t="s">
-        <v>25</v>
-      </c>
-      <c r="C92" s="2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="93" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A93" t="s">
-        <v>300</v>
       </c>
       <c r="B93" t="s">
         <v>25</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>298</v>
-      </c>
-      <c r="E93" t="s">
-        <v>299</v>
-      </c>
-      <c r="F93">
-        <v>1969</v>
-      </c>
-      <c r="H93" t="s">
-        <v>16</v>
-      </c>
-      <c r="I93" t="s">
-        <v>249</v>
+        <v>53</v>
       </c>
     </row>
     <row r="94" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>332</v>
+        <v>300</v>
       </c>
       <c r="B94" t="s">
-        <v>134</v>
+        <v>25</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>333</v>
+        <v>298</v>
       </c>
       <c r="E94" t="s">
-        <v>334</v>
+        <v>299</v>
+      </c>
+      <c r="F94">
+        <v>1969</v>
       </c>
       <c r="H94" t="s">
         <v>16</v>
       </c>
       <c r="I94" t="s">
-        <v>20</v>
+        <v>249</v>
       </c>
     </row>
     <row r="95" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>267</v>
+        <v>332</v>
       </c>
       <c r="B95" t="s">
-        <v>250</v>
+        <v>134</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>266</v>
-      </c>
-      <c r="D95" t="s">
-        <v>269</v>
+        <v>333</v>
       </c>
       <c r="E95" t="s">
-        <v>268</v>
-      </c>
-      <c r="F95">
-        <v>1970</v>
-      </c>
-      <c r="G95">
-        <v>2014</v>
+        <v>334</v>
       </c>
       <c r="H95" t="s">
         <v>16</v>
@@ -3873,97 +3891,100 @@
     </row>
     <row r="96" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>407</v>
+        <v>267</v>
       </c>
       <c r="B96" t="s">
-        <v>40</v>
+        <v>250</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>406</v>
+        <v>266</v>
       </c>
       <c r="D96" t="s">
-        <v>408</v>
+        <v>269</v>
       </c>
       <c r="E96" t="s">
-        <v>14</v>
+        <v>268</v>
       </c>
       <c r="F96">
-        <v>1949</v>
+        <v>1970</v>
       </c>
       <c r="G96">
-        <v>2013</v>
+        <v>2014</v>
       </c>
       <c r="H96" t="s">
-        <v>348</v>
+        <v>16</v>
       </c>
       <c r="I96" t="s">
-        <v>349</v>
+        <v>20</v>
       </c>
     </row>
     <row r="97" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>96</v>
+        <v>407</v>
       </c>
       <c r="B97" t="s">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>90</v>
+        <v>406</v>
+      </c>
+      <c r="D97" t="s">
+        <v>408</v>
       </c>
       <c r="E97" t="s">
-        <v>69</v>
+        <v>14</v>
       </c>
       <c r="F97">
-        <v>1995</v>
+        <v>1949</v>
+      </c>
+      <c r="G97">
+        <v>2013</v>
+      </c>
+      <c r="H97" t="s">
+        <v>348</v>
+      </c>
+      <c r="I97" t="s">
+        <v>349</v>
       </c>
     </row>
     <row r="98" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>404</v>
+        <v>96</v>
       </c>
       <c r="B98" t="s">
-        <v>83</v>
+        <v>25</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>403</v>
-      </c>
-      <c r="D98" t="s">
-        <v>405</v>
+        <v>90</v>
       </c>
       <c r="E98" t="s">
-        <v>14</v>
+        <v>69</v>
       </c>
       <c r="F98">
-        <v>1875</v>
-      </c>
-      <c r="G98">
-        <v>2004</v>
-      </c>
-      <c r="H98" t="s">
-        <v>348</v>
-      </c>
-      <c r="I98" t="s">
-        <v>349</v>
+        <v>1995</v>
       </c>
     </row>
     <row r="99" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>454</v>
+        <v>404</v>
       </c>
       <c r="B99" t="s">
-        <v>25</v>
+        <v>83</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>455</v>
+        <v>403</v>
+      </c>
+      <c r="D99" t="s">
+        <v>405</v>
       </c>
       <c r="E99" t="s">
-        <v>456</v>
+        <v>14</v>
       </c>
       <c r="F99">
-        <v>2006</v>
+        <v>1875</v>
       </c>
       <c r="G99">
-        <v>2016</v>
+        <v>2004</v>
       </c>
       <c r="H99" t="s">
         <v>348</v>
@@ -3971,80 +3992,83 @@
       <c r="I99" t="s">
         <v>349</v>
       </c>
-      <c r="J99" s="2" t="s">
-        <v>457</v>
-      </c>
-      <c r="L99" s="2" t="s">
-        <v>458</v>
-      </c>
-      <c r="Q99" t="s">
-        <v>459</v>
-      </c>
     </row>
     <row r="100" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>11</v>
+        <v>454</v>
       </c>
       <c r="B100" t="s">
         <v>25</v>
       </c>
       <c r="C100" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D100" t="s">
-        <v>95</v>
+        <v>455</v>
       </c>
       <c r="E100" t="s">
-        <v>10</v>
+        <v>456</v>
       </c>
       <c r="F100">
-        <v>2007</v>
+        <v>2006</v>
+      </c>
+      <c r="G100">
+        <v>2016</v>
       </c>
       <c r="H100" t="s">
-        <v>16</v>
+        <v>348</v>
       </c>
       <c r="I100" t="s">
-        <v>21</v>
+        <v>349</v>
+      </c>
+      <c r="J100" s="2" t="s">
+        <v>457</v>
+      </c>
+      <c r="L100" s="2" t="s">
+        <v>458</v>
+      </c>
+      <c r="Q100" t="s">
+        <v>459</v>
       </c>
     </row>
     <row r="101" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>223</v>
+        <v>11</v>
       </c>
       <c r="B101" t="s">
-        <v>124</v>
+        <v>25</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>222</v>
+        <v>12</v>
+      </c>
+      <c r="D101" t="s">
+        <v>95</v>
+      </c>
+      <c r="E101" t="s">
+        <v>10</v>
       </c>
       <c r="F101">
-        <v>1</v>
-      </c>
-      <c r="G101">
-        <v>2010</v>
+        <v>2007</v>
       </c>
       <c r="H101" t="s">
         <v>16</v>
       </c>
       <c r="I101" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="102" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="B102" t="s">
-        <v>40</v>
+        <v>124</v>
       </c>
       <c r="C102" s="2" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="F102">
-        <v>1946</v>
+        <v>1</v>
       </c>
       <c r="G102">
-        <v>2016</v>
+        <v>2010</v>
       </c>
       <c r="H102" t="s">
         <v>16</v>
@@ -4055,122 +4079,122 @@
     </row>
     <row r="103" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>97</v>
+        <v>226</v>
       </c>
       <c r="B103" t="s">
-        <v>128</v>
+        <v>40</v>
       </c>
       <c r="C103" s="2" t="s">
-        <v>98</v>
+        <v>225</v>
+      </c>
+      <c r="F103">
+        <v>1946</v>
+      </c>
+      <c r="G103">
+        <v>2016</v>
+      </c>
+      <c r="H103" t="s">
+        <v>16</v>
+      </c>
+      <c r="I103" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="104" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>278</v>
+        <v>97</v>
       </c>
       <c r="B104" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="C104" s="2" t="s">
-        <v>279</v>
-      </c>
-      <c r="E104" t="s">
-        <v>280</v>
-      </c>
-      <c r="F104">
-        <v>1890</v>
-      </c>
-      <c r="G104">
-        <v>1996</v>
-      </c>
-      <c r="H104" t="s">
-        <v>16</v>
-      </c>
-      <c r="I104" t="s">
-        <v>20</v>
+        <v>98</v>
       </c>
     </row>
     <row r="105" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>156</v>
+        <v>278</v>
       </c>
       <c r="B105" t="s">
-        <v>25</v>
+        <v>124</v>
       </c>
       <c r="C105" s="2" t="s">
-        <v>154</v>
+        <v>279</v>
+      </c>
+      <c r="E105" t="s">
+        <v>280</v>
+      </c>
+      <c r="F105">
+        <v>1890</v>
+      </c>
+      <c r="G105">
+        <v>1996</v>
+      </c>
+      <c r="H105" t="s">
+        <v>16</v>
+      </c>
+      <c r="I105" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="106" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>413</v>
+        <v>156</v>
       </c>
       <c r="B106" t="s">
-        <v>128</v>
+        <v>25</v>
       </c>
       <c r="C106" s="2" t="s">
-        <v>414</v>
-      </c>
-      <c r="E106" t="s">
-        <v>415</v>
-      </c>
-      <c r="F106">
-        <v>1946</v>
-      </c>
-      <c r="G106">
-        <v>2014</v>
-      </c>
-      <c r="H106" t="s">
-        <v>348</v>
-      </c>
-      <c r="I106" t="s">
-        <v>349</v>
-      </c>
-      <c r="N106" s="2" t="s">
-        <v>416</v>
-      </c>
-      <c r="Q106" t="s">
-        <v>417</v>
+        <v>154</v>
       </c>
     </row>
     <row r="107" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>229</v>
+        <v>413</v>
       </c>
       <c r="B107" t="s">
-        <v>40</v>
+        <v>128</v>
       </c>
       <c r="C107" s="2" t="s">
-        <v>225</v>
+        <v>414</v>
+      </c>
+      <c r="E107" t="s">
+        <v>415</v>
       </c>
       <c r="F107">
-        <v>1952</v>
+        <v>1946</v>
       </c>
       <c r="G107">
-        <v>1997</v>
+        <v>2014</v>
       </c>
       <c r="H107" t="s">
-        <v>16</v>
+        <v>348</v>
       </c>
       <c r="I107" t="s">
-        <v>20</v>
+        <v>349</v>
+      </c>
+      <c r="N107" s="2" t="s">
+        <v>416</v>
+      </c>
+      <c r="Q107" t="s">
+        <v>417</v>
       </c>
     </row>
     <row r="108" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>293</v>
+        <v>229</v>
       </c>
       <c r="B108" t="s">
         <v>40</v>
       </c>
       <c r="C108" s="2" t="s">
-        <v>294</v>
+        <v>225</v>
       </c>
       <c r="F108">
-        <v>2004</v>
+        <v>1952</v>
       </c>
       <c r="G108">
-        <v>2006</v>
+        <v>1997</v>
       </c>
       <c r="H108" t="s">
         <v>16</v>
@@ -4181,221 +4205,218 @@
     </row>
     <row r="109" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>102</v>
+        <v>293</v>
       </c>
       <c r="B109" t="s">
-        <v>99</v>
+        <v>40</v>
       </c>
       <c r="C109" s="2" t="s">
-        <v>103</v>
+        <v>294</v>
+      </c>
+      <c r="F109">
+        <v>2004</v>
+      </c>
+      <c r="G109">
+        <v>2006</v>
+      </c>
+      <c r="H109" t="s">
+        <v>16</v>
+      </c>
+      <c r="I109" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="110" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>289</v>
+        <v>102</v>
       </c>
       <c r="B110" t="s">
-        <v>124</v>
+        <v>99</v>
       </c>
       <c r="C110" s="2" t="s">
-        <v>290</v>
+        <v>103</v>
       </c>
     </row>
     <row r="111" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>246</v>
+        <v>289</v>
       </c>
       <c r="B111" t="s">
-        <v>165</v>
+        <v>124</v>
       </c>
       <c r="C111" s="2" t="s">
-        <v>247</v>
-      </c>
-      <c r="E111" t="s">
-        <v>14</v>
-      </c>
-      <c r="F111">
-        <v>1960</v>
-      </c>
-      <c r="G111">
-        <v>2006</v>
-      </c>
-      <c r="H111" t="s">
-        <v>16</v>
-      </c>
-      <c r="I111" t="s">
-        <v>249</v>
+        <v>290</v>
       </c>
     </row>
     <row r="112" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>365</v>
+        <v>246</v>
       </c>
       <c r="B112" t="s">
-        <v>128</v>
+        <v>165</v>
       </c>
       <c r="C112" s="2" t="s">
-        <v>364</v>
-      </c>
-      <c r="D112" t="s">
-        <v>370</v>
+        <v>247</v>
       </c>
       <c r="E112" t="s">
-        <v>366</v>
+        <v>14</v>
       </c>
       <c r="F112">
-        <v>1906</v>
+        <v>1960</v>
       </c>
       <c r="G112">
-        <v>2013</v>
+        <v>2006</v>
       </c>
       <c r="H112" t="s">
-        <v>367</v>
+        <v>16</v>
       </c>
       <c r="I112" t="s">
-        <v>368</v>
-      </c>
-      <c r="Q112" t="s">
-        <v>369</v>
+        <v>249</v>
       </c>
     </row>
     <row r="113" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>208</v>
+        <v>365</v>
       </c>
       <c r="B113" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="C113" s="2" t="s">
-        <v>209</v>
+        <v>364</v>
+      </c>
+      <c r="D113" t="s">
+        <v>370</v>
+      </c>
+      <c r="E113" t="s">
+        <v>366</v>
       </c>
       <c r="F113">
-        <v>1932</v>
+        <v>1906</v>
       </c>
       <c r="G113">
-        <v>2014</v>
+        <v>2013</v>
       </c>
       <c r="H113" t="s">
-        <v>16</v>
+        <v>367</v>
       </c>
       <c r="I113" t="s">
-        <v>20</v>
+        <v>368</v>
+      </c>
+      <c r="Q113" t="s">
+        <v>369</v>
       </c>
     </row>
     <row r="114" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>137</v>
+        <v>208</v>
       </c>
       <c r="B114" t="s">
-        <v>259</v>
+        <v>124</v>
       </c>
       <c r="C114" s="2" t="s">
-        <v>138</v>
+        <v>209</v>
+      </c>
+      <c r="F114">
+        <v>1932</v>
+      </c>
+      <c r="G114">
+        <v>2014</v>
+      </c>
+      <c r="H114" t="s">
+        <v>16</v>
+      </c>
+      <c r="I114" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="115" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>155</v>
+        <v>137</v>
       </c>
       <c r="B115" t="s">
         <v>259</v>
       </c>
       <c r="C115" s="2" t="s">
-        <v>154</v>
+        <v>138</v>
       </c>
     </row>
     <row r="116" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>57</v>
+        <v>155</v>
       </c>
       <c r="B116" t="s">
-        <v>128</v>
+        <v>259</v>
       </c>
       <c r="C116" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="Q116" t="s">
-        <v>17</v>
+        <v>154</v>
       </c>
     </row>
     <row r="117" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>129</v>
+        <v>57</v>
       </c>
       <c r="B117" t="s">
-        <v>259</v>
+        <v>128</v>
       </c>
       <c r="C117" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="E117" t="s">
-        <v>131</v>
-      </c>
-      <c r="F117">
-        <v>1945</v>
-      </c>
-      <c r="G117">
-        <v>2008</v>
-      </c>
-      <c r="I117" t="s">
-        <v>20</v>
+        <v>58</v>
+      </c>
+      <c r="Q117" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="118" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>148</v>
+        <v>129</v>
       </c>
       <c r="B118" t="s">
-        <v>128</v>
+        <v>259</v>
       </c>
       <c r="C118" s="2" t="s">
-        <v>147</v>
+        <v>130</v>
+      </c>
+      <c r="E118" t="s">
+        <v>131</v>
+      </c>
+      <c r="F118">
+        <v>1945</v>
+      </c>
+      <c r="G118">
+        <v>2008</v>
+      </c>
+      <c r="I118" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="119" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>233</v>
+        <v>148</v>
       </c>
       <c r="B119" t="s">
-        <v>165</v>
+        <v>128</v>
       </c>
       <c r="C119" s="2" t="s">
-        <v>234</v>
-      </c>
-      <c r="E119" t="s">
-        <v>14</v>
-      </c>
-      <c r="F119">
-        <v>2012</v>
-      </c>
-      <c r="G119">
-        <v>2016</v>
-      </c>
-      <c r="H119" t="s">
-        <v>16</v>
-      </c>
-      <c r="I119" t="s">
-        <v>20</v>
+        <v>147</v>
       </c>
     </row>
     <row r="120" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>35</v>
+        <v>233</v>
       </c>
       <c r="B120" t="s">
-        <v>25</v>
+        <v>165</v>
       </c>
       <c r="C120" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="D120" t="s">
-        <v>37</v>
+        <v>234</v>
       </c>
       <c r="E120" t="s">
         <v>14</v>
       </c>
       <c r="F120">
-        <v>2001</v>
+        <v>2012</v>
+      </c>
+      <c r="G120">
+        <v>2016</v>
       </c>
       <c r="H120" t="s">
         <v>16</v>
@@ -4406,148 +4427,148 @@
     </row>
     <row r="121" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>185</v>
+        <v>35</v>
       </c>
       <c r="B121" t="s">
-        <v>128</v>
+        <v>25</v>
       </c>
       <c r="C121" s="2" t="s">
-        <v>186</v>
+        <v>36</v>
+      </c>
+      <c r="D121" t="s">
+        <v>37</v>
+      </c>
+      <c r="E121" t="s">
+        <v>14</v>
+      </c>
+      <c r="F121">
+        <v>2001</v>
+      </c>
+      <c r="H121" t="s">
+        <v>16</v>
+      </c>
+      <c r="I121" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="122" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>210</v>
+        <v>185</v>
       </c>
       <c r="B122" t="s">
-        <v>40</v>
+        <v>128</v>
       </c>
       <c r="C122" s="2" t="s">
-        <v>211</v>
-      </c>
-      <c r="F122">
-        <v>1976</v>
-      </c>
-      <c r="G122">
-        <v>2016</v>
-      </c>
-      <c r="H122" t="s">
-        <v>16</v>
-      </c>
-      <c r="I122" t="s">
-        <v>20</v>
+        <v>186</v>
       </c>
     </row>
     <row r="123" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>426</v>
+        <v>210</v>
       </c>
       <c r="B123" t="s">
-        <v>86</v>
+        <v>40</v>
       </c>
       <c r="C123" s="2" t="s">
-        <v>427</v>
-      </c>
-      <c r="E123" t="s">
-        <v>34</v>
+        <v>211</v>
       </c>
       <c r="F123">
-        <v>2015</v>
+        <v>1976</v>
       </c>
       <c r="G123">
         <v>2016</v>
       </c>
       <c r="H123" t="s">
-        <v>348</v>
+        <v>16</v>
       </c>
       <c r="I123" t="s">
-        <v>349</v>
-      </c>
-      <c r="K123" s="2" t="s">
-        <v>428</v>
+        <v>20</v>
       </c>
     </row>
     <row r="124" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>144</v>
+        <v>426</v>
       </c>
       <c r="B124" t="s">
-        <v>60</v>
+        <v>86</v>
       </c>
       <c r="C124" s="2" t="s">
-        <v>143</v>
+        <v>427</v>
+      </c>
+      <c r="E124" t="s">
+        <v>34</v>
       </c>
       <c r="F124">
-        <v>1800</v>
+        <v>2015</v>
       </c>
       <c r="G124">
-        <v>2013</v>
+        <v>2016</v>
+      </c>
+      <c r="H124" t="s">
+        <v>348</v>
+      </c>
+      <c r="I124" t="s">
+        <v>349</v>
+      </c>
+      <c r="K124" s="2" t="s">
+        <v>428</v>
       </c>
     </row>
     <row r="125" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>472</v>
+        <v>144</v>
       </c>
       <c r="B125" t="s">
-        <v>25</v>
+        <v>60</v>
       </c>
       <c r="C125" s="2" t="s">
-        <v>473</v>
-      </c>
-      <c r="D125" t="s">
-        <v>474</v>
-      </c>
-      <c r="E125" t="s">
-        <v>112</v>
+        <v>143</v>
       </c>
       <c r="F125">
-        <v>1943</v>
-      </c>
-      <c r="H125" t="s">
-        <v>348</v>
-      </c>
-      <c r="I125" t="s">
-        <v>349</v>
-      </c>
-      <c r="N125" s="2" t="s">
-        <v>475</v>
+        <v>1800</v>
+      </c>
+      <c r="G125">
+        <v>2013</v>
       </c>
     </row>
     <row r="126" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>122</v>
+        <v>472</v>
       </c>
       <c r="B126" t="s">
-        <v>259</v>
+        <v>25</v>
       </c>
       <c r="C126" s="2" t="s">
-        <v>121</v>
+        <v>473</v>
+      </c>
+      <c r="D126" t="s">
+        <v>474</v>
+      </c>
+      <c r="E126" t="s">
+        <v>112</v>
+      </c>
+      <c r="F126">
+        <v>1943</v>
+      </c>
+      <c r="H126" t="s">
+        <v>348</v>
       </c>
       <c r="I126" t="s">
-        <v>20</v>
+        <v>349</v>
+      </c>
+      <c r="N126" s="2" t="s">
+        <v>475</v>
       </c>
     </row>
     <row r="127" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>318</v>
+        <v>122</v>
       </c>
       <c r="B127" t="s">
-        <v>250</v>
+        <v>259</v>
       </c>
       <c r="C127" s="2" t="s">
-        <v>319</v>
-      </c>
-      <c r="E127" t="s">
-        <v>320</v>
-      </c>
-      <c r="F127">
-        <v>1975</v>
-      </c>
-      <c r="G127">
-        <v>1989</v>
-      </c>
-      <c r="H127" t="s">
-        <v>16</v>
+        <v>121</v>
       </c>
       <c r="I127" t="s">
         <v>20</v>
@@ -4555,22 +4576,22 @@
     </row>
     <row r="128" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="B128" t="s">
         <v>250</v>
       </c>
       <c r="C128" s="2" t="s">
-        <v>317</v>
+        <v>319</v>
       </c>
       <c r="E128" t="s">
-        <v>105</v>
+        <v>320</v>
       </c>
       <c r="F128">
-        <v>1950</v>
+        <v>1975</v>
       </c>
       <c r="G128">
-        <v>1996</v>
+        <v>1989</v>
       </c>
       <c r="H128" t="s">
         <v>16</v>
@@ -4581,19 +4602,22 @@
     </row>
     <row r="129" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>322</v>
+        <v>316</v>
       </c>
       <c r="B129" t="s">
-        <v>25</v>
+        <v>250</v>
       </c>
       <c r="C129" s="2" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="E129" t="s">
-        <v>77</v>
+        <v>105</v>
       </c>
       <c r="F129">
-        <v>2010</v>
+        <v>1950</v>
+      </c>
+      <c r="G129">
+        <v>1996</v>
       </c>
       <c r="H129" t="s">
         <v>16</v>
@@ -4604,121 +4628,118 @@
     </row>
     <row r="130" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
-        <v>141</v>
+        <v>322</v>
       </c>
       <c r="B130" t="s">
-        <v>237</v>
+        <v>25</v>
       </c>
       <c r="C130" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="Q130" t="s">
-        <v>17</v>
+        <v>321</v>
+      </c>
+      <c r="E130" t="s">
+        <v>77</v>
+      </c>
+      <c r="F130">
+        <v>2010</v>
+      </c>
+      <c r="H130" t="s">
+        <v>16</v>
+      </c>
+      <c r="I130" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="131" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>308</v>
+        <v>141</v>
       </c>
       <c r="B131" t="s">
-        <v>250</v>
+        <v>237</v>
       </c>
       <c r="C131" s="2" t="s">
-        <v>309</v>
-      </c>
-      <c r="E131" t="s">
-        <v>310</v>
-      </c>
-      <c r="F131">
-        <v>1950</v>
-      </c>
-      <c r="G131">
-        <v>2010</v>
-      </c>
-      <c r="H131" t="s">
-        <v>16</v>
-      </c>
-      <c r="I131" t="s">
-        <v>20</v>
+        <v>142</v>
+      </c>
+      <c r="Q131" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="132" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>287</v>
+        <v>308</v>
       </c>
       <c r="B132" t="s">
-        <v>134</v>
+        <v>250</v>
       </c>
       <c r="C132" s="2" t="s">
-        <v>288</v>
+        <v>309</v>
+      </c>
+      <c r="E132" t="s">
+        <v>310</v>
       </c>
       <c r="F132">
-        <v>1990</v>
+        <v>1950</v>
       </c>
       <c r="G132">
-        <v>2008</v>
+        <v>2010</v>
+      </c>
+      <c r="H132" t="s">
+        <v>16</v>
+      </c>
+      <c r="I132" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="133" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
-        <v>274</v>
+        <v>287</v>
       </c>
       <c r="B133" t="s">
-        <v>55</v>
+        <v>134</v>
       </c>
       <c r="C133" s="2" t="s">
-        <v>275</v>
-      </c>
-      <c r="H133" t="s">
-        <v>16</v>
-      </c>
-      <c r="I133" t="s">
-        <v>20</v>
+        <v>288</v>
+      </c>
+      <c r="F133">
+        <v>1990</v>
+      </c>
+      <c r="G133">
+        <v>2008</v>
       </c>
     </row>
     <row r="134" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
-        <v>157</v>
+        <v>274</v>
       </c>
       <c r="B134" t="s">
-        <v>128</v>
+        <v>55</v>
       </c>
       <c r="C134" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="Q134" t="s">
-        <v>18</v>
+        <v>275</v>
+      </c>
+      <c r="H134" t="s">
+        <v>16</v>
+      </c>
+      <c r="I134" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="135" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
-        <v>439</v>
+        <v>157</v>
       </c>
       <c r="B135" t="s">
-        <v>259</v>
+        <v>128</v>
       </c>
       <c r="C135" s="2" t="s">
-        <v>438</v>
-      </c>
-      <c r="H135" t="s">
-        <v>348</v>
-      </c>
-      <c r="I135" t="s">
-        <v>349</v>
-      </c>
-      <c r="J135" s="2" t="s">
-        <v>440</v>
-      </c>
-      <c r="K135" s="2" t="s">
-        <v>442</v>
-      </c>
-      <c r="L135" s="2" t="s">
-        <v>441</v>
+        <v>154</v>
+      </c>
+      <c r="Q135" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="136" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
-        <v>443</v>
+        <v>439</v>
       </c>
       <c r="B136" t="s">
         <v>259</v>
@@ -4726,15 +4747,6 @@
       <c r="C136" s="2" t="s">
         <v>438</v>
       </c>
-      <c r="D136" t="s">
-        <v>447</v>
-      </c>
-      <c r="F136">
-        <v>1990</v>
-      </c>
-      <c r="G136">
-        <v>2014</v>
-      </c>
       <c r="H136" t="s">
         <v>348</v>
       </c>
@@ -4742,87 +4754,99 @@
         <v>349</v>
       </c>
       <c r="J136" s="2" t="s">
-        <v>444</v>
+        <v>440</v>
       </c>
       <c r="K136" s="2" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
       <c r="L136" s="2" t="s">
-        <v>446</v>
+        <v>441</v>
       </c>
     </row>
     <row r="137" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
-        <v>194</v>
+        <v>443</v>
       </c>
       <c r="B137" t="s">
-        <v>99</v>
+        <v>259</v>
       </c>
       <c r="C137" s="2" t="s">
-        <v>193</v>
+        <v>438</v>
+      </c>
+      <c r="D137" t="s">
+        <v>447</v>
+      </c>
+      <c r="F137">
+        <v>1990</v>
+      </c>
+      <c r="G137">
+        <v>2014</v>
+      </c>
+      <c r="H137" t="s">
+        <v>348</v>
+      </c>
+      <c r="I137" t="s">
+        <v>349</v>
+      </c>
+      <c r="J137" s="2" t="s">
+        <v>444</v>
+      </c>
+      <c r="K137" s="2" t="s">
+        <v>445</v>
+      </c>
+      <c r="L137" s="2" t="s">
+        <v>446</v>
       </c>
     </row>
     <row r="138" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
-        <v>295</v>
+        <v>194</v>
       </c>
       <c r="B138" t="s">
-        <v>40</v>
+        <v>99</v>
       </c>
       <c r="C138" s="2" t="s">
-        <v>296</v>
-      </c>
-      <c r="E138" t="s">
-        <v>297</v>
-      </c>
-      <c r="F138">
-        <v>1990</v>
-      </c>
-      <c r="G138">
-        <v>2015</v>
-      </c>
-      <c r="H138" t="s">
-        <v>16</v>
-      </c>
-      <c r="I138" t="s">
-        <v>249</v>
+        <v>193</v>
       </c>
     </row>
     <row r="139" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
-        <v>256</v>
+        <v>295</v>
       </c>
       <c r="B139" t="s">
-        <v>250</v>
+        <v>40</v>
       </c>
       <c r="C139" s="2" t="s">
-        <v>257</v>
+        <v>296</v>
       </c>
       <c r="E139" t="s">
-        <v>258</v>
+        <v>297</v>
+      </c>
+      <c r="F139">
+        <v>1990</v>
+      </c>
+      <c r="G139">
+        <v>2015</v>
       </c>
       <c r="H139" t="s">
         <v>16</v>
       </c>
       <c r="I139" t="s">
-        <v>20</v>
+        <v>249</v>
       </c>
     </row>
     <row r="140" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
-        <v>227</v>
+        <v>256</v>
       </c>
       <c r="B140" t="s">
-        <v>40</v>
+        <v>250</v>
       </c>
       <c r="C140" s="2" t="s">
-        <v>225</v>
-      </c>
-      <c r="F140">
-        <v>1955</v>
-      </c>
-      <c r="G140">
-        <v>2016</v>
+        <v>257</v>
+      </c>
+      <c r="E140" t="s">
+        <v>258</v>
       </c>
       <c r="H140" t="s">
         <v>16</v>
@@ -4833,7 +4857,7 @@
     </row>
     <row r="141" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="B141" t="s">
         <v>40</v>
@@ -4842,7 +4866,7 @@
         <v>225</v>
       </c>
       <c r="F141">
-        <v>1995</v>
+        <v>1955</v>
       </c>
       <c r="G141">
         <v>2016</v>
@@ -4856,657 +4880,709 @@
     </row>
     <row r="142" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
-        <v>452</v>
+        <v>230</v>
       </c>
       <c r="B142" t="s">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="C142" s="2" t="s">
-        <v>453</v>
-      </c>
-      <c r="E142" t="s">
-        <v>9</v>
+        <v>225</v>
+      </c>
+      <c r="F142">
+        <v>1995</v>
+      </c>
+      <c r="G142">
+        <v>2016</v>
       </c>
       <c r="H142" t="s">
-        <v>348</v>
+        <v>16</v>
       </c>
       <c r="I142" t="s">
-        <v>435</v>
+        <v>20</v>
       </c>
     </row>
     <row r="143" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
-        <v>109</v>
+        <v>452</v>
       </c>
       <c r="B143" t="s">
         <v>25</v>
       </c>
       <c r="C143" s="2" t="s">
-        <v>110</v>
+        <v>453</v>
       </c>
       <c r="E143" t="s">
-        <v>111</v>
-      </c>
-      <c r="F143">
-        <v>1956</v>
+        <v>9</v>
+      </c>
+      <c r="H143" t="s">
+        <v>348</v>
+      </c>
+      <c r="I143" t="s">
+        <v>435</v>
       </c>
     </row>
     <row r="144" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
-        <v>326</v>
+        <v>109</v>
       </c>
       <c r="B144" t="s">
         <v>25</v>
       </c>
       <c r="C144" s="2" t="s">
-        <v>327</v>
+        <v>110</v>
       </c>
       <c r="E144" t="s">
         <v>111</v>
       </c>
       <c r="F144">
-        <v>1998</v>
-      </c>
-      <c r="H144" t="s">
-        <v>16</v>
-      </c>
-      <c r="I144" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="145" spans="1:17" x14ac:dyDescent="0.2">
+        <v>1956</v>
+      </c>
+    </row>
+    <row r="145" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
-        <v>91</v>
+        <v>326</v>
       </c>
       <c r="B145" t="s">
         <v>25</v>
       </c>
       <c r="C145" s="2" t="s">
+        <v>327</v>
+      </c>
+      <c r="E145" t="s">
+        <v>111</v>
+      </c>
+      <c r="F145">
+        <v>1998</v>
+      </c>
+      <c r="H145" t="s">
+        <v>16</v>
+      </c>
+      <c r="I145" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="146" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A146" t="s">
+        <v>91</v>
+      </c>
+      <c r="B146" t="s">
+        <v>25</v>
+      </c>
+      <c r="C146" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="E145" t="s">
+      <c r="E146" t="s">
         <v>92</v>
       </c>
-      <c r="F145">
+      <c r="F146">
         <v>1999</v>
       </c>
     </row>
-    <row r="146" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A146" t="s">
+    <row r="147" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A147" t="s">
         <v>314</v>
       </c>
-      <c r="B146" t="s">
+      <c r="B147" t="s">
         <v>40</v>
       </c>
-      <c r="C146" s="2" t="s">
+      <c r="C147" s="2" t="s">
         <v>313</v>
       </c>
-      <c r="E146" t="s">
+      <c r="E147" t="s">
         <v>315</v>
       </c>
-      <c r="F146">
+      <c r="F147">
         <v>1950</v>
       </c>
-      <c r="G146">
+      <c r="G147">
         <v>2004</v>
       </c>
-      <c r="H146" t="s">
-        <v>16</v>
-      </c>
-      <c r="I146" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="147" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A147" t="s">
+      <c r="H147" t="s">
+        <v>16</v>
+      </c>
+      <c r="I147" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="148" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A148" t="s">
         <v>161</v>
       </c>
-      <c r="B147" t="s">
+      <c r="B148" t="s">
         <v>25</v>
       </c>
-      <c r="C147" s="2" t="s">
+      <c r="C148" s="2" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="148" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A148" t="s">
+    <row r="149" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A149" t="s">
         <v>168</v>
-      </c>
-      <c r="B148" t="s">
-        <v>40</v>
-      </c>
-      <c r="C148" s="2" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="149" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A149" t="s">
-        <v>399</v>
       </c>
       <c r="B149" t="s">
         <v>40</v>
       </c>
       <c r="C149" s="2" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="150" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A150" t="s">
+        <v>399</v>
+      </c>
+      <c r="B150" t="s">
+        <v>40</v>
+      </c>
+      <c r="C150" s="2" t="s">
         <v>400</v>
       </c>
-      <c r="E149" t="s">
+      <c r="E150" t="s">
         <v>14</v>
       </c>
-      <c r="F149">
+      <c r="F150">
         <v>2000</v>
       </c>
-      <c r="G149">
+      <c r="G150">
         <v>2014</v>
       </c>
-      <c r="H149" t="s">
+      <c r="H150" t="s">
         <v>348</v>
       </c>
-      <c r="I149" t="s">
+      <c r="I150" t="s">
         <v>349</v>
       </c>
-      <c r="J149" s="2" t="s">
+      <c r="J150" s="2" t="s">
         <v>402</v>
       </c>
-      <c r="N149" s="2" t="s">
+      <c r="N150" s="2" t="s">
         <v>401</v>
       </c>
     </row>
-    <row r="150" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A150" t="s">
+    <row r="151" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A151" t="s">
         <v>213</v>
       </c>
-      <c r="B150" t="s">
+      <c r="B151" t="s">
         <v>55</v>
       </c>
-      <c r="C150" s="2" t="s">
+      <c r="C151" s="2" t="s">
         <v>212</v>
       </c>
-      <c r="H150" t="s">
-        <v>16</v>
-      </c>
-      <c r="I150" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="151" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A151" t="s">
+      <c r="H151" t="s">
+        <v>16</v>
+      </c>
+      <c r="I151" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="152" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A152" t="s">
         <v>395</v>
-      </c>
-      <c r="B151" t="s">
-        <v>25</v>
-      </c>
-      <c r="C151" s="2" t="s">
-        <v>394</v>
-      </c>
-      <c r="D151" t="s">
-        <v>396</v>
-      </c>
-      <c r="E151" t="s">
-        <v>111</v>
-      </c>
-      <c r="F151">
-        <v>1986</v>
-      </c>
-      <c r="G151">
-        <v>2015</v>
-      </c>
-      <c r="H151" t="s">
-        <v>367</v>
-      </c>
-      <c r="I151" t="s">
-        <v>398</v>
-      </c>
-      <c r="J151" s="2" t="s">
-        <v>397</v>
-      </c>
-    </row>
-    <row r="152" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A152" t="s">
-        <v>323</v>
       </c>
       <c r="B152" t="s">
         <v>25</v>
       </c>
       <c r="C152" s="2" t="s">
+        <v>394</v>
+      </c>
+      <c r="D152" t="s">
+        <v>396</v>
+      </c>
+      <c r="E152" t="s">
+        <v>111</v>
+      </c>
+      <c r="F152">
+        <v>1986</v>
+      </c>
+      <c r="G152">
+        <v>2015</v>
+      </c>
+      <c r="H152" t="s">
+        <v>367</v>
+      </c>
+      <c r="I152" t="s">
+        <v>398</v>
+      </c>
+      <c r="J152" s="2" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="153" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A153" t="s">
+        <v>323</v>
+      </c>
+      <c r="B153" t="s">
+        <v>25</v>
+      </c>
+      <c r="C153" s="2" t="s">
         <v>324</v>
       </c>
-      <c r="E152" t="s">
+      <c r="E153" t="s">
         <v>325</v>
       </c>
-      <c r="F152">
+      <c r="F153">
         <v>1942</v>
       </c>
-      <c r="H152" t="s">
-        <v>16</v>
-      </c>
-      <c r="I152" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="153" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A153" t="s">
+      <c r="H153" t="s">
+        <v>16</v>
+      </c>
+      <c r="I153" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="154" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A154" t="s">
         <v>273</v>
       </c>
-      <c r="B153" t="s">
+      <c r="B154" t="s">
         <v>237</v>
       </c>
-      <c r="C153" s="2" t="s">
+      <c r="C154" s="2" t="s">
         <v>272</v>
       </c>
-      <c r="F153">
+      <c r="F154">
         <v>1996</v>
       </c>
-      <c r="G153">
+      <c r="G154">
         <v>2016</v>
       </c>
-      <c r="H153" t="s">
-        <v>16</v>
-      </c>
-      <c r="I153" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="154" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A154" t="s">
+      <c r="H154" t="s">
+        <v>16</v>
+      </c>
+      <c r="I154" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="155" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A155" t="s">
         <v>66</v>
       </c>
-      <c r="B154" t="s">
+      <c r="B155" t="s">
         <v>25</v>
       </c>
-      <c r="C154" s="2" t="s">
+      <c r="C155" s="2" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="155" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A155" t="s">
-        <v>383</v>
-      </c>
-      <c r="B155" t="s">
-        <v>40</v>
-      </c>
-      <c r="C155" s="2" t="s">
-        <v>384</v>
-      </c>
-      <c r="E155" t="s">
-        <v>386</v>
-      </c>
-      <c r="F155">
-        <v>1951</v>
-      </c>
-      <c r="H155" t="s">
-        <v>348</v>
-      </c>
-      <c r="I155" t="s">
-        <v>349</v>
-      </c>
-      <c r="N155" s="2" t="s">
-        <v>385</v>
-      </c>
-    </row>
-    <row r="156" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
-        <v>139</v>
+        <v>500</v>
       </c>
       <c r="B156" t="s">
         <v>40</v>
       </c>
       <c r="C156" s="2" t="s">
+        <v>499</v>
+      </c>
+      <c r="D156" t="s">
+        <v>501</v>
+      </c>
+      <c r="E156" t="s">
+        <v>14</v>
+      </c>
+      <c r="F156">
+        <v>1946</v>
+      </c>
+      <c r="G156">
+        <v>2015</v>
+      </c>
+      <c r="H156" t="s">
+        <v>348</v>
+      </c>
+      <c r="I156" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="157" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A157" t="s">
+        <v>383</v>
+      </c>
+      <c r="B157" t="s">
+        <v>40</v>
+      </c>
+      <c r="C157" s="2" t="s">
+        <v>384</v>
+      </c>
+      <c r="E157" t="s">
+        <v>386</v>
+      </c>
+      <c r="F157">
+        <v>1951</v>
+      </c>
+      <c r="H157" t="s">
+        <v>348</v>
+      </c>
+      <c r="I157" t="s">
+        <v>349</v>
+      </c>
+      <c r="N157" s="2" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="158" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A158" t="s">
+        <v>139</v>
+      </c>
+      <c r="B158" t="s">
+        <v>40</v>
+      </c>
+      <c r="C158" s="2" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="157" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A157" t="s">
+    <row r="159" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A159" t="s">
         <v>329</v>
       </c>
-      <c r="B157" t="s">
+      <c r="B159" t="s">
         <v>165</v>
       </c>
-      <c r="C157" s="2" t="s">
+      <c r="C159" s="2" t="s">
         <v>328</v>
       </c>
-      <c r="E157" t="s">
+      <c r="E159" t="s">
         <v>34</v>
       </c>
-      <c r="F157">
+      <c r="F159">
         <v>1789</v>
       </c>
-      <c r="H157" t="s">
-        <v>16</v>
-      </c>
-      <c r="I157" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="158" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A158" t="s">
+      <c r="H159" t="s">
+        <v>16</v>
+      </c>
+      <c r="I159" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="160" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A160" t="s">
         <v>172</v>
       </c>
-      <c r="B158" t="s">
+      <c r="B160" t="s">
         <v>60</v>
       </c>
-      <c r="C158" s="2" t="s">
+      <c r="C160" s="2" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="159" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A159" t="s">
+    <row r="161" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A161" t="s">
         <v>217</v>
       </c>
-      <c r="B159" t="s">
+      <c r="B161" t="s">
         <v>60</v>
       </c>
-      <c r="C159" s="2" t="s">
+      <c r="C161" s="2" t="s">
         <v>216</v>
       </c>
-      <c r="E159" t="s">
+      <c r="E161" t="s">
         <v>14</v>
       </c>
-      <c r="F159">
+      <c r="F161">
         <v>1900</v>
       </c>
-      <c r="H159" t="s">
-        <v>16</v>
-      </c>
-      <c r="I159" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="160" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A160" t="s">
+      <c r="H161" t="s">
+        <v>16</v>
+      </c>
+      <c r="I161" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="162" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A162" t="s">
         <v>132</v>
       </c>
-      <c r="B160" t="s">
+      <c r="B162" t="s">
         <v>259</v>
       </c>
-      <c r="C160" s="2" t="s">
+      <c r="C162" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="Q160" t="s">
+      <c r="Q162" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="161" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A161" t="s">
+    <row r="163" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A163" t="s">
         <v>182</v>
       </c>
-      <c r="B161" t="s">
+      <c r="B163" t="s">
         <v>165</v>
       </c>
-      <c r="C161" s="2" t="s">
+      <c r="C163" s="2" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="162" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A162" t="s">
+    <row r="164" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A164" t="s">
         <v>423</v>
       </c>
-      <c r="B162" t="s">
+      <c r="B164" t="s">
         <v>86</v>
       </c>
-      <c r="C162" s="2" t="s">
+      <c r="C164" s="2" t="s">
         <v>424</v>
       </c>
-      <c r="E162" t="s">
+      <c r="E164" t="s">
         <v>34</v>
       </c>
-      <c r="F162">
+      <c r="F164">
         <v>1996</v>
       </c>
-      <c r="G162">
+      <c r="G164">
         <v>2016</v>
       </c>
-      <c r="H162" t="s">
+      <c r="H164" t="s">
         <v>348</v>
       </c>
-      <c r="I162" t="s">
+      <c r="I164" t="s">
         <v>425</v>
       </c>
     </row>
-    <row r="163" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A163" t="s">
+    <row r="165" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A165" t="s">
         <v>115</v>
       </c>
-      <c r="B163" t="s">
+      <c r="B165" t="s">
         <v>128</v>
       </c>
-      <c r="C163" s="2" t="s">
+      <c r="C165" s="2" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="164" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A164" t="s">
+    <row r="166" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A166" t="s">
         <v>263</v>
       </c>
-      <c r="B164" t="s">
+      <c r="B166" t="s">
         <v>250</v>
       </c>
-      <c r="C164" s="2" t="s">
+      <c r="C166" s="2" t="s">
         <v>264</v>
       </c>
-      <c r="E164" t="s">
+      <c r="E166" t="s">
         <v>265</v>
       </c>
-      <c r="F164">
+      <c r="F166">
         <v>1500</v>
       </c>
-      <c r="G164">
+      <c r="G166">
         <v>2000</v>
       </c>
-      <c r="H164" t="s">
-        <v>16</v>
-      </c>
-      <c r="I164" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="165" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A165" t="s">
+      <c r="H166" t="s">
+        <v>16</v>
+      </c>
+      <c r="I166" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="167" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A167" t="s">
         <v>221</v>
       </c>
-      <c r="B165" t="s">
+      <c r="B167" t="s">
         <v>86</v>
       </c>
-      <c r="C165" s="2" t="s">
+      <c r="C167" s="2" t="s">
         <v>220</v>
       </c>
-      <c r="F165">
+      <c r="F167">
         <v>2013</v>
       </c>
-      <c r="H165" t="s">
-        <v>16</v>
-      </c>
-      <c r="I165" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="166" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A166" t="s">
+      <c r="H167" t="s">
+        <v>16</v>
+      </c>
+      <c r="I167" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="168" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A168" t="s">
         <v>13</v>
       </c>
-      <c r="B166" t="s">
+      <c r="B168" t="s">
         <v>25</v>
       </c>
-      <c r="C166" s="2" t="s">
+      <c r="C168" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="D166" s="1" t="s">
+      <c r="D168" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="E166" t="s">
+      <c r="E168" t="s">
         <v>14</v>
       </c>
-      <c r="F166">
+      <c r="F168">
         <v>1981</v>
       </c>
-      <c r="H166" t="s">
-        <v>16</v>
-      </c>
-      <c r="I166" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="167" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A167" t="s">
+      <c r="H168" t="s">
+        <v>16</v>
+      </c>
+      <c r="I168" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="169" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A169" t="s">
         <v>283</v>
       </c>
-      <c r="B167" t="s">
+      <c r="B169" t="s">
         <v>124</v>
       </c>
-      <c r="C167" s="2" t="s">
+      <c r="C169" s="2" t="s">
         <v>284</v>
       </c>
-      <c r="H167" t="s">
-        <v>16</v>
-      </c>
-      <c r="I167" t="s">
+      <c r="H169" t="s">
+        <v>16</v>
+      </c>
+      <c r="I169" t="s">
         <v>20</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:Q167">
+  <sortState ref="A2:Q169">
     <sortCondition ref="A2"/>
   </sortState>
   <hyperlinks>
     <hyperlink ref="C6" r:id="rId1"/>
-    <hyperlink ref="C62" r:id="rId2"/>
+    <hyperlink ref="C63" r:id="rId2"/>
     <hyperlink ref="C7" r:id="rId3"/>
     <hyperlink ref="C11" r:id="rId4"/>
-    <hyperlink ref="C100" r:id="rId5"/>
-    <hyperlink ref="C120" r:id="rId6"/>
-    <hyperlink ref="C166" r:id="rId7"/>
-    <hyperlink ref="C36" r:id="rId8"/>
-    <hyperlink ref="C31" r:id="rId9"/>
-    <hyperlink ref="C53" r:id="rId10"/>
-    <hyperlink ref="C60" r:id="rId11"/>
+    <hyperlink ref="C101" r:id="rId5"/>
+    <hyperlink ref="C121" r:id="rId6"/>
+    <hyperlink ref="C168" r:id="rId7"/>
+    <hyperlink ref="C37" r:id="rId8"/>
+    <hyperlink ref="C32" r:id="rId9"/>
+    <hyperlink ref="C54" r:id="rId10"/>
+    <hyperlink ref="C61" r:id="rId11"/>
     <hyperlink ref="C3" r:id="rId12"/>
     <hyperlink ref="C21" r:id="rId13"/>
-    <hyperlink ref="C64" r:id="rId14"/>
-    <hyperlink ref="C92" r:id="rId15"/>
-    <hyperlink ref="C30" r:id="rId16"/>
-    <hyperlink ref="C116" r:id="rId17"/>
-    <hyperlink ref="C44" r:id="rId18"/>
-    <hyperlink ref="C77" r:id="rId19"/>
+    <hyperlink ref="C65" r:id="rId14"/>
+    <hyperlink ref="C93" r:id="rId15"/>
+    <hyperlink ref="C31" r:id="rId16"/>
+    <hyperlink ref="C117" r:id="rId17"/>
+    <hyperlink ref="C45" r:id="rId18"/>
+    <hyperlink ref="C78" r:id="rId19"/>
     <hyperlink ref="C17" r:id="rId20"/>
-    <hyperlink ref="C154" r:id="rId21"/>
+    <hyperlink ref="C155" r:id="rId21"/>
     <hyperlink ref="C8" r:id="rId22"/>
-    <hyperlink ref="C40" r:id="rId23"/>
-    <hyperlink ref="C57" r:id="rId24"/>
-    <hyperlink ref="C54" r:id="rId25"/>
-    <hyperlink ref="C58" r:id="rId26"/>
-    <hyperlink ref="C59" r:id="rId27"/>
-    <hyperlink ref="C74" r:id="rId28"/>
-    <hyperlink ref="C97" r:id="rId29"/>
-    <hyperlink ref="C145" r:id="rId30"/>
-    <hyperlink ref="C103" r:id="rId31"/>
-    <hyperlink ref="C87" r:id="rId32"/>
-    <hyperlink ref="C109" r:id="rId33"/>
-    <hyperlink ref="C75" r:id="rId34"/>
+    <hyperlink ref="C41" r:id="rId23"/>
+    <hyperlink ref="C58" r:id="rId24"/>
+    <hyperlink ref="C55" r:id="rId25"/>
+    <hyperlink ref="C59" r:id="rId26"/>
+    <hyperlink ref="C60" r:id="rId27"/>
+    <hyperlink ref="C75" r:id="rId28"/>
+    <hyperlink ref="C98" r:id="rId29"/>
+    <hyperlink ref="C146" r:id="rId30"/>
+    <hyperlink ref="C104" r:id="rId31"/>
+    <hyperlink ref="C88" r:id="rId32"/>
+    <hyperlink ref="C110" r:id="rId33"/>
+    <hyperlink ref="C76" r:id="rId34"/>
     <hyperlink ref="C18" r:id="rId35"/>
-    <hyperlink ref="C143" r:id="rId36"/>
+    <hyperlink ref="C144" r:id="rId36"/>
     <hyperlink ref="C16" r:id="rId37"/>
-    <hyperlink ref="C163" r:id="rId38"/>
-    <hyperlink ref="C91" r:id="rId39"/>
-    <hyperlink ref="C61" r:id="rId40"/>
-    <hyperlink ref="C126" r:id="rId41"/>
+    <hyperlink ref="C165" r:id="rId38"/>
+    <hyperlink ref="C92" r:id="rId39"/>
+    <hyperlink ref="C62" r:id="rId40"/>
+    <hyperlink ref="C127" r:id="rId41"/>
     <hyperlink ref="C19" r:id="rId42"/>
-    <hyperlink ref="C55" r:id="rId43"/>
-    <hyperlink ref="C24" r:id="rId44"/>
-    <hyperlink ref="C117" r:id="rId45"/>
-    <hyperlink ref="C160" r:id="rId46"/>
-    <hyperlink ref="C28" r:id="rId47" display="http://comparativeconstitutionsproject.org/"/>
-    <hyperlink ref="C114" r:id="rId48"/>
-    <hyperlink ref="C156" r:id="rId49"/>
-    <hyperlink ref="C130" r:id="rId50"/>
-    <hyperlink ref="C124" r:id="rId51"/>
-    <hyperlink ref="C23" r:id="rId52"/>
-    <hyperlink ref="C118" r:id="rId53"/>
-    <hyperlink ref="C51" r:id="rId54"/>
-    <hyperlink ref="C81" r:id="rId55"/>
-    <hyperlink ref="C84" r:id="rId56"/>
-    <hyperlink ref="C115" r:id="rId57"/>
-    <hyperlink ref="C105" r:id="rId58"/>
-    <hyperlink ref="C134" r:id="rId59"/>
-    <hyperlink ref="C32" r:id="rId60"/>
-    <hyperlink ref="C147" r:id="rId61"/>
+    <hyperlink ref="C56" r:id="rId43"/>
+    <hyperlink ref="C25" r:id="rId44"/>
+    <hyperlink ref="C118" r:id="rId45"/>
+    <hyperlink ref="C162" r:id="rId46"/>
+    <hyperlink ref="C29" r:id="rId47" display="http://comparativeconstitutionsproject.org/"/>
+    <hyperlink ref="C115" r:id="rId48"/>
+    <hyperlink ref="C158" r:id="rId49"/>
+    <hyperlink ref="C131" r:id="rId50"/>
+    <hyperlink ref="C125" r:id="rId51"/>
+    <hyperlink ref="C24" r:id="rId52"/>
+    <hyperlink ref="C119" r:id="rId53"/>
+    <hyperlink ref="C52" r:id="rId54"/>
+    <hyperlink ref="C82" r:id="rId55"/>
+    <hyperlink ref="C85" r:id="rId56"/>
+    <hyperlink ref="C116" r:id="rId57"/>
+    <hyperlink ref="C106" r:id="rId58"/>
+    <hyperlink ref="C135" r:id="rId59"/>
+    <hyperlink ref="C33" r:id="rId60"/>
+    <hyperlink ref="C148" r:id="rId61"/>
     <hyperlink ref="C9" r:id="rId62"/>
-    <hyperlink ref="C34" r:id="rId63"/>
-    <hyperlink ref="C148" r:id="rId64"/>
+    <hyperlink ref="C35" r:id="rId63"/>
+    <hyperlink ref="C149" r:id="rId64"/>
     <hyperlink ref="C15" r:id="rId65"/>
-    <hyperlink ref="C158" r:id="rId66"/>
-    <hyperlink ref="C26" r:id="rId67"/>
-    <hyperlink ref="C25" r:id="rId68"/>
-    <hyperlink ref="C27" r:id="rId69"/>
-    <hyperlink ref="C56" r:id="rId70"/>
-    <hyperlink ref="C161" r:id="rId71"/>
-    <hyperlink ref="C29" r:id="rId72"/>
-    <hyperlink ref="C121" r:id="rId73"/>
-    <hyperlink ref="C33" r:id="rId74"/>
-    <hyperlink ref="C48" r:id="rId75"/>
-    <hyperlink ref="C137" r:id="rId76"/>
-    <hyperlink ref="C45" r:id="rId77"/>
-    <hyperlink ref="C41" r:id="rId78"/>
-    <hyperlink ref="C72" r:id="rId79"/>
+    <hyperlink ref="C160" r:id="rId66"/>
+    <hyperlink ref="C27" r:id="rId67"/>
+    <hyperlink ref="C26" r:id="rId68"/>
+    <hyperlink ref="C28" r:id="rId69"/>
+    <hyperlink ref="C57" r:id="rId70"/>
+    <hyperlink ref="C163" r:id="rId71"/>
+    <hyperlink ref="C30" r:id="rId72"/>
+    <hyperlink ref="C122" r:id="rId73"/>
+    <hyperlink ref="C34" r:id="rId74"/>
+    <hyperlink ref="C49" r:id="rId75"/>
+    <hyperlink ref="C138" r:id="rId76"/>
+    <hyperlink ref="C46" r:id="rId77"/>
+    <hyperlink ref="C42" r:id="rId78"/>
+    <hyperlink ref="C73" r:id="rId79"/>
     <hyperlink ref="C5" r:id="rId80"/>
-    <hyperlink ref="C71" r:id="rId81"/>
+    <hyperlink ref="C72" r:id="rId81"/>
     <hyperlink ref="C13" r:id="rId82"/>
-    <hyperlink ref="C113" r:id="rId83"/>
-    <hyperlink ref="C122" r:id="rId84"/>
-    <hyperlink ref="C150" r:id="rId85"/>
-    <hyperlink ref="C37" r:id="rId86"/>
-    <hyperlink ref="C159" r:id="rId87"/>
-    <hyperlink ref="C47" r:id="rId88"/>
-    <hyperlink ref="C165" r:id="rId89"/>
-    <hyperlink ref="C101" r:id="rId90"/>
-    <hyperlink ref="C69" r:id="rId91"/>
-    <hyperlink ref="C102" r:id="rId92"/>
-    <hyperlink ref="C140" r:id="rId93"/>
-    <hyperlink ref="C85" r:id="rId94"/>
-    <hyperlink ref="C107" r:id="rId95"/>
-    <hyperlink ref="C141" r:id="rId96"/>
-    <hyperlink ref="C65" r:id="rId97"/>
-    <hyperlink ref="C119" r:id="rId98"/>
-    <hyperlink ref="C49" r:id="rId99"/>
-    <hyperlink ref="C46" r:id="rId100"/>
-    <hyperlink ref="C88" r:id="rId101"/>
-    <hyperlink ref="C63" r:id="rId102"/>
+    <hyperlink ref="C114" r:id="rId83"/>
+    <hyperlink ref="C123" r:id="rId84"/>
+    <hyperlink ref="C151" r:id="rId85"/>
+    <hyperlink ref="C38" r:id="rId86"/>
+    <hyperlink ref="C161" r:id="rId87"/>
+    <hyperlink ref="C48" r:id="rId88"/>
+    <hyperlink ref="C167" r:id="rId89"/>
+    <hyperlink ref="C102" r:id="rId90"/>
+    <hyperlink ref="C70" r:id="rId91"/>
+    <hyperlink ref="C103" r:id="rId92"/>
+    <hyperlink ref="C141" r:id="rId93"/>
+    <hyperlink ref="C86" r:id="rId94"/>
+    <hyperlink ref="C108" r:id="rId95"/>
+    <hyperlink ref="C142" r:id="rId96"/>
+    <hyperlink ref="C66" r:id="rId97"/>
+    <hyperlink ref="C120" r:id="rId98"/>
+    <hyperlink ref="C50" r:id="rId99"/>
+    <hyperlink ref="C47" r:id="rId100"/>
+    <hyperlink ref="C89" r:id="rId101"/>
+    <hyperlink ref="C64" r:id="rId102"/>
     <hyperlink ref="C2" r:id="rId103"/>
-    <hyperlink ref="C82" r:id="rId104"/>
-    <hyperlink ref="C86" r:id="rId105"/>
-    <hyperlink ref="C111" r:id="rId106"/>
-    <hyperlink ref="C50" r:id="rId107"/>
-    <hyperlink ref="C89" r:id="rId108"/>
-    <hyperlink ref="C139" r:id="rId109"/>
+    <hyperlink ref="C83" r:id="rId104"/>
+    <hyperlink ref="C87" r:id="rId105"/>
+    <hyperlink ref="C112" r:id="rId106"/>
+    <hyperlink ref="C51" r:id="rId107"/>
+    <hyperlink ref="C90" r:id="rId108"/>
+    <hyperlink ref="C140" r:id="rId109"/>
     <hyperlink ref="C14" r:id="rId110"/>
     <hyperlink ref="C4" r:id="rId111"/>
-    <hyperlink ref="C164" r:id="rId112"/>
-    <hyperlink ref="C95" r:id="rId113"/>
-    <hyperlink ref="C90" r:id="rId114"/>
-    <hyperlink ref="C153" r:id="rId115"/>
-    <hyperlink ref="C133" r:id="rId116"/>
-    <hyperlink ref="C67" r:id="rId117"/>
-    <hyperlink ref="C104" r:id="rId118"/>
-    <hyperlink ref="C79" r:id="rId119"/>
-    <hyperlink ref="C167" r:id="rId120"/>
-    <hyperlink ref="C70" r:id="rId121"/>
-    <hyperlink ref="C132" r:id="rId122"/>
-    <hyperlink ref="C110" r:id="rId123"/>
-    <hyperlink ref="C83" r:id="rId124"/>
-    <hyperlink ref="C108" r:id="rId125"/>
-    <hyperlink ref="C138" r:id="rId126"/>
-    <hyperlink ref="C93" r:id="rId127"/>
+    <hyperlink ref="C166" r:id="rId112"/>
+    <hyperlink ref="C96" r:id="rId113"/>
+    <hyperlink ref="C91" r:id="rId114"/>
+    <hyperlink ref="C154" r:id="rId115"/>
+    <hyperlink ref="C134" r:id="rId116"/>
+    <hyperlink ref="C68" r:id="rId117"/>
+    <hyperlink ref="C105" r:id="rId118"/>
+    <hyperlink ref="C80" r:id="rId119"/>
+    <hyperlink ref="C169" r:id="rId120"/>
+    <hyperlink ref="C71" r:id="rId121"/>
+    <hyperlink ref="C133" r:id="rId122"/>
+    <hyperlink ref="C111" r:id="rId123"/>
+    <hyperlink ref="C84" r:id="rId124"/>
+    <hyperlink ref="C109" r:id="rId125"/>
+    <hyperlink ref="C139" r:id="rId126"/>
+    <hyperlink ref="C94" r:id="rId127"/>
     <hyperlink ref="C12" r:id="rId128"/>
     <hyperlink ref="C20" r:id="rId129"/>
-    <hyperlink ref="C131" r:id="rId130"/>
-    <hyperlink ref="C78" r:id="rId131"/>
-    <hyperlink ref="C146" r:id="rId132"/>
-    <hyperlink ref="C128" r:id="rId133"/>
-    <hyperlink ref="C127" r:id="rId134"/>
-    <hyperlink ref="C129" r:id="rId135"/>
-    <hyperlink ref="C152" r:id="rId136"/>
-    <hyperlink ref="C144" r:id="rId137"/>
-    <hyperlink ref="C157" r:id="rId138"/>
-    <hyperlink ref="C39" r:id="rId139"/>
-    <hyperlink ref="C94" r:id="rId140"/>
+    <hyperlink ref="C132" r:id="rId130"/>
+    <hyperlink ref="C79" r:id="rId131"/>
+    <hyperlink ref="C147" r:id="rId132"/>
+    <hyperlink ref="C129" r:id="rId133"/>
+    <hyperlink ref="C128" r:id="rId134"/>
+    <hyperlink ref="C130" r:id="rId135"/>
+    <hyperlink ref="C153" r:id="rId136"/>
+    <hyperlink ref="C145" r:id="rId137"/>
+    <hyperlink ref="C159" r:id="rId138"/>
+    <hyperlink ref="C40" r:id="rId139"/>
+    <hyperlink ref="C95" r:id="rId140"/>
     <hyperlink ref="J2" r:id="rId141"/>
     <hyperlink ref="M3" r:id="rId142"/>
     <hyperlink ref="J3" r:id="rId143"/>
@@ -5514,77 +5590,79 @@
     <hyperlink ref="J4" r:id="rId145"/>
     <hyperlink ref="P5" r:id="rId146"/>
     <hyperlink ref="J5" r:id="rId147"/>
-    <hyperlink ref="C112" r:id="rId148"/>
-    <hyperlink ref="C35" r:id="rId149"/>
+    <hyperlink ref="C113" r:id="rId148"/>
+    <hyperlink ref="C36" r:id="rId149"/>
     <hyperlink ref="P7" r:id="rId150"/>
     <hyperlink ref="J7" r:id="rId151"/>
     <hyperlink ref="M8" r:id="rId152"/>
     <hyperlink ref="L8" r:id="rId153"/>
     <hyperlink ref="J8" r:id="rId154"/>
-    <hyperlink ref="C155" r:id="rId155"/>
-    <hyperlink ref="N155" r:id="rId156"/>
+    <hyperlink ref="C157" r:id="rId155"/>
+    <hyperlink ref="N157" r:id="rId156"/>
     <hyperlink ref="C22" r:id="rId157"/>
     <hyperlink ref="N22" r:id="rId158"/>
-    <hyperlink ref="C66" r:id="rId159"/>
-    <hyperlink ref="C151" r:id="rId160"/>
-    <hyperlink ref="J151" r:id="rId161"/>
-    <hyperlink ref="C149" r:id="rId162"/>
-    <hyperlink ref="N149" r:id="rId163"/>
-    <hyperlink ref="J149" r:id="rId164"/>
-    <hyperlink ref="C98" r:id="rId165"/>
-    <hyperlink ref="C96" r:id="rId166"/>
-    <hyperlink ref="C42" r:id="rId167"/>
-    <hyperlink ref="J42" r:id="rId168"/>
-    <hyperlink ref="K42" r:id="rId169"/>
-    <hyperlink ref="C106" r:id="rId170"/>
-    <hyperlink ref="N106" r:id="rId171"/>
-    <hyperlink ref="C80" r:id="rId172"/>
-    <hyperlink ref="K80" r:id="rId173"/>
-    <hyperlink ref="C162" r:id="rId174"/>
-    <hyperlink ref="C123" r:id="rId175"/>
-    <hyperlink ref="K123" r:id="rId176"/>
+    <hyperlink ref="C67" r:id="rId159"/>
+    <hyperlink ref="C152" r:id="rId160"/>
+    <hyperlink ref="J152" r:id="rId161"/>
+    <hyperlink ref="C150" r:id="rId162"/>
+    <hyperlink ref="N150" r:id="rId163"/>
+    <hyperlink ref="J150" r:id="rId164"/>
+    <hyperlink ref="C99" r:id="rId165"/>
+    <hyperlink ref="C97" r:id="rId166"/>
+    <hyperlink ref="C43" r:id="rId167"/>
+    <hyperlink ref="J43" r:id="rId168"/>
+    <hyperlink ref="K43" r:id="rId169"/>
+    <hyperlink ref="C107" r:id="rId170"/>
+    <hyperlink ref="N107" r:id="rId171"/>
+    <hyperlink ref="C81" r:id="rId172"/>
+    <hyperlink ref="K81" r:id="rId173"/>
+    <hyperlink ref="C164" r:id="rId174"/>
+    <hyperlink ref="C124" r:id="rId175"/>
+    <hyperlink ref="K124" r:id="rId176"/>
     <hyperlink ref="L9" r:id="rId177"/>
     <hyperlink ref="J9" r:id="rId178"/>
     <hyperlink ref="J11" r:id="rId179"/>
-    <hyperlink ref="C135" r:id="rId180"/>
-    <hyperlink ref="J135" r:id="rId181"/>
-    <hyperlink ref="L135" r:id="rId182"/>
-    <hyperlink ref="K135" r:id="rId183"/>
-    <hyperlink ref="C136" r:id="rId184"/>
-    <hyperlink ref="J136" r:id="rId185"/>
-    <hyperlink ref="K136" r:id="rId186"/>
-    <hyperlink ref="L136" r:id="rId187"/>
-    <hyperlink ref="C68" r:id="rId188"/>
-    <hyperlink ref="J68" r:id="rId189"/>
-    <hyperlink ref="N68" r:id="rId190"/>
-    <hyperlink ref="C142" r:id="rId191"/>
-    <hyperlink ref="C99" r:id="rId192"/>
-    <hyperlink ref="J99" r:id="rId193"/>
-    <hyperlink ref="L99" r:id="rId194"/>
-    <hyperlink ref="C76" r:id="rId195"/>
-    <hyperlink ref="C52" r:id="rId196"/>
-    <hyperlink ref="L52" r:id="rId197"/>
-    <hyperlink ref="K52" r:id="rId198"/>
-    <hyperlink ref="J52" r:id="rId199"/>
-    <hyperlink ref="C73" r:id="rId200"/>
-    <hyperlink ref="J73" r:id="rId201"/>
-    <hyperlink ref="K73" r:id="rId202"/>
-    <hyperlink ref="L73" r:id="rId203"/>
-    <hyperlink ref="C125" r:id="rId204"/>
-    <hyperlink ref="N125" r:id="rId205"/>
-    <hyperlink ref="C38" r:id="rId206"/>
-    <hyperlink ref="K38" r:id="rId207"/>
-    <hyperlink ref="J38" r:id="rId208"/>
+    <hyperlink ref="C136" r:id="rId180"/>
+    <hyperlink ref="J136" r:id="rId181"/>
+    <hyperlink ref="L136" r:id="rId182"/>
+    <hyperlink ref="K136" r:id="rId183"/>
+    <hyperlink ref="C137" r:id="rId184"/>
+    <hyperlink ref="J137" r:id="rId185"/>
+    <hyperlink ref="K137" r:id="rId186"/>
+    <hyperlink ref="L137" r:id="rId187"/>
+    <hyperlink ref="C69" r:id="rId188"/>
+    <hyperlink ref="J69" r:id="rId189"/>
+    <hyperlink ref="N69" r:id="rId190"/>
+    <hyperlink ref="C143" r:id="rId191"/>
+    <hyperlink ref="C100" r:id="rId192"/>
+    <hyperlink ref="J100" r:id="rId193"/>
+    <hyperlink ref="L100" r:id="rId194"/>
+    <hyperlink ref="C77" r:id="rId195"/>
+    <hyperlink ref="C53" r:id="rId196"/>
+    <hyperlink ref="L53" r:id="rId197"/>
+    <hyperlink ref="K53" r:id="rId198"/>
+    <hyperlink ref="J53" r:id="rId199"/>
+    <hyperlink ref="C74" r:id="rId200"/>
+    <hyperlink ref="J74" r:id="rId201"/>
+    <hyperlink ref="K74" r:id="rId202"/>
+    <hyperlink ref="L74" r:id="rId203"/>
+    <hyperlink ref="C126" r:id="rId204"/>
+    <hyperlink ref="N126" r:id="rId205"/>
+    <hyperlink ref="C39" r:id="rId206"/>
+    <hyperlink ref="K39" r:id="rId207"/>
+    <hyperlink ref="J39" r:id="rId208"/>
     <hyperlink ref="C10" r:id="rId209"/>
     <hyperlink ref="J10" r:id="rId210"/>
     <hyperlink ref="P10" r:id="rId211"/>
     <hyperlink ref="N10" r:id="rId212"/>
-    <hyperlink ref="C43" r:id="rId213"/>
-    <hyperlink ref="J43" r:id="rId214"/>
-    <hyperlink ref="K43" r:id="rId215"/>
-    <hyperlink ref="L43" r:id="rId216"/>
-    <hyperlink ref="M43" r:id="rId217"/>
-    <hyperlink ref="N43" r:id="rId218"/>
+    <hyperlink ref="C44" r:id="rId213"/>
+    <hyperlink ref="J44" r:id="rId214"/>
+    <hyperlink ref="K44" r:id="rId215"/>
+    <hyperlink ref="L44" r:id="rId216"/>
+    <hyperlink ref="M44" r:id="rId217"/>
+    <hyperlink ref="N44" r:id="rId218"/>
+    <hyperlink ref="C23" r:id="rId219"/>
+    <hyperlink ref="C156" r:id="rId220"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
add Correlates of State Policy
</commit_message>
<xml_diff>
--- a/PolData.xlsx
+++ b/PolData.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="913" uniqueCount="502">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="923" uniqueCount="508">
   <si>
     <t>name</t>
   </si>
@@ -1533,6 +1533,24 @@
   </si>
   <si>
     <t>United Nations, roll-calls</t>
+  </si>
+  <si>
+    <t>http://www.ippsr.msu.edu/public-policy/correlates-state-policy</t>
+  </si>
+  <si>
+    <t>Correlates of State Policy</t>
+  </si>
+  <si>
+    <t>http://ippsr.msu.edu/sites/default/files/CorrelatesCodebook.pdf</t>
+  </si>
+  <si>
+    <t>http://ippsr.msu.edu/sites/default/files/correlatesofstatepolicyprojectv1_13.xlsx</t>
+  </si>
+  <si>
+    <t>http://ippsr.msu.edu/sites/default/files/correlatesofstatepolicyprojectv1_13.dta</t>
+  </si>
+  <si>
+    <t>http://ippsr.msu.edu/sites/default/files/correlatesofstatepolicyprojectv1_13.csv</t>
   </si>
 </sst>
 </file>
@@ -1872,10 +1890,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q169"/>
+  <dimension ref="A1:Q170"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+    <sheetView tabSelected="1" topLeftCell="A133" workbookViewId="0">
+      <selection activeCell="E38" sqref="E38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2732,42 +2750,60 @@
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>39</v>
+        <v>503</v>
       </c>
       <c r="B37" t="s">
-        <v>40</v>
+        <v>99</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>41</v>
+        <v>502</v>
       </c>
       <c r="E37" t="s">
-        <v>14</v>
+        <v>34</v>
       </c>
       <c r="F37">
-        <v>1816</v>
+        <v>1900</v>
       </c>
       <c r="G37">
-        <v>2007</v>
+        <v>2016</v>
       </c>
       <c r="H37" t="s">
-        <v>16</v>
+        <v>348</v>
       </c>
       <c r="I37" t="s">
-        <v>20</v>
+        <v>349</v>
+      </c>
+      <c r="J37" s="2" t="s">
+        <v>504</v>
+      </c>
+      <c r="K37" s="2" t="s">
+        <v>507</v>
+      </c>
+      <c r="L37" s="2" t="s">
+        <v>506</v>
+      </c>
+      <c r="N37" s="2" t="s">
+        <v>505</v>
       </c>
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>215</v>
+        <v>39</v>
       </c>
       <c r="B38" t="s">
-        <v>237</v>
+        <v>40</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>214</v>
+        <v>41</v>
+      </c>
+      <c r="E38" t="s">
+        <v>14</v>
       </c>
       <c r="F38">
-        <v>1995</v>
+        <v>1816</v>
+      </c>
+      <c r="G38">
+        <v>2007</v>
       </c>
       <c r="H38" t="s">
         <v>16</v>
@@ -2778,140 +2814,134 @@
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>476</v>
+        <v>215</v>
       </c>
       <c r="B39" t="s">
-        <v>40</v>
+        <v>237</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>477</v>
-      </c>
-      <c r="D39" t="s">
-        <v>478</v>
-      </c>
-      <c r="E39" t="s">
-        <v>14</v>
+        <v>214</v>
       </c>
       <c r="F39">
-        <v>2002</v>
+        <v>1995</v>
       </c>
       <c r="H39" t="s">
-        <v>348</v>
+        <v>16</v>
       </c>
       <c r="I39" t="s">
-        <v>349</v>
-      </c>
-      <c r="J39" s="2" t="s">
-        <v>480</v>
-      </c>
-      <c r="K39" s="2" t="s">
-        <v>479</v>
+        <v>20</v>
       </c>
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>330</v>
+        <v>476</v>
       </c>
       <c r="B40" t="s">
-        <v>165</v>
+        <v>40</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>331</v>
+        <v>477</v>
+      </c>
+      <c r="D40" t="s">
+        <v>478</v>
       </c>
       <c r="E40" t="s">
-        <v>77</v>
+        <v>14</v>
       </c>
       <c r="F40">
-        <v>1953</v>
+        <v>2002</v>
       </c>
       <c r="H40" t="s">
-        <v>16</v>
+        <v>348</v>
       </c>
       <c r="I40" t="s">
-        <v>20</v>
+        <v>349</v>
+      </c>
+      <c r="J40" s="2" t="s">
+        <v>480</v>
+      </c>
+      <c r="K40" s="2" t="s">
+        <v>479</v>
       </c>
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>75</v>
+        <v>330</v>
       </c>
       <c r="B41" t="s">
-        <v>25</v>
+        <v>165</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>76</v>
+        <v>331</v>
       </c>
       <c r="E41" t="s">
         <v>77</v>
       </c>
       <c r="F41">
-        <v>1971</v>
+        <v>1953</v>
+      </c>
+      <c r="H41" t="s">
+        <v>16</v>
+      </c>
+      <c r="I41" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>197</v>
+        <v>75</v>
       </c>
       <c r="B42" t="s">
-        <v>55</v>
+        <v>25</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>198</v>
+        <v>76</v>
       </c>
       <c r="E42" t="s">
-        <v>199</v>
+        <v>77</v>
       </c>
       <c r="F42">
-        <v>1975</v>
-      </c>
-      <c r="G42">
-        <v>2015</v>
-      </c>
-      <c r="H42" t="s">
-        <v>16</v>
-      </c>
-      <c r="I42" t="s">
-        <v>20</v>
+        <v>1971</v>
       </c>
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>409</v>
+        <v>197</v>
       </c>
       <c r="B43" t="s">
-        <v>250</v>
+        <v>55</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>410</v>
+        <v>198</v>
       </c>
       <c r="E43" t="s">
-        <v>9</v>
+        <v>199</v>
+      </c>
+      <c r="F43">
+        <v>1975</v>
+      </c>
+      <c r="G43">
+        <v>2015</v>
       </c>
       <c r="H43" t="s">
-        <v>348</v>
+        <v>16</v>
       </c>
       <c r="I43" t="s">
-        <v>349</v>
-      </c>
-      <c r="J43" s="2" t="s">
-        <v>411</v>
-      </c>
-      <c r="K43" s="2" t="s">
-        <v>412</v>
+        <v>20</v>
       </c>
     </row>
     <row r="44" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>489</v>
+        <v>409</v>
       </c>
       <c r="B44" t="s">
-        <v>60</v>
+        <v>250</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>488</v>
+        <v>410</v>
       </c>
       <c r="E44" t="s">
-        <v>490</v>
+        <v>9</v>
       </c>
       <c r="H44" t="s">
         <v>348</v>
@@ -2920,81 +2950,84 @@
         <v>349</v>
       </c>
       <c r="J44" s="2" t="s">
-        <v>491</v>
+        <v>411</v>
       </c>
       <c r="K44" s="2" t="s">
-        <v>492</v>
-      </c>
-      <c r="L44" s="2" t="s">
-        <v>493</v>
-      </c>
-      <c r="M44" s="2" t="s">
-        <v>494</v>
-      </c>
-      <c r="N44" s="2" t="s">
-        <v>495</v>
+        <v>412</v>
       </c>
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>59</v>
+        <v>489</v>
       </c>
       <c r="B45" t="s">
         <v>60</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>61</v>
+        <v>488</v>
+      </c>
+      <c r="E45" t="s">
+        <v>490</v>
+      </c>
+      <c r="H45" t="s">
+        <v>348</v>
+      </c>
+      <c r="I45" t="s">
+        <v>349</v>
+      </c>
+      <c r="J45" s="2" t="s">
+        <v>491</v>
+      </c>
+      <c r="K45" s="2" t="s">
+        <v>492</v>
+      </c>
+      <c r="L45" s="2" t="s">
+        <v>493</v>
+      </c>
+      <c r="M45" s="2" t="s">
+        <v>494</v>
+      </c>
+      <c r="N45" s="2" t="s">
+        <v>495</v>
       </c>
     </row>
     <row r="46" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>196</v>
+        <v>59</v>
       </c>
       <c r="B46" t="s">
-        <v>165</v>
+        <v>60</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>195</v>
-      </c>
-      <c r="F46">
-        <v>1946</v>
-      </c>
-      <c r="G46">
-        <v>2016</v>
+        <v>61</v>
       </c>
     </row>
     <row r="47" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>238</v>
+        <v>196</v>
       </c>
       <c r="B47" t="s">
-        <v>237</v>
+        <v>165</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>243</v>
-      </c>
-      <c r="H47" t="s">
-        <v>16</v>
-      </c>
-      <c r="I47" t="s">
-        <v>20</v>
+        <v>195</v>
+      </c>
+      <c r="F47">
+        <v>1946</v>
+      </c>
+      <c r="G47">
+        <v>2016</v>
       </c>
     </row>
     <row r="48" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>219</v>
+        <v>238</v>
       </c>
       <c r="B48" t="s">
-        <v>124</v>
+        <v>237</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>218</v>
-      </c>
-      <c r="F48">
-        <v>1970</v>
-      </c>
-      <c r="G48">
-        <v>2015</v>
+        <v>243</v>
       </c>
       <c r="H48" t="s">
         <v>16</v>
@@ -3005,44 +3038,50 @@
     </row>
     <row r="49" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>191</v>
+        <v>219</v>
       </c>
       <c r="B49" t="s">
-        <v>25</v>
+        <v>124</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="E49" t="s">
-        <v>192</v>
+        <v>218</v>
+      </c>
+      <c r="F49">
+        <v>1970</v>
+      </c>
+      <c r="G49">
+        <v>2015</v>
+      </c>
+      <c r="H49" t="s">
+        <v>16</v>
+      </c>
+      <c r="I49" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="50" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>235</v>
+        <v>191</v>
       </c>
       <c r="B50" t="s">
-        <v>60</v>
+        <v>25</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>236</v>
-      </c>
-      <c r="H50" t="s">
-        <v>16</v>
-      </c>
-      <c r="I50" t="s">
-        <v>20</v>
+        <v>190</v>
+      </c>
+      <c r="E50" t="s">
+        <v>192</v>
       </c>
     </row>
     <row r="51" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>252</v>
+        <v>235</v>
       </c>
       <c r="B51" t="s">
-        <v>250</v>
+        <v>60</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>251</v>
+        <v>236</v>
       </c>
       <c r="H51" t="s">
         <v>16</v>
@@ -3053,129 +3092,129 @@
     </row>
     <row r="52" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>149</v>
+        <v>252</v>
       </c>
       <c r="B52" t="s">
-        <v>128</v>
+        <v>250</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>150</v>
+        <v>251</v>
+      </c>
+      <c r="H52" t="s">
+        <v>16</v>
+      </c>
+      <c r="I52" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="53" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>462</v>
+        <v>149</v>
       </c>
       <c r="B53" t="s">
-        <v>250</v>
+        <v>128</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>464</v>
-      </c>
-      <c r="D53" t="s">
-        <v>463</v>
-      </c>
-      <c r="E53" t="s">
-        <v>14</v>
-      </c>
-      <c r="F53">
-        <v>1946</v>
-      </c>
-      <c r="G53">
-        <v>2010</v>
-      </c>
-      <c r="H53" t="s">
-        <v>348</v>
-      </c>
-      <c r="I53" t="s">
-        <v>349</v>
-      </c>
-      <c r="J53" s="2" t="s">
-        <v>467</v>
-      </c>
-      <c r="K53" s="2" t="s">
-        <v>466</v>
-      </c>
-      <c r="L53" s="2" t="s">
-        <v>465</v>
+        <v>150</v>
       </c>
     </row>
     <row r="54" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>28</v>
+        <v>462</v>
       </c>
       <c r="B54" t="s">
-        <v>25</v>
+        <v>250</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>48</v>
+        <v>464</v>
+      </c>
+      <c r="D54" t="s">
+        <v>463</v>
+      </c>
+      <c r="E54" t="s">
+        <v>14</v>
+      </c>
+      <c r="F54">
+        <v>1946</v>
+      </c>
+      <c r="G54">
+        <v>2010</v>
+      </c>
+      <c r="H54" t="s">
+        <v>348</v>
+      </c>
+      <c r="I54" t="s">
+        <v>349</v>
+      </c>
+      <c r="J54" s="2" t="s">
+        <v>467</v>
+      </c>
+      <c r="K54" s="2" t="s">
+        <v>466</v>
+      </c>
+      <c r="L54" s="2" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="55" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>80</v>
+        <v>28</v>
       </c>
       <c r="B55" t="s">
-        <v>128</v>
+        <v>25</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="E55" t="s">
-        <v>9</v>
-      </c>
-      <c r="F55">
-        <v>1979</v>
+        <v>48</v>
       </c>
     </row>
     <row r="56" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>125</v>
+        <v>80</v>
       </c>
       <c r="B56" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>126</v>
+        <v>81</v>
+      </c>
+      <c r="E56" t="s">
+        <v>9</v>
+      </c>
+      <c r="F56">
+        <v>1979</v>
       </c>
     </row>
     <row r="57" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>179</v>
+        <v>125</v>
       </c>
       <c r="B57" t="s">
-        <v>165</v>
+        <v>124</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>180</v>
+        <v>126</v>
       </c>
     </row>
     <row r="58" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
+        <v>179</v>
+      </c>
+      <c r="B58" t="s">
+        <v>165</v>
+      </c>
+      <c r="C58" s="2" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="59" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
         <v>78</v>
       </c>
-      <c r="B58" t="s">
+      <c r="B59" t="s">
         <v>25</v>
       </c>
-      <c r="C58" s="2" t="s">
+      <c r="C59" s="2" t="s">
         <v>79</v>
-      </c>
-      <c r="E58" t="s">
-        <v>9</v>
-      </c>
-      <c r="F58">
-        <v>1979</v>
-      </c>
-    </row>
-    <row r="59" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A59" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="B59" t="s">
-        <v>83</v>
-      </c>
-      <c r="C59" s="2" t="s">
-        <v>84</v>
       </c>
       <c r="E59" t="s">
         <v>9</v>
@@ -3186,13 +3225,13 @@
     </row>
     <row r="60" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A60" s="3" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B60" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="E60" t="s">
         <v>9</v>
@@ -3200,225 +3239,225 @@
       <c r="F60">
         <v>1979</v>
       </c>
-      <c r="G60">
+    </row>
+    <row r="61" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A61" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="B61" t="s">
+        <v>86</v>
+      </c>
+      <c r="C61" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="E61" t="s">
+        <v>9</v>
+      </c>
+      <c r="F61">
+        <v>1979</v>
+      </c>
+      <c r="G61">
         <v>2009</v>
-      </c>
-    </row>
-    <row r="61" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A61" t="s">
-        <v>27</v>
-      </c>
-      <c r="B61" t="s">
-        <v>25</v>
-      </c>
-      <c r="C61" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="Q61" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="62" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>120</v>
+        <v>27</v>
       </c>
       <c r="B62" t="s">
-        <v>259</v>
+        <v>25</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="I62" t="s">
-        <v>20</v>
+        <v>49</v>
+      </c>
+      <c r="Q62" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="63" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>5</v>
+        <v>120</v>
       </c>
       <c r="B63" t="s">
-        <v>25</v>
+        <v>259</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D63" t="s">
-        <v>94</v>
-      </c>
-      <c r="E63" t="s">
-        <v>9</v>
-      </c>
-      <c r="F63">
-        <v>2002</v>
-      </c>
-      <c r="H63" t="s">
-        <v>16</v>
+        <v>119</v>
       </c>
       <c r="I63" t="s">
-        <v>248</v>
-      </c>
-      <c r="Q63" t="s">
-        <v>44</v>
+        <v>20</v>
       </c>
     </row>
     <row r="64" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
+        <v>5</v>
+      </c>
+      <c r="B64" t="s">
+        <v>25</v>
+      </c>
+      <c r="C64" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D64" t="s">
+        <v>94</v>
+      </c>
+      <c r="E64" t="s">
+        <v>9</v>
+      </c>
+      <c r="F64">
+        <v>2002</v>
+      </c>
+      <c r="H64" t="s">
+        <v>16</v>
+      </c>
+      <c r="I64" t="s">
+        <v>248</v>
+      </c>
+      <c r="Q64" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="65" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
         <v>240</v>
       </c>
-      <c r="B64" t="s">
+      <c r="B65" t="s">
         <v>237</v>
       </c>
-      <c r="C64" s="2" t="s">
+      <c r="C65" s="2" t="s">
         <v>243</v>
       </c>
-      <c r="H64" t="s">
-        <v>16</v>
-      </c>
-      <c r="I64" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="65" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A65" s="1" t="s">
+      <c r="H65" t="s">
+        <v>16</v>
+      </c>
+      <c r="I65" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="66" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A66" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B65" t="s">
+      <c r="B66" t="s">
         <v>25</v>
       </c>
-      <c r="C65" s="2" t="s">
+      <c r="C66" s="2" t="s">
         <v>52</v>
-      </c>
-    </row>
-    <row r="66" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A66" t="s">
-        <v>232</v>
-      </c>
-      <c r="B66" t="s">
-        <v>250</v>
-      </c>
-      <c r="C66" s="2" t="s">
-        <v>231</v>
       </c>
     </row>
     <row r="67" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>390</v>
+        <v>232</v>
       </c>
       <c r="B67" t="s">
-        <v>83</v>
+        <v>250</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>392</v>
-      </c>
-      <c r="D67" t="s">
-        <v>391</v>
-      </c>
-      <c r="E67" t="s">
-        <v>9</v>
-      </c>
-      <c r="F67">
-        <v>2007</v>
-      </c>
-      <c r="G67">
-        <v>2015</v>
-      </c>
-      <c r="H67" t="s">
-        <v>348</v>
-      </c>
-      <c r="I67" t="s">
-        <v>349</v>
-      </c>
-      <c r="Q67" t="s">
-        <v>393</v>
+        <v>231</v>
       </c>
     </row>
     <row r="68" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>276</v>
+        <v>390</v>
       </c>
       <c r="B68" t="s">
-        <v>124</v>
+        <v>83</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>277</v>
+        <v>392</v>
+      </c>
+      <c r="D68" t="s">
+        <v>391</v>
+      </c>
+      <c r="E68" t="s">
+        <v>9</v>
       </c>
       <c r="F68">
-        <v>1948</v>
+        <v>2007</v>
       </c>
       <c r="G68">
-        <v>2000</v>
+        <v>2015</v>
       </c>
       <c r="H68" t="s">
-        <v>16</v>
+        <v>348</v>
       </c>
       <c r="I68" t="s">
-        <v>20</v>
+        <v>349</v>
+      </c>
+      <c r="Q68" t="s">
+        <v>393</v>
       </c>
     </row>
     <row r="69" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>449</v>
+        <v>276</v>
       </c>
       <c r="B69" t="s">
-        <v>250</v>
+        <v>124</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>448</v>
-      </c>
-      <c r="E69" t="s">
-        <v>14</v>
+        <v>277</v>
       </c>
       <c r="F69">
-        <v>-4000</v>
+        <v>1948</v>
       </c>
       <c r="G69">
         <v>2000</v>
       </c>
       <c r="H69" t="s">
-        <v>348</v>
+        <v>16</v>
       </c>
       <c r="I69" t="s">
-        <v>349</v>
-      </c>
-      <c r="J69" s="2" t="s">
-        <v>450</v>
-      </c>
-      <c r="N69" s="2" t="s">
-        <v>451</v>
+        <v>20</v>
       </c>
     </row>
     <row r="70" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>224</v>
+        <v>449</v>
       </c>
       <c r="B70" t="s">
-        <v>40</v>
+        <v>250</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>225</v>
+        <v>448</v>
+      </c>
+      <c r="E70" t="s">
+        <v>14</v>
       </c>
       <c r="F70">
-        <v>1964</v>
+        <v>-4000</v>
       </c>
       <c r="G70">
-        <v>2008</v>
+        <v>2000</v>
       </c>
       <c r="H70" t="s">
-        <v>16</v>
+        <v>348</v>
       </c>
       <c r="I70" t="s">
-        <v>20</v>
+        <v>349</v>
+      </c>
+      <c r="J70" s="2" t="s">
+        <v>450</v>
+      </c>
+      <c r="N70" s="2" t="s">
+        <v>451</v>
       </c>
     </row>
     <row r="71" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>285</v>
+        <v>224</v>
       </c>
       <c r="B71" t="s">
-        <v>250</v>
+        <v>40</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>286</v>
+        <v>225</v>
+      </c>
+      <c r="F71">
+        <v>1964</v>
+      </c>
+      <c r="G71">
+        <v>2008</v>
       </c>
       <c r="H71" t="s">
         <v>16</v>
@@ -3429,259 +3468,259 @@
     </row>
     <row r="72" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>205</v>
+        <v>285</v>
       </c>
       <c r="B72" t="s">
-        <v>40</v>
+        <v>250</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>204</v>
-      </c>
-      <c r="F72">
-        <v>2006</v>
+        <v>286</v>
+      </c>
+      <c r="H72" t="s">
+        <v>16</v>
+      </c>
+      <c r="I72" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="73" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>200</v>
+        <v>205</v>
       </c>
       <c r="B73" t="s">
-        <v>99</v>
+        <v>40</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="F73">
-        <v>1980</v>
-      </c>
-      <c r="G73">
-        <v>2007</v>
-      </c>
-      <c r="Q73" t="s">
-        <v>18</v>
+        <v>2006</v>
       </c>
     </row>
     <row r="74" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>468</v>
+        <v>200</v>
       </c>
       <c r="B74" t="s">
-        <v>40</v>
+        <v>99</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>464</v>
-      </c>
-      <c r="E74" t="s">
-        <v>14</v>
+        <v>201</v>
       </c>
       <c r="F74">
-        <v>1816</v>
+        <v>1980</v>
       </c>
       <c r="G74">
-        <v>2001</v>
-      </c>
-      <c r="H74" t="s">
-        <v>348</v>
-      </c>
-      <c r="I74" t="s">
-        <v>349</v>
-      </c>
-      <c r="J74" s="2" t="s">
-        <v>469</v>
-      </c>
-      <c r="K74" s="2" t="s">
-        <v>470</v>
-      </c>
-      <c r="L74" s="2" t="s">
-        <v>471</v>
+        <v>2007</v>
+      </c>
+      <c r="Q74" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="75" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>89</v>
+        <v>468</v>
       </c>
       <c r="B75" t="s">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>88</v>
+        <v>464</v>
       </c>
       <c r="E75" t="s">
-        <v>34</v>
+        <v>14</v>
       </c>
       <c r="F75">
-        <v>1972</v>
+        <v>1816</v>
+      </c>
+      <c r="G75">
+        <v>2001</v>
       </c>
       <c r="H75" t="s">
-        <v>16</v>
+        <v>348</v>
       </c>
       <c r="I75" t="s">
-        <v>20</v>
+        <v>349</v>
+      </c>
+      <c r="J75" s="2" t="s">
+        <v>469</v>
+      </c>
+      <c r="K75" s="2" t="s">
+        <v>470</v>
+      </c>
+      <c r="L75" s="2" t="s">
+        <v>471</v>
       </c>
     </row>
     <row r="76" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>104</v>
+        <v>89</v>
       </c>
       <c r="B76" t="s">
         <v>25</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>106</v>
+        <v>88</v>
       </c>
       <c r="E76" t="s">
-        <v>105</v>
+        <v>34</v>
       </c>
       <c r="F76">
-        <v>1980</v>
+        <v>1972</v>
+      </c>
+      <c r="H76" t="s">
+        <v>16</v>
+      </c>
+      <c r="I76" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="77" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>460</v>
+        <v>104</v>
       </c>
       <c r="B77" t="s">
         <v>25</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>461</v>
-      </c>
-      <c r="D77" t="s">
-        <v>363</v>
+        <v>106</v>
       </c>
       <c r="E77" t="s">
         <v>105</v>
       </c>
       <c r="F77">
-        <v>2009</v>
-      </c>
-      <c r="H77" t="s">
-        <v>348</v>
-      </c>
-      <c r="I77" t="s">
-        <v>301</v>
+        <v>1980</v>
       </c>
     </row>
     <row r="78" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>62</v>
+        <v>460</v>
       </c>
       <c r="B78" t="s">
         <v>25</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>63</v>
+        <v>461</v>
+      </c>
+      <c r="D78" t="s">
+        <v>363</v>
+      </c>
+      <c r="E78" t="s">
+        <v>105</v>
+      </c>
+      <c r="F78">
+        <v>2009</v>
+      </c>
+      <c r="H78" t="s">
+        <v>348</v>
+      </c>
+      <c r="I78" t="s">
+        <v>301</v>
       </c>
     </row>
     <row r="79" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>311</v>
+        <v>62</v>
       </c>
       <c r="B79" t="s">
-        <v>165</v>
+        <v>25</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>312</v>
-      </c>
-      <c r="E79" t="s">
-        <v>14</v>
-      </c>
-      <c r="H79" t="s">
-        <v>16</v>
-      </c>
-      <c r="I79" t="s">
-        <v>301</v>
+        <v>63</v>
       </c>
     </row>
     <row r="80" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>281</v>
+        <v>311</v>
       </c>
       <c r="B80" t="s">
-        <v>237</v>
+        <v>165</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>282</v>
+        <v>312</v>
+      </c>
+      <c r="E80" t="s">
+        <v>14</v>
       </c>
       <c r="H80" t="s">
         <v>16</v>
       </c>
       <c r="I80" t="s">
-        <v>20</v>
+        <v>301</v>
       </c>
     </row>
     <row r="81" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>418</v>
+        <v>281</v>
       </c>
       <c r="B81" t="s">
-        <v>86</v>
+        <v>237</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>419</v>
-      </c>
-      <c r="E81" t="s">
-        <v>420</v>
-      </c>
-      <c r="F81">
-        <v>1948</v>
-      </c>
-      <c r="G81">
-        <v>2012</v>
+        <v>282</v>
       </c>
       <c r="H81" t="s">
-        <v>348</v>
+        <v>16</v>
       </c>
       <c r="I81" t="s">
-        <v>349</v>
-      </c>
-      <c r="K81" s="2" t="s">
-        <v>421</v>
-      </c>
-      <c r="Q81" t="s">
-        <v>422</v>
+        <v>20</v>
       </c>
     </row>
     <row r="82" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>151</v>
+        <v>418</v>
       </c>
       <c r="B82" t="s">
-        <v>40</v>
+        <v>86</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>152</v>
+        <v>419</v>
       </c>
       <c r="E82" t="s">
-        <v>14</v>
+        <v>420</v>
+      </c>
+      <c r="F82">
+        <v>1948</v>
+      </c>
+      <c r="G82">
+        <v>2012</v>
+      </c>
+      <c r="H82" t="s">
+        <v>348</v>
+      </c>
+      <c r="I82" t="s">
+        <v>349</v>
+      </c>
+      <c r="K82" s="2" t="s">
+        <v>421</v>
+      </c>
+      <c r="Q82" t="s">
+        <v>422</v>
       </c>
     </row>
     <row r="83" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>242</v>
+        <v>151</v>
       </c>
       <c r="B83" t="s">
-        <v>237</v>
+        <v>40</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>243</v>
-      </c>
-      <c r="H83" t="s">
-        <v>16</v>
-      </c>
-      <c r="I83" t="s">
-        <v>20</v>
+        <v>152</v>
+      </c>
+      <c r="E83" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="84" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>292</v>
+        <v>242</v>
       </c>
       <c r="B84" t="s">
-        <v>99</v>
+        <v>237</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>291</v>
+        <v>243</v>
       </c>
       <c r="H84" t="s">
         <v>16</v>
@@ -3692,47 +3731,47 @@
     </row>
     <row r="85" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>153</v>
+        <v>292</v>
       </c>
       <c r="B85" t="s">
-        <v>259</v>
+        <v>99</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>154</v>
+        <v>291</v>
+      </c>
+      <c r="H85" t="s">
+        <v>16</v>
+      </c>
+      <c r="I85" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="86" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>228</v>
+        <v>153</v>
       </c>
       <c r="B86" t="s">
-        <v>40</v>
+        <v>259</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>225</v>
-      </c>
-      <c r="F86">
-        <v>1989</v>
-      </c>
-      <c r="G86">
-        <v>2017</v>
-      </c>
-      <c r="H86" t="s">
-        <v>16</v>
-      </c>
-      <c r="I86" t="s">
-        <v>20</v>
+        <v>154</v>
       </c>
     </row>
     <row r="87" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>245</v>
+        <v>228</v>
       </c>
       <c r="B87" t="s">
-        <v>237</v>
+        <v>40</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>244</v>
+        <v>225</v>
+      </c>
+      <c r="F87">
+        <v>1989</v>
+      </c>
+      <c r="G87">
+        <v>2017</v>
       </c>
       <c r="H87" t="s">
         <v>16</v>
@@ -3743,50 +3782,41 @@
     </row>
     <row r="88" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>100</v>
+        <v>245</v>
       </c>
       <c r="B88" t="s">
-        <v>99</v>
+        <v>237</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>101</v>
+        <v>244</v>
+      </c>
+      <c r="H88" t="s">
+        <v>16</v>
+      </c>
+      <c r="I88" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="89" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>239</v>
+        <v>100</v>
       </c>
       <c r="B89" t="s">
-        <v>237</v>
+        <v>99</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>243</v>
-      </c>
-      <c r="H89" t="s">
-        <v>16</v>
-      </c>
-      <c r="I89" t="s">
-        <v>20</v>
+        <v>101</v>
       </c>
     </row>
     <row r="90" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>254</v>
+        <v>239</v>
       </c>
       <c r="B90" t="s">
-        <v>55</v>
+        <v>237</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>253</v>
-      </c>
-      <c r="E90" t="s">
-        <v>255</v>
-      </c>
-      <c r="F90">
-        <v>1960</v>
-      </c>
-      <c r="G90">
-        <v>2014</v>
+        <v>243</v>
       </c>
       <c r="H90" t="s">
         <v>16</v>
@@ -3797,19 +3827,22 @@
     </row>
     <row r="91" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>270</v>
+        <v>254</v>
       </c>
       <c r="B91" t="s">
         <v>55</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>271</v>
+        <v>253</v>
+      </c>
+      <c r="E91" t="s">
+        <v>255</v>
       </c>
       <c r="F91">
-        <v>1990</v>
+        <v>1960</v>
       </c>
       <c r="G91">
-        <v>2010</v>
+        <v>2014</v>
       </c>
       <c r="H91" t="s">
         <v>16</v>
@@ -3820,96 +3853,90 @@
     </row>
     <row r="92" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>117</v>
+        <v>270</v>
       </c>
       <c r="B92" t="s">
         <v>55</v>
       </c>
       <c r="C92" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="F92">
+        <v>1990</v>
+      </c>
+      <c r="G92">
+        <v>2010</v>
+      </c>
+      <c r="H92" t="s">
+        <v>16</v>
+      </c>
+      <c r="I92" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="93" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A93" t="s">
+        <v>117</v>
+      </c>
+      <c r="B93" t="s">
+        <v>55</v>
+      </c>
+      <c r="C93" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="I92" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q92" t="s">
+      <c r="I93" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q93" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="93" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A93" s="1" t="s">
+    <row r="94" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A94" s="1" t="s">
         <v>23</v>
-      </c>
-      <c r="B93" t="s">
-        <v>25</v>
-      </c>
-      <c r="C93" s="2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="94" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A94" t="s">
-        <v>300</v>
       </c>
       <c r="B94" t="s">
         <v>25</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>298</v>
-      </c>
-      <c r="E94" t="s">
-        <v>299</v>
-      </c>
-      <c r="F94">
-        <v>1969</v>
-      </c>
-      <c r="H94" t="s">
-        <v>16</v>
-      </c>
-      <c r="I94" t="s">
-        <v>249</v>
+        <v>53</v>
       </c>
     </row>
     <row r="95" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>332</v>
+        <v>300</v>
       </c>
       <c r="B95" t="s">
-        <v>134</v>
+        <v>25</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>333</v>
+        <v>298</v>
       </c>
       <c r="E95" t="s">
-        <v>334</v>
+        <v>299</v>
+      </c>
+      <c r="F95">
+        <v>1969</v>
       </c>
       <c r="H95" t="s">
         <v>16</v>
       </c>
       <c r="I95" t="s">
-        <v>20</v>
+        <v>249</v>
       </c>
     </row>
     <row r="96" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>267</v>
+        <v>332</v>
       </c>
       <c r="B96" t="s">
-        <v>250</v>
+        <v>134</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>266</v>
-      </c>
-      <c r="D96" t="s">
-        <v>269</v>
+        <v>333</v>
       </c>
       <c r="E96" t="s">
-        <v>268</v>
-      </c>
-      <c r="F96">
-        <v>1970</v>
-      </c>
-      <c r="G96">
-        <v>2014</v>
+        <v>334</v>
       </c>
       <c r="H96" t="s">
         <v>16</v>
@@ -3920,97 +3947,100 @@
     </row>
     <row r="97" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>407</v>
+        <v>267</v>
       </c>
       <c r="B97" t="s">
-        <v>40</v>
+        <v>250</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>406</v>
+        <v>266</v>
       </c>
       <c r="D97" t="s">
-        <v>408</v>
+        <v>269</v>
       </c>
       <c r="E97" t="s">
-        <v>14</v>
+        <v>268</v>
       </c>
       <c r="F97">
-        <v>1949</v>
+        <v>1970</v>
       </c>
       <c r="G97">
-        <v>2013</v>
+        <v>2014</v>
       </c>
       <c r="H97" t="s">
-        <v>348</v>
+        <v>16</v>
       </c>
       <c r="I97" t="s">
-        <v>349</v>
+        <v>20</v>
       </c>
     </row>
     <row r="98" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>96</v>
+        <v>407</v>
       </c>
       <c r="B98" t="s">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>90</v>
+        <v>406</v>
+      </c>
+      <c r="D98" t="s">
+        <v>408</v>
       </c>
       <c r="E98" t="s">
-        <v>69</v>
+        <v>14</v>
       </c>
       <c r="F98">
-        <v>1995</v>
+        <v>1949</v>
+      </c>
+      <c r="G98">
+        <v>2013</v>
+      </c>
+      <c r="H98" t="s">
+        <v>348</v>
+      </c>
+      <c r="I98" t="s">
+        <v>349</v>
       </c>
     </row>
     <row r="99" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>404</v>
+        <v>96</v>
       </c>
       <c r="B99" t="s">
-        <v>83</v>
+        <v>25</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>403</v>
-      </c>
-      <c r="D99" t="s">
-        <v>405</v>
+        <v>90</v>
       </c>
       <c r="E99" t="s">
-        <v>14</v>
+        <v>69</v>
       </c>
       <c r="F99">
-        <v>1875</v>
-      </c>
-      <c r="G99">
-        <v>2004</v>
-      </c>
-      <c r="H99" t="s">
-        <v>348</v>
-      </c>
-      <c r="I99" t="s">
-        <v>349</v>
+        <v>1995</v>
       </c>
     </row>
     <row r="100" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>454</v>
+        <v>404</v>
       </c>
       <c r="B100" t="s">
-        <v>25</v>
+        <v>83</v>
       </c>
       <c r="C100" s="2" t="s">
-        <v>455</v>
+        <v>403</v>
+      </c>
+      <c r="D100" t="s">
+        <v>405</v>
       </c>
       <c r="E100" t="s">
-        <v>456</v>
+        <v>14</v>
       </c>
       <c r="F100">
-        <v>2006</v>
+        <v>1875</v>
       </c>
       <c r="G100">
-        <v>2016</v>
+        <v>2004</v>
       </c>
       <c r="H100" t="s">
         <v>348</v>
@@ -4018,80 +4048,83 @@
       <c r="I100" t="s">
         <v>349</v>
       </c>
-      <c r="J100" s="2" t="s">
-        <v>457</v>
-      </c>
-      <c r="L100" s="2" t="s">
-        <v>458</v>
-      </c>
-      <c r="Q100" t="s">
-        <v>459</v>
-      </c>
     </row>
     <row r="101" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>11</v>
+        <v>454</v>
       </c>
       <c r="B101" t="s">
         <v>25</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D101" t="s">
-        <v>95</v>
+        <v>455</v>
       </c>
       <c r="E101" t="s">
-        <v>10</v>
+        <v>456</v>
       </c>
       <c r="F101">
-        <v>2007</v>
+        <v>2006</v>
+      </c>
+      <c r="G101">
+        <v>2016</v>
       </c>
       <c r="H101" t="s">
-        <v>16</v>
+        <v>348</v>
       </c>
       <c r="I101" t="s">
-        <v>21</v>
+        <v>349</v>
+      </c>
+      <c r="J101" s="2" t="s">
+        <v>457</v>
+      </c>
+      <c r="L101" s="2" t="s">
+        <v>458</v>
+      </c>
+      <c r="Q101" t="s">
+        <v>459</v>
       </c>
     </row>
     <row r="102" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>223</v>
+        <v>11</v>
       </c>
       <c r="B102" t="s">
-        <v>124</v>
+        <v>25</v>
       </c>
       <c r="C102" s="2" t="s">
-        <v>222</v>
+        <v>12</v>
+      </c>
+      <c r="D102" t="s">
+        <v>95</v>
+      </c>
+      <c r="E102" t="s">
+        <v>10</v>
       </c>
       <c r="F102">
-        <v>1</v>
-      </c>
-      <c r="G102">
-        <v>2010</v>
+        <v>2007</v>
       </c>
       <c r="H102" t="s">
         <v>16</v>
       </c>
       <c r="I102" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="103" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="B103" t="s">
-        <v>40</v>
+        <v>124</v>
       </c>
       <c r="C103" s="2" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="F103">
-        <v>1946</v>
+        <v>1</v>
       </c>
       <c r="G103">
-        <v>2016</v>
+        <v>2010</v>
       </c>
       <c r="H103" t="s">
         <v>16</v>
@@ -4102,122 +4135,122 @@
     </row>
     <row r="104" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>97</v>
+        <v>226</v>
       </c>
       <c r="B104" t="s">
-        <v>128</v>
+        <v>40</v>
       </c>
       <c r="C104" s="2" t="s">
-        <v>98</v>
+        <v>225</v>
+      </c>
+      <c r="F104">
+        <v>1946</v>
+      </c>
+      <c r="G104">
+        <v>2016</v>
+      </c>
+      <c r="H104" t="s">
+        <v>16</v>
+      </c>
+      <c r="I104" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="105" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>278</v>
+        <v>97</v>
       </c>
       <c r="B105" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="C105" s="2" t="s">
-        <v>279</v>
-      </c>
-      <c r="E105" t="s">
-        <v>280</v>
-      </c>
-      <c r="F105">
-        <v>1890</v>
-      </c>
-      <c r="G105">
-        <v>1996</v>
-      </c>
-      <c r="H105" t="s">
-        <v>16</v>
-      </c>
-      <c r="I105" t="s">
-        <v>20</v>
+        <v>98</v>
       </c>
     </row>
     <row r="106" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>156</v>
+        <v>278</v>
       </c>
       <c r="B106" t="s">
-        <v>25</v>
+        <v>124</v>
       </c>
       <c r="C106" s="2" t="s">
-        <v>154</v>
+        <v>279</v>
+      </c>
+      <c r="E106" t="s">
+        <v>280</v>
+      </c>
+      <c r="F106">
+        <v>1890</v>
+      </c>
+      <c r="G106">
+        <v>1996</v>
+      </c>
+      <c r="H106" t="s">
+        <v>16</v>
+      </c>
+      <c r="I106" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="107" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>413</v>
+        <v>156</v>
       </c>
       <c r="B107" t="s">
-        <v>128</v>
+        <v>25</v>
       </c>
       <c r="C107" s="2" t="s">
-        <v>414</v>
-      </c>
-      <c r="E107" t="s">
-        <v>415</v>
-      </c>
-      <c r="F107">
-        <v>1946</v>
-      </c>
-      <c r="G107">
-        <v>2014</v>
-      </c>
-      <c r="H107" t="s">
-        <v>348</v>
-      </c>
-      <c r="I107" t="s">
-        <v>349</v>
-      </c>
-      <c r="N107" s="2" t="s">
-        <v>416</v>
-      </c>
-      <c r="Q107" t="s">
-        <v>417</v>
+        <v>154</v>
       </c>
     </row>
     <row r="108" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>229</v>
+        <v>413</v>
       </c>
       <c r="B108" t="s">
-        <v>40</v>
+        <v>128</v>
       </c>
       <c r="C108" s="2" t="s">
-        <v>225</v>
+        <v>414</v>
+      </c>
+      <c r="E108" t="s">
+        <v>415</v>
       </c>
       <c r="F108">
-        <v>1952</v>
+        <v>1946</v>
       </c>
       <c r="G108">
-        <v>1997</v>
+        <v>2014</v>
       </c>
       <c r="H108" t="s">
-        <v>16</v>
+        <v>348</v>
       </c>
       <c r="I108" t="s">
-        <v>20</v>
+        <v>349</v>
+      </c>
+      <c r="N108" s="2" t="s">
+        <v>416</v>
+      </c>
+      <c r="Q108" t="s">
+        <v>417</v>
       </c>
     </row>
     <row r="109" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>293</v>
+        <v>229</v>
       </c>
       <c r="B109" t="s">
         <v>40</v>
       </c>
       <c r="C109" s="2" t="s">
-        <v>294</v>
+        <v>225</v>
       </c>
       <c r="F109">
-        <v>2004</v>
+        <v>1952</v>
       </c>
       <c r="G109">
-        <v>2006</v>
+        <v>1997</v>
       </c>
       <c r="H109" t="s">
         <v>16</v>
@@ -4228,221 +4261,218 @@
     </row>
     <row r="110" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>102</v>
+        <v>293</v>
       </c>
       <c r="B110" t="s">
-        <v>99</v>
+        <v>40</v>
       </c>
       <c r="C110" s="2" t="s">
-        <v>103</v>
+        <v>294</v>
+      </c>
+      <c r="F110">
+        <v>2004</v>
+      </c>
+      <c r="G110">
+        <v>2006</v>
+      </c>
+      <c r="H110" t="s">
+        <v>16</v>
+      </c>
+      <c r="I110" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="111" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>289</v>
+        <v>102</v>
       </c>
       <c r="B111" t="s">
-        <v>124</v>
+        <v>99</v>
       </c>
       <c r="C111" s="2" t="s">
-        <v>290</v>
+        <v>103</v>
       </c>
     </row>
     <row r="112" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>246</v>
+        <v>289</v>
       </c>
       <c r="B112" t="s">
-        <v>165</v>
+        <v>124</v>
       </c>
       <c r="C112" s="2" t="s">
-        <v>247</v>
-      </c>
-      <c r="E112" t="s">
-        <v>14</v>
-      </c>
-      <c r="F112">
-        <v>1960</v>
-      </c>
-      <c r="G112">
-        <v>2006</v>
-      </c>
-      <c r="H112" t="s">
-        <v>16</v>
-      </c>
-      <c r="I112" t="s">
-        <v>249</v>
+        <v>290</v>
       </c>
     </row>
     <row r="113" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>365</v>
+        <v>246</v>
       </c>
       <c r="B113" t="s">
-        <v>128</v>
+        <v>165</v>
       </c>
       <c r="C113" s="2" t="s">
-        <v>364</v>
-      </c>
-      <c r="D113" t="s">
-        <v>370</v>
+        <v>247</v>
       </c>
       <c r="E113" t="s">
-        <v>366</v>
+        <v>14</v>
       </c>
       <c r="F113">
-        <v>1906</v>
+        <v>1960</v>
       </c>
       <c r="G113">
-        <v>2013</v>
+        <v>2006</v>
       </c>
       <c r="H113" t="s">
-        <v>367</v>
+        <v>16</v>
       </c>
       <c r="I113" t="s">
-        <v>368</v>
-      </c>
-      <c r="Q113" t="s">
-        <v>369</v>
+        <v>249</v>
       </c>
     </row>
     <row r="114" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>208</v>
+        <v>365</v>
       </c>
       <c r="B114" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="C114" s="2" t="s">
-        <v>209</v>
+        <v>364</v>
+      </c>
+      <c r="D114" t="s">
+        <v>370</v>
+      </c>
+      <c r="E114" t="s">
+        <v>366</v>
       </c>
       <c r="F114">
-        <v>1932</v>
+        <v>1906</v>
       </c>
       <c r="G114">
-        <v>2014</v>
+        <v>2013</v>
       </c>
       <c r="H114" t="s">
-        <v>16</v>
+        <v>367</v>
       </c>
       <c r="I114" t="s">
-        <v>20</v>
+        <v>368</v>
+      </c>
+      <c r="Q114" t="s">
+        <v>369</v>
       </c>
     </row>
     <row r="115" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>137</v>
+        <v>208</v>
       </c>
       <c r="B115" t="s">
-        <v>259</v>
+        <v>124</v>
       </c>
       <c r="C115" s="2" t="s">
-        <v>138</v>
+        <v>209</v>
+      </c>
+      <c r="F115">
+        <v>1932</v>
+      </c>
+      <c r="G115">
+        <v>2014</v>
+      </c>
+      <c r="H115" t="s">
+        <v>16</v>
+      </c>
+      <c r="I115" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="116" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>155</v>
+        <v>137</v>
       </c>
       <c r="B116" t="s">
         <v>259</v>
       </c>
       <c r="C116" s="2" t="s">
-        <v>154</v>
+        <v>138</v>
       </c>
     </row>
     <row r="117" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>57</v>
+        <v>155</v>
       </c>
       <c r="B117" t="s">
-        <v>128</v>
+        <v>259</v>
       </c>
       <c r="C117" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="Q117" t="s">
-        <v>17</v>
+        <v>154</v>
       </c>
     </row>
     <row r="118" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>129</v>
+        <v>57</v>
       </c>
       <c r="B118" t="s">
-        <v>259</v>
+        <v>128</v>
       </c>
       <c r="C118" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="E118" t="s">
-        <v>131</v>
-      </c>
-      <c r="F118">
-        <v>1945</v>
-      </c>
-      <c r="G118">
-        <v>2008</v>
-      </c>
-      <c r="I118" t="s">
-        <v>20</v>
+        <v>58</v>
+      </c>
+      <c r="Q118" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="119" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>148</v>
+        <v>129</v>
       </c>
       <c r="B119" t="s">
-        <v>128</v>
+        <v>259</v>
       </c>
       <c r="C119" s="2" t="s">
-        <v>147</v>
+        <v>130</v>
+      </c>
+      <c r="E119" t="s">
+        <v>131</v>
+      </c>
+      <c r="F119">
+        <v>1945</v>
+      </c>
+      <c r="G119">
+        <v>2008</v>
+      </c>
+      <c r="I119" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="120" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>233</v>
+        <v>148</v>
       </c>
       <c r="B120" t="s">
-        <v>165</v>
+        <v>128</v>
       </c>
       <c r="C120" s="2" t="s">
-        <v>234</v>
-      </c>
-      <c r="E120" t="s">
-        <v>14</v>
-      </c>
-      <c r="F120">
-        <v>2012</v>
-      </c>
-      <c r="G120">
-        <v>2016</v>
-      </c>
-      <c r="H120" t="s">
-        <v>16</v>
-      </c>
-      <c r="I120" t="s">
-        <v>20</v>
+        <v>147</v>
       </c>
     </row>
     <row r="121" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>35</v>
+        <v>233</v>
       </c>
       <c r="B121" t="s">
-        <v>25</v>
+        <v>165</v>
       </c>
       <c r="C121" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="D121" t="s">
-        <v>37</v>
+        <v>234</v>
       </c>
       <c r="E121" t="s">
         <v>14</v>
       </c>
       <c r="F121">
-        <v>2001</v>
+        <v>2012</v>
+      </c>
+      <c r="G121">
+        <v>2016</v>
       </c>
       <c r="H121" t="s">
         <v>16</v>
@@ -4453,148 +4483,148 @@
     </row>
     <row r="122" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>185</v>
+        <v>35</v>
       </c>
       <c r="B122" t="s">
-        <v>128</v>
+        <v>25</v>
       </c>
       <c r="C122" s="2" t="s">
-        <v>186</v>
+        <v>36</v>
+      </c>
+      <c r="D122" t="s">
+        <v>37</v>
+      </c>
+      <c r="E122" t="s">
+        <v>14</v>
+      </c>
+      <c r="F122">
+        <v>2001</v>
+      </c>
+      <c r="H122" t="s">
+        <v>16</v>
+      </c>
+      <c r="I122" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="123" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>210</v>
+        <v>185</v>
       </c>
       <c r="B123" t="s">
-        <v>40</v>
+        <v>128</v>
       </c>
       <c r="C123" s="2" t="s">
-        <v>211</v>
-      </c>
-      <c r="F123">
-        <v>1976</v>
-      </c>
-      <c r="G123">
-        <v>2016</v>
-      </c>
-      <c r="H123" t="s">
-        <v>16</v>
-      </c>
-      <c r="I123" t="s">
-        <v>20</v>
+        <v>186</v>
       </c>
     </row>
     <row r="124" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>426</v>
+        <v>210</v>
       </c>
       <c r="B124" t="s">
-        <v>86</v>
+        <v>40</v>
       </c>
       <c r="C124" s="2" t="s">
-        <v>427</v>
-      </c>
-      <c r="E124" t="s">
-        <v>34</v>
+        <v>211</v>
       </c>
       <c r="F124">
-        <v>2015</v>
+        <v>1976</v>
       </c>
       <c r="G124">
         <v>2016</v>
       </c>
       <c r="H124" t="s">
-        <v>348</v>
+        <v>16</v>
       </c>
       <c r="I124" t="s">
-        <v>349</v>
-      </c>
-      <c r="K124" s="2" t="s">
-        <v>428</v>
+        <v>20</v>
       </c>
     </row>
     <row r="125" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>144</v>
+        <v>426</v>
       </c>
       <c r="B125" t="s">
-        <v>60</v>
+        <v>86</v>
       </c>
       <c r="C125" s="2" t="s">
-        <v>143</v>
+        <v>427</v>
+      </c>
+      <c r="E125" t="s">
+        <v>34</v>
       </c>
       <c r="F125">
-        <v>1800</v>
+        <v>2015</v>
       </c>
       <c r="G125">
-        <v>2013</v>
+        <v>2016</v>
+      </c>
+      <c r="H125" t="s">
+        <v>348</v>
+      </c>
+      <c r="I125" t="s">
+        <v>349</v>
+      </c>
+      <c r="K125" s="2" t="s">
+        <v>428</v>
       </c>
     </row>
     <row r="126" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>472</v>
+        <v>144</v>
       </c>
       <c r="B126" t="s">
-        <v>25</v>
+        <v>60</v>
       </c>
       <c r="C126" s="2" t="s">
-        <v>473</v>
-      </c>
-      <c r="D126" t="s">
-        <v>474</v>
-      </c>
-      <c r="E126" t="s">
-        <v>112</v>
+        <v>143</v>
       </c>
       <c r="F126">
-        <v>1943</v>
-      </c>
-      <c r="H126" t="s">
-        <v>348</v>
-      </c>
-      <c r="I126" t="s">
-        <v>349</v>
-      </c>
-      <c r="N126" s="2" t="s">
-        <v>475</v>
+        <v>1800</v>
+      </c>
+      <c r="G126">
+        <v>2013</v>
       </c>
     </row>
     <row r="127" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>122</v>
+        <v>472</v>
       </c>
       <c r="B127" t="s">
-        <v>259</v>
+        <v>25</v>
       </c>
       <c r="C127" s="2" t="s">
-        <v>121</v>
+        <v>473</v>
+      </c>
+      <c r="D127" t="s">
+        <v>474</v>
+      </c>
+      <c r="E127" t="s">
+        <v>112</v>
+      </c>
+      <c r="F127">
+        <v>1943</v>
+      </c>
+      <c r="H127" t="s">
+        <v>348</v>
       </c>
       <c r="I127" t="s">
-        <v>20</v>
+        <v>349</v>
+      </c>
+      <c r="N127" s="2" t="s">
+        <v>475</v>
       </c>
     </row>
     <row r="128" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>318</v>
+        <v>122</v>
       </c>
       <c r="B128" t="s">
-        <v>250</v>
+        <v>259</v>
       </c>
       <c r="C128" s="2" t="s">
-        <v>319</v>
-      </c>
-      <c r="E128" t="s">
-        <v>320</v>
-      </c>
-      <c r="F128">
-        <v>1975</v>
-      </c>
-      <c r="G128">
-        <v>1989</v>
-      </c>
-      <c r="H128" t="s">
-        <v>16</v>
+        <v>121</v>
       </c>
       <c r="I128" t="s">
         <v>20</v>
@@ -4602,22 +4632,22 @@
     </row>
     <row r="129" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="B129" t="s">
         <v>250</v>
       </c>
       <c r="C129" s="2" t="s">
-        <v>317</v>
+        <v>319</v>
       </c>
       <c r="E129" t="s">
-        <v>105</v>
+        <v>320</v>
       </c>
       <c r="F129">
-        <v>1950</v>
+        <v>1975</v>
       </c>
       <c r="G129">
-        <v>1996</v>
+        <v>1989</v>
       </c>
       <c r="H129" t="s">
         <v>16</v>
@@ -4628,19 +4658,22 @@
     </row>
     <row r="130" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
-        <v>322</v>
+        <v>316</v>
       </c>
       <c r="B130" t="s">
-        <v>25</v>
+        <v>250</v>
       </c>
       <c r="C130" s="2" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="E130" t="s">
-        <v>77</v>
+        <v>105</v>
       </c>
       <c r="F130">
-        <v>2010</v>
+        <v>1950</v>
+      </c>
+      <c r="G130">
+        <v>1996</v>
       </c>
       <c r="H130" t="s">
         <v>16</v>
@@ -4651,121 +4684,118 @@
     </row>
     <row r="131" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>141</v>
+        <v>322</v>
       </c>
       <c r="B131" t="s">
-        <v>237</v>
+        <v>25</v>
       </c>
       <c r="C131" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="Q131" t="s">
-        <v>17</v>
+        <v>321</v>
+      </c>
+      <c r="E131" t="s">
+        <v>77</v>
+      </c>
+      <c r="F131">
+        <v>2010</v>
+      </c>
+      <c r="H131" t="s">
+        <v>16</v>
+      </c>
+      <c r="I131" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="132" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>308</v>
+        <v>141</v>
       </c>
       <c r="B132" t="s">
-        <v>250</v>
+        <v>237</v>
       </c>
       <c r="C132" s="2" t="s">
-        <v>309</v>
-      </c>
-      <c r="E132" t="s">
-        <v>310</v>
-      </c>
-      <c r="F132">
-        <v>1950</v>
-      </c>
-      <c r="G132">
-        <v>2010</v>
-      </c>
-      <c r="H132" t="s">
-        <v>16</v>
-      </c>
-      <c r="I132" t="s">
-        <v>20</v>
+        <v>142</v>
+      </c>
+      <c r="Q132" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="133" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
-        <v>287</v>
+        <v>308</v>
       </c>
       <c r="B133" t="s">
-        <v>134</v>
+        <v>250</v>
       </c>
       <c r="C133" s="2" t="s">
-        <v>288</v>
+        <v>309</v>
+      </c>
+      <c r="E133" t="s">
+        <v>310</v>
       </c>
       <c r="F133">
-        <v>1990</v>
+        <v>1950</v>
       </c>
       <c r="G133">
-        <v>2008</v>
+        <v>2010</v>
+      </c>
+      <c r="H133" t="s">
+        <v>16</v>
+      </c>
+      <c r="I133" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="134" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
-        <v>274</v>
+        <v>287</v>
       </c>
       <c r="B134" t="s">
-        <v>55</v>
+        <v>134</v>
       </c>
       <c r="C134" s="2" t="s">
-        <v>275</v>
-      </c>
-      <c r="H134" t="s">
-        <v>16</v>
-      </c>
-      <c r="I134" t="s">
-        <v>20</v>
+        <v>288</v>
+      </c>
+      <c r="F134">
+        <v>1990</v>
+      </c>
+      <c r="G134">
+        <v>2008</v>
       </c>
     </row>
     <row r="135" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
-        <v>157</v>
+        <v>274</v>
       </c>
       <c r="B135" t="s">
-        <v>128</v>
+        <v>55</v>
       </c>
       <c r="C135" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="Q135" t="s">
-        <v>18</v>
+        <v>275</v>
+      </c>
+      <c r="H135" t="s">
+        <v>16</v>
+      </c>
+      <c r="I135" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="136" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
-        <v>439</v>
+        <v>157</v>
       </c>
       <c r="B136" t="s">
-        <v>259</v>
+        <v>128</v>
       </c>
       <c r="C136" s="2" t="s">
-        <v>438</v>
-      </c>
-      <c r="H136" t="s">
-        <v>348</v>
-      </c>
-      <c r="I136" t="s">
-        <v>349</v>
-      </c>
-      <c r="J136" s="2" t="s">
-        <v>440</v>
-      </c>
-      <c r="K136" s="2" t="s">
-        <v>442</v>
-      </c>
-      <c r="L136" s="2" t="s">
-        <v>441</v>
+        <v>154</v>
+      </c>
+      <c r="Q136" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="137" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
-        <v>443</v>
+        <v>439</v>
       </c>
       <c r="B137" t="s">
         <v>259</v>
@@ -4773,15 +4803,6 @@
       <c r="C137" s="2" t="s">
         <v>438</v>
       </c>
-      <c r="D137" t="s">
-        <v>447</v>
-      </c>
-      <c r="F137">
-        <v>1990</v>
-      </c>
-      <c r="G137">
-        <v>2014</v>
-      </c>
       <c r="H137" t="s">
         <v>348</v>
       </c>
@@ -4789,87 +4810,99 @@
         <v>349</v>
       </c>
       <c r="J137" s="2" t="s">
-        <v>444</v>
+        <v>440</v>
       </c>
       <c r="K137" s="2" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
       <c r="L137" s="2" t="s">
-        <v>446</v>
+        <v>441</v>
       </c>
     </row>
     <row r="138" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
-        <v>194</v>
+        <v>443</v>
       </c>
       <c r="B138" t="s">
-        <v>99</v>
+        <v>259</v>
       </c>
       <c r="C138" s="2" t="s">
-        <v>193</v>
+        <v>438</v>
+      </c>
+      <c r="D138" t="s">
+        <v>447</v>
+      </c>
+      <c r="F138">
+        <v>1990</v>
+      </c>
+      <c r="G138">
+        <v>2014</v>
+      </c>
+      <c r="H138" t="s">
+        <v>348</v>
+      </c>
+      <c r="I138" t="s">
+        <v>349</v>
+      </c>
+      <c r="J138" s="2" t="s">
+        <v>444</v>
+      </c>
+      <c r="K138" s="2" t="s">
+        <v>445</v>
+      </c>
+      <c r="L138" s="2" t="s">
+        <v>446</v>
       </c>
     </row>
     <row r="139" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
-        <v>295</v>
+        <v>194</v>
       </c>
       <c r="B139" t="s">
-        <v>40</v>
+        <v>99</v>
       </c>
       <c r="C139" s="2" t="s">
-        <v>296</v>
-      </c>
-      <c r="E139" t="s">
-        <v>297</v>
-      </c>
-      <c r="F139">
-        <v>1990</v>
-      </c>
-      <c r="G139">
-        <v>2015</v>
-      </c>
-      <c r="H139" t="s">
-        <v>16</v>
-      </c>
-      <c r="I139" t="s">
-        <v>249</v>
+        <v>193</v>
       </c>
     </row>
     <row r="140" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
-        <v>256</v>
+        <v>295</v>
       </c>
       <c r="B140" t="s">
-        <v>250</v>
+        <v>40</v>
       </c>
       <c r="C140" s="2" t="s">
-        <v>257</v>
+        <v>296</v>
       </c>
       <c r="E140" t="s">
-        <v>258</v>
+        <v>297</v>
+      </c>
+      <c r="F140">
+        <v>1990</v>
+      </c>
+      <c r="G140">
+        <v>2015</v>
       </c>
       <c r="H140" t="s">
         <v>16</v>
       </c>
       <c r="I140" t="s">
-        <v>20</v>
+        <v>249</v>
       </c>
     </row>
     <row r="141" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
-        <v>227</v>
+        <v>256</v>
       </c>
       <c r="B141" t="s">
-        <v>40</v>
+        <v>250</v>
       </c>
       <c r="C141" s="2" t="s">
-        <v>225</v>
-      </c>
-      <c r="F141">
-        <v>1955</v>
-      </c>
-      <c r="G141">
-        <v>2016</v>
+        <v>257</v>
+      </c>
+      <c r="E141" t="s">
+        <v>258</v>
       </c>
       <c r="H141" t="s">
         <v>16</v>
@@ -4880,7 +4913,7 @@
     </row>
     <row r="142" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="B142" t="s">
         <v>40</v>
@@ -4889,7 +4922,7 @@
         <v>225</v>
       </c>
       <c r="F142">
-        <v>1995</v>
+        <v>1955</v>
       </c>
       <c r="G142">
         <v>2016</v>
@@ -4903,248 +4936,248 @@
     </row>
     <row r="143" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
-        <v>452</v>
+        <v>230</v>
       </c>
       <c r="B143" t="s">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="C143" s="2" t="s">
-        <v>453</v>
-      </c>
-      <c r="E143" t="s">
-        <v>9</v>
+        <v>225</v>
+      </c>
+      <c r="F143">
+        <v>1995</v>
+      </c>
+      <c r="G143">
+        <v>2016</v>
       </c>
       <c r="H143" t="s">
-        <v>348</v>
+        <v>16</v>
       </c>
       <c r="I143" t="s">
-        <v>435</v>
+        <v>20</v>
       </c>
     </row>
     <row r="144" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
-        <v>109</v>
+        <v>452</v>
       </c>
       <c r="B144" t="s">
         <v>25</v>
       </c>
       <c r="C144" s="2" t="s">
-        <v>110</v>
+        <v>453</v>
       </c>
       <c r="E144" t="s">
-        <v>111</v>
-      </c>
-      <c r="F144">
-        <v>1956</v>
+        <v>9</v>
+      </c>
+      <c r="H144" t="s">
+        <v>348</v>
+      </c>
+      <c r="I144" t="s">
+        <v>435</v>
       </c>
     </row>
     <row r="145" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
-        <v>326</v>
+        <v>109</v>
       </c>
       <c r="B145" t="s">
         <v>25</v>
       </c>
       <c r="C145" s="2" t="s">
-        <v>327</v>
+        <v>110</v>
       </c>
       <c r="E145" t="s">
         <v>111</v>
       </c>
       <c r="F145">
-        <v>1998</v>
-      </c>
-      <c r="H145" t="s">
-        <v>16</v>
-      </c>
-      <c r="I145" t="s">
-        <v>20</v>
+        <v>1956</v>
       </c>
     </row>
     <row r="146" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
-        <v>91</v>
+        <v>326</v>
       </c>
       <c r="B146" t="s">
         <v>25</v>
       </c>
       <c r="C146" s="2" t="s">
-        <v>93</v>
+        <v>327</v>
       </c>
       <c r="E146" t="s">
-        <v>92</v>
+        <v>111</v>
       </c>
       <c r="F146">
-        <v>1999</v>
+        <v>1998</v>
+      </c>
+      <c r="H146" t="s">
+        <v>16</v>
+      </c>
+      <c r="I146" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="147" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
-        <v>314</v>
+        <v>91</v>
       </c>
       <c r="B147" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="C147" s="2" t="s">
-        <v>313</v>
+        <v>93</v>
       </c>
       <c r="E147" t="s">
-        <v>315</v>
+        <v>92</v>
       </c>
       <c r="F147">
-        <v>1950</v>
-      </c>
-      <c r="G147">
-        <v>2004</v>
-      </c>
-      <c r="H147" t="s">
-        <v>16</v>
-      </c>
-      <c r="I147" t="s">
-        <v>20</v>
+        <v>1999</v>
       </c>
     </row>
     <row r="148" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
-        <v>161</v>
+        <v>314</v>
       </c>
       <c r="B148" t="s">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="C148" s="2" t="s">
-        <v>160</v>
+        <v>313</v>
+      </c>
+      <c r="E148" t="s">
+        <v>315</v>
+      </c>
+      <c r="F148">
+        <v>1950</v>
+      </c>
+      <c r="G148">
+        <v>2004</v>
+      </c>
+      <c r="H148" t="s">
+        <v>16</v>
+      </c>
+      <c r="I148" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="149" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="B149" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="C149" s="2" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
     </row>
     <row r="150" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
-        <v>399</v>
+        <v>168</v>
       </c>
       <c r="B150" t="s">
         <v>40</v>
       </c>
       <c r="C150" s="2" t="s">
-        <v>400</v>
-      </c>
-      <c r="E150" t="s">
-        <v>14</v>
-      </c>
-      <c r="F150">
-        <v>2000</v>
-      </c>
-      <c r="G150">
-        <v>2014</v>
-      </c>
-      <c r="H150" t="s">
-        <v>348</v>
-      </c>
-      <c r="I150" t="s">
-        <v>349</v>
-      </c>
-      <c r="J150" s="2" t="s">
-        <v>402</v>
-      </c>
-      <c r="N150" s="2" t="s">
-        <v>401</v>
+        <v>167</v>
       </c>
     </row>
     <row r="151" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
-        <v>213</v>
+        <v>399</v>
       </c>
       <c r="B151" t="s">
-        <v>55</v>
+        <v>40</v>
       </c>
       <c r="C151" s="2" t="s">
-        <v>212</v>
+        <v>400</v>
+      </c>
+      <c r="E151" t="s">
+        <v>14</v>
+      </c>
+      <c r="F151">
+        <v>2000</v>
+      </c>
+      <c r="G151">
+        <v>2014</v>
       </c>
       <c r="H151" t="s">
-        <v>16</v>
+        <v>348</v>
       </c>
       <c r="I151" t="s">
-        <v>20</v>
+        <v>349</v>
+      </c>
+      <c r="J151" s="2" t="s">
+        <v>402</v>
+      </c>
+      <c r="N151" s="2" t="s">
+        <v>401</v>
       </c>
     </row>
     <row r="152" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
-        <v>395</v>
+        <v>213</v>
       </c>
       <c r="B152" t="s">
-        <v>25</v>
+        <v>55</v>
       </c>
       <c r="C152" s="2" t="s">
-        <v>394</v>
-      </c>
-      <c r="D152" t="s">
-        <v>396</v>
-      </c>
-      <c r="E152" t="s">
-        <v>111</v>
-      </c>
-      <c r="F152">
-        <v>1986</v>
-      </c>
-      <c r="G152">
-        <v>2015</v>
+        <v>212</v>
       </c>
       <c r="H152" t="s">
-        <v>367</v>
+        <v>16</v>
       </c>
       <c r="I152" t="s">
-        <v>398</v>
-      </c>
-      <c r="J152" s="2" t="s">
-        <v>397</v>
+        <v>20</v>
       </c>
     </row>
     <row r="153" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
-        <v>323</v>
+        <v>395</v>
       </c>
       <c r="B153" t="s">
         <v>25</v>
       </c>
       <c r="C153" s="2" t="s">
-        <v>324</v>
+        <v>394</v>
+      </c>
+      <c r="D153" t="s">
+        <v>396</v>
       </c>
       <c r="E153" t="s">
-        <v>325</v>
+        <v>111</v>
       </c>
       <c r="F153">
-        <v>1942</v>
+        <v>1986</v>
+      </c>
+      <c r="G153">
+        <v>2015</v>
       </c>
       <c r="H153" t="s">
-        <v>16</v>
+        <v>367</v>
       </c>
       <c r="I153" t="s">
-        <v>20</v>
+        <v>398</v>
+      </c>
+      <c r="J153" s="2" t="s">
+        <v>397</v>
       </c>
     </row>
     <row r="154" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
-        <v>273</v>
+        <v>323</v>
       </c>
       <c r="B154" t="s">
-        <v>237</v>
+        <v>25</v>
       </c>
       <c r="C154" s="2" t="s">
-        <v>272</v>
+        <v>324</v>
+      </c>
+      <c r="E154" t="s">
+        <v>325</v>
       </c>
       <c r="F154">
-        <v>1996</v>
-      </c>
-      <c r="G154">
-        <v>2016</v>
+        <v>1942</v>
       </c>
       <c r="H154" t="s">
         <v>16</v>
@@ -5155,59 +5188,59 @@
     </row>
     <row r="155" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
-        <v>66</v>
+        <v>273</v>
       </c>
       <c r="B155" t="s">
-        <v>25</v>
+        <v>237</v>
       </c>
       <c r="C155" s="2" t="s">
-        <v>67</v>
+        <v>272</v>
+      </c>
+      <c r="F155">
+        <v>1996</v>
+      </c>
+      <c r="G155">
+        <v>2016</v>
+      </c>
+      <c r="H155" t="s">
+        <v>16</v>
+      </c>
+      <c r="I155" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="156" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
-        <v>500</v>
+        <v>66</v>
       </c>
       <c r="B156" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="C156" s="2" t="s">
-        <v>499</v>
-      </c>
-      <c r="D156" t="s">
-        <v>501</v>
-      </c>
-      <c r="E156" t="s">
-        <v>14</v>
-      </c>
-      <c r="F156">
-        <v>1946</v>
-      </c>
-      <c r="G156">
-        <v>2015</v>
-      </c>
-      <c r="H156" t="s">
-        <v>348</v>
-      </c>
-      <c r="I156" t="s">
-        <v>349</v>
+        <v>67</v>
       </c>
     </row>
     <row r="157" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
-        <v>383</v>
+        <v>500</v>
       </c>
       <c r="B157" t="s">
         <v>40</v>
       </c>
       <c r="C157" s="2" t="s">
-        <v>384</v>
+        <v>499</v>
+      </c>
+      <c r="D157" t="s">
+        <v>501</v>
       </c>
       <c r="E157" t="s">
-        <v>386</v>
+        <v>14</v>
       </c>
       <c r="F157">
-        <v>1951</v>
+        <v>1946</v>
+      </c>
+      <c r="G157">
+        <v>2015</v>
       </c>
       <c r="H157" t="s">
         <v>348</v>
@@ -5215,178 +5248,181 @@
       <c r="I157" t="s">
         <v>349</v>
       </c>
-      <c r="N157" s="2" t="s">
-        <v>385</v>
-      </c>
     </row>
     <row r="158" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
-        <v>139</v>
+        <v>383</v>
       </c>
       <c r="B158" t="s">
         <v>40</v>
       </c>
       <c r="C158" s="2" t="s">
-        <v>140</v>
+        <v>384</v>
+      </c>
+      <c r="E158" t="s">
+        <v>386</v>
+      </c>
+      <c r="F158">
+        <v>1951</v>
+      </c>
+      <c r="H158" t="s">
+        <v>348</v>
+      </c>
+      <c r="I158" t="s">
+        <v>349</v>
+      </c>
+      <c r="N158" s="2" t="s">
+        <v>385</v>
       </c>
     </row>
     <row r="159" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
-        <v>329</v>
+        <v>139</v>
       </c>
       <c r="B159" t="s">
-        <v>165</v>
+        <v>40</v>
       </c>
       <c r="C159" s="2" t="s">
-        <v>328</v>
-      </c>
-      <c r="E159" t="s">
-        <v>34</v>
-      </c>
-      <c r="F159">
-        <v>1789</v>
-      </c>
-      <c r="H159" t="s">
-        <v>16</v>
-      </c>
-      <c r="I159" t="s">
-        <v>20</v>
+        <v>140</v>
       </c>
     </row>
     <row r="160" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
-        <v>172</v>
+        <v>329</v>
       </c>
       <c r="B160" t="s">
-        <v>60</v>
+        <v>165</v>
       </c>
       <c r="C160" s="2" t="s">
-        <v>171</v>
+        <v>328</v>
+      </c>
+      <c r="E160" t="s">
+        <v>34</v>
+      </c>
+      <c r="F160">
+        <v>1789</v>
+      </c>
+      <c r="H160" t="s">
+        <v>16</v>
+      </c>
+      <c r="I160" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="161" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
-        <v>217</v>
+        <v>172</v>
       </c>
       <c r="B161" t="s">
         <v>60</v>
       </c>
       <c r="C161" s="2" t="s">
-        <v>216</v>
-      </c>
-      <c r="E161" t="s">
-        <v>14</v>
-      </c>
-      <c r="F161">
-        <v>1900</v>
-      </c>
-      <c r="H161" t="s">
-        <v>16</v>
-      </c>
-      <c r="I161" t="s">
-        <v>20</v>
+        <v>171</v>
       </c>
     </row>
     <row r="162" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
-        <v>132</v>
+        <v>217</v>
       </c>
       <c r="B162" t="s">
-        <v>259</v>
+        <v>60</v>
       </c>
       <c r="C162" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="Q162" t="s">
-        <v>17</v>
+        <v>216</v>
+      </c>
+      <c r="E162" t="s">
+        <v>14</v>
+      </c>
+      <c r="F162">
+        <v>1900</v>
+      </c>
+      <c r="H162" t="s">
+        <v>16</v>
+      </c>
+      <c r="I162" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="163" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
-        <v>182</v>
+        <v>132</v>
       </c>
       <c r="B163" t="s">
-        <v>165</v>
+        <v>259</v>
       </c>
       <c r="C163" s="2" t="s">
-        <v>181</v>
+        <v>133</v>
+      </c>
+      <c r="Q163" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="164" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
-        <v>423</v>
+        <v>182</v>
       </c>
       <c r="B164" t="s">
-        <v>86</v>
+        <v>165</v>
       </c>
       <c r="C164" s="2" t="s">
-        <v>424</v>
-      </c>
-      <c r="E164" t="s">
-        <v>34</v>
-      </c>
-      <c r="F164">
-        <v>1996</v>
-      </c>
-      <c r="G164">
-        <v>2016</v>
-      </c>
-      <c r="H164" t="s">
-        <v>348</v>
-      </c>
-      <c r="I164" t="s">
-        <v>425</v>
+        <v>181</v>
       </c>
     </row>
     <row r="165" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
-        <v>115</v>
+        <v>423</v>
       </c>
       <c r="B165" t="s">
-        <v>128</v>
+        <v>86</v>
       </c>
       <c r="C165" s="2" t="s">
-        <v>116</v>
+        <v>424</v>
+      </c>
+      <c r="E165" t="s">
+        <v>34</v>
+      </c>
+      <c r="F165">
+        <v>1996</v>
+      </c>
+      <c r="G165">
+        <v>2016</v>
+      </c>
+      <c r="H165" t="s">
+        <v>348</v>
+      </c>
+      <c r="I165" t="s">
+        <v>425</v>
       </c>
     </row>
     <row r="166" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
-        <v>263</v>
+        <v>115</v>
       </c>
       <c r="B166" t="s">
-        <v>250</v>
+        <v>128</v>
       </c>
       <c r="C166" s="2" t="s">
-        <v>264</v>
-      </c>
-      <c r="E166" t="s">
-        <v>265</v>
-      </c>
-      <c r="F166">
-        <v>1500</v>
-      </c>
-      <c r="G166">
-        <v>2000</v>
-      </c>
-      <c r="H166" t="s">
-        <v>16</v>
-      </c>
-      <c r="I166" t="s">
-        <v>20</v>
+        <v>116</v>
       </c>
     </row>
     <row r="167" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
-        <v>221</v>
+        <v>263</v>
       </c>
       <c r="B167" t="s">
-        <v>86</v>
+        <v>250</v>
       </c>
       <c r="C167" s="2" t="s">
-        <v>220</v>
+        <v>264</v>
+      </c>
+      <c r="E167" t="s">
+        <v>265</v>
       </c>
       <c r="F167">
-        <v>2013</v>
+        <v>1500</v>
+      </c>
+      <c r="G167">
+        <v>2000</v>
       </c>
       <c r="H167" t="s">
         <v>16</v>
@@ -5397,22 +5433,16 @@
     </row>
     <row r="168" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
-        <v>13</v>
+        <v>221</v>
       </c>
       <c r="B168" t="s">
-        <v>25</v>
+        <v>86</v>
       </c>
       <c r="C168" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="D168" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="E168" t="s">
-        <v>14</v>
+        <v>220</v>
       </c>
       <c r="F168">
-        <v>1981</v>
+        <v>2013</v>
       </c>
       <c r="H168" t="s">
         <v>16</v>
@@ -5423,166 +5453,192 @@
     </row>
     <row r="169" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
+        <v>13</v>
+      </c>
+      <c r="B169" t="s">
+        <v>25</v>
+      </c>
+      <c r="C169" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D169" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E169" t="s">
+        <v>14</v>
+      </c>
+      <c r="F169">
+        <v>1981</v>
+      </c>
+      <c r="H169" t="s">
+        <v>16</v>
+      </c>
+      <c r="I169" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="170" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A170" t="s">
         <v>283</v>
       </c>
-      <c r="B169" t="s">
+      <c r="B170" t="s">
         <v>124</v>
       </c>
-      <c r="C169" s="2" t="s">
+      <c r="C170" s="2" t="s">
         <v>284</v>
       </c>
-      <c r="H169" t="s">
-        <v>16</v>
-      </c>
-      <c r="I169" t="s">
+      <c r="H170" t="s">
+        <v>16</v>
+      </c>
+      <c r="I170" t="s">
         <v>20</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:Q169">
+  <sortState ref="A2:Q170">
     <sortCondition ref="A2"/>
   </sortState>
   <hyperlinks>
     <hyperlink ref="C6" r:id="rId1"/>
-    <hyperlink ref="C63" r:id="rId2"/>
+    <hyperlink ref="C64" r:id="rId2"/>
     <hyperlink ref="C7" r:id="rId3"/>
     <hyperlink ref="C11" r:id="rId4"/>
-    <hyperlink ref="C101" r:id="rId5"/>
-    <hyperlink ref="C121" r:id="rId6"/>
-    <hyperlink ref="C168" r:id="rId7"/>
-    <hyperlink ref="C37" r:id="rId8"/>
+    <hyperlink ref="C102" r:id="rId5"/>
+    <hyperlink ref="C122" r:id="rId6"/>
+    <hyperlink ref="C169" r:id="rId7"/>
+    <hyperlink ref="C38" r:id="rId8"/>
     <hyperlink ref="C32" r:id="rId9"/>
-    <hyperlink ref="C54" r:id="rId10"/>
-    <hyperlink ref="C61" r:id="rId11"/>
+    <hyperlink ref="C55" r:id="rId10"/>
+    <hyperlink ref="C62" r:id="rId11"/>
     <hyperlink ref="C3" r:id="rId12"/>
     <hyperlink ref="C21" r:id="rId13"/>
-    <hyperlink ref="C65" r:id="rId14"/>
-    <hyperlink ref="C93" r:id="rId15"/>
+    <hyperlink ref="C66" r:id="rId14"/>
+    <hyperlink ref="C94" r:id="rId15"/>
     <hyperlink ref="C31" r:id="rId16"/>
-    <hyperlink ref="C117" r:id="rId17"/>
-    <hyperlink ref="C45" r:id="rId18"/>
-    <hyperlink ref="C78" r:id="rId19"/>
+    <hyperlink ref="C118" r:id="rId17"/>
+    <hyperlink ref="C46" r:id="rId18"/>
+    <hyperlink ref="C79" r:id="rId19"/>
     <hyperlink ref="C17" r:id="rId20"/>
-    <hyperlink ref="C155" r:id="rId21"/>
+    <hyperlink ref="C156" r:id="rId21"/>
     <hyperlink ref="C8" r:id="rId22"/>
-    <hyperlink ref="C41" r:id="rId23"/>
-    <hyperlink ref="C58" r:id="rId24"/>
-    <hyperlink ref="C55" r:id="rId25"/>
-    <hyperlink ref="C59" r:id="rId26"/>
-    <hyperlink ref="C60" r:id="rId27"/>
-    <hyperlink ref="C75" r:id="rId28"/>
-    <hyperlink ref="C98" r:id="rId29"/>
-    <hyperlink ref="C146" r:id="rId30"/>
-    <hyperlink ref="C104" r:id="rId31"/>
-    <hyperlink ref="C88" r:id="rId32"/>
-    <hyperlink ref="C110" r:id="rId33"/>
-    <hyperlink ref="C76" r:id="rId34"/>
+    <hyperlink ref="C42" r:id="rId23"/>
+    <hyperlink ref="C59" r:id="rId24"/>
+    <hyperlink ref="C56" r:id="rId25"/>
+    <hyperlink ref="C60" r:id="rId26"/>
+    <hyperlink ref="C61" r:id="rId27"/>
+    <hyperlink ref="C76" r:id="rId28"/>
+    <hyperlink ref="C99" r:id="rId29"/>
+    <hyperlink ref="C147" r:id="rId30"/>
+    <hyperlink ref="C105" r:id="rId31"/>
+    <hyperlink ref="C89" r:id="rId32"/>
+    <hyperlink ref="C111" r:id="rId33"/>
+    <hyperlink ref="C77" r:id="rId34"/>
     <hyperlink ref="C18" r:id="rId35"/>
-    <hyperlink ref="C144" r:id="rId36"/>
+    <hyperlink ref="C145" r:id="rId36"/>
     <hyperlink ref="C16" r:id="rId37"/>
-    <hyperlink ref="C165" r:id="rId38"/>
-    <hyperlink ref="C92" r:id="rId39"/>
-    <hyperlink ref="C62" r:id="rId40"/>
-    <hyperlink ref="C127" r:id="rId41"/>
+    <hyperlink ref="C166" r:id="rId38"/>
+    <hyperlink ref="C93" r:id="rId39"/>
+    <hyperlink ref="C63" r:id="rId40"/>
+    <hyperlink ref="C128" r:id="rId41"/>
     <hyperlink ref="C19" r:id="rId42"/>
-    <hyperlink ref="C56" r:id="rId43"/>
+    <hyperlink ref="C57" r:id="rId43"/>
     <hyperlink ref="C25" r:id="rId44"/>
-    <hyperlink ref="C118" r:id="rId45"/>
-    <hyperlink ref="C162" r:id="rId46"/>
+    <hyperlink ref="C119" r:id="rId45"/>
+    <hyperlink ref="C163" r:id="rId46"/>
     <hyperlink ref="C29" r:id="rId47" display="http://comparativeconstitutionsproject.org/"/>
-    <hyperlink ref="C115" r:id="rId48"/>
-    <hyperlink ref="C158" r:id="rId49"/>
-    <hyperlink ref="C131" r:id="rId50"/>
-    <hyperlink ref="C125" r:id="rId51"/>
+    <hyperlink ref="C116" r:id="rId48"/>
+    <hyperlink ref="C159" r:id="rId49"/>
+    <hyperlink ref="C132" r:id="rId50"/>
+    <hyperlink ref="C126" r:id="rId51"/>
     <hyperlink ref="C24" r:id="rId52"/>
-    <hyperlink ref="C119" r:id="rId53"/>
-    <hyperlink ref="C52" r:id="rId54"/>
-    <hyperlink ref="C82" r:id="rId55"/>
-    <hyperlink ref="C85" r:id="rId56"/>
-    <hyperlink ref="C116" r:id="rId57"/>
-    <hyperlink ref="C106" r:id="rId58"/>
-    <hyperlink ref="C135" r:id="rId59"/>
+    <hyperlink ref="C120" r:id="rId53"/>
+    <hyperlink ref="C53" r:id="rId54"/>
+    <hyperlink ref="C83" r:id="rId55"/>
+    <hyperlink ref="C86" r:id="rId56"/>
+    <hyperlink ref="C117" r:id="rId57"/>
+    <hyperlink ref="C107" r:id="rId58"/>
+    <hyperlink ref="C136" r:id="rId59"/>
     <hyperlink ref="C33" r:id="rId60"/>
-    <hyperlink ref="C148" r:id="rId61"/>
+    <hyperlink ref="C149" r:id="rId61"/>
     <hyperlink ref="C9" r:id="rId62"/>
     <hyperlink ref="C35" r:id="rId63"/>
-    <hyperlink ref="C149" r:id="rId64"/>
+    <hyperlink ref="C150" r:id="rId64"/>
     <hyperlink ref="C15" r:id="rId65"/>
-    <hyperlink ref="C160" r:id="rId66"/>
+    <hyperlink ref="C161" r:id="rId66"/>
     <hyperlink ref="C27" r:id="rId67"/>
     <hyperlink ref="C26" r:id="rId68"/>
     <hyperlink ref="C28" r:id="rId69"/>
-    <hyperlink ref="C57" r:id="rId70"/>
-    <hyperlink ref="C163" r:id="rId71"/>
+    <hyperlink ref="C58" r:id="rId70"/>
+    <hyperlink ref="C164" r:id="rId71"/>
     <hyperlink ref="C30" r:id="rId72"/>
-    <hyperlink ref="C122" r:id="rId73"/>
+    <hyperlink ref="C123" r:id="rId73"/>
     <hyperlink ref="C34" r:id="rId74"/>
-    <hyperlink ref="C49" r:id="rId75"/>
-    <hyperlink ref="C138" r:id="rId76"/>
-    <hyperlink ref="C46" r:id="rId77"/>
-    <hyperlink ref="C42" r:id="rId78"/>
-    <hyperlink ref="C73" r:id="rId79"/>
+    <hyperlink ref="C50" r:id="rId75"/>
+    <hyperlink ref="C139" r:id="rId76"/>
+    <hyperlink ref="C47" r:id="rId77"/>
+    <hyperlink ref="C43" r:id="rId78"/>
+    <hyperlink ref="C74" r:id="rId79"/>
     <hyperlink ref="C5" r:id="rId80"/>
-    <hyperlink ref="C72" r:id="rId81"/>
+    <hyperlink ref="C73" r:id="rId81"/>
     <hyperlink ref="C13" r:id="rId82"/>
-    <hyperlink ref="C114" r:id="rId83"/>
-    <hyperlink ref="C123" r:id="rId84"/>
-    <hyperlink ref="C151" r:id="rId85"/>
-    <hyperlink ref="C38" r:id="rId86"/>
-    <hyperlink ref="C161" r:id="rId87"/>
-    <hyperlink ref="C48" r:id="rId88"/>
-    <hyperlink ref="C167" r:id="rId89"/>
-    <hyperlink ref="C102" r:id="rId90"/>
-    <hyperlink ref="C70" r:id="rId91"/>
-    <hyperlink ref="C103" r:id="rId92"/>
-    <hyperlink ref="C141" r:id="rId93"/>
-    <hyperlink ref="C86" r:id="rId94"/>
-    <hyperlink ref="C108" r:id="rId95"/>
-    <hyperlink ref="C142" r:id="rId96"/>
-    <hyperlink ref="C66" r:id="rId97"/>
-    <hyperlink ref="C120" r:id="rId98"/>
-    <hyperlink ref="C50" r:id="rId99"/>
-    <hyperlink ref="C47" r:id="rId100"/>
-    <hyperlink ref="C89" r:id="rId101"/>
-    <hyperlink ref="C64" r:id="rId102"/>
+    <hyperlink ref="C115" r:id="rId83"/>
+    <hyperlink ref="C124" r:id="rId84"/>
+    <hyperlink ref="C152" r:id="rId85"/>
+    <hyperlink ref="C39" r:id="rId86"/>
+    <hyperlink ref="C162" r:id="rId87"/>
+    <hyperlink ref="C49" r:id="rId88"/>
+    <hyperlink ref="C168" r:id="rId89"/>
+    <hyperlink ref="C103" r:id="rId90"/>
+    <hyperlink ref="C71" r:id="rId91"/>
+    <hyperlink ref="C104" r:id="rId92"/>
+    <hyperlink ref="C142" r:id="rId93"/>
+    <hyperlink ref="C87" r:id="rId94"/>
+    <hyperlink ref="C109" r:id="rId95"/>
+    <hyperlink ref="C143" r:id="rId96"/>
+    <hyperlink ref="C67" r:id="rId97"/>
+    <hyperlink ref="C121" r:id="rId98"/>
+    <hyperlink ref="C51" r:id="rId99"/>
+    <hyperlink ref="C48" r:id="rId100"/>
+    <hyperlink ref="C90" r:id="rId101"/>
+    <hyperlink ref="C65" r:id="rId102"/>
     <hyperlink ref="C2" r:id="rId103"/>
-    <hyperlink ref="C83" r:id="rId104"/>
-    <hyperlink ref="C87" r:id="rId105"/>
-    <hyperlink ref="C112" r:id="rId106"/>
-    <hyperlink ref="C51" r:id="rId107"/>
-    <hyperlink ref="C90" r:id="rId108"/>
-    <hyperlink ref="C140" r:id="rId109"/>
+    <hyperlink ref="C84" r:id="rId104"/>
+    <hyperlink ref="C88" r:id="rId105"/>
+    <hyperlink ref="C113" r:id="rId106"/>
+    <hyperlink ref="C52" r:id="rId107"/>
+    <hyperlink ref="C91" r:id="rId108"/>
+    <hyperlink ref="C141" r:id="rId109"/>
     <hyperlink ref="C14" r:id="rId110"/>
     <hyperlink ref="C4" r:id="rId111"/>
-    <hyperlink ref="C166" r:id="rId112"/>
-    <hyperlink ref="C96" r:id="rId113"/>
-    <hyperlink ref="C91" r:id="rId114"/>
-    <hyperlink ref="C154" r:id="rId115"/>
-    <hyperlink ref="C134" r:id="rId116"/>
-    <hyperlink ref="C68" r:id="rId117"/>
-    <hyperlink ref="C105" r:id="rId118"/>
-    <hyperlink ref="C80" r:id="rId119"/>
-    <hyperlink ref="C169" r:id="rId120"/>
-    <hyperlink ref="C71" r:id="rId121"/>
-    <hyperlink ref="C133" r:id="rId122"/>
-    <hyperlink ref="C111" r:id="rId123"/>
-    <hyperlink ref="C84" r:id="rId124"/>
-    <hyperlink ref="C109" r:id="rId125"/>
-    <hyperlink ref="C139" r:id="rId126"/>
-    <hyperlink ref="C94" r:id="rId127"/>
+    <hyperlink ref="C167" r:id="rId112"/>
+    <hyperlink ref="C97" r:id="rId113"/>
+    <hyperlink ref="C92" r:id="rId114"/>
+    <hyperlink ref="C155" r:id="rId115"/>
+    <hyperlink ref="C135" r:id="rId116"/>
+    <hyperlink ref="C69" r:id="rId117"/>
+    <hyperlink ref="C106" r:id="rId118"/>
+    <hyperlink ref="C81" r:id="rId119"/>
+    <hyperlink ref="C170" r:id="rId120"/>
+    <hyperlink ref="C72" r:id="rId121"/>
+    <hyperlink ref="C134" r:id="rId122"/>
+    <hyperlink ref="C112" r:id="rId123"/>
+    <hyperlink ref="C85" r:id="rId124"/>
+    <hyperlink ref="C110" r:id="rId125"/>
+    <hyperlink ref="C140" r:id="rId126"/>
+    <hyperlink ref="C95" r:id="rId127"/>
     <hyperlink ref="C12" r:id="rId128"/>
     <hyperlink ref="C20" r:id="rId129"/>
-    <hyperlink ref="C132" r:id="rId130"/>
-    <hyperlink ref="C79" r:id="rId131"/>
-    <hyperlink ref="C147" r:id="rId132"/>
-    <hyperlink ref="C129" r:id="rId133"/>
-    <hyperlink ref="C128" r:id="rId134"/>
-    <hyperlink ref="C130" r:id="rId135"/>
-    <hyperlink ref="C153" r:id="rId136"/>
-    <hyperlink ref="C145" r:id="rId137"/>
-    <hyperlink ref="C159" r:id="rId138"/>
-    <hyperlink ref="C40" r:id="rId139"/>
-    <hyperlink ref="C95" r:id="rId140"/>
+    <hyperlink ref="C133" r:id="rId130"/>
+    <hyperlink ref="C80" r:id="rId131"/>
+    <hyperlink ref="C148" r:id="rId132"/>
+    <hyperlink ref="C130" r:id="rId133"/>
+    <hyperlink ref="C129" r:id="rId134"/>
+    <hyperlink ref="C131" r:id="rId135"/>
+    <hyperlink ref="C154" r:id="rId136"/>
+    <hyperlink ref="C146" r:id="rId137"/>
+    <hyperlink ref="C160" r:id="rId138"/>
+    <hyperlink ref="C41" r:id="rId139"/>
+    <hyperlink ref="C96" r:id="rId140"/>
     <hyperlink ref="J2" r:id="rId141"/>
     <hyperlink ref="M3" r:id="rId142"/>
     <hyperlink ref="J3" r:id="rId143"/>
@@ -5590,79 +5646,84 @@
     <hyperlink ref="J4" r:id="rId145"/>
     <hyperlink ref="P5" r:id="rId146"/>
     <hyperlink ref="J5" r:id="rId147"/>
-    <hyperlink ref="C113" r:id="rId148"/>
+    <hyperlink ref="C114" r:id="rId148"/>
     <hyperlink ref="C36" r:id="rId149"/>
     <hyperlink ref="P7" r:id="rId150"/>
     <hyperlink ref="J7" r:id="rId151"/>
     <hyperlink ref="M8" r:id="rId152"/>
     <hyperlink ref="L8" r:id="rId153"/>
     <hyperlink ref="J8" r:id="rId154"/>
-    <hyperlink ref="C157" r:id="rId155"/>
-    <hyperlink ref="N157" r:id="rId156"/>
+    <hyperlink ref="C158" r:id="rId155"/>
+    <hyperlink ref="N158" r:id="rId156"/>
     <hyperlink ref="C22" r:id="rId157"/>
     <hyperlink ref="N22" r:id="rId158"/>
-    <hyperlink ref="C67" r:id="rId159"/>
-    <hyperlink ref="C152" r:id="rId160"/>
-    <hyperlink ref="J152" r:id="rId161"/>
-    <hyperlink ref="C150" r:id="rId162"/>
-    <hyperlink ref="N150" r:id="rId163"/>
-    <hyperlink ref="J150" r:id="rId164"/>
-    <hyperlink ref="C99" r:id="rId165"/>
-    <hyperlink ref="C97" r:id="rId166"/>
-    <hyperlink ref="C43" r:id="rId167"/>
-    <hyperlink ref="J43" r:id="rId168"/>
-    <hyperlink ref="K43" r:id="rId169"/>
-    <hyperlink ref="C107" r:id="rId170"/>
-    <hyperlink ref="N107" r:id="rId171"/>
-    <hyperlink ref="C81" r:id="rId172"/>
-    <hyperlink ref="K81" r:id="rId173"/>
-    <hyperlink ref="C164" r:id="rId174"/>
-    <hyperlink ref="C124" r:id="rId175"/>
-    <hyperlink ref="K124" r:id="rId176"/>
+    <hyperlink ref="C68" r:id="rId159"/>
+    <hyperlink ref="C153" r:id="rId160"/>
+    <hyperlink ref="J153" r:id="rId161"/>
+    <hyperlink ref="C151" r:id="rId162"/>
+    <hyperlink ref="N151" r:id="rId163"/>
+    <hyperlink ref="J151" r:id="rId164"/>
+    <hyperlink ref="C100" r:id="rId165"/>
+    <hyperlink ref="C98" r:id="rId166"/>
+    <hyperlink ref="C44" r:id="rId167"/>
+    <hyperlink ref="J44" r:id="rId168"/>
+    <hyperlink ref="K44" r:id="rId169"/>
+    <hyperlink ref="C108" r:id="rId170"/>
+    <hyperlink ref="N108" r:id="rId171"/>
+    <hyperlink ref="C82" r:id="rId172"/>
+    <hyperlink ref="K82" r:id="rId173"/>
+    <hyperlink ref="C165" r:id="rId174"/>
+    <hyperlink ref="C125" r:id="rId175"/>
+    <hyperlink ref="K125" r:id="rId176"/>
     <hyperlink ref="L9" r:id="rId177"/>
     <hyperlink ref="J9" r:id="rId178"/>
     <hyperlink ref="J11" r:id="rId179"/>
-    <hyperlink ref="C136" r:id="rId180"/>
-    <hyperlink ref="J136" r:id="rId181"/>
-    <hyperlink ref="L136" r:id="rId182"/>
-    <hyperlink ref="K136" r:id="rId183"/>
-    <hyperlink ref="C137" r:id="rId184"/>
-    <hyperlink ref="J137" r:id="rId185"/>
-    <hyperlink ref="K137" r:id="rId186"/>
-    <hyperlink ref="L137" r:id="rId187"/>
-    <hyperlink ref="C69" r:id="rId188"/>
-    <hyperlink ref="J69" r:id="rId189"/>
-    <hyperlink ref="N69" r:id="rId190"/>
-    <hyperlink ref="C143" r:id="rId191"/>
-    <hyperlink ref="C100" r:id="rId192"/>
-    <hyperlink ref="J100" r:id="rId193"/>
-    <hyperlink ref="L100" r:id="rId194"/>
-    <hyperlink ref="C77" r:id="rId195"/>
-    <hyperlink ref="C53" r:id="rId196"/>
-    <hyperlink ref="L53" r:id="rId197"/>
-    <hyperlink ref="K53" r:id="rId198"/>
-    <hyperlink ref="J53" r:id="rId199"/>
-    <hyperlink ref="C74" r:id="rId200"/>
-    <hyperlink ref="J74" r:id="rId201"/>
-    <hyperlink ref="K74" r:id="rId202"/>
-    <hyperlink ref="L74" r:id="rId203"/>
-    <hyperlink ref="C126" r:id="rId204"/>
-    <hyperlink ref="N126" r:id="rId205"/>
-    <hyperlink ref="C39" r:id="rId206"/>
-    <hyperlink ref="K39" r:id="rId207"/>
-    <hyperlink ref="J39" r:id="rId208"/>
+    <hyperlink ref="C137" r:id="rId180"/>
+    <hyperlink ref="J137" r:id="rId181"/>
+    <hyperlink ref="L137" r:id="rId182"/>
+    <hyperlink ref="K137" r:id="rId183"/>
+    <hyperlink ref="C138" r:id="rId184"/>
+    <hyperlink ref="J138" r:id="rId185"/>
+    <hyperlink ref="K138" r:id="rId186"/>
+    <hyperlink ref="L138" r:id="rId187"/>
+    <hyperlink ref="C70" r:id="rId188"/>
+    <hyperlink ref="J70" r:id="rId189"/>
+    <hyperlink ref="N70" r:id="rId190"/>
+    <hyperlink ref="C144" r:id="rId191"/>
+    <hyperlink ref="C101" r:id="rId192"/>
+    <hyperlink ref="J101" r:id="rId193"/>
+    <hyperlink ref="L101" r:id="rId194"/>
+    <hyperlink ref="C78" r:id="rId195"/>
+    <hyperlink ref="C54" r:id="rId196"/>
+    <hyperlink ref="L54" r:id="rId197"/>
+    <hyperlink ref="K54" r:id="rId198"/>
+    <hyperlink ref="J54" r:id="rId199"/>
+    <hyperlink ref="C75" r:id="rId200"/>
+    <hyperlink ref="J75" r:id="rId201"/>
+    <hyperlink ref="K75" r:id="rId202"/>
+    <hyperlink ref="L75" r:id="rId203"/>
+    <hyperlink ref="C127" r:id="rId204"/>
+    <hyperlink ref="N127" r:id="rId205"/>
+    <hyperlink ref="C40" r:id="rId206"/>
+    <hyperlink ref="K40" r:id="rId207"/>
+    <hyperlink ref="J40" r:id="rId208"/>
     <hyperlink ref="C10" r:id="rId209"/>
     <hyperlink ref="J10" r:id="rId210"/>
     <hyperlink ref="P10" r:id="rId211"/>
     <hyperlink ref="N10" r:id="rId212"/>
-    <hyperlink ref="C44" r:id="rId213"/>
-    <hyperlink ref="J44" r:id="rId214"/>
-    <hyperlink ref="K44" r:id="rId215"/>
-    <hyperlink ref="L44" r:id="rId216"/>
-    <hyperlink ref="M44" r:id="rId217"/>
-    <hyperlink ref="N44" r:id="rId218"/>
+    <hyperlink ref="C45" r:id="rId213"/>
+    <hyperlink ref="J45" r:id="rId214"/>
+    <hyperlink ref="K45" r:id="rId215"/>
+    <hyperlink ref="L45" r:id="rId216"/>
+    <hyperlink ref="M45" r:id="rId217"/>
+    <hyperlink ref="N45" r:id="rId218"/>
     <hyperlink ref="C23" r:id="rId219"/>
-    <hyperlink ref="C156" r:id="rId220"/>
+    <hyperlink ref="C157" r:id="rId220"/>
+    <hyperlink ref="C37" r:id="rId221"/>
+    <hyperlink ref="J37" r:id="rId222"/>
+    <hyperlink ref="N37" r:id="rId223"/>
+    <hyperlink ref="L37" r:id="rId224"/>
+    <hyperlink ref="K37" r:id="rId225"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
add 'UCDP Peacemakers at Risk'
</commit_message>
<xml_diff>
--- a/PolData.xlsx
+++ b/PolData.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="923" uniqueCount="508">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="931" uniqueCount="513">
   <si>
     <t>name</t>
   </si>
@@ -1551,6 +1551,21 @@
   </si>
   <si>
     <t>http://ippsr.msu.edu/sites/default/files/correlatesofstatepolicyprojectv1_13.csv</t>
+  </si>
+  <si>
+    <t>UCDP Peacemakers at Risk</t>
+  </si>
+  <si>
+    <t>https://www.prio.org/JPR/Datasets/</t>
+  </si>
+  <si>
+    <t>sub-Saharan Africa</t>
+  </si>
+  <si>
+    <t>Peacekeeping, violence, conflict, events</t>
+  </si>
+  <si>
+    <t>http://file.prio.no/Journals/JPR/2018/55/1/Sara%20Lindberg%20Bromley.zip</t>
   </si>
 </sst>
 </file>
@@ -1890,10 +1905,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q170"/>
+  <dimension ref="A1:Q171"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A133" workbookViewId="0">
-      <selection activeCell="E38" sqref="E38"/>
+    <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
+      <selection activeCell="A156" sqref="A156"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4977,7 +4992,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="145" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
         <v>109</v>
       </c>
@@ -4994,7 +5009,7 @@
         <v>1956</v>
       </c>
     </row>
-    <row r="146" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
         <v>326</v>
       </c>
@@ -5017,7 +5032,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="147" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
         <v>91</v>
       </c>
@@ -5034,7 +5049,7 @@
         <v>1999</v>
       </c>
     </row>
-    <row r="148" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
         <v>314</v>
       </c>
@@ -5060,7 +5075,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="149" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
         <v>161</v>
       </c>
@@ -5071,7 +5086,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="150" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
         <v>168</v>
       </c>
@@ -5082,7 +5097,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="151" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
         <v>399</v>
       </c>
@@ -5114,7 +5129,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="152" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
         <v>213</v>
       </c>
@@ -5131,7 +5146,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="153" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
         <v>395</v>
       </c>
@@ -5163,7 +5178,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="154" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
         <v>323</v>
       </c>
@@ -5186,7 +5201,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="155" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
         <v>273</v>
       </c>
@@ -5209,61 +5224,70 @@
         <v>20</v>
       </c>
     </row>
-    <row r="156" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
+        <v>508</v>
+      </c>
+      <c r="B156" t="s">
+        <v>40</v>
+      </c>
+      <c r="C156" s="2" t="s">
+        <v>509</v>
+      </c>
+      <c r="D156" t="s">
+        <v>511</v>
+      </c>
+      <c r="E156" t="s">
+        <v>510</v>
+      </c>
+      <c r="F156">
+        <v>1989</v>
+      </c>
+      <c r="G156">
+        <v>2009</v>
+      </c>
+      <c r="H156" t="s">
+        <v>348</v>
+      </c>
+      <c r="I156" t="s">
+        <v>349</v>
+      </c>
+      <c r="P156" s="2" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="157" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A157" t="s">
         <v>66</v>
       </c>
-      <c r="B156" t="s">
+      <c r="B157" t="s">
         <v>25</v>
       </c>
-      <c r="C156" s="2" t="s">
+      <c r="C157" s="2" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="157" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A157" t="s">
+    <row r="158" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A158" t="s">
         <v>500</v>
-      </c>
-      <c r="B157" t="s">
-        <v>40</v>
-      </c>
-      <c r="C157" s="2" t="s">
-        <v>499</v>
-      </c>
-      <c r="D157" t="s">
-        <v>501</v>
-      </c>
-      <c r="E157" t="s">
-        <v>14</v>
-      </c>
-      <c r="F157">
-        <v>1946</v>
-      </c>
-      <c r="G157">
-        <v>2015</v>
-      </c>
-      <c r="H157" t="s">
-        <v>348</v>
-      </c>
-      <c r="I157" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="158" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A158" t="s">
-        <v>383</v>
       </c>
       <c r="B158" t="s">
         <v>40</v>
       </c>
       <c r="C158" s="2" t="s">
-        <v>384</v>
+        <v>499</v>
+      </c>
+      <c r="D158" t="s">
+        <v>501</v>
       </c>
       <c r="E158" t="s">
-        <v>386</v>
+        <v>14</v>
       </c>
       <c r="F158">
-        <v>1951</v>
+        <v>1946</v>
+      </c>
+      <c r="G158">
+        <v>2015</v>
       </c>
       <c r="H158" t="s">
         <v>348</v>
@@ -5271,178 +5295,181 @@
       <c r="I158" t="s">
         <v>349</v>
       </c>
-      <c r="N158" s="2" t="s">
-        <v>385</v>
-      </c>
-    </row>
-    <row r="159" spans="1:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="159" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
-        <v>139</v>
+        <v>383</v>
       </c>
       <c r="B159" t="s">
         <v>40</v>
       </c>
       <c r="C159" s="2" t="s">
+        <v>384</v>
+      </c>
+      <c r="E159" t="s">
+        <v>386</v>
+      </c>
+      <c r="F159">
+        <v>1951</v>
+      </c>
+      <c r="H159" t="s">
+        <v>348</v>
+      </c>
+      <c r="I159" t="s">
+        <v>349</v>
+      </c>
+      <c r="N159" s="2" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="160" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A160" t="s">
+        <v>139</v>
+      </c>
+      <c r="B160" t="s">
+        <v>40</v>
+      </c>
+      <c r="C160" s="2" t="s">
         <v>140</v>
-      </c>
-    </row>
-    <row r="160" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A160" t="s">
-        <v>329</v>
-      </c>
-      <c r="B160" t="s">
-        <v>165</v>
-      </c>
-      <c r="C160" s="2" t="s">
-        <v>328</v>
-      </c>
-      <c r="E160" t="s">
-        <v>34</v>
-      </c>
-      <c r="F160">
-        <v>1789</v>
-      </c>
-      <c r="H160" t="s">
-        <v>16</v>
-      </c>
-      <c r="I160" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="161" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
-        <v>172</v>
+        <v>329</v>
       </c>
       <c r="B161" t="s">
-        <v>60</v>
+        <v>165</v>
       </c>
       <c r="C161" s="2" t="s">
-        <v>171</v>
+        <v>328</v>
+      </c>
+      <c r="E161" t="s">
+        <v>34</v>
+      </c>
+      <c r="F161">
+        <v>1789</v>
+      </c>
+      <c r="H161" t="s">
+        <v>16</v>
+      </c>
+      <c r="I161" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="162" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
-        <v>217</v>
+        <v>172</v>
       </c>
       <c r="B162" t="s">
         <v>60</v>
       </c>
       <c r="C162" s="2" t="s">
-        <v>216</v>
-      </c>
-      <c r="E162" t="s">
-        <v>14</v>
-      </c>
-      <c r="F162">
-        <v>1900</v>
-      </c>
-      <c r="H162" t="s">
-        <v>16</v>
-      </c>
-      <c r="I162" t="s">
-        <v>20</v>
+        <v>171</v>
       </c>
     </row>
     <row r="163" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
-        <v>132</v>
+        <v>217</v>
       </c>
       <c r="B163" t="s">
-        <v>259</v>
+        <v>60</v>
       </c>
       <c r="C163" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="Q163" t="s">
-        <v>17</v>
+        <v>216</v>
+      </c>
+      <c r="E163" t="s">
+        <v>14</v>
+      </c>
+      <c r="F163">
+        <v>1900</v>
+      </c>
+      <c r="H163" t="s">
+        <v>16</v>
+      </c>
+      <c r="I163" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="164" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
-        <v>182</v>
+        <v>132</v>
       </c>
       <c r="B164" t="s">
-        <v>165</v>
+        <v>259</v>
       </c>
       <c r="C164" s="2" t="s">
-        <v>181</v>
+        <v>133</v>
+      </c>
+      <c r="Q164" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="165" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
-        <v>423</v>
+        <v>182</v>
       </c>
       <c r="B165" t="s">
-        <v>86</v>
+        <v>165</v>
       </c>
       <c r="C165" s="2" t="s">
-        <v>424</v>
-      </c>
-      <c r="E165" t="s">
-        <v>34</v>
-      </c>
-      <c r="F165">
-        <v>1996</v>
-      </c>
-      <c r="G165">
-        <v>2016</v>
-      </c>
-      <c r="H165" t="s">
-        <v>348</v>
-      </c>
-      <c r="I165" t="s">
-        <v>425</v>
+        <v>181</v>
       </c>
     </row>
     <row r="166" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
-        <v>115</v>
+        <v>423</v>
       </c>
       <c r="B166" t="s">
-        <v>128</v>
+        <v>86</v>
       </c>
       <c r="C166" s="2" t="s">
-        <v>116</v>
+        <v>424</v>
+      </c>
+      <c r="E166" t="s">
+        <v>34</v>
+      </c>
+      <c r="F166">
+        <v>1996</v>
+      </c>
+      <c r="G166">
+        <v>2016</v>
+      </c>
+      <c r="H166" t="s">
+        <v>348</v>
+      </c>
+      <c r="I166" t="s">
+        <v>425</v>
       </c>
     </row>
     <row r="167" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
-        <v>263</v>
+        <v>115</v>
       </c>
       <c r="B167" t="s">
-        <v>250</v>
+        <v>128</v>
       </c>
       <c r="C167" s="2" t="s">
-        <v>264</v>
-      </c>
-      <c r="E167" t="s">
-        <v>265</v>
-      </c>
-      <c r="F167">
-        <v>1500</v>
-      </c>
-      <c r="G167">
-        <v>2000</v>
-      </c>
-      <c r="H167" t="s">
-        <v>16</v>
-      </c>
-      <c r="I167" t="s">
-        <v>20</v>
+        <v>116</v>
       </c>
     </row>
     <row r="168" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
-        <v>221</v>
+        <v>263</v>
       </c>
       <c r="B168" t="s">
-        <v>86</v>
+        <v>250</v>
       </c>
       <c r="C168" s="2" t="s">
-        <v>220</v>
+        <v>264</v>
+      </c>
+      <c r="E168" t="s">
+        <v>265</v>
       </c>
       <c r="F168">
-        <v>2013</v>
+        <v>1500</v>
+      </c>
+      <c r="G168">
+        <v>2000</v>
       </c>
       <c r="H168" t="s">
         <v>16</v>
@@ -5453,22 +5480,16 @@
     </row>
     <row r="169" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
-        <v>13</v>
+        <v>221</v>
       </c>
       <c r="B169" t="s">
-        <v>25</v>
+        <v>86</v>
       </c>
       <c r="C169" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="D169" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="E169" t="s">
-        <v>14</v>
+        <v>220</v>
       </c>
       <c r="F169">
-        <v>1981</v>
+        <v>2013</v>
       </c>
       <c r="H169" t="s">
         <v>16</v>
@@ -5479,23 +5500,49 @@
     </row>
     <row r="170" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
+        <v>13</v>
+      </c>
+      <c r="B170" t="s">
+        <v>25</v>
+      </c>
+      <c r="C170" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D170" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E170" t="s">
+        <v>14</v>
+      </c>
+      <c r="F170">
+        <v>1981</v>
+      </c>
+      <c r="H170" t="s">
+        <v>16</v>
+      </c>
+      <c r="I170" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="171" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A171" t="s">
         <v>283</v>
       </c>
-      <c r="B170" t="s">
+      <c r="B171" t="s">
         <v>124</v>
       </c>
-      <c r="C170" s="2" t="s">
+      <c r="C171" s="2" t="s">
         <v>284</v>
       </c>
-      <c r="H170" t="s">
-        <v>16</v>
-      </c>
-      <c r="I170" t="s">
+      <c r="H171" t="s">
+        <v>16</v>
+      </c>
+      <c r="I171" t="s">
         <v>20</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:Q170">
+  <sortState ref="A2:Q171">
     <sortCondition ref="A2"/>
   </sortState>
   <hyperlinks>
@@ -5505,7 +5552,7 @@
     <hyperlink ref="C11" r:id="rId4"/>
     <hyperlink ref="C102" r:id="rId5"/>
     <hyperlink ref="C122" r:id="rId6"/>
-    <hyperlink ref="C169" r:id="rId7"/>
+    <hyperlink ref="C170" r:id="rId7"/>
     <hyperlink ref="C38" r:id="rId8"/>
     <hyperlink ref="C32" r:id="rId9"/>
     <hyperlink ref="C55" r:id="rId10"/>
@@ -5519,7 +5566,7 @@
     <hyperlink ref="C46" r:id="rId18"/>
     <hyperlink ref="C79" r:id="rId19"/>
     <hyperlink ref="C17" r:id="rId20"/>
-    <hyperlink ref="C156" r:id="rId21"/>
+    <hyperlink ref="C157" r:id="rId21"/>
     <hyperlink ref="C8" r:id="rId22"/>
     <hyperlink ref="C42" r:id="rId23"/>
     <hyperlink ref="C59" r:id="rId24"/>
@@ -5536,7 +5583,7 @@
     <hyperlink ref="C18" r:id="rId35"/>
     <hyperlink ref="C145" r:id="rId36"/>
     <hyperlink ref="C16" r:id="rId37"/>
-    <hyperlink ref="C166" r:id="rId38"/>
+    <hyperlink ref="C167" r:id="rId38"/>
     <hyperlink ref="C93" r:id="rId39"/>
     <hyperlink ref="C63" r:id="rId40"/>
     <hyperlink ref="C128" r:id="rId41"/>
@@ -5544,10 +5591,10 @@
     <hyperlink ref="C57" r:id="rId43"/>
     <hyperlink ref="C25" r:id="rId44"/>
     <hyperlink ref="C119" r:id="rId45"/>
-    <hyperlink ref="C163" r:id="rId46"/>
+    <hyperlink ref="C164" r:id="rId46"/>
     <hyperlink ref="C29" r:id="rId47" display="http://comparativeconstitutionsproject.org/"/>
     <hyperlink ref="C116" r:id="rId48"/>
-    <hyperlink ref="C159" r:id="rId49"/>
+    <hyperlink ref="C160" r:id="rId49"/>
     <hyperlink ref="C132" r:id="rId50"/>
     <hyperlink ref="C126" r:id="rId51"/>
     <hyperlink ref="C24" r:id="rId52"/>
@@ -5564,12 +5611,12 @@
     <hyperlink ref="C35" r:id="rId63"/>
     <hyperlink ref="C150" r:id="rId64"/>
     <hyperlink ref="C15" r:id="rId65"/>
-    <hyperlink ref="C161" r:id="rId66"/>
+    <hyperlink ref="C162" r:id="rId66"/>
     <hyperlink ref="C27" r:id="rId67"/>
     <hyperlink ref="C26" r:id="rId68"/>
     <hyperlink ref="C28" r:id="rId69"/>
     <hyperlink ref="C58" r:id="rId70"/>
-    <hyperlink ref="C164" r:id="rId71"/>
+    <hyperlink ref="C165" r:id="rId71"/>
     <hyperlink ref="C30" r:id="rId72"/>
     <hyperlink ref="C123" r:id="rId73"/>
     <hyperlink ref="C34" r:id="rId74"/>
@@ -5585,9 +5632,9 @@
     <hyperlink ref="C124" r:id="rId84"/>
     <hyperlink ref="C152" r:id="rId85"/>
     <hyperlink ref="C39" r:id="rId86"/>
-    <hyperlink ref="C162" r:id="rId87"/>
+    <hyperlink ref="C163" r:id="rId87"/>
     <hyperlink ref="C49" r:id="rId88"/>
-    <hyperlink ref="C168" r:id="rId89"/>
+    <hyperlink ref="C169" r:id="rId89"/>
     <hyperlink ref="C103" r:id="rId90"/>
     <hyperlink ref="C71" r:id="rId91"/>
     <hyperlink ref="C104" r:id="rId92"/>
@@ -5610,7 +5657,7 @@
     <hyperlink ref="C141" r:id="rId109"/>
     <hyperlink ref="C14" r:id="rId110"/>
     <hyperlink ref="C4" r:id="rId111"/>
-    <hyperlink ref="C167" r:id="rId112"/>
+    <hyperlink ref="C168" r:id="rId112"/>
     <hyperlink ref="C97" r:id="rId113"/>
     <hyperlink ref="C92" r:id="rId114"/>
     <hyperlink ref="C155" r:id="rId115"/>
@@ -5618,7 +5665,7 @@
     <hyperlink ref="C69" r:id="rId117"/>
     <hyperlink ref="C106" r:id="rId118"/>
     <hyperlink ref="C81" r:id="rId119"/>
-    <hyperlink ref="C170" r:id="rId120"/>
+    <hyperlink ref="C171" r:id="rId120"/>
     <hyperlink ref="C72" r:id="rId121"/>
     <hyperlink ref="C134" r:id="rId122"/>
     <hyperlink ref="C112" r:id="rId123"/>
@@ -5636,7 +5683,7 @@
     <hyperlink ref="C131" r:id="rId135"/>
     <hyperlink ref="C154" r:id="rId136"/>
     <hyperlink ref="C146" r:id="rId137"/>
-    <hyperlink ref="C160" r:id="rId138"/>
+    <hyperlink ref="C161" r:id="rId138"/>
     <hyperlink ref="C41" r:id="rId139"/>
     <hyperlink ref="C96" r:id="rId140"/>
     <hyperlink ref="J2" r:id="rId141"/>
@@ -5653,8 +5700,8 @@
     <hyperlink ref="M8" r:id="rId152"/>
     <hyperlink ref="L8" r:id="rId153"/>
     <hyperlink ref="J8" r:id="rId154"/>
-    <hyperlink ref="C158" r:id="rId155"/>
-    <hyperlink ref="N158" r:id="rId156"/>
+    <hyperlink ref="C159" r:id="rId155"/>
+    <hyperlink ref="N159" r:id="rId156"/>
     <hyperlink ref="C22" r:id="rId157"/>
     <hyperlink ref="N22" r:id="rId158"/>
     <hyperlink ref="C68" r:id="rId159"/>
@@ -5672,7 +5719,7 @@
     <hyperlink ref="N108" r:id="rId171"/>
     <hyperlink ref="C82" r:id="rId172"/>
     <hyperlink ref="K82" r:id="rId173"/>
-    <hyperlink ref="C165" r:id="rId174"/>
+    <hyperlink ref="C166" r:id="rId174"/>
     <hyperlink ref="C125" r:id="rId175"/>
     <hyperlink ref="K125" r:id="rId176"/>
     <hyperlink ref="L9" r:id="rId177"/>
@@ -5718,12 +5765,14 @@
     <hyperlink ref="M45" r:id="rId217"/>
     <hyperlink ref="N45" r:id="rId218"/>
     <hyperlink ref="C23" r:id="rId219"/>
-    <hyperlink ref="C157" r:id="rId220"/>
+    <hyperlink ref="C158" r:id="rId220"/>
     <hyperlink ref="C37" r:id="rId221"/>
     <hyperlink ref="J37" r:id="rId222"/>
     <hyperlink ref="N37" r:id="rId223"/>
     <hyperlink ref="L37" r:id="rId224"/>
     <hyperlink ref="K37" r:id="rId225"/>
+    <hyperlink ref="C156" r:id="rId226"/>
+    <hyperlink ref="P156" r:id="rId227"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
add 'Militant Group Electoral Participation Dataset'
</commit_message>
<xml_diff>
--- a/PolData.xlsx
+++ b/PolData.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="931" uniqueCount="513">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="938" uniqueCount="516">
   <si>
     <t>name</t>
   </si>
@@ -1566,6 +1566,15 @@
   </si>
   <si>
     <t>http://file.prio.no/Journals/JPR/2018/55/1/Sara%20Lindberg%20Bromley.zip</t>
+  </si>
+  <si>
+    <t>http://dx.doi.org/10.7910/DVN/FB0R8A</t>
+  </si>
+  <si>
+    <t>Militant Group Electoral Participation Dataset</t>
+  </si>
+  <si>
+    <t>Militant group electoral participation, rebel parties, post-conflict elections, wartime elections</t>
   </si>
 </sst>
 </file>
@@ -1905,10 +1914,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q171"/>
+  <dimension ref="A1:Q172"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
-      <selection activeCell="A156" sqref="A156"/>
+    <sheetView tabSelected="1" topLeftCell="A149" workbookViewId="0">
+      <selection activeCell="A175" sqref="A175"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4276,244 +4285,247 @@
     </row>
     <row r="110" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>293</v>
+        <v>514</v>
       </c>
       <c r="B110" t="s">
         <v>40</v>
       </c>
       <c r="C110" s="2" t="s">
-        <v>294</v>
+        <v>513</v>
+      </c>
+      <c r="D110" t="s">
+        <v>515</v>
+      </c>
+      <c r="E110" t="s">
+        <v>14</v>
       </c>
       <c r="F110">
-        <v>2004</v>
+        <v>1970</v>
       </c>
       <c r="G110">
-        <v>2006</v>
+        <v>2010</v>
       </c>
       <c r="H110" t="s">
-        <v>16</v>
+        <v>348</v>
       </c>
       <c r="I110" t="s">
-        <v>20</v>
+        <v>349</v>
       </c>
     </row>
     <row r="111" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>102</v>
+        <v>293</v>
       </c>
       <c r="B111" t="s">
-        <v>99</v>
+        <v>40</v>
       </c>
       <c r="C111" s="2" t="s">
-        <v>103</v>
+        <v>294</v>
+      </c>
+      <c r="F111">
+        <v>2004</v>
+      </c>
+      <c r="G111">
+        <v>2006</v>
+      </c>
+      <c r="H111" t="s">
+        <v>16</v>
+      </c>
+      <c r="I111" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="112" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>289</v>
+        <v>102</v>
       </c>
       <c r="B112" t="s">
-        <v>124</v>
+        <v>99</v>
       </c>
       <c r="C112" s="2" t="s">
-        <v>290</v>
+        <v>103</v>
       </c>
     </row>
     <row r="113" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>246</v>
+        <v>289</v>
       </c>
       <c r="B113" t="s">
-        <v>165</v>
+        <v>124</v>
       </c>
       <c r="C113" s="2" t="s">
-        <v>247</v>
-      </c>
-      <c r="E113" t="s">
-        <v>14</v>
-      </c>
-      <c r="F113">
-        <v>1960</v>
-      </c>
-      <c r="G113">
-        <v>2006</v>
-      </c>
-      <c r="H113" t="s">
-        <v>16</v>
-      </c>
-      <c r="I113" t="s">
-        <v>249</v>
+        <v>290</v>
       </c>
     </row>
     <row r="114" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>365</v>
+        <v>246</v>
       </c>
       <c r="B114" t="s">
-        <v>128</v>
+        <v>165</v>
       </c>
       <c r="C114" s="2" t="s">
-        <v>364</v>
-      </c>
-      <c r="D114" t="s">
-        <v>370</v>
+        <v>247</v>
       </c>
       <c r="E114" t="s">
-        <v>366</v>
+        <v>14</v>
       </c>
       <c r="F114">
-        <v>1906</v>
+        <v>1960</v>
       </c>
       <c r="G114">
-        <v>2013</v>
+        <v>2006</v>
       </c>
       <c r="H114" t="s">
-        <v>367</v>
+        <v>16</v>
       </c>
       <c r="I114" t="s">
-        <v>368</v>
-      </c>
-      <c r="Q114" t="s">
-        <v>369</v>
+        <v>249</v>
       </c>
     </row>
     <row r="115" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>208</v>
+        <v>365</v>
       </c>
       <c r="B115" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="C115" s="2" t="s">
-        <v>209</v>
+        <v>364</v>
+      </c>
+      <c r="D115" t="s">
+        <v>370</v>
+      </c>
+      <c r="E115" t="s">
+        <v>366</v>
       </c>
       <c r="F115">
-        <v>1932</v>
+        <v>1906</v>
       </c>
       <c r="G115">
-        <v>2014</v>
+        <v>2013</v>
       </c>
       <c r="H115" t="s">
-        <v>16</v>
+        <v>367</v>
       </c>
       <c r="I115" t="s">
-        <v>20</v>
+        <v>368</v>
+      </c>
+      <c r="Q115" t="s">
+        <v>369</v>
       </c>
     </row>
     <row r="116" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>137</v>
+        <v>208</v>
       </c>
       <c r="B116" t="s">
-        <v>259</v>
+        <v>124</v>
       </c>
       <c r="C116" s="2" t="s">
-        <v>138</v>
+        <v>209</v>
+      </c>
+      <c r="F116">
+        <v>1932</v>
+      </c>
+      <c r="G116">
+        <v>2014</v>
+      </c>
+      <c r="H116" t="s">
+        <v>16</v>
+      </c>
+      <c r="I116" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="117" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>155</v>
+        <v>137</v>
       </c>
       <c r="B117" t="s">
         <v>259</v>
       </c>
       <c r="C117" s="2" t="s">
-        <v>154</v>
+        <v>138</v>
       </c>
     </row>
     <row r="118" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>57</v>
+        <v>155</v>
       </c>
       <c r="B118" t="s">
-        <v>128</v>
+        <v>259</v>
       </c>
       <c r="C118" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="Q118" t="s">
-        <v>17</v>
+        <v>154</v>
       </c>
     </row>
     <row r="119" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>129</v>
+        <v>57</v>
       </c>
       <c r="B119" t="s">
-        <v>259</v>
+        <v>128</v>
       </c>
       <c r="C119" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="E119" t="s">
-        <v>131</v>
-      </c>
-      <c r="F119">
-        <v>1945</v>
-      </c>
-      <c r="G119">
-        <v>2008</v>
-      </c>
-      <c r="I119" t="s">
-        <v>20</v>
+        <v>58</v>
+      </c>
+      <c r="Q119" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="120" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>148</v>
+        <v>129</v>
       </c>
       <c r="B120" t="s">
-        <v>128</v>
+        <v>259</v>
       </c>
       <c r="C120" s="2" t="s">
-        <v>147</v>
+        <v>130</v>
+      </c>
+      <c r="E120" t="s">
+        <v>131</v>
+      </c>
+      <c r="F120">
+        <v>1945</v>
+      </c>
+      <c r="G120">
+        <v>2008</v>
+      </c>
+      <c r="I120" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="121" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>233</v>
+        <v>148</v>
       </c>
       <c r="B121" t="s">
-        <v>165</v>
+        <v>128</v>
       </c>
       <c r="C121" s="2" t="s">
-        <v>234</v>
-      </c>
-      <c r="E121" t="s">
-        <v>14</v>
-      </c>
-      <c r="F121">
-        <v>2012</v>
-      </c>
-      <c r="G121">
-        <v>2016</v>
-      </c>
-      <c r="H121" t="s">
-        <v>16</v>
-      </c>
-      <c r="I121" t="s">
-        <v>20</v>
+        <v>147</v>
       </c>
     </row>
     <row r="122" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>35</v>
+        <v>233</v>
       </c>
       <c r="B122" t="s">
-        <v>25</v>
+        <v>165</v>
       </c>
       <c r="C122" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="D122" t="s">
-        <v>37</v>
+        <v>234</v>
       </c>
       <c r="E122" t="s">
         <v>14</v>
       </c>
       <c r="F122">
-        <v>2001</v>
+        <v>2012</v>
+      </c>
+      <c r="G122">
+        <v>2016</v>
       </c>
       <c r="H122" t="s">
         <v>16</v>
@@ -4524,148 +4536,148 @@
     </row>
     <row r="123" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>185</v>
+        <v>35</v>
       </c>
       <c r="B123" t="s">
-        <v>128</v>
+        <v>25</v>
       </c>
       <c r="C123" s="2" t="s">
-        <v>186</v>
+        <v>36</v>
+      </c>
+      <c r="D123" t="s">
+        <v>37</v>
+      </c>
+      <c r="E123" t="s">
+        <v>14</v>
+      </c>
+      <c r="F123">
+        <v>2001</v>
+      </c>
+      <c r="H123" t="s">
+        <v>16</v>
+      </c>
+      <c r="I123" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="124" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>210</v>
+        <v>185</v>
       </c>
       <c r="B124" t="s">
-        <v>40</v>
+        <v>128</v>
       </c>
       <c r="C124" s="2" t="s">
-        <v>211</v>
-      </c>
-      <c r="F124">
-        <v>1976</v>
-      </c>
-      <c r="G124">
-        <v>2016</v>
-      </c>
-      <c r="H124" t="s">
-        <v>16</v>
-      </c>
-      <c r="I124" t="s">
-        <v>20</v>
+        <v>186</v>
       </c>
     </row>
     <row r="125" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>426</v>
+        <v>210</v>
       </c>
       <c r="B125" t="s">
-        <v>86</v>
+        <v>40</v>
       </c>
       <c r="C125" s="2" t="s">
-        <v>427</v>
-      </c>
-      <c r="E125" t="s">
-        <v>34</v>
+        <v>211</v>
       </c>
       <c r="F125">
-        <v>2015</v>
+        <v>1976</v>
       </c>
       <c r="G125">
         <v>2016</v>
       </c>
       <c r="H125" t="s">
-        <v>348</v>
+        <v>16</v>
       </c>
       <c r="I125" t="s">
-        <v>349</v>
-      </c>
-      <c r="K125" s="2" t="s">
-        <v>428</v>
+        <v>20</v>
       </c>
     </row>
     <row r="126" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>144</v>
+        <v>426</v>
       </c>
       <c r="B126" t="s">
-        <v>60</v>
+        <v>86</v>
       </c>
       <c r="C126" s="2" t="s">
-        <v>143</v>
+        <v>427</v>
+      </c>
+      <c r="E126" t="s">
+        <v>34</v>
       </c>
       <c r="F126">
-        <v>1800</v>
+        <v>2015</v>
       </c>
       <c r="G126">
-        <v>2013</v>
+        <v>2016</v>
+      </c>
+      <c r="H126" t="s">
+        <v>348</v>
+      </c>
+      <c r="I126" t="s">
+        <v>349</v>
+      </c>
+      <c r="K126" s="2" t="s">
+        <v>428</v>
       </c>
     </row>
     <row r="127" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>472</v>
+        <v>144</v>
       </c>
       <c r="B127" t="s">
-        <v>25</v>
+        <v>60</v>
       </c>
       <c r="C127" s="2" t="s">
-        <v>473</v>
-      </c>
-      <c r="D127" t="s">
-        <v>474</v>
-      </c>
-      <c r="E127" t="s">
-        <v>112</v>
+        <v>143</v>
       </c>
       <c r="F127">
-        <v>1943</v>
-      </c>
-      <c r="H127" t="s">
-        <v>348</v>
-      </c>
-      <c r="I127" t="s">
-        <v>349</v>
-      </c>
-      <c r="N127" s="2" t="s">
-        <v>475</v>
+        <v>1800</v>
+      </c>
+      <c r="G127">
+        <v>2013</v>
       </c>
     </row>
     <row r="128" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>122</v>
+        <v>472</v>
       </c>
       <c r="B128" t="s">
-        <v>259</v>
+        <v>25</v>
       </c>
       <c r="C128" s="2" t="s">
-        <v>121</v>
+        <v>473</v>
+      </c>
+      <c r="D128" t="s">
+        <v>474</v>
+      </c>
+      <c r="E128" t="s">
+        <v>112</v>
+      </c>
+      <c r="F128">
+        <v>1943</v>
+      </c>
+      <c r="H128" t="s">
+        <v>348</v>
       </c>
       <c r="I128" t="s">
-        <v>20</v>
+        <v>349</v>
+      </c>
+      <c r="N128" s="2" t="s">
+        <v>475</v>
       </c>
     </row>
     <row r="129" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>318</v>
+        <v>122</v>
       </c>
       <c r="B129" t="s">
-        <v>250</v>
+        <v>259</v>
       </c>
       <c r="C129" s="2" t="s">
-        <v>319</v>
-      </c>
-      <c r="E129" t="s">
-        <v>320</v>
-      </c>
-      <c r="F129">
-        <v>1975</v>
-      </c>
-      <c r="G129">
-        <v>1989</v>
-      </c>
-      <c r="H129" t="s">
-        <v>16</v>
+        <v>121</v>
       </c>
       <c r="I129" t="s">
         <v>20</v>
@@ -4673,22 +4685,22 @@
     </row>
     <row r="130" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="B130" t="s">
         <v>250</v>
       </c>
       <c r="C130" s="2" t="s">
-        <v>317</v>
+        <v>319</v>
       </c>
       <c r="E130" t="s">
-        <v>105</v>
+        <v>320</v>
       </c>
       <c r="F130">
-        <v>1950</v>
+        <v>1975</v>
       </c>
       <c r="G130">
-        <v>1996</v>
+        <v>1989</v>
       </c>
       <c r="H130" t="s">
         <v>16</v>
@@ -4699,19 +4711,22 @@
     </row>
     <row r="131" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>322</v>
+        <v>316</v>
       </c>
       <c r="B131" t="s">
-        <v>25</v>
+        <v>250</v>
       </c>
       <c r="C131" s="2" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="E131" t="s">
-        <v>77</v>
+        <v>105</v>
       </c>
       <c r="F131">
-        <v>2010</v>
+        <v>1950</v>
+      </c>
+      <c r="G131">
+        <v>1996</v>
       </c>
       <c r="H131" t="s">
         <v>16</v>
@@ -4722,121 +4737,118 @@
     </row>
     <row r="132" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>141</v>
+        <v>322</v>
       </c>
       <c r="B132" t="s">
-        <v>237</v>
+        <v>25</v>
       </c>
       <c r="C132" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="Q132" t="s">
-        <v>17</v>
+        <v>321</v>
+      </c>
+      <c r="E132" t="s">
+        <v>77</v>
+      </c>
+      <c r="F132">
+        <v>2010</v>
+      </c>
+      <c r="H132" t="s">
+        <v>16</v>
+      </c>
+      <c r="I132" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="133" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
-        <v>308</v>
+        <v>141</v>
       </c>
       <c r="B133" t="s">
-        <v>250</v>
+        <v>237</v>
       </c>
       <c r="C133" s="2" t="s">
-        <v>309</v>
-      </c>
-      <c r="E133" t="s">
-        <v>310</v>
-      </c>
-      <c r="F133">
-        <v>1950</v>
-      </c>
-      <c r="G133">
-        <v>2010</v>
-      </c>
-      <c r="H133" t="s">
-        <v>16</v>
-      </c>
-      <c r="I133" t="s">
-        <v>20</v>
+        <v>142</v>
+      </c>
+      <c r="Q133" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="134" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
-        <v>287</v>
+        <v>308</v>
       </c>
       <c r="B134" t="s">
-        <v>134</v>
+        <v>250</v>
       </c>
       <c r="C134" s="2" t="s">
-        <v>288</v>
+        <v>309</v>
+      </c>
+      <c r="E134" t="s">
+        <v>310</v>
       </c>
       <c r="F134">
-        <v>1990</v>
+        <v>1950</v>
       </c>
       <c r="G134">
-        <v>2008</v>
+        <v>2010</v>
+      </c>
+      <c r="H134" t="s">
+        <v>16</v>
+      </c>
+      <c r="I134" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="135" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
-        <v>274</v>
+        <v>287</v>
       </c>
       <c r="B135" t="s">
-        <v>55</v>
+        <v>134</v>
       </c>
       <c r="C135" s="2" t="s">
-        <v>275</v>
-      </c>
-      <c r="H135" t="s">
-        <v>16</v>
-      </c>
-      <c r="I135" t="s">
-        <v>20</v>
+        <v>288</v>
+      </c>
+      <c r="F135">
+        <v>1990</v>
+      </c>
+      <c r="G135">
+        <v>2008</v>
       </c>
     </row>
     <row r="136" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
-        <v>157</v>
+        <v>274</v>
       </c>
       <c r="B136" t="s">
-        <v>128</v>
+        <v>55</v>
       </c>
       <c r="C136" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="Q136" t="s">
-        <v>18</v>
+        <v>275</v>
+      </c>
+      <c r="H136" t="s">
+        <v>16</v>
+      </c>
+      <c r="I136" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="137" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
-        <v>439</v>
+        <v>157</v>
       </c>
       <c r="B137" t="s">
-        <v>259</v>
+        <v>128</v>
       </c>
       <c r="C137" s="2" t="s">
-        <v>438</v>
-      </c>
-      <c r="H137" t="s">
-        <v>348</v>
-      </c>
-      <c r="I137" t="s">
-        <v>349</v>
-      </c>
-      <c r="J137" s="2" t="s">
-        <v>440</v>
-      </c>
-      <c r="K137" s="2" t="s">
-        <v>442</v>
-      </c>
-      <c r="L137" s="2" t="s">
-        <v>441</v>
+        <v>154</v>
+      </c>
+      <c r="Q137" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="138" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
-        <v>443</v>
+        <v>439</v>
       </c>
       <c r="B138" t="s">
         <v>259</v>
@@ -4844,15 +4856,6 @@
       <c r="C138" s="2" t="s">
         <v>438</v>
       </c>
-      <c r="D138" t="s">
-        <v>447</v>
-      </c>
-      <c r="F138">
-        <v>1990</v>
-      </c>
-      <c r="G138">
-        <v>2014</v>
-      </c>
       <c r="H138" t="s">
         <v>348</v>
       </c>
@@ -4860,87 +4863,99 @@
         <v>349</v>
       </c>
       <c r="J138" s="2" t="s">
-        <v>444</v>
+        <v>440</v>
       </c>
       <c r="K138" s="2" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
       <c r="L138" s="2" t="s">
-        <v>446</v>
+        <v>441</v>
       </c>
     </row>
     <row r="139" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
-        <v>194</v>
+        <v>443</v>
       </c>
       <c r="B139" t="s">
-        <v>99</v>
+        <v>259</v>
       </c>
       <c r="C139" s="2" t="s">
-        <v>193</v>
+        <v>438</v>
+      </c>
+      <c r="D139" t="s">
+        <v>447</v>
+      </c>
+      <c r="F139">
+        <v>1990</v>
+      </c>
+      <c r="G139">
+        <v>2014</v>
+      </c>
+      <c r="H139" t="s">
+        <v>348</v>
+      </c>
+      <c r="I139" t="s">
+        <v>349</v>
+      </c>
+      <c r="J139" s="2" t="s">
+        <v>444</v>
+      </c>
+      <c r="K139" s="2" t="s">
+        <v>445</v>
+      </c>
+      <c r="L139" s="2" t="s">
+        <v>446</v>
       </c>
     </row>
     <row r="140" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
-        <v>295</v>
+        <v>194</v>
       </c>
       <c r="B140" t="s">
-        <v>40</v>
+        <v>99</v>
       </c>
       <c r="C140" s="2" t="s">
-        <v>296</v>
-      </c>
-      <c r="E140" t="s">
-        <v>297</v>
-      </c>
-      <c r="F140">
-        <v>1990</v>
-      </c>
-      <c r="G140">
-        <v>2015</v>
-      </c>
-      <c r="H140" t="s">
-        <v>16</v>
-      </c>
-      <c r="I140" t="s">
-        <v>249</v>
+        <v>193</v>
       </c>
     </row>
     <row r="141" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
-        <v>256</v>
+        <v>295</v>
       </c>
       <c r="B141" t="s">
-        <v>250</v>
+        <v>40</v>
       </c>
       <c r="C141" s="2" t="s">
-        <v>257</v>
+        <v>296</v>
       </c>
       <c r="E141" t="s">
-        <v>258</v>
+        <v>297</v>
+      </c>
+      <c r="F141">
+        <v>1990</v>
+      </c>
+      <c r="G141">
+        <v>2015</v>
       </c>
       <c r="H141" t="s">
         <v>16</v>
       </c>
       <c r="I141" t="s">
-        <v>20</v>
+        <v>249</v>
       </c>
     </row>
     <row r="142" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
-        <v>227</v>
+        <v>256</v>
       </c>
       <c r="B142" t="s">
-        <v>40</v>
+        <v>250</v>
       </c>
       <c r="C142" s="2" t="s">
-        <v>225</v>
-      </c>
-      <c r="F142">
-        <v>1955</v>
-      </c>
-      <c r="G142">
-        <v>2016</v>
+        <v>257</v>
+      </c>
+      <c r="E142" t="s">
+        <v>258</v>
       </c>
       <c r="H142" t="s">
         <v>16</v>
@@ -4951,7 +4966,7 @@
     </row>
     <row r="143" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="B143" t="s">
         <v>40</v>
@@ -4960,7 +4975,7 @@
         <v>225</v>
       </c>
       <c r="F143">
-        <v>1995</v>
+        <v>1955</v>
       </c>
       <c r="G143">
         <v>2016</v>
@@ -4974,248 +4989,248 @@
     </row>
     <row r="144" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
-        <v>452</v>
+        <v>230</v>
       </c>
       <c r="B144" t="s">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="C144" s="2" t="s">
-        <v>453</v>
-      </c>
-      <c r="E144" t="s">
-        <v>9</v>
+        <v>225</v>
+      </c>
+      <c r="F144">
+        <v>1995</v>
+      </c>
+      <c r="G144">
+        <v>2016</v>
       </c>
       <c r="H144" t="s">
-        <v>348</v>
+        <v>16</v>
       </c>
       <c r="I144" t="s">
-        <v>435</v>
+        <v>20</v>
       </c>
     </row>
     <row r="145" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
-        <v>109</v>
+        <v>452</v>
       </c>
       <c r="B145" t="s">
         <v>25</v>
       </c>
       <c r="C145" s="2" t="s">
-        <v>110</v>
+        <v>453</v>
       </c>
       <c r="E145" t="s">
-        <v>111</v>
-      </c>
-      <c r="F145">
-        <v>1956</v>
+        <v>9</v>
+      </c>
+      <c r="H145" t="s">
+        <v>348</v>
+      </c>
+      <c r="I145" t="s">
+        <v>435</v>
       </c>
     </row>
     <row r="146" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
-        <v>326</v>
+        <v>109</v>
       </c>
       <c r="B146" t="s">
         <v>25</v>
       </c>
       <c r="C146" s="2" t="s">
-        <v>327</v>
+        <v>110</v>
       </c>
       <c r="E146" t="s">
         <v>111</v>
       </c>
       <c r="F146">
-        <v>1998</v>
-      </c>
-      <c r="H146" t="s">
-        <v>16</v>
-      </c>
-      <c r="I146" t="s">
-        <v>20</v>
+        <v>1956</v>
       </c>
     </row>
     <row r="147" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
-        <v>91</v>
+        <v>326</v>
       </c>
       <c r="B147" t="s">
         <v>25</v>
       </c>
       <c r="C147" s="2" t="s">
-        <v>93</v>
+        <v>327</v>
       </c>
       <c r="E147" t="s">
-        <v>92</v>
+        <v>111</v>
       </c>
       <c r="F147">
-        <v>1999</v>
+        <v>1998</v>
+      </c>
+      <c r="H147" t="s">
+        <v>16</v>
+      </c>
+      <c r="I147" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="148" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
-        <v>314</v>
+        <v>91</v>
       </c>
       <c r="B148" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="C148" s="2" t="s">
-        <v>313</v>
+        <v>93</v>
       </c>
       <c r="E148" t="s">
-        <v>315</v>
+        <v>92</v>
       </c>
       <c r="F148">
-        <v>1950</v>
-      </c>
-      <c r="G148">
-        <v>2004</v>
-      </c>
-      <c r="H148" t="s">
-        <v>16</v>
-      </c>
-      <c r="I148" t="s">
-        <v>20</v>
+        <v>1999</v>
       </c>
     </row>
     <row r="149" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
-        <v>161</v>
+        <v>314</v>
       </c>
       <c r="B149" t="s">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="C149" s="2" t="s">
-        <v>160</v>
+        <v>313</v>
+      </c>
+      <c r="E149" t="s">
+        <v>315</v>
+      </c>
+      <c r="F149">
+        <v>1950</v>
+      </c>
+      <c r="G149">
+        <v>2004</v>
+      </c>
+      <c r="H149" t="s">
+        <v>16</v>
+      </c>
+      <c r="I149" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="150" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="B150" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="C150" s="2" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
     </row>
     <row r="151" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
-        <v>399</v>
+        <v>168</v>
       </c>
       <c r="B151" t="s">
         <v>40</v>
       </c>
       <c r="C151" s="2" t="s">
-        <v>400</v>
-      </c>
-      <c r="E151" t="s">
-        <v>14</v>
-      </c>
-      <c r="F151">
-        <v>2000</v>
-      </c>
-      <c r="G151">
-        <v>2014</v>
-      </c>
-      <c r="H151" t="s">
-        <v>348</v>
-      </c>
-      <c r="I151" t="s">
-        <v>349</v>
-      </c>
-      <c r="J151" s="2" t="s">
-        <v>402</v>
-      </c>
-      <c r="N151" s="2" t="s">
-        <v>401</v>
+        <v>167</v>
       </c>
     </row>
     <row r="152" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
-        <v>213</v>
+        <v>399</v>
       </c>
       <c r="B152" t="s">
-        <v>55</v>
+        <v>40</v>
       </c>
       <c r="C152" s="2" t="s">
-        <v>212</v>
+        <v>400</v>
+      </c>
+      <c r="E152" t="s">
+        <v>14</v>
+      </c>
+      <c r="F152">
+        <v>2000</v>
+      </c>
+      <c r="G152">
+        <v>2014</v>
       </c>
       <c r="H152" t="s">
-        <v>16</v>
+        <v>348</v>
       </c>
       <c r="I152" t="s">
-        <v>20</v>
+        <v>349</v>
+      </c>
+      <c r="J152" s="2" t="s">
+        <v>402</v>
+      </c>
+      <c r="N152" s="2" t="s">
+        <v>401</v>
       </c>
     </row>
     <row r="153" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
-        <v>395</v>
+        <v>213</v>
       </c>
       <c r="B153" t="s">
-        <v>25</v>
+        <v>55</v>
       </c>
       <c r="C153" s="2" t="s">
-        <v>394</v>
-      </c>
-      <c r="D153" t="s">
-        <v>396</v>
-      </c>
-      <c r="E153" t="s">
-        <v>111</v>
-      </c>
-      <c r="F153">
-        <v>1986</v>
-      </c>
-      <c r="G153">
-        <v>2015</v>
+        <v>212</v>
       </c>
       <c r="H153" t="s">
-        <v>367</v>
+        <v>16</v>
       </c>
       <c r="I153" t="s">
-        <v>398</v>
-      </c>
-      <c r="J153" s="2" t="s">
-        <v>397</v>
+        <v>20</v>
       </c>
     </row>
     <row r="154" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
-        <v>323</v>
+        <v>395</v>
       </c>
       <c r="B154" t="s">
         <v>25</v>
       </c>
       <c r="C154" s="2" t="s">
-        <v>324</v>
+        <v>394</v>
+      </c>
+      <c r="D154" t="s">
+        <v>396</v>
       </c>
       <c r="E154" t="s">
-        <v>325</v>
+        <v>111</v>
       </c>
       <c r="F154">
-        <v>1942</v>
+        <v>1986</v>
+      </c>
+      <c r="G154">
+        <v>2015</v>
       </c>
       <c r="H154" t="s">
-        <v>16</v>
+        <v>367</v>
       </c>
       <c r="I154" t="s">
-        <v>20</v>
+        <v>398</v>
+      </c>
+      <c r="J154" s="2" t="s">
+        <v>397</v>
       </c>
     </row>
     <row r="155" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
-        <v>273</v>
+        <v>323</v>
       </c>
       <c r="B155" t="s">
-        <v>237</v>
+        <v>25</v>
       </c>
       <c r="C155" s="2" t="s">
-        <v>272</v>
+        <v>324</v>
+      </c>
+      <c r="E155" t="s">
+        <v>325</v>
       </c>
       <c r="F155">
-        <v>1996</v>
-      </c>
-      <c r="G155">
-        <v>2016</v>
+        <v>1942</v>
       </c>
       <c r="H155" t="s">
         <v>16</v>
@@ -5226,91 +5241,91 @@
     </row>
     <row r="156" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
-        <v>508</v>
+        <v>273</v>
       </c>
       <c r="B156" t="s">
-        <v>40</v>
+        <v>237</v>
       </c>
       <c r="C156" s="2" t="s">
-        <v>509</v>
-      </c>
-      <c r="D156" t="s">
-        <v>511</v>
-      </c>
-      <c r="E156" t="s">
-        <v>510</v>
+        <v>272</v>
       </c>
       <c r="F156">
-        <v>1989</v>
+        <v>1996</v>
       </c>
       <c r="G156">
-        <v>2009</v>
+        <v>2016</v>
       </c>
       <c r="H156" t="s">
-        <v>348</v>
+        <v>16</v>
       </c>
       <c r="I156" t="s">
-        <v>349</v>
-      </c>
-      <c r="P156" s="2" t="s">
-        <v>512</v>
+        <v>20</v>
       </c>
     </row>
     <row r="157" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
-        <v>66</v>
+        <v>508</v>
       </c>
       <c r="B157" t="s">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="C157" s="2" t="s">
-        <v>67</v>
+        <v>509</v>
+      </c>
+      <c r="D157" t="s">
+        <v>511</v>
+      </c>
+      <c r="E157" t="s">
+        <v>510</v>
+      </c>
+      <c r="F157">
+        <v>1989</v>
+      </c>
+      <c r="G157">
+        <v>2009</v>
+      </c>
+      <c r="H157" t="s">
+        <v>348</v>
+      </c>
+      <c r="I157" t="s">
+        <v>349</v>
+      </c>
+      <c r="P157" s="2" t="s">
+        <v>512</v>
       </c>
     </row>
     <row r="158" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
-        <v>500</v>
+        <v>66</v>
       </c>
       <c r="B158" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="C158" s="2" t="s">
-        <v>499</v>
-      </c>
-      <c r="D158" t="s">
-        <v>501</v>
-      </c>
-      <c r="E158" t="s">
-        <v>14</v>
-      </c>
-      <c r="F158">
-        <v>1946</v>
-      </c>
-      <c r="G158">
-        <v>2015</v>
-      </c>
-      <c r="H158" t="s">
-        <v>348</v>
-      </c>
-      <c r="I158" t="s">
-        <v>349</v>
+        <v>67</v>
       </c>
     </row>
     <row r="159" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
-        <v>383</v>
+        <v>500</v>
       </c>
       <c r="B159" t="s">
         <v>40</v>
       </c>
       <c r="C159" s="2" t="s">
-        <v>384</v>
+        <v>499</v>
+      </c>
+      <c r="D159" t="s">
+        <v>501</v>
       </c>
       <c r="E159" t="s">
-        <v>386</v>
+        <v>14</v>
       </c>
       <c r="F159">
-        <v>1951</v>
+        <v>1946</v>
+      </c>
+      <c r="G159">
+        <v>2015</v>
       </c>
       <c r="H159" t="s">
         <v>348</v>
@@ -5318,178 +5333,181 @@
       <c r="I159" t="s">
         <v>349</v>
       </c>
-      <c r="N159" s="2" t="s">
-        <v>385</v>
-      </c>
     </row>
     <row r="160" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
-        <v>139</v>
+        <v>383</v>
       </c>
       <c r="B160" t="s">
         <v>40</v>
       </c>
       <c r="C160" s="2" t="s">
-        <v>140</v>
+        <v>384</v>
+      </c>
+      <c r="E160" t="s">
+        <v>386</v>
+      </c>
+      <c r="F160">
+        <v>1951</v>
+      </c>
+      <c r="H160" t="s">
+        <v>348</v>
+      </c>
+      <c r="I160" t="s">
+        <v>349</v>
+      </c>
+      <c r="N160" s="2" t="s">
+        <v>385</v>
       </c>
     </row>
     <row r="161" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
-        <v>329</v>
+        <v>139</v>
       </c>
       <c r="B161" t="s">
-        <v>165</v>
+        <v>40</v>
       </c>
       <c r="C161" s="2" t="s">
-        <v>328</v>
-      </c>
-      <c r="E161" t="s">
-        <v>34</v>
-      </c>
-      <c r="F161">
-        <v>1789</v>
-      </c>
-      <c r="H161" t="s">
-        <v>16</v>
-      </c>
-      <c r="I161" t="s">
-        <v>20</v>
+        <v>140</v>
       </c>
     </row>
     <row r="162" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
-        <v>172</v>
+        <v>329</v>
       </c>
       <c r="B162" t="s">
-        <v>60</v>
+        <v>165</v>
       </c>
       <c r="C162" s="2" t="s">
-        <v>171</v>
+        <v>328</v>
+      </c>
+      <c r="E162" t="s">
+        <v>34</v>
+      </c>
+      <c r="F162">
+        <v>1789</v>
+      </c>
+      <c r="H162" t="s">
+        <v>16</v>
+      </c>
+      <c r="I162" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="163" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
-        <v>217</v>
+        <v>172</v>
       </c>
       <c r="B163" t="s">
         <v>60</v>
       </c>
       <c r="C163" s="2" t="s">
-        <v>216</v>
-      </c>
-      <c r="E163" t="s">
-        <v>14</v>
-      </c>
-      <c r="F163">
-        <v>1900</v>
-      </c>
-      <c r="H163" t="s">
-        <v>16</v>
-      </c>
-      <c r="I163" t="s">
-        <v>20</v>
+        <v>171</v>
       </c>
     </row>
     <row r="164" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
-        <v>132</v>
+        <v>217</v>
       </c>
       <c r="B164" t="s">
-        <v>259</v>
+        <v>60</v>
       </c>
       <c r="C164" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="Q164" t="s">
-        <v>17</v>
+        <v>216</v>
+      </c>
+      <c r="E164" t="s">
+        <v>14</v>
+      </c>
+      <c r="F164">
+        <v>1900</v>
+      </c>
+      <c r="H164" t="s">
+        <v>16</v>
+      </c>
+      <c r="I164" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="165" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
-        <v>182</v>
+        <v>132</v>
       </c>
       <c r="B165" t="s">
-        <v>165</v>
+        <v>259</v>
       </c>
       <c r="C165" s="2" t="s">
-        <v>181</v>
+        <v>133</v>
+      </c>
+      <c r="Q165" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="166" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
-        <v>423</v>
+        <v>182</v>
       </c>
       <c r="B166" t="s">
-        <v>86</v>
+        <v>165</v>
       </c>
       <c r="C166" s="2" t="s">
-        <v>424</v>
-      </c>
-      <c r="E166" t="s">
-        <v>34</v>
-      </c>
-      <c r="F166">
-        <v>1996</v>
-      </c>
-      <c r="G166">
-        <v>2016</v>
-      </c>
-      <c r="H166" t="s">
-        <v>348</v>
-      </c>
-      <c r="I166" t="s">
-        <v>425</v>
+        <v>181</v>
       </c>
     </row>
     <row r="167" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
-        <v>115</v>
+        <v>423</v>
       </c>
       <c r="B167" t="s">
-        <v>128</v>
+        <v>86</v>
       </c>
       <c r="C167" s="2" t="s">
-        <v>116</v>
+        <v>424</v>
+      </c>
+      <c r="E167" t="s">
+        <v>34</v>
+      </c>
+      <c r="F167">
+        <v>1996</v>
+      </c>
+      <c r="G167">
+        <v>2016</v>
+      </c>
+      <c r="H167" t="s">
+        <v>348</v>
+      </c>
+      <c r="I167" t="s">
+        <v>425</v>
       </c>
     </row>
     <row r="168" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
-        <v>263</v>
+        <v>115</v>
       </c>
       <c r="B168" t="s">
-        <v>250</v>
+        <v>128</v>
       </c>
       <c r="C168" s="2" t="s">
-        <v>264</v>
-      </c>
-      <c r="E168" t="s">
-        <v>265</v>
-      </c>
-      <c r="F168">
-        <v>1500</v>
-      </c>
-      <c r="G168">
-        <v>2000</v>
-      </c>
-      <c r="H168" t="s">
-        <v>16</v>
-      </c>
-      <c r="I168" t="s">
-        <v>20</v>
+        <v>116</v>
       </c>
     </row>
     <row r="169" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
-        <v>221</v>
+        <v>263</v>
       </c>
       <c r="B169" t="s">
-        <v>86</v>
+        <v>250</v>
       </c>
       <c r="C169" s="2" t="s">
-        <v>220</v>
+        <v>264</v>
+      </c>
+      <c r="E169" t="s">
+        <v>265</v>
       </c>
       <c r="F169">
-        <v>2013</v>
+        <v>1500</v>
+      </c>
+      <c r="G169">
+        <v>2000</v>
       </c>
       <c r="H169" t="s">
         <v>16</v>
@@ -5500,22 +5518,16 @@
     </row>
     <row r="170" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
-        <v>13</v>
+        <v>221</v>
       </c>
       <c r="B170" t="s">
-        <v>25</v>
+        <v>86</v>
       </c>
       <c r="C170" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="D170" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="E170" t="s">
-        <v>14</v>
+        <v>220</v>
       </c>
       <c r="F170">
-        <v>1981</v>
+        <v>2013</v>
       </c>
       <c r="H170" t="s">
         <v>16</v>
@@ -5526,23 +5538,49 @@
     </row>
     <row r="171" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
+        <v>13</v>
+      </c>
+      <c r="B171" t="s">
+        <v>25</v>
+      </c>
+      <c r="C171" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D171" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E171" t="s">
+        <v>14</v>
+      </c>
+      <c r="F171">
+        <v>1981</v>
+      </c>
+      <c r="H171" t="s">
+        <v>16</v>
+      </c>
+      <c r="I171" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="172" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A172" t="s">
         <v>283</v>
       </c>
-      <c r="B171" t="s">
+      <c r="B172" t="s">
         <v>124</v>
       </c>
-      <c r="C171" s="2" t="s">
+      <c r="C172" s="2" t="s">
         <v>284</v>
       </c>
-      <c r="H171" t="s">
-        <v>16</v>
-      </c>
-      <c r="I171" t="s">
+      <c r="H172" t="s">
+        <v>16</v>
+      </c>
+      <c r="I172" t="s">
         <v>20</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:Q171">
+  <sortState ref="A2:Q172">
     <sortCondition ref="A2"/>
   </sortState>
   <hyperlinks>
@@ -5551,8 +5589,8 @@
     <hyperlink ref="C7" r:id="rId3"/>
     <hyperlink ref="C11" r:id="rId4"/>
     <hyperlink ref="C102" r:id="rId5"/>
-    <hyperlink ref="C122" r:id="rId6"/>
-    <hyperlink ref="C170" r:id="rId7"/>
+    <hyperlink ref="C123" r:id="rId6"/>
+    <hyperlink ref="C171" r:id="rId7"/>
     <hyperlink ref="C38" r:id="rId8"/>
     <hyperlink ref="C32" r:id="rId9"/>
     <hyperlink ref="C55" r:id="rId10"/>
@@ -5562,11 +5600,11 @@
     <hyperlink ref="C66" r:id="rId14"/>
     <hyperlink ref="C94" r:id="rId15"/>
     <hyperlink ref="C31" r:id="rId16"/>
-    <hyperlink ref="C118" r:id="rId17"/>
+    <hyperlink ref="C119" r:id="rId17"/>
     <hyperlink ref="C46" r:id="rId18"/>
     <hyperlink ref="C79" r:id="rId19"/>
     <hyperlink ref="C17" r:id="rId20"/>
-    <hyperlink ref="C157" r:id="rId21"/>
+    <hyperlink ref="C158" r:id="rId21"/>
     <hyperlink ref="C8" r:id="rId22"/>
     <hyperlink ref="C42" r:id="rId23"/>
     <hyperlink ref="C59" r:id="rId24"/>
@@ -5575,75 +5613,75 @@
     <hyperlink ref="C61" r:id="rId27"/>
     <hyperlink ref="C76" r:id="rId28"/>
     <hyperlink ref="C99" r:id="rId29"/>
-    <hyperlink ref="C147" r:id="rId30"/>
+    <hyperlink ref="C148" r:id="rId30"/>
     <hyperlink ref="C105" r:id="rId31"/>
     <hyperlink ref="C89" r:id="rId32"/>
-    <hyperlink ref="C111" r:id="rId33"/>
+    <hyperlink ref="C112" r:id="rId33"/>
     <hyperlink ref="C77" r:id="rId34"/>
     <hyperlink ref="C18" r:id="rId35"/>
-    <hyperlink ref="C145" r:id="rId36"/>
+    <hyperlink ref="C146" r:id="rId36"/>
     <hyperlink ref="C16" r:id="rId37"/>
-    <hyperlink ref="C167" r:id="rId38"/>
+    <hyperlink ref="C168" r:id="rId38"/>
     <hyperlink ref="C93" r:id="rId39"/>
     <hyperlink ref="C63" r:id="rId40"/>
-    <hyperlink ref="C128" r:id="rId41"/>
+    <hyperlink ref="C129" r:id="rId41"/>
     <hyperlink ref="C19" r:id="rId42"/>
     <hyperlink ref="C57" r:id="rId43"/>
     <hyperlink ref="C25" r:id="rId44"/>
-    <hyperlink ref="C119" r:id="rId45"/>
-    <hyperlink ref="C164" r:id="rId46"/>
+    <hyperlink ref="C120" r:id="rId45"/>
+    <hyperlink ref="C165" r:id="rId46"/>
     <hyperlink ref="C29" r:id="rId47" display="http://comparativeconstitutionsproject.org/"/>
-    <hyperlink ref="C116" r:id="rId48"/>
-    <hyperlink ref="C160" r:id="rId49"/>
-    <hyperlink ref="C132" r:id="rId50"/>
-    <hyperlink ref="C126" r:id="rId51"/>
+    <hyperlink ref="C117" r:id="rId48"/>
+    <hyperlink ref="C161" r:id="rId49"/>
+    <hyperlink ref="C133" r:id="rId50"/>
+    <hyperlink ref="C127" r:id="rId51"/>
     <hyperlink ref="C24" r:id="rId52"/>
-    <hyperlink ref="C120" r:id="rId53"/>
+    <hyperlink ref="C121" r:id="rId53"/>
     <hyperlink ref="C53" r:id="rId54"/>
     <hyperlink ref="C83" r:id="rId55"/>
     <hyperlink ref="C86" r:id="rId56"/>
-    <hyperlink ref="C117" r:id="rId57"/>
+    <hyperlink ref="C118" r:id="rId57"/>
     <hyperlink ref="C107" r:id="rId58"/>
-    <hyperlink ref="C136" r:id="rId59"/>
+    <hyperlink ref="C137" r:id="rId59"/>
     <hyperlink ref="C33" r:id="rId60"/>
-    <hyperlink ref="C149" r:id="rId61"/>
+    <hyperlink ref="C150" r:id="rId61"/>
     <hyperlink ref="C9" r:id="rId62"/>
     <hyperlink ref="C35" r:id="rId63"/>
-    <hyperlink ref="C150" r:id="rId64"/>
+    <hyperlink ref="C151" r:id="rId64"/>
     <hyperlink ref="C15" r:id="rId65"/>
-    <hyperlink ref="C162" r:id="rId66"/>
+    <hyperlink ref="C163" r:id="rId66"/>
     <hyperlink ref="C27" r:id="rId67"/>
     <hyperlink ref="C26" r:id="rId68"/>
     <hyperlink ref="C28" r:id="rId69"/>
     <hyperlink ref="C58" r:id="rId70"/>
-    <hyperlink ref="C165" r:id="rId71"/>
+    <hyperlink ref="C166" r:id="rId71"/>
     <hyperlink ref="C30" r:id="rId72"/>
-    <hyperlink ref="C123" r:id="rId73"/>
+    <hyperlink ref="C124" r:id="rId73"/>
     <hyperlink ref="C34" r:id="rId74"/>
     <hyperlink ref="C50" r:id="rId75"/>
-    <hyperlink ref="C139" r:id="rId76"/>
+    <hyperlink ref="C140" r:id="rId76"/>
     <hyperlink ref="C47" r:id="rId77"/>
     <hyperlink ref="C43" r:id="rId78"/>
     <hyperlink ref="C74" r:id="rId79"/>
     <hyperlink ref="C5" r:id="rId80"/>
     <hyperlink ref="C73" r:id="rId81"/>
     <hyperlink ref="C13" r:id="rId82"/>
-    <hyperlink ref="C115" r:id="rId83"/>
-    <hyperlink ref="C124" r:id="rId84"/>
-    <hyperlink ref="C152" r:id="rId85"/>
+    <hyperlink ref="C116" r:id="rId83"/>
+    <hyperlink ref="C125" r:id="rId84"/>
+    <hyperlink ref="C153" r:id="rId85"/>
     <hyperlink ref="C39" r:id="rId86"/>
-    <hyperlink ref="C163" r:id="rId87"/>
+    <hyperlink ref="C164" r:id="rId87"/>
     <hyperlink ref="C49" r:id="rId88"/>
-    <hyperlink ref="C169" r:id="rId89"/>
+    <hyperlink ref="C170" r:id="rId89"/>
     <hyperlink ref="C103" r:id="rId90"/>
     <hyperlink ref="C71" r:id="rId91"/>
     <hyperlink ref="C104" r:id="rId92"/>
-    <hyperlink ref="C142" r:id="rId93"/>
+    <hyperlink ref="C143" r:id="rId93"/>
     <hyperlink ref="C87" r:id="rId94"/>
     <hyperlink ref="C109" r:id="rId95"/>
-    <hyperlink ref="C143" r:id="rId96"/>
+    <hyperlink ref="C144" r:id="rId96"/>
     <hyperlink ref="C67" r:id="rId97"/>
-    <hyperlink ref="C121" r:id="rId98"/>
+    <hyperlink ref="C122" r:id="rId98"/>
     <hyperlink ref="C51" r:id="rId99"/>
     <hyperlink ref="C48" r:id="rId100"/>
     <hyperlink ref="C90" r:id="rId101"/>
@@ -5651,39 +5689,39 @@
     <hyperlink ref="C2" r:id="rId103"/>
     <hyperlink ref="C84" r:id="rId104"/>
     <hyperlink ref="C88" r:id="rId105"/>
-    <hyperlink ref="C113" r:id="rId106"/>
+    <hyperlink ref="C114" r:id="rId106"/>
     <hyperlink ref="C52" r:id="rId107"/>
     <hyperlink ref="C91" r:id="rId108"/>
-    <hyperlink ref="C141" r:id="rId109"/>
+    <hyperlink ref="C142" r:id="rId109"/>
     <hyperlink ref="C14" r:id="rId110"/>
     <hyperlink ref="C4" r:id="rId111"/>
-    <hyperlink ref="C168" r:id="rId112"/>
+    <hyperlink ref="C169" r:id="rId112"/>
     <hyperlink ref="C97" r:id="rId113"/>
     <hyperlink ref="C92" r:id="rId114"/>
-    <hyperlink ref="C155" r:id="rId115"/>
-    <hyperlink ref="C135" r:id="rId116"/>
+    <hyperlink ref="C156" r:id="rId115"/>
+    <hyperlink ref="C136" r:id="rId116"/>
     <hyperlink ref="C69" r:id="rId117"/>
     <hyperlink ref="C106" r:id="rId118"/>
     <hyperlink ref="C81" r:id="rId119"/>
-    <hyperlink ref="C171" r:id="rId120"/>
+    <hyperlink ref="C172" r:id="rId120"/>
     <hyperlink ref="C72" r:id="rId121"/>
-    <hyperlink ref="C134" r:id="rId122"/>
-    <hyperlink ref="C112" r:id="rId123"/>
+    <hyperlink ref="C135" r:id="rId122"/>
+    <hyperlink ref="C113" r:id="rId123"/>
     <hyperlink ref="C85" r:id="rId124"/>
-    <hyperlink ref="C110" r:id="rId125"/>
-    <hyperlink ref="C140" r:id="rId126"/>
+    <hyperlink ref="C111" r:id="rId125"/>
+    <hyperlink ref="C141" r:id="rId126"/>
     <hyperlink ref="C95" r:id="rId127"/>
     <hyperlink ref="C12" r:id="rId128"/>
     <hyperlink ref="C20" r:id="rId129"/>
-    <hyperlink ref="C133" r:id="rId130"/>
+    <hyperlink ref="C134" r:id="rId130"/>
     <hyperlink ref="C80" r:id="rId131"/>
-    <hyperlink ref="C148" r:id="rId132"/>
-    <hyperlink ref="C130" r:id="rId133"/>
-    <hyperlink ref="C129" r:id="rId134"/>
-    <hyperlink ref="C131" r:id="rId135"/>
-    <hyperlink ref="C154" r:id="rId136"/>
-    <hyperlink ref="C146" r:id="rId137"/>
-    <hyperlink ref="C161" r:id="rId138"/>
+    <hyperlink ref="C149" r:id="rId132"/>
+    <hyperlink ref="C131" r:id="rId133"/>
+    <hyperlink ref="C130" r:id="rId134"/>
+    <hyperlink ref="C132" r:id="rId135"/>
+    <hyperlink ref="C155" r:id="rId136"/>
+    <hyperlink ref="C147" r:id="rId137"/>
+    <hyperlink ref="C162" r:id="rId138"/>
     <hyperlink ref="C41" r:id="rId139"/>
     <hyperlink ref="C96" r:id="rId140"/>
     <hyperlink ref="J2" r:id="rId141"/>
@@ -5693,23 +5731,23 @@
     <hyperlink ref="J4" r:id="rId145"/>
     <hyperlink ref="P5" r:id="rId146"/>
     <hyperlink ref="J5" r:id="rId147"/>
-    <hyperlink ref="C114" r:id="rId148"/>
+    <hyperlink ref="C115" r:id="rId148"/>
     <hyperlink ref="C36" r:id="rId149"/>
     <hyperlink ref="P7" r:id="rId150"/>
     <hyperlink ref="J7" r:id="rId151"/>
     <hyperlink ref="M8" r:id="rId152"/>
     <hyperlink ref="L8" r:id="rId153"/>
     <hyperlink ref="J8" r:id="rId154"/>
-    <hyperlink ref="C159" r:id="rId155"/>
-    <hyperlink ref="N159" r:id="rId156"/>
+    <hyperlink ref="C160" r:id="rId155"/>
+    <hyperlink ref="N160" r:id="rId156"/>
     <hyperlink ref="C22" r:id="rId157"/>
     <hyperlink ref="N22" r:id="rId158"/>
     <hyperlink ref="C68" r:id="rId159"/>
-    <hyperlink ref="C153" r:id="rId160"/>
-    <hyperlink ref="J153" r:id="rId161"/>
-    <hyperlink ref="C151" r:id="rId162"/>
-    <hyperlink ref="N151" r:id="rId163"/>
-    <hyperlink ref="J151" r:id="rId164"/>
+    <hyperlink ref="C154" r:id="rId160"/>
+    <hyperlink ref="J154" r:id="rId161"/>
+    <hyperlink ref="C152" r:id="rId162"/>
+    <hyperlink ref="N152" r:id="rId163"/>
+    <hyperlink ref="J152" r:id="rId164"/>
     <hyperlink ref="C100" r:id="rId165"/>
     <hyperlink ref="C98" r:id="rId166"/>
     <hyperlink ref="C44" r:id="rId167"/>
@@ -5719,24 +5757,24 @@
     <hyperlink ref="N108" r:id="rId171"/>
     <hyperlink ref="C82" r:id="rId172"/>
     <hyperlink ref="K82" r:id="rId173"/>
-    <hyperlink ref="C166" r:id="rId174"/>
-    <hyperlink ref="C125" r:id="rId175"/>
-    <hyperlink ref="K125" r:id="rId176"/>
+    <hyperlink ref="C167" r:id="rId174"/>
+    <hyperlink ref="C126" r:id="rId175"/>
+    <hyperlink ref="K126" r:id="rId176"/>
     <hyperlink ref="L9" r:id="rId177"/>
     <hyperlink ref="J9" r:id="rId178"/>
     <hyperlink ref="J11" r:id="rId179"/>
-    <hyperlink ref="C137" r:id="rId180"/>
-    <hyperlink ref="J137" r:id="rId181"/>
-    <hyperlink ref="L137" r:id="rId182"/>
-    <hyperlink ref="K137" r:id="rId183"/>
-    <hyperlink ref="C138" r:id="rId184"/>
-    <hyperlink ref="J138" r:id="rId185"/>
-    <hyperlink ref="K138" r:id="rId186"/>
-    <hyperlink ref="L138" r:id="rId187"/>
+    <hyperlink ref="C138" r:id="rId180"/>
+    <hyperlink ref="J138" r:id="rId181"/>
+    <hyperlink ref="L138" r:id="rId182"/>
+    <hyperlink ref="K138" r:id="rId183"/>
+    <hyperlink ref="C139" r:id="rId184"/>
+    <hyperlink ref="J139" r:id="rId185"/>
+    <hyperlink ref="K139" r:id="rId186"/>
+    <hyperlink ref="L139" r:id="rId187"/>
     <hyperlink ref="C70" r:id="rId188"/>
     <hyperlink ref="J70" r:id="rId189"/>
     <hyperlink ref="N70" r:id="rId190"/>
-    <hyperlink ref="C144" r:id="rId191"/>
+    <hyperlink ref="C145" r:id="rId191"/>
     <hyperlink ref="C101" r:id="rId192"/>
     <hyperlink ref="J101" r:id="rId193"/>
     <hyperlink ref="L101" r:id="rId194"/>
@@ -5749,8 +5787,8 @@
     <hyperlink ref="J75" r:id="rId201"/>
     <hyperlink ref="K75" r:id="rId202"/>
     <hyperlink ref="L75" r:id="rId203"/>
-    <hyperlink ref="C127" r:id="rId204"/>
-    <hyperlink ref="N127" r:id="rId205"/>
+    <hyperlink ref="C128" r:id="rId204"/>
+    <hyperlink ref="N128" r:id="rId205"/>
     <hyperlink ref="C40" r:id="rId206"/>
     <hyperlink ref="K40" r:id="rId207"/>
     <hyperlink ref="J40" r:id="rId208"/>
@@ -5765,14 +5803,15 @@
     <hyperlink ref="M45" r:id="rId217"/>
     <hyperlink ref="N45" r:id="rId218"/>
     <hyperlink ref="C23" r:id="rId219"/>
-    <hyperlink ref="C158" r:id="rId220"/>
+    <hyperlink ref="C159" r:id="rId220"/>
     <hyperlink ref="C37" r:id="rId221"/>
     <hyperlink ref="J37" r:id="rId222"/>
     <hyperlink ref="N37" r:id="rId223"/>
     <hyperlink ref="L37" r:id="rId224"/>
     <hyperlink ref="K37" r:id="rId225"/>
-    <hyperlink ref="C156" r:id="rId226"/>
-    <hyperlink ref="P156" r:id="rId227"/>
+    <hyperlink ref="C157" r:id="rId226"/>
+    <hyperlink ref="P157" r:id="rId227"/>
+    <hyperlink ref="C110" r:id="rId228"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
add 'Change in Source of Leader Support' and 'Peace Accords Matrix Implementation'
</commit_message>
<xml_diff>
--- a/PolData.xlsx
+++ b/PolData.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="971" uniqueCount="534">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="990" uniqueCount="545">
   <si>
     <t>name</t>
   </si>
@@ -1629,6 +1629,39 @@
   </si>
   <si>
     <t>http://dx.doi.org/10.7910/DVN/F8ITEB</t>
+  </si>
+  <si>
+    <t>Change in Source of Leader Support</t>
+  </si>
+  <si>
+    <t>http://www.chisols.org/</t>
+  </si>
+  <si>
+    <t>Leader transitions</t>
+  </si>
+  <si>
+    <t>http://www.chisols.org/uploads/1/1/2/6/11264284/chisolsusermanualv4.0.pdf</t>
+  </si>
+  <si>
+    <t>http://www.chisols.org/uploads/1/1/2/6/11264284/chisolsstyr4_0.zip</t>
+  </si>
+  <si>
+    <t>zip file is for the state-year datasets</t>
+  </si>
+  <si>
+    <t>https://peaceaccords.nd.edu/research</t>
+  </si>
+  <si>
+    <t>Peace Accords Matrix Implementation</t>
+  </si>
+  <si>
+    <t>Intrastate peace, peace agreements, implementation</t>
+  </si>
+  <si>
+    <t>http://peaceaccords.nd.edu/sites/default/files/PAM_ID%20V.1.5%20Updated%2029JULY2015.xlsx</t>
+  </si>
+  <si>
+    <t>http://peaceaccords.nd.edu/sites/default/files/PAM_ID%20CODEBOOK%20V.1.5%2029July2015.pdf</t>
   </si>
 </sst>
 </file>
@@ -1968,10 +2001,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q176"/>
+  <dimension ref="A1:Q178"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A36" sqref="A36"/>
+    <sheetView tabSelected="1" topLeftCell="A107" workbookViewId="0">
+      <selection activeCell="I125" sqref="I125"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2649,201 +2682,213 @@
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>146</v>
+        <v>534</v>
       </c>
       <c r="B24" t="s">
-        <v>128</v>
+        <v>40</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>145</v>
+        <v>535</v>
+      </c>
+      <c r="D24" t="s">
+        <v>536</v>
+      </c>
+      <c r="E24" t="s">
+        <v>14</v>
+      </c>
+      <c r="F24">
+        <v>1919</v>
+      </c>
+      <c r="G24">
+        <v>2008</v>
+      </c>
+      <c r="H24" t="s">
+        <v>348</v>
+      </c>
+      <c r="I24" t="s">
+        <v>349</v>
+      </c>
+      <c r="J24" s="2" t="s">
+        <v>537</v>
+      </c>
+      <c r="P24" s="2" t="s">
+        <v>538</v>
+      </c>
+      <c r="Q24" t="s">
+        <v>539</v>
       </c>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>127</v>
+        <v>146</v>
       </c>
       <c r="B25" t="s">
-        <v>259</v>
+        <v>128</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="I25" t="s">
-        <v>20</v>
+        <v>145</v>
       </c>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>173</v>
+        <v>127</v>
       </c>
       <c r="B26" t="s">
-        <v>128</v>
+        <v>259</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>175</v>
+        <v>121</v>
+      </c>
+      <c r="I26" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B27" t="s">
-        <v>86</v>
+        <v>128</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="E27" t="s">
-        <v>176</v>
-      </c>
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="B28" t="s">
-        <v>25</v>
+        <v>86</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>175</v>
       </c>
       <c r="E28" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>135</v>
+        <v>177</v>
       </c>
       <c r="B29" t="s">
-        <v>134</v>
+        <v>25</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>136</v>
+        <v>175</v>
+      </c>
+      <c r="E29" t="s">
+        <v>178</v>
       </c>
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>184</v>
+        <v>135</v>
       </c>
       <c r="B30" t="s">
-        <v>128</v>
+        <v>134</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>183</v>
+        <v>136</v>
       </c>
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
+        <v>184</v>
+      </c>
+      <c r="B31" t="s">
+        <v>128</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
         <v>54</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B32" t="s">
         <v>55</v>
       </c>
-      <c r="C31" s="2" t="s">
+      <c r="C32" s="2" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A32" s="1" t="s">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A33" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B33" t="s">
         <v>25</v>
       </c>
-      <c r="C32" s="2" t="s">
+      <c r="C33" s="2" t="s">
         <v>47</v>
-      </c>
-    </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
-        <v>158</v>
-      </c>
-      <c r="B33" t="s">
-        <v>99</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>187</v>
+        <v>158</v>
       </c>
       <c r="B34" t="s">
         <v>99</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>188</v>
-      </c>
-      <c r="F34">
-        <v>1960</v>
-      </c>
-      <c r="G34">
-        <v>2011</v>
-      </c>
-      <c r="H34" t="s">
-        <v>16</v>
-      </c>
-      <c r="I34" t="s">
-        <v>189</v>
+        <v>159</v>
       </c>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>164</v>
+        <v>187</v>
       </c>
       <c r="B35" t="s">
-        <v>165</v>
+        <v>99</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>166</v>
+        <v>188</v>
+      </c>
+      <c r="F35">
+        <v>1960</v>
+      </c>
+      <c r="G35">
+        <v>2011</v>
+      </c>
+      <c r="H35" t="s">
+        <v>16</v>
+      </c>
+      <c r="I35" t="s">
+        <v>189</v>
       </c>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>531</v>
+        <v>164</v>
       </c>
       <c r="B36" t="s">
-        <v>134</v>
+        <v>165</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>533</v>
-      </c>
-      <c r="E36" t="s">
-        <v>532</v>
-      </c>
-      <c r="F36">
-        <v>1982</v>
-      </c>
-      <c r="G36">
-        <v>2011</v>
-      </c>
-      <c r="H36" t="s">
-        <v>348</v>
-      </c>
-      <c r="I36" t="s">
-        <v>349</v>
+        <v>166</v>
       </c>
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>371</v>
+        <v>531</v>
       </c>
       <c r="B37" t="s">
-        <v>25</v>
+        <v>134</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>372</v>
-      </c>
-      <c r="D37" t="s">
-        <v>363</v>
+        <v>533</v>
       </c>
       <c r="E37" t="s">
-        <v>34</v>
+        <v>532</v>
       </c>
       <c r="F37">
-        <v>2006</v>
+        <v>1982</v>
+      </c>
+      <c r="G37">
+        <v>2011</v>
       </c>
       <c r="H37" t="s">
         <v>348</v>
@@ -2854,22 +2899,22 @@
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>503</v>
+        <v>371</v>
       </c>
       <c r="B38" t="s">
-        <v>99</v>
+        <v>25</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>502</v>
+        <v>372</v>
+      </c>
+      <c r="D38" t="s">
+        <v>363</v>
       </c>
       <c r="E38" t="s">
         <v>34</v>
       </c>
       <c r="F38">
-        <v>1900</v>
-      </c>
-      <c r="G38">
-        <v>2016</v>
+        <v>2006</v>
       </c>
       <c r="H38" t="s">
         <v>348</v>
@@ -2877,57 +2922,63 @@
       <c r="I38" t="s">
         <v>349</v>
       </c>
-      <c r="J38" s="2" t="s">
-        <v>504</v>
-      </c>
-      <c r="K38" s="2" t="s">
-        <v>507</v>
-      </c>
-      <c r="L38" s="2" t="s">
-        <v>506</v>
-      </c>
-      <c r="N38" s="2" t="s">
-        <v>505</v>
-      </c>
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>39</v>
+        <v>503</v>
       </c>
       <c r="B39" t="s">
-        <v>40</v>
+        <v>99</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>41</v>
+        <v>502</v>
       </c>
       <c r="E39" t="s">
-        <v>14</v>
+        <v>34</v>
       </c>
       <c r="F39">
-        <v>1816</v>
+        <v>1900</v>
       </c>
       <c r="G39">
-        <v>2007</v>
+        <v>2016</v>
       </c>
       <c r="H39" t="s">
-        <v>16</v>
+        <v>348</v>
       </c>
       <c r="I39" t="s">
-        <v>20</v>
+        <v>349</v>
+      </c>
+      <c r="J39" s="2" t="s">
+        <v>504</v>
+      </c>
+      <c r="K39" s="2" t="s">
+        <v>507</v>
+      </c>
+      <c r="L39" s="2" t="s">
+        <v>506</v>
+      </c>
+      <c r="N39" s="2" t="s">
+        <v>505</v>
       </c>
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>215</v>
+        <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>237</v>
+        <v>40</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>214</v>
+        <v>41</v>
+      </c>
+      <c r="E40" t="s">
+        <v>14</v>
       </c>
       <c r="F40">
-        <v>1995</v>
+        <v>1816</v>
+      </c>
+      <c r="G40">
+        <v>2007</v>
       </c>
       <c r="H40" t="s">
         <v>16</v>
@@ -2938,140 +2989,134 @@
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>476</v>
+        <v>215</v>
       </c>
       <c r="B41" t="s">
-        <v>40</v>
+        <v>237</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>477</v>
-      </c>
-      <c r="D41" t="s">
-        <v>478</v>
-      </c>
-      <c r="E41" t="s">
-        <v>14</v>
+        <v>214</v>
       </c>
       <c r="F41">
-        <v>2002</v>
+        <v>1995</v>
       </c>
       <c r="H41" t="s">
-        <v>348</v>
+        <v>16</v>
       </c>
       <c r="I41" t="s">
-        <v>349</v>
-      </c>
-      <c r="J41" s="2" t="s">
-        <v>480</v>
-      </c>
-      <c r="K41" s="2" t="s">
-        <v>479</v>
+        <v>20</v>
       </c>
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>330</v>
+        <v>476</v>
       </c>
       <c r="B42" t="s">
-        <v>165</v>
+        <v>40</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>331</v>
+        <v>477</v>
+      </c>
+      <c r="D42" t="s">
+        <v>478</v>
       </c>
       <c r="E42" t="s">
-        <v>77</v>
+        <v>14</v>
       </c>
       <c r="F42">
-        <v>1953</v>
+        <v>2002</v>
       </c>
       <c r="H42" t="s">
-        <v>16</v>
+        <v>348</v>
       </c>
       <c r="I42" t="s">
-        <v>20</v>
+        <v>349</v>
+      </c>
+      <c r="J42" s="2" t="s">
+        <v>480</v>
+      </c>
+      <c r="K42" s="2" t="s">
+        <v>479</v>
       </c>
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>75</v>
+        <v>330</v>
       </c>
       <c r="B43" t="s">
-        <v>25</v>
+        <v>165</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>76</v>
+        <v>331</v>
       </c>
       <c r="E43" t="s">
         <v>77</v>
       </c>
       <c r="F43">
-        <v>1971</v>
+        <v>1953</v>
+      </c>
+      <c r="H43" t="s">
+        <v>16</v>
+      </c>
+      <c r="I43" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="44" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>197</v>
+        <v>75</v>
       </c>
       <c r="B44" t="s">
-        <v>55</v>
+        <v>25</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>198</v>
+        <v>76</v>
       </c>
       <c r="E44" t="s">
-        <v>199</v>
+        <v>77</v>
       </c>
       <c r="F44">
-        <v>1975</v>
-      </c>
-      <c r="G44">
-        <v>2015</v>
-      </c>
-      <c r="H44" t="s">
-        <v>16</v>
-      </c>
-      <c r="I44" t="s">
-        <v>20</v>
+        <v>1971</v>
       </c>
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>409</v>
+        <v>197</v>
       </c>
       <c r="B45" t="s">
-        <v>250</v>
+        <v>55</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>410</v>
+        <v>198</v>
       </c>
       <c r="E45" t="s">
-        <v>9</v>
+        <v>199</v>
+      </c>
+      <c r="F45">
+        <v>1975</v>
+      </c>
+      <c r="G45">
+        <v>2015</v>
       </c>
       <c r="H45" t="s">
-        <v>348</v>
+        <v>16</v>
       </c>
       <c r="I45" t="s">
-        <v>349</v>
-      </c>
-      <c r="J45" s="2" t="s">
-        <v>411</v>
-      </c>
-      <c r="K45" s="2" t="s">
-        <v>412</v>
+        <v>20</v>
       </c>
     </row>
     <row r="46" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>489</v>
+        <v>409</v>
       </c>
       <c r="B46" t="s">
-        <v>60</v>
+        <v>250</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>488</v>
+        <v>410</v>
       </c>
       <c r="E46" t="s">
-        <v>490</v>
+        <v>9</v>
       </c>
       <c r="H46" t="s">
         <v>348</v>
@@ -3080,81 +3125,84 @@
         <v>349</v>
       </c>
       <c r="J46" s="2" t="s">
-        <v>491</v>
+        <v>411</v>
       </c>
       <c r="K46" s="2" t="s">
-        <v>492</v>
-      </c>
-      <c r="L46" s="2" t="s">
-        <v>493</v>
-      </c>
-      <c r="M46" s="2" t="s">
-        <v>494</v>
-      </c>
-      <c r="N46" s="2" t="s">
-        <v>495</v>
+        <v>412</v>
       </c>
     </row>
     <row r="47" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>59</v>
+        <v>489</v>
       </c>
       <c r="B47" t="s">
         <v>60</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>61</v>
+        <v>488</v>
+      </c>
+      <c r="E47" t="s">
+        <v>490</v>
+      </c>
+      <c r="H47" t="s">
+        <v>348</v>
+      </c>
+      <c r="I47" t="s">
+        <v>349</v>
+      </c>
+      <c r="J47" s="2" t="s">
+        <v>491</v>
+      </c>
+      <c r="K47" s="2" t="s">
+        <v>492</v>
+      </c>
+      <c r="L47" s="2" t="s">
+        <v>493</v>
+      </c>
+      <c r="M47" s="2" t="s">
+        <v>494</v>
+      </c>
+      <c r="N47" s="2" t="s">
+        <v>495</v>
       </c>
     </row>
     <row r="48" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>196</v>
+        <v>59</v>
       </c>
       <c r="B48" t="s">
-        <v>165</v>
+        <v>60</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>195</v>
-      </c>
-      <c r="F48">
-        <v>1946</v>
-      </c>
-      <c r="G48">
-        <v>2016</v>
+        <v>61</v>
       </c>
     </row>
     <row r="49" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>238</v>
+        <v>196</v>
       </c>
       <c r="B49" t="s">
-        <v>237</v>
+        <v>165</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>243</v>
-      </c>
-      <c r="H49" t="s">
-        <v>16</v>
-      </c>
-      <c r="I49" t="s">
-        <v>20</v>
+        <v>195</v>
+      </c>
+      <c r="F49">
+        <v>1946</v>
+      </c>
+      <c r="G49">
+        <v>2016</v>
       </c>
     </row>
     <row r="50" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>219</v>
+        <v>238</v>
       </c>
       <c r="B50" t="s">
-        <v>124</v>
+        <v>237</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>218</v>
-      </c>
-      <c r="F50">
-        <v>1970</v>
-      </c>
-      <c r="G50">
-        <v>2015</v>
+        <v>243</v>
       </c>
       <c r="H50" t="s">
         <v>16</v>
@@ -3165,44 +3213,50 @@
     </row>
     <row r="51" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>191</v>
+        <v>219</v>
       </c>
       <c r="B51" t="s">
-        <v>25</v>
+        <v>124</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="E51" t="s">
-        <v>192</v>
+        <v>218</v>
+      </c>
+      <c r="F51">
+        <v>1970</v>
+      </c>
+      <c r="G51">
+        <v>2015</v>
+      </c>
+      <c r="H51" t="s">
+        <v>16</v>
+      </c>
+      <c r="I51" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="52" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>235</v>
+        <v>191</v>
       </c>
       <c r="B52" t="s">
-        <v>60</v>
+        <v>25</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>236</v>
-      </c>
-      <c r="H52" t="s">
-        <v>16</v>
-      </c>
-      <c r="I52" t="s">
-        <v>20</v>
+        <v>190</v>
+      </c>
+      <c r="E52" t="s">
+        <v>192</v>
       </c>
     </row>
     <row r="53" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>252</v>
+        <v>235</v>
       </c>
       <c r="B53" t="s">
-        <v>250</v>
+        <v>60</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>251</v>
+        <v>236</v>
       </c>
       <c r="H53" t="s">
         <v>16</v>
@@ -3213,129 +3267,129 @@
     </row>
     <row r="54" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>149</v>
+        <v>252</v>
       </c>
       <c r="B54" t="s">
-        <v>128</v>
+        <v>250</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>150</v>
+        <v>251</v>
+      </c>
+      <c r="H54" t="s">
+        <v>16</v>
+      </c>
+      <c r="I54" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="55" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>462</v>
+        <v>149</v>
       </c>
       <c r="B55" t="s">
-        <v>250</v>
+        <v>128</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>464</v>
-      </c>
-      <c r="D55" t="s">
-        <v>463</v>
-      </c>
-      <c r="E55" t="s">
-        <v>14</v>
-      </c>
-      <c r="F55">
-        <v>1946</v>
-      </c>
-      <c r="G55">
-        <v>2010</v>
-      </c>
-      <c r="H55" t="s">
-        <v>348</v>
-      </c>
-      <c r="I55" t="s">
-        <v>349</v>
-      </c>
-      <c r="J55" s="2" t="s">
-        <v>467</v>
-      </c>
-      <c r="K55" s="2" t="s">
-        <v>466</v>
-      </c>
-      <c r="L55" s="2" t="s">
-        <v>465</v>
+        <v>150</v>
       </c>
     </row>
     <row r="56" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>28</v>
+        <v>462</v>
       </c>
       <c r="B56" t="s">
-        <v>25</v>
+        <v>250</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>48</v>
+        <v>464</v>
+      </c>
+      <c r="D56" t="s">
+        <v>463</v>
+      </c>
+      <c r="E56" t="s">
+        <v>14</v>
+      </c>
+      <c r="F56">
+        <v>1946</v>
+      </c>
+      <c r="G56">
+        <v>2010</v>
+      </c>
+      <c r="H56" t="s">
+        <v>348</v>
+      </c>
+      <c r="I56" t="s">
+        <v>349</v>
+      </c>
+      <c r="J56" s="2" t="s">
+        <v>467</v>
+      </c>
+      <c r="K56" s="2" t="s">
+        <v>466</v>
+      </c>
+      <c r="L56" s="2" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="57" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>80</v>
+        <v>28</v>
       </c>
       <c r="B57" t="s">
-        <v>128</v>
+        <v>25</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="E57" t="s">
-        <v>9</v>
-      </c>
-      <c r="F57">
-        <v>1979</v>
+        <v>48</v>
       </c>
     </row>
     <row r="58" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>125</v>
+        <v>80</v>
       </c>
       <c r="B58" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>126</v>
+        <v>81</v>
+      </c>
+      <c r="E58" t="s">
+        <v>9</v>
+      </c>
+      <c r="F58">
+        <v>1979</v>
       </c>
     </row>
     <row r="59" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>179</v>
+        <v>125</v>
       </c>
       <c r="B59" t="s">
-        <v>165</v>
+        <v>124</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>180</v>
+        <v>126</v>
       </c>
     </row>
     <row r="60" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
+        <v>179</v>
+      </c>
+      <c r="B60" t="s">
+        <v>165</v>
+      </c>
+      <c r="C60" s="2" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="61" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
         <v>78</v>
       </c>
-      <c r="B60" t="s">
+      <c r="B61" t="s">
         <v>25</v>
       </c>
-      <c r="C60" s="2" t="s">
+      <c r="C61" s="2" t="s">
         <v>79</v>
-      </c>
-      <c r="E60" t="s">
-        <v>9</v>
-      </c>
-      <c r="F60">
-        <v>1979</v>
-      </c>
-    </row>
-    <row r="61" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A61" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="B61" t="s">
-        <v>83</v>
-      </c>
-      <c r="C61" s="2" t="s">
-        <v>84</v>
       </c>
       <c r="E61" t="s">
         <v>9</v>
@@ -3346,13 +3400,13 @@
     </row>
     <row r="62" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A62" s="3" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B62" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="E62" t="s">
         <v>9</v>
@@ -3360,225 +3414,225 @@
       <c r="F62">
         <v>1979</v>
       </c>
-      <c r="G62">
+    </row>
+    <row r="63" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A63" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="B63" t="s">
+        <v>86</v>
+      </c>
+      <c r="C63" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="E63" t="s">
+        <v>9</v>
+      </c>
+      <c r="F63">
+        <v>1979</v>
+      </c>
+      <c r="G63">
         <v>2009</v>
-      </c>
-    </row>
-    <row r="63" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A63" t="s">
-        <v>27</v>
-      </c>
-      <c r="B63" t="s">
-        <v>25</v>
-      </c>
-      <c r="C63" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="Q63" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="64" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>120</v>
+        <v>27</v>
       </c>
       <c r="B64" t="s">
-        <v>259</v>
+        <v>25</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="I64" t="s">
-        <v>20</v>
+        <v>49</v>
+      </c>
+      <c r="Q64" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="65" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>5</v>
+        <v>120</v>
       </c>
       <c r="B65" t="s">
-        <v>25</v>
+        <v>259</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D65" t="s">
-        <v>94</v>
-      </c>
-      <c r="E65" t="s">
-        <v>9</v>
-      </c>
-      <c r="F65">
-        <v>2002</v>
-      </c>
-      <c r="H65" t="s">
-        <v>16</v>
+        <v>119</v>
       </c>
       <c r="I65" t="s">
-        <v>248</v>
-      </c>
-      <c r="Q65" t="s">
-        <v>44</v>
+        <v>20</v>
       </c>
     </row>
     <row r="66" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>240</v>
+        <v>5</v>
       </c>
       <c r="B66" t="s">
-        <v>237</v>
+        <v>25</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>243</v>
+        <v>6</v>
+      </c>
+      <c r="D66" t="s">
+        <v>94</v>
+      </c>
+      <c r="E66" t="s">
+        <v>9</v>
+      </c>
+      <c r="F66">
+        <v>2002</v>
       </c>
       <c r="H66" t="s">
         <v>16</v>
       </c>
       <c r="I66" t="s">
+        <v>248</v>
+      </c>
+      <c r="Q66" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="67" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
+        <v>240</v>
+      </c>
+      <c r="B67" t="s">
+        <v>237</v>
+      </c>
+      <c r="C67" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="H67" t="s">
+        <v>16</v>
+      </c>
+      <c r="I67" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="67" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A67" s="1" t="s">
+    <row r="68" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A68" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B67" t="s">
+      <c r="B68" t="s">
         <v>25</v>
       </c>
-      <c r="C67" s="2" t="s">
+      <c r="C68" s="2" t="s">
         <v>52</v>
-      </c>
-    </row>
-    <row r="68" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A68" t="s">
-        <v>232</v>
-      </c>
-      <c r="B68" t="s">
-        <v>250</v>
-      </c>
-      <c r="C68" s="2" t="s">
-        <v>231</v>
       </c>
     </row>
     <row r="69" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>390</v>
+        <v>232</v>
       </c>
       <c r="B69" t="s">
-        <v>83</v>
+        <v>250</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>392</v>
-      </c>
-      <c r="D69" t="s">
-        <v>391</v>
-      </c>
-      <c r="E69" t="s">
-        <v>9</v>
-      </c>
-      <c r="F69">
-        <v>2007</v>
-      </c>
-      <c r="G69">
-        <v>2015</v>
-      </c>
-      <c r="H69" t="s">
-        <v>348</v>
-      </c>
-      <c r="I69" t="s">
-        <v>349</v>
-      </c>
-      <c r="Q69" t="s">
-        <v>393</v>
+        <v>231</v>
       </c>
     </row>
     <row r="70" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>276</v>
+        <v>390</v>
       </c>
       <c r="B70" t="s">
-        <v>124</v>
+        <v>83</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>277</v>
+        <v>392</v>
+      </c>
+      <c r="D70" t="s">
+        <v>391</v>
+      </c>
+      <c r="E70" t="s">
+        <v>9</v>
       </c>
       <c r="F70">
-        <v>1948</v>
+        <v>2007</v>
       </c>
       <c r="G70">
-        <v>2000</v>
+        <v>2015</v>
       </c>
       <c r="H70" t="s">
-        <v>16</v>
+        <v>348</v>
       </c>
       <c r="I70" t="s">
-        <v>20</v>
+        <v>349</v>
+      </c>
+      <c r="Q70" t="s">
+        <v>393</v>
       </c>
     </row>
     <row r="71" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>449</v>
+        <v>276</v>
       </c>
       <c r="B71" t="s">
-        <v>250</v>
+        <v>124</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>448</v>
-      </c>
-      <c r="E71" t="s">
-        <v>14</v>
+        <v>277</v>
       </c>
       <c r="F71">
-        <v>-4000</v>
+        <v>1948</v>
       </c>
       <c r="G71">
         <v>2000</v>
       </c>
       <c r="H71" t="s">
-        <v>348</v>
+        <v>16</v>
       </c>
       <c r="I71" t="s">
-        <v>349</v>
-      </c>
-      <c r="J71" s="2" t="s">
-        <v>450</v>
-      </c>
-      <c r="N71" s="2" t="s">
-        <v>451</v>
+        <v>20</v>
       </c>
     </row>
     <row r="72" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>224</v>
+        <v>449</v>
       </c>
       <c r="B72" t="s">
-        <v>40</v>
+        <v>250</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>225</v>
+        <v>448</v>
+      </c>
+      <c r="E72" t="s">
+        <v>14</v>
       </c>
       <c r="F72">
-        <v>1964</v>
+        <v>-4000</v>
       </c>
       <c r="G72">
-        <v>2008</v>
+        <v>2000</v>
       </c>
       <c r="H72" t="s">
-        <v>16</v>
+        <v>348</v>
       </c>
       <c r="I72" t="s">
-        <v>20</v>
+        <v>349</v>
+      </c>
+      <c r="J72" s="2" t="s">
+        <v>450</v>
+      </c>
+      <c r="N72" s="2" t="s">
+        <v>451</v>
       </c>
     </row>
     <row r="73" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>285</v>
+        <v>224</v>
       </c>
       <c r="B73" t="s">
-        <v>250</v>
+        <v>40</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>286</v>
+        <v>225</v>
+      </c>
+      <c r="F73">
+        <v>1964</v>
+      </c>
+      <c r="G73">
+        <v>2008</v>
       </c>
       <c r="H73" t="s">
         <v>16</v>
@@ -3589,94 +3643,76 @@
     </row>
     <row r="74" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>205</v>
+        <v>285</v>
       </c>
       <c r="B74" t="s">
-        <v>40</v>
+        <v>250</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>204</v>
-      </c>
-      <c r="F74">
-        <v>2006</v>
+        <v>286</v>
+      </c>
+      <c r="H74" t="s">
+        <v>16</v>
+      </c>
+      <c r="I74" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="75" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>200</v>
+        <v>205</v>
       </c>
       <c r="B75" t="s">
-        <v>99</v>
+        <v>40</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="F75">
-        <v>1980</v>
-      </c>
-      <c r="G75">
-        <v>2007</v>
-      </c>
-      <c r="Q75" t="s">
-        <v>18</v>
+        <v>2006</v>
       </c>
     </row>
     <row r="76" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>521</v>
+        <v>200</v>
       </c>
       <c r="B76" t="s">
-        <v>165</v>
+        <v>99</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>520</v>
-      </c>
-      <c r="D76" t="s">
-        <v>525</v>
-      </c>
-      <c r="E76" t="s">
-        <v>14</v>
+        <v>201</v>
       </c>
       <c r="F76">
-        <v>1975</v>
+        <v>1980</v>
       </c>
       <c r="G76">
-        <v>2012</v>
-      </c>
-      <c r="H76" t="s">
-        <v>348</v>
-      </c>
-      <c r="I76" t="s">
-        <v>349</v>
-      </c>
-      <c r="J76" s="2" t="s">
-        <v>522</v>
-      </c>
-      <c r="K76" s="2" t="s">
-        <v>523</v>
-      </c>
-      <c r="N76" s="2" t="s">
-        <v>524</v>
+        <v>2007</v>
+      </c>
+      <c r="Q76" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="77" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>468</v>
+        <v>521</v>
       </c>
       <c r="B77" t="s">
-        <v>40</v>
+        <v>165</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>464</v>
+        <v>520</v>
+      </c>
+      <c r="D77" t="s">
+        <v>525</v>
       </c>
       <c r="E77" t="s">
         <v>14</v>
       </c>
       <c r="F77">
-        <v>1816</v>
+        <v>1975</v>
       </c>
       <c r="G77">
-        <v>2001</v>
+        <v>2012</v>
       </c>
       <c r="H77" t="s">
         <v>348</v>
@@ -3685,201 +3721,219 @@
         <v>349</v>
       </c>
       <c r="J77" s="2" t="s">
-        <v>469</v>
+        <v>522</v>
       </c>
       <c r="K77" s="2" t="s">
-        <v>470</v>
-      </c>
-      <c r="L77" s="2" t="s">
-        <v>471</v>
+        <v>523</v>
+      </c>
+      <c r="N77" s="2" t="s">
+        <v>524</v>
       </c>
     </row>
     <row r="78" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>89</v>
+        <v>468</v>
       </c>
       <c r="B78" t="s">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>88</v>
+        <v>464</v>
       </c>
       <c r="E78" t="s">
-        <v>34</v>
+        <v>14</v>
       </c>
       <c r="F78">
-        <v>1972</v>
+        <v>1816</v>
+      </c>
+      <c r="G78">
+        <v>2001</v>
       </c>
       <c r="H78" t="s">
-        <v>16</v>
+        <v>348</v>
       </c>
       <c r="I78" t="s">
-        <v>20</v>
+        <v>349</v>
+      </c>
+      <c r="J78" s="2" t="s">
+        <v>469</v>
+      </c>
+      <c r="K78" s="2" t="s">
+        <v>470</v>
+      </c>
+      <c r="L78" s="2" t="s">
+        <v>471</v>
       </c>
     </row>
     <row r="79" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>104</v>
+        <v>89</v>
       </c>
       <c r="B79" t="s">
         <v>25</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>106</v>
+        <v>88</v>
       </c>
       <c r="E79" t="s">
-        <v>105</v>
+        <v>34</v>
       </c>
       <c r="F79">
-        <v>1980</v>
+        <v>1972</v>
+      </c>
+      <c r="H79" t="s">
+        <v>16</v>
+      </c>
+      <c r="I79" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="80" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>460</v>
+        <v>104</v>
       </c>
       <c r="B80" t="s">
         <v>25</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>461</v>
-      </c>
-      <c r="D80" t="s">
-        <v>363</v>
+        <v>106</v>
       </c>
       <c r="E80" t="s">
         <v>105</v>
       </c>
       <c r="F80">
-        <v>2009</v>
-      </c>
-      <c r="H80" t="s">
-        <v>348</v>
-      </c>
-      <c r="I80" t="s">
-        <v>301</v>
+        <v>1980</v>
       </c>
     </row>
     <row r="81" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>62</v>
+        <v>460</v>
       </c>
       <c r="B81" t="s">
         <v>25</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>63</v>
+        <v>461</v>
+      </c>
+      <c r="D81" t="s">
+        <v>363</v>
+      </c>
+      <c r="E81" t="s">
+        <v>105</v>
+      </c>
+      <c r="F81">
+        <v>2009</v>
+      </c>
+      <c r="H81" t="s">
+        <v>348</v>
+      </c>
+      <c r="I81" t="s">
+        <v>301</v>
       </c>
     </row>
     <row r="82" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>311</v>
+        <v>62</v>
       </c>
       <c r="B82" t="s">
-        <v>165</v>
+        <v>25</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>312</v>
-      </c>
-      <c r="E82" t="s">
-        <v>14</v>
-      </c>
-      <c r="H82" t="s">
-        <v>16</v>
-      </c>
-      <c r="I82" t="s">
-        <v>301</v>
+        <v>63</v>
       </c>
     </row>
     <row r="83" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>281</v>
+        <v>311</v>
       </c>
       <c r="B83" t="s">
-        <v>237</v>
+        <v>165</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>282</v>
+        <v>312</v>
+      </c>
+      <c r="E83" t="s">
+        <v>14</v>
       </c>
       <c r="H83" t="s">
         <v>16</v>
       </c>
       <c r="I83" t="s">
-        <v>20</v>
+        <v>301</v>
       </c>
     </row>
     <row r="84" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>418</v>
+        <v>281</v>
       </c>
       <c r="B84" t="s">
-        <v>86</v>
+        <v>237</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>419</v>
-      </c>
-      <c r="E84" t="s">
-        <v>420</v>
-      </c>
-      <c r="F84">
-        <v>1948</v>
-      </c>
-      <c r="G84">
-        <v>2012</v>
+        <v>282</v>
       </c>
       <c r="H84" t="s">
-        <v>348</v>
+        <v>16</v>
       </c>
       <c r="I84" t="s">
-        <v>349</v>
-      </c>
-      <c r="K84" s="2" t="s">
-        <v>421</v>
-      </c>
-      <c r="Q84" t="s">
-        <v>422</v>
+        <v>20</v>
       </c>
     </row>
     <row r="85" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>151</v>
+        <v>418</v>
       </c>
       <c r="B85" t="s">
-        <v>40</v>
+        <v>86</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>152</v>
+        <v>419</v>
       </c>
       <c r="E85" t="s">
-        <v>14</v>
+        <v>420</v>
+      </c>
+      <c r="F85">
+        <v>1948</v>
+      </c>
+      <c r="G85">
+        <v>2012</v>
+      </c>
+      <c r="H85" t="s">
+        <v>348</v>
+      </c>
+      <c r="I85" t="s">
+        <v>349</v>
+      </c>
+      <c r="K85" s="2" t="s">
+        <v>421</v>
+      </c>
+      <c r="Q85" t="s">
+        <v>422</v>
       </c>
     </row>
     <row r="86" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>242</v>
+        <v>151</v>
       </c>
       <c r="B86" t="s">
-        <v>237</v>
+        <v>40</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>243</v>
-      </c>
-      <c r="H86" t="s">
-        <v>16</v>
-      </c>
-      <c r="I86" t="s">
-        <v>20</v>
+        <v>152</v>
+      </c>
+      <c r="E86" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="87" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>292</v>
+        <v>242</v>
       </c>
       <c r="B87" t="s">
-        <v>99</v>
+        <v>237</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>291</v>
+        <v>243</v>
       </c>
       <c r="H87" t="s">
         <v>16</v>
@@ -3890,47 +3944,47 @@
     </row>
     <row r="88" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>153</v>
+        <v>292</v>
       </c>
       <c r="B88" t="s">
-        <v>259</v>
+        <v>99</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>154</v>
+        <v>291</v>
+      </c>
+      <c r="H88" t="s">
+        <v>16</v>
+      </c>
+      <c r="I88" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="89" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>228</v>
+        <v>153</v>
       </c>
       <c r="B89" t="s">
-        <v>40</v>
+        <v>259</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>225</v>
-      </c>
-      <c r="F89">
-        <v>1989</v>
-      </c>
-      <c r="G89">
-        <v>2017</v>
-      </c>
-      <c r="H89" t="s">
-        <v>16</v>
-      </c>
-      <c r="I89" t="s">
-        <v>20</v>
+        <v>154</v>
       </c>
     </row>
     <row r="90" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>245</v>
+        <v>228</v>
       </c>
       <c r="B90" t="s">
-        <v>237</v>
+        <v>40</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>244</v>
+        <v>225</v>
+      </c>
+      <c r="F90">
+        <v>1989</v>
+      </c>
+      <c r="G90">
+        <v>2017</v>
       </c>
       <c r="H90" t="s">
         <v>16</v>
@@ -3941,50 +3995,41 @@
     </row>
     <row r="91" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>100</v>
+        <v>245</v>
       </c>
       <c r="B91" t="s">
-        <v>99</v>
+        <v>237</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>101</v>
+        <v>244</v>
+      </c>
+      <c r="H91" t="s">
+        <v>16</v>
+      </c>
+      <c r="I91" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="92" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>239</v>
+        <v>100</v>
       </c>
       <c r="B92" t="s">
-        <v>237</v>
+        <v>99</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>243</v>
-      </c>
-      <c r="H92" t="s">
-        <v>16</v>
-      </c>
-      <c r="I92" t="s">
-        <v>20</v>
+        <v>101</v>
       </c>
     </row>
     <row r="93" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>254</v>
+        <v>239</v>
       </c>
       <c r="B93" t="s">
-        <v>55</v>
+        <v>237</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>253</v>
-      </c>
-      <c r="E93" t="s">
-        <v>255</v>
-      </c>
-      <c r="F93">
-        <v>1960</v>
-      </c>
-      <c r="G93">
-        <v>2014</v>
+        <v>243</v>
       </c>
       <c r="H93" t="s">
         <v>16</v>
@@ -3995,19 +4040,22 @@
     </row>
     <row r="94" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>270</v>
+        <v>254</v>
       </c>
       <c r="B94" t="s">
         <v>55</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>271</v>
+        <v>253</v>
+      </c>
+      <c r="E94" t="s">
+        <v>255</v>
       </c>
       <c r="F94">
-        <v>1990</v>
+        <v>1960</v>
       </c>
       <c r="G94">
-        <v>2010</v>
+        <v>2014</v>
       </c>
       <c r="H94" t="s">
         <v>16</v>
@@ -4018,96 +4066,90 @@
     </row>
     <row r="95" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>117</v>
+        <v>270</v>
       </c>
       <c r="B95" t="s">
         <v>55</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>118</v>
+        <v>271</v>
+      </c>
+      <c r="F95">
+        <v>1990</v>
+      </c>
+      <c r="G95">
+        <v>2010</v>
+      </c>
+      <c r="H95" t="s">
+        <v>16</v>
       </c>
       <c r="I95" t="s">
         <v>20</v>
       </c>
-      <c r="Q95" t="s">
+    </row>
+    <row r="96" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A96" t="s">
+        <v>117</v>
+      </c>
+      <c r="B96" t="s">
+        <v>55</v>
+      </c>
+      <c r="C96" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="I96" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q96" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="96" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A96" s="1" t="s">
+    <row r="97" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A97" s="1" t="s">
         <v>23</v>
-      </c>
-      <c r="B96" t="s">
-        <v>25</v>
-      </c>
-      <c r="C96" s="2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="97" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A97" t="s">
-        <v>300</v>
       </c>
       <c r="B97" t="s">
         <v>25</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>298</v>
-      </c>
-      <c r="E97" t="s">
-        <v>299</v>
-      </c>
-      <c r="F97">
-        <v>1969</v>
-      </c>
-      <c r="H97" t="s">
-        <v>16</v>
-      </c>
-      <c r="I97" t="s">
-        <v>249</v>
+        <v>53</v>
       </c>
     </row>
     <row r="98" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>332</v>
+        <v>300</v>
       </c>
       <c r="B98" t="s">
-        <v>134</v>
+        <v>25</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>333</v>
+        <v>298</v>
       </c>
       <c r="E98" t="s">
-        <v>334</v>
+        <v>299</v>
+      </c>
+      <c r="F98">
+        <v>1969</v>
       </c>
       <c r="H98" t="s">
         <v>16</v>
       </c>
       <c r="I98" t="s">
-        <v>20</v>
+        <v>249</v>
       </c>
     </row>
     <row r="99" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>267</v>
+        <v>332</v>
       </c>
       <c r="B99" t="s">
-        <v>250</v>
+        <v>134</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>266</v>
-      </c>
-      <c r="D99" t="s">
-        <v>269</v>
+        <v>333</v>
       </c>
       <c r="E99" t="s">
-        <v>268</v>
-      </c>
-      <c r="F99">
-        <v>1970</v>
-      </c>
-      <c r="G99">
-        <v>2014</v>
+        <v>334</v>
       </c>
       <c r="H99" t="s">
         <v>16</v>
@@ -4118,97 +4160,100 @@
     </row>
     <row r="100" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>407</v>
+        <v>267</v>
       </c>
       <c r="B100" t="s">
-        <v>40</v>
+        <v>250</v>
       </c>
       <c r="C100" s="2" t="s">
-        <v>406</v>
+        <v>266</v>
       </c>
       <c r="D100" t="s">
-        <v>408</v>
+        <v>269</v>
       </c>
       <c r="E100" t="s">
-        <v>14</v>
+        <v>268</v>
       </c>
       <c r="F100">
-        <v>1949</v>
+        <v>1970</v>
       </c>
       <c r="G100">
-        <v>2013</v>
+        <v>2014</v>
       </c>
       <c r="H100" t="s">
-        <v>348</v>
+        <v>16</v>
       </c>
       <c r="I100" t="s">
-        <v>349</v>
+        <v>20</v>
       </c>
     </row>
     <row r="101" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>96</v>
+        <v>407</v>
       </c>
       <c r="B101" t="s">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>90</v>
+        <v>406</v>
+      </c>
+      <c r="D101" t="s">
+        <v>408</v>
       </c>
       <c r="E101" t="s">
-        <v>69</v>
+        <v>14</v>
       </c>
       <c r="F101">
-        <v>1995</v>
+        <v>1949</v>
+      </c>
+      <c r="G101">
+        <v>2013</v>
+      </c>
+      <c r="H101" t="s">
+        <v>348</v>
+      </c>
+      <c r="I101" t="s">
+        <v>349</v>
       </c>
     </row>
     <row r="102" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>404</v>
+        <v>96</v>
       </c>
       <c r="B102" t="s">
-        <v>83</v>
+        <v>25</v>
       </c>
       <c r="C102" s="2" t="s">
-        <v>403</v>
-      </c>
-      <c r="D102" t="s">
-        <v>405</v>
+        <v>90</v>
       </c>
       <c r="E102" t="s">
-        <v>14</v>
+        <v>69</v>
       </c>
       <c r="F102">
-        <v>1875</v>
-      </c>
-      <c r="G102">
-        <v>2004</v>
-      </c>
-      <c r="H102" t="s">
-        <v>348</v>
-      </c>
-      <c r="I102" t="s">
-        <v>349</v>
+        <v>1995</v>
       </c>
     </row>
     <row r="103" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>454</v>
+        <v>404</v>
       </c>
       <c r="B103" t="s">
-        <v>25</v>
+        <v>83</v>
       </c>
       <c r="C103" s="2" t="s">
-        <v>455</v>
+        <v>403</v>
+      </c>
+      <c r="D103" t="s">
+        <v>405</v>
       </c>
       <c r="E103" t="s">
-        <v>456</v>
+        <v>14</v>
       </c>
       <c r="F103">
-        <v>2006</v>
+        <v>1875</v>
       </c>
       <c r="G103">
-        <v>2016</v>
+        <v>2004</v>
       </c>
       <c r="H103" t="s">
         <v>348</v>
@@ -4216,80 +4261,83 @@
       <c r="I103" t="s">
         <v>349</v>
       </c>
-      <c r="J103" s="2" t="s">
-        <v>457</v>
-      </c>
-      <c r="L103" s="2" t="s">
-        <v>458</v>
-      </c>
-      <c r="Q103" t="s">
-        <v>459</v>
-      </c>
     </row>
     <row r="104" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>11</v>
+        <v>454</v>
       </c>
       <c r="B104" t="s">
         <v>25</v>
       </c>
       <c r="C104" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D104" t="s">
-        <v>95</v>
+        <v>455</v>
       </c>
       <c r="E104" t="s">
-        <v>10</v>
+        <v>456</v>
       </c>
       <c r="F104">
-        <v>2007</v>
+        <v>2006</v>
+      </c>
+      <c r="G104">
+        <v>2016</v>
       </c>
       <c r="H104" t="s">
-        <v>16</v>
+        <v>348</v>
       </c>
       <c r="I104" t="s">
-        <v>21</v>
+        <v>349</v>
+      </c>
+      <c r="J104" s="2" t="s">
+        <v>457</v>
+      </c>
+      <c r="L104" s="2" t="s">
+        <v>458</v>
+      </c>
+      <c r="Q104" t="s">
+        <v>459</v>
       </c>
     </row>
     <row r="105" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>223</v>
+        <v>11</v>
       </c>
       <c r="B105" t="s">
-        <v>124</v>
+        <v>25</v>
       </c>
       <c r="C105" s="2" t="s">
-        <v>222</v>
+        <v>12</v>
+      </c>
+      <c r="D105" t="s">
+        <v>95</v>
+      </c>
+      <c r="E105" t="s">
+        <v>10</v>
       </c>
       <c r="F105">
-        <v>1</v>
-      </c>
-      <c r="G105">
-        <v>2010</v>
+        <v>2007</v>
       </c>
       <c r="H105" t="s">
         <v>16</v>
       </c>
       <c r="I105" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="106" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="B106" t="s">
-        <v>40</v>
+        <v>124</v>
       </c>
       <c r="C106" s="2" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="F106">
-        <v>1946</v>
+        <v>1</v>
       </c>
       <c r="G106">
-        <v>2016</v>
+        <v>2010</v>
       </c>
       <c r="H106" t="s">
         <v>16</v>
@@ -4300,468 +4348,474 @@
     </row>
     <row r="107" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>97</v>
+        <v>226</v>
       </c>
       <c r="B107" t="s">
-        <v>128</v>
+        <v>40</v>
       </c>
       <c r="C107" s="2" t="s">
-        <v>98</v>
+        <v>225</v>
+      </c>
+      <c r="F107">
+        <v>1946</v>
+      </c>
+      <c r="G107">
+        <v>2016</v>
+      </c>
+      <c r="H107" t="s">
+        <v>16</v>
+      </c>
+      <c r="I107" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="108" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>278</v>
+        <v>97</v>
       </c>
       <c r="B108" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="C108" s="2" t="s">
-        <v>279</v>
-      </c>
-      <c r="E108" t="s">
-        <v>280</v>
-      </c>
-      <c r="F108">
-        <v>1890</v>
-      </c>
-      <c r="G108">
-        <v>1996</v>
-      </c>
-      <c r="H108" t="s">
-        <v>16</v>
-      </c>
-      <c r="I108" t="s">
-        <v>20</v>
+        <v>98</v>
       </c>
     </row>
     <row r="109" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>156</v>
+        <v>278</v>
       </c>
       <c r="B109" t="s">
-        <v>25</v>
+        <v>124</v>
       </c>
       <c r="C109" s="2" t="s">
-        <v>154</v>
+        <v>279</v>
+      </c>
+      <c r="E109" t="s">
+        <v>280</v>
+      </c>
+      <c r="F109">
+        <v>1890</v>
+      </c>
+      <c r="G109">
+        <v>1996</v>
+      </c>
+      <c r="H109" t="s">
+        <v>16</v>
+      </c>
+      <c r="I109" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="110" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>413</v>
+        <v>156</v>
       </c>
       <c r="B110" t="s">
-        <v>128</v>
+        <v>25</v>
       </c>
       <c r="C110" s="2" t="s">
-        <v>414</v>
-      </c>
-      <c r="E110" t="s">
-        <v>415</v>
-      </c>
-      <c r="F110">
-        <v>1946</v>
-      </c>
-      <c r="G110">
-        <v>2014</v>
-      </c>
-      <c r="H110" t="s">
-        <v>348</v>
-      </c>
-      <c r="I110" t="s">
-        <v>349</v>
-      </c>
-      <c r="N110" s="2" t="s">
-        <v>416</v>
-      </c>
-      <c r="Q110" t="s">
-        <v>417</v>
+        <v>154</v>
       </c>
     </row>
     <row r="111" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>229</v>
+        <v>413</v>
       </c>
       <c r="B111" t="s">
-        <v>40</v>
+        <v>128</v>
       </c>
       <c r="C111" s="2" t="s">
-        <v>225</v>
+        <v>414</v>
+      </c>
+      <c r="E111" t="s">
+        <v>415</v>
       </c>
       <c r="F111">
-        <v>1952</v>
+        <v>1946</v>
       </c>
       <c r="G111">
-        <v>1997</v>
+        <v>2014</v>
       </c>
       <c r="H111" t="s">
-        <v>16</v>
+        <v>348</v>
       </c>
       <c r="I111" t="s">
-        <v>20</v>
+        <v>349</v>
+      </c>
+      <c r="N111" s="2" t="s">
+        <v>416</v>
+      </c>
+      <c r="Q111" t="s">
+        <v>417</v>
       </c>
     </row>
     <row r="112" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>514</v>
+        <v>229</v>
       </c>
       <c r="B112" t="s">
         <v>40</v>
       </c>
       <c r="C112" s="2" t="s">
-        <v>513</v>
-      </c>
-      <c r="D112" t="s">
-        <v>515</v>
-      </c>
-      <c r="E112" t="s">
-        <v>14</v>
+        <v>225</v>
       </c>
       <c r="F112">
-        <v>1970</v>
+        <v>1952</v>
       </c>
       <c r="G112">
-        <v>2010</v>
+        <v>1997</v>
       </c>
       <c r="H112" t="s">
-        <v>348</v>
+        <v>16</v>
       </c>
       <c r="I112" t="s">
-        <v>349</v>
+        <v>20</v>
       </c>
     </row>
     <row r="113" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>293</v>
+        <v>514</v>
       </c>
       <c r="B113" t="s">
         <v>40</v>
       </c>
       <c r="C113" s="2" t="s">
-        <v>294</v>
+        <v>513</v>
+      </c>
+      <c r="D113" t="s">
+        <v>515</v>
+      </c>
+      <c r="E113" t="s">
+        <v>14</v>
       </c>
       <c r="F113">
-        <v>2004</v>
+        <v>1970</v>
       </c>
       <c r="G113">
-        <v>2006</v>
+        <v>2010</v>
       </c>
       <c r="H113" t="s">
-        <v>16</v>
+        <v>348</v>
       </c>
       <c r="I113" t="s">
-        <v>20</v>
+        <v>349</v>
       </c>
     </row>
     <row r="114" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>102</v>
+        <v>293</v>
       </c>
       <c r="B114" t="s">
-        <v>99</v>
+        <v>40</v>
       </c>
       <c r="C114" s="2" t="s">
-        <v>103</v>
+        <v>294</v>
+      </c>
+      <c r="F114">
+        <v>2004</v>
+      </c>
+      <c r="G114">
+        <v>2006</v>
+      </c>
+      <c r="H114" t="s">
+        <v>16</v>
+      </c>
+      <c r="I114" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="115" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>289</v>
+        <v>102</v>
       </c>
       <c r="B115" t="s">
-        <v>124</v>
+        <v>99</v>
       </c>
       <c r="C115" s="2" t="s">
-        <v>290</v>
+        <v>103</v>
       </c>
     </row>
     <row r="116" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>246</v>
+        <v>289</v>
       </c>
       <c r="B116" t="s">
-        <v>165</v>
+        <v>124</v>
       </c>
       <c r="C116" s="2" t="s">
-        <v>247</v>
-      </c>
-      <c r="E116" t="s">
-        <v>14</v>
-      </c>
-      <c r="F116">
-        <v>1960</v>
-      </c>
-      <c r="G116">
-        <v>2006</v>
-      </c>
-      <c r="H116" t="s">
-        <v>16</v>
-      </c>
-      <c r="I116" t="s">
-        <v>249</v>
+        <v>290</v>
       </c>
     </row>
     <row r="117" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>365</v>
+        <v>246</v>
       </c>
       <c r="B117" t="s">
-        <v>128</v>
+        <v>165</v>
       </c>
       <c r="C117" s="2" t="s">
-        <v>364</v>
-      </c>
-      <c r="D117" t="s">
-        <v>370</v>
+        <v>247</v>
       </c>
       <c r="E117" t="s">
-        <v>366</v>
+        <v>14</v>
       </c>
       <c r="F117">
-        <v>1906</v>
+        <v>1960</v>
       </c>
       <c r="G117">
-        <v>2013</v>
+        <v>2006</v>
       </c>
       <c r="H117" t="s">
-        <v>367</v>
+        <v>16</v>
       </c>
       <c r="I117" t="s">
-        <v>368</v>
-      </c>
-      <c r="Q117" t="s">
-        <v>369</v>
+        <v>249</v>
       </c>
     </row>
     <row r="118" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>208</v>
+        <v>365</v>
       </c>
       <c r="B118" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="C118" s="2" t="s">
-        <v>209</v>
+        <v>364</v>
+      </c>
+      <c r="D118" t="s">
+        <v>370</v>
+      </c>
+      <c r="E118" t="s">
+        <v>366</v>
       </c>
       <c r="F118">
-        <v>1932</v>
+        <v>1906</v>
       </c>
       <c r="G118">
-        <v>2014</v>
+        <v>2013</v>
       </c>
       <c r="H118" t="s">
-        <v>16</v>
+        <v>367</v>
       </c>
       <c r="I118" t="s">
-        <v>20</v>
+        <v>368</v>
+      </c>
+      <c r="Q118" t="s">
+        <v>369</v>
       </c>
     </row>
     <row r="119" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>137</v>
+        <v>208</v>
       </c>
       <c r="B119" t="s">
-        <v>259</v>
+        <v>124</v>
       </c>
       <c r="C119" s="2" t="s">
-        <v>138</v>
+        <v>209</v>
+      </c>
+      <c r="F119">
+        <v>1932</v>
+      </c>
+      <c r="G119">
+        <v>2014</v>
+      </c>
+      <c r="H119" t="s">
+        <v>16</v>
+      </c>
+      <c r="I119" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="120" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>155</v>
+        <v>137</v>
       </c>
       <c r="B120" t="s">
         <v>259</v>
       </c>
       <c r="C120" s="2" t="s">
-        <v>154</v>
+        <v>138</v>
       </c>
     </row>
     <row r="121" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>57</v>
+        <v>155</v>
       </c>
       <c r="B121" t="s">
-        <v>128</v>
+        <v>259</v>
       </c>
       <c r="C121" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="Q121" t="s">
-        <v>17</v>
+        <v>154</v>
       </c>
     </row>
     <row r="122" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>129</v>
+        <v>57</v>
       </c>
       <c r="B122" t="s">
-        <v>259</v>
+        <v>128</v>
       </c>
       <c r="C122" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="E122" t="s">
-        <v>131</v>
-      </c>
-      <c r="F122">
-        <v>1945</v>
-      </c>
-      <c r="G122">
-        <v>2008</v>
-      </c>
-      <c r="I122" t="s">
-        <v>20</v>
+        <v>58</v>
+      </c>
+      <c r="Q122" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="123" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>148</v>
+        <v>129</v>
       </c>
       <c r="B123" t="s">
-        <v>128</v>
+        <v>259</v>
       </c>
       <c r="C123" s="2" t="s">
-        <v>147</v>
+        <v>130</v>
+      </c>
+      <c r="E123" t="s">
+        <v>131</v>
+      </c>
+      <c r="F123">
+        <v>1945</v>
+      </c>
+      <c r="G123">
+        <v>2008</v>
+      </c>
+      <c r="I123" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="124" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>233</v>
+        <v>148</v>
       </c>
       <c r="B124" t="s">
-        <v>165</v>
+        <v>128</v>
       </c>
       <c r="C124" s="2" t="s">
-        <v>234</v>
-      </c>
-      <c r="E124" t="s">
-        <v>14</v>
-      </c>
-      <c r="F124">
-        <v>2012</v>
-      </c>
-      <c r="G124">
-        <v>2016</v>
-      </c>
-      <c r="H124" t="s">
-        <v>16</v>
-      </c>
-      <c r="I124" t="s">
-        <v>20</v>
+        <v>147</v>
       </c>
     </row>
     <row r="125" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>35</v>
+        <v>541</v>
       </c>
       <c r="B125" t="s">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="C125" s="2" t="s">
-        <v>36</v>
+        <v>540</v>
       </c>
       <c r="D125" t="s">
-        <v>37</v>
+        <v>542</v>
       </c>
       <c r="E125" t="s">
         <v>14</v>
       </c>
       <c r="F125">
-        <v>2001</v>
+        <v>1989</v>
+      </c>
+      <c r="G125">
+        <v>2012</v>
       </c>
       <c r="H125" t="s">
-        <v>16</v>
+        <v>348</v>
       </c>
       <c r="I125" t="s">
-        <v>20</v>
+        <v>349</v>
+      </c>
+      <c r="J125" s="2" t="s">
+        <v>544</v>
+      </c>
+      <c r="N125" s="2" t="s">
+        <v>543</v>
       </c>
     </row>
     <row r="126" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>185</v>
+        <v>233</v>
       </c>
       <c r="B126" t="s">
-        <v>128</v>
+        <v>165</v>
       </c>
       <c r="C126" s="2" t="s">
-        <v>186</v>
+        <v>234</v>
+      </c>
+      <c r="E126" t="s">
+        <v>14</v>
+      </c>
+      <c r="F126">
+        <v>2012</v>
+      </c>
+      <c r="G126">
+        <v>2016</v>
+      </c>
+      <c r="H126" t="s">
+        <v>16</v>
+      </c>
+      <c r="I126" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="127" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>516</v>
+        <v>35</v>
       </c>
       <c r="B127" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="C127" s="2" t="s">
-        <v>517</v>
+        <v>36</v>
       </c>
       <c r="D127" t="s">
-        <v>518</v>
+        <v>37</v>
       </c>
       <c r="E127" t="s">
         <v>14</v>
       </c>
       <c r="F127">
-        <v>1975</v>
-      </c>
-      <c r="G127">
-        <v>2011</v>
+        <v>2001</v>
       </c>
       <c r="H127" t="s">
-        <v>348</v>
+        <v>16</v>
       </c>
       <c r="I127" t="s">
-        <v>349</v>
-      </c>
-      <c r="P127" s="2" t="s">
-        <v>519</v>
+        <v>20</v>
       </c>
     </row>
     <row r="128" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>210</v>
+        <v>185</v>
       </c>
       <c r="B128" t="s">
-        <v>40</v>
+        <v>128</v>
       </c>
       <c r="C128" s="2" t="s">
-        <v>211</v>
-      </c>
-      <c r="F128">
-        <v>1976</v>
-      </c>
-      <c r="G128">
-        <v>2016</v>
-      </c>
-      <c r="H128" t="s">
-        <v>16</v>
-      </c>
-      <c r="I128" t="s">
-        <v>20</v>
+        <v>186</v>
       </c>
     </row>
     <row r="129" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>426</v>
+        <v>516</v>
       </c>
       <c r="B129" t="s">
-        <v>86</v>
+        <v>40</v>
       </c>
       <c r="C129" s="2" t="s">
-        <v>427</v>
+        <v>517</v>
+      </c>
+      <c r="D129" t="s">
+        <v>518</v>
       </c>
       <c r="E129" t="s">
-        <v>34</v>
+        <v>14</v>
       </c>
       <c r="F129">
-        <v>2015</v>
+        <v>1975</v>
       </c>
       <c r="G129">
-        <v>2016</v>
+        <v>2011</v>
       </c>
       <c r="H129" t="s">
         <v>348</v>
@@ -4769,45 +4823,51 @@
       <c r="I129" t="s">
         <v>349</v>
       </c>
-      <c r="K129" s="2" t="s">
-        <v>428</v>
+      <c r="P129" s="2" t="s">
+        <v>519</v>
       </c>
     </row>
     <row r="130" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
-        <v>144</v>
+        <v>210</v>
       </c>
       <c r="B130" t="s">
-        <v>60</v>
+        <v>40</v>
       </c>
       <c r="C130" s="2" t="s">
-        <v>143</v>
+        <v>211</v>
       </c>
       <c r="F130">
-        <v>1800</v>
+        <v>1976</v>
       </c>
       <c r="G130">
-        <v>2013</v>
+        <v>2016</v>
+      </c>
+      <c r="H130" t="s">
+        <v>16</v>
+      </c>
+      <c r="I130" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="131" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>472</v>
+        <v>426</v>
       </c>
       <c r="B131" t="s">
-        <v>25</v>
+        <v>86</v>
       </c>
       <c r="C131" s="2" t="s">
-        <v>473</v>
-      </c>
-      <c r="D131" t="s">
-        <v>474</v>
+        <v>427</v>
       </c>
       <c r="E131" t="s">
-        <v>112</v>
+        <v>34</v>
       </c>
       <c r="F131">
-        <v>1943</v>
+        <v>2015</v>
+      </c>
+      <c r="G131">
+        <v>2016</v>
       </c>
       <c r="H131" t="s">
         <v>348</v>
@@ -4815,71 +4875,65 @@
       <c r="I131" t="s">
         <v>349</v>
       </c>
-      <c r="N131" s="2" t="s">
-        <v>475</v>
+      <c r="K131" s="2" t="s">
+        <v>428</v>
       </c>
     </row>
     <row r="132" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>122</v>
+        <v>144</v>
       </c>
       <c r="B132" t="s">
-        <v>259</v>
+        <v>60</v>
       </c>
       <c r="C132" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="I132" t="s">
-        <v>20</v>
+        <v>143</v>
+      </c>
+      <c r="F132">
+        <v>1800</v>
+      </c>
+      <c r="G132">
+        <v>2013</v>
       </c>
     </row>
     <row r="133" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
-        <v>318</v>
+        <v>472</v>
       </c>
       <c r="B133" t="s">
-        <v>250</v>
+        <v>25</v>
       </c>
       <c r="C133" s="2" t="s">
-        <v>319</v>
+        <v>473</v>
+      </c>
+      <c r="D133" t="s">
+        <v>474</v>
       </c>
       <c r="E133" t="s">
-        <v>320</v>
+        <v>112</v>
       </c>
       <c r="F133">
-        <v>1975</v>
-      </c>
-      <c r="G133">
-        <v>1989</v>
+        <v>1943</v>
       </c>
       <c r="H133" t="s">
-        <v>16</v>
+        <v>348</v>
       </c>
       <c r="I133" t="s">
-        <v>20</v>
+        <v>349</v>
+      </c>
+      <c r="N133" s="2" t="s">
+        <v>475</v>
       </c>
     </row>
     <row r="134" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
-        <v>316</v>
+        <v>122</v>
       </c>
       <c r="B134" t="s">
-        <v>250</v>
+        <v>259</v>
       </c>
       <c r="C134" s="2" t="s">
-        <v>317</v>
-      </c>
-      <c r="E134" t="s">
-        <v>105</v>
-      </c>
-      <c r="F134">
-        <v>1950</v>
-      </c>
-      <c r="G134">
-        <v>1996</v>
-      </c>
-      <c r="H134" t="s">
-        <v>16</v>
+        <v>121</v>
       </c>
       <c r="I134" t="s">
         <v>20</v>
@@ -4887,19 +4941,22 @@
     </row>
     <row r="135" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
       <c r="B135" t="s">
-        <v>25</v>
+        <v>250</v>
       </c>
       <c r="C135" s="2" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="E135" t="s">
-        <v>77</v>
+        <v>320</v>
       </c>
       <c r="F135">
-        <v>2010</v>
+        <v>1975</v>
+      </c>
+      <c r="G135">
+        <v>1989</v>
       </c>
       <c r="H135" t="s">
         <v>16</v>
@@ -4910,35 +4967,44 @@
     </row>
     <row r="136" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
-        <v>141</v>
+        <v>316</v>
       </c>
       <c r="B136" t="s">
-        <v>237</v>
+        <v>250</v>
       </c>
       <c r="C136" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="Q136" t="s">
-        <v>17</v>
+        <v>317</v>
+      </c>
+      <c r="E136" t="s">
+        <v>105</v>
+      </c>
+      <c r="F136">
+        <v>1950</v>
+      </c>
+      <c r="G136">
+        <v>1996</v>
+      </c>
+      <c r="H136" t="s">
+        <v>16</v>
+      </c>
+      <c r="I136" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="137" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
-        <v>308</v>
+        <v>322</v>
       </c>
       <c r="B137" t="s">
-        <v>250</v>
+        <v>25</v>
       </c>
       <c r="C137" s="2" t="s">
-        <v>309</v>
+        <v>321</v>
       </c>
       <c r="E137" t="s">
-        <v>310</v>
+        <v>77</v>
       </c>
       <c r="F137">
-        <v>1950</v>
-      </c>
-      <c r="G137">
         <v>2010</v>
       </c>
       <c r="H137" t="s">
@@ -4950,243 +5016,237 @@
     </row>
     <row r="138" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
-        <v>287</v>
+        <v>141</v>
       </c>
       <c r="B138" t="s">
-        <v>134</v>
+        <v>237</v>
       </c>
       <c r="C138" s="2" t="s">
-        <v>288</v>
-      </c>
-      <c r="F138">
-        <v>1990</v>
-      </c>
-      <c r="G138">
-        <v>2008</v>
+        <v>142</v>
+      </c>
+      <c r="Q138" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="139" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
-        <v>526</v>
+        <v>308</v>
       </c>
       <c r="B139" t="s">
-        <v>40</v>
+        <v>250</v>
       </c>
       <c r="C139" s="2" t="s">
-        <v>527</v>
-      </c>
-      <c r="D139" t="s">
-        <v>528</v>
+        <v>309</v>
       </c>
       <c r="E139" t="s">
-        <v>14</v>
+        <v>310</v>
       </c>
       <c r="F139">
-        <v>1980</v>
+        <v>1950</v>
       </c>
       <c r="G139">
-        <v>2011</v>
+        <v>2010</v>
       </c>
       <c r="H139" t="s">
-        <v>348</v>
+        <v>16</v>
       </c>
       <c r="I139" t="s">
-        <v>349</v>
-      </c>
-      <c r="J139" s="2" t="s">
-        <v>529</v>
-      </c>
-      <c r="L139" s="2" t="s">
-        <v>530</v>
+        <v>20</v>
       </c>
     </row>
     <row r="140" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
-        <v>274</v>
+        <v>287</v>
       </c>
       <c r="B140" t="s">
-        <v>55</v>
+        <v>134</v>
       </c>
       <c r="C140" s="2" t="s">
-        <v>275</v>
-      </c>
-      <c r="H140" t="s">
-        <v>16</v>
-      </c>
-      <c r="I140" t="s">
-        <v>20</v>
+        <v>288</v>
+      </c>
+      <c r="F140">
+        <v>1990</v>
+      </c>
+      <c r="G140">
+        <v>2008</v>
       </c>
     </row>
     <row r="141" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
-        <v>157</v>
+        <v>526</v>
       </c>
       <c r="B141" t="s">
-        <v>128</v>
+        <v>40</v>
       </c>
       <c r="C141" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="Q141" t="s">
-        <v>18</v>
+        <v>527</v>
+      </c>
+      <c r="D141" t="s">
+        <v>528</v>
+      </c>
+      <c r="E141" t="s">
+        <v>14</v>
+      </c>
+      <c r="F141">
+        <v>1980</v>
+      </c>
+      <c r="G141">
+        <v>2011</v>
+      </c>
+      <c r="H141" t="s">
+        <v>348</v>
+      </c>
+      <c r="I141" t="s">
+        <v>349</v>
+      </c>
+      <c r="J141" s="2" t="s">
+        <v>529</v>
+      </c>
+      <c r="L141" s="2" t="s">
+        <v>530</v>
       </c>
     </row>
     <row r="142" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
-        <v>439</v>
+        <v>274</v>
       </c>
       <c r="B142" t="s">
-        <v>259</v>
+        <v>55</v>
       </c>
       <c r="C142" s="2" t="s">
-        <v>438</v>
+        <v>275</v>
       </c>
       <c r="H142" t="s">
-        <v>348</v>
+        <v>16</v>
       </c>
       <c r="I142" t="s">
-        <v>349</v>
-      </c>
-      <c r="J142" s="2" t="s">
-        <v>440</v>
-      </c>
-      <c r="K142" s="2" t="s">
-        <v>442</v>
-      </c>
-      <c r="L142" s="2" t="s">
-        <v>441</v>
+        <v>20</v>
       </c>
     </row>
     <row r="143" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
-        <v>443</v>
+        <v>157</v>
       </c>
       <c r="B143" t="s">
-        <v>259</v>
+        <v>128</v>
       </c>
       <c r="C143" s="2" t="s">
-        <v>438</v>
-      </c>
-      <c r="D143" t="s">
-        <v>447</v>
-      </c>
-      <c r="F143">
-        <v>1990</v>
-      </c>
-      <c r="G143">
-        <v>2014</v>
-      </c>
-      <c r="H143" t="s">
-        <v>348</v>
-      </c>
-      <c r="I143" t="s">
-        <v>349</v>
-      </c>
-      <c r="J143" s="2" t="s">
-        <v>444</v>
-      </c>
-      <c r="K143" s="2" t="s">
-        <v>445</v>
-      </c>
-      <c r="L143" s="2" t="s">
-        <v>446</v>
+        <v>154</v>
+      </c>
+      <c r="Q143" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="144" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
-        <v>194</v>
+        <v>439</v>
       </c>
       <c r="B144" t="s">
-        <v>99</v>
+        <v>259</v>
       </c>
       <c r="C144" s="2" t="s">
-        <v>193</v>
+        <v>438</v>
+      </c>
+      <c r="H144" t="s">
+        <v>348</v>
+      </c>
+      <c r="I144" t="s">
+        <v>349</v>
+      </c>
+      <c r="J144" s="2" t="s">
+        <v>440</v>
+      </c>
+      <c r="K144" s="2" t="s">
+        <v>442</v>
+      </c>
+      <c r="L144" s="2" t="s">
+        <v>441</v>
       </c>
     </row>
     <row r="145" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
-        <v>295</v>
+        <v>443</v>
       </c>
       <c r="B145" t="s">
-        <v>40</v>
+        <v>259</v>
       </c>
       <c r="C145" s="2" t="s">
-        <v>296</v>
-      </c>
-      <c r="E145" t="s">
-        <v>297</v>
+        <v>438</v>
+      </c>
+      <c r="D145" t="s">
+        <v>447</v>
       </c>
       <c r="F145">
         <v>1990</v>
       </c>
       <c r="G145">
-        <v>2015</v>
+        <v>2014</v>
       </c>
       <c r="H145" t="s">
-        <v>16</v>
+        <v>348</v>
       </c>
       <c r="I145" t="s">
-        <v>249</v>
+        <v>349</v>
+      </c>
+      <c r="J145" s="2" t="s">
+        <v>444</v>
+      </c>
+      <c r="K145" s="2" t="s">
+        <v>445</v>
+      </c>
+      <c r="L145" s="2" t="s">
+        <v>446</v>
       </c>
     </row>
     <row r="146" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
-        <v>256</v>
+        <v>194</v>
       </c>
       <c r="B146" t="s">
-        <v>250</v>
+        <v>99</v>
       </c>
       <c r="C146" s="2" t="s">
-        <v>257</v>
-      </c>
-      <c r="E146" t="s">
-        <v>258</v>
-      </c>
-      <c r="H146" t="s">
-        <v>16</v>
-      </c>
-      <c r="I146" t="s">
-        <v>20</v>
+        <v>193</v>
       </c>
     </row>
     <row r="147" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
-        <v>227</v>
+        <v>295</v>
       </c>
       <c r="B147" t="s">
         <v>40</v>
       </c>
       <c r="C147" s="2" t="s">
-        <v>225</v>
+        <v>296</v>
+      </c>
+      <c r="E147" t="s">
+        <v>297</v>
       </c>
       <c r="F147">
-        <v>1955</v>
+        <v>1990</v>
       </c>
       <c r="G147">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="H147" t="s">
         <v>16</v>
       </c>
       <c r="I147" t="s">
-        <v>20</v>
+        <v>249</v>
       </c>
     </row>
     <row r="148" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
-        <v>230</v>
+        <v>256</v>
       </c>
       <c r="B148" t="s">
-        <v>40</v>
+        <v>250</v>
       </c>
       <c r="C148" s="2" t="s">
-        <v>225</v>
-      </c>
-      <c r="F148">
-        <v>1995</v>
-      </c>
-      <c r="G148">
-        <v>2016</v>
+        <v>257</v>
+      </c>
+      <c r="E148" t="s">
+        <v>258</v>
       </c>
       <c r="H148" t="s">
         <v>16</v>
@@ -5197,99 +5257,102 @@
     </row>
     <row r="149" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
-        <v>452</v>
+        <v>227</v>
       </c>
       <c r="B149" t="s">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="C149" s="2" t="s">
-        <v>453</v>
-      </c>
-      <c r="E149" t="s">
-        <v>9</v>
+        <v>225</v>
+      </c>
+      <c r="F149">
+        <v>1955</v>
+      </c>
+      <c r="G149">
+        <v>2016</v>
       </c>
       <c r="H149" t="s">
-        <v>348</v>
+        <v>16</v>
       </c>
       <c r="I149" t="s">
-        <v>435</v>
+        <v>20</v>
       </c>
     </row>
     <row r="150" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
-        <v>109</v>
+        <v>230</v>
       </c>
       <c r="B150" t="s">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="C150" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="E150" t="s">
-        <v>111</v>
+        <v>225</v>
       </c>
       <c r="F150">
-        <v>1956</v>
+        <v>1995</v>
+      </c>
+      <c r="G150">
+        <v>2016</v>
+      </c>
+      <c r="H150" t="s">
+        <v>16</v>
+      </c>
+      <c r="I150" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="151" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
-        <v>326</v>
+        <v>452</v>
       </c>
       <c r="B151" t="s">
         <v>25</v>
       </c>
       <c r="C151" s="2" t="s">
-        <v>327</v>
+        <v>453</v>
       </c>
       <c r="E151" t="s">
-        <v>111</v>
-      </c>
-      <c r="F151">
-        <v>1998</v>
+        <v>9</v>
       </c>
       <c r="H151" t="s">
-        <v>16</v>
+        <v>348</v>
       </c>
       <c r="I151" t="s">
-        <v>20</v>
+        <v>435</v>
       </c>
     </row>
     <row r="152" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
-        <v>91</v>
+        <v>109</v>
       </c>
       <c r="B152" t="s">
         <v>25</v>
       </c>
       <c r="C152" s="2" t="s">
-        <v>93</v>
+        <v>110</v>
       </c>
       <c r="E152" t="s">
-        <v>92</v>
+        <v>111</v>
       </c>
       <c r="F152">
-        <v>1999</v>
+        <v>1956</v>
       </c>
     </row>
     <row r="153" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
-        <v>314</v>
+        <v>326</v>
       </c>
       <c r="B153" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="C153" s="2" t="s">
-        <v>313</v>
+        <v>327</v>
       </c>
       <c r="E153" t="s">
-        <v>315</v>
+        <v>111</v>
       </c>
       <c r="F153">
-        <v>1950</v>
-      </c>
-      <c r="G153">
-        <v>2004</v>
+        <v>1998</v>
       </c>
       <c r="H153" t="s">
         <v>16</v>
@@ -5300,122 +5363,110 @@
     </row>
     <row r="154" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
-        <v>161</v>
+        <v>91</v>
       </c>
       <c r="B154" t="s">
         <v>25</v>
       </c>
       <c r="C154" s="2" t="s">
-        <v>160</v>
+        <v>93</v>
+      </c>
+      <c r="E154" t="s">
+        <v>92</v>
+      </c>
+      <c r="F154">
+        <v>1999</v>
       </c>
     </row>
     <row r="155" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
-        <v>168</v>
+        <v>314</v>
       </c>
       <c r="B155" t="s">
         <v>40</v>
       </c>
       <c r="C155" s="2" t="s">
-        <v>167</v>
+        <v>313</v>
+      </c>
+      <c r="E155" t="s">
+        <v>315</v>
+      </c>
+      <c r="F155">
+        <v>1950</v>
+      </c>
+      <c r="G155">
+        <v>2004</v>
+      </c>
+      <c r="H155" t="s">
+        <v>16</v>
+      </c>
+      <c r="I155" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="156" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
-        <v>399</v>
+        <v>161</v>
       </c>
       <c r="B156" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="C156" s="2" t="s">
-        <v>400</v>
-      </c>
-      <c r="E156" t="s">
-        <v>14</v>
-      </c>
-      <c r="F156">
-        <v>2000</v>
-      </c>
-      <c r="G156">
-        <v>2014</v>
-      </c>
-      <c r="H156" t="s">
-        <v>348</v>
-      </c>
-      <c r="I156" t="s">
-        <v>349</v>
-      </c>
-      <c r="J156" s="2" t="s">
-        <v>402</v>
-      </c>
-      <c r="N156" s="2" t="s">
-        <v>401</v>
+        <v>160</v>
       </c>
     </row>
     <row r="157" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
-        <v>213</v>
+        <v>168</v>
       </c>
       <c r="B157" t="s">
-        <v>55</v>
+        <v>40</v>
       </c>
       <c r="C157" s="2" t="s">
-        <v>212</v>
-      </c>
-      <c r="H157" t="s">
-        <v>16</v>
-      </c>
-      <c r="I157" t="s">
-        <v>20</v>
+        <v>167</v>
       </c>
     </row>
     <row r="158" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
-        <v>395</v>
+        <v>399</v>
       </c>
       <c r="B158" t="s">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="C158" s="2" t="s">
-        <v>394</v>
-      </c>
-      <c r="D158" t="s">
-        <v>396</v>
+        <v>400</v>
       </c>
       <c r="E158" t="s">
-        <v>111</v>
+        <v>14</v>
       </c>
       <c r="F158">
-        <v>1986</v>
+        <v>2000</v>
       </c>
       <c r="G158">
-        <v>2015</v>
+        <v>2014</v>
       </c>
       <c r="H158" t="s">
-        <v>367</v>
+        <v>348</v>
       </c>
       <c r="I158" t="s">
-        <v>398</v>
+        <v>349</v>
       </c>
       <c r="J158" s="2" t="s">
-        <v>397</v>
+        <v>402</v>
+      </c>
+      <c r="N158" s="2" t="s">
+        <v>401</v>
       </c>
     </row>
     <row r="159" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
-        <v>323</v>
+        <v>213</v>
       </c>
       <c r="B159" t="s">
-        <v>25</v>
+        <v>55</v>
       </c>
       <c r="C159" s="2" t="s">
-        <v>324</v>
-      </c>
-      <c r="E159" t="s">
-        <v>325</v>
-      </c>
-      <c r="F159">
-        <v>1942</v>
+        <v>212</v>
       </c>
       <c r="H159" t="s">
         <v>16</v>
@@ -5426,91 +5477,103 @@
     </row>
     <row r="160" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
-        <v>273</v>
+        <v>395</v>
       </c>
       <c r="B160" t="s">
-        <v>237</v>
+        <v>25</v>
       </c>
       <c r="C160" s="2" t="s">
-        <v>272</v>
+        <v>394</v>
+      </c>
+      <c r="D160" t="s">
+        <v>396</v>
+      </c>
+      <c r="E160" t="s">
+        <v>111</v>
       </c>
       <c r="F160">
-        <v>1996</v>
+        <v>1986</v>
       </c>
       <c r="G160">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="H160" t="s">
-        <v>16</v>
+        <v>367</v>
       </c>
       <c r="I160" t="s">
-        <v>20</v>
+        <v>398</v>
+      </c>
+      <c r="J160" s="2" t="s">
+        <v>397</v>
       </c>
     </row>
     <row r="161" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
-        <v>508</v>
+        <v>323</v>
       </c>
       <c r="B161" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="C161" s="2" t="s">
-        <v>509</v>
-      </c>
-      <c r="D161" t="s">
-        <v>511</v>
+        <v>324</v>
       </c>
       <c r="E161" t="s">
-        <v>510</v>
+        <v>325</v>
       </c>
       <c r="F161">
-        <v>1989</v>
-      </c>
-      <c r="G161">
-        <v>2009</v>
+        <v>1942</v>
       </c>
       <c r="H161" t="s">
-        <v>348</v>
+        <v>16</v>
       </c>
       <c r="I161" t="s">
-        <v>349</v>
-      </c>
-      <c r="P161" s="2" t="s">
-        <v>512</v>
+        <v>20</v>
       </c>
     </row>
     <row r="162" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
-        <v>66</v>
+        <v>273</v>
       </c>
       <c r="B162" t="s">
-        <v>25</v>
+        <v>237</v>
       </c>
       <c r="C162" s="2" t="s">
-        <v>67</v>
+        <v>272</v>
+      </c>
+      <c r="F162">
+        <v>1996</v>
+      </c>
+      <c r="G162">
+        <v>2016</v>
+      </c>
+      <c r="H162" t="s">
+        <v>16</v>
+      </c>
+      <c r="I162" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="163" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
-        <v>500</v>
+        <v>508</v>
       </c>
       <c r="B163" t="s">
         <v>40</v>
       </c>
       <c r="C163" s="2" t="s">
-        <v>499</v>
+        <v>509</v>
       </c>
       <c r="D163" t="s">
-        <v>501</v>
+        <v>511</v>
       </c>
       <c r="E163" t="s">
-        <v>14</v>
+        <v>510</v>
       </c>
       <c r="F163">
-        <v>1946</v>
+        <v>1989</v>
       </c>
       <c r="G163">
-        <v>2015</v>
+        <v>2009</v>
       </c>
       <c r="H163" t="s">
         <v>348</v>
@@ -5518,93 +5581,102 @@
       <c r="I163" t="s">
         <v>349</v>
       </c>
+      <c r="P163" s="2" t="s">
+        <v>512</v>
+      </c>
     </row>
     <row r="164" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
-        <v>383</v>
+        <v>66</v>
       </c>
       <c r="B164" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="C164" s="2" t="s">
-        <v>384</v>
-      </c>
-      <c r="E164" t="s">
-        <v>386</v>
-      </c>
-      <c r="F164">
-        <v>1951</v>
-      </c>
-      <c r="H164" t="s">
-        <v>348</v>
-      </c>
-      <c r="I164" t="s">
-        <v>349</v>
-      </c>
-      <c r="N164" s="2" t="s">
-        <v>385</v>
+        <v>67</v>
       </c>
     </row>
     <row r="165" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
-        <v>139</v>
+        <v>500</v>
       </c>
       <c r="B165" t="s">
         <v>40</v>
       </c>
       <c r="C165" s="2" t="s">
-        <v>140</v>
+        <v>499</v>
+      </c>
+      <c r="D165" t="s">
+        <v>501</v>
+      </c>
+      <c r="E165" t="s">
+        <v>14</v>
+      </c>
+      <c r="F165">
+        <v>1946</v>
+      </c>
+      <c r="G165">
+        <v>2015</v>
+      </c>
+      <c r="H165" t="s">
+        <v>348</v>
+      </c>
+      <c r="I165" t="s">
+        <v>349</v>
       </c>
     </row>
     <row r="166" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
-        <v>329</v>
+        <v>383</v>
       </c>
       <c r="B166" t="s">
-        <v>165</v>
+        <v>40</v>
       </c>
       <c r="C166" s="2" t="s">
-        <v>328</v>
+        <v>384</v>
       </c>
       <c r="E166" t="s">
-        <v>34</v>
+        <v>386</v>
       </c>
       <c r="F166">
-        <v>1789</v>
+        <v>1951</v>
       </c>
       <c r="H166" t="s">
-        <v>16</v>
+        <v>348</v>
       </c>
       <c r="I166" t="s">
-        <v>20</v>
+        <v>349</v>
+      </c>
+      <c r="N166" s="2" t="s">
+        <v>385</v>
       </c>
     </row>
     <row r="167" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
-        <v>172</v>
+        <v>139</v>
       </c>
       <c r="B167" t="s">
-        <v>60</v>
+        <v>40</v>
       </c>
       <c r="C167" s="2" t="s">
-        <v>171</v>
+        <v>140</v>
       </c>
     </row>
     <row r="168" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
-        <v>217</v>
+        <v>329</v>
       </c>
       <c r="B168" t="s">
-        <v>60</v>
+        <v>165</v>
       </c>
       <c r="C168" s="2" t="s">
-        <v>216</v>
+        <v>328</v>
       </c>
       <c r="E168" t="s">
-        <v>14</v>
+        <v>34</v>
       </c>
       <c r="F168">
-        <v>1900</v>
+        <v>1789</v>
       </c>
       <c r="H168" t="s">
         <v>16</v>
@@ -5615,130 +5687,118 @@
     </row>
     <row r="169" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
-        <v>132</v>
+        <v>172</v>
       </c>
       <c r="B169" t="s">
-        <v>259</v>
+        <v>60</v>
       </c>
       <c r="C169" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="Q169" t="s">
-        <v>17</v>
+        <v>171</v>
       </c>
     </row>
     <row r="170" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
-        <v>182</v>
+        <v>217</v>
       </c>
       <c r="B170" t="s">
-        <v>165</v>
+        <v>60</v>
       </c>
       <c r="C170" s="2" t="s">
-        <v>181</v>
+        <v>216</v>
+      </c>
+      <c r="E170" t="s">
+        <v>14</v>
+      </c>
+      <c r="F170">
+        <v>1900</v>
+      </c>
+      <c r="H170" t="s">
+        <v>16</v>
+      </c>
+      <c r="I170" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="171" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
-        <v>423</v>
+        <v>132</v>
       </c>
       <c r="B171" t="s">
-        <v>86</v>
+        <v>259</v>
       </c>
       <c r="C171" s="2" t="s">
-        <v>424</v>
-      </c>
-      <c r="E171" t="s">
-        <v>34</v>
-      </c>
-      <c r="F171">
-        <v>1996</v>
-      </c>
-      <c r="G171">
-        <v>2016</v>
-      </c>
-      <c r="H171" t="s">
-        <v>348</v>
-      </c>
-      <c r="I171" t="s">
-        <v>425</v>
+        <v>133</v>
+      </c>
+      <c r="Q171" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="172" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
-        <v>115</v>
+        <v>182</v>
       </c>
       <c r="B172" t="s">
-        <v>128</v>
+        <v>165</v>
       </c>
       <c r="C172" s="2" t="s">
-        <v>116</v>
+        <v>181</v>
       </c>
     </row>
     <row r="173" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
-        <v>263</v>
+        <v>423</v>
       </c>
       <c r="B173" t="s">
-        <v>250</v>
+        <v>86</v>
       </c>
       <c r="C173" s="2" t="s">
-        <v>264</v>
+        <v>424</v>
       </c>
       <c r="E173" t="s">
-        <v>265</v>
+        <v>34</v>
       </c>
       <c r="F173">
-        <v>1500</v>
+        <v>1996</v>
       </c>
       <c r="G173">
-        <v>2000</v>
+        <v>2016</v>
       </c>
       <c r="H173" t="s">
-        <v>16</v>
+        <v>348</v>
       </c>
       <c r="I173" t="s">
-        <v>20</v>
+        <v>425</v>
       </c>
     </row>
     <row r="174" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
-        <v>221</v>
+        <v>115</v>
       </c>
       <c r="B174" t="s">
-        <v>86</v>
+        <v>128</v>
       </c>
       <c r="C174" s="2" t="s">
-        <v>220</v>
-      </c>
-      <c r="F174">
-        <v>2013</v>
-      </c>
-      <c r="H174" t="s">
-        <v>16</v>
-      </c>
-      <c r="I174" t="s">
-        <v>20</v>
+        <v>116</v>
       </c>
     </row>
     <row r="175" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
-        <v>13</v>
+        <v>263</v>
       </c>
       <c r="B175" t="s">
-        <v>25</v>
+        <v>250</v>
       </c>
       <c r="C175" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="D175" s="1" t="s">
-        <v>42</v>
+        <v>264</v>
       </c>
       <c r="E175" t="s">
-        <v>14</v>
+        <v>265</v>
       </c>
       <c r="F175">
-        <v>1981</v>
+        <v>1500</v>
+      </c>
+      <c r="G175">
+        <v>2000</v>
       </c>
       <c r="H175" t="s">
         <v>16</v>
@@ -5749,13 +5809,16 @@
     </row>
     <row r="176" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
-        <v>283</v>
+        <v>221</v>
       </c>
       <c r="B176" t="s">
-        <v>124</v>
+        <v>86</v>
       </c>
       <c r="C176" s="2" t="s">
-        <v>284</v>
+        <v>220</v>
+      </c>
+      <c r="F176">
+        <v>2013</v>
       </c>
       <c r="H176" t="s">
         <v>16</v>
@@ -5764,151 +5827,194 @@
         <v>20</v>
       </c>
     </row>
+    <row r="177" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A177" t="s">
+        <v>13</v>
+      </c>
+      <c r="B177" t="s">
+        <v>25</v>
+      </c>
+      <c r="C177" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D177" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E177" t="s">
+        <v>14</v>
+      </c>
+      <c r="F177">
+        <v>1981</v>
+      </c>
+      <c r="H177" t="s">
+        <v>16</v>
+      </c>
+      <c r="I177" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="178" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A178" t="s">
+        <v>283</v>
+      </c>
+      <c r="B178" t="s">
+        <v>124</v>
+      </c>
+      <c r="C178" s="2" t="s">
+        <v>284</v>
+      </c>
+      <c r="H178" t="s">
+        <v>16</v>
+      </c>
+      <c r="I178" t="s">
+        <v>20</v>
+      </c>
+    </row>
   </sheetData>
-  <sortState ref="A2:Q176">
+  <sortState ref="A2:Q178">
     <sortCondition ref="A2"/>
   </sortState>
   <hyperlinks>
     <hyperlink ref="C6" r:id="rId1"/>
-    <hyperlink ref="C65" r:id="rId2"/>
+    <hyperlink ref="C66" r:id="rId2"/>
     <hyperlink ref="C7" r:id="rId3"/>
     <hyperlink ref="C11" r:id="rId4"/>
-    <hyperlink ref="C104" r:id="rId5"/>
-    <hyperlink ref="C125" r:id="rId6"/>
-    <hyperlink ref="C175" r:id="rId7"/>
-    <hyperlink ref="C39" r:id="rId8"/>
-    <hyperlink ref="C32" r:id="rId9"/>
-    <hyperlink ref="C56" r:id="rId10"/>
-    <hyperlink ref="C63" r:id="rId11"/>
+    <hyperlink ref="C105" r:id="rId5"/>
+    <hyperlink ref="C127" r:id="rId6"/>
+    <hyperlink ref="C177" r:id="rId7"/>
+    <hyperlink ref="C40" r:id="rId8"/>
+    <hyperlink ref="C33" r:id="rId9"/>
+    <hyperlink ref="C57" r:id="rId10"/>
+    <hyperlink ref="C64" r:id="rId11"/>
     <hyperlink ref="C3" r:id="rId12"/>
     <hyperlink ref="C21" r:id="rId13"/>
-    <hyperlink ref="C67" r:id="rId14"/>
-    <hyperlink ref="C96" r:id="rId15"/>
-    <hyperlink ref="C31" r:id="rId16"/>
-    <hyperlink ref="C121" r:id="rId17"/>
-    <hyperlink ref="C47" r:id="rId18"/>
-    <hyperlink ref="C81" r:id="rId19"/>
+    <hyperlink ref="C68" r:id="rId14"/>
+    <hyperlink ref="C97" r:id="rId15"/>
+    <hyperlink ref="C32" r:id="rId16"/>
+    <hyperlink ref="C122" r:id="rId17"/>
+    <hyperlink ref="C48" r:id="rId18"/>
+    <hyperlink ref="C82" r:id="rId19"/>
     <hyperlink ref="C17" r:id="rId20"/>
-    <hyperlink ref="C162" r:id="rId21"/>
+    <hyperlink ref="C164" r:id="rId21"/>
     <hyperlink ref="C8" r:id="rId22"/>
-    <hyperlink ref="C43" r:id="rId23"/>
-    <hyperlink ref="C60" r:id="rId24"/>
-    <hyperlink ref="C57" r:id="rId25"/>
-    <hyperlink ref="C61" r:id="rId26"/>
-    <hyperlink ref="C62" r:id="rId27"/>
-    <hyperlink ref="C78" r:id="rId28"/>
-    <hyperlink ref="C101" r:id="rId29"/>
-    <hyperlink ref="C152" r:id="rId30"/>
-    <hyperlink ref="C107" r:id="rId31"/>
-    <hyperlink ref="C91" r:id="rId32"/>
-    <hyperlink ref="C114" r:id="rId33"/>
-    <hyperlink ref="C79" r:id="rId34"/>
+    <hyperlink ref="C44" r:id="rId23"/>
+    <hyperlink ref="C61" r:id="rId24"/>
+    <hyperlink ref="C58" r:id="rId25"/>
+    <hyperlink ref="C62" r:id="rId26"/>
+    <hyperlink ref="C63" r:id="rId27"/>
+    <hyperlink ref="C79" r:id="rId28"/>
+    <hyperlink ref="C102" r:id="rId29"/>
+    <hyperlink ref="C154" r:id="rId30"/>
+    <hyperlink ref="C108" r:id="rId31"/>
+    <hyperlink ref="C92" r:id="rId32"/>
+    <hyperlink ref="C115" r:id="rId33"/>
+    <hyperlink ref="C80" r:id="rId34"/>
     <hyperlink ref="C18" r:id="rId35"/>
-    <hyperlink ref="C150" r:id="rId36"/>
+    <hyperlink ref="C152" r:id="rId36"/>
     <hyperlink ref="C16" r:id="rId37"/>
-    <hyperlink ref="C172" r:id="rId38"/>
-    <hyperlink ref="C95" r:id="rId39"/>
-    <hyperlink ref="C64" r:id="rId40"/>
-    <hyperlink ref="C132" r:id="rId41"/>
+    <hyperlink ref="C174" r:id="rId38"/>
+    <hyperlink ref="C96" r:id="rId39"/>
+    <hyperlink ref="C65" r:id="rId40"/>
+    <hyperlink ref="C134" r:id="rId41"/>
     <hyperlink ref="C19" r:id="rId42"/>
-    <hyperlink ref="C58" r:id="rId43"/>
-    <hyperlink ref="C25" r:id="rId44"/>
-    <hyperlink ref="C122" r:id="rId45"/>
-    <hyperlink ref="C169" r:id="rId46"/>
-    <hyperlink ref="C29" r:id="rId47" display="http://comparativeconstitutionsproject.org/"/>
-    <hyperlink ref="C119" r:id="rId48"/>
-    <hyperlink ref="C165" r:id="rId49"/>
-    <hyperlink ref="C136" r:id="rId50"/>
-    <hyperlink ref="C130" r:id="rId51"/>
-    <hyperlink ref="C24" r:id="rId52"/>
-    <hyperlink ref="C123" r:id="rId53"/>
-    <hyperlink ref="C54" r:id="rId54"/>
-    <hyperlink ref="C85" r:id="rId55"/>
-    <hyperlink ref="C88" r:id="rId56"/>
-    <hyperlink ref="C120" r:id="rId57"/>
-    <hyperlink ref="C109" r:id="rId58"/>
-    <hyperlink ref="C141" r:id="rId59"/>
-    <hyperlink ref="C33" r:id="rId60"/>
-    <hyperlink ref="C154" r:id="rId61"/>
+    <hyperlink ref="C59" r:id="rId43"/>
+    <hyperlink ref="C26" r:id="rId44"/>
+    <hyperlink ref="C123" r:id="rId45"/>
+    <hyperlink ref="C171" r:id="rId46"/>
+    <hyperlink ref="C30" r:id="rId47" display="http://comparativeconstitutionsproject.org/"/>
+    <hyperlink ref="C120" r:id="rId48"/>
+    <hyperlink ref="C167" r:id="rId49"/>
+    <hyperlink ref="C138" r:id="rId50"/>
+    <hyperlink ref="C132" r:id="rId51"/>
+    <hyperlink ref="C25" r:id="rId52"/>
+    <hyperlink ref="C124" r:id="rId53"/>
+    <hyperlink ref="C55" r:id="rId54"/>
+    <hyperlink ref="C86" r:id="rId55"/>
+    <hyperlink ref="C89" r:id="rId56"/>
+    <hyperlink ref="C121" r:id="rId57"/>
+    <hyperlink ref="C110" r:id="rId58"/>
+    <hyperlink ref="C143" r:id="rId59"/>
+    <hyperlink ref="C34" r:id="rId60"/>
+    <hyperlink ref="C156" r:id="rId61"/>
     <hyperlink ref="C9" r:id="rId62"/>
-    <hyperlink ref="C35" r:id="rId63"/>
-    <hyperlink ref="C155" r:id="rId64"/>
+    <hyperlink ref="C36" r:id="rId63"/>
+    <hyperlink ref="C157" r:id="rId64"/>
     <hyperlink ref="C15" r:id="rId65"/>
-    <hyperlink ref="C167" r:id="rId66"/>
-    <hyperlink ref="C27" r:id="rId67"/>
-    <hyperlink ref="C26" r:id="rId68"/>
-    <hyperlink ref="C28" r:id="rId69"/>
-    <hyperlink ref="C59" r:id="rId70"/>
-    <hyperlink ref="C170" r:id="rId71"/>
-    <hyperlink ref="C30" r:id="rId72"/>
-    <hyperlink ref="C126" r:id="rId73"/>
-    <hyperlink ref="C34" r:id="rId74"/>
-    <hyperlink ref="C51" r:id="rId75"/>
-    <hyperlink ref="C144" r:id="rId76"/>
-    <hyperlink ref="C48" r:id="rId77"/>
-    <hyperlink ref="C44" r:id="rId78"/>
-    <hyperlink ref="C75" r:id="rId79"/>
+    <hyperlink ref="C169" r:id="rId66"/>
+    <hyperlink ref="C28" r:id="rId67"/>
+    <hyperlink ref="C27" r:id="rId68"/>
+    <hyperlink ref="C29" r:id="rId69"/>
+    <hyperlink ref="C60" r:id="rId70"/>
+    <hyperlink ref="C172" r:id="rId71"/>
+    <hyperlink ref="C31" r:id="rId72"/>
+    <hyperlink ref="C128" r:id="rId73"/>
+    <hyperlink ref="C35" r:id="rId74"/>
+    <hyperlink ref="C52" r:id="rId75"/>
+    <hyperlink ref="C146" r:id="rId76"/>
+    <hyperlink ref="C49" r:id="rId77"/>
+    <hyperlink ref="C45" r:id="rId78"/>
+    <hyperlink ref="C76" r:id="rId79"/>
     <hyperlink ref="C5" r:id="rId80"/>
-    <hyperlink ref="C74" r:id="rId81"/>
+    <hyperlink ref="C75" r:id="rId81"/>
     <hyperlink ref="C13" r:id="rId82"/>
-    <hyperlink ref="C118" r:id="rId83"/>
-    <hyperlink ref="C128" r:id="rId84"/>
-    <hyperlink ref="C157" r:id="rId85"/>
-    <hyperlink ref="C40" r:id="rId86"/>
-    <hyperlink ref="C168" r:id="rId87"/>
-    <hyperlink ref="C50" r:id="rId88"/>
-    <hyperlink ref="C174" r:id="rId89"/>
-    <hyperlink ref="C105" r:id="rId90"/>
-    <hyperlink ref="C72" r:id="rId91"/>
-    <hyperlink ref="C106" r:id="rId92"/>
-    <hyperlink ref="C147" r:id="rId93"/>
-    <hyperlink ref="C89" r:id="rId94"/>
-    <hyperlink ref="C111" r:id="rId95"/>
-    <hyperlink ref="C148" r:id="rId96"/>
-    <hyperlink ref="C68" r:id="rId97"/>
-    <hyperlink ref="C124" r:id="rId98"/>
-    <hyperlink ref="C52" r:id="rId99"/>
-    <hyperlink ref="C49" r:id="rId100"/>
-    <hyperlink ref="C92" r:id="rId101"/>
-    <hyperlink ref="C66" r:id="rId102"/>
+    <hyperlink ref="C119" r:id="rId83"/>
+    <hyperlink ref="C130" r:id="rId84"/>
+    <hyperlink ref="C159" r:id="rId85"/>
+    <hyperlink ref="C41" r:id="rId86"/>
+    <hyperlink ref="C170" r:id="rId87"/>
+    <hyperlink ref="C51" r:id="rId88"/>
+    <hyperlink ref="C176" r:id="rId89"/>
+    <hyperlink ref="C106" r:id="rId90"/>
+    <hyperlink ref="C73" r:id="rId91"/>
+    <hyperlink ref="C107" r:id="rId92"/>
+    <hyperlink ref="C149" r:id="rId93"/>
+    <hyperlink ref="C90" r:id="rId94"/>
+    <hyperlink ref="C112" r:id="rId95"/>
+    <hyperlink ref="C150" r:id="rId96"/>
+    <hyperlink ref="C69" r:id="rId97"/>
+    <hyperlink ref="C126" r:id="rId98"/>
+    <hyperlink ref="C53" r:id="rId99"/>
+    <hyperlink ref="C50" r:id="rId100"/>
+    <hyperlink ref="C93" r:id="rId101"/>
+    <hyperlink ref="C67" r:id="rId102"/>
     <hyperlink ref="C2" r:id="rId103"/>
-    <hyperlink ref="C86" r:id="rId104"/>
-    <hyperlink ref="C90" r:id="rId105"/>
-    <hyperlink ref="C116" r:id="rId106"/>
-    <hyperlink ref="C53" r:id="rId107"/>
-    <hyperlink ref="C93" r:id="rId108"/>
-    <hyperlink ref="C146" r:id="rId109"/>
+    <hyperlink ref="C87" r:id="rId104"/>
+    <hyperlink ref="C91" r:id="rId105"/>
+    <hyperlink ref="C117" r:id="rId106"/>
+    <hyperlink ref="C54" r:id="rId107"/>
+    <hyperlink ref="C94" r:id="rId108"/>
+    <hyperlink ref="C148" r:id="rId109"/>
     <hyperlink ref="C14" r:id="rId110"/>
     <hyperlink ref="C4" r:id="rId111"/>
-    <hyperlink ref="C173" r:id="rId112"/>
-    <hyperlink ref="C99" r:id="rId113"/>
-    <hyperlink ref="C94" r:id="rId114"/>
-    <hyperlink ref="C160" r:id="rId115"/>
-    <hyperlink ref="C140" r:id="rId116"/>
-    <hyperlink ref="C70" r:id="rId117"/>
-    <hyperlink ref="C108" r:id="rId118"/>
-    <hyperlink ref="C83" r:id="rId119"/>
-    <hyperlink ref="C176" r:id="rId120"/>
-    <hyperlink ref="C73" r:id="rId121"/>
-    <hyperlink ref="C138" r:id="rId122"/>
-    <hyperlink ref="C115" r:id="rId123"/>
-    <hyperlink ref="C87" r:id="rId124"/>
-    <hyperlink ref="C113" r:id="rId125"/>
-    <hyperlink ref="C145" r:id="rId126"/>
-    <hyperlink ref="C97" r:id="rId127"/>
+    <hyperlink ref="C175" r:id="rId112"/>
+    <hyperlink ref="C100" r:id="rId113"/>
+    <hyperlink ref="C95" r:id="rId114"/>
+    <hyperlink ref="C162" r:id="rId115"/>
+    <hyperlink ref="C142" r:id="rId116"/>
+    <hyperlink ref="C71" r:id="rId117"/>
+    <hyperlink ref="C109" r:id="rId118"/>
+    <hyperlink ref="C84" r:id="rId119"/>
+    <hyperlink ref="C178" r:id="rId120"/>
+    <hyperlink ref="C74" r:id="rId121"/>
+    <hyperlink ref="C140" r:id="rId122"/>
+    <hyperlink ref="C116" r:id="rId123"/>
+    <hyperlink ref="C88" r:id="rId124"/>
+    <hyperlink ref="C114" r:id="rId125"/>
+    <hyperlink ref="C147" r:id="rId126"/>
+    <hyperlink ref="C98" r:id="rId127"/>
     <hyperlink ref="C12" r:id="rId128"/>
     <hyperlink ref="C20" r:id="rId129"/>
-    <hyperlink ref="C137" r:id="rId130"/>
-    <hyperlink ref="C82" r:id="rId131"/>
-    <hyperlink ref="C153" r:id="rId132"/>
-    <hyperlink ref="C134" r:id="rId133"/>
-    <hyperlink ref="C133" r:id="rId134"/>
-    <hyperlink ref="C135" r:id="rId135"/>
-    <hyperlink ref="C159" r:id="rId136"/>
-    <hyperlink ref="C151" r:id="rId137"/>
-    <hyperlink ref="C166" r:id="rId138"/>
-    <hyperlink ref="C42" r:id="rId139"/>
-    <hyperlink ref="C98" r:id="rId140"/>
+    <hyperlink ref="C139" r:id="rId130"/>
+    <hyperlink ref="C83" r:id="rId131"/>
+    <hyperlink ref="C155" r:id="rId132"/>
+    <hyperlink ref="C136" r:id="rId133"/>
+    <hyperlink ref="C135" r:id="rId134"/>
+    <hyperlink ref="C137" r:id="rId135"/>
+    <hyperlink ref="C161" r:id="rId136"/>
+    <hyperlink ref="C153" r:id="rId137"/>
+    <hyperlink ref="C168" r:id="rId138"/>
+    <hyperlink ref="C43" r:id="rId139"/>
+    <hyperlink ref="C99" r:id="rId140"/>
     <hyperlink ref="J2" r:id="rId141"/>
     <hyperlink ref="M3" r:id="rId142"/>
     <hyperlink ref="J3" r:id="rId143"/>
@@ -5916,97 +6022,103 @@
     <hyperlink ref="J4" r:id="rId145"/>
     <hyperlink ref="P5" r:id="rId146"/>
     <hyperlink ref="J5" r:id="rId147"/>
-    <hyperlink ref="C117" r:id="rId148"/>
-    <hyperlink ref="C37" r:id="rId149"/>
+    <hyperlink ref="C118" r:id="rId148"/>
+    <hyperlink ref="C38" r:id="rId149"/>
     <hyperlink ref="P7" r:id="rId150"/>
     <hyperlink ref="J7" r:id="rId151"/>
     <hyperlink ref="M8" r:id="rId152"/>
     <hyperlink ref="L8" r:id="rId153"/>
     <hyperlink ref="J8" r:id="rId154"/>
-    <hyperlink ref="C164" r:id="rId155"/>
-    <hyperlink ref="N164" r:id="rId156"/>
+    <hyperlink ref="C166" r:id="rId155"/>
+    <hyperlink ref="N166" r:id="rId156"/>
     <hyperlink ref="C22" r:id="rId157"/>
     <hyperlink ref="N22" r:id="rId158"/>
-    <hyperlink ref="C69" r:id="rId159"/>
-    <hyperlink ref="C158" r:id="rId160"/>
-    <hyperlink ref="J158" r:id="rId161"/>
-    <hyperlink ref="C156" r:id="rId162"/>
-    <hyperlink ref="N156" r:id="rId163"/>
-    <hyperlink ref="J156" r:id="rId164"/>
-    <hyperlink ref="C102" r:id="rId165"/>
-    <hyperlink ref="C100" r:id="rId166"/>
-    <hyperlink ref="C45" r:id="rId167"/>
-    <hyperlink ref="J45" r:id="rId168"/>
-    <hyperlink ref="K45" r:id="rId169"/>
-    <hyperlink ref="C110" r:id="rId170"/>
-    <hyperlink ref="N110" r:id="rId171"/>
-    <hyperlink ref="C84" r:id="rId172"/>
-    <hyperlink ref="K84" r:id="rId173"/>
-    <hyperlink ref="C171" r:id="rId174"/>
-    <hyperlink ref="C129" r:id="rId175"/>
-    <hyperlink ref="K129" r:id="rId176"/>
+    <hyperlink ref="C70" r:id="rId159"/>
+    <hyperlink ref="C160" r:id="rId160"/>
+    <hyperlink ref="J160" r:id="rId161"/>
+    <hyperlink ref="C158" r:id="rId162"/>
+    <hyperlink ref="N158" r:id="rId163"/>
+    <hyperlink ref="J158" r:id="rId164"/>
+    <hyperlink ref="C103" r:id="rId165"/>
+    <hyperlink ref="C101" r:id="rId166"/>
+    <hyperlink ref="C46" r:id="rId167"/>
+    <hyperlink ref="J46" r:id="rId168"/>
+    <hyperlink ref="K46" r:id="rId169"/>
+    <hyperlink ref="C111" r:id="rId170"/>
+    <hyperlink ref="N111" r:id="rId171"/>
+    <hyperlink ref="C85" r:id="rId172"/>
+    <hyperlink ref="K85" r:id="rId173"/>
+    <hyperlink ref="C173" r:id="rId174"/>
+    <hyperlink ref="C131" r:id="rId175"/>
+    <hyperlink ref="K131" r:id="rId176"/>
     <hyperlink ref="L9" r:id="rId177"/>
     <hyperlink ref="J9" r:id="rId178"/>
     <hyperlink ref="J11" r:id="rId179"/>
-    <hyperlink ref="C142" r:id="rId180"/>
-    <hyperlink ref="J142" r:id="rId181"/>
-    <hyperlink ref="L142" r:id="rId182"/>
-    <hyperlink ref="K142" r:id="rId183"/>
-    <hyperlink ref="C143" r:id="rId184"/>
-    <hyperlink ref="J143" r:id="rId185"/>
-    <hyperlink ref="K143" r:id="rId186"/>
-    <hyperlink ref="L143" r:id="rId187"/>
-    <hyperlink ref="C71" r:id="rId188"/>
-    <hyperlink ref="J71" r:id="rId189"/>
-    <hyperlink ref="N71" r:id="rId190"/>
-    <hyperlink ref="C149" r:id="rId191"/>
-    <hyperlink ref="C103" r:id="rId192"/>
-    <hyperlink ref="J103" r:id="rId193"/>
-    <hyperlink ref="L103" r:id="rId194"/>
-    <hyperlink ref="C80" r:id="rId195"/>
-    <hyperlink ref="C55" r:id="rId196"/>
-    <hyperlink ref="L55" r:id="rId197"/>
-    <hyperlink ref="K55" r:id="rId198"/>
-    <hyperlink ref="J55" r:id="rId199"/>
-    <hyperlink ref="C77" r:id="rId200"/>
-    <hyperlink ref="J77" r:id="rId201"/>
-    <hyperlink ref="K77" r:id="rId202"/>
-    <hyperlink ref="L77" r:id="rId203"/>
-    <hyperlink ref="C131" r:id="rId204"/>
-    <hyperlink ref="N131" r:id="rId205"/>
-    <hyperlink ref="C41" r:id="rId206"/>
-    <hyperlink ref="K41" r:id="rId207"/>
-    <hyperlink ref="J41" r:id="rId208"/>
+    <hyperlink ref="C144" r:id="rId180"/>
+    <hyperlink ref="J144" r:id="rId181"/>
+    <hyperlink ref="L144" r:id="rId182"/>
+    <hyperlink ref="K144" r:id="rId183"/>
+    <hyperlink ref="C145" r:id="rId184"/>
+    <hyperlink ref="J145" r:id="rId185"/>
+    <hyperlink ref="K145" r:id="rId186"/>
+    <hyperlink ref="L145" r:id="rId187"/>
+    <hyperlink ref="C72" r:id="rId188"/>
+    <hyperlink ref="J72" r:id="rId189"/>
+    <hyperlink ref="N72" r:id="rId190"/>
+    <hyperlink ref="C151" r:id="rId191"/>
+    <hyperlink ref="C104" r:id="rId192"/>
+    <hyperlink ref="J104" r:id="rId193"/>
+    <hyperlink ref="L104" r:id="rId194"/>
+    <hyperlink ref="C81" r:id="rId195"/>
+    <hyperlink ref="C56" r:id="rId196"/>
+    <hyperlink ref="L56" r:id="rId197"/>
+    <hyperlink ref="K56" r:id="rId198"/>
+    <hyperlink ref="J56" r:id="rId199"/>
+    <hyperlink ref="C78" r:id="rId200"/>
+    <hyperlink ref="J78" r:id="rId201"/>
+    <hyperlink ref="K78" r:id="rId202"/>
+    <hyperlink ref="L78" r:id="rId203"/>
+    <hyperlink ref="C133" r:id="rId204"/>
+    <hyperlink ref="N133" r:id="rId205"/>
+    <hyperlink ref="C42" r:id="rId206"/>
+    <hyperlink ref="K42" r:id="rId207"/>
+    <hyperlink ref="J42" r:id="rId208"/>
     <hyperlink ref="C10" r:id="rId209"/>
     <hyperlink ref="J10" r:id="rId210"/>
     <hyperlink ref="P10" r:id="rId211"/>
     <hyperlink ref="N10" r:id="rId212"/>
-    <hyperlink ref="C46" r:id="rId213"/>
-    <hyperlink ref="J46" r:id="rId214"/>
-    <hyperlink ref="K46" r:id="rId215"/>
-    <hyperlink ref="L46" r:id="rId216"/>
-    <hyperlink ref="M46" r:id="rId217"/>
-    <hyperlink ref="N46" r:id="rId218"/>
+    <hyperlink ref="C47" r:id="rId213"/>
+    <hyperlink ref="J47" r:id="rId214"/>
+    <hyperlink ref="K47" r:id="rId215"/>
+    <hyperlink ref="L47" r:id="rId216"/>
+    <hyperlink ref="M47" r:id="rId217"/>
+    <hyperlink ref="N47" r:id="rId218"/>
     <hyperlink ref="C23" r:id="rId219"/>
-    <hyperlink ref="C163" r:id="rId220"/>
-    <hyperlink ref="C38" r:id="rId221"/>
-    <hyperlink ref="J38" r:id="rId222"/>
-    <hyperlink ref="N38" r:id="rId223"/>
-    <hyperlink ref="L38" r:id="rId224"/>
-    <hyperlink ref="K38" r:id="rId225"/>
-    <hyperlink ref="C161" r:id="rId226"/>
-    <hyperlink ref="P161" r:id="rId227"/>
-    <hyperlink ref="C112" r:id="rId228"/>
-    <hyperlink ref="C127" r:id="rId229"/>
-    <hyperlink ref="P127" r:id="rId230"/>
-    <hyperlink ref="C76" r:id="rId231"/>
-    <hyperlink ref="J76" r:id="rId232"/>
-    <hyperlink ref="K76" r:id="rId233"/>
-    <hyperlink ref="N76" r:id="rId234"/>
-    <hyperlink ref="C139" r:id="rId235"/>
-    <hyperlink ref="J139" r:id="rId236"/>
-    <hyperlink ref="L139" r:id="rId237"/>
-    <hyperlink ref="C36" r:id="rId238"/>
+    <hyperlink ref="C165" r:id="rId220"/>
+    <hyperlink ref="C39" r:id="rId221"/>
+    <hyperlink ref="J39" r:id="rId222"/>
+    <hyperlink ref="N39" r:id="rId223"/>
+    <hyperlink ref="L39" r:id="rId224"/>
+    <hyperlink ref="K39" r:id="rId225"/>
+    <hyperlink ref="C163" r:id="rId226"/>
+    <hyperlink ref="P163" r:id="rId227"/>
+    <hyperlink ref="C113" r:id="rId228"/>
+    <hyperlink ref="C129" r:id="rId229"/>
+    <hyperlink ref="P129" r:id="rId230"/>
+    <hyperlink ref="C77" r:id="rId231"/>
+    <hyperlink ref="J77" r:id="rId232"/>
+    <hyperlink ref="K77" r:id="rId233"/>
+    <hyperlink ref="N77" r:id="rId234"/>
+    <hyperlink ref="C141" r:id="rId235"/>
+    <hyperlink ref="J141" r:id="rId236"/>
+    <hyperlink ref="L141" r:id="rId237"/>
+    <hyperlink ref="C37" r:id="rId238"/>
+    <hyperlink ref="C24" r:id="rId239"/>
+    <hyperlink ref="J24" r:id="rId240"/>
+    <hyperlink ref="P24" r:id="rId241"/>
+    <hyperlink ref="C125" r:id="rId242"/>
+    <hyperlink ref="N125" r:id="rId243"/>
+    <hyperlink ref="J125" r:id="rId244"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
add 'The American Ideology Project'
</commit_message>
<xml_diff>
--- a/PolData.xlsx
+++ b/PolData.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="990" uniqueCount="545">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="998" uniqueCount="549">
   <si>
     <t>name</t>
   </si>
@@ -1662,6 +1662,18 @@
   </si>
   <si>
     <t>http://peaceaccords.nd.edu/sites/default/files/PAM_ID%20CODEBOOK%20V.1.5%2029July2015.pdf</t>
+  </si>
+  <si>
+    <t>The American Ideology Project</t>
+  </si>
+  <si>
+    <t>http://americanideologyproject.com/</t>
+  </si>
+  <si>
+    <t>Ideology, representation, policy preferences</t>
+  </si>
+  <si>
+    <t>http://americanideologyproject.com/estimates/estimates2015/codebook.pdf</t>
   </si>
 </sst>
 </file>
@@ -2001,10 +2013,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q178"/>
+  <dimension ref="A1:Q179"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A107" workbookViewId="0">
-      <selection activeCell="I125" sqref="I125"/>
+    <sheetView tabSelected="1" topLeftCell="A153" workbookViewId="0">
+      <selection activeCell="A157" sqref="A157"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5417,134 +5429,143 @@
     </row>
     <row r="157" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
-        <v>168</v>
+        <v>545</v>
       </c>
       <c r="B157" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="C157" s="2" t="s">
-        <v>167</v>
+        <v>546</v>
+      </c>
+      <c r="D157" t="s">
+        <v>547</v>
+      </c>
+      <c r="E157" t="s">
+        <v>34</v>
+      </c>
+      <c r="F157">
+        <v>2000</v>
+      </c>
+      <c r="G157">
+        <v>2011</v>
+      </c>
+      <c r="H157" t="s">
+        <v>348</v>
+      </c>
+      <c r="I157" t="s">
+        <v>349</v>
+      </c>
+      <c r="J157" s="2" t="s">
+        <v>548</v>
       </c>
     </row>
     <row r="158" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
-        <v>399</v>
+        <v>168</v>
       </c>
       <c r="B158" t="s">
         <v>40</v>
       </c>
       <c r="C158" s="2" t="s">
-        <v>400</v>
-      </c>
-      <c r="E158" t="s">
-        <v>14</v>
-      </c>
-      <c r="F158">
-        <v>2000</v>
-      </c>
-      <c r="G158">
-        <v>2014</v>
-      </c>
-      <c r="H158" t="s">
-        <v>348</v>
-      </c>
-      <c r="I158" t="s">
-        <v>349</v>
-      </c>
-      <c r="J158" s="2" t="s">
-        <v>402</v>
-      </c>
-      <c r="N158" s="2" t="s">
-        <v>401</v>
+        <v>167</v>
       </c>
     </row>
     <row r="159" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
-        <v>213</v>
+        <v>399</v>
       </c>
       <c r="B159" t="s">
-        <v>55</v>
+        <v>40</v>
       </c>
       <c r="C159" s="2" t="s">
-        <v>212</v>
+        <v>400</v>
+      </c>
+      <c r="E159" t="s">
+        <v>14</v>
+      </c>
+      <c r="F159">
+        <v>2000</v>
+      </c>
+      <c r="G159">
+        <v>2014</v>
       </c>
       <c r="H159" t="s">
-        <v>16</v>
+        <v>348</v>
       </c>
       <c r="I159" t="s">
-        <v>20</v>
+        <v>349</v>
+      </c>
+      <c r="J159" s="2" t="s">
+        <v>402</v>
+      </c>
+      <c r="N159" s="2" t="s">
+        <v>401</v>
       </c>
     </row>
     <row r="160" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
-        <v>395</v>
+        <v>213</v>
       </c>
       <c r="B160" t="s">
-        <v>25</v>
+        <v>55</v>
       </c>
       <c r="C160" s="2" t="s">
-        <v>394</v>
-      </c>
-      <c r="D160" t="s">
-        <v>396</v>
-      </c>
-      <c r="E160" t="s">
-        <v>111</v>
-      </c>
-      <c r="F160">
-        <v>1986</v>
-      </c>
-      <c r="G160">
-        <v>2015</v>
+        <v>212</v>
       </c>
       <c r="H160" t="s">
-        <v>367</v>
+        <v>16</v>
       </c>
       <c r="I160" t="s">
-        <v>398</v>
-      </c>
-      <c r="J160" s="2" t="s">
-        <v>397</v>
+        <v>20</v>
       </c>
     </row>
     <row r="161" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
-        <v>323</v>
+        <v>395</v>
       </c>
       <c r="B161" t="s">
         <v>25</v>
       </c>
       <c r="C161" s="2" t="s">
-        <v>324</v>
+        <v>394</v>
+      </c>
+      <c r="D161" t="s">
+        <v>396</v>
       </c>
       <c r="E161" t="s">
-        <v>325</v>
+        <v>111</v>
       </c>
       <c r="F161">
-        <v>1942</v>
+        <v>1986</v>
+      </c>
+      <c r="G161">
+        <v>2015</v>
       </c>
       <c r="H161" t="s">
-        <v>16</v>
+        <v>367</v>
       </c>
       <c r="I161" t="s">
-        <v>20</v>
+        <v>398</v>
+      </c>
+      <c r="J161" s="2" t="s">
+        <v>397</v>
       </c>
     </row>
     <row r="162" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
-        <v>273</v>
+        <v>323</v>
       </c>
       <c r="B162" t="s">
-        <v>237</v>
+        <v>25</v>
       </c>
       <c r="C162" s="2" t="s">
-        <v>272</v>
+        <v>324</v>
+      </c>
+      <c r="E162" t="s">
+        <v>325</v>
       </c>
       <c r="F162">
-        <v>1996</v>
-      </c>
-      <c r="G162">
-        <v>2016</v>
+        <v>1942</v>
       </c>
       <c r="H162" t="s">
         <v>16</v>
@@ -5555,91 +5576,91 @@
     </row>
     <row r="163" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
-        <v>508</v>
+        <v>273</v>
       </c>
       <c r="B163" t="s">
-        <v>40</v>
+        <v>237</v>
       </c>
       <c r="C163" s="2" t="s">
-        <v>509</v>
-      </c>
-      <c r="D163" t="s">
-        <v>511</v>
-      </c>
-      <c r="E163" t="s">
-        <v>510</v>
+        <v>272</v>
       </c>
       <c r="F163">
-        <v>1989</v>
+        <v>1996</v>
       </c>
       <c r="G163">
-        <v>2009</v>
+        <v>2016</v>
       </c>
       <c r="H163" t="s">
-        <v>348</v>
+        <v>16</v>
       </c>
       <c r="I163" t="s">
-        <v>349</v>
-      </c>
-      <c r="P163" s="2" t="s">
-        <v>512</v>
+        <v>20</v>
       </c>
     </row>
     <row r="164" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
-        <v>66</v>
+        <v>508</v>
       </c>
       <c r="B164" t="s">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="C164" s="2" t="s">
-        <v>67</v>
+        <v>509</v>
+      </c>
+      <c r="D164" t="s">
+        <v>511</v>
+      </c>
+      <c r="E164" t="s">
+        <v>510</v>
+      </c>
+      <c r="F164">
+        <v>1989</v>
+      </c>
+      <c r="G164">
+        <v>2009</v>
+      </c>
+      <c r="H164" t="s">
+        <v>348</v>
+      </c>
+      <c r="I164" t="s">
+        <v>349</v>
+      </c>
+      <c r="P164" s="2" t="s">
+        <v>512</v>
       </c>
     </row>
     <row r="165" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
-        <v>500</v>
+        <v>66</v>
       </c>
       <c r="B165" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="C165" s="2" t="s">
-        <v>499</v>
-      </c>
-      <c r="D165" t="s">
-        <v>501</v>
-      </c>
-      <c r="E165" t="s">
-        <v>14</v>
-      </c>
-      <c r="F165">
-        <v>1946</v>
-      </c>
-      <c r="G165">
-        <v>2015</v>
-      </c>
-      <c r="H165" t="s">
-        <v>348</v>
-      </c>
-      <c r="I165" t="s">
-        <v>349</v>
+        <v>67</v>
       </c>
     </row>
     <row r="166" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
-        <v>383</v>
+        <v>500</v>
       </c>
       <c r="B166" t="s">
         <v>40</v>
       </c>
       <c r="C166" s="2" t="s">
-        <v>384</v>
+        <v>499</v>
+      </c>
+      <c r="D166" t="s">
+        <v>501</v>
       </c>
       <c r="E166" t="s">
-        <v>386</v>
+        <v>14</v>
       </c>
       <c r="F166">
-        <v>1951</v>
+        <v>1946</v>
+      </c>
+      <c r="G166">
+        <v>2015</v>
       </c>
       <c r="H166" t="s">
         <v>348</v>
@@ -5647,178 +5668,181 @@
       <c r="I166" t="s">
         <v>349</v>
       </c>
-      <c r="N166" s="2" t="s">
-        <v>385</v>
-      </c>
     </row>
     <row r="167" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
-        <v>139</v>
+        <v>383</v>
       </c>
       <c r="B167" t="s">
         <v>40</v>
       </c>
       <c r="C167" s="2" t="s">
-        <v>140</v>
+        <v>384</v>
+      </c>
+      <c r="E167" t="s">
+        <v>386</v>
+      </c>
+      <c r="F167">
+        <v>1951</v>
+      </c>
+      <c r="H167" t="s">
+        <v>348</v>
+      </c>
+      <c r="I167" t="s">
+        <v>349</v>
+      </c>
+      <c r="N167" s="2" t="s">
+        <v>385</v>
       </c>
     </row>
     <row r="168" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
-        <v>329</v>
+        <v>139</v>
       </c>
       <c r="B168" t="s">
-        <v>165</v>
+        <v>40</v>
       </c>
       <c r="C168" s="2" t="s">
-        <v>328</v>
-      </c>
-      <c r="E168" t="s">
-        <v>34</v>
-      </c>
-      <c r="F168">
-        <v>1789</v>
-      </c>
-      <c r="H168" t="s">
-        <v>16</v>
-      </c>
-      <c r="I168" t="s">
-        <v>20</v>
+        <v>140</v>
       </c>
     </row>
     <row r="169" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
-        <v>172</v>
+        <v>329</v>
       </c>
       <c r="B169" t="s">
-        <v>60</v>
+        <v>165</v>
       </c>
       <c r="C169" s="2" t="s">
-        <v>171</v>
+        <v>328</v>
+      </c>
+      <c r="E169" t="s">
+        <v>34</v>
+      </c>
+      <c r="F169">
+        <v>1789</v>
+      </c>
+      <c r="H169" t="s">
+        <v>16</v>
+      </c>
+      <c r="I169" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="170" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
-        <v>217</v>
+        <v>172</v>
       </c>
       <c r="B170" t="s">
         <v>60</v>
       </c>
       <c r="C170" s="2" t="s">
-        <v>216</v>
-      </c>
-      <c r="E170" t="s">
-        <v>14</v>
-      </c>
-      <c r="F170">
-        <v>1900</v>
-      </c>
-      <c r="H170" t="s">
-        <v>16</v>
-      </c>
-      <c r="I170" t="s">
-        <v>20</v>
+        <v>171</v>
       </c>
     </row>
     <row r="171" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
-        <v>132</v>
+        <v>217</v>
       </c>
       <c r="B171" t="s">
-        <v>259</v>
+        <v>60</v>
       </c>
       <c r="C171" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="Q171" t="s">
-        <v>17</v>
+        <v>216</v>
+      </c>
+      <c r="E171" t="s">
+        <v>14</v>
+      </c>
+      <c r="F171">
+        <v>1900</v>
+      </c>
+      <c r="H171" t="s">
+        <v>16</v>
+      </c>
+      <c r="I171" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="172" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
-        <v>182</v>
+        <v>132</v>
       </c>
       <c r="B172" t="s">
-        <v>165</v>
+        <v>259</v>
       </c>
       <c r="C172" s="2" t="s">
-        <v>181</v>
+        <v>133</v>
+      </c>
+      <c r="Q172" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="173" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
-        <v>423</v>
+        <v>182</v>
       </c>
       <c r="B173" t="s">
-        <v>86</v>
+        <v>165</v>
       </c>
       <c r="C173" s="2" t="s">
-        <v>424</v>
-      </c>
-      <c r="E173" t="s">
-        <v>34</v>
-      </c>
-      <c r="F173">
-        <v>1996</v>
-      </c>
-      <c r="G173">
-        <v>2016</v>
-      </c>
-      <c r="H173" t="s">
-        <v>348</v>
-      </c>
-      <c r="I173" t="s">
-        <v>425</v>
+        <v>181</v>
       </c>
     </row>
     <row r="174" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
-        <v>115</v>
+        <v>423</v>
       </c>
       <c r="B174" t="s">
-        <v>128</v>
+        <v>86</v>
       </c>
       <c r="C174" s="2" t="s">
-        <v>116</v>
+        <v>424</v>
+      </c>
+      <c r="E174" t="s">
+        <v>34</v>
+      </c>
+      <c r="F174">
+        <v>1996</v>
+      </c>
+      <c r="G174">
+        <v>2016</v>
+      </c>
+      <c r="H174" t="s">
+        <v>348</v>
+      </c>
+      <c r="I174" t="s">
+        <v>425</v>
       </c>
     </row>
     <row r="175" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
-        <v>263</v>
+        <v>115</v>
       </c>
       <c r="B175" t="s">
-        <v>250</v>
+        <v>128</v>
       </c>
       <c r="C175" s="2" t="s">
-        <v>264</v>
-      </c>
-      <c r="E175" t="s">
-        <v>265</v>
-      </c>
-      <c r="F175">
-        <v>1500</v>
-      </c>
-      <c r="G175">
-        <v>2000</v>
-      </c>
-      <c r="H175" t="s">
-        <v>16</v>
-      </c>
-      <c r="I175" t="s">
-        <v>20</v>
+        <v>116</v>
       </c>
     </row>
     <row r="176" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
-        <v>221</v>
+        <v>263</v>
       </c>
       <c r="B176" t="s">
-        <v>86</v>
+        <v>250</v>
       </c>
       <c r="C176" s="2" t="s">
-        <v>220</v>
+        <v>264</v>
+      </c>
+      <c r="E176" t="s">
+        <v>265</v>
       </c>
       <c r="F176">
-        <v>2013</v>
+        <v>1500</v>
+      </c>
+      <c r="G176">
+        <v>2000</v>
       </c>
       <c r="H176" t="s">
         <v>16</v>
@@ -5829,22 +5853,16 @@
     </row>
     <row r="177" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
-        <v>13</v>
+        <v>221</v>
       </c>
       <c r="B177" t="s">
-        <v>25</v>
+        <v>86</v>
       </c>
       <c r="C177" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="D177" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="E177" t="s">
-        <v>14</v>
+        <v>220</v>
       </c>
       <c r="F177">
-        <v>1981</v>
+        <v>2013</v>
       </c>
       <c r="H177" t="s">
         <v>16</v>
@@ -5855,13 +5873,22 @@
     </row>
     <row r="178" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
-        <v>283</v>
+        <v>13</v>
       </c>
       <c r="B178" t="s">
-        <v>124</v>
+        <v>25</v>
       </c>
       <c r="C178" s="2" t="s">
-        <v>284</v>
+        <v>38</v>
+      </c>
+      <c r="D178" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E178" t="s">
+        <v>14</v>
+      </c>
+      <c r="F178">
+        <v>1981</v>
       </c>
       <c r="H178" t="s">
         <v>16</v>
@@ -5870,8 +5897,25 @@
         <v>20</v>
       </c>
     </row>
+    <row r="179" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A179" t="s">
+        <v>283</v>
+      </c>
+      <c r="B179" t="s">
+        <v>124</v>
+      </c>
+      <c r="C179" s="2" t="s">
+        <v>284</v>
+      </c>
+      <c r="H179" t="s">
+        <v>16</v>
+      </c>
+      <c r="I179" t="s">
+        <v>20</v>
+      </c>
+    </row>
   </sheetData>
-  <sortState ref="A2:Q178">
+  <sortState ref="A2:Q179">
     <sortCondition ref="A2"/>
   </sortState>
   <hyperlinks>
@@ -5881,7 +5925,7 @@
     <hyperlink ref="C11" r:id="rId4"/>
     <hyperlink ref="C105" r:id="rId5"/>
     <hyperlink ref="C127" r:id="rId6"/>
-    <hyperlink ref="C177" r:id="rId7"/>
+    <hyperlink ref="C178" r:id="rId7"/>
     <hyperlink ref="C40" r:id="rId8"/>
     <hyperlink ref="C33" r:id="rId9"/>
     <hyperlink ref="C57" r:id="rId10"/>
@@ -5895,7 +5939,7 @@
     <hyperlink ref="C48" r:id="rId18"/>
     <hyperlink ref="C82" r:id="rId19"/>
     <hyperlink ref="C17" r:id="rId20"/>
-    <hyperlink ref="C164" r:id="rId21"/>
+    <hyperlink ref="C165" r:id="rId21"/>
     <hyperlink ref="C8" r:id="rId22"/>
     <hyperlink ref="C44" r:id="rId23"/>
     <hyperlink ref="C61" r:id="rId24"/>
@@ -5912,7 +5956,7 @@
     <hyperlink ref="C18" r:id="rId35"/>
     <hyperlink ref="C152" r:id="rId36"/>
     <hyperlink ref="C16" r:id="rId37"/>
-    <hyperlink ref="C174" r:id="rId38"/>
+    <hyperlink ref="C175" r:id="rId38"/>
     <hyperlink ref="C96" r:id="rId39"/>
     <hyperlink ref="C65" r:id="rId40"/>
     <hyperlink ref="C134" r:id="rId41"/>
@@ -5920,10 +5964,10 @@
     <hyperlink ref="C59" r:id="rId43"/>
     <hyperlink ref="C26" r:id="rId44"/>
     <hyperlink ref="C123" r:id="rId45"/>
-    <hyperlink ref="C171" r:id="rId46"/>
+    <hyperlink ref="C172" r:id="rId46"/>
     <hyperlink ref="C30" r:id="rId47" display="http://comparativeconstitutionsproject.org/"/>
     <hyperlink ref="C120" r:id="rId48"/>
-    <hyperlink ref="C167" r:id="rId49"/>
+    <hyperlink ref="C168" r:id="rId49"/>
     <hyperlink ref="C138" r:id="rId50"/>
     <hyperlink ref="C132" r:id="rId51"/>
     <hyperlink ref="C25" r:id="rId52"/>
@@ -5938,14 +5982,14 @@
     <hyperlink ref="C156" r:id="rId61"/>
     <hyperlink ref="C9" r:id="rId62"/>
     <hyperlink ref="C36" r:id="rId63"/>
-    <hyperlink ref="C157" r:id="rId64"/>
+    <hyperlink ref="C158" r:id="rId64"/>
     <hyperlink ref="C15" r:id="rId65"/>
-    <hyperlink ref="C169" r:id="rId66"/>
+    <hyperlink ref="C170" r:id="rId66"/>
     <hyperlink ref="C28" r:id="rId67"/>
     <hyperlink ref="C27" r:id="rId68"/>
     <hyperlink ref="C29" r:id="rId69"/>
     <hyperlink ref="C60" r:id="rId70"/>
-    <hyperlink ref="C172" r:id="rId71"/>
+    <hyperlink ref="C173" r:id="rId71"/>
     <hyperlink ref="C31" r:id="rId72"/>
     <hyperlink ref="C128" r:id="rId73"/>
     <hyperlink ref="C35" r:id="rId74"/>
@@ -5959,11 +6003,11 @@
     <hyperlink ref="C13" r:id="rId82"/>
     <hyperlink ref="C119" r:id="rId83"/>
     <hyperlink ref="C130" r:id="rId84"/>
-    <hyperlink ref="C159" r:id="rId85"/>
+    <hyperlink ref="C160" r:id="rId85"/>
     <hyperlink ref="C41" r:id="rId86"/>
-    <hyperlink ref="C170" r:id="rId87"/>
+    <hyperlink ref="C171" r:id="rId87"/>
     <hyperlink ref="C51" r:id="rId88"/>
-    <hyperlink ref="C176" r:id="rId89"/>
+    <hyperlink ref="C177" r:id="rId89"/>
     <hyperlink ref="C106" r:id="rId90"/>
     <hyperlink ref="C73" r:id="rId91"/>
     <hyperlink ref="C107" r:id="rId92"/>
@@ -5986,15 +6030,15 @@
     <hyperlink ref="C148" r:id="rId109"/>
     <hyperlink ref="C14" r:id="rId110"/>
     <hyperlink ref="C4" r:id="rId111"/>
-    <hyperlink ref="C175" r:id="rId112"/>
+    <hyperlink ref="C176" r:id="rId112"/>
     <hyperlink ref="C100" r:id="rId113"/>
     <hyperlink ref="C95" r:id="rId114"/>
-    <hyperlink ref="C162" r:id="rId115"/>
+    <hyperlink ref="C163" r:id="rId115"/>
     <hyperlink ref="C142" r:id="rId116"/>
     <hyperlink ref="C71" r:id="rId117"/>
     <hyperlink ref="C109" r:id="rId118"/>
     <hyperlink ref="C84" r:id="rId119"/>
-    <hyperlink ref="C178" r:id="rId120"/>
+    <hyperlink ref="C179" r:id="rId120"/>
     <hyperlink ref="C74" r:id="rId121"/>
     <hyperlink ref="C140" r:id="rId122"/>
     <hyperlink ref="C116" r:id="rId123"/>
@@ -6010,9 +6054,9 @@
     <hyperlink ref="C136" r:id="rId133"/>
     <hyperlink ref="C135" r:id="rId134"/>
     <hyperlink ref="C137" r:id="rId135"/>
-    <hyperlink ref="C161" r:id="rId136"/>
+    <hyperlink ref="C162" r:id="rId136"/>
     <hyperlink ref="C153" r:id="rId137"/>
-    <hyperlink ref="C168" r:id="rId138"/>
+    <hyperlink ref="C169" r:id="rId138"/>
     <hyperlink ref="C43" r:id="rId139"/>
     <hyperlink ref="C99" r:id="rId140"/>
     <hyperlink ref="J2" r:id="rId141"/>
@@ -6029,16 +6073,16 @@
     <hyperlink ref="M8" r:id="rId152"/>
     <hyperlink ref="L8" r:id="rId153"/>
     <hyperlink ref="J8" r:id="rId154"/>
-    <hyperlink ref="C166" r:id="rId155"/>
-    <hyperlink ref="N166" r:id="rId156"/>
+    <hyperlink ref="C167" r:id="rId155"/>
+    <hyperlink ref="N167" r:id="rId156"/>
     <hyperlink ref="C22" r:id="rId157"/>
     <hyperlink ref="N22" r:id="rId158"/>
     <hyperlink ref="C70" r:id="rId159"/>
-    <hyperlink ref="C160" r:id="rId160"/>
-    <hyperlink ref="J160" r:id="rId161"/>
-    <hyperlink ref="C158" r:id="rId162"/>
-    <hyperlink ref="N158" r:id="rId163"/>
-    <hyperlink ref="J158" r:id="rId164"/>
+    <hyperlink ref="C161" r:id="rId160"/>
+    <hyperlink ref="J161" r:id="rId161"/>
+    <hyperlink ref="C159" r:id="rId162"/>
+    <hyperlink ref="N159" r:id="rId163"/>
+    <hyperlink ref="J159" r:id="rId164"/>
     <hyperlink ref="C103" r:id="rId165"/>
     <hyperlink ref="C101" r:id="rId166"/>
     <hyperlink ref="C46" r:id="rId167"/>
@@ -6048,7 +6092,7 @@
     <hyperlink ref="N111" r:id="rId171"/>
     <hyperlink ref="C85" r:id="rId172"/>
     <hyperlink ref="K85" r:id="rId173"/>
-    <hyperlink ref="C173" r:id="rId174"/>
+    <hyperlink ref="C174" r:id="rId174"/>
     <hyperlink ref="C131" r:id="rId175"/>
     <hyperlink ref="K131" r:id="rId176"/>
     <hyperlink ref="L9" r:id="rId177"/>
@@ -6094,14 +6138,14 @@
     <hyperlink ref="M47" r:id="rId217"/>
     <hyperlink ref="N47" r:id="rId218"/>
     <hyperlink ref="C23" r:id="rId219"/>
-    <hyperlink ref="C165" r:id="rId220"/>
+    <hyperlink ref="C166" r:id="rId220"/>
     <hyperlink ref="C39" r:id="rId221"/>
     <hyperlink ref="J39" r:id="rId222"/>
     <hyperlink ref="N39" r:id="rId223"/>
     <hyperlink ref="L39" r:id="rId224"/>
     <hyperlink ref="K39" r:id="rId225"/>
-    <hyperlink ref="C163" r:id="rId226"/>
-    <hyperlink ref="P163" r:id="rId227"/>
+    <hyperlink ref="C164" r:id="rId226"/>
+    <hyperlink ref="P164" r:id="rId227"/>
     <hyperlink ref="C113" r:id="rId228"/>
     <hyperlink ref="C129" r:id="rId229"/>
     <hyperlink ref="P129" r:id="rId230"/>
@@ -6119,6 +6163,8 @@
     <hyperlink ref="C125" r:id="rId242"/>
     <hyperlink ref="N125" r:id="rId243"/>
     <hyperlink ref="J125" r:id="rId244"/>
+    <hyperlink ref="C157" r:id="rId245"/>
+    <hyperlink ref="J157" r:id="rId246"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
add 'Nonviolent & Violent Campaigns and Outcomes'
</commit_message>
<xml_diff>
--- a/PolData.xlsx
+++ b/PolData.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="998" uniqueCount="549">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1005" uniqueCount="552">
   <si>
     <t>name</t>
   </si>
@@ -1674,6 +1674,15 @@
   </si>
   <si>
     <t>http://americanideologyproject.com/estimates/estimates2015/codebook.pdf</t>
+  </si>
+  <si>
+    <t>Nonviolent &amp; Violent Campaigns and Outcomes</t>
+  </si>
+  <si>
+    <t>https://www.du.edu/korbel/sie/research/chenow_navco_data.html</t>
+  </si>
+  <si>
+    <t>Nonviolent campaigns, violent campaigns</t>
   </si>
 </sst>
 </file>
@@ -2013,10 +2022,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q179"/>
+  <dimension ref="A1:Q180"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A153" workbookViewId="0">
-      <selection activeCell="A157" sqref="A157"/>
+    <sheetView tabSelected="1" topLeftCell="A99" workbookViewId="0">
+      <selection activeCell="A118" sqref="A118"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4586,208 +4595,211 @@
     </row>
     <row r="118" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>365</v>
+        <v>549</v>
       </c>
       <c r="B118" t="s">
-        <v>128</v>
+        <v>40</v>
       </c>
       <c r="C118" s="2" t="s">
-        <v>364</v>
+        <v>550</v>
       </c>
       <c r="D118" t="s">
-        <v>370</v>
+        <v>551</v>
       </c>
       <c r="E118" t="s">
-        <v>366</v>
+        <v>14</v>
       </c>
       <c r="F118">
-        <v>1906</v>
+        <v>1900</v>
       </c>
       <c r="G118">
-        <v>2013</v>
+        <v>2011</v>
       </c>
       <c r="H118" t="s">
-        <v>367</v>
+        <v>348</v>
       </c>
       <c r="I118" t="s">
-        <v>368</v>
-      </c>
-      <c r="Q118" t="s">
-        <v>369</v>
+        <v>248</v>
       </c>
     </row>
     <row r="119" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>208</v>
+        <v>365</v>
       </c>
       <c r="B119" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="C119" s="2" t="s">
-        <v>209</v>
+        <v>364</v>
+      </c>
+      <c r="D119" t="s">
+        <v>370</v>
+      </c>
+      <c r="E119" t="s">
+        <v>366</v>
       </c>
       <c r="F119">
-        <v>1932</v>
+        <v>1906</v>
       </c>
       <c r="G119">
-        <v>2014</v>
+        <v>2013</v>
       </c>
       <c r="H119" t="s">
-        <v>16</v>
+        <v>367</v>
       </c>
       <c r="I119" t="s">
-        <v>20</v>
+        <v>368</v>
+      </c>
+      <c r="Q119" t="s">
+        <v>369</v>
       </c>
     </row>
     <row r="120" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>137</v>
+        <v>208</v>
       </c>
       <c r="B120" t="s">
-        <v>259</v>
+        <v>124</v>
       </c>
       <c r="C120" s="2" t="s">
-        <v>138</v>
+        <v>209</v>
+      </c>
+      <c r="F120">
+        <v>1932</v>
+      </c>
+      <c r="G120">
+        <v>2014</v>
+      </c>
+      <c r="H120" t="s">
+        <v>16</v>
+      </c>
+      <c r="I120" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="121" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>155</v>
+        <v>137</v>
       </c>
       <c r="B121" t="s">
         <v>259</v>
       </c>
       <c r="C121" s="2" t="s">
-        <v>154</v>
+        <v>138</v>
       </c>
     </row>
     <row r="122" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>57</v>
+        <v>155</v>
       </c>
       <c r="B122" t="s">
-        <v>128</v>
+        <v>259</v>
       </c>
       <c r="C122" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="Q122" t="s">
-        <v>17</v>
+        <v>154</v>
       </c>
     </row>
     <row r="123" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>129</v>
+        <v>57</v>
       </c>
       <c r="B123" t="s">
-        <v>259</v>
+        <v>128</v>
       </c>
       <c r="C123" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="E123" t="s">
-        <v>131</v>
-      </c>
-      <c r="F123">
-        <v>1945</v>
-      </c>
-      <c r="G123">
-        <v>2008</v>
-      </c>
-      <c r="I123" t="s">
-        <v>20</v>
+        <v>58</v>
+      </c>
+      <c r="Q123" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="124" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>148</v>
+        <v>129</v>
       </c>
       <c r="B124" t="s">
-        <v>128</v>
+        <v>259</v>
       </c>
       <c r="C124" s="2" t="s">
-        <v>147</v>
+        <v>130</v>
+      </c>
+      <c r="E124" t="s">
+        <v>131</v>
+      </c>
+      <c r="F124">
+        <v>1945</v>
+      </c>
+      <c r="G124">
+        <v>2008</v>
+      </c>
+      <c r="I124" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="125" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>541</v>
+        <v>148</v>
       </c>
       <c r="B125" t="s">
-        <v>40</v>
+        <v>128</v>
       </c>
       <c r="C125" s="2" t="s">
-        <v>540</v>
-      </c>
-      <c r="D125" t="s">
-        <v>542</v>
-      </c>
-      <c r="E125" t="s">
-        <v>14</v>
-      </c>
-      <c r="F125">
-        <v>1989</v>
-      </c>
-      <c r="G125">
-        <v>2012</v>
-      </c>
-      <c r="H125" t="s">
-        <v>348</v>
-      </c>
-      <c r="I125" t="s">
-        <v>349</v>
-      </c>
-      <c r="J125" s="2" t="s">
-        <v>544</v>
-      </c>
-      <c r="N125" s="2" t="s">
-        <v>543</v>
+        <v>147</v>
       </c>
     </row>
     <row r="126" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>233</v>
+        <v>541</v>
       </c>
       <c r="B126" t="s">
-        <v>165</v>
+        <v>40</v>
       </c>
       <c r="C126" s="2" t="s">
-        <v>234</v>
+        <v>540</v>
+      </c>
+      <c r="D126" t="s">
+        <v>542</v>
       </c>
       <c r="E126" t="s">
         <v>14</v>
       </c>
       <c r="F126">
+        <v>1989</v>
+      </c>
+      <c r="G126">
         <v>2012</v>
       </c>
-      <c r="G126">
-        <v>2016</v>
-      </c>
       <c r="H126" t="s">
-        <v>16</v>
+        <v>348</v>
       </c>
       <c r="I126" t="s">
-        <v>20</v>
+        <v>349</v>
+      </c>
+      <c r="J126" s="2" t="s">
+        <v>544</v>
+      </c>
+      <c r="N126" s="2" t="s">
+        <v>543</v>
       </c>
     </row>
     <row r="127" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>35</v>
+        <v>233</v>
       </c>
       <c r="B127" t="s">
-        <v>25</v>
+        <v>165</v>
       </c>
       <c r="C127" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="D127" t="s">
-        <v>37</v>
+        <v>234</v>
       </c>
       <c r="E127" t="s">
         <v>14</v>
       </c>
       <c r="F127">
-        <v>2001</v>
+        <v>2012</v>
+      </c>
+      <c r="G127">
+        <v>2016</v>
       </c>
       <c r="H127" t="s">
         <v>16</v>
@@ -4798,180 +4810,180 @@
     </row>
     <row r="128" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>185</v>
+        <v>35</v>
       </c>
       <c r="B128" t="s">
-        <v>128</v>
+        <v>25</v>
       </c>
       <c r="C128" s="2" t="s">
-        <v>186</v>
+        <v>36</v>
+      </c>
+      <c r="D128" t="s">
+        <v>37</v>
+      </c>
+      <c r="E128" t="s">
+        <v>14</v>
+      </c>
+      <c r="F128">
+        <v>2001</v>
+      </c>
+      <c r="H128" t="s">
+        <v>16</v>
+      </c>
+      <c r="I128" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="129" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>516</v>
+        <v>185</v>
       </c>
       <c r="B129" t="s">
-        <v>40</v>
+        <v>128</v>
       </c>
       <c r="C129" s="2" t="s">
-        <v>517</v>
-      </c>
-      <c r="D129" t="s">
-        <v>518</v>
-      </c>
-      <c r="E129" t="s">
-        <v>14</v>
-      </c>
-      <c r="F129">
-        <v>1975</v>
-      </c>
-      <c r="G129">
-        <v>2011</v>
-      </c>
-      <c r="H129" t="s">
-        <v>348</v>
-      </c>
-      <c r="I129" t="s">
-        <v>349</v>
-      </c>
-      <c r="P129" s="2" t="s">
-        <v>519</v>
+        <v>186</v>
       </c>
     </row>
     <row r="130" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
-        <v>210</v>
+        <v>516</v>
       </c>
       <c r="B130" t="s">
         <v>40</v>
       </c>
       <c r="C130" s="2" t="s">
-        <v>211</v>
+        <v>517</v>
+      </c>
+      <c r="D130" t="s">
+        <v>518</v>
+      </c>
+      <c r="E130" t="s">
+        <v>14</v>
       </c>
       <c r="F130">
-        <v>1976</v>
+        <v>1975</v>
       </c>
       <c r="G130">
-        <v>2016</v>
+        <v>2011</v>
       </c>
       <c r="H130" t="s">
-        <v>16</v>
+        <v>348</v>
       </c>
       <c r="I130" t="s">
-        <v>20</v>
+        <v>349</v>
+      </c>
+      <c r="P130" s="2" t="s">
+        <v>519</v>
       </c>
     </row>
     <row r="131" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>426</v>
+        <v>210</v>
       </c>
       <c r="B131" t="s">
-        <v>86</v>
+        <v>40</v>
       </c>
       <c r="C131" s="2" t="s">
-        <v>427</v>
-      </c>
-      <c r="E131" t="s">
-        <v>34</v>
+        <v>211</v>
       </c>
       <c r="F131">
-        <v>2015</v>
+        <v>1976</v>
       </c>
       <c r="G131">
         <v>2016</v>
       </c>
       <c r="H131" t="s">
-        <v>348</v>
+        <v>16</v>
       </c>
       <c r="I131" t="s">
-        <v>349</v>
-      </c>
-      <c r="K131" s="2" t="s">
-        <v>428</v>
+        <v>20</v>
       </c>
     </row>
     <row r="132" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>144</v>
+        <v>426</v>
       </c>
       <c r="B132" t="s">
-        <v>60</v>
+        <v>86</v>
       </c>
       <c r="C132" s="2" t="s">
-        <v>143</v>
+        <v>427</v>
+      </c>
+      <c r="E132" t="s">
+        <v>34</v>
       </c>
       <c r="F132">
-        <v>1800</v>
+        <v>2015</v>
       </c>
       <c r="G132">
-        <v>2013</v>
+        <v>2016</v>
+      </c>
+      <c r="H132" t="s">
+        <v>348</v>
+      </c>
+      <c r="I132" t="s">
+        <v>349</v>
+      </c>
+      <c r="K132" s="2" t="s">
+        <v>428</v>
       </c>
     </row>
     <row r="133" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
-        <v>472</v>
+        <v>144</v>
       </c>
       <c r="B133" t="s">
-        <v>25</v>
+        <v>60</v>
       </c>
       <c r="C133" s="2" t="s">
-        <v>473</v>
-      </c>
-      <c r="D133" t="s">
-        <v>474</v>
-      </c>
-      <c r="E133" t="s">
-        <v>112</v>
+        <v>143</v>
       </c>
       <c r="F133">
-        <v>1943</v>
-      </c>
-      <c r="H133" t="s">
-        <v>348</v>
-      </c>
-      <c r="I133" t="s">
-        <v>349</v>
-      </c>
-      <c r="N133" s="2" t="s">
-        <v>475</v>
+        <v>1800</v>
+      </c>
+      <c r="G133">
+        <v>2013</v>
       </c>
     </row>
     <row r="134" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
-        <v>122</v>
+        <v>472</v>
       </c>
       <c r="B134" t="s">
-        <v>259</v>
+        <v>25</v>
       </c>
       <c r="C134" s="2" t="s">
-        <v>121</v>
+        <v>473</v>
+      </c>
+      <c r="D134" t="s">
+        <v>474</v>
+      </c>
+      <c r="E134" t="s">
+        <v>112</v>
+      </c>
+      <c r="F134">
+        <v>1943</v>
+      </c>
+      <c r="H134" t="s">
+        <v>348</v>
       </c>
       <c r="I134" t="s">
-        <v>20</v>
+        <v>349</v>
+      </c>
+      <c r="N134" s="2" t="s">
+        <v>475</v>
       </c>
     </row>
     <row r="135" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
-        <v>318</v>
+        <v>122</v>
       </c>
       <c r="B135" t="s">
-        <v>250</v>
+        <v>259</v>
       </c>
       <c r="C135" s="2" t="s">
-        <v>319</v>
-      </c>
-      <c r="E135" t="s">
-        <v>320</v>
-      </c>
-      <c r="F135">
-        <v>1975</v>
-      </c>
-      <c r="G135">
-        <v>1989</v>
-      </c>
-      <c r="H135" t="s">
-        <v>16</v>
+        <v>121</v>
       </c>
       <c r="I135" t="s">
         <v>20</v>
@@ -4979,22 +4991,22 @@
     </row>
     <row r="136" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="B136" t="s">
         <v>250</v>
       </c>
       <c r="C136" s="2" t="s">
-        <v>317</v>
+        <v>319</v>
       </c>
       <c r="E136" t="s">
-        <v>105</v>
+        <v>320</v>
       </c>
       <c r="F136">
-        <v>1950</v>
+        <v>1975</v>
       </c>
       <c r="G136">
-        <v>1996</v>
+        <v>1989</v>
       </c>
       <c r="H136" t="s">
         <v>16</v>
@@ -5005,19 +5017,22 @@
     </row>
     <row r="137" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
-        <v>322</v>
+        <v>316</v>
       </c>
       <c r="B137" t="s">
-        <v>25</v>
+        <v>250</v>
       </c>
       <c r="C137" s="2" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="E137" t="s">
-        <v>77</v>
+        <v>105</v>
       </c>
       <c r="F137">
-        <v>2010</v>
+        <v>1950</v>
+      </c>
+      <c r="G137">
+        <v>1996</v>
       </c>
       <c r="H137" t="s">
         <v>16</v>
@@ -5028,156 +5043,153 @@
     </row>
     <row r="138" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
-        <v>141</v>
+        <v>322</v>
       </c>
       <c r="B138" t="s">
-        <v>237</v>
+        <v>25</v>
       </c>
       <c r="C138" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="Q138" t="s">
-        <v>17</v>
+        <v>321</v>
+      </c>
+      <c r="E138" t="s">
+        <v>77</v>
+      </c>
+      <c r="F138">
+        <v>2010</v>
+      </c>
+      <c r="H138" t="s">
+        <v>16</v>
+      </c>
+      <c r="I138" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="139" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
-        <v>308</v>
+        <v>141</v>
       </c>
       <c r="B139" t="s">
-        <v>250</v>
+        <v>237</v>
       </c>
       <c r="C139" s="2" t="s">
-        <v>309</v>
-      </c>
-      <c r="E139" t="s">
-        <v>310</v>
-      </c>
-      <c r="F139">
-        <v>1950</v>
-      </c>
-      <c r="G139">
-        <v>2010</v>
-      </c>
-      <c r="H139" t="s">
-        <v>16</v>
-      </c>
-      <c r="I139" t="s">
-        <v>20</v>
+        <v>142</v>
+      </c>
+      <c r="Q139" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="140" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
-        <v>287</v>
+        <v>308</v>
       </c>
       <c r="B140" t="s">
-        <v>134</v>
+        <v>250</v>
       </c>
       <c r="C140" s="2" t="s">
-        <v>288</v>
+        <v>309</v>
+      </c>
+      <c r="E140" t="s">
+        <v>310</v>
       </c>
       <c r="F140">
-        <v>1990</v>
+        <v>1950</v>
       </c>
       <c r="G140">
-        <v>2008</v>
+        <v>2010</v>
+      </c>
+      <c r="H140" t="s">
+        <v>16</v>
+      </c>
+      <c r="I140" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="141" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
-        <v>526</v>
+        <v>287</v>
       </c>
       <c r="B141" t="s">
-        <v>40</v>
+        <v>134</v>
       </c>
       <c r="C141" s="2" t="s">
-        <v>527</v>
-      </c>
-      <c r="D141" t="s">
-        <v>528</v>
-      </c>
-      <c r="E141" t="s">
-        <v>14</v>
+        <v>288</v>
       </c>
       <c r="F141">
-        <v>1980</v>
+        <v>1990</v>
       </c>
       <c r="G141">
-        <v>2011</v>
-      </c>
-      <c r="H141" t="s">
-        <v>348</v>
-      </c>
-      <c r="I141" t="s">
-        <v>349</v>
-      </c>
-      <c r="J141" s="2" t="s">
-        <v>529</v>
-      </c>
-      <c r="L141" s="2" t="s">
-        <v>530</v>
+        <v>2008</v>
       </c>
     </row>
     <row r="142" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
-        <v>274</v>
+        <v>526</v>
       </c>
       <c r="B142" t="s">
-        <v>55</v>
+        <v>40</v>
       </c>
       <c r="C142" s="2" t="s">
-        <v>275</v>
+        <v>527</v>
+      </c>
+      <c r="D142" t="s">
+        <v>528</v>
+      </c>
+      <c r="E142" t="s">
+        <v>14</v>
+      </c>
+      <c r="F142">
+        <v>1980</v>
+      </c>
+      <c r="G142">
+        <v>2011</v>
       </c>
       <c r="H142" t="s">
-        <v>16</v>
+        <v>348</v>
       </c>
       <c r="I142" t="s">
-        <v>20</v>
+        <v>349</v>
+      </c>
+      <c r="J142" s="2" t="s">
+        <v>529</v>
+      </c>
+      <c r="L142" s="2" t="s">
+        <v>530</v>
       </c>
     </row>
     <row r="143" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
-        <v>157</v>
+        <v>274</v>
       </c>
       <c r="B143" t="s">
-        <v>128</v>
+        <v>55</v>
       </c>
       <c r="C143" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="Q143" t="s">
-        <v>18</v>
+        <v>275</v>
+      </c>
+      <c r="H143" t="s">
+        <v>16</v>
+      </c>
+      <c r="I143" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="144" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
-        <v>439</v>
+        <v>157</v>
       </c>
       <c r="B144" t="s">
-        <v>259</v>
+        <v>128</v>
       </c>
       <c r="C144" s="2" t="s">
-        <v>438</v>
-      </c>
-      <c r="H144" t="s">
-        <v>348</v>
-      </c>
-      <c r="I144" t="s">
-        <v>349</v>
-      </c>
-      <c r="J144" s="2" t="s">
-        <v>440</v>
-      </c>
-      <c r="K144" s="2" t="s">
-        <v>442</v>
-      </c>
-      <c r="L144" s="2" t="s">
-        <v>441</v>
+        <v>154</v>
+      </c>
+      <c r="Q144" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="145" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
-        <v>443</v>
+        <v>439</v>
       </c>
       <c r="B145" t="s">
         <v>259</v>
@@ -5185,15 +5197,6 @@
       <c r="C145" s="2" t="s">
         <v>438</v>
       </c>
-      <c r="D145" t="s">
-        <v>447</v>
-      </c>
-      <c r="F145">
-        <v>1990</v>
-      </c>
-      <c r="G145">
-        <v>2014</v>
-      </c>
       <c r="H145" t="s">
         <v>348</v>
       </c>
@@ -5201,87 +5204,99 @@
         <v>349</v>
       </c>
       <c r="J145" s="2" t="s">
-        <v>444</v>
+        <v>440</v>
       </c>
       <c r="K145" s="2" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
       <c r="L145" s="2" t="s">
-        <v>446</v>
+        <v>441</v>
       </c>
     </row>
     <row r="146" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
-        <v>194</v>
+        <v>443</v>
       </c>
       <c r="B146" t="s">
-        <v>99</v>
+        <v>259</v>
       </c>
       <c r="C146" s="2" t="s">
-        <v>193</v>
+        <v>438</v>
+      </c>
+      <c r="D146" t="s">
+        <v>447</v>
+      </c>
+      <c r="F146">
+        <v>1990</v>
+      </c>
+      <c r="G146">
+        <v>2014</v>
+      </c>
+      <c r="H146" t="s">
+        <v>348</v>
+      </c>
+      <c r="I146" t="s">
+        <v>349</v>
+      </c>
+      <c r="J146" s="2" t="s">
+        <v>444</v>
+      </c>
+      <c r="K146" s="2" t="s">
+        <v>445</v>
+      </c>
+      <c r="L146" s="2" t="s">
+        <v>446</v>
       </c>
     </row>
     <row r="147" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
-        <v>295</v>
+        <v>194</v>
       </c>
       <c r="B147" t="s">
-        <v>40</v>
+        <v>99</v>
       </c>
       <c r="C147" s="2" t="s">
-        <v>296</v>
-      </c>
-      <c r="E147" t="s">
-        <v>297</v>
-      </c>
-      <c r="F147">
-        <v>1990</v>
-      </c>
-      <c r="G147">
-        <v>2015</v>
-      </c>
-      <c r="H147" t="s">
-        <v>16</v>
-      </c>
-      <c r="I147" t="s">
-        <v>249</v>
+        <v>193</v>
       </c>
     </row>
     <row r="148" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
-        <v>256</v>
+        <v>295</v>
       </c>
       <c r="B148" t="s">
-        <v>250</v>
+        <v>40</v>
       </c>
       <c r="C148" s="2" t="s">
-        <v>257</v>
+        <v>296</v>
       </c>
       <c r="E148" t="s">
-        <v>258</v>
+        <v>297</v>
+      </c>
+      <c r="F148">
+        <v>1990</v>
+      </c>
+      <c r="G148">
+        <v>2015</v>
       </c>
       <c r="H148" t="s">
         <v>16</v>
       </c>
       <c r="I148" t="s">
-        <v>20</v>
+        <v>249</v>
       </c>
     </row>
     <row r="149" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
-        <v>227</v>
+        <v>256</v>
       </c>
       <c r="B149" t="s">
-        <v>40</v>
+        <v>250</v>
       </c>
       <c r="C149" s="2" t="s">
-        <v>225</v>
-      </c>
-      <c r="F149">
-        <v>1955</v>
-      </c>
-      <c r="G149">
-        <v>2016</v>
+        <v>257</v>
+      </c>
+      <c r="E149" t="s">
+        <v>258</v>
       </c>
       <c r="H149" t="s">
         <v>16</v>
@@ -5292,7 +5307,7 @@
     </row>
     <row r="150" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="B150" t="s">
         <v>40</v>
@@ -5301,7 +5316,7 @@
         <v>225</v>
       </c>
       <c r="F150">
-        <v>1995</v>
+        <v>1955</v>
       </c>
       <c r="G150">
         <v>2016</v>
@@ -5315,280 +5330,280 @@
     </row>
     <row r="151" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
-        <v>452</v>
+        <v>230</v>
       </c>
       <c r="B151" t="s">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="C151" s="2" t="s">
-        <v>453</v>
-      </c>
-      <c r="E151" t="s">
-        <v>9</v>
+        <v>225</v>
+      </c>
+      <c r="F151">
+        <v>1995</v>
+      </c>
+      <c r="G151">
+        <v>2016</v>
       </c>
       <c r="H151" t="s">
-        <v>348</v>
+        <v>16</v>
       </c>
       <c r="I151" t="s">
-        <v>435</v>
+        <v>20</v>
       </c>
     </row>
     <row r="152" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
-        <v>109</v>
+        <v>452</v>
       </c>
       <c r="B152" t="s">
         <v>25</v>
       </c>
       <c r="C152" s="2" t="s">
-        <v>110</v>
+        <v>453</v>
       </c>
       <c r="E152" t="s">
-        <v>111</v>
-      </c>
-      <c r="F152">
-        <v>1956</v>
+        <v>9</v>
+      </c>
+      <c r="H152" t="s">
+        <v>348</v>
+      </c>
+      <c r="I152" t="s">
+        <v>435</v>
       </c>
     </row>
     <row r="153" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
-        <v>326</v>
+        <v>109</v>
       </c>
       <c r="B153" t="s">
         <v>25</v>
       </c>
       <c r="C153" s="2" t="s">
-        <v>327</v>
+        <v>110</v>
       </c>
       <c r="E153" t="s">
         <v>111</v>
       </c>
       <c r="F153">
-        <v>1998</v>
-      </c>
-      <c r="H153" t="s">
-        <v>16</v>
-      </c>
-      <c r="I153" t="s">
-        <v>20</v>
+        <v>1956</v>
       </c>
     </row>
     <row r="154" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
-        <v>91</v>
+        <v>326</v>
       </c>
       <c r="B154" t="s">
         <v>25</v>
       </c>
       <c r="C154" s="2" t="s">
-        <v>93</v>
+        <v>327</v>
       </c>
       <c r="E154" t="s">
-        <v>92</v>
+        <v>111</v>
       </c>
       <c r="F154">
-        <v>1999</v>
+        <v>1998</v>
+      </c>
+      <c r="H154" t="s">
+        <v>16</v>
+      </c>
+      <c r="I154" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="155" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
-        <v>314</v>
+        <v>91</v>
       </c>
       <c r="B155" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="C155" s="2" t="s">
-        <v>313</v>
+        <v>93</v>
       </c>
       <c r="E155" t="s">
-        <v>315</v>
+        <v>92</v>
       </c>
       <c r="F155">
-        <v>1950</v>
-      </c>
-      <c r="G155">
-        <v>2004</v>
-      </c>
-      <c r="H155" t="s">
-        <v>16</v>
-      </c>
-      <c r="I155" t="s">
-        <v>20</v>
+        <v>1999</v>
       </c>
     </row>
     <row r="156" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
-        <v>161</v>
+        <v>314</v>
       </c>
       <c r="B156" t="s">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="C156" s="2" t="s">
-        <v>160</v>
+        <v>313</v>
+      </c>
+      <c r="E156" t="s">
+        <v>315</v>
+      </c>
+      <c r="F156">
+        <v>1950</v>
+      </c>
+      <c r="G156">
+        <v>2004</v>
+      </c>
+      <c r="H156" t="s">
+        <v>16</v>
+      </c>
+      <c r="I156" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="157" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
-        <v>545</v>
+        <v>161</v>
       </c>
       <c r="B157" t="s">
         <v>25</v>
       </c>
       <c r="C157" s="2" t="s">
-        <v>546</v>
-      </c>
-      <c r="D157" t="s">
-        <v>547</v>
-      </c>
-      <c r="E157" t="s">
-        <v>34</v>
-      </c>
-      <c r="F157">
-        <v>2000</v>
-      </c>
-      <c r="G157">
-        <v>2011</v>
-      </c>
-      <c r="H157" t="s">
-        <v>348</v>
-      </c>
-      <c r="I157" t="s">
-        <v>349</v>
-      </c>
-      <c r="J157" s="2" t="s">
-        <v>548</v>
+        <v>160</v>
       </c>
     </row>
     <row r="158" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
-        <v>168</v>
+        <v>545</v>
       </c>
       <c r="B158" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="C158" s="2" t="s">
-        <v>167</v>
+        <v>546</v>
+      </c>
+      <c r="D158" t="s">
+        <v>547</v>
+      </c>
+      <c r="E158" t="s">
+        <v>34</v>
+      </c>
+      <c r="F158">
+        <v>2000</v>
+      </c>
+      <c r="G158">
+        <v>2011</v>
+      </c>
+      <c r="H158" t="s">
+        <v>348</v>
+      </c>
+      <c r="I158" t="s">
+        <v>349</v>
+      </c>
+      <c r="J158" s="2" t="s">
+        <v>548</v>
       </c>
     </row>
     <row r="159" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
-        <v>399</v>
+        <v>168</v>
       </c>
       <c r="B159" t="s">
         <v>40</v>
       </c>
       <c r="C159" s="2" t="s">
-        <v>400</v>
-      </c>
-      <c r="E159" t="s">
-        <v>14</v>
-      </c>
-      <c r="F159">
-        <v>2000</v>
-      </c>
-      <c r="G159">
-        <v>2014</v>
-      </c>
-      <c r="H159" t="s">
-        <v>348</v>
-      </c>
-      <c r="I159" t="s">
-        <v>349</v>
-      </c>
-      <c r="J159" s="2" t="s">
-        <v>402</v>
-      </c>
-      <c r="N159" s="2" t="s">
-        <v>401</v>
+        <v>167</v>
       </c>
     </row>
     <row r="160" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
-        <v>213</v>
+        <v>399</v>
       </c>
       <c r="B160" t="s">
-        <v>55</v>
+        <v>40</v>
       </c>
       <c r="C160" s="2" t="s">
-        <v>212</v>
+        <v>400</v>
+      </c>
+      <c r="E160" t="s">
+        <v>14</v>
+      </c>
+      <c r="F160">
+        <v>2000</v>
+      </c>
+      <c r="G160">
+        <v>2014</v>
       </c>
       <c r="H160" t="s">
-        <v>16</v>
+        <v>348</v>
       </c>
       <c r="I160" t="s">
-        <v>20</v>
+        <v>349</v>
+      </c>
+      <c r="J160" s="2" t="s">
+        <v>402</v>
+      </c>
+      <c r="N160" s="2" t="s">
+        <v>401</v>
       </c>
     </row>
     <row r="161" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
-        <v>395</v>
+        <v>213</v>
       </c>
       <c r="B161" t="s">
-        <v>25</v>
+        <v>55</v>
       </c>
       <c r="C161" s="2" t="s">
-        <v>394</v>
-      </c>
-      <c r="D161" t="s">
-        <v>396</v>
-      </c>
-      <c r="E161" t="s">
-        <v>111</v>
-      </c>
-      <c r="F161">
-        <v>1986</v>
-      </c>
-      <c r="G161">
-        <v>2015</v>
+        <v>212</v>
       </c>
       <c r="H161" t="s">
-        <v>367</v>
+        <v>16</v>
       </c>
       <c r="I161" t="s">
-        <v>398</v>
-      </c>
-      <c r="J161" s="2" t="s">
-        <v>397</v>
+        <v>20</v>
       </c>
     </row>
     <row r="162" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
-        <v>323</v>
+        <v>395</v>
       </c>
       <c r="B162" t="s">
         <v>25</v>
       </c>
       <c r="C162" s="2" t="s">
-        <v>324</v>
+        <v>394</v>
+      </c>
+      <c r="D162" t="s">
+        <v>396</v>
       </c>
       <c r="E162" t="s">
-        <v>325</v>
+        <v>111</v>
       </c>
       <c r="F162">
-        <v>1942</v>
+        <v>1986</v>
+      </c>
+      <c r="G162">
+        <v>2015</v>
       </c>
       <c r="H162" t="s">
-        <v>16</v>
+        <v>367</v>
       </c>
       <c r="I162" t="s">
-        <v>20</v>
+        <v>398</v>
+      </c>
+      <c r="J162" s="2" t="s">
+        <v>397</v>
       </c>
     </row>
     <row r="163" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
-        <v>273</v>
+        <v>323</v>
       </c>
       <c r="B163" t="s">
-        <v>237</v>
+        <v>25</v>
       </c>
       <c r="C163" s="2" t="s">
-        <v>272</v>
+        <v>324</v>
+      </c>
+      <c r="E163" t="s">
+        <v>325</v>
       </c>
       <c r="F163">
-        <v>1996</v>
-      </c>
-      <c r="G163">
-        <v>2016</v>
+        <v>1942</v>
       </c>
       <c r="H163" t="s">
         <v>16</v>
@@ -5599,91 +5614,91 @@
     </row>
     <row r="164" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
-        <v>508</v>
+        <v>273</v>
       </c>
       <c r="B164" t="s">
-        <v>40</v>
+        <v>237</v>
       </c>
       <c r="C164" s="2" t="s">
-        <v>509</v>
-      </c>
-      <c r="D164" t="s">
-        <v>511</v>
-      </c>
-      <c r="E164" t="s">
-        <v>510</v>
+        <v>272</v>
       </c>
       <c r="F164">
-        <v>1989</v>
+        <v>1996</v>
       </c>
       <c r="G164">
-        <v>2009</v>
+        <v>2016</v>
       </c>
       <c r="H164" t="s">
-        <v>348</v>
+        <v>16</v>
       </c>
       <c r="I164" t="s">
-        <v>349</v>
-      </c>
-      <c r="P164" s="2" t="s">
-        <v>512</v>
+        <v>20</v>
       </c>
     </row>
     <row r="165" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
-        <v>66</v>
+        <v>508</v>
       </c>
       <c r="B165" t="s">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="C165" s="2" t="s">
-        <v>67</v>
+        <v>509</v>
+      </c>
+      <c r="D165" t="s">
+        <v>511</v>
+      </c>
+      <c r="E165" t="s">
+        <v>510</v>
+      </c>
+      <c r="F165">
+        <v>1989</v>
+      </c>
+      <c r="G165">
+        <v>2009</v>
+      </c>
+      <c r="H165" t="s">
+        <v>348</v>
+      </c>
+      <c r="I165" t="s">
+        <v>349</v>
+      </c>
+      <c r="P165" s="2" t="s">
+        <v>512</v>
       </c>
     </row>
     <row r="166" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
-        <v>500</v>
+        <v>66</v>
       </c>
       <c r="B166" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="C166" s="2" t="s">
-        <v>499</v>
-      </c>
-      <c r="D166" t="s">
-        <v>501</v>
-      </c>
-      <c r="E166" t="s">
-        <v>14</v>
-      </c>
-      <c r="F166">
-        <v>1946</v>
-      </c>
-      <c r="G166">
-        <v>2015</v>
-      </c>
-      <c r="H166" t="s">
-        <v>348</v>
-      </c>
-      <c r="I166" t="s">
-        <v>349</v>
+        <v>67</v>
       </c>
     </row>
     <row r="167" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
-        <v>383</v>
+        <v>500</v>
       </c>
       <c r="B167" t="s">
         <v>40</v>
       </c>
       <c r="C167" s="2" t="s">
-        <v>384</v>
+        <v>499</v>
+      </c>
+      <c r="D167" t="s">
+        <v>501</v>
       </c>
       <c r="E167" t="s">
-        <v>386</v>
+        <v>14</v>
       </c>
       <c r="F167">
-        <v>1951</v>
+        <v>1946</v>
+      </c>
+      <c r="G167">
+        <v>2015</v>
       </c>
       <c r="H167" t="s">
         <v>348</v>
@@ -5691,178 +5706,181 @@
       <c r="I167" t="s">
         <v>349</v>
       </c>
-      <c r="N167" s="2" t="s">
-        <v>385</v>
-      </c>
     </row>
     <row r="168" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
-        <v>139</v>
+        <v>383</v>
       </c>
       <c r="B168" t="s">
         <v>40</v>
       </c>
       <c r="C168" s="2" t="s">
-        <v>140</v>
+        <v>384</v>
+      </c>
+      <c r="E168" t="s">
+        <v>386</v>
+      </c>
+      <c r="F168">
+        <v>1951</v>
+      </c>
+      <c r="H168" t="s">
+        <v>348</v>
+      </c>
+      <c r="I168" t="s">
+        <v>349</v>
+      </c>
+      <c r="N168" s="2" t="s">
+        <v>385</v>
       </c>
     </row>
     <row r="169" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
-        <v>329</v>
+        <v>139</v>
       </c>
       <c r="B169" t="s">
-        <v>165</v>
+        <v>40</v>
       </c>
       <c r="C169" s="2" t="s">
-        <v>328</v>
-      </c>
-      <c r="E169" t="s">
-        <v>34</v>
-      </c>
-      <c r="F169">
-        <v>1789</v>
-      </c>
-      <c r="H169" t="s">
-        <v>16</v>
-      </c>
-      <c r="I169" t="s">
-        <v>20</v>
+        <v>140</v>
       </c>
     </row>
     <row r="170" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
-        <v>172</v>
+        <v>329</v>
       </c>
       <c r="B170" t="s">
-        <v>60</v>
+        <v>165</v>
       </c>
       <c r="C170" s="2" t="s">
-        <v>171</v>
+        <v>328</v>
+      </c>
+      <c r="E170" t="s">
+        <v>34</v>
+      </c>
+      <c r="F170">
+        <v>1789</v>
+      </c>
+      <c r="H170" t="s">
+        <v>16</v>
+      </c>
+      <c r="I170" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="171" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
-        <v>217</v>
+        <v>172</v>
       </c>
       <c r="B171" t="s">
         <v>60</v>
       </c>
       <c r="C171" s="2" t="s">
-        <v>216</v>
-      </c>
-      <c r="E171" t="s">
-        <v>14</v>
-      </c>
-      <c r="F171">
-        <v>1900</v>
-      </c>
-      <c r="H171" t="s">
-        <v>16</v>
-      </c>
-      <c r="I171" t="s">
-        <v>20</v>
+        <v>171</v>
       </c>
     </row>
     <row r="172" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
-        <v>132</v>
+        <v>217</v>
       </c>
       <c r="B172" t="s">
-        <v>259</v>
+        <v>60</v>
       </c>
       <c r="C172" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="Q172" t="s">
-        <v>17</v>
+        <v>216</v>
+      </c>
+      <c r="E172" t="s">
+        <v>14</v>
+      </c>
+      <c r="F172">
+        <v>1900</v>
+      </c>
+      <c r="H172" t="s">
+        <v>16</v>
+      </c>
+      <c r="I172" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="173" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
-        <v>182</v>
+        <v>132</v>
       </c>
       <c r="B173" t="s">
-        <v>165</v>
+        <v>259</v>
       </c>
       <c r="C173" s="2" t="s">
-        <v>181</v>
+        <v>133</v>
+      </c>
+      <c r="Q173" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="174" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
-        <v>423</v>
+        <v>182</v>
       </c>
       <c r="B174" t="s">
-        <v>86</v>
+        <v>165</v>
       </c>
       <c r="C174" s="2" t="s">
-        <v>424</v>
-      </c>
-      <c r="E174" t="s">
-        <v>34</v>
-      </c>
-      <c r="F174">
-        <v>1996</v>
-      </c>
-      <c r="G174">
-        <v>2016</v>
-      </c>
-      <c r="H174" t="s">
-        <v>348</v>
-      </c>
-      <c r="I174" t="s">
-        <v>425</v>
+        <v>181</v>
       </c>
     </row>
     <row r="175" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
-        <v>115</v>
+        <v>423</v>
       </c>
       <c r="B175" t="s">
-        <v>128</v>
+        <v>86</v>
       </c>
       <c r="C175" s="2" t="s">
-        <v>116</v>
+        <v>424</v>
+      </c>
+      <c r="E175" t="s">
+        <v>34</v>
+      </c>
+      <c r="F175">
+        <v>1996</v>
+      </c>
+      <c r="G175">
+        <v>2016</v>
+      </c>
+      <c r="H175" t="s">
+        <v>348</v>
+      </c>
+      <c r="I175" t="s">
+        <v>425</v>
       </c>
     </row>
     <row r="176" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
-        <v>263</v>
+        <v>115</v>
       </c>
       <c r="B176" t="s">
-        <v>250</v>
+        <v>128</v>
       </c>
       <c r="C176" s="2" t="s">
-        <v>264</v>
-      </c>
-      <c r="E176" t="s">
-        <v>265</v>
-      </c>
-      <c r="F176">
-        <v>1500</v>
-      </c>
-      <c r="G176">
-        <v>2000</v>
-      </c>
-      <c r="H176" t="s">
-        <v>16</v>
-      </c>
-      <c r="I176" t="s">
-        <v>20</v>
+        <v>116</v>
       </c>
     </row>
     <row r="177" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
-        <v>221</v>
+        <v>263</v>
       </c>
       <c r="B177" t="s">
-        <v>86</v>
+        <v>250</v>
       </c>
       <c r="C177" s="2" t="s">
-        <v>220</v>
+        <v>264</v>
+      </c>
+      <c r="E177" t="s">
+        <v>265</v>
       </c>
       <c r="F177">
-        <v>2013</v>
+        <v>1500</v>
+      </c>
+      <c r="G177">
+        <v>2000</v>
       </c>
       <c r="H177" t="s">
         <v>16</v>
@@ -5873,22 +5891,16 @@
     </row>
     <row r="178" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
-        <v>13</v>
+        <v>221</v>
       </c>
       <c r="B178" t="s">
-        <v>25</v>
+        <v>86</v>
       </c>
       <c r="C178" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="D178" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="E178" t="s">
-        <v>14</v>
+        <v>220</v>
       </c>
       <c r="F178">
-        <v>1981</v>
+        <v>2013</v>
       </c>
       <c r="H178" t="s">
         <v>16</v>
@@ -5899,13 +5911,22 @@
     </row>
     <row r="179" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
-        <v>283</v>
+        <v>13</v>
       </c>
       <c r="B179" t="s">
-        <v>124</v>
+        <v>25</v>
       </c>
       <c r="C179" s="2" t="s">
-        <v>284</v>
+        <v>38</v>
+      </c>
+      <c r="D179" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E179" t="s">
+        <v>14</v>
+      </c>
+      <c r="F179">
+        <v>1981</v>
       </c>
       <c r="H179" t="s">
         <v>16</v>
@@ -5914,8 +5935,25 @@
         <v>20</v>
       </c>
     </row>
+    <row r="180" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A180" t="s">
+        <v>283</v>
+      </c>
+      <c r="B180" t="s">
+        <v>124</v>
+      </c>
+      <c r="C180" s="2" t="s">
+        <v>284</v>
+      </c>
+      <c r="H180" t="s">
+        <v>16</v>
+      </c>
+      <c r="I180" t="s">
+        <v>20</v>
+      </c>
+    </row>
   </sheetData>
-  <sortState ref="A2:Q179">
+  <sortState ref="A2:Q180">
     <sortCondition ref="A2"/>
   </sortState>
   <hyperlinks>
@@ -5924,8 +5962,8 @@
     <hyperlink ref="C7" r:id="rId3"/>
     <hyperlink ref="C11" r:id="rId4"/>
     <hyperlink ref="C105" r:id="rId5"/>
-    <hyperlink ref="C127" r:id="rId6"/>
-    <hyperlink ref="C178" r:id="rId7"/>
+    <hyperlink ref="C128" r:id="rId6"/>
+    <hyperlink ref="C179" r:id="rId7"/>
     <hyperlink ref="C40" r:id="rId8"/>
     <hyperlink ref="C33" r:id="rId9"/>
     <hyperlink ref="C57" r:id="rId10"/>
@@ -5935,11 +5973,11 @@
     <hyperlink ref="C68" r:id="rId14"/>
     <hyperlink ref="C97" r:id="rId15"/>
     <hyperlink ref="C32" r:id="rId16"/>
-    <hyperlink ref="C122" r:id="rId17"/>
+    <hyperlink ref="C123" r:id="rId17"/>
     <hyperlink ref="C48" r:id="rId18"/>
     <hyperlink ref="C82" r:id="rId19"/>
     <hyperlink ref="C17" r:id="rId20"/>
-    <hyperlink ref="C165" r:id="rId21"/>
+    <hyperlink ref="C166" r:id="rId21"/>
     <hyperlink ref="C8" r:id="rId22"/>
     <hyperlink ref="C44" r:id="rId23"/>
     <hyperlink ref="C61" r:id="rId24"/>
@@ -5948,75 +5986,75 @@
     <hyperlink ref="C63" r:id="rId27"/>
     <hyperlink ref="C79" r:id="rId28"/>
     <hyperlink ref="C102" r:id="rId29"/>
-    <hyperlink ref="C154" r:id="rId30"/>
+    <hyperlink ref="C155" r:id="rId30"/>
     <hyperlink ref="C108" r:id="rId31"/>
     <hyperlink ref="C92" r:id="rId32"/>
     <hyperlink ref="C115" r:id="rId33"/>
     <hyperlink ref="C80" r:id="rId34"/>
     <hyperlink ref="C18" r:id="rId35"/>
-    <hyperlink ref="C152" r:id="rId36"/>
+    <hyperlink ref="C153" r:id="rId36"/>
     <hyperlink ref="C16" r:id="rId37"/>
-    <hyperlink ref="C175" r:id="rId38"/>
+    <hyperlink ref="C176" r:id="rId38"/>
     <hyperlink ref="C96" r:id="rId39"/>
     <hyperlink ref="C65" r:id="rId40"/>
-    <hyperlink ref="C134" r:id="rId41"/>
+    <hyperlink ref="C135" r:id="rId41"/>
     <hyperlink ref="C19" r:id="rId42"/>
     <hyperlink ref="C59" r:id="rId43"/>
     <hyperlink ref="C26" r:id="rId44"/>
-    <hyperlink ref="C123" r:id="rId45"/>
-    <hyperlink ref="C172" r:id="rId46"/>
+    <hyperlink ref="C124" r:id="rId45"/>
+    <hyperlink ref="C173" r:id="rId46"/>
     <hyperlink ref="C30" r:id="rId47" display="http://comparativeconstitutionsproject.org/"/>
-    <hyperlink ref="C120" r:id="rId48"/>
-    <hyperlink ref="C168" r:id="rId49"/>
-    <hyperlink ref="C138" r:id="rId50"/>
-    <hyperlink ref="C132" r:id="rId51"/>
+    <hyperlink ref="C121" r:id="rId48"/>
+    <hyperlink ref="C169" r:id="rId49"/>
+    <hyperlink ref="C139" r:id="rId50"/>
+    <hyperlink ref="C133" r:id="rId51"/>
     <hyperlink ref="C25" r:id="rId52"/>
-    <hyperlink ref="C124" r:id="rId53"/>
+    <hyperlink ref="C125" r:id="rId53"/>
     <hyperlink ref="C55" r:id="rId54"/>
     <hyperlink ref="C86" r:id="rId55"/>
     <hyperlink ref="C89" r:id="rId56"/>
-    <hyperlink ref="C121" r:id="rId57"/>
+    <hyperlink ref="C122" r:id="rId57"/>
     <hyperlink ref="C110" r:id="rId58"/>
-    <hyperlink ref="C143" r:id="rId59"/>
+    <hyperlink ref="C144" r:id="rId59"/>
     <hyperlink ref="C34" r:id="rId60"/>
-    <hyperlink ref="C156" r:id="rId61"/>
+    <hyperlink ref="C157" r:id="rId61"/>
     <hyperlink ref="C9" r:id="rId62"/>
     <hyperlink ref="C36" r:id="rId63"/>
-    <hyperlink ref="C158" r:id="rId64"/>
+    <hyperlink ref="C159" r:id="rId64"/>
     <hyperlink ref="C15" r:id="rId65"/>
-    <hyperlink ref="C170" r:id="rId66"/>
+    <hyperlink ref="C171" r:id="rId66"/>
     <hyperlink ref="C28" r:id="rId67"/>
     <hyperlink ref="C27" r:id="rId68"/>
     <hyperlink ref="C29" r:id="rId69"/>
     <hyperlink ref="C60" r:id="rId70"/>
-    <hyperlink ref="C173" r:id="rId71"/>
+    <hyperlink ref="C174" r:id="rId71"/>
     <hyperlink ref="C31" r:id="rId72"/>
-    <hyperlink ref="C128" r:id="rId73"/>
+    <hyperlink ref="C129" r:id="rId73"/>
     <hyperlink ref="C35" r:id="rId74"/>
     <hyperlink ref="C52" r:id="rId75"/>
-    <hyperlink ref="C146" r:id="rId76"/>
+    <hyperlink ref="C147" r:id="rId76"/>
     <hyperlink ref="C49" r:id="rId77"/>
     <hyperlink ref="C45" r:id="rId78"/>
     <hyperlink ref="C76" r:id="rId79"/>
     <hyperlink ref="C5" r:id="rId80"/>
     <hyperlink ref="C75" r:id="rId81"/>
     <hyperlink ref="C13" r:id="rId82"/>
-    <hyperlink ref="C119" r:id="rId83"/>
-    <hyperlink ref="C130" r:id="rId84"/>
-    <hyperlink ref="C160" r:id="rId85"/>
+    <hyperlink ref="C120" r:id="rId83"/>
+    <hyperlink ref="C131" r:id="rId84"/>
+    <hyperlink ref="C161" r:id="rId85"/>
     <hyperlink ref="C41" r:id="rId86"/>
-    <hyperlink ref="C171" r:id="rId87"/>
+    <hyperlink ref="C172" r:id="rId87"/>
     <hyperlink ref="C51" r:id="rId88"/>
-    <hyperlink ref="C177" r:id="rId89"/>
+    <hyperlink ref="C178" r:id="rId89"/>
     <hyperlink ref="C106" r:id="rId90"/>
     <hyperlink ref="C73" r:id="rId91"/>
     <hyperlink ref="C107" r:id="rId92"/>
-    <hyperlink ref="C149" r:id="rId93"/>
+    <hyperlink ref="C150" r:id="rId93"/>
     <hyperlink ref="C90" r:id="rId94"/>
     <hyperlink ref="C112" r:id="rId95"/>
-    <hyperlink ref="C150" r:id="rId96"/>
+    <hyperlink ref="C151" r:id="rId96"/>
     <hyperlink ref="C69" r:id="rId97"/>
-    <hyperlink ref="C126" r:id="rId98"/>
+    <hyperlink ref="C127" r:id="rId98"/>
     <hyperlink ref="C53" r:id="rId99"/>
     <hyperlink ref="C50" r:id="rId100"/>
     <hyperlink ref="C93" r:id="rId101"/>
@@ -6027,36 +6065,36 @@
     <hyperlink ref="C117" r:id="rId106"/>
     <hyperlink ref="C54" r:id="rId107"/>
     <hyperlink ref="C94" r:id="rId108"/>
-    <hyperlink ref="C148" r:id="rId109"/>
+    <hyperlink ref="C149" r:id="rId109"/>
     <hyperlink ref="C14" r:id="rId110"/>
     <hyperlink ref="C4" r:id="rId111"/>
-    <hyperlink ref="C176" r:id="rId112"/>
+    <hyperlink ref="C177" r:id="rId112"/>
     <hyperlink ref="C100" r:id="rId113"/>
     <hyperlink ref="C95" r:id="rId114"/>
-    <hyperlink ref="C163" r:id="rId115"/>
-    <hyperlink ref="C142" r:id="rId116"/>
+    <hyperlink ref="C164" r:id="rId115"/>
+    <hyperlink ref="C143" r:id="rId116"/>
     <hyperlink ref="C71" r:id="rId117"/>
     <hyperlink ref="C109" r:id="rId118"/>
     <hyperlink ref="C84" r:id="rId119"/>
-    <hyperlink ref="C179" r:id="rId120"/>
+    <hyperlink ref="C180" r:id="rId120"/>
     <hyperlink ref="C74" r:id="rId121"/>
-    <hyperlink ref="C140" r:id="rId122"/>
+    <hyperlink ref="C141" r:id="rId122"/>
     <hyperlink ref="C116" r:id="rId123"/>
     <hyperlink ref="C88" r:id="rId124"/>
     <hyperlink ref="C114" r:id="rId125"/>
-    <hyperlink ref="C147" r:id="rId126"/>
+    <hyperlink ref="C148" r:id="rId126"/>
     <hyperlink ref="C98" r:id="rId127"/>
     <hyperlink ref="C12" r:id="rId128"/>
     <hyperlink ref="C20" r:id="rId129"/>
-    <hyperlink ref="C139" r:id="rId130"/>
+    <hyperlink ref="C140" r:id="rId130"/>
     <hyperlink ref="C83" r:id="rId131"/>
-    <hyperlink ref="C155" r:id="rId132"/>
-    <hyperlink ref="C136" r:id="rId133"/>
-    <hyperlink ref="C135" r:id="rId134"/>
-    <hyperlink ref="C137" r:id="rId135"/>
-    <hyperlink ref="C162" r:id="rId136"/>
-    <hyperlink ref="C153" r:id="rId137"/>
-    <hyperlink ref="C169" r:id="rId138"/>
+    <hyperlink ref="C156" r:id="rId132"/>
+    <hyperlink ref="C137" r:id="rId133"/>
+    <hyperlink ref="C136" r:id="rId134"/>
+    <hyperlink ref="C138" r:id="rId135"/>
+    <hyperlink ref="C163" r:id="rId136"/>
+    <hyperlink ref="C154" r:id="rId137"/>
+    <hyperlink ref="C170" r:id="rId138"/>
     <hyperlink ref="C43" r:id="rId139"/>
     <hyperlink ref="C99" r:id="rId140"/>
     <hyperlink ref="J2" r:id="rId141"/>
@@ -6066,23 +6104,23 @@
     <hyperlink ref="J4" r:id="rId145"/>
     <hyperlink ref="P5" r:id="rId146"/>
     <hyperlink ref="J5" r:id="rId147"/>
-    <hyperlink ref="C118" r:id="rId148"/>
+    <hyperlink ref="C119" r:id="rId148"/>
     <hyperlink ref="C38" r:id="rId149"/>
     <hyperlink ref="P7" r:id="rId150"/>
     <hyperlink ref="J7" r:id="rId151"/>
     <hyperlink ref="M8" r:id="rId152"/>
     <hyperlink ref="L8" r:id="rId153"/>
     <hyperlink ref="J8" r:id="rId154"/>
-    <hyperlink ref="C167" r:id="rId155"/>
-    <hyperlink ref="N167" r:id="rId156"/>
+    <hyperlink ref="C168" r:id="rId155"/>
+    <hyperlink ref="N168" r:id="rId156"/>
     <hyperlink ref="C22" r:id="rId157"/>
     <hyperlink ref="N22" r:id="rId158"/>
     <hyperlink ref="C70" r:id="rId159"/>
-    <hyperlink ref="C161" r:id="rId160"/>
-    <hyperlink ref="J161" r:id="rId161"/>
-    <hyperlink ref="C159" r:id="rId162"/>
-    <hyperlink ref="N159" r:id="rId163"/>
-    <hyperlink ref="J159" r:id="rId164"/>
+    <hyperlink ref="C162" r:id="rId160"/>
+    <hyperlink ref="J162" r:id="rId161"/>
+    <hyperlink ref="C160" r:id="rId162"/>
+    <hyperlink ref="N160" r:id="rId163"/>
+    <hyperlink ref="J160" r:id="rId164"/>
     <hyperlink ref="C103" r:id="rId165"/>
     <hyperlink ref="C101" r:id="rId166"/>
     <hyperlink ref="C46" r:id="rId167"/>
@@ -6092,24 +6130,24 @@
     <hyperlink ref="N111" r:id="rId171"/>
     <hyperlink ref="C85" r:id="rId172"/>
     <hyperlink ref="K85" r:id="rId173"/>
-    <hyperlink ref="C174" r:id="rId174"/>
-    <hyperlink ref="C131" r:id="rId175"/>
-    <hyperlink ref="K131" r:id="rId176"/>
+    <hyperlink ref="C175" r:id="rId174"/>
+    <hyperlink ref="C132" r:id="rId175"/>
+    <hyperlink ref="K132" r:id="rId176"/>
     <hyperlink ref="L9" r:id="rId177"/>
     <hyperlink ref="J9" r:id="rId178"/>
     <hyperlink ref="J11" r:id="rId179"/>
-    <hyperlink ref="C144" r:id="rId180"/>
-    <hyperlink ref="J144" r:id="rId181"/>
-    <hyperlink ref="L144" r:id="rId182"/>
-    <hyperlink ref="K144" r:id="rId183"/>
-    <hyperlink ref="C145" r:id="rId184"/>
-    <hyperlink ref="J145" r:id="rId185"/>
-    <hyperlink ref="K145" r:id="rId186"/>
-    <hyperlink ref="L145" r:id="rId187"/>
+    <hyperlink ref="C145" r:id="rId180"/>
+    <hyperlink ref="J145" r:id="rId181"/>
+    <hyperlink ref="L145" r:id="rId182"/>
+    <hyperlink ref="K145" r:id="rId183"/>
+    <hyperlink ref="C146" r:id="rId184"/>
+    <hyperlink ref="J146" r:id="rId185"/>
+    <hyperlink ref="K146" r:id="rId186"/>
+    <hyperlink ref="L146" r:id="rId187"/>
     <hyperlink ref="C72" r:id="rId188"/>
     <hyperlink ref="J72" r:id="rId189"/>
     <hyperlink ref="N72" r:id="rId190"/>
-    <hyperlink ref="C151" r:id="rId191"/>
+    <hyperlink ref="C152" r:id="rId191"/>
     <hyperlink ref="C104" r:id="rId192"/>
     <hyperlink ref="J104" r:id="rId193"/>
     <hyperlink ref="L104" r:id="rId194"/>
@@ -6122,8 +6160,8 @@
     <hyperlink ref="J78" r:id="rId201"/>
     <hyperlink ref="K78" r:id="rId202"/>
     <hyperlink ref="L78" r:id="rId203"/>
-    <hyperlink ref="C133" r:id="rId204"/>
-    <hyperlink ref="N133" r:id="rId205"/>
+    <hyperlink ref="C134" r:id="rId204"/>
+    <hyperlink ref="N134" r:id="rId205"/>
     <hyperlink ref="C42" r:id="rId206"/>
     <hyperlink ref="K42" r:id="rId207"/>
     <hyperlink ref="J42" r:id="rId208"/>
@@ -6138,33 +6176,34 @@
     <hyperlink ref="M47" r:id="rId217"/>
     <hyperlink ref="N47" r:id="rId218"/>
     <hyperlink ref="C23" r:id="rId219"/>
-    <hyperlink ref="C166" r:id="rId220"/>
+    <hyperlink ref="C167" r:id="rId220"/>
     <hyperlink ref="C39" r:id="rId221"/>
     <hyperlink ref="J39" r:id="rId222"/>
     <hyperlink ref="N39" r:id="rId223"/>
     <hyperlink ref="L39" r:id="rId224"/>
     <hyperlink ref="K39" r:id="rId225"/>
-    <hyperlink ref="C164" r:id="rId226"/>
-    <hyperlink ref="P164" r:id="rId227"/>
+    <hyperlink ref="C165" r:id="rId226"/>
+    <hyperlink ref="P165" r:id="rId227"/>
     <hyperlink ref="C113" r:id="rId228"/>
-    <hyperlink ref="C129" r:id="rId229"/>
-    <hyperlink ref="P129" r:id="rId230"/>
+    <hyperlink ref="C130" r:id="rId229"/>
+    <hyperlink ref="P130" r:id="rId230"/>
     <hyperlink ref="C77" r:id="rId231"/>
     <hyperlink ref="J77" r:id="rId232"/>
     <hyperlink ref="K77" r:id="rId233"/>
     <hyperlink ref="N77" r:id="rId234"/>
-    <hyperlink ref="C141" r:id="rId235"/>
-    <hyperlink ref="J141" r:id="rId236"/>
-    <hyperlink ref="L141" r:id="rId237"/>
+    <hyperlink ref="C142" r:id="rId235"/>
+    <hyperlink ref="J142" r:id="rId236"/>
+    <hyperlink ref="L142" r:id="rId237"/>
     <hyperlink ref="C37" r:id="rId238"/>
     <hyperlink ref="C24" r:id="rId239"/>
     <hyperlink ref="J24" r:id="rId240"/>
     <hyperlink ref="P24" r:id="rId241"/>
-    <hyperlink ref="C125" r:id="rId242"/>
-    <hyperlink ref="N125" r:id="rId243"/>
-    <hyperlink ref="J125" r:id="rId244"/>
-    <hyperlink ref="C157" r:id="rId245"/>
-    <hyperlink ref="J157" r:id="rId246"/>
+    <hyperlink ref="C126" r:id="rId242"/>
+    <hyperlink ref="N126" r:id="rId243"/>
+    <hyperlink ref="J126" r:id="rId244"/>
+    <hyperlink ref="C158" r:id="rId245"/>
+    <hyperlink ref="J158" r:id="rId246"/>
+    <hyperlink ref="C118" r:id="rId247"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
add 'Sexual Violence in Armed Conflict'
</commit_message>
<xml_diff>
--- a/PolData.xlsx
+++ b/PolData.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1014" uniqueCount="557">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1023" uniqueCount="563">
   <si>
     <t>name</t>
   </si>
@@ -1698,6 +1698,24 @@
   </si>
   <si>
     <t>http://sites.psu.edu/dictators/wp-content/uploads/sites/12570/2016/05/GWF-Autocratic-Regimes-1.2.zip</t>
+  </si>
+  <si>
+    <t>http://www.sexualviolencedata.org/dataset/</t>
+  </si>
+  <si>
+    <t>Sexual Violence in Armed Conflict</t>
+  </si>
+  <si>
+    <t>Conflict-related sexual violence, armed conflict actors, government military, state military, insurgent forces</t>
+  </si>
+  <si>
+    <t>Asia, Africa, Middle East, Americas, Europe</t>
+  </si>
+  <si>
+    <t>http://www.sexualviolencedata.org/wp-content/uploads/2013/01/SVAC-coding-manual-10-25-13.pdf</t>
+  </si>
+  <si>
+    <t>http://www.sexualviolencedata.org/wp-content/uploads/2013/01/SVAC_dataset-update-2016-June-21.xlsx.zip</t>
   </si>
 </sst>
 </file>
@@ -2037,10 +2055,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q181"/>
+  <dimension ref="A1:Q182"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A162" workbookViewId="0">
-      <selection activeCell="A184" sqref="A184"/>
+    <sheetView tabSelected="1" topLeftCell="A167" workbookViewId="0">
+      <selection activeCell="A180" sqref="A180"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5300,76 +5318,88 @@
     </row>
     <row r="148" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
-        <v>194</v>
+        <v>558</v>
       </c>
       <c r="B148" t="s">
-        <v>99</v>
+        <v>40</v>
       </c>
       <c r="C148" s="2" t="s">
-        <v>193</v>
+        <v>557</v>
+      </c>
+      <c r="D148" t="s">
+        <v>559</v>
+      </c>
+      <c r="E148" t="s">
+        <v>560</v>
+      </c>
+      <c r="F148">
+        <v>1989</v>
+      </c>
+      <c r="G148">
+        <v>2009</v>
+      </c>
+      <c r="H148" t="s">
+        <v>348</v>
+      </c>
+      <c r="I148" t="s">
+        <v>349</v>
+      </c>
+      <c r="J148" s="2" t="s">
+        <v>561</v>
+      </c>
+      <c r="P148" s="2" t="s">
+        <v>562</v>
       </c>
     </row>
     <row r="149" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
-        <v>295</v>
+        <v>194</v>
       </c>
       <c r="B149" t="s">
-        <v>40</v>
+        <v>99</v>
       </c>
       <c r="C149" s="2" t="s">
-        <v>296</v>
-      </c>
-      <c r="E149" t="s">
-        <v>297</v>
-      </c>
-      <c r="F149">
-        <v>1990</v>
-      </c>
-      <c r="G149">
-        <v>2015</v>
-      </c>
-      <c r="H149" t="s">
-        <v>16</v>
-      </c>
-      <c r="I149" t="s">
-        <v>249</v>
+        <v>193</v>
       </c>
     </row>
     <row r="150" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
-        <v>256</v>
+        <v>295</v>
       </c>
       <c r="B150" t="s">
-        <v>250</v>
+        <v>40</v>
       </c>
       <c r="C150" s="2" t="s">
-        <v>257</v>
+        <v>296</v>
       </c>
       <c r="E150" t="s">
-        <v>258</v>
+        <v>297</v>
+      </c>
+      <c r="F150">
+        <v>1990</v>
+      </c>
+      <c r="G150">
+        <v>2015</v>
       </c>
       <c r="H150" t="s">
         <v>16</v>
       </c>
       <c r="I150" t="s">
-        <v>20</v>
+        <v>249</v>
       </c>
     </row>
     <row r="151" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
-        <v>227</v>
+        <v>256</v>
       </c>
       <c r="B151" t="s">
-        <v>40</v>
+        <v>250</v>
       </c>
       <c r="C151" s="2" t="s">
-        <v>225</v>
-      </c>
-      <c r="F151">
-        <v>1955</v>
-      </c>
-      <c r="G151">
-        <v>2016</v>
+        <v>257</v>
+      </c>
+      <c r="E151" t="s">
+        <v>258</v>
       </c>
       <c r="H151" t="s">
         <v>16</v>
@@ -5380,7 +5410,7 @@
     </row>
     <row r="152" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="B152" t="s">
         <v>40</v>
@@ -5389,7 +5419,7 @@
         <v>225</v>
       </c>
       <c r="F152">
-        <v>1995</v>
+        <v>1955</v>
       </c>
       <c r="G152">
         <v>2016</v>
@@ -5403,280 +5433,280 @@
     </row>
     <row r="153" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
-        <v>452</v>
+        <v>230</v>
       </c>
       <c r="B153" t="s">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="C153" s="2" t="s">
-        <v>453</v>
-      </c>
-      <c r="E153" t="s">
-        <v>9</v>
+        <v>225</v>
+      </c>
+      <c r="F153">
+        <v>1995</v>
+      </c>
+      <c r="G153">
+        <v>2016</v>
       </c>
       <c r="H153" t="s">
-        <v>348</v>
+        <v>16</v>
       </c>
       <c r="I153" t="s">
-        <v>435</v>
+        <v>20</v>
       </c>
     </row>
     <row r="154" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
-        <v>109</v>
+        <v>452</v>
       </c>
       <c r="B154" t="s">
         <v>25</v>
       </c>
       <c r="C154" s="2" t="s">
-        <v>110</v>
+        <v>453</v>
       </c>
       <c r="E154" t="s">
-        <v>111</v>
-      </c>
-      <c r="F154">
-        <v>1956</v>
+        <v>9</v>
+      </c>
+      <c r="H154" t="s">
+        <v>348</v>
+      </c>
+      <c r="I154" t="s">
+        <v>435</v>
       </c>
     </row>
     <row r="155" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
-        <v>326</v>
+        <v>109</v>
       </c>
       <c r="B155" t="s">
         <v>25</v>
       </c>
       <c r="C155" s="2" t="s">
-        <v>327</v>
+        <v>110</v>
       </c>
       <c r="E155" t="s">
         <v>111</v>
       </c>
       <c r="F155">
-        <v>1998</v>
-      </c>
-      <c r="H155" t="s">
-        <v>16</v>
-      </c>
-      <c r="I155" t="s">
-        <v>20</v>
+        <v>1956</v>
       </c>
     </row>
     <row r="156" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
-        <v>91</v>
+        <v>326</v>
       </c>
       <c r="B156" t="s">
         <v>25</v>
       </c>
       <c r="C156" s="2" t="s">
-        <v>93</v>
+        <v>327</v>
       </c>
       <c r="E156" t="s">
-        <v>92</v>
+        <v>111</v>
       </c>
       <c r="F156">
-        <v>1999</v>
+        <v>1998</v>
+      </c>
+      <c r="H156" t="s">
+        <v>16</v>
+      </c>
+      <c r="I156" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="157" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
-        <v>314</v>
+        <v>91</v>
       </c>
       <c r="B157" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="C157" s="2" t="s">
-        <v>313</v>
+        <v>93</v>
       </c>
       <c r="E157" t="s">
-        <v>315</v>
+        <v>92</v>
       </c>
       <c r="F157">
-        <v>1950</v>
-      </c>
-      <c r="G157">
-        <v>2004</v>
-      </c>
-      <c r="H157" t="s">
-        <v>16</v>
-      </c>
-      <c r="I157" t="s">
-        <v>20</v>
+        <v>1999</v>
       </c>
     </row>
     <row r="158" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
-        <v>161</v>
+        <v>314</v>
       </c>
       <c r="B158" t="s">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="C158" s="2" t="s">
-        <v>160</v>
+        <v>313</v>
+      </c>
+      <c r="E158" t="s">
+        <v>315</v>
+      </c>
+      <c r="F158">
+        <v>1950</v>
+      </c>
+      <c r="G158">
+        <v>2004</v>
+      </c>
+      <c r="H158" t="s">
+        <v>16</v>
+      </c>
+      <c r="I158" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="159" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
-        <v>545</v>
+        <v>161</v>
       </c>
       <c r="B159" t="s">
         <v>25</v>
       </c>
       <c r="C159" s="2" t="s">
-        <v>546</v>
-      </c>
-      <c r="D159" t="s">
-        <v>547</v>
-      </c>
-      <c r="E159" t="s">
-        <v>34</v>
-      </c>
-      <c r="F159">
-        <v>2000</v>
-      </c>
-      <c r="G159">
-        <v>2011</v>
-      </c>
-      <c r="H159" t="s">
-        <v>348</v>
-      </c>
-      <c r="I159" t="s">
-        <v>349</v>
-      </c>
-      <c r="J159" s="2" t="s">
-        <v>548</v>
+        <v>160</v>
       </c>
     </row>
     <row r="160" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
-        <v>168</v>
+        <v>545</v>
       </c>
       <c r="B160" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="C160" s="2" t="s">
-        <v>167</v>
+        <v>546</v>
+      </c>
+      <c r="D160" t="s">
+        <v>547</v>
+      </c>
+      <c r="E160" t="s">
+        <v>34</v>
+      </c>
+      <c r="F160">
+        <v>2000</v>
+      </c>
+      <c r="G160">
+        <v>2011</v>
+      </c>
+      <c r="H160" t="s">
+        <v>348</v>
+      </c>
+      <c r="I160" t="s">
+        <v>349</v>
+      </c>
+      <c r="J160" s="2" t="s">
+        <v>548</v>
       </c>
     </row>
     <row r="161" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
-        <v>399</v>
+        <v>168</v>
       </c>
       <c r="B161" t="s">
         <v>40</v>
       </c>
       <c r="C161" s="2" t="s">
-        <v>400</v>
-      </c>
-      <c r="E161" t="s">
-        <v>14</v>
-      </c>
-      <c r="F161">
-        <v>2000</v>
-      </c>
-      <c r="G161">
-        <v>2014</v>
-      </c>
-      <c r="H161" t="s">
-        <v>348</v>
-      </c>
-      <c r="I161" t="s">
-        <v>349</v>
-      </c>
-      <c r="J161" s="2" t="s">
-        <v>402</v>
-      </c>
-      <c r="N161" s="2" t="s">
-        <v>401</v>
+        <v>167</v>
       </c>
     </row>
     <row r="162" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
-        <v>213</v>
+        <v>399</v>
       </c>
       <c r="B162" t="s">
-        <v>55</v>
+        <v>40</v>
       </c>
       <c r="C162" s="2" t="s">
-        <v>212</v>
+        <v>400</v>
+      </c>
+      <c r="E162" t="s">
+        <v>14</v>
+      </c>
+      <c r="F162">
+        <v>2000</v>
+      </c>
+      <c r="G162">
+        <v>2014</v>
       </c>
       <c r="H162" t="s">
-        <v>16</v>
+        <v>348</v>
       </c>
       <c r="I162" t="s">
-        <v>20</v>
+        <v>349</v>
+      </c>
+      <c r="J162" s="2" t="s">
+        <v>402</v>
+      </c>
+      <c r="N162" s="2" t="s">
+        <v>401</v>
       </c>
     </row>
     <row r="163" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
-        <v>395</v>
+        <v>213</v>
       </c>
       <c r="B163" t="s">
-        <v>25</v>
+        <v>55</v>
       </c>
       <c r="C163" s="2" t="s">
-        <v>394</v>
-      </c>
-      <c r="D163" t="s">
-        <v>396</v>
-      </c>
-      <c r="E163" t="s">
-        <v>111</v>
-      </c>
-      <c r="F163">
-        <v>1986</v>
-      </c>
-      <c r="G163">
-        <v>2015</v>
+        <v>212</v>
       </c>
       <c r="H163" t="s">
-        <v>367</v>
+        <v>16</v>
       </c>
       <c r="I163" t="s">
-        <v>398</v>
-      </c>
-      <c r="J163" s="2" t="s">
-        <v>397</v>
+        <v>20</v>
       </c>
     </row>
     <row r="164" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
-        <v>323</v>
+        <v>395</v>
       </c>
       <c r="B164" t="s">
         <v>25</v>
       </c>
       <c r="C164" s="2" t="s">
-        <v>324</v>
+        <v>394</v>
+      </c>
+      <c r="D164" t="s">
+        <v>396</v>
       </c>
       <c r="E164" t="s">
-        <v>325</v>
+        <v>111</v>
       </c>
       <c r="F164">
-        <v>1942</v>
+        <v>1986</v>
+      </c>
+      <c r="G164">
+        <v>2015</v>
       </c>
       <c r="H164" t="s">
-        <v>16</v>
+        <v>367</v>
       </c>
       <c r="I164" t="s">
-        <v>20</v>
+        <v>398</v>
+      </c>
+      <c r="J164" s="2" t="s">
+        <v>397</v>
       </c>
     </row>
     <row r="165" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
-        <v>273</v>
+        <v>323</v>
       </c>
       <c r="B165" t="s">
-        <v>237</v>
+        <v>25</v>
       </c>
       <c r="C165" s="2" t="s">
-        <v>272</v>
+        <v>324</v>
+      </c>
+      <c r="E165" t="s">
+        <v>325</v>
       </c>
       <c r="F165">
-        <v>1996</v>
-      </c>
-      <c r="G165">
-        <v>2016</v>
+        <v>1942</v>
       </c>
       <c r="H165" t="s">
         <v>16</v>
@@ -5687,91 +5717,91 @@
     </row>
     <row r="166" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
-        <v>508</v>
+        <v>273</v>
       </c>
       <c r="B166" t="s">
-        <v>40</v>
+        <v>237</v>
       </c>
       <c r="C166" s="2" t="s">
-        <v>509</v>
-      </c>
-      <c r="D166" t="s">
-        <v>511</v>
-      </c>
-      <c r="E166" t="s">
-        <v>510</v>
+        <v>272</v>
       </c>
       <c r="F166">
-        <v>1989</v>
+        <v>1996</v>
       </c>
       <c r="G166">
-        <v>2009</v>
+        <v>2016</v>
       </c>
       <c r="H166" t="s">
-        <v>348</v>
+        <v>16</v>
       </c>
       <c r="I166" t="s">
-        <v>349</v>
-      </c>
-      <c r="P166" s="2" t="s">
-        <v>512</v>
+        <v>20</v>
       </c>
     </row>
     <row r="167" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
-        <v>66</v>
+        <v>508</v>
       </c>
       <c r="B167" t="s">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="C167" s="2" t="s">
-        <v>67</v>
+        <v>509</v>
+      </c>
+      <c r="D167" t="s">
+        <v>511</v>
+      </c>
+      <c r="E167" t="s">
+        <v>510</v>
+      </c>
+      <c r="F167">
+        <v>1989</v>
+      </c>
+      <c r="G167">
+        <v>2009</v>
+      </c>
+      <c r="H167" t="s">
+        <v>348</v>
+      </c>
+      <c r="I167" t="s">
+        <v>349</v>
+      </c>
+      <c r="P167" s="2" t="s">
+        <v>512</v>
       </c>
     </row>
     <row r="168" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
-        <v>500</v>
+        <v>66</v>
       </c>
       <c r="B168" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="C168" s="2" t="s">
-        <v>499</v>
-      </c>
-      <c r="D168" t="s">
-        <v>501</v>
-      </c>
-      <c r="E168" t="s">
-        <v>14</v>
-      </c>
-      <c r="F168">
-        <v>1946</v>
-      </c>
-      <c r="G168">
-        <v>2015</v>
-      </c>
-      <c r="H168" t="s">
-        <v>348</v>
-      </c>
-      <c r="I168" t="s">
-        <v>349</v>
+        <v>67</v>
       </c>
     </row>
     <row r="169" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
-        <v>383</v>
+        <v>500</v>
       </c>
       <c r="B169" t="s">
         <v>40</v>
       </c>
       <c r="C169" s="2" t="s">
-        <v>384</v>
+        <v>499</v>
+      </c>
+      <c r="D169" t="s">
+        <v>501</v>
       </c>
       <c r="E169" t="s">
-        <v>386</v>
+        <v>14</v>
       </c>
       <c r="F169">
-        <v>1951</v>
+        <v>1946</v>
+      </c>
+      <c r="G169">
+        <v>2015</v>
       </c>
       <c r="H169" t="s">
         <v>348</v>
@@ -5779,178 +5809,181 @@
       <c r="I169" t="s">
         <v>349</v>
       </c>
-      <c r="N169" s="2" t="s">
-        <v>385</v>
-      </c>
     </row>
     <row r="170" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
-        <v>139</v>
+        <v>383</v>
       </c>
       <c r="B170" t="s">
         <v>40</v>
       </c>
       <c r="C170" s="2" t="s">
-        <v>140</v>
+        <v>384</v>
+      </c>
+      <c r="E170" t="s">
+        <v>386</v>
+      </c>
+      <c r="F170">
+        <v>1951</v>
+      </c>
+      <c r="H170" t="s">
+        <v>348</v>
+      </c>
+      <c r="I170" t="s">
+        <v>349</v>
+      </c>
+      <c r="N170" s="2" t="s">
+        <v>385</v>
       </c>
     </row>
     <row r="171" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
-        <v>329</v>
+        <v>139</v>
       </c>
       <c r="B171" t="s">
-        <v>165</v>
+        <v>40</v>
       </c>
       <c r="C171" s="2" t="s">
-        <v>328</v>
-      </c>
-      <c r="E171" t="s">
-        <v>34</v>
-      </c>
-      <c r="F171">
-        <v>1789</v>
-      </c>
-      <c r="H171" t="s">
-        <v>16</v>
-      </c>
-      <c r="I171" t="s">
-        <v>20</v>
+        <v>140</v>
       </c>
     </row>
     <row r="172" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
-        <v>172</v>
+        <v>329</v>
       </c>
       <c r="B172" t="s">
-        <v>60</v>
+        <v>165</v>
       </c>
       <c r="C172" s="2" t="s">
-        <v>171</v>
+        <v>328</v>
+      </c>
+      <c r="E172" t="s">
+        <v>34</v>
+      </c>
+      <c r="F172">
+        <v>1789</v>
+      </c>
+      <c r="H172" t="s">
+        <v>16</v>
+      </c>
+      <c r="I172" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="173" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
-        <v>217</v>
+        <v>172</v>
       </c>
       <c r="B173" t="s">
         <v>60</v>
       </c>
       <c r="C173" s="2" t="s">
-        <v>216</v>
-      </c>
-      <c r="E173" t="s">
-        <v>14</v>
-      </c>
-      <c r="F173">
-        <v>1900</v>
-      </c>
-      <c r="H173" t="s">
-        <v>16</v>
-      </c>
-      <c r="I173" t="s">
-        <v>20</v>
+        <v>171</v>
       </c>
     </row>
     <row r="174" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
-        <v>132</v>
+        <v>217</v>
       </c>
       <c r="B174" t="s">
-        <v>259</v>
+        <v>60</v>
       </c>
       <c r="C174" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="Q174" t="s">
-        <v>17</v>
+        <v>216</v>
+      </c>
+      <c r="E174" t="s">
+        <v>14</v>
+      </c>
+      <c r="F174">
+        <v>1900</v>
+      </c>
+      <c r="H174" t="s">
+        <v>16</v>
+      </c>
+      <c r="I174" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="175" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
-        <v>182</v>
+        <v>132</v>
       </c>
       <c r="B175" t="s">
-        <v>165</v>
+        <v>259</v>
       </c>
       <c r="C175" s="2" t="s">
-        <v>181</v>
+        <v>133</v>
+      </c>
+      <c r="Q175" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="176" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
-        <v>423</v>
+        <v>182</v>
       </c>
       <c r="B176" t="s">
-        <v>86</v>
+        <v>165</v>
       </c>
       <c r="C176" s="2" t="s">
-        <v>424</v>
-      </c>
-      <c r="E176" t="s">
-        <v>34</v>
-      </c>
-      <c r="F176">
-        <v>1996</v>
-      </c>
-      <c r="G176">
-        <v>2016</v>
-      </c>
-      <c r="H176" t="s">
-        <v>348</v>
-      </c>
-      <c r="I176" t="s">
-        <v>425</v>
+        <v>181</v>
       </c>
     </row>
     <row r="177" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
-        <v>115</v>
+        <v>423</v>
       </c>
       <c r="B177" t="s">
-        <v>128</v>
+        <v>86</v>
       </c>
       <c r="C177" s="2" t="s">
-        <v>116</v>
+        <v>424</v>
+      </c>
+      <c r="E177" t="s">
+        <v>34</v>
+      </c>
+      <c r="F177">
+        <v>1996</v>
+      </c>
+      <c r="G177">
+        <v>2016</v>
+      </c>
+      <c r="H177" t="s">
+        <v>348</v>
+      </c>
+      <c r="I177" t="s">
+        <v>425</v>
       </c>
     </row>
     <row r="178" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
-        <v>263</v>
+        <v>115</v>
       </c>
       <c r="B178" t="s">
-        <v>250</v>
+        <v>128</v>
       </c>
       <c r="C178" s="2" t="s">
-        <v>264</v>
-      </c>
-      <c r="E178" t="s">
-        <v>265</v>
-      </c>
-      <c r="F178">
-        <v>1500</v>
-      </c>
-      <c r="G178">
-        <v>2000</v>
-      </c>
-      <c r="H178" t="s">
-        <v>16</v>
-      </c>
-      <c r="I178" t="s">
-        <v>20</v>
+        <v>116</v>
       </c>
     </row>
     <row r="179" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
-        <v>221</v>
+        <v>263</v>
       </c>
       <c r="B179" t="s">
-        <v>86</v>
+        <v>250</v>
       </c>
       <c r="C179" s="2" t="s">
-        <v>220</v>
+        <v>264</v>
+      </c>
+      <c r="E179" t="s">
+        <v>265</v>
       </c>
       <c r="F179">
-        <v>2013</v>
+        <v>1500</v>
+      </c>
+      <c r="G179">
+        <v>2000</v>
       </c>
       <c r="H179" t="s">
         <v>16</v>
@@ -5961,22 +5994,16 @@
     </row>
     <row r="180" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
-        <v>13</v>
+        <v>221</v>
       </c>
       <c r="B180" t="s">
-        <v>25</v>
+        <v>86</v>
       </c>
       <c r="C180" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="D180" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="E180" t="s">
-        <v>14</v>
+        <v>220</v>
       </c>
       <c r="F180">
-        <v>1981</v>
+        <v>2013</v>
       </c>
       <c r="H180" t="s">
         <v>16</v>
@@ -5987,13 +6014,22 @@
     </row>
     <row r="181" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
-        <v>283</v>
+        <v>13</v>
       </c>
       <c r="B181" t="s">
-        <v>124</v>
+        <v>25</v>
       </c>
       <c r="C181" s="2" t="s">
-        <v>284</v>
+        <v>38</v>
+      </c>
+      <c r="D181" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E181" t="s">
+        <v>14</v>
+      </c>
+      <c r="F181">
+        <v>1981</v>
       </c>
       <c r="H181" t="s">
         <v>16</v>
@@ -6002,8 +6038,25 @@
         <v>20</v>
       </c>
     </row>
+    <row r="182" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A182" t="s">
+        <v>283</v>
+      </c>
+      <c r="B182" t="s">
+        <v>124</v>
+      </c>
+      <c r="C182" s="2" t="s">
+        <v>284</v>
+      </c>
+      <c r="H182" t="s">
+        <v>16</v>
+      </c>
+      <c r="I182" t="s">
+        <v>20</v>
+      </c>
+    </row>
   </sheetData>
-  <sortState ref="A2:Q181">
+  <sortState ref="A2:Q182">
     <sortCondition ref="A2"/>
   </sortState>
   <hyperlinks>
@@ -6013,7 +6066,7 @@
     <hyperlink ref="C11" r:id="rId4"/>
     <hyperlink ref="C106" r:id="rId5"/>
     <hyperlink ref="C129" r:id="rId6"/>
-    <hyperlink ref="C180" r:id="rId7"/>
+    <hyperlink ref="C181" r:id="rId7"/>
     <hyperlink ref="C41" r:id="rId8"/>
     <hyperlink ref="C34" r:id="rId9"/>
     <hyperlink ref="C58" r:id="rId10"/>
@@ -6027,7 +6080,7 @@
     <hyperlink ref="C49" r:id="rId18"/>
     <hyperlink ref="C83" r:id="rId19"/>
     <hyperlink ref="C18" r:id="rId20"/>
-    <hyperlink ref="C167" r:id="rId21"/>
+    <hyperlink ref="C168" r:id="rId21"/>
     <hyperlink ref="C8" r:id="rId22"/>
     <hyperlink ref="C45" r:id="rId23"/>
     <hyperlink ref="C62" r:id="rId24"/>
@@ -6036,15 +6089,15 @@
     <hyperlink ref="C64" r:id="rId27"/>
     <hyperlink ref="C80" r:id="rId28"/>
     <hyperlink ref="C103" r:id="rId29"/>
-    <hyperlink ref="C156" r:id="rId30"/>
+    <hyperlink ref="C157" r:id="rId30"/>
     <hyperlink ref="C109" r:id="rId31"/>
     <hyperlink ref="C93" r:id="rId32"/>
     <hyperlink ref="C116" r:id="rId33"/>
     <hyperlink ref="C81" r:id="rId34"/>
     <hyperlink ref="C19" r:id="rId35"/>
-    <hyperlink ref="C154" r:id="rId36"/>
+    <hyperlink ref="C155" r:id="rId36"/>
     <hyperlink ref="C17" r:id="rId37"/>
-    <hyperlink ref="C177" r:id="rId38"/>
+    <hyperlink ref="C178" r:id="rId38"/>
     <hyperlink ref="C97" r:id="rId39"/>
     <hyperlink ref="C66" r:id="rId40"/>
     <hyperlink ref="C136" r:id="rId41"/>
@@ -6052,10 +6105,10 @@
     <hyperlink ref="C60" r:id="rId43"/>
     <hyperlink ref="C27" r:id="rId44"/>
     <hyperlink ref="C125" r:id="rId45"/>
-    <hyperlink ref="C174" r:id="rId46"/>
+    <hyperlink ref="C175" r:id="rId46"/>
     <hyperlink ref="C31" r:id="rId47" display="http://comparativeconstitutionsproject.org/"/>
     <hyperlink ref="C122" r:id="rId48"/>
-    <hyperlink ref="C170" r:id="rId49"/>
+    <hyperlink ref="C171" r:id="rId49"/>
     <hyperlink ref="C140" r:id="rId50"/>
     <hyperlink ref="C134" r:id="rId51"/>
     <hyperlink ref="C26" r:id="rId52"/>
@@ -6067,22 +6120,22 @@
     <hyperlink ref="C111" r:id="rId58"/>
     <hyperlink ref="C145" r:id="rId59"/>
     <hyperlink ref="C35" r:id="rId60"/>
-    <hyperlink ref="C158" r:id="rId61"/>
+    <hyperlink ref="C159" r:id="rId61"/>
     <hyperlink ref="C9" r:id="rId62"/>
     <hyperlink ref="C37" r:id="rId63"/>
-    <hyperlink ref="C160" r:id="rId64"/>
+    <hyperlink ref="C161" r:id="rId64"/>
     <hyperlink ref="C16" r:id="rId65"/>
-    <hyperlink ref="C172" r:id="rId66"/>
+    <hyperlink ref="C173" r:id="rId66"/>
     <hyperlink ref="C29" r:id="rId67"/>
     <hyperlink ref="C28" r:id="rId68"/>
     <hyperlink ref="C30" r:id="rId69"/>
     <hyperlink ref="C61" r:id="rId70"/>
-    <hyperlink ref="C175" r:id="rId71"/>
+    <hyperlink ref="C176" r:id="rId71"/>
     <hyperlink ref="C32" r:id="rId72"/>
     <hyperlink ref="C130" r:id="rId73"/>
     <hyperlink ref="C36" r:id="rId74"/>
     <hyperlink ref="C53" r:id="rId75"/>
-    <hyperlink ref="C148" r:id="rId76"/>
+    <hyperlink ref="C149" r:id="rId76"/>
     <hyperlink ref="C50" r:id="rId77"/>
     <hyperlink ref="C46" r:id="rId78"/>
     <hyperlink ref="C77" r:id="rId79"/>
@@ -6091,18 +6144,18 @@
     <hyperlink ref="C13" r:id="rId82"/>
     <hyperlink ref="C121" r:id="rId83"/>
     <hyperlink ref="C132" r:id="rId84"/>
-    <hyperlink ref="C162" r:id="rId85"/>
+    <hyperlink ref="C163" r:id="rId85"/>
     <hyperlink ref="C42" r:id="rId86"/>
-    <hyperlink ref="C173" r:id="rId87"/>
+    <hyperlink ref="C174" r:id="rId87"/>
     <hyperlink ref="C52" r:id="rId88"/>
-    <hyperlink ref="C179" r:id="rId89"/>
+    <hyperlink ref="C180" r:id="rId89"/>
     <hyperlink ref="C107" r:id="rId90"/>
     <hyperlink ref="C74" r:id="rId91"/>
     <hyperlink ref="C108" r:id="rId92"/>
-    <hyperlink ref="C151" r:id="rId93"/>
+    <hyperlink ref="C152" r:id="rId93"/>
     <hyperlink ref="C91" r:id="rId94"/>
     <hyperlink ref="C113" r:id="rId95"/>
-    <hyperlink ref="C152" r:id="rId96"/>
+    <hyperlink ref="C153" r:id="rId96"/>
     <hyperlink ref="C70" r:id="rId97"/>
     <hyperlink ref="C128" r:id="rId98"/>
     <hyperlink ref="C54" r:id="rId99"/>
@@ -6115,36 +6168,36 @@
     <hyperlink ref="C118" r:id="rId106"/>
     <hyperlink ref="C55" r:id="rId107"/>
     <hyperlink ref="C95" r:id="rId108"/>
-    <hyperlink ref="C150" r:id="rId109"/>
+    <hyperlink ref="C151" r:id="rId109"/>
     <hyperlink ref="C15" r:id="rId110"/>
     <hyperlink ref="C4" r:id="rId111"/>
-    <hyperlink ref="C178" r:id="rId112"/>
+    <hyperlink ref="C179" r:id="rId112"/>
     <hyperlink ref="C101" r:id="rId113"/>
     <hyperlink ref="C96" r:id="rId114"/>
-    <hyperlink ref="C165" r:id="rId115"/>
+    <hyperlink ref="C166" r:id="rId115"/>
     <hyperlink ref="C144" r:id="rId116"/>
     <hyperlink ref="C72" r:id="rId117"/>
     <hyperlink ref="C110" r:id="rId118"/>
     <hyperlink ref="C85" r:id="rId119"/>
-    <hyperlink ref="C181" r:id="rId120"/>
+    <hyperlink ref="C182" r:id="rId120"/>
     <hyperlink ref="C75" r:id="rId121"/>
     <hyperlink ref="C142" r:id="rId122"/>
     <hyperlink ref="C117" r:id="rId123"/>
     <hyperlink ref="C89" r:id="rId124"/>
     <hyperlink ref="C115" r:id="rId125"/>
-    <hyperlink ref="C149" r:id="rId126"/>
+    <hyperlink ref="C150" r:id="rId126"/>
     <hyperlink ref="C99" r:id="rId127"/>
     <hyperlink ref="C12" r:id="rId128"/>
     <hyperlink ref="C21" r:id="rId129"/>
     <hyperlink ref="C141" r:id="rId130"/>
     <hyperlink ref="C84" r:id="rId131"/>
-    <hyperlink ref="C157" r:id="rId132"/>
+    <hyperlink ref="C158" r:id="rId132"/>
     <hyperlink ref="C138" r:id="rId133"/>
     <hyperlink ref="C137" r:id="rId134"/>
     <hyperlink ref="C139" r:id="rId135"/>
-    <hyperlink ref="C164" r:id="rId136"/>
-    <hyperlink ref="C155" r:id="rId137"/>
-    <hyperlink ref="C171" r:id="rId138"/>
+    <hyperlink ref="C165" r:id="rId136"/>
+    <hyperlink ref="C156" r:id="rId137"/>
+    <hyperlink ref="C172" r:id="rId138"/>
     <hyperlink ref="C44" r:id="rId139"/>
     <hyperlink ref="C100" r:id="rId140"/>
     <hyperlink ref="J2" r:id="rId141"/>
@@ -6161,16 +6214,16 @@
     <hyperlink ref="M8" r:id="rId152"/>
     <hyperlink ref="L8" r:id="rId153"/>
     <hyperlink ref="J8" r:id="rId154"/>
-    <hyperlink ref="C169" r:id="rId155"/>
-    <hyperlink ref="N169" r:id="rId156"/>
+    <hyperlink ref="C170" r:id="rId155"/>
+    <hyperlink ref="N170" r:id="rId156"/>
     <hyperlink ref="C23" r:id="rId157"/>
     <hyperlink ref="N23" r:id="rId158"/>
     <hyperlink ref="C71" r:id="rId159"/>
-    <hyperlink ref="C163" r:id="rId160"/>
-    <hyperlink ref="J163" r:id="rId161"/>
-    <hyperlink ref="C161" r:id="rId162"/>
-    <hyperlink ref="N161" r:id="rId163"/>
-    <hyperlink ref="J161" r:id="rId164"/>
+    <hyperlink ref="C164" r:id="rId160"/>
+    <hyperlink ref="J164" r:id="rId161"/>
+    <hyperlink ref="C162" r:id="rId162"/>
+    <hyperlink ref="N162" r:id="rId163"/>
+    <hyperlink ref="J162" r:id="rId164"/>
     <hyperlink ref="C104" r:id="rId165"/>
     <hyperlink ref="C102" r:id="rId166"/>
     <hyperlink ref="C47" r:id="rId167"/>
@@ -6180,7 +6233,7 @@
     <hyperlink ref="N112" r:id="rId171"/>
     <hyperlink ref="C86" r:id="rId172"/>
     <hyperlink ref="K86" r:id="rId173"/>
-    <hyperlink ref="C176" r:id="rId174"/>
+    <hyperlink ref="C177" r:id="rId174"/>
     <hyperlink ref="C133" r:id="rId175"/>
     <hyperlink ref="K133" r:id="rId176"/>
     <hyperlink ref="L9" r:id="rId177"/>
@@ -6197,7 +6250,7 @@
     <hyperlink ref="C73" r:id="rId188"/>
     <hyperlink ref="J73" r:id="rId189"/>
     <hyperlink ref="N73" r:id="rId190"/>
-    <hyperlink ref="C153" r:id="rId191"/>
+    <hyperlink ref="C154" r:id="rId191"/>
     <hyperlink ref="C105" r:id="rId192"/>
     <hyperlink ref="J105" r:id="rId193"/>
     <hyperlink ref="L105" r:id="rId194"/>
@@ -6226,14 +6279,14 @@
     <hyperlink ref="M48" r:id="rId217"/>
     <hyperlink ref="N48" r:id="rId218"/>
     <hyperlink ref="C24" r:id="rId219"/>
-    <hyperlink ref="C168" r:id="rId220"/>
+    <hyperlink ref="C169" r:id="rId220"/>
     <hyperlink ref="C40" r:id="rId221"/>
     <hyperlink ref="J40" r:id="rId222"/>
     <hyperlink ref="N40" r:id="rId223"/>
     <hyperlink ref="L40" r:id="rId224"/>
     <hyperlink ref="K40" r:id="rId225"/>
-    <hyperlink ref="C166" r:id="rId226"/>
-    <hyperlink ref="P166" r:id="rId227"/>
+    <hyperlink ref="C167" r:id="rId226"/>
+    <hyperlink ref="P167" r:id="rId227"/>
     <hyperlink ref="C114" r:id="rId228"/>
     <hyperlink ref="C131" r:id="rId229"/>
     <hyperlink ref="P131" r:id="rId230"/>
@@ -6251,12 +6304,15 @@
     <hyperlink ref="C127" r:id="rId242"/>
     <hyperlink ref="N127" r:id="rId243"/>
     <hyperlink ref="J127" r:id="rId244"/>
-    <hyperlink ref="C159" r:id="rId245"/>
-    <hyperlink ref="J159" r:id="rId246"/>
+    <hyperlink ref="C160" r:id="rId245"/>
+    <hyperlink ref="J160" r:id="rId246"/>
     <hyperlink ref="C119" r:id="rId247"/>
     <hyperlink ref="C14" r:id="rId248"/>
     <hyperlink ref="J14" r:id="rId249"/>
     <hyperlink ref="P14" r:id="rId250"/>
+    <hyperlink ref="C148" r:id="rId251"/>
+    <hyperlink ref="J148" r:id="rId252"/>
+    <hyperlink ref="P148" r:id="rId253"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
update information on Global Terrorism Database
</commit_message>
<xml_diff>
--- a/PolData.xlsx
+++ b/PolData.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1062" uniqueCount="582">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1066" uniqueCount="584">
   <si>
     <t>name</t>
   </si>
@@ -1773,6 +1773,12 @@
   </si>
   <si>
     <t>http://nesstar.ada.edu.au/webview/velocity?study=http://150.203.254.120:80/obj/fStudy/au.edu.anu.ada.ddi.00009&amp;format=pdf&amp;mode=transform&amp;s&amp;gs</t>
+  </si>
+  <si>
+    <t>http://www.start.umd.edu/gtd/downloads/Codebook.pdf</t>
+  </si>
+  <si>
+    <t>Terror, victims, attacks, casualties</t>
   </si>
 </sst>
 </file>
@@ -2114,8 +2120,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q186"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView tabSelected="1" topLeftCell="A65" workbookViewId="0">
+      <selection activeCell="A91" sqref="A91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4216,8 +4222,26 @@
       <c r="C91" s="2" t="s">
         <v>152</v>
       </c>
+      <c r="D91" t="s">
+        <v>583</v>
+      </c>
       <c r="E91" t="s">
         <v>14</v>
+      </c>
+      <c r="F91">
+        <v>1970</v>
+      </c>
+      <c r="G91">
+        <v>2015</v>
+      </c>
+      <c r="H91" t="s">
+        <v>348</v>
+      </c>
+      <c r="I91" t="s">
+        <v>249</v>
+      </c>
+      <c r="J91" s="2" t="s">
+        <v>582</v>
       </c>
     </row>
     <row r="92" spans="1:17" x14ac:dyDescent="0.2">
@@ -6531,6 +6555,7 @@
     <hyperlink ref="J12" r:id="rId263"/>
     <hyperlink ref="M15" r:id="rId264"/>
     <hyperlink ref="J15" r:id="rId265"/>
+    <hyperlink ref="J91" r:id="rId266"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
add 'Democracy Barometer' and 'Suicide Attack Database'
</commit_message>
<xml_diff>
--- a/PolData.xlsx
+++ b/PolData.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1066" uniqueCount="584">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1083" uniqueCount="593">
   <si>
     <t>name</t>
   </si>
@@ -1779,6 +1779,33 @@
   </si>
   <si>
     <t>Terror, victims, attacks, casualties</t>
+  </si>
+  <si>
+    <t>Suicide Attack Database</t>
+  </si>
+  <si>
+    <t>http://cpostdata.uchicago.edu/search_new.php</t>
+  </si>
+  <si>
+    <t>Suicide attacks, victims, campaign, weapon, target type</t>
+  </si>
+  <si>
+    <t>Democracy Barometer</t>
+  </si>
+  <si>
+    <t>http://www.democracybarometer.org/dataset_en.html</t>
+  </si>
+  <si>
+    <t>Democracy, freedom, control, equality</t>
+  </si>
+  <si>
+    <t>http://www.democracybarometer.org/Data/Codebook_all%20countries_1990-2014.pdf</t>
+  </si>
+  <si>
+    <t>http://www.democracybarometer.org/Data/DB_data_1990-2014_Standardized.dta</t>
+  </si>
+  <si>
+    <t>http://www.democracybarometer.org/Data/DB_data_1990-2014_Standardized.xlsx</t>
   </si>
 </sst>
 </file>
@@ -2118,10 +2145,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q186"/>
+  <dimension ref="A1:Q188"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A65" workbookViewId="0">
-      <selection activeCell="A91" sqref="A91"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A194" sqref="A194"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3434,16 +3461,25 @@
     </row>
     <row r="52" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>489</v>
+        <v>587</v>
       </c>
       <c r="B52" t="s">
         <v>60</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>488</v>
+        <v>588</v>
+      </c>
+      <c r="D52" t="s">
+        <v>589</v>
       </c>
       <c r="E52" t="s">
-        <v>490</v>
+        <v>14</v>
+      </c>
+      <c r="F52">
+        <v>1990</v>
+      </c>
+      <c r="G52">
+        <v>2014</v>
       </c>
       <c r="H52" t="s">
         <v>348</v>
@@ -3452,81 +3488,87 @@
         <v>349</v>
       </c>
       <c r="J52" s="2" t="s">
-        <v>491</v>
-      </c>
-      <c r="K52" s="2" t="s">
-        <v>492</v>
+        <v>590</v>
       </c>
       <c r="L52" s="2" t="s">
-        <v>493</v>
-      </c>
-      <c r="M52" s="2" t="s">
-        <v>494</v>
+        <v>591</v>
       </c>
       <c r="N52" s="2" t="s">
-        <v>495</v>
+        <v>592</v>
       </c>
     </row>
     <row r="53" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>59</v>
+        <v>489</v>
       </c>
       <c r="B53" t="s">
         <v>60</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>61</v>
+        <v>488</v>
+      </c>
+      <c r="E53" t="s">
+        <v>490</v>
+      </c>
+      <c r="H53" t="s">
+        <v>348</v>
+      </c>
+      <c r="I53" t="s">
+        <v>349</v>
+      </c>
+      <c r="J53" s="2" t="s">
+        <v>491</v>
+      </c>
+      <c r="K53" s="2" t="s">
+        <v>492</v>
+      </c>
+      <c r="L53" s="2" t="s">
+        <v>493</v>
+      </c>
+      <c r="M53" s="2" t="s">
+        <v>494</v>
+      </c>
+      <c r="N53" s="2" t="s">
+        <v>495</v>
       </c>
     </row>
     <row r="54" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>196</v>
+        <v>59</v>
       </c>
       <c r="B54" t="s">
-        <v>165</v>
+        <v>60</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>195</v>
-      </c>
-      <c r="F54">
-        <v>1946</v>
-      </c>
-      <c r="G54">
-        <v>2016</v>
+        <v>61</v>
       </c>
     </row>
     <row r="55" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>238</v>
+        <v>196</v>
       </c>
       <c r="B55" t="s">
-        <v>237</v>
+        <v>165</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>243</v>
-      </c>
-      <c r="H55" t="s">
-        <v>16</v>
-      </c>
-      <c r="I55" t="s">
-        <v>20</v>
+        <v>195</v>
+      </c>
+      <c r="F55">
+        <v>1946</v>
+      </c>
+      <c r="G55">
+        <v>2016</v>
       </c>
     </row>
     <row r="56" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>219</v>
+        <v>238</v>
       </c>
       <c r="B56" t="s">
-        <v>124</v>
+        <v>237</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>218</v>
-      </c>
-      <c r="F56">
-        <v>1970</v>
-      </c>
-      <c r="G56">
-        <v>2015</v>
+        <v>243</v>
       </c>
       <c r="H56" t="s">
         <v>16</v>
@@ -3537,44 +3579,50 @@
     </row>
     <row r="57" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>191</v>
+        <v>219</v>
       </c>
       <c r="B57" t="s">
-        <v>25</v>
+        <v>124</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="E57" t="s">
-        <v>192</v>
+        <v>218</v>
+      </c>
+      <c r="F57">
+        <v>1970</v>
+      </c>
+      <c r="G57">
+        <v>2015</v>
+      </c>
+      <c r="H57" t="s">
+        <v>16</v>
+      </c>
+      <c r="I57" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="58" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>235</v>
+        <v>191</v>
       </c>
       <c r="B58" t="s">
-        <v>60</v>
+        <v>25</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>236</v>
-      </c>
-      <c r="H58" t="s">
-        <v>16</v>
-      </c>
-      <c r="I58" t="s">
-        <v>20</v>
+        <v>190</v>
+      </c>
+      <c r="E58" t="s">
+        <v>192</v>
       </c>
     </row>
     <row r="59" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>252</v>
+        <v>235</v>
       </c>
       <c r="B59" t="s">
-        <v>250</v>
+        <v>60</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>251</v>
+        <v>236</v>
       </c>
       <c r="H59" t="s">
         <v>16</v>
@@ -3585,129 +3633,129 @@
     </row>
     <row r="60" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>149</v>
+        <v>252</v>
       </c>
       <c r="B60" t="s">
-        <v>128</v>
+        <v>250</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>150</v>
+        <v>251</v>
+      </c>
+      <c r="H60" t="s">
+        <v>16</v>
+      </c>
+      <c r="I60" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="61" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>462</v>
+        <v>149</v>
       </c>
       <c r="B61" t="s">
-        <v>250</v>
+        <v>128</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>464</v>
-      </c>
-      <c r="D61" t="s">
-        <v>463</v>
-      </c>
-      <c r="E61" t="s">
-        <v>14</v>
-      </c>
-      <c r="F61">
-        <v>1946</v>
-      </c>
-      <c r="G61">
-        <v>2010</v>
-      </c>
-      <c r="H61" t="s">
-        <v>348</v>
-      </c>
-      <c r="I61" t="s">
-        <v>349</v>
-      </c>
-      <c r="J61" s="2" t="s">
-        <v>467</v>
-      </c>
-      <c r="K61" s="2" t="s">
-        <v>466</v>
-      </c>
-      <c r="L61" s="2" t="s">
-        <v>465</v>
+        <v>150</v>
       </c>
     </row>
     <row r="62" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>28</v>
+        <v>462</v>
       </c>
       <c r="B62" t="s">
-        <v>25</v>
+        <v>250</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>48</v>
+        <v>464</v>
+      </c>
+      <c r="D62" t="s">
+        <v>463</v>
+      </c>
+      <c r="E62" t="s">
+        <v>14</v>
+      </c>
+      <c r="F62">
+        <v>1946</v>
+      </c>
+      <c r="G62">
+        <v>2010</v>
+      </c>
+      <c r="H62" t="s">
+        <v>348</v>
+      </c>
+      <c r="I62" t="s">
+        <v>349</v>
+      </c>
+      <c r="J62" s="2" t="s">
+        <v>467</v>
+      </c>
+      <c r="K62" s="2" t="s">
+        <v>466</v>
+      </c>
+      <c r="L62" s="2" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="63" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>80</v>
+        <v>28</v>
       </c>
       <c r="B63" t="s">
-        <v>128</v>
+        <v>25</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="E63" t="s">
-        <v>9</v>
-      </c>
-      <c r="F63">
-        <v>1979</v>
+        <v>48</v>
       </c>
     </row>
     <row r="64" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>125</v>
+        <v>80</v>
       </c>
       <c r="B64" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>126</v>
+        <v>81</v>
+      </c>
+      <c r="E64" t="s">
+        <v>9</v>
+      </c>
+      <c r="F64">
+        <v>1979</v>
       </c>
     </row>
     <row r="65" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>179</v>
+        <v>125</v>
       </c>
       <c r="B65" t="s">
-        <v>165</v>
+        <v>124</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>180</v>
+        <v>126</v>
       </c>
     </row>
     <row r="66" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
+        <v>179</v>
+      </c>
+      <c r="B66" t="s">
+        <v>165</v>
+      </c>
+      <c r="C66" s="2" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="67" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
         <v>78</v>
       </c>
-      <c r="B66" t="s">
+      <c r="B67" t="s">
         <v>25</v>
       </c>
-      <c r="C66" s="2" t="s">
+      <c r="C67" s="2" t="s">
         <v>79</v>
-      </c>
-      <c r="E66" t="s">
-        <v>9</v>
-      </c>
-      <c r="F66">
-        <v>1979</v>
-      </c>
-    </row>
-    <row r="67" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A67" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="B67" t="s">
-        <v>83</v>
-      </c>
-      <c r="C67" s="2" t="s">
-        <v>84</v>
       </c>
       <c r="E67" t="s">
         <v>9</v>
@@ -3718,13 +3766,13 @@
     </row>
     <row r="68" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A68" s="3" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B68" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="E68" t="s">
         <v>9</v>
@@ -3732,225 +3780,225 @@
       <c r="F68">
         <v>1979</v>
       </c>
-      <c r="G68">
+    </row>
+    <row r="69" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A69" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="B69" t="s">
+        <v>86</v>
+      </c>
+      <c r="C69" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="E69" t="s">
+        <v>9</v>
+      </c>
+      <c r="F69">
+        <v>1979</v>
+      </c>
+      <c r="G69">
         <v>2009</v>
-      </c>
-    </row>
-    <row r="69" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A69" t="s">
-        <v>27</v>
-      </c>
-      <c r="B69" t="s">
-        <v>25</v>
-      </c>
-      <c r="C69" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="Q69" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="70" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>120</v>
+        <v>27</v>
       </c>
       <c r="B70" t="s">
-        <v>259</v>
+        <v>25</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="I70" t="s">
-        <v>20</v>
+        <v>49</v>
+      </c>
+      <c r="Q70" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="71" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>5</v>
+        <v>120</v>
       </c>
       <c r="B71" t="s">
-        <v>25</v>
+        <v>259</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D71" t="s">
-        <v>94</v>
-      </c>
-      <c r="E71" t="s">
-        <v>9</v>
-      </c>
-      <c r="F71">
-        <v>2002</v>
-      </c>
-      <c r="H71" t="s">
-        <v>16</v>
+        <v>119</v>
       </c>
       <c r="I71" t="s">
-        <v>248</v>
-      </c>
-      <c r="Q71" t="s">
-        <v>44</v>
+        <v>20</v>
       </c>
     </row>
     <row r="72" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>240</v>
+        <v>5</v>
       </c>
       <c r="B72" t="s">
-        <v>237</v>
+        <v>25</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>243</v>
+        <v>6</v>
+      </c>
+      <c r="D72" t="s">
+        <v>94</v>
+      </c>
+      <c r="E72" t="s">
+        <v>9</v>
+      </c>
+      <c r="F72">
+        <v>2002</v>
       </c>
       <c r="H72" t="s">
         <v>16</v>
       </c>
       <c r="I72" t="s">
+        <v>248</v>
+      </c>
+      <c r="Q72" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="73" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A73" t="s">
+        <v>240</v>
+      </c>
+      <c r="B73" t="s">
+        <v>237</v>
+      </c>
+      <c r="C73" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="H73" t="s">
+        <v>16</v>
+      </c>
+      <c r="I73" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="73" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A73" s="1" t="s">
+    <row r="74" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A74" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B73" t="s">
+      <c r="B74" t="s">
         <v>25</v>
       </c>
-      <c r="C73" s="2" t="s">
+      <c r="C74" s="2" t="s">
         <v>52</v>
-      </c>
-    </row>
-    <row r="74" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A74" t="s">
-        <v>232</v>
-      </c>
-      <c r="B74" t="s">
-        <v>250</v>
-      </c>
-      <c r="C74" s="2" t="s">
-        <v>231</v>
       </c>
     </row>
     <row r="75" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>390</v>
+        <v>232</v>
       </c>
       <c r="B75" t="s">
-        <v>83</v>
+        <v>250</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>392</v>
-      </c>
-      <c r="D75" t="s">
-        <v>391</v>
-      </c>
-      <c r="E75" t="s">
-        <v>9</v>
-      </c>
-      <c r="F75">
-        <v>2007</v>
-      </c>
-      <c r="G75">
-        <v>2015</v>
-      </c>
-      <c r="H75" t="s">
-        <v>348</v>
-      </c>
-      <c r="I75" t="s">
-        <v>349</v>
-      </c>
-      <c r="Q75" t="s">
-        <v>393</v>
+        <v>231</v>
       </c>
     </row>
     <row r="76" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>276</v>
+        <v>390</v>
       </c>
       <c r="B76" t="s">
-        <v>124</v>
+        <v>83</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>277</v>
+        <v>392</v>
+      </c>
+      <c r="D76" t="s">
+        <v>391</v>
+      </c>
+      <c r="E76" t="s">
+        <v>9</v>
       </c>
       <c r="F76">
-        <v>1948</v>
+        <v>2007</v>
       </c>
       <c r="G76">
-        <v>2000</v>
+        <v>2015</v>
       </c>
       <c r="H76" t="s">
-        <v>16</v>
+        <v>348</v>
       </c>
       <c r="I76" t="s">
-        <v>20</v>
+        <v>349</v>
+      </c>
+      <c r="Q76" t="s">
+        <v>393</v>
       </c>
     </row>
     <row r="77" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>449</v>
+        <v>276</v>
       </c>
       <c r="B77" t="s">
-        <v>250</v>
+        <v>124</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>448</v>
-      </c>
-      <c r="E77" t="s">
-        <v>14</v>
+        <v>277</v>
       </c>
       <c r="F77">
-        <v>-4000</v>
+        <v>1948</v>
       </c>
       <c r="G77">
         <v>2000</v>
       </c>
       <c r="H77" t="s">
-        <v>348</v>
+        <v>16</v>
       </c>
       <c r="I77" t="s">
-        <v>349</v>
-      </c>
-      <c r="J77" s="2" t="s">
-        <v>450</v>
-      </c>
-      <c r="N77" s="2" t="s">
-        <v>451</v>
+        <v>20</v>
       </c>
     </row>
     <row r="78" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>224</v>
+        <v>449</v>
       </c>
       <c r="B78" t="s">
-        <v>40</v>
+        <v>250</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>225</v>
+        <v>448</v>
+      </c>
+      <c r="E78" t="s">
+        <v>14</v>
       </c>
       <c r="F78">
-        <v>1964</v>
+        <v>-4000</v>
       </c>
       <c r="G78">
-        <v>2008</v>
+        <v>2000</v>
       </c>
       <c r="H78" t="s">
-        <v>16</v>
+        <v>348</v>
       </c>
       <c r="I78" t="s">
-        <v>20</v>
+        <v>349</v>
+      </c>
+      <c r="J78" s="2" t="s">
+        <v>450</v>
+      </c>
+      <c r="N78" s="2" t="s">
+        <v>451</v>
       </c>
     </row>
     <row r="79" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>285</v>
+        <v>224</v>
       </c>
       <c r="B79" t="s">
-        <v>250</v>
+        <v>40</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>286</v>
+        <v>225</v>
+      </c>
+      <c r="F79">
+        <v>1964</v>
+      </c>
+      <c r="G79">
+        <v>2008</v>
       </c>
       <c r="H79" t="s">
         <v>16</v>
@@ -3961,94 +4009,76 @@
     </row>
     <row r="80" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>205</v>
+        <v>285</v>
       </c>
       <c r="B80" t="s">
-        <v>40</v>
+        <v>250</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>204</v>
-      </c>
-      <c r="F80">
-        <v>2006</v>
+        <v>286</v>
+      </c>
+      <c r="H80" t="s">
+        <v>16</v>
+      </c>
+      <c r="I80" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="81" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>200</v>
+        <v>205</v>
       </c>
       <c r="B81" t="s">
-        <v>99</v>
+        <v>40</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="F81">
-        <v>1980</v>
-      </c>
-      <c r="G81">
-        <v>2007</v>
-      </c>
-      <c r="Q81" t="s">
-        <v>18</v>
+        <v>2006</v>
       </c>
     </row>
     <row r="82" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>521</v>
+        <v>200</v>
       </c>
       <c r="B82" t="s">
-        <v>165</v>
+        <v>99</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>520</v>
-      </c>
-      <c r="D82" t="s">
-        <v>525</v>
-      </c>
-      <c r="E82" t="s">
-        <v>14</v>
+        <v>201</v>
       </c>
       <c r="F82">
-        <v>1975</v>
+        <v>1980</v>
       </c>
       <c r="G82">
-        <v>2012</v>
-      </c>
-      <c r="H82" t="s">
-        <v>348</v>
-      </c>
-      <c r="I82" t="s">
-        <v>349</v>
-      </c>
-      <c r="J82" s="2" t="s">
-        <v>522</v>
-      </c>
-      <c r="K82" s="2" t="s">
-        <v>523</v>
-      </c>
-      <c r="N82" s="2" t="s">
-        <v>524</v>
+        <v>2007</v>
+      </c>
+      <c r="Q82" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="83" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>468</v>
+        <v>521</v>
       </c>
       <c r="B83" t="s">
-        <v>40</v>
+        <v>165</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>464</v>
+        <v>520</v>
+      </c>
+      <c r="D83" t="s">
+        <v>525</v>
       </c>
       <c r="E83" t="s">
         <v>14</v>
       </c>
       <c r="F83">
-        <v>1816</v>
+        <v>1975</v>
       </c>
       <c r="G83">
-        <v>2001</v>
+        <v>2012</v>
       </c>
       <c r="H83" t="s">
         <v>348</v>
@@ -4057,219 +4087,237 @@
         <v>349</v>
       </c>
       <c r="J83" s="2" t="s">
-        <v>469</v>
+        <v>522</v>
       </c>
       <c r="K83" s="2" t="s">
-        <v>470</v>
-      </c>
-      <c r="L83" s="2" t="s">
-        <v>471</v>
+        <v>523</v>
+      </c>
+      <c r="N83" s="2" t="s">
+        <v>524</v>
       </c>
     </row>
     <row r="84" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>89</v>
+        <v>468</v>
       </c>
       <c r="B84" t="s">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>88</v>
+        <v>464</v>
       </c>
       <c r="E84" t="s">
-        <v>34</v>
+        <v>14</v>
       </c>
       <c r="F84">
-        <v>1972</v>
+        <v>1816</v>
+      </c>
+      <c r="G84">
+        <v>2001</v>
       </c>
       <c r="H84" t="s">
-        <v>16</v>
+        <v>348</v>
       </c>
       <c r="I84" t="s">
-        <v>20</v>
+        <v>349</v>
+      </c>
+      <c r="J84" s="2" t="s">
+        <v>469</v>
+      </c>
+      <c r="K84" s="2" t="s">
+        <v>470</v>
+      </c>
+      <c r="L84" s="2" t="s">
+        <v>471</v>
       </c>
     </row>
     <row r="85" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>104</v>
+        <v>89</v>
       </c>
       <c r="B85" t="s">
         <v>25</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>106</v>
+        <v>88</v>
       </c>
       <c r="E85" t="s">
-        <v>105</v>
+        <v>34</v>
       </c>
       <c r="F85">
-        <v>1980</v>
+        <v>1972</v>
+      </c>
+      <c r="H85" t="s">
+        <v>16</v>
+      </c>
+      <c r="I85" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="86" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>460</v>
+        <v>104</v>
       </c>
       <c r="B86" t="s">
         <v>25</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>461</v>
-      </c>
-      <c r="D86" t="s">
-        <v>363</v>
+        <v>106</v>
       </c>
       <c r="E86" t="s">
         <v>105</v>
       </c>
       <c r="F86">
-        <v>2009</v>
-      </c>
-      <c r="H86" t="s">
-        <v>348</v>
-      </c>
-      <c r="I86" t="s">
-        <v>301</v>
+        <v>1980</v>
       </c>
     </row>
     <row r="87" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>62</v>
+        <v>460</v>
       </c>
       <c r="B87" t="s">
         <v>25</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>63</v>
+        <v>461</v>
+      </c>
+      <c r="D87" t="s">
+        <v>363</v>
+      </c>
+      <c r="E87" t="s">
+        <v>105</v>
+      </c>
+      <c r="F87">
+        <v>2009</v>
+      </c>
+      <c r="H87" t="s">
+        <v>348</v>
+      </c>
+      <c r="I87" t="s">
+        <v>301</v>
       </c>
     </row>
     <row r="88" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>311</v>
+        <v>62</v>
       </c>
       <c r="B88" t="s">
-        <v>165</v>
+        <v>25</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>312</v>
-      </c>
-      <c r="E88" t="s">
-        <v>14</v>
-      </c>
-      <c r="H88" t="s">
-        <v>16</v>
-      </c>
-      <c r="I88" t="s">
-        <v>301</v>
+        <v>63</v>
       </c>
     </row>
     <row r="89" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>281</v>
+        <v>311</v>
       </c>
       <c r="B89" t="s">
-        <v>237</v>
+        <v>165</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>282</v>
+        <v>312</v>
+      </c>
+      <c r="E89" t="s">
+        <v>14</v>
       </c>
       <c r="H89" t="s">
         <v>16</v>
       </c>
       <c r="I89" t="s">
-        <v>20</v>
+        <v>301</v>
       </c>
     </row>
     <row r="90" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>418</v>
+        <v>281</v>
       </c>
       <c r="B90" t="s">
-        <v>86</v>
+        <v>237</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>419</v>
-      </c>
-      <c r="E90" t="s">
-        <v>420</v>
-      </c>
-      <c r="F90">
-        <v>1948</v>
-      </c>
-      <c r="G90">
-        <v>2012</v>
+        <v>282</v>
       </c>
       <c r="H90" t="s">
-        <v>348</v>
+        <v>16</v>
       </c>
       <c r="I90" t="s">
-        <v>349</v>
-      </c>
-      <c r="K90" s="2" t="s">
-        <v>421</v>
-      </c>
-      <c r="Q90" t="s">
-        <v>422</v>
+        <v>20</v>
       </c>
     </row>
     <row r="91" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>151</v>
+        <v>418</v>
       </c>
       <c r="B91" t="s">
-        <v>40</v>
+        <v>86</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="D91" t="s">
-        <v>583</v>
+        <v>419</v>
       </c>
       <c r="E91" t="s">
-        <v>14</v>
+        <v>420</v>
       </c>
       <c r="F91">
-        <v>1970</v>
+        <v>1948</v>
       </c>
       <c r="G91">
-        <v>2015</v>
+        <v>2012</v>
       </c>
       <c r="H91" t="s">
         <v>348</v>
       </c>
       <c r="I91" t="s">
-        <v>249</v>
-      </c>
-      <c r="J91" s="2" t="s">
-        <v>582</v>
+        <v>349</v>
+      </c>
+      <c r="K91" s="2" t="s">
+        <v>421</v>
+      </c>
+      <c r="Q91" t="s">
+        <v>422</v>
       </c>
     </row>
     <row r="92" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>242</v>
+        <v>151</v>
       </c>
       <c r="B92" t="s">
-        <v>237</v>
+        <v>40</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>243</v>
+        <v>152</v>
+      </c>
+      <c r="D92" t="s">
+        <v>583</v>
+      </c>
+      <c r="E92" t="s">
+        <v>14</v>
+      </c>
+      <c r="F92">
+        <v>1970</v>
+      </c>
+      <c r="G92">
+        <v>2015</v>
       </c>
       <c r="H92" t="s">
-        <v>16</v>
+        <v>348</v>
       </c>
       <c r="I92" t="s">
-        <v>20</v>
+        <v>249</v>
+      </c>
+      <c r="J92" s="2" t="s">
+        <v>582</v>
       </c>
     </row>
     <row r="93" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>292</v>
+        <v>242</v>
       </c>
       <c r="B93" t="s">
-        <v>99</v>
+        <v>237</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>291</v>
+        <v>243</v>
       </c>
       <c r="H93" t="s">
         <v>16</v>
@@ -4280,47 +4328,47 @@
     </row>
     <row r="94" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>153</v>
+        <v>292</v>
       </c>
       <c r="B94" t="s">
-        <v>259</v>
+        <v>99</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>154</v>
+        <v>291</v>
+      </c>
+      <c r="H94" t="s">
+        <v>16</v>
+      </c>
+      <c r="I94" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="95" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>228</v>
+        <v>153</v>
       </c>
       <c r="B95" t="s">
-        <v>40</v>
+        <v>259</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>225</v>
-      </c>
-      <c r="F95">
-        <v>1989</v>
-      </c>
-      <c r="G95">
-        <v>2017</v>
-      </c>
-      <c r="H95" t="s">
-        <v>16</v>
-      </c>
-      <c r="I95" t="s">
-        <v>20</v>
+        <v>154</v>
       </c>
     </row>
     <row r="96" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>245</v>
+        <v>228</v>
       </c>
       <c r="B96" t="s">
-        <v>237</v>
+        <v>40</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>244</v>
+        <v>225</v>
+      </c>
+      <c r="F96">
+        <v>1989</v>
+      </c>
+      <c r="G96">
+        <v>2017</v>
       </c>
       <c r="H96" t="s">
         <v>16</v>
@@ -4331,50 +4379,41 @@
     </row>
     <row r="97" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>100</v>
+        <v>245</v>
       </c>
       <c r="B97" t="s">
-        <v>99</v>
+        <v>237</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>101</v>
+        <v>244</v>
+      </c>
+      <c r="H97" t="s">
+        <v>16</v>
+      </c>
+      <c r="I97" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="98" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>239</v>
+        <v>100</v>
       </c>
       <c r="B98" t="s">
-        <v>237</v>
+        <v>99</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>243</v>
-      </c>
-      <c r="H98" t="s">
-        <v>16</v>
-      </c>
-      <c r="I98" t="s">
-        <v>20</v>
+        <v>101</v>
       </c>
     </row>
     <row r="99" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>254</v>
+        <v>239</v>
       </c>
       <c r="B99" t="s">
-        <v>55</v>
+        <v>237</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>253</v>
-      </c>
-      <c r="E99" t="s">
-        <v>255</v>
-      </c>
-      <c r="F99">
-        <v>1960</v>
-      </c>
-      <c r="G99">
-        <v>2014</v>
+        <v>243</v>
       </c>
       <c r="H99" t="s">
         <v>16</v>
@@ -4385,19 +4424,22 @@
     </row>
     <row r="100" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>270</v>
+        <v>254</v>
       </c>
       <c r="B100" t="s">
         <v>55</v>
       </c>
       <c r="C100" s="2" t="s">
-        <v>271</v>
+        <v>253</v>
+      </c>
+      <c r="E100" t="s">
+        <v>255</v>
       </c>
       <c r="F100">
-        <v>1990</v>
+        <v>1960</v>
       </c>
       <c r="G100">
-        <v>2010</v>
+        <v>2014</v>
       </c>
       <c r="H100" t="s">
         <v>16</v>
@@ -4408,96 +4450,90 @@
     </row>
     <row r="101" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>117</v>
+        <v>270</v>
       </c>
       <c r="B101" t="s">
         <v>55</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>118</v>
+        <v>271</v>
+      </c>
+      <c r="F101">
+        <v>1990</v>
+      </c>
+      <c r="G101">
+        <v>2010</v>
+      </c>
+      <c r="H101" t="s">
+        <v>16</v>
       </c>
       <c r="I101" t="s">
         <v>20</v>
       </c>
-      <c r="Q101" t="s">
+    </row>
+    <row r="102" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A102" t="s">
+        <v>117</v>
+      </c>
+      <c r="B102" t="s">
+        <v>55</v>
+      </c>
+      <c r="C102" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="I102" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q102" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="102" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A102" s="1" t="s">
+    <row r="103" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A103" s="1" t="s">
         <v>23</v>
-      </c>
-      <c r="B102" t="s">
-        <v>25</v>
-      </c>
-      <c r="C102" s="2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="103" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A103" t="s">
-        <v>300</v>
       </c>
       <c r="B103" t="s">
         <v>25</v>
       </c>
       <c r="C103" s="2" t="s">
-        <v>298</v>
-      </c>
-      <c r="E103" t="s">
-        <v>299</v>
-      </c>
-      <c r="F103">
-        <v>1969</v>
-      </c>
-      <c r="H103" t="s">
-        <v>16</v>
-      </c>
-      <c r="I103" t="s">
-        <v>249</v>
+        <v>53</v>
       </c>
     </row>
     <row r="104" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>332</v>
+        <v>300</v>
       </c>
       <c r="B104" t="s">
-        <v>134</v>
+        <v>25</v>
       </c>
       <c r="C104" s="2" t="s">
-        <v>333</v>
+        <v>298</v>
       </c>
       <c r="E104" t="s">
-        <v>334</v>
+        <v>299</v>
+      </c>
+      <c r="F104">
+        <v>1969</v>
       </c>
       <c r="H104" t="s">
         <v>16</v>
       </c>
       <c r="I104" t="s">
-        <v>20</v>
+        <v>249</v>
       </c>
     </row>
     <row r="105" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>267</v>
+        <v>332</v>
       </c>
       <c r="B105" t="s">
-        <v>250</v>
+        <v>134</v>
       </c>
       <c r="C105" s="2" t="s">
-        <v>266</v>
-      </c>
-      <c r="D105" t="s">
-        <v>269</v>
+        <v>333</v>
       </c>
       <c r="E105" t="s">
-        <v>268</v>
-      </c>
-      <c r="F105">
-        <v>1970</v>
-      </c>
-      <c r="G105">
-        <v>2014</v>
+        <v>334</v>
       </c>
       <c r="H105" t="s">
         <v>16</v>
@@ -4508,97 +4544,100 @@
     </row>
     <row r="106" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>407</v>
+        <v>267</v>
       </c>
       <c r="B106" t="s">
-        <v>40</v>
+        <v>250</v>
       </c>
       <c r="C106" s="2" t="s">
-        <v>406</v>
+        <v>266</v>
       </c>
       <c r="D106" t="s">
-        <v>408</v>
+        <v>269</v>
       </c>
       <c r="E106" t="s">
-        <v>14</v>
+        <v>268</v>
       </c>
       <c r="F106">
-        <v>1949</v>
+        <v>1970</v>
       </c>
       <c r="G106">
-        <v>2013</v>
+        <v>2014</v>
       </c>
       <c r="H106" t="s">
-        <v>348</v>
+        <v>16</v>
       </c>
       <c r="I106" t="s">
-        <v>349</v>
+        <v>20</v>
       </c>
     </row>
     <row r="107" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>96</v>
+        <v>407</v>
       </c>
       <c r="B107" t="s">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="C107" s="2" t="s">
-        <v>90</v>
+        <v>406</v>
+      </c>
+      <c r="D107" t="s">
+        <v>408</v>
       </c>
       <c r="E107" t="s">
-        <v>69</v>
+        <v>14</v>
       </c>
       <c r="F107">
-        <v>1995</v>
+        <v>1949</v>
+      </c>
+      <c r="G107">
+        <v>2013</v>
+      </c>
+      <c r="H107" t="s">
+        <v>348</v>
+      </c>
+      <c r="I107" t="s">
+        <v>349</v>
       </c>
     </row>
     <row r="108" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>404</v>
+        <v>96</v>
       </c>
       <c r="B108" t="s">
-        <v>83</v>
+        <v>25</v>
       </c>
       <c r="C108" s="2" t="s">
-        <v>403</v>
-      </c>
-      <c r="D108" t="s">
-        <v>405</v>
+        <v>90</v>
       </c>
       <c r="E108" t="s">
-        <v>14</v>
+        <v>69</v>
       </c>
       <c r="F108">
-        <v>1875</v>
-      </c>
-      <c r="G108">
-        <v>2004</v>
-      </c>
-      <c r="H108" t="s">
-        <v>348</v>
-      </c>
-      <c r="I108" t="s">
-        <v>349</v>
+        <v>1995</v>
       </c>
     </row>
     <row r="109" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>454</v>
+        <v>404</v>
       </c>
       <c r="B109" t="s">
-        <v>25</v>
+        <v>83</v>
       </c>
       <c r="C109" s="2" t="s">
-        <v>455</v>
+        <v>403</v>
+      </c>
+      <c r="D109" t="s">
+        <v>405</v>
       </c>
       <c r="E109" t="s">
-        <v>456</v>
+        <v>14</v>
       </c>
       <c r="F109">
-        <v>2006</v>
+        <v>1875</v>
       </c>
       <c r="G109">
-        <v>2016</v>
+        <v>2004</v>
       </c>
       <c r="H109" t="s">
         <v>348</v>
@@ -4606,80 +4645,83 @@
       <c r="I109" t="s">
         <v>349</v>
       </c>
-      <c r="J109" s="2" t="s">
-        <v>457</v>
-      </c>
-      <c r="L109" s="2" t="s">
-        <v>458</v>
-      </c>
-      <c r="Q109" t="s">
-        <v>459</v>
-      </c>
     </row>
     <row r="110" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>11</v>
+        <v>454</v>
       </c>
       <c r="B110" t="s">
         <v>25</v>
       </c>
       <c r="C110" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D110" t="s">
-        <v>95</v>
+        <v>455</v>
       </c>
       <c r="E110" t="s">
-        <v>10</v>
+        <v>456</v>
       </c>
       <c r="F110">
-        <v>2007</v>
+        <v>2006</v>
+      </c>
+      <c r="G110">
+        <v>2016</v>
       </c>
       <c r="H110" t="s">
-        <v>16</v>
+        <v>348</v>
       </c>
       <c r="I110" t="s">
-        <v>21</v>
+        <v>349</v>
+      </c>
+      <c r="J110" s="2" t="s">
+        <v>457</v>
+      </c>
+      <c r="L110" s="2" t="s">
+        <v>458</v>
+      </c>
+      <c r="Q110" t="s">
+        <v>459</v>
       </c>
     </row>
     <row r="111" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>223</v>
+        <v>11</v>
       </c>
       <c r="B111" t="s">
-        <v>124</v>
+        <v>25</v>
       </c>
       <c r="C111" s="2" t="s">
-        <v>222</v>
+        <v>12</v>
+      </c>
+      <c r="D111" t="s">
+        <v>95</v>
+      </c>
+      <c r="E111" t="s">
+        <v>10</v>
       </c>
       <c r="F111">
-        <v>1</v>
-      </c>
-      <c r="G111">
-        <v>2010</v>
+        <v>2007</v>
       </c>
       <c r="H111" t="s">
         <v>16</v>
       </c>
       <c r="I111" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="112" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="B112" t="s">
-        <v>40</v>
+        <v>124</v>
       </c>
       <c r="C112" s="2" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="F112">
-        <v>1946</v>
+        <v>1</v>
       </c>
       <c r="G112">
-        <v>2016</v>
+        <v>2010</v>
       </c>
       <c r="H112" t="s">
         <v>16</v>
@@ -4690,440 +4732,437 @@
     </row>
     <row r="113" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>97</v>
+        <v>226</v>
       </c>
       <c r="B113" t="s">
-        <v>128</v>
+        <v>40</v>
       </c>
       <c r="C113" s="2" t="s">
-        <v>98</v>
+        <v>225</v>
+      </c>
+      <c r="F113">
+        <v>1946</v>
+      </c>
+      <c r="G113">
+        <v>2016</v>
+      </c>
+      <c r="H113" t="s">
+        <v>16</v>
+      </c>
+      <c r="I113" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="114" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>278</v>
+        <v>97</v>
       </c>
       <c r="B114" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="C114" s="2" t="s">
-        <v>279</v>
-      </c>
-      <c r="E114" t="s">
-        <v>280</v>
-      </c>
-      <c r="F114">
-        <v>1890</v>
-      </c>
-      <c r="G114">
-        <v>1996</v>
-      </c>
-      <c r="H114" t="s">
-        <v>16</v>
-      </c>
-      <c r="I114" t="s">
-        <v>20</v>
+        <v>98</v>
       </c>
     </row>
     <row r="115" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>156</v>
+        <v>278</v>
       </c>
       <c r="B115" t="s">
-        <v>25</v>
+        <v>124</v>
       </c>
       <c r="C115" s="2" t="s">
-        <v>154</v>
+        <v>279</v>
+      </c>
+      <c r="E115" t="s">
+        <v>280</v>
+      </c>
+      <c r="F115">
+        <v>1890</v>
+      </c>
+      <c r="G115">
+        <v>1996</v>
+      </c>
+      <c r="H115" t="s">
+        <v>16</v>
+      </c>
+      <c r="I115" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="116" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>413</v>
+        <v>156</v>
       </c>
       <c r="B116" t="s">
-        <v>128</v>
+        <v>25</v>
       </c>
       <c r="C116" s="2" t="s">
-        <v>414</v>
-      </c>
-      <c r="E116" t="s">
-        <v>415</v>
-      </c>
-      <c r="F116">
-        <v>1946</v>
-      </c>
-      <c r="G116">
-        <v>2014</v>
-      </c>
-      <c r="H116" t="s">
-        <v>348</v>
-      </c>
-      <c r="I116" t="s">
-        <v>349</v>
-      </c>
-      <c r="N116" s="2" t="s">
-        <v>416</v>
-      </c>
-      <c r="Q116" t="s">
-        <v>417</v>
+        <v>154</v>
       </c>
     </row>
     <row r="117" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>229</v>
+        <v>413</v>
       </c>
       <c r="B117" t="s">
-        <v>40</v>
+        <v>128</v>
       </c>
       <c r="C117" s="2" t="s">
-        <v>225</v>
+        <v>414</v>
+      </c>
+      <c r="E117" t="s">
+        <v>415</v>
       </c>
       <c r="F117">
-        <v>1952</v>
+        <v>1946</v>
       </c>
       <c r="G117">
-        <v>1997</v>
+        <v>2014</v>
       </c>
       <c r="H117" t="s">
-        <v>16</v>
+        <v>348</v>
       </c>
       <c r="I117" t="s">
-        <v>20</v>
+        <v>349</v>
+      </c>
+      <c r="N117" s="2" t="s">
+        <v>416</v>
+      </c>
+      <c r="Q117" t="s">
+        <v>417</v>
       </c>
     </row>
     <row r="118" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>514</v>
+        <v>229</v>
       </c>
       <c r="B118" t="s">
         <v>40</v>
       </c>
       <c r="C118" s="2" t="s">
-        <v>513</v>
-      </c>
-      <c r="D118" t="s">
-        <v>515</v>
-      </c>
-      <c r="E118" t="s">
-        <v>14</v>
+        <v>225</v>
       </c>
       <c r="F118">
-        <v>1970</v>
+        <v>1952</v>
       </c>
       <c r="G118">
-        <v>2010</v>
+        <v>1997</v>
       </c>
       <c r="H118" t="s">
-        <v>348</v>
+        <v>16</v>
       </c>
       <c r="I118" t="s">
-        <v>349</v>
+        <v>20</v>
       </c>
     </row>
     <row r="119" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>293</v>
+        <v>514</v>
       </c>
       <c r="B119" t="s">
         <v>40</v>
       </c>
       <c r="C119" s="2" t="s">
-        <v>294</v>
+        <v>513</v>
+      </c>
+      <c r="D119" t="s">
+        <v>515</v>
+      </c>
+      <c r="E119" t="s">
+        <v>14</v>
       </c>
       <c r="F119">
-        <v>2004</v>
+        <v>1970</v>
       </c>
       <c r="G119">
-        <v>2006</v>
+        <v>2010</v>
       </c>
       <c r="H119" t="s">
-        <v>16</v>
+        <v>348</v>
       </c>
       <c r="I119" t="s">
-        <v>20</v>
+        <v>349</v>
       </c>
     </row>
     <row r="120" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>102</v>
+        <v>293</v>
       </c>
       <c r="B120" t="s">
-        <v>99</v>
+        <v>40</v>
       </c>
       <c r="C120" s="2" t="s">
-        <v>103</v>
+        <v>294</v>
+      </c>
+      <c r="F120">
+        <v>2004</v>
+      </c>
+      <c r="G120">
+        <v>2006</v>
+      </c>
+      <c r="H120" t="s">
+        <v>16</v>
+      </c>
+      <c r="I120" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="121" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>289</v>
+        <v>102</v>
       </c>
       <c r="B121" t="s">
-        <v>124</v>
+        <v>99</v>
       </c>
       <c r="C121" s="2" t="s">
-        <v>290</v>
+        <v>103</v>
       </c>
     </row>
     <row r="122" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>246</v>
+        <v>289</v>
       </c>
       <c r="B122" t="s">
-        <v>165</v>
+        <v>124</v>
       </c>
       <c r="C122" s="2" t="s">
-        <v>247</v>
-      </c>
-      <c r="E122" t="s">
-        <v>14</v>
-      </c>
-      <c r="F122">
-        <v>1960</v>
-      </c>
-      <c r="G122">
-        <v>2006</v>
-      </c>
-      <c r="H122" t="s">
-        <v>16</v>
-      </c>
-      <c r="I122" t="s">
-        <v>249</v>
+        <v>290</v>
       </c>
     </row>
     <row r="123" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>549</v>
+        <v>246</v>
       </c>
       <c r="B123" t="s">
-        <v>40</v>
+        <v>165</v>
       </c>
       <c r="C123" s="2" t="s">
-        <v>550</v>
-      </c>
-      <c r="D123" t="s">
-        <v>551</v>
+        <v>247</v>
       </c>
       <c r="E123" t="s">
         <v>14</v>
       </c>
       <c r="F123">
-        <v>1900</v>
+        <v>1960</v>
       </c>
       <c r="G123">
-        <v>2011</v>
+        <v>2006</v>
       </c>
       <c r="H123" t="s">
-        <v>348</v>
+        <v>16</v>
       </c>
       <c r="I123" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
     </row>
     <row r="124" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>365</v>
+        <v>549</v>
       </c>
       <c r="B124" t="s">
-        <v>128</v>
+        <v>40</v>
       </c>
       <c r="C124" s="2" t="s">
-        <v>364</v>
+        <v>550</v>
       </c>
       <c r="D124" t="s">
-        <v>370</v>
+        <v>551</v>
       </c>
       <c r="E124" t="s">
-        <v>366</v>
+        <v>14</v>
       </c>
       <c r="F124">
-        <v>1906</v>
+        <v>1900</v>
       </c>
       <c r="G124">
-        <v>2013</v>
+        <v>2011</v>
       </c>
       <c r="H124" t="s">
-        <v>367</v>
+        <v>348</v>
       </c>
       <c r="I124" t="s">
-        <v>368</v>
-      </c>
-      <c r="Q124" t="s">
-        <v>369</v>
+        <v>248</v>
       </c>
     </row>
     <row r="125" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>208</v>
+        <v>365</v>
       </c>
       <c r="B125" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="C125" s="2" t="s">
-        <v>209</v>
+        <v>364</v>
+      </c>
+      <c r="D125" t="s">
+        <v>370</v>
+      </c>
+      <c r="E125" t="s">
+        <v>366</v>
       </c>
       <c r="F125">
-        <v>1932</v>
+        <v>1906</v>
       </c>
       <c r="G125">
-        <v>2014</v>
+        <v>2013</v>
       </c>
       <c r="H125" t="s">
-        <v>16</v>
+        <v>367</v>
       </c>
       <c r="I125" t="s">
-        <v>20</v>
+        <v>368</v>
+      </c>
+      <c r="Q125" t="s">
+        <v>369</v>
       </c>
     </row>
     <row r="126" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>137</v>
+        <v>208</v>
       </c>
       <c r="B126" t="s">
-        <v>259</v>
+        <v>124</v>
       </c>
       <c r="C126" s="2" t="s">
-        <v>138</v>
+        <v>209</v>
+      </c>
+      <c r="F126">
+        <v>1932</v>
+      </c>
+      <c r="G126">
+        <v>2014</v>
+      </c>
+      <c r="H126" t="s">
+        <v>16</v>
+      </c>
+      <c r="I126" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="127" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>155</v>
+        <v>137</v>
       </c>
       <c r="B127" t="s">
         <v>259</v>
       </c>
       <c r="C127" s="2" t="s">
-        <v>154</v>
+        <v>138</v>
       </c>
     </row>
     <row r="128" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>57</v>
+        <v>155</v>
       </c>
       <c r="B128" t="s">
-        <v>128</v>
+        <v>259</v>
       </c>
       <c r="C128" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="Q128" t="s">
-        <v>17</v>
+        <v>154</v>
       </c>
     </row>
     <row r="129" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>129</v>
+        <v>57</v>
       </c>
       <c r="B129" t="s">
-        <v>259</v>
+        <v>128</v>
       </c>
       <c r="C129" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="E129" t="s">
-        <v>131</v>
-      </c>
-      <c r="F129">
-        <v>1945</v>
-      </c>
-      <c r="G129">
-        <v>2008</v>
-      </c>
-      <c r="I129" t="s">
-        <v>20</v>
+        <v>58</v>
+      </c>
+      <c r="Q129" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="130" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
-        <v>148</v>
+        <v>129</v>
       </c>
       <c r="B130" t="s">
-        <v>128</v>
+        <v>259</v>
       </c>
       <c r="C130" s="2" t="s">
-        <v>147</v>
+        <v>130</v>
+      </c>
+      <c r="E130" t="s">
+        <v>131</v>
+      </c>
+      <c r="F130">
+        <v>1945</v>
+      </c>
+      <c r="G130">
+        <v>2008</v>
+      </c>
+      <c r="I130" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="131" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>541</v>
+        <v>148</v>
       </c>
       <c r="B131" t="s">
-        <v>40</v>
+        <v>128</v>
       </c>
       <c r="C131" s="2" t="s">
-        <v>540</v>
-      </c>
-      <c r="D131" t="s">
-        <v>542</v>
-      </c>
-      <c r="E131" t="s">
-        <v>14</v>
-      </c>
-      <c r="F131">
-        <v>1989</v>
-      </c>
-      <c r="G131">
-        <v>2012</v>
-      </c>
-      <c r="H131" t="s">
-        <v>348</v>
-      </c>
-      <c r="I131" t="s">
-        <v>349</v>
-      </c>
-      <c r="J131" s="2" t="s">
-        <v>544</v>
-      </c>
-      <c r="N131" s="2" t="s">
-        <v>543</v>
+        <v>147</v>
       </c>
     </row>
     <row r="132" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>233</v>
+        <v>541</v>
       </c>
       <c r="B132" t="s">
-        <v>165</v>
+        <v>40</v>
       </c>
       <c r="C132" s="2" t="s">
-        <v>234</v>
+        <v>540</v>
+      </c>
+      <c r="D132" t="s">
+        <v>542</v>
       </c>
       <c r="E132" t="s">
         <v>14</v>
       </c>
       <c r="F132">
+        <v>1989</v>
+      </c>
+      <c r="G132">
         <v>2012</v>
       </c>
-      <c r="G132">
-        <v>2016</v>
-      </c>
       <c r="H132" t="s">
-        <v>16</v>
+        <v>348</v>
       </c>
       <c r="I132" t="s">
-        <v>20</v>
+        <v>349</v>
+      </c>
+      <c r="J132" s="2" t="s">
+        <v>544</v>
+      </c>
+      <c r="N132" s="2" t="s">
+        <v>543</v>
       </c>
     </row>
     <row r="133" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
-        <v>35</v>
+        <v>233</v>
       </c>
       <c r="B133" t="s">
-        <v>25</v>
+        <v>165</v>
       </c>
       <c r="C133" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="D133" t="s">
-        <v>37</v>
+        <v>234</v>
       </c>
       <c r="E133" t="s">
         <v>14</v>
       </c>
       <c r="F133">
-        <v>2001</v>
+        <v>2012</v>
+      </c>
+      <c r="G133">
+        <v>2016</v>
       </c>
       <c r="H133" t="s">
         <v>16</v>
@@ -5134,180 +5173,180 @@
     </row>
     <row r="134" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
-        <v>185</v>
+        <v>35</v>
       </c>
       <c r="B134" t="s">
-        <v>128</v>
+        <v>25</v>
       </c>
       <c r="C134" s="2" t="s">
-        <v>186</v>
+        <v>36</v>
+      </c>
+      <c r="D134" t="s">
+        <v>37</v>
+      </c>
+      <c r="E134" t="s">
+        <v>14</v>
+      </c>
+      <c r="F134">
+        <v>2001</v>
+      </c>
+      <c r="H134" t="s">
+        <v>16</v>
+      </c>
+      <c r="I134" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="135" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
-        <v>516</v>
+        <v>185</v>
       </c>
       <c r="B135" t="s">
-        <v>40</v>
+        <v>128</v>
       </c>
       <c r="C135" s="2" t="s">
-        <v>517</v>
-      </c>
-      <c r="D135" t="s">
-        <v>518</v>
-      </c>
-      <c r="E135" t="s">
-        <v>14</v>
-      </c>
-      <c r="F135">
-        <v>1975</v>
-      </c>
-      <c r="G135">
-        <v>2011</v>
-      </c>
-      <c r="H135" t="s">
-        <v>348</v>
-      </c>
-      <c r="I135" t="s">
-        <v>349</v>
-      </c>
-      <c r="P135" s="2" t="s">
-        <v>519</v>
+        <v>186</v>
       </c>
     </row>
     <row r="136" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
-        <v>210</v>
+        <v>516</v>
       </c>
       <c r="B136" t="s">
         <v>40</v>
       </c>
       <c r="C136" s="2" t="s">
-        <v>211</v>
+        <v>517</v>
+      </c>
+      <c r="D136" t="s">
+        <v>518</v>
+      </c>
+      <c r="E136" t="s">
+        <v>14</v>
       </c>
       <c r="F136">
-        <v>1976</v>
+        <v>1975</v>
       </c>
       <c r="G136">
-        <v>2016</v>
+        <v>2011</v>
       </c>
       <c r="H136" t="s">
-        <v>16</v>
+        <v>348</v>
       </c>
       <c r="I136" t="s">
-        <v>20</v>
+        <v>349</v>
+      </c>
+      <c r="P136" s="2" t="s">
+        <v>519</v>
       </c>
     </row>
     <row r="137" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
-        <v>426</v>
+        <v>210</v>
       </c>
       <c r="B137" t="s">
-        <v>86</v>
+        <v>40</v>
       </c>
       <c r="C137" s="2" t="s">
-        <v>427</v>
-      </c>
-      <c r="E137" t="s">
-        <v>34</v>
+        <v>211</v>
       </c>
       <c r="F137">
-        <v>2015</v>
+        <v>1976</v>
       </c>
       <c r="G137">
         <v>2016</v>
       </c>
       <c r="H137" t="s">
-        <v>348</v>
+        <v>16</v>
       </c>
       <c r="I137" t="s">
-        <v>349</v>
-      </c>
-      <c r="K137" s="2" t="s">
-        <v>428</v>
+        <v>20</v>
       </c>
     </row>
     <row r="138" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
-        <v>144</v>
+        <v>426</v>
       </c>
       <c r="B138" t="s">
-        <v>60</v>
+        <v>86</v>
       </c>
       <c r="C138" s="2" t="s">
-        <v>143</v>
+        <v>427</v>
+      </c>
+      <c r="E138" t="s">
+        <v>34</v>
       </c>
       <c r="F138">
-        <v>1800</v>
+        <v>2015</v>
       </c>
       <c r="G138">
-        <v>2013</v>
+        <v>2016</v>
+      </c>
+      <c r="H138" t="s">
+        <v>348</v>
+      </c>
+      <c r="I138" t="s">
+        <v>349</v>
+      </c>
+      <c r="K138" s="2" t="s">
+        <v>428</v>
       </c>
     </row>
     <row r="139" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
-        <v>472</v>
+        <v>144</v>
       </c>
       <c r="B139" t="s">
-        <v>25</v>
+        <v>60</v>
       </c>
       <c r="C139" s="2" t="s">
-        <v>473</v>
-      </c>
-      <c r="D139" t="s">
-        <v>474</v>
-      </c>
-      <c r="E139" t="s">
-        <v>112</v>
+        <v>143</v>
       </c>
       <c r="F139">
-        <v>1943</v>
-      </c>
-      <c r="H139" t="s">
-        <v>348</v>
-      </c>
-      <c r="I139" t="s">
-        <v>349</v>
-      </c>
-      <c r="N139" s="2" t="s">
-        <v>475</v>
+        <v>1800</v>
+      </c>
+      <c r="G139">
+        <v>2013</v>
       </c>
     </row>
     <row r="140" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
-        <v>122</v>
+        <v>472</v>
       </c>
       <c r="B140" t="s">
-        <v>259</v>
+        <v>25</v>
       </c>
       <c r="C140" s="2" t="s">
-        <v>121</v>
+        <v>473</v>
+      </c>
+      <c r="D140" t="s">
+        <v>474</v>
+      </c>
+      <c r="E140" t="s">
+        <v>112</v>
+      </c>
+      <c r="F140">
+        <v>1943</v>
+      </c>
+      <c r="H140" t="s">
+        <v>348</v>
       </c>
       <c r="I140" t="s">
-        <v>20</v>
+        <v>349</v>
+      </c>
+      <c r="N140" s="2" t="s">
+        <v>475</v>
       </c>
     </row>
     <row r="141" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
-        <v>318</v>
+        <v>122</v>
       </c>
       <c r="B141" t="s">
-        <v>250</v>
+        <v>259</v>
       </c>
       <c r="C141" s="2" t="s">
-        <v>319</v>
-      </c>
-      <c r="E141" t="s">
-        <v>320</v>
-      </c>
-      <c r="F141">
-        <v>1975</v>
-      </c>
-      <c r="G141">
-        <v>1989</v>
-      </c>
-      <c r="H141" t="s">
-        <v>16</v>
+        <v>121</v>
       </c>
       <c r="I141" t="s">
         <v>20</v>
@@ -5315,22 +5354,22 @@
     </row>
     <row r="142" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="B142" t="s">
         <v>250</v>
       </c>
       <c r="C142" s="2" t="s">
-        <v>317</v>
+        <v>319</v>
       </c>
       <c r="E142" t="s">
-        <v>105</v>
+        <v>320</v>
       </c>
       <c r="F142">
-        <v>1950</v>
+        <v>1975</v>
       </c>
       <c r="G142">
-        <v>1996</v>
+        <v>1989</v>
       </c>
       <c r="H142" t="s">
         <v>16</v>
@@ -5341,19 +5380,22 @@
     </row>
     <row r="143" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
-        <v>322</v>
+        <v>316</v>
       </c>
       <c r="B143" t="s">
-        <v>25</v>
+        <v>250</v>
       </c>
       <c r="C143" s="2" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="E143" t="s">
-        <v>77</v>
+        <v>105</v>
       </c>
       <c r="F143">
-        <v>2010</v>
+        <v>1950</v>
+      </c>
+      <c r="G143">
+        <v>1996</v>
       </c>
       <c r="H143" t="s">
         <v>16</v>
@@ -5364,156 +5406,153 @@
     </row>
     <row r="144" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
-        <v>141</v>
+        <v>322</v>
       </c>
       <c r="B144" t="s">
-        <v>237</v>
+        <v>25</v>
       </c>
       <c r="C144" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="Q144" t="s">
-        <v>17</v>
+        <v>321</v>
+      </c>
+      <c r="E144" t="s">
+        <v>77</v>
+      </c>
+      <c r="F144">
+        <v>2010</v>
+      </c>
+      <c r="H144" t="s">
+        <v>16</v>
+      </c>
+      <c r="I144" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="145" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
-        <v>308</v>
+        <v>141</v>
       </c>
       <c r="B145" t="s">
-        <v>250</v>
+        <v>237</v>
       </c>
       <c r="C145" s="2" t="s">
-        <v>309</v>
-      </c>
-      <c r="E145" t="s">
-        <v>310</v>
-      </c>
-      <c r="F145">
-        <v>1950</v>
-      </c>
-      <c r="G145">
-        <v>2010</v>
-      </c>
-      <c r="H145" t="s">
-        <v>16</v>
-      </c>
-      <c r="I145" t="s">
-        <v>20</v>
+        <v>142</v>
+      </c>
+      <c r="Q145" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="146" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
-        <v>287</v>
+        <v>308</v>
       </c>
       <c r="B146" t="s">
-        <v>134</v>
+        <v>250</v>
       </c>
       <c r="C146" s="2" t="s">
-        <v>288</v>
+        <v>309</v>
+      </c>
+      <c r="E146" t="s">
+        <v>310</v>
       </c>
       <c r="F146">
-        <v>1990</v>
+        <v>1950</v>
       </c>
       <c r="G146">
-        <v>2008</v>
+        <v>2010</v>
+      </c>
+      <c r="H146" t="s">
+        <v>16</v>
+      </c>
+      <c r="I146" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="147" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
-        <v>526</v>
+        <v>287</v>
       </c>
       <c r="B147" t="s">
-        <v>40</v>
+        <v>134</v>
       </c>
       <c r="C147" s="2" t="s">
-        <v>527</v>
-      </c>
-      <c r="D147" t="s">
-        <v>528</v>
-      </c>
-      <c r="E147" t="s">
-        <v>14</v>
+        <v>288</v>
       </c>
       <c r="F147">
-        <v>1980</v>
+        <v>1990</v>
       </c>
       <c r="G147">
-        <v>2011</v>
-      </c>
-      <c r="H147" t="s">
-        <v>348</v>
-      </c>
-      <c r="I147" t="s">
-        <v>349</v>
-      </c>
-      <c r="J147" s="2" t="s">
-        <v>529</v>
-      </c>
-      <c r="L147" s="2" t="s">
-        <v>530</v>
+        <v>2008</v>
       </c>
     </row>
     <row r="148" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
-        <v>274</v>
+        <v>526</v>
       </c>
       <c r="B148" t="s">
-        <v>55</v>
+        <v>40</v>
       </c>
       <c r="C148" s="2" t="s">
-        <v>275</v>
+        <v>527</v>
+      </c>
+      <c r="D148" t="s">
+        <v>528</v>
+      </c>
+      <c r="E148" t="s">
+        <v>14</v>
+      </c>
+      <c r="F148">
+        <v>1980</v>
+      </c>
+      <c r="G148">
+        <v>2011</v>
       </c>
       <c r="H148" t="s">
-        <v>16</v>
+        <v>348</v>
       </c>
       <c r="I148" t="s">
-        <v>20</v>
+        <v>349</v>
+      </c>
+      <c r="J148" s="2" t="s">
+        <v>529</v>
+      </c>
+      <c r="L148" s="2" t="s">
+        <v>530</v>
       </c>
     </row>
     <row r="149" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
-        <v>157</v>
+        <v>274</v>
       </c>
       <c r="B149" t="s">
-        <v>128</v>
+        <v>55</v>
       </c>
       <c r="C149" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="Q149" t="s">
-        <v>18</v>
+        <v>275</v>
+      </c>
+      <c r="H149" t="s">
+        <v>16</v>
+      </c>
+      <c r="I149" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="150" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
-        <v>439</v>
+        <v>157</v>
       </c>
       <c r="B150" t="s">
-        <v>259</v>
+        <v>128</v>
       </c>
       <c r="C150" s="2" t="s">
-        <v>438</v>
-      </c>
-      <c r="H150" t="s">
-        <v>348</v>
-      </c>
-      <c r="I150" t="s">
-        <v>349</v>
-      </c>
-      <c r="J150" s="2" t="s">
-        <v>440</v>
-      </c>
-      <c r="K150" s="2" t="s">
-        <v>442</v>
-      </c>
-      <c r="L150" s="2" t="s">
-        <v>441</v>
+        <v>154</v>
+      </c>
+      <c r="Q150" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="151" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
-        <v>443</v>
+        <v>439</v>
       </c>
       <c r="B151" t="s">
         <v>259</v>
@@ -5521,15 +5560,6 @@
       <c r="C151" s="2" t="s">
         <v>438</v>
       </c>
-      <c r="D151" t="s">
-        <v>447</v>
-      </c>
-      <c r="F151">
-        <v>1990</v>
-      </c>
-      <c r="G151">
-        <v>2014</v>
-      </c>
       <c r="H151" t="s">
         <v>348</v>
       </c>
@@ -5537,36 +5567,33 @@
         <v>349</v>
       </c>
       <c r="J151" s="2" t="s">
-        <v>444</v>
+        <v>440</v>
       </c>
       <c r="K151" s="2" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
       <c r="L151" s="2" t="s">
-        <v>446</v>
+        <v>441</v>
       </c>
     </row>
     <row r="152" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
-        <v>558</v>
+        <v>443</v>
       </c>
       <c r="B152" t="s">
-        <v>40</v>
+        <v>259</v>
       </c>
       <c r="C152" s="2" t="s">
-        <v>557</v>
+        <v>438</v>
       </c>
       <c r="D152" t="s">
-        <v>559</v>
-      </c>
-      <c r="E152" t="s">
-        <v>560</v>
+        <v>447</v>
       </c>
       <c r="F152">
-        <v>1989</v>
+        <v>1990</v>
       </c>
       <c r="G152">
-        <v>2009</v>
+        <v>2014</v>
       </c>
       <c r="H152" t="s">
         <v>348</v>
@@ -5575,84 +5602,99 @@
         <v>349</v>
       </c>
       <c r="J152" s="2" t="s">
-        <v>561</v>
-      </c>
-      <c r="P152" s="2" t="s">
-        <v>562</v>
+        <v>444</v>
+      </c>
+      <c r="K152" s="2" t="s">
+        <v>445</v>
+      </c>
+      <c r="L152" s="2" t="s">
+        <v>446</v>
       </c>
     </row>
     <row r="153" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
-        <v>194</v>
+        <v>558</v>
       </c>
       <c r="B153" t="s">
-        <v>99</v>
+        <v>40</v>
       </c>
       <c r="C153" s="2" t="s">
-        <v>193</v>
+        <v>557</v>
+      </c>
+      <c r="D153" t="s">
+        <v>559</v>
+      </c>
+      <c r="E153" t="s">
+        <v>560</v>
+      </c>
+      <c r="F153">
+        <v>1989</v>
+      </c>
+      <c r="G153">
+        <v>2009</v>
+      </c>
+      <c r="H153" t="s">
+        <v>348</v>
+      </c>
+      <c r="I153" t="s">
+        <v>349</v>
+      </c>
+      <c r="J153" s="2" t="s">
+        <v>561</v>
+      </c>
+      <c r="P153" s="2" t="s">
+        <v>562</v>
       </c>
     </row>
     <row r="154" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
-        <v>295</v>
+        <v>194</v>
       </c>
       <c r="B154" t="s">
-        <v>40</v>
+        <v>99</v>
       </c>
       <c r="C154" s="2" t="s">
-        <v>296</v>
-      </c>
-      <c r="E154" t="s">
-        <v>297</v>
-      </c>
-      <c r="F154">
-        <v>1990</v>
-      </c>
-      <c r="G154">
-        <v>2015</v>
-      </c>
-      <c r="H154" t="s">
-        <v>16</v>
-      </c>
-      <c r="I154" t="s">
-        <v>249</v>
+        <v>193</v>
       </c>
     </row>
     <row r="155" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
-        <v>256</v>
+        <v>295</v>
       </c>
       <c r="B155" t="s">
-        <v>250</v>
+        <v>40</v>
       </c>
       <c r="C155" s="2" t="s">
-        <v>257</v>
+        <v>296</v>
       </c>
       <c r="E155" t="s">
-        <v>258</v>
+        <v>297</v>
+      </c>
+      <c r="F155">
+        <v>1990</v>
+      </c>
+      <c r="G155">
+        <v>2015</v>
       </c>
       <c r="H155" t="s">
         <v>16</v>
       </c>
       <c r="I155" t="s">
-        <v>20</v>
+        <v>249</v>
       </c>
     </row>
     <row r="156" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
-        <v>227</v>
+        <v>256</v>
       </c>
       <c r="B156" t="s">
-        <v>40</v>
+        <v>250</v>
       </c>
       <c r="C156" s="2" t="s">
-        <v>225</v>
-      </c>
-      <c r="F156">
-        <v>1955</v>
-      </c>
-      <c r="G156">
-        <v>2016</v>
+        <v>257</v>
+      </c>
+      <c r="E156" t="s">
+        <v>258</v>
       </c>
       <c r="H156" t="s">
         <v>16</v>
@@ -5663,7 +5705,7 @@
     </row>
     <row r="157" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="B157" t="s">
         <v>40</v>
@@ -5672,7 +5714,7 @@
         <v>225</v>
       </c>
       <c r="F157">
-        <v>1995</v>
+        <v>1955</v>
       </c>
       <c r="G157">
         <v>2016</v>
@@ -5686,99 +5728,108 @@
     </row>
     <row r="158" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
-        <v>452</v>
+        <v>230</v>
       </c>
       <c r="B158" t="s">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="C158" s="2" t="s">
-        <v>453</v>
-      </c>
-      <c r="E158" t="s">
-        <v>9</v>
+        <v>225</v>
+      </c>
+      <c r="F158">
+        <v>1995</v>
+      </c>
+      <c r="G158">
+        <v>2016</v>
       </c>
       <c r="H158" t="s">
-        <v>348</v>
+        <v>16</v>
       </c>
       <c r="I158" t="s">
-        <v>435</v>
+        <v>20</v>
       </c>
     </row>
     <row r="159" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
-        <v>109</v>
+        <v>584</v>
       </c>
       <c r="B159" t="s">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="C159" s="2" t="s">
-        <v>110</v>
+        <v>585</v>
+      </c>
+      <c r="D159" t="s">
+        <v>586</v>
       </c>
       <c r="E159" t="s">
-        <v>111</v>
+        <v>14</v>
       </c>
       <c r="F159">
-        <v>1956</v>
+        <v>1974</v>
+      </c>
+      <c r="G159">
+        <v>2016</v>
+      </c>
+      <c r="H159" t="s">
+        <v>348</v>
+      </c>
+      <c r="I159" t="s">
+        <v>349</v>
       </c>
     </row>
     <row r="160" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
-        <v>326</v>
+        <v>452</v>
       </c>
       <c r="B160" t="s">
         <v>25</v>
       </c>
       <c r="C160" s="2" t="s">
-        <v>327</v>
+        <v>453</v>
       </c>
       <c r="E160" t="s">
-        <v>111</v>
-      </c>
-      <c r="F160">
-        <v>1998</v>
+        <v>9</v>
       </c>
       <c r="H160" t="s">
-        <v>16</v>
+        <v>348</v>
       </c>
       <c r="I160" t="s">
-        <v>20</v>
+        <v>435</v>
       </c>
     </row>
     <row r="161" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
-        <v>91</v>
+        <v>109</v>
       </c>
       <c r="B161" t="s">
         <v>25</v>
       </c>
       <c r="C161" s="2" t="s">
-        <v>93</v>
+        <v>110</v>
       </c>
       <c r="E161" t="s">
-        <v>92</v>
+        <v>111</v>
       </c>
       <c r="F161">
-        <v>1999</v>
+        <v>1956</v>
       </c>
     </row>
     <row r="162" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
-        <v>314</v>
+        <v>326</v>
       </c>
       <c r="B162" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="C162" s="2" t="s">
-        <v>313</v>
+        <v>327</v>
       </c>
       <c r="E162" t="s">
-        <v>315</v>
+        <v>111</v>
       </c>
       <c r="F162">
-        <v>1950</v>
-      </c>
-      <c r="G162">
-        <v>2004</v>
+        <v>1998</v>
       </c>
       <c r="H162" t="s">
         <v>16</v>
@@ -5789,76 +5840,79 @@
     </row>
     <row r="163" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
-        <v>161</v>
+        <v>91</v>
       </c>
       <c r="B163" t="s">
         <v>25</v>
       </c>
       <c r="C163" s="2" t="s">
-        <v>160</v>
+        <v>93</v>
+      </c>
+      <c r="E163" t="s">
+        <v>92</v>
+      </c>
+      <c r="F163">
+        <v>1999</v>
       </c>
     </row>
     <row r="164" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
-        <v>545</v>
+        <v>314</v>
       </c>
       <c r="B164" t="s">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="C164" s="2" t="s">
-        <v>546</v>
-      </c>
-      <c r="D164" t="s">
-        <v>547</v>
+        <v>313</v>
       </c>
       <c r="E164" t="s">
-        <v>34</v>
+        <v>315</v>
       </c>
       <c r="F164">
-        <v>2000</v>
+        <v>1950</v>
       </c>
       <c r="G164">
-        <v>2011</v>
+        <v>2004</v>
       </c>
       <c r="H164" t="s">
-        <v>348</v>
+        <v>16</v>
       </c>
       <c r="I164" t="s">
-        <v>349</v>
-      </c>
-      <c r="J164" s="2" t="s">
-        <v>548</v>
+        <v>20</v>
       </c>
     </row>
     <row r="165" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="B165" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="C165" s="2" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
     </row>
     <row r="166" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
-        <v>399</v>
+        <v>545</v>
       </c>
       <c r="B166" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="C166" s="2" t="s">
-        <v>400</v>
+        <v>546</v>
+      </c>
+      <c r="D166" t="s">
+        <v>547</v>
       </c>
       <c r="E166" t="s">
-        <v>14</v>
+        <v>34</v>
       </c>
       <c r="F166">
         <v>2000</v>
       </c>
       <c r="G166">
-        <v>2014</v>
+        <v>2011</v>
       </c>
       <c r="H166" t="s">
         <v>348</v>
@@ -5867,76 +5921,61 @@
         <v>349</v>
       </c>
       <c r="J166" s="2" t="s">
-        <v>402</v>
-      </c>
-      <c r="N166" s="2" t="s">
-        <v>401</v>
+        <v>548</v>
       </c>
     </row>
     <row r="167" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
-        <v>213</v>
+        <v>168</v>
       </c>
       <c r="B167" t="s">
-        <v>55</v>
+        <v>40</v>
       </c>
       <c r="C167" s="2" t="s">
-        <v>212</v>
-      </c>
-      <c r="H167" t="s">
-        <v>16</v>
-      </c>
-      <c r="I167" t="s">
-        <v>20</v>
+        <v>167</v>
       </c>
     </row>
     <row r="168" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
-        <v>395</v>
+        <v>399</v>
       </c>
       <c r="B168" t="s">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="C168" s="2" t="s">
-        <v>394</v>
-      </c>
-      <c r="D168" t="s">
-        <v>396</v>
+        <v>400</v>
       </c>
       <c r="E168" t="s">
-        <v>111</v>
+        <v>14</v>
       </c>
       <c r="F168">
-        <v>1986</v>
+        <v>2000</v>
       </c>
       <c r="G168">
-        <v>2015</v>
+        <v>2014</v>
       </c>
       <c r="H168" t="s">
-        <v>367</v>
+        <v>348</v>
       </c>
       <c r="I168" t="s">
-        <v>398</v>
+        <v>349</v>
       </c>
       <c r="J168" s="2" t="s">
-        <v>397</v>
+        <v>402</v>
+      </c>
+      <c r="N168" s="2" t="s">
+        <v>401</v>
       </c>
     </row>
     <row r="169" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
-        <v>323</v>
+        <v>213</v>
       </c>
       <c r="B169" t="s">
-        <v>25</v>
+        <v>55</v>
       </c>
       <c r="C169" s="2" t="s">
-        <v>324</v>
-      </c>
-      <c r="E169" t="s">
-        <v>325</v>
-      </c>
-      <c r="F169">
-        <v>1942</v>
+        <v>212</v>
       </c>
       <c r="H169" t="s">
         <v>16</v>
@@ -5947,91 +5986,103 @@
     </row>
     <row r="170" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
-        <v>273</v>
+        <v>395</v>
       </c>
       <c r="B170" t="s">
-        <v>237</v>
+        <v>25</v>
       </c>
       <c r="C170" s="2" t="s">
-        <v>272</v>
+        <v>394</v>
+      </c>
+      <c r="D170" t="s">
+        <v>396</v>
+      </c>
+      <c r="E170" t="s">
+        <v>111</v>
       </c>
       <c r="F170">
-        <v>1996</v>
+        <v>1986</v>
       </c>
       <c r="G170">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="H170" t="s">
-        <v>16</v>
+        <v>367</v>
       </c>
       <c r="I170" t="s">
-        <v>20</v>
+        <v>398</v>
+      </c>
+      <c r="J170" s="2" t="s">
+        <v>397</v>
       </c>
     </row>
     <row r="171" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
-        <v>508</v>
+        <v>323</v>
       </c>
       <c r="B171" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="C171" s="2" t="s">
-        <v>509</v>
-      </c>
-      <c r="D171" t="s">
-        <v>511</v>
+        <v>324</v>
       </c>
       <c r="E171" t="s">
-        <v>510</v>
+        <v>325</v>
       </c>
       <c r="F171">
-        <v>1989</v>
-      </c>
-      <c r="G171">
-        <v>2009</v>
+        <v>1942</v>
       </c>
       <c r="H171" t="s">
-        <v>348</v>
+        <v>16</v>
       </c>
       <c r="I171" t="s">
-        <v>349</v>
-      </c>
-      <c r="P171" s="2" t="s">
-        <v>512</v>
+        <v>20</v>
       </c>
     </row>
     <row r="172" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
-        <v>66</v>
+        <v>273</v>
       </c>
       <c r="B172" t="s">
-        <v>25</v>
+        <v>237</v>
       </c>
       <c r="C172" s="2" t="s">
-        <v>67</v>
+        <v>272</v>
+      </c>
+      <c r="F172">
+        <v>1996</v>
+      </c>
+      <c r="G172">
+        <v>2016</v>
+      </c>
+      <c r="H172" t="s">
+        <v>16</v>
+      </c>
+      <c r="I172" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="173" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
-        <v>500</v>
+        <v>508</v>
       </c>
       <c r="B173" t="s">
         <v>40</v>
       </c>
       <c r="C173" s="2" t="s">
-        <v>499</v>
+        <v>509</v>
       </c>
       <c r="D173" t="s">
-        <v>501</v>
+        <v>511</v>
       </c>
       <c r="E173" t="s">
-        <v>14</v>
+        <v>510</v>
       </c>
       <c r="F173">
-        <v>1946</v>
+        <v>1989</v>
       </c>
       <c r="G173">
-        <v>2015</v>
+        <v>2009</v>
       </c>
       <c r="H173" t="s">
         <v>348</v>
@@ -6039,93 +6090,102 @@
       <c r="I173" t="s">
         <v>349</v>
       </c>
+      <c r="P173" s="2" t="s">
+        <v>512</v>
+      </c>
     </row>
     <row r="174" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
-        <v>383</v>
+        <v>66</v>
       </c>
       <c r="B174" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="C174" s="2" t="s">
-        <v>384</v>
-      </c>
-      <c r="E174" t="s">
-        <v>386</v>
-      </c>
-      <c r="F174">
-        <v>1951</v>
-      </c>
-      <c r="H174" t="s">
-        <v>348</v>
-      </c>
-      <c r="I174" t="s">
-        <v>349</v>
-      </c>
-      <c r="N174" s="2" t="s">
-        <v>385</v>
+        <v>67</v>
       </c>
     </row>
     <row r="175" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
-        <v>139</v>
+        <v>500</v>
       </c>
       <c r="B175" t="s">
         <v>40</v>
       </c>
       <c r="C175" s="2" t="s">
-        <v>140</v>
+        <v>499</v>
+      </c>
+      <c r="D175" t="s">
+        <v>501</v>
+      </c>
+      <c r="E175" t="s">
+        <v>14</v>
+      </c>
+      <c r="F175">
+        <v>1946</v>
+      </c>
+      <c r="G175">
+        <v>2015</v>
+      </c>
+      <c r="H175" t="s">
+        <v>348</v>
+      </c>
+      <c r="I175" t="s">
+        <v>349</v>
       </c>
     </row>
     <row r="176" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
-        <v>329</v>
+        <v>383</v>
       </c>
       <c r="B176" t="s">
-        <v>165</v>
+        <v>40</v>
       </c>
       <c r="C176" s="2" t="s">
-        <v>328</v>
+        <v>384</v>
       </c>
       <c r="E176" t="s">
-        <v>34</v>
+        <v>386</v>
       </c>
       <c r="F176">
-        <v>1789</v>
+        <v>1951</v>
       </c>
       <c r="H176" t="s">
-        <v>16</v>
+        <v>348</v>
       </c>
       <c r="I176" t="s">
-        <v>20</v>
+        <v>349</v>
+      </c>
+      <c r="N176" s="2" t="s">
+        <v>385</v>
       </c>
     </row>
     <row r="177" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
-        <v>172</v>
+        <v>139</v>
       </c>
       <c r="B177" t="s">
-        <v>60</v>
+        <v>40</v>
       </c>
       <c r="C177" s="2" t="s">
-        <v>171</v>
+        <v>140</v>
       </c>
     </row>
     <row r="178" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
-        <v>217</v>
+        <v>329</v>
       </c>
       <c r="B178" t="s">
-        <v>60</v>
+        <v>165</v>
       </c>
       <c r="C178" s="2" t="s">
-        <v>216</v>
+        <v>328</v>
       </c>
       <c r="E178" t="s">
-        <v>14</v>
+        <v>34</v>
       </c>
       <c r="F178">
-        <v>1900</v>
+        <v>1789</v>
       </c>
       <c r="H178" t="s">
         <v>16</v>
@@ -6136,130 +6196,118 @@
     </row>
     <row r="179" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
-        <v>132</v>
+        <v>172</v>
       </c>
       <c r="B179" t="s">
-        <v>259</v>
+        <v>60</v>
       </c>
       <c r="C179" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="Q179" t="s">
-        <v>17</v>
+        <v>171</v>
       </c>
     </row>
     <row r="180" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
-        <v>182</v>
+        <v>217</v>
       </c>
       <c r="B180" t="s">
-        <v>165</v>
+        <v>60</v>
       </c>
       <c r="C180" s="2" t="s">
-        <v>181</v>
+        <v>216</v>
+      </c>
+      <c r="E180" t="s">
+        <v>14</v>
+      </c>
+      <c r="F180">
+        <v>1900</v>
+      </c>
+      <c r="H180" t="s">
+        <v>16</v>
+      </c>
+      <c r="I180" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="181" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
-        <v>423</v>
+        <v>132</v>
       </c>
       <c r="B181" t="s">
-        <v>86</v>
+        <v>259</v>
       </c>
       <c r="C181" s="2" t="s">
-        <v>424</v>
-      </c>
-      <c r="E181" t="s">
-        <v>34</v>
-      </c>
-      <c r="F181">
-        <v>1996</v>
-      </c>
-      <c r="G181">
-        <v>2016</v>
-      </c>
-      <c r="H181" t="s">
-        <v>348</v>
-      </c>
-      <c r="I181" t="s">
-        <v>425</v>
+        <v>133</v>
+      </c>
+      <c r="Q181" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="182" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
-        <v>115</v>
+        <v>182</v>
       </c>
       <c r="B182" t="s">
-        <v>128</v>
+        <v>165</v>
       </c>
       <c r="C182" s="2" t="s">
-        <v>116</v>
+        <v>181</v>
       </c>
     </row>
     <row r="183" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
-        <v>263</v>
+        <v>423</v>
       </c>
       <c r="B183" t="s">
-        <v>250</v>
+        <v>86</v>
       </c>
       <c r="C183" s="2" t="s">
-        <v>264</v>
+        <v>424</v>
       </c>
       <c r="E183" t="s">
-        <v>265</v>
+        <v>34</v>
       </c>
       <c r="F183">
-        <v>1500</v>
+        <v>1996</v>
       </c>
       <c r="G183">
-        <v>2000</v>
+        <v>2016</v>
       </c>
       <c r="H183" t="s">
-        <v>16</v>
+        <v>348</v>
       </c>
       <c r="I183" t="s">
-        <v>20</v>
+        <v>425</v>
       </c>
     </row>
     <row r="184" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
-        <v>221</v>
+        <v>115</v>
       </c>
       <c r="B184" t="s">
-        <v>86</v>
+        <v>128</v>
       </c>
       <c r="C184" s="2" t="s">
-        <v>220</v>
-      </c>
-      <c r="F184">
-        <v>2013</v>
-      </c>
-      <c r="H184" t="s">
-        <v>16</v>
-      </c>
-      <c r="I184" t="s">
-        <v>20</v>
+        <v>116</v>
       </c>
     </row>
     <row r="185" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
-        <v>13</v>
+        <v>263</v>
       </c>
       <c r="B185" t="s">
-        <v>25</v>
+        <v>250</v>
       </c>
       <c r="C185" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="D185" s="1" t="s">
-        <v>42</v>
+        <v>264</v>
       </c>
       <c r="E185" t="s">
-        <v>14</v>
+        <v>265</v>
       </c>
       <c r="F185">
-        <v>1981</v>
+        <v>1500</v>
+      </c>
+      <c r="G185">
+        <v>2000</v>
       </c>
       <c r="H185" t="s">
         <v>16</v>
@@ -6270,13 +6318,16 @@
     </row>
     <row r="186" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
-        <v>283</v>
+        <v>221</v>
       </c>
       <c r="B186" t="s">
-        <v>124</v>
+        <v>86</v>
       </c>
       <c r="C186" s="2" t="s">
-        <v>284</v>
+        <v>220</v>
+      </c>
+      <c r="F186">
+        <v>2013</v>
       </c>
       <c r="H186" t="s">
         <v>16</v>
@@ -6285,151 +6336,194 @@
         <v>20</v>
       </c>
     </row>
+    <row r="187" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A187" t="s">
+        <v>13</v>
+      </c>
+      <c r="B187" t="s">
+        <v>25</v>
+      </c>
+      <c r="C187" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D187" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E187" t="s">
+        <v>14</v>
+      </c>
+      <c r="F187">
+        <v>1981</v>
+      </c>
+      <c r="H187" t="s">
+        <v>16</v>
+      </c>
+      <c r="I187" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="188" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A188" t="s">
+        <v>283</v>
+      </c>
+      <c r="B188" t="s">
+        <v>124</v>
+      </c>
+      <c r="C188" s="2" t="s">
+        <v>284</v>
+      </c>
+      <c r="H188" t="s">
+        <v>16</v>
+      </c>
+      <c r="I188" t="s">
+        <v>20</v>
+      </c>
+    </row>
   </sheetData>
-  <sortState ref="A2:Q186">
+  <sortState ref="A2:Q188">
     <sortCondition ref="A2"/>
   </sortState>
   <hyperlinks>
     <hyperlink ref="C6" r:id="rId1"/>
-    <hyperlink ref="C71" r:id="rId2"/>
+    <hyperlink ref="C72" r:id="rId2"/>
     <hyperlink ref="C7" r:id="rId3"/>
     <hyperlink ref="C11" r:id="rId4"/>
-    <hyperlink ref="C110" r:id="rId5"/>
-    <hyperlink ref="C133" r:id="rId6"/>
-    <hyperlink ref="C185" r:id="rId7"/>
+    <hyperlink ref="C111" r:id="rId5"/>
+    <hyperlink ref="C134" r:id="rId6"/>
+    <hyperlink ref="C187" r:id="rId7"/>
     <hyperlink ref="C45" r:id="rId8"/>
     <hyperlink ref="C38" r:id="rId9"/>
-    <hyperlink ref="C62" r:id="rId10"/>
-    <hyperlink ref="C69" r:id="rId11"/>
+    <hyperlink ref="C63" r:id="rId10"/>
+    <hyperlink ref="C70" r:id="rId11"/>
     <hyperlink ref="C3" r:id="rId12"/>
     <hyperlink ref="C26" r:id="rId13"/>
-    <hyperlink ref="C73" r:id="rId14"/>
-    <hyperlink ref="C102" r:id="rId15"/>
+    <hyperlink ref="C74" r:id="rId14"/>
+    <hyperlink ref="C103" r:id="rId15"/>
     <hyperlink ref="C37" r:id="rId16"/>
-    <hyperlink ref="C128" r:id="rId17"/>
-    <hyperlink ref="C53" r:id="rId18"/>
-    <hyperlink ref="C87" r:id="rId19"/>
+    <hyperlink ref="C129" r:id="rId17"/>
+    <hyperlink ref="C54" r:id="rId18"/>
+    <hyperlink ref="C88" r:id="rId19"/>
     <hyperlink ref="C22" r:id="rId20"/>
-    <hyperlink ref="C172" r:id="rId21"/>
+    <hyperlink ref="C174" r:id="rId21"/>
     <hyperlink ref="C8" r:id="rId22"/>
     <hyperlink ref="C49" r:id="rId23"/>
-    <hyperlink ref="C66" r:id="rId24"/>
-    <hyperlink ref="C63" r:id="rId25"/>
-    <hyperlink ref="C67" r:id="rId26"/>
-    <hyperlink ref="C68" r:id="rId27"/>
-    <hyperlink ref="C84" r:id="rId28"/>
-    <hyperlink ref="C107" r:id="rId29"/>
-    <hyperlink ref="C161" r:id="rId30"/>
-    <hyperlink ref="C113" r:id="rId31"/>
-    <hyperlink ref="C97" r:id="rId32"/>
-    <hyperlink ref="C120" r:id="rId33"/>
-    <hyperlink ref="C85" r:id="rId34"/>
+    <hyperlink ref="C67" r:id="rId24"/>
+    <hyperlink ref="C64" r:id="rId25"/>
+    <hyperlink ref="C68" r:id="rId26"/>
+    <hyperlink ref="C69" r:id="rId27"/>
+    <hyperlink ref="C85" r:id="rId28"/>
+    <hyperlink ref="C108" r:id="rId29"/>
+    <hyperlink ref="C163" r:id="rId30"/>
+    <hyperlink ref="C114" r:id="rId31"/>
+    <hyperlink ref="C98" r:id="rId32"/>
+    <hyperlink ref="C121" r:id="rId33"/>
+    <hyperlink ref="C86" r:id="rId34"/>
     <hyperlink ref="C23" r:id="rId35"/>
-    <hyperlink ref="C159" r:id="rId36"/>
+    <hyperlink ref="C161" r:id="rId36"/>
     <hyperlink ref="C21" r:id="rId37"/>
-    <hyperlink ref="C182" r:id="rId38"/>
-    <hyperlink ref="C101" r:id="rId39"/>
-    <hyperlink ref="C70" r:id="rId40"/>
-    <hyperlink ref="C140" r:id="rId41"/>
+    <hyperlink ref="C184" r:id="rId38"/>
+    <hyperlink ref="C102" r:id="rId39"/>
+    <hyperlink ref="C71" r:id="rId40"/>
+    <hyperlink ref="C141" r:id="rId41"/>
     <hyperlink ref="C24" r:id="rId42"/>
-    <hyperlink ref="C64" r:id="rId43"/>
+    <hyperlink ref="C65" r:id="rId43"/>
     <hyperlink ref="C31" r:id="rId44"/>
-    <hyperlink ref="C129" r:id="rId45"/>
-    <hyperlink ref="C179" r:id="rId46"/>
+    <hyperlink ref="C130" r:id="rId45"/>
+    <hyperlink ref="C181" r:id="rId46"/>
     <hyperlink ref="C35" r:id="rId47" display="http://comparativeconstitutionsproject.org/"/>
-    <hyperlink ref="C126" r:id="rId48"/>
-    <hyperlink ref="C175" r:id="rId49"/>
-    <hyperlink ref="C144" r:id="rId50"/>
-    <hyperlink ref="C138" r:id="rId51"/>
+    <hyperlink ref="C127" r:id="rId48"/>
+    <hyperlink ref="C177" r:id="rId49"/>
+    <hyperlink ref="C145" r:id="rId50"/>
+    <hyperlink ref="C139" r:id="rId51"/>
     <hyperlink ref="C30" r:id="rId52"/>
-    <hyperlink ref="C130" r:id="rId53"/>
-    <hyperlink ref="C60" r:id="rId54"/>
-    <hyperlink ref="C91" r:id="rId55"/>
-    <hyperlink ref="C94" r:id="rId56"/>
-    <hyperlink ref="C127" r:id="rId57"/>
-    <hyperlink ref="C115" r:id="rId58"/>
-    <hyperlink ref="C149" r:id="rId59"/>
+    <hyperlink ref="C131" r:id="rId53"/>
+    <hyperlink ref="C61" r:id="rId54"/>
+    <hyperlink ref="C92" r:id="rId55"/>
+    <hyperlink ref="C95" r:id="rId56"/>
+    <hyperlink ref="C128" r:id="rId57"/>
+    <hyperlink ref="C116" r:id="rId58"/>
+    <hyperlink ref="C150" r:id="rId59"/>
     <hyperlink ref="C39" r:id="rId60"/>
-    <hyperlink ref="C163" r:id="rId61"/>
+    <hyperlink ref="C165" r:id="rId61"/>
     <hyperlink ref="C9" r:id="rId62"/>
     <hyperlink ref="C41" r:id="rId63"/>
-    <hyperlink ref="C165" r:id="rId64"/>
+    <hyperlink ref="C167" r:id="rId64"/>
     <hyperlink ref="C20" r:id="rId65"/>
-    <hyperlink ref="C177" r:id="rId66"/>
+    <hyperlink ref="C179" r:id="rId66"/>
     <hyperlink ref="C33" r:id="rId67"/>
     <hyperlink ref="C32" r:id="rId68"/>
     <hyperlink ref="C34" r:id="rId69"/>
-    <hyperlink ref="C65" r:id="rId70"/>
-    <hyperlink ref="C180" r:id="rId71"/>
+    <hyperlink ref="C66" r:id="rId70"/>
+    <hyperlink ref="C182" r:id="rId71"/>
     <hyperlink ref="C36" r:id="rId72"/>
-    <hyperlink ref="C134" r:id="rId73"/>
+    <hyperlink ref="C135" r:id="rId73"/>
     <hyperlink ref="C40" r:id="rId74"/>
-    <hyperlink ref="C57" r:id="rId75"/>
-    <hyperlink ref="C153" r:id="rId76"/>
-    <hyperlink ref="C54" r:id="rId77"/>
+    <hyperlink ref="C58" r:id="rId75"/>
+    <hyperlink ref="C154" r:id="rId76"/>
+    <hyperlink ref="C55" r:id="rId77"/>
     <hyperlink ref="C50" r:id="rId78"/>
-    <hyperlink ref="C81" r:id="rId79"/>
+    <hyperlink ref="C82" r:id="rId79"/>
     <hyperlink ref="C5" r:id="rId80"/>
-    <hyperlink ref="C80" r:id="rId81"/>
+    <hyperlink ref="C81" r:id="rId81"/>
     <hyperlink ref="C17" r:id="rId82"/>
-    <hyperlink ref="C125" r:id="rId83"/>
-    <hyperlink ref="C136" r:id="rId84"/>
-    <hyperlink ref="C167" r:id="rId85"/>
+    <hyperlink ref="C126" r:id="rId83"/>
+    <hyperlink ref="C137" r:id="rId84"/>
+    <hyperlink ref="C169" r:id="rId85"/>
     <hyperlink ref="C46" r:id="rId86"/>
-    <hyperlink ref="C178" r:id="rId87"/>
-    <hyperlink ref="C56" r:id="rId88"/>
-    <hyperlink ref="C184" r:id="rId89"/>
-    <hyperlink ref="C111" r:id="rId90"/>
-    <hyperlink ref="C78" r:id="rId91"/>
-    <hyperlink ref="C112" r:id="rId92"/>
-    <hyperlink ref="C156" r:id="rId93"/>
-    <hyperlink ref="C95" r:id="rId94"/>
-    <hyperlink ref="C117" r:id="rId95"/>
-    <hyperlink ref="C157" r:id="rId96"/>
-    <hyperlink ref="C74" r:id="rId97"/>
-    <hyperlink ref="C132" r:id="rId98"/>
-    <hyperlink ref="C58" r:id="rId99"/>
-    <hyperlink ref="C55" r:id="rId100"/>
-    <hyperlink ref="C98" r:id="rId101"/>
-    <hyperlink ref="C72" r:id="rId102"/>
+    <hyperlink ref="C180" r:id="rId87"/>
+    <hyperlink ref="C57" r:id="rId88"/>
+    <hyperlink ref="C186" r:id="rId89"/>
+    <hyperlink ref="C112" r:id="rId90"/>
+    <hyperlink ref="C79" r:id="rId91"/>
+    <hyperlink ref="C113" r:id="rId92"/>
+    <hyperlink ref="C157" r:id="rId93"/>
+    <hyperlink ref="C96" r:id="rId94"/>
+    <hyperlink ref="C118" r:id="rId95"/>
+    <hyperlink ref="C158" r:id="rId96"/>
+    <hyperlink ref="C75" r:id="rId97"/>
+    <hyperlink ref="C133" r:id="rId98"/>
+    <hyperlink ref="C59" r:id="rId99"/>
+    <hyperlink ref="C56" r:id="rId100"/>
+    <hyperlink ref="C99" r:id="rId101"/>
+    <hyperlink ref="C73" r:id="rId102"/>
     <hyperlink ref="C2" r:id="rId103"/>
-    <hyperlink ref="C92" r:id="rId104"/>
-    <hyperlink ref="C96" r:id="rId105"/>
-    <hyperlink ref="C122" r:id="rId106"/>
-    <hyperlink ref="C59" r:id="rId107"/>
-    <hyperlink ref="C99" r:id="rId108"/>
-    <hyperlink ref="C155" r:id="rId109"/>
+    <hyperlink ref="C93" r:id="rId104"/>
+    <hyperlink ref="C97" r:id="rId105"/>
+    <hyperlink ref="C123" r:id="rId106"/>
+    <hyperlink ref="C60" r:id="rId107"/>
+    <hyperlink ref="C100" r:id="rId108"/>
+    <hyperlink ref="C156" r:id="rId109"/>
     <hyperlink ref="C19" r:id="rId110"/>
     <hyperlink ref="C4" r:id="rId111"/>
-    <hyperlink ref="C183" r:id="rId112"/>
-    <hyperlink ref="C105" r:id="rId113"/>
-    <hyperlink ref="C100" r:id="rId114"/>
-    <hyperlink ref="C170" r:id="rId115"/>
-    <hyperlink ref="C148" r:id="rId116"/>
-    <hyperlink ref="C76" r:id="rId117"/>
-    <hyperlink ref="C114" r:id="rId118"/>
-    <hyperlink ref="C89" r:id="rId119"/>
-    <hyperlink ref="C186" r:id="rId120"/>
-    <hyperlink ref="C79" r:id="rId121"/>
-    <hyperlink ref="C146" r:id="rId122"/>
-    <hyperlink ref="C121" r:id="rId123"/>
-    <hyperlink ref="C93" r:id="rId124"/>
-    <hyperlink ref="C119" r:id="rId125"/>
-    <hyperlink ref="C154" r:id="rId126"/>
-    <hyperlink ref="C103" r:id="rId127"/>
+    <hyperlink ref="C185" r:id="rId112"/>
+    <hyperlink ref="C106" r:id="rId113"/>
+    <hyperlink ref="C101" r:id="rId114"/>
+    <hyperlink ref="C172" r:id="rId115"/>
+    <hyperlink ref="C149" r:id="rId116"/>
+    <hyperlink ref="C77" r:id="rId117"/>
+    <hyperlink ref="C115" r:id="rId118"/>
+    <hyperlink ref="C90" r:id="rId119"/>
+    <hyperlink ref="C188" r:id="rId120"/>
+    <hyperlink ref="C80" r:id="rId121"/>
+    <hyperlink ref="C147" r:id="rId122"/>
+    <hyperlink ref="C122" r:id="rId123"/>
+    <hyperlink ref="C94" r:id="rId124"/>
+    <hyperlink ref="C120" r:id="rId125"/>
+    <hyperlink ref="C155" r:id="rId126"/>
+    <hyperlink ref="C104" r:id="rId127"/>
     <hyperlink ref="C16" r:id="rId128"/>
     <hyperlink ref="C25" r:id="rId129"/>
-    <hyperlink ref="C145" r:id="rId130"/>
-    <hyperlink ref="C88" r:id="rId131"/>
-    <hyperlink ref="C162" r:id="rId132"/>
-    <hyperlink ref="C142" r:id="rId133"/>
-    <hyperlink ref="C141" r:id="rId134"/>
-    <hyperlink ref="C143" r:id="rId135"/>
-    <hyperlink ref="C169" r:id="rId136"/>
-    <hyperlink ref="C160" r:id="rId137"/>
-    <hyperlink ref="C176" r:id="rId138"/>
+    <hyperlink ref="C146" r:id="rId130"/>
+    <hyperlink ref="C89" r:id="rId131"/>
+    <hyperlink ref="C164" r:id="rId132"/>
+    <hyperlink ref="C143" r:id="rId133"/>
+    <hyperlink ref="C142" r:id="rId134"/>
+    <hyperlink ref="C144" r:id="rId135"/>
+    <hyperlink ref="C171" r:id="rId136"/>
+    <hyperlink ref="C162" r:id="rId137"/>
+    <hyperlink ref="C178" r:id="rId138"/>
     <hyperlink ref="C48" r:id="rId139"/>
-    <hyperlink ref="C104" r:id="rId140"/>
+    <hyperlink ref="C105" r:id="rId140"/>
     <hyperlink ref="J2" r:id="rId141"/>
     <hyperlink ref="M3" r:id="rId142"/>
     <hyperlink ref="J3" r:id="rId143"/>
@@ -6437,64 +6531,64 @@
     <hyperlink ref="J4" r:id="rId145"/>
     <hyperlink ref="P5" r:id="rId146"/>
     <hyperlink ref="J5" r:id="rId147"/>
-    <hyperlink ref="C124" r:id="rId148"/>
+    <hyperlink ref="C125" r:id="rId148"/>
     <hyperlink ref="C43" r:id="rId149"/>
     <hyperlink ref="P7" r:id="rId150"/>
     <hyperlink ref="J7" r:id="rId151"/>
     <hyperlink ref="M8" r:id="rId152"/>
     <hyperlink ref="L8" r:id="rId153"/>
     <hyperlink ref="J8" r:id="rId154"/>
-    <hyperlink ref="C174" r:id="rId155"/>
-    <hyperlink ref="N174" r:id="rId156"/>
+    <hyperlink ref="C176" r:id="rId155"/>
+    <hyperlink ref="N176" r:id="rId156"/>
     <hyperlink ref="C27" r:id="rId157"/>
     <hyperlink ref="N27" r:id="rId158"/>
-    <hyperlink ref="C75" r:id="rId159"/>
-    <hyperlink ref="C168" r:id="rId160"/>
-    <hyperlink ref="J168" r:id="rId161"/>
-    <hyperlink ref="C166" r:id="rId162"/>
-    <hyperlink ref="N166" r:id="rId163"/>
-    <hyperlink ref="J166" r:id="rId164"/>
-    <hyperlink ref="C108" r:id="rId165"/>
-    <hyperlink ref="C106" r:id="rId166"/>
+    <hyperlink ref="C76" r:id="rId159"/>
+    <hyperlink ref="C170" r:id="rId160"/>
+    <hyperlink ref="J170" r:id="rId161"/>
+    <hyperlink ref="C168" r:id="rId162"/>
+    <hyperlink ref="N168" r:id="rId163"/>
+    <hyperlink ref="J168" r:id="rId164"/>
+    <hyperlink ref="C109" r:id="rId165"/>
+    <hyperlink ref="C107" r:id="rId166"/>
     <hyperlink ref="C51" r:id="rId167"/>
     <hyperlink ref="J51" r:id="rId168"/>
     <hyperlink ref="K51" r:id="rId169"/>
-    <hyperlink ref="C116" r:id="rId170"/>
-    <hyperlink ref="N116" r:id="rId171"/>
-    <hyperlink ref="C90" r:id="rId172"/>
-    <hyperlink ref="K90" r:id="rId173"/>
-    <hyperlink ref="C181" r:id="rId174"/>
-    <hyperlink ref="C137" r:id="rId175"/>
-    <hyperlink ref="K137" r:id="rId176"/>
+    <hyperlink ref="C117" r:id="rId170"/>
+    <hyperlink ref="N117" r:id="rId171"/>
+    <hyperlink ref="C91" r:id="rId172"/>
+    <hyperlink ref="K91" r:id="rId173"/>
+    <hyperlink ref="C183" r:id="rId174"/>
+    <hyperlink ref="C138" r:id="rId175"/>
+    <hyperlink ref="K138" r:id="rId176"/>
     <hyperlink ref="L9" r:id="rId177"/>
     <hyperlink ref="J9" r:id="rId178"/>
     <hyperlink ref="J11" r:id="rId179"/>
-    <hyperlink ref="C150" r:id="rId180"/>
-    <hyperlink ref="J150" r:id="rId181"/>
-    <hyperlink ref="L150" r:id="rId182"/>
-    <hyperlink ref="K150" r:id="rId183"/>
-    <hyperlink ref="C151" r:id="rId184"/>
-    <hyperlink ref="J151" r:id="rId185"/>
-    <hyperlink ref="K151" r:id="rId186"/>
-    <hyperlink ref="L151" r:id="rId187"/>
-    <hyperlink ref="C77" r:id="rId188"/>
-    <hyperlink ref="J77" r:id="rId189"/>
-    <hyperlink ref="N77" r:id="rId190"/>
-    <hyperlink ref="C158" r:id="rId191"/>
-    <hyperlink ref="C109" r:id="rId192"/>
-    <hyperlink ref="J109" r:id="rId193"/>
-    <hyperlink ref="L109" r:id="rId194"/>
-    <hyperlink ref="C86" r:id="rId195"/>
-    <hyperlink ref="C61" r:id="rId196"/>
-    <hyperlink ref="L61" r:id="rId197"/>
-    <hyperlink ref="K61" r:id="rId198"/>
-    <hyperlink ref="J61" r:id="rId199"/>
-    <hyperlink ref="C83" r:id="rId200"/>
-    <hyperlink ref="J83" r:id="rId201"/>
-    <hyperlink ref="K83" r:id="rId202"/>
-    <hyperlink ref="L83" r:id="rId203"/>
-    <hyperlink ref="C139" r:id="rId204"/>
-    <hyperlink ref="N139" r:id="rId205"/>
+    <hyperlink ref="C151" r:id="rId180"/>
+    <hyperlink ref="J151" r:id="rId181"/>
+    <hyperlink ref="L151" r:id="rId182"/>
+    <hyperlink ref="K151" r:id="rId183"/>
+    <hyperlink ref="C152" r:id="rId184"/>
+    <hyperlink ref="J152" r:id="rId185"/>
+    <hyperlink ref="K152" r:id="rId186"/>
+    <hyperlink ref="L152" r:id="rId187"/>
+    <hyperlink ref="C78" r:id="rId188"/>
+    <hyperlink ref="J78" r:id="rId189"/>
+    <hyperlink ref="N78" r:id="rId190"/>
+    <hyperlink ref="C160" r:id="rId191"/>
+    <hyperlink ref="C110" r:id="rId192"/>
+    <hyperlink ref="J110" r:id="rId193"/>
+    <hyperlink ref="L110" r:id="rId194"/>
+    <hyperlink ref="C87" r:id="rId195"/>
+    <hyperlink ref="C62" r:id="rId196"/>
+    <hyperlink ref="L62" r:id="rId197"/>
+    <hyperlink ref="K62" r:id="rId198"/>
+    <hyperlink ref="J62" r:id="rId199"/>
+    <hyperlink ref="C84" r:id="rId200"/>
+    <hyperlink ref="J84" r:id="rId201"/>
+    <hyperlink ref="K84" r:id="rId202"/>
+    <hyperlink ref="L84" r:id="rId203"/>
+    <hyperlink ref="C140" r:id="rId204"/>
+    <hyperlink ref="N140" r:id="rId205"/>
     <hyperlink ref="C47" r:id="rId206"/>
     <hyperlink ref="K47" r:id="rId207"/>
     <hyperlink ref="J47" r:id="rId208"/>
@@ -6502,47 +6596,47 @@
     <hyperlink ref="J10" r:id="rId210"/>
     <hyperlink ref="P10" r:id="rId211"/>
     <hyperlink ref="N10" r:id="rId212"/>
-    <hyperlink ref="C52" r:id="rId213"/>
-    <hyperlink ref="J52" r:id="rId214"/>
-    <hyperlink ref="K52" r:id="rId215"/>
-    <hyperlink ref="L52" r:id="rId216"/>
-    <hyperlink ref="M52" r:id="rId217"/>
-    <hyperlink ref="N52" r:id="rId218"/>
+    <hyperlink ref="C53" r:id="rId213"/>
+    <hyperlink ref="J53" r:id="rId214"/>
+    <hyperlink ref="K53" r:id="rId215"/>
+    <hyperlink ref="L53" r:id="rId216"/>
+    <hyperlink ref="M53" r:id="rId217"/>
+    <hyperlink ref="N53" r:id="rId218"/>
     <hyperlink ref="C28" r:id="rId219"/>
-    <hyperlink ref="C173" r:id="rId220"/>
+    <hyperlink ref="C175" r:id="rId220"/>
     <hyperlink ref="C44" r:id="rId221"/>
     <hyperlink ref="J44" r:id="rId222"/>
     <hyperlink ref="N44" r:id="rId223"/>
     <hyperlink ref="L44" r:id="rId224"/>
     <hyperlink ref="K44" r:id="rId225"/>
-    <hyperlink ref="C171" r:id="rId226"/>
-    <hyperlink ref="P171" r:id="rId227"/>
-    <hyperlink ref="C118" r:id="rId228"/>
-    <hyperlink ref="C135" r:id="rId229"/>
-    <hyperlink ref="P135" r:id="rId230"/>
-    <hyperlink ref="C82" r:id="rId231"/>
-    <hyperlink ref="J82" r:id="rId232"/>
-    <hyperlink ref="K82" r:id="rId233"/>
-    <hyperlink ref="N82" r:id="rId234"/>
-    <hyperlink ref="C147" r:id="rId235"/>
-    <hyperlink ref="J147" r:id="rId236"/>
-    <hyperlink ref="L147" r:id="rId237"/>
+    <hyperlink ref="C173" r:id="rId226"/>
+    <hyperlink ref="P173" r:id="rId227"/>
+    <hyperlink ref="C119" r:id="rId228"/>
+    <hyperlink ref="C136" r:id="rId229"/>
+    <hyperlink ref="P136" r:id="rId230"/>
+    <hyperlink ref="C83" r:id="rId231"/>
+    <hyperlink ref="J83" r:id="rId232"/>
+    <hyperlink ref="K83" r:id="rId233"/>
+    <hyperlink ref="N83" r:id="rId234"/>
+    <hyperlink ref="C148" r:id="rId235"/>
+    <hyperlink ref="J148" r:id="rId236"/>
+    <hyperlink ref="L148" r:id="rId237"/>
     <hyperlink ref="C42" r:id="rId238"/>
     <hyperlink ref="C29" r:id="rId239"/>
     <hyperlink ref="J29" r:id="rId240"/>
     <hyperlink ref="P29" r:id="rId241"/>
-    <hyperlink ref="C131" r:id="rId242"/>
-    <hyperlink ref="N131" r:id="rId243"/>
-    <hyperlink ref="J131" r:id="rId244"/>
-    <hyperlink ref="C164" r:id="rId245"/>
-    <hyperlink ref="J164" r:id="rId246"/>
-    <hyperlink ref="C123" r:id="rId247"/>
+    <hyperlink ref="C132" r:id="rId242"/>
+    <hyperlink ref="N132" r:id="rId243"/>
+    <hyperlink ref="J132" r:id="rId244"/>
+    <hyperlink ref="C166" r:id="rId245"/>
+    <hyperlink ref="J166" r:id="rId246"/>
+    <hyperlink ref="C124" r:id="rId247"/>
     <hyperlink ref="C18" r:id="rId248"/>
     <hyperlink ref="J18" r:id="rId249"/>
     <hyperlink ref="P18" r:id="rId250"/>
-    <hyperlink ref="C152" r:id="rId251"/>
-    <hyperlink ref="J152" r:id="rId252"/>
-    <hyperlink ref="P152" r:id="rId253"/>
+    <hyperlink ref="C153" r:id="rId251"/>
+    <hyperlink ref="J153" r:id="rId252"/>
+    <hyperlink ref="P153" r:id="rId253"/>
     <hyperlink ref="C14" r:id="rId254"/>
     <hyperlink ref="C12" r:id="rId255"/>
     <hyperlink ref="C13" r:id="rId256"/>
@@ -6555,7 +6649,12 @@
     <hyperlink ref="J12" r:id="rId263"/>
     <hyperlink ref="M15" r:id="rId264"/>
     <hyperlink ref="J15" r:id="rId265"/>
-    <hyperlink ref="J91" r:id="rId266"/>
+    <hyperlink ref="J92" r:id="rId266"/>
+    <hyperlink ref="C159" r:id="rId267"/>
+    <hyperlink ref="C52" r:id="rId268"/>
+    <hyperlink ref="J52" r:id="rId269"/>
+    <hyperlink ref="L52" r:id="rId270"/>
+    <hyperlink ref="N52" r:id="rId271"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
add 'Domestic Terrorist Victims dataset', 'Konstanz One-Sided Violence Event Dataset' and 'Ill-Treatment and Torture'
</commit_message>
<xml_diff>
--- a/PolData.xlsx
+++ b/PolData.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1107" uniqueCount="605">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1131" uniqueCount="619">
   <si>
     <t>name</t>
   </si>
@@ -1842,6 +1842,48 @@
   </si>
   <si>
     <t>http://ps.au.dk/fileadmin/Statskundskab/Dokumenter/Forskning/Forskningscentre/DEDERE/CLD_cow.xls</t>
+  </si>
+  <si>
+    <t>Ill-Treatment and Torture</t>
+  </si>
+  <si>
+    <t>http://faculty.ucmerced.edu/cconrad2/Academic/Data.html</t>
+  </si>
+  <si>
+    <t>Human rights, torture</t>
+  </si>
+  <si>
+    <t>http://faculty.ucmerced.edu/cconrad2/Academic/Data_files/CY.zip</t>
+  </si>
+  <si>
+    <t>http://faculty.ucmerced.edu/cconrad2/Academic/Data_files/ITT_CY_UsersGuide19July11.pdf</t>
+  </si>
+  <si>
+    <t>Konstanz One-Sided Violence Event Dataset</t>
+  </si>
+  <si>
+    <t>https://cms.uni-konstanz.de/fileadmin/archive/kosved/polver/gschneider/forschung/kosved/data/</t>
+  </si>
+  <si>
+    <t>Mass killings, massacres, one-sided violence, political violence</t>
+  </si>
+  <si>
+    <t>https://cms.uni-konstanz.de/fileadmin/polver/gschneider/KOSVED/Coders_and_sources_kosved_webappendix_20130527.pdf</t>
+  </si>
+  <si>
+    <t>https://cms.uni-konstanz.de/fileadmin/polver/gschneider/KOSVED/KOSVED_Gesamtdatensatz_20130529_ohneGIS.xlsx</t>
+  </si>
+  <si>
+    <t>http://hdl.handle.net/1902.1/14717</t>
+  </si>
+  <si>
+    <t>Political violence, target selection, terrorism, victims</t>
+  </si>
+  <si>
+    <t>Western Europe</t>
+  </si>
+  <si>
+    <t>Domestic Terrorist Victims dataset</t>
   </si>
 </sst>
 </file>
@@ -2181,10 +2223,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q191"/>
+  <dimension ref="A1:Q194"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A161" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" topLeftCell="A166" workbookViewId="0">
+      <selection activeCell="B200" sqref="B200"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3682,22 +3724,25 @@
     </row>
     <row r="59" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>594</v>
+        <v>618</v>
       </c>
       <c r="B59" t="s">
-        <v>259</v>
+        <v>40</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>593</v>
+        <v>615</v>
       </c>
       <c r="D59" t="s">
-        <v>595</v>
+        <v>616</v>
       </c>
       <c r="E59" t="s">
-        <v>10</v>
+        <v>617</v>
       </c>
       <c r="F59">
-        <v>1945</v>
+        <v>1965</v>
+      </c>
+      <c r="G59">
+        <v>2005</v>
       </c>
       <c r="H59" t="s">
         <v>348</v>
@@ -3708,67 +3753,76 @@
     </row>
     <row r="60" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>219</v>
+        <v>594</v>
       </c>
       <c r="B60" t="s">
-        <v>124</v>
+        <v>259</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>218</v>
+        <v>593</v>
+      </c>
+      <c r="D60" t="s">
+        <v>595</v>
+      </c>
+      <c r="E60" t="s">
+        <v>10</v>
       </c>
       <c r="F60">
-        <v>1970</v>
-      </c>
-      <c r="G60">
-        <v>2015</v>
+        <v>1945</v>
       </c>
       <c r="H60" t="s">
-        <v>16</v>
+        <v>348</v>
       </c>
       <c r="I60" t="s">
-        <v>20</v>
+        <v>349</v>
       </c>
     </row>
     <row r="61" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>191</v>
+        <v>219</v>
       </c>
       <c r="B61" t="s">
-        <v>25</v>
+        <v>124</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="E61" t="s">
-        <v>192</v>
+        <v>218</v>
+      </c>
+      <c r="F61">
+        <v>1970</v>
+      </c>
+      <c r="G61">
+        <v>2015</v>
+      </c>
+      <c r="H61" t="s">
+        <v>16</v>
+      </c>
+      <c r="I61" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="62" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>235</v>
+        <v>191</v>
       </c>
       <c r="B62" t="s">
-        <v>60</v>
+        <v>25</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>236</v>
-      </c>
-      <c r="H62" t="s">
-        <v>16</v>
-      </c>
-      <c r="I62" t="s">
-        <v>20</v>
+        <v>190</v>
+      </c>
+      <c r="E62" t="s">
+        <v>192</v>
       </c>
     </row>
     <row r="63" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>252</v>
+        <v>235</v>
       </c>
       <c r="B63" t="s">
-        <v>250</v>
+        <v>60</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>251</v>
+        <v>236</v>
       </c>
       <c r="H63" t="s">
         <v>16</v>
@@ -3779,129 +3833,129 @@
     </row>
     <row r="64" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>149</v>
+        <v>252</v>
       </c>
       <c r="B64" t="s">
-        <v>128</v>
+        <v>250</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>150</v>
+        <v>251</v>
+      </c>
+      <c r="H64" t="s">
+        <v>16</v>
+      </c>
+      <c r="I64" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="65" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>462</v>
+        <v>149</v>
       </c>
       <c r="B65" t="s">
-        <v>250</v>
+        <v>128</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>464</v>
-      </c>
-      <c r="D65" t="s">
-        <v>463</v>
-      </c>
-      <c r="E65" t="s">
-        <v>14</v>
-      </c>
-      <c r="F65">
-        <v>1946</v>
-      </c>
-      <c r="G65">
-        <v>2010</v>
-      </c>
-      <c r="H65" t="s">
-        <v>348</v>
-      </c>
-      <c r="I65" t="s">
-        <v>349</v>
-      </c>
-      <c r="J65" s="2" t="s">
-        <v>467</v>
-      </c>
-      <c r="K65" s="2" t="s">
-        <v>466</v>
-      </c>
-      <c r="L65" s="2" t="s">
-        <v>465</v>
+        <v>150</v>
       </c>
     </row>
     <row r="66" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>28</v>
+        <v>462</v>
       </c>
       <c r="B66" t="s">
-        <v>25</v>
+        <v>250</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>48</v>
+        <v>464</v>
+      </c>
+      <c r="D66" t="s">
+        <v>463</v>
+      </c>
+      <c r="E66" t="s">
+        <v>14</v>
+      </c>
+      <c r="F66">
+        <v>1946</v>
+      </c>
+      <c r="G66">
+        <v>2010</v>
+      </c>
+      <c r="H66" t="s">
+        <v>348</v>
+      </c>
+      <c r="I66" t="s">
+        <v>349</v>
+      </c>
+      <c r="J66" s="2" t="s">
+        <v>467</v>
+      </c>
+      <c r="K66" s="2" t="s">
+        <v>466</v>
+      </c>
+      <c r="L66" s="2" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="67" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>80</v>
+        <v>28</v>
       </c>
       <c r="B67" t="s">
-        <v>128</v>
+        <v>25</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="E67" t="s">
-        <v>9</v>
-      </c>
-      <c r="F67">
-        <v>1979</v>
+        <v>48</v>
       </c>
     </row>
     <row r="68" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>125</v>
+        <v>80</v>
       </c>
       <c r="B68" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>126</v>
+        <v>81</v>
+      </c>
+      <c r="E68" t="s">
+        <v>9</v>
+      </c>
+      <c r="F68">
+        <v>1979</v>
       </c>
     </row>
     <row r="69" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>179</v>
+        <v>125</v>
       </c>
       <c r="B69" t="s">
-        <v>165</v>
+        <v>124</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>180</v>
+        <v>126</v>
       </c>
     </row>
     <row r="70" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
+        <v>179</v>
+      </c>
+      <c r="B70" t="s">
+        <v>165</v>
+      </c>
+      <c r="C70" s="2" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="71" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A71" t="s">
         <v>78</v>
       </c>
-      <c r="B70" t="s">
+      <c r="B71" t="s">
         <v>25</v>
       </c>
-      <c r="C70" s="2" t="s">
+      <c r="C71" s="2" t="s">
         <v>79</v>
-      </c>
-      <c r="E70" t="s">
-        <v>9</v>
-      </c>
-      <c r="F70">
-        <v>1979</v>
-      </c>
-    </row>
-    <row r="71" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A71" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="B71" t="s">
-        <v>83</v>
-      </c